<commit_message>
residues forces added with contributions
</commit_message>
<xml_diff>
--- a/results_test/forces/force_results.xlsx
+++ b/results_test/forces/force_results.xlsx
@@ -467,7 +467,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>{6500: {'frame': 6500, 'ionic_force': [10.081943392753601, 8.897971272468567, -2.1222930885851383], 'ionic_force_magnitude': 13.613361204868552, 'motion_vector': [0.8403472900390625, -0.8082695007324219, 0.09564208984375], 'ionic_force_x': 10.081943392753601, 'ionic_force_y': 8.897971272468567, 'ionic_force_z': -2.1222930885851383, 'radial_force': 13.446913227219245, 'axial_force': -2.1222930885851383, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-0.4597816467285156, 6.867312431335449, 4.928182125091553], 'asn_force_magnitude': 8.465126003215468, 'residue_force': [-0.4597816467285156, 6.867312431335449, 4.928182125091553], 'residue_force_magnitude': 8.465126003215468, 'total_force': [9.622161746025085, 15.765283703804016, 2.8058890365064144], 'total_force_magnitude': 18.6816268085326, 'motion_component_total': -3.751035137079949, 'cosine_total_motion': -0.20078739263578002, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.5519086046032223, 'cosine_residue_motion': -0.5519086046032223, 'cosine_ionic_motion': 0.06764976917058485, 'motion_component_glu': None, 'motion_component_asn': -4.6719758802251015, 'motion_component_residue': -4.6719758802251015, 'motion_component_ionic': 0.9209407431451524}, 6501: {'frame': 6501, 'ionic_force': [10.483401715755463, 8.962290167808533, -2.592883415520191], 'ionic_force_magnitude': 14.033794960465316, 'motion_vector': [-0.46063232421875, -0.98577880859375, -0.43386077880859375], 'ionic_force_x': 10.483401715755463, 'ionic_force_y': 8.962290167808533, 'ionic_force_z': -2.592883415520191, 'radial_force': 13.79218461977297, 'axial_force': -2.592883415520191, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [1.1594171524047852, 8.153244018554688, 8.414933681488037], 'asn_force_magnitude': 11.774155809366123, 'residue_force': [1.1594171524047852, 8.153244018554688, 8.414933681488037], 'residue_force_magnitude': 11.774155809366123, 'total_force': [11.642818868160248, 17.11553418636322, 5.822050265967846], 'total_force_magnitude': 21.50332557956589, 'motion_component_total': -21.138089026666297, 'cosine_total_motion': -0.9830148805798361, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.8861699521672649, 'cosine_residue_motion': -0.8861699521672649, 'cosine_ionic_motion': -0.762743503551621, 'motion_component_glu': None, 'motion_component_asn': -10.433903090395901, 'motion_component_residue': -10.433903090395901, 'motion_component_ionic': -10.704185936270399}, 6502: {'frame': 6502, 'ionic_force': [11.625001519918442, 8.640661865472794, -4.613270275294781], 'ionic_force_magnitude': 15.201445998471996, 'motion_vector': [-0.4776763916015625, 0.31816864013671875, -0.33734130859375], 'ionic_force_x': 11.625001519918442, 'ionic_force_y': 8.640661865472794, 'ionic_force_z': -4.613270275294781, 'radial_force': 14.484533054660128, 'axial_force': -4.613270275294781, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [4.454033255577087, -0.38120079040527344, 29.511417388916016], 'asn_force_magnitude': 29.848073347993616, 'residue_force': [4.454033255577087, -0.38120079040527344, 29.511417388916016], 'residue_force_magnitude': 29.848073347993616, 'total_force': [16.07903477549553, 8.25946107506752, 24.898147113621235], 'total_force_magnitude': 30.768031887881218, 'motion_component_total': -20.20596221345819, 'cosine_total_motion': -0.656719360116655, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.6141775272041401, 'cosine_residue_motion': -0.6141775272041401, 'cosine_ionic_motion': -0.1232742156876414, 'motion_component_glu': None, 'motion_component_asn': -18.33201588067852, 'motion_component_residue': -18.33201588067852, 'motion_component_ionic': -1.8739463327796702}, 6503: {'frame': 6503, 'ionic_force': [11.245525449514389, 9.056975394487381, -5.633130311965942], 'ionic_force_magnitude': 15.499122653996102, 'motion_vector': [0.24894332885742188, 0.13856887817382812, -0.48906707763671875], 'ionic_force_x': 11.245525449514389, 'ionic_force_y': 9.056975394487381, 'ionic_force_z': -5.633130311965942, 'radial_force': 14.439205169676953, 'axial_force': -5.633130311965942, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-17.786433219909668, 19.308142960071564, 38.5463604927063], 'asn_force_magnitude': 46.63671835031423, 'residue_force': [-17.786433219909668, 19.308142960071564, 38.5463604927063], 'residue_force_magnitude': 46.63671835031423, 'total_force': [-6.540907770395279, 28.365118354558945, 32.913230180740356], 'total_force_magnitude': 43.93909574239497, 'motion_component_total': -24.37185294337288, 'cosine_total_motion': -0.5546735209631889, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.7805581220149096, 'cosine_residue_motion': -0.7805581220149096, 'cosine_ionic_motion': 0.7762256366159407, 'motion_component_glu': None, 'motion_component_asn': -36.40266929245955, 'motion_component_residue': -36.40266929245955, 'motion_component_ionic': 12.030816349086672}, 6504: {'frame': 6504, 'ionic_force': [9.827082574367523, 8.00064042210579, -3.6161573603749275], 'ionic_force_magnitude': 13.177951022153053, 'motion_vector': [-1.3946723937988281, 1.9302940368652344, 2.1039581298828125], 'ionic_force_x': 9.827082574367523, 'ionic_force_y': 8.00064042210579, 'ionic_force_z': -3.6161573603749275, 'radial_force': 12.672087400553664, 'axial_force': -3.6161573603749275, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-17.627061367034912, 83.77625507116318, 67.12841844558716], 'asn_force_magnitude': 108.79061893928012, 'residue_force': [-17.627061367034912, 83.77625507116318, 67.12841844558716], 'residue_force_magnitude': 108.79061893928012, 'total_force': [-7.799978792667389, 91.77689549326897, 63.51226108521223], 'total_force_magnitude': 111.88228422634496, 'motion_component_total': 101.22472079757716, 'cosine_total_motion': 0.9047430654239516, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.9474349623830411, 'cosine_residue_motion': 0.9474349623830411, 'cosine_ionic_motion': -0.14018227580919085, 'motion_component_glu': None, 'motion_component_asn': 103.07203596236462, 'motion_component_residue': 103.07203596236462, 'motion_component_ionic': -1.8473151647874677}, 6505: {'frame': 6505, 'ionic_force': [8.954921334981918, 11.337874412536621, 0.06668257713317871], 'ionic_force_magnitude': 14.44792230309466, 'motion_vector': [1.2258834838867188, -0.9209442138671875, -0.31507110595703125], 'ionic_force_x': 8.954921334981918, 'ionic_force_y': 11.337874412536621, 'ionic_force_z': 0.06668257713317871, 'radial_force': 14.447768419730675, 'axial_force': 0.06668257713317871, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-0.48206377029418945, 0.9736707210540771, 0.43469953536987305], 'asn_force_magnitude': 1.1702067499886502, 'residue_force': [-0.48206377029418945, 0.9736707210540771, 0.43469953536987305], 'residue_force_magnitude': 1.1702067499886502, 'total_force': [8.472857564687729, 12.311545133590698, 0.5013821125030518], 'total_force_magnitude': 14.953756815953136, 'motion_component_total': -0.7087932192891095, 'cosine_total_motion': -0.047399006685259634, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.8869239070081387, 'cosine_residue_motion': -0.8869239070081387, 'cosine_ionic_motion': 0.022777747313025818, 'motion_component_glu': None, 'motion_component_asn': -1.0378843427072297, 'motion_component_residue': -1.0378843427072297, 'motion_component_ionic': 0.3290911234181202}, 6506: {'frame': 6506, 'ionic_force': [8.623957127332687, 13.234449625015259, -0.3938300022855401], 'ionic_force_magnitude': 15.801215000177645, 'motion_vector': [0.202423095703125, -0.7250022888183594, -0.397186279296875], 'ionic_force_x': 8.623957127332687, 'ionic_force_y': 13.234449625015259, 'ionic_force_z': -0.3938300022855401, 'radial_force': 15.796306321768352, 'axial_force': -0.3938300022855401, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-0.8118951320648193, 4.410116195678711, 5.561502456665039], 'asn_force_magnitude': 7.144131027658261, 'residue_force': [-0.8118951320648193, 4.410116195678711, 5.561502456665039], 'residue_force_magnitude': 7.144131027658261, 'total_force': [7.812061995267868, 17.64456582069397, 5.167672454379499], 'total_force_magnitude': 19.976582646049927, 'motion_component_total': -15.584111210437268, 'cosine_total_motion': -0.7801189766318112, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.9161753387152256, 'cosine_residue_motion': -0.9161753387152256, 'cosine_ionic_motion': -0.5720341471364631, 'motion_component_glu': None, 'motion_component_asn': -6.5452766640907605, 'motion_component_residue': -6.5452766640907605, 'motion_component_ionic': -9.038834546346507}, 6507: {'frame': 6507, 'ionic_force': [7.709233731031418, 10.224741041660309, -1.3882663855329156], 'ionic_force_magnitude': 12.88040751086261, 'motion_vector': [-0.5508842468261719, 0.7071418762207031, 0.5803451538085938], 'ionic_force_x': 7.709233731031418, 'ionic_force_y': 10.224741041660309, 'ionic_force_z': -1.3882663855329156, 'radial_force': 12.805374422041917, 'axial_force': -1.3882663855329156, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-1.127873182296753, 5.707294940948486, 11.358274936676025], 'asn_force_magnitude': 12.761493760349655, 'residue_force': [-1.127873182296753, 5.707294940948486, 11.358274936676025], 'residue_force_magnitude': 12.761493760349655, 'total_force': [6.581360548734665, 15.932035982608795, 9.97000855114311], 'total_force_magnitude': 19.9134413834839, 'motion_component_total': 12.573460355545087, 'cosine_total_motion': 0.631405697961049, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.8254580715079681, 'cosine_residue_motion': 0.8254580715079681, 'cosine_ionic_motion': 0.15833212767887905, 'motion_component_glu': None, 'motion_component_asn': 10.534078028979195, 'motion_component_residue': 10.534078028979195, 'motion_component_ionic': 2.0393823265658915}, 6508: {'frame': 6508, 'ionic_force': [8.196878910064697, 9.545158743858337, -0.845391895622015], 'ionic_force_magnitude': 12.61005815882314, 'motion_vector': [0.4479179382324219, -0.00655364990234375, -0.4083099365234375], 'ionic_force_x': 8.196878910064697, 'ionic_force_y': 9.545158743858337, 'ionic_force_z': -0.845391895622015, 'radial_force': 12.581688253637454, 'axial_force': -0.845391895622015, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-1.3246822357177734, 3.438356876373291, 5.006871700286865], 'asn_force_magnitude': 6.216578259626691, 'residue_force': [-1.3246822357177734, 3.438356876373291, 5.006871700286865], 'residue_force_magnitude': 6.216578259626691, 'total_force': [6.872196674346924, 12.983515620231628, 4.16147980466485], 'total_force_magnitude': 15.26815899695628, 'motion_component_total': 2.1347279550177696, 'cosine_total_motion': 0.13981567492474561, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.7060007510426008, 'cosine_residue_motion': -0.7060007510426008, 'cosine_ionic_motion': 0.5173359863265016, 'motion_component_glu': None, 'motion_component_asn': -4.3889089202115485, 'motion_component_residue': -4.3889089202115485, 'motion_component_ionic': 6.523636875229318}, 6509: {'frame': 6509, 'ionic_force': [8.639953941106796, 9.225626945495605, -1.5821315441280603], 'ionic_force_magnitude': 12.738294111254712, 'motion_vector': [0.6326484680175781, 0.24243927001953125, -0.14005279541015625], 'ionic_force_x': 8.639953941106796, 'ionic_force_y': 9.225626945495605, 'ionic_force_z': -1.5821315441280603, 'radial_force': 12.639659672708813, 'axial_force': -1.5821315441280603, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-0.6517491340637207, 5.48417067527771, 6.172529220581055], 'asn_force_magnitude': 8.282573386831881, 'residue_force': [-0.6517491340637207, 5.48417067527771, 6.172529220581055], 'residue_force_magnitude': 8.282573386831881, 'total_force': [7.988204807043076, 14.709797620773315, 4.590397676452994], 'total_force_magnitude': 17.35688085202406, 'motion_component_total': 11.53029283891268, 'cosine_total_motion': 0.6643067344423284, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.009209195305889378, 'cosine_residue_motion': 0.009209195305889378, 'cosine_ionic_motion': 0.899179819756083, 'motion_component_glu': None, 'motion_component_asn': 0.07627583595469645, 'motion_component_residue': 0.07627583595469645, 'motion_component_ionic': 11.454017002957984}, 6510: {'frame': 6510, 'ionic_force': [8.169408738613129, 10.510639429092407, -0.9569092690944672], 'ionic_force_magnitude': 13.34647727665242, 'motion_vector': [-0.5427474975585938, -0.5374031066894531, -0.217681884765625], 'ionic_force_x': 8.169408738613129, 'ionic_force_y': 10.510639429092407, 'ionic_force_z': -0.9569092690944672, 'radial_force': 13.312129068895047, 'axial_force': -0.9569092690944672, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [1.0689871311187744, 6.226802349090576, 4.6353254318237305], 'asn_force_magnitude': 7.835945561325023, 'residue_force': [1.0689871311187744, 6.226802349090576, 4.6353254318237305], 'residue_force_magnitude': 7.835945561325023, 'total_force': [9.238395869731903, 16.737441778182983, 3.6784161627292633], 'total_force_magnitude': 19.468452968589276, 'motion_component_total': -18.64705599815435, 'cosine_total_motion': -0.9578088216993831, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.7930646120050037, 'cosine_residue_motion': -0.7930646120050037, 'cosine_ionic_motion': -0.9315300670101739, 'motion_component_glu': None, 'motion_component_asn': -6.21441112628456, 'motion_component_residue': -6.21441112628456, 'motion_component_ionic': -12.432644871869792}, 6511: {'frame': 6511, 'ionic_force': [9.239876329898834, 10.888403356075287, -0.996029619127512], 'ionic_force_magnitude': 14.315191833803542, 'motion_vector': [-0.13922500610351562, -0.4607810974121094, -0.42333984375], 'ionic_force_x': 9.239876329898834, 'ionic_force_y': 10.888403356075287, 'ionic_force_z': -0.996029619127512, 'radial_force': 14.280498669038709, 'axial_force': -0.996029619127512, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-0.5281887054443359, 8.032324314117432, 9.187541007995605], 'asn_force_magnitude': 12.215077853592335, 'residue_force': [-0.5281887054443359, 8.032324314117432, 9.187541007995605], 'residue_force_magnitude': 12.215077853592335, 'total_force': [8.711687624454498, 18.92072767019272, 8.191511388868093], 'total_force_magnitude': 22.382767828613726, 'motion_component_total': -20.90228388229539, 'cosine_total_motion': -0.9338560826054, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.9600045854600323, 'cosine_residue_motion': -0.9600045854600323, 'cosine_ionic_motion': -0.6409801026506722, 'motion_component_glu': None, 'motion_component_asn': -11.726530751199931, 'motion_component_residue': -11.726530751199931, 'motion_component_ionic': -9.175753131095458}, 6512: {'frame': 6512, 'ionic_force': [9.706706315279007, 9.800261914730072, -2.3819656521081924], 'ionic_force_magnitude': 13.997822739848125, 'motion_vector': [0.5918121337890625, 0.91455078125, 0.193389892578125], 'ionic_force_x': 9.706706315279007, 'ionic_force_y': 9.800261914730072, 'ionic_force_z': -2.3819656521081924, 'radial_force': 13.793668152032152, 'axial_force': -2.3819656521081924, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-7.006870269775391, 13.963640421628952, 17.046968698501587], 'asn_force_magnitude': 23.123118877212587, 'residue_force': [-7.006870269775391, 13.963640421628952, 17.046968698501587], 'residue_force_magnitude': 23.123118877212587, 'total_force': [2.6998360455036163, 23.763902336359024, 14.665003046393394], 'total_force_magnitude': 28.054847767816135, 'motion_component_total': 23.65146010885213, 'cosine_total_motion': 0.8430436088833293, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.4659577686498877, 'cosine_residue_motion': 0.4659577686498877, 'cosine_ionic_motion': 0.9199332976222395, 'motion_component_glu': None, 'motion_component_asn': 10.774396876252073, 'motion_component_residue': 10.774396876252073, 'motion_component_ionic': 12.877063232600058}, 6513: {'frame': 6513, 'ionic_force': [8.15608811378479, 11.545685589313507, -1.4180032014846802], 'ionic_force_magnitude': 14.206877282729092, 'motion_vector': [0.8010101318359375, -0.8122329711914062, -0.20128631591796875], 'ionic_force_x': 8.15608811378479, 'ionic_force_y': 11.545685589313507, 'ionic_force_z': -1.4180032014846802, 'radial_force': 14.135933964443351, 'axial_force': -1.4180032014846802, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [1.8882267475128174, 8.692317008972168, 4.966899871826172], 'asn_force_magnitude': 10.187829482830802, 'residue_force': [1.8882267475128174, 8.692317008972168, 4.966899871826172], 'residue_force_magnitude': 10.187829482830802, 'total_force': [10.044314861297607, 20.238002598285675, 3.5488966703414917], 'total_force_magnitude': 22.870497978353306, 'motion_component_total': -7.861564525915503, 'cosine_total_motion': -0.3437426038277082, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.5548028390659743, 'cosine_residue_motion': -0.5548028390659743, 'cosine_ionic_motion': -0.15551114864677235, 'motion_component_glu': None, 'motion_component_asn': -5.652236720994566, 'motion_component_residue': -5.652236720994566, 'motion_component_ionic': -2.209327804920937}, 6514: {'frame': 6514, 'ionic_force': [7.400987505912781, 7.646649926900864, -1.3441858291625977], 'ionic_force_magnitude': 10.726262476304205, 'motion_vector': [-0.7476043701171875, -0.9638442993164062, 0.5952987670898438], 'ionic_force_x': 7.400987505912781, 'ionic_force_y': 7.646649926900864, 'ionic_force_z': -1.3441858291625977, 'radial_force': 10.64170433564333, 'axial_force': -1.3441858291625977, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-0.5413827896118164, 16.18848466873169, 4.1756744384765625], 'asn_force_magnitude': 16.727115358327488, 'residue_force': [-0.5413827896118164, 16.18848466873169, 4.1756744384765625], 'residue_force_magnitude': 16.727115358327488, 'total_force': [6.859604716300964, 23.835134595632553, 2.831488609313965], 'total_force_magnitude': 24.963676528117666, 'motion_component_total': -19.462068456028888, 'cosine_total_motion': -0.7796154718680127, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.5599338128269465, 'cosine_residue_motion': -0.5599338128269465, 'cosine_ionic_motion': -0.9412403433300128, 'motion_component_glu': None, 'motion_component_asn': -9.366077480184487, 'motion_component_residue': -9.366077480184487, 'motion_component_ionic': -10.095990975844403}, 6515: {'frame': 6515, 'ionic_force': [7.8542662262916565, 10.365837097167969, -1.8927641795016825], 'ionic_force_magnitude': 13.14239829398326, 'motion_vector': [-0.4972648620605469, 0.8793983459472656, -0.0349578857421875], 'ionic_force_x': 7.8542662262916565, 'ionic_force_y': 10.365837097167969, 'ionic_force_z': -1.8927641795016825, 'radial_force': 13.005386448640788, 'axial_force': -1.8927641795016825, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-2.053715705871582, -2.341998517513275, 13.487313270568848], 'asn_force_magnitude': 13.84233811590515, 'residue_force': [-2.053715705871582, -2.341998517513275, 13.487313270568848], 'residue_force_magnitude': 13.84233811590515, 'total_force': [5.8005505204200745, 8.023838579654694, 11.594549091067165], 'total_force_magnitude': 15.24670261130147, 'motion_component_total': 3.7259593912871645, 'cosine_total_motion': 0.24437804594715012, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.1078992681831266, 'cosine_residue_motion': -0.1078992681831266, 'cosine_ionic_motion': 0.3971525917249284, 'motion_component_glu': None, 'motion_component_asn': -1.4935781526495653, 'motion_component_residue': -1.4935781526495653, 'motion_component_ionic': 5.219537543936729}, 6516: {'frame': 6516, 'ionic_force': [8.564916908740997, 8.454901933670044, -2.339739290997386], 'ionic_force_magnitude': 12.260405715613649, 'motion_vector': [0.10906982421875, -0.23324966430664062, -0.46515655517578125], 'ionic_force_x': 8.564916908740997, 'ionic_force_y': 8.454901933670044, 'ionic_force_z': -2.339739290997386, 'radial_force': 12.035080737644218, 'axial_force': -2.339739290997386, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-1.1611855030059814, 5.971788644790649, 12.154028415679932], 'asn_force_magnitude': 13.591578941373847, 'residue_force': [-1.1611855030059814, 5.971788644790649, 12.154028415679932], 'residue_force_magnitude': 13.591578941373847, 'total_force': [7.403731405735016, 14.426690578460693, 9.814289124682546], 'total_force_magnitude': 18.954284760912916, 'motion_component_total': -13.396819656339938, 'cosine_total_motion': -0.7067963695452412, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.9926474078878975, 'cosine_residue_motion': -0.9926474078878975, 'cosine_ionic_motion': 0.007734323897437115, 'motion_component_glu': None, 'motion_component_asn': -13.491645605258483, 'motion_component_residue': -13.491645605258483, 'motion_component_ionic': 0.09482594891854523}, 6517: {'frame': 6517, 'ionic_force': [7.82864648103714, 6.85845959931612, -3.1483363062143326], 'ionic_force_magnitude': 10.8737387911212, 'motion_vector': [0.41172027587890625, -0.2516136169433594, -0.4042510986328125], 'ionic_force_x': 7.82864648103714, 'ionic_force_y': 6.85845959931612, 'ionic_force_z': -3.1483363062143326, 'radial_force': 10.407986058815924, 'axial_force': -3.1483363062143326, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [1.1644930839538574, 10.149431228637695, 22.4260311126709], 'asn_force_magnitude': 24.64333317296801, 'residue_force': [1.1644930839538574, 10.149431228637695, 22.4260311126709], 'residue_force_magnitude': 24.64333317296801, 'total_force': [8.993139564990997, 17.007890827953815, 19.277694806456566], 'total_force_magnitude': 27.235536100871677, 'motion_component_total': -13.296405477132883, 'cosine_total_motion': -0.48820061510400486, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.7181364562871924, 'cosine_residue_motion': -0.7181364562871924, 'cosine_ionic_motion': 0.4047246824064274, 'motion_component_glu': None, 'motion_component_asn': -17.69727595593986, 'motion_component_residue': -17.69727595593986, 'motion_component_ionic': 4.4008704788069775}, 6518: {'frame': 6518, 'ionic_force': [8.416690051555634, 6.887873167172074, -3.1172511354088783], 'ionic_force_magnitude': 11.31374044391211, 'motion_vector': [0.5746345520019531, 0.6277122497558594, 0.5345230102539062], 'ionic_force_x': 8.416690051555634, 'ionic_force_y': 6.887873167172074, 'ionic_force_z': -3.1172511354088783, 'radial_force': 10.875820345656903, 'axial_force': -3.1172511354088783, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [27.00638771057129, 9.658788204193115, 29.760422706604004], 'asn_force_magnitude': 41.33182703949714, 'residue_force': [27.00638771057129, 9.658788204193115, 29.760422706604004], 'residue_force_magnitude': 41.33182703949714, 'total_force': [35.42307776212692, 16.54666137136519, 26.643171571195126], 'total_force_magnitude': 47.312208065703935, 'motion_component_total': 44.76129027944969, 'cosine_total_motion': 0.9460833072362274, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.9025583792564235, 'cosine_residue_motion': 0.9025583792564235, 'cosine_ionic_motion': 0.6591015139459799, 'motion_component_glu': None, 'motion_component_asn': 37.30438682447536, 'motion_component_residue': 37.30438682447536, 'motion_component_ionic': 7.456903454974334}, 6519: {'frame': 6519, 'ionic_force': [9.411851108074188, 7.655534982681274, -1.22977040335536], 'ionic_force_magnitude': 12.194363140262098, 'motion_vector': [-0.2264251708984375, -0.23356246948242188, 0.3396759033203125], 'ionic_force_x': 9.411851108074188, 'ionic_force_y': 7.655534982681274, 'ionic_force_z': -1.22977040335536, 'radial_force': 12.132195067324549, 'axial_force': -1.22977040335536, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.6944136619567871, 12.099075317382812, 7.111443519592285], 'asn_force_magnitude': 14.051422091801433, 'residue_force': [0.6944136619567871, 12.099075317382812, 7.111443519592285], 'residue_force_magnitude': 14.051422091801433, 'total_force': [10.106264770030975, 19.754610300064087, 5.881673116236925], 'total_force_magnitude': 22.95594246280539, 'motion_component_total': -10.427795614093622, 'cosine_total_motion': -0.4542525592660536, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.08587790474756599, 'cosine_residue_motion': -0.08587790474756599, 'cosine_ionic_motion': -0.7561763431237181, 'motion_component_glu': None, 'motion_component_asn': -1.2067066879675679, 'motion_component_residue': -1.2067066879675679, 'motion_component_ionic': -9.221088926126052}, 6520: {'frame': 6520, 'ionic_force': [10.359990179538727, 7.922158852219582, -1.979037795215845], 'ionic_force_magnitude': 13.191155673208952, 'motion_vector': [-0.3358879089355469, 0.9568252563476562, -0.047332763671875], 'ionic_force_x': 10.359990179538727, 'ionic_force_y': 7.922158852219582, 'ionic_force_z': -1.979037795215845, 'radial_force': 13.041855596499293, 'axial_force': -1.979037795215845, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-0.49257922172546387, 7.493866920471191, 10.708334922790527], 'asn_force_magnitude': 13.079339147298814, 'residue_force': [-0.49257922172546387, 7.493866920471191, 10.708334922790527], 'residue_force_magnitude': 13.079339147298814, 'total_force': [9.867410957813263, 15.416025772690773, 8.729297127574682], 'total_force_magnitude': 20.278566960614427, 'motion_component_total': 10.858169401952216, 'cosine_total_motion': 0.5354505287795357, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.5143113766990952, 'cosine_residue_motion': 0.5143113766990952, 'cosine_ionic_motion': 0.3131883650786743, 'motion_component_glu': None, 'motion_component_asn': 6.726852923161623, 'motion_component_residue': 6.726852923161623, 'motion_component_ionic': 4.131316478790591}, 6521: {'frame': 6521, 'ionic_force': [8.523545622825623, 8.435715436935425, -0.3902862071990967], 'ionic_force_magnitude': 11.998518585261694, 'motion_vector': [-0.5778541564941406, -0.9405899047851562, 0.7363662719726562], 'ionic_force_x': 8.523545622825623, 'ionic_force_y': 8.435715436935425, 'ionic_force_z': -0.3902862071990967, 'radial_force': 11.992169316572395, 'axial_force': -0.3902862071990967, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [1.2788491249084473, 7.075196266174316, 5.13110876083374], 'asn_force_magnitude': 8.833013891343704, 'residue_force': [1.2788491249084473, 7.075196266174316, 5.13110876083374], 'residue_force_magnitude': 8.833013891343704, 'total_force': [9.80239474773407, 15.510911703109741, 4.7408225536346436], 'total_force_magnitude': 18.95127233557478, 'motion_component_total': -12.632334402748914, 'cosine_total_motion': -0.6665691980498776, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.3084562326945369, 'cosine_residue_motion': -0.3084562326945369, 'cosine_ionic_motion': -0.8257466239754488, 'motion_component_glu': None, 'motion_component_asn': -2.724598188262391, 'motion_component_residue': -2.724598188262391, 'motion_component_ionic': -9.907736214486523}, 6522: {'frame': 6522, 'ionic_force': [8.201929569244385, 7.852409273386002, -1.7952950298786163], 'ionic_force_magnitude': 11.495871619842957, 'motion_vector': [1.0019340515136719, -0.547149658203125, -1.1143798828125], 'ionic_force_x': 8.201929569244385, 'ionic_force_y': 7.852409273386002, 'ionic_force_z': -1.7952950298786163, 'radial_force': 11.354821885683801, 'axial_force': -1.7952950298786163, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-1.1752307415008545, 2.312664270401001, 7.7411885261535645], 'asn_force_magnitude': 8.164287055267572, 'residue_force': [-1.1752307415008545, 2.312664270401001, 7.7411885261535645], 'residue_force_magnitude': 8.164287055267572, 'total_force': [7.02669882774353, 10.165073543787003, 5.945893496274948], 'total_force_magnitude': 13.713382734958413, 'motion_component_total': -3.226607063881107, 'cosine_total_motion': -0.2352889236917292, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.8498817613268737, 'cosine_residue_motion': -0.8498817613268737, 'cosine_ionic_motion': 0.3229047541049872, 'motion_component_glu': None, 'motion_component_asn': -6.938678662508998, 'motion_component_residue': -6.938678662508998, 'motion_component_ionic': 3.712071598627891}, 6523: {'frame': 6523, 'ionic_force': [8.875896751880646, 7.546073779463768, -2.6961287893354893], 'ionic_force_magnitude': 11.958004979253005, 'motion_vector': [-1.1348419189453125, 1.6291122436523438, 1.2769622802734375], 'ionic_force_x': 8.875896751880646, 'ionic_force_y': 7.546073779463768, 'ionic_force_z': -2.6961287893354893, 'radial_force': 11.65009753758122, 'axial_force': -2.6961287893354893, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-9.646163940429688, 6.588872909545898, 13.30817985534668], 'asn_force_magnitude': 17.70789022006995, 'residue_force': [-9.646163940429688, 6.588872909545898, 13.30817985534668], 'residue_force_magnitude': 17.70789022006995, 'total_force': [-0.7702671885490417, 14.134946689009666, 10.61205106601119], 'total_force_magnitude': 17.691965896149863, 'motion_component_total': 15.865665487518713, 'cosine_total_motion': 0.8967723304831494, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.9252038814612272, 'cosine_residue_motion': 0.9252038814612272, 'cosine_ionic_motion': -0.04329679386131599, 'motion_component_glu': None, 'motion_component_asn': 16.38340876409802, 'motion_component_residue': 16.38340876409802, 'motion_component_ionic': -0.5177432765793075}, 6524: {'frame': 6524, 'ionic_force': [7.49516898393631, 8.840759873390198, -1.1478295773267746], 'ionic_force_magnitude': 11.647064264238148, 'motion_vector': [3.0123634338378906, -2.144947052001953, -2.431182861328125], 'ionic_force_x': 7.49516898393631, 'ionic_force_y': 8.840759873390198, 'ionic_force_z': -1.1478295773267746, 'radial_force': 11.590366397862802, 'axial_force': -1.1478295773267746, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-0.46462464332580566, 3.2130324840545654, 4.136907577514648], 'asn_force_magnitude': 5.258655541835156, 'residue_force': [-0.46462464332580566, 3.2130324840545654, 4.136907577514648], 'residue_force_magnitude': 5.258655541835156, 'total_force': [7.030544340610504, 12.053792357444763, 2.989078000187874], 'total_force_magnitude': 14.270846198207424, 'motion_component_total': -2.6986703349409025, 'cosine_total_motion': -0.18910373620871096, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.7884366861205669, 'cosine_residue_motion': -0.7884366861205669, 'cosine_ionic_motion': 0.1242756613232993, 'motion_component_glu': None, 'motion_component_asn': -4.146116948854065, 'motion_component_residue': -4.146116948854065, 'motion_component_ionic': 1.4474466139131623}, 6525: {'frame': 6525, 'ionic_force': [9.840662479400635, 7.653836600482464, -2.6271378248929977], 'ionic_force_magnitude': 12.740553594383249, 'motion_vector': [-2.0359725952148438, 0.5774726867675781, 0.655609130859375], 'ionic_force_x': 9.840662479400635, 'ionic_force_y': 7.653836600482464, 'ionic_force_z': -2.6271378248929977, 'radial_force': 12.46674988681366, 'axial_force': -2.6271378248929977, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [85.96767401695251, -10.053918957710266, -64.23384380340576], 'asn_force_magnitude': 107.78454876304649, 'residue_force': [85.96767401695251, -10.053918957710266, -64.23384380340576], 'residue_force_magnitude': 107.78454876304649, 'total_force': [95.80833649635315, -2.4000823572278023, -66.86098162829876], 'total_force_magnitude': 116.85627326686239, 'motion_component_total': -108.4553178787265, 'cosine_total_motion': -0.9281086487419398, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.9336186342065317, 'cosine_residue_motion': -0.9336186342065317, 'cosine_ionic_motion': -0.6142319182624612, 'motion_component_glu': None, 'motion_component_asn': -100.62966320472277, 'motion_component_residue': -100.62966320472277, 'motion_component_ionic': -7.825654674003718}, 6526: {'frame': 6526, 'ionic_force': [8.668226391077042, 8.704079300165176, -1.1561321690678596], 'ionic_force_magnitude': 12.338386718808986, 'motion_vector': [1.2026252746582031, -0.27906036376953125, -0.46521759033203125], 'ionic_force_x': 8.668226391077042, 'ionic_force_y': 8.704079300165176, 'ionic_force_z': -1.1561321690678596, 'radial_force': 12.28410131961343, 'axial_force': -1.1561321690678596, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [20</t>
+          <t>{6500: {'frame': 6500, 'ionic_force': [10.081943392753601, 8.897971272468567, -2.1222930885851383], 'ionic_force_magnitude': 13.613361204868552, 'motion_vector': [0.8403472900390625, -0.8082695007324219, 0.09564208984375], 'ionic_force_x': 10.081943392753601, 'ionic_force_y': 8.897971272468567, 'ionic_force_z': -2.1222930885851383, 'radial_force': 13.446913227219245, 'axial_force': -2.1222930885851383, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-0.4597816467285156, 6.867312431335449, 4.928182125091553], 'asn_force_magnitude': 8.465126003215468, 'residue_force': [-0.4597816467285156, 6.867312431335449, 4.928182125091553], 'residue_force_magnitude': 8.465126003215468, 'total_force': [9.622161746025085, 15.765283703804016, 2.8058890365064144], 'total_force_magnitude': 18.6816268085326, 'motion_component_total': -3.751035137079949, 'cosine_total_motion': -0.20078739263578002, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.5519086046032223, 'cosine_residue_motion': -0.5519086046032223, 'cosine_ionic_motion': 0.06764976917058485, 'motion_component_glu': None, 'motion_component_asn': -4.6719758802251015, 'motion_component_residue': -4.6719758802251015, 'motion_component_ionic': 0.9209407431451524, 'ionic_contributions': [{'ion_id': 1327, 'distance': 14.501358032226562, 'force': [0.9640901684761047, 1.2501052618026733, -0.017418090254068375], 'magnitude': 1.5787769556045532}, {'ion_id': 1330, 'distance': 10.892683982849121, 'force': [1.6772516965866089, 2.190032482147217, -0.4691789448261261], 'magnitude': 2.7981324195861816}, {'ion_id': 1355, 'distance': 6.828861236572266, 'force': [6.430893898010254, 2.644869804382324, 1.5276371240615845], 'magnitude': 7.119368553161621}, {'ion_id': 1359, 'distance': 14.681105613708496, 'force': [0.31147414445877075, 0.8422232866287231, -1.251532793045044], 'magnitude': 1.5403540134429932}, {'ion_id': 1465, 'distance': 10.825296401977539, 'force': [0.6982334852218628, 1.9707404375076294, -1.9118003845214844], 'magnitude': 2.8330776691436768}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.53505802154541, 'force': [-4.579796314239502, 7.029941558837891, 7.878915309906006], 'magnitude': 11.509644508361816}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.32102108001709, 'force': [3.9151611328125, -4.018174171447754, -4.110124111175537], 'magnitude': 6.954662322998047}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.325368642807007, 'force': [11.173625946044922, -19.582983016967773, -15.909395217895508], 'magnitude': 27.594419479370117}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.286119222640991, 'force': [-7.981685161590576, 9.01579475402832, 4.629401683807373], 'magnitude': 12.9005126953125}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 2.688101053237915, 'force': [-2.9870872497558594, 14.422733306884766, 12.439384460449219], 'magnitude': 19.278905868530273}]}, 6501: {'frame': 6501, 'ionic_force': [10.483401715755463, 8.962290167808533, -2.592883415520191], 'ionic_force_magnitude': 14.033794960465316, 'motion_vector': [-0.46063232421875, -0.98577880859375, -0.43386077880859375], 'ionic_force_x': 10.483401715755463, 'ionic_force_y': 8.962290167808533, 'ionic_force_z': -2.592883415520191, 'radial_force': 13.79218461977297, 'axial_force': -2.592883415520191, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [1.1594171524047852, 8.153244018554688, 8.414933681488037], 'asn_force_magnitude': 11.774155809366123, 'residue_force': [1.1594171524047852, 8.153244018554688, 8.414933681488037], 'residue_force_magnitude': 11.774155809366123, 'total_force': [11.642818868160248, 17.11553418636322, 5.822050265967846], 'total_force_magnitude': 21.50332557956589, 'motion_component_total': -21.138089026666297, 'cosine_total_motion': -0.9830148805798361, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.8861699521672649, 'cosine_residue_motion': -0.8861699521672649, 'cosine_ionic_motion': -0.762743503551621, 'motion_component_glu': None, 'motion_component_asn': -10.433903090395901, 'motion_component_residue': -10.433903090395901, 'motion_component_ionic': -10.704185936270399, 'ionic_contributions': [{'ion_id': 1327, 'distance': 14.337858200073242, 'force': [1.1554292440414429, 1.1262600421905518, -0.06863195449113846], 'magnitude': 1.6149888038635254}, {'ion_id': 1330, 'distance': 8.436062812805176, 'force': [2.076904535293579, 4.1037421226501465, -0.780176043510437], 'magnitude': 4.665072917938232}, {'ion_id': 1355, 'distance': 7.409305572509766, 'force': [5.77974796295166, 0.7983136177062988, 1.5908108949661255], 'magnitude': 6.047600269317627}, {'ion_id': 1359, 'distance': 14.33599853515625, 'force': [0.37562042474746704, 0.8487633466720581, -1.3221392631530762], 'magnitude': 1.6154077053070068}, {'ion_id': 1465, 'distance': 10.35150146484375, 'force': [1.0956995487213135, 2.0852110385894775, -2.012747049331665], 'magnitude': 3.0983564853668213}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.875383138656616, 'force': [-3.9214677810668945, 7.978348731994629, 13.015137672424316], 'magnitude': 15.761528015136719}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.503239631652832, 'force': [4.646948337554932, -4.8860578536987305, -6.986770153045654], 'magnitude': 9.709924697875977}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 2.591418504714966, 'force': [8.875370025634766, -27.20709800720215, -35.29412841796875], 'magnitude': 45.438682556152344}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 2.294158458709717, 'force': [-13.76177978515625, 17.170976638793945, 14.708637237548828], 'magnitude': 26.468339920043945}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 2.2305688858032227, 'force': [5.320346355438232, 15.097074508666992, 22.972057342529297], 'magnitude': 27.99898338317871}]}, 6502: {'frame': 6502, 'ionic_force': [11.625001519918442, 8.640661865472794, -4.613270275294781], 'ionic_force_magnitude': 15.201445998471996, 'motion_vector': [-0.4776763916015625, 0.31816864013671875, -0.33734130859375], 'ionic_force_x': 11.625001519918442, 'ionic_force_y': 8.640661865472794, 'ionic_force_z': -4.613270275294781, 'radial_force': 14.484533054660128, 'axial_force': -4.613270275294781, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [4.454033255577087, -0.38120079040527344, 29.511417388916016], 'asn_force_magnitude': 29.848073347993616, 'residue_force': [4.454033255577087, -0.38120079040527344, 29.511417388916016], 'residue_force_magnitude': 29.848073347993616, 'total_force': [16.07903477549553, 8.25946107506752, 24.898147113621235], 'total_force_magnitude': 30.768031887881218, 'motion_component_total': -20.20596221345819, 'cosine_total_motion': -0.656719360116655, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.6141775272041401, 'cosine_residue_motion': -0.6141775272041401, 'cosine_ionic_motion': -0.1232742156876414, 'motion_component_glu': None, 'motion_component_asn': -18.33201588067852, 'motion_component_residue': -18.33201588067852, 'motion_component_ionic': -1.8739463327796702, 'ionic_contributions': [{'ion_id': 1327, 'distance': 13.427719116210938, 'force': [1.394202709197998, 1.199537992477417, -0.08850883692502975], 'magnitude': 1.8413381576538086}, {'ion_id': 1330, 'distance': 7.558098316192627, 'force': [2.795842409133911, 4.828749656677246, -1.6259845495224], 'magnitude': 5.811831474304199}, {'ion_id': 1355, 'distance': 7.420594215393066, 'force': [5.975593090057373, 0.20818576216697693, 0.7748332023620605], 'magnitude': 6.029213905334473}, {'ion_id': 1359, 'distance': 14.30691909790039, 'force': [0.39647552371025085, 0.6920129656791687, -1.4123555421829224], 'magnitude': 1.6219812631607056}, {'ion_id': 1465, 'distance': 10.469426155090332, 'force': [1.0628877878189087, 1.7121754884719849, -2.2612545490264893], 'magnitude': 3.028951406478882}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.2610840797424316, 'force': [-9.725320816040039, 6.661158561706543, 18.88135528564453], 'magnitude': 22.25889778137207}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.044439792633057, 'force': [7.785599708557129, -3.810567855834961, -8.353086471557617], 'magnitude': 12.037858963012695}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 1.9360193014144897, 'force': [40.65467071533203, -23.795244216918945, -66.39793395996094], 'magnitude': 81.41069793701172}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 1.92190420627594, 'force': [-32.44646453857422, 9.861348152160645, 16.503801345825195], 'magnitude': 37.71464920043945}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 1.413465142250061, 'force': [-1.814451813697815, 10.702104568481445, 68.87728118896484], 'magnitude': 69.72737884521484}]}, 6503: {'frame': 6503, 'ionic_force': [11.245525449514389, 9.056975394487381, -5.633130311965942], 'ionic_force_magnitude': 15.499122653996102, 'motion_vector': [0.24894332885742188, 0.13856887817382812, -0.48906707763671875], 'ionic_force_x': 11.245525449514389, 'ionic_force_y': 9.056975394487381, 'ionic_force_z': -5.633130311965942, 'radial_force': 14.439205169676953, 'axial_force': -5.633130311965942, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-17.786433219909668, 19.308142960071564, 38.5463604927063], 'asn_force_magnitude': 46.63671835031423, 'residue_force': [-17.786433219909668, 19.308142960071564, 38.5463604927063], 'residue_force_magnitude': 46.63671835031423, 'total_force': [-6.540907770395279, 28.365118354558945, 32.913230180740356], 'total_force_magnitude': 43.93909574239497, 'motion_component_total': -24.37185294337288, 'cosine_total_motion': -0.5546735209631889, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.7805581220149096, 'cosine_residue_motion': -0.7805581220149096, 'cosine_ionic_motion': 0.7762256366159407, 'motion_component_glu': None, 'motion_component_asn': -36.40266929245955, 'motion_component_residue': -36.40266929245955, 'motion_component_ionic': 12.030816349086672, 'ionic_contributions': [{'ion_id': 1327, 'distance': 12.726118087768555, 'force': [1.3975937366485596, 1.4927356243133545, -0.144304096698761], 'magnitude': 2.0499637126922607}, {'ion_id': 1330, 'distance': 7.7350287437438965, 'force': [2.3191373348236084, 4.516908645629883, -2.2384073734283447], 'magnitude': 5.5489935874938965}, {'ion_id': 1355, 'distance': 7.14366340637207, 'force': [6.450554847717285, 0.43755224347114563, 0.7234833836555481], 'magnitude': 6.505731105804443}, {'ion_id': 1359, 'distance': 14.138544082641602, 'force': [0.3285345733165741, 0.7057961225509644, -1.4670779705047607], 'magnitude': 1.6608434915542603}, {'ion_id': 1465, 'distance': 10.129035949707031, 'force': [0.7497049570083618, 1.9039827585220337, -2.506824254989624], 'magnitude': 3.235950469970703}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.754899978637695, 'force': [-4.836879253387451, 0.8949549794197083, -3.339604377746582], 'magnitude': 5.945528030395508}, {'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.3457064628601074, 'force': [-12.025126457214355, 8.179439544677734, 15.352368354797363], 'magnitude': 21.147153854370117}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.2685956954956055, 'force': [7.831679821014404, -4.046734809875488, -6.251003742218018], 'magnitude': 10.806772232055664}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 2.0999464988708496, 'force': [47.59791564941406, -29.130535125732422, -40.91468811035156], 'magnitude': 69.19654083251953}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 2.3385672569274902, 'force': [-23.21302032470703, 8.939334869384766, 5.486260414123535], 'magnitude': 25.472633361816406}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 1.2931607961654663, 'force': [-33.1410026550293, 34.471683502197266, 68.21302795410156], 'magnitude': 83.30450439453125}]}, 6504: {'frame': 6504, 'ionic_force': [9.827082574367523, 8.00064042210579, -3.6161573603749275], 'ionic_force_magnitude': 13.177951022153053, 'motion_vector': [-1.3946723937988281, 1.9302940368652344, 2.1039581298828125], 'ionic_force_x': 9.827082574367523, 'ionic_force_y': 8.00064042210579, 'ionic_force_z': -3.6161573603749275, 'radial_force': 12.672087400553664, 'axial_force': -3.6161573603749275, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-17.627061367034912, 83.77625507116318, 67.12841844558716], 'asn_force_magnitude': 108.79061893928012, 'residue_force': [-17.627061367034912, 83.77625507116318, 67.12841844558716], 'residue_force_magnitude': 108.79061893928012, 'total_force': [-7.799978792667389, 91.77689549326897, 63.51226108521223], 'total_force_magnitude': 111.88228422634496, 'motion_component_total': 101.22472079757716, 'cosine_total_motion': 0.9047430654239516, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.9474349623830411, 'cosine_residue_motion': 0.9474349623830411, 'cosine_ionic_motion': -0.14018227580919085, 'motion_component_glu': None, 'motion_component_asn': 103.07203596236462, 'motion_component_residue': 103.07203596236462, 'motion_component_ionic': -1.8473151647874677, 'ionic_contributions': [{'ion_id': 1327, 'distance': 13.917710304260254, 'force': [1.23141348361969, 1.187270998954773, -0.10812932997941971], 'magnitude': 1.713967204093933}, {'ion_id': 1330, 'distance': 7.934230327606201, 'force': [2.0249695777893066, 4.583828449249268, -1.6436532735824585], 'magnitude': 5.273858547210693}, {'ion_id': 1355, 'distance': 7.617783069610596, 'force': [5.697000026702881, 0.46980372071266174, 0.2337888479232788], 'magnitude': 5.72111701965332}, {'ion_id': 1465, 'distance': 10.747157096862793, 'force': [0.8736994862556458, 1.759737253189087, -2.098163604736328], 'magnitude': 2.874424695968628}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.6893157958984375, 'force': [-5.272274494171143, 0.7780961394309998, -2.9334909915924072], 'magnitude': 6.0833940505981445}, {'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 2.923990249633789, 'force': [-15.6574125289917, 13.565571784973145, 18.368186950683594], 'magnitude': 27.686992645263672}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.8767197132110596, 'force': [9.613481521606445, -5.87046480178833, -6.691837787628174], 'magnitude': 13.101987838745117}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 1.7439719438552856, 'force': [68.77738189697266, -58.82910919189453, -43.295536041259766], 'magnitude': 100.32794189453125}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 2.112577438354492, 'force': [-27.80966567993164, 14.173375129699707, 0.21587109565734863], 'magnitude': 31.213916778564453}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 0.9214372038841248, 'force': [-47.27857208251953, 119.95878601074219, 101.46522521972656], 'magnitude': 164.0748748779297}]}, 6505: {'frame': 6505, 'ionic_force': [8.954921334981918, 11.337874412536621, 0.06668257713317871], 'ionic_force_magnitude': 14.44792230309466, 'motion_vector': [1.2258834838867188, -0.9209442138671875, -0.31507110595703125], 'ionic_force_x': 8.954921334981918, 'ionic_force_y': 11.337874412536621, 'ionic_force_z': 0.06668257713317871, 'radial_force': 14.447768419730675, 'axial_force': 0.06668257713317871, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-0.48206377029418945, 0.9736707210540771, 0.43469953536987305], 'asn_force_magnitude': 1.1702067499886502, 'residue_force': [-0.48206377029418945, 0.9736707210540771, 0.43469953536987305], 'residue_force_magnitude': 1.1702067499886502, 'total_force': [8.472857564687729, 12.311545133590698, 0.5013821125030518], 'total_force_magnitude': 14.953756815953136, 'motion_component_total': -0.7087932192891095, 'cosine_total_motion': -0.047399006685259634, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.8869239070081387, 'cosine_residue_motion': -0.8869239070081387, 'cosine_ionic_motion': 0.022777747313025818, 'motion_component_glu': None, 'motion_component_asn': -1.0378843427072297, 'motion_component_residue': -1.0378843427072297, 'motion_component_ionic': 0.3290911234181202, 'ionic_contributions': [{'ion_id': 1327, 'distance': 14.51010513305664, 'force': [0.9046583771705627, 1.2874258756637573, 0.10324346274137497], 'magnitude': 1.5768738985061646}, {'ion_id': 1330, 'distance': 10.13671875, 'force': [0.6813580989837646, 3.155944347381592, 0.12422109395265579], 'magnitude': 3.2310469150543213}, {'ion_id': 1355, 'distance': 6.801566123962402, 'force': [6.166740417480469, 2.169691801071167, 2.961028814315796], 'magnitude': 7.176624774932861}, {'ion_id': 1359, 'distance': 13.200652122497559, 'force': [0.27677449584007263, 1.2362631559371948, -1.4230068922042847], 'magnitude': 1.9052294492721558}, {'ion_id': 1465, 'distance': 9.122966766357422, 'force': [0.9253899455070496, 3.48854923248291, -1.6988039016723633], 'magnitude': 3.9890170097351074}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.8568220138549805, 'force': [6.898890495300293, -7.8649067878723145, -7.608279228210449], 'magnitude': 12.935894012451172}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.855471611022949, 'force': [-3.9878201484680176, 3.5164992809295654, 2.578230857849121], 'magnitude': 5.908955097198486}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.084853649139404, 'force': [-3.393134117126465, 5.322078227996826, 5.464747905731201], 'magnitude': 8.348732948303223}]}, 6506: {'frame': 6506, 'ionic_force': [8.623957127332687, 13.234449625015259, -0.3938300022855401], 'ionic_force_magnitude': 15.801215000177645, 'motion_vector': [0.202423095703125, -0.7250022888183594, -0.397186279296875], 'ionic_force_x': 8.623957127332687, 'ionic_force_y': 13.234449625015259, 'ionic_force_z': -0.3938300022855401, 'radial_force': 15.796306321768352, 'axial_force': -0.3938300022855401, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-0.8118951320648193, 4.410116195678711, 5.561502456665039], 'asn_force_magnitude': 7.144131027658261, 'residue_force': [-0.8118951320648193, 4.410116195678711, 5.561502456665039], 'residue_force_magnitude': 7.144131027658261, 'total_force': [7.812061995267868, 17.64456582069397, 5.167672454379499], 'total_force_magnitude': 19.976582646049927, 'motion_component_total': -15.584111210437268, 'cosine_total_motion': -0.7801189766318112, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.9161753387152256, 'cosine_residue_motion': -0.9161753387152256, 'cosine_ionic_motion': -0.5720341471364631, 'motion_component_glu': None, 'motion_component_asn': -6.5452766640907605, 'motion_component_residue': -6.5452766640907605, 'motion_component_ionic': -9.038834546346507, 'ionic_contributions': [{'ion_id': 1327, 'distance': 13.775360107421875, 'force': [1.1759207248687744, 1.295444130897522, 0.006512581370770931], 'magnitude': 1.7495734691619873}, {'ion_id': 1330, 'distance': 7.36737060546875, 'force': [0.41796424984931946, 5.998465061187744, 1.121175765991211], 'magnitude': 6.116641998291016}, {'ion_id': 1355, 'distance': 7.552302837371826, 'force': [5.303382396697998, 1.6648468971252441, 1.7273120880126953], 'magnitude': 5.8207550048828125}, {'ion_id': 1359, 'distance': 13.520206451416016, 'force': [0.40036541223526, 1.0453904867172241, -1.4302330017089844], 'magnitude': 1.816232442855835}, {'ion_id': 1465, 'distance': 9.182841300964355, 'force': [1.3263243436813354, 3.2303030490875244, -1.818597435951233], 'magnitude': 3.9371678829193115}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.815361976623535, 'force': [-3.863424777984619, 5.1770853996276855, 7.904995441436768], 'magnitude': 10.208683013916016}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.5522236824035645, 'force': [3.46663236618042, -3.1595187187194824, -4.335928916931152], 'magnitude': 6.38751745223999}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.528366804122925, 'force': [9.477591514587402, -14.115449905395508, -17.654951095581055], 'magnitude': 24.510568618774414}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.3666739463806152, 'force': [-7.487356662750244, 7.186718940734863, 6.5839409828186035], 'magnitude': 12.29055404663086}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 2.9299724102020264, 'force': [-2.4053375720977783, 9.321280479431152, 13.063446044921875], 'magnitude': 16.22730827331543}]}, 6507: {'frame': 6507, 'ionic_force': [7.709233731031418, 10.224741041660309, -1.3882663855329156], 'ionic_force_magnitude': 12.88040751086261, 'motion_vector': [-0.5508842468261719, 0.7071418762207031, 0.5803451538085938], 'ionic_force_x': 7.709233731031418, 'ionic_force_y': 10.224741041660309, 'ionic_force_z': -1.3882663855329156, 'radial_force': 12.805374422041917, 'axial_force': -1.3882663855329156, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-1.127873182296753, 5.707294940948486, 11.358274936676025], 'asn_force_magnitude': 12.761493760349655, 'residue_force': [-1.127873182296753, 5.707294940948486, 11.358274936676025], 'residue_force_magnitude': 12.761493760349655, 'total_force': [6.581360548734665, 15.932035982608795, 9.97000855114311], 'total_force_magnitude': 19.9134413834839, 'motion_component_total': 12.573460355545087, 'cosine_total_motion': 0.631405697961049, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.8254580715079681, 'cosine_residue_motion': 0.8254580715079681, 'cosine_ionic_motion': 0.15833212767887905, 'motion_component_glu': None, 'motion_component_asn': 10.534078028979195, 'motion_component_residue': 10.534078028979195, 'motion_component_ionic': 2.0393823265658915, 'ionic_contributions': [{'ion_id': 1327, 'distance': 13.825602531433105, 'force': [1.2036428451538086, 1.2521857023239136, 0.0053549399599432945], 'magnitude': 1.7368805408477783}, {'ion_id': 1330, 'distance': 9.18973445892334, 'force': [-0.9935823678970337, 3.679025173187256, 0.9656085968017578], 'magnitude': 3.9312634468078613}, {'ion_id': 1355, 'distance': 7.734027862548828, 'force': [5.284008026123047, 0.8967590928077698, 1.443036437034607], 'magnitude': 5.550429821014404}, {'ion_id': 1359, 'distance': 12.886669158935547, 'force': [0.4560973346233368, 1.0773588418960571, -1.6211364269256592], 'magnitude': 1.9992023706436157}, {'ion_id': 1465, 'distance': 8.742290496826172, 'force': [1.7590678930282593, 3.3194122314453125, -2.1811299324035645], 'magnitude': 4.343977928161621}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.083062648773193, 'force': [-5.63332462310791, 5.970870018005371, 11.585503578186035], 'magnitude': 14.19892692565918}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.8327507972717285, 'force': [4.903711795806885, -3.526336193084717, -5.882151126861572], 'magnitude': 8.430963516235352}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 2.7669761180877686, 'force': [16.736114501953125, -18.825477600097656, -30.88652992248535], 'magnitude': 39.85566329956055}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 2.634650230407715, 'force': [-14.081010818481445, 9.473031997680664, 10.712381362915039], 'magnitude': 20.069087982177734}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 2.195261240005493, 'force': [-3.0533640384674072, 12.615206718444824, 25.829071044921875], 'magnitude': 28.906875610351562}]}, 6508: {'frame': 6508, 'ionic_force': [8.196878910064697, 9.545158743858337, -0.845391895622015], 'ionic_force_magnitude': 12.61005815882314, 'motion_vector': [0.4479179382324219, -0.00655364990234375, -0.4083099365234375], 'ionic_force_x': 8.196878910064697, 'ionic_force_y': 9.545158743858337, 'ionic_force_z': -0.845391895622015, 'radial_force': 12.581688253637454, 'axial_force': -0.845391895622015, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-1.3246822357177734, 3.438356876373291, 5.006871700286865], 'asn_force_magnitude': 6.216578259626691, 'residue_force': [-1.3246822357177734, 3.438356876373291, 5.006871700286865], 'residue_force_magnitude': 6.216578259626691, 'total_force': [6.872196674346924, 12.983515620231628, 4.16147980466485], 'total_force_magnitude': 15.26815899695628, 'motion_component_total': 2.1347279550177696, 'cosine_total_motion': 0.13981567492474561, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.7060007510426008, 'cosine_residue_motion': -0.7060007510426008, 'cosine_ionic_motion': 0.5173359863265016, 'motion_component_glu': None, 'motion_component_asn': -4.3889089202115485, 'motion_component_residue': -4.3889089202115485, 'motion_component_ionic': 6.523636875229318, 'ionic_contributions': [{'ion_id': 1327, 'distance': 13.767386436462402, 'force': [1.1328179836273193, 1.335171103477478, 0.0463273860514164], 'magnitude': 1.7516005039215088}, {'ion_id': 1330, 'distance': 12.729866027832031, 'force': [-0.5327326059341431, 1.9765138626098633, 0.0836285948753357], 'magnitude': 2.0487568378448486}, {'ion_id': 1355, 'distance': 7.018674850463867, 'force': [6.056460380554199, 1.6252503395080566, 2.4695637226104736], 'magnitude': 6.739502906799316}, {'ion_id': 1359, 'distance': 13.185367584228516, 'force': [0.32606077194213867, 1.136378526687622, -1.499696135520935], 'magnitude': 1.9096492528915405}, {'ion_id': 1465, 'distance': 8.932685852050781, 'force': [1.214272379875183, 3.4718449115753174, -1.9452154636383057], 'magnitude': 4.160772323608398}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.088389873504639, 'force': [-3.9003937244415283, 4.3555498123168945, 7.028666019439697], 'magnitude': 9.142539978027344}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.8621697425842285, 'force': [3.2859272956848145, -2.6669387817382812, -3.8629274368286133], 'magnitude': 5.729928970336914}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.7965641021728516, 'force': [9.550633430480957, -11.230769157409668, -15.192797660827637], 'magnitude': 21.16992950439453}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.6755244731903076, 'force': [-6.731670379638672, 5.472902774810791, 5.57363224029541], 'magnitude': 10.311810493469238}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 3.1379330158233643, 'force': [-3.5291788578033447, 7.507612228393555, 11.460298538208008], 'magnitude': 14.147713661193848}]}, 6509: {'frame': 6509, 'ionic_force': [8.639953941106796, 9.225626945495605, -1.5821315441280603], 'ionic_force_magnitude': 12.738294111254712, 'motion_vector': [0.6326484680175781, 0.24243927001953125, -0.14005279541015625], 'ionic_force_x': 8.639953941106796, 'ionic_force_y': 9.225626945495605, 'ionic_force_z': -1.5821315441280603, 'radial_force': 12.639659672708813, 'axial_force': -1.5821315441280603, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-0.6517491340637207, 5.48417067527771, 6.172529220581055], 'asn_force_magnitude': 8.282573386831881, 'residue_force': [-0.6517491340637207, 5.48417067527771, 6.172529220581055], 'residue_force_magnitude': 8.282573386831881, 'total_force': [7.988204807043076, 14.709797620773315, 4.590397676452994], 'total_force_magnitude': 17.35688085202406, 'motion_component_total': 11.53029283891268, 'cosine_total_motion': 0.6643067344423284, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.009209195305889378, 'cosine_residue_motion': 0.009209195305889378, 'cosine_ionic_motion': 0.899179819756083, 'motion_component_glu': None, 'motion_component_asn': 0.07627583595469645, 'motion_component_residue': 0.07627583595469645, 'motion_component_ionic': 11.454017002957984, 'ionic_contributions': [{'ion_id': 1327, 'distance': 13.967348098754883, 'force': [1.1541345119476318, 1.2506355047225952, -0.005397135391831398], 'magnitude': 1.7018063068389893}, {'ion_id': 1330, 'distance': 12.75448226928711, 'force': [-0.1657010018825531, 2.027735948562622, 0.1610119491815567], 'magnitude': 2.04085636138916}, {'ion_id': 1355, 'distance': 7.376007556915283, 'force': [5.690523624420166, 1.5907838344573975, 1.5250321626663208], 'magnitude': 6.102325439453125}, {'ion_id': 1359, 'distance': 13.528180122375488, 'force': [0.4454243779182434, 1.0431405305862427, -1.415763020515442], 'magnitude': 1.8140920400619507}, {'ion_id': 1465, 'distance': 9.015236854553223, 'force': [1.515572428703308, 3.313331127166748, -1.8470155000686646], 'magnitude': 4.084921836853027}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.592179298400879, 'force': [-4.211427688598633, 5.909515380859375, 8.56412410736084], 'magnitude': 11.225092887878418}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.334578514099121, 'force': [3.779480457305908, -3.5305588245391846, -4.596541404724121], 'magnitude': 6.919357776641846}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.3159492015838623, 'force': [10.585783958435059, -16.80129051208496, -19.385528564453125], 'magnitude': 27.75141143798828}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.1748175621032715, 'force': [-8.495471954345703, 8.463653564453125, 6.870993614196777], 'magnitude': 13.820891380310059}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 2.7230899333953857, 'force': [-2.3101139068603516, 11.442851066589355, 14.719481468200684], 'magnitude': 18.786659240722656}]}, 6510: {'frame': 6510, 'ionic_force': [8.169408738613129, 10.510639429092407, -0.9569092690944672], 'ionic_force_magnitude': 13.34647727665242, 'motion_vector': [-0.5427474975585938, -0.5374031066894531, -0.217681884765625], 'ionic_force_x': 8.169408738613129, 'ionic_force_y': 10.510639429092407, 'ionic_force_z': -0.9569092690944672, 'radial_force': 13.312129068895047, 'axial_force': -0.9569092690944672, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [1.0689871311187744, 6.226802349090576, 4.6353254318237305], 'asn_force_magnitude': 7.835945561325023, 'residue_force': [1.0689871311187744, 6.226802349090576, 4.6353254318237305], 'residue_force_magnitude': 7.835945561325023, 'total_force': [9.238395869731903, 16.737441778182983, 3.6784161627292633], 'total_force_magnitude': 19.468452968589276, 'motion_component_total': -18.64705599815435, 'cosine_total_motion': -0.9578088216993831, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.7930646120050037, 'cosine_residue_motion': -0.7930646120050037, 'cosine_ionic_motion': -0.9315300670101739, 'motion_component_glu': None, 'motion_component_asn': -6.21441112628456, 'motion_component_residue': -6.21441112628456, 'motion_component_ionic': -12.432644871869792, 'ionic_contributions': [{'ion_id': 1327, 'distance': 14.943717956542969, 'force': [1.0011017322540283, 1.0972646474838257, 0.06368693709373474], 'magnitude': 1.4866911172866821}, {'ion_id': 1330, 'distance': 8.376114845275879, 'force': [-0.3688025176525116, 4.693726539611816, 0.4749440550804138], 'magnitude': 4.732088088989258}, {'ion_id': 1355, 'distance': 7.593198776245117, 'force': [5.465493679046631, 0.39318275451660156, 1.7694438695907593], 'magnitude': 5.758224010467529}, {'ion_id': 1359, 'distance': 13.399306297302246, 'force': [0.4867585003376007, 1.0545459985733032, -1.4388798475265503], 'magnitude': 1.8491555452346802}, {'ion_id': 1465, 'distance': 9.033523559570312, 'force': [1.5848573446273804, 3.2719194889068604, -1.8261042833328247], 'magnitude': 4.0684013366</t>
         </is>
       </c>
     </row>
@@ -483,7 +483,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>{6500: {'frame': 6500, 'ionic_force': [-6.2898120284080505, 8.96427071094513, -9.324965059757233], 'ionic_force_magnitude': 14.383144930699562, 'motion_vector': [-0.07231521606445312, 0.7506103515625, -0.3880615234375], 'ionic_force_x': -6.2898120284080505, 'ionic_force_y': 8.96427071094513, 'ionic_force_z': -9.324965059757233, 'radial_force': 10.950793794598422, 'axial_force': -9.324965059757233, 'glu_force': [1.275538682937622, 6.072243690490723, -0.026713132858276367], 'glu_force_magnitude': 6.204825215897845, 'asn_force': [9.176877975463867, 7.638951301574707, -4.474958419799805], 'asn_force_magnitude': 12.751232066875769, 'residue_force': [10.45241665840149, 13.71119499206543, -4.501671552658081], 'residue_force_magnitude': 17.81894859073565, 'total_force': [4.162604629993439, 22.67546570301056, -13.826636612415314], 'total_force_magnitude': 26.88270637725738, 'motion_component_total': 26.041228518789573, 'cosine_total_motion': 0.9686981717294768, 'cosine_glu_motion': 0.8506009999111716, 'cosine_asn_motion': 0.6294413349467401, 'cosine_residue_motion': 0.7466199815079814, 'cosine_ionic_motion': 0.88556748283168, 'motion_component_glu': 5.277830532916758, 'motion_component_asn': 8.026152534389965, 'motion_component_residue': 13.303983067306723, 'motion_component_ionic': 12.737245451482849}, 6501: {'frame': 6501, 'ionic_force': [-7.69091010093689, 7.941129088401794, -6.768357574939728], 'ionic_force_magnitude': 12.96234136418256, 'motion_vector': [-0.7340888977050781, -0.2639427185058594, 0.5615005493164062], 'ionic_force_x': -7.69091010093689, 'ionic_force_y': 7.941129088401794, 'ionic_force_z': -6.768357574939728, 'radial_force': 11.05493687812618, 'axial_force': -6.768357574939728, 'glu_force': [-2.225094795227051, 18.632317543029785, 2.9421894550323486], 'glu_force_magnitude': 18.99396700695633, 'asn_force': [-1.990316390991211, 18.064454317092896, -58.507577896118164], 'asn_force_magnitude': 61.2651821215029, 'residue_force': [-4.215411186218262, 36.69677186012268, -55.565388441085815], 'residue_force_magnitude': 66.72282329931444, 'total_force': [-11.906321287155151, 44.637900948524475, -62.33374601602554], 'total_force_magnitude': 77.58736095572286, 'motion_component_total': -39.579097630069555, 'cosine_total_motion': -0.5101230038312083, 'cosine_glu_motion': -0.08941599763732135, 'cosine_asn_motion': -0.6140515241110238, 'cosine_residue_motion': -0.589278765817298, 'cosine_ionic_motion': -0.020116324441538897, 'motion_component_glu': -1.6983645090173667, 'motion_component_asn': -37.619978456648305, 'motion_component_residue': -39.31834296566567, 'motion_component_ionic': -0.2607546644038763}, 6502: {'frame': 6502, 'ionic_force': [-8.320663809776306, 9.290036588907242, -5.847688972949982], 'ionic_force_magnitude': 13.774385372237749, 'motion_vector': [-0.20615386962890625, 0.09394073486328125, -0.17812347412109375], 'ionic_force_x': -8.320663809776306, 'ionic_force_y': 9.290036588907242, 'ionic_force_z': -5.847688972949982, 'radial_force': 12.471496544463157, 'axial_force': -5.847688972949982, 'glu_force': [1.934384047985077, 16.60329246520996, -0.24690335988998413], 'glu_force_magnitude': 16.71741976500925, 'asn_force': [16.836238384246826, 0.9645018577575684, 0.03910636901855469], 'asn_force_magnitude': 16.863887928734044, 'residue_force': [18.770622432231903, 17.56779432296753, -0.20779699087142944], 'residue_force_magnitude': 25.710053353832482, 'total_force': [10.449958622455597, 26.85783091187477, -6.055485963821411], 'total_force_magnitude': 29.44849107781124, 'motion_component_total': 5.022310360760915, 'cosine_total_motion': 0.17054559255652696, 'cosine_glu_motion': 0.2501005666023938, 'cosine_asn_motion': -0.696962482712588, 'cosine_residue_motion': -0.29453307386892913, 'cosine_ionic_motion': 0.9143617710728573, 'motion_component_glu': 4.181036155358871, 'motion_component_asn': -11.753497198997323, 'motion_component_residue': -7.572461043638452, 'motion_component_ionic': 12.594771404399367}, 6503: {'frame': 6503, 'ionic_force': [-9.341202855110168, 8.491201132535934, -6.012524664402008], 'ionic_force_magnitude': 13.982454015427349, 'motion_vector': [-0.2536506652832031, -0.006526947021484375, -0.0059356689453125], 'ionic_force_x': -9.341202855110168, 'ionic_force_y': 8.491201132535934, 'ionic_force_z': -6.012524664402008, 'radial_force': 12.623730330353936, 'axial_force': -6.012524664402008, 'glu_force': [3.123059034347534, 16.97547721862793, 0.5465711951255798], 'glu_force_magnitude': 17.269020371854236, 'asn_force': [23.1798152923584, 3.1644234657287598, 4.686254501342773], 'asn_force_magnitude': 23.85955561425364, 'residue_force': [26.302874326705933, 20.13990068435669, 5.232825696468353], 'residue_force_magnitude': 33.538623439131435, 'total_force': [16.961671471595764, 28.631101816892624, -0.7796989679336548], 'total_force_magnitude': 33.287328232229974, 'motion_component_total': -17.669476464404937, 'cosine_total_motion': -0.530816902490141, 'cosine_glu_motion': -0.20675773652892054, 'cosine_asn_motion': -0.9789277053915527, 'cosine_residue_motion': -0.8028738460941797, 'cosine_ionic_motion': 0.6621017396989426, 'motion_component_glu': -3.5705035641563994, 'motion_component_asn': -23.356780029123456, 'motion_component_residue': -26.927283593279856, 'motion_component_ionic': 9.257807128874914}, 6504: {'frame': 6504, 'ionic_force': [-8.52401351928711, 8.355697363615036, -4.412103891372681], 'ionic_force_magnitude': 12.72568841586099, 'motion_vector': [0.3465385437011719, 0.4995460510253906, -0.39102935791015625], 'ionic_force_x': -8.52401351928711, 'ionic_force_y': 8.355697363615036, 'ionic_force_z': -4.412103891372681, 'radial_force': 11.936351406912946, 'axial_force': -4.412103891372681, 'glu_force': [4.236848592758179, 16.042572021484375, 0.4770299792289734], 'glu_force_magnitude': 16.599474710470613, 'asn_force': [18.614683628082275, 1.9146413803100586, 15.819032669067383], 'asn_force_magnitude': 24.50334860327892, 'residue_force': [22.851532220840454, 17.957213401794434, 16.296062648296356], 'residue_force_magnitude': 33.319899397130456, 'total_force': [14.327518701553345, 26.31291076540947, 11.883958756923676], 'total_force_magnitude': 32.231592278819015, 'motion_component_total': 18.623812524041618, 'cosine_total_motion': 0.5778123638117703, 'cosine_glu_motion': 0.7746908355694081, 'cosine_asn_motion': 0.06895903243732909, 'cosine_residue_motion': 0.43665162284005643, 'cosine_ionic_motion': 0.320188916014844, 'motion_component_glu': 12.859460933467737, 'motion_component_asn': 1.6897272111566934, 'motion_component_residue': 14.54918814462443, 'motion_component_ionic': 4.0746243794171875}, 6505: {'frame': 6505, 'ionic_force': [-8.858786135911942, 7.233338475227356, -8.380332887172699], 'ionic_force_magnitude': 14.178478641901547, 'motion_vector': [0.18931961059570312, -1.0247459411621094, 0.25006103515625], 'ionic_force_x': -8.858786135911942, 'ionic_force_y': 7.233338475227356, 'ionic_force_z': -8.380332887172699, 'radial_force': 11.436751168886646, 'axial_force': -8.380332887172699, 'glu_force': [3.9833587408065796, 22.36219024658203, 3.877466082572937], 'glu_force_magnitude': 23.04277419721402, 'asn_force': [56.45589256286621, -4.4363179206848145, -59.9253044128418], 'asn_force_magnitude': 82.44992923426338, 'residue_force': [60.43925130367279, 17.925872325897217, -56.04783833026886], 'residue_force_magnitude': 84.35401696593254, 'total_force': [51.58046516776085, 25.159210801124573, -64.42817121744156], 'total_force_magnitude': 86.28162910771897, 'motion_component_total': -29.97898549300942, 'cosine_total_motion': -0.34745502377547743, 'cosine_glu_motion': -0.8581686507113183, 'cosine_asn_motion': 0.0028216880162019124, 'cosine_residue_motion': -0.2316657720296116, 'cosine_ionic_motion': -0.7361189653982468, 'motion_component_glu': -19.774586441468735, 'motion_component_asn': 0.2326479772570167, 'motion_component_residue': -19.541938464211718, 'motion_component_ionic': -10.437047028797707}, 6506: {'frame': 6506, 'ionic_force': [-9.954873204231262, 8.362967252731323, -7.493973910808563], 'ionic_force_magnitude': 15.006610768539893, 'motion_vector': [-0.2793464660644531, 0.185546875, -0.166778564453125], 'ionic_force_x': -9.954873204231262, 'ionic_force_y': 8.362967252731323, 'ionic_force_z': -7.493973910808563, 'radial_force': 13.001489214031524, 'axial_force': -7.493973910808563, 'glu_force': [1.001715674996376, 13.158740997314453, 0.8407977223396301], 'glu_force_magnitude': 13.223571368500611, 'asn_force': [22.252627849578857, 6.001870155334473, 6.600922584533691], 'asn_force_magnitude': 23.974446198824992, 'residue_force': [23.254343524575233, 19.160611152648926, 7.4417203068733215], 'residue_force_magnitude': 31.03663502423707, 'total_force': [13.299470320343971, 27.52357840538025, -0.0522536039352417], 'total_force_magnitude': 30.568382513275843, 'motion_component_total': 3.7392105927982033, 'cosine_total_motion': 0.12232281479644089, 'cosine_glu_motion': 0.4081630960287514, 'cosine_asn_motion': -0.6908626051379012, 'cosine_residue_motion': -0.3597578963896971, 'cosine_ionic_motion': 0.9932212776104898, 'motion_component_glu': 5.397373830324362, 'motion_component_asn': -16.563048357658687, 'motion_component_residue': -11.165674527334323, 'motion_component_ionic': 14.904885120132528}, 6507: {'frame': 6507, 'ionic_force': [-8.238221824169159, 7.098378419876099, -6.328981935977936], 'ionic_force_magnitude': 12.582181343547498, 'motion_vector': [0.5045700073242188, 0.26412200927734375, 0.01922607421875], 'ionic_force_x': -8.238221824169159, 'ionic_force_y': 7.098378419876099, 'ionic_force_z': -6.328981935977936, 'radial_force': 10.874524128254059, 'axial_force': -6.328981935977936, 'glu_force': [2.1811296939849854, 13.869128227233887, 1.4779795408248901], 'glu_force_magnitude': 14.117169264712233, 'asn_force': [34.64919185638428, 5.912895679473877, 22.317228317260742], 'asn_force_magnitude': 41.63637245704304, 'residue_force': [36.83032155036926, 19.782023906707764, 23.795207858085632], 'residue_force_magnitude': 48.10418871947278, 'total_force': [28.592099726200104, 26.880402326583862, 17.466225922107697], 'total_force_magnitude': 42.95501418873115, 'motion_component_total': 38.365359227638, 'cosine_total_motion': 0.8931520557547109, 'cosine_glu_motion': 0.5956926090886951, 'cosine_asn_motion': 0.820769768846677, 'cosine_residue_motion': 0.8852320415953007, 'cosine_ionic_motion': -0.3352367802225039, 'motion_component_glu': 8.409493392243165, 'motion_component_asn': 34.17387579718136, 'motion_component_residue': 42.58336918942452, 'motion_component_ionic': -4.218009961786522}, 6508: {'frame': 6508, 'ionic_force': [-7.880868673324585, 5.787855744361877, -7.391227200627327], 'ionic_force_magnitude': 12.257145046666652, 'motion_vector': [-0.12299728393554688, -0.23679351806640625, 0.32021331787109375], 'ionic_force_x': -7.880868673324585, 'ionic_force_y': 5.787855744361877, 'ionic_force_z': -7.391227200627327, 'radial_force': 9.77790187942851, 'axial_force': -7.391227200627327, 'glu_force': [0.3374987840652466, 16.64457607269287, 1.9459850788116455], 'glu_force_magnitude': 16.761344695335847, 'asn_force': [28.803736805915833, 23.728214263916016, -26.18156623840332], 'asn_force_magnitude': 45.5868162612249, 'residue_force': [29.14123558998108, 40.37279033660889, -24.235581159591675], 'residue_force_magnitude': 55.37632350939989, 'total_force': [21.260366916656494, 46.160646080970764, -31.626808360219], 'total_force_magnitude': 59.8586957350185, 'motion_component_total': -56.79436806245683, 'cosine_total_motion': -0.948807309699383, 'cosine_glu_motion': -0.480892259044313, 'cosine_asn_motion': -0.9233640396004629, 'cosine_residue_motion': -0.9056872062323855, 'cosine_ionic_motion': -0.5417852449754305, 'motion_component_glu': -8.060400915160468, 'motion_component_asn': -42.09322681548869, 'motion_component_residue': -50.153627730649156, 'motion_component_ionic': -6.640740331807676}, 6509: {'frame': 6509, 'ionic_force': [-7.748109370470047, 7.134311139583588, -6.899723134934902], 'ionic_force_magnitude': 12.591178403624822, 'motion_vector': [0.30371856689453125, 1.6467742919921875, -0.6300277709960938], 'ionic_force_x': -7.748109370470047, 'ionic_force_y': 7.134311139583588, 'ionic_force_z': -6.899723134934902, 'radial_force': 10.532406859457728, 'axial_force': -6.899723134934902, 'glu_force': [0.8246764540672302, 14.861669540405273, 0.38165515661239624], 'glu_force_magnitude': 14.88942488616238, 'asn_force': [18.72737431526184, 6.037736892700195, -1.6329612731933594], 'asn_force_magnitude': 19.744249239947088, 'residue_force': [19.55205076932907, 20.89940643310547, -1.2513061165809631], 'residue_force_magnitude': 28.646703921043777, 'total_force': [11.803941398859024, 28.033717572689056, -8.151029251515865], 'total_force_magnitude': 31.490659430251068, 'motion_component_total': 30.67700369607958, 'cosine_total_motion': 0.974161997592535, 'cosine_glu_motion': 0.9190846923595447, 'cosine_asn_motion': 0.47160040464692216, 'cosine_residue_motion': 0.8027463992122673, 'cosine_ionic_motion': 0.610027515133175, 'motion_component_glu': 13.6846424909091, 'motion_component_asn': 9.311395931008732, 'motion_component_residue': 22.99603842191783, 'motion_component_ionic': 7.680965274161747}, 6510: {'frame': 6510, 'ionic_force': [-7.857691705226898, 6.3123403787612915, -4.668317198753357], 'ionic_force_magnitude': 11.107751593365249, 'motion_vector': [-0.013092041015625, -2.068023681640625, 0.45330047607421875], 'ionic_force_x': -7.857691705226898, 'ionic_force_y': 6.3123403787612915, 'ionic_force_z': -4.668317198753357, 'radial_force': 10.079134883100426, 'axial_force': -4.668317198753357, 'glu_force': [-3.5615577697753906, 39.58858013153076, 14.60868525505066], 'glu_force_magnitude': 42.348011233813736, 'asn_force': [469.7030258178711, -661.1516205221415, 541.8322277069092], 'asn_force_magnitude': 975.3586831332099, 'residue_force': [466.1414680480957, -621.5630403906107, 556.4409129619598], 'residue_force_magnitude': 955.6437469222478, 'total_force': [458.2837763428688, -615.2507000118494, 551.7725957632065], 'total_force_magnitude': 944.9922967725283, 'motion_component_total': 716.2758181020616, 'cosine_total_motion': 0.7579700073200474, 'cosine_glu_motion': -0.8387617984979163, 'cosine_asn_motion': 0.7780855303615919, 'cosine_residue_motion': 0.7569688877502381, 'cosine_ionic_motion': -0.6407026688815439, 'motion_component_glu': -35.51989406528357, 'motion_component_asn': 758.9124782584875, 'motion_component_residue': 723.3925841932039, 'motion_component_ionic': -7.116766091142337}, 6511: {'frame': 6511, 'ionic_force': [-9.913389056921005, 7.8386406898498535, -6.242726296186447], 'ionic_force_magnitude': 14.095786677853376, 'motion_vector': [-0.5040168762207031, 0.45391082763671875, 0.05902099609375], 'ionic_force_x': -9.913389056921005, 'ionic_force_y': 7.8386406898498535, 'ionic_force_z': -6.242726296186447, 'radial_force': 12.638020828375419, 'axial_force': -6.242726296186447, 'glu_force': [1.9401975870132446, 5.208596229553223, 0.1543828248977661], 'glu_force_magnitude': 5.56036648214769, 'asn_force': [14.662186980247498, 7.6265058517456055, 0.9824576377868652], 'asn_force_magnitude': 16.556223650352603, 'residue_force': [16.602384567260742, 12.835102081298828, 1.1368404626846313], 'residue_force_magnitude': 21.01598022920121, 'total_force': [6.688995510339737, 20.67374277114868, -5.105885833501816], 'total_force_magnitude': 22.320760991725216, 'motion_component_total': 8.388554055344535, 'cosine_total_motion': 0.37581846149664666, 'cosine_glu_motion': 0.3686076048840523, 'cosine_asn_motion': -0.3433434891160181, 'cosine_residue_motion': -0.17295782465500223, 'cosine_ionic_motion': 0.8529805787760929, 'motion_component_glu': 2.0495933712620236, 'motion_component_asn': -5.6844715946972, 'motion_component_residue': -3.6348782234351766, 'motion_component_ionic': 12.023432278779712}, 6512: {'frame': 6512, 'ionic_force': [-8.842867404222488, 8.652108788490295, -5.702980926260352], 'ionic_force_magnitude': 13.62274868966689, 'motion_vector': [0.0037841796875, -0.05219268798828125, -0.3178558349609375], 'ionic_force_x': -8.842867404222488, 'ionic_force_y': 8.652108788490295, 'ionic_force_z': -5.702980926260352, 'radial_force': 12.371551657594596, 'axial_force': -5.702980926260352, 'glu_force': [1.7136732041835785, 14.80975341796875, 0.8006877303123474], 'glu_force_magnitude': 14.930056027799983, 'asn_force': [24.94244956970215, 6.792237281799316, 5.134651184082031], 'asn_force_magnitude': 26.35573790679355, 'residue_force': [26.656122773885727, 21.601990699768066, 5.935338914394379], 'residue_force_magnitude': 34.81986690896534, 'total_force': [17.81325536966324, 30.254099488258362, 0.23235798813402653], 'total_force_magnitude': 35.10949434191442, 'motion_component_total': -4.921825506617761, 'cosine_total_motion': -0.14018502968702648, 'cosine_glu_motion': -0.21228438004485323, 'cosine_asn_motion': -0.22287112026413936, 'cosine_residue_motion': -0.25971812425977725, 'cosine_ionic_motion': 0.3025472397563979, 'motion_component_glu': -3.1694176878964435, 'motion_component_asn': -5.873932832675122, 'motion_component_residue': -9.043350520571565, 'motion_component_ionic': 4.121525013953804}, 6513: {'frame': 6513, 'ionic_force': [-9.518068015575409, 8.962327480316162, -6.766226708889008], 'ionic_force_magnitude': 14.720691440609466, 'motion_vector': [-0.08514022827148438, 0.5365028381347656, 0.13083648681640625], 'ionic_force_x': -9.518068015575409, 'ionic_force_y': 8.962327480316162, 'ionic_force_z': -6.766226708889008, 'radial_force': 13.073520283900196, 'axial_force': -6.766226708889008, 'glu_force': [1.5315049886703491, 14.068401336669922, 1.8692872524261475], 'glu_force_magnitude': 14.274440743231278, 'asn_force': [43.200369358062744, 15.308669090270996, 13.813036918640137], 'asn_force_magnitude': 47.86885470641825, 'residue_force': [44.73187434673309, 29.377070426940918, 15.682324171066284], 'residue_force_magnitude': 55.76637105682756, 'total_force': [35.213806331157684, 38.33939790725708, 8.916097462177277], 'total_force_magnitude': 52.81494468589656, 'motion_component_total': 33.53487553365118, 'cosine_total_motion': 0.634950499959648, 'cosine_glu_motion': 0.9606389194451976, 'cosine_asn_motion': 0.23712424783761368, 'cosine_residue_motion': 0.4494366232443071, 'cosine_ionic_motion': 0.575477454266293, 'motion_component_glu': 13.712583331262199, 'motion_component_asn': 11.35086616710744, 'motion_component_residue': 25.06344949836964, 'motion_component_ionic': 8.471426035281546}, 6514: {'frame': 6514, 'ionic_force': [-7.190410137176514, 8.119710952043533, -4.648743212223053], 'ionic_force_magnitude': 11.800106666413502, 'motion_vector': [-0.034603118896484375, 0.70941162109375, -0.40940093994140625], 'ionic_force_x': -7.190410137176514, 'ionic_force_y': 8.119710952043533, 'ionic_force_z': -4.648743212223053, 'radial_force': 10.845815040168556, 'axial_force': -4.648743212223053, 'glu_force': [3.0865814685821533, 18.94169521331787, 2.2641639709472656], 'glu_force_magnitude': 19.32462784127445, 'asn_force': [45.49425029754639, 14.21488332748413, -16.488208770751953], 'asn_force_magnitude': 50.434618533480425, 'residue_force': [48.58083176612854, 33.156578540802, -14.224044799804688], 'residue_force_magnitude': 60.51263806915136, 'total_force': [41.390421628952026, 41.276289492845535, -18.87278801202774], 'total_force_magnitude': 61.42541171426162, 'motion_component_total': 43.39619343996504, 'cosine_total_motion': 0.7064860003191383, 'cosine_glu_motion': 0.7829473158595802, 'cosine_asn_motion': 0.3690839877203677, 'cosine_residue_motion': 0.5576483971371653, 'cosine_ionic_motion': 0.8179093703984975, 'motion_component_glu': 15.130165498311143, 'motion_component_asn': 18.61461012749252, 'motion_component_residue': 33.74477562580366, 'motion_component_ionic': 9.65141781416138}, 6515: {'frame': 6515, 'ionic_force': [-6.9467833042144775, 6.8754576444625854, -4.343690901994705], 'ionic_force_magnitude': 10.695670467464094, 'motion_vector': [-0.9353866577148438, -0.8836402893066406, 0.4879302978515625], 'ionic_force_x': -6.9467833042144775, 'ionic_force_y': 6.8754576444625854, 'ionic_force_z': -4.343690901994705, 'radial_force': 9.773930432354838, 'axial_force': -4.343690901994705, 'glu_force': [5.9062042236328125, 26.99496555328369, 8.591544389724731], 'glu_force_magnitude': 28.938314542399347, 'asn_force': [49.67412567138672, -162.68043851852417, -178.85716819763184], 'asn_force_magnitude': 246.82449322032855, 'residue_force': [55.58032989501953, -135.68547296524048, -170.2656238079071], 'residue_force_magnitude': 224.7000295855253, 'total_force': [48.633546590805054, -128.8100153207779, -174.6093147099018], 'total_force_magnitude': 222.36378905838194, 'motion_component_total': -12.256203442724619, 'cosine_total_motion': -0.05511780265404065, 'cosine_glu_motion': -0.6324407661122937, 'cosine_asn_motion': 0.029489138489490387, 'cosine_residue_motion': -0.04905708368776784, 'cosine_ionic_motion': -0.11528732962132443, 'motion_component_glu': -18.301769819193574, 'motion_component_asn': 7.27864166317255, 'motion_component_residue': -11.023128156021023, 'motion_component_ionic': -1.2330752867035981}, 6516: {'frame': 6516, 'ionic_force': [-7.070002973079681, 8.471872210502625, -5.481831818819046], 'ionic_force_magnitude': 12.321040576195628, 'motion_vector': [-0.17266464233398438, 0.45489501953125, -0.0809326171875], 'ionic_force_x': -7.070002973079681, 'ionic_force_y': 8.471872210502625, 'ionic_force_z': -5.481831818819046, 'radial_force': 11.034380852156689, 'axial_force': -5.481831818819046, 'glu_force': [6.1050180196762085, 13.263955116271973, 0.9374845027923584], 'glu_force_magnitude': 14.631562716949427, 'asn_force': [-2.8178529739379883, 1.4964325428009033, 32.67200469970703], 'asn_force_magnitude': 32.827419893064445, 'residue_force': [3.28716504573822, 14.760387659072876, 33.60948920249939], 'residue_force_magnitude': 36.85474545207112, 'total_force': [-3.782837927341461, 23.2322598695755, 28.127657383680344], 'total_force_magnitude': 36.67714371820315, 'motion_component_total': 18.134842117438005, 'cosine_total_motion': 0.4944453214997095, 'cosine_glu_motion': 0.6794693874722222, 'cosine_asn_motion': -0.09121572630490409, 'cosine_residue_motion': 0.188505494301133, 'cosine_ionic_motion': 0.9080012389754891, 'motion_component_glu': 9.94169895704703, 'motion_component_asn': -2.9943769482619302, 'motion_component_residue': 6.9473220087851, 'motion_component_ionic': 11.187520108652905}, 6517: {'frame': 6517, 'ionic_force': [-5.969686806201935, 6.511586420238018, -3.3341631777584553], 'ionic_force_magnitude': 9.442169367697764, 'motion_vector': [-0.13305282592773438, -0.13154983520507812, -0.19814300537109375], 'ionic_force_x': -5.969686806201935, 'ionic_force_y': 6.511586420238018, 'ionic_force_z': -3.3341631777584553, 'radial_force': 8.833907304945509, 'axial_force': -3.3341631777584553, 'glu_force': [9.087771832942963, 14.550921440124512, 1.424428939819336], 'glu_force_magnitude': 17.214700388008545, 'asn_force': [-6.729728698730469, 9.10070514678955, 23.480726718902588], 'asn_force_magnitude': 26.06638850656347, 'residue_force': [2.358043134212494, 23.651626586914062, 24.905155658721924], 'residue_force_magnitude': 34.427119920417326, 'total_force': [-3.611643671989441, 30.16321300715208, 21.57099248096347], 'total_force_magnitude': 37.25816830631952, 'motion_component_total': -28.480358690282166, 'cosine_total_motion': -0.7644057661699781, 'cosine_glu_motion': -0.7259150529211152, 'cosine_asn_motion': -0.6974289200687955, 'cosine_residue_motion': -0.8910377458329294, 'cosine_ionic_motion': 0.23252120922945732, 'motion_component_glu': -12.496410143182366, 'motion_component_asn': -18.179453186226226, 'motion_component_residue': -30.675863329408593, 'motion_component_ionic': 2.1955046391264244}, 6518: {'frame': 6518, 'ionic_force': [-6.401425421237946, 8.129929726943374, -4.4058263301849365], 'ionic_force_magnitude': 11.246568829668, 'motion_vector': [1.0821189880371094, -0.35472869873046875, 0.2816925048828125], 'ionic_force_x': -6.401425421237946, 'ionic_force_y': 8.129929726943374, 'ionic_force_z': -4.4058263301849365, 'radial_force': 10.347656970962507, 'axial_force': -4.4058263301849365, 'glu_force': [7.954393357038498, 12.848433494567871, 1.9196135997772217], 'glu_force_magnitude': 15.232843901100063, 'asn_force': [-16.768634796142578, 11.704121828079224, 30.165756225585938], 'asn_force_magnitude': 36.443743349914, 'residue_force': [-8.81424143910408, 24.552555322647095, 32.08536982536316], 'residue_force_magnitude': 41.35202270565238, 'total_force': [-15.215666860342026, 32.68248504959047, 27.679543495178223], 'total_force_magnitude': 45.45127583603213, 'motion_component_total': -17.271715197800035, 'cosine_total_motion': -0.3800050687269738, 'cosine_glu_motion': 0.25689541930248583, 'cosine_asn_motion': -0.32279011283736025, 'cosine_residue_motion': -0.1898439711854543, 'cosine_ionic_motion': -0.8377028704038997, 'motion_component_glu': 3.9132478211424147, 'motion_component_asn': -11.763680028134537, 'motion_component_residue': -7.850432206992123, 'motion_component_ionic': -9.42128299080791}, 6519: {'frame': 6519, 'ionic_force': [-7.852996408939362, 10.710128724575043, -3.5803879499435425], 'ionic_force_magnitude': 13.754838703811936, 'motion_vector': [-0.20067977905273438, 0.5549964904785156, 0.33962249755859375], 'ionic_force_x': -7.852996408939362, 'ionic_force_y': 10.710128724575043, 'ionic_force_z': -3.5803879499435425, 'radial_force': 13.280678066114769, 'axial_force': -3.5803879499435425, 'glu_force': [3.4995651245117188, 16.404654502868652, 1.4007641077041626], 'glu_force_magnitude': 16.83216520548143, 'asn_force': [32.96016883850098, 8.857699871063232, 14.641231536865234], 'asn_force_magnitude': 37.137544854021, 'residue_force': [36.459733963012695, 25.262354373931885, 16.041995644569397], 'residue_force_magnitude': 47.16825599307399, 'total_force': [28.606737554073334, 35.97248309850693, 12.461607694625854], 'total_force_magnitude': 47.61991852255477, 'motion_component_total': 27.105022287564452, 'cosine_total_motion': 0.5691950580454351, 'cosine_glu_motion': 0.7746123861912061, 'cosine_asn_motion': 0.1294739355712791, 'cosine_residue_motion': 0.37836352793938605, 'cosine_ionic_motion': 0.6730921926922415, 'motion_component_glu': 13.038403654582563, 'motion_component_asn': 4.8083440897050025, 'motion_component_residue': 17.846747744287565, 'motion_component_ionic': 9.258274543276885}, 6520: {'frame': 6520, 'ionic_force': [-8.18613851070404, 11.724495336413383, -4.51964670419693], 'ionic_force_magnitude': 14.996795022296235, 'motion_vector': [0.20529937744140625, -0.8965682983398438, -0.5561676025390625], 'ionic_force_x': -8.18613851070404, 'ionic_force_y': 11.724495336413383, 'ionic_force_z': -4.51964670419693, 'radial_force': 14.299533370359011, 'axial_force': -4.51964670419693, 'glu_force': [7.752428770065308, 21.772496223449707, -0.2848648428916931], 'glu_force_magnitude': 23.113262245165302, 'asn_force': [8.307072967290878, -7.535544157028198, 8.230011940002441], 'asn_force_magnitude': 13.911325729742634, 'residue_force': [16.059501737356186, 14.236952066421509, 7.945147097110748], 'residue_force_magnitude': 22.885011745429743, 'total_force': [7.873363226652145, 25.961447402834892, 3.4255003929138184], 'total_force_magnitude': 27.34448121085521, 'motion_component_total': -21.92393410132354, 'cosine_total_motion': -0.8017681495679712, 'cosine_glu_motion': -0.7153041699446999, 'cosine_asn_motion': 0.25977418287387527, 'cosine_residue_motion': -0.5645271120927418, 'cosine_ionic_motion': -0.6004432611821384, 'motion_component_glu': -16.533012864992138, 'motion_component_asn': 3.6138032741362096, 'motion_component_residue': -12.919209590855928, 'motion_component_ionic': -9.00472451046761}, 6521: {'frame': 6521, 'ionic_force': [-6.109072804450989, 11.851601839065552, -4.16014552116394], 'ionic_force_magnitude': 13.96739229201661, 'motion_vector': [-0.6643180847167969, 0.7580108642578125, -0.02217864990234375], 'ionic_force_x': -6.109072804450989, 'ionic_force_y': 11.851601839065552, 'ionic_force_z': -4.16014552116394, 'radial_force': 13.333463041604181, 'axial_force': -4.16014552116394, 'glu_force': [2.4853821992874146, 13.518867492675781, 1.7603836059570312], 'glu_force_magnitude': 13.857700148335688, 'asn_force': [38.435476303100586, 1.742910385131836, 36.7315731048584], 'asn_force_magnitude': 53.19334580579007, 'residue_force': [40.920858502388, 15.261777877807617, 38.49195671081543], 'residue_force_magnitude': 58.21571313650025, 'total_force': [34.81178569793701, 27.11337971687317, 34.33181118965149], 'total_force_magnitude': 55.90768321717795, 'motion_component_total': -3.30829247941508, 'cosine_total_motion': -0.05917420091552977, 'cosine_glu_motion': 0.6125143850499072, 'cosine_asn_motion': -0.4666800678123039, 'cosine_residue_motion': -0.2806155359626276, 'cosine_ionic_motion': 0.9327396833607189, 'motion_component_glu': 8.488040684563842, 'motion_component_asn': -24.82427422780944, 'motion_component_residue': -16.336233543245598, 'motion_component_ionic': 13.027941063830518}, 6522: {'frame': 6522, 'ionic_force': [-5.653996646404266, 6.742477625608444, -4.252717904746532], 'ionic_force_magnitude': 9.773141367376864, 'motion_vector': [0.6198005676269531, -0.474945068359375, 0.15839385986328125], 'ionic_force_x': -5.653996646404266, 'ionic_force_y': 6.742477625608444, 'ionic_force_z': -4.252717904746532, 'radial_force': 8.799356942946522, 'axial_force': -4.252717904746532, 'glu_force': [7.8894155621528625, 16.059277534484863, 2.5062453746795654], 'glu_force_magnitude': 18.067222772746582, 'asn_force': [3.0838565826416016, 19.16446280479431, 38.87880754470825], 'asn_force_magnitude': 43.45513182717445, 'residue_force': [10.973272144794464, 35.223740339279175, 41.38505291938782], 'residue_force_magnitude': 55.4422870216698, 'total_force': [5.319275498390198, 41.96621796488762, 37.132335014641285], 'total_force_magnitude': 56.28737376840197, 'motion_component_total': -13.496320076352376, 'cosine_total_motion': -0.23977526704095053, 'cosine_glu_motion': -0.1625856178423463, 'cosine_asn_motion': -0.029821996682133565, 'cosine_residue_motion': -0.07635668731918203, 'cosine_ionic_motion': -0.9477946091006545, 'motion_component_glu': -2.937470577202312, 'motion_component_asn': -1.295918797171673, 'motion_component_residue': -4.233389374373985, 'motion_component_ionic': -9.26293070197839}, 6523: {'frame': 6523, 'ionic_force': [-6.722442984580994, 8.549417868256569, -5.158254951238632], 'ionic_force_magnitude': 12.037083521725052, 'motion_vector': [-0.4757804870605469, 0.21879196166992188, 0.0498046875], 'ionic_force_x': -6.722442984580994, 'ionic_force_y': 8.549417868256569, 'ionic_force_z': -5.158254951238632, 'radial_force': 10.87583493654657, 'axial_force': -5.158254951238632, 'glu_force': [3.4419965744018555, 15.669902801513672, 1.6421400308609009], 'glu_force_magnitude': 16.12730039740179, 'asn_force': [36.404226303100586, 10.063498497009277, 24.31576156616211], 'asn_force_magnitude': 44.91990600245191, 'residue_force': [39.84622287750244, 25.73340129852295, 25.95790159702301], 'residue_force_magnitude': 54.07163836351874, 'total_force': [33.12377989292145, 34.28281916677952, 20.799646645784378], 'total_force_magnitude': 52.01078527580892, 'motion_component_total': -13.730764297232273, 'cosine_total_motion': -0.2639984038775642, 'cosine_glu_motion': 0.2207318915159569, 'cosine_asn_motion': -0.5885645511974676, 'cosine_residue_motion': -0.4231137706719966, 'cosine_ionic_motion': 0.7599590449512609, 'motion_component_glu': 3.5598095217645405, 'motion_component_asn': -26.438264316165544, 'motion_component_residue': -22.878454794401, 'motion_component_ionic': 9.14769049716873}, 6524: {'frame': 6524, 'ionic_force': [-6.786805152893066, 7.711427450180054, -5.358022391796112], 'ionic_force_magnitude': 11.585993330470842, 'motion_vector': [0.6155433654785156, -0.20136642456054688, -0.29674530029296875], 'ionic_force_x': -6.786805152893066, 'ionic_force_y': 7.711427450180054, 'ionic_force_z': -5.358022391796112, 'radial_force': 10.272625638205955, 'axial_force': -5.358022391796112, 'glu_force': [6.157494306564331, 15.414989471435547, 1.3578473329544067], 'glu_force_magnitude': 16.654740644016414, 'asn_force': [9.74406623840332, 6.530340194702148, 34.181721687316895], 'asn_force_magnitude': 36.13837665731714, 'residue_force': [15.901560544967651, 21.945329666137695, 35.5395690202713], 'residue_force_magnitude': 44.69360231696884, 'total_force': [9.114755392074585, 29.65675711631775, 30.18154662847519], 'total_force_magnitude': 43.2842669500182, 'motion_component_total': -13.079319635036033, 'cosine_total_</t>
+          <t>{6500: {'frame': 6500, 'ionic_force': [-6.2898120284080505, 8.96427071094513, -9.324965059757233], 'ionic_force_magnitude': 14.383144930699562, 'motion_vector': [-0.07231521606445312, 0.7506103515625, -0.3880615234375], 'ionic_force_x': -6.2898120284080505, 'ionic_force_y': 8.96427071094513, 'ionic_force_z': -9.324965059757233, 'radial_force': 10.950793794598422, 'axial_force': -9.324965059757233, 'glu_force': [1.275538682937622, 6.072243690490723, -0.026713132858276367], 'glu_force_magnitude': 6.204825215897845, 'asn_force': [9.176877975463867, 7.638951301574707, -4.474958419799805], 'asn_force_magnitude': 12.751232066875769, 'residue_force': [10.45241665840149, 13.71119499206543, -4.501671552658081], 'residue_force_magnitude': 17.81894859073565, 'total_force': [4.162604629993439, 22.67546570301056, -13.826636612415314], 'total_force_magnitude': 26.88270637725738, 'motion_component_total': 26.041228518789573, 'cosine_total_motion': 0.9686981717294768, 'cosine_glu_motion': 0.8506009999111716, 'cosine_asn_motion': 0.6294413349467401, 'cosine_residue_motion': 0.7466199815079814, 'cosine_ionic_motion': 0.88556748283168, 'motion_component_glu': 5.277830532916758, 'motion_component_asn': 8.026152534389965, 'motion_component_residue': 13.303983067306723, 'motion_component_ionic': 12.737245451482849, 'ionic_contributions': [{'ion_id': 1327, 'distance': 9.480656623840332, 'force': [1.0468125343322754, 3.485199213027954, -0.6332185864448547], 'magnitude': 3.6936967372894287}, {'ion_id': 1330, 'distance': 6.843091011047363, 'force': [0.373801052570343, 6.2043938636779785, -3.4104108810424805], 'magnitude': 7.0897908210754395}, {'ion_id': 1341, 'distance': 6.828861236572266, 'force': [-6.430893898010254, -2.644869804382324, -1.5276371240615845], 'magnitude': 7.119368553161621}, {'ion_id': 1359, 'distance': 14.824708938598633, 'force': [-0.3260658383369446, 0.5594664812088013, -1.3648301362991333], 'magnitude': 1.510656476020813}, {'ion_id': 1465, 'distance': 10.682046890258789, 'force': [-0.9534658789634705, 1.3600809574127197, -2.3888683319091797], 'magnitude': 2.909572124481201}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 4.882998466491699, 'force': [4.382442951202393, -10.2682523727417, -1.0584074258804321], 'magnitude': 11.214411735534668}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 4.038802623748779, 'force': [-3.1069042682647705, 16.340496063232422, 1.0316942930221558], 'magnitude': 16.665205001831055}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 2.782015323638916, 'force': [-4.050301551818848, -13.726561546325684, 27.02996826171875], 'magnitude': 30.585006713867188}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.407395362854004, 'force': [6.912156581878662, 9.592981338500977, -12.158613204956055], 'magnitude': 16.959808349609375}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 2.083928108215332, 'force': [-18.50306510925293, 44.984893798828125, -50.70583724975586], 'magnitude': 70.26439666748047}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 2.333038806915283, 'force': [5.486478328704834, -23.15191078186035, 9.429458618164062], 'magnitude': 25.593496322631836}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 2.1227025985717773, 'force': [19.33160972595215, -10.06045150756836, 21.930065155029297], 'magnitude': 30.91684913635254}]}, 6501: {'frame': 6501, 'ionic_force': [-7.69091010093689, 7.941129088401794, -6.768357574939728], 'ionic_force_magnitude': 12.96234136418256, 'motion_vector': [-0.7340888977050781, -0.2639427185058594, 0.5615005493164062], 'ionic_force_x': -7.69091010093689, 'ionic_force_y': 7.941129088401794, 'ionic_force_z': -6.768357574939728, 'radial_force': 11.05493687812618, 'axial_force': -6.768357574939728, 'glu_force': [-2.225094795227051, 18.632317543029785, 2.9421894550323486], 'glu_force_magnitude': 18.99396700695633, 'asn_force': [-1.990316390991211, 18.064454317092896, -58.507577896118164], 'asn_force_magnitude': 61.2651821215029, 'residue_force': [-4.215411186218262, 36.69677186012268, -55.565388441085815], 'residue_force_magnitude': 66.72282329931444, 'total_force': [-11.906321287155151, 44.637900948524475, -62.33374601602554], 'total_force_magnitude': 77.58736095572286, 'motion_component_total': -39.579097630069555, 'cosine_total_motion': -0.5101230038312083, 'cosine_glu_motion': -0.08941599763732135, 'cosine_asn_motion': -0.6140515241110238, 'cosine_residue_motion': -0.589278765817298, 'cosine_ionic_motion': -0.020116324441538897, 'motion_component_glu': -1.6983645090173667, 'motion_component_asn': -37.619978456648305, 'motion_component_residue': -39.31834296566567, 'motion_component_ionic': -0.2607546644038763, 'ionic_contributions': [{'ion_id': 1327, 'distance': 9.900136947631836, 'force': [1.086919903755188, 3.0864734649658203, -0.8753246665000916], 'magnitude': 3.387315511703491}, {'ion_id': 1330, 'distance': 7.9911088943481445, 'force': [-2.163508176803589, 4.191789627075195, -2.1859216690063477], 'magnitude': 5.199049949645996}, {'ion_id': 1341, 'distance': 7.409305572509766, 'force': [-5.77974796295166, -0.7983136177062988, -1.5908108949661255], 'magnitude': 6.047600269317627}, {'ion_id': 1465, 'distance': 11.081165313720703, 'force': [-0.8345738649368286, 1.4611796140670776, -2.116300344467163], 'magnitude': 2.703754186630249}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 4.234692096710205, 'force': [6.464458465576172, -13.100109100341797, -2.9891550540924072], 'magnitude': 14.91097354888916}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 5.420766830444336, 'force': [-3.73416805267334, 8.36577320098877, 1.2857370376586914], 'magnitude': 9.251123428344727}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 3.3423523902893066, 'force': [-4.955385208129883, 23.366653442382812, 4.6456074714660645], 'magnitude': 24.333885192871094}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 2.1747500896453857, 'force': [-10.143157958984375, -11.460227966308594, 47.6533088684082], 'magnitude': 50.05055618286133}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.7822988033294678, 'force': [13.35721206665039, 10.757869720458984, -18.78488540649414], 'magnitude': 25.43656349182129}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 1.3463107347488403, 'force': [-59.578208923339844, 72.97209167480469, -139.52366638183594], 'magnitude': 168.348876953125}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 1.501520037651062, 'force': [17.60514259338379, -55.95954895019531, 19.402860641479492], 'magnitude': 61.789024353027344}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 1.6815459728240967, 'force': [36.76869583129883, 1.7542698383331299, 32.74480438232422], 'magnitude': 49.26699447631836}]}, 6502: {'frame': 6502, 'ionic_force': [-8.320663809776306, 9.290036588907242, -5.847688972949982], 'ionic_force_magnitude': 13.774385372237749, 'motion_vector': [-0.20615386962890625, 0.09394073486328125, -0.17812347412109375], 'ionic_force_x': -8.320663809776306, 'ionic_force_y': 9.290036588907242, 'ionic_force_z': -5.847688972949982, 'radial_force': 12.471496544463157, 'axial_force': -5.847688972949982, 'glu_force': [1.934384047985077, 16.60329246520996, -0.24690335988998413], 'glu_force_magnitude': 16.71741976500925, 'asn_force': [16.836238384246826, 0.9645018577575684, 0.03910636901855469], 'asn_force_magnitude': 16.863887928734044, 'residue_force': [18.770622432231903, 17.56779432296753, -0.20779699087142944], 'residue_force_magnitude': 25.710053353832482, 'total_force': [10.449958622455597, 26.85783091187477, -6.055485963821411], 'total_force_magnitude': 29.44849107781124, 'motion_component_total': 5.022310360760915, 'cosine_total_motion': 0.17054559255652696, 'cosine_glu_motion': 0.2501005666023938, 'cosine_asn_motion': -0.696962482712588, 'cosine_residue_motion': -0.29453307386892913, 'cosine_ionic_motion': 0.9143617710728573, 'motion_component_glu': 4.181036155358871, 'motion_component_asn': -11.753497198997323, 'motion_component_residue': -7.572461043638452, 'motion_component_ionic': 12.594771404399367, 'ionic_contributions': [{'ion_id': 1327, 'distance': 9.086702346801758, 'force': [1.2445228099822998, 3.7574269771575928, -0.7076037526130676], 'magnitude': 4.0209197998046875}, {'ion_id': 1330, 'distance': 7.715169906616211, 'force': [-2.6883904933929443, 4.354552745819092, -2.218109607696533], 'magnitude': 5.577596664428711}, {'ion_id': 1341, 'distance': 7.420594215393066, 'force': [-5.975593090057373, -0.20818576216697693, -0.7748332023620605], 'magnitude': 6.029213905334473}, {'ion_id': 1465, 'distance': 11.068405151367188, 'force': [-0.9012030363082886, 1.3862426280975342, -2.1471424102783203], 'magnitude': 2.709991931915283}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 4.143868446350098, 'force': [4.140351295471191, -14.972335815429688, -1.0800418853759766], 'magnitude': 15.57176399230957}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 5.370075702667236, 'force': [-2.552300453186035, 9.068246841430664, 0.33683720231056213], 'magnitude': 9.426600456237793}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 3.4746975898742676, 'force': [0.34633320569992065, 22.507381439208984, 0.4963013231754303], 'magnitude': 22.51551628112793}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 2.981372594833374, 'force': [-10.494219779968262, -6.805779457092285, 23.511438369750977], 'magnitude': 26.631465911865234}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.7065768241882324, 'force': [8.488018989562988, 5.570678234100342, -10.116313934326172], 'magnitude': 14.332436561584473}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 1.896828532218933, 'force': [11.519098281860352, 37.893272399902344, -74.99378204345703], 'magnitude': 84.80953216552734}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 1.9487519264221191, 'force': [-5.76513147354126, -30.565887451171875, 19.444923400878906], 'magnitude': 36.6826286315918}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 1.7698607444763184, 'force': [13.088472366333008, -5.127781867980957, 42.192840576171875], 'magnitude': 44.47289276123047}]}, 6503: {'frame': 6503, 'ionic_force': [-9.341202855110168, 8.491201132535934, -6.012524664402008], 'ionic_force_magnitude': 13.982454015427349, 'motion_vector': [-0.2536506652832031, -0.006526947021484375, -0.0059356689453125], 'ionic_force_x': -9.341202855110168, 'ionic_force_y': 8.491201132535934, 'ionic_force_z': -6.012524664402008, 'radial_force': 12.623730330353936, 'axial_force': -6.012524664402008, 'glu_force': [3.123059034347534, 16.97547721862793, 0.5465711951255798], 'glu_force_magnitude': 17.269020371854236, 'asn_force': [23.1798152923584, 3.1644234657287598, 4.686254501342773], 'asn_force_magnitude': 23.85955561425364, 'residue_force': [26.302874326705933, 20.13990068435669, 5.232825696468353], 'residue_force_magnitude': 33.538623439131435, 'total_force': [16.961671471595764, 28.631101816892624, -0.7796989679336548], 'total_force_magnitude': 33.287328232229974, 'motion_component_total': -17.669476464404937, 'cosine_total_motion': -0.530816902490141, 'cosine_glu_motion': -0.20675773652892054, 'cosine_asn_motion': -0.9789277053915527, 'cosine_residue_motion': -0.8028738460941797, 'cosine_ionic_motion': 0.6621017396989426, 'motion_component_glu': -3.5705035641563994, 'motion_component_asn': -23.356780029123456, 'motion_component_residue': -26.927283593279856, 'motion_component_ionic': 9.257807128874914, 'ionic_contributions': [{'ion_id': 1327, 'distance': 9.088233947753906, 'force': [0.7046208381652832, 3.886070966720581, -0.7475728988647461], 'magnitude': 4.019565105438232}, {'ion_id': 1330, 'distance': 7.998379707336426, 'force': [-2.498203992843628, 3.7735369205474854, -2.5399537086486816], 'magnitude': 5.189601898193359}, {'ion_id': 1341, 'distance': 7.14366340637207, 'force': [-6.450554847717285, -0.43755224347114563, -0.7234833836555481], 'magnitude': 6.505731105804443}, {'ion_id': 1465, 'distance': 11.2750244140625, 'force': [-1.0970648527145386, 1.2691454887390137, -2.0015146732330322], 'magnitude': 2.6115784645080566}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 4.01923131942749, 'force': [3.6885898113250732, -16.02198028564453, -1.9172371625900269], 'magnitude': 16.55250358581543}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 5.236320972442627, 'force': [-2.3625972270965576, 9.603191375732422, 0.700569212436676], 'magnitude': 9.91433048248291}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 3.399014711380005, 'force': [1.7970664501190186, 23.39426612854004, 1.7632391452789307], 'magnitude': 23.529346466064453}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 2.893994092941284, 'force': [-13.48714828491211, -6.52357816696167, 23.966407775878906], 'magnitude': 28.263916015625}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.6775176525115967, 'force': [9.507019996643066, 5.331854820251465, -9.652809143066406], 'magnitude': 14.559836387634277}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 1.7408254146575928, 'force': [26.825870513916016, 43.58721160888672, -86.7132797241211], 'magnitude': 100.6909408569336}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 1.8258906602859497, 'force': [-11.726789474487305, -35.0107421875, 19.56388282775879], 'magnitude': 41.78534698486328}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 1.5375877618789673, 'force': [12.06086254119873, -4.220322608947754, 57.52205276489258], 'magnitude': 58.92420959472656}]}, 6504: {'frame': 6504, 'ionic_force': [-8.52401351928711, 8.355697363615036, -4.412103891372681], 'ionic_force_magnitude': 12.72568841586099, 'motion_vector': [0.3465385437011719, 0.4995460510253906, -0.39102935791015625], 'ionic_force_x': -8.52401351928711, 'ionic_force_y': 8.355697363615036, 'ionic_force_z': -4.412103891372681, 'radial_force': 11.936351406912946, 'axial_force': -4.412103891372681, 'glu_force': [4.236848592758179, 16.042572021484375, 0.4770299792289734], 'glu_force_magnitude': 16.599474710470613, 'asn_force': [18.614683628082275, 1.9146413803100586, 15.819032669067383], 'asn_force_magnitude': 24.50334860327892, 'residue_force': [22.851532220840454, 17.957213401794434, 16.296062648296356], 'residue_force_magnitude': 33.319899397130456, 'total_force': [14.327518701553345, 26.31291076540947, 11.883958756923676], 'total_force_magnitude': 32.231592278819015, 'motion_component_total': 18.623812524041618, 'cosine_total_motion': 0.5778123638117703, 'cosine_glu_motion': 0.7746908355694081, 'cosine_asn_motion': 0.06895903243732909, 'cosine_residue_motion': 0.43665162284005643, 'cosine_ionic_motion': 0.320188916014844, 'motion_component_glu': 12.859460933467737, 'motion_component_asn': 1.6897272111566934, 'motion_component_residue': 14.54918814462443, 'motion_component_ionic': 4.0746243794171875, 'ionic_contributions': [{'ion_id': 1327, 'distance': 9.408270835876465, 'force': [0.9622269868850708, 3.594086170196533, -0.4741421937942505], 'magnitude': 3.7507529258728027}, {'ion_id': 1330, 'distance': 8.226515769958496, 'force': [-2.706892490386963, 3.7393572330474854, -1.6602444648742676], 'magnitude': 4.905758857727051}, {'ion_id': 1341, 'distance': 7.617783069610596, 'force': [-5.697000026702881, -0.46980372071266174, -0.2337888479232788], 'magnitude': 5.72111701965332}, {'ion_id': 1465, 'distance': 10.982931137084961, 'force': [-1.0823479890823364, 1.4920576810836792, -2.043928384780884], 'magnitude': 2.7523365020751953}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.9775094985961914, 'force': [2.72805118560791, -16.559207916259766, -2.003427028656006], 'magnitude': 16.901578903198242}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 5.1885504722595215, 'force': [-1.9348127841949463, 9.883590698242188, 0.7316498160362244], 'magnitude': 10.09773063659668}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 3.4346113204956055, 'force': [3.443610191345215, 22.718189239501953, 1.7488071918487549], 'magnitude': 23.044151306152344}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.0198965072631836, 'force': [-14.049777030944824, -5.797299385070801, 21.041074752807617], 'magnitude': 25.956342697143555}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.8464739322662354, 'force': [9.186090469360352, 4.682243347167969, -8.415327072143555], 'magnitude': 13.308845520019531}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 1.82269287109375, 'force': [36.153018951416016, 38.30272674560547, -75.24677276611328], 'magnitude': 91.848876953125}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 1.9152203798294067, 'force': [-15.191081047058105, -30.466201782226562, 16.834383010864258], 'magnitude': 37.97834777832031}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 1.500850796699524, 'force': [2.516432285308838, -4.806827545166016, 61.605674743652344], 'magnitude': 61.84413528442383}]}, 6505: {'frame': 6505, 'ionic_force': [-8.858786135911942, 7.233338475227356, -8.380332887172699], 'ionic_force_magnitude': 14.178478641901547, 'motion_vector': [0.18931961059570312, -1.0247459411621094, 0.25006103515625], 'ionic_force_x': -8.858786135911942, 'ionic_force_y': 7.233338475227356, 'ionic_force_z': -8.380332887172699, 'radial_force': 11.436751168886646, 'axial_force': -8.380332887172699, 'glu_force': [3.9833587408065796, 22.36219024658203, 3.877466082572937], 'glu_force_magnitude': 23.04277419721402, 'asn_force': [56.45589256286621, -4.4363179206848145, -59.9253044128418], 'asn_force_magnitude': 82.44992923426338, 'residue_force': [60.43925130367279, 17.925872325897217, -56.04783833026886], 'residue_force_magnitude': 84.35401696593254, 'total_force': [51.58046516776085, 25.159210801124573, -64.42817121744156], 'total_force_magnitude': 86.28162910771897, 'motion_component_total': -29.97898549300942, 'cosine_total_motion': -0.34745502377547743, 'cosine_glu_motion': -0.8581686507113183, 'cosine_asn_motion': 0.0028216880162019124, 'cosine_residue_motion': -0.2316657720296116, 'cosine_ionic_motion': -0.7361189653982468, 'motion_component_glu': -19.774586441468735, 'motion_component_asn': 0.2326479772570167, 'motion_component_residue': -19.541938464211718, 'motion_component_ionic': -10.437047028797707, 'ionic_contributions': [{'ion_id': 1327, 'distance': 10.268755912780762, 'force': [0.760402500629425, 3.0018088817596436, -0.5691439509391785], 'magnitude': 3.1484906673431396}, {'ion_id': 1330, 'distance': 9.006739616394043, 'force': [-1.6843782663345337, 3.5646517276763916, -1.0980793237686157], 'magnitude': 4.0926337242126465}, {'ion_id': 1341, 'distance': 6.801566123962402, 'force': [-6.166740417480469, -2.169691801071167, -2.961028814315796], 'magnitude': 7.176624774932861}, {'ion_id': 1359, 'distance': 14.772037506103516, 'force': [-0.4044402539730072, 0.6704288721084595, -1.30451500415802], 'magnitude': 1.5214487314224243}, {'ion_id': 1465, 'distance': 9.682229042053223, 'force': [-1.363629698753357, 2.1661407947540283, -2.447565793991089], 'magnitude': 3.541501045227051}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.641894817352295, 'force': [5.472200870513916, -18.806726455688477, -4.774502754211426], 'magnitude': 20.16020393371582}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 4.832467079162598, 'force': [-3.2295644283294678, 11.03004264831543, 1.8475264310836792], 'magnitude': 11.640673637390137}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.963825225830078, 'force': [1.7407222986221313, 30.138874053955078, 6.804442405700684], 'magnitude': 30.946443557739258}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 2.4333138465881348, 'force': [-21.163040161132812, -2.8742685317993164, 33.79615783691406], 'magnitude': 39.978946685791016}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.1974546909332275, 'force': [13.904720306396484, 5.142300128936768, -12.294902801513672], 'magnitude': 19.260040283203125}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 1.1917656660079956, 'force': [66.86273956298828, 46.97012710571289, -198.69639587402344], 'magnitude': 214.84197998046875}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 1.2086108922958374, 'force': [-33.1042594909668, -81.81383514404297, 36.13267517089844], 'magnitude': 95.3675308227539}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 1.2375956773757935, 'force': [29.955732345581055, 28.139358520507812, 81.13716125488281], 'magnitude': 90.9527816772461}]}, 6506: {'frame': 6506, 'ionic_force': [-9.954873204231262, 8.362967252731323, -7.493973910808563], 'ionic_force_magnitude': 15.006610768539893, 'motion_vector': [-0.2793464660644531, 0.185546875, -0.166778564453125], 'ionic_force_x': -9.954873204231262, 'ionic_force_y': 8.362967252731323, 'ionic_force_z': -7.493973910808563, 'radial_force': 13.001489214031524, 'axial_force': -7.493973910808563, 'glu_force': [1.001715674996376, 13.158740997314453, 0.8407977223396301], 'glu_force_magnitude': 13.223571368500611, 'asn_force': [22.252627849578857, 6.001870155334473, 6.600922584533691], 'asn_force_magnitude': 23.974446198824992, 'residue_force': [23.254343524575233, 19.160611152648926, 7.4417203068733215], 'residue_force_magnitude': 31.03663502423707, 'total_force': [13.299470320343971, 27.52357840538025, -0.0522536039352417], 'total_force_magnitude': 30.568382513275843, 'motion_component_total': 3.7392105927982033, 'cosine_total_motion': 0.12232281479644089, 'cosine_glu_motion': 0.4081630960287514, 'cosine_asn_motion': -0.6908626051379012, 'cosine_residue_motion': -0.3597578963896971, 'cosine_ionic_motion': 0.9932212776104898, 'motion_component_glu': 5.397373830324362, 'motion_component_asn': -16.563048357658687, 'motion_component_residue': -11.165674527334323, 'motion_component_ionic': 14.904885120132528, 'ionic_contributions': [{'ion_id': 1327, 'distance': 8.665142059326172, 'force': [1.2132747173309326, 4.102494239807129, -1.1174546480178833], 'magnitude': 4.421673774719238}, {'ion_id': 1330, 'distance': 8.192713737487793, 'force': [-3.8504509925842285, 3.057932138442993, -0.5377671122550964], 'magnitude': 4.946323394775391}, {'ion_id': 1341, 'distance': 7.552302837371826, 'force': [-5.303382396697998, -1.6648468971252441, -1.7273120880126953], 'magnitude': 5.8207550048828125}, {'ion_id': 1359, 'distance': 14.59177017211914, 'force': [-0.4168241024017334, 0.6007530689239502, -1.3772019147872925], 'magnitude': 1.5592727661132812}, {'ion_id': 1465, 'distance': 9.233230590820312, 'force': [-1.5974904298782349, 2.266634702682495, -2.7342381477355957], 'magnitude': 3.8943121433258057}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 4.617114543914795, 'force': [3.199863910675049, -12.013513565063477, -1.6638062000274658], 'magnitude': 12.543201446533203}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 5.831795692443848, 'force': [-2.0970499515533447, 7.680425643920898, 0.7084800601005554], 'magnitude': 7.993028163909912}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 3.931859016418457, 'force': [-0.10109828412532806, 17.49182891845703, 1.7961238622665405], 'magnitude': 17.58409309387207}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 2.822953462600708, 'force': [-11.5617036819458, -12.623644828796387, 24.275903701782227], 'magnitude': 29.70435905456543}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.642610549926758, 'force': [8.633233070373535, 7.652902603149414, -9.334488868713379], 'magnitude': 14.840226173400879}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 1.8744544982910156, 'force': [8.412850379943848, 59.54972457885742, -62.65240478515625], 'magnitude': 86.84623718261719}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 2.1918890476226807, 'force': [-3.0454764366149902, -27.27217674255371, 9.36563491821289], 'magnitude': 28.99588966369629}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 1.6130322217941284, 'force': [19.813724517822266, -21.304935455322266, 44.9462776184082], 'magnitude': 53.54112243652344}]}, 6507: {'frame': 6507, 'ionic_force': [-8.238221824169159, 7.098378419876099, -6.328981935977936], 'ionic_force_magnitude': 12.582181343547498, 'motion_vector': [0.5045700073242188, 0.26412200927734375, 0.01922607421875], 'ionic_force_x': -8.238221824169159, 'ionic_force_y': 7.098378419876099, 'ionic_force_z': -6.328981935977936, 'radial_force': 10.874524128254059, 'axial_force': -6.328981935977936, 'glu_force': [2.1811296939849854, 13.869128227233887, 1.4779795408248901], 'glu_force_magnitude': 14.117169264712233, 'asn_force': [34.64919185638428, 5.912895679473877, 22.317228317260742], 'asn_force_magnitude': 41.63637245704304, 'residue_force': [36.83032155036926, 19.782023906707764, 23.795207858085632], 'residue_force_magnitude': 48.10418871947278, 'total_force': [28.592099726200104, 26.880402326583862, 17.466225922107697], 'total_force_magnitude': 42.95501418873115, 'motion_component_total': 38.365359227638, 'cosine_total_motion': 0.8931520557547109, 'cosine_glu_motion': 0.5956926090886951, 'cosine_asn_motion': 0.820769768846677, 'cosine_residue_motion': 0.8852320415953007, 'cosine_ionic_motion': -0.3352367802225039, 'motion_component_glu': 8.409493392243165, 'motion_component_asn': 34.17387579718136, 'motion_component_residue': 42.58336918942452, 'motion_component_ionic': -4.218009961786522, 'ionic_contributions': [{'ion_id': 1327, 'distance': 9.208434104919434, 'force': [0.9431630373001099, 3.706730842590332, -0.8368191123008728], 'magnitude': 3.9153130054473877}, {'ion_id': 1330, 'distance': 12.161338806152344, 'force': [-1.7877682447433472, 1.3567931652069092, 0.0454939603805542], 'magnitude': 2.2447879314422607}, {'ion_id': 1341, 'distance': 7.734027862548828, 'force': [-5.284008026123047, -0.8967590928077698, -1.443036437034607], 'magnitude': 5.550429821014404}, {'ion_id': 1359, 'distance': 14.396419525146484, 'force': [-0.49212461709976196, 0.6336775422096252, -1.3864613771438599], 'magnitude': 1.6018767356872559}, {'ion_id': 1465, 'distance': 9.223329544067383, 'force': [-1.6174839735031128, 2.297935962677002, -2.7081589698791504], 'magnitude': 3.902677059173584}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 4.400365829467773, 'force': [2.8197336196899414, -13.295353889465332, -2.4453654289245605], 'magnitude': 13.809313774108887}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 5.6025190353393555, 'force': [-1.9333616495132446, 8.375652313232422, 1.0568832159042358], 'magnitude': 8.660625457763672}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 3.777524709701538, 'force': [1.2947577238082886, 18.788829803466797, 2.866461753845215], 'magnitude': 19.050277709960938}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 2.740161180496216, 'force': [-15.855650901794434, -11.668033599853516, 24.624658584594727], 'magnitude': 31.526473999023438}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.6237378120422363, 'force': [9.924775123596191, 7.005295276641846, -8.790956497192383], 'magnitude': 14.995206832885742}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 1.6814520359039307, 'force': [29.58548355102539, 70.58973693847656, -76.09283447265625], 'magnitude': 107.92743682861328}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 2.0179402828216553, 'force': [-8.638670921325684, -31.8046817779541, 9.174985885620117], 'magnitude': 34.21030044555664}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 1.3110281229019165, 'force': [19.633255004882812, -28.209421157836914, 73.40137481689453], 'magnitude': 81.04935455322266}]}, 6508: {'frame': 6508, 'ionic_force': [-7.880868673324585, 5.787855744361877, -7.391227200627327], 'ionic_force_magnitude': 12.257145046666652, 'motion_vector': [-0.12299728393554688, -0.23679351806640625, 0.32021331787109375], 'ionic_force_x': -7.880868673324585, 'ionic_force_y': 5.787855744361877, 'ionic_force_z': -7.391227200627327, 'radial_force': 9.77790187942851, 'axial_force': -7.391227200627327, 'glu_force': [0.3374987840652466, 16.64457607269287, 1.9459850788116455], 'glu_force_magnitude': 16.761344695335847, 'asn_force': [28.803736805915833, 23.728214263916016, -26.18156623840332], 'asn_force_magnitude': 45.5868162612249, 'residue_force': [29.14123558998108, 40.37279033660889, -24.235581159591675], 'residue_force_magnitude': 55.37632350939989, 'total_force': [21.260366916656494, 46.160646080970764, -31.626808360219], 'total_force_magnitude': 59.8586957350185, 'motion_component_total': -56.79436806245683, 'cosine_total_motion': -0.948807309699383, 'cosine_glu_motion': -0.480892259044313, 'cosine_asn_motion': -0.9233640396004629, 'cosine_residue_motion': -0.9056872062323855, 'cosine_ionic_motion': -0.5417852449754305, 'motion_component_glu': -8.060400915160468, 'motion_component_asn': -42.09322681548869, 'motion_component_residue': -50.153627730649156, 'motion_component_ionic': -6.640740331807676, 'ionic_contributions': [{'ion_id': 1327, 'distance': 9.438546180725098, 'force': [1.0252001285552979, 3.475285530090332, -0.871704638004303], 'magnitude': 3.72672963142395}, {'ion_id': 1330, 'distance': 14.450658798217773, 'force': [-1.0581204891204834, 1.1649466753005981, -0.22578908503055573], 'magnitude': 1.5898743867874146}, {'ion_id': 1341, 'distance': 7.018674850463867, 'force': [-6.056460380554199, -1.6252503395080566, -2.4695637226104736], 'magnitude': 6.739502906799316}, {'ion_id': 1359, 'distance': 14.880107879638672, 'force': [-0.40871429443359375, 0.6200888156890869, -1.3025859594345093], 'magnitude': 1.4994291067123413}, {'ion_id': 1465, 'distance': 9.613468170166016, 'force': [-1.3827736377716064, 2.152785062789917, -2.5215837955474854], 'magnitude': 3.592343330383301}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 4.280975341796875, 'force': [4.781951427459717, -13.538860321044922, -2.5901920795440674], 'magnitude': 14.590301513671875}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 5.4851298332214355, 'force': [-2.8913111686706543, 8.489922523498535, 1.0945320129394531], 'magnitude': 9.035289764404297}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 3.5136022567749023, 'force': [-1.553141474723816, 21.693513870239258, 3.4416451454162598], 'magnitude': 22.01966667175293}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 2.4472596645355225, 'force': [-14.108201026916504, -12.113224029541016, 34.87725067138672], 'magnitude': 39.524600982666016}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.1973865032196045, 'force': [11.408428192138672, 8.60685920715332, -12.91319465637207], 'magnitude': 19.2608642578125}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 1.4668028354644775, 'force': [-4.219973087310791, 80.79767608642578, -116.48468017578125], 'magnitude': 141.826492309570</t>
         </is>
       </c>
     </row>
@@ -499,7 +499,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>{6569: {'frame': 6569, 'ionic_force': [8.93659296631813, 4.198592029511929, -11.964962244033813], 'ionic_force_magnitude': 15.51293622681027, 'motion_vector': [0.9375572204589844, 4.542621612548828, 3.9090347290039062], 'ionic_force_x': 8.93659296631813, 'ionic_force_y': 4.198592029511929, 'ionic_force_z': -11.964962244033813, 'radial_force': 9.87374644579897, 'axial_force': -11.964962244033813, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [2.4234748482704163, 1.273831844329834, 1.2961934804916382], 'asn_force_magnitude': 3.029190559654029, 'residue_force': [2.4234748482704163, 1.273831844329834, 1.2961934804916382], 'residue_force_magnitude': 3.029190559654029, 'total_force': [11.360067814588547, 5.4724238738417625, -10.668768763542175], 'total_force_magnitude': 16.51729974108895, 'motion_component_total': -1.0212397170447503, 'cosine_total_motion': -0.061828490918783924, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.7143262405109572, 'cosine_residue_motion': 0.7143262405109572, 'cosine_ionic_motion': -0.20531703184656236, 'motion_component_glu': None, 'motion_component_asn': 2.163830304268945, 'motion_component_residue': 2.163830304268945, 'motion_component_ionic': -3.1850700213136953}, 6570: {'frame': 6570, 'ionic_force': [12.369088254868984, 9.554802000522614, -1.3525469191372395], 'ionic_force_magnitude': 15.688147395227915, 'motion_vector': [0.08165740966796875, 0.8572654724121094, 0.46636962890625], 'ionic_force_x': 12.369088254868984, 'ionic_force_y': 9.554802000522614, 'ionic_force_z': -1.3525469191372395, 'radial_force': 15.629734019679567, 'axial_force': -1.3525469191372395, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [2.14583683013916, -15.262238144874573, 15.3211669921875], 'asn_force_magnitude': 21.73197383798678, 'residue_force': [2.14583683013916, -15.262238144874573, 15.3211669921875], 'residue_force_magnitude': 21.73197383798678, 'total_force': [14.514925085008144, -5.707436144351959, 13.96862007305026], 'total_force_magnitude': 20.937531476047422, 'motion_component_total': 2.8662707759259183, 'cosine_total_motion': 0.13689630887026666, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.27079566203904465, 'cosine_residue_motion': -0.27079566203904465, 'cosine_ionic_motion': 0.557822080474634, 'motion_component_glu': None, 'motion_component_asn': -5.8849242428728274, 'motion_component_residue': -5.8849242428728274, 'motion_component_ionic': 8.751195018798747}, 6571: {'frame': 6571, 'ionic_force': [10.874882519245148, 11.021745204925537, -1.5739329904317856], 'ionic_force_magnitude': 15.563393017849684, 'motion_vector': [-0.7143974304199219, 2.6378211975097656, 0.46242523193359375], 'ionic_force_x': 10.874882519245148, 'ionic_force_y': 11.021745204925537, 'ionic_force_z': -1.5739329904317856, 'radial_force': 15.483602202642729, 'axial_force': -1.5739329904317856, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-1.605684757232666, 0.3110790252685547, 14.728298664093018], 'asn_force_magnitude': 14.81883177711035, 'residue_force': [-1.605684757232666, 0.3110790252685547, 14.728298664093018], 'residue_force_magnitude': 14.81883177711035, 'total_force': [9.269197762012482, 11.332824230194092, 13.154365673661232], 'total_force_magnitude': 19.682181496474634, 'motion_component_total': 10.590980308782694, 'cosine_total_motion': 0.5380999210214423, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.21372531110818835, 'cosine_residue_motion': 0.21372531110818835, 'cosine_ionic_motion': 0.4770052949537086, 'motion_component_glu': None, 'motion_component_asn': 3.1671594318228173, 'motion_component_residue': 3.1671594318228173, 'motion_component_ionic': 7.423820876959877}, 6572: {'frame': 6572, 'ionic_force': [4.297864839434624, 8.788159370422363, -1.320813924074173], 'ionic_force_magnitude': 9.871572150372959, 'motion_vector': [0.8923988342285156, -0.882781982421875, -0.6154251098632812], 'ionic_force_x': 4.297864839434624, 'ionic_force_y': 8.788159370422363, 'ionic_force_z': -1.320813924074173, 'radial_force': 9.782810807635544, 'axial_force': -1.320813924074173, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-2.9726831912994385, 5.858217239379883, 4.899883508682251], 'asn_force_magnitude': 8.195389739253294, 'residue_force': [-2.9726831912994385, 5.858217239379883, 4.899883508682251], 'residue_force_magnitude': 8.195389739253294, 'total_force': [1.3251816481351852, 14.646376609802246, 3.579069584608078], 'total_force_magnitude': 15.135461449463087, 'motion_component_total': -9.978205373607633, 'cosine_total_motion': -0.6592600699307782, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.9461156099804022, 'cosine_residue_motion': -0.9461156099804022, 'cosine_ionic_motion': -0.22533586115184634, 'motion_component_glu': None, 'motion_component_asn': -7.753786162180759, 'motion_component_residue': -7.753786162180759, 'motion_component_ionic': -2.2244192114268744}, 6573: {'frame': 6573, 'ionic_force': [6.707516588270664, 9.176944971084595, -0.1950500402599573], 'ionic_force_magnitude': 11.368603357600545, 'motion_vector': [-0.3231239318847656, -0.48430633544921875, 0.06146240234375], 'ionic_force_x': 6.707516588270664, 'ionic_force_y': 9.176944971084595, 'ionic_force_z': -0.1950500402599573, 'radial_force': 11.366930007008971, 'axial_force': -0.1950500402599573, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.6474916785955429, 6.648892879486084, 4.46166467666626], 'asn_force_magnitude': 8.033272912315544, 'residue_force': [0.6474916785955429, 6.648892879486084, 4.46166467666626], 'residue_force_magnitude': 8.033272912315544, 'total_force': [7.355008266866207, 15.825837850570679, 4.2666146364063025], 'total_force_magnitude': 17.965447134258092, 'motion_component_total': -16.703515181437325, 'cosine_total_motion': -0.9297578321658132, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.670869648568459, 'cosine_residue_motion': -0.670869648568459, 'cosine_ionic_motion': -0.9952177809364312, 'motion_component_glu': None, 'motion_component_asn': -5.38927897553965, 'motion_component_residue': -5.38927897553965, 'motion_component_ionic': -11.314236205897675}, 6574: {'frame': 6574, 'ionic_force': [9.922765612602234, 10.655503034591675, -1.8789064027369022], 'ionic_force_magnitude': 14.680984694259426, 'motion_vector': [0.2715606689453125, -0.07678985595703125, -0.05289459228515625], 'ionic_force_x': 9.922765612602234, 'ionic_force_y': 10.655503034591675, 'ionic_force_z': -1.8789064027369022, 'radial_force': 14.560254885228959, 'axial_force': -1.8789064027369022, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-0.7596144676208496, 7.04573130607605, 7.420785903930664], 'asn_force_magnitude': 10.26096521818562, 'residue_force': [-0.7596144676208496, 7.04573130607605, 7.420785903930664], 'residue_force_magnitude': 10.26096521818562, 'total_force': [9.163151144981384, 17.701234340667725, 5.541879501193762], 'total_force_magnitude': 20.68838960612352, 'motion_component_total': 2.9114362935133666, 'cosine_total_motion': 0.14072802905121315, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.3868904578765326, 'cosine_residue_motion': -0.3868904578765326, 'cosine_ionic_motion': 0.468722362180727, 'motion_component_glu': None, 'motion_component_asn': -3.9698695315190093, 'motion_component_residue': -3.9698695315190093, 'motion_component_ionic': 6.881305825032376}, 6575: {'frame': 6575, 'ionic_force': [6.102406769990921, 8.403478920459747, -1.6997588761150837], 'ionic_force_magnitude': 10.52364036776126, 'motion_vector': [-0.7413291931152344, 0.8488311767578125, 0.4405517578125], 'ionic_force_x': 6.102406769990921, 'ionic_force_y': 8.403478920459747, 'ionic_force_z': -1.6997588761150837, 'radial_force': 10.385462259959464, 'axial_force': -1.6997588761150837, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.24673700332641602, 7.761092662811279, 7.846946716308594], 'asn_force_magnitude': 11.039475134178245, 'residue_force': [0.24673700332641602, 7.761092662811279, 7.846946716308594], 'residue_force_magnitude': 11.039475134178245, 'total_force': [6.349143773317337, 16.164571583271027, 6.14718784019351], 'total_force_magnitude': 18.422619777533555, 'motion_component_total': 9.687656768826043, 'cosine_total_motion': 0.5258566309141425, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.738274537650366, 'cosine_residue_motion': 0.738274537650366, 'cosine_ionic_motion': 0.14609900324491662, 'motion_component_glu': None, 'motion_component_asn': 8.150163400588156, 'motion_component_residue': 8.150163400588156, 'motion_component_ionic': 1.5374933682378877}, 6576: {'frame': 6576, 'ionic_force': [5.697530130855739, 9.966541528701782, -1.1423418633639812], 'ionic_force_magnitude': 11.536842920320106, 'motion_vector': [0.1239013671875, -0.14241409301757812, -0.3520050048828125], 'ionic_force_x': 5.697530130855739, 'ionic_force_y': 9.966541528701782, 'ionic_force_z': -1.1423418633639812, 'radial_force': 11.480148066786693, 'axial_force': -1.1423418633639812, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-3.922982931137085, 7.049598693847656, 6.736132860183716], 'asn_force_magnitude': 10.5100962285004, 'residue_force': [-3.922982931137085, 7.049598693847656, 6.736132860183716], 'residue_force_magnitude': 10.5100962285004, 'total_force': [1.7745471997186542, 17.01614022254944, 5.593790996819735], 'total_force_magnitude': 17.999681762564464, 'motion_component_total': -10.446278808828731, 'cosine_total_motion': -0.5803590833786175, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.9197655379328833, 'cosine_residue_motion': -0.9197655379328833, 'cosine_ionic_motion': -0.06756220075795798, 'motion_component_glu': None, 'motion_component_asn': -9.666824311333038, 'motion_component_residue': -9.666824311333038, 'motion_component_ionic': -0.7794544974956932}, 6577: {'frame': 6577, 'ionic_force': [10.770041853189468, 11.033284544944763, -1.4359604306519032], 'ionic_force_magnitude': 15.48512679081343, 'motion_vector': [2.2769126892089844, -2.477092742919922, -0.91888427734375], 'ionic_force_x': 10.770041853189468, 'ionic_force_y': 11.033284544944763, 'ionic_force_z': -1.4359604306519032, 'radial_force': 15.41840359340648, 'axial_force': -1.4359604306519032, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-0.9619882106781006, 5.421460151672363, 4.095129013061523], 'asn_force_magnitude': 6.8620502131122025, 'residue_force': [-0.9619882106781006, 5.421460151672363, 4.095129013061523], 'residue_force_magnitude': 6.8620502131122025, 'total_force': [9.808053642511368, 16.454744696617126, 2.6591685824096203], 'total_force_magnitude': 19.33979619424425, 'motion_component_total': -5.984110926139508, 'cosine_total_motion': -0.30941954434454944, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.8098635667906998, 'cosine_residue_motion': -0.8098635667906998, 'cosine_ionic_motion': -0.027561057188422215, 'motion_component_glu': None, 'motion_component_asn': -5.55732446108793, 'motion_component_residue': -5.55732446108793, 'motion_component_ionic': -0.4267864650515779}, 6578: {'frame': 6578, 'ionic_force': [11.297083020210266, 8.097006931900978, -3.776877298951149], 'ionic_force_magnitude': 14.403138829856085, 'motion_vector': [-1.2792587280273438, 0.96728515625, 1.4186248779296875], 'ionic_force_x': 11.297083020210266, 'ionic_force_y': 8.097006931900978, 'ionic_force_z': -3.776877298951149, 'radial_force': 13.899122491034303, 'axial_force': -3.776877298951149, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-84.09410262107849, -24.021531105041504, 627.1876850128174], 'asn_force_magnitude': 633.2560653353523, 'residue_force': [-84.09410262107849, -24.021531105041504, 627.1876850128174], 'residue_force_magnitude': 633.2560653353523, 'total_force': [-72.79701960086823, -15.924524173140526, 623.4108077138662], 'total_force_magnitude': 627.8487331414831, 'motion_component_total': 449.33635608261034, 'cosine_total_motion': 0.7156761372031857, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.7183987378373606, 'cosine_residue_motion': 0.7183987378373606, 'cosine_ionic_motion': -0.38838770133661316, 'motion_component_glu': None, 'motion_component_asn': 454.9303580647703, 'motion_component_residue': 454.9303580647703, 'motion_component_ionic': -5.594001982159921}, 6579: {'frame': 6579, 'ionic_force': [9.608516097068787, 8.373697221279144, -1.9300379157066345], 'ionic_force_magnitude': 12.89059475343761, 'motion_vector': [2.924358367919922, -6.608238220214844, -2.4186172485351562], 'ionic_force_x': 9.608516097068787, 'ionic_force_y': 8.373697221279144, 'ionic_force_z': -1.9300379157066345, 'radial_force': 12.745288805723, 'axial_force': -1.9300379157066345, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-0.7262768745422363, 2.8879292011260986, 9.543179512023926], 'asn_force_magnitude': 9.9969939665844, 'residue_force': [-0.7262768745422363, 2.8879292011260986, 9.543179512023926], 'residue_force_magnitude': 9.9969939665844, 'total_force': [8.88223922252655, 11.261626422405243, 7.613141596317291], 'total_force_magnitude': 16.238175028296176, 'motion_component_total': -8.773554211712579, 'cosine_total_motion': -0.5403042026843556, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.5813693883990191, 'cosine_residue_motion': -0.5813693883990191, 'cosine_ionic_motion': -0.2297495189460466, 'motion_component_glu': None, 'motion_component_asn': -5.811946268181856, 'motion_component_residue': -5.811946268181856, 'motion_component_ionic': -2.9616079435307228}, 6580: {'frame': 6580, 'ionic_force': [9.401102185249329, 2.19012341927737, -3.330233727581799], 'ionic_force_magnitude': 10.211161519116729, 'motion_vector': [0.0558624267578125, 1.9655532836914062, -0.0980682373046875], 'ionic_force_x': 9.401102185249329, 'ionic_force_y': 2.19012341927737, 'ionic_force_z': -3.330233727581799, 'radial_force': 9.652842218184595, 'axial_force': -3.330233727581799, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [4.104503393173218, -0.697739839553833, 0.06686857342720032], 'asn_force_magnitude': 4.163923677780761, 'residue_force': [4.104503393173218, -0.697739839553833, 0.06686857342720032], 'residue_force_magnitude': 4.163923677780761, 'total_force': [13.505605578422546, 1.492383579723537, -3.2633651541545987], 'total_force_magnitude': 13.974195608989346, 'motion_component_total': 2.035689911724462, 'cosine_total_motion': 0.14567492603402085, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.1401231600253338, 'cosine_residue_motion': -0.1401231600253338, 'cosine_ionic_motion': 0.25649893507765903, 'motion_component_glu': None, 'motion_component_asn': -0.58346214383495, 'motion_component_residue': -0.58346214383495, 'motion_component_ionic': 2.619152055559412}, 6581: {'frame': 6581, 'ionic_force': [8.237632095813751, 2.8010704964399338, -3.125244453549385], 'ionic_force_magnitude': 9.245092285447901, 'motion_vector': [-1.0904083251953125, 0.6786651611328125, -0.0248260498046875], 'ionic_force_x': 8.237632095813751, 'ionic_force_y': 2.8010704964399338, 'ionic_force_z': -3.125244453549385, 'radial_force': 8.700837802878933, 'axial_force': -3.125244453549385, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [1.1421012878417969, 6.257309436798096, -4.232310585677624], 'asn_force_magnitude': 7.6400765462900475, 'residue_force': [1.1421012878417969, 6.257309436798096, -4.232310585677624], 'residue_force_magnitude': 7.6400765462900475, 'total_force': [9.379733383655548, 9.05837993323803, -7.357555039227009], 'total_force_magnitude': 14.972216319523522, 'motion_component_total': -3.0340012712975755, 'cosine_total_motion': -0.202642094299779, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.31650665882401713, 'cosine_residue_motion': 0.31650665882401713, 'cosine_ionic_motion': -0.5897330393018821, 'motion_component_glu': None, 'motion_component_asn': 2.418135100825999, 'motion_component_residue': 2.418135100825999, 'motion_component_ionic': -5.452136372123575}, 6582: {'frame': 6582, 'ionic_force': [13.439601302146912, 8.873756095767021, -5.538107238709927], 'ionic_force_magnitude': 17.030474514683455, 'motion_vector': [-3.5965843200683594, -4.00225830078125, 1.7977447509765625], 'ionic_force_x': 13.439601302146912, 'ionic_force_y': 8.873756095767021, 'ionic_force_z': -5.538107238709927, 'radial_force': 16.104857354470152, 'axial_force': -5.538107238709927, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [7.70050835609436, 7.685168266296387, -6.644646137952805], 'asn_force_magnitude': 12.747978762226552, 'residue_force': [7.70050835609436, 7.685168266296387, -6.644646137952805], 'residue_force_magnitude': 12.747978762226552, 'total_force': [21.140109658241272, 16.558924362063408, -12.182753376662731], 'total_force_magnitude': 29.487653216686983, 'motion_component_total': -28.944211484010033, 'cosine_total_motion': -0.9815705329724436, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.9734091900660689, 'cosine_residue_motion': -0.9734091900660689, 'cosine_ionic_motion': -0.9709190303438223, 'motion_component_glu': None, 'motion_component_asn': -12.408999681918395, 'motion_component_residue': -12.408999681918395, 'motion_component_ionic': -16.535211802091638}, 6617: {'frame': 6617, 'ionic_force': [25.495893580839038, -9.819616988301277, -19.05839467048645], 'ionic_force_magnitude': 33.31197794635483, 'motion_vector': [-0.17819976806640625, -0.8794822692871094, 1.2368545532226562], 'ionic_force_x': 25.495893580839038, 'ionic_force_y': -9.819616988301277, 'ionic_force_z': -19.05839467048645, 'radial_force': 27.321520222754888, 'axial_force': -19.05839467048645, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-0.04208803176879883, 1.0084843635559082, 0.9710139632225037], 'asn_force_magnitude': 1.4005999538512095, 'residue_force': [-0.04208803176879883, 1.0084843635559082, 0.9710139632225037], 'residue_force_magnitude': 1.4005999538512095, 'total_force': [25.45380554907024, -8.811132624745369, -18.087380707263947], 'total_force_magnitude': 32.445116980991685, 'motion_component_total': -12.537291219674534, 'cosine_total_motion': -0.38641534955844475, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.1502443559821742, 'cosine_residue_motion': 0.1502443559821742, 'cosine_ionic_motion': -0.3826768701113557, 'motion_component_glu': None, 'motion_component_asn': 0.21043223805503786, 'motion_component_residue': 0.21043223805503786, 'motion_component_ionic': -12.747723457729572}, 6618: {'frame': 6618, 'ionic_force': [7.006479242816567, -3.3669902831315994, -11.937614440917969], 'ionic_force_magnitude': 14.245490987913868, 'motion_vector': [0.8625411987304688, 1.1436653137207031, -2.8303680419921875], 'ionic_force_x': 7.006479242816567, 'ionic_force_y': -3.3669902831315994, 'ionic_force_z': -11.937614440917969, 'radial_force': 7.773504675931058, 'axial_force': -11.937614440917969, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [12.034701824188232, -3.1329400539398193, 1.9882113933563232], 'asn_force_magnitude': 12.593742331942952, 'residue_force': [12.034701824188232, -3.1329400539398193, 1.9882113933563232], 'residue_force_magnitude': 12.593742331942952, 'total_force': [19.0411810670048, -6.499930337071419, -9.949403047561646], 'total_force_magnitude': 22.445629681879552, 'motion_component_total': 11.711237034240074, 'cosine_total_motion': 0.5217602357440033, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.029287113027961772, 'cosine_residue_motion': 0.029287113027961772, 'cosine_ionic_motion': 0.7962100210334999, 'motion_component_glu': None, 'motion_component_asn': 0.3688343551206401, 'motion_component_residue': 0.3688343551206401, 'motion_component_ionic': 11.342402679119434}, 6619: {'frame': 6619, 'ionic_force': [4.875967264175415, -2.3995706290006638, -8.796449065208435], 'ionic_force_magnitude': 10.339753968140599, 'motion_vector': [-0.950592041015625, -1.9060783386230469, 2.1285781860351562], 'ionic_force_x': 4.875967264175415, 'ionic_force_y': -2.3995706290006638, 'ionic_force_z': -8.796449065208435, 'radial_force': 5.434426921476903, 'axial_force': -8.796449065208435, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-2.022278070449829, 0.42758893966674805, -0.34845590591430664], 'asn_force_magnitude': 2.0961541961206427, 'residue_force': [-2.022278070449829, 0.42758893966674805, -0.34845590591430664], 'residue_force_magnitude': 2.0961541961206427, 'total_force': [2.853689193725586, -1.9719816893339157, -9.144904971122742], 'total_force_magnitude': 9.780671793303355, 'motion_component_total': -6.116931290443129, 'cosine_total_motion': -0.625410137433635, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.057925494883231815, 'cosine_residue_motion': 0.057925494883231815, 'cosine_ionic_motion': -0.603336605380256, 'motion_component_glu': None, 'motion_component_asn': 0.12142076916185118, 'motion_component_residue': 0.12142076916185118, 'motion_component_ionic': -6.23835205960498}, 6620: {'frame': 6620, 'ionic_force': [6.493408654816449, -3.330855667591095, -9.856857150793076], 'ionic_force_magnitude': 12.264444069256033, 'motion_vector': [1.2603034973144531, 5.175846099853516, -1.229766845703125], 'ionic_force_x': 6.493408654816449, 'ionic_force_y': -3.330855667591095, 'ionic_force_z': -9.856857150793076, 'radial_force': 7.297873350282868, 'axial_force': -9.856857150793076, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [12.92377495765686, -1.314504623413086, 1.6151475310325623], 'asn_force_magnitude': 13.090476809808477, 'residue_force': [12.92377495765686, -1.314504623413086, 1.6151475310325623], 'residue_force_magnitude': 13.090476809808477, 'total_force': [19.41718361247331, -4.645360291004181, -8.241709619760513], 'total_force_magnitude': 21.59935575729502, 'motion_component_total': 1.9321209551582301, 'cosine_total_motion': 0.08945271224145984, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.10476677910042305, 'cosine_residue_motion': 0.10476677910042305, 'cosine_ionic_motion': 0.045715391561146, 'motion_component_glu': None, 'motion_component_asn': 1.3714470922524153, 'motion_component_residue': 1.3714470922524153, 'motion_component_ionic': 0.5606738629058143}, 6621: {'frame': 6621, 'ionic_force': [4.325476974248886, -1.8174557834863663, -10.630309104919434], 'ionic_force_magnitude': 11.619654394422337, 'motion_vector': [0.6217308044433594, -2.0323638916015625, 2.1789169311523438], 'ionic_force_x': 4.325476974248886, 'ionic_force_y': -1.8174557834863663, 'ionic_force_z': -10.630309104919434, 'radial_force': 4.691790338419369, 'axial_force': -10.630309104919434, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [1.0479178428649902, -2.747545003890991, -0.5306612551212311], 'asn_force_magnitude': 2.9880991820031677, 'residue_force': [1.0479178428649902, -2.747545003890991, -0.5306612551212311], 'residue_force_magnitude': 2.9880991820031677, 'total_force': [5.373394817113876, -4.5650007873773575, -11.160970360040665], 'total_force_magnitude': 13.201509891942225, 'motion_component_total': -3.843968680927876, 'cosine_total_motion': -0.29117644211849664, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.5584568712066338, 'cosine_residue_motion': 0.5584568712066338, 'cosine_ionic_motion': -0.4744283275422261, 'motion_component_glu': None, 'motion_component_asn': 1.6687245200365908, 'motion_component_residue': 1.6687245200365908, 'motion_component_ionic': -5.512693200964467}, 6623: {'frame': 6623, 'ionic_force': [6.283501505851746, -3.975326861254871, -7.835638165473938], 'ionic_force_magnitude': 10.801983164590077, 'motion_vector': [3.3156967163085938, 1.1702003479003906, 0.8474578857421875], 'ionic_force_x': 6.283501505851746, 'ionic_force_y': -3.975326861254871, 'ionic_force_z': -7.835638165473938, 'radial_force': 7.435429700283344, 'axial_force': -7.835638165473938, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [1.1770047545433044, 4.229018211364746, 2.5180851817131042], 'asn_force_magnitude': 5.060700367205643, 'residue_force': [1.1770047545433044, 4.229018211364746, 2.5180851817131042], 'residue_force_magnitude': 5.060700367205643, 'total_force': [7.46050626039505, 0.2536913501098752, -5.317552983760834], 'total_force_magnitude': 9.165144990539869, 'motion_component_total': 5.6754919464693705, 'cosine_total_motion': 0.619247371681248, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.6001731647165891, 'cosine_residue_motion': 0.6001731647165891, 'cosine_ionic_motion': 0.24423250353225961, 'motion_component_glu': None, 'motion_component_asn': 3.037296555068216, 'motion_component_residue': 3.037296555068216, 'motion_component_ionic': 2.6381953914011547}, 6624: {'frame': 6624, 'ionic_force': [7.87319028377533, -4.011160895228386, -5.9922478795051575], 'ionic_force_magnitude': 10.676308894996327, 'motion_vector': [-0.22956085205078125, 0.6142463684082031, -2.2589950561523438], 'ionic_force_x': 7.87319028377533, 'ionic_force_y': -4.011160895228386, 'ionic_force_z': -5.9922478795051575, 'radial_force': 8.836092856684092, 'axial_force': -5.9922478795051575, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [2.0391921401023865, 7.058685302734375, -2.3340597455389798], 'asn_force_magnitude': 7.709161931302202, 'residue_force': [2.0391921401023865, 7.058685302734375, -2.3340597455389798], 'residue_force_magnitude': 7.709161931302202, 'total_force': [9.912382423877716, 3.047524407505989, -8.326307625044137], 'total_force_magnitude': 13.299252948884487, 'motion_component_total': 7.824663324290154, 'cosine_total_motion': 0.588353598082851, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.5040457098339405, 'cosine_residue_motion': 0.5040457098339405, 'cosine_ionic_motion': 0.36893774479007324, 'motion_component_glu': None, 'motion_component_asn': 3.8857699978880103, 'motion_component_residue': 3.8857699978880103, 'motion_component_ionic': 3.9388933264021433}, 6625: {'frame': 6625, 'ionic_force': [5.6088151931762695, -2.546375662088394, -5.219111204147339], 'ionic_force_magnitude': 8.073534458026257, 'motion_vector': [0.36219024658203125, -0.22568130493164062, 1.1433563232421875], 'ionic_force_x': 5.6088151931762695, 'ionic_force_y': -2.546375662088394, 'ionic_force_z': -5.219111204147339, 'radial_force': 6.159775716994983, 'axial_force': -5.219111204147339, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [2.922158122062683, 5.9378697872161865, 1.7068880796432495], 'asn_force_magnitude': 6.834527973218043, 'residue_force': [2.922158122062683, 5.9378697872161865, 1.7068880796432495], 'residue_force_magnitude': 6.834527973218043, 'total_force': [8.530973315238953, 3.3914941251277924, -3.5122231245040894], 'total_force_magnitude': 9.8293158145619, 'motion_component_total': -1.3858432363344693, 'cosine_total_motion': -0.14099081385515919, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.20020619224530636, 'cosine_residue_motion': 0.20020619224530636, 'cosine_ionic_motion': -0.3411341181443097, 'motion_component_glu': None, 'motion_component_asn': 1.3683148213120155, 'motion_component_residue': 1.3683148213120155, 'motion_component_ionic': -2.754158057646485}, 6626: {'frame': 6626, 'ionic_force': [5.625236392021179, -4.34935262799263, -4.449422746896744], 'ionic_force_magnitude': 8.38793869370467, 'motion_vector': [-5.026386260986328, 0.7360191345214844, -1.5363540649414062], 'ionic_force_x': 5.625236392021179, 'ionic_force_y': -4.34935262799263, 'ionic_force_z': -4.449422746896744, 'radial_force': 7.110566274829724, 'axial_force': -4.449422746896744, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [1.5052151679992676, 5.914242506027222, -0.9589341282844543], 'asn_force_magnitude': 6.1776607048674075, 'residue_force': [1.5052151679992676, 5.914242506027222, -0.9589341282844543], 'residue_force_magnitude': 6.1776607048674075, 'total_force': [7.130451560020447, 1.5648898780345917, -5.408356875181198], 'total_force_magnitude': 9.08529272337952, 'motion_component_total': -4.970479063377123, 'cosine_total_motion': -0.547090689833956, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.0530568413702029, 'cosine_residue_motion': -0.0530568413702029, 'cosine_ionic_motion': -0.5534985493878839, 'motion_component_glu': None, 'motion_component_asn': -0.32776716405708584, 'motion_component_residue': -0.32776716405708584, 'motion_component_ionic': -4.642711899320037}, 6627: {'frame': 6627, 'ionic_force': [11.841566383838654, -8.76005607843399, -20.117031037807465], 'ionic_force_magnitude': 24.933034606647357, 'motion_vector': [4.9320220947265625, -0.5729293823242188, 1.6975784301757812], 'ionic_force_x': 11.841566383838654, 'ionic_force_y': -8.76005607843399, 'ionic_force_z': -20.117031037807465, 'radial_force': 14.72960545704351, 'axial_force': -20.117031037807465, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-0.0460205078125, -2.392179250717163, -0.8835080862045288], 'asn_force_magnitude': 2.55053445244126, 'residue_force': [-0.0460205078125, -2.392179250717163, -0.8835080862045288], 'residue_force_magnitude': 2.55053445244126, 'total_force': [11.795545876026154, -11.152235329151154, -21.000539124011993], 'total_force_magnitude': 26.54298210166603, 'motion_component_total': 5.510434363233532, 'cosine_total_motion': 0.20760419240487893, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.026618318443774686, 'cosine_residue_motion': -0.026618318443774686, 'cosine_ionic_motion': 0.22373230493183544, 'motion_component_glu': None, 'motion_component_asn': -0.06789093825689996, 'motion_component_residue': -0.06789093825689996, 'motion_component_ionic': 5.578325301490432}, 6628: {'frame': 6628, 'ionic_force': [7.13002073764801, -3.063589721918106, -6.835246443748474], 'ionic_force_magnitude': 10.341342835933306, 'motion_vector': [-1.2178421020507812, -2.2107009887695312, 0.6198348999023438], 'ionic_force_x': 7.13002073764801, 'ionic_force_y': -3.063589721918106, 'ionic_force_z': -6.835246443748474, 'radial_force': 7.760333607747346, 'axial_force': -6.835246443748474, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [1.8490533828735352, 6.5575597286224365, -1.4850602746009827], 'asn_force_magnitude': 6.973233971864473, 'residue_force': [1.8490533828735352, 6.5575597286224365, -1.4850602746009827], 'residue_force_magnitude': 6.973233971864473, 'total_force': [8.979074120521545, 3.4939700067043304, -8.320306718349457], 'total_force_magnitude': 12.73024360949076, 'motion_component_total': -9.16387307201277, 'cosine_total_motion': -0.7198505663458664, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.9749532381110365, 'cosine_residue_motion': -0.9749532381110365, 'cosine_ionic_motion': -0.228722330219908, 'motion_component_glu': None, 'motion_component_asn': -6.798577040975152, 'motion_component_residue': -6.798577040975152, 'motion_component_ionic': -2.3652960310376177}, 6629: {'frame': 6629, 'ionic_force': [10.198720812797546, -4.6738147884607315, -6.662026922218502], 'ionic_force_magnitude': 13.047645519655575, 'motion_vector': [0.7532005310058594, 1.959686279296875, -0.757354736328125], 'ionic_force_x': 10.198720812797546, 'ionic_force_y': -4.6738147884607315, 'ionic_force_z': -6.662026922218502, 'radial_force': 11.218665290230566, 'axial_force': -6.662026922218502, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.3608928322792053, 2.7624082565307617, 0.12063387036323547], 'asn_force_magnitude': 2.78849341810567, 'residue_force': [0.3608928322792053, 2.7624082565307617, 0.12063387036323547], 'residue_force_magnitude': 2.78849341810567, 'total_force': [10.559613645076752, -1.9114065319299698, -6.541393051855266], 'total_force_magnitude': 12.56776584451095, 'motion_component_total': 4.105024933345987, 'cosine_total_motion': 0.32663123932555466, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.8988274780326174, 'cosine_residue_motion': 0.8988274780326174, 'cosine_ionic_motion': 0.12252405420052483, 'motion_component_glu': None, 'motion_component_asn': 2.5063745065064724, 'motion_component_residue': 2.5063745065064724, 'motion_component_ionic': 1.5986504268395145}, 6630: {'frame': 6630, 'ionic_force': [7.65932685136795, -3.4130903966724873, -3.7145602703094482], 'ionic_force_magnitude': 9.171283000415233, 'motion_vector': [0.9477729797363281, 0.11902999877929688, -0.323333740234375], 'ionic_force_x': 7.65932685136795, 'ionic_force_y': -3.4130903966724873, 'ionic_force_z': -3.7145602703094482, 'radial_force': 8.38537261378074, 'axial_force': -3.7145602703094482, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [2.833851814270019</t>
+          <t xml:space="preserve">{6569: {'frame': 6569, 'ionic_force': [8.93659296631813, 4.198592029511929, -11.964962244033813], 'ionic_force_magnitude': 15.51293622681027, 'motion_vector': [0.9375572204589844, 4.542621612548828, 3.9090347290039062], 'ionic_force_x': 8.93659296631813, 'ionic_force_y': 4.198592029511929, 'ionic_force_z': -11.964962244033813, 'radial_force': 9.87374644579897, 'axial_force': -11.964962244033813, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [2.4234748482704163, 1.273831844329834, 1.2961934804916382], 'asn_force_magnitude': 3.029190559654029, 'residue_force': [2.4234748482704163, 1.273831844329834, 1.2961934804916382], 'residue_force_magnitude': 3.029190559654029, 'total_force': [11.360067814588547, 5.4724238738417625, -10.668768763542175], 'total_force_magnitude': 16.51729974108895, 'motion_component_total': -1.0212397170447503, 'cosine_total_motion': -0.061828490918783924, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.7143262405109572, 'cosine_residue_motion': 0.7143262405109572, 'cosine_ionic_motion': -0.20531703184656236, 'motion_component_glu': None, 'motion_component_asn': 2.163830304268945, 'motion_component_residue': 2.163830304268945, 'motion_component_ionic': -3.1850700213136953, 'ionic_contributions': [{'ion_id': 1327, 'distance': 10.281067848205566, 'force': [2.5776994228363037, 1.23420250415802, -1.3029985427856445], 'magnitude': 3.1409544944763184}, {'ion_id': 1330, 'distance': 7.982583522796631, 'force': [3.5478971004486084, -3.1198573112487793, -2.1965181827545166], 'magnitude': 5.210160732269287}, {'ion_id': 1341, 'distance': 6.964383125305176, 'force': [1.5748634338378906, 5.740958213806152, -3.378621816635132], 'magnitude': 6.844989776611328}, {'ion_id': 1359, 'distance': 9.398062705993652, 'force': [1.0105098485946655, 0.24263377487659454, -3.6123909950256348], 'magnitude': 3.7589054107666016}, {'ion_id': 1374, 'distance': 14.902193069458008, 'force': [0.22562316060066223, 0.10065484791994095, -1.4744327068328857], 'magnitude': 1.494987964630127}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.181301116943359, 'force': [-4.431948661804199, -7.413596153259277, -1.7737922668457031], 'magnitude': 8.817591667175293}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.641460418701172, 'force': [4.162238597869873, 4.443803787231445, 1.0990182161331177], 'magnitude': 6.187039852142334}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.682880401611328, 'force': [3.568387985229492, 7.924644947052002, 3.706906795501709], 'magnitude': 9.44852066040039}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.7848358154296875, 'force': [-0.8752030730247498, -3.681020736694336, -1.7359392642974854], 'magnitude': 4.1628570556640625}]}, 6570: {'frame': 6570, 'ionic_force': [12.369088254868984, 9.554802000522614, -1.3525469191372395], 'ionic_force_magnitude': 15.688147395227915, 'motion_vector': [0.08165740966796875, 0.8572654724121094, 0.46636962890625], 'ionic_force_x': 12.369088254868984, 'ionic_force_y': 9.554802000522614, 'ionic_force_z': -1.3525469191372395, 'radial_force': 15.629734019679567, 'axial_force': -1.3525469191372395, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [2.14583683013916, -15.262238144874573, 15.3211669921875], 'asn_force_magnitude': 21.73197383798678, 'residue_force': [2.14583683013916, -15.262238144874573, 15.3211669921875], 'residue_force_magnitude': 21.73197383798678, 'total_force': [14.514925085008144, -5.707436144351959, 13.96862007305026], 'total_force_magnitude': 20.937531476047422, 'motion_component_total': 2.8662707759259183, 'cosine_total_motion': 0.13689630887026666, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.27079566203904465, 'cosine_residue_motion': -0.27079566203904465, 'cosine_ionic_motion': 0.557822080474634, 'motion_component_glu': None, 'motion_component_asn': -5.8849242428728274, 'motion_component_residue': -5.8849242428728274, 'motion_component_ionic': 8.751195018798747, 'ionic_contributions': [{'ion_id': 1327, 'distance': 12.443742752075195, 'force': [1.5750917196273804, 1.453436017036438, -0.059865642338991165], 'magnitude': 2.1440553665161133}, {'ion_id': 1330, 'distance': 6.1113481521606445, 'force': [8.851373672485352, -0.5448993444442749, 0.612082302570343], 'magnitude': 8.889227867126465}, {'ion_id': 1341, 'distance': 7.490889549255371, 'force': [-0.1118030920624733, 4.923777103424072, 3.27870774269104], 'magnitude': 5.9165873527526855}, {'ion_id': 1359, 'distance': 8.462321281433105, 'force': [1.5930393934249878, 2.9040167331695557, -3.243910789489746], 'magnitude': 4.636167049407959}, {'ion_id': 1374, 'distance': 12.411674499511719, 'force': [0.4613865613937378, 0.8184714913368225, -1.9395605325698853], 'magnitude': 2.155149221420288}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.3212621212005615, 'force': [-10.76899528503418, 1.2038726806640625, 18.522775650024414], 'magnitude': 21.459585189819336}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.105748176574707, 'force': [8.130144119262695, -1.3959976434707642, -8.270342826843262], 'magnitude': 11.681036949157715}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 2.081256151199341, 'force': [40.91041946411133, 7.57208251953125, -56.84620666503906], 'magnitude': 70.4449462890625}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 2.1356611251831055, 'force': [-27.10550880432129, -4.105338096618652, 13.464783668518066], 'magnitude': 30.542802810668945}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 1.6265705823898315, 'force': [-9.020222663879395, -18.53685760498047, 48.450157165527344], 'magnitude': 52.65355682373047}]}, 6571: {'frame': 6571, 'ionic_force': [10.874882519245148, 11.021745204925537, -1.5739329904317856], 'ionic_force_magnitude': 15.563393017849684, 'motion_vector': [-0.7143974304199219, 2.6378211975097656, 0.46242523193359375], 'ionic_force_x': 10.874882519245148, 'ionic_force_y': 11.021745204925537, 'ionic_force_z': -1.5739329904317856, 'radial_force': 15.483602202642729, 'axial_force': -1.5739329904317856, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-1.605684757232666, 0.3110790252685547, 14.728298664093018], 'asn_force_magnitude': 14.81883177711035, 'residue_force': [-1.605684757232666, 0.3110790252685547, 14.728298664093018], 'residue_force_magnitude': 14.81883177711035, 'total_force': [9.269197762012482, 11.332824230194092, 13.154365673661232], 'total_force_magnitude': 19.682181496474634, 'motion_component_total': 10.590980308782694, 'cosine_total_motion': 0.5380999210214423, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.21372531110818835, 'cosine_residue_motion': 0.21372531110818835, 'cosine_ionic_motion': 0.4770052949537086, 'motion_component_glu': None, 'motion_component_asn': 3.1671594318228173, 'motion_component_residue': 3.1671594318228173, 'motion_component_ionic': 7.423820876959877, 'ionic_contributions': [{'ion_id': 1327, 'distance': 14.060022354125977, 'force': [0.9435466527938843, 1.3866626024246216, -0.0861724466085434], 'magnitude': 1.6794461011886597}, {'ion_id': 1330, 'distance': 6.742351531982422, 'force': [7.051734924316406, 1.6229393482208252, 0.9881018400192261], 'magnitude': 7.3032355308532715}, {'ion_id': 1341, 'distance': 8.82316780090332, 'force': [0.5937607288360596, 3.663236141204834, 2.101393938064575], 'magnitude': 4.264704704284668}, {'ion_id': 1359, 'distance': 8.525839805603027, 'force': [1.727158784866333, 3.3323826789855957, -2.602457046508789], 'magnitude': 4.5673441886901855}, {'ion_id': 1374, 'distance': 12.040011405944824, 'force': [0.5586814284324646, 1.0165244340896606, -1.9747992753982544], 'magnitude': 2.290257453918457}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.835495948791504, 'force': [-6.649723052978516, 4.378159999847412, 13.98338508605957], 'magnitude': 16.0910587310791}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.571895599365234, 'force': [5.7199931144714355, -2.777463912963867, -6.950753688812256], 'magnitude': 9.420488357543945}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 2.5052480697631836, 'force': [21.871545791625977, -12.295077323913574, -41.64374542236328], 'magnitude': 48.618255615234375}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 2.3657121658325195, 'force': [-19.082826614379883, 5.9995598793029785, 14.813304901123047], 'magnitude': 24.89142417907715}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 1.9933732748031616, 'force': [-3.4646739959716797, 5.0059003829956055, 34.52610778808594], 'magnitude': 35.058738708496094}]}, 6572: {'frame': 6572, 'ionic_force': [4.297864839434624, 8.788159370422363, -1.320813924074173], 'ionic_force_magnitude': 9.871572150372959, 'motion_vector': [0.8923988342285156, -0.882781982421875, -0.6154251098632812], 'ionic_force_x': 4.297864839434624, 'ionic_force_y': 8.788159370422363, 'ionic_force_z': -1.320813924074173, 'radial_force': 9.782810807635544, 'axial_force': -1.320813924074173, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-2.9726831912994385, 5.858217239379883, 4.899883508682251], 'asn_force_magnitude': 8.195389739253294, 'residue_force': [-2.9726831912994385, 5.858217239379883, 4.899883508682251], 'residue_force_magnitude': 8.195389739253294, 'total_force': [1.3251816481351852, 14.646376609802246, 3.579069584608078], 'total_force_magnitude': 15.135461449463087, 'motion_component_total': -9.978205373607633, 'cosine_total_motion': -0.6592600699307782, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.9461156099804022, 'cosine_residue_motion': -0.9461156099804022, 'cosine_ionic_motion': -0.22533586115184634, 'motion_component_glu': None, 'motion_component_asn': -7.753786162180759, 'motion_component_residue': -7.753786162180759, 'motion_component_ionic': -2.2244192114268744, 'ionic_contributions': [{'ion_id': 1330, 'distance': 8.661239624023438, 'force': [3.4389588832855225, 2.7700512409210205, 0.2946772277355194], 'magnitude': 4.425658702850342}, {'ion_id': 1341, 'distance': 11.687585830688477, 'force': [-0.10774736106395721, 2.0299341678619385, 1.3322513103485107], 'magnitude': 2.430459976196289}, {'ion_id': 1359, 'distance': 10.02340030670166, 'force': [0.6919946074485779, 2.870731830596924, -1.4831961393356323], 'magnitude': 3.304516315460205}, {'ion_id': 1374, 'distance': 13.351118087768555, 'force': [0.2746587097644806, 1.1174421310424805, -1.4645463228225708], 'magnitude': 1.8625279664993286}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.765955924987793, 'force': [-2.8394579887390137, 4.545980930328369, 4.686906814575195], 'magnitude': 7.120081424713135}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.571197032928467, 'force': [5.882512092590332, -10.45059871673584, -8.332319259643555], 'magnitude': 14.602962493896484}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.492272853851318, 'force': [-3.884735107421875, 4.929616928100586, 2.8739984035491943], 'magnitude': 6.903054237365723}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 3.9056949615478516, 'force': [-2.131002187728882, 6.833218097686768, 5.671297550201416], 'magnitude': 9.132231712341309}]}, 6573: {'frame': 6573, 'ionic_force': [6.707516588270664, 9.176944971084595, -0.1950500402599573], 'ionic_force_magnitude': 11.368603357600545, 'motion_vector': [-0.3231239318847656, -0.48430633544921875, 0.06146240234375], 'ionic_force_x': 6.707516588270664, 'ionic_force_y': 9.176944971084595, 'ionic_force_z': -0.1950500402599573, 'radial_force': 11.366930007008971, 'axial_force': -0.1950500402599573, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.6474916785955429, 6.648892879486084, 4.46166467666626], 'asn_force_magnitude': 8.033272912315544, 'residue_force': [0.6474916785955429, 6.648892879486084, 4.46166467666626], 'residue_force_magnitude': 8.033272912315544, 'total_force': [7.355008266866207, 15.825837850570679, 4.2666146364063025], 'total_force_magnitude': 17.965447134258092, 'motion_component_total': -16.703515181437325, 'cosine_total_motion': -0.9297578321658132, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.670869648568459, 'cosine_residue_motion': -0.670869648568459, 'cosine_ionic_motion': -0.9952177809364312, 'motion_component_glu': None, 'motion_component_asn': -5.38927897553965, 'motion_component_residue': -5.38927897553965, 'motion_component_ionic': -11.314236205897675, 'ionic_contributions': [{'ion_id': 1327, 'distance': 14.697473526000977, 'force': [0.9881269335746765, 1.1771571636199951, 0.006705602630972862], 'magnitude': 1.5369250774383545}, {'ion_id': 1330, 'distance': 8.471452713012695, 'force': [4.258534908294678, 1.36393404006958, 1.1857856512069702], 'magnitude': 4.62617826461792}, {'ion_id': 1341, 'distance': 10.060464859008789, 'force': [-0.05445399135351181, 2.8371944427490234, 1.6453436613082886], 'magnitude': 3.28021240234375}, {'ion_id': 1359, 'distance': 9.740442276000977, 'force': [1.1280900239944458, 2.8237078189849854, -1.7318087816238403], 'magnitude': 3.499296188354492}, {'ion_id': 1374, 'distance': 14.094215393066406, 'force': [0.387218713760376, 0.9749515056610107, -1.3010761737823486], 'magnitude': 1.6713072061538696}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.463759422302246, 'force': [-3.744825839996338, 7.448522567749023, 8.463831901550293], 'magnitude': 11.880263328552246}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.171883583068848, 'force': [3.697920799255371, -4.416711330413818, -4.583697319030762], 'magnitude': 7.361537933349609}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.252305269241333, 'force': [8.417840957641602, -21.18697166442871, -17.676794052124023], 'magnitude': 28.848169326782227}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.107545852661133, 'force': [-7.592984199523926, 10.794179916381836, 5.825342655181885], 'magnitude': 14.425752639770508}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 2.7270896434783936, 'force': [-0.13046003878116608, 14.009873390197754, 12.432981491088867], 'magnitude': 18.73159408569336}]}, 6574: {'frame': 6574, 'ionic_force': [9.922765612602234, 10.655503034591675, -1.8789064027369022], 'ionic_force_magnitude': 14.680984694259426, 'motion_vector': [0.2715606689453125, -0.07678985595703125, -0.05289459228515625], 'ionic_force_x': 9.922765612602234, 'ionic_force_y': 10.655503034591675, 'ionic_force_z': -1.8789064027369022, 'radial_force': 14.560254885228959, 'axial_force': -1.8789064027369022, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-0.7596144676208496, 7.04573130607605, 7.420785903930664], 'asn_force_magnitude': 10.26096521818562, 'residue_force': [-0.7596144676208496, 7.04573130607605, 7.420785903930664], 'residue_force_magnitude': 10.26096521818562, 'total_force': [9.163151144981384, 17.701234340667725, 5.541879501193762], 'total_force_magnitude': 20.68838960612352, 'motion_component_total': 2.9114362935133666, 'cosine_total_motion': 0.14072802905121315, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.3868904578765326, 'cosine_residue_motion': -0.3868904578765326, 'cosine_ionic_motion': 0.468722362180727, 'motion_component_glu': None, 'motion_component_asn': -3.9698695315190093, 'motion_component_residue': -3.9698695315190093, 'motion_component_ionic': 6.881305825032376, 'ionic_contributions': [{'ion_id': 1327, 'distance': 14.467777252197266, 'force': [0.8655595183372498, 1.3287378549575806, -0.03194442763924599], 'magnitude': 1.5861141681671143}, {'ion_id': 1330, 'distance': 6.830624103546143, 'force': [6.645339488983154, 1.9468575716018677, 1.6377795934677124], 'magnitude': 7.115694999694824}, {'ion_id': 1341, 'distance': 9.315082550048828, 'force': [0.7769212126731873, 3.7414112091064453, 0.19452917575836182], 'magnitude': 3.826173782348633}, {'ion_id': 1359, 'distance': 9.518845558166504, 'force': [1.2521162033081055, 2.632829427719116, -2.2195000648498535], 'magnitude': 3.664118766784668}, {'ion_id': 1374, 'distance': 13.530313491821289, 'force': [0.3828291893005371, 1.005666971206665, -1.459770679473877], 'magnitude': 1.8135199546813965}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.342501163482666, 'force': [-5.001438617706299, 6.690077304840088, 9.370508193969727], 'magnitude': 12.55300521850586}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.114717483520508, 'force': [4.298825740814209, -3.8537423610687256, -4.829565048217773], 'magnitude': 7.527013301849365}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.0765044689178467, 'force': [13.33101749420166, -19.95539093017578, -21.52764892578125], 'magnitude': 32.23931121826172}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 2.9930942058563232, 'force': [-10.176483154296875, 9.5642671585083, 6.838796615600586], 'magnitude': 15.550085067749023}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 2.4574155807495117, 'force': [-3.211535930633545, 14.600520133972168, 17.568695068359375], 'magnitude': 23.06833839416504}]}, 6575: {'frame': 6575, 'ionic_force': [6.102406769990921, 8.403478920459747, -1.6997588761150837], 'ionic_force_magnitude': 10.52364036776126, 'motion_vector': [-0.7413291931152344, 0.8488311767578125, 0.4405517578125], 'ionic_force_x': 6.102406769990921, 'ionic_force_y': 8.403478920459747, 'ionic_force_z': -1.6997588761150837, 'radial_force': 10.385462259959464, 'axial_force': -1.6997588761150837, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.24673700332641602, 7.761092662811279, 7.846946716308594], 'asn_force_magnitude': 11.039475134178245, 'residue_force': [0.24673700332641602, 7.761092662811279, 7.846946716308594], 'residue_force_magnitude': 11.039475134178245, 'total_force': [6.349143773317337, 16.164571583271027, 6.14718784019351], 'total_force_magnitude': 18.422619777533555, 'motion_component_total': 9.687656768826043, 'cosine_total_motion': 0.5258566309141425, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.738274537650366, 'cosine_residue_motion': 0.738274537650366, 'cosine_ionic_motion': 0.14609900324491662, 'motion_component_glu': None, 'motion_component_asn': 8.150163400588156, 'motion_component_residue': 8.150163400588156, 'motion_component_ionic': 1.5374933682378877, 'ionic_contributions': [{'ion_id': 1330, 'distance': 8.94628620147705, 'force': [3.698859691619873, 1.877339243888855, -0.03207122161984444], 'magnitude': 4.148131370544434}, {'ion_id': 1341, 'distance': 9.998907089233398, 'force': [0.6937668323516846, 2.8005433082580566, 1.644039273262024], 'magnitude': 3.320725917816162}, {'ion_id': 1359, 'distance': 9.653382301330566, 'force': [1.2716120481491089, 2.7411482334136963, -1.8873075246810913], 'magnitude': 3.5626986026763916}, {'ion_id': 1374, 'distance': 13.633832931518555, 'force': [0.4381681978702545, 0.9844481348991394, -1.4244194030761719], 'magnitude': 1.7860851287841797}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.159532070159912, 'force': [-4.797679901123047, 7.359748840332031, 10.48828411102295], 'magnitude': 13.681656837463379}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.889468669891357, 'force': [4.463278770446777, -4.281904697418213, -5.439150810241699], 'magnitude': 8.236499786376953}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 2.889049768447876, 'force': [12.661568641662598, -23.125553131103516, -25.32651710510254], 'magnitude': 36.55870819091797}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 2.7486746311187744, 'force': [-11.318129539489746, 11.834195137023926, 8.475379943847656], 'magnitude': 18.438554763793945}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 2.344921588897705, 'force': [-0.762300968170166, 15.97460651397705, 19.648950576782227], 'magnitude': 25.334766387939453}]}, 6576: {'frame': 6576, 'ionic_force': [5.697530130855739, 9.966541528701782, -1.1423418633639812], 'ionic_force_magnitude': 11.536842920320106, 'motion_vector': [0.1239013671875, -0.14241409301757812, -0.3520050048828125], 'ionic_force_x': 5.697530130855739, 'ionic_force_y': 9.966541528701782, 'ionic_force_z': -1.1423418633639812, 'radial_force': 11.480148066786693, 'axial_force': -1.1423418633639812, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-3.922982931137085, 7.049598693847656, 6.736132860183716], 'asn_force_magnitude': 10.5100962285004, 'residue_force': [-3.922982931137085, 7.049598693847656, 6.736132860183716], 'residue_force_magnitude': 10.5100962285004, 'total_force': [1.7745471997186542, 17.01614022254944, 5.593790996819735], 'total_force_magnitude': 17.999681762564464, 'motion_component_total': -10.446278808828731, 'cosine_total_motion': -0.5803590833786175, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.9197655379328833, 'cosine_residue_motion': -0.9197655379328833, 'cosine_ionic_motion': -0.06756220075795798, 'motion_component_glu': None, 'motion_component_asn': -9.666824311333038, 'motion_component_residue': -9.666824311333038, 'motion_component_ionic': -0.7794544974956932, 'ionic_contributions': [{'ion_id': 1327, 'distance': 14.209431648254395, 'force': [0.8476411700248718, 1.4078731536865234, 0.05625929310917854], 'magnitude': 1.6443136930465698}, {'ion_id': 1330, 'distance': 9.042120933532715, 'force': [3.670255661010742, 1.709186315536499, 0.31133517622947693], 'magnitude': 4.060667991638184}, {'ion_id': 1341, 'distance': 10.431806564331055, 'force': [0.002328316681087017, 2.6095755100250244, 1.5804171562194824], 'magnitude': 3.050837278366089}, {'ion_id': 1359, 'distance': 9.570117950439453, 'force': [0.9095866680145264, 3.105701446533203, -1.6332862377166748], 'magnitude': 3.624962568283081}, {'ion_id': 1374, 'distance': 13.339473724365234, 'force': [0.2677183151245117, 1.1342051029205322, -1.4570672512054443], 'magnitude': 1.8657810688018799}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.247533798217773, 'force': [-3.603886842727661, 5.0560173988342285, 5.9453301429748535], 'magnitude': 8.596409797668457}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.019979000091553, 'force': [8.181915283203125, -12.570965766906738, -11.470209121704102], 'magnitude': 18.882230758666992}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.9533658027648926, 'force': [-5.475440979003906, 5.891266345977783, 3.8418538570404053], 'magnitude': 8.913322448730469}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 3.343647003173828, 'force': [-3.0255703926086426, 8.673280715942383, 8.419157981872559], 'magnitude': 12.460421562194824}]}, 6577: {'frame': 6577, 'ionic_force': [10.770041853189468, 11.033284544944763, -1.4359604306519032], 'ionic_force_magnitude': 15.48512679081343, 'motion_vector': [2.2769126892089844, -2.477092742919922, -0.91888427734375], 'ionic_force_x': 10.770041853189468, 'ionic_force_y': 11.033284544944763, 'ionic_force_z': -1.4359604306519032, 'radial_force': 15.41840359340648, 'axial_force': -1.4359604306519032, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-0.9619882106781006, 5.421460151672363, 4.095129013061523], 'asn_force_magnitude': 6.8620502131122025, 'residue_force': [-0.9619882106781006, 5.421460151672363, 4.095129013061523], 'residue_force_magnitude': 6.8620502131122025, 'total_force': [9.808053642511368, 16.454744696617126, 2.6591685824096203], 'total_force_magnitude': 19.33979619424425, 'motion_component_total': -5.984110926139508, 'cosine_total_motion': -0.30941954434454944, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.8098635667906998, 'cosine_residue_motion': -0.8098635667906998, 'cosine_ionic_motion': -0.027561057188422215, 'motion_component_glu': None, 'motion_component_asn': -5.55732446108793, 'motion_component_residue': -5.55732446108793, 'motion_component_ionic': -0.4267864650515779, 'ionic_contributions': [{'ion_id': 1327, 'distance': 14.401464462280273, 'force': [1.0223180055618286, 1.2306550741195679, 0.052624136209487915], 'magnitude': 1.6007546186447144}, {'ion_id': 1330, 'distance': 6.132602691650391, 'force': [7.852027416229248, 3.727412223815918, 1.5429376363754272], 'magnitude': 8.827717781066895}, {'ion_id': 1341, 'distance': 12.76302719116211, 'force': [0.4523809254169464, 1.9864200353622437, 0.05863363668322563], 'magnitude': 2.0381243228912354}, {'ion_id': 1359, 'distance': 9.616036415100098, 'force': [1.0853403806686401, 2.987722158432007, -1.669343113899231], 'magnitude': 3.5904252529144287}, {'ion_id': 1374, 'distance': 13.458894729614258, 'force': [0.3579751253128052, 1.1010750532150269, -1.420812726020813], 'magnitude': 1.832817792892456}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.870000839233398, 'force': [-4.254752159118652, 6.033515930175781, 6.716550827026367], 'magnitude': 9.98089599609375}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.677136421203613, 'force': [3.515805959701538, -3.4957027435302734, -3.5700771808624268], 'magnitude': 6.109523773193359}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.6615095138549805, 'force': [10.05775260925293, -15.751140594482422, -12.991555213928223], 'magnitude': 22.760433197021484}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.6390881538391113, 'force': [-6.661928653717041, 7.141546249389648, 3.9081318378448486], 'magnitude': 10.51933765411377}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 2.980756998062134, 'force': [-3.618865966796875, 11.493241310119629, 10.032078742980957], 'magnitude': 15.67907428741455}]}, 6578: {'frame': 6578, 'ionic_force': [11.297083020210266, 8.097006931900978, -3.776877298951149], 'ionic_force_magnitude': 14.403138829856085, 'motion_vector': [-1.2792587280273438, 0.96728515625, 1.4186248779296875], 'ionic_force_x': 11.297083020210266, 'ionic_force_y': 8.097006931900978, 'ionic_force_z': -3.776877298951149, 'radial_force': 13.899122491034303, 'axial_force': -3.776877298951149, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-84.09410262107849, -24.021531105041504, 627.1876850128174], 'asn_force_magnitude': 633.2560653353523, 'residue_force': [-84.09410262107849, -24.021531105041504, 627.1876850128174], 'residue_force_magnitude': 633.2560653353523, 'total_force': [-72.79701960086823, -15.924524173140526, 623.4108077138662], 'total_force_magnitude': 627.8487331414831, 'motion_component_total': 449.33635608261034, 'cosine_total_motion': 0.7156761372031857, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.7183987378373606, 'cosine_residue_motion': 0.7183987378373606, 'cosine_ionic_motion': -0.38838770133661316, 'motion_component_glu': None, 'motion_component_asn': 454.9303580647703, 'motion_component_residue': 454.9303580647703, 'motion_component_ionic': -5.594001982159921, 'ionic_contributions': [{'ion_id': 1327, 'distance': 13.392813682556152, 'force': [1.3949049711227417, 1.2103792428970337, -0.1234259232878685], 'magnitude': 1.8509489297866821}, {'ion_id': 1330, 'distance': 8.506098747253418, 'force': [4.5826263427734375, 0.2037651091814041, 0.11392490565776825], 'magnitude': 4.588568687438965}, {'ion_id': 1341, 'distance': 8.48983097076416, 'force': [2.695676326751709, 3.7334976196289062, 0.10549106448888779], 'magnitude': 4.606170177459717}, {'ion_id': 1359, 'distance': 9.237970352172852, 'force': [2.0399694442749023, 2.267669677734375, -2.4146974086761475], 'magnitude': 3.8903167247772217}, {'ion_id': 1374, 'distance': 13.924551963806152, 'force': [0.5839059352874756, 0.681695282459259, -1.458169937133789], 'magnitude': 1.7122832536697388}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 2.412480354309082, 'force': [3.3867037296295166, 7.870773792266846, 39.75961685180664], 'magnitude': 40.67242431640625}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.707017660140991, 'force': [9.827856063842773, -7.655353546142578, -23.808813095092773], 'magnitude': 26.871002197265625}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 1.3449290990829468, 'force': [-82.64669799804688, -7.126943111419678, -146.89013671875], 'magnitude': 168.6949462890625}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 0.4340415298938751, 'force': [-47.24699401855469, -11.119616508483887, 737.8590087890625], 'magnitude': 739.4537963867188}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 1.893883466720581, 'force': [32.58502960205078, -5.990391731262207, 20.268009185791016], 'magnitude': 38.83891296386719}]}, 6579: {'frame': 6579, 'ionic_force': [9.608516097068787, 8.373697221279144, -1.9300379157066345], 'ionic_force_magnitude': 12.89059475343761, 'motion_vector': [2.924358367919922, -6.608238220214844, -2.4186172485351562], 'ionic_force_x': 9.608516097068787, 'ionic_force_y': 8.373697221279144, 'ionic_force_z': -1.9300379157066345, 'radial_force': 12.745288805723, 'axial_force': -1.9300379157066345, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-0.7262768745422363, 2.8879292011260986, 9.543179512023926], 'asn_force_magnitude': 9.9969939665844, 'residue_force': [-0.7262768745422363, 2.8879292011260986, 9.543179512023926], 'residue_force_magnitude': 9.9969939665844, 'total_force': [8.88223922252655, 11.261626422405243, 7.613141596317291], 'total_force_magnitude': 16.238175028296176, 'motion_component_total': -8.773554211712579, 'cosine_total_motion': -0.5403042026843556, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.5813693883990191, 'cosine_residue_motion': -0.5813693883990191, 'cosine_ionic_motion': -0.2297495189460466, 'motion_component_glu': None, 'motion_component_asn': -5.811946268181856, 'motion_component_residue': -5.811946268181856, 'motion_component_ionic': -2.9616079435307228, 'ionic_contributions': [{'ion_id': 1327, 'distance': 12.721465110778809, 'force': [1.3253157138824463, 1.562822699546814, 0.09811156988143921], 'magnitude': 2.0514633655548096}, {'ion_id': 1330, 'distance': 7.632896900177002, 'force': [5.451991558074951, 0.6885251402854919, 1.5081236362457275], 'magnitude': 5.698483943939209}, {'ion_id': 1341, 'distance': 14.535503387451172, 'force': [0.3505029082298279, 1.43211030960083, 0.5435124635696411], 'magnitude': 1.5713682174682617}, {'ion_id': 1359, 'distance': 8.499899864196777, 'force': [1.873288631439209, 3.515359878540039, -2.291175127029419], 'magnitude': 4.595263957977295}, {'ion_id': 1374, 'distance': 12.216654777526855, 'force': [0.6074172854423523, 1.1748791933059692, -1.7886104583740234], 'magnitude': 2.2245054244995117}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.1815185546875, 'force': [-3.4913713932037354, 4.643194198608398, 12.22835922241211], 'magnitude': 13.53815746307373}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.76894998550415, 'force': [4.119980335235596, -3.156247854232788, -6.930066108703613], 'magnitude': 8.65805721282959}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 2.853111982345581, 'force': [8.150490760803223, -13.455161094665527, -34.02484893798828], 'magnitude': 37.48549270629883}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 2.461745023727417, 'force': [-12.204421043395996, 8.97136402130127, 17.291080474853516], </t>
         </is>
       </c>
     </row>
@@ -515,7 +515,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>{6716: {'frame': 6716, 'ionic_force': [3.5372003354132175, 2.635218560695648, -13.300951480865479], 'ionic_force_magnitude': 14.013260625986366, 'motion_vector': [2.1366920471191406, 6.534908294677734, 0.9935302734375], 'ionic_force_x': 3.5372003354132175, 'ionic_force_y': 2.635218560695648, 'ionic_force_z': -13.300951480865479, 'radial_force': 4.4109140861597185, 'axial_force': -13.300951480865479, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [10.430237293243408, -2.519187092781067, 2.3031381368637085], 'asn_force_magnitude': 10.974543219618589, 'residue_force': [10.430237293243408, -2.519187092781067, 2.3031381368637085], 'residue_force_magnitude': 10.974543219618589, 'total_force': [13.967437628656626, 0.1160314679145813, -10.99781334400177], 'total_force_magnitude': 17.777926638431794, 'motion_component_total': 2.83235411582245, 'cosine_total_motion': 0.15931858497489526, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.10640135998621542, 'cosine_residue_motion': 0.10640135998621542, 'cosine_ionic_motion': 0.11879089645564639, 'motion_component_glu': None, 'motion_component_asn': 1.167706323794917, 'motion_component_residue': 1.167706323794917, 'motion_component_ionic': 1.6646477920275329}, 6717: {'frame': 6717, 'ionic_force': [0.5450510084629059, 4.748510509729385, -11.099060416221619], 'ionic_force_magnitude': 12.084476603716624, 'motion_vector': [-2.882415771484375, -8.947956085205078, 1.36480712890625], 'ionic_force_x': 0.5450510084629059, 'ionic_force_y': 4.748510509729385, 'ionic_force_z': -11.099060416221619, 'radial_force': 4.779689599005029, 'axial_force': -11.099060416221619, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-3.1488189697265625, -8.874019980430603, -0.7465218305587769], 'asn_force_magnitude': 9.445664950689933, 'residue_force': [-3.1488189697265625, -8.874019980430603, -0.7465218305587769], 'residue_force_magnitude': 9.445664950689933, 'total_force': [-2.6037679612636566, -4.125509470701218, -11.845582246780396], 'total_force_magnitude': 12.810825685887208, 'motion_component_total': 2.9742241709054857, 'cosine_total_motion': 0.23216490832296477, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.9747498067733612, 'cosine_residue_motion': 0.9747498067733612, 'cosine_ionic_motion': -0.5157803783333467, 'motion_component_glu': None, 'motion_component_asn': 9.207160085530923, 'motion_component_residue': 9.207160085530923, 'motion_component_ionic': -6.232935914625437}, 6718: {'frame': 6718, 'ionic_force': [-15.74527932703495, -6.038105010986328, -8.724657155573368], 'ionic_force_magnitude': 18.986631499356328, 'motion_vector': [-0.8591651916503906, -0.15292739868164062, -0.16278839111328125], 'ionic_force_x': -15.74527932703495, 'ionic_force_y': -6.038105010986328, 'ionic_force_z': -8.724657155573368, 'radial_force': 16.863348813626917, 'axial_force': -8.724657155573368, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [21.994686126708984, -2.6051195710897446, 2.344572961330414], 'asn_force_magnitude': 22.272177445483887, 'residue_force': [21.994686126708984, -2.6051195710897446, 2.344572961330414], 'residue_force_magnitude': 22.272177445483887, 'total_force': [6.249406799674034, -8.643224582076073, -6.380084194242954], 'total_force_magnitude': 12.428430747670637, 'motion_component_total': -3.3894402347929886, 'cosine_total_motion': -0.272716669031466, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.9549263311797028, 'cosine_residue_motion': -0.9549263311797028, 'cosine_ionic_motion': 0.9416545773910651, 'motion_component_glu': None, 'motion_component_asn': -21.268288695399253, 'motion_component_residue': -21.268288695399253, 'motion_component_ionic': 17.878848460606267}, 6719: {'frame': 6719, 'ionic_force': [-13.247648186981678, -7.324256241321564, -7.235395602881908], 'ionic_force_magnitude': 16.777838403822457, 'motion_vector': [3.021942138671875, 1.1164970397949219, -1.1178054809570312], 'ionic_force_x': -13.247648186981678, 'ionic_force_y': -7.324256241321564, 'ionic_force_z': -7.235395602881908, 'radial_force': 15.13753321960275, 'axial_force': -7.235395602881908, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [29.421308517456055, -4.946713283658028, 8.758866712450981], 'asn_force_magnitude': 31.09342556355817, 'residue_force': [29.421308517456055, -4.946713283658028, 8.758866712450981], 'residue_force_magnitude': 31.09342556355817, 'total_force': [16.173660330474377, -12.270969524979591, 1.5234711095690727], 'total_force_magnitude': 20.358903354312332, 'motion_component_total': 9.815921531206694, 'cosine_total_motion': 0.4821439229990514, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.6941101257523201, 'cosine_residue_motion': 0.6941101257523201, 'cosine_ionic_motion': -0.7013024987834178, 'motion_component_glu': None, 'motion_component_asn': 21.58226152799177, 'motion_component_residue': 21.58226152799177, 'motion_component_ionic': -11.766339996785078}, 6720: {'frame': 6720, 'ionic_force': [-13.875824749469757, -1.1168307960033417, -19.71669438481331], 'ionic_force_magnitude': 24.135738251999413, 'motion_vector': [-2.0362319946289062, -3.377918243408203, 1.4120712280273438], 'ionic_force_x': -13.875824749469757, 'ionic_force_y': -1.1168307960033417, 'ionic_force_z': -19.71669438481331, 'radial_force': 13.920697665882228, 'axial_force': -19.71669438481331, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-7.1707658767700195, -20.72485041618347, 13.114341616630554], 'asn_force_magnitude': 25.552402315052838, 'residue_force': [-7.1707658767700195, -20.72485041618347, 13.114341616630554], 'residue_force_magnitude': 25.552402315052838, 'total_force': [-21.046590626239777, -21.841681212186813, -6.6023527681827545], 'total_force_magnitude': 31.04205336698668, 'motion_component_total': 25.6155671172993, 'cosine_total_motion': 0.82518919784287, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.9633717340628261, 'cosine_residue_motion': 0.9633717340628261, 'cosine_ionic_motion': 0.041395252929257796, 'motion_component_glu': None, 'motion_component_asn': 24.616462127723423, 'motion_component_residue': 24.616462127723423, 'motion_component_ionic': 0.9991049895758781}, 6721: {'frame': 6721, 'ionic_force': [-14.872823670506477, -15.005800008773804, -8.68900191783905], 'ionic_force_magnitude': 22.84455454075444, 'motion_vector': [-1.2706642150878906, 0.12684249877929688, -0.00298309326171875], 'ionic_force_x': -14.872823670506477, 'ionic_force_y': -15.005800008773804, 'ionic_force_z': -8.68900191783905, 'radial_force': 21.127586654355333, 'axial_force': -8.68900191783905, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [15.174116134643555, -0.2986522912979126, 0.23915520310401917], 'asn_force_magnitude': 15.17893899025617, 'residue_force': [15.174116134643555, -0.2986522912979126, 0.23915520310401917], 'residue_force_magnitude': 15.17893899025617, 'total_force': [0.30129246413707733, -15.304452300071716, -8.449846714735031], 'total_force_magnitude': 17.48476327711172, 'motion_component_total': -1.8002511283057345, 'cosine_total_motion': -0.10296113820782107, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.9967268639087372, 'cosine_residue_motion': -0.9967268639087372, 'cosine_ionic_motion': 0.5834653113999466, 'motion_component_glu': None, 'motion_component_asn': -15.129256257220087, 'motion_component_residue': -15.129256257220087, 'motion_component_ionic': 13.329005128914353}, 6722: {'frame': 6722, 'ionic_force': [-6.684693541377783, -13.338738977909088, -3.4362437948584557], 'ionic_force_magnitude': 15.310612550797314, 'motion_vector': [1.3387413024902344, 0.14303207397460938, 0.6805572509765625], 'ionic_force_x': -6.684693541377783, 'ionic_force_y': -13.338738977909088, 'ionic_force_z': -3.4362437948584557, 'radial_force': 14.920022964557695, 'axial_force': -3.4362437948584557, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [4.270717620849609, -6.068329334259033, 1.5291308164596558], 'asn_force_magnitude': 7.576403563691061, 'residue_force': [4.270717620849609, -6.068329334259033, 1.5291308164596558], 'residue_force_magnitude': 7.576403563691061, 'total_force': [-2.4139759205281734, -19.40706831216812, -1.9071129783988], 'total_force_magnitude': 19.649393378179056, 'motion_component_total': -4.84254892780208, 'cosine_total_motion': -0.24644775716993905, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.5153317496321815, 'cosine_residue_motion': 0.5153317496321815, 'cosine_ionic_motion': -0.5712972099044454, 'motion_component_glu': None, 'motion_component_asn': 3.90436130439641, 'motion_component_residue': 3.90436130439641, 'motion_component_ionic': -8.74691023219849}, 6723: {'frame': 6723, 'ionic_force': [-0.5762564726173878, -13.915500342845917, 1.1806349530816078], 'ionic_force_magnitude': 13.977378874682344, 'motion_vector': [-0.162322998046875, 2.1346893310546875, 1.369384765625], 'ionic_force_x': -0.5762564726173878, 'ionic_force_y': -13.915500342845917, 'ionic_force_z': 1.1806349530816078, 'radial_force': 13.92742694520342, 'axial_force': 1.1806349530816078, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [15.259693145751953, -0.13366782665252686, -0.7264796169474721], 'asn_force_magnitude': 15.277561147782434, 'residue_force': [15.259693145751953, -0.13366782665252686, -0.7264796169474721], 'residue_force_magnitude': 15.277561147782434, 'total_force': [14.683436673134565, -14.049168169498444, 0.4541553361341357], 'total_force_magnitude': 20.327043460821855, 'motion_component_total': -12.494206561479418, 'cosine_total_motion': -0.6146593126324854, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.09677030005628524, 'cosine_residue_motion': -0.09677030005628524, 'cosine_ionic_motion': -0.7881157464389487, 'motion_component_glu': None, 'motion_component_asn': -1.4784141763991516, 'motion_component_residue': -1.4784141763991516, 'motion_component_ionic': -11.015792385080267}, 6725: {'frame': 6725, 'ionic_force': [-2.6017091274261475, -10.550699710845947, -2.3864916190505028], 'ionic_force_magnitude': 11.125713326343421, 'motion_vector': [-0.458587646484375, 0.23482513427734375, -0.8922119140625], 'ionic_force_x': -2.6017091274261475, 'ionic_force_y': -10.550699710845947, 'ionic_force_z': -2.3864916190505028, 'radial_force': 10.866745362443039, 'axial_force': -2.3864916190505028, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [14.904263019561768, -3.653952479362488, 1.1480313390493393], 'asn_force_magnitude': 15.38851522510067, 'residue_force': [14.904263019561768, -3.653952479362488, 1.1480313390493393], 'residue_force_magnitude': 15.38851522510067, 'total_force': [12.30255389213562, -14.204652190208435, -1.2384602800011635], 'total_force_magnitude': 18.83238593431101, 'motion_component_total': -7.641029267764303, 'cosine_total_motion': -0.40573877863468144, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.5498252854484987, 'cosine_residue_motion': -0.5498252854484987, 'cosine_ionic_motion': 0.0737000392202924, 'motion_component_glu': None, 'motion_component_asn': -8.460994776269544, 'motion_component_residue': -8.460994776269544, 'motion_component_ionic': 0.81996550850524}, 6726: {'frame': 6726, 'ionic_force': [-10.6773931235075, -23.184772670269012, 0.8381237238645554], 'ionic_force_magnitude': 25.539045774313546, 'motion_vector': [1.3153266906738281, 2.5401535034179688, 0.22161865234375], 'ionic_force_x': -10.6773931235075, 'ionic_force_y': -23.184772670269012, 'ionic_force_z': 0.8381237238645554, 'radial_force': 25.525289571050475, 'axial_force': 0.8381237238645554, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [7.387481212615967, -6.994044780731201, 0.925237700343132], 'asn_force_magnitude': 10.215067589779496, 'residue_force': [7.387481212615967, -6.994044780731201, 0.925237700343132], 'residue_force_magnitude': 10.215067589779496, 'total_force': [-3.289911910891533, -30.178817451000214, 1.7633614242076874], 'total_force_magnitude': 30.408781406603666, 'motion_component_total': -28.09107565792514, 'cosine_total_motion': -0.9237816958960675, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.26764046394851304, 'cosine_residue_motion': -0.26764046394851304, 'cosine_ionic_motion': -0.9928761807708024, 'motion_component_glu': None, 'motion_component_asn': -2.733965428994003, 'motion_component_residue': -2.733965428994003, 'motion_component_ionic': -25.357110228931134}, 6727: {'frame': 6727, 'ionic_force': [0.19401593878865242, -14.893805980682373, -1.1919869855046272], 'ionic_force_magnitude': 14.942688237004964, 'motion_vector': [1.3554725646972656, -0.12535858154296875, 0.22263336181640625], 'ionic_force_x': 0.19401593878865242, 'ionic_force_y': -14.893805980682373, 'ionic_force_z': -1.1919869855046272, 'radial_force': 14.895069612952941, 'axial_force': -1.1919869855046272, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [15.635623455047607, -4.838559329509735, 1.3787758648395538], 'asn_force_magnitude': 16.42514536004734, 'residue_force': [15.635623455047607, -4.838559329509735, 1.3787758648395538], 'residue_force_magnitude': 16.42514536004734, 'total_force': [15.82963939383626, -19.732365310192108, 0.1867888793349266], 'total_force_magnitude': 25.297798603024905, 'motion_component_total': 17.379182707049065, 'cosine_total_motion': 0.6869839933412627, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.9757798625021488, 'cosine_residue_motion': 0.9757798625021488, 'cosine_ionic_motion': 0.09046943927374791, 'motion_component_glu': None, 'motion_component_asn': 16.027326081004798, 'motion_component_residue': 16.027326081004798, 'motion_component_ionic': 1.3518566260442677}, 6728: {'frame': 6728, 'ionic_force': [2.4772856384515762, -9.180882215499878, -5.546252489089966], 'ionic_force_magnitude': 11.008472149308323, 'motion_vector': [-2.3235855102539062, 0.4115257263183594, -0.305999755859375], 'ionic_force_x': 2.4772856384515762, 'ionic_force_y': -9.180882215499878, 'ionic_force_z': -5.546252489089966, 'radial_force': 9.509234584831756, 'axial_force': -5.546252489089966, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [26.263432025909424, -33.52600917220116, -6.009776473045349], 'asn_force_magnitude': 43.01021467105286, 'residue_force': [26.263432025909424, -33.52600917220116, -6.009776473045349], 'residue_force_magnitude': 43.01021467105286, 'total_force': [28.740717664361, -42.706891387701035, -11.556028962135315], 'total_force_magnitude': 52.75840434695799, 'motion_component_total': -33.96521336303074, 'cosine_total_motion': -0.6437877298119831, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.7131232627027111, 'cosine_residue_motion': -0.7131232627027111, 'cosine_ionic_motion': -0.29919036016932293, 'motion_component_glu': None, 'motion_component_asn': -30.671584615765227, 'motion_component_residue': -30.671584615765227, 'motion_component_ionic': -3.293628747265518}, 6729: {'frame': 6729, 'ionic_force': [-0.1381404548883438, -10.870651245117188, -5.780998591333628], 'ionic_force_magnitude': 12.313004750719704, 'motion_vector': [6.845603942871094, -0.24485015869140625, 2.0646591186523438], 'ionic_force_x': -0.1381404548883438, 'ionic_force_y': -10.870651245117188, 'ionic_force_z': -5.780998591333628, 'radial_force': 10.871528930111193, 'axial_force': -5.780998591333628, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [19.96870183944702, 4.045881658792496, 3.3776470087468624], 'asn_force_magnitude': 20.652523111363053, 'residue_force': [19.96870183944702, 4.045881658792496, 3.3776470087468624], 'residue_force_magnitude': 20.652523111363053, 'total_force': [19.830561384558678, -6.824769586324692, -2.4033515825867653], 'total_force_magnitude': 21.109352040332613, 'motion_component_total': 18.514704458817842, 'cosine_total_motion': 0.8770853990895929, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.9656528813426598, 'cosine_residue_motion': 0.9656528813426598, 'cosine_ionic_motion': -0.11601262401707942, 'motion_component_glu': None, 'motion_component_asn': 19.943168449483604, 'motion_component_residue': 19.943168449483604, 'motion_component_ionic': -1.4284639906657577}, 6730: {'frame': 6730, 'ionic_force': [6.242489993572235, -8.63433450460434, -3.8057007491588593], 'ionic_force_magnitude': 11.313875191524735, 'motion_vector': [-1.2953071594238281, -0.1076507568359375, -0.698211669921875], 'ionic_force_x': 6.242489993572235, 'ionic_force_y': -8.63433450460434, 'ionic_force_z': -3.8057007491588593, 'radial_force': 10.654595893662535, 'axial_force': -3.8057007491588593, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-12.818450927734375, 8.374242305755615, 18.869015216827393], 'asn_force_magnitude': 24.29980151431499, 'residue_force': [-12.818450927734375, 8.374242305755615, 18.869015216827393], 'residue_force_magnitude': 24.29980151431499, 'total_force': [-6.57596093416214, -0.26009219884872437, 15.063314467668533], 'total_force_magnitude': 16.438197982485814, 'motion_component_total': -1.336211613549998, 'cosine_total_motion': -0.08128698869387468, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.070504190700785, 'cosine_residue_motion': 0.070504190700785, 'cosine_ionic_motion': -0.2695318272373059, 'motion_component_glu': None, 'motion_component_asn': 1.7132378399564878, 'motion_component_residue': 1.7132378399564878, 'motion_component_ionic': -3.0494494535064858}, 6731: {'frame': 6731, 'ionic_force': [5.921286433935165, -8.68039095401764, -5.1164384491276], 'ionic_force_magnitude': 11.68711951470537, 'motion_vector': [-3.020660400390625, -1.9799308776855469, -1.5014266967773438], 'ionic_force_x': 5.921286433935165, 'ionic_force_y': -8.68039095401764, 'ionic_force_z': -5.1164384491276, 'radial_force': 10.50765531159525, 'axial_force': -5.1164384491276, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-8.266975402832031, -86.22281551361084, -60.90032505989075], 'asn_force_magnitude': 105.88468439677929, 'residue_force': [-8.266975402832031, -86.22281551361084, -60.90032505989075], 'residue_force_magnitude': 105.88468439677929, 'total_force': [-2.345688968896866, -94.90320646762848, -66.01676350901835], 'total_force_magnitude': 115.63016007418558, 'motion_component_total': 75.19278984785117, 'cosine_total_motion': 0.6502869995130098, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.6932792135974126, 'cosine_residue_motion': 0.6932792135974126, 'cosine_ionic_motion': 0.15274414837596564, 'motion_component_glu': None, 'motion_component_asn': 73.40765073060938, 'motion_component_residue': 73.40765073060938, 'motion_component_ionic': 1.7851391172418007}, 6732: {'frame': 6732, 'ionic_force': [1.955627828836441, -8.962807416915894, -4.607766941189766], 'ionic_force_magnitude': 10.265861541145165, 'motion_vector': [-0.6335678100585938, -1.2690963745117188, -0.14817047119140625], 'ionic_force_x': 1.955627828836441, 'ionic_force_y': -8.962807416915894, 'ionic_force_z': -4.607766941189766, 'radial_force': 9.17367957788161, 'axial_force': -4.607766941189766, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [48.236093521118164, 46.80040621757507, 9.09523481503129], 'asn_force_magnitude': 67.82125062728241, 'residue_force': [48.236093521118164, 46.80040621757507, 9.09523481503129], 'residue_force_magnitude': 67.82125062728241, 'total_force': [50.191721349954605, 37.83759880065918, 4.487467873841524], 'total_force_magnitude': 63.016110186125374, 'motion_component_total': -56.43379263797134, 'cosine_total_motion': -0.8955454798985149, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.9439430068863643, 'cosine_residue_motion': -0.9439430068863643, 'cosine_ionic_motion': 0.7389153437864471, 'motion_component_glu': None, 'motion_component_asn': -64.01939524791068, 'motion_component_residue': -64.01939524791068, 'motion_component_ionic': 7.585602609939345}, 6733: {'frame': 6733, 'ionic_force': [0.8487526476383209, -7.318961501121521, -2.883708417415619], 'ionic_force_magnitude': 7.912228052100479, 'motion_vector': [-0.7289466857910156, 5.138896942138672, 0.6813125610351562], 'ionic_force_x': 0.8487526476383209, 'ionic_force_y': -7.318961501121521, 'ionic_force_z': -2.883708417415619, 'radial_force': 7.36801048531909, 'axial_force': -2.883708417415619, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [6.313289403915405, 11.005126357078552, 1.2774989604949951], 'asn_force_magnitude': 12.751565897054423, 'residue_force': [6.313289403915405, 11.005126357078552, 1.2774989604949951], 'residue_force_magnitude': 12.751565897054423, 'total_force': [7.162042051553726, 3.6861648559570312, -1.6062094569206238], 'total_force_magnitude': 8.213559917174639, 'motion_component_total': 2.4122384883373313, 'cosine_total_motion': 0.29368976578515193, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.7913164704901857, 'cosine_residue_motion': 0.7913164704901857, 'cosine_ionic_motion': -0.9704328009737309, 'motion_component_glu': None, 'motion_component_asn': 10.090524118880126, 'motion_component_residue': 10.090524118880126, 'motion_component_ionic': -7.678285630542795}, 6735: {'frame': 6735, 'ionic_force': [0.1152866929769516, -11.250973999500275, -6.662376455962658], 'ionic_force_magnitude': 13.07612201686625, 'motion_vector': [4.712928771972656, -0.7217674255371094, 0.44530487060546875], 'ionic_force_x': 0.1152866929769516, 'ionic_force_y': -11.250973999500275, 'ionic_force_z': -6.662376455962658, 'radial_force': 11.251564644928667, 'axial_force': -6.662376455962658, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [15.251408576965332, 4.214793831110001, 8.42385470867157], 'asn_force_magnitude': 17.925715572135545, 'residue_force': [15.251408576965332, 4.214793831110001, 8.42385470867157], 'residue_force_magnitude': 17.925715572135545, 'total_force': [15.366695269942284, -7.036180168390274, 1.761478252708912], 'total_force_magnitude': 16.992526607779126, 'motion_component_total': 16.34811697523501, 'cosine_total_motion': 0.9620768795942853, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.845622842165887, 'cosine_residue_motion': 0.845622842165887, 'cosine_ionic_motion': 0.09098434717371777, 'motion_component_glu': None, 'motion_component_asn': 15.158394549966559, 'motion_component_residue': 15.158394549966559, 'motion_component_ionic': 1.1897224252684535}, 6736: {'frame': 6736, 'ionic_force': [3.921821415424347, -9.079240322113037, -5.114391982555389], 'ionic_force_magnitude': 11.13419477970415, 'motion_vector': [-2.3464584350585938, -0.8663825988769531, -0.7218017578125], 'ionic_force_x': 3.921821415424347, 'ionic_force_y': -9.079240322113037, 'ionic_force_z': -5.114391982555389, 'radial_force': 9.890060062566064, 'axial_force': -5.114391982555389, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-1.2585983276367188, -22.61277985572815, 1.7097110748291016], 'asn_force_magnitude': 22.712221258902616, 'residue_force': [-1.2585983276367188, -22.61277985572815, 1.7097110748291016], 'residue_force_magnitude': 22.712221258902616, 'total_force': [2.663223087787628, -31.692020177841187, -3.404680907726288], 'total_force_magnitude': 31.98544594423304, 'motion_component_total': 9.090474460311343, 'cosine_total_motion': 0.28420658808886645, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.36041238970723644, 'cosine_residue_motion': 0.36041238970723644, 'cosine_ionic_motion': 0.08125495724934617, 'motion_component_glu': None, 'motion_component_asn': 8.18576593948059, 'motion_component_residue': 8.18576593948059, 'motion_component_ionic': 0.9047085208307539}, 6737: {'frame': 6737, 'ionic_force': [1.429343543946743, -8.786172986030579, -4.839783970266581], 'ionic_force_magnitude': 10.13229330339016, 'motion_vector': [-0.7057685852050781, 2.4183120727539062, -3.2960205078125], 'ionic_force_x': 1.429343543946743, 'ionic_force_y': -8.786172986030579, 'ionic_force_z': -4.839783970266581, 'radial_force': 8.901677297401637, 'axial_force': -4.839783970266581, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [50.38634920120239, 13.626427799463272, -12.629289656877518], 'asn_force_magnitude': 53.70253883790605, 'residue_force': [50.38634920120239, 13.626427799463272, -12.629289656877518], 'residue_force_magnitude': 53.70253883790605, 'total_force': [51.815692745149136, 4.8402548134326935, -17.4690736271441], 'total_force_magnitude': 54.89501447954305, 'motion_component_total': 7.885679895119946, 'cosine_total_motion': 0.1436502015690075, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.1751383815674174, 'cosine_residue_motion': 0.1751383815674174, 'cosine_ionic_motion': -0.14998537818716928, 'motion_component_glu': None, 'motion_component_asn': 9.405375738132241, 'motion_component_residue': 9.405375738132241, 'motion_component_ionic': -1.519695843012296}, 6738: {'frame': 6738, 'ionic_force': [0.9048817381262779, -7.781327426433563, -5.582104861736298], 'ionic_force_magnitude': 9.61913520877951, 'motion_vector': [0.6251106262207031, -3.9033660888671875, 2.5921707153320312], 'ionic_force_x': 0.9048817381262779, 'ionic_force_y': -7.781327426433563, 'ionic_force_z': -5.582104861736298, 'radial_force': 7.833764578882979, 'axial_force': -5.582104861736298, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [7.256131649017334, -3.746622681617737, 5.531697034835815], 'asn_force_magnitude': 9.863483163238778, 'residue_force': [7.256131649017334, -3.746622681617737, 5.531697034835815], 'residue_force_magnitude': 9.863483163238778, 'total_force': [8.161013387143612, -11.5279501080513, -0.05040782690048218], 'total_force_magnitude': 14.124387213180968, 'motion_component_total': 10.57046972511555, 'cosine_total_motion': 0.7483843062055904, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.7184614812294504, 'cosine_residue_motion': 0.7184614812294504, 'cosine_ionic_motion': 0.36218817242463114, 'motion_component_glu': None, 'motion_component_asn': 7.086532723542277, 'motion_component_residue': 7.086532723542277, 'motion_component_ionic': 3.483937001573273}, 6739: {'frame': 6739, 'ionic_force': [0.6931726336479187, -5.631544232368469, -2.902565985918045], 'ionic_force_magnitude': 6.373356105206216, 'motion_vector': [4.595001220703125, 3.0436325073242188, 2.2935104370117188], 'ionic_force_x': 0.6931726336479187, 'ionic_force_y': -5.631544232368469, 'ionic_force_z': -2.902565985918045, 'radial_force': 5.674044302009014, 'axial_force': -2.902565985918045, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [5.363488674163818, 15.868772983551025, 3.668878212571144], 'asn_force_magnitude': 17.147758865229058, 'residue_force': [5.363488674163818, 15.868772983551025, 3.668878212571144], 'residue_force_magnitude': 17.147758865229058, 'total_force': [6.056661307811737, 10.237228751182556, 0.7663122266530991], 'total_force_magnitude': 11.919363788822816, 'motion_component_total': 10.175679631232235, 'cosine_total_motion': 0.8537099640145482, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.7947667204863275, 'cosine_residue_motion': 0.7947667204863275, 'cosine_ionic_motion': -0.5417535735929965, 'motion_component_glu': None, 'motion_component_asn': 13.628468077008446, 'motion_component_residue': 13.628468077008446, 'motion_component_ionic': -3.4527884457762097}, 6740: {'frame': 6740, 'ionic_force': [6.653733730316162, -12.968421638011932, 0.5059778839349747], 'ionic_force_magnitude': 14.584517337033626, 'motion_vector': [-0.7445793151855469, -0.18370437622070312, -0.7890472412109375], 'ionic_force_x': 6.653733730316162, 'ionic_force_y': -12.968421638011932, 'ionic_force_z': 0.5059778839349747, 'radial_force': 14.575737797285019, 'axial_force': 0.5059778839349747, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-23.347854256629944, 7.471371650695801, 19.56956911087036], 'asn_force_magnitude': 31.367367245543342, 'residue_force': [-23.347854256629944, 7.471371650695801, 19.56956911087036], 'residue_force_magnitude': 31.367367245543342, 'total_force': [-16.69412052631378, -5.497049987316132, 20.075546994805336], 'total_force_magnitude': 26.68218142976284, 'motion_component_total': -2.181718330710801, 'cosine_total_motion': -0.08176686514383666, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.016528982330242022, 'cosine_residue_motion': 0.016528982330242022, 'cosine_ionic_motion': -0.18514078507090295, 'motion_component_glu': None, 'motion_component_asn': 0.5184706589477983, 'motion_component_residue': 0.5184706589477983, 'motion_component_ionic': -2.7001889896586}, 6741: {'frame': 6741, 'ionic_force': [4.5849082469940186, -8.226674973964691, -3.655347716063261], 'ionic_force_magnitude': 10.102530954465797, 'motion_vector': [-0.7228012084960938, -1.44598388671875, -0.26507568359375], 'ionic_force_x': 4.5849082469940186, 'ionic_force_y': -8.226674973964691, 'ionic_force_z': -3.655347716063261, 'radial_force': 9.418044635730428, 'axial_force': -3.655347716063261, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-133.1776237487793, -170.251784324646, -91.74122905731201], 'asn_force_magnitude': 234.8156780158501, 'residue_force': [-133.1776237487793, -170.251784324646, -91.74122905731201], 'residue_force_magnitude': 234.8156780158501, 'total_force': [-128.59271550178528, -178.4784592986107, -95.39657677337527], 'total_force_magnitude': 239.7731297994156, 'motion_component_total': 229.71548373213346, 'cosine_total_motion': 0.958053489664601, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.953451714378301, 'cosine_residue_motion': 0.953451714378301, 'cosine_ionic_motion': 0.5770903342237114, 'motion_component_glu': None, 'motion_component_asn': 223.8854107671154, 'motion_component_residue': 223.8854107671154, 'motion_component_ionic': 5.830072965018056}, 6742: {'frame': 6742, 'ionic_force': [3.3822226524353027, -9.729140877723694, -3.9997954964637756], 'ionic_force_magnitude': 11.04961430561142, 'motion_vector': [0.2605171203613281, 2.8099212646484375, 0.07628631591796875], 'ionic_force_x': 3.3822226524353027, 'ionic_force_y': -9.729140877723694, 'ionic_force_z': -3.9997954964637756, 'radial_force': 10.300272437622253, 'axial_force': -3.9997954964637756, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-233.61487197875977, 291.7616882324219, -474.73042488098145], 'asn_force_magnitude': 604.2100358629956, 'residue_force': [-233.61487197875977, 291.7616882324219, -474.73042488098145], 'residue_force_magnitude': 604.2100358629956, 'total_force': [-230.23264932632446, 282.0325473546982, -478.7302203774452], 'total_force_magnitude': 601.4416467836556, 'motion_component_total': 246.5421069784691, 'cosine_total_motion': 0.4099185819553874, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.42373034301333484, 'cosine_residue_motion': 0.42373034301333484, 'cosine_ionic_motion': -0.8579501969623554, 'motion_component_glu': None, 'motion_component_asn': 256.02212574832646, 'motion_component_residue': 256.02212574832646, 'motion_component_ionic': -9.480018769857379}, 6743: {'frame': 6743, 'ionic_force': [5.934663951396942, -9.266806989908218, -5.335296720266342], 'ionic_force_magnitude': 12.229445576047468, 'motion_vector': [-0.673370361328125, -1.9990310668945312, 0.34476470947265625], 'ionic_force_x': 5.934663951396942, 'ionic_force_y': -9.266806989908218, 'ionic_force_z': -5.335296720266342, 'radial_force': 11.0042695352405, 'axial_force': -5.335296720266342, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-6.261672288179398, -2.689249038696289, 10.86844289302826], 'asn_force_magnitude': 12.82823647878769, 'residue_force': [-6.261672288179398, -2.689249038696289, 10.86844289302826], 'residue_force_magnitude': 12.82823647878769, 'total_force': [-0.32700833678245544, -11.956056028604507, 5.533146172761917], 'total_force_magnitude': 13.178388246694103, 'motion_component_total': 12.17766437725035, 'cosine_total_motion': 0.9240632579105573, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.48650314911501713, 'cosine_residue_motion': 0.48650314911501713, 'cosine_ionic_motion': 0.48544203380368817, 'motion_component_glu': None, 'motion_component_asn': 6.2409774445223505, 'motion_component_residue': 6.2409774445223505, 'motion_component_ionic': 5.936686932728}, 6744: {'frame': 6744, 'ionic_force': [4.246630027890205, -8.969302654266357, -4.882513225078583], 'ionic_force_magnitude': 11.059891142804053, 'motion_vector': [-3.0384254455566406, 2.452880859375, -0.903594970703125], 'ionic_force_x': 4.246630027890205, 'ionic_force_y': -8.969302654266357, 'ionic_force_z': -4.882513225078583, 'radial_force': 9.923822685719868, 'axial_force': -4.882513225078583, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude'</t>
+          <t>{6716: {'frame': 6716, 'ionic_force': [3.5372003354132175, 2.635218560695648, -13.300951480865479], 'ionic_force_magnitude': 14.013260625986366, 'motion_vector': [2.1366920471191406, 6.534908294677734, 0.9935302734375], 'ionic_force_x': 3.5372003354132175, 'ionic_force_y': 2.635218560695648, 'ionic_force_z': -13.300951480865479, 'radial_force': 4.4109140861597185, 'axial_force': -13.300951480865479, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [10.430237293243408, -2.519187092781067, 2.3031381368637085], 'asn_force_magnitude': 10.974543219618589, 'residue_force': [10.430237293243408, -2.519187092781067, 2.3031381368637085], 'residue_force_magnitude': 10.974543219618589, 'total_force': [13.967437628656626, 0.1160314679145813, -10.99781334400177], 'total_force_magnitude': 17.777926638431794, 'motion_component_total': 2.83235411582245, 'cosine_total_motion': 0.15931858497489526, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.10640135998621542, 'cosine_residue_motion': 0.10640135998621542, 'cosine_ionic_motion': 0.11879089645564639, 'motion_component_glu': None, 'motion_component_asn': 1.167706323794917, 'motion_component_residue': 1.167706323794917, 'motion_component_ionic': 1.6646477920275329, 'ionic_contributions': [{'ion_id': 1327, 'distance': 10.33717155456543, 'force': [1.9013433456420898, -1.8896634578704834, -1.5707390308380127], 'magnitude': 3.106952667236328}, {'ion_id': 1330, 'distance': 10.157370567321777, 'force': [1.3640469312667847, -2.8642194271087646, -0.5391140580177307], 'magnitude': 3.217921733856201}, {'ion_id': 1341, 'distance': 5.020081996917725, 'force': [3.074054718017578, 10.045456886291504, -7.949360370635986], 'magnitude': 13.173964500427246}, {'ion_id': 1359, 'distance': 9.410994529724121, 'force': [-2.778268337249756, -2.3256843090057373, -0.9613978266716003], 'magnitude': 3.748582124710083}, {'ion_id': 1400, 'distance': 12.003229141235352, 'force': [-0.023976322263479233, -0.33067113161087036, -2.2803401947021484], 'magnitude': 2.3043153285980225}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.69844388961792, 'force': [-8.11705493927002, 5.659494876861572, -4.131341457366943], 'magnitude': 10.723079681396484}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.351180076599121, 'force': [5.809851169586182, -7.1534318923950195, 4.821128845214844], 'magnitude': 10.400444030761719}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.925340175628662, 'force': [6.605451583862305, -4.094982624053955, 3.890268087387085], 'magnitude': 8.691091537475586}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.583805084228516, 'force': [6.937869071960449, 2.409684896469116, -1.9237312078475952], 'magnitude': 7.592190265655518}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.175177097320557, 'force': [-9.122063636779785, -4.794681549072266, 4.858684062957764], 'magnitude': 11.39332389831543}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.925405025482178, 'force': [2.9580588340759277, 1.5856989622116089, -2.116126298904419], 'magnitude': 3.9676876068115234}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.368992805480957, 'force': [5.35812520980835, 3.869030237197876, -3.0957438945770264], 'magnitude': 7.2981181144714355}]}, 6717: {'frame': 6717, 'ionic_force': [0.5450510084629059, 4.748510509729385, -11.099060416221619], 'ionic_force_magnitude': 12.084476603716624, 'motion_vector': [-2.882415771484375, -8.947956085205078, 1.36480712890625], 'ionic_force_x': 0.5450510084629059, 'ionic_force_y': 4.748510509729385, 'ionic_force_z': -11.099060416221619, 'radial_force': 4.779689599005029, 'axial_force': -11.099060416221619, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-3.1488189697265625, -8.874019980430603, -0.7465218305587769], 'asn_force_magnitude': 9.445664950689933, 'residue_force': [-3.1488189697265625, -8.874019980430603, -0.7465218305587769], 'residue_force_magnitude': 9.445664950689933, 'total_force': [-2.6037679612636566, -4.125509470701218, -11.845582246780396], 'total_force_magnitude': 12.810825685887208, 'motion_component_total': 2.9742241709054857, 'cosine_total_motion': 0.23216490832296477, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.9747498067733612, 'cosine_residue_motion': 0.9747498067733612, 'cosine_ionic_motion': -0.5157803783333467, 'motion_component_glu': None, 'motion_component_asn': 9.207160085530923, 'motion_component_residue': 9.207160085530923, 'motion_component_ionic': -6.232935914625437, 'ionic_contributions': [{'ion_id': 1327, 'distance': 8.708318710327148, 'force': [3.7785017490386963, 0.381460577249527, -2.1780126094818115], 'magnitude': 4.377936363220215}, {'ion_id': 1330, 'distance': 6.242790222167969, 'force': [8.046460151672363, -2.481989860534668, -1.290306568145752], 'magnitude': 8.518842697143555}, {'ion_id': 1341, 'distance': 10.314593315124512, 'force': [0.29557427763938904, 3.0619518756866455, -0.5244418382644653], 'magnitude': 3.1205694675445557}, {'ion_id': 1359, 'distance': 4.99979305267334, 'force': [-12.195097923278809, 2.7431704998016357, -4.48800802230835], 'magnitude': 13.281100273132324}, {'ion_id': 1400, 'distance': 10.72553825378418, 'force': [0.6196127533912659, 1.0439174175262451, -2.6182913780212402], 'magnitude': 2.886023759841919}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.667177200317383, 'force': [6.549556732177734, -3.0372657775878906, 1.4838671684265137], 'magnitude': 7.370450496673584}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.145531177520752, 'force': [-5.8040971755981445, 4.356490135192871, -1.6261597871780396], 'magnitude': 7.437132835388184}, {'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 2.7258217334747314, 'force': [-30.02167320251465, -9.978987693786621, 3.757323741912842], 'magnitude': 31.859041213989258}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.816680908203125, 'force': [13.315171241760254, 1.9459177255630493, -1.2808949947357178], 'magnitude': 13.517436027526855}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 2.6079559326171875, 'force': [36.30823516845703, 21.74136734008789, 14.893804550170898], 'magnitude': 44.86424255371094}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.4868245124816895, 'force': [-9.192042350769043, -4.36124324798584, -5.270145416259766], 'magnitude': 11.458120346069336}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 2.257025957107544, 'force': [-14.303969383239746, -19.540298461914062, -12.704317092895508], 'magnitude': 27.346416473388672}]}, 6718: {'frame': 6718, 'ionic_force': [-15.74527932703495, -6.038105010986328, -8.724657155573368], 'ionic_force_magnitude': 18.986631499356328, 'motion_vector': [-0.8591651916503906, -0.15292739868164062, -0.16278839111328125], 'ionic_force_x': -15.74527932703495, 'ionic_force_y': -6.038105010986328, 'ionic_force_z': -8.724657155573368, 'radial_force': 16.863348813626917, 'axial_force': -8.724657155573368, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [21.994686126708984, -2.6051195710897446, 2.344572961330414], 'asn_force_magnitude': 22.272177445483887, 'residue_force': [21.994686126708984, -2.6051195710897446, 2.344572961330414], 'residue_force_magnitude': 22.272177445483887, 'total_force': [6.249406799674034, -8.643224582076073, -6.380084194242954], 'total_force_magnitude': 12.428430747670637, 'motion_component_total': -3.3894402347929886, 'cosine_total_motion': -0.272716669031466, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.9549263311797028, 'cosine_residue_motion': -0.9549263311797028, 'cosine_ionic_motion': 0.9416545773910651, 'motion_component_glu': None, 'motion_component_asn': -21.268288695399253, 'motion_component_residue': -21.268288695399253, 'motion_component_ionic': 17.878848460606267, 'ionic_contributions': [{'ion_id': 1327, 'distance': 9.429652214050293, 'force': [1.6139215230941772, -3.2655608654022217, -0.8199719190597534], 'magnitude': 3.733762741088867}, {'ion_id': 1330, 'distance': 11.5631685256958, 'force': [0.40082046389579773, -2.4494481086730957, 0.07108324021100998], 'magnitude': 2.483043670654297}, {'ion_id': 1340, 'distance': 13.527496337890625, 'force': [-0.1447393149137497, -0.5571725368499756, -1.720524549484253], 'magnitude': 1.8142755031585693}, {'ion_id': 1341, 'distance': 4.54123067855835, 'force': [-15.274748802185059, 4.401199817657471, -2.545541286468506], 'magnitude': 16.098703384399414}, {'ion_id': 1359, 'distance': 11.682413101196289, 'force': [-1.6921180486679077, -1.7458655834197998, -0.0793391764163971], 'magnitude': 2.432612895965576}, {'ion_id': 1400, 'distance': 8.67500114440918, 'force': [-0.6484151482582092, -2.421257734298706, -3.6303634643554688], 'magnitude': 4.4116291999816895}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.337597846984863, 'force': [-12.479039192199707, 0.19354380667209625, 1.5899094343185425], 'magnitude': 12.581402778625488}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.246819257736206, 'force': [18.27349090576172, -3.3349740505218506, -1.9637556076049805], 'magnitude': 18.678834915161133}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.270986080169678, 'force': [10.937370300292969, -0.7892783284187317, 0.6124639511108398], 'magnitude': 10.982902526855469}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.248615264892578, 'force': [-4.855237007141113, 1.112776517868042, -0.8721252083778381], 'magnitude': 5.056896209716797}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.503660202026367, 'force': [11.290244102478027, -1.6605662107467651, 2.4449565410614014], 'magnitude': 11.670685768127441}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.584572792053223, 'force': [-6.198419570922852, 1.028630018234253, -0.6202538013458252], 'magnitude': 6.3137311935424805}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.4092721939086914, 'force': [-26.1644287109375, 1.8108723163604736, -1.1657122373580933], 'magnitude': 26.252912521362305}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.758702278137207, 'force': [9.632721900939941, -0.11789679527282715, -2.103728771209717], 'magnitude': 9.860471725463867}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 2.5150418281555176, 'force': [21.5579833984375, -0.8482268452644348, 4.422818660736084], 'magnitude': 22.023338317871094}]}, 6719: {'frame': 6719, 'ionic_force': [-13.247648186981678, -7.324256241321564, -7.235395602881908], 'ionic_force_magnitude': 16.777838403822457, 'motion_vector': [3.021942138671875, 1.1164970397949219, -1.1178054809570312], 'ionic_force_x': -13.247648186981678, 'ionic_force_y': -7.324256241321564, 'ionic_force_z': -7.235395602881908, 'radial_force': 15.13753321960275, 'axial_force': -7.235395602881908, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [29.421308517456055, -4.946713283658028, 8.758866712450981], 'asn_force_magnitude': 31.09342556355817, 'residue_force': [29.421308517456055, -4.946713283658028, 8.758866712450981], 'residue_force_magnitude': 31.09342556355817, 'total_force': [16.173660330474377, -12.270969524979591, 1.5234711095690727], 'total_force_magnitude': 20.358903354312332, 'motion_component_total': 9.815921531206694, 'cosine_total_motion': 0.4821439229990514, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.6941101257523201, 'cosine_residue_motion': 0.6941101257523201, 'cosine_ionic_motion': -0.7013024987834178, 'motion_component_glu': None, 'motion_component_asn': 21.58226152799177, 'motion_component_residue': 21.58226152799177, 'motion_component_ionic': -11.766339996785078, 'ionic_contributions': [{'ion_id': 1327, 'distance': 9.7034273147583, 'force': [1.420046091079712, -3.122454881668091, -0.8165378570556641], 'magnitude': 3.5260443687438965}, {'ion_id': 1330, 'distance': 11.059231758117676, 'force': [0.10633199661970139, -2.712059497833252, -0.04335900396108627], 'magnitude': 2.714489459991455}, {'ion_id': 1340, 'distance': 13.822405815124512, 'force': [-0.22071534395217896, -0.5099888443946838, -1.6464329957962036], 'magnitude': 1.737683892250061}, {'ion_id': 1341, 'distance': 5.057727336883545, 'force': [-12.584758758544922, 2.7286531925201416, -1.619233250617981], 'magnitude': 12.978583335876465}, {'ion_id': 1359, 'distance': 11.801372528076172, 'force': [-1.4268096685409546, -1.9060715436935425, -0.11701104044914246], 'magnitude': 2.383817672729492}, {'ion_id': 1400, 'distance': 9.690614700317383, 'force': [-0.5417425036430359, -1.8023346662521362, -2.992821455001831], 'magnitude': 3.535374879837036}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.176555156707764, 'force': [-8.808028221130371, -0.14710111916065216, 0.6576032042503357], 'magnitude': 8.83376693725586}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.061956405639648, 'force': [11.856607437133789, -1.2538725137710571, -0.5246146321296692], 'magnitude': 11.934260368347168}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.6706011295318604, 'force': [16.741588592529297, -3.7991788387298584, 3.736842632293701], 'magnitude': 17.569250106811523}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.759651184082031, 'force': [-8.443126678466797, 1.9407836198806763, -0.7045970559120178], 'magnitude': 8.691920280456543}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 2.5681350231170654, 'force': [-45.73453903198242, 6.991687297821045, 0.20548425614833832], 'magnitude': 46.26633834838867}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 2.9801361560821533, 'force': [14.804438591003418, -1.0414575338363647, -5.077622413635254], 'magnitude': 15.68560791015625}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 1.6578047275543213, 'force': [49.00436782836914, -7.637574195861816, 10.465770721435547], 'magnitude': 50.688194274902344}]}, 6720: {'frame': 6720, 'ionic_force': [-13.875824749469757, -1.1168307960033417, -19.71669438481331], 'ionic_force_magnitude': 24.135738251999413, 'motion_vector': [-2.0362319946289062, -3.377918243408203, 1.4120712280273438], 'ionic_force_x': -13.875824749469757, 'ionic_force_y': -1.1168307960033417, 'ionic_force_z': -19.71669438481331, 'radial_force': 13.920697665882228, 'axial_force': -19.71669438481331, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-7.1707658767700195, -20.72485041618347, 13.114341616630554], 'asn_force_magnitude': 25.552402315052838, 'residue_force': [-7.1707658767700195, -20.72485041618347, 13.114341616630554], 'residue_force_magnitude': 25.552402315052838, 'total_force': [-21.046590626239777, -21.841681212186813, -6.6023527681827545], 'total_force_magnitude': 31.04205336698668, 'motion_component_total': 25.6155671172993, 'cosine_total_motion': 0.82518919784287, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.9633717340628261, 'cosine_residue_motion': 0.9633717340628261, 'cosine_ionic_motion': 0.041395252929257796, 'motion_component_glu': None, 'motion_component_asn': 24.616462127723423, 'motion_component_residue': 24.616462127723423, 'motion_component_ionic': 0.9991049895758781, 'ionic_contributions': [{'ion_id': 1327, 'distance': 9.959306716918945, 'force': [1.9507142305374146, -2.5765552520751953, -0.8716263175010681], 'magnitude': 3.3471860885620117}, {'ion_id': 1330, 'distance': 11.256476402282715, 'force': [0.7414261698722839, -2.502897262573242, -0.2262757122516632], 'magnitude': 2.620192527770996}, {'ion_id': 1340, 'distance': 14.40766429901123, 'force': [0.15693143010139465, -0.3897511661052704, -1.5432026386260986], 'magnitude': 1.5993773937225342}, {'ion_id': 1341, 'distance': 3.792005777359009, 'force': [-16.80057144165039, 8.428204536437988, -13.408795356750488], 'magnitude': 23.088733673095703}, {'ion_id': 1359, 'distance': 11.166389465332031, 'force': [-0.39115285873413086, -2.5806212425231934, -0.5263550877571106], 'magnitude': 2.6626408100128174}, {'ion_id': 1400, 'distance': 9.726400375366211, 'force': [0.46682772040367126, -1.4952104091644287, -3.14043927192688], 'magnitude': 3.5094075202941895}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 2.4850728511810303, 'force': [-33.00111389160156, 15.89177417755127, -11.297689437866211], 'magnitude': 38.33092498779297}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.0715231895446777, 'force': [22.452072143554688, -34.185150146484375, 20.805419921875], 'magnitude': 45.88665771484375}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.715735912322998, 'force': [18.35745620727539, -7.9843034744262695, 9.365213394165039], 'magnitude': 22.100961685180664}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.188111782073975, 'force': [-5.4549174308776855, 4.017484664916992, -4.145012378692627], 'magnitude': 7.9421305656433105}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.44715690612793, 'force': [-6.401937007904053, 1.6091984510421753, -2.457880735397339], 'magnitude': 7.043827056884766}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.720620632171631, 'force': [-9.063371658325195, -1.187255859375, 1.840545892715454], 'magnitude': 9.324263572692871}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.768670558929443, 'force': [5.941045761108398, 1.1134017705917358, -0.9962550401687622], 'magnitude': 6.126027584075928}]}, 6721: {'frame': 6721, 'ionic_force': [-14.872823670506477, -15.005800008773804, -8.68900191783905], 'ionic_force_magnitude': 22.84455454075444, 'motion_vector': [-1.2706642150878906, 0.12684249877929688, -0.00298309326171875], 'ionic_force_x': -14.872823670506477, 'ionic_force_y': -15.005800008773804, 'ionic_force_z': -8.68900191783905, 'radial_force': 21.127586654355333, 'axial_force': -8.68900191783905, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [15.174116134643555, -0.2986522912979126, 0.23915520310401917], 'asn_force_magnitude': 15.17893899025617, 'residue_force': [15.174116134643555, -0.2986522912979126, 0.23915520310401917], 'residue_force_magnitude': 15.17893899025617, 'total_force': [0.30129246413707733, -15.304452300071716, -8.449846714735031], 'total_force_magnitude': 17.48476327711172, 'motion_component_total': -1.8002511283057345, 'cosine_total_motion': -0.10296113820782107, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.9967268639087372, 'cosine_residue_motion': -0.9967268639087372, 'cosine_ionic_motion': 0.5834653113999466, 'motion_component_glu': None, 'motion_component_asn': -15.129256257220087, 'motion_component_residue': -15.129256257220087, 'motion_component_ionic': 13.329005128914353, 'ionic_contributions': [{'ion_id': 1327, 'distance': 12.513692855834961, 'force': [0.9067454934120178, -1.875288724899292, -0.39515984058380127], 'magnitude': 2.120152473449707}, {'ion_id': 1340, 'distance': 14.38318157196045, 'force': [-0.07977347075939178, -0.7151584625244141, -1.4344524145126343], 'magnitude': 1.604826807975769}, {'ion_id': 1341, 'distance': 4.348263740539551, 'force': [-14.652536392211914, -8.457913398742676, -4.700499534606934], 'magnitude': 17.55926513671875}, {'ion_id': 1359, 'distance': 12.728078842163086, 'force': [-0.839736819267273, -1.8682215213775635, -0.06597363948822021], 'magnitude': 2.0493321418762207}, {'ion_id': 1400, 'distance': 10.5826416015625, 'force': [-0.20752248167991638, -2.0892179012298584, -2.092916488647461], 'magnitude': 2.964489221572876}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.838408946990967, 'force': [-8.726812362670898, -4.90623140335083, 1.4203170537948608], 'magnitude': 10.11166000366211}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.590388298034668, 'force': [12.975239753723145, 7.8054046630859375, -2.011598825454712], 'magnitude': 15.275068283081055}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.5145978927612305, 'force': [9.320706367492676, 3.7037506103515625, 0.2956015169620514], 'magnitude': 10.033977508544922}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.13029670715332, 'force': [-5.068414688110352, -1.299284815788269, -0.7982254028320312], 'magnitude': 5.292837619781494}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.530855178833008, 'force': [6.2727460861206055, -4.274484157562256, 1.5040031671524048], 'magnitude': 7.738254547119141}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.418235778808594, 'force': [-12.468961715698242, 9.37389850616455, -1.0007495880126953], 'magnitude': 15.631586074829102}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.574459552764893, 'force': [5.527878284454346, -3.5790178775787354, -0.9756960868835449], 'magnitude': 6.657236099243164}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 3.6621646881103516, 'force': [7.341734409332275, -7.122687816619873, 1.8055033683776855], 'magnitude': 10.387184143066406}]}, 6722: {'frame': 6722, 'ionic_force': [-6.684693541377783, -13.338738977909088, -3.4362437948584557], 'ionic_force_magnitude': 15.310612550797314, 'motion_vector': [1.3387413024902344, 0.14303207397460938, 0.6805572509765625], 'ionic_force_x': -6.684693541377783, 'ionic_force_y': -13.338738977909088, 'ionic_force_z': -3.4362437948584557, 'radial_force': 14.920022964557695, 'axial_force': -3.4362437948584557, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [4.270717620849609, -6.068329334259033, 1.5291308164596558], 'asn_force_magnitude': 7.576403563691061, 'residue_force': [4.270717620849609, -6.068329334259033, 1.5291308164596558], 'residue_force_magnitude': 7.576403563691061, 'total_force': [-2.4139759205281734, -19.40706831216812, -1.9071129783988], 'total_force_magnitude': 19.649393378179056, 'motion_component_total': -4.84254892780208, 'cosine_total_motion': -0.24644775716993905, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.5153317496321815, 'cosine_residue_motion': 0.5153317496321815, 'cosine_ionic_motion': -0.5712972099044454, 'motion_component_glu': None, 'motion_component_asn': 3.90436130439641, 'motion_component_residue': 3.90436130439641, 'motion_component_ionic': -8.74691023219849, 'ionic_contributions': [{'ion_id': 1327, 'distance': 11.797014236450195, 'force': [0.81926029920578, -2.1865475177764893, -0.4886828362941742], 'magnitude': 2.3855793476104736}, {'ion_id': 1330, 'distance': 14.756539344787598, 'force': [0.03506458178162575, -1.515844464302063, 0.15978533029556274], 'magnitude': 1.5246459245681763}, {'ion_id': 1340, 'distance': 13.889774322509766, 'force': [-0.26287201046943665, -0.7818873524665833, -1.5102778673171997], 'magnitude': 1.7208685874938965}, {'ion_id': 1341, 'distance': 6.538846492767334, 'force': [-5.845895767211914, -5.08392858505249, 0.5223320126533508], 'magnitude': 7.764898777008057}, {'ion_id': 1359, 'distance': 13.870075225830078, 'force': [-0.7654677033424377, -1.5446780920028687, -0.07922738045454025], 'magnitude': 1.7257601022720337}, {'ion_id': 1400, 'distance': 10.362624168395996, 'force': [-0.6647829413414001, -2.2258529663085938, -2.040173053741455], 'magnitude': 3.0917088985443115}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.920578956604004, 'force': [-6.212218284606934, -2.5330309867858887, 0.7717737555503845], 'magnitude': 6.7530388832092285}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.669466018676758, 'force': [8.355960845947266, 3.3029634952545166, -0.908689022064209], 'magnitude': 9.030911445617676}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.4772539138793945, 'force': [8.473575592041016, -7.723418235778809, 2.827376127243042], 'magnitude': 11.808756828308105}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.431731700897217, 'force': [-5.330728530883789, 3.9286210536956787, -0.8319829106330872], 'magnitude': 6.67404842376709}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.3942880630493164, 'force': [-17.58504867553711, 19.68408966064453, -2.1838436126708984], 'magnitude': 26.485212326049805}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.504770517349243, 'force': [8.179596900939941, -7.547560691833496, -2.1791305541992188], 'magnitude': 11.341079711914062}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 2.796997308731079, 'force': [8.389579772949219, -15.179993629455566, 4.033627033233643], 'magnitude': 17.806947708129883}]}, 6723: {'frame': 6723, 'ionic_force': [-0.5762564726173878, -13.915500342845917, 1.1806349530816078], 'ionic_force_magnitude': 13.977378874682344, 'motion_vector': [-0.162322998046875, 2.1346893310546875, 1.369384765625], 'ionic_force_x': -0.5762564726173878, 'ionic_force_y': -13.915500342845917, 'ionic_force_z': 1.1806349530816078, 'radial_force': 13.92742694520342, 'axial_force': 1.1806349530816078, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [15.259693145751953, -0.13366782665252686, -0.7264796169474721], 'asn_force_magnitude': 15.277561147782434, 'residue_force': [15.259693145751953, -0.13366782665252686, -0.7264796169474721], 'residue_force_magnitude': 15.277561147782434, 'total_force': [14.683436673134565, -14.049168169498444, 0.4541553361341357], 'total_force_magnitude': 20.327043460821855, 'motion_component_total': -12.494206561479418, 'cosine_total_motion': -0.6146593126324854, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.09677030005628524, 'cosine_residue_motion': -0.09677030005628524, 'cosine_ionic_motion': -0.7881157464389487, 'motion_component_glu': None, 'motion_component_asn': -1.4784141763991516, 'motion_component_residue': -1.4784141763991516, 'motion_component_ionic': -11.015792385080267, 'ionic_contributions': [{'ion_id': 1327, 'distance': 12.17466926574707, 'force': [0.9342626333236694, -2.013418436050415, -0.30056488513946533], 'magnitude': 2.239874839782715}, {'ion_id': 1340, 'distance': 13.355932235717773, 'force': [-0.046403419226408005, -0.8943821787834167, -1.6315449476242065], 'magnitude': 1.8611855506896973}, {'ion_id': 1341, 'distance': 6.2200493812561035, 'force': [-0.5979642868041992, -6.457273483276367, 5.619952201843262], 'magnitude': 8.581247329711914}, {'ion_id': 1359, 'distance': 12.868754386901855, 'force': [-0.7437009215354919, -1.8613765239715576, 0.03603336960077286], 'magnitude': 2.004772424697876}, {'ion_id': 1400, 'distance': 9.46842098236084, 'force': [-0.12245047837495804, -2.68904972076416, -2.543240785598755], 'magnitude': 3.703249454498291}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.799175262451172, 'force': [-8.79680347442627, -4.4495954513549805, 2.906493663787842], 'magnitude': 10.277663230895996}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.5584704875946045, 'force': [13.030034065246582, 6.837989807128906, -5.027176380157471], 'magnitude': 15.550317764282227}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.378759384155273, 'force': [9.911370277404785, 3.462311029434204, -1.0100843906402588], 'magnitude': 10.547185897827148}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.945642471313477, 'force': [-5.5791916847229, -1.1395291090011597, -0.11071347445249557], 'magnitude': 5.695451259613037}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.616502285003662, 'force': [6.081092834472656, -3.7213315963745117, 2.3415303230285645], 'magnitude': 7.504049777984619}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.414801597595215, 'force': [-12.73949909210205, 8.438753128051758, -3.4059226512908936], 'magnitude': 15.655915260314941}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.443363189697266, 'force': [6.139840602874756, -3.476691961288452, 0.011327649466693401], 'magnitude': 7.0558600425720215}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 3.71586537361145, 'force': [7.2128496170043945, -6.085573673248291, 3.568065643310547], 'magnitude': 10.089127540588379}]}, 6725: {'frame': 6725, 'ionic_force': [-2.6017091274261475, -10.550699710845947, -2.3864916190505028], 'ionic_force_magnitude': 11.125713326343421, 'motion_vector': [-0.458587646484375, 0.23482513427734375, -0.8922119140625], 'ionic_force_x': -2.6017091274261475, 'ionic_force_y': -10.550699710845947, 'ionic_force_z': -2.3864916190505028, 'radial_force': 10.866745362443039, 'axial_force': -2.3864916190505028, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [14.904263019561768, -3.653952479362488, 1.1480313390493393], 'asn_force_magnitude': 15.38851522510067, 'residue_force': [14.904263019561768, -3.653952479362488, 1.1480313390493393], 'residue_force_magnitude': 15.38851522510067, 'total_force': [12.30255389213562, -14.204652190208435, -1.2384602800011635], 'total_force_magnitude': 18.83238593431101, 'motion_component_total': -7.641029267764303, 'cosine_total_motion': -0.40573877863468144, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.5498252854484987, 'cosine_residue_motion': -0.5498252854484987, 'cosine_ionic_motion': 0.0737000392202924, 'motion_component_glu': None, 'motion_component_asn': -8.460994776269544, 'motion_component_residue': -8.460994776269544, 'motion_component_ionic': 0.81996550850524, 'ionic_contributions': [{'ion_id': 1327, 'distance': 11.196022987365723, 'force': [1.0887424945831299, -2.387108087539673, -0.3622821271419525], 'magnitude': 2.648564338684082}, {'ion_id': 1340, 'distance': 14.0929594039917, 'force': [-0.1545937955379486, -0.8115612268447876, -1.4531803131103516], 'magnitude': 1.671605110168457}, {'ion_id': 1341, 'distance': 8.497982025146484, 'force': [-2.5049638748168945, -3.5627336502075195, 1.4722782373428345], 'magnitude': 4.5973381996154785}, {'ion_id': 1359, 'distance': 13.108739852905273, 'force': [-0.7145503759384155, -1.7946149110794067, 0.0394371822476387], 'magnitude': 1.9320404529571533}, {'ion_id': 1400, 'distance': 10.697546005249023, 'force': [-0.3163435757160187, -1.9946818351745605, -2.082744598388672], 'magnitude': 2.9011471271514893}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.217677593231201, 'force': [-7.770203113555908, -3.551813840866089, 1.616421103477478], 'magnitude': 8.69507122039795}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.9636013507843018, 'force': [11.184063911437988, 5.117713928222656, -2.4133527278900146], 'magnitude': 12.533896446228027}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.898542404174805, 'force': [8.340500831604004, 2.7049918174743652, -0.19015534222126007], 'magnitude': 8.77023983001709}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.520724296569824, 'force': [-4.47048282623291, -0.8636056184768677, -0.4001809358596802], 'magnitude': 4.5706868171691895}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.0887227058410645, 'force': [7.179224967956543, -5.099740505218506, 2.4526615142822266], 'magnitude': 9.14134407043457}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.9338300228118896, 'force': [-15.224953651428223, 12.196601867675781, -2</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
csv with forces added 6799
</commit_message>
<xml_diff>
--- a/results_test/forces/force_results.xlsx
+++ b/results_test/forces/force_results.xlsx
@@ -467,7 +467,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t xml:space="preserve">{7: {'frame': 7, 'ionic_force': [9.144094347953796, 1.0876708216965199, -9.02269172668457], 'ionic_force_magnitude': 12.892108254875644, 'motion_vector': [-0.4276580810546875, 0.11970901489257812, -0.5581741333007812], 'ionic_force_x': 9.144094347953796, 'ionic_force_y': 1.0876708216965199, 'ionic_force_z': -9.02269172668457, 'radial_force': 9.208555221132713, 'axial_force': -9.02269172668457, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-4.051599442958832, -2.439544200897217, -8.383115142583847], 'asn_force_magnitude': 9.625146931249109, 'residue_force': [-4.051599442958832, -2.439544200897217, -8.383115142583847], 'residue_force_magnitude': 9.625146931249109, 'total_force': [5.092494904994965, -1.351873379200697, -17.405806869268417], 'total_force_magnitude': 18.185796071689104, 'motion_component_total': 10.340551456485855, 'cosine_total_motion': 0.5686059282597806, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.8913988101045852, 'cosine_residue_motion': 0.8913988101045852, 'cosine_ionic_motion': 0.1365724596846074, 'motion_component_glu': None, 'motion_component_asn': 8.579844521597256, 'motion_component_residue': 8.579844521597256, 'motion_component_ionic': 1.7607069348885984, 'ionic_contributions': [{'ion_id': 1305, 'distance': 9.522394180297852, 'force': [2.1304941177368164, 0.16049018502235413, -2.973381996154785], 'magnitude': 3.6613881587982178}, {'ion_id': 1306, 'distance': 6.503903865814209, 'force': [6.327358722686768, 0.9067855477333069, -4.554352760314941], 'magnitude': 7.848557472229004}, {'ion_id': 2433, 'distance': 14.206185340881348, 'force': [0.6862415075302124, 0.02039508894085884, -1.4949569702148438], 'magnitude': 1.6450653076171875}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.7765116691589355, 'force': [5.549598693847656, -13.854113578796387, 7.262692451477051], 'magnitude': 16.597625732421875}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.6253390312194824, 'force': [-6.353938102722168, 23.14116096496582, -15.501691818237305], 'magnitude': 28.56900978088379}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.390173435211182, 'force': [-4.238785743713379, 14.97311019897461, -2.9142580032348633], 'magnitude': 15.832063674926758}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.1455769538879395, 'force': [1.5152294635772705, -7.9598588943481445, -0.22593210637569427], 'magnitude': 8.105942726135254}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.372169494628906, 'force': [1.5165494680404663, -4.495540618896484, 0.8886966109275818], 'magnitude': 4.826964855194092}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.7313129901885986, 'force': [4.9250664710998535, 16.107311248779297, 2.3177313804626465], 'magnitude': 17.002164840698242}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.653998851776123, 'force': [-5.827251434326172, -27.338464736938477, 0.38919597864151], 'magnitude': 27.955322265625}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.836911678314209, 'force': [-3.4048056602478027, -12.578286170959473, 0.5511159300804138], 'magnitude': 13.042611122131348}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.918816089630127, 'force': [0.993121325969696, 5.516653060913086, -1.3160080909729004], 'magnitude': 5.757744789123535}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.727032661437988, 'force': [1.273616075515747, 4.0484843254089355, 0.1653425246477127], 'magnitude': 4.247312068939209}]}, 8: {'frame': 8, 'ionic_force': [7.62947016954422, 1.5109903551638126, -9.45906412601471], 'ionic_force_magnitude': 12.246052468506804, 'motion_vector': [-0.19427871704101562, -0.08087539672851562, -0.9428253173828125], 'ionic_force_x': 7.62947016954422, 'ionic_force_y': 1.5109903551638126, 'ionic_force_z': -9.45906412601471, 'radial_force': 7.777654332854037, 'axial_force': -9.45906412601471, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-13.545484900474548, 7.169286251068115, -7.416431412100792], 'asn_force_magnitude': 17.025929678849657, 'residue_force': [-13.545484900474548, 7.169286251068115, -7.416431412100792], 'residue_force_magnitude': 17.025929678849657, 'total_force': [-5.916014730930328, 8.680276606231928, -16.8754955381155], 'total_force_magnitude': 19.877846510983982, 'motion_component_total': 16.93328490760541, 'cosine_total_motion': 0.8518671727467317, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.5498825242618762, 'cosine_residue_motion': 0.5498825242618762, 'cosine_ionic_motion': 0.6182419793941583, 'motion_component_glu': None, 'motion_component_asn': 9.362261189711045, 'motion_component_residue': 9.362261189711045, 'motion_component_ionic': 7.571023717894365, 'ionic_contributions': [{'ion_id': 1305, 'distance': 9.625224113464355, 'force': [1.8010152578353882, 0.23604314029216766, -3.0891149044036865], 'magnitude': 3.583574056625366}, {'ion_id': 1306, 'distance': 6.726587772369385, 'force': [5.301113605499268, 1.2464194297790527, -4.917684078216553], 'magnitude': 7.337505340576172}, {'ion_id': 2433, 'distance': 14.657554626464844, 'force': [0.5273413062095642, 0.02852778509259224, -1.4522651433944702], 'magnitude': 1.545307993888855}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.7580111026763916, 'force': [4.742934226989746, -15.444692611694336, 4.462300777435303], 'magnitude': 16.761445999145508}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.6038155555725098, 'force': [-4.184497356414795, 27.2148494720459, -9.23870849609375], 'magnitude': 29.04327392578125}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.55521821975708, 'force': [-3.5137319564819336, 14.276277542114258, -0.3098200559616089], 'magnitude': 14.705591201782227}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.368983745574951, 'force': [0.7845888137817383, -7.16344690322876, -1.154306411743164], 'magnitude': 7.2981486320495605}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.531222820281982, 'force': [1.302681565284729, -4.359643936157227, 0.1718807965517044], 'magnitude': 4.553352355957031}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.7761874198913574, 'force': [10.628662109375, 12.478887557983398, 2.6238648891448975], 'magnitude': 16.600475311279297}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.6729986667633057, 'force': [-21.140989303588867, -17.285573959350586, -3.7126452922821045], 'magnitude': 27.559322357177734}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.882439613342285, 'force': [-9.513001441955566, -8.159605026245117, -2.6031813621520996], 'magnitude': 12.800503730773926}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.100968837738037, 'force': [4.502735614776611, 2.5431928634643555, 1.3861900568008423], 'magnitude': 5.353875160217285}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.696345806121826, 'force': [2.845132827758789, 3.0690412521362305, 0.9579936861991882], 'magnitude': 4.2931976318359375}]}, 9: {'frame': 9, 'ionic_force': [6.004610300064087, 1.0871146023273468, -7.455634832382202], 'ionic_force_magnitude': 9.634503296385333, 'motion_vector': [0.5861968994140625, -0.18622207641601562, -0.679412841796875], 'ionic_force_x': 6.004610300064087, 'ionic_force_y': 1.0871146023273468, 'ionic_force_z': -7.455634832382202, 'radial_force': 6.102226070396693, 'axial_force': -7.455634832382202, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-8.106544971466064, 6.1816935539245605, 2.6727231964468956], 'asn_force_magnitude': 10.539110771495833, 'residue_force': [-8.106544971466064, 6.1816935539245605, 2.6727231964468956], 'residue_force_magnitude': 10.539110771495833, 'total_force': [-2.1019346714019775, 7.268808156251907, -4.7829116359353065], 'total_force_magnitude': 8.95153311407612, 'motion_component_total': 0.7243178029127049, 'cosine_total_motion': 0.08091550281747029, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.7991825462204285, 'cosine_residue_motion': -0.7991825462204285, 'cosine_ionic_motion': 0.9493993517660273, 'motion_component_glu': None, 'motion_component_asn': -8.422673381263184, 'motion_component_residue': -8.422673381263184, 'motion_component_ionic': 9.146991184175889, 'ionic_contributions': [{'ion_id': 1305, 'distance': 10.245689392089844, 'force': [1.5193254947662354, 0.22708097100257874, -2.7645342350006104], 'magnitude': 3.1626832485198975}, {'ion_id': 1306, 'distance': 7.1210856437683105, 'force': [4.485284805297852, 0.8600336313247681, -4.691100597381592], 'magnitude': 6.5470499992370605}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.6697676181793213, 'force': [3.7100274562835693, -17.103097915649414, -1.6367162466049194], 'magnitude': 17.577232360839844}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.5951249599456787, 'force': [-1.2680376768112183, 28.7652530670166, 5.081347942352295], 'magnitude': 29.238122940063477}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.66580057144165, 'force': [-2.666797399520874, 13.135809898376465, 4.099885940551758], 'magnitude': 14.016788482666016}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.704106330871582, 'force': [0.7792848348617554, -5.451210975646973, -3.050956964492798], 'magnitude': 6.295341491699219}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.552134990692139, 'force': [1.101813793182373, -4.27436637878418, -0.9686117172241211], 'magnitude': 4.519116401672363}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.9187076091766357, 'force': [8.90909194946289, 12.579450607299805, -0.07691972702741623], 'magnitude': 15.414941787719727}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.774747371673584, 'force': [-17.02199935913086, -19.037578582763672, -1.3832162618637085], 'magnitude': 25.575206756591797}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.945440769195557, 'force': [-8.725992202758789, -8.874736785888672, -0.8705098032951355], 'magnitude': 12.476445198059082}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.92160701751709, 'force': [4.453303337097168, 3.4134907722473145, 1.262007474899292], 'magnitude': 5.751216411590576}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.8923659324646, 'force': [2.62276029586792, 3.028679847717285, 0.21641255915164948], 'magnitude': 4.0123066902160645}]}, 10: {'frame': 10, 'ionic_force': [5.42918598651886, 0.30263806879520416, -6.82907509803772], 'ionic_force_magnitude': 8.729485492944915, 'motion_vector': [-0.07196044921875, 0.04669189453125, 0.901214599609375], 'ionic_force_x': 5.42918598651886, 'ionic_force_y': 0.30263806879520416, 'ionic_force_z': -6.82907509803772, 'radial_force': 5.437614392074603, 'axial_force': -6.82907509803772, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-14.167079448699951, 2.6101136207580566, 1.1775083541870117], 'asn_force_magnitude': 14.453558701690856, 'residue_force': [-14.167079448699951, 2.6101136207580566, 1.1775083541870117], 'residue_force_magnitude': 14.453558701690856, 'total_force': [-8.737893462181091, 2.912751689553261, -5.651566743850708], 'total_force_magnitude': 10.806253338767407, 'motion_component_total': -4.781340719998147, 'cosine_total_motion': -0.44246054299366633, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.16832940695395587, 'cosine_residue_motion': 0.16832940695395587, 'cosine_ionic_motion': -0.8264289677161939, 'motion_component_glu': None, 'motion_component_asn': 2.43295896462981, 'motion_component_residue': 2.43295896462981, 'motion_component_ionic': -7.214299684627957, 'ionic_contributions': [{'ion_id': 1305, 'distance': 10.641091346740723, 'force': [1.43716299533844, -0.03858654201030731, -2.5553414821624756], 'magnitude': 2.9320123195648193}, {'ion_id': 1306, 'distance': 7.528183460235596, 'force': [3.99202299118042, 0.3412246108055115, -4.273733615875244], 'magnitude': 5.858112335205078}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.8648178577423096, 'force': [4.2888054847717285, -15.22591781616211, -0.9648796319961548], 'magnitude': 15.847820281982422}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.595811605453491, 'force': [-9.037348747253418, 27.59457015991211, 3.290829658508301], 'magnitude': 29.222654342651367}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.748159885406494, 'force': [-2.317878246307373, 12.891724586486816, 3.408855438232422], 'magnitude': 13.534749031066895}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.702096462249756, 'force': [0.44413894414901733, -5.6640238761901855, -2.724097728729248], 'magnitude': 6.300724983215332}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.728267669677734, 'force': [0.7835658192634583, -4.078244209289551, -0.8820784091949463], 'magnitude': 4.245481491088867}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.8244564533233643, 'force': [9.10882568359375, 13.076884269714355, -2.8194022178649902], 'magnitude': 16.184085845947266}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.648843288421631, 'force': [-15.905418395996094, -23.071077346801758, 1.5314570665359497], 'magnitude': 28.064252853393555}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.680365085601807, 'force': [-9.934514999389648, -8.987592697143555, 3.816385507583618], 'magnitude': 13.929688453674316}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.605868816375732, 'force': [5.464865207672119, 3.0589096546173096, -1.9749726057052612], 'magnitude': 6.566749095916748}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.582308292388916, 'force': [2.937879800796509, 3.014880895614624, -1.5045887231826782], 'magnitude': 4.470395088195801}]}, 11: {'frame': 11, 'ionic_force': [5.892659664154053, 0.8582678958773613, -7.248329401016235], 'ionic_force_magnitude': 9.380743083800892, 'motion_vector': [-0.4045906066894531, -0.12989044189453125, -0.5406570434570312], 'ionic_force_x': 5.892659664154053, 'ionic_force_y': 0.8582678958773613, 'ionic_force_z': -7.248329401016235, 'radial_force': 5.954835152935966, 'axial_force': -7.248329401016235, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-16.013050824403763, 12.390702486038208, 2.0887385606765747], 'asn_force_magnitude': 20.354609639521676, 'residue_force': [-16.013050824403763, 12.390702486038208, 2.0887385606765747], 'residue_force_magnitude': 20.354609639521676, 'total_force': [-10.12039116024971, 13.24897038191557, -5.159590840339661], 'total_force_magnitude': 17.452189291233733, 'motion_component_total': 7.508472316008847, 'cosine_total_motion': 0.43023096934780364, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.26719982619857174, 'cosine_residue_motion': 0.26719982619857174, 'cosine_ionic_motion': 0.2206354165655574, 'motion_component_glu': None, 'motion_component_asn': 5.4387481580199655, 'motion_component_residue': 5.4387481580199655, 'motion_component_ionic': 2.0697241579888814, 'ionic_contributions': [{'ion_id': 1305, 'distance': 10.63266658782959, 'force': [1.4972081184387207, 0.10249637812376022, -2.524249315261841], 'magnitude': 2.936660051345825}, {'ion_id': 1306, 'distance': 7.148584365844727, 'force': [4.395451545715332, 0.7557715177536011, -4.7240800857543945], 'magnitude': 6.496777534484863}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.6431357860565186, 'force': [4.2307562828063965, -17.31977653503418, -0.4677724838256836], 'magnitude': 17.835155487060547}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.451476573944092, 'force': [-6.532306671142578, 31.873048782348633, 3.8709890842437744], 'magnitude': 32.7650260925293}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.627101898193359, 'force': [-1.4228527545928955, 13.917214393615723, 2.722613573074341], 'magnitude': 14.252227783203125}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.574159145355225, 'force': [-0.1490773856639862, -6.19175386428833, -2.443441152572632], 'magnitude': 6.658111095428467}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.604874610900879, 'force': [0.5936090350151062, -4.34055757522583, -0.686814546585083], 'magnitude': 4.434470176696777}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.590561866760254, 'force': [12.074233055114746, 13.726902961730957, -1.7092034816741943], 'magnitude': 18.36127281188965}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.642768383026123, 'force': [-22.88438606262207, -16.45588493347168, 0.6146681904792786], 'magnitude': 28.193422317504883}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.6935505867004395, 'force': [-10.414986610412598, -8.95059585571289, 1.8110318183898926], 'magnitude': 13.851531982421875}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.743936538696289, 'force': [5.4038896560668945, 2.9093825817108154, -0.8065250515937805], 'magnitude': 6.1900739669799805}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.5408501625061035, 'force': [3.0880706310272217, 3.2227225303649902, -0.8168073892593384], 'magnitude': 4.537542819976807}]}, 12: {'frame': 12, 'ionic_force': [5.195822477340698, 0.6290174052119255, -7.423855781555176], 'ionic_force_magnitude': 9.083274122111948, 'motion_vector': [-0.09729385375976562, -0.12824630737304688, 1.350921630859375], 'ionic_force_x': 5.195822477340698, 'ionic_force_y': 0.6290174052119255, 'ionic_force_z': -7.423855781555176, 'radial_force': 5.233759080440977, 'axial_force': -7.423855781555176, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-10.753758013248444, 1.3659706115722656, 5.102963149547577], 'asn_force_magnitude': 11.981211125125236, 'residue_force': [-10.753758013248444, 1.3659706115722656, 5.102963149547577], 'residue_force_magnitude': 11.981211125125236, 'total_force': [-5.557935535907745, 1.9949880167841911, -2.320892632007599], 'total_force_magnitude': 6.344853600968725, 'motion_component_total': -2.095174918870346, 'cosine_total_motion': -0.3302164321885153, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.47636256770378393, 'cosine_residue_motion': 0.47636256770378393, 'cosine_ionic_motion': -0.8590047277822297, 'motion_component_glu': None, 'motion_component_asn': 5.7074004957658, 'motion_component_residue': 5.7074004957658, 'motion_component_ionic': -7.802575414636146, 'ionic_contributions': [{'ion_id': 1305, 'distance': 10.819844245910645, 'force': [1.2942156791687012, 0.09223221987485886, -2.521709442138672], 'magnitude': 2.8359336853027344}, {'ion_id': 1306, 'distance': 7.2661638259887695, 'force': [3.901606798171997, 0.5367851853370667, -4.902146339416504], 'magnitude': 6.288219928741455}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.933993339538574, 'force': [2.192653179168701, -15.106833457946777, -0.9615597128868103], 'magnitude': 15.29538345336914}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.849979877471924, 'force': [-0.40807804465293884, 23.814319610595703, 4.519295692443848], 'magnitude': 24.242780685424805}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.984221458435059, 'force': [-0.9750038385391235, 11.97861385345459, 2.536829948425293], 'magnitude': 12.283050537109375}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.12647819519043, 'force': [-0.13282230496406555, -4.926605224609375, -1.9515657424926758], 'magnitude': 5.30072546005249}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.877471923828125, 'force': [0.5891918540000916, -3.9428844451904297, -0.6073876619338989], 'magnitude': 4.03266716003418}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.6245808601379395, 'force': [9.837677001953125, 14.555749893188477, -4.000843048095703], 'magnitude': 18.018226623535156}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.544515609741211, 'force': [-20.324533462524414, -22.1102352142334, 4.794425010681152], 'magnitude': 30.412755966186523}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.624504566192627, 'force': [-9.649621963500977, -9.741189956665039, 3.946732759475708], 'magnitude': 14.268240928649902}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.607882499694824, 'force': [5.359733581542969, 3.3871264457702637, -1.6874526739120483], 'magnitude': 6.56101131439209}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.464447021484375, 'force': [2.7570459842681885, 3.457909107208252, -1.4855114221572876], 'magnitude': 4.665317058563232}]}, 13: {'frame': 13, 'ionic_force': [8.770304501056671, 1.0512491520494223, -10.93020236492157], 'ionic_force_magnitude': 14.05320922633249, 'motion_vector': [0.20073699951171875, 0.05039215087890625, -1.1215057373046875], 'ionic_force_x': 8.770304501056671, 'ionic_force_y': 1.0512491520494223, 'ionic_force_z': -10.93020236492157, 'radial_force': 8.8330835963971, 'axial_force': -10.93020236492157, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-5.844012854620814, 10.237451314926147, -11.606195941567421], 'asn_force_magnitude': 16.542722868515707, 'residue_force': [-5.844012854620814, 10.237451314926147, -11.606195941567421], 'residue_force_magnitude': 16.542722868515707, 'total_force': [2.926291646435857, 11.28870046697557, -22.53639830648899], 'total_force_magnitude': 25.374932308516893, 'motion_component_total': 23.17606377949722, 'cosine_total_motion': 0.913344851435066, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.6551029818275638, 'cosine_residue_motion': 0.6551029818275638, 'cosine_ionic_motion': 0.8780113141463322, 'motion_component_glu': None, 'motion_component_asn': 10.837187078711668, 'motion_component_residue': 10.837187078711668, 'motion_component_ionic': 12.33887670078555, 'ionic_contributions': [{'ion_id': 1305, 'distance': 9.229276657104492, 'force': [1.7836300134658813, 0.13545437157154083, -3.462944746017456], 'magnitude': 3.8976492881774902}, {'ion_id': 1306, 'distance': 6.154598236083984, 'force': [6.408231735229492, 0.9370232224464417, -5.9056830406188965], 'magnitude': 8.764732360839844}, {'ion_id': 2433, 'distance': 14.119183540344238, 'force': [0.5784427523612976, -0.02122844196856022, -1.5615745782852173], 'magnitude': 1.6654014587402344}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.815457820892334, 'force': [1.919463872909546, -15.353157997131348, 5.000054836273193], 'magnitude': 16.260515213012695}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.671564817428589, 'force': [0.018672706559300423, 26.079233169555664, -9.001191139221191], 'magnitude': 27.58891487121582}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.64756965637207, 'force': [-0.6785356402397156, 14.055305480957031, -1.2487013339996338], 'magnitude': 14.126969337463379}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.566338539123535, 'force': [-0.5581166744232178, -6.632697105407715, -0.5751115083694458], 'magnitude': 6.680936813354492}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.554023265838623, 'force': [0.6111555695533752, -4.456416130065918, 0.4018724262714386], 'magnitude': 4.516044616699219}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.617870330810547, 'force': [8.831650733947754, 15.427783012390137, 3.3252580165863037], 'magnitude': 18.085128784179688}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.904789447784424, 'force': [-14.536104202270508, -15.853724479675293, -9.052940368652344], 'magnitude': 23.336551666259766}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.803957462310791, 'force': [-7.812679767608643, -10.577165603637695, -1.3824737071990967], 'magnitude': 13.22216510772705}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.004220485687256, 'force': [4.091086387634277, 3.689462184906006, 0.7724369764328003], 'magnitude': 5.562892913818359}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.576723575592041, 'force': [2.2693941593170166, 3.8588287830352783, 0.1545998603105545], 'magnitude': 4.479353904724121}]}, 14: {'frame': 14, 'ionic_force': [5.879561901092529, 0.938679963350296, -7.477024078369141], 'ionic_force_magnitude': 9.558046729896544, 'motion_vector': [0.3662147521972656, 0.29686737060546875, -1.0832748413085938], 'ionic_force_x': 5.879561901092529, 'ionic_force_y': 0.938679963350296, 'ionic_force_z': -7.477024078369141, 'radial_force': 5.954021180880541, 'axial_force': -7.477024078369141, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-10.626070022583008, 6.048847913742065, -6.461329698562622], 'asn_force_magnitude': 13.82934223605542, 'residue_force': [-10.626070022583008, 6.048847913742065, -6.461329698562622], 'residue_force_magnitude': 13.82934223605542, 'total_force': [-4.7465081214904785, 6.9875278770923615, -13.938353776931763], 'total_force_magnitude': 16.29823889846464, 'motion_component_total': 13.065070730806191, 'cosine_total_motion': 0.8016246916123542, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.30013733881706, 'cosine_residue_motion': 0.30013733881706, 'cosine_ionic_motion': 0.932655908304252, 'motion_component_glu': None, 'motion_component_asn': 4.150701976320043, 'motion_component_residue': 4.150701976320043, 'motion_component_ionic': 8.914368754486148, 'ionic_contributions': [{'ion_id': 1305, 'distance': 10.131610870361328, 'force': [1.52020263671875, 0.15927240252494812, -2.8503246307373047], 'magnitude': 3.2343058586120605}, {'ion_id': 1306, 'distance': 7.199889659881592, 'force': [4.359359264373779, 0.7794075608253479, -4.626699447631836], 'magnitude': 6.40451717376709}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.813807487487793, 'force': [3.9378724098205566, -15.717386245727539, 1.522908329963684], 'magnitude': 16.27459144592285}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.6664392948150635, 'force': [-4.383327484130859, 26.599225997924805, -6.347048282623291], 'magnitude': 27.695079803466797}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.396380424499512, 'force': [-2.550234794616699, 15.284669876098633, 3.0194106101989746], 'magnitude': 15.787389755249023}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.954076051712036, 'force': [0.6381100416183472, -8.202877044677734, -3.4199185371398926], 'magnitude': 8.91011905670166}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.405246257781982, 'force': [0.8146671056747437, -4.606374263763428, -0.9231047630310059], 'magnitude': 4.768069744110107}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.7858221530914307, 'force': [8.060348510742188, 14.023764610290527, -3.3385636806488037], 'magnitude': 16.516088485717773}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.8225815296173096, 'force': [-16.013404846191406, -18.634111404418945, 2.684539318084717], 'magnitude': 24.715702056884766}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.925962448120117, 'force': [-7.523538112640381, -9.593951225280762, 3.080723524093628], 'magnitude': 12.575308799743652}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.978542804718018, 'force': [4.191066265106201, 3.4991369247436523, -1.3342300653457642], 'magnitude': 5.620424270629883}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.701474189758301, 'force': [2.2023708820343018, 3.3967506885528564, -1.4060461521148682], 'magnitude': 4.285477638244629}]}, 15: {'frame': 15, 'ionic_force': [3.8807400465011597, 0.5396576374769211, -5.940748453140259], 'ionic_force_magnitude': 7.1164503692285646, 'motion_vector': [-0.24757003784179688, 0.37027740478515625, 0.4908905029296875], 'ionic_force_x': 3.8807400465011597, 'ionic_force_y': 0.5396576374769211, 'ionic_force_z': -5.940748453140259, 'radial_force': 3.918082908031043, 'axial_force': -5.940748453140259, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-13.650164723396301, 4.881107330322266, 12.207969665527344], 'asn_force_magnitude': 18.95222227340146, 'residue_force': [-13.650164723396301, 4.881107330322266, 12.207969665527344], 'residue_force_magnitude': 18.95222227340146, 'total_force': [-9.769424676895142, 5.420764967799187, 6.267221212387085], 'total_force_magnitude': 12.810324472028071, 'motion_component_total': 11.31828647660354, 'cosine_total_motion': 0.8835284774649959, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.8899131490653656, 'cosine_residue_motion': 0.8899131490653656, 'cosine_ionic_motion': -0.7795382586371186, 'motion_component_glu': None, 'motion_component_asn': 16.865831805109455, 'motion_component_residue': 16.865831805109455, 'motion_component_ionic': -5.547545328505914, 'ionic_contributions': [{'ion_id': 1305, 'distance': 11.883319854736328, 'force': [1.0295027494430542, 0.13269831240177155, -2.109494686126709], 'magnitude': 2.351053476333618}, {'ion_id': 1306, 'distance': 8.322646141052246, 'force': [2.8512372970581055, 0.40695932507514954, -3.83125376701355], 'magnitude': 4.793086051940918}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.6112968921661377, 'force': [4.75652551651001, -16.688488006591797, -5.322561740875244], 'magnitude': 18.15102767944336}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.553644895553589, 'force': [-5.721695899963379, 26.23341178894043, 13.814850807189941], 'magnitude': 30.19569206237793}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.750667095184326, 'force': [-2.043933391571045, 12.165769577026367, 5.533477306365967], 'magnitude': 13.520464897155762}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.153984069824219, 'force': [0.32161688804626465, -4.343551158905029, -2.9210941791534424], 'magnitude': 5.244298458099365}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.510556221008301, 'force': [0.8220828771591187, -4.3142476081848145, -1.3256118297576904], 'magnitude': 4.5875701904296875}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.7227942943573, 'force': [10.333606719970703, 12.264867782592773, -5.875219821929932], 'magnitude': 17.08006477355957}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.655656099319458, 'force': [-20.195674896240234, -17.893260955810547, 7.177550315856934], 'magnitude': 27.920446395874023}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.8049235343933105, 'force': [-9.658027648925781, -7.476167678833008, 5.051183223724365], 'magnitude': 13.216846466064453}, {'resid': </t>
+          <t>{7: {'frame': 7, 'motion_vector': [-0.4276580810546875, 0.11970901489257812, -0.5581741333007812], 'ionic_force': [9.144094347953796, 1.0876708216965199, -9.02269172668457], 'ionic_force_magnitude': 12.892108254875644, 'radial_force': 9.208555221132713, 'axial_force': -9.02269172668457, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-4.051599442958832, -2.439544200897217, -8.383115142583847], 'asn_force_magnitude': 9.625146931249109, 'residue_force': [-4.051599442958832, -2.439544200897217, -8.383115142583847], 'residue_force_magnitude': 9.625146931249109, 'total_force': [5.092494904994965, -1.351873379200697, -17.405806869268417], 'total_force_magnitude': 18.185796071689104, 'cosine_total_motion': 0.5686059282597806, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.8913988101045852, 'cosine_residue_motion': 0.8913988101045852, 'cosine_ionic_motion': 0.1365724596846074, 'motion_component_total': 10.340551456485855, 'motion_component_glu': None, 'motion_component_asn': 8.579844521597256, 'motion_component_residue': 8.579844521597256, 'motion_component_ionic': 1.7607069348885984, 'motion_component_percent_total': 56.86059282597806, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 89.13988101045852, 'motion_component_percent_residue': 89.13988101045852, 'motion_component_percent_ionic': 13.65724596846074, 'ionic_contributions': [{'ion_id': 1305, 'distance': 9.522394180297852, 'force': [2.1304941177368164, 0.16049018502235413, -2.973381996154785], 'magnitude': 3.6613881587982178, 'cosine_ionic_motion': 0.2939756512641907, 'motion_component_ionic': 1.0763589143753052, 'motion_component_percent_ionic': 29.397565126419067}, {'ion_id': 1306, 'distance': 6.503903865814209, 'force': [6.327358722686768, 0.9067855477333069, -4.554352760314941], 'magnitude': 7.848557472229004, 'cosine_ionic_motion': -0.00987331010401249, 'motion_component_ionic': -0.07749123871326447, 'motion_component_percent_ionic': 0.9873310104012489}, {'ion_id': 2433, 'distance': 14.206185340881348, 'force': [0.6862415075302124, 0.02039508894085884, -1.4949569702148438], 'magnitude': 1.6450653076171875, 'cosine_ionic_motion': 0.4631058871746063, 'motion_component_ionic': 0.7618394494056702, 'motion_component_percent_ionic': 46.31058871746063}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.7765116691589355, 'force': [5.549598693847656, -13.854113578796387, 7.262692451477051], 'magnitude': 16.597625732421875, 'cosine_with_motion': -0.68297278881073, 'motion_component': -11.335726737976074, 'motion_component_percent': 68.297278881073}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.6253390312194824, 'force': [-6.353938102722168, 23.14116096496582, -15.501691818237305], 'magnitude': 28.56900978088379, 'cosine_with_motion': 0.6938956379890442, 'motion_component': 19.823911666870117, 'motion_component_percent': 69.38956379890442}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.390173435211182, 'force': [-4.238785743713379, 14.97311019897461, -2.9142580032348633], 'magnitude': 15.832063674926758, 'cosine_with_motion': 0.4632880389690399, 'motion_component': 7.334805965423584, 'motion_component_percent': 46.32880389690399}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.1455769538879395, 'force': [1.5152294635772705, -7.9598588943481445, -0.22593210637569427], 'magnitude': 8.105942726135254, 'cosine_with_motion': -0.2550656795501709, 'motion_component': -2.0675477981567383, 'motion_component_percent': 25.50656795501709}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.372169494628906, 'force': [1.5165494680404663, -4.495540618896484, 0.8886966109275818], 'magnitude': 4.826964855194092, 'cosine_with_motion': -0.48874831199645996, 'motion_component': -2.359170913696289, 'motion_component_percent': 48.874831199645996}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.7313129901885986, 'force': [4.9250664710998535, 16.107311248779297, 2.3177313804626465], 'magnitude': 17.002164840698242, 'cosine_with_motion': -0.12135713547468185, 'motion_component': -2.0633339881896973, 'motion_component_percent': 12.135713547468185}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.653998851776123, 'force': [-5.827251434326172, -27.338464736938477, 0.38919597864151], 'magnitude': 27.955322265625, 'cosine_with_motion': -0.05004105344414711, 'motion_component': -1.3989137411117554, 'motion_component_percent': 5.004105344414711}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.836911678314209, 'force': [-3.4048056602478027, -12.578286170959473, 0.5511159300804138], 'magnitude': 13.042611122131348, 'cosine_with_motion': -0.03840212523937225, 'motion_component': -0.5008639693260193, 'motion_component_percent': 3.8402125239372253}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.918816089630127, 'force': [0.993121325969696, 5.516653060913086, -1.3160080909729004], 'magnitude': 5.757744789123535, 'cosine_with_motion': 0.2362441122531891, 'motion_component': 1.3602333068847656, 'motion_component_percent': 23.62441122531891}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.727032661437988, 'force': [1.273616075515747, 4.0484843254089355, 0.1653425246477127], 'magnitude': 4.247312068939209, 'cosine_with_motion': -0.05027863383293152, 'motion_component': -0.21354904770851135, 'motion_component_percent': 5.027863383293152}]}, 8: {'frame': 8, 'motion_vector': [-0.19427871704101562, -0.08087539672851562, -0.9428253173828125], 'ionic_force': [7.62947016954422, 1.5109903551638126, -9.45906412601471], 'ionic_force_magnitude': 12.246052468506804, 'radial_force': 7.777654332854037, 'axial_force': -9.45906412601471, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-13.545484900474548, 7.169286251068115, -7.416431412100792], 'asn_force_magnitude': 17.025929678849657, 'residue_force': [-13.545484900474548, 7.169286251068115, -7.416431412100792], 'residue_force_magnitude': 17.025929678849657, 'total_force': [-5.916014730930328, 8.680276606231928, -16.8754955381155], 'total_force_magnitude': 19.877846510983982, 'cosine_total_motion': 0.8518671727467317, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.5498825242618762, 'cosine_residue_motion': 0.5498825242618762, 'cosine_ionic_motion': 0.6182419793941583, 'motion_component_total': 16.93328490760541, 'motion_component_glu': None, 'motion_component_asn': 9.362261189711045, 'motion_component_residue': 9.362261189711045, 'motion_component_ionic': 7.571023717894365, 'motion_component_percent_total': 85.18671727467317, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 54.98825242618762, 'motion_component_percent_residue': 54.98825242618762, 'motion_component_percent_ionic': 61.824197939415825, 'ionic_contributions': [{'ion_id': 1305, 'distance': 9.625224113464355, 'force': [1.8010152578353882, 0.23604314029216766, -3.0891149044036865], 'magnitude': 3.583574056625366, 'cosine_ionic_motion': 0.7347304821014404, 'motion_component_ionic': 2.6329610347747803, 'motion_component_percent_ionic': 73.47304821014404}, {'ion_id': 1306, 'distance': 6.726587772369385, 'force': [5.301113605499268, 1.2464194297790527, -4.917684078216553], 'magnitude': 7.337505340576172, 'cosine_ionic_motion': 0.49459826946258545, 'motion_component_ionic': 3.629117488861084, 'motion_component_percent_ionic': 49.459826946258545}, {'ion_id': 2433, 'distance': 14.657554626464844, 'force': [0.5273413062095642, 0.02852778509259224, -1.4522651433944702], 'magnitude': 1.545307993888855, 'cosine_ionic_motion': 0.847044825553894, 'motion_component_ionic': 1.3089451789855957, 'motion_component_percent_ionic': 84.7044825553894}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.7580111026763916, 'force': [4.742934226989746, -15.444692611694336, 4.462300777435303], 'magnitude': 16.761445999145508, 'cosine_with_motion': -0.23959551751613617, 'motion_component': -4.01596736907959, 'motion_component_percent': 23.959551751613617}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.6038155555725098, 'force': [-4.184497356414795, 27.2148494720459, -9.23870849609375], 'magnitude': 29.04327392578125, 'cosine_with_motion': 0.2609885632991791, 'motion_component': 7.579962730407715, 'motion_component_percent': 26.098856329917908}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.55521821975708, 'force': [-3.5137319564819336, 14.276277542114258, -0.3098200559616089], 'magnitude': 14.705591201782227, 'cosine_with_motion': -0.01266016997396946, 'motion_component': -0.18617528676986694, 'motion_component_percent': 1.266016997396946}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.368983745574951, 'force': [0.7845888137817383, -7.16344690322876, -1.154306411743164], 'magnitude': 7.2981486320495605, 'cosine_with_motion': 0.21491986513137817, 'motion_component': 1.5685170888900757, 'motion_component_percent': 21.491986513137817}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.531222820281982, 'force': [1.302681565284729, -4.359643936157227, 0.1718807965517044], 'magnitude': 4.553352355957031, 'cosine_with_motion': -0.014220020733773708, 'motion_component': -0.06474876403808594, 'motion_component_percent': 1.4220020733773708}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.7761874198913574, 'force': [10.628662109375, 12.478887557983398, 2.6238648891448975], 'magnitude': 16.600475311279297, 'cosine_with_motion': -0.3459615409374237, 'motion_component': -5.743125915527344, 'motion_component_percent': 34.59615409374237}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.6729986667633057, 'force': [-21.140989303588867, -17.285573959350586, -3.7126452922821045], 'magnitude': 27.559322357177734, 'cosine_with_motion': 0.3382638692855835, 'motion_component': 9.322322845458984, 'motion_component_percent': 33.82638692855835}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.882439613342285, 'force': [-9.513001441955566, -8.159605026245117, -2.6031813621520996], 'magnitude': 12.800503730773926, 'cosine_with_motion': 0.4013090133666992, 'motion_component': 5.13695764541626, 'motion_component_percent': 40.13090133666992}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.100968837738037, 'force': [4.502735614776611, 2.5431928634643555, 1.3861900568008423], 'magnitude': 5.353875160217285, 'cosine_with_motion': -0.4616033732891083, 'motion_component': -2.4713668823242188, 'motion_component_percent': 46.16033732891083}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.696345806121826, 'force': [2.845132827758789, 3.0690412521362305, 0.9579936861991882], 'magnitude': 4.2931976318359375, 'cosine_with_motion': -0.4109092950820923, 'motion_component': -1.7641148567199707, 'motion_component_percent': 41.09092950820923}]}, 9: {'frame': 9, 'motion_vector': [0.5861968994140625, -0.18622207641601562, -0.679412841796875], 'ionic_force': [6.004610300064087, 1.0871146023273468, -7.455634832382202], 'ionic_force_magnitude': 9.634503296385333, 'radial_force': 6.102226070396693, 'axial_force': -7.455634832382202, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-8.106544971466064, 6.1816935539245605, 2.6727231964468956], 'asn_force_magnitude': 10.539110771495833, 'residue_force': [-8.106544971466064, 6.1816935539245605, 2.6727231964468956], 'residue_force_magnitude': 10.539110771495833, 'total_force': [-2.1019346714019775, 7.268808156251907, -4.7829116359353065], 'total_force_magnitude': 8.95153311407612, 'cosine_total_motion': 0.08091550281747029, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.7991825462204285, 'cosine_residue_motion': -0.7991825462204285, 'cosine_ionic_motion': 0.9493993517660273, 'motion_component_total': 0.7243178029127049, 'motion_component_glu': None, 'motion_component_asn': -8.422673381263184, 'motion_component_residue': -8.422673381263184, 'motion_component_ionic': 9.146991184175889, 'motion_component_percent_total': 8.091550281747029, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 79.91825462204285, 'motion_component_percent_residue': 79.91825462204285, 'motion_component_percent_ionic': 94.93993517660273, 'ionic_contributions': [{'ion_id': 1305, 'distance': 10.245689392089844, 'force': [1.5193254947662354, 0.22708097100257874, -2.7645342350006104], 'magnitude': 3.1626832485198975, 'cosine_ionic_motion': 0.9406964182853699, 'motion_component_ionic': 2.9751248359680176, 'motion_component_percent_ionic': 94.06964182853699}, {'ion_id': 1306, 'distance': 7.1210856437683105, 'force': [4.485284805297852, 0.8600336313247681, -4.691100597381592], 'magnitude': 6.5470499992370605, 'cosine_ionic_motion': 0.9426942467689514, 'motion_component_ionic': 6.171866416931152, 'motion_component_percent_ionic': 94.26942467689514}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.6697676181793213, 'force': [3.7100274562835693, -17.103097915649414, -1.6367162466049194], 'magnitude': 17.577232360839844, 'cosine_with_motion': 0.4017519950866699, 'motion_component': 7.061688423156738, 'motion_component_percent': 40.17519950866699}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.5951249599456787, 'force': [-1.2680376768112183, 28.7652530670166, 5.081347942352295], 'magnitude': 29.238122940063477, 'cosine_with_motion': -0.3564891517162323, 'motion_component': -10.423073768615723, 'motion_component_percent': 35.64891517162323}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.66580057144165, 'force': [-2.666797399520874, 13.135809898376465, 4.099885940551758], 'magnitude': 14.016788482666016, 'cosine_with_motion': -0.5289599299430847, 'motion_component': -7.4143195152282715, 'motion_component_percent': 52.89599299430847}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.704106330871582, 'force': [0.7792848348617554, -5.451210975646973, -3.050956964492798], 'magnitude': 6.295341491699219, 'cosine_with_motion': 0.6144095063209534, 'motion_component': 3.867917776107788, 'motion_component_percent': 61.44095063209534}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.552134990692139, 'force': [1.101813793182373, -4.27436637878418, -0.9686117172241211], 'magnitude': 4.519116401672363, 'cosine_with_motion': 0.5070367455482483, 'motion_component': 2.29135799407959, 'motion_component_percent': 50.70367455482483}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.9187076091766357, 'force': [8.90909194946289, 12.579450607299805, -0.07691972702741623], 'magnitude': 15.414941787719727, 'cosine_with_motion': 0.20755426585674286, 'motion_component': 3.199436902999878, 'motion_component_percent': 20.755426585674286}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.774747371673584, 'force': [-17.02199935913086, -19.037578582763672, -1.3832162618637085], 'magnitude': 25.575206756591797, 'cosine_with_motion': -0.23436598479747772, 'motion_component': -5.993958473205566, 'motion_component_percent': 23.436598479747772}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.945440769195557, 'force': [-8.725992202758789, -8.874736785888672, -0.8705098032951355], 'magnitude': 12.476445198059082, 'cosine_with_motion': -0.2510920763015747, 'motion_component': -3.1327366828918457, 'motion_component_percent': 25.10920763015747}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.92160701751709, 'force': [4.453303337097168, 3.4134907722473145, 1.262007474899292], 'magnitude': 5.751216411590576, 'cosine_with_motion': 0.21200276911258698, 'motion_component': 1.2192738056182861, 'motion_component_percent': 21.200276911258698}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.8923659324646, 'force': [2.62276029586792, 3.028679847717285, 0.21641255915164948], 'magnitude': 4.0123066902160645, 'cosine_with_motion': 0.22474370896816254, 'motion_component': 0.9017406702041626, 'motion_component_percent': 22.474370896816254}]}, 10: {'frame': 10, 'motion_vector': [-0.07196044921875, 0.04669189453125, 0.901214599609375], 'ionic_force': [5.42918598651886, 0.30263806879520416, -6.82907509803772], 'ionic_force_magnitude': 8.729485492944915, 'radial_force': 5.437614392074603, 'axial_force': -6.82907509803772, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-14.167079448699951, 2.6101136207580566, 1.1775083541870117], 'asn_force_magnitude': 14.453558701690856, 'residue_force': [-14.167079448699951, 2.6101136207580566, 1.1775083541870117], 'residue_force_magnitude': 14.453558701690856, 'total_force': [-8.737893462181091, 2.912751689553261, -5.651566743850708], 'total_force_magnitude': 10.806253338767407, 'cosine_total_motion': -0.44246054299366633, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.16832940695395587, 'cosine_residue_motion': 0.16832940695395587, 'cosine_ionic_motion': -0.8264289677161939, 'motion_component_total': -4.781340719998147, 'motion_component_glu': None, 'motion_component_asn': 2.43295896462981, 'motion_component_residue': 2.43295896462981, 'motion_component_ionic': -7.214299684627957, 'motion_component_percent_total': 44.246054299366634, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 16.83294069539559, 'motion_component_percent_residue': 16.83294069539559, 'motion_component_percent_ionic': 82.64289677161939, 'ionic_contributions': [{'ion_id': 1305, 'distance': 10.641091346740723, 'force': [1.43716299533844, -0.03858654201030731, -2.5553414821624756], 'magnitude': 2.9320123195648193, 'cosine_ionic_motion': -0.9072515964508057, 'motion_component_ionic': -2.6600728034973145, 'motion_component_percent_ionic': 90.72515964508057}, {'ion_id': 1306, 'distance': 7.528183460235596, 'force': [3.99202299118042, 0.3412246108055115, -4.273733615875244], 'magnitude': 5.858112335205078, 'cosine_ionic_motion': -0.7774222493171692, 'motion_component_ionic': -4.554226875305176, 'motion_component_percent_ionic': 77.74222493171692}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.8648178577423096, 'force': [4.2888054847717285, -15.22591781616211, -0.9648796319961548], 'magnitude': 15.847820281982422, 'cosine_with_motion': -0.1316746324300766, 'motion_component': -2.0867559909820557, 'motion_component_percent': 13.16746324300766}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.595811605453491, 'force': [-9.037348747253418, 27.59457015991211, 3.290829658508301], 'magnitude': 29.222654342651367, 'cosine_with_motion': 0.18539156019687653, 'motion_component': 5.417633533477783, 'motion_component_percent': 18.539156019687653}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.748159885406494, 'force': [-2.317878246307373, 12.891724586486816, 3.408855438232422], 'magnitude': 13.534749031066895, 'cosine_with_motion': 0.31346556544303894, 'motion_component': 4.242677688598633, 'motion_component_percent': 31.346556544303894}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.702096462249756, 'force': [0.44413894414901733, -5.6640238761901855, -2.724097728729248], 'magnitude': 6.300724983215332, 'cosine_with_motion': -0.4823695123195648, 'motion_component': -3.0392775535583496, 'motion_component_percent': 48.23695123195648}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.728267669677734, 'force': [0.7835658192634583, -4.078244209289551, -0.8820784091949463], 'magnitude': 4.245481491088867, 'cosine_with_motion': -0.2710499167442322, 'motion_component': -1.1507374048233032, 'motion_component_percent': 27.104991674423218}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.8244564533233643, 'force': [9.10882568359375, 13.076884269714355, -2.8194022178649902], 'magnitude': 16.184085845947266, 'cosine_with_motion': -0.17648841440677643, 'motion_component': -2.8563036918640137, 'motion_component_percent': 17.648841440677643}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.648843288421631, 'force': [-15.905418395996094, -23.071077346801758, 1.5314570665359497], 'magnitude': 28.064252853393555, 'cosine_with_motion': 0.05697422847151756, 'motion_component': 1.5989391803741455, 'motion_component_percent': 5.697422847151756}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.680365085601807, 'force': [-9.934514999389648, -8.987592697143555, 3.816385507583618], 'magnitude': 13.929688453674316, 'cosine_with_motion': 0.29615500569343567, 'motion_component': 4.125347137451172, 'motion_component_percent': 29.615500569343567}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.605868816375732, 'force': [5.464865207672119, 3.0589096546173096, -1.9749726057052612], 'magnitude': 6.566749095916748, 'cosine_with_motion': -0.3415257930755615, 'motion_component': -2.2427141666412354, 'motion_component_percent': 34.15257930755615}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.582308292388916, 'force': [2.937879800796509, 3.014880895614624, -1.5045887231826782], 'magnitude': 4.470395088195801, 'cosine_with_motion': -0.352508008480072, 'motion_component': -1.5758501291275024, 'motion_component_percent': 35.2508008480072}]}, 11: {'frame': 11, 'motion_vector': [-0.4045906066894531, -0.12989044189453125, -0.5406570434570312], 'ionic_force': [5.892659664154053, 0.8582678958773613, -7.248329401016235], 'ionic_force_magnitude': 9.380743083800892, 'radial_force': 5.954835152935966, 'axial_force': -7.248329401016235, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-16.013050824403763, 12.390702486038208, 2.0887385606765747], 'asn_force_magnitude': 20.354609639521676, 'residue_force': [-16.013050824403763, 12.390702486038208, 2.0887385606765747], 'residue_force_magnitude': 20.354609639521676, 'total_force': [-10.12039116024971, 13.24897038191557, -5.159590840339661], 'total_force_magnitude': 17.452189291233733, 'cosine_total_motion': 0.43023096934780364, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.26719982619857174, 'cosine_residue_motion': 0.26719982619857174, 'cosine_ionic_motion': 0.2206354165655574, 'motion_component_total': 7.508472316008847, 'motion_component_glu': None, 'motion_component_asn': 5.4387481580199655, 'motion_component_residue': 5.4387481580199655, 'motion_component_ionic': 2.0697241579888814, 'motion_component_percent_total': 43.02309693478036, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 26.719982619857173, 'motion_component_percent_residue': 26.719982619857173, 'motion_component_percent_ionic': 22.063541656555742, 'ionic_contributions': [{'ion_id': 1305, 'distance': 10.63266658782959, 'force': [1.4972081184387207, 0.10249637812376022, -2.524249315261841], 'magnitude': 2.936660051345825, 'cosine_ionic_motion': 0.36925607919692993, 'motion_component_ionic': 1.0843795537948608, 'motion_component_percent_ionic': 36.92560791969299}, {'ion_id': 1306, 'distance': 7.148584365844727, 'force': [4.395451545715332, 0.7557715177536011, -4.7240800857543945], 'magnitude': 6.496777534484863, 'cosine_ionic_motion': 0.15166667103767395, 'motion_component_ionic': 0.9853445887565613, 'motion_component_percent_ionic': 15.166667103767395}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.6431357860565186, 'force': [4.2307562828063965, -17.31977653503418, -0.4677724838256836], 'magnitude': 17.835155487060547, 'cosine_with_motion': 0.06448311358690262, 'motion_component': 1.1500663757324219, 'motion_component_percent': 6.448311358690262}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.451476573944092, 'force': [-6.532306671142578, 31.873048782348633, 3.8709890842437744], 'magnitude': 32.7650260925293, 'cosine_with_motion': -0.15933357179164886, 'motion_component': -5.220568656921387, 'motion_component_percent': 15.933357179164886}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.627101898193359, 'force': [-1.4228527545928955, 13.917214393615723, 2.722613573074341], 'magnitude': 14.252227783203125, 'cosine_with_motion': -0.27590349316596985, 'motion_component': -3.932239532470703, 'motion_component_percent': 27.590349316596985}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.574159145355225, 'force': [-0.1490773856639862, -6.19175386428833, -2.443441152572632], 'magnitude': 6.658111095428467, 'cosine_with_motion': 0.47736668586730957, 'motion_component': 3.1783604621887207, 'motion_component_percent': 47.73666858673096}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.604874610900879, 'force': [0.5936090350151062, -4.34055757522583, -0.686814546585083], 'magnitude': 4.434470176696777, 'cosine_with_motion': 0.22790010273456573, 'motion_component': 1.0106161832809448, 'motion_component_percent': 22.790010273456573}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.590561866760254, 'force': [12.074233055114746, 13.726902961730957, -1.7092034816741943], 'magnitude': 18.36127281188965, 'cosine_with_motion': -0.4549252986907959, 'motion_component': -8.353007316589355, 'motion_component_percent': 45.49252986907959}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.642768383026123, 'force': [-22.88438606262207, -16.45588493347168, 0.6146681904792786], 'magnitude': 28.193422317504883, 'cosine_with_motion': 0.5706751942634583, 'motion_component': 16.08928680419922, 'motion_component_percent': 57.067519426345825}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.6935505867004395, 'force': [-10.414986610412598, -8.95059585571289, 1.8110318183898926], 'magnitude': 13.851531982421875, 'cosine_with_motion': 0.4616476893424988, 'motion_component': 6.394527912139893, 'motion_component_percent': 46.16476893424988}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.743936538696289, 'force': [5.4038896560668945, 2.9093825817108154, -0.8065250515937805], 'magnitude': 6.1900739669799805, 'cosine_with_motion': -0.49997180700302124, 'motion_component': -3.094862461090088, 'motion_component_percent': 49.997180700302124}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.5408501625061035, 'force': [3.0880706310272217, 3.2227225303649902, -0.8168073892593384], 'magnitude': 4.537542819976807, 'cosine_with_motion': -0.39303892850875854, 'motion_component': -1.7834309339523315, 'motion_component_percent': 39.303892850875854}]}, 12: {'frame': 12, 'motion_vector': [-0.09729385375976562, -0.12824630737304688, 1.350921630859375], 'ionic_force': [5.195822477340698, 0.6290174052119255, -7.423855781555176], 'ionic_force_magnitude': 9.083274122111948, 'radial_force': 5.233759080440977, 'axial_force': -7.423855781555176, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-10.753758013248444, 1.3659706115722656, 5.102963149547577], 'asn_force_magnitude': 11.981211125125236, 'residue_force': [-10.753758013248444, 1.3659706115722656, 5.102963149547577], 'residue_force_magnitude': 11.981211125125236, 'total_force': [-5.557935535907745, 1.9949880167841911, -2.320892632007599], 'total_force_magnitude': 6.344853600968725, 'cosine_total_motion': -0.3302164321885153, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.47636256770378393, 'cosine_residue_motion': 0.47636256770378393, 'cosine_ionic_motion': -0.8590047277822297, 'motion_component_total': -2.095174918870346, 'motion_component_glu': None, 'motion_component_asn': 5.7074004957658, 'motion_component_residue': 5.7074004957658, 'motion_component_ionic': -7.802575414636146, 'motion_component_percent_total': 33.02164321885153, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 47.636256770378395, 'motion_component_percent_residue': 47.636256770378395, 'motion_component_percent_ionic': 85.90047277822296, 'ionic_contributions': [{'ion_id': 1305, 'distance': 10.819844245910645, 'force': [1.2942156791687012, 0.09223221987485886, -2.521709442138672], 'magnitude': 2.8359336853027344, 'cosine_ionic_motion': -0.9186549186706543, 'motion_component_ionic': -2.6052443981170654, 'motion_component_percent_ionic': 91.86549186706543}, {'ion_id': 1306, 'distance': 7.2661638259887695, 'force': [3.901606798171997, 0.5367851853370667, -4.902146339416504], 'magnitude': 6.288219928741455, 'cosine_ionic_motion': -0.8265186548233032, 'motion_component_ionic': -5.197330951690674, 'motion_component_percent_ionic': 82.65186548233032}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.933993339538574, 'force': [2.192653179168701, -15.106833457946777, -0.9615597128868103], 'magnitude': 15.29538345336914, 'cosine_with_motion': 0.0204272773116827, 'motion_component': 0.3124430477619171, 'motion_component_percent': 2.04272773116827}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.849979877471924, 'force': [-0.40807804465293884, 23.814319610595703, 4.519295692443848], 'magnitude': 24.242780685424805, 'cosine_with_motion': 0.09371290355920792, 'motion_component': 2.2718613147735596, 'motion_component_percent': 9.371290355920792}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.984221458435059, 'force': [-0.9750038385391235, 11.97861385345459, 2.536829948425293], 'magnitude': 12.283050537109375, 'cosine_with_motion': 0.11882756650447845, 'motion_component': 1.4595650434494019, 'motion_component_percent': 11.882756650447845}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.12647819519043, 'force': [-0.13282230496406555, -4.926605224609375, -1.9515657424926758], 'magnitude': 5.30072546005249, 'cosine_with_motion': -0.27617886662483215, 'motion_component': -1.463948369026184, 'motion_component_percent': 27.617886662483215}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.877471923828125, 'force': [0.5891918540000916, -3.9428844451904297, -0.6073876619338989], 'magnitude': 4.03266716003418, 'cosine_with_motion': -0.06784053891897202, 'motion_component': -0.27357831597328186, 'motion_component_percent': 6.7840538918972015}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.6245808601379395, 'force': [9.837677001953125, 14.555749893188477, -4.000843048095703], 'magnitude': 18.018226623535156, 'cosine_with_motion': -0.3356812000274658, 'motion_component': -6.048379898071289, 'motion_component_percent': 33.56812000274658}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.544515609741211, 'force': [-20.324533462524414, -22.1102352142334, 4.794425010681152], 'magnitude': 30.412755966186523, 'cosine_with_motion': 0.27286168932914734, 'motion_component': 8.298476219177246, 'motion_component_percent': 27.286168932914734}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.624504566192627, 'force': [-9.649621963500977, -9.741189956665039, 3.946732759475708], 'magnitude': 14.268240928649902, 'cosine_with_motion': 0.38738855719566345, 'motion_component': 5.527353286743164, 'motion_component_percent': 38.738855719566345}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.607882499694824, 'force': [5.359733581542969, 3.3871264457702637, -1.6874526739120483], 'magnitude': 6.56101131439209, 'cosine_with_motion': -0.3624725043773651, 'motion_component': -2.3781862258911133, 'motion_component_percent': 36.24725043773651}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.464447021484375, 'force': [2.7570459842681885, 3.457909107208252, -1.4855114221572876], 'magnitude': 4.665317058563232, 'cosine_with_motion': -0.42831093072891235, 'motion_component': -1.9982062578201294, 'motion_component_per</t>
         </is>
       </c>
     </row>
@@ -483,7 +483,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>{760: {'frame': 760, 'ionic_force': [6.2238762974739075, -3.591959446668625, -15.905625224113464], 'ionic_force_magnitude': 17.453587671385044, 'motion_vector': [0.43795013427734375, -0.21899032592773438, -0.324615478515625], 'ionic_force_x': 6.2238762974739075, 'ionic_force_y': -3.591959446668625, 'ionic_force_z': -15.905625224113464, 'radial_force': 7.186014808833161, 'axial_force': -15.905625224113464, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [6.150402218103409, 0.19301128387451172, -9.66019320487976], 'asn_force_magnitude': 11.45355986389207, 'residue_force': [6.150402218103409, 0.19301128387451172, -9.66019320487976], 'residue_force_magnitude': 11.45355986389207, 'total_force': [12.374278515577316, -3.398948162794113, -25.565818428993225], 'total_force_magnitude': 28.60571078191712, 'motion_component_total': 24.618239990362206, 'cosine_total_motion': 0.8606057782673394, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.8600653614153887, 'cosine_residue_motion': 0.8600653614153887, 'cosine_ionic_motion': 0.8460970984631494, 'motion_component_glu': None, 'motion_component_asn': 9.850810103831122, 'motion_component_residue': 9.850810103831122, 'motion_component_ionic': 14.767429886531083, 'ionic_contributions': [{'ion_id': 1305, 'distance': 5.483183860778809, 'force': [3.6287899017333984, -0.07852231711149216, -10.42906379699707], 'magnitude': 11.04262924194336}, {'ion_id': 1307, 'distance': 9.4274320602417, 'force': [1.388010025024414, -3.399308681488037, 0.6872068643569946], 'magnitude': 3.7355220317840576}, {'ion_id': 1313, 'distance': 12.530621528625488, 'force': [0.33516377210617065, -0.027667954564094543, -2.0875115394592285], 'magnitude': 2.1144278049468994}, {'ion_id': 2433, 'distance': 8.923480033874512, 'force': [0.8719125986099243, -0.08646049350500107, -4.07625675201416], 'magnitude': 4.169361591339111}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.825902462005615, 'force': [-3.0543558597564697, -5.7498459815979, 2.5002336502075195], 'magnitude': 6.974308967590332}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.650112152099609, 'force': [4.436252117156982, 7.244457721710205, -3.2804160118103027], 'magnitude': 9.106241226196289}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.588597059249878, 'force': [-5.562565326690674, 14.392956733703613, 9.988791465759277], 'magnitude': 18.381383895874023}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.9979047775268555, 'force': [7.43020486831665, -12.00178337097168, -16.756216049194336], 'magnitude': 21.909393310546875}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.7077767848968506, 'force': [0.47450941801071167, -20.36496925354004, -8.81492805480957], 'magnitude': 22.195947647094727}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.516462564468384, 'force': [2.7217092514038086, 9.680355072021484, 5.079469680786133], 'magnitude': 11.265788078308105}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.403622627258301, 'force': [-0.2953522503376007, 6.991840362548828, 1.6228721141815186], 'magnitude': 7.183785915374756}]}, 761: {'frame': 761, 'ionic_force': [12.738315880298615, -4.829882338643074, -23.65466946363449], 'ionic_force_magnitude': 27.297176452981475, 'motion_vector': [-0.29718780517578125, -0.07862472534179688, 0.7725677490234375], 'ionic_force_x': 12.738315880298615, 'ionic_force_y': -4.829882338643074, 'ionic_force_z': -23.65466946363449, 'radial_force': 13.62323217417233, 'axial_force': -23.65466946363449, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-1.240791916847229, -3.651379108428955, -13.70577585697174], 'asn_force_magnitude': 14.237992337964446, 'residue_force': [-1.240791916847229, -3.651379108428955, -13.70577585697174], 'residue_force_magnitude': 14.237992337964446, 'total_force': [11.497523963451385, -8.48126144707203, -37.36044532060623], 'total_force_magnitude': 39.99909658451972, 'motion_component_total': -38.02071102708291, 'cosine_total_motion': -0.9505392439737632, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.839015311282996, 'cosine_residue_motion': -0.839015311282996, 'cosine_ionic_motion': -0.9552203136655474, 'motion_component_glu': None, 'motion_component_asn': -11.945893573482152, 'motion_component_residue': -11.945893573482152, 'motion_component_ionic': -26.074817453600758, 'ionic_contributions': [{'ion_id': 1305, 'distance': 4.033351898193359, 'force': [9.497282028198242, -1.4192678928375244, -18.007890701293945], 'magnitude': 20.408252716064453}, {'ion_id': 1307, 'distance': 9.503510475158691, 'force': [1.7444636821746826, -3.1808838844299316, 0.5928385853767395], 'magnitude': 3.6759533882141113}, {'ion_id': 1313, 'distance': 12.466975212097168, 'force': [0.44171684980392456, -0.08128352463245392, -2.088320255279541], 'magnitude': 2.1360716819763184}, {'ion_id': 2433, 'distance': 8.801434516906738, 'force': [1.0548533201217651, -0.14844703674316406, -4.151297092437744], 'magnitude': 4.285792827606201}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.774477958679199, 'force': [-3.011371612548828, -5.84398889541626, 2.67887806892395], 'magnitude': 7.099081039428711}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.7205986976623535, 'force': [4.704928398132324, 6.611140727996826, -3.498167037963867], 'magnitude': 8.836328506469727}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.39385724067688, 'force': [1.5932810306549072, 17.216833114624023, 11.108569145202637], 'magnitude': 20.551355361938477}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.634606122970581, 'force': [-4.252919673919678, -17.376630783081055, -22.016599655151367], 'magnitude': 28.368385314941406}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.179434299468994, 'force': [-5.557168960571289, -15.215255737304688, -6.5403971672058105], 'magnitude': 17.468914031982422}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.321422576904297, 'force': [3.848464012145996, 5.593907833099365, 3.089388847351074], 'magnitude': 7.459678649902344}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.925113677978516, 'force': [1.4339948892593384, 5.362614631652832, 1.472551941871643], 'magnitude': 5.7430291175842285}]}, 768: {'frame': 768, 'ionic_force': [11.80370283126831, -3.687008783221245, -18.915793627500534], 'ionic_force_magnitude': 22.599307132180666, 'motion_vector': [-0.5820541381835938, -0.10816574096679688, -0.3086700439453125], 'ionic_force_x': 11.80370283126831, 'ionic_force_y': -3.687008783221245, 'ionic_force_z': -18.915793627500534, 'radial_force': 12.366140638713524, 'axial_force': -18.915793627500534, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [1.7805204391479492, -1.2756080627441406, -14.73203194141388], 'asn_force_magnitude': 14.89396502234379, 'residue_force': [1.7805204391479492, -1.2756080627441406, -14.73203194141388], 'residue_force_magnitude': 14.89396502234379, 'total_force': [13.58422327041626, -4.962616845965385, -33.64782556891441], 'total_force_magnitude': 36.624238604187646, 'motion_component_total': 4.517459250312436, 'cosine_total_motion': 0.12334616151708629, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.3669489184461005, 'cosine_residue_motion': 0.3669489184461005, 'cosine_ionic_motion': -0.04194221975331891, 'motion_component_glu': None, 'motion_component_asn': 5.465324356323105, 'motion_component_residue': 5.465324356323105, 'motion_component_ionic': -0.9478651060106689, 'ionic_contributions': [{'ion_id': 1305, 'distance': 4.501012802124023, 'force': [8.69870662689209, -0.5448192954063416, -13.87774658203125], 'magnitude': 16.387683868408203}, {'ion_id': 1307, 'distance': 10.221074104309082, 'force': [1.4806410074234009, -2.767298698425293, 0.4990297853946686], 'magnitude': 3.1779348850250244}, {'ion_id': 1313, 'distance': 13.009090423583984, 'force': [0.5215495824813843, -0.13493144512176514, -1.8863331079483032], 'magnitude': 1.9617525339126587}, {'ion_id': 2433, 'distance': 9.321123123168945, 'force': [1.1028056144714355, -0.23995934426784515, -3.6507437229156494], 'magnitude': 3.821215867996216}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.114900588989258, 'force': [3.308007001876831, 6.393937110900879, -2.196016311645508], 'magnitude': 7.526474952697754}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.494544506072998, 'force': [2.515502452850342, 17.18895721435547, 8.599810600280762], 'magnitude': 19.384136199951172}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.607819080352783, 'force': [-3.6708574295043945, -21.16065788269043, -19.41893768310547], 'magnitude': 28.95416831970215}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.376420021057129, 'force': [-5.88956880569458, -13.469000816345215, -6.141573429107666], 'magnitude': 15.931727409362793}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.470947742462158, 'force': [3.842482566833496, 4.988195896148682, 2.9868156909942627], 'magnitude': 6.9690632820129395}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.142477512359619, 'force': [1.6749546527862549, 4.782960414886475, 1.4378691911697388], 'magnitude': 5.267794132232666}]}, 774: {'frame': 774, 'ionic_force': [10.475233167409897, -4.618187832646072, -21.514216423034668], 'ionic_force_magnitude': 24.37046731325395, 'motion_vector': [-1.0657234191894531, -0.014034271240234375, 0.7283935546875], 'ionic_force_x': 10.475233167409897, 'ionic_force_y': -4.618187832646072, 'ionic_force_z': -21.514216423034668, 'radial_force': 11.448063974716625, 'axial_force': -21.514216423034668, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-2.79820716381073, -9.780909061431885, -10.804529368877411], 'asn_force_magnitude': 14.840283025688445, 'residue_force': [-2.79820716381073, -9.780909061431885, -10.804529368877411], 'residue_force_magnitude': 14.840283025688445, 'total_force': [7.677026003599167, -14.399096894077957, -32.31874579191208], 'total_force_magnitude': 36.20458602424861, 'motion_component_total': -24.41656901860525, 'cosine_total_motion': -0.6744054193093619, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.2479693068729528, 'cosine_residue_motion': -0.2479693068729528, 'cosine_ionic_motion': -0.8508919445975974, 'motion_component_glu': None, 'motion_component_asn': -3.6799346956784103, 'motion_component_residue': -3.6799346956784103, 'motion_component_ionic': -20.73663432292684, 'ionic_contributions': [{'ion_id': 1305, 'distance': 4.294199466705322, 'force': [7.753024101257324, -1.7171417474746704, -16.158370971679688], 'magnitude': 18.004192352294922}, {'ion_id': 1307, 'distance': 10.263452529907227, 'force': [1.444155216217041, -2.761002540588379, 0.4741096496582031], 'magnitude': 3.151745557785034}, {'ion_id': 1313, 'distance': 12.748905181884766, 'force': [0.4012247622013092, -0.01295121293514967, -2.0028076171875], 'magnitude': 2.04264235496521}, {'ion_id': 2433, 'distance': 9.19312572479248, 'force': [0.8768290877342224, -0.12709233164787292, -3.8271474838256836], 'magnitude': 3.92836332321167}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.502677917480469, 'force': [-2.555861711502075, -6.9205780029296875, 2.5864498615264893], 'magnitude': 7.817707538604736}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.477771759033203, 'force': [3.961638927459717, 8.154483795166016, -3.775686502456665], 'magnitude': 9.82069206237793}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.661566972732544, 'force': [2.3035364151000977, 16.415498733520508, 6.079585552215576], 'magnitude': 17.65605354309082}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.5984044075012207, 'force': [-6.747326850891113, -24.21038055419922, -14.794974327087402], 'magnitude': 29.164365768432617}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.412884712219238, 'force': [-5.652472019195557, -14.314430236816406, -2.9462690353393555], 'magnitude': 15.669519424438477}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.213598728179932, 'force': [4.4113688468933105, 6.305539131164551, 1.5313644409179688], 'magnitude': 7.846341609954834}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.257880210876465, 'force': [1.4809092283248901, 4.7889580726623535, 0.5150006413459778], 'magnitude': 5.039091110229492}]}, 777: {'frame': 777, 'ionic_force': [3.253043606877327, -2.876964196562767, -18.913673758506775], 'ionic_force_magnitude': 19.40583084384117, 'motion_vector': [-0.18167495727539062, -0.27399444580078125, 0.3039093017578125], 'ionic_force_x': 3.253043606877327, 'ionic_force_y': -2.876964196562767, 'ionic_force_z': -18.913673758506775, 'radial_force': 4.34271985011116, 'axial_force': -18.913673758506775, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [6.349842518568039, -4.249195218086243, -11.838613510131836], 'asn_force_magnitude': 14.090029448311935, 'residue_force': [6.349842518568039, -4.249195218086243, -11.838613510131836], 'residue_force_magnitude': 14.090029448311935, 'total_force': [9.602886125445366, -7.12615941464901, -30.75228726863861], 'total_force_magnitude': 32.995465479276604, 'motion_component_total': -20.41073018731494, 'cosine_total_motion': -0.6185919759226997, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.5686615983288297, 'cosine_residue_motion': -0.5686615983288297, 'cosine_ionic_motion': -0.6388941355052798, 'motion_component_glu': None, 'motion_component_asn': -8.012458666577343, 'motion_component_residue': -8.012458666577343, 'motion_component_ionic': -12.398271520737598, 'ionic_contributions': [{'ion_id': 1305, 'distance': 4.9131622314453125, 'force': [1.1015095710754395, 1.6659917831420898, -13.607799530029297], 'magnitude': 13.753582954406738}, {'ion_id': 1307, 'distance': 7.9652605056762695, 'force': [1.8268259763717651, -4.72895622253418, 1.297066569328308], 'magnitude': 5.232848167419434}, {'ion_id': 1313, 'distance': 12.369667053222656, 'force': [0.09195472300052643, 0.049325793981552124, -2.1673009395599365], 'magnitude': 2.169811487197876}, {'ion_id': 2433, 'distance': 8.643499374389648, 'force': [0.23275333642959595, 0.1366744488477707, -4.43563985824585], 'magnitude': 4.443844318389893}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.4169793128967285, 'force': [-8.892522811889648, 15.237275123596191, 9.989500045776367], 'magnitude': 20.27416229248047}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.622715473175049, 'force': [16.82961654663086, -14.755626678466797, -17.846418380737305], 'magnitude': 28.626197814941406}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.651845693588257, 'force': [2.0806901454925537, -20.070762634277344, -10.787858009338379], 'magnitude': 22.881053924560547}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.245034694671631, 'force': [1.875540852546692, 10.595893859863281, 7.69559383392334], 'magnitude': 13.229239463806152}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.528416633605957, 'force': [-0.41165056824684143, 6.314081192016602, 2.472215414047241], 'magnitude': 6.793300151824951}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.576260089874268, 'force': [-5.131831645965576, -1.5700560808181763, -3.3616464138031006], 'magnitude': 6.332569599151611}]}, 778: {'frame': 778, 'ionic_force': [2.2254137322306633, -2.9039981458336115, -20.00335383415222], 'ionic_force_magnitude': 20.33518714260821, 'motion_vector': [0.5508079528808594, 0.34873199462890625, -0.7382888793945312], 'ionic_force_x': 2.2254137322306633, 'ionic_force_y': -2.9039981458336115, 'ionic_force_z': -20.00335383415222, 'radial_force': 3.6586433975731856, 'axial_force': -20.00335383415222, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [4.0535277128219604, -2.6926302909851074, -13.897537469863892], 'asn_force_magnitude': 14.724907216305882, 'residue_force': [4.0535277128219604, -2.6926302909851074, -13.897537469863892], 'residue_force_magnitude': 14.724907216305882, 'total_force': [6.278941445052624, -5.596628436818719, -33.90089130401611], 'total_force_magnitude': 34.928753008616304, 'motion_component_total': 26.941608805627464, 'cosine_total_motion': 0.7713303935866661, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.7966753458909348, 'cosine_residue_motion': 0.7966753458909348, 'cosine_ionic_motion': 0.7479959810153054, 'motion_component_glu': None, 'motion_component_asn': 11.73097054976241, 'motion_component_residue': 11.73097054976241, 'motion_component_ionic': 15.210638255865053, 'ionic_contributions': [{'ion_id': 1305, 'distance': 4.80653715133667, 'force': [0.9331015348434448, 1.4339590072631836, -14.268352508544922], 'magnitude': 14.370553016662598}, {'ion_id': 1307, 'distance': 8.545356750488281, 'force': [1.0206871032714844, -4.311095237731934, 1.0214502811431885], 'magnitude': 4.546504974365234}, {'ion_id': 1313, 'distance': 12.240949630737305, 'force': [0.09539709240198135, -0.03691666200757027, -2.2133216857910156], 'magnitude': 2.215684175491333}, {'ion_id': 2433, 'distance': 8.545307159423828, 'force': [0.17622800171375275, 0.010054746642708778, -4.543129920959473], 'magnitude': 4.546557426452637}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.414400815963745, 'force': [-9.531901359558105, 12.459776878356934, 12.891138076782227], 'magnitude': 20.304792404174805}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.6359496116638184, 'force': [15.442631721496582, -9.4920654296875, -21.784208297729492], 'magnitude': 28.339475631713867}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.5600497722625732, 'force': [4.157824516296387, -19.82586097717285, -13.012040138244629], 'magnitude': 24.076242446899414}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.2483973503112793, 'force': [1.395737648010254, 10.621081352233887, 7.715811729431152], 'magnitude': 13.201863288879395}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.52667236328125, 'force': [-1.2605687379837036, 5.837601184844971, 3.248612403869629], 'magnitude': 6.798536777496338}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.229920387268066, 'force': [-6.150196075439453, -2.293163299560547, -2.9568512439727783], 'magnitude': 7.199060916900635}]}, 780: {'frame': 780, 'ionic_force': [1.5604924224317074, -2.2272028028964996, -19.57033908367157], 'ionic_force_magnitude': 19.758384062862525, 'motion_vector': [0.9329605102539062, -1.2980384826660156, -0.02295684814453125], 'ionic_force_x': 1.5604924224317074, 'ionic_force_y': -2.2272028028964996, 'ionic_force_z': -19.57033908367157, 'radial_force': 2.7194795321341916, 'axial_force': -19.57033908367157, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [6.659114956855774, -5.889174699783325, -12.39469289779663], 'asn_force_magnitude': 15.253019461204346, 'residue_force': [6.659114956855774, -5.889174699783325, -12.39469289779663], 'residue_force_magnitude': 15.253019461204346, 'total_force': [8.219607379287481, -8.116377502679825, -31.9650319814682], 'total_force_magnitude': 33.98824500929592, 'motion_component_total': 11.845712006036852, 'cosine_total_motion': 0.3485237911753608, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.5799301422415836, 'cosine_residue_motion': 0.5799301422415836, 'cosine_ionic_motion': 0.15183560815207364, 'motion_component_glu': None, 'motion_component_asn': 8.84568574574988, 'motion_component_residue': 8.84568574574988, 'motion_component_ionic': 3.000026260286971, 'ionic_contributions': [{'ion_id': 1305, 'distance': 4.863986492156982, 'force': [0.10441190004348755, 2.004671096801758, -13.888773918151855], 'magnitude': 14.033090591430664}, {'ion_id': 1307, 'distance': 8.17383098602295, 'force': [1.306268334388733, -4.686950206756592, 1.0095268487930298], 'magnitude': 4.969203472137451}, {'ion_id': 1313, 'distance': 12.230953216552734, 'force': [0.05755798891186714, 0.07618516683578491, -2.217252254486084], 'magnitude': 2.2193074226379395}, {'ion_id': 2433, 'distance': 8.598190307617188, 'force': [0.09225419908761978, 0.37889114022254944, -4.47383975982666], 'magnitude': 4.490802764892578}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.5328550338745117, 'force': [-9.332026481628418, 13.461036682128906, 9.561555862426758], 'magnitude': 18.96601104736328}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.5732314586639404, 'force': [18.028329849243164, -15.043168067932129, -18.248754501342773], 'magnitude': 29.737764358520508}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.821122407913208, 'force': [3.6600077152252197, -17.851118087768555, -10.232149124145508], 'magnitude': 20.898683547973633}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.3263204097747803, 'force': [0.8818273544311523, 10.723662376403809, 6.538188457489014], 'magnitude': 12.590570449829102}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.718008995056152, 'force': [-0.8394418954849243, 5.667860984802246, 2.5173287391662598], 'magnitude': 6.258295059204102}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.346384048461914, 'force': [-5.73958158493042, -2.8474485874176025, -2.530862331390381], 'magnitude': 6.888833522796631}]}, 783: {'frame': 783, 'ionic_force': [3.219554729759693, -2.991701401770115, -16.00367283821106], 'ionic_force_magnitude': 16.596184930512365, 'motion_vector': [-0.09017181396484375, -0.0724945068359375, 0.0356597900390625], 'ionic_force_x': 3.219554729759693, 'ionic_force_y': -2.991701401770115, 'ionic_force_z': -16.00367283821106, 'radial_force': 4.394975532954795, 'axial_force': -16.00367283821106, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [10.200632810592651, 3.30025053024292, -12.62721872329712], 'asn_force_magnitude': 16.564758253137693, 'residue_force': [10.200632810592651, 3.30025053024292, -12.62721872329712], 'residue_force_magnitude': 16.564758253137693, 'total_force': [13.420187540352345, 0.308549128472805, -28.63089156150818], 'total_force_magnitude': 31.62158420746421, 'motion_component_total': -18.612833219754705, 'cosine_total_motion': -0.5886116615043336, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.8024645243561229, 'cosine_residue_motion': -0.8024645243561229, 'cosine_ionic_motion': -0.3205677924988123, 'motion_component_glu': None, 'motion_component_asn': -13.2926308526783, 'motion_component_residue': -13.2926308526783, 'motion_component_ionic': -5.320202367076403, 'ionic_contributions': [{'ion_id': 1305, 'distance': 5.601700782775879, 'force': [1.1842836141586304, 1.1778639554977417, -10.447630882263184], 'magnitude': 10.580307006835938}, {'ion_id': 1307, 'distance': 8.383296966552734, 'force': [1.6591039896011353, -4.3603739738464355, 0.7419834136962891], 'magnitude': 4.723984241485596}, {'ion_id': 1313, 'distance': 12.37425422668457, 'force': [0.10796178132295609, 0.038376592099666595, -2.1651737689971924], 'magnitude': 2.168203353881836}, {'ion_id': 2433, 'distance': 8.95036792755127, 'force': [0.26820534467697144, 0.15243202447891235, -4.132851600646973], 'magnitude': 4.144349098205566}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.950982570648193, 'force': [1.7997841835021973, 5.123132228851318, -1.1957693099975586], 'magnitude': 5.560177326202393}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.347566604614258, 'force': [-8.996441841125488, 15.769462585449219, 10.798011779785156], 'magnitude': 21.123659133911133}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.683553457260132, 'force': [12.725552558898926, -13.314679145812988, -20.20932960510254], 'magnitude': 27.342958450317383}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.34283447265625, 'force': [3.8015289306640625, -25.622360229492188, -8.643223762512207], 'magnitude': 27.30681800842285}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.092778205871582, 'force': [2.3181164264678955, 13.321063041687012, 5.41120719909668], 'magnitude': 14.563843727111816}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.11101770401001, 'force': [-1.4479074478149414, 8.023632049560547, 1.2118849754333496], 'magnitude': 8.24280071258545}]}, 784: {'frame': 784, 'ionic_force': [3.5136116072535515, -2.7213201289996505, -16.896898567676544], 'ionic_force_magnitude': 17.471583528045628, 'motion_vector': [0.3027000427246094, 1.73797607421875, -0.552337646484375], 'ionic_force_x': 3.5136116072535515, 'ionic_force_y': -2.7213201289996505, 'ionic_force_z': -16.896898567676544, 'radial_force': 4.444215315567593, 'axial_force': -16.896898567676544, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.8413375616073608, -0.1391606330871582, -15.900920510292053], 'asn_force_magnitude': 15.923771150358796, 'residue_force': [0.8413375616073608, -0.1391606330871582, -15.900920510292053], 'residue_force_magnitude': 15.923771150358796, 'total_force': [4.354949168860912, -2.8604807620868087, -32.7978190779686], 'total_force_magnitude': 33.2091082193544, 'motion_component_total': 7.8234271242535325, 'cosine_total_motion': 0.23558076514966483, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.2987960842443145, 'cosine_residue_motion': 0.2987960842443145, 'cosine_ionic_motion': 0.1754544259370086, 'motion_component_glu': None, 'motion_component_asn': 4.757960466129791, 'motion_component_residue': 4.757960466129791, 'motion_component_ionic': 3.065466658123741, 'ionic_contributions': [{'ion_id': 1305, 'distance': 5.370963096618652, 'force': [1.555128574371338, 1.4112720489501953, -11.315679550170898], 'magnitude': 11.508896827697754}, {'ion_id': 1307, 'distance': 8.494441986083984, 'force': [1.60205078125, -4.257933616638184, 0.6886278986930847], 'magnitude': 4.601171016693115}, {'ion_id': 1313, 'distance': 12.510846138000488, 'force': [0.11199747771024704, -0.012419587932527065, -2.118122100830078], 'magnitude': 2.121117353439331}, {'ion_id': 2433, 'distance': 8.932231903076172, 'force': [0.24443477392196655, 0.13776102662086487, -4.151724815368652], 'magnitude': 4.161194801330566}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.502779960632324, 'force': [1.8940670490264893, 5.981349468231201, -1.709570050239563], 'magnitude': 6.502819538116455}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.4452998638153076, 'force': [-7.706871032714844, 16.02739906311035, 9.023236274719238], 'magnitude': 19.94222068786621}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.7065467834472656, 'force': [9.21245002746582, -16.67827796936035, -18.960988998413086], 'magnitude': 26.880352020263672}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.78139328956604, 'force': [2.7102136611938477, -20.456178665161133, -5.440663814544678], 'magnitude': 21.340133666992188}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.4678573608398438, 'force': [1.5724457502365112, 11.189437866210938, 2.5511484146118164], 'magnitude': 11.583802223205566}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.669490337371826, 'force': [-1.206805944442749, 6.191004753112793, 1.0172092914581299], 'magnitude': 6.38902473449707}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.475203037261963, 'force': [-5.634161949157715, -2.393895149230957, -2.381291627883911], 'magnitude': 6.568490505218506}]}, 787: {'frame': 787, 'ionic_force': [5.250772535800934, -1.1602076143026352, -20.863549679517746], 'ionic_force_magnitude': 21.545403202556045, 'motion_vector': [0.2198486328125, 0.18189239501953125, 0.66143798828125], 'ionic_force_x': 5.250772535800934, 'ionic_force_y': -1.1602076143026352, 'ionic_force_z': -20.863549679517746, 'radial_force': 5.377424470042064, 'axial_force': -20.863549679517746, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [13.392127335071564, -6.304686069488525, -10.969375014305115], 'asn_force_magnitude': 18.423499374386914, 'residue_force': [13.392127335071564, -6.304686069488525, -10.969375014305115], 'residue_force_magnitude': 18.423499374386914, 'total_force': [18.642899870872498, -7.464893683791161, -31.83292469382286], 'total_force_magnitude': 37.637978796267475, 'motion_component_total': -25.424368859467805, 'cosine_total_motion': -0.6754977199250964, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.4112627714919698, 'cosine_residue_motion': -0.4112627714919698, 'cosine_ionic_motion': -0.8283655347911767, 'motion_component_glu': None, 'motion_component_asn': -7.576899413290935, 'motion_component_residue': -7.576899413290935, 'motion_component_ionic': -17.84746944617687, 'ionic_contributions': [{'ion_id': 1305, 'distance': 4.506951808929443, 'force': [2.2521560192108154, 2.6821045875549316, -15.964882850646973], 'magnitude': 16.344520568847656}, {'ion_id': 1307, 'distance': 8.135137557983398, 'force': [2.457170009613037, -4.345483303070068, 0.495204359292984], 'magnitude': 5.0165863037109375}, {'ion_id': 1313, 'distance': 13.337339401245117, 'force': [0.2008456587791443, 0.1273030787706375, -1.8511680364608765], 'magnitude': 1.8663783073425293}, {'ion_id': 2433, 'distance': 9.631600379943848, 'force': [0.340600848197937, 0.375868022441864, -3.542703151702881], 'magnitude': 3.578831195831299}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.9658095836639404, 'force': [-10.246170043945312, -10.151110649108887, 4.301395416259766], 'magnitude': 15.050948143005371}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.8396174907684326, 'force': [18.93375587463379, 13.46406364440918, -7.521315574645996], 'magnitude': 24.420040130615234}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.792302131652832, 'force': [10.009074211120605, 8.68825912475586, -0.9301528334617615], 'magnitude': 13.2865571975708}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.714291095733643, 'force': [-5.201322078704834, -3.4440205097198486, -0.6123093366622925], 'magnitude': 6.26816987991333}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.733892440795898, 'force': [-2.9934804439544678, -2.9753687381744385, 0.37383022904396057], 'magnitude': 4.237156391143799}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.7736494541168213, 'force': [-4.752922534942627, 15.705157279968262, 2.6600139141082764], 'magnitude': 16.622812271118164}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.7370355129241943, 'force': [5.783012866973877, -23.988004684448242, -9.056739807128906], 'magnitude': 26.284828186035156}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.317617416381836, 'force': [1.5464798212051392, -16.278444290161133, 0.7435783743858337], 'magnitude': 16.368637084960938}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.228622913360596, 'force': [1.0967320203781128, 7.701969146</t>
+          <t>{760: {'frame': 760, 'motion_vector': [0.43795013427734375, -0.21899032592773438, -0.324615478515625], 'ionic_force': [6.2238762974739075, -3.591959446668625, -15.905625224113464], 'ionic_force_magnitude': 17.453587671385044, 'radial_force': 7.186014808833161, 'axial_force': -15.905625224113464, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [6.150402218103409, 0.19301128387451172, -9.66019320487976], 'asn_force_magnitude': 11.45355986389207, 'residue_force': [6.150402218103409, 0.19301128387451172, -9.66019320487976], 'residue_force_magnitude': 11.45355986389207, 'total_force': [12.374278515577316, -3.398948162794113, -25.565818428993225], 'total_force_magnitude': 28.60571078191712, 'cosine_total_motion': 0.8606057782673394, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.8600653614153887, 'cosine_residue_motion': 0.8600653614153887, 'cosine_ionic_motion': 0.8460970984631494, 'motion_component_total': 24.618239990362206, 'motion_component_glu': None, 'motion_component_asn': 9.850810103831122, 'motion_component_residue': 9.850810103831122, 'motion_component_ionic': 14.767429886531083, 'motion_component_percent_total': 86.06057782673395, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 86.00653614153887, 'motion_component_percent_residue': 86.00653614153887, 'motion_component_percent_ionic': 84.60970984631494, 'ionic_contributions': [{'ion_id': 1305, 'distance': 5.483183860778809, 'force': [3.6287899017333984, -0.07852231711149216, -10.42906379699707], 'magnitude': 11.04262924194336, 'cosine_ionic_motion': 0.7694795727729797, 'motion_component_ionic': 8.497077941894531, 'motion_component_percent_ionic': 76.94795727729797}, {'ion_id': 1307, 'distance': 9.4274320602417, 'force': [1.388010025024414, -3.399308681488037, 0.6872068643569946], 'magnitude': 3.7355220317840576, 'cosine_ionic_motion': 0.5145567059516907, 'motion_component_ionic': 1.922137975692749, 'motion_component_percent_ionic': 51.45567059516907}, {'ion_id': 1313, 'distance': 12.530621528625488, 'force': [0.33516377210617065, -0.027667954564094543, -2.0875115394592285], 'magnitude': 2.1144278049468994, 'cosine_ionic_motion': 0.668566882610321, 'motion_component_ionic': 1.4136364459991455, 'motion_component_percent_ionic': 66.8566882610321}, {'ion_id': 2433, 'distance': 8.923480033874512, 'force': [0.8719125986099243, -0.08646049350500107, -4.07625675201416], 'magnitude': 4.169361591339111, 'cosine_ionic_motion': 0.7038432955741882, 'motion_component_ionic': 2.934577226638794, 'motion_component_percent_ionic': 70.38432955741882}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.825902462005615, 'force': [-3.0543558597564697, -5.7498459815979, 2.5002336502075195], 'magnitude': 6.974308967590332, 'cosine_with_motion': -0.21724484860897064, 'motion_component': -1.5151326656341553, 'motion_component_percent': 21.724484860897064}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.650112152099609, 'force': [4.436252117156982, 7.244457721710205, -3.2804160118103027], 'magnitude': 9.106241226196289, 'cosine_with_motion': 0.2656703293323517, 'motion_component': 2.4192581176757812, 'motion_component_percent': 26.56703293323517}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.588597059249878, 'force': [-5.562565326690674, 14.392956733703613, 9.988791465759277], 'magnitude': 18.381383895874023, 'cosine_with_motion': -0.8177438378334045, 'motion_component': -15.03126335144043, 'motion_component_percent': 81.77438378334045}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.9979047775268555, 'force': [7.43020486831665, -12.00178337097168, -16.756216049194336], 'magnitude': 21.909393310546875, 'cosine_with_motion': 0.8796035051345825, 'motion_component': 19.27157974243164, 'motion_component_percent': 87.96035051345825}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.7077767848968506, 'force': [0.47450941801071167, -20.36496925354004, -8.81492805480957], 'magnitude': 22.195947647094727, 'cosine_with_motion': 0.5773923993110657, 'motion_component': 12.81577205657959, 'motion_component_percent': 57.73923993110657}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.516462564468384, 'force': [2.7217092514038086, 9.680355072021484, 5.079469680786133], 'magnitude': 11.265788078308105, 'cosine_with_motion': -0.3893384635448456, 'motion_component': -4.386204719543457, 'motion_component_percent': 38.93384635448456}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.403622627258301, 'force': [-0.2953522503376007, 6.991840362548828, 1.6228721141815186], 'magnitude': 7.183785915374756, 'cosine_with_motion': -0.5182783007621765, 'motion_component': -3.723200559616089, 'motion_component_percent': 51.82783007621765}]}, 761: {'frame': 761, 'motion_vector': [-0.29718780517578125, -0.07862472534179688, 0.7725677490234375], 'ionic_force': [12.738315880298615, -4.829882338643074, -23.65466946363449], 'ionic_force_magnitude': 27.297176452981475, 'radial_force': 13.62323217417233, 'axial_force': -23.65466946363449, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-1.240791916847229, -3.651379108428955, -13.70577585697174], 'asn_force_magnitude': 14.237992337964446, 'residue_force': [-1.240791916847229, -3.651379108428955, -13.70577585697174], 'residue_force_magnitude': 14.237992337964446, 'total_force': [11.497523963451385, -8.48126144707203, -37.36044532060623], 'total_force_magnitude': 39.99909658451972, 'cosine_total_motion': -0.9505392439737632, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.839015311282996, 'cosine_residue_motion': -0.839015311282996, 'cosine_ionic_motion': -0.9552203136655474, 'motion_component_total': -38.02071102708291, 'motion_component_glu': None, 'motion_component_asn': -11.945893573482152, 'motion_component_residue': -11.945893573482152, 'motion_component_ionic': -26.074817453600758, 'motion_component_percent_total': 95.05392439737632, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 83.9015311282996, 'motion_component_percent_residue': 83.9015311282996, 'motion_component_percent_ionic': 95.52203136655474, 'ionic_contributions': [{'ion_id': 1305, 'distance': 4.033351898193359, 'force': [9.497282028198242, -1.4192678928375244, -18.007890701293945], 'magnitude': 20.408252716064453, 'cosine_ionic_motion': -0.9796156287193298, 'motion_component_ionic': -19.99224281311035, 'motion_component_percent_ionic': 97.96156287193298}, {'ion_id': 1307, 'distance': 9.503510475158691, 'force': [1.7444636821746826, -3.1808838844299316, 0.5928385853767395], 'magnitude': 3.6759533882141113, 'cosine_ionic_motion': 0.062055058777332306, 'motion_component_ionic': 0.22811150550842285, 'motion_component_percent_ionic': 6.205505877733231}, {'ion_id': 1313, 'distance': 12.466975212097168, 'force': [0.44171684980392456, -0.08128352463245392, -2.088320255279541], 'magnitude': 2.1360716819763184, 'cosine_ionic_motion': -0.9786861538887024, 'motion_component_ionic': -2.090543746948242, 'motion_component_percent_ionic': 97.86861538887024}, {'ion_id': 2433, 'distance': 8.801434516906738, 'force': [1.0548533201217651, -0.14844703674316406, -4.151297092437744], 'magnitude': 4.285792827606201, 'cosine_ionic_motion': -0.9846820831298828, 'motion_component_ionic': -4.2201433181762695, 'motion_component_percent_ionic': 98.46820831298828}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.774477958679199, 'force': [-3.011371612548828, -5.84398889541626, 2.67887806892395], 'magnitude': 7.099081039428711, 'cosine_with_motion': 0.5800740718841553, 'motion_component': 4.117992877960205, 'motion_component_percent': 58.00740718841553}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.7205986976623535, 'force': [4.704928398132324, 6.611140727996826, -3.498167037963867], 'magnitude': 8.836328506469727, 'cosine_with_motion': -0.6288903951644897, 'motion_component': -5.557082176208496, 'motion_component_percent': 62.889039516448975}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.39385724067688, 'force': [1.5932810306549072, 17.216833114624023, 11.108569145202637], 'magnitude': 20.551355361938477, 'cosine_with_motion': 0.39530149102211, 'motion_component': 8.123981475830078, 'motion_component_percent': 39.530149102211}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.634606122970581, 'force': [-4.252919673919678, -17.376630783081055, -22.016599655151367], 'magnitude': 28.368385314941406, 'cosine_with_motion': -0.6096012592315674, 'motion_component': -17.29340362548828, 'motion_component_percent': 60.96012592315674}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.179434299468994, 'force': [-5.557168960571289, -15.215255737304688, -6.5403971672058105], 'magnitude': 17.468914031982422, 'cosine_with_motion': -0.15181182324886322, 'motion_component': -2.6519877910614014, 'motion_component_percent': 15.181182324886322}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.321422576904297, 'force': [3.848464012145996, 5.593907833099365, 3.089388847351074], 'magnitude': 7.459678649902344, 'cosine_with_motion': 0.1294984221458435, 'motion_component': 0.9660166501998901, 'motion_component_percent': 12.94984221458435}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.925113677978516, 'force': [1.4339948892593384, 5.362614631652832, 1.472551941871643], 'magnitude': 5.7430291175842285, 'cosine_with_motion': 0.060697875916957855, 'motion_component': 0.3485896587371826, 'motion_component_percent': 6.0697875916957855}]}, 768: {'frame': 768, 'motion_vector': [-0.5820541381835938, -0.10816574096679688, -0.3086700439453125], 'ionic_force': [11.80370283126831, -3.687008783221245, -18.915793627500534], 'ionic_force_magnitude': 22.599307132180666, 'radial_force': 12.366140638713524, 'axial_force': -18.915793627500534, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [1.7805204391479492, -1.2756080627441406, -14.73203194141388], 'asn_force_magnitude': 14.89396502234379, 'residue_force': [1.7805204391479492, -1.2756080627441406, -14.73203194141388], 'residue_force_magnitude': 14.89396502234379, 'total_force': [13.58422327041626, -4.962616845965385, -33.64782556891441], 'total_force_magnitude': 36.624238604187646, 'cosine_total_motion': 0.12334616151708629, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.3669489184461005, 'cosine_residue_motion': 0.3669489184461005, 'cosine_ionic_motion': -0.04194221975331891, 'motion_component_total': 4.517459250312436, 'motion_component_glu': None, 'motion_component_asn': 5.465324356323105, 'motion_component_residue': 5.465324356323105, 'motion_component_ionic': -0.9478651060106689, 'motion_component_percent_total': 12.334616151708628, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 36.69489184461005, 'motion_component_percent_residue': 36.69489184461005, 'motion_component_percent_ionic': 4.194221975331891, 'ionic_contributions': [{'ion_id': 1305, 'distance': 4.501012802124023, 'force': [8.69870662689209, -0.5448192954063416, -13.87774658203125], 'magnitude': 16.387683868408203, 'cosine_ionic_motion': -0.06585518270730972, 'motion_component_ionic': -1.0792138576507568, 'motion_component_percent_ionic': 6.585518270730972}, {'ion_id': 1307, 'distance': 10.221074104309082, 'force': [1.4806410074234009, -2.767298698425293, 0.4990297853946686], 'magnitude': 3.1779348850250244, 'cosine_ionic_motion': -0.3377006947994232, 'motion_component_ionic': -1.0731908082962036, 'motion_component_percent_ionic': 33.77006947994232}, {'ion_id': 1313, 'distance': 13.009090423583984, 'force': [0.5215495824813843, -0.13493144512176514, -1.8863331079483032], 'magnitude': 1.9617525339126587, 'cosine_ionic_motion': 0.22391581535339355, 'motion_component_ionic': 0.43926742672920227, 'motion_component_percent_ionic': 22.391581535339355}, {'ion_id': 2433, 'distance': 9.321123123168945, 'force': [1.1028056144714355, -0.23995934426784515, -3.6507437229156494], 'magnitude': 3.821215867996216, 'cosine_ionic_motion': 0.2002691626548767, 'motion_component_ionic': 0.7652717232704163, 'motion_component_percent_ionic': 20.02691626548767}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.114900588989258, 'force': [3.308007001876831, 6.393937110900879, -2.196016311645508], 'magnitude': 7.526474952697754, 'cosine_with_motion': -0.38590317964553833, 'motion_component': -2.9044907093048096, 'motion_component_percent': 38.59031796455383}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.494544506072998, 'force': [2.515502452850342, 17.18895721435547, 8.599810600280762], 'magnitude': 19.384136199951172, 'cosine_with_motion': -0.46190327405929565, 'motion_component': -8.953596115112305, 'motion_component_percent': 46.190327405929565}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.607819080352783, 'force': [-3.6708574295043945, -21.16065788269043, -19.41893768310547], 'magnitude': 28.95416831970215, 'cosine_with_motion': 0.5389952659606934, 'motion_component': 15.606159210205078, 'motion_component_percent': 53.899526596069336}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.376420021057129, 'force': [-5.88956880569458, -13.469000816345215, -6.141573429107666], 'magnitude': 15.931727409362793, 'cosine_with_motion': 0.6374645829200745, 'motion_component': 10.155912399291992, 'motion_component_percent': 63.746458292007446}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.470947742462158, 'force': [3.842482566833496, 4.988195896148682, 2.9868156909942627], 'magnitude': 6.9690632820129395, 'cosine_with_motion': -0.794772744178772, 'motion_component': -5.538821697235107, 'motion_component_percent': 79.4772744178772}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.142477512359619, 'force': [1.6749546527862549, 4.782960414886475, 1.4378691911697388], 'magnitude': 5.267794132232666, 'cosine_with_motion': -0.5504844784736633, 'motion_component': -2.899838924407959, 'motion_component_percent': 55.04844784736633}]}, 774: {'frame': 774, 'motion_vector': [-1.0657234191894531, -0.014034271240234375, 0.7283935546875], 'ionic_force': [10.475233167409897, -4.618187832646072, -21.514216423034668], 'ionic_force_magnitude': 24.37046731325395, 'radial_force': 11.448063974716625, 'axial_force': -21.514216423034668, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-2.79820716381073, -9.780909061431885, -10.804529368877411], 'asn_force_magnitude': 14.840283025688445, 'residue_force': [-2.79820716381073, -9.780909061431885, -10.804529368877411], 'residue_force_magnitude': 14.840283025688445, 'total_force': [7.677026003599167, -14.399096894077957, -32.31874579191208], 'total_force_magnitude': 36.20458602424861, 'cosine_total_motion': -0.6744054193093619, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.2479693068729528, 'cosine_residue_motion': -0.2479693068729528, 'cosine_ionic_motion': -0.8508919445975974, 'motion_component_total': -24.41656901860525, 'motion_component_glu': None, 'motion_component_asn': -3.6799346956784103, 'motion_component_residue': -3.6799346956784103, 'motion_component_ionic': -20.73663432292684, 'motion_component_percent_total': 67.44054193093619, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 24.79693068729528, 'motion_component_percent_residue': 24.79693068729528, 'motion_component_percent_ionic': 85.08919445975974, 'ionic_contributions': [{'ion_id': 1305, 'distance': 4.294199466705322, 'force': [7.753024101257324, -1.7171417474746704, -16.158370971679688], 'magnitude': 18.004192352294922, 'cosine_ionic_motion': -0.8608502745628357, 'motion_component_ionic': -15.498913764953613, 'motion_component_percent_ionic': 86.08502745628357}, {'ion_id': 1307, 'distance': 10.263452529907227, 'force': [1.444155216217041, -2.761002540588379, 0.4741096496582031], 'magnitude': 3.151745557785034, 'cosine_ionic_motion': -0.2838697135448456, 'motion_component_ionic': -0.8946851491928101, 'motion_component_percent_ionic': 28.386971354484558}, {'ion_id': 1313, 'distance': 12.748905181884766, 'force': [0.4012247622013092, -0.01295121293514967, -2.0028076171875], 'magnitude': 2.04264235496521, 'cosine_ionic_motion': -0.7153201699256897, 'motion_component_ionic': -1.4611432552337646, 'motion_component_percent_ionic': 71.53201699256897}, {'ion_id': 2433, 'distance': 9.19312572479248, 'force': [0.8768290877342224, -0.12709233164787292, -3.8271474838256836], 'magnitude': 3.92836332321167, 'cosine_ionic_motion': -0.7336113452911377, 'motion_component_ionic': -2.881891965866089, 'motion_component_percent_ionic': 73.36113452911377}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.502677917480469, 'force': [-2.555861711502075, -6.9205780029296875, 2.5864498615264893], 'magnitude': 7.817707538604736, 'cosine_with_motion': 0.46619492769241333, 'motion_component': 3.644575595855713, 'motion_component_percent': 46.61949276924133}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.477771759033203, 'force': [3.961638927459717, 8.154483795166016, -3.775686502456665], 'magnitude': 9.82069206237793, 'cosine_with_motion': -0.5589756965637207, 'motion_component': -5.489528179168701, 'motion_component_percent': 55.89756965637207}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.661566972732544, 'force': [2.3035364151000977, 16.415498733520508, 6.079585552215576], 'magnitude': 17.65605354309082, 'cosine_with_motion': 0.07647211849689484, 'motion_component': 1.3501957654953003, 'motion_component_percent': 7.647211849689484}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.5984044075012207, 'force': [-6.747326850891113, -24.21038055419922, -14.794974327087402], 'magnitude': 29.164365768432617, 'cosine_with_motion': -0.08621666580438614, 'motion_component': -2.5144543647766113, 'motion_component_percent': 8.621666580438614}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.412884712219238, 'force': [-5.652472019195557, -14.314430236816406, -2.9462690353393555], 'magnitude': 15.669519424438477, 'cosine_with_motion': 0.2016385942697525, 'motion_component': 3.1595797538757324, 'motion_component_percent': 20.16385942697525}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.213598728179932, 'force': [4.4113688468933105, 6.305539131164551, 1.5313644409179688], 'magnitude': 7.846341609954834, 'cosine_with_motion': -0.3627511262893677, 'motion_component': -2.846269369125366, 'motion_component_percent': 36.27511262893677}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.257880210876465, 'force': [1.4809092283248901, 4.7889580726623535, 0.5150006413459778], 'magnitude': 5.039091110229492, 'cosine_with_motion': -0.19527995586395264, 'motion_component': -0.984033465385437, 'motion_component_percent': 19.527995586395264}]}, 777: {'frame': 777, 'motion_vector': [-0.18167495727539062, -0.27399444580078125, 0.3039093017578125], 'ionic_force': [3.253043606877327, -2.876964196562767, -18.913673758506775], 'ionic_force_magnitude': 19.40583084384117, 'radial_force': 4.34271985011116, 'axial_force': -18.913673758506775, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [6.349842518568039, -4.249195218086243, -11.838613510131836], 'asn_force_magnitude': 14.090029448311935, 'residue_force': [6.349842518568039, -4.249195218086243, -11.838613510131836], 'residue_force_magnitude': 14.090029448311935, 'total_force': [9.602886125445366, -7.12615941464901, -30.75228726863861], 'total_force_magnitude': 32.995465479276604, 'cosine_total_motion': -0.6185919759226997, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.5686615983288297, 'cosine_residue_motion': -0.5686615983288297, 'cosine_ionic_motion': -0.6388941355052798, 'motion_component_total': -20.41073018731494, 'motion_component_glu': None, 'motion_component_asn': -8.012458666577343, 'motion_component_residue': -8.012458666577343, 'motion_component_ionic': -12.398271520737598, 'motion_component_percent_total': 61.859197592269965, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 56.86615983288297, 'motion_component_percent_residue': 56.86615983288297, 'motion_component_percent_ionic': 63.88941355052798, 'ionic_contributions': [{'ion_id': 1305, 'distance': 4.9131622314453125, 'force': [1.1015095710754395, 1.6659917831420898, -13.607799530029297], 'magnitude': 13.753582954406738, 'cosine_ionic_motion': -0.7782527208328247, 'motion_component_ionic': -10.703763008117676, 'motion_component_percent_ionic': 77.82527208328247}, {'ion_id': 1307, 'distance': 7.9652605056762695, 'force': [1.8268259763717651, -4.72895622253418, 1.297066569328308], 'magnitude': 5.232848167419434, 'cosine_ionic_motion': 0.5796595215797424, 'motion_component_ionic': 3.0332703590393066, 'motion_component_percent_ionic': 57.96595215797424}, {'ion_id': 1313, 'distance': 12.369667053222656, 'force': [0.09195472300052643, 0.049325793981552124, -2.1673009395599365], 'magnitude': 2.169811487197876, 'cosine_ionic_motion': -0.7091403603553772, 'motion_component_ionic': -1.5387009382247925, 'motion_component_percent_ionic': 70.91403603553772}, {'ion_id': 2433, 'distance': 8.643499374389648, 'force': [0.23275333642959595, 0.1366744488477707, -4.43563985824585], 'magnitude': 4.443844318389893, 'cosine_ionic_motion': -0.7176395058631897, 'motion_component_ionic': -3.1890783309936523, 'motion_component_percent_ionic': 71.76395058631897}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.4169793128967285, 'force': [-8.892522811889648, 15.237275123596191, 9.989500045776367], 'magnitude': 20.27416229248047, 'cosine_with_motion': 0.05249869450926781, 'motion_component': 1.0643670558929443, 'motion_component_percent': 5.249869450926781}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.622715473175049, 'force': [16.82961654663086, -14.755626678466797, -17.846418380737305], 'magnitude': 28.626197814941406, 'cosine_with_motion': -0.3463032841682434, 'motion_component': -9.913346290588379, 'motion_component_percent': 34.63032841682434}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.651845693588257, 'force': [2.0806901454925537, -20.070762634277344, -10.787858009338379], 'magnitude': 22.881053924560547, 'cosine_with_motion': 0.17988532781600952, 'motion_component': 4.115965843200684, 'motion_component_percent': 17.988532781600952}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.245034694671631, 'force': [1.875540852546692, 10.595893859863281, 7.69559383392334], 'magnitude': 13.229239463806152, 'cosine_with_motion': -0.15283194184303284, 'motion_component': -2.021850347518921, 'motion_component_percent': 15.283194184303284}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.528416633605957, 'force': [-0.41165056824684143, 6.314081192016602, 2.472215414047241], 'magnitude': 6.793300151824951, 'cosine_with_motion': -0.2972017228603363, 'motion_component': -2.0189805030822754, 'motion_component_percent': 29.72017228603363}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.576260089874268, 'force': [-5.131831645965576, -1.5700560808181763, -3.3616464138031006], 'magnitude': 6.332569599151611, 'cosine_with_motion': 0.12023338675498962, 'motion_component': 0.7613862752914429, 'motion_component_percent': 12.023338675498962}]}, 778: {'frame': 778, 'motion_vector': [0.5508079528808594, 0.34873199462890625, -0.7382888793945312], 'ionic_force': [2.2254137322306633, -2.9039981458336115, -20.00335383415222], 'ionic_force_magnitude': 20.33518714260821, 'radial_force': 3.6586433975731856, 'axial_force': -20.00335383415222, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [4.0535277128219604, -2.6926302909851074, -13.897537469863892], 'asn_force_magnitude': 14.724907216305882, 'residue_force': [4.0535277128219604, -2.6926302909851074, -13.897537469863892], 'residue_force_magnitude': 14.724907216305882, 'total_force': [6.278941445052624, -5.596628436818719, -33.90089130401611], 'total_force_magnitude': 34.928753008616304, 'cosine_total_motion': 0.7713303935866661, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.7966753458909348, 'cosine_residue_motion': 0.7966753458909348, 'cosine_ionic_motion': 0.7479959810153054, 'motion_component_total': 26.941608805627464, 'motion_component_glu': None, 'motion_component_asn': 11.73097054976241, 'motion_component_residue': 11.73097054976241, 'motion_component_ionic': 15.210638255865053, 'motion_component_percent_total': 77.13303935866661, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 79.66753458909348, 'motion_component_percent_residue': 79.66753458909348, 'motion_component_percent_ionic': 74.79959810153053, 'ionic_contributions': [{'ion_id': 1305, 'distance': 4.80653715133667, 'force': [0.9331015348434448, 1.4339590072631836, -14.268352508544922], 'magnitude': 14.370553016662598, 'cosine_ionic_motion': 0.8159022927284241, 'motion_component_ionic': 11.724967002868652, 'motion_component_percent_ionic': 81.59022927284241}, {'ion_id': 1307, 'distance': 8.545356750488281, 'force': [1.0206871032714844, -4.311095237731934, 1.0214502811431885], 'magnitude': 4.546504974365234, 'cosine_ionic_motion': -0.37859654426574707, 'motion_component_ionic': -1.7212910652160645, 'motion_component_percent_ionic': 37.85965442657471}, {'ion_id': 1313, 'distance': 12.240949630737305, 'force': [0.09539709240198135, -0.03691666200757027, -2.2133216857910156], 'magnitude': 2.215684175491333, 'cosine_ionic_motion': 0.7669698596000671, 'motion_component_ionic': 1.6993629932403564, 'motion_component_percent_ionic': 76.69698596000671}, {'ion_id': 2433, 'distance': 8.545307159423828, 'force': [0.17622800171375275, 0.010054746642708778, -4.543129920959473], 'magnitude': 4.546557426452637, 'cosine_ionic_motion': 0.7714846730232239, 'motion_component_ionic': 3.507599353790283, 'motion_component_percent_ionic': 77.14846730232239}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.414400815963745, 'force': [-9.531901359558105, 12.459776878356934, 12.891138076782227], 'magnitude': 20.304792404174805, 'cosine_with_motion': -0.5211602449417114, 'motion_component': -10.582050323486328, 'motion_component_percent': 52.11602449417114}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.6359496116638184, 'force': [15.442631721496582, -9.4920654296875, -21.784208297729492], 'magnitude': 28.339475631713867, 'cosine_with_motion': 0.7623465061187744, 'motion_component': 21.60449981689453, 'motion_component_percent': 76.23465061187744}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.5600497722625732, 'force': [4.157824516296387, -19.82586097717285, -13.012040138244629], 'magnitude': 24.076242446899414, 'cosine_with_motion': 0.21013124287128448, 'motion_component': 5.059170722961426, 'motion_component_percent': 21.01312428712845}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.2483973503112793, 'force': [1.395737648010254, 10.621081352233887, 7.715811729431152], 'magnitude': 13.201863288879395, 'cosine_with_motion': -0.09411829710006714, 'motion_component': -1.2425369024276733, 'motion_component_percent': 9.411829710006714}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.52667236328125, 'force': [-1.2605687379837036, 5.837601184844971, 3.248612403869629], 'magnitude': 6.798536777496338, 'cosine_with_motion': -0.1578526347875595, 'motion_component': -1.0731669664382935, 'motion_component_percent': 15.785263478755951}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.229920387268066, 'force': [-6.150196075439453, -2.293163299560547, -2.9568512439727783], 'magnitude': 7.199060916900635, 'cosine_with_motion': -0.2826682925224304, 'motion_component': -2.0349462032318115, 'motion_component_percent': 28.266829252243042}]}, 780: {'frame': 780, 'motion_vector': [0.9329605102539062, -1.2980384826660156, -0.02295684814453125], 'ionic_force': [1.5604924224317074, -2.2272028028964996, -19.57033908367157], 'ionic_force_magnitude': 19.758384062862525, 'radial_force': 2.7194795321341916, 'axial_force': -19.57033908367157, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [6.659114956855774, -5.889174699783325, -12.39469289779663], 'asn_force_magnitude': 15.253019461204346, 'residue_force': [6.659114956855774, -5.889174699783325, -12.39469289779663], 'residue_force_magnitude': 15.253019461204346, 'total_force': [8.219607379287481, -8.116377502679825, -31.9650319814682], 'total_force_magnitude': 33.98824500929592, 'cosine_total_motion': 0.3485237911753608, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.5799301422415836, 'cosine_residue_motion': 0.5799301422415836, 'cosine_ionic_motion': 0.15183560815207364, 'motion_component_total': 11.845712006036852, 'motion_component_glu': None, 'motion_component_asn': 8.84568574574988, 'motion_component_residue': 8.84568574574988, 'motion_component_ionic': 3.000026260286971, 'motion_component_percent_total': 34.85237911753608, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 57.99301422415836, 'motion_component_percent_residue': 57.99301422415836, 'motion_component_percent_ionic': 15.183560815207365, 'ionic_contributions': [{'ion_id': 1305, 'distance': 4.863986492156982, 'force': [0.10441190004348755, 2.004671096801758, -13.888773918151855], 'magnitude': 14.033090591430664, 'cosine_ionic_motion': -0.09743314981460571, 'motion_component_ionic': -1.3672882318496704, 'motion_component_percent_ionic': 9.743314981460571}, {'ion_id': 1307, 'distance': 8.17383098602295, 'force': [1.306268334388733, -4.686950206756592, 1.0095268487930298], 'magnitude': 4.969203472137451, 'cosine_ionic_motion': 0.916303277015686, 'motion_component_ionic': 4.553297519683838, 'motion_component_percent_ionic': 91.6303277015686}, {'ion_id': 1313, 'distance': 12.230953216552734, 'force': [0.05755798891186714, 0.07618516683578491, -2.217252254486084], 'magnitude': 2.2193074226379395, 'cosine_ionic_motion': 0.0016091226134449244, 'motion_component_ionic': 0.00357113778591156, 'motion_component_percent_ionic': 0.16091226134449244}, {'ion_id': 2433, 'distance': 8.598190307617188, 'force': [0.09225419908761978, 0.37889114022254944, -4.47383975982666], 'magnitude': 4.490802764892578, 'cosine_ionic_motion': -0.04220941290259361, 'motion_component_ionic': -0.1895541548728943, 'motion_component_percent_ionic': 4.220941290259361}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.5328550338745117, 'force': [-9.332026481628418, 13.461036682128906, 9.561555862426758], 'magnitude': 18.96601104736328, 'cosine_with_motion': -0.8706464171409607, 'motion_component': -16.5126895904541, 'motion_component_percent': 87.06464171409607}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.5732314586639404, 'force': [18.028329849243164, -15.043168067932129, -18.248754501342773], 'magnitude': 29.737764358520508, 'cosine_with_motion': 0.7733249664306641, 'motion_component': 22.99695587158203, 'motion_component_percent': 77.3324966430664}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.821122407913208, 'force': [3.6600077152252197, -17.851118087768555, -10.232149124145508], 'magnitude': 20.898683547973633, 'cosine_with_motion': 0.8027648329734802, 'motion_component': 16.7767276763916, 'motion_component_percent': 80.27648329734802}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.3263204097747803, 'force': [0.8818273544311523, 10.723662376403809, 6.538188457489014], 'magnitude': 12.590570449829102, 'cosine_with_motion': -0.6581251621246338, 'motion_component': -8.286170959472656, 'motion_component_percent': 65.81251621246338</t>
         </is>
       </c>
     </row>
@@ -499,7 +499,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>{2261: {'frame': 2261, 'ionic_force': [9.17229837179184, 1.028277650475502, -9.523530200123787], 'ionic_force_magnitude': 13.26220343006065, 'motion_vector': [-1.0795135498046875, -0.78814697265625, 0.6654815673828125], 'ionic_force_x': 9.17229837179184, 'ionic_force_y': 1.028277650475502, 'ionic_force_z': -9.523530200123787, 'radial_force': 9.229756895370683, 'axial_force': -9.523530200123787, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [7.0570900440216064, 7.893163204193115, -6.501342058181763], 'asn_force_magnitude': 12.424652663754431, 'residue_force': [7.0570900440216064, 7.893163204193115, -6.501342058181763], 'residue_force_magnitude': 12.424652663754431, 'total_force': [16.229388415813446, 8.921440854668617, -16.02487225830555], 'total_force_magnitude': 24.490440709993376, 'motion_component_total': -23.585269969968714, 'cosine_total_motion': -0.9630398345728705, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.9792086757705155, 'cosine_residue_motion': -0.9792086757705155, 'cosine_ionic_motion': -0.8610139595885321, 'motion_component_glu': None, 'motion_component_asn': -12.166327681783585, 'motion_component_residue': -12.166327681783585, 'motion_component_ionic': -11.418942288185132, 'ionic_contributions': [{'ion_id': 1306, 'distance': 11.144904136657715, 'force': [1.5889837741851807, 2.148843765258789, -0.045660361647605896], 'magnitude': 2.6729166507720947}, {'ion_id': 1307, 'distance': 9.503464698791504, 'force': [2.269397735595703, -2.8564016819000244, 0.45132771134376526], 'magnitude': 3.6759889125823975}, {'ion_id': 1313, 'distance': 10.139678955078125, 'force': [1.2523084878921509, 0.40465953946113586, -2.948805570602417], 'magnitude': 3.229161024093628}, {'ion_id': 1460, 'distance': 13.783182144165039, 'force': [0.5171981453895569, 0.2051517814397812, -1.6566481590270996], 'magnitude': 1.7475881576538086}, {'ion_id': 2433, 'distance': 7.150071144104004, 'force': [3.544410228729248, 1.1260242462158203, -5.32374382019043], 'magnitude': 6.494075775146484}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.8561618328094482, 'force': [-4.236083507537842, -14.082409858703613, 6.095686912536621], 'magnitude': 15.919047355651855}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.8134114742279053, 'force': [11.147245407104492, 19.2869873046875, -11.073408126831055], 'magnitude': 24.877084732055664}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.667447090148926, 'force': [4.180720329284668, 13.239962577819824, -1.8488456010818481], 'magnitude': 14.006900787353516}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.459536552429199, 'force': [-2.9634432792663574, -6.3406453132629395, -0.2847350239753723], 'magnitude': 7.0047736167907715}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.634800434112549, 'force': [-1.0713489055633545, -4.210731506347656, 0.6099597811698914], 'magnitude': 4.38749361038208}]}, 2265: {'frame': 2265, 'ionic_force': [9.130726605653763, 1.9627961963415146, -10.302303045988083], 'ionic_force_magnitude': 13.905401299744698, 'motion_vector': [0.6828193664550781, 0.2771263122558594, 0.02298736572265625], 'ionic_force_x': 9.130726605653763, 'ionic_force_y': 1.9627961963415146, 'ionic_force_z': -10.302303045988083, 'radial_force': 9.339311390866364, 'axial_force': -10.302303045988083, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [3.032887816429138, 11.611568927764893, -6.067251920700073], 'asn_force_magnitude': 13.447620136682852, 'residue_force': [3.032887816429138, 11.611568927764893, -6.067251920700073], 'residue_force_magnitude': 13.447620136682852, 'total_force': [12.163614422082901, 13.574365124106407, -16.369554966688156], 'total_force_magnitude': 24.498555756188658, 'motion_component_total': 15.857208265330689, 'cosine_total_motion': 0.6472711462317507, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.5193695335500276, 'cosine_residue_motion': 0.5193695335500276, 'cosine_ionic_motion': 0.638091909490355, 'motion_component_glu': None, 'motion_component_asn': 6.9842841977469305, 'motion_component_residue': 6.9842841977469305, 'motion_component_ionic': 8.872924067583758, 'ionic_contributions': [{'ion_id': 1306, 'distance': 10.167248725891113, 'force': [1.7125273942947388, 2.7137768268585205, 0.13229718804359436], 'magnitude': 3.211671829223633}, {'ion_id': 1307, 'distance': 9.260034561157227, 'force': [2.3590493202209473, -3.053358554840088, 0.3204958438873291], 'magnitude': 3.8717992305755615}, {'ion_id': 1313, 'distance': 10.266485214233398, 'force': [1.0728236436843872, 0.4622923731803894, -2.925252676010132], 'magnitude': 3.14988374710083}, {'ion_id': 1460, 'distance': 13.558910369873047, 'force': [0.4920254051685333, 0.18344132602214813, -1.7278474569320679], 'magnitude': 1.8058784008026123}, {'ion_id': 2433, 'distance': 6.779136657714844, 'force': [3.4943008422851562, 1.6566442251205444, -6.101995944976807], 'magnitude': 7.224193096160889}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.9743127822875977, 'force': [-3.029351234436035, -13.51841926574707, 5.716115474700928], 'magnitude': 14.986614227294922}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.7652649879455566, 'force': [5.912781238555908, 22.921756744384766, -10.136136054992676], 'magnitude': 25.750905990600586}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.7473063468933105, 'force': [4.9608964920043945, 12.30671215057373, -2.6936099529266357], 'magnitude': 13.539615631103516}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.4551544189453125, 'force': [-3.490391969680786, -6.0826497077941895, 0.2805880904197693], 'magnitude': 7.018560409545898}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.694264888763428, 'force': [-1.3210467100143433, -4.015830993652344, 0.7657905220985413], 'magnitude': 4.296335220336914}]}, 2266: {'frame': 2266, 'ionic_force': [9.680621922016144, 1.6852705627679825, -9.65313646197319], 'ionic_force_magnitude': 13.774527985387671, 'motion_vector': [-1.1436843872070312, -1.179443359375, 0.6229476928710938], 'ionic_force_x': 9.680621922016144, 'ionic_force_y': 1.6852705627679825, 'ionic_force_z': -9.65313646197319, 'radial_force': 9.826218889621371, 'axial_force': -9.65313646197319, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [1.8425058722496033, 9.913079738616943, -10.763621866703033], 'asn_force_magnitude': 14.74854343597427, 'residue_force': [1.8425058722496033, 9.913079738616943, -10.763621866703033], 'residue_force_magnitude': 14.74854343597427, 'total_force': [11.523127794265747, 11.598350301384926, -20.416758328676224], 'total_force_magnitude': 26.15622726098291, 'motion_component_total': -22.52490112947925, 'cosine_total_motion': -0.8611678169305217, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.791255363964706, 'cosine_residue_motion': -0.791255363964706, 'cosine_ionic_motion': -0.7880514698299226, 'motion_component_glu': None, 'motion_component_asn': -11.669864104381096, 'motion_component_residue': -11.669864104381096, 'motion_component_ionic': -10.855037025098156, 'ionic_contributions': [{'ion_id': 1306, 'distance': 11.234864234924316, 'force': [1.5262173414230347, 2.137537717819214, 0.14135095477104187], 'magnitude': 2.6302826404571533}, {'ion_id': 1307, 'distance': 9.184137344360352, 'force': [2.673102855682373, -2.871659517288208, 0.3172300457954407], 'magnitude': 3.936056613922119}, {'ion_id': 1313, 'distance': 10.04376220703125, 'force': [1.2430906295776367, 0.5733397603034973, -2.99291729927063], 'magnitude': 3.2911314964294434}, {'ion_id': 1460, 'distance': 13.551627159118652, 'force': [0.5830580592155457, 0.21003158390522003, -1.6982765197753906], 'magnitude': 1.8078199625015259}, {'ion_id': 2433, 'distance': 7.01875638961792, 'force': [3.6551530361175537, 1.6360210180282593, -5.420523643493652], 'magnitude': 6.739346027374268}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.790710687637329, 'force': [-1.2962645292282104, -14.231207847595215, 8.195677757263184], 'magnitude': 16.473514556884766}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.659165859222412, 'force': [3.3110499382019043, 21.939655303955078, -16.8265323638916], 'magnitude': 27.846790313720703}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.462449550628662, 'force': [3.25949764251709, 14.429506301879883, -3.996321439743042], 'magnitude': 15.323366165161133}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.120400428771973, 'force': [-2.7134130001068115, -7.720348358154297, 0.6005362868309021], 'magnitude': 8.205305099487305}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.4251909255981445, 'force': [-0.7183641791343689, -4.504525661468506, 1.2630178928375244], 'magnitude': 4.733076572418213}]}, 2268: {'frame': 2268, 'ionic_force': [10.473756790161133, 1.8430732190608978, -8.884076906368136], 'ionic_force_magnitude': 13.8572480193049, 'motion_vector': [-0.18704986572265625, -0.371490478515625, -0.394805908203125], 'ionic_force_x': 10.473756790161133, 'ionic_force_y': 1.8430732190608978, 'ionic_force_z': -8.884076906368136, 'radial_force': 10.634683831231936, 'axial_force': -8.884076906368136, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-4.8723388612270355, 12.627479553222656, -6.10999259352684], 'asn_force_magnitude': 14.850081997707361, 'residue_force': [-4.8723388612270355, 12.627479553222656, -6.10999259352684], 'residue_force_magnitude': 14.850081997707361, 'total_force': [5.601417928934097, 14.470552772283554, -14.994069499894977], 'total_force_magnitude': 21.577648169291027, 'motion_component_total': -0.8782893431034147, 'cosine_total_motion': -0.04070366409780388, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.16056266766432975, 'cosine_residue_motion': -0.16056266766432975, 'cosine_ionic_motion': 0.10868532015767929, 'motion_component_glu': None, 'motion_component_asn': -2.384368780585933, 'motion_component_residue': -2.384368780585933, 'motion_component_ionic': 1.5060794374825202, 'ionic_contributions': [{'ion_id': 1306, 'distance': 11.470409393310547, 'force': [1.6078039407730103, 1.9444148540496826, -0.03991365805268288], 'magnitude': 2.5233659744262695}, {'ion_id': 1307, 'distance': 10.841493606567383, 'force': [1.9502389430999756, -2.0432045459747314, 0.018825938925147057], 'magnitude': 2.8246188163757324}, {'ion_id': 1313, 'distance': 10.89434814453125, 'force': [1.217636227607727, 0.36708852648735046, -2.491459369659424], 'magnitude': 2.7972776889801025}, {'ion_id': 1460, 'distance': 14.645277976989746, 'force': [0.5479416847229004, 0.135992169380188, -1.441270112991333], 'magnitude': 1.5478997230529785}, {'ion_id': 2433, 'distance': 6.756194591522217, 'force': [5.1501359939575195, 1.4387822151184082, -4.930259704589844], 'magnitude': 7.273338794708252}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.8425087928771973, 'force': [2.948867082595825, -15.000923156738281, 4.828411102294922], 'magnitude': 16.03237533569336}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.6733570098876953, 'force': [-7.116278648376465, 24.974990844726562, -9.204205513000488], 'magnitude': 27.55193328857422}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.470522880554199, 'force': [-0.9130064845085144, 15.211467742919922, -0.9442872405052185], 'magnitude': 15.268072128295898}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.171175956726074, 'force': [-0.24993082880973816, -7.921639919281006, -1.137224793434143], 'magnitude': 8.006754875183105}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.4605889320373535, 'force': [0.4580100178718567, -4.636415958404541, 0.34731385111808777], 'magnitude': 4.671911239624023}]}, 2269: {'frame': 2269, 'ionic_force': [12.215474724769592, 1.5210530683398247, -10.407313026487827], 'ionic_force_magnitude': 16.119664686943523, 'motion_vector': [-1.0145034790039062, 0.823699951171875, 0.27971649169921875], 'ionic_force_x': 12.215474724769592, 'ionic_force_y': 1.5210530683398247, 'ionic_force_z': -10.407313026487827, 'radial_force': 12.309810119908054, 'axial_force': -10.407313026487827, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-2.13426174223423, 10.67313814163208, -3.368392623960972], 'asn_force_magnitude': 11.393727214738856, 'residue_force': [-2.13426174223423, 10.67313814163208, -3.368392623960972], 'residue_force_magnitude': 11.393727214738856, 'total_force': [10.081212982535362, 12.194191209971905, -13.7757056504488], 'total_force_magnitude': 20.97854190911281, 'motion_component_total': -3.0203462701425927, 'cosine_total_motion': -0.1439731265989746, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.6577022374570919, 'cosine_residue_motion': 0.6577022374570919, 'cosine_ionic_motion': -0.6522484404261935, 'motion_component_glu': None, 'motion_component_asn': 7.493679882109505, 'motion_component_residue': 7.493679882109505, 'motion_component_ionic': -10.514026152252097, 'ionic_contributions': [{'ion_id': 1306, 'distance': 11.17204475402832, 'force': [1.694044589996338, 2.045954465866089, -0.13997234404087067], 'magnitude': 2.659945249557495}, {'ion_id': 1307, 'distance': 11.321696281433105, 'force': [1.7108734846115112, -1.9433295726776123, 0.07040224224328995], 'magnitude': 2.5900914669036865}, {'ion_id': 1313, 'distance': 9.32046127319336, 'force': [1.9830888509750366, 0.3941100537776947, -3.2431273460388184], 'magnitude': 3.821758508682251}, {'ion_id': 1460, 'distance': 14.296980857849121, 'force': [0.5635555982589722, 0.1147402748465538, -1.5190082788467407], 'magnitude': 1.6242371797561646}, {'ion_id': 2433, 'distance': 6.273693561553955, 'force': [6.263912200927734, 0.9095778465270996, -5.5756072998046875], 'magnitude': 8.435124397277832}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.8535971641540527, 'force': [1.6794264316558838, -15.571176528930664, 2.968061923980713], 'magnitude': 15.940244674682617}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.657850980758667, 'force': [-1.5747489929199219, 27.27834129333496, -5.512861728668213], 'magnitude': 27.87434959411621}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.67467737197876, 'force': [0.1745680421590805, 13.957775115966797, 0.36374419927597046], 'magnitude': 13.963604927062988}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.5912089347839355, 'force': [-0.7262468338012695, -6.408841133117676, -1.4404574632644653], 'magnitude': 6.6087517738342285}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.642570495605469, 'force': [0.03614121675491333, -4.373770713806152, 0.11448761075735092], 'magnitude': 4.375418186187744}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.983630657196045, 'force': [-2.079843044281006, -8.262550354003906, -0.1973496377468109], 'magnitude': 8.522583961486816}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.841239929199219, 'force': [0.3564414381980896, 4.053360462188721, 0.33598247170448303], 'magnitude': 4.082850456237793}]}, 2270: {'frame': 2270, 'ionic_force': [11.086936205625534, 3.327737480401993, -11.238739222288132], 'ionic_force_magnitude': 16.133916154259637, 'motion_vector': [0.494598388671875, -1.7763481140136719, 0.808197021484375], 'ionic_force_x': 11.086936205625534, 'ionic_force_y': 3.327737480401993, 'ionic_force_z': -11.238739222288132, 'radial_force': 11.575577357785766, 'axial_force': -11.238739222288132, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [1.0553871393203735, 16.747479915618896, -7.028375923633575], 'asn_force_magnitude': 18.193130397537782, 'residue_force': [1.0553871393203735, 16.747479915618896, -7.028375923633575], 'residue_force_magnitude': 18.193130397537782, 'total_force': [12.142323344945908, 20.07521739602089, -18.267115145921707], 'total_force_magnitude': 29.734455862939214, 'motion_component_total': -22.062917220939244, 'cosine_total_motion': -0.7419983510926893, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.9530445913907333, 'cosine_residue_motion': -0.9530445913907333, 'cosine_ionic_motion': -0.29280260600909885, 'motion_component_glu': None, 'motion_component_asn': -17.338864525839725, 'motion_component_residue': -17.338864525839725, 'motion_component_ionic': -4.72405269509952, 'ionic_contributions': [{'ion_id': 1306, 'distance': 10.51248836517334, 'force': [1.6320011615753174, 2.514735221862793, -0.19447630643844604], 'magnitude': 3.0041873455047607}, {'ion_id': 1307, 'distance': 10.130454063415527, 'force': [2.1316187381744385, -2.4281625747680664, 0.16044160723686218], 'magnitude': 3.235044479370117}, {'ion_id': 1313, 'distance': 10.578052520751953, 'force': [1.0888550281524658, 0.4178965389728546, -2.7282259464263916], 'magnitude': 2.967062473297119}, {'ion_id': 1460, 'distance': 14.25514030456543, 'force': [0.45483729243278503, 0.18684375286102295, -1.5580334663391113], 'magnitude': 1.6337857246398926}, {'ion_id': 2433, 'distance': 5.9453535079956055, 'force': [5.779623985290527, 2.6364245414733887, -6.918445110321045], 'magnitude': 9.392533302307129}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.7779879570007324, 'force': [-0.8482921123504639, -15.651665687561035, 5.418171405792236], 'magnitude': 16.58465576171875}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.6543116569519043, 'force': [2.7832577228546143, 25.383670806884766, -11.36021614074707], 'magnitude': 27.948734283447266}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.565553665161133, 'force': [2.400338649749756, 14.367148399353027, -1.458168864250183], 'magnitude': 14.63908576965332}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.482104778289795, 'force': [-1.9207251071929932, -6.633512020111084, -0.6272006034851074], 'magnitude': 6.934410572052002}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.529580116271973, 'force': [-0.5192922949790955, -4.485893726348877, 0.6039515137672424], 'magnitude': 4.556057929992676}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.991696357727051, 'force': [-0.8398997187614441, 3.7677321434020996, 0.39508676528930664], 'magnitude': 3.880377769470215}]}, 2492: {'frame': 2492, 'ionic_force': [9.755406647920609, 0.5477147996425629, -11.056969352066517], 'ionic_force_magnitude': 14.755491236166263, 'motion_vector': [-2.5311126708984375, 2.8303871154785156, 0.9147491455078125], 'ionic_force_x': 9.755406647920609, 'ionic_force_y': 0.5477147996425629, 'ionic_force_z': -11.056969352066517, 'radial_force': 9.770770203420051, 'axial_force': -11.056969352066517, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-6.351130992174149, -11.85277271270752, -4.769610553979874], 'asn_force_magnitude': 14.267945566741385, 'residue_force': [-6.351130992174149, -11.85277271270752, -4.769610553979874], 'residue_force_magnitude': 14.267945566741385, 'total_force': [3.40427565574646, -11.305057913064957, -15.82657990604639], 'total_force_magnitude': 19.74522875736141, 'motion_component_total': -14.105496055631573, 'cosine_total_motion': -0.7143749119833704, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.3918360759131695, 'cosine_residue_motion': -0.3918360759131695, 'cosine_ionic_motion': -0.5770597614904768, 'motion_component_glu': None, 'motion_component_asn': -5.590695802214648, 'motion_component_residue': -5.590695802214648, 'motion_component_ionic': -8.514800253416924, 'ionic_contributions': [{'ion_id': 1306, 'distance': 7.256741523742676, 'force': [4.944879055023193, 3.794395685195923, -0.9477364420890808], 'magnitude': 6.304559707641602}, {'ion_id': 1307, 'distance': 11.3829984664917, 'force': [1.5883479118347168, -2.01047945022583, -0.018609173595905304], 'magnitude': 2.5622689723968506}, {'ion_id': 1313, 'distance': 10.91519832611084, 'force': [0.6676040887832642, -0.2546995282173157, -2.6934328079223633], 'magnitude': 2.7866015434265137}, {'ion_id': 1460, 'distance': 14.24957275390625, 'force': [0.2775050699710846, -0.13799616694450378, -1.6054214239120483], 'magnitude': 1.6350626945495605}, {'ion_id': 2433, 'distance': 7.270791053771973, 'force': [2.2770705223083496, -0.8435057401657104, -5.791769504547119], 'magnitude': 6.280218601226807}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.731081485748291, 'force': [0.8560025691986084, 16.429052352905273, 4.301031589508057], 'magnitude': 17.004276275634766}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.700852632522583, 'force': [-7.190485000610352, -24.634323120117188, -8.373350143432617], 'magnitude': 26.993812561035156}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.7179975509643555, 'force': [-2.3188703060150146, -13.459009170532227, -1.1819517612457275], 'magnitude': 13.708358764648438}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.948777198791504, 'force': [2.0353517532348633, 5.309359073638916, 0.15524470806121826], 'magnitude': 5.688238143920898}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.550324440002441, 'force': [0.26686999201774597, 4.502148151397705, 0.32941505312919617], 'magnitude': 4.522065162658691}]}, 2500: {'frame': 2500, 'ionic_force': [10.757028341293335, 3.463405579328537, -10.93871683627367], 'ionic_force_magnitude': 15.727821303870703, 'motion_vector': [-0.6099472045898438, -2.023162841796875, 0.6139450073242188], 'ionic_force_x': 10.757028341293335, 'ionic_force_y': 3.463405579328537, 'ionic_force_z': -10.93871683627367, 'radial_force': 11.300833462285517, 'axial_force': -10.93871683627367, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [9.913759469985962, 5.442253589630127, -2.4253696501255035], 'asn_force_magnitude': 11.56646743402359, 'residue_force': [9.913759469985962, 5.442253589630127, -2.4253696501255035], 'residue_force_magnitude': 11.56646743402359, 'total_force': [20.670787811279297, 8.905659168958664, -13.364086486399174], 'total_force_magnitude': 26.176154064120023, 'motion_component_total': -17.646305668873342, 'cosine_total_motion': -0.6741366827857019, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.7286878344692552, 'cosine_residue_motion': -0.7286878344692552, 'cosine_ionic_motion': -0.5860927196347875, 'motion_component_glu': None, 'motion_component_asn': -8.428344106957812, 'motion_component_residue': -8.428344106957812, 'motion_component_ionic': -9.21796156191553, 'ionic_contributions': [{'ion_id': 1306, 'distance': 10.85891342163086, 'force': [1.5857772827148438, 2.3122644424438477, -0.25718116760253906], 'magnitude': 2.815563678741455}, {'ion_id': 1307, 'distance': 9.445901870727539, 'force': [2.9505650997161865, -2.2636144161224365, 0.12457256764173508], 'magnitude': 3.7209277153015137}, {'ion_id': 1313, 'distance': 10.672607421875, 'force': [0.8667038679122925, 0.6107208728790283, -2.715040445327759], 'magnitude': 2.9147214889526367}, {'ion_id': 1460, 'distance': 14.710773468017578, 'force': [0.34449779987335205, 0.28117606043815613, -1.4682879447937012], 'magnitude': 1.5341473817825317}, {'ion_id': 2433, 'distance': 6.185005187988281, 'force': [5.00948429107666, 2.5228586196899414, -6.622779846191406], 'magnitude': 8.678765296936035}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.7058541774749756, 'force': [-7.429487228393555, -14.820969581604004, 4.7160420417785645], 'magnitude': 17.236574172973633}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.851870536804199, 'force': [15.849732398986816, 17.377857208251953, -5.740339756011963], 'magnitude': 24.210647583007812}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.658753395080566, 'force': [6.029250621795654, 12.662135124206543, -0.9901033639907837], 'magnitude': 14.059226036071777}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.696172714233398, 'force': [-3.002795696258545, -5.488577365875244, -0.8709450960159302], 'magnitude': 6.316629409790039}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.516839981079102, 'force': [-1.5329406261444092, -4.288191795349121, 0.45997652411460876], 'magnitude': 4.577125072479248}]}, 2502: {'frame': 2502, 'ionic_force': [11.108901798725128, 4.885472863912582, -9.020216885954142], 'ionic_force_magnitude': 15.120841806837237, 'motion_vector': [1.0041885375976562, -1.8047294616699219, -0.99957275390625], 'ionic_force_x': 11.108901798725128, 'ionic_force_y': 4.885472863912582, 'ionic_force_z': -9.020216885954142, 'radial_force': 12.135713587496394, 'axial_force': -9.020216885954142, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [11.695576667785645, 3.224666118621826, -7.130850836634636], 'asn_force_magnitude': 14.072456033790704, 'residue_force': [11.695576667785645, 3.224666118621826, -7.130850836634636], 'residue_force_magnitude': 14.072456033790704, 'total_force': [22.804478466510773, 8.110138982534409, -16.151067722588778], 'total_force_magnitude': 29.097690303961016, 'motion_component_total': 10.637561645192266, 'cosine_total_motion': 0.3655809630960363, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.40424890558602117, 'cosine_residue_motion': 0.40424890558602117, 'cosine_ionic_motion': 0.3272824858459445, 'motion_component_glu': None, 'motion_component_asn': 5.688774950567292, 'motion_component_residue': 5.688774950567292, 'motion_component_ionic': 4.948786694624974, 'ionic_contributions': [{'ion_id': 1306, 'distance': 10.935221672058105, 'force': [1.6125199794769287, 2.259916067123413, -0.03140765801072121], 'magnitude': 2.7764055728912354}, {'ion_id': 1307, 'distance': 8.901533126831055, 'force': [3.5420584678649902, -2.151763916015625, 0.6159398555755615], 'magnitude': 4.189945697784424}, {'ion_id': 1313, 'distance': 10.70211124420166, 'force': [1.0196746587753296, 0.8430778980255127, -2.579105854034424], 'magnitude': 2.8986728191375732}, {'ion_id': 1460, 'distance': 14.046440124511719, 'force': [0.4846588969230652, 0.40232810378074646, -1.56035315990448], 'magnitude': 1.6826955080032349}, {'ion_id': 2433, 'distance': 6.489561557769775, 'force': [4.4499897956848145, 3.531914710998535, -5.465290069580078], 'magnitude': 7.8832879066467285}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.520566940307617, 'force': [-10.391767501831055, -13.442659378051758, 8.721470832824707], 'magnitude': 19.0986385345459}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.628633499145508, 'force': [20.62630844116211, 14.287422180175781, -13.510346412658691], 'magnitude': 28.497447967529297}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.244329929351807, 'force': [9.724801063537598, 13.384598731994629, -3.6336734294891357], 'magnitude': 16.938796997070312}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.106366157531738, 'force': [-5.748861789703369, -5.9306135177612305, 0.17484469711780548], 'magnitude': 8.261486053466797}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.912648677825928, 'force': [-2.5149035453796387, -5.074081897735596, 1.1168534755706787], 'magnitude': 5.772210121154785}]}, 2503: {'frame': 2503, 'ionic_force': [10.486082792282104, 2.2957146763801575, -9.244423501193523], 'ionic_force_magnitude': 14.16642523967713, 'motion_vector': [0.7024688720703125, -0.047672271728515625, 0.34432220458984375], 'ionic_force_x': 10.486082792282104, 'ionic_force_y': 2.2957146763801575, 'ionic_force_z': -9.244423501193523, 'radial_force': 10.7344416809605, 'axial_force': -9.244423501193523, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-1.5346150398254395, 16.07801342010498, -3.536777164787054], 'asn_force_magnitude': 16.533794227910708, 'residue_force': [-1.5346150398254395, 16.07801342010498, -3.536777164787054], 'residue_force_magnitude': 16.533794227910708, 'total_force': [8.951467752456665, 18.373728096485138, -12.781200665980577], 'total_force_magnitude': 24.105637298169516, 'motion_component_total': 1.29038017695438, 'cosine_total_motion': 0.053530224527702744, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.2363118005060805, 'cosine_residue_motion': -0.2363118005060805, 'cosine_ionic_motion': 0.3668893720338059, 'motion_component_glu': None, 'motion_component_asn': -3.9071306831946204, 'motion_component_residue': -3.9071306831946204, 'motion_component_ionic': 5.197510860149, 'ionic_contributions': [{'ion_id': 1306, 'distance': 10.291056632995605, 'force': [2.275625705718994, 2.12125301361084, -0.38621312379837036], 'magnitude': 3.134860038757324}, {'ion_id': 1307, 'distance': 11.276666641235352, 'force': [2.049074649810791, -1.6138296127319336, 0.11496884375810623], 'magnitude': 2.6108181476593018}, {'ion_id': 1313, 'distance': 11.264599800109863, 'force': [1.04147207736969, 0.32502686977386475, -2.378091335296631], 'magnitude': 2.6164145469665527}, {'ion_id': 1460, 'distance': 14.645037651062012, 'force': [0.4698096513748169, 0.164600670337677, -1.465720534324646], 'magnitude': 1.5479506254196167}, {'ion_id': 2433, 'distance': 6.865213394165039, 'force': [4.6501007080078125, 1.2986637353897095, -5.129367351531982], 'magnitude': 7.044172763824463}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.886817693710327, 'force': [1.5360503196716309, -15.122956275939941, 3.8015801906585693], 'magnitude': 15.668927192687988}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.697760820388794, 'force': [-3.6142938137054443, 25.845338821411133, -7.13914155960083], 'magnitude': 27.055721282958984}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.610356330871582, 'force': [0.7917301058769226, 14.330216407775879, -0.33359259366989136], 'magnitude': 14.355947494506836}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.458778381347656, 'force': [-0.6242847442626953, -6.846532821655273, -1.3547999858856201], 'magnitude': 7.007155418395996}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.596306800842285, 'force': [-0.2617737352848053, -4.4305877685546875, 0.2942676842212677], 'magnitude': 4.448058605194092}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.860004901885986, 'force': [2.168656587600708, 6.463316917419434, 1.0203067064285278], 'magnitude': 6.893371105194092}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.896365165710449, 'force': [-1.6073572635650635, -8.625304222106934, 0.2264678180217743], 'magnitude': 8.776717185974121}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.585378646850586, 'force': [0.0766575038433075, 4.464522361755371, -0.05186542496085167], 'magnitude': 4.465481281280518}]}, 2504: {'frame': 2504, 'ionic_force': [10.3755504488945, 1.9541607946157455, -7.793602168560028], 'ionic_force_magnitude': 13.122919884330305, 'motion_vector': [-1.1085968017578125, 0.3018455505371094, 0.1440887451171875], 'ionic_force_x': 10.3755504488945, 'ionic_force_y': 1.9541607946157455, 'ionic_force_z': -7.793602168560028, 'radial_force': 10.557972889185127, 'axial_force': -7.793602168560028, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-3.3221406042575836, 14.862268924713135, -2.7153480648994446], 'asn_force_magnitude': 15.4692201</t>
+          <t>{2261: {'frame': 2261, 'motion_vector': [-1.0795135498046875, -0.78814697265625, 0.6654815673828125], 'ionic_force': [9.17229837179184, 1.028277650475502, -9.523530200123787], 'ionic_force_magnitude': 13.26220343006065, 'radial_force': 9.229756895370683, 'axial_force': -9.523530200123787, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [7.0570900440216064, 7.893163204193115, -6.501342058181763], 'asn_force_magnitude': 12.424652663754431, 'residue_force': [7.0570900440216064, 7.893163204193115, -6.501342058181763], 'residue_force_magnitude': 12.424652663754431, 'total_force': [16.229388415813446, 8.921440854668617, -16.02487225830555], 'total_force_magnitude': 24.490440709993376, 'cosine_total_motion': -0.9630398345728705, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.9792086757705155, 'cosine_residue_motion': -0.9792086757705155, 'cosine_ionic_motion': -0.8610139595885321, 'motion_component_total': -23.585269969968714, 'motion_component_glu': None, 'motion_component_asn': -12.166327681783585, 'motion_component_residue': -12.166327681783585, 'motion_component_ionic': -11.418942288185132, 'motion_component_percent_total': 96.30398345728705, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 97.92086757705155, 'motion_component_percent_residue': 97.92086757705155, 'motion_component_percent_ionic': 86.10139595885322, 'ionic_contributions': [{'ion_id': 1306, 'distance': 11.144904136657715, 'force': [1.5889837741851807, 2.148843765258789, -0.045660361647605896], 'magnitude': 2.6729166507720947, 'cosine_ionic_motion': -0.8617754578590393, 'motion_component_ionic': -2.3034539222717285, 'motion_component_percent_ionic': 86.17754578590393}, {'ion_id': 1307, 'distance': 9.503464698791504, 'force': [2.269397735595703, -2.8564016819000244, 0.45132771134376526], 'magnitude': 3.6759889125823975, 'cosine_ionic_motion': 0.018541615456342697, 'motion_component_ionic': 0.06815877556800842, 'motion_component_percent_ionic': 1.8541615456342697}, {'ion_id': 1313, 'distance': 10.139678955078125, 'force': [1.2523084878921509, 0.40465953946113586, -2.948805570602417], 'magnitude': 3.229161024093628, 'cosine_ionic_motion': -0.7535384297370911, 'motion_component_ionic': -2.4332969188690186, 'motion_component_percent_ionic': 75.3538429737091}, {'ion_id': 1460, 'distance': 13.783182144165039, 'force': [0.5171981453895569, 0.2051517814397812, -1.6566481590270996], 'magnitude': 1.7475881576538086, 'cosine_ionic_motion': -0.6984426975250244, 'motion_component_ionic': -1.2205902338027954, 'motion_component_percent_ionic': 69.84426975250244}, {'ion_id': 2433, 'distance': 7.150071144104004, 'force': [3.544410228729248, 1.1260242462158203, -5.32374382019043], 'magnitude': 6.494075775146484, 'cosine_ionic_motion': -0.851508378982544, 'motion_component_ionic': -5.529759883880615, 'motion_component_percent_ionic': 85.1508378982544}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.8561618328094482, 'force': [-4.236083507537842, -14.082409858703613, 6.095686912536621], 'magnitude': 15.919047355651855, 'cosine_with_motion': 0.8300103545188904, 'motion_component': 13.212974548339844, 'motion_component_percent': 83.00103545188904}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.8134114742279053, 'force': [11.147245407104492, 19.2869873046875, -11.073408126831055], 'magnitude': 24.877084732055664, 'cosine_with_motion': -0.9316018223762512, 'motion_component': -23.175537109375, 'motion_component_percent': 93.16018223762512}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.667447090148926, 'force': [4.180720329284668, 13.239962577819824, -1.8488456010818481], 'magnitude': 14.006900787353516, 'cosine_with_motion': -0.7735787630081177, 'motion_component': -10.835440635681152, 'motion_component_percent': 77.35787630081177}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.459536552429199, 'force': [-2.9634432792663574, -6.3406453132629395, -0.2847350239753723], 'magnitude': 7.0047736167907715, 'cosine_with_motion': 0.7655612826347351, 'motion_component': 5.362583637237549, 'motion_component_percent': 76.55612826347351}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.634800434112549, 'force': [-1.0713489055633545, -4.210731506347656, 0.6099597811698914], 'magnitude': 4.38749361038208, 'cosine_with_motion': 0.7450931668281555, 'motion_component': 3.2690916061401367, 'motion_component_percent': 74.50931668281555}]}, 2265: {'frame': 2265, 'motion_vector': [0.6828193664550781, 0.2771263122558594, 0.02298736572265625], 'ionic_force': [9.130726605653763, 1.9627961963415146, -10.302303045988083], 'ionic_force_magnitude': 13.905401299744698, 'radial_force': 9.339311390866364, 'axial_force': -10.302303045988083, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [3.032887816429138, 11.611568927764893, -6.067251920700073], 'asn_force_magnitude': 13.447620136682852, 'residue_force': [3.032887816429138, 11.611568927764893, -6.067251920700073], 'residue_force_magnitude': 13.447620136682852, 'total_force': [12.163614422082901, 13.574365124106407, -16.369554966688156], 'total_force_magnitude': 24.498555756188658, 'cosine_total_motion': 0.6472711462317507, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.5193695335500276, 'cosine_residue_motion': 0.5193695335500276, 'cosine_ionic_motion': 0.638091909490355, 'motion_component_total': 15.857208265330689, 'motion_component_glu': None, 'motion_component_asn': 6.9842841977469305, 'motion_component_residue': 6.9842841977469305, 'motion_component_ionic': 8.872924067583758, 'motion_component_percent_total': 64.72711462317507, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 51.93695335500276, 'motion_component_percent_residue': 51.93695335500276, 'motion_component_percent_ionic': 63.8091909490355, 'ionic_contributions': [{'ion_id': 1306, 'distance': 10.167248725891113, 'force': [1.7125273942947388, 2.7137768268585205, 0.13229718804359436], 'magnitude': 3.211671829223633, 'cosine_ionic_motion': 0.8127316236495972, 'motion_component_ionic': 2.610227346420288, 'motion_component_percent_ionic': 81.27316236495972}, {'ion_id': 1307, 'distance': 9.260034561157227, 'force': [2.3590493202209473, -3.053358554840088, 0.3204958438873291], 'magnitude': 3.8717992305755615, 'cosine_ionic_motion': 0.27044573426246643, 'motion_component_ionic': 1.0471116304397583, 'motion_component_percent_ionic': 27.044573426246643}, {'ion_id': 1313, 'distance': 10.266485214233398, 'force': [1.0728236436843872, 0.4622923731803894, -2.925252676010132], 'magnitude': 3.14988374710083, 'cosine_ionic_motion': 0.341647207736969, 'motion_component_ionic': 1.0761489868164062, 'motion_component_percent_ionic': 34.1647207736969}, {'ion_id': 1460, 'distance': 13.558910369873047, 'force': [0.4920254051685333, 0.18344132602214813, -1.7278474569320679], 'magnitude': 1.8058784008026123, 'cosine_ionic_motion': 0.26068514585494995, 'motion_component_ionic': 0.4707656502723694, 'motion_component_percent_ionic': 26.068514585494995}, {'ion_id': 2433, 'distance': 6.779136657714844, 'force': [3.4943008422851562, 1.6566442251205444, -6.101995944976807], 'magnitude': 7.224193096160889, 'cosine_ionic_motion': 0.5078311562538147, 'motion_component_ionic': 3.668670415878296, 'motion_component_percent_ionic': 50.78311562538147}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.9743127822875977, 'force': [-3.029351234436035, -13.51841926574707, 5.716115474700928], 'magnitude': 14.986614227294922, 'cosine_with_motion': -0.514372706413269, 'motion_component': -7.708705425262451, 'motion_component_percent': 51.437270641326904}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.7652649879455566, 'force': [5.912781238555908, 22.921756744384766, -10.136136054992676], 'magnitude': 25.750905990600586, 'cosine_with_motion': 0.5349674820899963, 'motion_component': 13.775897026062012, 'motion_component_percent': 53.496748208999634}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.7473063468933105, 'force': [4.9608964920043945, 12.30671215057373, -2.6936099529266357], 'magnitude': 13.539615631103516, 'cosine_with_motion': 0.6747882962226868, 'motion_component': 9.136374473571777, 'motion_component_percent': 67.47882962226868}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.4551544189453125, 'force': [-3.490391969680786, -6.0826497077941895, 0.2805880904197693], 'magnitude': 7.018560409545898, 'cosine_with_motion': -0.7850906848907471, 'motion_component': -5.51020622253418, 'motion_component_percent': 78.5090684890747}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.694264888763428, 'force': [-1.3210467100143433, -4.015830993652344, 0.7657905220985413], 'magnitude': 4.296335220336914, 'cosine_with_motion': -0.6305550932884216, 'motion_component': -2.709075927734375, 'motion_component_percent': 63.05550932884216}]}, 2266: {'frame': 2266, 'motion_vector': [-1.1436843872070312, -1.179443359375, 0.6229476928710938], 'ionic_force': [9.680621922016144, 1.6852705627679825, -9.65313646197319], 'ionic_force_magnitude': 13.774527985387671, 'radial_force': 9.826218889621371, 'axial_force': -9.65313646197319, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [1.8425058722496033, 9.913079738616943, -10.763621866703033], 'asn_force_magnitude': 14.74854343597427, 'residue_force': [1.8425058722496033, 9.913079738616943, -10.763621866703033], 'residue_force_magnitude': 14.74854343597427, 'total_force': [11.523127794265747, 11.598350301384926, -20.416758328676224], 'total_force_magnitude': 26.15622726098291, 'cosine_total_motion': -0.8611678169305217, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.791255363964706, 'cosine_residue_motion': -0.791255363964706, 'cosine_ionic_motion': -0.7880514698299226, 'motion_component_total': -22.52490112947925, 'motion_component_glu': None, 'motion_component_asn': -11.669864104381096, 'motion_component_residue': -11.669864104381096, 'motion_component_ionic': -10.855037025098156, 'motion_component_percent_total': 86.11678169305218, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 79.1255363964706, 'motion_component_percent_residue': 79.1255363964706, 'motion_component_percent_ionic': 78.80514698299226, 'ionic_contributions': [{'ion_id': 1306, 'distance': 11.234864234924316, 'force': [1.5262173414230347, 2.137537717819214, 0.14135095477104187], 'magnitude': 2.6302826404571533, 'cosine_ionic_motion': -0.904158353805542, 'motion_component_ionic': -2.3781919479370117, 'motion_component_percent_ionic': 90.4158353805542}, {'ion_id': 1307, 'distance': 9.184137344360352, 'force': [2.673102855682373, -2.871659517288208, 0.3172300457954407], 'magnitude': 3.936056613922119, 'cosine_ionic_motion': 0.07625913619995117, 'motion_component_ionic': 0.30016028881073, 'motion_component_percent_ionic': 7.625913619995117}, {'ion_id': 1313, 'distance': 10.04376220703125, 'force': [1.2430906295776367, 0.5733397603034973, -2.99291729927063], 'magnitude': 3.2911314964294434, 'cosine_ionic_motion': -0.6852173805236816, 'motion_component_ionic': -2.255140542984009, 'motion_component_percent_ionic': 68.52173805236816}, {'ion_id': 1460, 'distance': 13.551627159118652, 'force': [0.5830580592155457, 0.21003158390522003, -1.6982765197753906], 'magnitude': 1.8078199625015259, 'cosine_ionic_motion': -0.6209837794303894, 'motion_component_ionic': -1.1226269006729126, 'motion_component_percent_ionic': 62.09837794303894}, {'ion_id': 2433, 'distance': 7.01875638961792, 'force': [3.6551530361175537, 1.6360210180282593, -5.420523643493652], 'magnitude': 6.739346027374268, 'cosine_ionic_motion': -0.8011516332626343, 'motion_component_ionic': -5.399238109588623, 'motion_component_percent_ionic': 80.11516332626343}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.790710687637329, 'force': [-1.2962645292282104, -14.231207847595215, 8.195677757263184], 'magnitude': 16.473514556884766, 'cosine_with_motion': 0.807507336139679, 'motion_component': 13.302483558654785, 'motion_component_percent': 80.7507336139679}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.659165859222412, 'force': [3.3110499382019043, 21.939655303955078, -16.8265323638916], 'magnitude': 27.846790313720703, 'cosine_with_motion': -0.8205046653747559, 'motion_component': -22.848421096801758, 'motion_component_percent': 82.05046653747559}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.462449550628662, 'force': [3.25949764251709, 14.429506301879883, -3.996321439743042], 'magnitude': 15.323366165161133, 'cosine_with_motion': -0.8630373477935791, 'motion_component': -13.224637031555176, 'motion_component_percent': 86.30373477935791}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.120400428771973, 'force': [-2.7134130001068115, -7.720348358154297, 0.6005362868309021], 'magnitude': 8.205305099487305, 'cosine_with_motion': 0.872796893119812, 'motion_component': 7.161564826965332, 'motion_component_percent': 87.2796893119812}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.4251909255981445, 'force': [-0.7183641791343689, -4.504525661468506, 1.2630178928375244], 'magnitude': 4.733076572418213, 'cosine_with_motion': 0.8322591185569763, 'motion_component': 3.939146041870117, 'motion_component_percent': 83.22591185569763}]}, 2268: {'frame': 2268, 'motion_vector': [-0.18704986572265625, -0.371490478515625, -0.394805908203125], 'ionic_force': [10.473756790161133, 1.8430732190608978, -8.884076906368136], 'ionic_force_magnitude': 13.8572480193049, 'radial_force': 10.634683831231936, 'axial_force': -8.884076906368136, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-4.8723388612270355, 12.627479553222656, -6.10999259352684], 'asn_force_magnitude': 14.850081997707361, 'residue_force': [-4.8723388612270355, 12.627479553222656, -6.10999259352684], 'residue_force_magnitude': 14.850081997707361, 'total_force': [5.601417928934097, 14.470552772283554, -14.994069499894977], 'total_force_magnitude': 21.577648169291027, 'cosine_total_motion': -0.04070366409780388, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.16056266766432975, 'cosine_residue_motion': -0.16056266766432975, 'cosine_ionic_motion': 0.10868532015767929, 'motion_component_total': -0.8782893431034147, 'motion_component_glu': None, 'motion_component_asn': -2.384368780585933, 'motion_component_residue': -2.384368780585933, 'motion_component_ionic': 1.5060794374825202, 'motion_component_percent_total': 4.070366409780387, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 16.056266766432977, 'motion_component_percent_residue': 16.056266766432977, 'motion_component_percent_ionic': 10.86853201576793, 'ionic_contributions': [{'ion_id': 1306, 'distance': 11.470409393310547, 'force': [1.6078039407730103, 1.9444148540496826, -0.03991365805268288], 'magnitude': 2.5233659744262695, 'cosine_ionic_motion': -0.6961064338684082, 'motion_component_ionic': -1.7565313577651978, 'motion_component_percent_ionic': 69.61064338684082}, {'ion_id': 1307, 'distance': 10.841493606567383, 'force': [1.9502389430999756, -2.0432045459747314, 0.018825938925147057], 'magnitude': 2.8246188163757324, 'cosine_ionic_motion': 0.23879513144493103, 'motion_component_ionic': 0.6745052337646484, 'motion_component_percent_ionic': 23.879513144493103}, {'ion_id': 1313, 'distance': 10.89434814453125, 'force': [1.217636227607727, 0.36708852648735046, -2.491459369659424], 'magnitude': 2.7972776889801025, 'cosine_ionic_motion': 0.38619548082351685, 'motion_component_ionic': 1.0802960395812988, 'motion_component_percent_ionic': 38.619548082351685}, {'ion_id': 1460, 'distance': 14.645277976989746, 'force': [0.5479416847229004, 0.135992169380188, -1.441270112991333], 'magnitude': 1.5478997230529785, 'cosine_ionic_motion': 0.46865376830101013, 'motion_component_ionic': 0.7254290580749512, 'motion_component_percent_ionic': 46.86537683010101}, {'ion_id': 2433, 'distance': 6.756194591522217, 'force': [5.1501359939575195, 1.4387822151184082, -4.930259704589844], 'magnitude': 7.273338794708252, 'cosine_ionic_motion': 0.10756826400756836, 'motion_component_ionic': 0.7823804020881653, 'motion_component_percent_ionic': 10.756826400756836}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.8425087928771973, 'force': [2.948867082595825, -15.000923156738281, 4.828411102294922], 'magnitude': 16.03237533569336, 'cosine_with_motion': 0.33878791332244873, 'motion_component': 5.431574821472168, 'motion_component_percent': 33.87879133224487}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.6733570098876953, 'force': [-7.116278648376465, 24.974990844726562, -9.204205513000488], 'magnitude': 27.55193328857422, 'cosine_with_motion': -0.27297231554985046, 'motion_component': -7.5209150314331055, 'motion_component_percent': 27.297231554985046}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.470522880554199, 'force': [-0.9130064845085144, 15.211467742919922, -0.9442872405052185], 'magnitude': 15.268072128295898, 'cosine_with_motion': -0.5833121538162231, 'motion_component': -8.906051635742188, 'motion_component_percent': 58.331215381622314}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.171175956726074, 'force': [-0.24993082880973816, -7.921639919281006, -1.137224793434143], 'magnitude': 8.006754875183105, 'cosine_with_motion': 0.7488758563995361, 'motion_component': 5.996065616607666, 'motion_component_percent': 74.88758563995361}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.4605889320373535, 'force': [0.4580100178718567, -4.636415958404541, 0.34731385111808777], 'magnitude': 4.671911239624023, 'cosine_with_motion': 0.5597190260887146, 'motion_component': 2.614957571029663, 'motion_component_percent': 55.97190260887146}]}, 2269: {'frame': 2269, 'motion_vector': [-1.0145034790039062, 0.823699951171875, 0.27971649169921875], 'ionic_force': [12.215474724769592, 1.5210530683398247, -10.407313026487827], 'ionic_force_magnitude': 16.119664686943523, 'radial_force': 12.309810119908054, 'axial_force': -10.407313026487827, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-2.13426174223423, 10.67313814163208, -3.368392623960972], 'asn_force_magnitude': 11.393727214738856, 'residue_force': [-2.13426174223423, 10.67313814163208, -3.368392623960972], 'residue_force_magnitude': 11.393727214738856, 'total_force': [10.081212982535362, 12.194191209971905, -13.7757056504488], 'total_force_magnitude': 20.97854190911281, 'cosine_total_motion': -0.1439731265989746, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.6577022374570919, 'cosine_residue_motion': 0.6577022374570919, 'cosine_ionic_motion': -0.6522484404261935, 'motion_component_total': -3.0203462701425927, 'motion_component_glu': None, 'motion_component_asn': 7.493679882109505, 'motion_component_residue': 7.493679882109505, 'motion_component_ionic': -10.514026152252097, 'motion_component_percent_total': 14.39731265989746, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 65.77022374570919, 'motion_component_percent_residue': 65.77022374570919, 'motion_component_percent_ionic': 65.22484404261934, 'ionic_contributions': [{'ion_id': 1306, 'distance': 11.17204475402832, 'force': [1.694044589996338, 2.045954465866089, -0.13997234404087067], 'magnitude': 2.659945249557495, 'cosine_ionic_motion': -0.02039933018386364, 'motion_component_ionic': -0.05426110327243805, 'motion_component_percent_ionic': 2.039933018386364}, {'ion_id': 1307, 'distance': 11.321696281433105, 'force': [1.7108734846115112, -1.9433295726776123, 0.07040224224328995], 'magnitude': 2.5900914669036865, 'cosine_ionic_motion': -0.9582075476646423, 'motion_component_ionic': -2.4818451404571533, 'motion_component_percent_ionic': 95.82075476646423}, {'ion_id': 1313, 'distance': 9.32046127319336, 'force': [1.9830888509750366, 0.3941100537776947, -3.2431273460388184], 'magnitude': 3.821758508682251, 'cosine_ionic_motion': -0.5079683065414429, 'motion_component_ionic': -1.9413321018218994, 'motion_component_percent_ionic': 50.79683065414429}, {'ion_id': 1460, 'distance': 14.296980857849121, 'force': [0.5635555982589722, 0.1147402748465538, -1.5190082788467407], 'magnitude': 1.6242371797561646, 'cosine_ionic_motion': -0.41560065746307373, 'motion_component_ionic': -0.6750340461730957, 'motion_component_percent_ionic': 41.56006574630737}, {'ion_id': 2433, 'distance': 6.273693561553955, 'force': [6.263912200927734, 0.9095778465270996, -5.5756072998046875], 'magnitude': 8.435124397277832, 'cosine_ionic_motion': -0.6356223821640015, 'motion_component_ionic': -5.36155366897583, 'motion_component_percent_ionic': 63.56223821640015}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.8535971641540527, 'force': [1.6794264316558838, -15.571176528930664, 2.968061923980713], 'magnitude': 15.940244674682617, 'cosine_with_motion': -0.6430988311767578, 'motion_component': -10.251152992248535, 'motion_component_percent': 64.30988311767578}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.657850980758667, 'force': [-1.5747489929199219, 27.27834129333496, -5.512861728668213], 'magnitude': 27.87434959411621, 'cosine_with_motion': 0.6046738028526306, 'motion_component': 16.854888916015625, 'motion_component_percent': 60.46738028526306}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.67467737197876, 'force': [0.1745680421590805, 13.957775115966797, 0.36374419927597046], 'magnitude': 13.963604927062988, 'cosine_with_motion': 0.6120661497116089, 'motion_component': 8.546649932861328, 'motion_component_percent': 61.20661497116089}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.5912089347839355, 'force': [-0.7262468338012695, -6.408841133117676, -1.4404574632644653], 'magnitude': 6.6087517738342285, 'cosine_with_motion': -0.55991530418396, 'motion_component': -3.70034122467041, 'motion_component_percent': 55.991530418395996}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.642570495605469, 'force': [0.03614121675491333, -4.373770713806152, 0.11448761075735092], 'magnitude': 4.375418186187744, 'cosine_with_motion': -0.6169232726097107, 'motion_component': -2.6992974281311035, 'motion_component_percent': 61.69232726097107}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.983630657196045, 'force': [-2.079843044281006, -8.262550354003906, -0.1973496377468109], 'magnitude': 8.522583961486816, 'cosine_with_motion': -0.41714346408843994, 'motion_component': -3.555140256881714, 'motion_component_percent': 41.714346408843994}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.841239929199219, 'force': [0.3564414381980896, 4.053360462188721, 0.33598247170448303], 'magnitude': 4.082850456237793, 'cosine_with_motion': 0.5628595948219299, 'motion_component': 2.2980716228485107, 'motion_component_percent': 56.28595948219299}]}, 2270: {'frame': 2270, 'motion_vector': [0.494598388671875, -1.7763481140136719, 0.808197021484375], 'ionic_force': [11.086936205625534, 3.327737480401993, -11.238739222288132], 'ionic_force_magnitude': 16.133916154259637, 'radial_force': 11.575577357785766, 'axial_force': -11.238739222288132, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [1.0553871393203735, 16.747479915618896, -7.028375923633575], 'asn_force_magnitude': 18.193130397537782, 'residue_force': [1.0553871393203735, 16.747479915618896, -7.028375923633575], 'residue_force_magnitude': 18.193130397537782, 'total_force': [12.142323344945908, 20.07521739602089, -18.267115145921707], 'total_force_magnitude': 29.734455862939214, 'cosine_total_motion': -0.7419983510926893, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.9530445913907333, 'cosine_residue_motion': -0.9530445913907333, 'cosine_ionic_motion': -0.29280260600909885, 'motion_component_total': -22.062917220939244, 'motion_component_glu': None, 'motion_component_asn': -17.338864525839725, 'motion_component_residue': -17.338864525839725, 'motion_component_ionic': -4.72405269509952, 'motion_component_percent_total': 74.19983510926893, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 95.30445913907333, 'motion_component_percent_residue': 95.30445913907333, 'motion_component_percent_ionic': 29.280260600909884, 'ionic_contributions': [{'ion_id': 1306, 'distance': 10.51248836517334, 'force': [1.6320011615753174, 2.514735221862793, -0.19447630643844604], 'magnitude': 3.0041873455047607, 'cosine_ionic_motion': -0.6311010122299194, 'motion_component_ionic': -1.89594566822052, 'motion_component_percent_ionic': 63.11010122299194}, {'ion_id': 1307, 'distance': 10.130454063415527, 'force': [2.1316187381744385, -2.4281625747680664, 0.16044160723686218], 'magnitude': 3.235044479370117, 'cosine_ionic_motion': 0.844040036201477, 'motion_component_ionic': 2.7305071353912354, 'motion_component_percent_ionic': 84.4040036201477}, {'ion_id': 1313, 'distance': 10.578052520751953, 'force': [1.0888550281524658, 0.4178965389728546, -2.7282259464263916], 'magnitude': 2.967062473297119, 'cosine_ionic_motion': -0.40323740243911743, 'motion_component_ionic': -1.1964305639266968, 'motion_component_percent_ionic': 40.32374024391174}, {'ion_id': 1460, 'distance': 14.25514030456543, 'force': [0.45483729243278503, 0.18684375286102295, -1.5580334663391113], 'magnitude': 1.6337857246398926, 'cosine_ionic_motion': -0.4153349697589874, 'motion_component_ionic': -0.6785683631896973, 'motion_component_percent_ionic': 41.53349697589874}, {'ion_id': 2433, 'distance': 5.9453535079956055, 'force': [5.779623985290527, 2.6364245414733887, -6.918445110321045], 'magnitude': 9.392533302307129, 'cosine_ionic_motion': -0.3921854794025421, 'motion_component_ionic': -3.683615207672119, 'motion_component_percent_ionic': 39.21854794025421}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.7779879570007324, 'force': [-0.8482921123504639, -15.651665687561035, 5.418171405792236], 'magnitude': 16.58465576171875, 'cosine_with_motion': 0.9512698650360107, 'motion_component': 15.776483535766602, 'motion_component_percent': 95.12698650360107}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.6543116569519043, 'force': [2.7832577228546143, 25.383670806884766, -11.36021614074707], 'magnitude': 27.948734283447266, 'cosine_with_motion': -0.9400516152381897, 'motion_component': -26.273252487182617, 'motion_component_percent': 94.00516152381897}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.565553665161133, 'force': [2.400338649749756, 14.367148399353027, -1.458168864250183], 'magnitude': 14.63908576965332, 'cosine_with_motion': -0.8656375408172607, 'motion_component': -12.672142028808594, 'motion_component_percent': 86.56375408172607}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.482104778289795, 'force': [-1.9207251071929932, -6.633512020111084, -0.6272006034851074], 'magnitude': 6.934410572052002, 'cosine_with_motion': 0.7396817803382874, 'motion_component': 5.1292572021484375, 'motion_component_percent': 73.96817803382874}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.529580116271973, 'force': [-0.5192922949790955, -4.485893726348877, 0.6039515137672424], 'magnitude': 4.556057929992676, 'cosine_with_motion': 0.8939488530158997, 'motion_component': 4.072882652282715, 'motion_component_percent': 89.39488530158997}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.991696357727051, 'force': [-0.8398997187614441, 3.7677321434020996, 0.39508676528930664], 'magnitude': 3.880377769470215, 'cosine_with_motion': -0.8690118789672852, 'motion_component': -3.3720943927764893, 'motion_component_percent': 86.90118789672852}]}, 2492: {'frame': 2492, 'motion_vector': [-2.5311126708984375, 2.8303871154785156, 0.9147491455078125], 'ionic_force': [9.755406647920609, 0.5477147996425629, -11.056969352066517], 'ionic_force_magnitude': 14.755491236166263, 'radial_force': 9.770770203420051, 'axial_force': -11.056969352066517, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-6.351130992174149, -11.85277271270752, -4.769610553979874], 'asn_force_magnitude': 14.267945566741385, 'residue_force': [-6.351130992174149, -11.85277271270752, -4.769610553979874], 'residue_force_magnitude': 14.267945566741385, 'total_force': [3.40427565574646, -11.305057913064957, -15.82657990604639], 'total_force_magnitude': 19.74522875736141, 'cosine_total_motion': -0.7143749119833704, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.3918360759131695, 'cosine_residue_motion': -0.3918360759131695, 'cosine_ionic_motion': -0.5770597614904768, 'motion_component_total': -14.105496055631573, 'motion_component_glu': None, 'motion_component_asn': -5.590695802214648, 'motion_component_residue': -5.590695802214648, 'motion_component_ionic': -8.514800253416924, 'motion_component_percent_total': 71.43749119833704, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 39.18360759131695, 'motion_component_percent_residue': 39.18360759131695, 'motion_component_percent_ionic': 57.70597614904768, 'ionic_contributions': [{'ion_id': 1306, 'distance': 7.256741523742676, 'force': [4.944879055023193, 3.794395685195923, -0.9477364420890808], 'magnitude': 6.304559707641602, 'cosine_ionic_motion': -0.10735122859477997, 'motion_component_ionic': -0.6768022179603577, 'motion_component_percent_ionic': 10.735122859477997}, {'ion_id': 1307, 'distance': 11.3829984664917, 'force': [1.5883479118347168, -2.01047945022583, -0.018609173595905304], 'magnitude': 2.5622689723968506, 'cosine_ionic_motion': -0.9720533490180969, 'motion_component_ionic': -2.490662097930908, 'motion_component_percent_ionic': 97.20533490180969}, {'ion_id': 1313, 'distance': 10.91519832611084, 'force': [0.6676040887832642, -0.2546995282173157, -2.6934328079223633], 'magnitude': 2.7866015434265137, 'cosine_ionic_motion': -0.4478755593299866, 'motion_component_ionic': -1.2480506896972656, 'motion_component_percent_ionic': 44.78755593299866}, {'ion_id': 1460, 'distance': 14.24957275390625, 'force': [0.2775050699710846, -0.13799616694450378, -1.6054214239120483], 'magnitude': 1.6350626945495605, 'cosine_ionic_motion': -0.40111494064331055, 'motion_component_ionic': -0.6558480858802795, 'motion_component_percent_ionic': 40.111494064331055}, {'ion_id': 2433, 'distance': 7.270791053771973, 'force': [2.2770705223083496, -0.8435057401657104, -5.791769504547119], 'magnitude': 6.280218601226807, 'cosine_ionic_motion': -0.5482988953590393, 'motion_component_ionic': -3.443437099456787, 'motion_component_percent_ionic': 54.82988953590393}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.731081485748291, 'force': [0.8560025691986084, 16.429052352905273, 4.301031589508057], 'magnitude': 17.004276275634766, 'cosine_with_motion': 0.7267859578132629, 'motion_component': 12.358469009399414, 'motion_component_percent': 72.6785957813263}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.700852632522583, 'force': [-7.190485000610352, -24.634323120117188, -8.373350143432617], 'magnitude': 26.993812561035156, 'cosine_with_motion': -0.5613640546798706, 'motion_component': -15.153356552124023, 'motion_component_percent': 56.13640546798706}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.7179975509643555, 'force': [-2.3188703060150146, -13.459009170532227, -1.1819517612457275], 'magnitude': 13.708358764648438, 'cosine_with_motion': -0.6220719218254089, 'motion_component': -8.52758502960205, 'motion_component_percent': 62.207192182540894}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.948777198791504, 'force': [2.0353517532348633, 5.309359073638916, 0.15524470806121826], 'magnitude': 5.688238143920898, 'cosine_wit</t>
         </is>
       </c>
     </row>
@@ -515,7 +515,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>{3185: {'frame': 3185, 'ionic_force': [10.830740660429, 0.3619977980852127, -26.339956998825073], 'ionic_force_magnitude': 28.48208771068656, 'motion_vector': [3.3021926879882812, 1.7625465393066406, 0.34154510498046875], 'ionic_force_x': 10.830740660429, 'ionic_force_y': 0.3619977980852127, 'ionic_force_z': -26.339956998825073, 'radial_force': 10.83678853070819, 'axial_force': -26.339956998825073, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [8.105061918497086, -11.73450893163681, -7.371694318950176], 'asn_force_magnitude': 16.054052625470558, 'residue_force': [8.105061918497086, -11.73450893163681, -7.371694318950176], 'residue_force_magnitude': 16.054052625470558, 'total_force': [18.935802578926086, -11.372511133551598, -33.71165131777525], 'total_force_magnitude': 40.3035242052364, 'motion_component_total': 8.239864047768757, 'cosine_total_motion': 0.20444524915015247, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.05906475990435253, 'cosine_residue_motion': 0.05906475990435253, 'cosine_ionic_motion': 0.25600775329463143, 'motion_component_glu': None, 'motion_component_asn': 0.9482287638152589, 'motion_component_residue': 0.9482287638152589, 'motion_component_ionic': 7.291635283953498, 'ionic_contributions': [{'ion_id': 1306, 'distance': 4.375885963439941, 'force': [6.986976623535156, 8.647163391113281, -13.30506706237793], 'magnitude': 17.33828353881836}, {'ion_id': 1307, 'distance': 6.36940860748291, 'force': [2.498210906982422, -7.074841499328613, -3.267333745956421], 'magnitude': 8.183514595031738}, {'ion_id': 1313, 'distance': 6.8978657722473145, 'force': [1.0481852293014526, -0.9845649600028992, -6.827840805053711], 'magnitude': 6.9776411056518555}, {'ion_id': 1460, 'distance': 10.584712982177734, 'force': [0.2973679006099701, -0.2257591336965561, -2.9397153854370117], 'magnitude': 2.963329553604126}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.6301827430725098, 'force': [-6.580717086791992, 16.640785217285156, 1.5606398582458496], 'magnitude': 17.96265983581543}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.617792844772339, 'force': [13.598535537719727, -24.361940383911133, -6.871391773223877], 'magnitude': 28.733957290649414}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.141814708709717, 'force': [1.212706208229065, -17.740966796875, -0.435160756111145], 'magnitude': 17.787691116333008}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.6368229389190674, 'force': [1.6431950330734253, 10.392723083496094, 0.47288060188293457], 'magnitude': 10.532444953918457}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.140359401702881, 'force': [-0.31144198775291443, 5.2627949714660645, -0.03751295059919357], 'magnitude': 5.2721357345581055}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.496977806091309, 'force': [-5.725818634033203, -1.7442978620529175, -2.576413869857788], 'magnitude': 6.516554832458496}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.689517974853516, 'force': [4.2686028480529785, -0.18360716104507446, 0.5152645707130432], 'magnitude': 4.3035078048706055}]}, 3186: {'frame': 3186, 'ionic_force': [26.529620349407196, 4.835323363542557, -9.52608323097229], 'ionic_force_magnitude': 28.5997791886076, 'motion_vector': [-1.120147705078125, -0.510986328125, 0.8818283081054688], 'ionic_force_x': 26.529620349407196, 'ionic_force_y': 4.835323363542557, 'ionic_force_z': -9.52608323097229, 'radial_force': 26.966666607382177, 'axial_force': -9.52608323097229, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [6.062232851982117, 7.529888391494751, 1.958306908607483], 'asn_force_magnitude': 9.863308384528917, 'residue_force': [6.062232851982117, 7.529888391494751, 1.958306908607483], 'residue_force_magnitude': 9.863308384528917, 'total_force': [32.59185320138931, 12.365211755037308, -7.567776322364807], 'total_force_magnitude': 35.670696591364305, 'motion_component_total': -32.68559524290799, 'cosine_total_motion': -0.9163150251128264, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.5965909428690352, 'cosine_residue_motion': -0.5965909428690352, 'cosine_ionic_motion': -0.9371133468278592, 'motion_component_glu': None, 'motion_component_asn': -5.884360448934167, 'motion_component_residue': -5.884360448934167, 'motion_component_ionic': -26.801234793973823, 'ionic_contributions': [{'ion_id': 1306, 'distance': 3.9044389724731445, 'force': [20.750598907470703, 6.123347282409668, -2.4909238815307617], 'magnitude': 21.778141021728516}, {'ion_id': 1307, 'distance': 10.482446670532227, 'force': [1.9073935747146606, -2.2411868572235107, -0.6840906143188477], 'magnitude': 3.0214316844940186}, {'ion_id': 1313, 'distance': 8.069931030273438, 'force': [2.8922908306121826, 0.682626485824585, -4.142235279083252], 'magnitude': 5.0979838371276855}, {'ion_id': 1460, 'distance': 11.685558319091797, 'force': [0.9793370366096497, 0.2705364525318146, -2.2088334560394287], 'magnitude': 2.4313035011291504}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.986762523651123, 'force': [-3.3615376949310303, -14.398987770080566, -1.7819820642471313], 'magnitude': 14.89316177368164}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.037108898162842, 'force': [8.76229190826416, 19.110010147094727, 3.707000970840454], 'magnitude': 21.347414016723633}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.9858293533325195, 'force': [3.2005178928375244, 11.289494514465332, 3.603163003921509], 'magnitude': 12.275128364562988}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.024247646331787, 'force': [-1.8575721979141235, -4.551418304443359, -2.5078530311584473], 'magnitude': 5.518632888793945}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.816722869873047, 'force': [-0.6814670562744141, -3.919210195541382, -1.0620219707489014], 'magnitude': 4.117341041564941}]}, 3188: {'frame': 3188, 'ionic_force': [11.80595587193966, -1.4899064302444458, -16.767672687768936], 'ionic_force_magnitude': 20.56101317020206, 'motion_vector': [2.9478530883789062, -1.2035942077636719, 0.8451919555664062], 'ionic_force_x': 11.80595587193966, 'ionic_force_y': -1.4899064302444458, 'ionic_force_z': -16.767672687768936, 'radial_force': 11.89959727138151, 'axial_force': -16.767672687768936, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-9.493465304374695, -3.0462600626051426, -5.455596923828125], 'asn_force_magnitude': 11.365259418494242, 'residue_force': [-9.493465304374695, -3.0462600626051426, -5.455596923828125], 'residue_force_magnitude': 11.365259418494242, 'total_force': [2.3124905675649643, -4.536166492849588, -22.22326961159706], 'total_force_magnitude': 22.79908180839004, 'motion_component_total': -1.9749929026302495, 'cosine_total_motion': -0.08662598429308035, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.7726739540734446, 'cosine_residue_motion': -0.7726739540734446, 'cosine_ionic_motion': 0.33104628526733565, 'motion_component_glu': None, 'motion_component_asn': -8.781639933958404, 'motion_component_residue': -8.781639933958404, 'motion_component_ionic': 6.806647031328156, 'ionic_contributions': [{'ion_id': 1306, 'distance': 7.902102947235107, 'force': [0.704689621925354, 5.264189720153809, -0.24574843049049377], 'magnitude': 5.316829204559326}, {'ion_id': 1307, 'distance': 4.215550899505615, 'force': [11.88012981414795, -11.49898910522461, -8.6984281539917], 'magnitude': 18.682260513305664}, {'ion_id': 1313, 'distance': 7.252689838409424, 'force': [-0.5623465180397034, 3.5319478511810303, -5.200526714324951], 'magnitude': 6.311605930328369}, {'ion_id': 1460, 'distance': 10.703454971313477, 'force': [-0.21651704609394073, 1.2129451036453247, -2.622969388961792], 'magnitude': 2.897944688796997}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.9543068408966064, 'force': [9.581599235534668, -0.03208534047007561, 11.72050952911377], 'magnitude': 15.138640403747559}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.935325860977173, 'force': [-16.629323959350586, -3.5374836921691895, -15.272061347961426], 'magnitude': 22.853534698486328}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.479323863983154, 'force': [-6.031380653381348, -1.0252747535705566, -13.923310279846191], 'magnitude': 15.20813274383545}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.181246757507324, 'force': [1.7811845541000366, 1.6163733005523682, 7.596541881561279], 'magnitude': 7.96823263168335}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.400108337402344, 'force': [1.8044555187225342, -0.06778957694768906, 4.422723293304443], 'magnitude': 4.77714729309082}]}, 3189: {'frame': 3189, 'ionic_force': [12.04167953133583, 15.30772179365158, -8.939361959695816], 'ionic_force_magnitude': 21.429899315995037, 'motion_vector': [2.050933837890625, -1.666748046875, -0.683929443359375], 'ionic_force_x': 12.04167953133583, 'ionic_force_y': 15.30772179365158, 'ionic_force_z': -8.939361959695816, 'radial_force': 19.476354701206997, 'axial_force': -8.939361959695816, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [10.599079847335815, -1.189270257949829, 1.1911693885922432], 'asn_force_magnitude': 10.731902993829356, 'residue_force': [10.599079847335815, -1.189270257949829, 1.1911693885922432], 'residue_force_magnitude': 10.731902993829356, 'total_force': [22.640759378671646, 14.118451535701752, -7.748192571103573], 'total_force_magnitude': 27.78433276376764, 'motion_component_total': 10.330936865401501, 'cosine_total_motion': 0.371825983846322, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.7818501630954965, 'cosine_residue_motion': 0.7818501630954965, 'cosine_ionic_motion': 0.09053690503822516, 'motion_component_glu': None, 'motion_component_asn': 8.39074010605053, 'motion_component_residue': 8.39074010605053, 'motion_component_ionic': 1.940196759350969, 'ionic_contributions': [{'ion_id': 1306, 'distance': 4.907887935638428, 'force': [4.522043704986572, 13.012672424316406, 0.44386425614356995], 'magnitude': 13.783161163330078}, {'ion_id': 1307, 'distance': 7.745893955230713, 'force': [5.291672229766846, -1.454615592956543, -0.7079718708992004], 'magnitude': 5.5334367752075195}, {'ion_id': 1313, 'distance': 6.778944969177246, 'force': [1.8297994136810303, 3.0413978099823, -6.2925825119018555], 'magnitude': 7.2246012687683105}, {'ion_id': 1460, 'distance': 11.483993530273438, 'force': [0.39816418290138245, 0.7082671523094177, -2.38267183303833], 'magnitude': 2.517399787902832}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.5787932872772217, 'force': [-15.929393768310547, -8.559465408325195, 3.8187503814697266], 'magnitude': 18.48223114013672}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.848459243774414, 'force': [23.558996200561523, 5.480602741241455, -1.9761227369308472], 'magnitude': 24.2686710357666}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.693469524383545, 'force': [12.044590950012207, 6.841427326202393, -0.02992498129606247], 'magnitude': 13.852010726928711}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.8854546546936035, 'force': [-5.286684513092041, -2.261216640472412, -1.0021666288375854], 'magnitude': 5.836648941040039}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.466248512268066, 'force': [-3.788429021835327, -2.6906182765960693, 0.3806333541870117], 'magnitude': 4.662242412567139}]}, 3190: {'frame': 3190, 'ionic_force': [15.530074954032898, 11.720041185617447, -13.903977543115616], 'ionic_force_magnitude': 23.913661053672072, 'motion_vector': [-0.8215522766113281, -0.8835487365722656, -0.6362762451171875], 'ionic_force_x': 15.530074954032898, 'ionic_force_y': 11.720041185617447, 'ionic_force_z': -13.903977543115616, 'radial_force': 19.456171089668416, 'axial_force': -13.903977543115616, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [8.18987786769867, 3.4612741470336914, 1.6022478938102722], 'asn_force_magnitude': 9.034473782238994, 'residue_force': [8.18987786769867, 3.4612741470336914, 1.6022478938102722], 'residue_force_magnitude': 9.034473782238994, 'total_force': [23.719952821731567, 15.181315332651138, -12.301729649305344], 'total_force_magnitude': 30.731759621914886, 'motion_component_total': -18.382404112223956, 'cosine_total_motion': -0.5981565760756317, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.8769124628321204, 'cosine_residue_motion': -0.8769124628321204, 'cosine_ionic_motion': -0.437405273662284, 'motion_component_glu': None, 'motion_component_asn': -7.922442654775418, 'motion_component_residue': -7.922442654775418, 'motion_component_ionic': -10.459961457448536, 'ionic_contributions': [{'ion_id': 1306, 'distance': 4.505828857421875, 'force': [8.8020601272583, 11.90870189666748, -6.9365973472595215], 'magnitude': 16.352670669555664}, {'ion_id': 1307, 'distance': 9.605598449707031, 'force': [3.2317216396331787, -1.556819200515747, -0.28207412362098694], 'magnitude': 3.5982325077056885}, {'ion_id': 1313, 'distance': 7.852586269378662, 'force': [2.741168975830078, 1.0629887580871582, -4.5104899406433105], 'magnitude': 5.38409423828125}, {'ion_id': 1460, 'distance': 11.956610679626465, 'force': [0.7551242113113403, 0.3051697313785553, -2.174816131591797], 'magnitude': 2.3223190307617188}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.6500916481018066, 'force': [-8.962726593017578, -15.326889038085938, -0.6565071940422058], 'magnitude': 17.767244338989258}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.893784761428833, 'force': [16.062002182006836, 16.66604995727539, 4.144992828369141], 'magnitude': 23.514379501342773}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.771966457366943, 'force': [6.582432746887207, 11.42540454864502, 2.3859596252441406], 'magnitude': 13.400040626525879}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.9438042640686035, 'force': [-3.1666483879089355, -4.3073344230651855, -1.9762696027755737], 'magnitude': 5.699687480926514}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.423899173736572, 'force': [-1.6978040933609009, -4.361782550811768, -0.7181048393249512], 'magnitude': 4.735331058502197}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.702774524688721, 'force': [2.310697317123413, 6.742098808288574, 1.4780361652374268], 'magnitude': 7.278723239898682}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.810923099517822, 'force': [-2.938075304031372, -7.376273155212402, -3.055859088897705], 'magnitude': 8.507641792297363}]}, 3191: {'frame': 3191, 'ionic_force': [17.29844206571579, 1.1133021712303162, -8.736418187618256], 'ionic_force_magnitude': 19.41135086423247, 'motion_vector': [1.4482460021972656, 0.2650604248046875, 0.5260162353515625], 'ionic_force_x': 17.29844206571579, 'ionic_force_y': 1.1133021712303162, 'ionic_force_z': -8.736418187618256, 'radial_force': 17.334230286499363, 'axial_force': -8.736418187618256, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-0.12483274936676025, -8.143236875534058, -0.7974077761173248], 'asn_force_magnitude': 8.183138101473329, 'residue_force': [-0.12483274936676025, -8.143236875534058, -0.7974077761173248], 'residue_force_magnitude': 8.183138101473329, 'total_force': [17.17360931634903, -7.0299347043037415, -9.53382596373558], 'total_force_magnitude': 20.86256639064722, 'motion_component_total': 11.508740998012817, 'cosine_total_motion': 0.5516455062389752, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.21562519615260967, 'cosine_residue_motion': -0.21562519615260967, 'cosine_ionic_motion': 0.6837871227573488, 'motion_component_glu': None, 'motion_component_asn': -1.7644907582740803, 'motion_component_residue': -1.7644907582740803, 'motion_component_ionic': 13.273231756286897, 'ionic_contributions': [{'ion_id': 1306, 'distance': 5.4740495681762695, 'force': [10.922542572021484, 1.8332058191299438, -0.30494749546051025], 'magnitude': 11.079511642456055}, {'ion_id': 1307, 'distance': 10.684454917907715, 'force': [2.5171878337860107, -1.3357510566711426, -0.5809615254402161], 'magnitude': 2.9082610607147217}, {'ion_id': 1313, 'distance': 7.416356086730957, 'force': [2.9662954807281494, 0.4142634868621826, -5.240616798400879], 'magnitude': 6.036106586456299}, {'ion_id': 1460, 'distance': 10.956549644470215, 'force': [0.8924161791801453, 0.20158392190933228, -2.6098923683166504], 'magnitude': 2.7656068801879883}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.137293815612793, 'force': [-4.541301250457764, -7.616402626037598, -1.3473764657974243], 'magnitude': 8.969305038452148}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.479304790496826, 'force': [6.375889778137207, 7.045587539672852, 2.453929901123047], 'magnitude': 9.813972473144531}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.1367387771606445, 'force': [1.5254372358322144, 8.745102882385254, 1.2959271669387817], 'magnitude': 8.971242904663086}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.9513065814971924, 'force': [-2.616971015930176, -12.033166885375977, -2.7234742641448975], 'magnitude': 12.612016677856445}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.933863162994385, 'force': [-3.0954058170318604, -8.050671577453613, -0.840927243232727], 'magnitude': 8.666141510009766}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.632627010345459, 'force': [2.227518320083618, 3.7663137912750244, 0.3645131289958954], 'magnitude': 4.390880107879639}]}, 3192: {'frame': 3192, 'ionic_force': [14.277701735496521, 1.8772609233856201, -9.105208367109299], 'ionic_force_magnitude': 17.037655203423625, 'motion_vector': [-1.4279060363769531, -0.3152008056640625, 0.24273681640625], 'ionic_force_x': 14.277701735496521, 'ionic_force_y': 1.8772609233856201, 'ionic_force_z': -9.105208367109299, 'radial_force': 14.400585940241147, 'axial_force': -9.105208367109299, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [5.426489636301994, 5.107189655303955, -0.14802205562591553], 'asn_force_magnitude': 7.453327208508185, 'residue_force': [5.426489636301994, 5.107189655303955, -0.14802205562591553], 'residue_force_magnitude': 7.453327208508185, 'total_force': [19.704191371798515, 6.984450578689575, -9.253230422735214], 'total_force_magnitude': 22.8617580417353, 'motion_component_total': -21.981733151778457, 'cosine_total_motion': -0.9615066834164585, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.8503108684132783, 'cosine_residue_motion': -0.8503108684132783, 'cosine_ionic_motion': -0.9182066331169767, 'motion_component_glu': None, 'motion_component_asn': -6.33764513123491, 'motion_component_residue': -6.33764513123491, 'motion_component_ionic': -15.644088020543546, 'ionic_contributions': [{'ion_id': 1306, 'distance': 6.40054178237915, 'force': [7.416618824005127, 2.3804314136505127, -2.2368931770324707], 'magnitude': 8.104096412658691}, {'ion_id': 1307, 'distance': 10.719320297241211, 'force': [2.5377702713012695, -1.3266432285308838, -0.38498708605766296], 'magnitude': 2.8893728256225586}, {'ion_id': 1313, 'distance': 7.895941734313965, 'force': [3.2284295558929443, 0.5756868124008179, -4.195573329925537], 'magnitude': 5.325129985809326}, {'ion_id': 1460, 'distance': 11.41408634185791, 'force': [1.0948830842971802, 0.24778592586517334, -2.287754774093628], 'magnitude': 2.548330545425415}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.054739475250244, 'force': [-2.356449842453003, -14.174798011779785, -0.907854437828064], 'magnitude': 14.397984504699707}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.288381576538086, 'force': [7.63788366317749, 16.50430679321289, 0.9284068942070007], 'magnitude': 18.20965003967285}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.936164379119873, 'force': [1.7036049365997314, 11.97382926940918, 3.249650001525879], 'magnitude': 12.523381233215332}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.874608516693115, 'force': [-1.4094593524932861, -5.1374030113220215, -2.447693109512329], 'magnitude': 5.862651824951172}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.775841236114502, 'force': [-0.1490897685289383, -4.058745384216309, -0.9705314040184021], 'magnitude': 4.1758317947387695}]}, 3193: {'frame': 3193, 'ionic_force': [24.2664697766304, -1.6357786357402802, -8.331860184669495], 'ionic_force_magnitude': 25.70908830165204, 'motion_vector': [-1.265380859375, 0.5024642944335938, 1.421234130859375], 'ionic_force_x': 24.2664697766304, 'ionic_force_y': -1.6357786357402802, 'ionic_force_z': -8.331860184669495, 'radial_force': 24.32154039458153, 'axial_force': -8.331860184669495, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [4.683553457260132, 7.689526557922363, -0.025576263666152954], 'asn_force_magnitude': 9.0036184846577, 'residue_force': [4.683553457260132, 7.689526557922363, -0.025576263666152954], 'residue_force_magnitude': 9.0036184846577, 'total_force': [28.950023233890533, 6.053747922182083, -8.357436448335648], 'total_force_magnitude': 30.73432044370096, 'motion_component_total': -23.102493950159797, 'cosine_total_motion': -0.7516839030971542, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.11845788957196339, 'cosine_residue_motion': -0.11845788957196339, 'cosine_ionic_motion': -0.857126633484709, 'motion_component_glu': None, 'motion_component_asn': -1.0665496442036702, 'motion_component_residue': -1.0665496442036702, 'motion_component_ionic': -22.03594430595613, 'ionic_contributions': [{'ion_id': 1306, 'distance': 4.426405429840088, 'force': [16.86561393737793, 0.2729170322418213, 1.6130274534225464], 'magnitude': 16.94477081298828}, {'ion_id': 1307, 'distance': 9.166293144226074, 'force': [2.8553409576416016, -2.6237025260925293, -0.7594399452209473], 'magnitude': 3.9513967037200928}, {'ion_id': 1313, 'distance': 6.751701831817627, 'force': [3.558159112930298, 0.47408899664878845, -6.336966037750244], 'magnitude': 7.283020973205566}, {'ion_id': 1460, 'distance': 10.477368354797363, 'force': [0.9873557686805725, 0.2409178614616394, -2.8484816551208496], 'magnitude': 3.0243611335754395}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.573826313018799, 'force': [-4.482679843902588, -10.382486343383789, 0.38323065638542175], 'magnitude': 11.315357208251953}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.603158473968506, 'force': [8.293501853942871, 12.693092346191406, 0.3751336336135864], 'magnitude': 15.166986465454102}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.661822319030762, 'force': [4.1384501457214355, 8.515083312988281, 0.988288164138794], 'magnitude': 9.518935203552246}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.646981239318848, 'force': [-2.074617862701416, -3.6613059043884277, -1.1727513074874878], 'magnitude': 4.36858606338501}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.745528221130371, 'force': [1.4980759620666504, 6.869321823120117, 1.4101687669754028], 'magnitude': 7.170801162719727}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.237707614898682, 'force': [-2.6891767978668213, -6.344178676605225, -2.00964617729187], 'magnitude': 7.177670478820801}]}, 3195: {'frame': 3195, 'ionic_force': [13.184819161891937, 8.239660143852234, -7.467395126819611], 'ionic_force_magnitude': 17.247998306992876, 'motion_vector': [-2.6438636779785156, 0.3204536437988281, -0.75738525390625], 'ionic_force_x': 13.184819161891937, 'ionic_force_y': 8.239660143852234, 'ionic_force_z': -7.467395126819611, 'radial_force': 15.547715446906654, 'axial_force': -7.467395126819611, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [10.147289276123047, 0.8621158599853516, 4.081506751477718], 'asn_force_magnitude': 10.97129986700383, 'residue_force': [10.147289276123047, 0.8621158599853516, 4.081506751477718], 'residue_force_magnitude': 10.97129986700383, 'total_force': [23.332108438014984, 9.101776003837585, -3.3858883753418922], 'total_force_magnitude': 25.272393054034257, 'motion_component_total': -20.299583084250834, 'cosine_total_motion': -0.8032315357255173, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.97582263852606, 'cosine_residue_motion': -0.97582263852606, 'cosine_ionic_motion': -0.5562118066814178, 'motion_component_glu': None, 'motion_component_asn': -10.706042784280289, 'motion_component_residue': -10.706042784280289, 'motion_component_ionic': -9.593540299970543, 'ionic_contributions': [{'ion_id': 1306, 'distance': 6.083889961242676, 'force': [5.561399459838867, 6.935168266296387, 1.1953492164611816], 'magnitude': 8.969647407531738}, {'ion_id': 1307, 'distance': 9.575628280639648, 'force': [3.3571889400482178, -1.2759623527526855, -0.45971280336380005], 'magnitude': 3.6207916736602783}, {'ion_id': 1313, 'distance': 6.99928617477417, 'force': [3.318345785140991, 1.9544174671173096, -5.576297760009766], 'magnitude': 6.776891708374023}, {'ion_id': 1460, 'distance': 10.770756721496582, 'force': [0.9478849768638611, 0.6260367631912231, -2.6267337799072266], 'magnitude': 2.8618416786193848}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.5273516178131104, 'force': [-12.970773696899414, -13.918174743652344, -0.05629340559244156], 'magnitude': 19.025238037109375}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.842782735824585, 'force': [20.532848358154297, 12.34808349609375, 4.428743362426758], 'magnitude': 24.36568832397461}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.631701469421387, 'force': [9.123636245727539, 10.735398292541504, 1.9572348594665527], 'magnitude': 14.223933219909668}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.896658897399902, 'force': [-3.866205930709839, -3.9082860946655273, -1.879759430885315], 'magnitude': 5.809969425201416}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.19757080078125, 'force': [-2.672215700149536, -4.394905090332031, -0.3684186339378357], 'magnitude': 5.156710147857666}]}, 3196: {'frame': 3196, 'ionic_force': [6.619435306638479, 22.22155737876892, -13.786656141281128], 'ionic_force_magnitude': 26.975663544658474, 'motion_vector': [2.318988800048828, -2.4310836791992188, 0.22534942626953125], 'ionic_force_x': 6.619435306638479, 'ionic_force_y': 22.22155737876892, 'ionic_force_z': -13.786656141281128, 'radial_force': 23.186516256580926, 'axial_force': -13.786656141281128, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-1.7153337001800537, -4.505590200424194, -2.48662531375885], 'asn_force_magnitude': 5.4245753942735675, 'residue_force': [-1.7153337001800537, -4.505590200424194, -2.48662531375885], 'residue_force_magnitude': 5.4245753942735675, 'total_force': [4.9041016064584255, 17.715967178344727, -16.273281455039978], 'total_force_magnitude': 24.550466287742964, 'motion_component_total': -10.50209204771151, 'cosine_total_motion': -0.42777566522045135, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.3512110515384187, 'cosine_residue_motion': 0.3512110515384187, 'cosine_ionic_motion': -0.45994282422537697, 'motion_component_glu': None, 'motion_component_asn': 1.9051708283722517, 'motion_component_residue': 1.9051708283722517, 'motion_component_ionic': -12.407262876083761, 'ionic_contributions': [{'ion_id': 1306, 'distance': 3.882166862487793, 'force': [0.034611787647008896, 21.819107055664062, -3.03163743019104], 'magnitude': 22.02874183654785}, {'ion_id': 1307, 'distance': 6.965738296508789, 'force': [5.983163833618164, -2.2468509674072266, -2.4435293674468994], 'magnitude': 6.8423261642456055}, {'ion_id': 1313, 'distance': 7.424468994140625, 'force': [0.49341556429862976, 2.0448687076568604, -5.6436381340026855], 'magnitude': 6.022922515869141}, {'ion_id': 1460, 'distance': 11.01244068145752, 'force': [0.10824412107467651, 0.6044325828552246, -2.667851209640503], 'magnitude': 2.7376058101654053}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.898651599884033, 'force': [8.349928855895996, -3.975731372833252, 3.4322502613067627], 'magnitude': 9.864486694335938}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.3155388832092285, 'force': [-8.677992820739746, 2.6388981342315674, -5.432845115661621], 'magnitude': 10.572943687438965}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.494718074798584, 'force': [-11.389640808105469, 9.417529106140137, -3.1178841590881348], 'magnitude': 15.104137420654297}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.6145095825195312, 'force': [7.17305850982666, -7.618627548217773, 2.049612522125244], 'magnitude': 10.662887573242188}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.333044052124023, 'force': [3.5914595127105713, -3.2912018299102783, 0.5102007389068604], 'magnitude': 4.898050308227539}, {'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.7371015548706055, 'force': [-6.409738063812256, -2.9606735706329346, -1.3685144186019897], 'magnitude': 7.1918816566467285}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.743947505950928, 'force': [5.6475911140441895, 1.2842168807983398, 1.4405548572540283], 'magnitude': 5.968224048614502}]}, 3197: {'frame': 3197, 'ionic_force': [16.769740521907806, 8.663859937340021, -10.408290982246399], 'ionic_force_magnitude': 21.555026962568938, 'motion_vector': [-2.359294891357422, 1.4584197998046875, 2.7145614624023438], 'ionic_force_x': 16.769740521907806, 'ionic_force_y': 8.663859937340021, 'ionic_force_z': -10.408290982246399, 'radial_force': 18.87555737418003, 'axial_force': -10.408290982246399, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-0.717125654220581, -8.19782304763794, 0.9059391021728516], 'asn_force_magnitude': 8.278846391929907, 'residue_force': [-0.717125654220581, -8.19782304763794, 0.9059391021728516], 'residue_force_magnitude': 8.278846391929907, 'total_force': [16.052614867687225, 0.4660368897020817, -9.502351880073547], 'total_force_magnitude': 18.66007303644853, 'motion_component_total': -16.229840272209287, 'cosine_total_motion': -0.8697629554025703, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.24290987333967784, 'cosine_residue_motion': -0.24290987333967784, 'cosine_ionic_motion': -0.6596524684677239, 'motion_component_glu': None, 'motion_component_asn': -2.0110135284623425, 'motion_component_residue': -2.0110135284623425, 'motion_component_ionic': -14.218826743746943, 'ionic_contributions': [{'ion_id': 1306, 'distance': 4.667008399963379, 'force': [11.251453399658203, 10.151823997497559, -1.6383306980133057], 'magnitude': 15.242666244506836}, {'ion_id': 1307, 'distance': 10.15230655670166, 'force': [2.6972978115081787, -1.6630486249923706, -0.5784024000167847], 'magnitude': 3.221132516860962}, {'ion_id': 1313, 'distance': 7.379036903381348, 'force': [2.2362687587738037, 0.05940436199307442, -5.672110557556152], 'magnitude': 6.097315788269043}, {'ion_id': 1460, 'distance': 11.</t>
+          <t>{3185: {'frame': 3185, 'motion_vector': [3.3021926879882812, 1.7625465393066406, 0.34154510498046875], 'ionic_force': [10.830740660429, 0.3619977980852127, -26.339956998825073], 'ionic_force_magnitude': 28.48208771068656, 'radial_force': 10.83678853070819, 'axial_force': -26.339956998825073, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [8.105061918497086, -11.73450893163681, -7.371694318950176], 'asn_force_magnitude': 16.054052625470558, 'residue_force': [8.105061918497086, -11.73450893163681, -7.371694318950176], 'residue_force_magnitude': 16.054052625470558, 'total_force': [18.935802578926086, -11.372511133551598, -33.71165131777525], 'total_force_magnitude': 40.3035242052364, 'cosine_total_motion': 0.20444524915015247, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.05906475990435253, 'cosine_residue_motion': 0.05906475990435253, 'cosine_ionic_motion': 0.25600775329463143, 'motion_component_total': 8.239864047768757, 'motion_component_glu': None, 'motion_component_asn': 0.9482287638152589, 'motion_component_residue': 0.9482287638152589, 'motion_component_ionic': 7.291635283953498, 'motion_component_percent_total': 20.444524915015247, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 5.906475990435253, 'motion_component_percent_residue': 5.906475990435253, 'motion_component_percent_ionic': 25.600775329463143, 'ionic_contributions': [{'ion_id': 1306, 'distance': 4.375885963439941, 'force': [6.986976623535156, 8.647163391113281, -13.30506706237793], 'magnitude': 17.33828353881836, 'cosine_ionic_motion': 0.518176257610321, 'motion_component_ionic': 8.98428726196289, 'motion_component_percent_ionic': 51.817625761032104}, {'ion_id': 1307, 'distance': 6.36940860748291, 'force': [2.498210906982422, -7.074841499328613, -3.267333745956421], 'magnitude': 8.183514595031738, 'cosine_ionic_motion': -0.17347978055477142, 'motion_component_ionic': -1.419674277305603, 'motion_component_percent_ionic': 17.347978055477142}, {'ion_id': 1313, 'distance': 6.8978657722473145, 'force': [1.0481852293014526, -0.9845649600028992, -6.827840805053711], 'magnitude': 6.9776411056518555, 'cosine_ionic_motion': -0.02310800738632679, 'motion_component_ionic': -0.1612393856048584, 'motion_component_percent_ionic': 2.310800738632679}, {'ion_id': 1460, 'distance': 10.584712982177734, 'force': [0.2973679006099701, -0.2257591336965561, -2.9397153854370117], 'magnitude': 2.963329553604126, 'cosine_ionic_motion': -0.0377071313560009, 'motion_component_ionic': -0.1117386519908905, 'motion_component_percent_ionic': 3.77071313560009}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.6301827430725098, 'force': [-6.580717086791992, 16.640785217285156, 1.5606398582458496], 'magnitude': 17.96265983581543, 'cosine_with_motion': 0.120451420545578, 'motion_component': 2.163627862930298, 'motion_component_percent': 12.0451420545578}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.617792844772339, 'force': [13.598535537719727, -24.361940383911133, -6.871391773223877], 'magnitude': 28.733957290649414, 'cosine_with_motion': -0.0035273476969450712, 'motion_component': -0.10135465860366821, 'motion_component_percent': 0.3527347696945071}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.141814708709717, 'force': [1.212706208229065, -17.740966796875, -0.435160756111145], 'magnitude': 17.787691116333008, 'cosine_with_motion': -0.4100211560726166, 'motion_component': -7.29332971572876, 'motion_component_percent': 41.00211560726166}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.6368229389190674, 'force': [1.6431950330734253, 10.392723083496094, 0.47288060188293457], 'magnitude': 10.532444953918457, 'cosine_with_motion': 0.6038506627082825, 'motion_component': 6.3600239753723145, 'motion_component_percent': 60.38506627082825}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.140359401702881, 'force': [-0.31144198775291443, 5.2627949714660645, -0.03751295059919357], 'magnitude': 5.2721357345581055, 'cosine_with_motion': 0.41555044054985046, 'motion_component': 2.19083833694458, 'motion_component_percent': 41.555044054985046}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.496977806091309, 'force': [-5.725818634033203, -1.7442978620529175, -2.576413869857788], 'magnitude': 6.516554832458496, 'cosine_with_motion': -0.9333892464637756, 'motion_component': -6.08248233795166, 'motion_component_percent': 93.33892464637756}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.689517974853516, 'force': [4.2686028480529785, -0.18360716104507446, 0.5152645707130432], 'magnitude': 4.3035078048706055, 'cosine_with_motion': 0.8622978925704956, 'motion_component': 3.7109057903289795, 'motion_component_percent': 86.22978925704956}]}, 3186: {'frame': 3186, 'motion_vector': [-1.120147705078125, -0.510986328125, 0.8818283081054688], 'ionic_force': [26.529620349407196, 4.835323363542557, -9.52608323097229], 'ionic_force_magnitude': 28.5997791886076, 'radial_force': 26.966666607382177, 'axial_force': -9.52608323097229, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [6.062232851982117, 7.529888391494751, 1.958306908607483], 'asn_force_magnitude': 9.863308384528917, 'residue_force': [6.062232851982117, 7.529888391494751, 1.958306908607483], 'residue_force_magnitude': 9.863308384528917, 'total_force': [32.59185320138931, 12.365211755037308, -7.567776322364807], 'total_force_magnitude': 35.670696591364305, 'cosine_total_motion': -0.9163150251128264, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.5965909428690352, 'cosine_residue_motion': -0.5965909428690352, 'cosine_ionic_motion': -0.9371133468278592, 'motion_component_total': -32.68559524290799, 'motion_component_glu': None, 'motion_component_asn': -5.884360448934167, 'motion_component_residue': -5.884360448934167, 'motion_component_ionic': -26.801234793973823, 'motion_component_percent_total': 91.63150251128263, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 59.659094286903525, 'motion_component_percent_residue': 59.659094286903525, 'motion_component_percent_ionic': 93.71133468278592, 'ionic_contributions': [{'ion_id': 1306, 'distance': 3.9044389724731445, 'force': [20.750598907470703, 6.123347282409668, -2.4909238815307617], 'magnitude': 21.778141021728516, 'cosine_ionic_motion': -0.8662286400794983, 'motion_component_ionic': -18.864849090576172, 'motion_component_percent_ionic': 86.62286400794983}, {'ion_id': 1307, 'distance': 10.482446670532227, 'force': [1.9073935747146606, -2.2411868572235107, -0.6840906143188477], 'magnitude': 3.0214316844940186, 'cosine_ionic_motion': -0.3484918773174286, 'motion_component_ionic': -1.0529444217681885, 'motion_component_percent_ionic': 34.84918773174286}, {'ion_id': 1313, 'distance': 8.069931030273438, 'force': [2.8922908306121826, 0.682626485824585, -4.142235279083252], 'magnitude': 5.0979838371276855, 'cosine_ionic_motion': -0.9379406571388245, 'motion_component_ionic': -4.781606197357178, 'motion_component_percent_ionic': 93.79406571388245}, {'ion_id': 1460, 'distance': 11.685558319091797, 'force': [0.9793370366096497, 0.2705364525318146, -2.2088334560394287], 'magnitude': 2.4313035011291504, 'cosine_ionic_motion': -0.8644888401031494, 'motion_component_ionic': -2.101834774017334, 'motion_component_percent_ionic': 86.44888401031494}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.986762523651123, 'force': [-3.3615376949310303, -14.398987770080566, -1.7819820642471313], 'magnitude': 14.89316177368164, 'cosine_with_motion': 0.4234950542449951, 'motion_component': 6.307180404663086, 'motion_component_percent': 42.34950542449951}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.037108898162842, 'force': [8.76229190826416, 19.110010147094727, 3.707000970840454], 'magnitude': 21.347414016723633, 'cosine_with_motion': -0.5045356750488281, 'motion_component': -10.77053165435791, 'motion_component_percent': 50.45356750488281}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.9858293533325195, 'force': [3.2005178928375244, 11.289494514465332, 3.603163003921509], 'magnitude': 12.275128364562988, 'cosine_with_motion': -0.3322523534297943, 'motion_component': -4.078440189361572, 'motion_component_percent': 33.22523534297943}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.024247646331787, 'force': [-1.8575721979141235, -4.551418304443359, -2.5078530311584473], 'magnitude': 5.518632888793945, 'cosine_with_motion': 0.26263460516929626, 'motion_component': 1.4493839740753174, 'motion_component_percent': 26.263460516929626}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.816722869873047, 'force': [-0.6814670562744141, -3.919210195541382, -1.0620219707489014], 'magnitude': 4.117341041564941, 'cosine_with_motion': 0.29340440034866333, 'motion_component': 1.2080459594726562, 'motion_component_percent': 29.340440034866333}]}, 3188: {'frame': 3188, 'motion_vector': [2.9478530883789062, -1.2035942077636719, 0.8451919555664062], 'ionic_force': [11.80595587193966, -1.4899064302444458, -16.767672687768936], 'ionic_force_magnitude': 20.56101317020206, 'radial_force': 11.89959727138151, 'axial_force': -16.767672687768936, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-9.493465304374695, -3.0462600626051426, -5.455596923828125], 'asn_force_magnitude': 11.365259418494242, 'residue_force': [-9.493465304374695, -3.0462600626051426, -5.455596923828125], 'residue_force_magnitude': 11.365259418494242, 'total_force': [2.3124905675649643, -4.536166492849588, -22.22326961159706], 'total_force_magnitude': 22.79908180839004, 'cosine_total_motion': -0.08662598429308035, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.7726739540734446, 'cosine_residue_motion': -0.7726739540734446, 'cosine_ionic_motion': 0.33104628526733565, 'motion_component_total': -1.9749929026302495, 'motion_component_glu': None, 'motion_component_asn': -8.781639933958404, 'motion_component_residue': -8.781639933958404, 'motion_component_ionic': 6.806647031328156, 'motion_component_percent_total': 8.662598429308035, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 77.26739540734447, 'motion_component_percent_residue': 77.26739540734447, 'motion_component_percent_ionic': 33.10462852673356, 'ionic_contributions': [{'ion_id': 1306, 'distance': 7.902102947235107, 'force': [0.704689621925354, 5.264189720153809, -0.24574843049049377], 'magnitude': 5.316829204559326, 'cosine_ionic_motion': -0.25499215722084045, 'motion_component_ionic': -1.3557497262954712, 'motion_component_percent_ionic': 25.499215722084045}, {'ion_id': 1307, 'distance': 4.215550899505615, 'force': [11.88012981414795, -11.49898910522461, -8.6984281539917], 'magnitude': 18.682260513305664, 'cosine_ionic_motion': 0.6744394898414612, 'motion_component_ionic': 12.600054740905762, 'motion_component_percent_ionic': 67.44394898414612}, {'ion_id': 1313, 'distance': 7.252689838409424, 'force': [-0.5623465180397034, 3.5319478511810303, -5.200526714324951], 'magnitude': 6.311605930328369, 'cosine_ionic_motion': -0.4955672323703766, 'motion_component_ionic': -3.1278250217437744, 'motion_component_percent_ionic': 49.55672323703766}, {'ion_id': 1460, 'distance': 10.703454971313477, 'force': [-0.21651704609394073, 1.2129451036453247, -2.622969388961792], 'magnitude': 2.897944688796997, 'cosine_ionic_motion': -0.45198705792427063, 'motion_component_ionic': -1.3098335266113281, 'motion_component_percent_ionic': 45.19870579242706}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.9543068408966064, 'force': [9.581599235534668, -0.03208534047007561, 11.72050952911377], 'magnitude': 15.138640403747559, 'cosine_with_motion': 0.7657545804977417, 'motion_component': 11.592483520507812, 'motion_component_percent': 76.57545804977417}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.935325860977173, 'force': [-16.629323959350586, -3.5374836921691895, -15.272061347961426], 'magnitude': 22.853534698486328, 'cosine_with_motion': -0.7660059928894043, 'motion_component': -17.505945205688477, 'motion_component_percent': 76.60059928894043}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.479323863983154, 'force': [-6.031380653381348, -1.0252747535705566, -13.923310279846191], 'magnitude': 15.20813274383545, 'cosine_with_motion': -0.5651268362998962, 'motion_component': -8.594524383544922, 'motion_component_percent': 56.512683629989624}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.181246757507324, 'force': [1.7811845541000366, 1.6163733005523682, 7.596541881561279], 'magnitude': 7.96823263168335, 'cosine_with_motion': 0.37050122022628784, 'motion_component': 2.952239990234375, 'motion_component_percent': 37.050122022628784}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.400108337402344, 'force': [1.8044555187225342, -0.06778957694768906, 4.422723293304443], 'magnitude': 4.77714729309082, 'cosine_with_motion': 0.5807034969329834, 'motion_component': 2.774106025695801, 'motion_component_percent': 58.07034969329834}]}, 3189: {'frame': 3189, 'motion_vector': [2.050933837890625, -1.666748046875, -0.683929443359375], 'ionic_force': [12.04167953133583, 15.30772179365158, -8.939361959695816], 'ionic_force_magnitude': 21.429899315995037, 'radial_force': 19.476354701206997, 'axial_force': -8.939361959695816, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [10.599079847335815, -1.189270257949829, 1.1911693885922432], 'asn_force_magnitude': 10.731902993829356, 'residue_force': [10.599079847335815, -1.189270257949829, 1.1911693885922432], 'residue_force_magnitude': 10.731902993829356, 'total_force': [22.640759378671646, 14.118451535701752, -7.748192571103573], 'total_force_magnitude': 27.78433276376764, 'cosine_total_motion': 0.371825983846322, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.7818501630954965, 'cosine_residue_motion': 0.7818501630954965, 'cosine_ionic_motion': 0.09053690503822516, 'motion_component_total': 10.330936865401501, 'motion_component_glu': None, 'motion_component_asn': 8.39074010605053, 'motion_component_residue': 8.39074010605053, 'motion_component_ionic': 1.940196759350969, 'motion_component_percent_total': 37.1825983846322, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 78.18501630954965, 'motion_component_percent_residue': 78.18501630954965, 'motion_component_percent_ionic': 9.053690503822516, 'ionic_contributions': [{'ion_id': 1306, 'distance': 4.907887935638428, 'force': [4.522043704986572, 13.012672424316406, 0.44386425614356995], 'magnitude': 13.783161163330078, 'cosine_ionic_motion': -0.33801013231277466, 'motion_component_ionic': -4.658848285675049, 'motion_component_percent_ionic': 33.801013231277466}, {'ion_id': 1307, 'distance': 7.745893955230713, 'force': [5.291672229766846, -1.454615592956543, -0.7079718708992004], 'magnitude': 5.5334367752075195, 'cosine_ionic_motion': 0.9110285043716431, 'motion_component_ionic': 5.041118621826172, 'motion_component_percent_ionic': 91.1028504371643}, {'ion_id': 1313, 'distance': 6.778944969177246, 'force': [1.8297994136810303, 3.0413978099823, -6.2925825119018555], 'magnitude': 7.2246012687683105, 'cosine_ionic_motion': 0.1514660269021988, 'motion_component_ionic': 1.0942816734313965, 'motion_component_percent_ionic': 15.14660269021988}, {'ion_id': 1460, 'distance': 11.483993530273438, 'force': [0.39816418290138245, 0.7082671523094177, -2.38267183303833], 'magnitude': 2.517399787902832, 'cosine_ionic_motion': 0.1841759830713272, 'motion_component_ionic': 0.4636445939540863, 'motion_component_percent_ionic': 18.41759830713272}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.5787932872772217, 'force': [-15.929393768310547, -8.559465408325195, 3.8187503814697266], 'magnitude': 18.48223114013672, 'cosine_with_motion': -0.41652700304985046, 'motion_component': -7.698348522186279, 'motion_component_percent': 41.652700304985046}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.848459243774414, 'force': [23.558996200561523, 5.480602741241455, -1.9761227369308472], 'magnitude': 24.2686710357666, 'cosine_with_motion': 0.6118435263633728, 'motion_component': 14.84862995147705, 'motion_component_percent': 61.18435263633728}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.693469524383545, 'force': [12.044590950012207, 6.841427326202393, -0.02992498129606247], 'magnitude': 13.852010726928711, 'cosine_with_motion': 0.3522550165653229, 'motion_component': 4.8794403076171875, 'motion_component_percent': 35.22550165653229}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.8854546546936035, 'force': [-5.286684513092041, -2.261216640472412, -1.0021666288375854], 'magnitude': 5.836648941040039, 'cosine_with_motion': -0.40094494819641113, 'motion_component': -2.340174913406372, 'motion_component_percent': 40.09449481964111}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.466248512268066, 'force': [-3.788429021835327, -2.6906182765960693, 0.3806333541870117], 'magnitude': 4.662242412567139, 'cosine_with_motion': -0.27857986092567444, 'motion_component': -1.2988067865371704, 'motion_component_percent': 27.857986092567444}]}, 3190: {'frame': 3190, 'motion_vector': [-0.8215522766113281, -0.8835487365722656, -0.6362762451171875], 'ionic_force': [15.530074954032898, 11.720041185617447, -13.903977543115616], 'ionic_force_magnitude': 23.913661053672072, 'radial_force': 19.456171089668416, 'axial_force': -13.903977543115616, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [8.18987786769867, 3.4612741470336914, 1.6022478938102722], 'asn_force_magnitude': 9.034473782238994, 'residue_force': [8.18987786769867, 3.4612741470336914, 1.6022478938102722], 'residue_force_magnitude': 9.034473782238994, 'total_force': [23.719952821731567, 15.181315332651138, -12.301729649305344], 'total_force_magnitude': 30.731759621914886, 'cosine_total_motion': -0.5981565760756317, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.8769124628321204, 'cosine_residue_motion': -0.8769124628321204, 'cosine_ionic_motion': -0.437405273662284, 'motion_component_total': -18.382404112223956, 'motion_component_glu': None, 'motion_component_asn': -7.922442654775418, 'motion_component_residue': -7.922442654775418, 'motion_component_ionic': -10.459961457448536, 'motion_component_percent_total': 59.81565760756317, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 87.69124628321204, 'motion_component_percent_residue': 87.69124628321204, 'motion_component_percent_ionic': 43.7405273662284, 'ionic_contributions': [{'ion_id': 1306, 'distance': 4.505828857421875, 'force': [8.8020601272583, 11.90870189666748, -6.9365973472595215], 'magnitude': 16.352670669555664, 'cosine_ionic_motion': -0.5980634093284607, 'motion_component_ionic': -9.77993392944336, 'motion_component_percent_ionic': 59.80634093284607}, {'ion_id': 1307, 'distance': 9.605598449707031, 'force': [3.2317216396331787, -1.556819200515747, -0.28207412362098694], 'magnitude': 3.5982325077056885, 'cosine_ionic_motion': -0.22413209080696106, 'motion_component_ionic': -0.8064793944358826, 'motion_component_percent_ionic': 22.413209080696106}, {'ion_id': 1313, 'distance': 7.852586269378662, 'force': [2.741168975830078, 1.0629887580871582, -4.5104899406433105], 'magnitude': 5.38409423828125, 'cosine_ionic_motion': -0.04375084862112999, 'motion_component_ionic': -0.23555868864059448, 'motion_component_percent_ionic': 4.375084862112999}, {'ion_id': 1460, 'distance': 11.956610679626465, 'force': [0.7551242113113403, 0.3051697313785553, -2.174816131591797], 'magnitude': 2.3223190307617188, 'cosine_ionic_motion': 0.15588343143463135, 'motion_component_ionic': 0.36201104521751404, 'motion_component_percent_ionic': 15.588343143463135}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.6500916481018066, 'force': [-8.962726593017578, -15.326889038085938, -0.6565071940422058], 'magnitude': 17.767244338989258, 'cosine_with_motion': 0.8798756003379822, 'motion_component': 15.632965087890625, 'motion_component_percent': 87.98756003379822}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.893784761428833, 'force': [16.062002182006836, 16.66604995727539, 4.144992828369141], 'magnitude': 23.514379501342773, 'cosine_with_motion': -0.9527691006660461, 'motion_component': -22.40377426147461, 'motion_component_percent': 95.27691006660461}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.771966457366943, 'force': [6.582432746887207, 11.42540454864502, 2.3859596252441406], 'magnitude': 13.400040626525879, 'cosine_with_motion': -0.9312483072280884, 'motion_component': -12.478765487670898, 'motion_component_percent': 93.12483072280884}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.9438042640686035, 'force': [-3.1666483879089355, -4.3073344230651855, -1.9762696027755737], 'magnitude': 5.699687480926514, 'cosine_with_motion': 0.9859118461608887, 'motion_component': 5.619389533996582, 'motion_component_percent': 98.59118461608887}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.423899173736572, 'force': [-1.6978040933609009, -4.361782550811768, -0.7181048393249512], 'magnitude': 4.735331058502197, 'cosine_with_motion': 0.8833670616149902, 'motion_component': 4.183035373687744, 'motion_component_percent': 88.33670616149902}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.702774524688721, 'force': [2.310697317123413, 6.742098808288574, 1.4780361652374268], 'magnitude': 7.278723239898682, 'cosine_with_motion': -0.8859500288963318, 'motion_component': -6.448585033416748, 'motion_component_percent': 88.59500288963318}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.810923099517822, 'force': [-2.938075304031372, -7.376273155212402, -3.055859088897705], 'magnitude': 8.507641792297363, 'cosine_with_motion': 0.9371920228004456, 'motion_component': 7.973293781280518, 'motion_component_percent': 93.71920228004456}]}, 3191: {'frame': 3191, 'motion_vector': [1.4482460021972656, 0.2650604248046875, 0.5260162353515625], 'ionic_force': [17.29844206571579, 1.1133021712303162, -8.736418187618256], 'ionic_force_magnitude': 19.41135086423247, 'radial_force': 17.334230286499363, 'axial_force': -8.736418187618256, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-0.12483274936676025, -8.143236875534058, -0.7974077761173248], 'asn_force_magnitude': 8.183138101473329, 'residue_force': [-0.12483274936676025, -8.143236875534058, -0.7974077761173248], 'residue_force_magnitude': 8.183138101473329, 'total_force': [17.17360931634903, -7.0299347043037415, -9.53382596373558], 'total_force_magnitude': 20.86256639064722, 'cosine_total_motion': 0.5516455062389752, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.21562519615260967, 'cosine_residue_motion': -0.21562519615260967, 'cosine_ionic_motion': 0.6837871227573488, 'motion_component_total': 11.508740998012817, 'motion_component_glu': None, 'motion_component_asn': -1.7644907582740803, 'motion_component_residue': -1.7644907582740803, 'motion_component_ionic': 13.273231756286897, 'motion_component_percent_total': 55.164550623897526, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 21.562519615260967, 'motion_component_percent_residue': 21.562519615260967, 'motion_component_percent_ionic': 68.37871227573487, 'ionic_contributions': [{'ion_id': 1306, 'distance': 5.4740495681762695, 'force': [10.922542572021484, 1.8332058191299438, -0.30494749546051025], 'magnitude': 11.079511642456055, 'cosine_ionic_motion': 0.931983470916748, 'motion_component_ionic': 10.325922012329102, 'motion_component_percent_ionic': 93.1983470916748}, {'ion_id': 1307, 'distance': 10.684454917907715, 'force': [2.5171878337860107, -1.3357510566711426, -0.5809615254402161], 'magnitude': 2.9082610607147217, 'cosine_ionic_motion': 0.6566780805587769, 'motion_component_ionic': 1.9097912311553955, 'motion_component_percent_ionic': 65.66780805587769}, {'ion_id': 1313, 'distance': 7.416356086730957, 'force': [2.9662954807281494, 0.4142634868621826, -5.240616798400879], 'magnitude': 6.036106586456299, 'cosine_ionic_motion': 0.17474383115768433, 'motion_component_ionic': 1.0547723770141602, 'motion_component_percent_ionic': 17.474383115768433}, {'ion_id': 1460, 'distance': 10.956549644470215, 'force': [0.8924161791801453, 0.20158392190933228, -2.6098923683166504], 'magnitude': 2.7656068801879883, 'cosine_ionic_motion': -0.006238765548914671, 'motion_component_ionic': -0.017253972589969635, 'motion_component_percent_ionic': 0.6238765548914671}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.137293815612793, 'force': [-4.541301250457764, -7.616402626037598, -1.3473764657974243], 'magnitude': 8.969305038452148, 'cosine_with_motion': -0.6635134220123291, 'motion_component': -5.951254367828369, 'motion_component_percent': 66.35134220123291}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.479304790496826, 'force': [6.375889778137207, 7.045587539672852, 2.453929901123047], 'magnitude': 9.813972473144531, 'cosine_with_motion': 0.8076428771018982, 'motion_component': 7.926185131072998, 'motion_component_percent': 80.76428771018982}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.1367387771606445, 'force': [1.5254372358322144, 8.745102882385254, 1.2959271669387817], 'magnitude': 8.971242904663086, 'cosine_with_motion': 0.3713706135749817, 'motion_component': 3.331655979156494, 'motion_component_percent': 37.13706135749817}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.9513065814971924, 'force': [-2.616971015930176, -12.033166885375977, -2.7234742641448975], 'magnitude': 12.612016677856445, 'cosine_with_motion': -0.426616907119751, 'motion_component': -5.380499362945557, 'motion_component_percent': 42.6616907119751}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.933863162994385, 'force': [-3.0954058170318604, -8.050671577453613, -0.840927243232727], 'magnitude': 8.666141510009766, 'cosine_with_motion': -0.5210080146789551, 'motion_component': -4.515129089355469, 'motion_component_percent': 52.10080146789551}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.632627010345459, 'force': [2.227518320083618, 3.7663137912750244, 0.3645131289958954], 'magnitude': 4.390880107879639, 'cosine_with_motion': 0.6432766318321228, 'motion_component': 2.8245506286621094, 'motion_component_percent': 64.32766318321228}]}, 3192: {'frame': 3192, 'motion_vector': [-1.4279060363769531, -0.3152008056640625, 0.24273681640625], 'ionic_force': [14.277701735496521, 1.8772609233856201, -9.105208367109299], 'ionic_force_magnitude': 17.037655203423625, 'radial_force': 14.400585940241147, 'axial_force': -9.105208367109299, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [5.426489636301994, 5.107189655303955, -0.14802205562591553], 'asn_force_magnitude': 7.453327208508185, 'residue_force': [5.426489636301994, 5.107189655303955, -0.14802205562591553], 'residue_force_magnitude': 7.453327208508185, 'total_force': [19.704191371798515, 6.984450578689575, -9.253230422735214], 'total_force_magnitude': 22.8617580417353, 'cosine_total_motion': -0.9615066834164585, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.8503108684132783, 'cosine_residue_motion': -0.8503108684132783, 'cosine_ionic_motion': -0.9182066331169767, 'motion_component_total': -21.981733151778457, 'motion_component_glu': None, 'motion_component_asn': -6.33764513123491, 'motion_component_residue': -6.33764513123491, 'motion_component_ionic': -15.644088020543546, 'motion_component_percent_total': 96.15066834164585, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 85.03108684132783, 'motion_component_percent_residue': 85.03108684132783, 'motion_component_percent_ionic': 91.82066331169767, 'ionic_contributions': [{'ion_id': 1306, 'distance': 6.40054178237915, 'force': [7.416618824005127, 2.3804314136505127, -2.2368931770324707], 'magnitude': 8.104096412658691, 'cosine_ionic_motion': -0.9892522096633911, 'motion_component_ionic': -8.016995429992676, 'motion_component_percent_ionic': 98.92522096633911}, {'ion_id': 1307, 'distance': 10.719320297241211, 'force': [2.5377702713012695, -1.3266432285308838, -0.38498708605766296], 'magnitude': 2.8893728256225586, 'cosine_ionic_motion': -0.7702711224555969, 'motion_component_ionic': -2.225600481033325, 'motion_component_percent_ionic': 77.02711224555969}, {'ion_id': 1313, 'distance': 7.895941734313965, 'force': [3.2284295558929443, 0.5756868124008179, -4.195573329925537], 'magnitude': 5.325129985809326, 'cosine_ionic_motion': -0.7360293865203857, 'motion_component_ionic': -3.91945219039917, 'motion_component_percent_ionic': 73.60293865203857}, {'ion_id': 1460, 'distance': 11.41408634185791, 'force': [1.0948830842971802, 0.24778592586517334, -2.287754774093628], 'magnitude': 2.548330545425415, 'cosine_ionic_motion': -0.5815727114677429, 'motion_component_ionic': -1.4820395708084106, 'motion_component_percent_ionic': 58.15727114677429}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.054739475250244, 'force': [-2.356449842453003, -14.174798011779785, -0.907854437828064], 'magnitude': 14.397984504699707, 'cosine_with_motion': 0.35668274760246277, 'motion_component': 5.135512828826904, 'motion_component_percent': 35.66827476024628}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.288381576538086, 'force': [7.63788366317749, 16.50430679321289, 0.9284068942070007], 'magnitude': 18.20965003967285, 'cosine_with_motion': -0.5884330868721008, 'motion_component': -10.715160369873047, 'motion_component_percent': 58.84330868721008}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.936164379119873, 'force': [1.7036049365997314, 11.97382926940918, 3.249650001525879], 'magnitude': 12.523381233215332, 'cosine_with_motion': -0.2918628752231598, 'motion_component': -3.6551098823547363, 'motion_component_percent': 29.18628752231598}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.874608516693115, 'force': [-1.4094593524932861, -5.1374030113220215, -2.447693109512329], 'magnitude': 5.862651824951172, 'cosine_with_motion': 0.34956133365631104, 'motion_component': 2.049356460571289, 'motion_component_percent': 34.9561333656311}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.775841236114502, 'force': [-0.1490897685289383, -4.058745384216309, -0.9705314040184021], 'magnitude': 4.1758317947387695, 'cosine_with_motion': 0.20301499962806702, 'motion_component': 0.8477565050125122, 'motion_component_percent': 20.3014999628067}]}, 3193: {'frame': 3193, 'motion_vector': [-1.265380859375, 0.5024642944335938, 1.421234130859375], 'ionic_force': [24.2664697766304, -1.6357786357402802, -8.331860184669495], 'ionic_force_magnitude': 25.70908830165204, 'radial_force': 24.32154039458153, 'axial_force': -8.331860184669495, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [4.683553457260132, 7.689526557922363, -0.025576263666152954], 'asn_force_magnitude': 9.0036184846577, 'residue_force': [4.683553457260132, 7.689526557922363, -0.025576263666152954], 'residue_force_magnitude': 9.0036184846577, 'total_force': [28.950023233890533, 6.053747922182083, -8.357436448335648], 'total_force_magnitude': 30.73432044370096, 'cosine_total_motion': -0.7516839030971542, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.11845788957196339, 'cosine_residue_motion': -0.11845788957196339, 'cosine_ionic_motion': -0.857126633484709, 'motion_component_total': -23.102493950159797, 'motion_component_glu': None, 'motion_co</t>
         </is>
       </c>
     </row>
@@ -531,7 +531,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>{3320: {'frame': 3320, 'ionic_force': [14.295079827308655, -1.2250978574156761, -4.31649112701416], 'ionic_force_magnitude': 14.982732316869418, 'motion_vector': [-0.18167495727539062, 0.760711669921875, 0.7443389892578125], 'ionic_force_x': 14.295079827308655, 'ionic_force_y': -1.2250978574156761, 'ionic_force_z': -4.31649112701416, 'radial_force': 14.347479640319108, 'axial_force': -4.31649112701416, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [1.7637792229652405, 1.4510164260864258, 2.6891615092754364], 'asn_force_magnitude': 3.528166016375226, 'residue_force': [1.7637792229652405, 1.4510164260864258, 2.6891615092754364], 'residue_force_magnitude': 3.528166016375226, 'total_force': [16.058859050273895, 0.22591856867074966, -1.6273296177387238], 'total_force_magnitude': 16.142682394230636, 'motion_component_total': -3.664868296375276, 'cosine_total_motion': -0.2270296972258522, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.7311059634752681, 'cosine_residue_motion': 0.7311059634752681, 'cosine_ionic_motion': -0.416768542547299, 'motion_component_glu': None, 'motion_component_asn': 2.5794632147027086, 'motion_component_residue': 2.5794632147027086, 'motion_component_ionic': -6.244331511077984, 'ionic_contributions': [{'ion_id': 1306, 'distance': 6.092681884765625, 'force': [6.963980674743652, -2.6537961959838867, 4.944848537445068], 'magnitude': 8.943778991699219}, {'ion_id': 1307, 'distance': 10.376346588134766, 'force': [2.457754135131836, -1.7556523084640503, -0.6207482814788818], 'magnitude': 3.0835366249084473}, {'ion_id': 1387, 'distance': 12.950896263122559, 'force': [0.3318135738372803, -0.0069795772433280945, -1.9514002799987793], 'magnitude': 1.9794220924377441}, {'ion_id': 1460, 'distance': 7.725468635559082, 'force': [1.624815821647644, -0.2846843898296356, -5.312528133392334], 'magnitude': 5.562735557556152}, {'ion_id': 2433, 'distance': 8.367491722106934, 'force': [2.916715621948242, 3.4760146141052246, -1.3766629695892334], 'magnitude': 4.741846561431885}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.929006576538086, 'force': [3.87831449508667, 4.029547691345215, 0.3129032552242279], 'magnitude': 5.601471900939941}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.0385870933532715, 'force': [-2.164111852645874, 13.85459041595459, 3.7423644065856934], 'magnitude': 14.513384819030762}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.556410312652588, 'force': [-0.5534653067588806, -9.418764114379883, -0.9688898324966431], 'magnitude': 9.48462963104248}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.316054105758667, 'force': [1.9426721334457397, -23.71256446838379, -14.282292366027832], 'magnitude': 27.749658584594727}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.6567134857177734, 'force': [1.9972094297409058, 8.327070236206055, 5.933754920959473], 'magnitude': 10.41817569732666}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 3.4046263694763184, 'force': [-3.3368396759033203, 8.371136665344238, 7.951321125030518], 'magnitude': 12.01806640625}]}, 3321: {'frame': 3321, 'ionic_force': [12.688717484474182, 1.7846734374761581, -5.118914902210236], 'ionic_force_magnitude': 13.798257152818387, 'motion_vector': [3.44659423828125, 0.5642127990722656, -0.29720306396484375], 'ionic_force_x': 12.688717484474182, 'ionic_force_y': 1.7846734374761581, 'ionic_force_z': -5.118914902210236, 'radial_force': 12.813610368636693, 'axial_force': -5.118914902210236, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-0.9511253759264946, -2.4715158939361572, 3.0370868146419525], 'asn_force_magnitude': 4.029506993961216, 'residue_force': [-0.9511253759264946, -2.4715158939361572, 3.0370868146419525], 'residue_force_magnitude': 4.029506993961216, 'total_force': [11.737592108547688, -0.6868424564599991, -2.081828087568283], 'total_force_magnitude': 11.94055397596046, 'motion_component_total': 11.607656968542669, 'cosine_total_motion': 0.9721204721248274, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.3947405667618458, 'cosine_residue_motion': -0.3947405667618458, 'cosine_ionic_motion': 0.9565169497086744, 'motion_component_glu': None, 'motion_component_asn': -1.590609874567072, 'motion_component_residue': -1.590609874567072, 'motion_component_ionic': 13.198266843109742, 'ionic_contributions': [{'ion_id': 1306, 'distance': 6.783074855804443, 'force': [4.35039758682251, -0.736777126789093, 5.709558963775635], 'magnitude': 7.215806484222412}, {'ion_id': 1307, 'distance': 8.998174667358398, 'force': [3.376248836517334, -2.3066442012786865, -0.3063477873802185], 'magnitude': 4.100428581237793}, {'ion_id': 1387, 'distance': 11.853490829467773, 'force': [0.4181758165359497, 0.16234956681728363, -2.319929599761963], 'magnitude': 2.362901210784912}, {'ion_id': 1460, 'distance': 6.62709379196167, 'force': [2.362652540206909, 0.5963982939720154, -7.155970096588135], 'magnitude': 7.559479236602783}, {'ion_id': 2433, 'distance': 8.374307632446289, 'force': [2.1812427043914795, 4.069346904754639, -1.0462263822555542], 'magnitude': 4.734130859375}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.841907024383545, 'force': [-4.671124458312988, -5.110078811645508, 0.42171603441238403], 'magnitude': 6.936148166656494}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.702136516571045, 'force': [4.938201904296875, 3.471296548843384, -0.49013134837150574], 'magnitude': 6.0560688972473145}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.446988105773926, 'force': [-3.116992473602295, 10.654122352600098, 4.478387832641602], 'magnitude': 11.97004222869873}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.780481815338135, 'force': [0.4535975754261017, -8.364376068115234, -2.0181007385253906], 'magnitude': 8.616336822509766}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.754653215408325, 'force': [5.390667915344238, -16.270679473876953, -13.218152046203613], 'magnitude': 21.64518165588379}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.599644422531128, 'force': [0.08243153244256973, 7.747219085693359, 7.453906536102295], 'magnitude': 10.75113582611084}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 3.87046480178833, 'force': [-4.027907371520996, 5.400980472564697, 6.409460544586182], 'magnitude': 9.299237251281738}]}, 3322: {'frame': 3322, 'ionic_force': [11.341214001178741, 1.8453324884176254, -4.039094507694244], 'ionic_force_magnitude': 12.179600627911743, 'motion_vector': [-1.1910209655761719, 1.1273345947265625, 1.091339111328125], 'ionic_force_x': 11.341214001178741, 'ionic_force_y': 1.8453324884176254, 'ionic_force_z': -4.039094507694244, 'radial_force': 11.490360612850333, 'axial_force': -4.039094507694244, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [9.554869204759598, 12.884615182876587, 1.8226514756679535], 'asn_force_magnitude': 16.144066784197587, 'residue_force': [9.554869204759598, 12.884615182876587, 1.8226514756679535], 'residue_force_magnitude': 16.144066784197587, 'total_force': [20.89608320593834, 14.729947671294212, -2.216443032026291], 'total_force_magnitude': 25.661844662120103, 'motion_component_total': -5.432296779366711, 'cosine_total_motion': -0.21168769630132703, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.16144797816748313, 'cosine_residue_motion': 0.16144797816748313, 'cosine_ionic_motion': -0.6600153787189091, 'motion_component_glu': None, 'motion_component_asn': 2.606426941709522, 'motion_component_residue': 2.606426941709522, 'motion_component_ionic': -8.038723721076233, 'ionic_contributions': [{'ion_id': 1306, 'distance': 8.663389205932617, 'force': [4.151607990264893, 0.16926394402980804, 1.5174075365066528], 'magnitude': 4.423462867736816}, {'ion_id': 1307, 'distance': 12.226007461547852, 'force': [2.0877387523651123, -0.7246052622795105, -0.22269701957702637], 'magnitude': 2.2211034297943115}, {'ion_id': 1387, 'distance': 13.204231262207031, 'force': [0.8166144490242004, 0.16744935512542725, -1.7120360136032104], 'magnitude': 1.904196858406067}, {'ion_id': 1460, 'distance': 8.941094398498535, 'force': [2.6996209621429443, 0.5092499852180481, -3.1144349575042725], 'magnitude': 4.152949810028076}, {'ion_id': 2433, 'distance': 11.769852638244629, 'force': [1.5856318473815918, 1.7239744663238525, -0.5073340535163879], 'magnitude': 2.3966026306152344}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.1563720703125, 'force': [-2.6074059009552, -13.449638366699219, 0.2574821412563324], 'magnitude': 13.702468872070312}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.21524977684021, 'force': [7.510493278503418, 17.48997688293457, -0.7057549357414246], 'magnitude': 19.04743766784668}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.132801055908203, 'force': [2.618009328842163, 11.14928150177002, 1.728433609008789], 'magnitude': 11.58222484588623}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.191195011138916, 'force': [-1.855749249458313, -4.612452030181885, -1.4156352281570435], 'magnitude': 5.169384956359863}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.901503562927246, 'force': [-0.4347606599330902, -3.929887056350708, -0.6050654053688049], 'magnitude': 3.999891757965088}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.67315149307251, 'force': [3.523135185241699, 6.240754127502441, 1.65395987033844], 'magnitude': 7.354935646057129}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.831563472747803, 'force': [-7.883199691772461, -9.597227096557617, -4.07584810256958], 'magnitude': 13.071500778198242}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.132293224334717, 'force': [3.936645746231079, 3.2974867820739746, 1.2648983001708984], 'magnitude': 5.288720607757568}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 3.9971368312835693, 'force': [4.747701168060303, 6.29632043838501, 3.7201812267303467], 'magnitude': 8.719178199768066}]}, 3323: {'frame': 3323, 'ionic_force': [11.9672349691391, 4.672180593013763, -4.230508267879486], 'ionic_force_magnitude': 13.525575200519821, 'motion_vector': [-0.09119033813476562, -1.4596443176269531, 0.58355712890625], 'ionic_force_x': 11.9672349691391, 'ionic_force_y': 4.672180593013763, 'ionic_force_z': -4.230508267879486, 'radial_force': 12.8469445511499, 'axial_force': -4.230508267879486, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [12.794849157333374, 12.295886993408203, -3.5123274326324463], 'asn_force_magnitude': 18.089594962508198, 'residue_force': [12.794849157333374, 12.295886993408203, -3.5123274326324463], 'residue_force_magnitude': 18.089594962508198, 'total_force': [24.762084126472473, 16.968067586421967, -7.742835700511932], 'total_force_magnitude': 31.00044568371568, 'motion_component_total': -20.03268705084889, 'cosine_total_motion': -0.6462064208764561, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.7430103328275136, 'cosine_residue_motion': -0.7430103328275136, 'cosine_ionic_motion': -0.48736789225699, 'motion_component_glu': None, 'motion_component_asn': -13.44075597380813, 'motion_component_residue': -13.44075597380813, 'motion_component_ionic': -6.59193107704076, 'ionic_contributions': [{'ion_id': 1306, 'distance': 8.208459854125977, 'force': [3.659790277481079, 1.3112963438034058, 3.027434825897217], 'magnitude': 4.927364826202393}, {'ion_id': 1307, 'distance': 11.098809242248535, 'force': [2.6004390716552734, -0.6885156631469727, -0.16605886816978455], 'magnitude': 2.695164680480957}, {'ion_id': 1387, 'distance': 11.813334465026855, 'force': [0.8393199443817139, 0.3989105820655823, -2.18998122215271], 'magnitude': 2.3789925575256348}, {'ion_id': 1460, 'distance': 7.422881603240967, 'force': [3.4794766902923584, 1.5985596179962158, -4.6523637771606445], 'magnitude': 6.02549934387207}, {'ion_id': 2433, 'distance': 11.547141075134277, 'force': [1.3882089853286743, 2.0519297122955322, -0.24953922629356384], 'magnitude': 2.4899415969848633}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.5001673698425293, 'force': [-6.819509029388428, -17.08074951171875, 5.922703266143799], 'magnitude': 19.32190704345703}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.5544488430023193, 'force': [17.15321159362793, 22.74156951904297, -9.96096420288086], 'magnitude': 30.176687240600586}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.368577003479004, 'force': [6.918120384216309, 14.368143081665039, -1.1591911315917969], 'magnitude': 15.988986015319824}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.267806529998779, 'force': [-3.960157871246338, -6.458460330963135, -1.0496279001235962], 'magnitude': 7.648285865783691}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.107175350189209, 'force': [-1.6006189584732056, -5.089155197143555, 0.2518254518508911], 'magnitude': 5.340870380401611}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.4539008140563965, 'force': [1.103803038597107, 3.8145394325256348, 2.482927083969116], 'magnitude': 4.683376789093018}]}, 3325: {'frame': 3325, 'ionic_force': [13.136695861816406, 2.739805907011032, -4.366748213768005], 'ionic_force_magnitude': 14.111973800160023, 'motion_vector': [-1.0484428405761719, -1.0520210266113281, -0.158599853515625], 'ionic_force_x': 13.136695861816406, 'ionic_force_y': 2.739805907011032, 'ionic_force_z': -4.366748213768005, 'radial_force': 13.419363419102892, 'axial_force': -4.366748213768005, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [2.0107651948928833, 4.5555925369262695, 1.0442612171173096], 'asn_force_magnitude': 5.087934897487021, 'residue_force': [2.0107651948928833, 4.5555925369262695, 1.0442612171173096], 'residue_force_magnitude': 5.087934897487021, 'total_force': [15.14746105670929, 7.295398443937302, -3.322486996650696], 'total_force_magnitude': 17.137891782924765, 'motion_component_total': -15.417579498011303, 'cosine_total_motion': -0.89961937520066, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.9298052315041389, 'cosine_residue_motion': -0.9298052315041389, 'cosine_ionic_motion': -0.7572853495982408, 'motion_component_glu': None, 'motion_component_asn': -4.730788485235907, 'motion_component_residue': -4.730788485235907, 'motion_component_ionic': -10.686791012775398, 'ionic_contributions': [{'ion_id': 1306, 'distance': 8.27988052368164, 'force': [4.4394755363464355, 0.9520545601844788, 1.6842352151870728], 'magnitude': 4.842726230621338}, {'ion_id': 1307, 'distance': 10.302607536315918, 'force': [2.6720001697540283, -1.5414988994598389, -0.5172479152679443], 'magnitude': 3.1278345584869385}, {'ion_id': 1387, 'distance': 12.010658264160156, 'force': [1.0765461921691895, 0.23434945940971375, -2.0206117630004883], 'magnitude': 2.3014655113220215}, {'ion_id': 1460, 'distance': 9.120766639709473, 'force': [2.5632970333099365, 0.5630773901939392, -3.0066704750061035], 'magnitude': 3.9909415245056152}, {'ion_id': 2433, 'distance': 9.718379974365234, 'force': [2.3853769302368164, 2.5318233966827393, -0.506453275680542], 'magnitude': 3.515202283859253}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.9098193645477295, 'force': [-2.2039787769317627, -15.255782127380371, -1.4805901050567627], 'magnitude': 15.485107421875}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.873441457748413, 'force': [7.1205620765686035, 22.27750015258789, 4.664998531341553], 'magnitude': 23.848514556884766}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.024945259094238, 'force': [2.1752514839172363, 11.53020191192627, 2.8921031951904297], 'magnitude': 12.08476448059082}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.167775630950928, 'force': [-1.2281134128570557, -4.590771198272705, -2.151001453399658], 'magnitude': 5.216344356536865}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.832415580749512, 'force': [-0.3578742742538452, -4.011233806610107, -0.7434439659118652], 'magnitude': 4.095213890075684}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.391584873199463, 'force': [-3.495081901550293, -5.394322395324707, -2.1378049850463867], 'magnitude': 6.773811340332031}]}, 3326: {'frame': 3326, 'ionic_force': [13.417050004005432, 2.1709354370832443, -3.8333840072155], 'ionic_force_magnitude': 14.121792535961626, 'motion_vector': [0.80645751953125, 0.5555877685546875, -0.410614013671875], 'ionic_force_x': 13.417050004005432, 'ionic_force_y': 2.1709354370832443, 'ionic_force_z': -3.8333840072155, 'radial_force': 13.591548531420766, 'axial_force': -3.8333840072155, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [2.8685702085494995, 5.435973882675171, -1.2763834595680237], 'asn_force_magnitude': 6.277552216458508, 'residue_force': [2.8685702085494995, 5.435973882675171, -1.2763834595680237], 'residue_force_magnitude': 6.277552216458508, 'total_force': [16.28562021255493, 7.606909319758415, -5.109767466783524], 'total_force_magnitude': 18.686792626644213, 'motion_component_total': 18.323668383769725, 'cosine_total_motion': 0.9805678668282146, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.8787073227483828, 'cosine_residue_motion': 0.8787073227483828, 'cosine_ionic_motion': 0.9069342471656812, 'motion_component_glu': None, 'motion_component_asn': 5.516131101537432, 'motion_component_residue': 5.516131101537432, 'motion_component_ionic': 12.807537282232293, 'ionic_contributions': [{'ion_id': 1306, 'distance': 7.224223613739014, 'force': [5.361866474151611, 1.3586233854293823, 3.1420536041259766], 'magnitude': 6.361443996429443}, {'ion_id': 1307, 'distance': 10.580955505371094, 'force': [2.534034490585327, -1.4627076387405396, -0.48265519738197327], 'magnitude': 2.9654343128204346}, {'ion_id': 1387, 'distance': 12.873809814453125, 'force': [0.7306075096130371, 0.05163702368736267, -1.8644970655441284], 'magnitude': 2.0031981468200684}, {'ion_id': 1460, 'distance': 8.178290367126465, 'force': [2.9076755046844482, 0.214521124958992, -4.017284393310547], 'magnitude': 4.963785648345947}, {'ion_id': 2433, 'distance': 10.849812507629395, 'force': [1.8828660249710083, 2.008861541748047, -0.6110009551048279], 'magnitude': 2.820289134979248}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.632572650909424, 'force': [-2.9538981914520264, -10.626333236694336, -0.1438537836074829], 'magnitude': 11.030193328857422}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.869371175765991, 'force': [6.285953044891357, 11.549616813659668, 0.2510470747947693], 'magnitude': 13.151801109313965}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.474891185760498, 'force': [2.559556722640991, 9.622541427612305, 2.1186726093292236], 'magnitude': 10.180049896240234}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.540660858154297, 'force': [-1.4735945463180542, -3.9685699939727783, -1.6343446969985962], 'magnitude': 4.537853240966797}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.17544412612915, 'force': [2.6576550006866455, 8.071651458740234, 2.4264745712280273], 'magnitude': 8.837559700012207}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.230767250061035, 'force': [-4.207101821899414, -9.212932586669922, -4.294379234313965], 'magnitude': 11.000887870788574}]}, 3327: {'frame': 3327, 'ionic_force': [21.70894306898117, 0.4854571521282196, -6.7340773940086365], 'ionic_force_magnitude': 22.734592060719194, 'motion_vector': [-0.40179443359375, 0.5124359130859375, 0.6054840087890625], 'ionic_force_x': 21.70894306898117, 'ionic_force_y': 0.4854571521282196, 'ionic_force_z': -6.7340773940086365, 'radial_force': 21.714370306753498, 'axial_force': -6.7340773940086365, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [6.768657088279724, 10.94654893875122, 7.805947452783585], 'asn_force_magnitude': 15.052390776312357, 'residue_force': [6.768657088279724, 10.94654893875122, 7.805947452783585], 'residue_force_magnitude': 15.052390776312357, 'total_force': [28.477600157260895, 11.43200609087944, 1.0718700587749481], 'total_force_magnitude': 30.70526631380403, 'motion_component_total': -5.550026569359918, 'cosine_total_motion': -0.18075161806575235, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.5690387661741516, 'cosine_residue_motion': 0.5690387661741516, 'cosine_ionic_motion': -0.6208785452135951, 'motion_component_glu': None, 'motion_component_asn': 8.565393875323965, 'motion_component_residue': 8.565393875323965, 'motion_component_ionic': -14.115420444683883, 'ionic_contributions': [{'ion_id': 1306, 'distance': 4.783001899719238, 'force': [14.490052223205566, -0.3445451557636261, -0.7261050343513489], 'magnitude': 14.512324333190918}, {'ion_id': 1307, 'distance': 11.25306510925293, 'force': [2.2564868927001953, -1.2306782007217407, -0.5171406269073486], 'magnitude': 2.62178111076355}, {'ion_id': 1387, 'distance': 13.600533485412598, 'force': [0.7123898863792419, 0.10276107490062714, -1.644201397895813], 'magnitude': 1.7948418855667114}, {'ion_id': 1460, 'distance': 8.987810134887695, 'force': [2.544466972351074, 0.2279723435640335, -3.2194597721099854], 'magnitude': 4.109890937805176}, {'ion_id': 2433, 'distance': 11.503260612487793, 'force': [1.7055470943450928, 1.7299470901489258, -0.6271705627441406], 'magnitude': 2.508974075317383}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.7508065700531006, 'force': [-2.514101505279541, -16.386459350585938, -2.8764758110046387], 'magnitude': 16.825899124145508}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.843489170074463, 'force': [8.262893676757812, 21.46953582763672, 7.9925360679626465], 'magnitude': 24.35358428955078}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.933146953582764, 'force': [2.124559164047241, 11.826533317565918, 3.5830864906311035], 'magnitude': 12.53870677947998}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.150247097015381, 'force': [-1.2134851217269897, -4.523586273193359, -2.376384735107422], 'magnitude': 5.251912593841553}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.775523662567139, 'force': [-0.3407745361328125, -4.044666290283203, -0.9828341603279114], 'magnitude': 4.1762919425964355}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.117613315582275, 'force': [3.9065439701080322, 8.021707534790039, 1.4436801671981812], 'magnitude': 9.038423538208008}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.984063625335693, 'force': [-2.978884696960449, -4.613879680633545, -0.2755874693393707], 'magnitude': 5.498871803283691}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.313364505767822, 'force': [-8.800670623779297, -12.824962615966797, -5.201835632324219], 'magnitude': 16.40093231201172}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.629553318023682, 'force': [4.55888557434082, 4.193305492401123, 1.9695806503295898], 'magnitude': 6.499730587005615}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 3.770855665206909, 'force': [3.7636911869049072, 7.829020977020264, 4.530181884765625], 'magnitude': 9.797014236450195}]}, 3328: {'frame': 3328, 'ionic_force': [13.955669224262238, 4.043034732341766, -8.50230523943901], 'ionic_force_magnitude': 16.834370428635996, 'motion_vector': [-1.1094818115234375, 0.8973617553710938, 1.1634902954101562], 'ionic_force_x': 13.955669224262238, 'ionic_force_y': 4.043034732341766, 'ionic_force_z': -8.50230523943901, 'radial_force': 14.529515936325684, 'axial_force': -8.50230523943901, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [11.620216339826584, 18.754841327667236, 4.205258876085281], 'asn_force_magnitude': 22.46013586836112, 'residue_force': [11.620216339826584, 18.754841327667236, 4.205258876085281], 'residue_force_magnitude': 22.46013586836112, 'total_force': [25.57588556408882, 22.797876060009003, -4.297046363353729], 'total_force_magnitude': 34.530185094837094, 'motion_component_total': -7.015966705819842, 'cosine_total_motion': -0.20318358232226388, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.21353320906450965, 'cosine_residue_motion': 0.21353320906450965, 'cosine_ionic_motion': -0.7016568658678941, 'motion_component_glu': None, 'motion_component_asn': 4.795984887996047, 'motion_component_residue': 4.795984887996047, 'motion_component_ionic': -11.81195159381589, 'ionic_contributions': [{'ion_id': 1306, 'distance': 7.073066234588623, 'force': [5.705695152282715, 2.9352493286132812, -1.6938565969467163], 'magnitude': 6.636248588562012}, {'ion_id': 1307, 'distance': 10.411755561828613, 'force': [2.587146282196045, -1.5906908512115479, -0.39483076333999634], 'magnitude': 3.0625994205474854}, {'ion_id': 1387, 'distance': 13.023557662963867, 'force': [0.7809037566184998, 0.18411484360694885, -1.7854108810424805], 'magnitude': 1.9573965072631836}, {'ion_id': 1460, 'distance': 7.9806437492370605, 'force': [3.093663454055786, 0.4853256046772003, -4.167239665985107], 'magnitude': 5.21269416809082}, {'ion_id': 2433, 'distance': 11.000399589538574, 'force': [1.788260579109192, 2.029035806655884, -0.4609673321247101], 'magnitude': 2.7436022758483887}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.647946357727051, 'force': [-2.7626218795776367, -17.568330764770508, -0.3739224970340729], 'magnitude': 17.78814697265625}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.6879703998565674, 'force': [9.981447219848633, 25.31687355041504, 1.4703444242477417], 'magnitude': 27.253170013427734}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.691813945770264, 'force': [2.5192792415618896, 13.330267906188965, 2.847168445587158], 'magnitude': 13.861788749694824}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.801128387451172, 'force': [-1.6162699460983276, -5.344393730163574, -2.312736988067627], 'magnitude': 6.043478012084961}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.548980712890625, 'force': [-0.4456850588321686, -4.4534759521484375, -0.6609137654304504], 'magnitude': 4.524255752563477}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.121576309204102, 'force': [3.765683889389038, 8.019159317016602, 1.7185007333755493], 'magnitude': 9.02444076538086}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.264307022094727, 'force': [-9.371210098266602, -12.917621612548828, -5.186461448669434], 'magnitude': 16.78046226501465}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.641579627990723, 'force': [4.653621673583984, 4.182854175567627, 1.630305290222168], 'magnitude': 6.466093063354492}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 3.590463876724243, 'force': [4.895971298217773, 8.189508438110352, 5.072974681854248], 'magnitude': 10.806185722351074}]}, 3329: {'frame': 3329, 'ionic_force': [22.60821044445038, 6.519129231572151, -6.981471963226795], 'ionic_force_magnitude': 24.543251133698966, 'motion_vector': [0.8754844665527344, -1.0129776000976562, 0.6521530151367188], 'ionic_force_x': 22.60821044445038, 'ionic_force_y': 6.519129231572151, 'ionic_force_z': -6.981471963226795, 'radial_force': 23.529348172834997, 'axial_force': -6.981471963226795, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [8.299520455300808, -0.5748426914215088, -2.9503413140773773], 'asn_force_magnitude': 8.827060540031946, 'residue_force': [8.299520455300808, -0.5748426914215088, -2.9503413140773773], 'residue_force_magnitude': 8.827060540031946, 'total_force': [30.907730899751186, 5.944286540150642, -9.931813277304173], 'total_force_magnitude': 33.003988953126346, 'motion_component_total': 9.777157770185832, 'cosine_total_motion': 0.29624169927070826, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.4506632212891813, 'cosine_residue_motion': 0.4506632212891813, 'cosine_ionic_motion': 0.23628190907185725, 'motion_component_glu': None, 'motion_component_asn': 3.9780315374854167, 'motion_component_residue': 3.9780315374854167, 'motion_component_ionic': 5.7991262327004165, 'ionic_contributions': [{'ion_id': 1306, 'distance': 5.082821369171143, 'force': [12.494484901428223, 2.5334689617156982, 1.6158926486968994], 'magnitude': 12.850748062133789}, {'ion_id': 1307, 'distance': 8.874921798706055, 'force': [3.9902992248535156, -1.354427695274353, 0.10097753256559372], 'magnitude': 4.215110778808594}, {'ion_id': 1316, 'distance': 14.969817161560059, 'force': [0.37819957733154297, 0.24994249641895294, -1.4104505777359009], 'magnitude': 1.4815117120742798}, {'ion_id': 1387, 'distance': 11.019346237182617, 'force': [0.9713860750198364, 0.7008095979690552, -2.4578428268432617], 'magnitude': 2.734175682067871}, {'ion_id': 1460, 'distance': 7.456501483917236, 'force': [3.2983713150024414, 2.064893960952759, -4.52915096282959], 'magnitude': 5.971285343170166}, {'ion_id': 2433, 'distance': 10.948685646057129, 'force': [1.4754693508148193, 2.324441909790039, -0.3008977770805359], 'magnitude': 2.7695810794830322}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.5852224826812744, 'force': [-10.43619441986084, -13.890335083007812, 6.106855869293213], 'magnitude': 18.416006088256836}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.00884747505188, 'force': [17.004352569580078, 11.41319751739502, -7.325798988342285], 'magnitude': 21.750320434570312}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.323683738708496, 'force': [9.170852661132812, 13.453458786010742, -1.1539982557296753], 'magnitude': 16.322738647460938}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.381967067718506, 'force': [-4.952744483947754, -5.251922607421875, -0.7225998640060425], 'magnitude': 7.254965305328369}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.999220371246338, 'force': [-2.3799679279327393, -5.03740930557251, 0.1732882559299469], 'magnitude': 5.574026107788086}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.753434181213379, 'force': [-1.476701021194458, -6.900729179382324, -5.9308247566223145], 'magnitude': 9.218210220336914}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.724883079528809, 'force': [1.2969675064086914, 2.8016138076782227, 2.921576976776123], 'magnitude': 4.250503063201904}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.817553997039795, 'force': [0.07295557111501694, 2.8372833728790283, 2.9811594486236572], 'magnitude': 4.116164684295654}]}, 3330: {'frame': 3330, 'ionic_force': [14.08597069978714, 0.9935656264424324, -8.829362889751792], 'ionic_force_magnitude': 16.654110370963554, 'motion_vector': [1.0237197875976562, -1.2902107238769531, 0.8571853637695312], 'ionic_force_x': 14.08597069978714, 'ionic_force_y': 0.9935656264424324, 'ionic_force_z': -8.829362889751792, 'radial_force': 14.120968210760541, 'axial_force': -8.829362889751792,</t>
+          <t>{3320: {'frame': 3320, 'motion_vector': [-0.18167495727539062, 0.760711669921875, 0.7443389892578125], 'ionic_force': [14.295079827308655, -1.2250978574156761, -4.31649112701416], 'ionic_force_magnitude': 14.982732316869418, 'radial_force': 14.347479640319108, 'axial_force': -4.31649112701416, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [1.7637792229652405, 1.4510164260864258, 2.6891615092754364], 'asn_force_magnitude': 3.528166016375226, 'residue_force': [1.7637792229652405, 1.4510164260864258, 2.6891615092754364], 'residue_force_magnitude': 3.528166016375226, 'total_force': [16.058859050273895, 0.22591856867074966, -1.6273296177387238], 'total_force_magnitude': 16.142682394230636, 'cosine_total_motion': -0.2270296972258522, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.7311059634752681, 'cosine_residue_motion': 0.7311059634752681, 'cosine_ionic_motion': -0.416768542547299, 'motion_component_total': -3.664868296375276, 'motion_component_glu': None, 'motion_component_asn': 2.5794632147027086, 'motion_component_residue': 2.5794632147027086, 'motion_component_ionic': -6.244331511077984, 'motion_component_percent_total': 22.70296972258522, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 73.11059634752681, 'motion_component_percent_residue': 73.11059634752681, 'motion_component_percent_ionic': 41.6768542547299, 'ionic_contributions': [{'ion_id': 1306, 'distance': 6.092681884765625, 'force': [6.963980674743652, -2.6537961959838867, 4.944848537445068], 'magnitude': 8.943778991699219, 'cosine_ionic_motion': 0.04107999801635742, 'motion_component_ionic': 0.36741042137145996, 'motion_component_percent_ionic': 4.107999801635742}, {'ion_id': 1307, 'distance': 10.376346588134766, 'force': [2.457754135131836, -1.7556523084640503, -0.6207482814788818], 'magnitude': 3.0835366249084473, 'cosine_ionic_motion': -0.6740549206733704, 'motion_component_ionic': -2.0784730911254883, 'motion_component_percent_ionic': 67.40549206733704}, {'ion_id': 1387, 'distance': 12.950896263122559, 'force': [0.3318135738372803, -0.0069795772433280945, -1.9514002799987793], 'magnitude': 1.9794220924377441, 'cosine_ionic_motion': -0.7103326916694641, 'motion_component_ionic': -1.4060481786727905, 'motion_component_percent_ionic': 71.03326916694641}, {'ion_id': 1460, 'distance': 7.725468635559082, 'force': [1.624815821647644, -0.2846843898296356, -5.312528133392334], 'magnitude': 5.562735557556152, 'cosine_ionic_motion': -0.7435988187789917, 'motion_component_ionic': -4.136443614959717, 'motion_component_percent_ionic': 74.35988187789917}, {'ion_id': 2433, 'distance': 8.367491722106934, 'force': [2.916715621948242, 3.4760146141052246, -1.3766629695892334], 'magnitude': 4.741846561431885, 'cosine_ionic_motion': 0.2128332555294037, 'motion_component_ionic': 1.0092226266860962, 'motion_component_percent_ionic': 21.28332555294037}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.929006576538086, 'force': [3.87831449508667, 4.029547691345215, 0.3129032552242279], 'magnitude': 5.601471900939941, 'cosine_with_motion': 0.428852915763855, 'motion_component': 2.402207612991333, 'motion_component_percent': 42.8852915763855}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.0385870933532715, 'force': [-2.164111852645874, 13.85459041595459, 3.7423644065856934], 'magnitude': 14.513384819030762, 'cosine_with_motion': 0.8754403591156006, 'motion_component': 12.705602645874023, 'motion_component_percent': 87.54403591156006}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.556410312652588, 'force': [-0.5534653067588806, -9.418764114379883, -0.9688898324966431], 'magnitude': 9.48462963104248, 'cosine_with_motion': -0.7602785229682922, 'motion_component': -7.210960388183594, 'motion_component_percent': 76.02785229682922}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.316054105758667, 'force': [1.9426721334457397, -23.71256446838379, -14.282292366027832], 'magnitude': 27.749658584594727, 'cosine_with_motion': -0.968666672706604, 'motion_component': -26.880168914794922, 'motion_component_percent': 96.8666672706604}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.6567134857177734, 'force': [1.9972094297409058, 8.327070236206055, 5.933754920959473], 'magnitude': 10.41817569732666, 'cosine_with_motion': 0.9235438704490662, 'motion_component': 9.621642112731934, 'motion_component_percent': 92.35438704490662}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 3.4046263694763184, 'force': [-3.3368396759033203, 8.371136665344238, 7.951321125030518], 'magnitude': 12.01806640625, 'cosine_with_motion': 0.9935991168022156, 'motion_component': 11.941140174865723, 'motion_component_percent': 99.35991168022156}]}, 3321: {'frame': 3321, 'motion_vector': [3.44659423828125, 0.5642127990722656, -0.29720306396484375], 'ionic_force': [12.688717484474182, 1.7846734374761581, -5.118914902210236], 'ionic_force_magnitude': 13.798257152818387, 'radial_force': 12.813610368636693, 'axial_force': -5.118914902210236, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-0.9511253759264946, -2.4715158939361572, 3.0370868146419525], 'asn_force_magnitude': 4.029506993961216, 'residue_force': [-0.9511253759264946, -2.4715158939361572, 3.0370868146419525], 'residue_force_magnitude': 4.029506993961216, 'total_force': [11.737592108547688, -0.6868424564599991, -2.081828087568283], 'total_force_magnitude': 11.94055397596046, 'cosine_total_motion': 0.9721204721248274, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.3947405667618458, 'cosine_residue_motion': -0.3947405667618458, 'cosine_ionic_motion': 0.9565169497086744, 'motion_component_total': 11.607656968542669, 'motion_component_glu': None, 'motion_component_asn': -1.590609874567072, 'motion_component_residue': -1.590609874567072, 'motion_component_ionic': 13.198266843109742, 'motion_component_percent_total': 97.21204721248274, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 39.47405667618458, 'motion_component_percent_residue': 39.47405667618458, 'motion_component_percent_ionic': 95.65169497086744, 'ionic_contributions': [{'ion_id': 1306, 'distance': 6.783074855804443, 'force': [4.35039758682251, -0.736777126789093, 5.709558963775635], 'magnitude': 7.215806484222412, 'cosine_ionic_motion': 0.5093080997467041, 'motion_component_ionic': 3.6750688552856445, 'motion_component_percent_ionic': 50.93080997467041}, {'ion_id': 1307, 'distance': 8.998174667358398, 'force': [3.376248836517334, -2.3066442012786865, -0.3063477873802185], 'magnitude': 4.100428581237793, 'cosine_ionic_motion': 0.7254307866096497, 'motion_component_ionic': 2.9745771884918213, 'motion_component_percent_ionic': 72.54307866096497}, {'ion_id': 1387, 'distance': 11.853490829467773, 'force': [0.4181758165359497, 0.16234956681728363, -2.319929599761963], 'magnitude': 2.362901210784912, 'cosine_ionic_motion': 0.26833152770996094, 'motion_component_ionic': 0.634040892124176, 'motion_component_percent_ionic': 26.833152770996094}, {'ion_id': 1460, 'distance': 6.62709379196167, 'force': [2.362652540206909, 0.5963982939720154, -7.155970096588135], 'magnitude': 7.559479236602783, 'cosine_ionic_motion': 0.4002908170223236, 'motion_component_ionic': 3.0259900093078613, 'motion_component_percent_ionic': 40.02908170223236}, {'ion_id': 2433, 'distance': 8.374307632446289, 'force': [2.1812427043914795, 4.069346904754639, -1.0462263822555542], 'magnitude': 4.734130859375, 'cosine_ionic_motion': 0.6101627349853516, 'motion_component_ionic': 2.8885903358459473, 'motion_component_percent_ionic': 61.016273498535156}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.841907024383545, 'force': [-4.671124458312988, -5.110078811645508, 0.42171603441238403], 'magnitude': 6.936148166656494, 'cosine_with_motion': -0.7859534025192261, 'motion_component': -5.451489448547363, 'motion_component_percent': 78.59534025192261}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.702136516571045, 'force': [4.938201904296875, 3.471296548843384, -0.49013134837150574], 'magnitude': 6.0560688972473145, 'cosine_with_motion': 0.9009337425231934, 'motion_component': 5.456116676330566, 'motion_component_percent': 90.09337425231934}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.446988105773926, 'force': [-3.116992473602295, 10.654122352600098, 4.478387832641602], 'magnitude': 11.97004222869873, 'cosine_with_motion': -0.14450354874134064, 'motion_component': -1.7297135591506958, 'motion_component_percent': 14.450354874134064}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.780481815338135, 'force': [0.4535975754261017, -8.364376068115234, -2.0181007385253906], 'magnitude': 8.616336822509766, 'cosine_with_motion': -0.08463726192712784, 'motion_component': -0.729263186454773, 'motion_component_percent': 8.463726192712784}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.754653215408325, 'force': [5.390667915344238, -16.270679473876953, -13.218152046203613], 'magnitude': 21.64518165588379, 'cosine_with_motion': 0.17566996812820435, 'motion_component': 3.802408218383789, 'motion_component_percent': 17.566996812820435}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.599644422531128, 'force': [0.08243153244256973, 7.747219085693359, 7.453906536102295], 'magnitude': 10.75113582611084, 'cosine_with_motion': 0.06474582850933075, 'motion_component': 0.6960912346839905, 'motion_component_percent': 6.474582850933075}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 3.87046480178833, 'force': [-4.027907371520996, 5.400980472564697, 6.409460544586182], 'magnitude': 9.299237251281738, 'cosine_with_motion': -0.3908664286136627, 'motion_component': -3.6347596645355225, 'motion_component_percent': 39.08664286136627}]}, 3322: {'frame': 3322, 'motion_vector': [-1.1910209655761719, 1.1273345947265625, 1.091339111328125], 'ionic_force': [11.341214001178741, 1.8453324884176254, -4.039094507694244], 'ionic_force_magnitude': 12.179600627911743, 'radial_force': 11.490360612850333, 'axial_force': -4.039094507694244, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [9.554869204759598, 12.884615182876587, 1.8226514756679535], 'asn_force_magnitude': 16.144066784197587, 'residue_force': [9.554869204759598, 12.884615182876587, 1.8226514756679535], 'residue_force_magnitude': 16.144066784197587, 'total_force': [20.89608320593834, 14.729947671294212, -2.216443032026291], 'total_force_magnitude': 25.661844662120103, 'cosine_total_motion': -0.21168769630132703, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.16144797816748313, 'cosine_residue_motion': 0.16144797816748313, 'cosine_ionic_motion': -0.6600153787189091, 'motion_component_total': -5.432296779366711, 'motion_component_glu': None, 'motion_component_asn': 2.606426941709522, 'motion_component_residue': 2.606426941709522, 'motion_component_ionic': -8.038723721076233, 'motion_component_percent_total': 21.168769630132704, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 16.144797816748312, 'motion_component_percent_residue': 16.144797816748312, 'motion_component_percent_ionic': 66.00153787189092, 'ionic_contributions': [{'ion_id': 1306, 'distance': 8.663389205932617, 'force': [4.151607990264893, 0.16926394402980804, 1.5174075365066528], 'magnitude': 4.423462867736816, 'cosine_ionic_motion': -0.35551244020462036, 'motion_component_ionic': -1.5725960731506348, 'motion_component_percent_ionic': 35.551244020462036}, {'ion_id': 1307, 'distance': 12.226007461547852, 'force': [2.0877387523651123, -0.7246052622795105, -0.22269701957702637], 'magnitude': 2.2211034297943115, 'cosine_ionic_motion': -0.8105596303939819, 'motion_component_ionic': -1.8003367185592651, 'motion_component_percent_ionic': 81.0559630393982}, {'ion_id': 1387, 'distance': 13.204231262207031, 'force': [0.8166144490242004, 0.16744935512542725, -1.7120360136032104], 'magnitude': 1.904196858406067, 'cosine_ionic_motion': -0.707068681716919, 'motion_component_ionic': -1.3463979959487915, 'motion_component_percent_ionic': 70.7068681716919}, {'ion_id': 1460, 'distance': 8.941094398498535, 'force': [2.6996209621429443, 0.5092499852180481, -3.1144349575042725], 'magnitude': 4.152949810028076, 'cosine_ionic_motion': -0.7383261322975159, 'motion_component_ionic': -3.0662314891815186, 'motion_component_percent_ionic': 73.83261322975159}, {'ion_id': 2433, 'distance': 11.769852638244629, 'force': [1.5856318473815918, 1.7239744663238525, -0.5073340535163879], 'magnitude': 2.3966026306152344, 'cosine_ionic_motion': -0.10563347488641739, 'motion_component_ionic': -0.2531614601612091, 'motion_component_percent_ionic': 10.563347488641739}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.1563720703125, 'force': [-2.6074059009552, -13.449638366699219, 0.2574821412563324], 'magnitude': 13.702468872070312, 'cosine_with_motion': -0.4362647533416748, 'motion_component': -5.977904319763184, 'motion_component_percent': 43.62647533416748}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.21524977684021, 'force': [7.510493278503418, 17.48997688293457, -0.7057549357414246], 'magnitude': 19.04743766784668, 'cosine_with_motion': 0.26656079292297363, 'motion_component': 5.077300071716309, 'motion_component_percent': 26.656079292297363}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.132801055908203, 'force': [2.618009328842163, 11.14928150177002, 1.728433609008789], 'magnitude': 11.58222484588623, 'cosine_with_motion': 0.4969041049480438, 'motion_component': 5.755255222320557, 'motion_component_percent': 49.69041049480438}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.191195011138916, 'force': [-1.855749249458313, -4.612452030181885, -1.4156352281570435], 'magnitude': 5.169384956359863, 'cosine_with_motion': -0.44529542326927185, 'motion_component': -2.301903486251831, 'motion_component_percent': 44.529542326927185}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.901503562927246, 'force': [-0.4347606599330902, -3.929887056350708, -0.6050654053688049], 'magnitude': 3.999891757965088, 'cosine_with_motion': -0.5803574919700623, 'motion_component': -2.3213672637939453, 'motion_component_percent': 58.035749197006226}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.67315149307251, 'force': [3.523135185241699, 6.240754127502441, 1.65395987033844], 'magnitude': 7.354935646057129, 'cosine_with_motion': 0.3205554187297821, 'motion_component': 2.3576645851135254, 'motion_component_percent': 32.05554187297821}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.831563472747803, 'force': [-7.883199691772461, -9.597227096557617, -4.07584810256958], 'magnitude': 13.071500778198242, 'cosine_with_motion': -0.22829198837280273, 'motion_component': -2.984118938446045, 'motion_component_percent': 22.829198837280273}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.132293224334717, 'force': [3.936645746231079, 3.2974867820739746, 1.2648983001708984], 'magnitude': 5.288720607757568, 'cosine_with_motion': 0.039275337010622025, 'motion_component': 0.20771628618240356, 'motion_component_percent': 3.9275337010622025}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 3.9971368312835693, 'force': [4.747701168060303, 6.29632043838501, 3.7201812267303467], 'magnitude': 8.719178199768066, 'cosine_with_motion': 0.3204183876514435, 'motion_component': 2.7937850952148438, 'motion_component_percent': 32.04183876514435}]}, 3323: {'frame': 3323, 'motion_vector': [-0.09119033813476562, -1.4596443176269531, 0.58355712890625], 'ionic_force': [11.9672349691391, 4.672180593013763, -4.230508267879486], 'ionic_force_magnitude': 13.525575200519821, 'radial_force': 12.8469445511499, 'axial_force': -4.230508267879486, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [12.794849157333374, 12.295886993408203, -3.5123274326324463], 'asn_force_magnitude': 18.089594962508198, 'residue_force': [12.794849157333374, 12.295886993408203, -3.5123274326324463], 'residue_force_magnitude': 18.089594962508198, 'total_force': [24.762084126472473, 16.968067586421967, -7.742835700511932], 'total_force_magnitude': 31.00044568371568, 'cosine_total_motion': -0.6462064208764561, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.7430103328275136, 'cosine_residue_motion': -0.7430103328275136, 'cosine_ionic_motion': -0.48736789225699, 'motion_component_total': -20.03268705084889, 'motion_component_glu': None, 'motion_component_asn': -13.44075597380813, 'motion_component_residue': -13.44075597380813, 'motion_component_ionic': -6.59193107704076, 'motion_component_percent_total': 64.6206420876456, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 74.30103328275136, 'motion_component_percent_residue': 74.30103328275136, 'motion_component_percent_ionic': 48.736789225699, 'ionic_contributions': [{'ion_id': 1306, 'distance': 8.208459854125977, 'force': [3.659790277481079, 1.3112963438034058, 3.027434825897217], 'magnitude': 4.927364826202393, 'cosine_ionic_motion': -0.06200550124049187, 'motion_component_ionic': -0.30552372336387634, 'motion_component_percent_ionic': 6.200550124049187}, {'ion_id': 1307, 'distance': 11.098809242248535, 'force': [2.6004390716552734, -0.6885156631469727, -0.16605886816978455], 'magnitude': 2.695164680480957, 'cosine_ionic_motion': 0.1580989509820938, 'motion_component_ionic': 0.4261026978492737, 'motion_component_percent_ionic': 15.809895098209381}, {'ion_id': 1387, 'distance': 11.813334465026855, 'force': [0.8393199443817139, 0.3989105820655823, -2.18998122215271], 'magnitude': 2.3789925575256348, 'cosine_ionic_motion': -0.5170273780822754, 'motion_component_ionic': -1.2300043106079102, 'motion_component_percent_ionic': 51.70273780822754}, {'ion_id': 1460, 'distance': 7.422881603240967, 'force': [3.4794766902923584, 1.5985596179962158, -4.6523637771606445], 'magnitude': 6.02549934387207, 'cosine_ionic_motion': -0.5655173659324646, 'motion_component_ionic': -3.407524585723877, 'motion_component_percent_ionic': 56.55173659324646}, {'ion_id': 2433, 'distance': 11.547141075134277, 'force': [1.3882089853286743, 2.0519297122955322, -0.24953922629356384], 'magnitude': 2.4899415969848633, 'cosine_ionic_motion': -0.833345353603363, 'motion_component_ionic': -2.074981212615967, 'motion_component_percent_ionic': 83.3345353603363}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.5001673698425293, 'force': [-6.819509029388428, -17.08074951171875, 5.922703266143799], 'magnitude': 19.32190704345703, 'cosine_with_motion': 0.9535027742385864, 'motion_component': 18.423492431640625, 'motion_component_percent': 95.35027742385864}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.5544488430023193, 'force': [17.15321159362793, 22.74156951904297, -9.96096420288086], 'magnitude': 30.176687240600586, 'cosine_with_motion': -0.8538387417793274, 'motion_component': -25.76602554321289, 'motion_component_percent': 85.38387417793274}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.368577003479004, 'force': [6.918120384216309, 14.368143081665039, -1.1591911315917969], 'magnitude': 15.988986015319824, 'cosine_with_motion': -0.8849396705627441, 'motion_component': -14.149288177490234, 'motion_component_percent': 88.49396705627441}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.267806529998779, 'force': [-3.960157871246338, -6.458460330963135, -1.0496279001235962], 'magnitude': 7.648285865783691, 'cosine_with_motion': 0.7619013786315918, 'motion_component': 5.827239513397217, 'motion_component_percent': 76.19013786315918}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.107175350189209, 'force': [-1.6006189584732056, -5.089155197143555, 0.2518254518508911], 'magnitude': 5.340870380401611, 'cosine_with_motion': 0.918125569820404, 'motion_component': 4.903589725494385, 'motion_component_percent': 91.8125569820404}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.4539008140563965, 'force': [1.103803038597107, 3.8145394325256348, 2.482927083969116], 'magnitude': 4.683376789093018, 'cosine_with_motion': -0.5721858739852905, 'motion_component': -2.679762125015259, 'motion_component_percent': 57.21858739852905}]}, 3325: {'frame': 3325, 'motion_vector': [-1.0484428405761719, -1.0520210266113281, -0.158599853515625], 'ionic_force': [13.136695861816406, 2.739805907011032, -4.366748213768005], 'ionic_force_magnitude': 14.111973800160023, 'radial_force': 13.419363419102892, 'axial_force': -4.366748213768005, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [2.0107651948928833, 4.5555925369262695, 1.0442612171173096], 'asn_force_magnitude': 5.087934897487021, 'residue_force': [2.0107651948928833, 4.5555925369262695, 1.0442612171173096], 'residue_force_magnitude': 5.087934897487021, 'total_force': [15.14746105670929, 7.295398443937302, -3.322486996650696], 'total_force_magnitude': 17.137891782924765, 'cosine_total_motion': -0.89961937520066, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.9298052315041389, 'cosine_residue_motion': -0.9298052315041389, 'cosine_ionic_motion': -0.7572853495982408, 'motion_component_total': -15.417579498011303, 'motion_component_glu': None, 'motion_component_asn': -4.730788485235907, 'motion_component_residue': -4.730788485235907, 'motion_component_ionic': -10.686791012775398, 'motion_component_percent_total': 89.961937520066, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 92.98052315041389, 'motion_component_percent_residue': 92.98052315041389, 'motion_component_percent_ionic': 75.72853495982407, 'ionic_contributions': [{'ion_id': 1306, 'distance': 8.27988052368164, 'force': [4.4394755363464355, 0.9520545601844788, 1.6842352151870728], 'magnitude': 4.842726230621338, 'cosine_ionic_motion': -0.8188536763191223, 'motion_component_ionic': -3.965484142303467, 'motion_component_percent_ionic': 81.88536763191223}, {'ion_id': 1307, 'distance': 10.302607536315918, 'force': [2.6720001697540283, -1.5414988994598389, -0.5172479152679443], 'magnitude': 3.1278345584869385, 'cosine_ionic_motion': -0.23495399951934814, 'motion_component_ionic': -0.734897255897522, 'motion_component_percent_ionic': 23.495399951934814}, {'ion_id': 1387, 'distance': 12.010658264160156, 'force': [1.0765461921691895, 0.23434945940971375, -2.0206117630004883], 'magnitude': 2.3014655113220215, 'cosine_ionic_motion': -0.3068244457244873, 'motion_component_ionic': -0.7061458826065063, 'motion_component_percent_ionic': 30.68244457244873}, {'ion_id': 1460, 'distance': 9.120766639709473, 'force': [2.5632970333099365, 0.5630773901939392, -3.0066704750061035], 'magnitude': 3.9909415245056152, 'cosine_ionic_motion': -0.4701994061470032, 'motion_component_ionic': -1.8765382766723633, 'motion_component_percent_ionic': 47.01994061470032}, {'ion_id': 2433, 'distance': 9.718379974365234, 'force': [2.3853769302368164, 2.5318233966827393, -0.506453275680542], 'magnitude': 3.515202283859253, 'cosine_ionic_motion': -0.9682872891426086, 'motion_component_ionic': -3.4037256240844727, 'motion_component_percent_ionic': 96.82872891426086}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.9098193645477295, 'force': [-2.2039787769317627, -15.255782127380371, -1.4805901050567627], 'magnitude': 15.485107421875, 'cosine_with_motion': 0.8039302229881287, 'motion_component': 12.448945999145508, 'motion_component_percent': 80.39302229881287}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.873441457748413, 'force': [7.1205620765686035, 22.27750015258789, 4.664998531341553], 'magnitude': 23.848514556884766, 'cosine_with_motion': -0.8882526159286499, 'motion_component': -21.18350601196289, 'motion_component_percent': 88.82526159286499}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.024945259094238, 'force': [2.1752514839172363, 11.53020191192627, 2.8921031951904297], 'magnitude': 12.08476448059082, 'cosine_with_motion': -0.8237401843070984, 'motion_component': -9.954706192016602, 'motion_component_percent': 82.37401843070984}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.167775630950928, 'force': [-1.2281134128570557, -4.590771198272705, -2.151001453399658], 'magnitude': 5.216344356536865, 'cosine_with_motion': 0.8288804888725281, 'motion_component': 4.323726177215576, 'motion_component_percent': 82.88804888725281}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.832415580749512, 'force': [-0.3578742742538452, -4.011233806610107, -0.7434439659118652], 'magnitude': 4.095213890075684, 'cosine_with_motion': 0.7704776525497437, 'motion_component': 3.15527081489563, 'motion_component_percent': 77.04776525497437}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.391584873199463, 'force': [-3.495081901550293, -5.394322395324707, -2.1378049850463867], 'magnitude': 6.773811340332031, 'cosine_with_motion': 0.9565487504005432, 'motion_component': 6.479480743408203, 'motion_component_percent': 95.65487504005432}]}, 3326: {'frame': 3326, 'motion_vector': [0.80645751953125, 0.5555877685546875, -0.410614013671875], 'ionic_force': [13.417050004005432, 2.1709354370832443, -3.8333840072155], 'ionic_force_magnitude': 14.121792535961626, 'radial_force': 13.591548531420766, 'axial_force': -3.8333840072155, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [2.8685702085494995, 5.435973882675171, -1.2763834595680237], 'asn_force_magnitude': 6.277552216458508, 'residue_force': [2.8685702085494995, 5.435973882675171, -1.2763834595680237], 'residue_force_magnitude': 6.277552216458508, 'total_force': [16.28562021255493, 7.606909319758415, -5.109767466783524], 'total_force_magnitude': 18.686792626644213, 'cosine_total_motion': 0.9805678668282146, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.8787073227483828, 'cosine_residue_motion': 0.8787073227483828, 'cosine_ionic_motion': 0.9069342471656812, 'motion_component_total': 18.323668383769725, 'motion_component_glu': None, 'motion_component_asn': 5.516131101537432, 'motion_component_residue': 5.516131101537432, 'motion_component_ionic': 12.807537282232293, 'motion_component_percent_total': 98.05678668282147, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 87.87073227483828, 'motion_component_percent_residue': 87.87073227483828, 'motion_component_percent_ionic': 90.69342471656812, 'ionic_contributions': [{'ion_id': 1306, 'distance': 7.224223613739014, 'force': [5.361866474151611, 1.3586233854293823, 3.1420536041259766], 'magnitude': 6.361443996429443, 'cosine_ionic_motion': 0.5608614683151245, 'motion_component_ionic': 3.5678887367248535, 'motion_component_percent_ionic': 56.08614683151245}, {'ion_id': 1307, 'distance': 10.580955505371094, 'force': [2.534034490585327, -1.4627076387405396, -0.48265519738197327], 'magnitude': 2.9654343128204346, 'cosine_ionic_motion': 0.4538269639015198, 'motion_component_ionic': 1.3457940816879272, 'motion_component_percent_ionic': 45.38269639015198}, {'ion_id': 1387, 'distance': 12.873809814453125, 'force': [0.7306075096130371, 0.05163702368736267, -1.8644970655441284], 'magnitude': 2.0031981468200684, 'cosine_ionic_motion': 0.6503711342811584, 'motion_component_ionic': 1.302822232246399, 'motion_component_percent_ionic': 65.03711342811584}, {'ion_id': 1460, 'distance': 8.178290367126465, 'force': [2.9076755046844482, 0.214521124958992, -4.017284393310547], 'magnitude': 4.963785648345947, 'cosine_ionic_motion': 0.7804169654846191, 'motion_component_ionic': 3.8738224506378174, 'motion_component_percent_ionic': 78.04169654846191}, {'ion_id': 2433, 'distance': 10.849812507629395, 'force': [1.8828660249710083, 2.008861541748047, -0.6110009551048279], 'magnitude': 2.820289134979248, 'cosine_ionic_motion': 0.9634509086608887, 'motion_component_ionic': 2.717210054397583, 'motion_component_percent_ionic': 96.34509086608887}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.632572650909424, 'force': [-2.9538981914520264, -10.626333236694336, -0.1438537836074829], 'magnitude': 11.030193328857422, 'cosine_with_motion': -0.702375590801239, 'motion_component': -7.747338771820068, 'motion_component_percent': 70.2375590801239}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.869371175765991, 'force': [6.285953044891357, 11.549616813659668, 0.2510470747947693], 'magnitude': 13.151801109313965, 'cosine_with_motion': 0.8150550723075867, 'motion_component': 10.719442367553711, 'motion_component_percent': 81.50550723075867}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.474891185760498, 'force': [2.559556722640991, 9.622541427612305, 2.1186726093292236], 'magnitude': 10.180049896240234, 'cosine_with_motion': 0.6050135493278503, 'motion_component': 6.1590681076049805, 'motion_component_percent': 60.501354932785034}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.540660858154297, 'force': [-1.4735945463180542, -3.9685699939727783, -1.6343446969985962], 'magnitude': 4.537853240966797, 'cosine_with_motion': -0.5649118423461914, 'motion_component': -2.5634870529174805, 'motion_component_percent': 56.49118423461914}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.17544412612915, 'force': [2.6576550006866455, 8.071651458740234, 2.4264745712280273], 'magnitude': 8.837559700012207, 'cosine_with_motion': 0.600067138671875, 'motion_component': 5.303129196166992, 'motion_component_percent': 60.0067138671875}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.230767250061035, 'force': [-4.207101821899414, -9.212932586669922, -4.294379234313965], 'magnitude': 11.000887870788574, 'cosine_with_motion': -0.5776517987251282, 'motion_component': -6.354682922363281, 'motion_component_percent': 57.76517987251282}]}, 3327: {'frame': 3327, 'motion_vector': [-0.40179443359375, 0.5124359130859375, 0.6054840087890625], 'ionic_force': [21.70894306898117, 0.4854571521282196, -6.7340773940086365], 'ionic_force_magnitude': 22.734592060719194, 'radial_force': 21.714370306753498, 'axial_force': -6.7340773940086365, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [6.768657088279724, 10.94654893875122, 7.805947452783585], 'asn_force_magnitude': 15.052390776312357, 'residue_force': [6.768657088279724, 10.94654893875122, 7.805947452783585], 'residue_force_magnitude': 15.052390776312357, 'total_force': [28.477600157260895, 11.43200609087944, 1.0718700587749481], 'total_force_magnitude': 30.70526631380403, 'cosine_total_motion': -0.18075161806575235, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.5690387661741516, 'cosine_residue_motion': 0.5690387661741516, 'cosine_ionic_motion': -0.6208785452135951, 'motion_component_total': -5.550026569359918, 'motion_component_glu': None, 'motion_component_asn': 8.565393875323965, 'motion_component_residue': 8.565393875323965, 'motion_component_ionic': -14.115420444683883, 'motion_component_percent_total': 18.075161806575235, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 56.903876617415165, 'motion_component_percent_residue': 56.903876617415165, 'motion_component_percent_ionic': 62.08785452135951, 'ionic_contributions': [{'ion_id': 1306, 'distance': 4.783001899719238, 'force': [14.490052223205566, -0.3445451557636261, -0.7261050343513489], 'magnitude': 14.512324333190918, 'cosine_ionic_motion': -0.49893006682395935, 'motion_component_ionic': -7.240634918212891, 'motion_component_percent_ionic': 49.893006682395935}, {'ion_id': 1307, 'distance': 11.25306510925293, 'force': [2.2564868927001953, -1.2306782007217407, -0.5171406269073486], 'magnitude': 2.62178111076355, 'cosine_ionic_motion': -0.7937460541725159, 'motion_component_ionic': -2.</t>
         </is>
       </c>
     </row>
@@ -547,7 +547,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>{4333: {'frame': 4333, 'ionic_force': [10.218847453594208, 2.7001716569066048, -15.040524646639824], 'ionic_force_magnitude': 18.382958192379444, 'motion_vector': [-1.0914764404296875, 2.8184471130371094, 0.5848388671875], 'ionic_force_x': 10.218847453594208, 'ionic_force_y': 2.7001716569066048, 'ionic_force_z': -15.040524646639824, 'radial_force': 10.569568120627757, 'axial_force': -15.040524646639824, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [3.5677709579467773, 4.624752044677734, 1.8411636352539062], 'asn_force_magnitude': 6.124312583049687, 'residue_force': [3.5677709579467773, 4.624752044677734, 1.8411636352539062], 'residue_force_magnitude': 6.124312583049687, 'total_force': [13.786618411540985, 7.324923701584339, -13.199361011385918], 'total_force_magnitude': 20.443788434836815, 'motion_component_total': -0.689419172472987, 'cosine_total_motion': -0.0337226720316767, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.5419283245041114, 'cosine_residue_motion': 0.5419283245041114, 'cosine_ionic_motion': -0.21804747567810898, 'motion_component_glu': None, 'motion_component_asn': 3.318938456871564, 'motion_component_residue': 3.318938456871564, 'motion_component_ionic': -4.008357629344551, 'ionic_contributions': [{'ion_id': 1306, 'distance': 7.030627250671387, 'force': [1.9004194736480713, 6.339089393615723, 1.1476751565933228], 'magnitude': 6.716607093811035}, {'ion_id': 1307, 'distance': 8.677374839782715, 'force': [2.6483633518218994, -3.5226809978485107, -0.1344403475522995], 'magnitude': 4.409215927124023}, {'ion_id': 1308, 'distance': 14.20415210723877, 'force': [0.17358297109603882, -0.07655664533376694, -1.6345635652542114], 'magnitude': 1.6455363035202026}, {'ion_id': 1316, 'distance': 9.113018035888672, 'force': [0.8972761631011963, -0.14553450047969818, -3.8930156230926514], 'magnitude': 3.9977312088012695}, {'ion_id': 1387, 'distance': 5.375945568084717, 'force': [4.599205493927002, 0.10585440695285797, -10.526180267333984], 'magnitude': 11.487574577331543}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.533482551574707, 'force': [4.31558895111084, 4.671905040740967, -0.9512782096862793], 'magnitude': 6.430858135223389}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.743353366851807, 'force': [-0.9748809337615967, 8.454612731933594, 6.185499668121338], 'magnitude': 10.520992279052734}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.188126087188721, 'force': [-0.8626163005828857, -6.304483890533447, -3.609175205230713], 'magnitude': 7.315515518188477}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.913429021835327, 'force': [1.696218729019165, -12.744790077209473, -15.22091007232666], 'magnitude': 19.92443084716797}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.5858659744262695, 'force': [1.7662837505340576, 6.371105670928955, 8.582714080810547], 'magnitude': 10.833915710449219}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.079699516296387, 'force': [-2.3728232383728027, 4.176402568817139, 6.854313373565674], 'magnitude': 8.369841575622559}]}, 4335: {'frame': 4335, 'ionic_force': [9.905854746699333, 2.9460261538624763, -22.515233606100082], 'ionic_force_magnitude': 24.773792053280943, 'motion_vector': [-2.4897499084472656, -1.9592094421386719, -2.6416397094726562], 'ionic_force_x': 9.905854746699333, 'ionic_force_y': 2.9460261538624763, 'ionic_force_z': -22.515233606100082, 'radial_force': 10.334651825869484, 'axial_force': -22.515233606100082, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [4.829582959413528, 6.925490617752075, 6.043889671564102], 'asn_force_magnitude': 10.383443273811862, 'residue_force': [4.829582959413528, 6.925490617752075, 6.043889671564102], 'residue_force_magnitude': 10.383443273811862, 'total_force': [14.735437706112862, 9.871516771614552, -16.47134393453598], 'total_force_magnitude': 24.205064320773353, 'motion_component_total': -3.0343199210512886, 'cosine_total_motion': -0.1253588869188488, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.9702796276735125, 'cosine_residue_motion': -0.9702796276735125, 'cosine_ionic_motion': 0.2841924053245415, 'motion_component_glu': None, 'motion_component_asn': -10.074843473683211, 'motion_component_residue': -10.074843473683211, 'motion_component_ionic': 7.040523552631923, 'ionic_contributions': [{'ion_id': 1306, 'distance': 8.269227981567383, 'force': [-0.3307041525840759, 4.825318336486816, 0.4242839515209198], 'magnitude': 4.8552117347717285}, {'ion_id': 1307, 'distance': 8.450594902038574, 'force': [3.035064935684204, -3.5079329013824463, -0.3104632496833801], 'magnitude': 4.649043083190918}, {'ion_id': 1308, 'distance': 14.563118934631348, 'force': [0.17067889869213104, -0.07447502017021179, -1.5542986392974854], 'magnitude': 1.565414309501648}, {'ion_id': 1316, 'distance': 9.559685707092285, 'force': [0.7298926711082458, 0.04116610437631607, -3.5585622787475586], 'magnitude': 3.632878065109253}, {'ion_id': 1387, 'distance': 4.214784622192383, 'force': [6.300922393798828, 1.661949634552002, -17.516193389892578], 'magnitude': 18.68905258178711}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.76469612121582, 'force': [-4.433062553405762, -5.54639196395874, 0.5704285502433777], 'magnitude': 7.123194217681885}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.975369930267334, 'force': [5.955981254577637, 5.24924373626709, -0.496473103761673], 'magnitude': 7.954543113708496}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.314467430114746, 'force': [-0.821997344493866, 7.551161766052246, 3.5425148010253906], 'magnitude': 8.381237030029297}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.3444623947143555, 'force': [-0.7999061346054077, -13.655682563781738, -8.617050170898438], 'magnitude': 16.166975021362305}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.364649295806885, 'force': [1.9568079710006714, 6.213186264038086, 3.322962522506714], 'magnitude': 7.312650680541992}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.044857978820801, 'force': [-0.38029196858406067, 6.085940361022949, 5.942730903625488], 'magnitude': 8.514655113220215}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.952569007873535, 'force': [3.3520517349243164, 1.0280330181121826, 1.7787761688232422], 'magnitude': 3.9315578937530518}]}, 4336: {'frame': 4336, 'ionic_force': [-1.1519034951925278, -1.205802470445633, -12.496924042701721], 'ionic_force_magnitude': 12.607694150360162, 'motion_vector': [0.6896553039550781, 0.1011199951171875, 0.940399169921875], 'ionic_force_x': -1.1519034951925278, 'ionic_force_y': -1.205802470445633, 'ionic_force_z': -12.496924042701721, 'radial_force': 1.667585458070906, 'axial_force': -12.496924042701721, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-1.998314619064331, -11.548934876918793, -1.6533186435699463], 'asn_force_magnitude': 11.83657976973304, 'residue_force': [-1.998314619064331, -11.548934876918793, -1.6533186435699463], 'residue_force_magnitude': 11.83657976973304, 'total_force': [-3.150218114256859, -12.754737347364426, -14.150242686271667], 'total_force_magnitude': 19.308976333509495, 'motion_component_total': -14.325846576919169, 'cosine_total_motion': -0.7419267769290067, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.2959686083944419, 'cosine_residue_motion': -0.2959686083944419, 'cosine_ionic_motion': -0.858411570367315, 'motion_component_glu': None, 'motion_component_asn': -3.503256042597691, 'motion_component_residue': -3.503256042597691, 'motion_component_ionic': -10.822590534321478, 'ionic_contributions': [{'ion_id': 1306, 'distance': 8.297228813171387, 'force': [-1.9411698579788208, 3.975846767425537, -1.9185880422592163], 'magnitude': 4.8224968910217285}, {'ion_id': 1307, 'distance': 9.114627838134766, 'force': [1.3281068801879883, -3.4387872219085693, -1.5431928634643555], 'magnitude': 3.996319532394409}, {'ion_id': 1316, 'distance': 11.616941452026367, 'force': [-0.19560758769512177, -0.3452792465686798, -2.427891969680786], 'magnitude': 2.4601097106933594}, {'ion_id': 1387, 'distance': 7.006906032562256, 'force': [-0.3432329297065735, -1.397582769393921, -6.607251167297363], 'magnitude': 6.762160301208496}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.808727264404297, 'force': [-3.573249340057373, 7.851780414581299, -2.714258909225464], 'magnitude': 9.043548583984375}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.166891574859619, 'force': [1.3632164001464844, -4.737532138824463, 1.7106449604034424], 'magnitude': 5.218129634857178}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.609676837921143, 'force': [2.4141554832458496, -3.4597537517547607, 1.341355323791504], 'magnitude': 4.426881313323975}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.236931800842285, 'force': [-10.689862251281738, 7.426120281219482, -2.1117420196533203], 'magnitude': 13.186351776123047}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.4410440921783447, 'force': [15.346685409545898, -6.299398899078369, 1.1598154306411743], 'magnitude': 16.629743576049805}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.193416118621826, 'force': [10.235634803771973, -13.267374038696289, 4.5079779624938965], 'magnitude': 17.352615356445312}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.423757553100586, 'force': [-5.362268447875977, 10.251153945922852, -2.718930959701538], 'magnitude': 11.884135246276855}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.135996341705322, 'force': [-2.7916762828826904, 4.2870192527771, -1.3107243776321411], 'magnitude': 5.281097412109375}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.594569444656372, 'force': [15.601705551147461, 7.704370498657227, 5.7327880859375], 'magnitude': 18.320354461669922}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.546199321746826, 'force': [-23.320262908935547, -18.13536262512207, -7.054473876953125], 'magnitude': 30.372547149658203}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.983973264694214, 'force': [-16.482017517089844, -2.8371663093566895, -9.481409072875977], 'magnitude': 19.225074768066406}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.3962671756744385, 'force': [9.966341972351074, -0.7564395070075989, 6.779455661773682], 'magnitude': 12.077301025390625}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.8707661628723145, 'force': [5.293282508850098, 0.42364799976348877, 2.50618314743042], 'magnitude': 5.871905326843262}]}, 4337: {'frame': 4337, 'ionic_force': [-0.19163120537996292, 0.32513704895973206, -11.826547503471375], 'ionic_force_magnitude': 11.832567873092747, 'motion_vector': [-1.2149238586425781, 0.8994140625, 1.17535400390625], 'ionic_force_x': -0.19163120537996292, 'ionic_force_y': 0.32513704895973206, 'ionic_force_z': -11.826547503471375, 'radial_force': 0.3774077628793832, 'axial_force': -11.826547503471375, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [8.216361999511719, -4.510262191295624, 1.8031255006790161], 'asn_force_magnitude': 9.544754114824014, 'residue_force': [8.216361999511719, -4.510262191295624, 1.8031255006790161], 'residue_force_magnitude': 9.544754114824014, 'total_force': [8.024730794131756, -4.185125142335892, -10.023422002792358], 'total_force_magnitude': 13.50483489056273, 'motion_component_total': -13.210111786226161, 'cosine_total_motion': -0.9781764748162509, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.652187027568698, 'cosine_residue_motion': -0.652187027568698, 'cosine_ionic_motion': -0.5903322969386221, 'motion_component_glu': None, 'motion_component_asn': -6.224964815021172, 'motion_component_residue': -6.224964815021172, 'motion_component_ionic': -6.985146971204988, 'ionic_contributions': [{'ion_id': 1306, 'distance': 7.549276828765869, 'force': [-1.3619964122772217, 5.054660320281982, -2.5555646419525146], 'magnitude': 5.825421333312988}, {'ion_id': 1307, 'distance': 9.575133323669434, 'force': [1.334238886833191, -3.2292449474334717, -0.951119065284729], 'magnitude': 3.621166229248047}, {'ion_id': 1316, 'distance': 11.058213233947754, 'force': [-0.0917414203286171, -0.38027724623680115, -2.686659812927246], 'magnitude': 2.714989423751831}, {'ion_id': 1387, 'distance': 7.602648735046387, 'force': [-0.07213225960731506, -1.1200010776519775, -5.633203983306885], 'magnitude': 5.743917942047119}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.7457780838012695, 'force': [1.3774666786193848, -3.620861530303955, 1.6725267171859741], 'magnitude': 4.219644546508789}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.334958076477051, 'force': [-8.543743133544922, 9.23127555847168, -0.6823439598083496], 'magnitude': 12.596729278564453}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.4750232696533203, 'force': [10.193188667297363, -12.466917991638184, -2.5620980262756348], 'magnitude': 16.30611801147461}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.377269744873047, 'force': [9.8428373336792, -11.224483489990234, 5.545485019683838], 'magnitude': 15.925541877746582}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.88883900642395, 'force': [-4.0889387130737305, 7.124800205230713, -4.1678314208984375], 'magnitude': 9.211569786071777}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.285560607910156, 'force': [-3.191173553466797, 3.2229580879211426, -2.072108507156372], 'magnitude': 4.986449718475342}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.623368263244629, 'force': [9.301969528198242, 3.4288275241851807, 4.93491792678833], 'magnitude': 11.0741548538208}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.064777851104736, 'force': [-6.665158748626709, -0.7033438086509705, -3.7422866821289062], 'magnitude': 7.676179885864258}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.4305453300476074, 'force': [-19.863107681274414, -10.691112518310547, -12.784184455871582], 'magnitude': 25.92833137512207}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 2.922518253326416, 'force': [12.110390663146973, 2.985849380493164, 10.509305953979492], 'magnitude': 16.310192108154297}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 3.351707935333252, 'force': [7.742630958557129, 8.202746391296387, 5.151742935180664], 'magnitude': 12.400557518005371}]}, 4338: {'frame': 4338, 'ionic_force': [-1.9880583882331848, -1.188404381275177, -12.07487940788269], 'ionic_force_magnitude': 12.295014999721138, 'motion_vector': [1.5186386108398438, 5.265224456787109, -0.11255645751953125], 'ionic_force_x': -1.9880583882331848, 'ionic_force_y': -1.188404381275177, 'ionic_force_z': -12.07487940788269, 'radial_force': 2.3161781296908845, 'axial_force': -12.07487940788269, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-4.661213755607605, 3.588160276412964, 0.14355164766311646], 'asn_force_magnitude': 5.884081484840289, 'residue_force': [-4.661213755607605, 3.588160276412964, 0.14355164766311646], 'residue_force_magnitude': 5.884081484840289, 'total_force': [-6.64927214384079, 2.399755895137787, -11.931327760219574], 'total_force_magnitude': 13.868245401668226, 'motion_component_total': 0.7079639008624337, 'cosine_total_motion': 0.051049276989089905, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.3658090951674374, 'cosine_residue_motion': 0.3658090951674374, 'cosine_ionic_motion': -0.11748555191117914, 'motion_component_glu': None, 'motion_component_asn': 2.1524505238608977, 'motion_component_residue': 2.1524505238608977, 'motion_component_ionic': -1.4444866229984639, 'ionic_contributions': [{'ion_id': 1306, 'distance': 6.735961437225342, 'force': [-1.6397868394851685, 7.1292724609375, -0.15652811527252197], 'magnitude': 7.317098140716553}, {'ion_id': 1307, 'distance': 6.5452165603637695, 'force': [2.079728841781616, -7.2433953285217285, -1.8075493574142456], 'magnitude': 7.749792098999023}, {'ion_id': 1316, 'distance': 10.65501594543457, 'force': [-0.5445583462715149, -0.3111899495124817, -2.85630202293396], 'magnitude': 2.92435359954834}, {'ion_id': 1387, 'distance': 6.638399124145508, 'force': [-1.8834420442581177, -0.7630915641784668, -7.254499912261963], 'magnitude': 7.533752918243408}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.675151824951172, 'force': [-4.804211139678955, 5.200509071350098, 1.9730955362319946], 'magnitude': 7.3497514724731445}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.7113447189331055, 'force': [2.861213445663452, -4.979075908660889, -1.860718846321106], 'magnitude': 6.036556243896484}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.587115287780762, 'force': [11.007375717163086, -8.942174911499023, -3.029362201690674], 'magnitude': 14.501788139343262}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.7125494480133057, 'force': [-6.810189723968506, 7.069425582885742, 2.4081523418426514], 'magnitude': 10.107158660888672}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.801830768585205, 'force': [-5.306699275970459, 2.746837854385376, 0.8922334313392639], 'magnitude': 6.0417094230651855}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.047773838043213, 'force': [4.33180570602417, 5.8324785232543945, 5.790213584899902], 'magnitude': 9.29025936126709}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.836606502532959, 'force': [-4.4443440437316895, -3.5129165649414062, -6.2259111404418945], 'magnitude': 8.417526245117188}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.563413143157959, 'force': [-3.881063461303711, -11.172825813293457, -8.649303436279297], 'magnitude': 14.652820587158203}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.8671276569366455, 'force': [1.2050726413726807, 6.649488925933838, 6.411457061767578], 'magnitude': 9.315293312072754}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.069983005523682, 'force': [1.1798263788223267, 4.696413516998291, 2.4336953163146973], 'magnitude': 5.4195170402526855}]}, 4339: {'frame': 4339, 'ionic_force': [7.982106583658606, -1.4821966588497162, -13.919581286609173], 'ionic_force_magnitude': 16.114145203606412, 'motion_vector': [-0.3119239807128906, 0.11574172973632812, 2.2965164184570312], 'ionic_force_x': 7.982106583658606, 'ionic_force_y': -1.4821966588497162, 'ionic_force_z': -13.919581286609173, 'radial_force': 8.118554825114586, 'axial_force': -13.919581286609173, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-7.585148334503174, 0.5071490556001663, -5.471320137381554], 'asn_force_magnitude': 9.366270307156917, 'residue_force': [-7.585148334503174, 0.5071490556001663, -5.471320137381554], 'residue_force_magnitude': 9.366270307156917, 'total_force': [0.396958249155432, -0.9750476032495499, -19.390901423990726], 'total_force_magnitude': 19.419458069552324, 'motion_component_total': -19.292551592710545, 'cosine_total_motion': -0.9934649836062751, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.4665558962243783, 'cosine_residue_motion': -0.4665558962243783, 'cosine_ionic_motion': -0.9260598540427335, 'motion_component_glu': None, 'motion_component_asn': -4.369888637435379, 'motion_component_residue': -4.369888637435379, 'motion_component_ionic': -14.922662955275168, 'ionic_contributions': [{'ion_id': 1306, 'distance': 12.086974143981934, 'force': [-0.076982282102108, 2.2683990001678467, -0.11256872862577438], 'magnitude': 2.2724947929382324}, {'ion_id': 1307, 'distance': 4.773991107940674, 'force': [8.069611549377441, -11.067646980285645, -4.958900451660156], 'magnitude': 14.567159652709961}, {'ion_id': 1308, 'distance': 14.942962646484375, 'force': [0.015117759816348553, 0.40834537148475647, -1.4295883178710938], 'magnitude': 1.4868414402008057}, {'ion_id': 1316, 'distance': 10.61767578125, 'force': [-0.007704783696681261, 1.2880055904388428, -2.648350715637207], 'magnitude': 2.944958209991455}, {'ion_id': 1387, 'distance': 6.710808753967285, 'force': [-0.017935659736394882, 5.620700359344482, -4.770173072814941], 'magnitude': 7.37205171585083}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.018038272857666, 'force': [6.271729946136475, 0.11264830827713013, 7.001832485198975], 'magnitude': 9.400688171386719}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.0668745040893555, 'force': [-6.8335700035095215, 1.300106167793274, -9.661827087402344], 'magnitude': 11.905412673950195}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.531255722045898, 'force': [-5.787351131439209, -2.1102218627929688, -7.843906879425049], 'magnitude': 9.9736328125}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.363516807556152, 'force': [2.0502943992614746, 1.2441344261169434, 4.206985950469971], 'magnitude': 4.8425517082214355}, {'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.54049825668335, 'force': [-7.7058868408203125, 0.24992693960666656, -0.14709018170833588], 'magnitude': 7.711341857910156}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.7624359130859375, 'force': [8.936247825622559, 1.0477044582366943, 1.8685365915298462], 'magnitude': 9.189430236816406}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.390146732330322, 'force': [-4.516612529754639, -1.3371493816375732, -0.8958510160446167], 'magnitude': 4.794820785522461}]}, 4342: {'frame': 4342, 'ionic_force': [0.36002762615680695, -0.6625969856977463, -12.154103636741638], 'ionic_force_magnitude': 12.17747469181144, 'motion_vector': [-2.657154083251953, -1.6822662353515625, 5.648590087890625], 'ionic_force_x': 0.36002762615680695, 'ionic_force_y': -0.6625969856977463, 'ionic_force_z': -12.154103636741638, 'radial_force': 0.7540919420414496, 'axial_force': -12.154103636741638, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-1.7132823467254639, 6.230952024459839, 3.035045027732849], 'asn_force_magnitude': 7.139439603434374, 'residue_force': [-1.7132823467254639, 6.230952024459839, 3.035045027732849], 'residue_force_magnitude': 7.139439603434374, 'total_force': [-1.353254720568657, 5.568355038762093, -9.119058609008789], 'total_force_magnitude': 10.770102417850344, 'motion_component_total': -8.86015509442096, 'cosine_total_motion': -0.8226621020554232, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.24295504586859484, 'cosine_residue_motion': 0.24295504586859484, 'cosine_ionic_motion': -0.8700258665184236, 'motion_component_glu': None, 'motion_component_asn': 1.7345628763284608, 'motion_component_residue': 1.7345628763284608, 'motion_component_ionic': -10.594717970749421, 'ionic_contributions': [{'ion_id': 1306, 'distance': 10.719278335571289, 'force': [-0.24011437594890594, 2.6392462253570557, -1.151229977607727], 'magnitude': 2.8893954753875732}, {'ion_id': 1307, 'distance': 7.315350532531738, 'force': [1.9842231273651123, -4.65313720703125, -3.5916688442230225], 'magnitude': 6.203943252563477}, {'ion_id': 1316, 'distance': 12.332013130187988, 'force': [-0.2974294424057007, 0.23622436821460724, -2.1497864723205566], 'magnitude': 2.183082342147827}, {'ion_id': 1387, 'distance': 7.778631687164307, 'force': [-1.0866516828536987, 1.1150696277618408, -5.261418342590332], 'magnitude': 5.4869585037231445}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.704615592956543, 'force': [12.616436958312988, -10.850533485412598, 4.537448883056641], 'magnitude': 17.24810218811035}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.030694007873535, 'force': [-11.430656433105469, 17.945898056030273, -2.6205928325653076], 'magnitude': 21.43787956237793}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.750706911087036, 'force': [-16.150854110717773, 8.964676856994629, -11.369834899902344], 'magnitude': 21.690750122070312}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.1222000122070312, 'force': [9.01647663116455, -4.638064384460449, 10.070466995239258], 'magnitude': 14.290654182434082}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.455587863922119, 'force': [5.754631042480469, -1.7799017429351807, 3.599611520767212], 'magnitude': 7.017195224761963}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.711827278137207, 'force': [4.374838352203369, -7.956341743469238, 2.2440872192382812], 'magnitude': 9.352994918823242}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.976241111755371, 'force': [-1.970184087753296, 5.045817852020264, -1.5184667110443115], 'magnitude': 5.62562370300293}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.733818531036377, 'force': [-2.60467529296875, 3.191467761993408, -0.9922808408737183], 'magnitude': 4.2372660636901855}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.692897319793701, 'force': [4.100759506225586, 6.0411057472229, 0.1930396556854248], 'magnitude': 7.304002285003662}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.079403877258301, 'force': [-3.1928701400756836, -6.847381114959717, -1.080253005027771], 'magnitude': 7.632037162780762}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.297802448272705, 'force': [-7.500580787658691, -7.770613670349121, 1.2486629486083984], 'magnitude': 10.871996879577637}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.368214130401611, 'force': [5.273396015167236, 4.884821891784668, -1.2768439054489136], 'magnitude': 7.300720691680908}]}, 4344: {'frame': 4344, 'ionic_force': [9.202361762523651, 8.81113064289093, -18.928253769874573], 'ionic_force_magnitude': 22.81662279986282, 'motion_vector': [1.4634857177734375, -1.2306327819824219, 0.8022537231445312], 'ionic_force_x': 9.202361762523651, 'ionic_force_y': 8.81113064289093, 'ionic_force_z': -18.928253769874573, 'radial_force': 12.74046644414752, 'axial_force': -18.928253769874573, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-1.3671069145202637, 2.4705255199223757, -14.21933102607727], 'asn_force_magnitude': 14.496960112019364, 'residue_force': [-1.3671069145202637, 2.4705255199223757, -14.21933102607727], 'residue_force_magnitude': 14.496960112019364, 'total_force': [7.8352548480033875, 11.281656162813306, -33.14758479595184], 'total_force_magnitude': 35.880765907571174, 'motion_component_total': -13.989884438962582, 'cosine_total_motion': -0.38989927012707903, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.547172058914251, 'cosine_residue_motion': -0.547172058914251, 'cosine_ionic_motion': -0.2654885860894187, 'motion_component_glu': None, 'motion_component_asn': -7.932331512491407, 'motion_component_residue': -7.932331512491407, 'motion_component_ionic': -6.057552926471175, 'ionic_contributions': [{'ion_id': 1306, 'distance': 13.459346771240234, 'force': [-0.3357532024383545, 1.7316968441009521, -0.49725770950317383], 'magnitude': 1.8326945304870605}, {'ion_id': 1307, 'distance': 4.361624717712402, 'force': [10.69202995300293, 3.909050941467285, -13.227506637573242], 'magnitude': 17.45185089111328}, {'ion_id': 1316, 'distance': 12.345357894897461, 'force': [-0.2957773804664612, 0.846617579460144, -1.985202670097351], 'magnitude': 2.1783652305603027}, {'ion_id': 1387, 'distance': 9.041485786437988, 'force': [-0.8581376075744629, 2.323765277862549, -3.2182867527008057], 'magnitude': 4.061237812042236}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.4186930656433105, 'force': [12.080121994018555, 2.4292454719543457, 16.07443618774414], 'magnitude': 20.253841400146484}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.586261749267578, 'force': [-10.830937385559082, -0.01949642412364483, -27.3740234375], 'magnitude': 29.43886375427246}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.272101879119873, 'force': [-8.195077896118164, -5.821994304656982, -13.359621047973633], 'magnitude': 16.719282150268555}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.195068359375, 'force': [2.3199331760406494, 3.7860662937164307, 6.5531439781188965], 'magnitude': 7.9158124923706055}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.038047790527344, 'force': [3.2588531970977783, 2.0967044830322266, 3.886733293533325], 'magnitude': 5.488441467285156}]}, 4345: {'frame': 4345, 'ionic_force': [14.981032002717257, 2.010621815919876, -19.484798073768616], 'ionic_force_magnitude': 24.66031783916478, 'motion_vector': [-1.1395187377929688, 0.0416717529296875, -1.0085220336914062], 'ionic_force_x': 14.981032002717257, 'ionic_force_y': 2.010621815919876, 'ionic_force_z': -19.484798073768616, 'radial_force': 15.115353781936154, 'axial_force': -19.484798073768616, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-11.528387069702148, -2.641897439956665, -3.2413852512836456], 'asn_force_magnitude': 12.263356345608017, 'residue_force': [-11.528387069702148, -2.641897439956665, -3.2413852512836456], 'residue_force_magnitude': 12.263356345608017, 'total_force': [3.452644933015108, -0.6312756240367889, -22.72618332505226], 'total_force_magnitude': 22.99562294157002, 'motion_component_total': 12.454421663036875, 'cosine_total_motion': 0.5415996641918566, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.8729072036061416, 'cosine_residue_motion': 0.8729072036061416, 'cosine_ionic_motion': 0.0709500007249627, 'motion_component_glu': None, 'motion_component_asn': 10.704772094470325, 'motion_component_residue': 10.704772094470325, 'motion_component_ionic': 1.7496495685665518, 'ionic_contributions': [{'ion_id': 1306, 'distance': 9.631107330322266, 'force': [-0.47127556800842285, 3.423821449279785, -0.9305918216705322], 'magnitude': 3.579197406768799}, {'ion_id': 1307, 'distance': 4.17344856262207, 'force': [15.362360000610352, -7.023677349090576, -8.83127212524414], 'magnitude': 19.061100006103516}, {'ion_id': 1308, 'distance': 14.868091583251953, 'force': [-0.04955724999308586, 0.3378300964832306, -1.4625250101089478], 'magnitude': 1.5018537044525146}, {'ion_id': 1316, 'distance': 10.493775367736816, 'force': [-0.044318169355392456, 1.0932285785675049, -2.809373140335083], 'magnitude': 3.014911413192749}, {'ion_id': 1387, 'distance': 6.951023101806641, 'force': [0.18382298946380615, 4.179419040679932, -5.451035976409912], 'magnitude': 6.871326446533203}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.7250189781188965, 'force': [4.933323860168457, -0.14927417039871216, 5.272686004638672], 'magnitude': 7.2222700119018555}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.608229637145996, 'force': [-5.709897994995117, 0.44179612398147583, -7.292564392089844], 'magnitude': 9.2725191116333}</t>
+          <t>{4333: {'frame': 4333, 'motion_vector': [-1.0914764404296875, 2.8184471130371094, 0.5848388671875], 'ionic_force': [10.218847453594208, 2.7001716569066048, -15.040524646639824], 'ionic_force_magnitude': 18.382958192379444, 'radial_force': 10.569568120627757, 'axial_force': -15.040524646639824, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [3.5677709579467773, 4.624752044677734, 1.8411636352539062], 'asn_force_magnitude': 6.124312583049687, 'residue_force': [3.5677709579467773, 4.624752044677734, 1.8411636352539062], 'residue_force_magnitude': 6.124312583049687, 'total_force': [13.786618411540985, 7.324923701584339, -13.199361011385918], 'total_force_magnitude': 20.443788434836815, 'cosine_total_motion': -0.0337226720316767, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.5419283245041114, 'cosine_residue_motion': 0.5419283245041114, 'cosine_ionic_motion': -0.21804747567810898, 'motion_component_total': -0.689419172472987, 'motion_component_glu': None, 'motion_component_asn': 3.318938456871564, 'motion_component_residue': 3.318938456871564, 'motion_component_ionic': -4.008357629344551, 'motion_component_percent_total': 3.3722672031676697, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 54.192832450411146, 'motion_component_percent_residue': 54.192832450411146, 'motion_component_percent_ionic': 21.804747567810896, 'ionic_contributions': [{'ion_id': 1306, 'distance': 7.030627250671387, 'force': [1.9004194736480713, 6.339089393615723, 1.1476751565933228], 'magnitude': 6.716607093811035, 'cosine_ionic_motion': 0.7962185144424438, 'motion_component_ionic': 5.34788703918457, 'motion_component_percent_ionic': 79.62185144424438}, {'ion_id': 1307, 'distance': 8.677374839782715, 'force': [2.6483633518218994, -3.5226809978485107, -0.1344403475522995], 'magnitude': 4.409215927124023, 'cosine_ionic_motion': -0.950204074382782, 'motion_component_ionic': -4.18965482711792, 'motion_component_percent_ionic': 95.0204074382782}, {'ion_id': 1308, 'distance': 14.20415210723877, 'force': [0.17358297109603882, -0.07655664533376694, -1.6345635652542114], 'magnitude': 1.6455363035202026, 'cosine_ionic_motion': -0.2687048017978668, 'motion_component_ionic': -0.44216352701187134, 'motion_component_percent_ionic': 26.870480179786682}, {'ion_id': 1316, 'distance': 9.113018035888672, 'force': [0.8972761631011963, -0.14553450047969818, -3.8930156230926514], 'magnitude': 3.9977312088012695, 'cosine_ionic_motion': -0.2979077398777008, 'motion_component_ionic': -1.1909550428390503, 'motion_component_percent_ionic': 29.79077398777008}, {'ion_id': 1387, 'distance': 5.375945568084717, 'force': [4.599205493927002, 0.10585440695285797, -10.526180267333984], 'magnitude': 11.487574577331543, 'cosine_ionic_motion': -0.3075907230377197, 'motion_component_ionic': -3.5334713459014893, 'motion_component_percent_ionic': 30.759072303771973}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.533482551574707, 'force': [4.31558895111084, 4.671905040740967, -0.9512782096862793], 'magnitude': 6.430858135223389, 'cosine_with_motion': 0.3990866243839264, 'motion_component': 2.566469430923462, 'motion_component_percent': 39.90866243839264}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.743353366851807, 'force': [-0.9748809337615967, 8.454612731933594, 6.185499668121338], 'magnitude': 10.520992279052734, 'cosine_with_motion': 0.8802621364593506, 'motion_component': 9.261231422424316, 'motion_component_percent': 88.02621364593506}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.188126087188721, 'force': [-0.8626163005828857, -6.304483890533447, -3.609175205230713], 'magnitude': 7.315515518188477, 'cosine_with_motion': -0.8409232497215271, 'motion_component': -6.151787281036377, 'motion_component_percent': 84.09232497215271}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.913429021835327, 'force': [1.696218729019165, -12.744790077209473, -15.22091007232666], 'magnitude': 19.92443084716797, 'cosine_with_motion': -0.760940432548523, 'motion_component': -15.161304473876953, 'motion_component_percent': 76.0940432548523}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.5858659744262695, 'force': [1.7662837505340576, 6.371105670928955, 8.582714080810547], 'magnitude': 10.833915710449219, 'cosine_with_motion': 0.6310961246490479, 'motion_component': 6.837242126464844, 'motion_component_percent': 63.109612464904785}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.079699516296387, 'force': [-2.3728232383728027, 4.176402568817139, 6.854313373565674], 'magnitude': 8.369841575622559, 'cosine_with_motion': 0.7129271030426025, 'motion_component': 5.9670867919921875, 'motion_component_percent': 71.29271030426025}]}, 4335: {'frame': 4335, 'motion_vector': [-2.4897499084472656, -1.9592094421386719, -2.6416397094726562], 'ionic_force': [9.905854746699333, 2.9460261538624763, -22.515233606100082], 'ionic_force_magnitude': 24.773792053280943, 'radial_force': 10.334651825869484, 'axial_force': -22.515233606100082, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [4.829582959413528, 6.925490617752075, 6.043889671564102], 'asn_force_magnitude': 10.383443273811862, 'residue_force': [4.829582959413528, 6.925490617752075, 6.043889671564102], 'residue_force_magnitude': 10.383443273811862, 'total_force': [14.735437706112862, 9.871516771614552, -16.47134393453598], 'total_force_magnitude': 24.205064320773353, 'cosine_total_motion': -0.1253588869188488, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.9702796276735125, 'cosine_residue_motion': -0.9702796276735125, 'cosine_ionic_motion': 0.2841924053245415, 'motion_component_total': -3.0343199210512886, 'motion_component_glu': None, 'motion_component_asn': -10.074843473683211, 'motion_component_residue': -10.074843473683211, 'motion_component_ionic': 7.040523552631923, 'motion_component_percent_total': 12.53588869188488, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 97.02796276735126, 'motion_component_percent_residue': 97.02796276735126, 'motion_component_percent_ionic': 28.419240532454147, 'ionic_contributions': [{'ion_id': 1306, 'distance': 8.269227981567383, 'force': [-0.3307041525840759, 4.825318336486816, 0.4242839515209198], 'magnitude': 4.8552117347717285, 'cosine_ionic_motion': -0.48688679933547974, 'motion_component_ionic': -2.363938570022583, 'motion_component_percent_ionic': 48.688679933547974}, {'ion_id': 1307, 'distance': 8.450594902038574, 'force': [3.035064935684204, -3.5079329013824463, -0.3104632496833801], 'magnitude': 4.649043083190918, 'cosine_ionic_motion': 0.007110195234417915, 'motion_component_ionic': 0.03305560350418091, 'motion_component_percent_ionic': 0.7110195234417915}, {'ion_id': 1308, 'distance': 14.563118934631348, 'force': [0.17067889869213104, -0.07447502017021179, -1.5542986392974854], 'magnitude': 1.565414309501648, 'cosine_ionic_motion': 0.5926381349563599, 'motion_component_ionic': 0.9277241826057434, 'motion_component_percent_ionic': 59.263813495635986}, {'ion_id': 1316, 'distance': 9.559685707092285, 'force': [0.7298926711082458, 0.04116610437631607, -3.5585622787475586], 'magnitude': 3.632878065109253, 'cosine_ionic_motion': 0.5006490349769592, 'motion_component_ionic': 1.818796992301941, 'motion_component_percent_ionic': 50.06490349769592}, {'ion_id': 1387, 'distance': 4.214784622192383, 'force': [6.300922393798828, 1.661949634552002, -17.516193389892578], 'magnitude': 18.68905258178711, 'cosine_ionic_motion': 0.35447943210601807, 'motion_component_ionic': 6.624884605407715, 'motion_component_percent_ionic': 35.44794321060181}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.76469612121582, 'force': [-4.433062553405762, -5.54639196395874, 0.5704285502433777], 'magnitude': 7.123194217681885, 'cosine_with_motion': 0.694169282913208, 'motion_component': 4.944702625274658, 'motion_component_percent': 69.4169282913208}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.975369930267334, 'force': [5.955981254577637, 5.24924373626709, -0.496473103761673], 'magnitude': 7.954543113708496, 'cosine_with_motion': -0.7253876328468323, 'motion_component': -5.770127296447754, 'motion_component_percent': 72.53876328468323}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.314467430114746, 'force': [-0.821997344493866, 7.551161766052246, 3.5425148010253906], 'magnitude': 8.381237030029297, 'cosine_with_motion': -0.6394019722938538, 'motion_component': -5.35897970199585, 'motion_component_percent': 63.940197229385376}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.3444623947143555, 'force': [-0.7999061346054077, -13.655682563781738, -8.617050170898438], 'magnitude': 16.166975021362305, 'cosine_with_motion': 0.7723798155784607, 'motion_component': 12.487045288085938, 'motion_component_percent': 77.23798155784607}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.364649295806885, 'force': [1.9568079710006714, 6.213186264038086, 3.322962522506714], 'magnitude': 7.312650680541992, 'cosine_with_motion': -0.8560663461685181, 'motion_component': -6.2601141929626465, 'motion_component_percent': 85.6066346168518}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.044857978820801, 'force': [-0.38029196858406067, 6.085940361022949, 5.942730903625488], 'magnitude': 8.514655113220215, 'cosine_with_motion': -0.759485125541687, 'motion_component': -6.466753959655762, 'motion_component_percent': 75.9485125541687}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.952569007873535, 'force': [3.3520517349243164, 1.0280330181121826, 1.7787761688232422], 'magnitude': 3.9315578937530518, 'cosine_with_motion': -0.9285419583320618, 'motion_component': -3.650616407394409, 'motion_component_percent': 92.85419583320618}]}, 4336: {'frame': 4336, 'motion_vector': [0.6896553039550781, 0.1011199951171875, 0.940399169921875], 'ionic_force': [-1.1519034951925278, -1.205802470445633, -12.496924042701721], 'ionic_force_magnitude': 12.607694150360162, 'radial_force': 1.667585458070906, 'axial_force': -12.496924042701721, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-1.998314619064331, -11.548934876918793, -1.6533186435699463], 'asn_force_magnitude': 11.83657976973304, 'residue_force': [-1.998314619064331, -11.548934876918793, -1.6533186435699463], 'residue_force_magnitude': 11.83657976973304, 'total_force': [-3.150218114256859, -12.754737347364426, -14.150242686271667], 'total_force_magnitude': 19.308976333509495, 'cosine_total_motion': -0.7419267769290067, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.2959686083944419, 'cosine_residue_motion': -0.2959686083944419, 'cosine_ionic_motion': -0.858411570367315, 'motion_component_total': -14.325846576919169, 'motion_component_glu': None, 'motion_component_asn': -3.503256042597691, 'motion_component_residue': -3.503256042597691, 'motion_component_ionic': -10.822590534321478, 'motion_component_percent_total': 74.19267769290066, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 29.59686083944419, 'motion_component_percent_residue': 29.59686083944419, 'motion_component_percent_ionic': 85.8411570367315, 'ionic_contributions': [{'ion_id': 1306, 'distance': 8.297228813171387, 'force': [-1.9411698579788208, 3.975846767425537, -1.9185880422592163], 'magnitude': 4.8224968910217285, 'cosine_ionic_motion': -0.4855515658855438, 'motion_component_ionic': -2.3415708541870117, 'motion_component_percent_ionic': 48.55515658855438}, {'ion_id': 1307, 'distance': 9.114627838134766, 'force': [1.3281068801879883, -3.4387872219085693, -1.5431928634643555], 'magnitude': 3.996319532394409, 'cosine_ionic_motion': -0.18876178562641144, 'motion_component_ionic': -0.7543523907661438, 'motion_component_percent_ionic': 18.876178562641144}, {'ion_id': 1316, 'distance': 11.616941452026367, 'force': [-0.19560758769512177, -0.3452792465686798, -2.427891969680786], 'magnitude': 2.4601097106933594, 'cosine_ionic_motion': -0.8518276214599609, 'motion_component_ionic': -2.0955893993377686, 'motion_component_percent_ionic': 85.1827621459961}, {'ion_id': 1387, 'distance': 7.006906032562256, 'force': [-0.3432329297065735, -1.397582769393921, -6.607251167297363], 'magnitude': 6.762160301208496, 'cosine_ionic_motion': -0.8327334523200989, 'motion_component_ionic': -5.631077289581299, 'motion_component_percent_ionic': 83.27334523200989}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.808727264404297, 'force': [-3.573249340057373, 7.851780414581299, -2.714258909225464], 'magnitude': 9.043548583984375, 'cosine_with_motion': -0.39890748262405396, 'motion_component': -3.607539176940918, 'motion_component_percent': 39.890748262405396}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.166891574859619, 'force': [1.3632164001464844, -4.737532138824463, 1.7106449604034424], 'magnitude': 5.218129634857178, 'cosine_with_motion': 0.3388575315475464, 'motion_component': 1.768202543258667, 'motion_component_percent': 33.88575315475464}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.609676837921143, 'force': [2.4141554832458496, -3.4597537517547607, 1.341355323791504], 'magnitude': 4.426881313323975, 'cosine_with_motion': 0.4972093403339386, 'motion_component': 2.2010867595672607, 'motion_component_percent': 49.72093403339386}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.236931800842285, 'force': [-10.689862251281738, 7.426120281219482, -2.1117420196533203], 'magnitude': 13.186351776123047, 'cosine_with_motion': -0.5576333999633789, 'motion_component': -7.353150367736816, 'motion_component_percent': 55.76333999633789}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.4410440921783447, 'force': [15.346685409545898, -6.299398899078369, 1.1598154306411743], 'magnitude': 16.629743576049805, 'cosine_with_motion': 0.5670191645622253, 'motion_component': 9.429383277893066, 'motion_component_percent': 56.701916456222534}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.193416118621826, 'force': [10.235634803771973, -13.267374038696289, 4.5079779624938965], 'magnitude': 17.352615356445312, 'cosine_with_motion': 0.49018627405166626, 'motion_component': 8.506013870239258, 'motion_component_percent': 49.018627405166626}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.423757553100586, 'force': [-5.362268447875977, 10.251153945922852, -2.718930959701538], 'magnitude': 11.884135246276855, 'cosine_with_motion': -0.37512654066085815, 'motion_component': -4.458054542541504, 'motion_component_percent': 37.512654066085815}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.135996341705322, 'force': [-2.7916762828826904, 4.2870192527771, -1.3107243776321411], 'magnitude': 5.281097412109375, 'cosine_with_motion': -0.44071099162101746, 'motion_component': -2.32743763923645, 'motion_component_percent': 44.071099162101746}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.594569444656372, 'force': [15.601705551147461, 7.704370498657227, 5.7327880859375], 'magnitude': 18.320354461669922, 'cosine_with_motion': 0.7894604206085205, 'motion_component': 14.463194847106934, 'motion_component_percent': 78.94604206085205}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.546199321746826, 'force': [-23.320262908935547, -18.13536262512207, -7.054473876953125], 'magnitude': 30.372547149658203, 'cosine_with_motion': -0.6905459761619568, 'motion_component': -20.97364044189453, 'motion_component_percent': 69.05459761619568}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.983973264694214, 'force': [-16.482017517089844, -2.8371663093566895, -9.481409072875977], 'magnitude': 19.225074768066406, 'cosine_with_motion': -0.9140639901161194, 'motion_component': -17.572948455810547, 'motion_component_percent': 91.40639901161194}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.3962671756744385, 'force': [9.966341972351074, -0.7564395070075989, 6.779455661773682], 'magnitude': 12.077301025390625, 'cosine_with_motion': 0.9317466616630554, 'motion_component': 11.252985000610352, 'motion_component_percent': 93.17466616630554}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.8707661628723145, 'force': [5.293282508850098, 0.42364799976348877, 2.50618314743042], 'magnitude': 5.871905326843262, 'cosine_with_motion': 0.880233883857727, 'motion_component': 5.168650150299072, 'motion_component_percent': 88.0233883857727}]}, 4337: {'frame': 4337, 'motion_vector': [-1.2149238586425781, 0.8994140625, 1.17535400390625], 'ionic_force': [-0.19163120537996292, 0.32513704895973206, -11.826547503471375], 'ionic_force_magnitude': 11.832567873092747, 'radial_force': 0.3774077628793832, 'axial_force': -11.826547503471375, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [8.216361999511719, -4.510262191295624, 1.8031255006790161], 'asn_force_magnitude': 9.544754114824014, 'residue_force': [8.216361999511719, -4.510262191295624, 1.8031255006790161], 'residue_force_magnitude': 9.544754114824014, 'total_force': [8.024730794131756, -4.185125142335892, -10.023422002792358], 'total_force_magnitude': 13.50483489056273, 'cosine_total_motion': -0.9781764748162509, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.652187027568698, 'cosine_residue_motion': -0.652187027568698, 'cosine_ionic_motion': -0.5903322969386221, 'motion_component_total': -13.210111786226161, 'motion_component_glu': None, 'motion_component_asn': -6.224964815021172, 'motion_component_residue': -6.224964815021172, 'motion_component_ionic': -6.985146971204988, 'motion_component_percent_total': 97.81764748162509, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 65.21870275686979, 'motion_component_percent_residue': 65.21870275686979, 'motion_component_percent_ionic': 59.03322969386221, 'ionic_contributions': [{'ion_id': 1306, 'distance': 7.549276828765869, 'force': [-1.3619964122772217, 5.054660320281982, -2.5555646419525146], 'magnitude': 5.825421333312988, 'cosine_ionic_motion': 0.2866344153881073, 'motion_component_ionic': 1.6697661876678467, 'motion_component_percent_ionic': 28.66344153881073}, {'ion_id': 1307, 'distance': 9.575133323669434, 'force': [1.334238886833191, -3.2292449474334717, -0.951119065284729], 'magnitude': 3.621166229248047, 'cosine_ionic_motion': -0.8138875961303711, 'motion_component_ionic': -2.9472222328186035, 'motion_component_percent_ionic': 81.38875961303711}, {'ion_id': 1316, 'distance': 11.058213233947754, 'force': [-0.0917414203286171, -0.38027724623680115, -2.686659812927246], 'magnitude': 2.714989423751831, 'cosine_ionic_motion': -0.6517738103866577, 'motion_component_ionic': -1.7695590257644653, 'motion_component_percent_ionic': 65.17738103866577}, {'ion_id': 1387, 'distance': 7.602648735046387, 'force': [-0.07213225960731506, -1.1200010776519775, -5.633203983306885], 'magnitude': 5.743917942047119, 'cosine_ionic_motion': -0.6856177449226379, 'motion_component_ionic': -3.9381320476531982, 'motion_component_percent_ionic': 68.5617744922638}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.7457780838012695, 'force': [1.3774666786193848, -3.620861530303955, 1.6725267171859741], 'magnitude': 4.219644546508789, 'cosine_with_motion': -0.3668872117996216, 'motion_component': -1.5481336116790771, 'motion_component_percent': 36.68872117996216}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.334958076477051, 'force': [-8.543743133544922, 9.23127555847168, -0.6823439598083496], 'magnitude': 12.596729278564453, 'cosine_with_motion': 0.7413191795349121, 'motion_component': 9.338196754455566, 'motion_component_percent': 74.13191795349121}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.4750232696533203, 'force': [10.193188667297363, -12.466917991638184, -2.5620980262756348], 'magnitude': 16.30611801147461, 'cosine_with_motion': -0.8522031307220459, 'motion_component': -13.896124839782715, 'motion_component_percent': 85.22031307220459}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.377269744873047, 'force': [9.8428373336792, -11.224483489990234, 5.545485019683838], 'magnitude': 15.925541877746582, 'cosine_with_motion': -0.5094696283340454, 'motion_component': -8.113579750061035, 'motion_component_percent': 50.94696283340454}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.88883900642395, 'force': [-4.0889387130737305, 7.124800205230713, -4.1678314208984375], 'magnitude': 9.211569786071777, 'cosine_with_motion': 0.36722511053085327, 'motion_component': 3.3827197551727295, 'motion_component_percent': 36.72251105308533}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.285560607910156, 'force': [-3.191173553466797, 3.2229580879211426, -2.072108507156372], 'magnitude': 4.986449718475342, 'cosine_with_motion': 0.4545800983905792, 'motion_component': 2.2667407989501953, 'motion_component_percent': 45.45800983905792}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.623368263244629, 'force': [9.301969528198242, 3.4288275241851807, 4.93491792678833], 'magnitude': 11.0741548538208, 'cosine_with_motion': -0.11398262530565262, 'motion_component': -1.2622612714767456, 'motion_component_percent': 11.398262530565262}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.064777851104736, 'force': [-6.665158748626709, -0.7033438086509705, -3.7422866821289062], 'magnitude': 7.676179885864258, 'cosine_with_motion': 0.20863282680511475, 'motion_component': 1.6015031337738037, 'motion_component_percent': 20.863282680511475}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.4305453300476074, 'force': [-19.863107681274414, -10.691112518310547, -12.784184455871582], 'magnitude': 25.92833137512207, 'cosine_with_motion': -0.010262681171298027, 'motion_component': -0.2660942077636719, 'motion_component_percent': 1.0262681171298027}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 2.922518253326416, 'force': [12.110390663146973, 2.985849380493164, 10.509305953979492], 'magnitude': 16.310192108154297, 'cosine_with_motion': 0.01038939505815506, 'motion_component': 0.16945302486419678, 'motion_component_percent': 1.038939505815506}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 3.351707935333252, 'force': [7.742630958557129, 8.202746391296387, 5.151742935180664], 'magnitude': 12.400557518005371, 'cosine_with_motion': 0.16955818235874176, 'motion_component': 2.10261607170105, 'motion_component_percent': 16.955818235874176}]}, 4338: {'frame': 4338, 'motion_vector': [1.5186386108398438, 5.265224456787109, -0.11255645751953125], 'ionic_force': [-1.9880583882331848, -1.188404381275177, -12.07487940788269], 'ionic_force_magnitude': 12.295014999721138, 'radial_force': 2.3161781296908845, 'axial_force': -12.07487940788269, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-4.661213755607605, 3.588160276412964, 0.14355164766311646], 'asn_force_magnitude': 5.884081484840289, 'residue_force': [-4.661213755607605, 3.588160276412964, 0.14355164766311646], 'residue_force_magnitude': 5.884081484840289, 'total_force': [-6.64927214384079, 2.399755895137787, -11.931327760219574], 'total_force_magnitude': 13.868245401668226, 'cosine_total_motion': 0.051049276989089905, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.3658090951674374, 'cosine_residue_motion': 0.3658090951674374, 'cosine_ionic_motion': -0.11748555191117914, 'motion_component_total': 0.7079639008624337, 'motion_component_glu': None, 'motion_component_asn': 2.1524505238608977, 'motion_component_residue': 2.1524505238608977, 'motion_component_ionic': -1.4444866229984639, 'motion_component_percent_total': 5.10492769890899, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 36.580909516743745, 'motion_component_percent_residue': 36.580909516743745, 'motion_component_percent_ionic': 11.748555191117914, 'ionic_contributions': [{'ion_id': 1306, 'distance': 6.735961437225342, 'force': [-1.6397868394851685, 7.1292724609375, -0.15652811527252197], 'magnitude': 7.317098140716553, 'cosine_ionic_motion': 0.8743170499801636, 'motion_component_ionic': 6.397463798522949, 'motion_component_percent_ionic': 87.43170499801636}, {'ion_id': 1307, 'distance': 6.5452165603637695, 'force': [2.079728841781616, -7.2433953285217285, -1.8075493574142456], 'magnitude': 7.749792098999023, 'cosine_ionic_motion': -0.8187141418457031, 'motion_component_ionic': -6.344864368438721, 'motion_component_percent_ionic': 81.87141418457031}, {'ion_id': 1316, 'distance': 10.65501594543457, 'force': [-0.5445583462715149, -0.3111899495124817, -2.85630202293396], 'magnitude': 2.92435359954834, 'cosine_ionic_motion': -0.13376092910766602, 'motion_component_ionic': -0.39116424322128296, 'motion_component_percent_ionic': 13.376092910766602}, {'ion_id': 1387, 'distance': 6.638399124145508, 'force': [-1.8834420442581177, -0.7630915641784668, -7.254499912261963], 'magnitude': 7.533752918243408, 'cosine_ionic_motion': -0.14679564535617828, 'motion_component_ionic': -1.1059221029281616, 'motion_component_percent_ionic': 14.679564535617828}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.675151824951172, 'force': [-4.804211139678955, 5.200509071350098, 1.9730955362319946], 'magnitude': 7.3497514724731445, 'cosine_with_motion': 0.49309539794921875, 'motion_component': 3.624128580093384, 'motion_component_percent': 49.309539794921875}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.7113447189331055, 'force': [2.861213445663452, -4.979075908660889, -1.860718846321106], 'magnitude': 6.036556243896484, 'cosine_with_motion': -0.6546899080276489, 'motion_component': -3.9520723819732666, 'motion_component_percent': 65.46899080276489}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.587115287780762, 'force': [11.007375717163086, -8.942174911499023, -3.029362201690674], 'magnitude': 14.501788139343262, 'cosine_with_motion': -0.37775108218193054, 'motion_component': -5.4780659675598145, 'motion_component_percent': 37.775108218193054}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.7125494480133057, 'force': [-6.810189723968506, 7.069425582885742, 2.4081523418426514], 'magnitude': 10.107158660888672, 'cosine_with_motion': 0.480325847864151, 'motion_component': 4.854729652404785, 'motion_component_percent': 48.0325847864151}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.801830768585205, 'force': [-5.306699275970459, 2.746837854385376, 0.8922334313392639], 'magnitude': 6.0417094230651855, 'cosine_with_motion': 0.1903485208749771, 'motion_component': 1.150030493736267, 'motion_component_percent': 19.03485208749771}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.047773838043213, 'force': [4.33180570602417, 5.8324785232543945, 5.790213584899902], 'magnitude': 9.29025936126709, 'cosine_with_motion': 0.7194814682006836, 'motion_component': 6.684169292449951, 'motion_component_percent': 71.94814682006836}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.836606502532959, 'force': [-4.4443440437316895, -3.5129165649414062, -6.2259111404418945], 'magnitude': 8.417526245117188, 'cosine_with_motion': -0.532004714012146, 'motion_component': -4.478163719177246, 'motion_component_percent': 53.2004714012146}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.563413143157959, 'force': [-3.881063461303711, -11.172825813293457, -8.649303436279297], 'magnitude': 14.652820587158203, 'cosine_with_motion': -0.7937490940093994, 'motion_component': -11.63066291809082, 'motion_component_percent': 79.37490940093994}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.8671276569366455, 'force': [1.2050726413726807, 6.649488925933838, 6.411457061767578], 'magnitude': 9.315293312072754, 'cosine_with_motion': 0.7074306607246399, 'motion_component': 6.589923858642578, 'motion_component_percent': 70.74306607246399}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.069983005523682, 'force': [1.1798263788223267, 4.696413516998291, 2.4336953163146973], 'magnitude': 5.4195170402526855, 'cosine_with_motion': 0.8835535645484924, 'motion_component': 4.78843355178833, 'motion_component_percent': 88.35535645484924}]}, 4339: {'frame': 4339, 'motion_vector': [-0.3119239807128906, 0.11574172973632812, 2.2965164184570312], 'ionic_force': [7.982106583658606, -1.4821966588497162, -13.919581286609173], 'ionic_force_magnitude': 16.114145203606412, 'radial_force': 8.118554825114586, 'axial_force': -13.919581286609173, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-7.585148334503174, 0.5071490556001663, -5.471320137381554], 'asn_force_magnitude': 9.366270307156917, 'residue_force': [-7.585148334503174, 0.5071490556001663, -5.471320137381554], 'residue_force_magnitude': 9.366270307156917, 'total_force': [0.396958249155432, -0.9750476032495499, -19.390901423990726], 'total_force_magnitude': 19.419458069552324, 'cosine_total_motion': -0.9934649836062751, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.4665558962243783, 'cosine_residue_motion': -0.4665558962243783, 'cosine_ionic_motion': -0.9260598540427335, 'motion_component_total': -19.292551592710545, 'motion_component_glu': None, 'motion_component_asn': -4.369888637435379, 'motion_component_residue': -4.369888637435379, 'motion_component_ionic': -14.922662955275168, 'motion_component_percent_total': 99.3464983606275, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 46.65558962243783, 'motion_component_percent_residue': 46.65558962243783, 'motion_component_percent_ionic': 92.60598540427335, 'ionic_contributions': [{'ion_id': 1306, 'distance': 12.086974143981934, 'force': [-0.076982282102108, 2.2683990001678467, -0.11256872862577438], 'magnitude': 2.2724947929382324, 'cosine_ionic_motion': 0.005318314302712679, 'motion_component_ionic': 0.012085841968655586, 'motion_component_percent_ionic': 0.5318314302712679}, {'ion_id': 1307, 'distance': 4.773991107940674, 'force': [8.069611549377441, -11.067646980285645, -4.958900451660156], 'magnitude': 14.567159652709961, 'cosine_ionic_motion': -0.4492591321468353, 'motion_component_ionic': -6.544429302215576, 'motion_component_percent_ionic': 44.92591321468353}, {'ion_id': 1308, 'distance': 14.942962646484375, 'force': [0.015117759816348553, 0.40834537148475647, -1.4295883178710938], 'magnitude': 1.4868414402008057, 'cosine_ionic_motion': -0.9392277002334595, 'motion_component_ionic': -1.3964827060699463, 'motion_component_percent_ionic': 93.92277002334595}, {'ion_id': 1316, 'distance': 10.61767578125, 'force': [-0.007704783696681261, 1.2880055904388428, -2.648350715637207], 'magnitude': 2.944958209991455, 'cosine_ionic_motion': -0.8678253293037415, 'motion_component_ionic': -2.5557093620300293, 'motion_component_percent_ionic': 86.78253293037415}, {'ion_id': 1387, 'distance': 6.710808753967285, 'force': [-0.017935659736394882, 5.620700359344482, -4.770173072814941], 'magnitude': 7.37205171585083, 'cosine_ionic_motion': -0.6020206809043884, 'motion_component_ionic': -4.438127517700195, 'motion_component_percent_ionic': 60.20206809043884}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.018038272857666, 'force': [6.271729946136475, 0.11264830827713013, 7.001832485198975], 'magnitude': 9.400688171386719, 'cosine_with_motion': 0.6480434536933899, 'motion_component': 6.09205436706543, 'motion_component_percent': 64.80434536933899}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance'</t>
         </is>
       </c>
     </row>
@@ -563,7 +563,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>{4408: {'frame': 4408, 'ionic_force': [9.049361620098352, -12.949827790260315, -9.676596252247691], 'ionic_force_magnitude': 18.52634611999143, 'motion_vector': [0.9472541809082031, 6.171745300292969, -2.0280227661132812], 'ionic_force_x': 9.049361620098352, 'ionic_force_y': -12.949827790260315, 'ionic_force_z': -9.676596252247691, 'radial_force': 15.798385535513033, 'axial_force': -9.676596252247691, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [3.5434560775756836, 4.623234510421753, -10.538706541061401], 'asn_force_magnitude': 12.04137508221852, 'residue_force': [3.5434560775756836, 4.623234510421753, -10.538706541061401], 'residue_force_magnitude': 12.04137508221852, 'total_force': [12.592817697674036, -8.326593279838562, -20.215302793309093], 'total_force_magnitude': 25.230332543188478, 'motion_component_total': 0.2339763904153358, 'cosine_total_motion': 0.009273615003481325, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.6737605041827468, 'cosine_residue_motion': 0.6737605041827468, 'cosine_ionic_motion': -0.42528766897708287, 'motion_component_glu': None, 'motion_component_asn': 8.113002946449114, 'motion_component_residue': 8.113002946449114, 'motion_component_ionic': -7.879026556033779, 'ionic_contributions': [{'ion_id': 1306, 'distance': 7.103499889373779, 'force': [-1.5873969793319702, -6.355767250061035, -0.6117986440658569], 'magnitude': 6.5795063972473145}, {'ion_id': 1307, 'distance': 10.374420166015625, 'force': [1.3527055978775024, -2.772169589996338, -0.023000208660960197], 'magnitude': 3.0846824645996094}, {'ion_id': 1308, 'distance': 13.471064567565918, 'force': [0.0392477847635746, -0.5659531354904175, -1.739326000213623], 'magnitude': 1.8295077085494995}, {'ion_id': 1316, 'distance': 8.044059753417969, 'force': [0.1305760145187378, -2.5276927947998047, -4.4630842208862305], 'magnitude': 5.130828380584717}, {'ion_id': 1460, 'distance': 5.888736724853516, 'force': [9.114229202270508, -0.7282450199127197, -2.8393871784210205], 'magnitude': 9.574007987976074}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.416689395904541, 'force': [-12.96794605255127, 8.339502334594727, 13.170660972595215], 'magnitude': 20.277603149414062}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.828958034515381, 'force': [12.381628036499023, -3.9192512035369873, -20.89765167236328], 'magnitude': 24.604412078857422}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.574815034866333, 'force': [11.49341106414795, -17.1616268157959, -11.980310440063477], 'magnitude': 23.87776756286621}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.129112958908081, 'force': [-3.6253979206085205, 12.196083068847656, 6.366799354553223], 'magnitude': 14.227581977844238}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.471631050109863, 'force': [-3.738239049911499, 5.168527126312256, 2.801795244216919], 'magnitude': 6.966933250427246}]}, 4409: {'frame': 4409, 'ionic_force': [8.281869903206825, -9.407124474644661, -19.244575142860413], 'ionic_force_magnitude': 22.96599730915909, 'motion_vector': [1.2028884887695312, 0.22224044799804688, -0.367950439453125], 'ionic_force_x': 8.281869903206825, 'ionic_force_y': -9.407124474644661, 'ionic_force_z': -19.244575142860413, 'radial_force': 12.53329006985403, 'axial_force': -19.244575142860413, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [4.813360691070557, 6.736542046070099, -4.601872891187668], 'asn_force_magnitude': 9.472416480891319, 'residue_force': [4.813360691070557, 6.736542046070099, -4.601872891187668], 'residue_force_magnitude': 9.472416480891319, 'total_force': [13.095230594277382, -2.670582428574562, -23.84644803404808], 'total_force_magnitude': 27.33624258499447, 'motion_component_total': 18.735817698421133, 'cosine_total_motion': 0.6853837955295905, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.7421792013658787, 'cosine_residue_motion': 0.7421792013658787, 'cosine_ionic_motion': 0.5096920914015745, 'motion_component_glu': None, 'motion_component_asn': 7.030230498792906, 'motion_component_residue': 7.030230498792906, 'motion_component_ionic': 11.705587199628228, 'ionic_contributions': [{'ion_id': 1306, 'distance': 4.740226745605469, 'force': [4.004691123962402, -8.651683807373047, -11.288216590881348], 'magnitude': 14.775419235229492}, {'ion_id': 1307, 'distance': 8.134659767150879, 'force': [1.8958126306533813, -4.239731788635254, -1.8980571031570435], 'magnitude': 5.017175674438477}, {'ion_id': 1308, 'distance': 14.995219230651855, 'force': [0.11879675090312958, 0.2119782418012619, -1.456363558769226], 'magnitude': 1.4764965772628784}, {'ion_id': 1316, 'distance': 9.502534866333008, 'force': [0.3882765471935272, 1.0418009757995605, -3.5045788288116455], 'magnitude': 3.6767079830169678}, {'ion_id': 1460, 'distance': 10.326704025268555, 'force': [1.8742928504943848, 2.2305119037628174, -1.09735906124115], 'magnitude': 3.1132545471191406}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.89084005355835, 'force': [8.498285293579102, -3.1778390407562256, 3.9511711597442627], 'magnitude': 9.89602279663086}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.35770320892334, 'force': [-7.495138168334961, 4.818055152893066, -5.303986549377441], 'magnitude': 10.369331359863281}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.541079998016357, 'force': [-13.760960578918457, 0.9053523540496826, -5.364368915557861], 'magnitude': 14.79730224609375}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.812704563140869, 'force': [8.416282653808594, 0.5008266568183899, 4.5553998947143555], 'magnitude': 9.583126068115234}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.284165382385254, 'force': [4.813093662261963, 0.14431548118591309, 1.3054699897766113], 'magnitude': 4.9890828132629395}, {'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.9146533012390137, 'force': [-11.325387954711914, -10.452134132385254, -1.0463273525238037], 'magnitude': 15.446887016296387}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.011950731277466, 'force': [13.774523735046387, 16.59543228149414, -2.446213960647583], 'magnitude': 21.70552635192871}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.9798951148986816, 'force': [16.72966194152832, 8.269248008728027, 4.781069755554199], 'magnitude': 19.26449203491211}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.451082944869995, 'force': [-11.090353012084961, -2.473383665084839, -2.7746827602386475], 'magnitude': 11.696683883666992}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.9062395095825195, 'force': [-4.9672088623046875, -2.2703304290771484, -1.9144953489303589], 'magnitude': 5.787301540374756}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.611631870269775, 'force': [1.2205619812011719, -6.123000621795654, -0.34490880370140076], 'magnitude': 6.252989292144775}]}, 4410: {'frame': 4410, 'ionic_force': [15.673005670309067, -6.354610577225685, -18.238948702812195], 'ionic_force_magnitude': 24.8733478268114, 'motion_vector': [-0.20865249633789062, -4.049587249755859, 2.408935546875], 'ionic_force_x': 15.673005670309067, 'ionic_force_y': -6.354610577225685, 'ionic_force_z': -18.238948702812195, 'radial_force': 16.9122494757418, 'axial_force': -18.238948702812195, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-2.721809506416321, 10.137011382728815, 0.07277804613113403], 'asn_force_magnitude': 10.496310942745097, 'residue_force': [-2.721809506416321, 10.137011382728815, 0.07277804613113403], 'residue_force_magnitude': 10.496310942745097, 'total_force': [12.951196163892746, 3.78240080550313, -18.16617065668106], 'total_force_magnitude': 22.628517279237737, 'motion_component_total': -13.098736594388683, 'cosine_total_motion': -0.5788596942852778, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.8141910275658907, 'cosine_residue_motion': -0.8141910275658907, 'cosine_ionic_motion': -0.18303665569925734, 'motion_component_glu': None, 'motion_component_asn': -8.546002192124734, 'motion_component_residue': -8.546002192124734, 'motion_component_ionic': -4.552734402263949, 'ionic_contributions': [{'ion_id': 1306, 'distance': 4.458994388580322, 'force': [10.753595352172852, -6.403841495513916, -11.053228378295898], 'magnitude': 16.69799041748047}, {'ion_id': 1307, 'distance': 9.301104545593262, 'force': [2.1814122200012207, -2.955780029296875, -1.1102296113967896], 'magnitude': 3.8376822471618652}, {'ion_id': 1308, 'distance': 14.55396556854248, 'force': [0.2570955455303192, 0.21237300336360931, -1.531499981880188], 'magnitude': 1.5673840045928955}, {'ion_id': 1316, 'distance': 9.078113555908203, 'force': [1.0977156162261963, 1.1136078834533691, -3.712677240371704], 'magnitude': 4.0285325050354}, {'ion_id': 1460, 'distance': 11.939895629882812, 'force': [1.383186936378479, 1.6790300607681274, -0.8313134908676147], 'magnitude': 2.3288259506225586}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.73225736618042, 'force': [6.547236442565918, -2.216608762741089, 2.029426336288452], 'magnitude': 7.204042911529541}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.05270528793335, 'force': [-6.328794479370117, 3.563107967376709, -2.5960657596588135], 'magnitude': 7.712906837463379}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.484741687774658, 'force': [-9.65060806274414, 0.8191473484039307, -3.01424503326416], 'magnitude': 10.143515586853027}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.884988784790039, 'force': [5.276494979858398, -0.04528632387518883, 2.4972031116485596], 'magnitude': 5.837762832641602}, {'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.5908331871032715, 'force': [-12.240410804748535, -13.4556245803833, -2.4805119037628174], 'magnitude': 18.358497619628906}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.6594109535217285, 'force': [12.675597190856934, 24.51116943359375, 3.6999547481536865], 'magnitude': 27.841655731201172}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.7416653633117676, 'force': [19.326404571533203, 9.764897346496582, 2.487921953201294], 'magnitude': 21.79570770263672}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.178309679031372, 'force': [-13.40526294708252, -3.137441635131836, -0.7964059710502625], 'magnitude': 13.790535926818848}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.718949794769287, 'force': [-5.611135005950928, -2.574636936187744, -1.010662317276001], 'magnitude': 6.255799770355225}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.2427778244018555, 'force': [0.6886686086654663, -7.091712474822998, -0.7438371181488037], 'magnitude': 7.163794040679932}]}, 4411: {'frame': 4411, 'ionic_force': [8.995075047016144, -8.02235746383667, -9.743937104940414], 'ionic_force_magnitude': 15.498835591232748, 'motion_vector': [-2.447307586669922, -1.137054443359375, 2.16204833984375], 'ionic_force_x': 8.995075047016144, 'ionic_force_y': -8.02235746383667, 'ionic_force_z': -9.743937104940414, 'radial_force': 12.052783677600308, 'axial_force': -9.743937104940414, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-2.7447137013077736, -6.466000556945801, -3.4784128069877625], 'asn_force_magnitude': 7.838492977632021, 'residue_force': [-2.7447137013077736, -6.466000556945801, -3.4784128069877625], 'residue_force_magnitude': 7.838492977632021, 'total_force': [6.25036134570837, -14.48835802078247, -13.222349911928177], 'total_force_magnitude': 20.58664791275559, 'motion_component_total': -7.926873524314079, 'cosine_total_motion': -0.3850492590103777, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.24161728779535188, 'cosine_residue_motion': 0.24161728779535188, 'cosine_ionic_motion': -0.6336468878686462, 'motion_component_glu': None, 'motion_component_asn': 1.8939154136583607, 'motion_component_residue': 1.8939154136583607, 'motion_component_ionic': -9.82078893797244, 'ionic_contributions': [{'ion_id': 1306, 'distance': 7.156948566436768, 'force': [1.557535171508789, -6.21755838394165, 0.962909996509552], 'magnitude': 6.481600284576416}, {'ion_id': 1307, 'distance': 11.11915111541748, 'force': [1.0693477392196655, -2.452256441116333, -0.23202911019325256], 'magnitude': 2.685312509536743}, {'ion_id': 1308, 'distance': 12.464065551757812, 'force': [0.3361741900444031, -0.34610939025878906, -2.0818889141082764], 'magnitude': 2.1370694637298584}, {'ion_id': 1316, 'distance': 6.50744104385376, 'force': [2.108905553817749, -1.8903121948242188, -7.310626983642578], 'magnitude': 7.840027332305908}, {'ion_id': 1460, 'distance': 8.158514022827148, 'force': [3.923112392425537, 2.8838789463043213, -1.0823020935058594], 'magnitude': 4.987879753112793}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.379117012023926, 'force': [-2.057718515396118, -3.9980130195617676, 1.7207963466644287], 'magnitude': 4.814504623413086}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.32531213760376, 'force': [-1.0138967037200928, 11.15296459197998, 5.889075756072998], 'magnitude': 12.652976989746094}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.63965106010437, 'force': [-0.12175191938877106, -11.074440002441406, -9.914205551147461], 'magnitude': 14.864370346069336}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.949275970458984, 'force': [-1.204451322555542, -11.803104400634766, -3.7968087196350098], 'magnitude': 12.45711612701416}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.030297756195068, 'force': [1.6128840446472168, 4.96711540222168, 1.7422451972961426], 'magnitude': 5.505365371704102}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.640200614929199, 'force': [0.0402207151055336, 4.2894768714904785, 0.8804841637611389], 'magnitude': 4.379096031188965}]}, 4414: {'frame': 4414, 'ionic_force': [1.0051689818501472, 3.150031417608261, -16.299150347709656], 'ionic_force_magnitude': 16.631156444193426, 'motion_vector': [-0.04938507080078125, -0.9767036437988281, 0.471405029296875], 'ionic_force_x': 1.0051689818501472, 'ionic_force_y': 3.150031417608261, 'ionic_force_z': -16.299150347709656, 'radial_force': 3.3065182010678202, 'axial_force': -16.299150347709656, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-9.326332688331604, 6.6415345668792725, 9.811745405197144], 'asn_force_magnitude': 15.078488343096668, 'residue_force': [-9.326332688331604, 6.6415345668792725, 9.811745405197144], 'residue_force_magnitude': 15.078488343096668, 'total_force': [-8.321163706481457, 9.791565984487534, -6.487404942512512], 'total_force_magnitude': 14.394545937499151, 'motion_component_total': -11.24749092609025, 'cosine_total_motion': -0.7813717066815894, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.08557976932595379, 'cosine_residue_motion': -0.08557976932595379, 'cosine_ionic_motion': -0.5987002410394829, 'motion_component_glu': None, 'motion_component_asn': -1.290413554186296, 'motion_component_residue': -1.290413554186296, 'motion_component_ionic': -9.957077371903955, 'ionic_contributions': [{'ion_id': 1306, 'distance': 5.7553391456604, 'force': [-0.07259159535169601, 3.9749860763549805, -9.200763702392578], 'magnitude': 10.022965431213379}, {'ion_id': 1307, 'distance': 8.831177711486816, 'force': [0.6202806830406189, -2.786587715148926, -3.157846212387085], 'magnitude': 4.256971836090088}, {'ion_id': 1316, 'distance': 12.10187816619873, 'force': [-0.3398584723472595, 0.2946309745311737, -2.221829891204834], 'magnitude': 2.2669007778167725}, {'ion_id': 1460, 'distance': 11.469853401184082, 'force': [0.7973383665084839, 1.6670020818710327, -1.7187105417251587], 'magnitude': 2.5236105918884277}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.720937967300415, 'force': [7.105258464813232, -12.653792381286621, -9.039254188537598], 'magnitude': 17.09711265563965}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.6477584838867188, 'force': [-14.25243091583252, 16.973936080932617, 17.252464294433594], 'magnitude': 28.08725357055664}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.404152870178223, 'force': [-2.494011402130127, 12.281402587890625, 9.509675979614258], 'magnitude': 15.731715202331543}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.1764421463012695, 'force': [-0.5048230290412903, -6.006754398345947, -5.239223003387451], 'magnitude': 7.986576080322266}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.36414909362793, 'force': [0.8196741938591003, -3.9532573223114014, -2.671917676925659], 'magnitude': 4.841410160064697}]}, 4415: {'frame': 4415, 'ionic_force': [-1.2431654334068298, -0.5947210304439068, -11.592971801757812], 'ionic_force_magnitude': 11.674594151199504, 'motion_vector': [-1.1576690673828125, 0.13907241821289062, -4.969749450683594], 'ionic_force_x': -1.2431654334068298, 'ionic_force_y': -0.5947210304439068, 'ionic_force_z': -11.592971801757812, 'radial_force': 1.3780977464860225, 'axial_force': -11.592971801757812, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-3.074497163295746, 7.075682878494263, 1.2083042860031128], 'asn_force_magnitude': 7.808829633927477, 'residue_force': [-3.074497163295746, 7.075682878494263, 1.2083042860031128], 'residue_force_magnitude': 7.808829633927477, 'total_force': [-4.317662596702576, 6.480961848050356, -10.3846675157547], 'total_force_magnitude': 12.980230975896369, 'motion_component_total': 11.265884049548912, 'cosine_total_motion': 0.867926315831289, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.036668940161641315, 'cosine_residue_motion': -0.036668940161641315, 'cosine_ionic_motion': 0.9895183855227138, 'motion_component_glu': None, 'motion_component_asn': -0.2863415065789381, 'motion_component_residue': -0.2863415065789381, 'motion_component_ionic': 11.55222555612785, 'ionic_contributions': [{'ion_id': 1306, 'distance': 8.39176082611084, 'force': [-1.8574953079223633, 0.8867517709732056, -4.2414045333862305], 'magnitude': 4.714459419250488}, {'ion_id': 1307, 'distance': 8.712069511413574, 'force': [0.4999687671661377, -3.111016035079956, -3.033966064453125], 'magnitude': 4.374167442321777}, {'ion_id': 1316, 'distance': 11.873608589172363, 'force': [-0.3461155891418457, 0.052372146397829056, -2.328737497329712], 'magnitude': 2.35490083694458}, {'ion_id': 1460, 'distance': 11.344376564025879, 'force': [0.46047669649124146, 1.5771710872650146, -1.9888637065887451], 'magnitude': 2.5797455310821533}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.848116159439087, 'force': [5.775625228881836, -14.440893173217773, -3.6939024925231934], 'magnitude': 15.985686302185059}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.7618367671966553, 'force': [-10.727200508117676, 23.33286476135254, 2.629127264022827], 'magnitude': 25.81487464904785}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.397829532623291, 'force': [-1.4129245281219482, 14.79317569732666, 5.298953056335449], 'magnitude': 15.776986122131348}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.9046380519866943, 'force': [-1.0952177047729492, -8.42005443572998, -3.3750810623168945], 'magnitude': 9.137176513671875}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.36522102355957, 'force': [0.5878484845161438, -4.434353828430176, -1.8470145463943481], 'magnitude': 4.839475631713867}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.839544773101807, 'force': [3.7973718643188477, -3.755056142807007, 2.1962220668792725], 'magnitude': 5.774415493011475}]}}</t>
+          <t>{4408: {'frame': 4408, 'motion_vector': [0.9472541809082031, 6.171745300292969, -2.0280227661132812], 'ionic_force': [9.049361620098352, -12.949827790260315, -9.676596252247691], 'ionic_force_magnitude': 18.52634611999143, 'radial_force': 15.798385535513033, 'axial_force': -9.676596252247691, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [3.5434560775756836, 4.623234510421753, -10.538706541061401], 'asn_force_magnitude': 12.04137508221852, 'residue_force': [3.5434560775756836, 4.623234510421753, -10.538706541061401], 'residue_force_magnitude': 12.04137508221852, 'total_force': [12.592817697674036, -8.326593279838562, -20.215302793309093], 'total_force_magnitude': 25.230332543188478, 'cosine_total_motion': 0.009273615003481325, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.6737605041827468, 'cosine_residue_motion': 0.6737605041827468, 'cosine_ionic_motion': -0.42528766897708287, 'motion_component_total': 0.2339763904153358, 'motion_component_glu': None, 'motion_component_asn': 8.113002946449114, 'motion_component_residue': 8.113002946449114, 'motion_component_ionic': -7.879026556033779, 'motion_component_percent_total': 0.9273615003481326, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 67.37605041827467, 'motion_component_percent_residue': 67.37605041827467, 'motion_component_percent_ionic': 42.52876689770829, 'ionic_contributions': [{'ion_id': 1306, 'distance': 7.103499889373779, 'force': [-1.5873969793319702, -6.355767250061035, -0.6117986440658569], 'magnitude': 6.5795063972473145, 'cosine_ionic_motion': -0.9142022132873535, 'motion_component_ionic': -6.0149993896484375, 'motion_component_percent_ionic': 91.42022132873535}, {'ion_id': 1307, 'distance': 10.374420166015625, 'force': [1.3527055978775024, -2.772169589996338, -0.023000208660960197], 'magnitude': 3.0846824645996094, 'cosine_ionic_motion': -0.7792661190032959, 'motion_component_ionic': -2.4037885665893555, 'motion_component_percent_ionic': 77.92661190032959}, {'ion_id': 1308, 'distance': 13.471064567565918, 'force': [0.0392477847635746, -0.5659531354904175, -1.739326000213623], 'magnitude': 1.8295077085494995, 'cosine_ionic_motion': 0.005965552292764187, 'motion_component_ionic': 0.010914023965597153, 'motion_component_percent_ionic': 0.5965552292764187}, {'ion_id': 1316, 'distance': 8.044059753417969, 'force': [0.1305760145187378, -2.5276927947998047, -4.4630842208862305], 'magnitude': 5.130828380584717, 'cosine_ionic_motion': -0.19075140357017517, 'motion_component_ionic': -0.9787126779556274, 'motion_component_percent_ionic': 19.075140357017517}, {'ion_id': 1460, 'distance': 5.888736724853516, 'force': [9.114229202270508, -0.7282450199127197, -2.8393871784210205], 'magnitude': 9.574007987976074, 'cosine_ionic_motion': 0.15746384859085083, 'motion_component_ionic': 1.507560133934021, 'motion_component_percent_ionic': 15.746384859085083}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.416689395904541, 'force': [-12.96794605255127, 8.339502334594727, 13.170660972595215], 'magnitude': 20.277603149414062, 'cosine_with_motion': 0.09370879083871841, 'motion_component': 1.9001896381378174, 'motion_component_percent': 9.370879083871841}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.828958034515381, 'force': [12.381628036499023, -3.9192512035369873, -20.89765167236328], 'magnitude': 24.604412078857422, 'cosine_with_motion': 0.18523332476615906, 'motion_component': 4.557557106018066, 'motion_component_percent': 18.523332476615906}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.574815034866333, 'force': [11.49341106414795, -17.1616268157959, -11.980310440063477], 'magnitude': 23.87776756286621, 'cosine_with_motion': -0.4512225091457367, 'motion_component': -10.774186134338379, 'motion_component_percent': 45.12225091457367}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.129112958908081, 'force': [-3.6253979206085205, 12.196083068847656, 6.366799354553223], 'magnitude': 14.227581977844238, 'cosine_with_motion': 0.6308503150939941, 'motion_component': 8.97547435760498, 'motion_component_percent': 63.085031509399414}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.471631050109863, 'force': [-3.738239049911499, 5.168527126312256, 2.801795244216919], 'magnitude': 6.966933250427246, 'cosine_with_motion': 0.4957659840583801, 'motion_component': 3.4539685249328613, 'motion_component_percent': 49.57659840583801}]}, 4409: {'frame': 4409, 'motion_vector': [1.2028884887695312, 0.22224044799804688, -0.367950439453125], 'ionic_force': [8.281869903206825, -9.407124474644661, -19.244575142860413], 'ionic_force_magnitude': 22.96599730915909, 'radial_force': 12.53329006985403, 'axial_force': -19.244575142860413, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [4.813360691070557, 6.736542046070099, -4.601872891187668], 'asn_force_magnitude': 9.472416480891319, 'residue_force': [4.813360691070557, 6.736542046070099, -4.601872891187668], 'residue_force_magnitude': 9.472416480891319, 'total_force': [13.095230594277382, -2.670582428574562, -23.84644803404808], 'total_force_magnitude': 27.33624258499447, 'cosine_total_motion': 0.6853837955295905, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.7421792013658787, 'cosine_residue_motion': 0.7421792013658787, 'cosine_ionic_motion': 0.5096920914015745, 'motion_component_total': 18.735817698421133, 'motion_component_glu': None, 'motion_component_asn': 7.030230498792906, 'motion_component_residue': 7.030230498792906, 'motion_component_ionic': 11.705587199628228, 'motion_component_percent_total': 68.53837955295904, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 74.21792013658786, 'motion_component_percent_residue': 74.21792013658786, 'motion_component_percent_ionic': 50.969209140157446, 'ionic_contributions': [{'ion_id': 1306, 'distance': 4.740226745605469, 'force': [4.004691123962402, -8.651683807373047, -11.288216590881348], 'magnitude': 14.775419235229492, 'cosine_ionic_motion': 0.37342217564582825, 'motion_component_ionic': 5.51746940612793, 'motion_component_percent_ionic': 37.342217564582825}, {'ion_id': 1307, 'distance': 8.134659767150879, 'force': [1.8958126306533813, -4.239731788635254, -1.8980571031570435], 'magnitude': 5.017175674438477, 'cosine_ionic_motion': 0.31777825951576233, 'motion_component_ionic': 1.5943493843078613, 'motion_component_percent_ionic': 31.777825951576233}, {'ion_id': 1308, 'distance': 14.995219230651855, 'force': [0.11879675090312958, 0.2119782418012619, -1.456363558769226], 'magnitude': 1.4764965772628784, 'cosine_ionic_motion': 0.3848656117916107, 'motion_component_ionic': 0.5682527422904968, 'motion_component_percent_ionic': 38.48656117916107}, {'ion_id': 1316, 'distance': 9.502534866333008, 'force': [0.3882765471935272, 1.0418009757995605, -3.5045788288116455], 'magnitude': 3.6767079830169678, 'cosine_ionic_motion': 0.42330682277679443, 'motion_component_ionic': 1.5563756227493286, 'motion_component_percent_ionic': 42.33068227767944}, {'ion_id': 1460, 'distance': 10.326704025268555, 'force': [1.8742928504943848, 2.2305119037628174, -1.09735906124115], 'magnitude': 3.1132545471191406, 'cosine_ionic_motion': 0.7931057214736938, 'motion_component_ionic': 2.46914005279541, 'motion_component_percent_ionic': 79.31057214736938}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.89084005355835, 'force': [8.498285293579102, -3.1778390407562256, 3.9511711597442627], 'magnitude': 9.89602279663086, 'cosine_with_motion': 0.637795627117157, 'motion_component': 6.311639785766602, 'motion_component_percent': 63.7795627117157}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.35770320892334, 'force': [-7.495138168334961, 4.818055152893066, -5.303986549377441], 'magnitude': 10.369331359863281, 'cosine_with_motion': -0.45248380303382874, 'motion_component': -4.691954612731934, 'motion_component_percent': 45.24838030338287}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.541079998016357, 'force': [-13.760960578918457, 0.9053523540496826, -5.364368915557861], 'magnitude': 14.79730224609375, 'cosine_with_motion': -0.7606579065322876, 'motion_component': -11.255684852600098, 'motion_component_percent': 76.06579065322876}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.812704563140869, 'force': [8.416282653808594, 0.5008266568183899, 4.5553998947143555], 'magnitude': 9.583126068115234, 'cosine_with_motion': 0.6991859674453735, 'motion_component': 6.700387477874756, 'motion_component_percent': 69.91859674453735}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.284165382385254, 'force': [4.813093662261963, 0.14431548118591309, 1.3054699897766113], 'magnitude': 4.9890828132629395, 'cosine_with_motion': 0.8381209969520569, 'motion_component': 4.181455135345459, 'motion_component_percent': 83.81209969520569}, {'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.9146533012390137, 'force': [-11.325387954711914, -10.452134132385254, -1.0463273525238037], 'magnitude': 15.446887016296387, 'cosine_with_motion': -0.7886344790458679, 'motion_component': -12.181947708129883, 'motion_component_percent': 78.86344790458679}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.011950731277466, 'force': [13.774523735046387, 16.59543228149414, -2.446213960647583], 'magnitude': 21.70552635192871, 'cosine_with_motion': 0.763081431388855, 'motion_component': 16.56308364868164, 'motion_component_percent': 76.3081431388855}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.9798951148986816, 'force': [16.72966194152832, 8.269248008728027, 4.781069755554199], 'magnitude': 19.26449203491211, 'cosine_with_motion': 0.8209646940231323, 'motion_component': 15.815467834472656, 'motion_component_percent': 82.09646940231323}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.451082944869995, 'force': [-11.090353012084961, -2.473383665084839, -2.7746827602386475], 'magnitude': 11.696683883666992, 'cosine_with_motion': -0.8613229393959045, 'motion_component': -10.07462215423584, 'motion_component_percent': 86.13229393959045}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.9062395095825195, 'force': [-4.9672088623046875, -2.2703304290771484, -1.9144953489303589], 'magnitude': 5.787301540374756, 'cosine_with_motion': -0.7811997532844543, 'motion_component': -4.52103853225708, 'motion_component_percent': 78.11997532844543}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.611631870269775, 'force': [1.2205619812011719, -6.123000621795654, -0.34490880370140076], 'magnitude': 6.252989292144775, 'cosine_with_motion': 0.029337240383028984, 'motion_component': 0.18344545364379883, 'motion_component_percent': 2.9337240383028984}]}, 4410: {'frame': 4410, 'motion_vector': [-0.20865249633789062, -4.049587249755859, 2.408935546875], 'ionic_force': [15.673005670309067, -6.354610577225685, -18.238948702812195], 'ionic_force_magnitude': 24.8733478268114, 'radial_force': 16.9122494757418, 'axial_force': -18.238948702812195, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-2.721809506416321, 10.137011382728815, 0.07277804613113403], 'asn_force_magnitude': 10.496310942745097, 'residue_force': [-2.721809506416321, 10.137011382728815, 0.07277804613113403], 'residue_force_magnitude': 10.496310942745097, 'total_force': [12.951196163892746, 3.78240080550313, -18.16617065668106], 'total_force_magnitude': 22.628517279237737, 'cosine_total_motion': -0.5788596942852778, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.8141910275658907, 'cosine_residue_motion': -0.8141910275658907, 'cosine_ionic_motion': -0.18303665569925734, 'motion_component_total': -13.098736594388683, 'motion_component_glu': None, 'motion_component_asn': -8.546002192124734, 'motion_component_residue': -8.546002192124734, 'motion_component_ionic': -4.552734402263949, 'motion_component_percent_total': 57.88596942852779, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 81.41910275658907, 'motion_component_percent_residue': 81.41910275658907, 'motion_component_percent_ionic': 18.303665569925734, 'ionic_contributions': [{'ion_id': 1306, 'distance': 4.458994388580322, 'force': [10.753595352172852, -6.403841495513916, -11.053228378295898], 'magnitude': 16.69799041748047, 'cosine_ionic_motion': -0.03729673847556114, 'motion_component_ionic': -0.6227805614471436, 'motion_component_percent_ionic': 3.729673847556114}, {'ion_id': 1307, 'distance': 9.301104545593262, 'force': [2.1814122200012207, -2.955780029296875, -1.1102296113967896], 'magnitude': 3.8376822471618652, 'cosine_ionic_motion': 0.4883864223957062, 'motion_component_ionic': 1.8742718696594238, 'motion_component_percent_ionic': 48.83864223957062}, {'ion_id': 1308, 'distance': 14.55396556854248, 'force': [0.2570955455303192, 0.21237300336360931, -1.531499981880188], 'magnitude': 1.5673840045928955, 'cosine_ionic_motion': -0.6226418018341064, 'motion_component_ionic': -0.9759188294410706, 'motion_component_percent_ionic': 62.264180183410645}, {'ion_id': 1316, 'distance': 9.078113555908203, 'force': [1.0977156162261963, 1.1136078834533691, -3.712677240371704], 'magnitude': 4.0285325050354, 'cosine_ionic_motion': -0.7200942635536194, 'motion_component_ionic': -2.900923252105713, 'motion_component_percent_ionic': 72.00942635536194}, {'ion_id': 1460, 'distance': 11.939895629882812, 'force': [1.383186936378479, 1.6790300607681274, -0.8313134908676147], 'magnitude': 2.3288259506225586, 'cosine_ionic_motion': -0.8276203274726868, 'motion_component_ionic': -1.9273836612701416, 'motion_component_percent_ionic': 82.76203274726868}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.73225736618042, 'force': [6.547236442565918, -2.216608762741089, 2.029426336288452], 'magnitude': 7.204042911529541, 'cosine_with_motion': 0.3678550124168396, 'motion_component': 2.650043249130249, 'motion_component_percent': 36.78550124168396}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.05270528793335, 'force': [-6.328794479370117, 3.563107967376709, -2.5960657596588135], 'magnitude': 7.712906837463379, 'cosine_with_motion': -0.5322520732879639, 'motion_component': -4.105210781097412, 'motion_component_percent': 53.22520732879639}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.484741687774658, 'force': [-9.65060806274414, 0.8191473484039307, -3.01424503326416], 'magnitude': 10.143515586853027, 'cosine_with_motion': -0.17901991307735443, 'motion_component': -1.8158912658691406, 'motion_component_percent': 17.901991307735443}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.884988784790039, 'force': [5.276494979858398, -0.04528632387518883, 2.4972031116485596], 'magnitude': 5.837762832641602, 'cosine_with_motion': 0.18515437841415405, 'motion_component': 1.0808873176574707, 'motion_component_percent': 18.515437841415405}, {'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.5908331871032715, 'force': [-12.240410804748535, -13.4556245803833, -2.4805119037628174], 'magnitude': 18.358497619628906, 'cosine_with_motion': 0.5897823572158813, 'motion_component': 10.827518463134766, 'motion_component_percent': 58.978235721588135}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.6594109535217285, 'force': [12.675597190856934, 24.51116943359375, 3.6999547481536865], 'magnitude': 27.841655731201172, 'cosine_with_motion': -0.7081539630889893, 'motion_component': -19.71617889404297, 'motion_component_percent': 70.81539630889893}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.7416653633117676, 'force': [19.326404571533203, 9.764897346496582, 2.487921953201294], 'magnitude': 21.79570770263672, 'cosine_with_motion': -0.3655935525894165, 'motion_component': -7.968369960784912, 'motion_component_percent': 36.55935525894165}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.178309679031372, 'force': [-13.40526294708252, -3.137441635131836, -0.7964059710502625], 'magnitude': 13.790535926818848, 'cosine_with_motion': 0.20884327590465546, 'motion_component': 2.8800606727600098, 'motion_component_percent': 20.884327590465546}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.718949794769287, 'force': [-5.611135005950928, -2.574636936187744, -1.010662317276001], 'magnitude': 6.255799770355225, 'cosine_with_motion': 0.31052926182746887, 'motion_component': 1.9426088333129883, 'motion_component_percent': 31.052926182746887}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.2427778244018555, 'force': [0.6886686086654663, -7.091712474822998, -0.7438371181488037], 'magnitude': 7.163794040679932, 'cosine_with_motion': 0.792670726776123, 'motion_component': 5.678529739379883, 'motion_component_percent': 79.2670726776123}]}, 4411: {'frame': 4411, 'motion_vector': [-2.447307586669922, -1.137054443359375, 2.16204833984375], 'ionic_force': [8.995075047016144, -8.02235746383667, -9.743937104940414], 'ionic_force_magnitude': 15.498835591232748, 'radial_force': 12.052783677600308, 'axial_force': -9.743937104940414, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-2.7447137013077736, -6.466000556945801, -3.4784128069877625], 'asn_force_magnitude': 7.838492977632021, 'residue_force': [-2.7447137013077736, -6.466000556945801, -3.4784128069877625], 'residue_force_magnitude': 7.838492977632021, 'total_force': [6.25036134570837, -14.48835802078247, -13.222349911928177], 'total_force_magnitude': 20.58664791275559, 'cosine_total_motion': -0.3850492590103777, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.24161728779535188, 'cosine_residue_motion': 0.24161728779535188, 'cosine_ionic_motion': -0.6336468878686462, 'motion_component_total': -7.926873524314079, 'motion_component_glu': None, 'motion_component_asn': 1.8939154136583607, 'motion_component_residue': 1.8939154136583607, 'motion_component_ionic': -9.82078893797244, 'motion_component_percent_total': 38.504925901037765, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 24.16172877953519, 'motion_component_percent_residue': 24.16172877953519, 'motion_component_percent_ionic': 63.36468878686462, 'ionic_contributions': [{'ion_id': 1306, 'distance': 7.156948566436768, 'force': [1.557535171508789, -6.21755838394165, 0.962909996509552], 'magnitude': 6.481600284576416, 'cosine_ionic_motion': 0.23825237154960632, 'motion_component_ionic': 1.5442566871643066, 'motion_component_percent_ionic': 23.825237154960632}, {'ion_id': 1307, 'distance': 11.11915111541748, 'force': [1.0693477392196655, -2.452256441116333, -0.23202911019325256], 'magnitude': 2.685312509536743, 'cosine_ionic_motion': -0.03557547181844711, 'motion_component_ionic': -0.09553125500679016, 'motion_component_percent_ionic': 3.5575471818447113}, {'ion_id': 1308, 'distance': 12.464065551757812, 'force': [0.3361741900444031, -0.34610939025878906, -2.0818889141082764], 'magnitude': 2.1370694637298584, 'cosine_ionic_motion': -0.6671931743621826, 'motion_component_ionic': -1.4258381128311157, 'motion_component_percent_ionic': 66.71931743621826}, {'ion_id': 1316, 'distance': 6.50744104385376, 'force': [2.108905553817749, -1.8903121948242188, -7.310626983642578], 'magnitude': 7.840027332305908, 'cosine_ionic_motion': -0.6941344141960144, 'motion_component_ionic': -5.442032814025879, 'motion_component_percent_ionic': 69.41344141960144}, {'ion_id': 1460, 'distance': 8.158514022827148, 'force': [3.923112392425537, 2.8838789463043213, -1.0823020935058594], 'magnitude': 4.987879753112793, 'cosine_ionic_motion': -0.8824678063392639, 'motion_component_ionic': -4.4016432762146, 'motion_component_percent_ionic': 88.24678063392639}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.379117012023926, 'force': [-2.057718515396118, -3.9980130195617676, 1.7207963466644287], 'magnitude': 4.814504623413086, 'cosine_with_motion': 0.7990415096282959, 'motion_component': 3.8469889163970947, 'motion_component_percent': 79.90415096282959}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.32531213760376, 'force': [-1.0138967037200928, 11.15296459197998, 5.889075756072998], 'magnitude': 12.652976989746094, 'cosine_with_motion': 0.05787748843431473, 'motion_component': 0.7323225140571594, 'motion_component_percent': 5.787748843431473}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.63965106010437, 'force': [-0.12175191938877106, -11.074440002441406, -9.914205551147461], 'magnitude': 14.864370346069336, 'cosine_with_motion': -0.16624541580677032, 'motion_component': -2.4711334705352783, 'motion_component_percent': 16.624541580677032}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.949275970458984, 'force': [-1.204451322555542, -11.803104400634766, -3.7968087196350098], 'magnitude': 12.45711612701416, 'cosine_with_motion': 0.18942785263061523, 'motion_component': 2.359724760055542, 'motion_component_percent': 18.942785263061523}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.030297756195068, 'force': [1.6128840446472168, 4.96711540222168, 1.7422451972961426], 'magnitude': 5.505365371704102, 'cosine_with_motion': -0.30616089701652527, 'motion_component': -1.6855276823043823, 'motion_component_percent': 30.616089701652527}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.640200614929199, 'force': [0.0402207151055336, 4.2894768714904785, 0.8804841637611389], 'magnitude': 4.379096031188965, 'cosine_with_motion': -0.20288658142089844, 'motion_component': -0.8884598016738892, 'motion_component_percent': 20.288658142089844}]}, 4414: {'frame': 4414, 'motion_vector': [-0.04938507080078125, -0.9767036437988281, 0.471405029296875], 'ionic_force': [1.0051689818501472, 3.150031417608261, -16.299150347709656], 'ionic_force_magnitude': 16.631156444193426, 'radial_force': 3.3065182010678202, 'axial_force': -16.299150347709656, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-9.326332688331604, 6.6415345668792725, 9.811745405197144], 'asn_force_magnitude': 15.078488343096668, 'residue_force': [-9.326332688331604, 6.6415345668792725, 9.811745405197144], 'residue_force_magnitude': 15.078488343096668, 'total_force': [-8.321163706481457, 9.791565984487534, -6.487404942512512], 'total_force_magnitude': 14.394545937499151, 'cosine_total_motion': -0.7813717066815894, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.08557976932595379, 'cosine_residue_motion': -0.08557976932595379, 'cosine_ionic_motion': -0.5987002410394829, 'motion_component_total': -11.24749092609025, 'motion_component_glu': None, 'motion_component_asn': -1.290413554186296, 'motion_component_residue': -1.290413554186296, 'motion_component_ionic': -9.957077371903955, 'motion_component_percent_total': 78.13717066815894, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 8.557976932595379, 'motion_component_percent_residue': 8.557976932595379, 'motion_component_percent_ionic': 59.870024103948296, 'ionic_contributions': [{'ion_id': 1306, 'distance': 5.7553391456604, 'force': [-0.07259159535169601, 3.9749860763549805, -9.200763702392578], 'magnitude': 10.022965431213379, 'cosine_ionic_motion': -0.7550632357597351, 'motion_component_ionic': -7.567972660064697, 'motion_component_percent_ionic': 75.50632357597351}, {'ion_id': 1307, 'distance': 8.831177711486816, 'force': [0.6202806830406189, -2.786587715148926, -3.157846212387085], 'magnitude': 4.256971836090088, 'cosine_ionic_motion': 0.2601761817932129, 'motion_component_ionic': 1.1075626611709595, 'motion_component_percent_ionic': 26.01761817932129}, {'ion_id': 1316, 'distance': 12.10187816619873, 'force': [-0.3398584723472595, 0.2946309745311737, -2.221829891204834], 'magnitude': 2.2669007778167725, 'cosine_ionic_motion': -0.5356953144073486, 'motion_component_ionic': -1.2143681049346924, 'motion_component_percent_ionic': 53.56953144073486}, {'ion_id': 1460, 'distance': 11.469853401184082, 'force': [0.7973383665084839, 1.6670020818710327, -1.7187105417251587], 'magnitude': 2.5236105918884277, 'cosine_ionic_motion': -0.9043784737586975, 'motion_component_ionic': -2.282299041748047, 'motion_component_percent_ionic': 90.43784737586975}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.720937967300415, 'force': [7.105258464813232, -12.653792381286621, -9.039254188537598], 'magnitude': 17.09711265563965, 'cosine_with_motion': 0.4173719584941864, 'motion_component': 7.135855197906494, 'motion_component_percent': 41.73719584941864}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.6477584838867188, 'force': [-14.25243091583252, 16.973936080932617, 17.252464294433594], 'magnitude': 28.08725357055664, 'cosine_with_motion': -0.2538893222808838, 'motion_component': -7.131053924560547, 'motion_component_percent': 25.38893222808838}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.404152870178223, 'force': [-2.494011402130127, 12.281402587890625, 9.509675979614258], 'magnitude': 15.731715202331543, 'cosine_with_motion': -0.4326501786708832, 'motion_component': -6.806329250335693, 'motion_component_percent': 43.26501786708832}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.1764421463012695, 'force': [-0.5048230290412903, -6.006754398345947, -5.239223003387451], 'magnitude': 7.986576080322266, 'cosine_with_motion': 0.3946644961833954, 'motion_component': 3.1520180702209473, 'motion_component_percent': 39.46644961833954}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.36414909362793, 'force': [0.8196741938591003, -3.9532573223114014, -2.671917676925659], 'magnitude': 4.841410160064697, 'cosine_with_motion': 0.4872744679450989, 'motion_component': 2.359095573425293, 'motion_component_percent': 48.72744679450989}]}, 4415: {'frame': 4415, 'motion_vector': [-1.1576690673828125, 0.13907241821289062, -4.969749450683594], 'ionic_force': [-1.2431654334068298, -0.5947210304439068, -11.592971801757812], 'ionic_force_magnitude': 11.674594151199504, 'radial_force': 1.3780977464860225, 'axial_force': -11.592971801757812, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-3.074497163295746, 7.075682878494263, 1.2083042860031128], 'asn_force_magnitude': 7.808829633927477, 'residue_force': [-3.074497163295746, 7.075682878494263, 1.2083042860031128], 'residue_force_magnitude': 7.808829633927477, 'total_force': [-4.317662596702576, 6.480961848050356, -10.3846675157547], 'total_force_magnitude': 12.980230975896369, 'cosine_total_motion': 0.867926315831289, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.036668940161641315, 'cosine_residue_motion': -0.036668940161641315, 'cosine_ionic_motion': 0.9895183855227138, 'motion_component_total': 11.265884049548912, 'motion_component_glu': None, 'motion_component_asn': -0.2863415065789381, 'motion_component_residue': -0.2863415065789381, 'motion_component_ionic': 11.55222555612785, 'motion_component_percent_total': 86.7926315831289, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 3.6668940161641315, 'motion_component_percent_residue': 3.6668940161641315, 'motion_component_percent_ionic': 98.95183855227138, 'ionic_contributions': [{'ion_id': 1306, 'distance': 8.39176082611084, 'force': [-1.8574953079223633, 0.8867517709732056, -4.2414045333862305], 'magnitude': 4.714459419250488, 'cosine_ionic_motion': 0.9703527092933655, 'motion_component_ionic': 4.57468843460083, 'motion_component_percent_ionic': 97.03527092933655}, {'ion_id': 1307, 'distance': 8.712069511413574, 'force': [0.4999687671661377, -3.111016035079956, -3.033966064453125], 'magnitude': 4.374167442321777, 'cosine_ionic_motion': 0.6299753189086914, 'motion_component_ionic': 2.755617618560791, 'motion_component_percent_ionic': 62.99753189086914}, {'ion_id': 1316, 'distance': 11.873608589172363, 'force': [-0.3461155891418457, 0.052372146397829056, -2.328737497329712], 'magnitude': 2.35490083694458, 'cosine_ionic_motion': 0.996685266494751, 'motion_component_ionic': 2.347095012664795, 'motion_component_percent_ionic': 99.6685266494751}, {'ion_id': 1460, 'distance': 11.344376564025879, 'force': [0.46047669649124146, 1.5771710872650146, -1.9888637065887451], 'magnitude': 2.5797455310821533, 'cosine_ionic_motion': 0.726747989654541, 'motion_component_ionic': 1.87482488155365, 'motion_component_percent_ionic': 72.6747989654541}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.848116159439087, 'force': [5.775625228881836, -14.440893173217773, -3.6939024925231934], 'magnitude': 15.985686302185059, 'cosine_with_motion': 0.11841823905706406, 'motion_component': 1.8929967880249023, 'motion_component_percent': 11.841823905706406}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.7618367671966553, 'force': [-10.727200508117676, 23.33286476135254, 2.629127264022827], 'magnitude': 25.81487464904785, 'cosine_with_motion': 0.019710563123226166, 'motion_component': 0.5088257193565369, 'motion_component_percent': 1.9710563123226166}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.397829532623291, 'force': [-1.4129245281219482, 14.79317569732666, 5.298953056335449], 'magnitude': 15.776986122131348, 'cosine_with_motion': -0.2811318337917328, 'motion_component': -4.435412883758545, 'motion_component_percent': 28.11318337917328}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.9046380519866943, 'force': [-1.0952177047729492, -8.42005443572998, -3.3750810623168945], 'magnitude': 9.137176513671875, 'cosine_with_motion': 0.36169153451919556, 'motion_component': 3.3048393726348877, 'motion_component_percent': 36.169153451919556}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.36522102355957, 'force': [0.5878484845161438, -4.434353828430176, -1.8470145463943481], 'magnitude': 4.839475631713867, 'cosine_with_motion': 0.31905555725097656, 'motion_component': 1.5440616607666016, 'motion_component_percent': 31.905555725097656}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.839544773101807, 'force': [3.7973718643188477, -3.755056142807007, 2.1962220668792725], 'magnitude': 5.774415493011475, 'cosine_with_motion': -0.537136971950531, 'motion_component': -3.101651906967163, 'motion_component_percent': 53.7136971950531}]}}</t>
         </is>
       </c>
     </row>
@@ -579,7 +579,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>{4857: {'frame': 4857, 'ionic_force': [-24.356317825615406, 5.643100440502167, 5.592016190290451], 'ionic_force_magnitude': 25.619239756020416, 'motion_vector': [0.9804725646972656, -0.3909263610839844, 0.2857513427734375], 'ionic_force_x': -24.356317825615406, 'ionic_force_y': 5.643100440502167, 'ionic_force_z': 5.592016190290451, 'radial_force': 25.001495967321368, 'axial_force': 5.592016190290451, 'glu_force': [-10.987810134887695, 14.360766410827637, -2.7645459175109863], 'glu_force_magnitude': 18.292246925862408, 'asn_force': [1.3874993324279785, -0.3169316053390503, -0.6931047439575195], 'asn_force_magnitude': 1.5830332359263, 'residue_force': [-9.600310802459717, 14.043834805488586, -3.457650661468506], 'residue_force_magnitude': 17.359453091743156, 'total_force': [-33.95662862807512, 19.686935245990753, 2.134365528821945], 'total_force_magnitude': 39.30882297112784, 'motion_component_total': -36.92615122325311, 'cosine_total_motion': -0.9393858282242439, 'cosine_glu_motion': -0.8587285038781322, 'cosine_asn_motion': 0.7430262111290231, 'cosine_residue_motion': -0.8371138520916579, 'cosine_ionic_motion': -0.8741208868290865, 'motion_component_glu': -15.708073835215188, 'motion_component_asn': 1.1762351873816357, 'motion_component_residue': -14.531838647833553, 'motion_component_ionic': -22.394312575419555, 'ionic_contributions': [{'ion_id': 1306, 'distance': 8.758042335510254, 'force': [-0.837573766708374, 2.762312173843384, 3.2253456115722656], 'magnitude': 4.328366279602051}, {'ion_id': 1307, 'distance': 11.013960838317871, 'force': [0.08748745173215866, 2.7204031944274902, -0.2865326702594757], 'magnitude': 2.7368502616882324}, {'ion_id': 1308, 'distance': 10.233463287353516, 'force': [-1.2521235942840576, 1.593077540397644, -2.4381844997406006], 'magnitude': 3.1702449321746826}, {'ion_id': 1320, 'distance': 13.275734901428223, 'force': [-0.6172628998756409, 0.6778424382209778, -1.6455979347229004], 'magnitude': 1.8837400674819946}, {'ion_id': 1460, 'distance': 3.8113815784454346, 'force': [-21.736845016479492, -2.110534906387329, 6.736985683441162], 'magnitude': 22.854578018188477}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.83697247505188, 'force': [9.213166236877441, -15.410645484924316, -2.738801956176758], 'magnitude': 18.162363052368164}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 3.656285047531128, 'force': [-7.278402328491211, 18.777568817138672, -2.814974069595337], 'magnitude': 20.33460807800293}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 3.9761993885040283, 'force': [-12.922574043273926, 10.993843078613281, 2.7892301082611084], 'magnitude': 17.194107055664062}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.785486698150635, 'force': [-1.0566141605377197, 1.7043412923812866, 6.781833171844482], 'magnitude': 7.072091102600098}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.924427509307861, 'force': [2.4441134929656982, -2.021272897720337, -7.474937915802002], 'magnitude': 8.11997127532959}]}, 4858: {'frame': 4858, 'ionic_force': [-9.28166988492012, 11.450447499752045, 3.758600100874901], 'ionic_force_magnitude': 15.211483113605581, 'motion_vector': [-0.14766693115234375, 1.5113677978515625, -0.5906982421875], 'ionic_force_x': -9.28166988492012, 'ionic_force_y': 11.450447499752045, 'ionic_force_z': 3.758600100874901, 'radial_force': 14.73981491733227, 'axial_force': 3.758600100874901, 'glu_force': [-13.212425708770752, 22.319079399108887, -0.6105731129646301], 'glu_force_magnitude': 25.943829668339028, 'asn_force': [1.2593601942062378, -0.28960487246513367, -5.6734819412231445], 'asn_force_magnitude': 5.818784788793263, 'residue_force': [-11.953065514564514, 22.029474526643753, -6.284055054187775], 'residue_force_magnitude': 25.839173188002366, 'total_force': [-21.234735399484634, 33.4799220263958, -2.525454953312874], 'total_force_magnitude': 39.72652878242549, 'motion_component_total': 33.89452367006175, 'cosine_total_motion': 0.8531962068897461, 'cosine_glu_motion': 0.8526488047331512, 'cosine_asn_motion': 0.2876916306146544, 'cosine_residue_motion': 0.9208882524167568, 'cosine_ionic_motion': 0.6639413496791131, 'motion_component_glu': 22.12097535690974, 'motion_component_asn': 1.674015684083681, 'motion_component_residue': 23.794991040993416, 'motion_component_ionic': 10.099532629068328, 'ionic_contributions': [{'ion_id': 1306, 'distance': 8.15285587310791, 'force': [-2.1441845893859863, 4.504876136779785, 0.23799630999565125], 'magnitude': 4.994805335998535}, {'ion_id': 1307, 'distance': 9.122523307800293, 'force': [1.3651424646377563, 3.7462639808654785, -0.13131223618984222], 'magnitude': 3.9894046783447266}, {'ion_id': 1308, 'distance': 9.799673080444336, 'force': [-1.0608267784118652, 1.5705699920654297, -2.8913075923919678], 'magnitude': 3.4571235179901123}, {'ion_id': 1320, 'distance': 13.182660102844238, 'force': [-0.4662999212741852, 0.6704815030097961, -1.7270715236663818], 'magnitude': 1.9104337692260742}, {'ion_id': 1460, 'distance': 5.5286970138549805, 'force': [-6.97550106048584, 0.9582558870315552, 8.270295143127441], 'magnitude': 10.861567497253418}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.764124870300293, 'force': [9.685281753540039, -15.975787162780762, -2.669835090637207], 'magnitude': 18.872161865234375}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 3.528026819229126, 'force': [-4.353703022003174, 21.1895809173584, 3.005239725112915], 'magnitude': 21.839975357055664}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 3.281412124633789, 'force': [-18.544004440307617, 17.10528564453125, -0.9459777474403381], 'magnitude': 25.246105194091797}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.8172383308410645, 'force': [1.2593601942062378, -0.28960487246513367, -5.6734819412231445], 'magnitude': 5.818784713745117}]}, 4859: {'frame': 4859, 'ionic_force': [-11.826732784509659, 21.502933859825134, 4.421850718557835], 'ionic_force_magnitude': 24.93592863146308, 'motion_vector': [-0.5728759765625, -0.2980232238769531, -0.14586639404296875], 'ionic_force_x': -11.826732784509659, 'ionic_force_y': 21.502933859825134, 'ionic_force_z': 4.421850718557835, 'radial_force': 24.540737008822898, 'axial_force': 4.421850718557835, 'glu_force': [-25.724108695983887, 18.06024932861328, -1.9480111598968506], 'glu_force_magnitude': 31.49122292788187, 'asn_force': [0.7898761257529259, -1.310462236404419, -0.060089111328125], 'asn_force_magnitude': 1.5312825566748702, 'residue_force': [-24.93423257023096, 16.749787092208862, -2.0081002712249756], 'residue_force_magnitude': 30.104879807100822, 'total_force': [-36.76096535474062, 38.252720952034, 2.413750447332859], 'total_force_magnitude': 53.108054241034104, 'motion_component_total': 14.058594196187208, 'cosine_total_motion': 0.26471680043824297, 'cosine_glu_motion': 0.46232058577826657, 'cosine_asn_motion': -0.05246634818604452, 'cosine_residue_motion': 0.48094195757883484, 'cosine_ionic_motion': -0.016847402682462258, 'motion_component_glu': 14.559040630892326, 'motion_component_asn': -0.0803408037897202, 'motion_component_residue': 14.478699827102606, 'motion_component_ionic': -0.42010563091539854, 'ionic_contributions': [{'ion_id': 1306, 'distance': 7.285847187042236, 'force': [-3.3123834133148193, 5.30451774597168, 0.07961202412843704], 'magnitude': 6.254289150238037}, {'ion_id': 1307, 'distance': 10.17105484008789, 'force': [1.019066572189331, 3.0403809547424316, -0.13036009669303894], 'magnitude': 3.209268808364868}, {'ion_id': 1308, 'distance': 10.916866302490234, 'force': [-0.8318650126457214, 1.5506973266601562, -2.159569263458252], 'magnitude': 2.785749673843384}, {'ion_id': 1320, 'distance': 14.021308898925781, 'force': [-0.4241594970226288, 0.7252730131149292, -1.4648845195770264], 'magnitude': 1.6887328624725342}, {'ion_id': 1460, 'distance': 4.570935249328613, 'force': [-8.27739143371582, 10.882064819335938, 8.097052574157715], 'magnitude': 15.890148162841797}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.507916212081909, 'force': [17.08523178100586, -11.745720863342285, -6.504417419433594], 'magnitude': 21.729578018188477}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 2.6400349140167236, 'force': [-30.043292999267578, 24.848541259765625, 1.0838556289672852], 'magnitude': 39.002872467041016}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 4.386460304260254, 'force': [-12.766047477722168, 4.957428932189941, 3.472550630569458], 'magnitude': 14.128222465515137}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.7132649421691895, 'force': [0.1196339949965477, 2.5797061920166016, 6.776618957519531], 'magnitude': 7.252017974853516}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.994253158569336, 'force': [0.6702421307563782, -3.8901684284210205, -6.836708068847656], 'magnitude': 7.894505023956299}]}, 4860: {'frame': 4860, 'ionic_force': [-4.794602394104004, 12.35471922159195, -2.0622036159038544], 'ionic_force_magnitude': 13.411934346520205, 'motion_vector': [0.6911888122558594, -0.11594009399414062, 0.5926361083984375], 'ionic_force_x': -4.794602394104004, 'ionic_force_y': 12.35471922159195, 'ionic_force_z': -2.0622036159038544, 'radial_force': 13.25244502580265, 'axial_force': -2.0622036159038544, 'glu_force': [-19.473167419433594, 22.178525924682617, 0.19907911121845245], 'glu_force_magnitude': 29.51492663093765, 'asn_force': [-0.04808613657951355, -0.5574445724487305, 1.5964374542236328], 'asn_force_magnitude': 1.691646911483518, 'residue_force': [-19.521253556013107, 21.621081352233887, 1.7955165654420853], 'residue_force_magnitude': 29.185173958276266, 'total_force': [-24.31585595011711, 33.975800573825836, -0.2666870504617691], 'total_force_magnitude': 41.78141928180653, 'motion_component_total': -22.7756549592314, 'cosine_total_motion': -0.5451144396415687, 'cosine_glu_motion': -0.587423963429649, 'cosine_asn_motion': 0.6295749638971516, 'cosine_residue_motion': -0.5575692871291635, 'cosine_ionic_motion': -0.4848590928468034, 'motion_component_glu': -17.33777518188069, 'motion_component_asn': 1.0650185432239638, 'motion_component_residue': -16.272756638656727, 'motion_component_ionic': -6.502898320574672, 'ionic_contributions': [{'ion_id': 1306, 'distance': 9.515270233154297, 'force': [-2.5619351863861084, 2.5342040061950684, 0.6784204840660095], 'magnitude': 3.66687273979187}, {'ion_id': 1307, 'distance': 10.100597381591797, 'force': [0.7434799671173096, 3.142179489135742, -0.4046603739261627], 'magnitude': 3.2541980743408203}, {'ion_id': 1308, 'distance': 10.912854194641113, 'force': [-0.9280287027359009, 1.4536443948745728, -2.190319776535034], 'magnitude': 2.7877984046936035}, {'ion_id': 1320, 'distance': 14.029218673706055, 'force': [-0.4511340856552124, 0.7071818709373474, -1.4634768962860107], 'magnitude': 1.6868292093276978}, {'ion_id': 1460, 'distance': 8.173669815063477, 'force': [-1.5969843864440918, 4.517509460449219, 1.3178329467773438], 'magnitude': 4.969399929046631}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.5046865940093994, 'force': [13.607168197631836, -15.845686912536621, -6.138125419616699], 'magnitude': 21.769643783569336}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 2.8582470417022705, 'force': [-16.38758087158203, 28.959178924560547, 0.17417438328266144], 'magnitude': 33.274871826171875}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 3.689500570297241, 'force': [-16.6927547454834, 9.065033912658691, 6.16303014755249], 'magnitude': 19.970123291015625}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.874335765838623, 'force': [-0.44713327288627625, 2.8439011573791504, 6.226464748382568], 'magnitude': 6.859778881072998}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.847378730773926, 'force': [0.3990471363067627, -3.401345729827881, -4.6300272941589355], 'magnitude': 5.758953094482422}]}, 4861: {'frame': 4861, 'ionic_force': [-6.5610339641571045, 14.756245732307434, 0.32843945175409317], 'ionic_force_magnitude': 16.152455765750698, 'motion_vector': [0.4648017883300781, 0.24734878540039062, -0.2841033935546875], 'ionic_force_x': -6.5610339641571045, 'ionic_force_y': 14.756245732307434, 'ionic_force_z': 0.32843945175409317, 'radial_force': 16.14911622321991, 'axial_force': 0.32843945175409317, 'glu_force': [-24.28467082977295, 14.03956127166748, -4.462919235229492], 'glu_force_magnitude': 28.40373507325246, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [-24.28467082977295, 14.03956127166748, -4.462919235229492], 'residue_force_magnitude': 28.40373507325246, 'total_force': [-30.845704793930054, 28.795807003974915, -4.134479783475399], 'total_force_magnitude': 42.39988123007442, 'motion_component_total': -10.09548801673443, 'cosine_total_motion': -0.2381017994355526, 'cosine_glu_motion': -0.3852662650484079, 'cosine_asn_motion': None, 'cosine_residue_motion': -0.3852662650484079, 'cosine_ionic_motion': 0.05246960094817645, 'motion_component_glu': -10.943000925096442, 'motion_component_asn': None, 'motion_component_residue': -10.943000925096442, 'motion_component_ionic': 0.847512908362011, 'ionic_contributions': [{'ion_id': 1306, 'distance': 7.293181419372559, 'force': [-4.193318843841553, 3.516507863998413, 3.0015461444854736], 'magnitude': 6.2417168617248535}, {'ion_id': 1307, 'distance': 11.440825462341309, 'force': [0.5813269019126892, 2.4661834239959717, -0.11614765971899033], 'magnitude': 2.536432981491089}, {'ion_id': 1308, 'distance': 10.164334297180176, 'force': [-0.8082016706466675, 1.8407821655273438, -2.506990909576416], 'magnitude': 3.2135140895843506}, {'ion_id': 1320, 'distance': 13.986430168151855, 'force': [-0.4184555411338806, 0.7065335512161255, -1.485287070274353], 'magnitude': 1.6971659660339355}, {'ion_id': 1460, 'distance': 7.0830183029174805, 'force': [-1.7223848104476929, 6.22623872756958, 1.435318946838379], 'magnitude': 6.617612838745117}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.7518699169158936, 'force': [15.4595308303833, -10.6598539352417, -2.864459991455078], 'magnitude': 18.995649337768555}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 2.808248519897461, 'force': [-27.88861846923828, 19.966638565063477, -3.4291157722473145], 'magnitude': 34.47028350830078}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 4.591255187988281, 'force': [-11.855583190917969, 4.732776641845703, 1.8306565284729004], 'magnitude': 12.895942687988281}], 'asn_contributions': []}, 4862: {'frame': 4862, 'ionic_force': [-3.6536727249622345, 22.094812095165253, -0.211676687002182], 'ionic_force_magnitude': 22.395866871403168, 'motion_vector': [-0.7869873046875, 0.3434638977050781, -0.23621368408203125], 'ionic_force_x': -3.6536727249622345, 'ionic_force_y': 22.094812095165253, 'ionic_force_z': -0.211676687002182, 'radial_force': 22.394866507791328, 'axial_force': -0.211676687002182, 'glu_force': [-24.35048484802246, 16.70631217956543, -6.922949433326721], 'glu_force_magnitude': 30.33107660191551, 'asn_force': [0.6463719010353088, -1.5418689846992493, -3.0950231552124023], 'asn_force_magnitude': 3.5177158685326515, 'residue_force': [-23.704112946987152, 15.16444319486618, -10.017972588539124], 'residue_force_magnitude': 29.869802188808823, 'total_force': [-27.357785671949387, 37.25925529003143, -10.229649275541306], 'total_force_magnitude': 47.34285865830915, 'motion_component_total': 41.25881202745113, 'cosine_total_motion': 0.8714896648981671, 'cosine_glu_motion': 0.9824119865927807, 'cosine_asn_motion': -0.09805255670832731, 'cosine_residue_motion': 0.9860357293004586, 'cosine_ionic_motion': 0.5271561895745854, 'motion_component_glu': 29.797613219985625, 'motion_component_asn': -0.34492103468308066, 'motion_component_residue': 29.452692185302542, 'motion_component_ionic': 11.806119842148586, 'ionic_contributions': [{'ion_id': 1306, 'distance': 9.68929386138916, 'force': [-1.5576599836349487, 2.6959004402160645, 1.676754355430603], 'magnitude': 3.5363383293151855}, {'ion_id': 1307, 'distance': 10.900853157043457, 'force': [0.7250994443893433, 2.6796772480010986, -0.3156937062740326], 'magnitude': 2.793940305709839}, {'ion_id': 1308, 'distance': 10.722567558288574, 'force': [-0.5865727663040161, 1.652468204498291, -2.294264078140259], 'magnitude': 2.8876230716705322}, {'ion_id': 1320, 'distance': 14.130182266235352, 'force': [-0.32260993123054504, 0.7156185507774353, -1.465861201286316], 'magnitude': 1.6628097295761108}, {'ion_id': 1460, 'distance': 4.761733531951904, 'force': [-1.9119294881820679, 14.351147651672363, 2.1873879432678223], 'magnitude': 14.642252922058105}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.4525365829467773, 'force': [18.71674919128418, -12.027681350708008, -2.8678622245788574], 'magnitude': 22.43226432800293}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 2.7261617183685303, 'force': [-26.637910842895508, 24.350927352905273, -5.946378231048584], 'magnitude': 36.577388763427734}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 3.986100435256958, 'force': [-16.429323196411133, 4.383066177368164, 1.8912910223007202], 'magnitude': 17.108797073364258}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.824161529541016, 'force': [1.4364039897918701, -2.5230722427368164, -8.514288902282715], 'magnitude': 8.995680809020996}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.003833293914795, 'force': [-0.7900320887565613, 0.9812032580375671, 5.4192657470703125], 'magnitude': 5.563753128051758}]}, 4863: {'frame': 4863, 'ionic_force': [-0.5461589097976685, 16.03918308019638, -1.5026157051324844], 'ionic_force_magnitude': 16.118670459815228, 'motion_vector': [1.4510307312011719, -0.018299102783203125, -1.9164810180664062], 'ionic_force_x': -0.5461589097976685, 'ionic_force_y': 16.03918308019638, 'ionic_force_z': -1.5026157051324844, 'radial_force': 16.048479162674862, 'axial_force': -1.5026157051324844, 'glu_force': [-28.76598358154297, 12.570500135421753, -4.275290012359619], 'glu_force_magnitude': 31.682446082302732, 'asn_force': [-6.290740668773651, 2.413153886795044, -6.250876426696777], 'asn_force_magnitude': 9.190766341549015, 'residue_force': [-35.05672425031662, 14.983654022216797, -10.526166439056396], 'residue_force_magnitude': 39.55103011203309, 'total_force': [-35.60288316011429, 31.022837102413177, -12.028782144188881], 'total_force_magnitude': 48.730619851054335, 'motion_component_total': -12.136803217678604, 'cosine_total_motion': -0.24905907732704557, 'cosine_glu_motion': -0.4434905291726908, 'cosine_asn_motion': 0.12707127026887044, 'cosine_residue_motion': -0.3257306418636394, 'cosine_ionic_motion': 0.04629285082428669, 'motion_component_glu': -14.050864778525682, 'motion_component_asn': 1.1678823537650125, 'motion_component_residue': -12.88298242476067, 'motion_component_ionic': 0.7461792070820629, 'ionic_contributions': [{'ion_id': 1306, 'distance': 8.00169563293457, 'force': [2.4124746322631836, 4.2648186683654785, 1.696656584739685], 'magnitude': 5.185301780700684}, {'ion_id': 1307, 'distance': 11.148056983947754, 'force': [0.740688681602478, 2.5558183193206787, -0.2357446402311325], 'magnitude': 2.6714046001434326}, {'ion_id': 1308, 'distance': 11.235227584838867, 'force': [-0.7104681134223938, 1.5558724403381348, -1.9979960918426514], 'magnitude': 2.630112648010254}, {'ion_id': 1320, 'distance': 14.331863403320312, 'force': [-0.3768095374107361, 0.7196657061576843, -1.397373080253601], 'magnitude': 1.6163402795791626}, {'ion_id': 1460, 'distance': 6.684293746948242, 'force': [-2.6120445728302, 6.943007946014404, 0.43184152245521545], 'magnitude': 7.430654048919678}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.412463903427124, 'force': [20.048564910888672, -9.693181037902832, -5.600008487701416], 'magnitude': 22.962203979492188}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 2.6289806365966797, 'force': [-34.114402770996094, 19.421701431274414, -2.4446840286254883], 'magnitude': 39.33155822753906}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 4.196050643920898, 'force': [-14.700145721435547, 2.841979742050171, 3.769402503967285], 'magnitude': 15.439544677734375}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.010080337524414, 'force': [0.6761043667793274, 5.067225933074951, 13.804279327392578], 'magnitude': 14.720462799072266}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.168339490890503, 'force': [-4.438760280609131, -3.2980196475982666, -18.820043563842773], 'magnitude': 19.615646362304688}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.986429214477539, 'force': [3.7379581928253174, -10.324305534362793, -15.752140045166016], 'magnitude': 19.20139503479004}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.2126219272613525, 'force': [-4.629650592803955, 7.972245216369629, 9.858650207519531], 'magnitude': 13.497530937194824}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.911325931549072, 'force': [-1.63639235496521, 2.9960079193115234, 4.658377647399902], 'magnitude': 5.775320053100586}]}, 4864: {'frame': 4864, 'ionic_force': [-0.0066828131675720215, 12.786956429481506, -2.553470253944397], 'ionic_force_magnitude': 13.039421372408713, 'motion_vector': [-1.0789031982421875, -0.15365219116210938, 2.0991592407226562], 'ionic_force_x': -0.0066828131675720215, 'ionic_force_y': 12.786956429481506, 'ionic_force_z': -2.553470253944397, 'radial_force': 12.786958175791858, 'axial_force': -2.553470253944397, 'glu_force': [-13.438095569610596, 5.978214502334595, 8.480800151824951], 'glu_force_magnitude': 16.977792329661288, 'asn_force': [6.788048714399338, -6.09087598323822, -10.219190120697021], 'asn_force_magnitude': 13.697015087791874, 'residue_force': [-6.650046855211258, -0.11266148090362549, -1.7383899688720703], 'residue_force_magnitude': 6.87443201069438, 'total_force': [-6.65672966837883, 12.67429494857788, -4.291860222816467], 'total_force_magnitude': 14.945563438479525, 'motion_component_total': -1.595968659938916, 'cosine_total_motion': -0.10678544616323148, 'cosine_glu_motion': 0.7815184969893078, 'cosine_asn_motion': -0.8593491410928418, 'cosine_residue_motion': 0.2179002701770179, 'cosine_ionic_motion': -0.23727350808138184, 'motion_component_glu': 13.268458743673488, 'motion_component_asn': -11.770518151229641, 'motion_component_residue': 1.4979405924438458, 'motion_component_ionic': -3.093909252382762, 'ionic_contributions': [{'ion_id': 1306, 'distance': 7.938421249389648, 'force': [2.984558343887329, 4.312427520751953, 0.5002753138542175], 'magnitude': 5.268291473388672}, {'ion_id': 1307, 'distance': 11.211475372314453, 'force': [0.9359217882156372, 2.3722565174102783, -0.6875678896903992], 'magnitude': 2.641268730163574}, {'ion_id': 1308, 'distance': 12.457712173461914, 'force': [-0.32004624605178833, 1.0951236486434937, -1.809603214263916], 'magnitude': 2.139249563217163}, {'ion_id': 1460, 'distance': 7.319933891296387, 'force': [-3.60711669921875, 5.007148742675781, -0.5565744638442993], 'magnitude': 6.196176528930664}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 4.956602573394775, 'force': [7.967339992523193, -4.023813724517822, -6.228005886077881], 'magnitude': 10.883824348449707}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 3.730639934539795, 'force': [-14.370619773864746, 8.182292938232422, 10.394174575805664], 'magnitude': 19.532114028930664}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 5.671643257141113, 'force': [-7.034815788269043, 1.8197352886199951, 4.314631462097168], 'magnitude': 8.4508056640625}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.068402290344238, 'force': [3.4139113426208496, 7.137356758117676, 11.913630485534668], 'magnitude': 14.30144214630127}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.0277693271636963, 'force': [-1.581360101699829, -10.28913688659668, -18.788131713867188], 'magnitude': 21.47931480407715}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.136965274810791, 'force': [-1.2526359558105469, -6.987586975097656, -9.12786865234375], 'magnitude': 11.563453674316406}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.248579502105713, 'force': [-0.36216965317726135, 3.3420257568359375, 3.777909755706787], 'magnitude': 5.0569658279418945}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.948750019073486, 'force': [0.8462134599685669, 2.300140857696533, 3.0806093215942383], 'magnitude': 3.936607599258423}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.710508823394775, 'force': [5.724089622497559, -1.5936754941940308, -1.0753393173217773], 'magnitude': 6.038323879241943}]}, 4865: {'frame': 4865, 'ionic_force': [-0.5236209034919739, 12.514497458934784, -1.6652111858129501], 'ionic_force_magnitude': 12.635654070669057, 'motion_vector': [3.705402374267578, -1.9471969604492188, -2.8583602905273438], 'ionic_force_x': -0.5236209034919739, 'ionic_force_y': 12.514497458934784, 'ionic_force_z': -1.6652111858129501, 'radial_force': 12.525447117778228, 'axial_force': -1.6652111858129501, 'glu_force': [-26.459341049194336, 15.009342908859253, -8.259520530700684], 'glu_force_magnitude': 31.521370254326985, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [-26.459341049194336, 15.009342908859253, -8.259520530700684], 'residue_force_magnitude': 31.521370254326985, 'total_force': [-26.98296195268631, 27.523840367794037, -9.924731716513634], 'total_force_magnitude': 39.80128545633542, 'motion_component_total': -24.702270575205873, 'cosine_total_motion': -0.6206400193357036, 'cosine_glu_motion': -0.6487967344702084, 'cosine_asn_motion': None, 'cosine_residue_motion': -0.6487967344702084, 'cosine_ionic_motion': -0.33645337743462417, 'motion_component_glu': -20.45096208703371, 'motion_component_asn': None, 'motion_component_residue': -20.45096208703371, 'motion_component_ionic': -4.251308488172161, 'ionic_contributions': [{'ion_id': 1306, 'distance': 7.624697208404541, 'force': [2.304857015609741, 4.980421543121338, 1.5797655582427979], 'magnitude': 5.7107462882995605}, {'ion_id': 1307, 'distance': 12.682141304016113, 'force': [0.3401249349117279, 2.030419111251831, -0.1505231112241745], 'magnitude': 2.0642054080963135}, {'ion_id': 1308, 'distance': 10.608867645263672, 'force': [-0.8212441205978394, 1.7357362508773804, -2.2392847537994385], 'magnitude': 2.949850559234619}, {'ion_id': 1320, 'distance': 13.407963752746582, 'force': [-0.41535165905952454, 0.8550887703895569, -1.5833065509796143], 'magnitude': 1.8467683792114258}, {'ion_id': 1460, 'distance': 9.643028259277344, 'force': [-1.932007074356079, 2.9128317832946777, 0.7281376719474792], 'magnitude': 3.5703535079956055}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.2503302097320557, 'force': [22.10988426208496, -11.621963500976562, -4.084951400756836], 'magnitude': 25.31015396118164}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 2.6411478519439697, 'force': [-30.125837326049805, 23.55825424194336, -7.490272045135498], 'magnitude': 38.970008850097656}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 3.7835781574249268, 'force': [-18.443387985229492, 3.073052167892456, 3.3157029151916504], 'magnitude': 18.989368438720703}], 'asn_contributions': []}, 4866: {'frame': 4866, 'ionic_force': [-1.7787259072065353, 16.205128252506256, -4.119738966226578], 'ionic_force_magnitude': 16.814942660710734, 'motion_vector': [-0.006435394287109375, 0.24068450927734375, 0.5570297241210938], 'ionic_force_x': -1.7787259072065353, 'ionic_force_y': 16.205128252506256, 'ionic_force_z': -4.119738966226578, 'radial_force': 16.302455260884607, 'axial_force': -4.119738966226578, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-1.5362493991851807, -0.5545862279832363, -10.290606021881104], 'asn_force_magnitude': 10.41941459000174, 'residue_force': [-1.5362493991851807, -0.5545862279832363, -10.290606021881104], 'residue_force_magnitude': 10.41941459000174, 'total_force': [-3.314975306391716, 15.65054202452302, -14.410344988107681], 'total_force_magnitude': 21.531060578142178, 'motion_component_total': -6.98508197401825, 'cosine_total_motion': -0.32441885287849404, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.9261207270813271, 'cosine_residue_motion': -0.9261207270813271, 'cosine_ionic_motion': 0.1584634509674458, 'motion_component_glu': None, 'motion_component_asn': -9.649635815854198, 'motion_component_residue': -9.649635815854198, 'motion_component_ionic': 2.6645538418359482, 'ionic_contributions': [{'ion_id': 1306, 'distance': 8.056601524353027, 'force': [4.388768196105957, 2.6268601417541504, -0.013402372598648071], 'magnitude': 5.114866733551025}, {'ion_id': 1307, 'distance': 10.70998477935791, 'force': [1.5909762382507324, 2.1847963333129883, -1.0358966588974], 'magnitude': 2.8944122791290283}, {'ion_id': 1308, 'distance': 12.196389198303223, 'force': [0.049068644642829895, 0.7890864014625549, -2.0871825218200684], 'magnitude': 2.2319042682647705}, {'ion_id': 1460, 'distance': 5.0141401290893555, 'force': [-7.807538986206055, 10.604385375976562, -0.9832574129104614], 'magnitude': 13.205204963684082}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.074389934539795, 'force': [6.744213104248047, 0.7544726133346558, 6.201504707336426], 'magnitude': 9.1930570602417}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.062393665313721, 'force': [-7.771589279174805, -0.08954380452632904, -9.053156852722168], 'magnitude': 11.93169116973877}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.783505439758301, 'force': [-5.697414875030518, -2.1214683055877686, -6.801517486572266], 'magnitude': 9.122598648071289}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.562329292297363, 'force': [2.1707088947296143, 1.3069082498550415, 3.721978187561035], 'magnitude': 4.502566814422607}, {'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.264837741851807, 'force': [-12.754512786865234, -1.3772611618041992, 2.190645217895508], 'magnitude': 13.014352798461914}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.7559070587158203, 'force': [12.72143840789795, 0.10482407361268997, -5.743832111358643], 'magnitude': 13.958423614501953}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.600454330444336, 'force': [14.3584623336792, -0.9895721077919006, 0.853628933429718], 'magnitude': 14.417814254760742}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.507758140563965, 'force': [-6.535667419433594, 1.8898481130599976, -0.8451385498046875], 'magnitude': 6.855708122253418}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.364349365234375, 'force': [-4.77188777923584, -0.03279389813542366, -0.8147180676460266], 'magnitude': 4.841048717498779}]}, 4867: {'frame': 4867, 'ionic_force': [5.378923777490854, 8.464651763439178, -4.732402980327606], 'ionic_force_magnitude': 11.089580174585695, 'motion_vector': [-0.9177093505859375, 0.6418495178222656, 2.0229339599609375], 'ionic_force_x': 5.378923777490854,</t>
+          <t>{4857: {'frame': 4857, 'motion_vector': [0.9804725646972656, -0.3909263610839844, 0.2857513427734375], 'ionic_force': [-24.356317825615406, 5.643100440502167, 5.592016190290451], 'ionic_force_magnitude': 25.619239756020416, 'radial_force': 25.001495967321368, 'axial_force': 5.592016190290451, 'glu_force': [-10.987810134887695, 14.360766410827637, -2.7645459175109863], 'glu_force_magnitude': 18.292246925862408, 'asn_force': [1.3874993324279785, -0.3169316053390503, -0.6931047439575195], 'asn_force_magnitude': 1.5830332359263, 'residue_force': [-9.600310802459717, 14.043834805488586, -3.457650661468506], 'residue_force_magnitude': 17.359453091743156, 'total_force': [-33.95662862807512, 19.686935245990753, 2.134365528821945], 'total_force_magnitude': 39.30882297112784, 'cosine_total_motion': -0.9393858282242439, 'cosine_glu_motion': -0.8587285038781322, 'cosine_asn_motion': 0.7430262111290231, 'cosine_residue_motion': -0.8371138520916579, 'cosine_ionic_motion': -0.8741208868290865, 'motion_component_total': -36.92615122325311, 'motion_component_glu': -15.708073835215188, 'motion_component_asn': 1.1762351873816357, 'motion_component_residue': -14.531838647833553, 'motion_component_ionic': -22.394312575419555, 'motion_component_percent_total': 93.9385828224244, 'motion_component_percent_glu': 85.87285038781322, 'motion_component_percent_asn': 74.30262111290232, 'motion_component_percent_residue': 83.71138520916578, 'motion_component_percent_ionic': 87.41208868290865, 'ionic_contributions': [{'ion_id': 1306, 'distance': 8.758042335510254, 'force': [-0.837573766708374, 2.762312173843384, 3.2253456115722656], 'magnitude': 4.328366279602051, 'cosine_ionic_motion': -0.20692846179008484, 'motion_component_ionic': -0.8956621885299683, 'motion_component_percent_ionic': 20.692846179008484}, {'ion_id': 1307, 'distance': 11.013960838317871, 'force': [0.08748745173215866, 2.7204031944274902, -0.2865326702594757], 'magnitude': 2.7368502616882324, 'cosine_ionic_motion': -0.354038804769516, 'motion_component_ionic': -0.9689511656761169, 'motion_component_percent_ionic': 35.4038804769516}, {'ion_id': 1308, 'distance': 10.233463287353516, 'force': [-1.2521235942840576, 1.593077540397644, -2.4381844997406006], 'magnitude': 3.1702449321746826, 'cosine_ionic_motion': -0.7347405552864075, 'motion_component_ionic': -2.3293075561523438, 'motion_component_percent_ionic': 73.47405552864075}, {'ion_id': 1320, 'distance': 13.275734901428223, 'force': [-0.6172628998756409, 0.6778424382209778, -1.6455979347229004], 'magnitude': 1.8837400674819946, 'cosine_ionic_motion': -0.6507173776626587, 'motion_component_ionic': -1.2257823944091797, 'motion_component_percent_ionic': 65.07173776626587}, {'ion_id': 1460, 'distance': 3.8113815784454346, 'force': [-21.736845016479492, -2.110534906387329, 6.736985683441162], 'magnitude': 22.854578018188477, 'cosine_ionic_motion': -0.7427225112915039, 'motion_component_ionic': -16.974609375, 'motion_component_percent_ionic': 74.27225112915039}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.83697247505188, 'force': [9.213166236877441, -15.410645484924316, -2.738801956176758], 'magnitude': 18.162363052368164, 'cosine_with_motion': 0.7187466621398926, 'motion_component': 13.05413818359375, 'motion_component_percent': 71.87466621398926}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 3.656285047531128, 'force': [-7.278402328491211, 18.777568817138672, -2.814974069595337], 'magnitude': 20.33460807800293, 'cosine_with_motion': -0.6872181296348572, 'motion_component': -13.974311828613281, 'motion_component_percent': 68.72181296348572}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 3.9761993885040283, 'force': [-12.922574043273926, 10.993843078613281, 2.7892301082611084], 'magnitude': 17.194107055664062, 'cosine_with_motion': -0.8600563406944275, 'motion_component': -14.787900924682617, 'motion_component_percent': 86.00563406944275}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.785486698150635, 'force': [-1.0566141605377197, 1.7043412923812866, 6.781833171844482], 'magnitude': 7.072091102600098, 'cosine_with_motion': 0.03047313168644905, 'motion_component': 0.21550875902175903, 'motion_component_percent': 3.047313168644905}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.924427509307861, 'force': [2.4441134929656982, -2.021272897720337, -7.474937915802002], 'magnitude': 8.11997127532959, 'cosine_with_motion': 0.11831647157669067, 'motion_component': 0.9607263207435608, 'motion_component_percent': 11.831647157669067}]}, 4858: {'frame': 4858, 'motion_vector': [-0.14766693115234375, 1.5113677978515625, -0.5906982421875], 'ionic_force': [-9.28166988492012, 11.450447499752045, 3.758600100874901], 'ionic_force_magnitude': 15.211483113605581, 'radial_force': 14.73981491733227, 'axial_force': 3.758600100874901, 'glu_force': [-13.212425708770752, 22.319079399108887, -0.6105731129646301], 'glu_force_magnitude': 25.943829668339028, 'asn_force': [1.2593601942062378, -0.28960487246513367, -5.6734819412231445], 'asn_force_magnitude': 5.818784788793263, 'residue_force': [-11.953065514564514, 22.029474526643753, -6.284055054187775], 'residue_force_magnitude': 25.839173188002366, 'total_force': [-21.234735399484634, 33.4799220263958, -2.525454953312874], 'total_force_magnitude': 39.72652878242549, 'cosine_total_motion': 0.8531962068897461, 'cosine_glu_motion': 0.8526488047331512, 'cosine_asn_motion': 0.2876916306146544, 'cosine_residue_motion': 0.9208882524167568, 'cosine_ionic_motion': 0.6639413496791131, 'motion_component_total': 33.89452367006175, 'motion_component_glu': 22.12097535690974, 'motion_component_asn': 1.674015684083681, 'motion_component_residue': 23.794991040993416, 'motion_component_ionic': 10.099532629068328, 'motion_component_percent_total': 85.31962068897461, 'motion_component_percent_glu': 85.26488047331512, 'motion_component_percent_asn': 28.76916306146544, 'motion_component_percent_residue': 92.08882524167568, 'motion_component_percent_ionic': 66.39413496791131, 'ionic_contributions': [{'ion_id': 1306, 'distance': 8.15285587310791, 'force': [-2.1441845893859863, 4.504876136779785, 0.23799630999565125], 'magnitude': 4.994805335998535, 'cosine_ionic_motion': 0.8582062721252441, 'motion_component_ionic': 4.28657341003418, 'motion_component_percent_ionic': 85.82062721252441}, {'ion_id': 1307, 'distance': 9.122523307800293, 'force': [1.3651424646377563, 3.7462639808654785, -0.13131223618984222], 'magnitude': 3.9894046783447266, 'cosine_ionic_motion': 0.8519472479820251, 'motion_component_ionic': 3.3987622261047363, 'motion_component_percent_ionic': 85.19472479820251}, {'ion_id': 1308, 'distance': 9.799673080444336, 'force': [-1.0608267784118652, 1.5705699920654297, -2.8913075923919678], 'magnitude': 3.4571235179901123, 'cosine_ionic_motion': 0.7523887753486633, 'motion_component_ionic': 2.6011009216308594, 'motion_component_percent_ionic': 75.23887753486633}, {'ion_id': 1320, 'distance': 13.182660102844238, 'force': [-0.4662999212741852, 0.6704815030097961, -1.7270715236663818], 'magnitude': 1.9104337692260742, 'cosine_ionic_motion': 0.6753826141357422, 'motion_component_ionic': 1.2902737855911255, 'motion_component_percent_ionic': 67.53826141357422}, {'ion_id': 1460, 'distance': 5.5286970138549805, 'force': [-6.97550106048584, 0.9582558870315552, 8.270295143127441], 'magnitude': 10.861567497253418, 'cosine_ionic_motion': -0.1360003799200058, 'motion_component_ionic': -1.4771772623062134, 'motion_component_percent_ionic': 13.60003799200058}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.764124870300293, 'force': [9.685281753540039, -15.975787162780762, -2.669835090637207], 'magnitude': 18.872161865234375, 'cosine_with_motion': -0.7804260849952698, 'motion_component': -14.728327751159668, 'motion_component_percent': 78.04260849952698}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 3.528026819229126, 'force': [-4.353703022003174, 21.1895809173584, 3.005239725112915], 'magnitude': 21.839975357055664, 'cosine_with_motion': 0.8681167364120483, 'motion_component': 18.95964813232422, 'motion_component_percent': 86.81167364120483}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 3.281412124633789, 'force': [-18.544004440307617, 17.10528564453125, -0.9459777474403381], 'magnitude': 25.246105194091797, 'cosine_with_motion': 0.708610475063324, 'motion_component': 17.8896541595459, 'motion_component_percent': 70.8610475063324}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.8172383308410645, 'force': [1.2593601942062378, -0.28960487246513367, -5.6734819412231445], 'magnitude': 5.818784713745117, 'cosine_with_motion': 0.2876916229724884, 'motion_component': 1.6740156412124634, 'motion_component_percent': 28.76916229724884}]}, 4859: {'frame': 4859, 'motion_vector': [-0.5728759765625, -0.2980232238769531, -0.14586639404296875], 'ionic_force': [-11.826732784509659, 21.502933859825134, 4.421850718557835], 'ionic_force_magnitude': 24.93592863146308, 'radial_force': 24.540737008822898, 'axial_force': 4.421850718557835, 'glu_force': [-25.724108695983887, 18.06024932861328, -1.9480111598968506], 'glu_force_magnitude': 31.49122292788187, 'asn_force': [0.7898761257529259, -1.310462236404419, -0.060089111328125], 'asn_force_magnitude': 1.5312825566748702, 'residue_force': [-24.93423257023096, 16.749787092208862, -2.0081002712249756], 'residue_force_magnitude': 30.104879807100822, 'total_force': [-36.76096535474062, 38.252720952034, 2.413750447332859], 'total_force_magnitude': 53.108054241034104, 'cosine_total_motion': 0.26471680043824297, 'cosine_glu_motion': 0.46232058577826657, 'cosine_asn_motion': -0.05246634818604452, 'cosine_residue_motion': 0.48094195757883484, 'cosine_ionic_motion': -0.016847402682462258, 'motion_component_total': 14.058594196187208, 'motion_component_glu': 14.559040630892326, 'motion_component_asn': -0.0803408037897202, 'motion_component_residue': 14.478699827102606, 'motion_component_ionic': -0.42010563091539854, 'motion_component_percent_total': 26.471680043824296, 'motion_component_percent_glu': 46.232058577826656, 'motion_component_percent_asn': 5.246634818604452, 'motion_component_percent_residue': 48.09419575788348, 'motion_component_percent_ionic': 1.6847402682462258, 'ionic_contributions': [{'ion_id': 1306, 'distance': 7.285847187042236, 'force': [-3.3123834133148193, 5.30451774597168, 0.07961202412843704], 'magnitude': 6.254289150238037, 'cosine_ionic_motion': 0.0736871212720871, 'motion_component_ionic': 0.46086055040359497, 'motion_component_percent_ionic': 7.36871212720871}, {'ion_id': 1307, 'distance': 10.17105484008789, 'force': [1.019066572189331, 3.0403809547424316, -0.13036009669303894], 'magnitude': 3.209268808364868, 'cosine_ionic_motion': -0.6923038363456726, 'motion_component_ionic': -2.2217891216278076, 'motion_component_percent_ionic': 69.23038363456726}, {'ion_id': 1308, 'distance': 10.916866302490234, 'force': [-0.8318650126457214, 1.5506973266601562, -2.159569263458252], 'magnitude': 2.785749673843384, 'cosine_ionic_motion': 0.1786206066608429, 'motion_component_ionic': 0.4975923001766205, 'motion_component_percent_ionic': 17.86206066608429}, {'ion_id': 1320, 'distance': 14.021308898925781, 'force': [-0.4241594970226288, 0.7252730131149292, -1.4648845195770264], 'magnitude': 1.6887328624725342, 'cosine_ionic_motion': 0.21513624489307404, 'motion_component_ionic': 0.3633076548576355, 'motion_component_percent_ionic': 21.513624489307404}, {'ion_id': 1460, 'distance': 4.570935249328613, 'force': [-8.27739143371582, 10.882064819335938, 8.097052574157715], 'magnitude': 15.890148162841797, 'cosine_ionic_motion': 0.030202558264136314, 'motion_component_ionic': 0.4799231290817261, 'motion_component_percent_ionic': 3.0202558264136314}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.507916212081909, 'force': [17.08523178100586, -11.745720863342285, -6.504417419433594], 'magnitude': 21.729578018188477, 'cosine_with_motion': -0.3710964620113373, 'motion_component': -8.063769340515137, 'motion_component_percent': 37.10964620113373}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 2.6400349140167236, 'force': [-30.043292999267578, 24.848541259765625, 1.0838556289672852], 'magnitude': 39.002872467041016, 'cosine_with_motion': 0.37363138794898987, 'motion_component': 14.572697639465332, 'motion_component_percent': 37.36313879489899}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 4.386460304260254, 'force': [-12.766047477722168, 4.957428932189941, 3.472550630569458], 'magnitude': 14.128222465515137, 'cosine_with_motion': 0.5697895884513855, 'motion_component': 8.050113677978516, 'motion_component_percent': 56.97895884513855}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.7132649421691895, 'force': [0.1196339949965477, 2.5797061920166016, 6.776618957519531], 'magnitude': 7.252017974853516, 'cosine_with_motion': -0.3802984356880188, 'motion_component': -2.7579309940338135, 'motion_component_percent': 38.02984356880188}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.994253158569336, 'force': [0.6702421307563782, -3.8901684284210205, -6.836708068847656], 'magnitude': 7.894505023956299, 'cosine_with_motion': 0.3391713500022888, 'motion_component': 2.6775898933410645, 'motion_component_percent': 33.91713500022888}]}, 4860: {'frame': 4860, 'motion_vector': [0.6911888122558594, -0.11594009399414062, 0.5926361083984375], 'ionic_force': [-4.794602394104004, 12.35471922159195, -2.0622036159038544], 'ionic_force_magnitude': 13.411934346520205, 'radial_force': 13.25244502580265, 'axial_force': -2.0622036159038544, 'glu_force': [-19.473167419433594, 22.178525924682617, 0.19907911121845245], 'glu_force_magnitude': 29.51492663093765, 'asn_force': [-0.04808613657951355, -0.5574445724487305, 1.5964374542236328], 'asn_force_magnitude': 1.691646911483518, 'residue_force': [-19.521253556013107, 21.621081352233887, 1.7955165654420853], 'residue_force_magnitude': 29.185173958276266, 'total_force': [-24.31585595011711, 33.975800573825836, -0.2666870504617691], 'total_force_magnitude': 41.78141928180653, 'cosine_total_motion': -0.5451144396415687, 'cosine_glu_motion': -0.587423963429649, 'cosine_asn_motion': 0.6295749638971516, 'cosine_residue_motion': -0.5575692871291635, 'cosine_ionic_motion': -0.4848590928468034, 'motion_component_total': -22.7756549592314, 'motion_component_glu': -17.33777518188069, 'motion_component_asn': 1.0650185432239638, 'motion_component_residue': -16.272756638656727, 'motion_component_ionic': -6.502898320574672, 'motion_component_percent_total': 54.51144396415687, 'motion_component_percent_glu': 58.742396342964895, 'motion_component_percent_asn': 62.95749638971516, 'motion_component_percent_residue': 55.756928712916356, 'motion_component_percent_ionic': 48.48590928468034, 'ionic_contributions': [{'ion_id': 1306, 'distance': 9.515270233154297, 'force': [-2.5619351863861084, 2.5342040061950684, 0.6784204840660095], 'magnitude': 3.66687273979187, 'cosine_ionic_motion': -0.49398836493492126, 'motion_component_ionic': -1.8113924264907837, 'motion_component_percent_ionic': 49.39883649349213}, {'ion_id': 1307, 'distance': 10.100597381591797, 'force': [0.7434799671173096, 3.142179489135742, -0.4046603739261627], 'magnitude': 3.2541980743408203, 'cosine_ionic_motion': -0.03021174483001232, 'motion_component_ionic': -0.09831500053405762, 'motion_component_percent_ionic': 3.021174483001232}, {'ion_id': 1308, 'distance': 10.912854194641113, 'force': [-0.9280287027359009, 1.4536443948745728, -2.190319776535034], 'magnitude': 2.7877984046936035, 'cosine_ionic_motion': -0.823868989944458, 'motion_component_ionic': -2.296780586242676, 'motion_component_percent_ionic': 82.3868989944458}, {'ion_id': 1320, 'distance': 14.029218673706055, 'force': [-0.4511340856552124, 0.7071818709373474, -1.4634768962860107], 'magnitude': 1.6868292093276978, 'cosine_ionic_motion': -0.814564049243927, 'motion_component_ionic': -1.3740304708480835, 'motion_component_percent_ionic': 81.4564049243927}, {'ion_id': 1460, 'distance': 8.173669815063477, 'force': [-1.5969843864440918, 4.517509460449219, 1.3178329467773438], 'magnitude': 4.969399929046631, 'cosine_ionic_motion': -0.18561193346977234, 'motion_component_ionic': -0.9223799109458923, 'motion_component_percent_ionic': 18.561193346977234}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.5046865940093994, 'force': [13.607168197631836, -15.845686912536621, -6.138125419616699], 'magnitude': 21.769643783569336, 'cosine_with_motion': 0.38059693574905396, 'motion_component': 8.285459518432617, 'motion_component_percent': 38.059693574905396}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 2.8582470417022705, 'force': [-16.38758087158203, 28.959178924560547, 0.17417438328266144], 'magnitude': 33.274871826171875, 'cosine_with_motion': -0.47743895649909973, 'motion_component': -15.886719703674316, 'motion_component_percent': 47.74389564990997}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 3.689500570297241, 'force': [-16.6927547454834, 9.065033912658691, 6.16303014755249], 'magnitude': 19.970123291015625, 'cosine_with_motion': -0.48755407333374023, 'motion_component': -9.736515045166016, 'motion_component_percent': 48.75540733337402}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.874335765838623, 'force': [-0.44713327288627625, 2.8439011573791504, 6.226464748382568], 'magnitude': 6.859778881072998, 'cosine_with_motion': 0.4846278727054596, 'motion_component': 3.3244400024414062, 'motion_component_percent': 48.46278727054596}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.847378730773926, 'force': [0.3990471363067627, -3.401345729827881, -4.6300272941589355], 'magnitude': 5.758953094482422, 'cosine_with_motion': -0.39233195781707764, 'motion_component': -2.2594213485717773, 'motion_component_percent': 39.233195781707764}]}, 4861: {'frame': 4861, 'motion_vector': [0.4648017883300781, 0.24734878540039062, -0.2841033935546875], 'ionic_force': [-6.5610339641571045, 14.756245732307434, 0.32843945175409317], 'ionic_force_magnitude': 16.152455765750698, 'radial_force': 16.14911622321991, 'axial_force': 0.32843945175409317, 'glu_force': [-24.28467082977295, 14.03956127166748, -4.462919235229492], 'glu_force_magnitude': 28.40373507325246, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [-24.28467082977295, 14.03956127166748, -4.462919235229492], 'residue_force_magnitude': 28.40373507325246, 'total_force': [-30.845704793930054, 28.795807003974915, -4.134479783475399], 'total_force_magnitude': 42.39988123007442, 'cosine_total_motion': -0.2381017994355526, 'cosine_glu_motion': -0.3852662650484079, 'cosine_asn_motion': None, 'cosine_residue_motion': -0.3852662650484079, 'cosine_ionic_motion': 0.05246960094817645, 'motion_component_total': -10.09548801673443, 'motion_component_glu': -10.943000925096442, 'motion_component_asn': None, 'motion_component_residue': -10.943000925096442, 'motion_component_ionic': 0.847512908362011, 'motion_component_percent_total': 23.81017994355526, 'motion_component_percent_glu': 38.52662650484079, 'motion_component_percent_asn': None, 'motion_component_percent_residue': 38.52662650484079, 'motion_component_percent_ionic': 5.246960094817645, 'ionic_contributions': [{'ion_id': 1306, 'distance': 7.293181419372559, 'force': [-4.193318843841553, 3.516507863998413, 3.0015461444854736], 'magnitude': 6.2417168617248535, 'cosine_ionic_motion': -0.5173704028129578, 'motion_component_ionic': -3.2292795181274414, 'motion_component_percent_ionic': 51.737040281295776}, {'ion_id': 1307, 'distance': 11.440825462341309, 'force': [0.5813269019126892, 2.4661834239959717, -0.11614765971899033], 'magnitude': 2.536432981491089, 'cosine_ionic_motion': 0.6017869114875793, 'motion_component_ionic': 1.5263922214508057, 'motion_component_percent_ionic': 60.178691148757935}, {'ion_id': 1308, 'distance': 10.164334297180176, 'force': [-0.8082016706466675, 1.8407821655273438, -2.506990909576416], 'magnitude': 3.2135140895843506, 'cosine_ionic_motion': 0.4118986427783966, 'motion_component_ionic': 1.3236421346664429, 'motion_component_percent_ionic': 41.18986427783966}, {'ion_id': 1320, 'distance': 13.986430168151855, 'force': [-0.4184555411338806, 0.7065335512161255, -1.485287070274353], 'magnitude': 1.6971659660339355, 'cosine_ionic_motion': 0.39614471793174744, 'motion_component_ionic': 0.6723233461380005, 'motion_component_percent_ionic': 39.614471793174744}, {'ion_id': 1460, 'distance': 7.0830183029174805, 'force': [-1.7223848104476929, 6.22623872756958, 1.435318946838379], 'magnitude': 6.617612838745117, 'cosine_ionic_motion': 0.0837816521525383, 'motion_component_ionic': 0.5544345378875732, 'motion_component_percent_ionic': 8.37816521525383}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.7518699169158936, 'force': [15.4595308303833, -10.6598539352417, -2.864459991455078], 'magnitude': 18.995649337768555, 'cosine_with_motion': 0.4718756675720215, 'motion_component': 8.963584899902344, 'motion_component_percent': 47.18756675720215}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 2.808248519897461, 'force': [-27.88861846923828, 19.966638565063477, -3.4291157722473145], 'magnitude': 34.47028350830078, 'cosine_with_motion': -0.34184131026268005, 'motion_component': -11.783367156982422, 'motion_component_percent': 34.184131026268005}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 4.591255187988281, 'force': [-11.855583190917969, 4.732776641845703, 1.8306565284729004], 'magnitude': 12.895942687988281, 'cosine_with_motion': -0.6299050450325012, 'motion_component': -8.12321949005127, 'motion_component_percent': 62.99050450325012}], 'asn_contributions': []}, 4862: {'frame': 4862, 'motion_vector': [-0.7869873046875, 0.3434638977050781, -0.23621368408203125], 'ionic_force': [-3.6536727249622345, 22.094812095165253, -0.211676687002182], 'ionic_force_magnitude': 22.395866871403168, 'radial_force': 22.394866507791328, 'axial_force': -0.211676687002182, 'glu_force': [-24.35048484802246, 16.70631217956543, -6.922949433326721], 'glu_force_magnitude': 30.33107660191551, 'asn_force': [0.6463719010353088, -1.5418689846992493, -3.0950231552124023], 'asn_force_magnitude': 3.5177158685326515, 'residue_force': [-23.704112946987152, 15.16444319486618, -10.017972588539124], 'residue_force_magnitude': 29.869802188808823, 'total_force': [-27.357785671949387, 37.25925529003143, -10.229649275541306], 'total_force_magnitude': 47.34285865830915, 'cosine_total_motion': 0.8714896648981671, 'cosine_glu_motion': 0.9824119865927807, 'cosine_asn_motion': -0.09805255670832731, 'cosine_residue_motion': 0.9860357293004586, 'cosine_ionic_motion': 0.5271561895745854, 'motion_component_total': 41.25881202745113, 'motion_component_glu': 29.797613219985625, 'motion_component_asn': -0.34492103468308066, 'motion_component_residue': 29.452692185302542, 'motion_component_ionic': 11.806119842148586, 'motion_component_percent_total': 87.14896648981671, 'motion_component_percent_glu': 98.24119865927807, 'motion_component_percent_asn': 9.80525567083273, 'motion_component_percent_residue': 98.60357293004586, 'motion_component_percent_ionic': 52.715618957458545, 'ionic_contributions': [{'ion_id': 1306, 'distance': 9.68929386138916, 'force': [-1.5576599836349487, 2.6959004402160645, 1.676754355430603], 'magnitude': 3.5363383293151855, 'cosine_ionic_motion': 0.557489275932312, 'motion_component_ionic': 1.971470594406128, 'motion_component_percent_ionic': 55.7489275932312}, {'ion_id': 1307, 'distance': 10.900853157043457, 'force': [0.7250994443893433, 2.6796772480010986, -0.3156937062740326], 'magnitude': 2.793940305709839, 'cosine_ionic_motion': 0.17052489519119263, 'motion_component_ionic': 0.4764363765716553, 'motion_component_percent_ionic': 17.052489519119263}, {'ion_id': 1308, 'distance': 10.722567558288574, 'force': [-0.5865727663040161, 1.652468204498291, -2.294264078140259], 'magnitude': 2.8876230716705322, 'cosine_ionic_motion': 0.6109457612037659, 'motion_component_ionic': 1.7641810178756714, 'motion_component_percent_ionic': 61.09457612037659}, {'ion_id': 1320, 'distance': 14.130182266235352, 'force': [-0.32260993123054504, 0.7156185507774353, -1.465861201286316], 'magnitude': 1.6628097295761108, 'cosine_ionic_motion': 0.5712511539459229, 'motion_component_ionic': 0.9498819708824158, 'motion_component_percent_ionic': 57.125115394592285}, {'ion_id': 1460, 'distance': 4.761733531951904, 'force': [-1.9119294881820679, 14.351147651672363, 2.1873879432678223], 'magnitude': 14.642252922058105, 'cosine_ionic_motion': 0.45376554131507874, 'motion_component_ionic': 6.6441497802734375, 'motion_component_percent_ionic': 45.37655413150787}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.4525365829467773, 'force': [18.71674919128418, -12.027681350708008, -2.8678622245788574], 'magnitude': 22.43226432800293, 'cosine_with_motion': -0.9101992845535278, 'motion_component': -20.417831420898438, 'motion_component_percent': 91.01992845535278}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 2.7261617183685303, 'force': [-26.637910842895508, 24.350927352905273, -5.946378231048584], 'magnitude': 36.577388763427734, 'cosine_with_motion': 0.9434311389923096, 'motion_component': 34.50824737548828, 'motion_component_percent': 94.34311389923096}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 3.986100435256958, 'force': [-16.429323196411133, 4.383066177368164, 1.8912910223007202], 'magnitude': 17.108797073364258, 'cosine_with_motion': 0.918077290058136, 'motion_component': 15.707198143005371, 'motion_component_percent': 91.8077290058136}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.824161529541016, 'force': [1.4364039897918701, -2.5230722427368164, -8.514288902282715], 'magnitude': 8.995680809020996, 'cosine_with_motion': 0.0017694580601528287, 'motion_component': 0.015917479991912842, 'motion_component_percent': 0.17694580601528287}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.003833293914795, 'force': [-0.7900320887565613, 0.9812032580375671, 5.4192657470703125], 'magnitude': 5.563753128051758, 'cosine_with_motion': -0.06485523283481598, 'motion_component': -0.36083850264549255, 'motion_component_percent': 6.485523283481598}]}, 4863: {'frame': 4863, 'motion_vector': [1.4510307312011719, -0.018299102783203125, -1.9164810180664062], 'ionic_force': [-0.5461589097976685, 16.03918308019638, -1.5026157051324844], 'ionic_force_magnitude': 16.118670459815228, 'radial_force': 16.048479162674862, 'axial_force': -1.5026157051324844, 'glu_force': [-28.76598358154297, 12.570500135421753, -4.275290012359619], 'glu_force_magnitude': 31.682446082302732, 'asn_force': [-6.290740668773651, 2.413153886795044, -6.250876426696777], 'asn_force_magnitude': 9.190766341549015, 'residue_force': [-35.05672425031662, 14.983654022216797, -10.526166439056396], 'residue_force_magnitude': 39.55103011203309, 'total_force': [-35.60288316011429, 31.022837102413177, -12.028782144188881], 'total_force_magnitude': 48.730619851054335, 'cosine_total_motion': -0.24905907732704557, 'cosine_glu_motion': -0.4434905291726908, 'cosine_asn_motion': 0.12707127026887044, 'cosine_residue_motion': -0.3257306418636394, 'cosine_ionic_motion': 0.04629285082428669, 'motion_component_total': -12.136803217678604, 'motion_component_glu': -14.050864778525682, 'motion_component_asn': 1.1678823537650125, 'motion_component_residue': -12.88298242476067, 'motion_component_ionic': 0.7461792070820629, 'motion_component_percent_total': 24.905907732704556, 'motion_component_percent_glu': 44.34905291726908, 'motion_component_percent_asn': 12.707127026887044, 'motion_component_percent_residue': 32.57306418636394, 'motion_component_percent_ionic': 4.6292850824286695, 'ionic_contributions': [{'ion_id': 1306, 'distance': 8.00169563293457, 'force': [2.4124746322631836, 4.2648186683654785, 1.696656584739685], 'magnitude': 5.185301780700684, 'cosine_ionic_motion': 0.013712235726416111, 'motion_component_ionic': 0.0711020827293396, 'motion_component_percent_ionic': 1.371223572641611}, {'ion_id': 1307, 'distance': 11.148056983947754, 'force': [0.740688681602478, 2.5558183193206787, -0.2357446402311325], 'magnitude': 2.6714046001434326, 'cosine_ionic_motion': 0.23043334484100342, 'motion_component_ionic': 0.615580677986145, 'motion_component_percent_ionic': 23.043334484100342}, {'ion_id': 1308, 'distance': 11.235227584838867, 'force': [-0.7104681134223938, 1.5558724403381348, -1.9979960918426514], 'magnitude': 2.630112648010254, 'cosine_ionic_motion': 0.43807509541511536, 'motion_component_ionic': 1.1521868705749512, 'motion_component_percent_ionic': 43.807509541511536}, {'ion_id': 1320, 'distance': 14.331863403320312, 'force': [-0.3768095374107361, 0.7196657061576843, -1.397373080253601], 'magnitude': 1.6163402795791626, 'cosine_ionic_motion': 0.5451289415359497, 'motion_component_ionic': 0.8811138868331909, 'motion_component_percent_ionic': 54.51289415359497}, {'ion_id': 1460, 'distance': 6.684293746948242, 'force': [-2.6120445728302, 6.943007946014404, 0.43184152245521545], 'magnitude': 7.430654048919678, 'cosine_ionic_motion': -0.26562997698783875, 'motion_component_ionic': -1.9738043546676636, 'motion_component_percent_ionic': 26.562997698783875}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.412463903427124, 'force': [20.048564910888672, -9.693181037902832, -5.600008487701416], 'magnitude': 22.962203979492188, 'cosine_with_motion': 0.724667489528656, 'motion_component': 16.639963150024414, 'motion_component_percent': 72.4667489528656}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 2.6289806365966797, 'force': [-34.114402770996094, 19.421701431274414, -2.4446840286254883], 'magnitude': 39.33155822753906, 'cosine_with_motion': -0.47775474190711975, 'motion_component': -18.79083824157715, 'motion_component_percent': 47.775474190711975}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 4.196050643920898, 'force': [-14.700145721435547, 2.841979742050171, 3.769402503967285], 'magnitude': 15.439544677734375, 'cosine_with_motion': -0.7707474231719971, 'motion_component': -11.899989128112793, 'motion_component_percent': 77.0747423171997}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.010080337524414, 'force': [0.6761043667793274, 5.067225933074951, 13.804279327392578], 'magnitude': 14.720462799072266, 'cosine_with_motion': -0.7225163578987122, 'motion_component': -10.635775566101074, 'motion_component_percent': 72.25163578987122}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.168339490890503, 'force': [-4.438760280609131, -3.2980196475982666, -18.820043563842773], 'magnitude': 19.615646362304688, 'cosine_with_motion': 0.6295929551124573, 'motion_component': 12.349872589111328, 'motion_component_percent': 62.95929551124573}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.986429214477539, 'force': [3.7379581928253174, -10.324305534362793, -15.752140045166016], 'magnitude': 19.20139503479004, 'cosine_with_motion': 0.7756260633468628, 'motion_component': 14.893102645874023, 'motion_component_percent': 77.56260633468628}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.2126219272613525, 'force': [-4.629650592803955, 7.972245216369629, 9.858650207519531], 'magnitude': 13.497530937194824, 'cosine_with_motion': -0.7938428521156311, 'motion_component': -10.71491813659668, 'motion_component_percent': 79.38428521156311}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.911325931549072, 'force': [-1.63639235496521, 2.9960079193115234, 4.658377647399902], 'magnitude': 5.775320053100586, 'cosine_with_motion': -0.818032443523407, 'motion_component': -4.724399089813232,</t>
         </is>
       </c>
     </row>
@@ -595,7 +595,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>{4992: {'frame': 4992, 'ionic_force': [-19.95671159029007, -2.516607314348221, 0.35591466911137104], 'ionic_force_magnitude': 20.117910555630214, 'motion_vector': [1.30914306640625, -2.567424774169922, 0.49839019775390625], 'ionic_force_x': -19.95671159029007, 'ionic_force_y': -2.516607314348221, 'ionic_force_z': 0.35591466911137104, 'radial_force': 20.114761988963455, 'axial_force': 0.35591466911137104, 'glu_force': [-11.418001174926758, -14.587153434753418, 6.207677364349365], 'glu_force_magnitude': 19.53691517152907, 'asn_force': [1.6953658312559128, -0.3065730333328247, 1.8747434616088867], 'asn_force_magnitude': 2.546156981295971, 'residue_force': [-9.722635343670845, -14.893726468086243, 8.082420825958252], 'residue_force_magnitude': 19.536587535699624, 'total_force': [-29.679346933960915, -17.410333782434464, 8.438335495069623], 'total_force_magnitude': 35.42864466458667, 'motion_component_total': 3.436511463555302, 'cosine_total_motion': 0.09699810692985182, 'cosine_glu_motion': 0.44797979935668564, 'cosine_asn_motion': 0.529214031111739, 'cosine_residue_motion': 0.5169585179627656, 'cosine_ionic_motion': -0.3312020826678284, 'motion_component_glu': 8.75214333859018, 'motion_component_asn': 1.3474619999149375, 'motion_component_residue': 10.099605338505118, 'motion_component_ionic': -6.663093874949816, 'ionic_contributions': [{'ion_id': 1306, 'distance': 13.177733421325684, 'force': [-1.3452452421188354, -1.3558294773101807, -0.08520316332578659], 'magnitude': 1.9118623733520508}, {'ion_id': 1307, 'distance': 6.083970069885254, 'force': [-8.701690673828125, 2.1244421005249023, 0.4665580689907074], 'magnitude': 8.969411849975586}, {'ion_id': 1309, 'distance': 13.56334114074707, 'force': [-0.8666126132011414, -0.2845568358898163, -1.5572242736816406], 'magnitude': 1.8046987056732178}, {'ion_id': 1316, 'distance': 7.383633136749268, 'force': [-3.8274505138397217, -1.5964282751083374, 4.4594645500183105], 'magnitude': 6.089727878570557}, {'ion_id': 1320, 'distance': 8.708598136901855, 'force': [-3.069931983947754, -1.0022555589675903, -2.9554810523986816], 'magnitude': 4.377655506134033}, {'ion_id': 1460, 'distance': 12.331439971923828, 'force': [-2.145780563354492, -0.4019792675971985, 0.027800539508461952], 'magnitude': 2.1832852363586426}], 'glu_contributions': [{'resid': 1073, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 4.3583550453186035, 'force': [7.864422798156738, 10.202507972717285, -5.675961494445801], 'magnitude': 14.076820373535156}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 4.242438793182373, 'force': [-10.68781852722168, -7.506555557250977, 7.585867881774902], 'magnitude': 15.10374927520752}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 3.707674503326416, 'force': [-8.594605445861816, -17.283105850219727, 4.297770977020264], 'magnitude': 19.77482795715332}], 'asn_contributions': [{'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.846770286560059, 'force': [-3.5097014904022217, 0.9241728782653809, 9.400524139404297], 'magnitude': 10.076803207397461}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.594653606414795, 'force': [3.1878349781036377, -0.4439716339111328, -5.405299663543701], 'magnitude': 6.290998935699463}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.240706443786621, 'force': [4.4877848625183105, 2.487294912338257, -16.173370361328125], 'magnitude': 16.967756271362305}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.6650214195251465, 'force': [-2.232736825942993, -2.049315929412842, 5.638392925262451], 'magnitude': 6.401272296905518}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.046799182891846, 'force': [-0.23781569302082062, -1.2247532606124878, 8.414496421813965], 'magnitude': 8.506487846374512}]}, 4993: {'frame': 4993, 'ionic_force': [-11.465587615966797, -15.185635328292847, -2.6171058416366577], 'ionic_force_magnitude': 19.207094071973398, 'motion_vector': [-1.2147407531738281, 0.47171783447265625, 0.3584442138671875], 'ionic_force_x': -11.465587615966797, 'ionic_force_y': -15.185635328292847, 'ionic_force_z': -2.6171058416366577, 'radial_force': 19.02795889482913, 'axial_force': -2.6171058416366577, 'glu_force': [-24.02146816253662, -7.26126941666007, 1.3423142433166504], 'glu_force_magnitude': 25.130833128905497, 'asn_force': [1.0738476812839508, -1.3141849040985107, 1.2803244590759277], 'asn_force_magnitude': 2.1259025201705266, 'residue_force': [-22.94762048125267, -8.575454320758581, 2.622638702392578], 'residue_force_magnitude': 24.6375716401254, 'total_force': [-34.41320809721947, -23.761089649051428, 0.00553286075592041], 'total_force_magnitude': 41.81935321672657, 'motion_component_total': 22.638711862524833, 'cosine_total_motion': 0.5413453370548539, 'cosine_glu_motion': 0.7724406385233468, 'cosine_asn_motion': -0.5100412913173472, 'cosine_residue_motion': 0.7438955019521386, 'cosine_ionic_motion': 0.22444483919628416, 'motion_component_glu': 19.41207678871544, 'motion_component_asn': -1.084298066602578, 'motion_component_residue': 18.32777872211286, 'motion_component_ionic': 4.310933140411972, 'ionic_contributions': [{'ion_id': 1307, 'distance': 5.823085308074951, 'force': [-4.743855953216553, -8.147418975830078, -2.642191171646118], 'magnitude': 9.791107177734375}, {'ion_id': 1309, 'distance': 13.311628341674805, 'force': [-0.767593502998352, -0.664334774017334, -1.574743628501892], 'magnitude': 1.873594880104065}, {'ion_id': 1316, 'distance': 10.68295955657959, 'force': [-0.9619420766830444, -1.5705485343933105, 2.251835346221924], 'magnitude': 2.9090750217437744}, {'ion_id': 1320, 'distance': 8.882369041442871, 'force': [-2.390256643295288, -2.211256742477417, -2.6654586791992188], 'magnitude': 4.2080464363098145}, {'ion_id': 1460, 'distance': 8.903144836425781, 'force': [-2.6019394397735596, -2.592076301574707, 2.0134522914886475], 'magnitude': 4.18842887878418}], 'glu_contributions': [{'resid': 1073, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.7476274967193604, 'force': [16.813922882080078, 5.647915363311768, -6.918410301208496], 'magnitude': 19.038681030273438}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 4.11309289932251, 'force': [-14.870831489562988, 0.05484262481331825, 6.0873823165893555], 'magnitude': 16.06863021850586}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 3.0562846660614014, 'force': [-25.96455955505371, -12.964027404785156, 2.173342227935791], 'magnitude': 29.102367401123047}], 'asn_contributions': [{'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.204658508300781, 'force': [-1.6403664350509644, -3.485567331314087, 7.843697547912598], 'magnitude': 8.738625526428223}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.89402437210083, 'force': [2.018101692199707, 1.864999771118164, -4.957528591156006], 'magnitude': 5.668160915374756}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.256622314453125, 'force': [1.1413710117340088, 6.642326354980469, -8.747842788696289], 'magnitude': 11.04300594329834}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.769192218780518, 'force': [-0.895393431186676, -2.824409008026123, 2.9561948776245117], 'magnitude': 4.1854634284973145}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.04091739654541, 'force': [0.45013484358787537, -3.5115346908569336, 4.185803413391113], 'magnitude': 5.482193470001221}]}, 4994: {'frame': 4994, 'ionic_force': [-15.226321399211884, -15.62778353691101, -3.6030957102775574], 'ionic_force_magnitude': 22.114492540550533, 'motion_vector': [0.4574928283691406, 1.3063774108886719, 0.06430816650390625], 'ionic_force_x': -15.226321399211884, 'ionic_force_y': -15.62778353691101, 'ionic_force_z': -3.6030957102775574, 'radial_force': 21.81899359797891, 'axial_force': -3.6030957102775574, 'glu_force': [-32.275760650634766, -17.716858863830566, 1.9284021854400635], 'glu_force_magnitude': 36.86910018656226, 'asn_force': [-0.4553137421607971, -1.938793420791626, 3.4184200763702393], 'asn_force_magnitude': 3.9562389147821286, 'residue_force': [-32.73107439279556, -19.655652284622192, 5.346822261810303], 'residue_force_magnitude': 38.55199613431296, 'total_force': [-47.957395792007446, -35.2834358215332, 1.7437265515327454], 'total_force_magnitude': 59.564026364996735, 'motion_component_total': -49.017401899278966, 'cosine_total_motion': -0.8229363407857939, 'cosine_glu_motion': -0.7396406325537873, 'cosine_asn_motion': -0.459916685487585, 'cosine_residue_motion': -0.7545504199319684, 'cosine_ionic_motion': -0.9011274841770078, 'motion_component_glu': -27.269884583677864, 'motion_component_asn': -1.819540288683597, 'motion_component_residue': -29.089424872361462, 'motion_component_ionic': -19.927977026917507, 'ionic_contributions': [{'ion_id': 1306, 'distance': 14.929139137268066, 'force': [-0.8425669074058533, -1.2280627489089966, -0.028977513313293457], 'magnitude': 1.4895961284637451}, {'ion_id': 1307, 'distance': 5.389379024505615, 'force': [-5.873695373535156, -9.419403076171875, -2.7254559993743896], 'magnitude': 11.430378913879395}, {'ion_id': 1309, 'distance': 13.295854568481445, 'force': [-0.9202994108200073, -0.567900538444519, -1.5354427099227905], 'magnitude': 1.8780431747436523}, {'ion_id': 1316, 'distance': 9.752813339233398, 'force': [-1.8541682958602905, -1.3925756216049194, 2.6088037490844727], 'magnitude': 3.490424633026123}, {'ion_id': 1320, 'distance': 9.194694519042969, 'force': [-2.610811948776245, -1.7711108922958374, -2.3384480476379395], 'magnitude': 3.927023410797119}, {'ion_id': 1460, 'distance': 9.89516544342041, 'force': [-3.124779462814331, -1.2487306594848633, 0.41642481088638306], 'magnitude': 3.3907203674316406}], 'glu_contributions': [{'resid': 1073, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 2.875811815261841, 'force': [22.783946990966797, 20.381959915161133, -10.526509284973145], 'magnitude': 32.33171463012695}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 2.790276288986206, 'force': [-29.792335510253906, -8.531960487365723, 16.085168838500977], 'magnitude': 34.9157600402832}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.6380455493927, 'force': [-25.267372131347656, -29.566858291625977, -3.6302573680877686], 'magnitude': 39.06172180175781}], 'asn_contributions': [{'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.933972358703613, 'force': [-0.4553137421607971, -1.938793420791626, 3.4184200763702393], 'magnitude': 3.9562387466430664}]}, 4995: {'frame': 4995, 'ionic_force': [-16.513193786144257, -9.016636848449707, -1.008799159899354], 'ionic_force_magnitude': 18.841522890164374, 'motion_vector': [0.29911041259765625, -1.0097732543945312, -0.8112640380859375], 'ionic_force_x': -16.513193786144257, 'ionic_force_y': -9.016636848449707, 'ionic_force_z': -1.008799159899354, 'radial_force': 18.814497311264375, 'axial_force': -1.008799159899354, 'glu_force': [-25.47502326965332, -17.447433471679688, 1.9919557571411133], 'glu_force_magnitude': 30.94119637435622, 'asn_force': [0.016815880313515663, 0.7998800724744797, 2.303154945373535], 'asn_force_magnitude': 2.438157830529244, 'residue_force': [-25.458207389339805, -16.647553399205208, 4.295110702514648], 'residue_force_magnitude': 30.71985243462085, 'total_force': [-41.97140117548406, -25.664190247654915, 3.2863115426152945], 'total_force_magnitude': 49.30566926080993, 'motion_component_total': 8.044985611733257, 'cosine_total_motion': 0.16316552908303641, 'cosine_glu_motion': 0.20378209048134185, 'cosine_asn_motion': -0.8241076025223907, 'cosine_residue_motion': 0.13984303095251502, 'cosine_ionic_motion': 0.19897692764627548, 'motion_component_glu': 6.305261679160026, 'motion_component_asn': -2.0093044042886485, 'motion_component_residue': 4.295957274871378, 'motion_component_ionic': 3.7490283368618798, 'ionic_contributions': [{'ion_id': 1306, 'distance': 12.820343971252441, 'force': [-1.3241117000579834, -1.5251678228378296, 0.027443215250968933], 'magnitude': 2.0199410915374756}, {'ion_id': 1307, 'distance': 6.259469985961914, 'force': [-7.239418983459473, -4.05126953125, 1.7257643938064575], 'magnitude': 8.473502159118652}, {'ion_id': 1309, 'distance': 12.917562484741211, 'force': [-0.9697037935256958, -0.4882330298423767, -1.6673376560211182], 'magnitude': 1.989651083946228}, {'ion_id': 1316, 'distance': 13.020878791809082, 'force': [-0.7669690251350403, -0.3876888155937195, 1.759548544883728], 'magnitude': 1.9582020044326782}, {'ion_id': 1320, 'distance': 8.06869125366211, 'force': [-3.7609140872955322, -1.9077779054641724, -2.8672845363616943], 'magnitude': 5.099550247192383}, {'ion_id': 1460, 'distance': 11.43622875213623, 'force': [-2.4520761966705322, -0.6564997434616089, 0.013066878542304039], 'magnitude': 2.5384721755981445}], 'glu_contributions': [{'resid': 1073, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.393834114074707, 'force': [17.07512855529785, 13.89212417602539, -7.374588489532471], 'magnitude': 23.214988708496094}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 3.4763989448547363, 'force': [-18.829477310180664, -6.357393264770508, 10.535232543945312], 'magnitude': 22.49348258972168}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.808281421661377, 'force': [-23.720674514770508, -24.98216438293457, -1.1686882972717285], 'magnitude': 34.46947479248047}], 'asn_contributions': [{'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.829130172729492, 'force': [-1.6747750043869019, -0.2213338166475296, 6.758659839630127], 'magnitude': 6.966587543487549}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.607299327850342, 'force': [1.7109771966934204, 2.448659896850586, -9.233780860900879], 'magnitude': 9.704951286315918}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.285283088684082, 'force': [-0.01938631199300289, -1.4274460077285767, 4.778275966644287], 'magnitude': 4.986972808837891}]}, 4996: {'frame': 4996, 'ionic_force': [-3.4634814858436584, -24.222798764705658, -7.885996222496033], 'ionic_force_magnitude': 25.708532054931286, 'motion_vector': [-0.20244598388671875, 1.0721435546875, 1.0912857055664062], 'ionic_force_x': -3.4634814858436584, 'ionic_force_y': -24.222798764705658, 'ionic_force_z': -7.885996222496033, 'radial_force': 24.469157811379773, 'axial_force': -7.885996222496033, 'glu_force': [-29.198650360107422, -18.053829431533813, 4.87490177154541], 'glu_force_magnitude': 34.67371637533154, 'asn_force': [2.0548769496381283, 1.2744672298431396, -1.7439651489257812], 'asn_force_magnitude': 2.9813085111685216, 'residue_force': [-27.143773410469294, -16.779362201690674, 3.130936622619629], 'residue_force_magnitude': 32.06453172883219, 'total_force': [-30.607254896312952, -41.00216096639633, -4.755059599876404], 'total_force_magnitude': 51.38668940494732, 'motion_component_total': -27.834233351081092, 'cosine_total_motion': -0.5416623190440697, 'cosine_glu_motion': -0.15185225902643873, 'cosine_asn_motion': -0.20709014120287902, 'cosine_residue_motion': -0.18346382884156343, 'cosine_ionic_motion': -0.8538625053812476, 'motion_component_glu': -5.265282160436115, 'motion_component_asn': -0.6173996005472342, 'motion_component_residue': -5.882681760983349, 'motion_component_ionic': -21.951551590097743, 'ionic_contributions': [{'ion_id': 1306, 'distance': 13.125436782836914, 'force': [-1.1426242589950562, -1.551206111907959, -0.044628992676734924], 'magnitude': 1.9271279573440552}, {'ion_id': 1307, 'distance': 4.0804619789123535, 'force': [3.4352829456329346, -19.294559478759766, -3.6758644580841064], 'magnitude': 19.939739227294922}, {'ion_id': 1309, 'distance': 13.257035255432129, 'force': [-0.8596774935722351, -0.5392806529998779, -1.5933207273483276], 'magnitude': 1.889057993888855}, {'ion_id': 1320, 'distance': 8.773033142089844, 'force': [-2.712550401687622, -1.9728121757507324, -2.712400197982788], 'magnitude': 4.313587188720703}, {'ion_id': 1460, 'distance': 11.878056526184082, 'force': [-2.1839122772216797, -0.864940345287323, 0.14021815359592438], 'magnitude': 2.353137493133545}], 'glu_contributions': [{'resid': 1073, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.334083318710327, 'force': [18.76300621032715, 11.122505187988281, -10.14197826385498], 'magnitude': 24.054527282714844}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 3.643115997314453, 'force': [-17.8575382232666, -2.6054956912994385, 9.686452865600586], 'magnitude': 20.48188591003418}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.590609312057495, 'force': [-30.10411834716797, -26.570838928222656, 5.330427169799805], 'magnitude': 40.50531768798828}], 'asn_contributions': [{'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.199516296386719, 'force': [-2.6778736114501953, -1.6790857315063477, 8.165523529052734], 'magnitude': 8.755918502807617}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.779223442077637, 'force': [2.8431921005249023, 0.8961319923400879, -5.086368560791016], 'magnitude': 5.8955864906311035}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.50897216796875, 'force': [1.9459538459777832, 4.046713352203369, -8.996109008789062], 'magnitude': 10.054481506347656}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.489260196685791, 'force': [-0.056395385414361954, -1.9892923831939697, 4.1729888916015625], 'magnitude': 4.623234748840332}]}, 4997: {'frame': 4997, 'ionic_force': [-12.324485659599304, -21.485591620206833, 0.6895290873944759], 'ionic_force_magnitude': 24.77900410440932, 'motion_vector': [-0.3025016784667969, -0.6528167724609375, -0.76025390625], 'ionic_force_x': -12.324485659599304, 'ionic_force_y': -21.485591620206833, 'ionic_force_z': 0.6895290873944759, 'radial_force': 24.76940843144969, 'axial_force': 0.6895290873944759, 'glu_force': [-26.104713439941406, -19.13771677017212, 1.6138575077056885], 'glu_force_magnitude': 32.40852978788089, 'asn_force': [-0.256849005818367, 0.3470843434333801, 2.765280246734619], 'asn_force_magnitude': 2.7987879155497186, 'residue_force': [-26.361562445759773, -18.79063242673874, 4.379137754440308], 'residue_force_magnitude': 32.667976506830996, 'total_force': [-38.68604810535908, -40.27622404694557, 5.0686668418347836], 'total_force_magnitude': 56.07562683593853, 'motion_component_total': 32.6175943815771, 'cosine_total_motion': 0.5816715072487193, 'cosine_glu_motion': 0.5648982393926534, 'cosine_asn_motion': -0.768432407705826, 'cosine_residue_motion': 0.49457737544582775, 'cosine_ionic_motion': 0.6643024162853077, 'motion_component_glu': 18.307521418478274, 'motion_component_asn': -2.15067933660384, 'motion_component_residue': 16.156842081874434, 'motion_component_ionic': 16.46075229970267, 'ionic_contributions': [{'ion_id': 1306, 'distance': 12.2718505859375, 'force': [-1.535698652267456, -1.5813456773757935, -0.031177494674921036], 'magnitude': 2.2045400142669678}, {'ion_id': 1307, 'distance': 4.242607593536377, 'force': [-4.548783779144287, -17.15741729736328, 5.0139594078063965], 'magnitude': 18.444732666015625}, {'ion_id': 1309, 'distance': 12.592719078063965, 'force': [-1.0400985479354858, -0.5203492045402527, -1.7408907413482666], 'magnitude': 2.093625783920288}, {'ion_id': 1320, 'distance': 8.438592910766602, 'force': [-3.253243923187256, -1.7816591262817383, -2.824697256088257], 'magnitude': 4.662276268005371}, {'ion_id': 1460, 'distance': 12.835030555725098, 'force': [-1.9466607570648193, -0.4448203146457672, 0.2723351716995239], 'magnitude': 2.0153212547302246}], 'glu_contributions': [{'resid': 1073, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.519207239151001, 'force': [15.38404655456543, 13.974355697631836, -5.8474297523498535], 'magnitude': 21.59036636352539}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 3.6334826946258545, 'force': [-17.216053009033203, -7.235029697418213, 8.673872947692871], 'magnitude': 20.590633392333984}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.7672173976898193, 'force': [-24.272706985473633, -25.877042770385742, -1.212585687637329], 'magnitude': 35.500083923339844}], 'asn_contributions': [{'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.68773078918457, 'force': [-1.9383807182312012, -0.6893336176872253, 7.022111892700195], 'magnitude': 7.317277908325195}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.708172798156738, 'force': [1.9283785820007324, 2.883417844772339, -8.698851585388184], 'magnitude': 9.364975929260254}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.377700328826904, 'force': [-0.24684686958789825, -1.8469998836517334, 4.442019939422607], 'magnitude': 4.817040920257568}]}, 4998: {'frame': 4998, 'ionic_force': [-8.595291793346405, -8.897465407848358, -3.6955340802669525], 'ionic_force_magnitude': 12.91127041909667, 'motion_vector': [1.2956390380859375, -1.7068977355957031, 0.36876678466796875], 'ionic_force_x': -8.595291793346405, 'ionic_force_y': -8.897465407848358, 'ionic_force_z': -3.6955340802669525, 'radial_force': 12.371092582978521, 'axial_force': -3.6955340802669525, 'glu_force': [-24.26844882965088, -17.303970336914062, 4.667385101318359], 'glu_force_magnitude': 30.16901525907323, 'asn_force': [-0.7594750616699457, 0.1303102970123291, 3.0745785236358643], 'asn_force_magnitude': 3.1696713143177635, 'residue_force': [-25.027923891320825, -17.173660039901733, 7.741963624954224], 'residue_force_magnitude': 31.325222652775825, 'total_force': [-33.62321568466723, -26.07112544775009, 4.046429544687271], 'total_force_magnitude': 42.7387155533492, 'motion_component_total': 1.1172486486236832, 'cosine_total_motion': 0.026141371685095727, 'cosine_glu_motion': -0.0028332656432715347, 'cosine_asn_motion': -0.010537839293686381, 'cosine_residue_motion': -0.0037949713132660167, 'cosine_ionic_motion': 0.09574015026006427, 'motion_component_glu': -0.08547683442486687, 'motion_component_asn': -0.033401486924088286, 'motion_component_residue': -0.11887832134895504, 'motion_component_ionic': 1.2361269699726383, 'ionic_contributions': [{'ion_id': 1306, 'distance': 12.126421928405762, 'force': [-1.212032675743103, -1.8853203058242798, 0.2718568742275238], 'magnitude': 2.2577338218688965}, {'ion_id': 1307, 'distance': 8.477420806884766, 'force': [-1.4655177593231201, -4.378549098968506, 0.14790880680084229], 'magnitude': 4.619665622711182}, {'ion_id': 1309, 'distance': 13.297412872314453, 'force': [-0.8881041407585144, -0.46092355251312256, -1.5887774229049683], 'magnitude': 1.8776030540466309}, {'ion_id': 1320, 'distance': 8.557500839233398, 'force': [-3.2808942794799805, -1.594046950340271, -2.6922800540924072], 'magnitude': 4.533610820770264}, {'ion_id': 1460, 'distance': 13.39831829071045, 'force': [-1.748742938041687, -0.578625500202179, 0.16575771570205688], 'magnitude': 1.8494282960891724}], 'glu_contributions': [{'resid': 1073, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.517155170440674, 'force': [15.353458404541016, 12.796353340148926, -8.231489181518555], 'magnitude': 21.615568161010742}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 3.8038060665130615, 'force': [-15.194540977478027, -5.650843620300293, 9.49634838104248], 'magnitude': 18.787940979003906}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.7977993488311768, 'force': [-24.427366256713867, -24.449480056762695, 3.4025259017944336], 'magnitude': 34.72823715209961}], 'asn_contributions': [{'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.376643657684326, 'force': [-2.3995699882507324, -1.6088228225708008, 7.661952495574951], 'magnitude': 8.188514709472656}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.680517196655273, 'force': [1.6689785718917847, 3.7069311141967773, -8.537936210632324], 'magnitude': 9.456382751464844}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.618100643157959, 'force': [-0.028883645310997963, -1.9677979946136475, 3.9505622386932373], 'magnitude': 4.413615703582764}]}, 4999: {'frame': 4999, 'ionic_force': [-13.94003438949585, -13.628098368644714, 0.2862973641604185], 'ionic_force_magnitude': 19.496963612483583, 'motion_vector': [-0.551971435546875, 1.3257789611816406, 0.19469451904296875], 'ionic_force_x': -13.94003438949585, 'ionic_force_y': -13.628098368644714, 'ionic_force_z': 0.2862973641604185, 'radial_force': 19.494861474906244, 'axial_force': 0.2862973641604185, 'glu_force': [-29.7453670501709, -4.709474802017212, 0.7009942531585693], 'glu_force_magnitude': 30.124033707377052, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [-29.7453670501709, -4.709474802017212, 0.7009942531585693], 'residue_force_magnitude': 30.124033707377052, 'total_force': [-43.68540143966675, -18.337573170661926, 0.9872916173189878], 'total_force_magnitude': 47.38834913216376, 'motion_component_total': -0.0043155269347410485, 'cosine_total_motion': -9.10672562723225e-05, 'cosine_glu_motion': 0.23619190233075033, 'cosine_asn_motion': None, 'cosine_residue_motion': 0.23619190233075033, 'cosine_ionic_motion': -0.36515267175230093, 'motion_component_glu': 7.115052827221032, 'motion_component_asn': None, 'motion_component_residue': 7.115052827221032, 'motion_component_ionic': -7.119368354155773, 'ionic_contributions': [{'ion_id': 1306, 'distance': 8.779632568359375, 'force': [-1.312923789024353, -3.71425461769104, 1.741175651550293], 'magnitude': 4.307104587554932}, {'ion_id': 1307, 'distance': 10.189913749694824, 'force': [-0.6792678236961365, -3.1243350505828857, -0.02229972369968891], 'magnitude': 3.1974008083343506}, {'ion_id': 1309, 'distance': 13.085969924926758, 'force': [-0.7131099104881287, -0.7815901041030884, -1.624629020690918], 'magnitude': 1.938769817352295}, {'ion_id': 1320, 'distance': 8.737730026245117, 'force': [-2.2887518405914307, -2.6869468688964844, -2.5399811267852783], 'magnitude': 4.348513603210449}, {'ion_id': 1460, 'distance': 5.783412456512451, 'force': [-8.9459810256958, -3.320971727371216, 2.7320315837860107], 'magnitude': 9.925896644592285}], 'glu_contributions': [{'resid': 1073, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.7607743740081787, 'force': [17.93753433227539, 3.140578508377075, -5.080453872680664], 'magnitude': 18.905803680419922}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 4.463375568389893, 'force': [-13.11652946472168, 1.0732035636901855, 3.606135368347168], 'magnitude': 13.645487785339355}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.7569198608398438, 'force': [-34.56637191772461, -8.923256874084473, 2.1753127574920654], 'magnitude': 35.76577377319336}], 'asn_contributions': []}, 5000: {'frame': 5000, 'ionic_force': [-10.132799685001373, -11.112239122390747, -2.420377552509308], 'ionic_force_magnitude': 15.231996430745589, 'motion_vector': [-0.7812538146972656, 0.4613761901855469, -0.36583709716796875], 'ionic_force_x': -10.132799685001373, 'ionic_force_y': -11.112239122390747, 'ionic_force_z': -2.420377552509308, 'radial_force': 15.038466935481004, 'axial_force': -2.420377552509308, 'glu_force': [-26.04249668121338, -13.600052833557129, -0.6666277348995209], 'glu_force_magnitude': 29.387369106530997, 'asn_force': [0.10181431472301483, 0.09704506397247314, 2.6466970443725586], 'asn_force_magnitude': 2.650431878734931, 'residue_force': [-25.940682366490364, -13.503007769584656, 1.9800693094730377], 'residue_force_magnitude': 29.311617064483574, 'total_force': [-36.07348205149174, -24.615246891975403, -0.44030824303627014], 'total_force_magnitude': 43.673794868560336, 'motion_component_total': 17.36360475737407, 'cosine_total_motion': 0.3975749029739958, 'cosine_glu_motion': 0.4979189155424071, 'cosine_asn_motion': -0.3868356705900173, 'cosine_residue_motion': 0.4642270446243121, 'cosine_ionic_motion': 0.24660978693424204, 'motion_component_glu': 14.63252695616835, 'motion_component_asn': -1.0252815931635864, 'motion_component_residue': 13.607245363004763, 'motion_component_ionic': 3.756359394369305, 'ionic_contributions': [{'ion_id': 1306, 'distance': 12.127389907836914, 'force': [-0.8784706592559814, -1.9305158853530884, 0.7727431654930115], 'magnitude': 2.257373332977295}, {'ion_id': 1307, 'distance': 8.653753280639648, 'force': [-0.2424018383026123, -4.398298740386963, 0.5005394816398621], 'magnitude': 4.43332052230835}, {'ion_id': 1309, 'distance': 12.70804214477539, 'force': [-0.9397225975990295, -0.6545020341873169, -1.707296371459961], 'magnitude': 2.055799722671509}, {'ion_id': 1320, 'distance': 7.755664825439453, 'force': [-3.7437233924865723, -2.7520456314086914, -2.9792110919952393], 'magnitude': 5.519503593444824}, {'ion_id': 1460, 'distance': 8.450234413146973, 'force': [-4.328481197357178, -1.3768768310546875, 0.9928472638130188], 'magnitude': 4.649439334869385}], 'glu_contributions': [{'resid': 1073, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.594980001449585, 'force': [17.792102813720703, 8.923538208007812, -5.646260738372803], 'magnitude': 20.689821243286133}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 4.129591464996338, 'force': [-14.833268165588379, -2.4058408737182617, 5.3183979988098145], 'magnitude': 15.940491676330566}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.7751455307006836, 'force': [-29.001331329345703, -20.11775016784668, -0.3387649953365326], 'magnitude': 35.29753494262695}], 'asn_contributions': [{'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.842946529388428, 'force': [-1.1452957391738892, -1.3808842897415161, 6.697564601898193], 'magnitude': 6.933680057525635}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.831326007843018, 'force': [1.1115437746047974, 3.6620640754699707, -8.116592407226562], 'magnitude': 8.973589897155762}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.4928202629089355, 'force': [0.13556627929210663, -2.1841347217559814, 4.065724849700928], 'magnitude': 4.617243766784668}]}, 5001: {'frame': 5001, 'ionic_force': [-8.440096318721771, -11.586323291063309, -2.215720146894455], 'ionic_force_magnitude': 14.504741605547162, 'motion_vector': [-0.016719818115234375, -0.3343772888183594, 0.31487274169921875], 'ionic_force_x': -8.440096318721771, 'ionic_force_y': -11.586323291063309, 'ionic_force_z': -2.215720146894455, 'radial_force': 14.33450777928342, 'axial_force': -2.215720146894455, 'glu_force': [-27.27439785003662, -29.413665771484375, 0.45595622062683105], 'glu_force_magnitude': 40.11563795172404, 'asn_force': [-0.3014219403266907, 0.4341629147529602, 2.2152905464172363], 'asn_force_magnitude': 2.277468952083139, 'residue_force': [-27.57581979036331, -28.979502856731415, 2.6712467670440674], 'residue_force_magnitude': 40.09205634816379, 'total_force': [-36.01591610908508, -40.56582614779472, 0.4555266201496124], 'total_force_magnitude': 54.24887066779755, 'motion_component_total': 31.135528907390537, 'cosine_total_motion': 0.5739387479244388, 'cosine_glu_motion': 0.565968388959146, 'cosine_asn_motion': 0.5325178181943959, 'cosine_residue_motion': 0.5965514857426318, 'cosine_ionic_motion': 0.4976685088726757, 'motion_component_glu': 22.70418298360563, 'motion_component_asn': 1.2127927973687902, 'motion_component_residue': 23.916975780974422, 'motion_component_ionic': 7.218553126416117, 'ionic_contributions': [{'ion_id': 1306, 'distance': 12.427327156066895, 'force': [-1.3881559371948242, -1.5592139959335327, 0.5130171179771423], 'magnitude': 2.149723529815674}, {'ion_id': 1307, 'distance': 6.923681735992432, 'force': [-0.7212875485420227, -6.880537509918213, -0.3214363157749176], 'magnitude': 6.925704002380371}, {'ion_id': 1309, 'distance': 13.290054321289062, 'force': [-0.9957014322280884, -0.493723243474</t>
+          <t>{4992: {'frame': 4992, 'motion_vector': [1.30914306640625, -2.567424774169922, 0.49839019775390625], 'ionic_force': [-19.95671159029007, -2.516607314348221, 0.35591466911137104], 'ionic_force_magnitude': 20.117910555630214, 'radial_force': 20.114761988963455, 'axial_force': 0.35591466911137104, 'glu_force': [-11.418001174926758, -14.587153434753418, 6.207677364349365], 'glu_force_magnitude': 19.53691517152907, 'asn_force': [1.6953658312559128, -0.3065730333328247, 1.8747434616088867], 'asn_force_magnitude': 2.546156981295971, 'residue_force': [-9.722635343670845, -14.893726468086243, 8.082420825958252], 'residue_force_magnitude': 19.536587535699624, 'total_force': [-29.679346933960915, -17.410333782434464, 8.438335495069623], 'total_force_magnitude': 35.42864466458667, 'cosine_total_motion': 0.09699810692985182, 'cosine_glu_motion': 0.44797979935668564, 'cosine_asn_motion': 0.529214031111739, 'cosine_residue_motion': 0.5169585179627656, 'cosine_ionic_motion': -0.3312020826678284, 'motion_component_total': 3.436511463555302, 'motion_component_glu': 8.75214333859018, 'motion_component_asn': 1.3474619999149375, 'motion_component_residue': 10.099605338505118, 'motion_component_ionic': -6.663093874949816, 'motion_component_percent_total': 9.699810692985182, 'motion_component_percent_glu': 44.797979935668565, 'motion_component_percent_asn': 52.9214031111739, 'motion_component_percent_residue': 51.69585179627656, 'motion_component_percent_ionic': 33.12020826678284, 'ionic_contributions': [{'ion_id': 1306, 'distance': 13.177733421325684, 'force': [-1.3452452421188354, -1.3558294773101807, -0.08520316332578659], 'magnitude': 1.9118623733520508, 'cosine_ionic_motion': 0.299984872341156, 'motion_component_ionic': 0.5735297799110413, 'motion_component_percent_ionic': 29.9984872341156}, {'ion_id': 1307, 'distance': 6.083970069885254, 'force': [-8.701690673828125, 2.1244421005249023, 0.4665580689907074], 'magnitude': 8.969411849975586, 'cosine_ionic_motion': -0.6333103179931641, 'motion_component_ionic': -5.680420875549316, 'motion_component_percent_ionic': 63.331031799316406}, {'ion_id': 1309, 'distance': 13.56334114074707, 'force': [-0.8666126132011414, -0.2845568358898163, -1.5572242736816406], 'magnitude': 1.8046987056732178, 'cosine_ionic_motion': -0.22356922924518585, 'motion_component_ionic': -0.4034751057624817, 'motion_component_percent_ionic': 22.356922924518585}, {'ion_id': 1316, 'distance': 7.383633136749268, 'force': [-3.8274505138397217, -1.5964282751083374, 4.4594645500183105], 'magnitude': 6.089727878570557, 'cosine_ionic_motion': 0.07358409464359283, 'motion_component_ionic': 0.44810712337493896, 'motion_component_percent_ionic': 7.3584094643592834}, {'ion_id': 1320, 'distance': 8.708598136901855, 'force': [-3.069931983947754, -1.0022555589675903, -2.9554810523986816], 'magnitude': 4.377655506134033, 'cosine_ionic_motion': -0.22796718776226044, 'motion_component_ionic': -0.9979618191719055, 'motion_component_percent_ionic': 22.796718776226044}, {'ion_id': 1460, 'distance': 12.331439971923828, 'force': [-2.145780563354492, -0.4019792675971985, 0.027800539508461952], 'magnitude': 2.1832852363586426, 'cosine_ionic_motion': -0.2761309742927551, 'motion_component_ionic': -0.6028726696968079, 'motion_component_percent_ionic': 27.613097429275513}], 'glu_contributions': [{'resid': 1073, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 4.3583550453186035, 'force': [7.864422798156738, 10.202507972717285, -5.675961494445801], 'magnitude': 14.076820373535156, 'cosine_with_motion': -0.4548722505569458, 'motion_component': -6.4031548500061035, 'motion_component_percent': 45.48722505569458}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 4.242438793182373, 'force': [-10.68781852722168, -7.506555557250977, 7.585867881774902], 'magnitude': 15.10374927520752, 'cosine_with_motion': 0.20512840151786804, 'motion_component': 3.098207950592041, 'motion_component_percent': 20.512840151786804}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 3.707674503326416, 'force': [-8.594605445861816, -17.283105850219727, 4.297770977020264], 'magnitude': 19.77482795715332, 'cosine_with_motion': 0.6097190976142883, 'motion_component': 12.057089805603027, 'motion_component_percent': 60.97190976142883}], 'asn_contributions': [{'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.846770286560059, 'force': [-3.5097014904022217, 0.9241728782653809, 9.400524139404297], 'magnitude': 10.076803207397461, 'cosine_with_motion': -0.07744093239307404, 'motion_component': -0.7803570628166199, 'motion_component_percent': 7.744093239307404}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.594653606414795, 'force': [3.1878349781036377, -0.4439716339111328, -5.405299663543701], 'magnitude': 6.290998935699463, 'cosine_with_motion': 0.1423555314540863, 'motion_component': 0.8955584764480591, 'motion_component_percent': 14.23555314540863}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.240706443786621, 'force': [4.4877848625183105, 2.487294912338257, -16.173370361328125], 'magnitude': 16.967756271362305, 'cosine_with_motion': -0.17272165417671204, 'motion_component': -2.930698871612549, 'motion_component_percent': 17.272165417671204}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.6650214195251465, 'force': [-2.232736825942993, -2.049315929412842, 5.638392925262451], 'magnitude': 6.401272296905518, 'cosine_with_motion': 0.2750054597854614, 'motion_component': 1.7603847980499268, 'motion_component_percent': 27.500545978546143}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.046799182891846, 'force': [-0.23781569302082062, -1.2247532606124878, 8.414496421813965], 'magnitude': 8.506487846374512, 'cosine_with_motion': 0.2824402451515198, 'motion_component': 2.4025745391845703, 'motion_component_percent': 28.244024515151978}]}, 4993: {'frame': 4993, 'motion_vector': [-1.2147407531738281, 0.47171783447265625, 0.3584442138671875], 'ionic_force': [-11.465587615966797, -15.185635328292847, -2.6171058416366577], 'ionic_force_magnitude': 19.207094071973398, 'radial_force': 19.02795889482913, 'axial_force': -2.6171058416366577, 'glu_force': [-24.02146816253662, -7.26126941666007, 1.3423142433166504], 'glu_force_magnitude': 25.130833128905497, 'asn_force': [1.0738476812839508, -1.3141849040985107, 1.2803244590759277], 'asn_force_magnitude': 2.1259025201705266, 'residue_force': [-22.94762048125267, -8.575454320758581, 2.622638702392578], 'residue_force_magnitude': 24.6375716401254, 'total_force': [-34.41320809721947, -23.761089649051428, 0.00553286075592041], 'total_force_magnitude': 41.81935321672657, 'cosine_total_motion': 0.5413453370548539, 'cosine_glu_motion': 0.7724406385233468, 'cosine_asn_motion': -0.5100412913173472, 'cosine_residue_motion': 0.7438955019521386, 'cosine_ionic_motion': 0.22444483919628416, 'motion_component_total': 22.638711862524833, 'motion_component_glu': 19.41207678871544, 'motion_component_asn': -1.084298066602578, 'motion_component_residue': 18.32777872211286, 'motion_component_ionic': 4.310933140411972, 'motion_component_percent_total': 54.13453370548539, 'motion_component_percent_glu': 77.24406385233468, 'motion_component_percent_asn': 51.00412913173472, 'motion_component_percent_residue': 74.38955019521386, 'motion_component_percent_ionic': 22.444483919628418, 'ionic_contributions': [{'ion_id': 1307, 'distance': 5.823085308074951, 'force': [-4.743855953216553, -8.147418975830078, -2.642191171646118], 'magnitude': 9.791107177734375, 'cosine_ionic_motion': 0.07346829771995544, 'motion_component_ionic': 0.7193359732627869, 'motion_component_percent_ionic': 7.346829771995544}, {'ion_id': 1309, 'distance': 13.311628341674805, 'force': [-0.767593502998352, -0.664334774017334, -1.574743628501892], 'magnitude': 1.873594880104065, 'cosine_ionic_motion': 0.021558674052357674, 'motion_component_ionic': 0.04039222002029419, 'motion_component_percent_ionic': 2.1558674052357674}, {'ion_id': 1316, 'distance': 10.68295955657959, 'force': [-0.9619420766830444, -1.5705485343933105, 2.251835346221924], 'magnitude': 2.9090750217437744, 'cosine_ionic_motion': 0.3140687644481659, 'motion_component_ionic': 0.9136495590209961, 'motion_component_percent_ionic': 31.40687644481659}, {'ion_id': 1320, 'distance': 8.882369041442871, 'force': [-2.390256643295288, -2.211256742477417, -2.6654586791992188], 'magnitude': 4.2080464363098145, 'cosine_ionic_motion': 0.159134179353714, 'motion_component_ionic': 0.6696439981460571, 'motion_component_percent_ionic': 15.913417935371399}, {'ion_id': 1460, 'distance': 8.903144836425781, 'force': [-2.6019394397735596, -2.592076301574707, 2.0134522914886475], 'magnitude': 4.18842887878418, 'cosine_ionic_motion': 0.4698447287082672, 'motion_component_ionic': 1.9679112434387207, 'motion_component_percent_ionic': 46.98447287082672}], 'glu_contributions': [{'resid': 1073, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.7476274967193604, 'force': [16.813922882080078, 5.647915363311768, -6.918410301208496], 'magnitude': 19.038681030273438, 'cosine_with_motion': -0.7866051197052002, 'motion_component': -14.975923538208008, 'motion_component_percent': 78.66051197052002}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 4.11309289932251, 'force': [-14.870831489562988, 0.05484262481331825, 6.0873823165893555], 'magnitude': 16.06863021850586, 'cosine_with_motion': 0.9334647059440613, 'motion_component': 14.999499320983887, 'motion_component_percent': 93.34647059440613}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 3.0562846660614014, 'force': [-25.96455955505371, -12.964027404785156, 2.173342227935791], 'magnitude': 29.102367401123047, 'cosine_with_motion': 0.6662172675132751, 'motion_component': 19.388500213623047, 'motion_component_percent': 66.62172675132751}], 'asn_contributions': [{'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.204658508300781, 'force': [-1.6403664350509644, -3.485567331314087, 7.843697547912598], 'magnitude': 8.738625526428223, 'cosine_with_motion': 0.26755622029304504, 'motion_component': 2.33807373046875, 'motion_component_percent': 26.755622029304504}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.89402437210083, 'force': [2.018101692199707, 1.864999771118164, -4.957528591156006], 'magnitude': 5.668160915374756, 'cosine_with_motion': -0.43713414669036865, 'motion_component': -2.4777467250823975, 'motion_component_percent': 43.713414669036865}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.256622314453125, 'force': [1.1413710117340088, 6.642326354980469, -8.747842788696289], 'magnitude': 11.04300594329834, 'cosine_with_motion': -0.09305184334516525, 'motion_component': -1.0275720357894897, 'motion_component_percent': 9.305184334516525}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.769192218780518, 'force': [-0.895393431186676, -2.824409008026123, 2.9561948776245117], 'magnitude': 4.1854634284973145, 'cosine_with_motion': 0.144072487950325, 'motion_component': 0.6030101180076599, 'motion_component_percent': 14.407248795032501}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.04091739654541, 'force': [0.45013484358787537, -3.5115346908569336, 4.185803413391113], 'magnitude': 5.482193470001221, 'cosine_with_motion': -0.09486406296491623, 'motion_component': -0.5200631618499756, 'motion_component_percent': 9.486406296491623}]}, 4994: {'frame': 4994, 'motion_vector': [0.4574928283691406, 1.3063774108886719, 0.06430816650390625], 'ionic_force': [-15.226321399211884, -15.62778353691101, -3.6030957102775574], 'ionic_force_magnitude': 22.114492540550533, 'radial_force': 21.81899359797891, 'axial_force': -3.6030957102775574, 'glu_force': [-32.275760650634766, -17.716858863830566, 1.9284021854400635], 'glu_force_magnitude': 36.86910018656226, 'asn_force': [-0.4553137421607971, -1.938793420791626, 3.4184200763702393], 'asn_force_magnitude': 3.9562389147821286, 'residue_force': [-32.73107439279556, -19.655652284622192, 5.346822261810303], 'residue_force_magnitude': 38.55199613431296, 'total_force': [-47.957395792007446, -35.2834358215332, 1.7437265515327454], 'total_force_magnitude': 59.564026364996735, 'cosine_total_motion': -0.8229363407857939, 'cosine_glu_motion': -0.7396406325537873, 'cosine_asn_motion': -0.459916685487585, 'cosine_residue_motion': -0.7545504199319684, 'cosine_ionic_motion': -0.9011274841770078, 'motion_component_total': -49.017401899278966, 'motion_component_glu': -27.269884583677864, 'motion_component_asn': -1.819540288683597, 'motion_component_residue': -29.089424872361462, 'motion_component_ionic': -19.927977026917507, 'motion_component_percent_total': 82.29363407857939, 'motion_component_percent_glu': 73.96406325537873, 'motion_component_percent_asn': 45.991668548758504, 'motion_component_percent_residue': 75.45504199319683, 'motion_component_percent_ionic': 90.11274841770079, 'ionic_contributions': [{'ion_id': 1306, 'distance': 14.929139137268066, 'force': [-0.8425669074058533, -1.2280627489089966, -0.028977513313293457], 'magnitude': 1.4895961284637451, 'cosine_ionic_motion': -0.964909017086029, 'motion_component_ionic': -1.4373247623443604, 'motion_component_percent_ionic': 96.4909017086029}, {'ion_id': 1307, 'distance': 5.389379024505615, 'force': [-5.873695373535156, -9.419403076171875, -2.7254559993743896], 'magnitude': 11.430378913879395, 'cosine_ionic_motion': -0.9576418995857239, 'motion_component_ionic': -10.946209907531738, 'motion_component_percent_ionic': 95.76418995857239}, {'ion_id': 1309, 'distance': 13.295854568481445, 'force': [-0.9202994108200073, -0.567900538444519, -1.5354427099227905], 'magnitude': 1.8780431747436523, 'cosine_ionic_motion': -0.48482075333595276, 'motion_component_ionic': -0.9105142951011658, 'motion_component_percent_ionic': 48.482075333595276}, {'ion_id': 1316, 'distance': 9.752813339233398, 'force': [-1.8541682958602905, -1.3925756216049194, 2.6088037490844727], 'magnitude': 3.490424633026123, 'cosine_ionic_motion': -0.5168421268463135, 'motion_component_ionic': -1.8039984703063965, 'motion_component_percent_ionic': 51.68421268463135}, {'ion_id': 1320, 'distance': 9.194694519042969, 'force': [-2.610811948776245, -1.7711108922958374, -2.3384480476379395], 'magnitude': 3.927023410797119, 'cosine_ionic_motion': -0.6723389625549316, 'motion_component_ionic': -2.6402907371520996, 'motion_component_percent_ionic': 67.23389625549316}, {'ion_id': 1460, 'distance': 9.89516544342041, 'force': [-3.124779462814331, -1.2487306594848633, 0.41642481088638306], 'magnitude': 3.3907203674316406, 'cosine_ionic_motion': -0.6457740664482117, 'motion_component_ionic': -2.1896393299102783, 'motion_component_percent_ionic': 64.57740664482117}], 'glu_contributions': [{'resid': 1073, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 2.875811815261841, 'force': [22.783946990966797, 20.381959915161133, -10.526509284973145], 'magnitude': 32.33171463012695, 'cosine_with_motion': 0.8118846416473389, 'motion_component': 26.249622344970703, 'motion_component_percent': 81.18846416473389}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 2.790276288986206, 'force': [-29.792335510253906, -8.531960487365723, 16.085168838500977], 'magnitude': 34.9157600402832, 'cosine_with_motion': -0.49071186780929565, 'motion_component': -17.133577346801758, 'motion_component_percent': 49.071186780929565}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.6380455493927, 'force': [-25.267372131347656, -29.566858291625977, -3.6302573680877686], 'magnitude': 39.06172180175781, 'cosine_with_motion': -0.9314983487129211, 'motion_component': -36.385929107666016, 'motion_component_percent': 93.14983487129211}], 'asn_contributions': [{'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.933972358703613, 'force': [-0.4553137421607971, -1.938793420791626, 3.4184200763702393], 'magnitude': 3.9562387466430664, 'cosine_with_motion': -0.45991674065589905, 'motion_component': -1.8195403814315796, 'motion_component_percent': 45.991674065589905}]}, 4995: {'frame': 4995, 'motion_vector': [0.29911041259765625, -1.0097732543945312, -0.8112640380859375], 'ionic_force': [-16.513193786144257, -9.016636848449707, -1.008799159899354], 'ionic_force_magnitude': 18.841522890164374, 'radial_force': 18.814497311264375, 'axial_force': -1.008799159899354, 'glu_force': [-25.47502326965332, -17.447433471679688, 1.9919557571411133], 'glu_force_magnitude': 30.94119637435622, 'asn_force': [0.016815880313515663, 0.7998800724744797, 2.303154945373535], 'asn_force_magnitude': 2.438157830529244, 'residue_force': [-25.458207389339805, -16.647553399205208, 4.295110702514648], 'residue_force_magnitude': 30.71985243462085, 'total_force': [-41.97140117548406, -25.664190247654915, 3.2863115426152945], 'total_force_magnitude': 49.30566926080993, 'cosine_total_motion': 0.16316552908303641, 'cosine_glu_motion': 0.20378209048134185, 'cosine_asn_motion': -0.8241076025223907, 'cosine_residue_motion': 0.13984303095251502, 'cosine_ionic_motion': 0.19897692764627548, 'motion_component_total': 8.044985611733257, 'motion_component_glu': 6.305261679160026, 'motion_component_asn': -2.0093044042886485, 'motion_component_residue': 4.295957274871378, 'motion_component_ionic': 3.7490283368618798, 'motion_component_percent_total': 16.316552908303642, 'motion_component_percent_glu': 20.378209048134185, 'motion_component_percent_asn': 82.41076025223907, 'motion_component_percent_residue': 13.984303095251502, 'motion_component_percent_ionic': 19.897692764627546, 'ionic_contributions': [{'ion_id': 1306, 'distance': 12.820343971252441, 'force': [-1.3241117000579834, -1.5251678228378296, 0.027443215250968933], 'magnitude': 2.0199410915374756, 'cosine_ionic_motion': 0.41774290800094604, 'motion_component_ionic': 0.8438160419464111, 'motion_component_percent_ionic': 41.774290800094604}, {'ion_id': 1307, 'distance': 6.259469985961914, 'force': [-7.239418983459473, -4.05126953125, 1.7257643938064575], 'magnitude': 8.473502159118652, 'cosine_ionic_motion': 0.046644438058137894, 'motion_component_ionic': 0.39524173736572266, 'motion_component_percent_ionic': 4.664443805813789}, {'ion_id': 1309, 'distance': 12.917562484741211, 'force': [-0.9697037935256958, -0.4882330298423767, -1.6673376560211182], 'magnitude': 1.989651083946228, 'cosine_ionic_motion': 0.5881295800209045, 'motion_component_ionic': 1.1701726913452148, 'motion_component_percent_ionic': 58.812958002090454}, {'ion_id': 1316, 'distance': 13.020878791809082, 'force': [-0.7669690251350403, -0.3876888155937195, 1.759548544883728], 'magnitude': 1.9582020044326782, 'cosine_ionic_motion': -0.486089825630188, 'motion_component_ionic': -0.951862096786499, 'motion_component_percent_ionic': 48.6089825630188}, {'ion_id': 1320, 'distance': 8.06869125366211, 'force': [-3.7609140872955322, -1.9077779054641724, -2.8672845363616943], 'magnitude': 5.099550247192383, 'cosine_ionic_motion': 0.46135154366493225, 'motion_component_ionic': 2.3526854515075684, 'motion_component_percent_ionic': 46.135154366493225}, {'ion_id': 1460, 'distance': 11.43622875213623, 'force': [-2.4520761966705322, -0.6564997434616089, 0.013066878542304039], 'magnitude': 2.5384721755981445, 'cosine_ionic_motion': -0.024040281772613525, 'motion_component_ionic': -0.06102558597922325, 'motion_component_percent_ionic': 2.4040281772613525}], 'glu_contributions': [{'resid': 1073, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.393834114074707, 'force': [17.07512855529785, 13.89212417602539, -7.374588489532471], 'magnitude': 23.214988708496094, 'cosine_with_motion': -0.09519301354885101, 'motion_component': -2.209904670715332, 'motion_component_percent': 9.519301354885101}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 3.4763989448547363, 'force': [-18.829477310180664, -6.357393264770508, 10.535232543945312], 'magnitude': 22.49348258972168, 'cosine_with_motion': -0.2594912052154541, 'motion_component': -5.8368611335754395, 'motion_component_percent': 25.94912052154541}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.808281421661377, 'force': [-23.720674514770508, -24.98216438293457, -1.1686882972717285], 'magnitude': 34.46947479248047, 'cosine_with_motion': 0.41636916995048523, 'motion_component': 14.35202693939209, 'motion_component_percent': 41.63691699504852}], 'asn_contributions': [{'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.829130172729492, 'force': [-1.6747750043869019, -0.2213338166475296, 6.758659839630127], 'magnitude': 6.966587543487549, 'cosine_with_motion': -0.6219998598098755, 'motion_component': -4.333216667175293, 'motion_component_percent': 62.19998598098755}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.607299327850342, 'force': [1.7109771966934204, 2.448659896850586, -9.233780860900879], 'magnitude': 9.704951286315918, 'cosine_with_motion': 0.4286457896232605, 'motion_component': 4.15998649597168, 'motion_component_percent': 42.86457896232605}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.285283088684082, 'force': [-0.01938631199300289, -1.4274460077285767, 4.778275966644287], 'magnitude': 4.986972808837891, 'cosine_with_motion': -0.3681740462779999, 'motion_component': -1.8360739946365356, 'motion_component_percent': 36.81740462779999}]}, 4996: {'frame': 4996, 'motion_vector': [-0.20244598388671875, 1.0721435546875, 1.0912857055664062], 'ionic_force': [-3.4634814858436584, -24.222798764705658, -7.885996222496033], 'ionic_force_magnitude': 25.708532054931286, 'radial_force': 24.469157811379773, 'axial_force': -7.885996222496033, 'glu_force': [-29.198650360107422, -18.053829431533813, 4.87490177154541], 'glu_force_magnitude': 34.67371637533154, 'asn_force': [2.0548769496381283, 1.2744672298431396, -1.7439651489257812], 'asn_force_magnitude': 2.9813085111685216, 'residue_force': [-27.143773410469294, -16.779362201690674, 3.130936622619629], 'residue_force_magnitude': 32.06453172883219, 'total_force': [-30.607254896312952, -41.00216096639633, -4.755059599876404], 'total_force_magnitude': 51.38668940494732, 'cosine_total_motion': -0.5416623190440697, 'cosine_glu_motion': -0.15185225902643873, 'cosine_asn_motion': -0.20709014120287902, 'cosine_residue_motion': -0.18346382884156343, 'cosine_ionic_motion': -0.8538625053812476, 'motion_component_total': -27.834233351081092, 'motion_component_glu': -5.265282160436115, 'motion_component_asn': -0.6173996005472342, 'motion_component_residue': -5.882681760983349, 'motion_component_ionic': -21.951551590097743, 'motion_component_percent_total': 54.16623190440697, 'motion_component_percent_glu': 15.185225902643873, 'motion_component_percent_asn': 20.709014120287904, 'motion_component_percent_residue': 18.34638288415634, 'motion_component_percent_ionic': 85.38625053812477, 'ionic_contributions': [{'ion_id': 1306, 'distance': 13.125436782836914, 'force': [-1.1426242589950562, -1.551206111907959, -0.044628992676734924], 'magnitude': 1.9271279573440552, 'cosine_ionic_motion': -0.49783241748809814, 'motion_component_ionic': -0.9593867659568787, 'motion_component_percent_ionic': 49.783241748809814}, {'ion_id': 1307, 'distance': 4.0804619789123535, 'force': [3.4352829456329346, -19.294559478759766, -3.6758644580841064], 'magnitude': 19.939739227294922, 'cosine_ionic_motion': -0.8252533078193665, 'motion_component_ionic': -16.45533561706543, 'motion_component_percent_ionic': 82.52533078193665}, {'ion_id': 1309, 'distance': 13.257035255432129, 'force': [-0.8596774935722351, -0.5392806529998779, -1.5933207273483276], 'magnitude': 1.889057993888855, 'cosine_ionic_motion': -0.7350984215736389, 'motion_component_ionic': -1.388643503189087, 'motion_component_percent_ionic': 73.50984215736389}, {'ion_id': 1320, 'distance': 8.773033142089844, 'force': [-2.712550401687622, -1.9728121757507324, -2.712400197982788], 'magnitude': 4.313587188720703, 'cosine_ionic_motion': -0.6799253821372986, 'motion_component_ionic': -2.932917356491089, 'motion_component_percent_ionic': 67.99253821372986}, {'ion_id': 1460, 'distance': 11.878056526184082, 'force': [-2.1839122772216797, -0.864940345287323, 0.14021815359592438], 'magnitude': 2.353137493133545, 'cosine_ionic_motion': -0.09148188680410385, 'motion_component_ionic': -0.21526946127414703, 'motion_component_percent_ionic': 9.148188680410385}], 'glu_contributions': [{'resid': 1073, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.334083318710327, 'force': [18.76300621032715, 11.122505187988281, -10.14197826385498], 'magnitude': 24.054527282714844, 'cosine_with_motion': -0.07923884689807892, 'motion_component': -1.906053066253662, 'motion_component_percent': 7.923884689807892}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 3.643115997314453, 'force': [-17.8575382232666, -2.6054956912994385, 9.686452865600586], 'magnitude': 20.48188591003418, 'cosine_with_motion': 0.3604385256767273, 'motion_component': 7.382460594177246, 'motion_component_percent': 36.04385256767273}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.590609312057495, 'force': [-30.10411834716797, -26.570838928222656, 5.330427169799805], 'magnitude': 40.50531768798828, 'cosine_with_motion': -0.2651921212673187, 'motion_component': -10.741690635681152, 'motion_component_percent': 26.519212126731873}], 'asn_contributions': [{'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.199516296386719, 'force': [-2.6778736114501953, -1.6790857315063477, 8.165523529052734], 'magnitude': 8.755918502807617, 'cosine_with_motion': 0.5663769245147705, 'motion_component': 4.959150314331055, 'motion_component_percent': 56.63769245147705}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.779223442077637, 'force': [2.8431921005249023, 0.8961319923400879, -5.086368560791016], 'magnitude': 5.8955864906311035, 'cosine_with_motion': -0.5677671432495117, 'motion_component': -3.347320318222046, 'motion_component_percent': 56.77671432495117}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.50897216796875, 'force': [1.9459538459777832, 4.046713352203369, -8.996109008789062], 'magnitude': 10.054481506347656, 'cosine_with_motion': -0.3784928321838379, 'motion_component': -3.805549144744873, 'motion_component_percent': 37.84928321838379}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.489260196685791, 'force': [-0.056395385414361954, -1.9892923831939697, 4.1729888916015625], 'magnitude': 4.623234748840332, 'cosine_with_motion': 0.3409560024738312, 'motion_component': 1.576319694519043, 'motion_component_percent': 34.09560024738312}]}, 4997: {'frame': 4997, 'motion_vector': [-0.3025016784667969, -0.6528167724609375, -0.76025390625], 'ionic_force': [-12.324485659599304, -21.485591620206833, 0.6895290873944759], 'ionic_force_magnitude': 24.77900410440932, 'radial_force': 24.76940843144969, 'axial_force': 0.6895290873944759, 'glu_force': [-26.104713439941406, -19.13771677017212, 1.6138575077056885], 'glu_force_magnitude': 32.40852978788089, 'asn_force': [-0.256849005818367, 0.3470843434333801, 2.765280246734619], 'asn_force_magnitude': 2.7987879155497186, 'residue_force': [-26.361562445759773, -18.79063242673874, 4.379137754440308], 'residue_force_magnitude': 32.667976506830996, 'total_force': [-38.68604810535908, -40.27622404694557, 5.0686668418347836], 'total_force_magnitude': 56.07562683593853, 'cosine_total_motion': 0.5816715072487193, 'cosine_glu_motion': 0.5648982393926534, 'cosine_asn_motion': -0.768432407705826, 'cosine_residue_motion': 0.49457737544582775, 'cosine_ionic_motion': 0.6643024162853077, 'motion_component_total': 32.6175943815771, 'motion_component_glu': 18.307521418478274, 'motion_component_asn': -2.15067933660384, 'motion_component_residue': 16.156842081874434, 'motion_component_ionic': 16.46075229970267, 'motion_component_percent_total': 58.16715072487193, 'motion_component_percent_glu': 56.489823939265335, 'motion_component_percent_asn': 76.8432407705826, 'motion_component_percent_residue': 49.45773754458278, 'motion_component_percent_ionic': 66.43024162853078, 'ionic_contributions': [{'ion_id': 1306, 'distance': 12.2718505859375, 'force': [-1.535698652267456, -1.5813456773757935, -0.031177494674921036], 'magnitude': 2.2045400142669678, 'cosine_ionic_motion': 0.6589518785476685, 'motion_component_ionic': 1.452685832977295, 'motion_component_percent_ionic': 65.89518785476685}, {'ion_id': 1307, 'distance': 4.242607593536377, 'force': [-4.548783779144287, -17.15741729736328, 5.0139594078063965], 'magnitude': 18.444732666015625, 'cosine_ionic_motion': 0.4539732336997986, 'motion_component_ionic': 8.373414993286133, 'motion_component_percent_ionic': 45.39732336997986}, {'ion_id': 1309, 'distance': 12.592719078063965, 'force': [-1.0400985479354858, -0.5203492045402527, -1.7408907413482666], 'magnitude': 2.093625783920288, 'cosine_ionic_motion': 0.9025148153305054, 'motion_component_ionic': 1.8895282745361328, 'motion_component_percent_ionic': 90.25148153305054}, {'ion_id': 1320, 'distance': 8.438592910766602, 'force': [-3.253243923187256, -1.7816591262817383, -2.824697256088257], 'magnitude': 4.662276268005371, 'cosine_ionic_motion': 0.8800268173217773, 'motion_component_ionic': 4.102928161621094, 'motion_component_percent_ionic': 88.00268173217773}, {'ion_id': 1460, 'distance': 12.835030555725098, 'force': [-1.9466607570648193, -0.4448203146457672, 0.2723351716995239], 'magnitude': 2.0153212547302246, 'cosine_ionic_motion': 0.3186562657356262, 'motion_component_ionic': 0.6421947479248047, 'motion_component_percent_ionic': 31.865626573562622}], 'glu_contributions': [{'resid': 1073, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.519207239151001, 'force': [15.38404655456543, 13.974355697631836, -5.8474297523498535], 'magnitude': 21.59036636352539, 'cosine_with_motion': -0.41287946701049805, 'motion_component': -8.91421890258789, 'motion_component_percent': 41.287946701049805}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 3.6334826946258545, 'force': [-17.216053009033203, -7.235029697418213, 8.673872947692871], 'magnitude': 20.590633392333984, 'cosine_with_motion': 0.1548129916191101, 'motion_component': 3.187697410583496, 'motion_component_percent': 15.48129916191101}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.7672173976898193, 'force': [-24.272706985473633, -25.877042770385742, -1.212585687637329], 'magnitude': 35.500083923339844, 'cosine_with_motion': 0.6770136952400208, 'motion_component': 24.034042358398438, 'motion_component_percent': 67.70136952400208}], 'asn_contributions': [{'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.68773078918457, 'force': [-1.9383807182312012, -0.6893336176872253, 7.022111892700195], 'magnitude': 7.317277908325195, 'cosine_with_motion': -0.5616996884346008, 'motion_component': -4.11011266708374, 'motion_component_percent': 56.16996884346008}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.708172798156738, 'force': [1.9283785820007324, 2.883417844772339, -8.698851585388184], 'magnitude': 9.364975929260254, 'cosine_with_motion': 0.4231140613555908, 'motion_component': 3.9624528884887695, 'motion_component_percent': 42.31140613555908}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.377700328826904, 'force': [-0.24684686958789825, -1.8469998836517334, 4.442019939422607], 'magnitude': 4.817040920257568, 'cosine_with_motion': -0.4158194661140442, 'motion_component': -2.003019332885742, 'motion_component_percent': 41.58194661140442}]}, 4998: {'frame': 4998, 'motion_vector': [1.2956390380859375, -1.7068977355957031, 0.36876678466796875], 'ionic_force': [-8.595291793346405, -8.897465407848358, -3.6955340802669525], 'ionic_force_magnitude': 12.91127041909667, 'radial_force': 12.371092582978521, 'axial_force': -3.6955340802669525, 'glu_force': [-24.26844882965088, -17.303970336914062, 4.667385101318359], 'glu_force_magnitude': 30.16901525907323, 'asn_force': [-0.7594750616699457, 0.1303102970123291, 3.0745785236358643], 'asn_force_magnitude': 3.1696713143177635, 'residue_force': [-25.027923891320825,</t>
         </is>
       </c>
     </row>
@@ -611,7 +611,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>{5173: {'frame': 5173, 'ionic_force': [-0.03178515285253525, 10.060459554195404, -0.028999194502830505], 'ionic_force_magnitude': 10.06055155997052, 'motion_vector': [-0.32863616943359375, 0.4364585876464844, -0.3377685546875], 'ionic_force_x': -0.03178515285253525, 'ionic_force_y': 10.060459554195404, 'ionic_force_z': -0.028999194502830505, 'radial_force': 10.060509765292386, 'axial_force': -0.028999194502830505, 'glu_force': [-6.758579730987549, 7.259679794311523, 1.6593886613845825], 'glu_force_magnitude': 10.056585972664006, 'asn_force': [-7.390199303627014, -2.865291476249695, 7.459710121154785], 'asn_force_magnitude': 10.884494296147043, 'residue_force': [-14.148779034614563, 4.394388318061829, 9.119098782539368], 'residue_force_magnitude': 17.397027316929115, 'total_force': [-14.180564187467098, 14.454847872257233, 9.090099588036537], 'total_force_magnitude': 22.195966710314643, 'motion_component_total': 12.297202498985062, 'cosine_total_motion': 0.5540286962707712, 'cosine_glu_motion': 0.7475932094883707, 'cosine_asn_motion': -0.19188523890942097, 'cosine_residue_motion': 0.31210283782744785, 'cosine_ionic_motion': 0.6826207154421637, 'motion_component_glu': 7.518235383799613, 'motion_component_asn': -2.088573788424405, 'motion_component_residue': 5.429661595375208, 'motion_component_ionic': 6.867540903609853, 'ionic_contributions': [{'ion_id': 1306, 'distance': 12.007840156555176, 'force': [-1.142738938331604, 1.9904721975326538, -0.18408028781414032], 'magnitude': 2.3025457859039307}, {'ion_id': 1307, 'distance': 7.160901069641113, 'force': [0.9537079930305481, 3.515716075897217, 5.352444171905518], 'magnitude': 6.474447727203369}, {'ion_id': 1308, 'distance': 11.22840404510498, 'force': [0.7354629039764404, 2.4643869400024414, -0.565873920917511], 'magnitude': 2.633310079574585}, {'ion_id': 1309, 'distance': 9.778471946716309, 'force': [-0.48083266615867615, 1.5299593210220337, -3.0795645713806152], 'magnitude': 3.4721310138702393}, {'ion_id': 1403, 'distance': 14.173266410827637, 'force': [-0.09738444536924362, 0.5599250197410583, -1.5519245862960815], 'magnitude': 1.652715802192688}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 5.199153900146484, 'force': [-6.758579730987549, 7.259679794311523, 1.6593886613845825], 'magnitude': 10.056586265563965}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.7128424644470215, 'force': [4.685451984405518, 0.9295059442520142, 9.52723503112793], 'magnitude': 10.6576566696167}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.261452674865723, 'force': [-2.8056347370147705, -2.153184175491333, -6.171500205993652], 'magnitude': 7.113030433654785}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.9321959018707275, 'force': [-4.595969200134277, 0.7100307941436768, -19.178930282592773], 'magnitude': 19.73470115661621}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.785325765609741, 'force': [0.3094111680984497, 1.22603440284729, 9.639676094055176], 'magnitude': 9.72225570678711}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 3.5840225219726562, 'force': [2.689281940460205, -3.0791029930114746, 10.045012474060059], 'magnitude': 10.845063209533691}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.799994468688965, 'force': [-3.7066445350646973, 0.42509329319000244, 1.7969428300857544], 'magnitude': 4.141125679016113}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.5933098793029785, 'force': [-3.9660959243774414, -0.9236687421798706, 1.8012741804122925], 'magnitude': 4.452826976776123}]}, 5174: {'frame': 5174, 'ionic_force': [-0.6643470674753189, 10.092601358890533, -2.0427508652210236], 'ionic_force_magnitude': 10.318662234655388, 'motion_vector': [-2.1065216064453125, -0.9170722961425781, 2.1868057250976562], 'ionic_force_x': -0.6643470674753189, 'ionic_force_y': 10.092601358890533, 'ionic_force_z': -2.0427508652210236, 'radial_force': 10.114443099624522, 'axial_force': -2.0427508652210236, 'glu_force': [-7.780902862548828, 6.3519370555877686, 1.3226341009140015], 'glu_force_magnitude': 10.131086549796628, 'asn_force': [-7.848422586917877, -0.6536328196525574, 8.752897500991821], 'asn_force_magnitude': 11.774471861983386, 'residue_force': [-15.629325449466705, 5.698304235935211, 10.075531601905823], 'residue_force_magnitude': 19.44897997920785, 'total_force': [-16.293672516942024, 15.790905594825745, 8.0327807366848], 'total_force_magnitude': 24.069940381266118, 'motion_component_total': 11.793688128885574, 'cosine_total_motion': 0.4899757931292893, 'cosine_glu_motion': 0.4187999273624166, 'cosine_asn_motion': 0.9712541380581925, 'cosine_residue_motion': 0.8061555334685936, 'cosine_ionic_motion': -0.37652310089423896, 'motion_component_glu': 4.242898311157184, 'motion_component_asn': 11.436004519401115, 'motion_component_residue': 15.678902830558298, 'motion_component_ionic': -3.885214701672724, 'ionic_contributions': [{'ion_id': 1306, 'distance': 12.4862642288208, 'force': [-0.6169819831848145, 2.007314682006836, -0.35312172770500183], 'magnitude': 2.1294772624969482}, {'ion_id': 1307, 'distance': 7.873819828033447, 'force': [0.5131598114967346, 2.890629529953003, 4.478611946105957], 'magnitude': 5.3550944328308105}, {'ion_id': 1308, 'distance': 11.81053352355957, 'force': [0.4955497980117798, 2.235003709793091, -0.6512793898582458], 'magnitude': 2.3801209926605225}, {'ion_id': 1309, 'distance': 8.462942123413086, 'force': [-0.8381993174552917, 2.3942766189575195, -3.879767417907715], 'magnitude': 4.635486602783203}, {'ion_id': 1403, 'distance': 13.790569305419922, 'force': [-0.2178753763437271, 0.5653768181800842, -1.637194275856018], 'magnitude': 1.7457164525985718}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 5.600811004638672, 'force': [6.262893199920654, -5.221066474914551, -2.4852945804595947], 'magnitude': 8.524086952209473}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 5.847188949584961, 'force': [-6.818350791931152, 3.4854533672332764, 2.1401119232177734], 'magnitude': 7.950997829437256}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 4.977415561676025, 'force': [-7.22544527053833, 8.087550163269043, 1.6678167581558228], 'magnitude': 10.972562789916992}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.760137557983398, 'force': [3.6300151348114014, 2.7228000164031982, 9.4099760055542], 'magnitude': 10.446928024291992}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.740535736083984, 'force': [-1.890036940574646, -2.368476390838623, -5.150002479553223], 'magnitude': 5.975319862365723}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.941314697265625, 'force': [-2.2430100440979004, -4.7319841384887695, -18.932613372802734], 'magnitude': 19.64348793029785}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.324524879455566, 'force': [-0.5797222256660461, 2.653454542160034, 6.936166286468506], 'magnitude': 7.44897985458374}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 3.2011022567749023, 'force': [1.3044353723526, 0.6891797184944153, 13.514564514160156], 'magnitude': 13.594850540161133}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.879083156585693, 'force': [-3.7527353763580322, 0.8021993637084961, 1.2320884466171265], 'magnitude': 4.030457496643066}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.458897590637207, 'force': [-4.317368507385254, -0.4208059310913086, 1.7427181005477905], 'magnitude': 4.674806594848633}]}, 5175: {'frame': 5175, 'ionic_force': [-4.48947374522686, 8.996800035238266, -3.1096643209457397], 'ionic_force_magnitude': 10.524628144124973, 'motion_vector': [0.8205947875976562, 1.4489250183105469, -0.349456787109375], 'ionic_force_x': -4.48947374522686, 'ionic_force_y': 8.996800035238266, 'ionic_force_z': -3.1096643209457397, 'radial_force': 10.05473944879451, 'axial_force': -3.1096643209457397, 'glu_force': [-12.236773014068604, 14.97885513305664, -4.509521113708615], 'glu_force_magnitude': 19.860526064782842, 'asn_force': [-1.377406358718872, -0.5415080785751343, 3.917880058288574], 'asn_force_magnitude': 4.18810976782326, 'residue_force': [-13.614179372787476, 14.437347054481506, -0.5916410554200411], 'residue_force_magnitude': 19.85278089095924, 'total_force': [-18.103653118014336, 23.434147089719772, -3.701305376365781], 'total_force_magnitude': 29.842941670169278, 'motion_component_total': 11.985183039674084, 'cosine_total_motion': 0.4016086340326952, 'cosine_glu_motion': 0.3917474294886923, 'cosine_asn_motion': -0.4608646553582442, 'cosine_residue_motion': 0.2946770178723724, 'cosine_ionic_motion': 0.5829208107155092, 'motion_component_glu': 7.780310034171852, 'motion_component_asn': -1.930151764750363, 'motion_component_residue': 5.850158269421489, 'motion_component_ionic': 6.135024770252594, 'ionic_contributions': [{'ion_id': 1306, 'distance': 12.98525619506836, 'force': [-1.0581152439117432, 1.6551977396011353, 0.1323573887348175], 'magnitude': 1.9689606428146362}, {'ion_id': 1307, 'distance': 10.564190864562988, 'force': [-0.3703985810279846, 0.40683475136756897, 2.9235332012176514], 'magnitude': 2.974853992462158}, {'ion_id': 1308, 'distance': 9.630842208862305, 'force': [0.23377586901187897, 3.548218250274658, -0.4093410074710846], 'magnitude': 3.5793943405151367}, {'ion_id': 1309, 'distance': 7.792961597442627, 'force': [-2.680544376373291, 2.8133533000946045, -3.845205307006836], 'magnitude': 5.466797828674316}, {'ion_id': 1403, 'distance': 12.611123085021973, 'force': [-0.6141914129257202, 0.5731959939002991, -1.911008596420288], 'magnitude': 2.087519645690918}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.8696460723876953, 'force': [9.367057800292969, -15.202912330627441, 0.016476763412356377], 'magnitude': 17.85694694519043}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 3.822664499282837, 'force': [-14.11198616027832, 12.011738777160645, 1.6255600452423096], 'magnitude': 18.603023529052734}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 3.633172035217285, 'force': [-7.491844654083252, 18.170028686523438, -6.151557922363281], 'magnitude': 20.594158172607422}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.767369270324707, 'force': [-1.377406358718872, -0.5415080785751343, 3.917880058288574], 'magnitude': 4.188109874725342}]}, 5176: {'frame': 5176, 'ionic_force': [-1.6972591429948807, 9.394513070583344, -1.1074041053652763], 'ionic_force_magnitude': 9.610614355202319, 'motion_vector': [-0.2884254455566406, 1.5469932556152344, -1.362060546875], 'ionic_force_x': -1.6972591429948807, 'ionic_force_y': 9.394513070583344, 'ionic_force_z': -1.1074041053652763, 'radial_force': 9.546599626665035, 'axial_force': -1.1074041053652763, 'glu_force': [-19.01718759536743, 20.73361301422119, -1.6225908994674683], 'glu_force_magnitude': 28.1810030674551, 'asn_force': [-0.6952297687530518, -0.1736546754837036, 0.5019161701202393], 'asn_force_magnitude': 0.8748829747491611, 'residue_force': [-19.712417364120483, 20.559958338737488, -1.120674729347229], 'residue_force_magnitude': 28.505213506951623, 'total_force': [-21.409676507115364, 29.95447140932083, -2.2280788347125053], 'total_force_magnitude': 36.88643301872439, 'motion_component_total': 26.69037067059993, 'cosine_total_motion': 0.7235823170283582, 'cosine_glu_motion': 0.678069463817084, 'cosine_asn_motion': -0.4128632695551034, 'cosine_residue_motion': 0.6576856752808345, 'cosine_ionic_motion': 0.8264716263384885, 'motion_component_glu': 19.10867763977688, 'motion_component_asn': -0.3612070454330336, 'motion_component_residue': 18.747470594343845, 'motion_component_ionic': 7.942900076256084, 'ionic_contributions': [{'ion_id': 1306, 'distance': 14.89237117767334, 'force': [-0.5284325480461121, 1.4004030227661133, 0.022839702665805817], 'magnitude': 1.4969606399536133}, {'ion_id': 1307, 'distance': 8.6985502243042, 'force': [-0.19438980519771576, 2.0637528896331787, 3.8672609329223633], 'magnitude': 4.387775421142578}, {'ion_id': 1308, 'distance': 10.563375473022461, 'force': [0.5721141695976257, 2.9097232818603516, -0.24224546551704407], 'magnitude': 2.9753129482269287}, {'ion_id': 1309, 'distance': 9.11813735961914, 'force': [-1.1644694805145264, 2.285262107849121, -3.060650587081909], 'magnitude': 3.99324369430542}, {'ion_id': 1403, 'distance': 13.266416549682617, 'force': [-0.3820814788341522, 0.7353717684745789, -1.6946086883544922], 'magnitude': 1.8863871097564697}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.7171125411987305, 'force': [11.659213066101074, -15.12153434753418, -3.1501314640045166], 'magnitude': 19.352554321289062}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 2.8986754417419434, 'force': [-25.04872703552246, 20.474231719970703, -0.30672621726989746], 'magnitude': 32.3531608581543}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 4.061368465423584, 'force': [-5.627673625946045, 15.380915641784668, 1.8342667818069458], 'magnitude': 16.480527877807617}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.233702182769775, 'force': [1.5910654067993164, -1.8462071418762207, -10.870063781738281], 'magnitude': 11.13994026184082}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.719921112060547, 'force': [-1.17593252658844, 1.0421768426895142, 3.9573471546173096], 'magnitude': 4.257880687713623}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.302978038787842, 'force': [-1.1103626489639282, 0.6303756237030029, 7.414632797241211], 'magnitude': 7.52376651763916}]}, 5177: {'frame': 5177, 'ionic_force': [-1.3824736773967743, 8.549700021743774, -0.875838428735733], 'ionic_force_magnitude': 8.70492371498744, 'motion_vector': [1.0473556518554688, -0.16293716430664062, -0.0436553955078125], 'ionic_force_x': -1.3824736773967743, 'ionic_force_y': 8.549700021743774, 'ionic_force_z': -0.875838428735733, 'radial_force': 8.660750771757634, 'axial_force': -0.875838428735733, 'glu_force': [-25.912687301635742, 22.428939819335938, 8.468029022216797], 'glu_force_magnitude': 35.30201439199828, 'asn_force': [0.774412602186203, 1.5036826133728027, 2.5479869842529297], 'asn_force_magnitude': 3.058269764443092, 'residue_force': [-25.13827469944954, 23.93262243270874, 11.016016006469727], 'residue_force_magnitude': 36.415050185690745, 'total_force': [-26.520748376846313, 32.482322454452515, 10.140177577733994], 'total_force_magnitude': 43.142491441860486, 'motion_component_total': -31.58959986054271, 'cosine_total_motion': -0.7322154749248397, 'cosine_glu_motion': -0.832143931429355, 'cosine_asn_motion': 0.14019541199527244, 'cosine_residue_motion': -0.7949351025551864, 'cosine_ionic_motion': -0.3035061872029496, 'motion_component_glu': -29.37635704353312, 'motion_component_asn': 0.4287553896187841, 'motion_component_residue': -28.947601653914333, 'motion_component_ionic': -2.6419982066283736, 'ionic_contributions': [{'ion_id': 1307, 'distance': 8.939340591430664, 'force': [-0.45594823360443115, 2.804142475128174, 3.031407594680786], 'magnitude': 4.154580116271973}, {'ion_id': 1308, 'distance': 11.303756713867188, 'force': [0.689740777015686, 2.4730772972106934, -0.39926019310951233], 'magnitude': 2.5983190536499023}, {'ion_id': 1309, 'distance': 9.676535606384277, 'force': [-1.2035044431686401, 2.5528600215911865, -2.146219491958618], 'magnitude': 3.5456700325012207}, {'ion_id': 1403, 'distance': 14.429394721984863, 'force': [-0.41276177763938904, 0.7196202278137207, -1.3617663383483887], 'magnitude': 1.594563603401184}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.2737128734588623, 'force': [17.63517189025879, -13.619305610656738, -11.225502967834473], 'magnitude': 24.94988441467285}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 2.769817352294922, 'force': [-32.05121612548828, 13.869439125061035, 5.990726470947266], 'magnitude': 35.433467864990234}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 3.0888047218322754, 'force': [-11.49664306640625, 22.17880630493164, 13.702805519104004], 'magnitude': 28.49279022216797}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.723537921905518, 'force': [0.3901461064815521, 4.517452716827393, 5.626331806182861], 'magnitude': 7.226008892059326}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.737008094787598, 'force': [1.5527937412261963, -5.17930793762207, -7.531026363372803], 'magnitude': 9.271071434020996}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.232869625091553, 'force': [-1.1685272455215454, 2.1655378341674805, 4.452681541442871], 'magnitude': 5.087374687194824}]}, 5178: {'frame': 5178, 'ionic_force': [-1.344180654734373, 9.261112630367279, -1.605331540107727], 'ionic_force_magnitude': 9.494846925494645, 'motion_vector': [-0.499969482421875, -1.2579994201660156, 0.6877059936523438], 'ionic_force_x': -1.344180654734373, 'ionic_force_y': 9.261112630367279, 'ionic_force_z': -1.605331540107727, 'radial_force': 9.358153064836591, 'axial_force': -1.605331540107727, 'glu_force': [-16.422406673431396, 21.141526222229004, 4.929273366928101], 'glu_force_magnitude': 27.220530999204758, 'asn_force': [-0.13263589143753052, -2.4197518825531006, -2.994140148162842], 'asn_force_magnitude': 3.8519691950556028, 'residue_force': [-16.555042564868927, 18.721774339675903, 1.9351332187652588], 'residue_force_magnitude': 25.066292293132182, 'total_force': [-17.8992232196033, 27.982886970043182, 0.32980167865753174], 'total_force_magnitude': 33.21946604312965, 'motion_component_total': -17.14104347223333, 'cosine_total_motion': -0.5159939491495346, 'cosine_glu_motion': -0.36281276984807215, 'cosine_asn_motion': 0.17974320918784045, 'cosine_residue_motion': -0.36637213179952305, 'cosine_ionic_motion': -0.8380811813955584, 'motion_component_glu': -9.87595624855679, 'motion_component_asn': 0.6923653048119967, 'motion_component_residue': -9.183590943744793, 'motion_component_ionic': -7.957452528488538, 'ionic_contributions': [{'ion_id': 1306, 'distance': 14.052817344665527, 'force': [-0.6633750796318054, 1.5338643789291382, -0.1830899715423584], 'magnitude': 1.681168794631958}, {'ion_id': 1307, 'distance': 9.598557472229004, 'force': [0.008810419589281082, 2.18619704246521, 2.864572048187256], 'magnitude': 3.603513479232788}, {'ion_id': 1308, 'distance': 12.033468246459961, 'force': [0.52821284532547, 2.203639030456543, -0.34880292415618896], 'magnitude': 2.2927489280700684}, {'ion_id': 1309, 'distance': 9.426063537597656, 'force': [-0.9532740116119385, 2.5756494998931885, -2.5336785316467285], 'magnitude': 3.7366065979003906}, {'ion_id': 1403, 'distance': 14.318366050720215, 'force': [-0.26455482840538025, 0.7617626786231995, -1.404332160949707], 'magnitude': 1.6193888187408447}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.7478668689727783, 'force': [12.879548072814941, -12.15123462677002, -6.988813400268555], 'magnitude': 19.0362491607666}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 3.1079115867614746, 'force': [-21.525930404663086, 18.075557708740234, 1.4024779796600342], 'magnitude': 28.143531799316406}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 3.6807591915130615, 'force': [-7.776024341583252, 15.217203140258789, 10.515608787536621], 'magnitude': 20.06509017944336}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.4385528564453125, 'force': [0.3637133538722992, -4.931046485900879, -9.054475784301758], 'magnitude': 10.31654167175293}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.601647853851318, 'force': [-0.4963492453098297, 2.5112946033477783, 6.060335636138916], 'magnitude': 6.57880163192749}]}, 5179: {'frame': 5179, 'ionic_force': [-2.9875034540891647, 9.438717722892761, -3.671563595533371], 'ionic_force_magnitude': 10.559116836965606, 'motion_vector': [0.006259918212890625, 2.1265487670898438, -1.1589584350585938], 'ionic_force_x': -2.9875034540891647, 'ionic_force_y': 9.438717722892761, 'ionic_force_z': -3.671563595533371, 'radial_force': 9.90023076198957, 'axial_force': -3.671563595533371, 'glu_force': [-23.799495220184326, 22.224249839782715, -1.1507561802864075], 'glu_force_magnitude': 32.58308600275802, 'asn_force': [0.31184569001197815, 1.3416973948478699, 8.548349380493164], 'asn_force_magnitude': 8.658618640678112, 'residue_force': [-23.487649530172348, 23.565947234630585, 7.397593200206757], 'residue_force_magnitude': 34.08442363710062, 'total_force': [-26.475152984261513, 33.004664957523346, 3.7260296046733856], 'total_force_magnitude': 42.47499183182174, 'motion_component_total': 27.12866424526647, 'cosine_total_motion': 0.6386973387230179, 'cosine_glu_motion': 0.6139209778471686, 'cosine_asn_motion': -0.3362918949524588, 'cosine_residue_motion': 0.501449487065499, 'cosine_ionic_motion': 0.9505574803738571, 'motion_component_glu': 20.0034400200916, 'motion_component_asn': -2.911823270344325, 'motion_component_residue': 17.091616749747274, 'motion_component_ionic': 10.037047495519198, 'ionic_contributions': [{'ion_id': 1306, 'distance': 11.857600212097168, 'force': [-0.7968317866325378, 2.22175669670105, 0.06649583578109741], 'magnitude': 2.3612635135650635}, {'ion_id': 1307, 'distance': 13.191850662231445, 'force': [-0.160544291138649, 0.86920565366745, 1.6906518936157227], 'magnitude': 1.9077726602554321}, {'ion_id': 1308, 'distance': 11.75716495513916, 'force': [0.29383471608161926, 2.3622288703918457, -0.319489985704422], 'magnitude': 2.401777982711792}, {'ion_id': 1309, 'distance': 8.050174713134766, 'force': [-1.8343040943145752, 3.2689404487609863, -3.492114543914795], 'magnitude': 5.123036861419678}, {'ion_id': 1403, 'distance': 13.449821472167969, 'force': [-0.489657998085022, 0.7165860533714294, -1.6171067953109741], 'magnitude': 1.8352915048599243}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.613638401031494, 'force': [13.778266906738281, -14.792187690734863, -3.262894868850708], 'magnitude': 20.476716995239258}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 2.716130256652832, 'force': [-30.349185943603516, 20.880599975585938, -0.8410678505897522], 'magnitude': 36.84806442260742}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 3.8941898345947266, 'force': [-7.228576183319092, 16.13583755493164, 2.9532065391540527], 'magnitude': 17.925931930541992}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.184726238250732, 'force': [1.2996680736541748, 2.6859867572784424, 8.284985542297363], 'magnitude': 8.805943489074707}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.05418586730957, 'force': [-0.11354377865791321, -5.14473819732666, -17.837482452392578], 'magnitude': 18.564939498901367}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.1461873054504395, 'force': [-1.6079875230789185, 3.2112555503845215, 7.264286041259766], 'magnitude': 8.103557586669922}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 3.5787012577056885, 'force': [0.733708918094635, 0.5891932845115662, 10.836560249328613], 'magnitude': 10.877339363098145}]}, 5180: {'frame': 5180, 'ionic_force': [-0.47080206871032715, 4.05627167224884, -2.3710789382457733], 'ionic_force_magnitude': 4.721970965432023, 'motion_vector': [0.3277015686035156, -0.06797409057617188, 1.3685455322265625], 'ionic_force_x': -0.47080206871032715, 'ionic_force_y': 4.05627167224884, 'ionic_force_z': -2.3710789382457733, 'radial_force': 4.083502720335855, 'axial_force': -2.3710789382457733, 'glu_force': [-25.0678653717041, 16.978437423706055, 15.715483665466309], 'glu_force_magnitude': 34.112191933150854, 'asn_force': [-0.317492350935936, 4.530882358551025, 6.887574195861816], 'asn_force_magnitude': 8.250356031313634, 'residue_force': [-25.385357722640038, 21.50931978225708, 22.603057861328125], 'residue_force_magnitude': 40.22394124006676, 'total_force': [-25.856159791350365, 25.56559145450592, 20.23197892308235], 'total_force_magnitude': 41.610977358367805, 'motion_component_total': 12.40528550877519, 'cosine_total_motion': 0.2981253096253106, 'cosine_glu_motion': 0.25257051941981307, 'cosine_asn_motion': 0.7754781064382247, 'cosine_residue_motion': 0.3732529445114025, 'cosine_ionic_motion': -0.5524004738759996, 'motion_component_glu': 8.615734035104268, 'motion_component_asn': 6.397970472604284, 'motion_component_residue': 15.013704507708551, 'motion_component_ionic': -2.6084189989333604, 'ionic_contributions': [{'ion_id': 1308, 'distance': 13.69267463684082, 'force': [0.32464051246643066, 1.7187424898147583, -0.2759523093700409], 'magnitude': 1.770767331123352}, {'ion_id': 1309, 'distance': 10.125423431396484, 'force': [-0.7954425811767578, 2.337529182434082, -2.0951266288757324], 'magnitude': 3.238259792327881}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.236091136932373, 'force': [19.283445358276367, -9.734607696533203, -13.613936424255371], 'magnitude': 25.53337287902832}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 3.0544145107269287, 'force': [-27.631637573242188, 3.6904678344726562, 8.479211807250977], 'magnitude': 29.138015747070312}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.776036262512207, 'force': [-16.71967315673828, 23.0225772857666, 20.850208282470703], 'magnitude': 35.27488708496094}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.677863597869873, 'force': [0.23208953440189362, 4.414318561553955, 5.863074779510498], 'magnitude': 7.3427324295043945}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.794473171234131, 'force': [2.0497195720672607, -7.793473243713379, -10.548626899719238], 'magnitude': 13.274528503417969}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.327760696411133, 'force': [-1.5611531734466553, 2.8427305221557617, 3.6834611892700195], 'magnitude': 4.907769680023193}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 3.8427014350891113, 'force': [-1.038148283958435, 5.0673065185546875, 7.889665126800537], 'magnitude': 9.43409538269043}]}, 5181: {'frame': 5181, 'ionic_force': [-0.8457868248224258, 6.44456821680069, -2.367974877357483], 'ionic_force_magnitude': 6.917739506069667, 'motion_vector': [-0.3796195983886719, -1.8383750915527344, -0.54205322265625], 'ionic_force_x': -0.8457868248224258, 'ionic_force_y': 6.44456821680069, 'ionic_force_z': -2.367974877357483, 'radial_force': 6.4998319096758825, 'axial_force': -2.367974877357483, 'glu_force': [-26.373924255371094, 25.822315216064453, 1.338186264038086], 'glu_force_magnitude': 36.93462584382175, 'asn_force': [-0.8362669944763184, 2.2442076206207275, 3.8984904289245605], 'asn_force_magnitude': 4.575372985333437, 'residue_force': [-27.210191249847412, 28.06652283668518, 5.2366766929626465], 'residue_force_magnitude': 39.44042335956932, 'total_force': [-28.055978074669838, 34.51109105348587, 2.8687018156051636], 'total_force_magnitude': 44.5688541644858, 'motion_component_total': -27.816125757040833, 'cosine_total_motion': -0.624115792934291, 'cosine_glu_motion': -0.5291267397122088, 'cosine_asn_motion': -0.6623793528239298, 'cosine_residue_motion': -0.5723501126340709, 'cosine_ionic_motion': -0.7578190824121356, 'motion_component_glu': -19.54309815523169, 'motion_component_asn': -3.0306325969532537, 'motion_component_residue': -22.573730752184943, 'motion_component_ionic': -5.242395004855895, 'ionic_contributions': [{'ion_id': 1307, 'distance': 13.534213066101074, 'force': [-0.15910173952579498, 1.1764719486236572, 1.3695497512817383], 'magnitude': 1.8124750852584839}, {'ion_id': 1308, 'distance': 13.662712097167969, 'force': [0.3693566620349884, 1.7314714193344116, -0.16969358921051025], 'magnitude': 1.7785425186157227}, {'ion_id': 1309, 'distance': 9.666790008544922, 'force': [-0.789997935295105, 2.699798583984375, -2.170147180557251], 'magnitude': 3.5528225898742676}, {'ion_id': 1403, 'distance': 14.182221412658691, 'force': [-0.2660438120365143, 0.8368262648582458, -1.39768385887146], 'magnitude': 1.6506295204162598}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 2.99792218208313, 'force': [24.841527938842773, -15.354774475097656, -5.681687355041504], 'magnitude': 29.751506805419922}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 2.7962822914123535, 'force': [-31.13483238220215, 13.418130874633789, -7.697152137756348], 'magnitude': 34.765933990478516}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.700066328048706, 'force': [-20.08061981201172, 27.75895881652832, 14.717025756835938], 'magnitude': 37.28782653808594}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.5178961753845215, 'force': [-0.8362669944763184, 2.2442076206207275, 3.8984904289245605], 'magnitude': 4.57537317276001}]}, 5182: {'frame': 5182, 'ionic_force': [-2.513504236936569, 7.566243886947632, -3.646450847387314], 'ionic_force_magnitude': 8.767117764024967, 'motion_vector': [3.399822235107422, 1.0570564270019531, -0.6069412231445312], 'ionic_force_x': -2.513504236936569, 'ionic_force_y': 7.566243886947632, 'ionic_force_z': -3.646450847387314, 'radial_force': 7.972813186439934, 'axial_force': -3.646450847387314, 'glu_force': [-11.87851095199585, 24.449152946472168, -2.7236955165863037], 'glu_force_magnitude': 27.318100583747515, 'asn_force': [0.09131675958633423, 1.8928513526916504, 6.783854246139526], 'asn_force_magnitude': 7.043571780484191, 'residue_force': [-11.787194192409515, 26.34200429916382, 4.060158729553223], 'residue_force_magnitude': 29.143164315768885, 'total_force': [-14.300698429346085, 33.90824818611145, 0.4137078821659088], 'total_force_magnitude': 36.80285892196146, 'motion_component_total': -3.6071427110328105, 'cosine_total_motion': -0.09801256795515718, 'cosine_glu_motion': -0.1306189387689052, 'cosine_asn_motion': -0.07099568140915338, 'cosine_residue_motion': -0.13959789820557564, 'cosine_ionic_motion': 0.05260357929725482, 'motion_component_glu': -3.5682613074313103, 'motion_component_asn': -0.5000631781097589, 'motion_component_residue': -4.068324485541069, 'motion_component_ionic': 0.4611817745082587, 'ionic_contributions': [{'ion_id': 1306, 'distance': 14.191061019897461, 'force': [-0.7537117600440979, 1.4613643884658813, -0.11885979771614075], 'magnitude': 1.648573637008667}, {'ion_id': 1307, 'distance': 14.717589378356934, 'force': [-0.25020793080329895, 0.5931304693222046, 1.390986442565918], 'magnitude': 1.5327266454696655}, {'ion_id': 1308, 'distance': 12.26911449432373, 'force': [0.24988240003585815, 2.1664843559265137, -0.3289939761161804], 'magnitude': 2.2055232524871826}, {'ion_id': 1309, 'distance': 8.785860061645508, 'force': [-1.407989263534546, 2.6396069526672363, -3.090088129043579], 'magnitude': 4.301000118255615}, {'ion_id': 1403, 'distance': 13.999079704284668, 'force': [-0.3514776825904846, 0.7056577205657959, -1.4994953870773315], 'magnitude': 1.694100260734558}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.5990183353424072, 'force': [10.65865707397461, -17.07918930053711, -4.5656328201293945], 'magnitude': 20.643417358398438}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 2.884697914123535, 'force': [-18.52711296081543, 26.6701908</t>
+          <t>{5173: {'frame': 5173, 'motion_vector': [-0.32863616943359375, 0.4364585876464844, -0.3377685546875], 'ionic_force': [-0.03178515285253525, 10.060459554195404, -0.028999194502830505], 'ionic_force_magnitude': 10.06055155997052, 'radial_force': 10.060509765292386, 'axial_force': -0.028999194502830505, 'glu_force': [-6.758579730987549, 7.259679794311523, 1.6593886613845825], 'glu_force_magnitude': 10.056585972664006, 'asn_force': [-7.390199303627014, -2.865291476249695, 7.459710121154785], 'asn_force_magnitude': 10.884494296147043, 'residue_force': [-14.148779034614563, 4.394388318061829, 9.119098782539368], 'residue_force_magnitude': 17.397027316929115, 'total_force': [-14.180564187467098, 14.454847872257233, 9.090099588036537], 'total_force_magnitude': 22.195966710314643, 'cosine_total_motion': 0.5540286962707712, 'cosine_glu_motion': 0.7475932094883707, 'cosine_asn_motion': -0.19188523890942097, 'cosine_residue_motion': 0.31210283782744785, 'cosine_ionic_motion': 0.6826207154421637, 'motion_component_total': 12.297202498985062, 'motion_component_glu': 7.518235383799613, 'motion_component_asn': -2.088573788424405, 'motion_component_residue': 5.429661595375208, 'motion_component_ionic': 6.867540903609853, 'motion_component_percent_total': 55.40286962707712, 'motion_component_percent_glu': 74.75932094883707, 'motion_component_percent_asn': 19.188523890942097, 'motion_component_percent_residue': 31.210283782744785, 'motion_component_percent_ionic': 68.26207154421637, 'ionic_contributions': [{'ion_id': 1306, 'distance': 12.007840156555176, 'force': [-1.142738938331604, 1.9904721975326538, -0.18408028781414032], 'magnitude': 2.3025457859039307, 'cosine_ionic_motion': 0.883359968662262, 'motion_component_ionic': 2.0339767932891846, 'motion_component_percent_ionic': 88.3359968662262}, {'ion_id': 1307, 'distance': 7.160901069641113, 'force': [0.9537079930305481, 3.515716075897217, 5.352444171905518], 'magnitude': 6.474447727203369, 'cosine_ionic_motion': -0.14111211895942688, 'motion_component_ionic': -0.913623034954071, 'motion_component_percent_ionic': 14.111211895942688}, {'ion_id': 1308, 'distance': 11.22840404510498, 'force': [0.7354629039764404, 2.4643869400024414, -0.565873920917511], 'magnitude': 2.633310079574585, 'cosine_ionic_motion': 0.6060114502906799, 'motion_component_ionic': 1.5958161354064941, 'motion_component_percent_ionic': 60.60114502906799}, {'ion_id': 1309, 'distance': 9.778471946716309, 'force': [-0.48083266615867615, 1.5299593210220337, -3.0795645713806152], 'magnitude': 3.4721310138702393, 'cosine_ionic_motion': 0.8366618156433105, 'motion_component_ionic': 2.9049994945526123, 'motion_component_percent_ionic': 83.66618156433105}, {'ion_id': 1403, 'distance': 14.173266410827637, 'force': [-0.09738444536924362, 0.5599250197410583, -1.5519245862960815], 'magnitude': 1.652715802192688, 'cosine_ionic_motion': 0.7541354298591614, 'motion_component_ionic': 1.2463715076446533, 'motion_component_percent_ionic': 75.41354298591614}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 5.199153900146484, 'force': [-6.758579730987549, 7.259679794311523, 1.6593886613845825], 'magnitude': 10.056586265563965, 'cosine_with_motion': 0.7475931644439697, 'motion_component': 7.518235206604004, 'motion_component_percent': 74.75931644439697}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.7128424644470215, 'force': [4.685451984405518, 0.9295059442520142, 9.52723503112793], 'magnitude': 10.6576566696167, 'cosine_with_motion': -0.6357436180114746, 'motion_component': -6.775537490844727, 'motion_component_percent': 63.57436180114746}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.261452674865723, 'force': [-2.8056347370147705, -2.153184175491333, -6.171500205993652], 'magnitude': 7.113030433654785, 'cosine_with_motion': 0.4523618817329407, 'motion_component': 3.2176637649536133, 'motion_component_percent': 45.23618817329407}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.9321959018707275, 'force': [-4.595969200134277, 0.7100307941436768, -19.178930282592773], 'magnitude': 19.73470115661621, 'cosine_with_motion': 0.6546418070793152, 'motion_component': 12.919160842895508, 'motion_component_percent': 65.46418070793152}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.785325765609741, 'force': [0.3094111680984497, 1.22603440284729, 9.639676094055176], 'magnitude': 9.72225570678711, 'cosine_with_motion': -0.4519783854484558, 'motion_component': -4.394249439239502, 'motion_component_percent': 45.19783854484558}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 3.5840225219726562, 'force': [2.689281940460205, -3.0791029930114746, 10.045012474060059], 'magnitude': 10.845063209533691, 'cosine_with_motion': -0.806849479675293, 'motion_component': -8.750333786010742, 'motion_component_percent': 80.6849479675293}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.799994468688965, 'force': [-3.7066445350646973, 0.42509329319000244, 1.7969428300857544], 'magnitude': 4.141125679016113, 'cosine_with_motion': 0.2995240092277527, 'motion_component': 1.2403665781021118, 'motion_component_percent': 29.95240092277527}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.5933098793029785, 'force': [-3.9660959243774414, -0.9236687421798706, 1.8012741804122925], 'magnitude': 4.452826976776123, 'cosine_with_motion': 0.10203768312931061, 'motion_component': 0.4543561339378357, 'motion_component_percent': 10.20376831293106}]}, 5174: {'frame': 5174, 'motion_vector': [-2.1065216064453125, -0.9170722961425781, 2.1868057250976562], 'ionic_force': [-0.6643470674753189, 10.092601358890533, -2.0427508652210236], 'ionic_force_magnitude': 10.318662234655388, 'radial_force': 10.114443099624522, 'axial_force': -2.0427508652210236, 'glu_force': [-7.780902862548828, 6.3519370555877686, 1.3226341009140015], 'glu_force_magnitude': 10.131086549796628, 'asn_force': [-7.848422586917877, -0.6536328196525574, 8.752897500991821], 'asn_force_magnitude': 11.774471861983386, 'residue_force': [-15.629325449466705, 5.698304235935211, 10.075531601905823], 'residue_force_magnitude': 19.44897997920785, 'total_force': [-16.293672516942024, 15.790905594825745, 8.0327807366848], 'total_force_magnitude': 24.069940381266118, 'cosine_total_motion': 0.4899757931292893, 'cosine_glu_motion': 0.4187999273624166, 'cosine_asn_motion': 0.9712541380581925, 'cosine_residue_motion': 0.8061555334685936, 'cosine_ionic_motion': -0.37652310089423896, 'motion_component_total': 11.793688128885574, 'motion_component_glu': 4.242898311157184, 'motion_component_asn': 11.436004519401115, 'motion_component_residue': 15.678902830558298, 'motion_component_ionic': -3.885214701672724, 'motion_component_percent_total': 48.99757931292893, 'motion_component_percent_glu': 41.87999273624166, 'motion_component_percent_asn': 97.12541380581925, 'motion_component_percent_residue': 80.61555334685936, 'motion_component_percent_ionic': 37.6523100894239, 'ionic_contributions': [{'ion_id': 1306, 'distance': 12.4862642288208, 'force': [-0.6169819831848145, 2.007314682006836, -0.35312172770500183], 'magnitude': 2.1294772624969482, 'cosine_ionic_motion': -0.19444845616817474, 'motion_component_ionic': -0.41407355666160583, 'motion_component_percent_ionic': 19.444845616817474}, {'ion_id': 1307, 'distance': 7.873819828033447, 'force': [0.5131598114967346, 2.890629529953003, 4.478611946105957], 'magnitude': 5.3550944328308105, 'cosine_ionic_motion': 0.35688990354537964, 'motion_component_ionic': 1.9111790657043457, 'motion_component_percent_ionic': 35.688990354537964}, {'ion_id': 1308, 'distance': 11.81053352355957, 'force': [0.4955497980117798, 2.235003709793091, -0.6512793898582458], 'magnitude': 2.3801209926605225, 'cosine_ionic_motion': -0.5984301567077637, 'motion_component_ionic': -1.4243361949920654, 'motion_component_percent_ionic': 59.84301567077637}, {'ion_id': 1309, 'distance': 8.462942123413086, 'force': [-0.8381993174552917, 2.3942766189575195, -3.879767417907715], 'magnitude': 4.635486602783203, 'cosine_ionic_motion': -0.606292724609375, 'motion_component_ionic': -2.8104617595672607, 'motion_component_percent_ionic': 60.6292724609375}, {'ion_id': 1403, 'distance': 13.790569305419922, 'force': [-0.2178753763437271, 0.5653768181800842, -1.637194275856018], 'magnitude': 1.7457164525985718, 'cosine_ionic_motion': -0.6573360562324524, 'motion_component_ionic': -1.1475223302841187, 'motion_component_percent_ionic': 65.73360562324524}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 5.600811004638672, 'force': [6.262893199920654, -5.221066474914551, -2.4852945804595947], 'magnitude': 8.524086952209473, 'cosine_with_motion': -0.5118784308433533, 'motion_component': -4.363296031951904, 'motion_component_percent': 51.18784308433533}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 5.847188949584961, 'force': [-6.818350791931152, 3.4854533672332764, 2.1401119232177734], 'magnitude': 7.950997829437256, 'cosine_with_motion': 0.6283521056175232, 'motion_component': 4.996026039123535, 'motion_component_percent': 62.83521056175232}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 4.977415561676025, 'force': [-7.22544527053833, 8.087550163269043, 1.6678167581558228], 'magnitude': 10.972562789916992, 'cosine_with_motion': 0.3290177881717682, 'motion_component': 3.61016845703125, 'motion_component_percent': 32.90177881717682}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.760137557983398, 'force': [3.6300151348114014, 2.7228000164031982, 9.4099760055542], 'magnitude': 10.446928024291992, 'cosine_with_motion': 0.31488659977912903, 'motion_component': 3.289597749710083, 'motion_component_percent': 31.488659977912903}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.740535736083984, 'force': [-1.890036940574646, -2.368476390838623, -5.150002479553223], 'magnitude': 5.975319862365723, 'cosine_with_motion': -0.2695431411266327, 'motion_component': -1.6106064319610596, 'motion_component_percent': 26.95431411266327}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.941314697265625, 'force': [-2.2430100440979004, -4.7319841384887695, -18.932613372802734], 'magnitude': 19.64348793029785, 'cosine_with_motion': -0.5190096497535706, 'motion_component': -10.195159912109375, 'motion_component_percent': 51.900964975357056}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.324524879455566, 'force': [-0.5797222256660461, 2.653454542160034, 6.936166286468506], 'magnitude': 7.44897985458374, 'cosine_with_motion': 0.5906738042831421, 'motion_component': 4.399917125701904, 'motion_component_percent': 59.06738042831421}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 3.2011022567749023, 'force': [1.3044353723526, 0.6891797184944153, 13.514564514160156], 'magnitude': 13.594850540161133, 'cosine_with_motion': 0.6069909930229187, 'motion_component': 8.251952171325684, 'motion_component_percent': 60.69909930229187}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.879083156585693, 'force': [-3.7527353763580322, 0.8021993637084961, 1.2320884466171265], 'magnitude': 4.030457496643066, 'cosine_with_motion': 0.7715820670127869, 'motion_component': 3.1098287105560303, 'motion_component_percent': 77.15820670127869}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.458897590637207, 'force': [-4.317368507385254, -0.4208059310913086, 1.7427181005477905], 'magnitude': 4.674806594848633, 'cosine_with_motion': 0.8963958024978638, 'motion_component': 4.190476894378662, 'motion_component_percent': 89.63958024978638}]}, 5175: {'frame': 5175, 'motion_vector': [0.8205947875976562, 1.4489250183105469, -0.349456787109375], 'ionic_force': [-4.48947374522686, 8.996800035238266, -3.1096643209457397], 'ionic_force_magnitude': 10.524628144124973, 'radial_force': 10.05473944879451, 'axial_force': -3.1096643209457397, 'glu_force': [-12.236773014068604, 14.97885513305664, -4.509521113708615], 'glu_force_magnitude': 19.860526064782842, 'asn_force': [-1.377406358718872, -0.5415080785751343, 3.917880058288574], 'asn_force_magnitude': 4.18810976782326, 'residue_force': [-13.614179372787476, 14.437347054481506, -0.5916410554200411], 'residue_force_magnitude': 19.85278089095924, 'total_force': [-18.103653118014336, 23.434147089719772, -3.701305376365781], 'total_force_magnitude': 29.842941670169278, 'cosine_total_motion': 0.4016086340326952, 'cosine_glu_motion': 0.3917474294886923, 'cosine_asn_motion': -0.4608646553582442, 'cosine_residue_motion': 0.2946770178723724, 'cosine_ionic_motion': 0.5829208107155092, 'motion_component_total': 11.985183039674084, 'motion_component_glu': 7.780310034171852, 'motion_component_asn': -1.930151764750363, 'motion_component_residue': 5.850158269421489, 'motion_component_ionic': 6.135024770252594, 'motion_component_percent_total': 40.160863403269516, 'motion_component_percent_glu': 39.17474294886923, 'motion_component_percent_asn': 46.08646553582442, 'motion_component_percent_residue': 29.46770178723724, 'motion_component_percent_ionic': 58.29208107155092, 'ionic_contributions': [{'ion_id': 1306, 'distance': 12.98525619506836, 'force': [-1.0581152439117432, 1.6551977396011353, 0.1323573887348175], 'magnitude': 1.9689606428146362, 'cosine_ionic_motion': 0.44289395213127136, 'motion_component_ionic': 0.8720407485961914, 'motion_component_percent_ionic': 44.289395213127136}, {'ion_id': 1307, 'distance': 10.564190864562988, 'force': [-0.3703985810279846, 0.40683475136756897, 2.9235332012176514], 'magnitude': 2.974853992462158, 'cosine_ionic_motion': -0.1454351246356964, 'motion_component_ionic': -0.432648241519928, 'motion_component_percent_ionic': 14.543512463569641}, {'ion_id': 1308, 'distance': 9.630842208862305, 'force': [0.23377586901187897, 3.548218250274658, -0.4093410074710846], 'magnitude': 3.5793943405151367, 'cosine_ionic_motion': 0.8991609215736389, 'motion_component_ionic': 3.218451499938965, 'motion_component_percent_ionic': 89.91609215736389}, {'ion_id': 1309, 'distance': 7.792961597442627, 'force': [-2.680544376373291, 2.8133533000946045, -3.845205307006836], 'magnitude': 5.466797828674316, 'cosine_ionic_motion': 0.34623077511787415, 'motion_component_ionic': 1.8927736282348633, 'motion_component_percent_ionic': 34.623077511787415}, {'ion_id': 1403, 'distance': 12.611123085021973, 'force': [-0.6141914129257202, 0.5731959939002991, -1.911008596420288], 'magnitude': 2.087519645690918, 'cosine_ionic_motion': 0.27995291352272034, 'motion_component_ionic': 0.5844072103500366, 'motion_component_percent_ionic': 27.995291352272034}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.8696460723876953, 'force': [9.367057800292969, -15.202912330627441, 0.016476763412356377], 'magnitude': 17.85694694519043, 'cosine_with_motion': -0.4722163677215576, 'motion_component': -8.432342529296875, 'motion_component_percent': 47.22163677215576}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 3.822664499282837, 'force': [-14.11198616027832, 12.011738777160645, 1.6255600452423096], 'magnitude': 18.603023529052734, 'cosine_with_motion': 0.16605117917060852, 'motion_component': 3.0890538692474365, 'motion_component_percent': 16.605117917060852}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 3.633172035217285, 'force': [-7.491844654083252, 18.170028686523438, -6.151557922363281], 'magnitude': 20.594158172607422, 'cosine_with_motion': 0.6372485756874084, 'motion_component': 13.123598098754883, 'motion_component_percent': 63.724857568740845}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.767369270324707, 'force': [-1.377406358718872, -0.5415080785751343, 3.917880058288574], 'magnitude': 4.188109874725342, 'cosine_with_motion': -0.4608646631240845, 'motion_component': -1.9301518201828003, 'motion_component_percent': 46.08646631240845}]}, 5176: {'frame': 5176, 'motion_vector': [-0.2884254455566406, 1.5469932556152344, -1.362060546875], 'ionic_force': [-1.6972591429948807, 9.394513070583344, -1.1074041053652763], 'ionic_force_magnitude': 9.610614355202319, 'radial_force': 9.546599626665035, 'axial_force': -1.1074041053652763, 'glu_force': [-19.01718759536743, 20.73361301422119, -1.6225908994674683], 'glu_force_magnitude': 28.1810030674551, 'asn_force': [-0.6952297687530518, -0.1736546754837036, 0.5019161701202393], 'asn_force_magnitude': 0.8748829747491611, 'residue_force': [-19.712417364120483, 20.559958338737488, -1.120674729347229], 'residue_force_magnitude': 28.505213506951623, 'total_force': [-21.409676507115364, 29.95447140932083, -2.2280788347125053], 'total_force_magnitude': 36.88643301872439, 'cosine_total_motion': 0.7235823170283582, 'cosine_glu_motion': 0.678069463817084, 'cosine_asn_motion': -0.4128632695551034, 'cosine_residue_motion': 0.6576856752808345, 'cosine_ionic_motion': 0.8264716263384885, 'motion_component_total': 26.69037067059993, 'motion_component_glu': 19.10867763977688, 'motion_component_asn': -0.3612070454330336, 'motion_component_residue': 18.747470594343845, 'motion_component_ionic': 7.942900076256084, 'motion_component_percent_total': 72.35823170283582, 'motion_component_percent_glu': 67.8069463817084, 'motion_component_percent_asn': 41.28632695551034, 'motion_component_percent_residue': 65.76856752808345, 'motion_component_percent_ionic': 82.64716263384885, 'ionic_contributions': [{'ion_id': 1306, 'distance': 14.89237117767334, 'force': [-0.5284325480461121, 1.4004030227661133, 0.022839702665805817], 'magnitude': 1.4969606399536133, 'cosine_ionic_motion': 0.7342918515205383, 'motion_component_ionic': 1.0992059707641602, 'motion_component_percent_ionic': 73.42918515205383}, {'ion_id': 1307, 'distance': 8.6985502243042, 'force': [-0.19438980519771576, 2.0637528896331787, 3.8672609329223633], 'magnitude': 4.387775421142578, 'cosine_ionic_motion': -0.22106388211250305, 'motion_component_ionic': -0.9699786901473999, 'motion_component_percent_ionic': 22.106388211250305}, {'ion_id': 1308, 'distance': 10.563375473022461, 'force': [0.5721141695976257, 2.9097232818603516, -0.24224546551704407], 'magnitude': 2.9753129482269287, 'cosine_ionic_motion': 0.7535516619682312, 'motion_component_ionic': 2.2420520782470703, 'motion_component_percent_ionic': 75.35516619682312}, {'ion_id': 1309, 'distance': 9.11813735961914, 'force': [-1.1644694805145264, 2.285262107849121, -3.060650587081909], 'magnitude': 3.99324369430542, 'cosine_ionic_motion': 0.9673940539360046, 'motion_component_ionic': 3.8630402088165283, 'motion_component_percent_ionic': 96.73940539360046}, {'ion_id': 1403, 'distance': 13.266416549682617, 'force': [-0.3820814788341522, 0.7353717684745789, -1.6946086883544922], 'magnitude': 1.8863871097564697, 'cosine_ionic_motion': 0.9057421088218689, 'motion_component_ionic': 1.7085802555084229, 'motion_component_percent_ionic': 90.57421088218689}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.7171125411987305, 'force': [11.659213066101074, -15.12153434753418, -3.1501314640045166], 'magnitude': 19.352554321289062, 'cosine_with_motion': -0.5577578544616699, 'motion_component': -10.794038772583008, 'motion_component_percent': 55.77578544616699}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 2.8986754417419434, 'force': [-25.04872703552246, 20.474231719970703, -0.30672621726989746], 'magnitude': 32.3531608581543, 'cosine_with_motion': 0.5838869214057922, 'motion_component': 18.890586853027344, 'motion_component_percent': 58.388692140579224}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 4.061368465423584, 'force': [-5.627673625946045, 15.380915641784668, 1.8342667818069458], 'magnitude': 16.480527877807617, 'cosine_with_motion': 0.6681903004646301, 'motion_component': 11.012128829956055, 'motion_component_percent': 66.81903004646301}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.233702182769775, 'force': [1.5910654067993164, -1.8462071418762207, -10.870063781738281], 'magnitude': 11.13994026184082, 'cosine_with_motion': 0.4956105351448059, 'motion_component': 5.521071910858154, 'motion_component_percent': 49.56105351448059}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.719921112060547, 'force': [-1.17593252658844, 1.0421768426895142, 3.9573471546173096], 'magnitude': 4.257880687713623, 'cosine_with_motion': -0.38804492354393005, 'motion_component': -1.6522489786148071, 'motion_component_percent': 38.804492354393005}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.302978038787842, 'force': [-1.1103626489639282, 0.6303756237030029, 7.414632797241211], 'magnitude': 7.52376651763916, 'cosine_with_motion': -0.562222421169281, 'motion_component': -4.230030059814453, 'motion_component_percent': 56.2222421169281}]}, 5177: {'frame': 5177, 'motion_vector': [1.0473556518554688, -0.16293716430664062, -0.0436553955078125], 'ionic_force': [-1.3824736773967743, 8.549700021743774, -0.875838428735733], 'ionic_force_magnitude': 8.70492371498744, 'radial_force': 8.660750771757634, 'axial_force': -0.875838428735733, 'glu_force': [-25.912687301635742, 22.428939819335938, 8.468029022216797], 'glu_force_magnitude': 35.30201439199828, 'asn_force': [0.774412602186203, 1.5036826133728027, 2.5479869842529297], 'asn_force_magnitude': 3.058269764443092, 'residue_force': [-25.13827469944954, 23.93262243270874, 11.016016006469727], 'residue_force_magnitude': 36.415050185690745, 'total_force': [-26.520748376846313, 32.482322454452515, 10.140177577733994], 'total_force_magnitude': 43.142491441860486, 'cosine_total_motion': -0.7322154749248397, 'cosine_glu_motion': -0.832143931429355, 'cosine_asn_motion': 0.14019541199527244, 'cosine_residue_motion': -0.7949351025551864, 'cosine_ionic_motion': -0.3035061872029496, 'motion_component_total': -31.58959986054271, 'motion_component_glu': -29.37635704353312, 'motion_component_asn': 0.4287553896187841, 'motion_component_residue': -28.947601653914333, 'motion_component_ionic': -2.6419982066283736, 'motion_component_percent_total': 73.22154749248398, 'motion_component_percent_glu': 83.2143931429355, 'motion_component_percent_asn': 14.019541199527245, 'motion_component_percent_residue': 79.49351025551864, 'motion_component_percent_ionic': 30.350618720294957, 'ionic_contributions': [{'ion_id': 1307, 'distance': 8.939340591430664, 'force': [-0.45594823360443115, 2.804142475128174, 3.031407594680786], 'magnitude': 4.154580116271973, 'cosine_ionic_motion': -0.24204227328300476, 'motion_component_ionic': -1.0055840015411377, 'motion_component_percent_ionic': 24.204227328300476}, {'ion_id': 1308, 'distance': 11.303756713867188, 'force': [0.689740777015686, 2.4730772972106934, -0.39926019310951233], 'magnitude': 2.5983190536499023, 'cosine_ionic_motion': 0.12221500277519226, 'motion_component_ionic': 0.3175535798072815, 'motion_component_percent_ionic': 12.221500277519226}, {'ion_id': 1309, 'distance': 9.676535606384277, 'force': [-1.2035044431686401, 2.5528600215911865, -2.146219491958618], 'magnitude': 3.5456700325012207, 'cosine_ionic_motion': -0.4207861125469208, 'motion_component_ionic': -1.4919687509536743, 'motion_component_percent_ionic': 42.07861125469208}, {'ion_id': 1403, 'distance': 14.429394721984863, 'force': [-0.41276177763938904, 0.7196202278137207, -1.3617663383483887], 'magnitude': 1.594563603401184, 'cosine_ionic_motion': -0.2897338271141052, 'motion_component_ionic': -0.46199899911880493, 'motion_component_percent_ionic': 28.973382711410522}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.2737128734588623, 'force': [17.63517189025879, -13.619305610656738, -11.225502967834473], 'magnitude': 24.94988441467285, 'cosine_with_motion': 0.8001859784126282, 'motion_component': 19.964548110961914, 'motion_component_percent': 80.01859784126282}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 2.769817352294922, 'force': [-32.05121612548828, 13.869439125061035, 5.990726470947266], 'magnitude': 35.433467864990234, 'cosine_with_motion': -0.9601144194602966, 'motion_component': -34.02018356323242, 'motion_component_percent': 96.01144194602966}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 3.0888047218322754, 'force': [-11.49664306640625, 22.17880630493164, 13.702805519104004], 'magnitude': 28.49279022216797, 'cosine_with_motion': -0.5377052426338196, 'motion_component': -15.320722579956055, 'motion_component_percent': 53.77052426338196}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.723537921905518, 'force': [0.3901461064815521, 4.517452716827393, 5.626331806182861], 'magnitude': 7.226008892059326, 'cosine_with_motion': -0.0747559517621994, 'motion_component': -0.5401871800422668, 'motion_component_percent': 7.47559517621994}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.737008094787598, 'force': [1.5527937412261963, -5.17930793762207, -7.531026363372803], 'magnitude': 9.271071434020996, 'cosine_with_motion': 0.2845887839794159, 'motion_component': 2.6384429931640625, 'motion_component_percent': 28.45887839794159}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.232869625091553, 'force': [-1.1685272455215454, 2.1655378341674805, 4.452681541442871], 'magnitude': 5.087374687194824, 'cosine_with_motion': -0.3281654119491577, 'motion_component': -1.669500470161438, 'motion_component_percent': 32.81654119491577}]}, 5178: {'frame': 5178, 'motion_vector': [-0.499969482421875, -1.2579994201660156, 0.6877059936523438], 'ionic_force': [-1.344180654734373, 9.261112630367279, -1.605331540107727], 'ionic_force_magnitude': 9.494846925494645, 'radial_force': 9.358153064836591, 'axial_force': -1.605331540107727, 'glu_force': [-16.422406673431396, 21.141526222229004, 4.929273366928101], 'glu_force_magnitude': 27.220530999204758, 'asn_force': [-0.13263589143753052, -2.4197518825531006, -2.994140148162842], 'asn_force_magnitude': 3.8519691950556028, 'residue_force': [-16.555042564868927, 18.721774339675903, 1.9351332187652588], 'residue_force_magnitude': 25.066292293132182, 'total_force': [-17.8992232196033, 27.982886970043182, 0.32980167865753174], 'total_force_magnitude': 33.21946604312965, 'cosine_total_motion': -0.5159939491495346, 'cosine_glu_motion': -0.36281276984807215, 'cosine_asn_motion': 0.17974320918784045, 'cosine_residue_motion': -0.36637213179952305, 'cosine_ionic_motion': -0.8380811813955584, 'motion_component_total': -17.14104347223333, 'motion_component_glu': -9.87595624855679, 'motion_component_asn': 0.6923653048119967, 'motion_component_residue': -9.183590943744793, 'motion_component_ionic': -7.957452528488538, 'motion_component_percent_total': 51.59939491495346, 'motion_component_percent_glu': 36.281276984807214, 'motion_component_percent_asn': 17.974320918784045, 'motion_component_percent_residue': 36.637213179952305, 'motion_component_percent_ionic': 83.80811813955584, 'ionic_contributions': [{'ion_id': 1306, 'distance': 14.052817344665527, 'force': [-0.6633750796318054, 1.5338643789291382, -0.1830899715423584], 'magnitude': 1.681168794631958, 'cosine_ionic_motion': -0.6753159761428833, 'motion_component_ionic': -1.1353201866149902, 'motion_component_percent_ionic': 67.53159761428833}, {'ion_id': 1307, 'distance': 9.598557472229004, 'force': [0.008810419589281082, 2.18619704246521, 2.864572048187256], 'magnitude': 3.603513479232788, 'cosine_ionic_motion': -0.14340798556804657, 'motion_component_ionic': -0.5167726278305054, 'motion_component_percent_ionic': 14.340798556804657}, {'ion_id': 1308, 'distance': 12.033468246459961, 'force': [0.52821284532547, 2.203639030456543, -0.34880292415618896], 'magnitude': 2.2927489280700684, 'cosine_ionic_motion': -0.9410790801048279, 'motion_component_ionic': -2.157658100128174, 'motion_component_percent_ionic': 94.10790801048279}, {'ion_id': 1309, 'distance': 9.426063537597656, 'force': [-0.9532740116119385, 2.5756494998931885, -2.5336785316467285], 'magnitude': 3.7366065979003906, 'cosine_ionic_motion': -0.7942044734954834, 'motion_component_ionic': -2.9676296710968018, 'motion_component_percent_ionic': 79.42044734954834}, {'ion_id': 1403, 'distance': 14.318366050720215, 'force': [-0.26455482840538025, 0.7617626786231995, -1.404332160949707], 'magnitude': 1.6193888187408447, 'cosine_ionic_motion': -0.7287143468856812, 'motion_component_ionic': -1.1800718307495117, 'motion_component_percent_ionic': 72.87143468856812}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.7478668689727783, 'force': [12.879548072814941, -12.15123462677002, -6.988813400268555], 'magnitude': 19.0362491607666, 'cosine_with_motion': 0.1397933065891266, 'motion_component': 2.661140203475952, 'motion_component_percent': 13.979330658912659}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 3.1079115867614746, 'force': [-21.525930404663086, 18.075557708740234, 1.4024779796600342], 'magnitude': 28.143531799316406, 'cosine_with_motion': -0.2577016353607178, 'motion_component': -7.252634048461914, 'motion_component_percent': 25.770163536071777}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 3.6807591915130615, 'force': [-7.776024341583252, 15.217203140258789, 10.515608787536621], 'magnitude': 20.06509017944336, 'cosine_with_motion': -0.2633659541606903, 'motion_component': -5.284461498260498, 'motion_component_percent': 26.33659541606903}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.4385528564453125, 'force': [0.3637133538722992, -4.931046485900879, -9.054475784301758], 'magnitude': 10.31654167175293, 'cosine_with_motion': -0.013113133609294891, 'motion_component': -0.13528218865394592, 'motion_component_percent': 1.3113133609294891}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.601647853851318, 'force': [-0.4963492453098297, 2.5112946033477783, 6.060335636138916], 'magnitude': 6.57880163192749, 'cosine_with_motion': 0.12580516934394836, 'motion_component': 0.8276472687721252, 'motion_component_percent': 12.580516934394836}]}, 5179: {'frame': 5179, 'motion_vector': [0.006259918212890625, 2.1265487670898438, -1.1589584350585938], 'ionic_force': [-2.9875034540891647, 9.438717722892761, -3.671563595533371], 'ionic_force_magnitude': 10.559116836965606, 'radial_force': 9.90023076198957, 'axial_force': -3.671563595533371, 'glu_force': [-23.799495220184326, 22.224249839782715, -1.1507561802864075], 'glu_force_magnitude': 32.58308600275802, 'asn_force': [0.31184569001197815, 1.3416973948478699, 8.548349380493164], 'asn_force_magnitude': 8.658618640678112, 'residue_force': [-23.487649530172348, 23.565947234630585, 7.397593200206757], 'residue_force_magnitude': 34.08442363710062, 'total_force': [-26.475152984261513, 33.004664957523346, 3.7260296046733856], 'total_force_magnitude': 42.47499183182174, 'cosine_total_motion': 0.6386973387230179, 'cosine_glu_motion': 0.6139209778471686, 'cosine_asn_motion': -0.3362918949524588, 'cosine_residue_motion': 0.501449487065499, 'cosine_ionic_motion': 0.9505574803738571, 'motion_component_total': 27.12866424526647, 'motion_component_glu': 20.0034400200916, 'motion_component_asn': -2.911823270344325, 'motion_component_residue': 17.091616749747274, 'motion_component_ionic': 10.037047495519198, 'motion_component_percent_total': 63.869733872301794, 'motion_component_percent_glu': 61.39209778471686, 'motion_component_percent_asn': 33.62918949524588, 'motion_component_percent_residue': 50.1449487065499, 'motion_component_percent_ionic': 95.05574803738571, 'ionic_contributions': [{'ion_id': 1306, 'distance': 11.857600212097168, 'force': [-0.7968317866325378, 2.22175669670105, 0.06649583578109741], 'magnitude': 2.3612635135650635, 'cosine_ionic_motion': 0.8118366003036499, 'motion_component_ionic': 1.9169601202011108, 'motion_component_percent_ionic': 81.18366003036499}, {'ion_id': 1307, 'distance': 13.191850662231445, 'force': [-0.160544291138649, 0.8</t>
         </is>
       </c>
     </row>
@@ -627,7 +627,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>{5213: {'frame': 5213, 'ionic_force': [8.349748060107231, 9.205024123191833, -18.89620530605316], 'ionic_force_magnitude': 22.61674903128917, 'motion_vector': [-0.08104324340820312, -3.535572052001953, 0.40856170654296875], 'ionic_force_x': 8.349748060107231, 'ionic_force_y': 9.205024123191833, 'ionic_force_z': -18.89620530605316, 'radial_force': 12.427822084975631, 'axial_force': -18.89620530605316, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-11.033990144729614, 1.9732149839401245, -5.10729056596756], 'asn_force_magnitude': 12.317748690895481, 'residue_force': [-11.033990144729614, 1.9732149839401245, -5.10729056596756], 'residue_force_magnitude': 12.317748690895481, 'total_force': [-2.684242084622383, 11.178239107131958, -24.00349587202072], 'total_force_magnitude': 26.61439458607293, 'motion_component_total': -13.79509228795936, 'cosine_total_motion': -0.5183319967450323, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.18628470386856832, 'cosine_residue_motion': -0.18628470386856832, 'cosine_ionic_motion': -0.5084941299405185, 'motion_component_glu': None, 'motion_component_asn': -2.2946081672109098, 'motion_component_residue': -2.2946081672109098, 'motion_component_ionic': -11.50048412074845, 'ionic_contributions': [{'ion_id': 1306, 'distance': 11.115274429321289, 'force': [-0.7094604969024658, 2.2941157817840576, -1.2060950994491577], 'magnitude': 2.687185764312744}, {'ion_id': 1308, 'distance': 4.756705284118652, 'force': [4.778199672698975, 9.435524940490723, -10.170702934265137], 'magnitude': 14.673224449157715}, {'ion_id': 1320, 'distance': 6.789470195770264, 'force': [4.232130527496338, -3.0712902545928955, -4.9525957107543945], 'magnitude': 7.202219009399414}, {'ion_id': 1403, 'distance': 11.246515274047852, 'force': [0.04887835681438446, 0.5466736555099487, -2.5668115615844727], 'magnitude': 2.624835729598999}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.5150952339172363, 'force': [16.992422103881836, -6.173070430755615, 6.33919095993042], 'magnitude': 19.158145904541016}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.725060224533081, 'force': [-19.537765502929688, 15.083691596984863, -9.688909530639648], 'magnitude': 26.516353607177734}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.6749155521392822, 'force': [-20.53214454650879, -0.5899879932403564, -9.412881851196289], 'magnitude': 22.594676971435547}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.237393856048584, 'force': [10.7410888671875, 3.150566339492798, 7.1675543785095215], 'magnitude': 13.291760444641113}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.4853692054748535, 'force': [6.563553333282471, 0.7515674829483032, 2.0739171504974365], 'magnitude': 6.924320697784424}, {'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.766394138336182, 'force': [-6.361416816711426, -3.1261937618255615, -0.6628996729850769], 'magnitude': 7.118999004364014}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.568770885467529, 'force': [12.717414855957031, 7.166444301605225, 0.7805547118186951], 'magnitude': 14.618475914001465}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.9164936542510986, 'force': [-8.516819953918457, -2.9974727630615234, -0.9801065325737], 'magnitude': 9.081942558288574}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.460243225097656, 'force': [-5.205928802490234, -4.682491779327393, -0.09132105112075806], 'magnitude': 7.002553939819336}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.316735744476318, 'force': [2.1056063175201416, -6.609838008880615, -0.6323891282081604], 'magnitude': 6.965877532958984}]}, 5214: {'frame': 5214, 'ionic_force': [-0.392241433262825, -3.0962782502174377, -10.358314990997314], 'ionic_force_magnitude': 10.818293848729445, 'motion_vector': [-2.800647735595703, -0.17963790893554688, 2.6386032104492188], 'ionic_force_x': -0.392241433262825, 'ionic_force_y': -3.0962782502174377, 'ionic_force_z': -10.358314990997314, 'radial_force': 3.121024246098968, 'axial_force': -10.358314990997314, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [16.765697956085205, -12.439022541046143, 0.22667193412780762], 'asn_force_magnitude': 20.8774828438932, 'residue_force': [16.765697956085205, -12.439022541046143, 0.22667193412780762], 'residue_force_magnitude': 20.8774828438932, 'total_force': [16.37345652282238, -15.53530079126358, -10.131643056869507], 'total_force_magnitude': 24.740368635321538, 'motion_component_total': -18.12004705530107, 'cosine_total_motion': -0.7324081270733893, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.5486425501739778, 'cosine_residue_motion': -0.5486425501739778, 'cosine_ionic_motion': -0.6161573830236546, 'motion_component_glu': None, 'motion_component_asn': -11.454275428687035, 'motion_component_residue': -11.454275428687035, 'motion_component_ionic': -6.665771626614035, 'ionic_contributions': [{'ion_id': 1306, 'distance': 8.311978340148926, 'force': [-1.26851487159729, 3.9690990447998047, -2.3935248851776123], 'magnitude': 4.805397033691406}, {'ion_id': 1308, 'distance': 8.85319995880127, 'force': [-1.3250770568847656, -3.1238503456115723, -2.5353305339813232], 'magnitude': 4.2358198165893555}, {'ion_id': 1320, 'distance': 8.383258819580078, 'force': [2.0835518836975098, -3.640300989151001, -2.173349618911743], 'magnitude': 4.724026679992676}, {'ion_id': 1403, 'distance': 10.072875022888184, 'force': [0.11779861152172089, -0.3012259602546692, -3.2561099529266357], 'magnitude': 3.272134780883789}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.220438480377197, 'force': [-7.028218746185303, 7.975660800933838, -3.5152876377105713], 'magnitude': 11.196619033813477}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.340437412261963, 'force': [4.018090724945068, -5.689406394958496, 2.4826714992523193], 'magnitude': 7.394461154937744}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.443244934082031, 'force': [3.4803147315979004, -2.686570167541504, 1.6661407947540283], 'magnitude': 4.701731204986572}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.7183046340942383, 'force': [-10.050923347473145, 13.65013599395752, -2.4068522453308105], 'magnitude': 17.121337890625}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.5175106525421143, 'force': [20.784893035888672, -22.801639556884766, 3.652261972427368], 'magnitude': 31.068723678588867}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.250736236572266, 'force': [5.533113479614258, -15.4774751663208, 3.876791000366211], 'magnitude': 16.887779235839844}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.822483539581299, 'force': [-1.0360026359558105, 9.108904838562012, -2.6181509494781494], 'magnitude': 9.534157752990723}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.256087779998779, 'force': [-1.7162542343139648, 4.579953193664551, -1.2270251512527466], 'magnitude': 5.04252815246582}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.542922496795654, 'force': [7.132328510284424, 2.891019582748413, -0.3643268942832947], 'magnitude': 7.704598426818848}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.470865249633789, 'force': [-8.900879859924316, -4.187804698944092, -0.5291113257408142], 'magnitude': 9.851057052612305}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.4902024269104, 'force': [4.549236297607422, 0.19819903373718262, -0.7904391288757324], 'magnitude': 4.621647834777832}]}, 5215: {'frame': 5215, 'ionic_force': [-7.000141829252243, -6.792514324188232, -8.448651671409607], 'ionic_force_magnitude': 12.904260983828621, 'motion_vector': [0.9844284057617188, -0.2884941101074219, -5.571617126464844], 'ionic_force_x': -7.000141829252243, 'ionic_force_y': -6.792514324188232, 'ionic_force_z': -8.448651671409607, 'radial_force': 9.753985671198684, 'axial_force': -8.448651671409607, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [3.558483213186264, 0.47542114555835724, -0.7009260654449463], 'asn_force_magnitude': 3.6578853718224402, 'residue_force': [3.558483213186264, 0.47542114555835724, -0.7009260654449463], 'residue_force_magnitude': 3.6578853718224402, 'total_force': [-3.441658616065979, -6.317093178629875, -9.149577736854553], 'total_force_magnitude': 11.638962712363064, 'motion_component_total': 8.72197646011732, 'cosine_total_motion': 0.7493774725176083, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.35087796957467987, 'cosine_residue_motion': 0.35087796957467987, 'cosine_ionic_motion': 0.5764378973144713, 'motion_component_glu': None, 'motion_component_asn': 1.2834713922019807, 'motion_component_residue': 1.2834713922019807, 'motion_component_ionic': 7.43850506791534, 'ionic_contributions': [{'ion_id': 1306, 'distance': 8.160512924194336, 'force': [-3.8426830768585205, 2.8841068744659424, -1.3305236101150513], 'magnitude': 4.98543643951416}, {'ion_id': 1308, 'distance': 9.352710723876953, 'force': [-2.1365599632263184, -3.032615900039673, -0.8023586273193359], 'magnitude': 3.7954483032226562}, {'ion_id': 1320, 'distance': 7.378998756408691, 'force': [0.5601136684417725, -6.005922317504883, -0.8906189203262329], 'magnitude': 6.097379207611084}, {'ion_id': 1403, 'distance': 9.133903503417969, 'force': [-1.2336101531982422, -0.5227363109588623, -3.747150182723999], 'magnitude': 3.9794700145721436}, {'ion_id': 1469, 'distance': 13.903539657592773, 'force': [-0.34740230441093445, -0.11534667015075684, -1.6780003309249878], 'magnitude': 1.7174626588821411}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.461219310760498, 'force': [-1.7710473537445068, 7.48703670501709, -6.744088649749756], 'magnitude': 10.231082916259766}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.108263969421387, 'force': [0.19433173537254333, -3.524526357650757, 4.005063533782959], 'magnitude': 5.33859395980835}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.204665660858154, 'force': [1.7985098361968994, -3.607750654220581, 3.1931893825531006], 'magnitude': 5.142660617828369}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.722692489624023, 'force': [-5.9168829917907715, 3.027146816253662, 2.8412938117980957], 'magnitude': 7.228144645690918}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.113308906555176, 'force': [6.542529582977295, -1.7497735023498535, -3.294235944747925], 'magnitude': 7.531161308288574}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.2527875900268555, 'force': [7.63437032699585, -6.52311372756958, -4.633557319641113], 'magnitude': 11.059135437011719}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.436313629150391, 'force': [-4.377902507781982, 4.1760382652282715, 3.6738297939300537], 'magnitude': 7.078301429748535}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.813601493835449, 'force': [-2.6524696350097656, 2.8659005165100098, 1.3190717697143555], 'magnitude': 4.121763229370117}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.534676551818848, 'force': [6.397800922393799, 4.249890327453613, 8.574560165405273], 'magnitude': 11.511581420898438}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.575444221496582, 'force': [-2.910076379776001, -4.051925182342529, -7.973955154418945], 'magnitude': 9.40588092803955}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.497517108917236, 'force': [-9.882165908813477, -1.5354973077774048, -11.29392147064209], 'magnitude': 15.085344314575195}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.384892463684082, 'force': [3.943589925765991, -0.5436141490936279, 6.053659439086914], 'magnitude': 7.245288848876953}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.9015960693359375, 'force': [4.557895660400391, 0.20560939610004425, 3.578164577484131], 'magnitude': 5.798271179199219}]}, 5216: {'frame': 5216, 'ionic_force': [-1.1580060422420502, -1.9418916404247284, -7.661372423171997], 'ionic_force_magnitude': 7.988025321915354, 'motion_vector': [0.49591064453125, 1.3578147888183594, -0.21898651123046875], 'ionic_force_x': -1.1580060422420502, 'ionic_force_y': -1.9418916404247284, 'ionic_force_z': -7.661372423171997, 'radial_force': 2.2609558016512707, 'axial_force': -7.661372423171997, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-3.7864845395088196, -14.654212445020676, 9.05460637807846], 'asn_force_magnitude': 17.637156919800802, 'residue_force': [-3.7864845395088196, -14.654212445020676, 9.05460637807846], 'residue_force_magnitude': 17.637156919800802, 'total_force': [-4.94449058175087, -16.596104085445404, 1.3932339549064636], 'total_force_magnitude': 17.37296056465521, 'motion_component_total': -17.298886898540218, 'cosine_total_motion': -0.9957362669512017, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.9213599580828115, 'cosine_residue_motion': -0.9213599580828115, 'cosine_ionic_motion': -0.13128610588344053, 'motion_component_glu': None, 'motion_component_asn': -16.250170160327635, 'motion_component_residue': -16.250170160327635, 'motion_component_ionic': -1.0487167382125833, 'ionic_contributions': [{'ion_id': 1306, 'distance': 10.266419410705566, 'force': [-1.4940450191497803, 1.5567138195037842, -2.294883966445923], 'magnitude': 3.1499240398406982}, {'ion_id': 1308, 'distance': 12.706043243408203, 'force': [-0.5920225381851196, -1.5384231805801392, -1.2295265197753906], 'magnitude': 2.0564465522766113}, {'ion_id': 1320, 'distance': 10.449557304382324, 'force': [1.186414122581482, -1.7023833990097046, -2.2223496437072754], 'magnitude': 3.0404810905456543}, {'ion_id': 1403, 'distance': 13.051283836364746, 'force': [-0.2583526074886322, -0.2577988803386688, -1.9146122932434082], 'magnitude': 1.9490886926651}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.96173620223999, 'force': [1.6038880348205566, -6.3169097900390625, -1.371645450592041], 'magnitude': 6.660121440887451}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.816272258758545, 'force': [-2.506654739379883, 8.01327133178711, 1.2502413988113403], 'magnitude': 8.488753318786621}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.8918938636779785, 'force': [-0.36741095781326294, -3.8968489170074463, -0.8850693106651306], 'magnitude': 4.012950420379639}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.597157955169678, 'force': [-5.129405498504639, 3.937967300415039, -3.9083101749420166], 'magnitude': 7.556009292602539}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.731990814208984, 'force': [6.930484294891357, -3.6226212978363037, 4.022002696990967], 'magnitude': 8.79383373260498}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.536361217498779, 'force': [4.822237014770508, -5.848729133605957, 6.453319072723389], 'magnitude': 9.955246925354004}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.722114562988281, 'force': [-2.436523914337158, 3.613025188446045, -4.476563930511475], 'magnitude': 6.247417449951172}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.7144429683685303, 'force': [12.244051933288574, 6.392899036407471, -10.1771879196167], 'magnitude': 17.15695571899414}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.6490366458892822, 'force': [-17.539894104003906, -14.308707237243652, 16.582679748535156], 'magnitude': 28.06015396118164}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.133080005645752, 'force': [-13.984121322631836, -1.2258847951889038, 11.046565055847168], 'magnitude': 17.862951278686523}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.625009536743164, 'force': [8.369632720947266, -1.6478105783462524, -6.29440450668335], 'magnitude': 10.601205825805664}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.134454250335693, 'force': [4.2072319984436035, 0.2561364471912384, -3.1870203018188477], 'magnitude': 5.2842698097229}]}, 5217: {'frame': 5217, 'ionic_force': [-1.6522649973630905, -0.9567364044487476, -8.501810789108276], 'ionic_force_magnitude': 8.713559023895268, 'motion_vector': [1.0223388671875, -0.4985237121582031, 2.0433120727539062], 'ionic_force_x': -1.6522649973630905, 'ionic_force_y': -0.9567364044487476, 'ionic_force_z': -8.501810789108276, 'radial_force': 1.9092732044180507, 'axial_force': -8.501810789108276, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-1.3066682368516922, -0.37906181812286377, 3.6236820220947266], 'asn_force_magnitude': 3.870677090692047, 'residue_force': [-1.3066682368516922, -0.37906181812286377, 3.6236820220947266], 'residue_force_magnitude': 3.870677090692047, 'total_force': [-2.9589332342147827, -1.3357982225716114, -4.87812876701355], 'total_force_magnitude': 5.859674312069858, 'motion_component_total': -5.271058070309653, 'cosine_total_motion': -0.8995479594236555, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.6912923510244952, 'cosine_residue_motion': 0.6912923510244952, 'cosine_ionic_motion': -0.9120070816755999, 'motion_component_glu': None, 'motion_component_asn': 2.675769466081158, 'motion_component_residue': 2.675769466081158, 'motion_component_ionic': -7.946827536390812, 'ionic_contributions': [{'ion_id': 1306, 'distance': 11.288458824157715, 'force': [-1.082576036453247, 1.5340907573699951, -1.8062469959259033], 'magnitude': 2.6053662300109863}, {'ion_id': 1308, 'distance': 9.986126899719238, 'force': [-1.6062496900558472, -1.6342322826385498, -2.415165901184082], 'magnitude': 3.329231023788452}, {'ion_id': 1320, 'distance': 10.916261672973633, 'force': [1.2217909097671509, -0.8660487532615662, -2.349320888519287], 'magnitude': 2.7860584259033203}, {'ion_id': 1403, 'distance': 13.08194351196289, 'force': [-0.18523018062114716, 0.009453874081373215, -1.931077003479004], 'magnitude': 1.939963459968567}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.3549933433532715, 'force': [3.173546075820923, -7.269976615905762, -2.2844626903533936], 'magnitude': 8.254860877990723}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.493684768676758, 'force': [-3.743788242340088, 8.962427139282227, 0.8637454509735107], 'magnitude': 9.751261711120605}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.609076023101807, 'force': [-1.943361520767212, 8.57589340209961, 4.0919671058654785], 'magnitude': 9.698803901672363}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.2177839279174805, 'force': [0.15768615901470184, -4.663626194000244, -2.099456787109375], 'magnitude': 5.1168341636657715}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.941163539886475, 'force': [5.086411952972412, -4.929412841796875, 3.856743812561035], 'magnitude': 8.065058708190918}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.714658260345459, 'force': [-1.1342309713363647, 2.9586288928985596, -2.8559513092041016], 'magnitude': 4.265726566314697}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.690225601196289, 'force': [4.250235557556152, 4.45625114440918, -3.940310478210449], 'magnitude': 7.310863494873047}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.7684526443481445, 'force': [-4.517857074737549, -6.293577194213867, 3.8695077896118164], 'magnitude': 8.659863471984863}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.785881519317627, 'force': [-5.477853775024414, -3.934474229812622, 6.131738662719727], 'magnitude': 9.115107536315918}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.165782928466797, 'force': [2.842543601989746, 1.7588046789169312, -4.0098395347595215], 'magnitude': 5.220369815826416}]}, 5218: {'frame': 5218, 'ionic_force': [2.5373760387301445, -1.672971323132515, -10.462154865264893], 'ionic_force_magnitude': 10.894668174604103, 'motion_vector': [-0.7376747131347656, 0.12036895751953125, 5.263938903808594], 'ionic_force_x': 2.5373760387301445, 'ionic_force_y': -1.672971323132515, 'ionic_force_z': -10.462154865264893, 'radial_force': 3.0392614579771906, 'axial_force': -10.462154865264893, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [2.102584421634674, -2.3916987776756287, 2.5022700428962708], 'asn_force_magnitude': 4.049992550710682, 'residue_force': [2.102584421634674, -2.3916987776756287, 2.5022700428962708], 'residue_force_magnitude': 4.049992550710682, 'total_force': [4.639960460364819, -4.064670100808144, -7.959884822368622], 'total_force_magnitude': 10.070280159336528, 'motion_component_total': -8.616634641110503, 'cosine_total_motion': -0.8556499426802643, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.5263093413579796, 'cosine_residue_motion': 0.5263093413579796, 'cosine_ionic_motion': -0.98655446689365, 'motion_component_glu': None, 'motion_component_asn': 2.1315489118692628, 'motion_component_residue': 2.1315489118692628, 'motion_component_ionic': -10.748183552979766, 'ionic_contributions': [{'ion_id': 1306, 'distance': 8.952473640441895, 'force': [-1.6688743829727173, 2.59674072265625, -2.762474775314331], 'magnitude': 4.142399311065674}, {'ion_id': 1308, 'distance': 9.649384498596191, 'force': [-1.0178943872451782, -2.646784543991089, -2.161548376083374], 'magnitude': 3.5656511783599854}, {'ion_id': 1320, 'distance': 7.298971652984619, 'force': [5.3220672607421875, -1.4583486318588257, -2.8955790996551514], 'magnitude': 6.231818199157715}, {'ion_id': 1403, 'distance': 11.194082260131836, 'force': [-0.09792245179414749, -0.1645788699388504, -2.642552614212036], 'magnitude': 2.6494827270507812}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.576210975646973, 'force': [4.152886867523193, -6.326608180999756, 0.826778769493103], 'magnitude': 7.612884044647217}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.947748184204102, 'force': [-5.19920539855957, 5.87307071685791, -1.7818294763565063], 'magnitude': 8.043606758117676}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.439992904663086, 'force': [-3.47602915763855, 9.667176246643066, -0.8839237093925476], 'magnitude': 10.311080932617188}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.6349406242370605, 'force': [1.550364375114441, -6.216604232788086, 1.0003122091293335], 'magnitude': 6.4846296310424805}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.114135265350342, 'force': [-6.343599796295166, 11.510722160339355, -4.780110836029053], 'magnitude': 13.985258102416992}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.1825482845306396, 'force': [11.394954681396484, -13.194110870361328, 8.603394508361816], 'magnitude': 19.44088363647461}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.1792473793029785, 'force': [2.8414037227630615, -16.464763641357422, 5.104458332061768], 'magnitude': 17.470474243164062}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.527759313583374, 'force': [0.3850836157798767, 10.552276611328125, -3.71500301361084], 'magnitude': 11.193751335144043}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.126480579376221, 'force': [-0.543602705001831, 5.102504730224609, -1.329128384590149], 'magnitude': 5.300720691680908}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.188117027282715, 'force': [-6.258123874664307, -3.698328733444214, 0.8218269348144531], 'magnitude': 7.315541744232178}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.952728748321533, 'force': [3.598452091217041, 0.8029664158821106, -1.3645052909851074], 'magnitude': 3.9313466548919678}]}, 5222: {'frame': 5222, 'ionic_force': [-11.94608449935913, 3.242609441280365, -10.622156023979187], 'ionic_force_magnitude': 16.31115107686353, 'motion_vector': [-3.9730682373046875, -1.5599021911621094, 2.0731430053710938], 'ionic_force_x': -11.94608449935913, 'ionic_force_y': 3.242609441280365, 'ionic_force_z': -10.622156023979187, 'radial_force': 12.378346046807266, 'axial_force': -10.622156023979187, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [5.115164041519165, 5.246052503585815, -3.320834696292877], 'asn_force_magnitude': 8.044495827715512, 'residue_force': [5.115164041519165, 5.246052503585815, -3.320834696292877], 'residue_force_magnitude': 8.044495827715512, 'total_force': [-6.830920457839966, 8.48866194486618, -13.942990720272064], 'total_force_magnitude': 17.695362277759354, 'motion_component_total': -3.162717724619622, 'cosine_total_motion': -0.1787314481034799, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.9271309648884625, 'cosine_residue_motion': -0.9271309648884625, 'cosine_ionic_motion': 0.26335256377243166, 'motion_component_glu': None, 'motion_component_asn': -7.458301178791093, 'motion_component_residue': -7.458301178791093, 'motion_component_ionic': 4.295583454171471, 'ionic_contributions': [{'ion_id': 1306, 'distance': 11.967347145080566, 'force': [-1.2669048309326172, 1.7904175519943237, -0.7504638433456421], 'magnitude': 2.3181540966033936}, {'ion_id': 1308, 'distance': 8.632686614990234, 'force': [-2.3145053386688232, -2.909573793411255, -2.4544501304626465], 'magnitude': 4.454983711242676}, {'ion_id': 1320, 'distance': 6.0926737785339355, 'force': [-7.233617305755615, 3.4570906162261963, -3.964205026626587], 'magnitude': 8.943802833557129}, {'ion_id': 1403, 'distance': 9.4161376953125, 'force': [-1.1310570240020752, 0.9046750664710999, -3.4530370235443115], 'magnitude': 3.74448823928833}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.4582486152648926, 'force': [3.716090440750122, -13.011960983276367, 14.444682121276855], 'magnitude': 19.793163299560547}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.1675169467926025, 'force': [3.275346517562866, 13.932584762573242, -13.4286470413208], 'magnitude': 19.62583351135254}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.677961826324463, 'force': [-7.439981460571289, 7.759405612945557, -19.83099937438965], 'magnitude': 22.557266235351562}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.7630958557128906, 'force': [1.382826805114746, -1.7291169166564941, 9.585070610046387], 'magnitude': 9.8374605178833}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.366880893707275, 'force': [3.6315255165100098, -2.2304391860961914, 5.933194637298584], 'magnitude': 7.305178642272949}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.433842182159424, 'force': [-4.09097957611084, -9.394994735717773, -1.3410942554473877], 'magnitude': 10.334436416625977}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.454866409301758, 'force': [2.5107436180114746, 6.456911563873291, 1.1302156448364258], 'magnitude': 7.019467830657959}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.850269317626953, 'force': [2.129592180252075, 3.4636623859405518, 0.18674296140670776], 'magnitude': 4.070257186889648}]}, 5223: {'frame': 5223, 'ionic_force': [-10.693952560424805, 0.50745789706707, -4.039891541004181], 'ionic_force_magnitude': 11.442851853667822, 'motion_vector': [1.1881523132324219, 0.9744796752929688, 2.5615386962890625], 'ionic_force_x': -10.693952560424805, 'ionic_force_y': 0.50745789706707, 'ionic_force_z': -4.039891541004181, 'radial_force': 10.705985936937894, 'axial_force': -4.039891541004181, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-0.4661531448364258, 3.332392692565918, -1.5015206933021545], 'asn_force_magnitude': 3.684657949433326, 'residue_force': [-0.4661531448364258, 3.332392692565918, -1.5015206933021545], 'residue_force_magnitude': 3.684657949433326, 'total_force': [-11.16010570526123, 3.839850589632988, -5.5414122343063354], 'total_force_magnitude': 13.038391827745821, 'motion_component_total': -7.938317948374027, 'cosine_total_motion': -0.6088417999128705, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.10473077513392179, 'cosine_residue_motion': -0.10473077513392179, 'cosine_ionic_motion': -0.6600121160185869, 'motion_component_glu': None, 'motion_component_asn': -0.385897083147519, 'motion_component_residue': -0.385897083147519, 'motion_component_ionic': -7.552420865226508, 'ionic_contributions': [{'ion_id': 1306, 'distance': 12.668959617614746, 'force': [-1.6322910785675049, 1.243991732597351, -0.25848662853240967], 'magnitude': 2.068502902984619}, {'ion_id': 1308, 'distance': 10.760255813598633, 'force': [-2.0935752391815186, -1.8744561672210693, -0.5705388188362122], 'magnitude': 2.8674304485321045}, {'ion_id': 1320, 'distance': 8.908306121826172, 'force': [-4.028995990753174, 0.7997772693634033, 0.7936450242996216], 'magnitude': 4.183578014373779}, {'ion_id': 1403, 'distance': 9.706404685974121, 'force': [-2.2542738914489746, 0.2554945647716522, -2.6964259147644043], 'magnitude': 3.523881435394287}, {'ion_id': 1469, 'distance': 14.983464241027832, 'force': [-0.6848163604736328, 0.08265049755573273, -1.3080852031707764], 'magnitude': 1.4788141250610352}], 'glu_contributions': [], 'asn_contributions': [{'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.253961563110352, 'force': [-2.46748423576355, 7.1519575119018555, 4.037117004394531], 'magnitude': 8.57538890838623}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.061633586883545, 'force': [3.046874761581421, -5.271973133087158, -4.689686298370361], 'magnitude': 7.685720920562744}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.454590797424316, 'force': [3.5123116970062256, -14.31281566619873, -4.390205383300781], 'magnitude': 15.377480506896973}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.5357630252838135, 'force': [-3.6557726860046387, 10.125402450561523, 2.877659559249878], 'magnitude': 11.143131256103516}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.922157287597656, 'force': [-0.9020826816558838, 5.639821529388428, 0.6635944247245789], 'magnitude': 5.749930381774902}]}, 5224: {'frame': 5224, 'ionic_force': [-13.356659054756165, 2.8882558345794678, -2.429133066907525], 'ionic_force_magnitude': 13.879591144112485, 'motion_vector': [0.0398406982421875, 2.6087303161621094, -0.5442276000976562], 'ionic_force_x': -13.356659054756165, 'ionic_force_y': 2.8882558345794678, 'ionic_force_z': -2.429133066907525, 'radial_force': 13.66537093792123, 'axial_force': -2.429133066907525, 'glu_force': [-2.154943585395813, 10.995372772216797, -1.4237671867012978], 'glu_force_magnitude': 11.294649939602927, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [-2.154943585395813, 10.995372772216797, -1.4237671867012978], 'residue_force_magnitude': 11.294649939602927, 'total_force': [-15.511602640151978, 13.883628606796265, -3.852900253608823], 'total_force_ma</t>
+          <t>{5213: {'frame': 5213, 'motion_vector': [-0.08104324340820312, -3.535572052001953, 0.40856170654296875], 'ionic_force': [8.349748060107231, 9.205024123191833, -18.89620530605316], 'ionic_force_magnitude': 22.61674903128917, 'radial_force': 12.427822084975631, 'axial_force': -18.89620530605316, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-11.033990144729614, 1.9732149839401245, -5.10729056596756], 'asn_force_magnitude': 12.317748690895481, 'residue_force': [-11.033990144729614, 1.9732149839401245, -5.10729056596756], 'residue_force_magnitude': 12.317748690895481, 'total_force': [-2.684242084622383, 11.178239107131958, -24.00349587202072], 'total_force_magnitude': 26.61439458607293, 'cosine_total_motion': -0.5183319967450323, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.18628470386856832, 'cosine_residue_motion': -0.18628470386856832, 'cosine_ionic_motion': -0.5084941299405185, 'motion_component_total': -13.79509228795936, 'motion_component_glu': None, 'motion_component_asn': -2.2946081672109098, 'motion_component_residue': -2.2946081672109098, 'motion_component_ionic': -11.50048412074845, 'motion_component_percent_total': 51.83319967450323, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 18.628470386856833, 'motion_component_percent_residue': 18.628470386856833, 'motion_component_percent_ionic': 50.849412994051846, 'ionic_contributions': [{'ion_id': 1306, 'distance': 11.115274429321289, 'force': [-0.7094604969024658, 2.2941157817840576, -1.2060950994491577], 'magnitude': 2.687185764312744, 'cosine_ionic_motion': -0.8933602571487427, 'motion_component_ionic': -2.400624990463257, 'motion_component_percent_ionic': 89.33602571487427}, {'ion_id': 1308, 'distance': 4.756705284118652, 'force': [4.778199672698975, 9.435524940490723, -10.170702934265137], 'magnitude': 14.673224449157715, 'cosine_ionic_motion': -0.7255885601043701, 'motion_component_ionic': -10.646723747253418, 'motion_component_percent_ionic': 72.55885601043701}, {'ion_id': 1320, 'distance': 6.789470195770264, 'force': [4.232130527496338, -3.0712902545928955, -4.9525957107543945], 'magnitude': 7.202219009399414, 'cosine_ionic_motion': 0.33121374249458313, 'motion_component_ionic': 2.3854739665985107, 'motion_component_percent_ionic': 33.12137424945831}, {'ion_id': 1403, 'distance': 11.246515274047852, 'force': [0.04887835681438446, 0.5466736555099487, -2.5668115615844727], 'magnitude': 2.624835729598999, 'cosine_ionic_motion': -0.3194900155067444, 'motion_component_ionic': -0.8386088013648987, 'motion_component_percent_ionic': 31.94900155067444}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.5150952339172363, 'force': [16.992422103881836, -6.173070430755615, 6.33919095993042], 'magnitude': 19.158145904541016, 'cosine_with_motion': 0.3377859890460968, 'motion_component': 6.471353530883789, 'motion_component_percent': 33.77859890460968}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.725060224533081, 'force': [-19.537765502929688, 15.083691596984863, -9.688909530639648], 'magnitude': 26.516353607177734, 'cosine_with_motion': -0.5900984406471252, 'motion_component': -15.647258758544922, 'motion_component_percent': 59.009844064712524}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.6749155521392822, 'force': [-20.53214454650879, -0.5899879932403564, -9.412881851196289], 'magnitude': 22.594676971435547, 'cosine_with_motion': -0.0011910652974620461, 'motion_component': -0.02691173553466797, 'motion_component_percent': 0.11910652974620461}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.237393856048584, 'force': [10.7410888671875, 3.150566339492798, 7.1675543785095215], 'magnitude': 13.291760444641113, 'cosine_with_motion': -0.19191370904445648, 'motion_component': -2.5508711338043213, 'motion_component_percent': 19.191370904445648}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.4853692054748535, 'force': [6.563553333282471, 0.7515674829483032, 2.0739171504974365], 'magnitude': 6.924320697784424, 'cosine_with_motion': -0.09500038623809814, 'motion_component': -0.6578131318092346, 'motion_component_percent': 9.500038623809814}, {'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.766394138336182, 'force': [-6.361416816711426, -3.1261937618255615, -0.6628996729850769], 'magnitude': 7.118999004364014, 'cosine_with_motion': 0.445773720741272, 'motion_component': 3.1734626293182373, 'motion_component_percent': 44.5773720741272}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.568770885467529, 'force': [12.717414855957031, 7.166444301605225, 0.7805547118186951], 'magnitude': 14.618475914001465, 'cosine_with_motion': -0.5005415678024292, 'motion_component': -7.317154884338379, 'motion_component_percent': 50.05415678024292}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.9164936542510986, 'force': [-8.516819953918457, -2.9974727630615234, -0.9801065325737], 'magnitude': 9.081942558288574, 'cosine_with_motion': 0.33674392104148865, 'motion_component': 3.058289051055908, 'motion_component_percent': 33.674392104148865}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.460243225097656, 'force': [-5.205928802490234, -4.682491779327393, -0.09132105112075806], 'magnitude': 7.002553939819336, 'cosine_with_motion': 0.6795183420181274, 'motion_component': 4.758363723754883, 'motion_component_percent': 67.95183420181274}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.316735744476318, 'force': [2.1056063175201416, -6.609838008880615, -0.6323891282081604], 'magnitude': 6.965877532958984, 'cosine_with_motion': 0.925071120262146, 'motion_component': 6.443932056427002, 'motion_component_percent': 92.5071120262146}]}, 5214: {'frame': 5214, 'motion_vector': [-2.800647735595703, -0.17963790893554688, 2.6386032104492188], 'ionic_force': [-0.392241433262825, -3.0962782502174377, -10.358314990997314], 'ionic_force_magnitude': 10.818293848729445, 'radial_force': 3.121024246098968, 'axial_force': -10.358314990997314, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [16.765697956085205, -12.439022541046143, 0.22667193412780762], 'asn_force_magnitude': 20.8774828438932, 'residue_force': [16.765697956085205, -12.439022541046143, 0.22667193412780762], 'residue_force_magnitude': 20.8774828438932, 'total_force': [16.37345652282238, -15.53530079126358, -10.131643056869507], 'total_force_magnitude': 24.740368635321538, 'cosine_total_motion': -0.7324081270733893, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.5486425501739778, 'cosine_residue_motion': -0.5486425501739778, 'cosine_ionic_motion': -0.6161573830236546, 'motion_component_total': -18.12004705530107, 'motion_component_glu': None, 'motion_component_asn': -11.454275428687035, 'motion_component_residue': -11.454275428687035, 'motion_component_ionic': -6.665771626614035, 'motion_component_percent_total': 73.24081270733893, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 54.86425501739778, 'motion_component_percent_residue': 54.86425501739778, 'motion_component_percent_ionic': 61.615738302365465, 'ionic_contributions': [{'ion_id': 1306, 'distance': 8.311978340148926, 'force': [-1.26851487159729, 3.9690990447998047, -2.3935248851776123], 'magnitude': 4.805397033691406, 'cosine_ionic_motion': -0.18777962028980255, 'motion_component_ionic': -0.9023556113243103, 'motion_component_percent_ionic': 18.777962028980255}, {'ion_id': 1308, 'distance': 8.85319995880127, 'force': [-1.3250770568847656, -3.1238503456115723, -2.5353305339813232], 'magnitude': 4.2358198165893555, 'cosine_ionic_motion': -0.1481626033782959, 'motion_component_ionic': -0.6275901198387146, 'motion_component_percent_ionic': 14.81626033782959}, {'ion_id': 1320, 'distance': 8.383258819580078, 'force': [2.0835518836975098, -3.640300989151001, -2.173349618911743], 'magnitude': 4.724026679992676, 'cosine_ionic_motion': -0.5998743772506714, 'motion_component_ionic': -2.83382248878479, 'motion_component_percent_ionic': 59.98743772506714}, {'ion_id': 1403, 'distance': 10.072875022888184, 'force': [0.11779861152172089, -0.3012259602546692, -3.2561099529266357], 'magnitude': 3.272134780883789, 'cosine_ionic_motion': -0.7035171985626221, 'motion_component_ionic': -2.3020031452178955, 'motion_component_percent_ionic': 70.3517198562622}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.220438480377197, 'force': [-7.028218746185303, 7.975660800933838, -3.5152876377105713], 'magnitude': 11.196619033813477, 'cosine_with_motion': 0.20810221135616302, 'motion_component': 2.3300411701202393, 'motion_component_percent': 20.810221135616302}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.340437412261963, 'force': [4.018090724945068, -5.689406394958496, 2.4826714992523193], 'magnitude': 7.394461154937744, 'cosine_with_motion': -0.12921223044395447, 'motion_component': -0.9554547667503357, 'motion_component_percent': 12.921223044395447}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.443244934082031, 'force': [3.4803147315979004, -2.686570167541504, 1.6661407947540283], 'magnitude': 4.701731204986572, 'cosine_with_motion': -0.26879724860191345, 'motion_component': -1.2638124227523804, 'motion_component_percent': 26.879724860191345}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.7183046340942383, 'force': [-10.050923347473145, 13.65013599395752, -2.4068522453308105], 'magnitude': 17.121337890625, 'cosine_with_motion': 0.2933393716812134, 'motion_component': 5.02236270904541, 'motion_component_percent': 29.333937168121338}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.5175106525421143, 'force': [20.784893035888672, -22.801639556884766, 3.652261972427368], 'magnitude': 31.068723678588867, 'cosine_with_motion': -0.3716505765914917, 'motion_component': -11.546709060668945, 'motion_component_percent': 37.16505765914917}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.250736236572266, 'force': [5.533113479614258, -15.4774751663208, 3.876791000366211], 'magnitude': 16.887779235839844, 'cosine_with_motion': -0.038225430995225906, 'motion_component': -0.6455426216125488, 'motion_component_percent': 3.8225430995225906}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.822483539581299, 'force': [-1.0360026359558105, 9.108904838562012, -2.6181509494781494], 'magnitude': 9.534157752990723, 'cosine_with_motion': -0.15365438163280487, 'motion_component': -1.4649651050567627, 'motion_component_percent': 15.365438163280487}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.256087779998779, 'force': [-1.7162542343139648, 4.579953193664551, -1.2270251512527466], 'magnitude': 5.04252815246582, 'cosine_with_motion': 0.038419459015131, 'motion_component': 0.19373120367527008, 'motion_component_percent': 3.8419459015130997}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.542922496795654, 'force': [7.132328510284424, 2.891019582748413, -0.3643268942832947], 'magnitude': 7.704598426818848, 'cosine_with_motion': -0.7229446172714233, 'motion_component': -5.569997787475586, 'motion_component_percent': 72.29446172714233}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.470865249633789, 'force': [-8.900879859924316, -4.187804698944092, -0.5291113257408142], 'magnitude': 9.851057052612305, 'cosine_with_motion': 0.6399633288383484, 'motion_component': 6.304315090179443, 'motion_component_percent': 63.99633288383484}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.4902024269104, 'force': [4.549236297607422, 0.19819903373718262, -0.7904391288757324], 'magnitude': 4.621647834777832, 'cosine_with_motion': -0.834820032119751, 'motion_component': -3.8582441806793213, 'motion_component_percent': 83.4820032119751}]}, 5215: {'frame': 5215, 'motion_vector': [0.9844284057617188, -0.2884941101074219, -5.571617126464844], 'ionic_force': [-7.000141829252243, -6.792514324188232, -8.448651671409607], 'ionic_force_magnitude': 12.904260983828621, 'radial_force': 9.753985671198684, 'axial_force': -8.448651671409607, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [3.558483213186264, 0.47542114555835724, -0.7009260654449463], 'asn_force_magnitude': 3.6578853718224402, 'residue_force': [3.558483213186264, 0.47542114555835724, -0.7009260654449463], 'residue_force_magnitude': 3.6578853718224402, 'total_force': [-3.441658616065979, -6.317093178629875, -9.149577736854553], 'total_force_magnitude': 11.638962712363064, 'cosine_total_motion': 0.7493774725176083, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.35087796957467987, 'cosine_residue_motion': 0.35087796957467987, 'cosine_ionic_motion': 0.5764378973144713, 'motion_component_total': 8.72197646011732, 'motion_component_glu': None, 'motion_component_asn': 1.2834713922019807, 'motion_component_residue': 1.2834713922019807, 'motion_component_ionic': 7.43850506791534, 'motion_component_percent_total': 74.93774725176084, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 35.08779695746799, 'motion_component_percent_residue': 35.08779695746799, 'motion_component_percent_ionic': 57.64378973144713, 'ionic_contributions': [{'ion_id': 1306, 'distance': 8.160512924194336, 'force': [-3.8426830768585205, 2.8841068744659424, -1.3305236101150513], 'magnitude': 4.98543643951416, 'cosine_ionic_motion': 0.09907559305429459, 'motion_component_ionic': 0.49393507838249207, 'motion_component_percent_ionic': 9.907559305429459}, {'ion_id': 1308, 'distance': 9.352710723876953, 'force': [-2.1365599632263184, -3.032615900039673, -0.8023586273193359], 'magnitude': 3.7954483032226562, 'cosine_ionic_motion': 0.15077678859233856, 'motion_component_ionic': 0.5722655057907104, 'motion_component_percent_ionic': 15.077678859233856}, {'ion_id': 1320, 'distance': 7.378998756408691, 'force': [0.5601136684417725, -6.005922317504883, -0.8906189203262329], 'magnitude': 6.097379207611084, 'cosine_ionic_motion': 0.20977315306663513, 'motion_component_ionic': 1.2790664434432983, 'motion_component_percent_ionic': 20.977315306663513}, {'ion_id': 1403, 'distance': 9.133903503417969, 'force': [-1.2336101531982422, -0.5227363109588623, -3.747150182723999], 'magnitude': 3.9794700145721436, 'cosine_ionic_motion': 0.8788779377937317, 'motion_component_ionic': 3.4974684715270996, 'motion_component_percent_ionic': 87.88779377937317}, {'ion_id': 1469, 'distance': 13.903539657592773, 'force': [-0.34740230441093445, -0.11534667015075684, -1.6780003309249878], 'magnitude': 1.7174626588821411, 'cosine_ionic_motion': 0.9291436672210693, 'motion_component_ionic': 1.5957695245742798, 'motion_component_percent_ionic': 92.91436672210693}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.461219310760498, 'force': [-1.7710473537445068, 7.48703670501709, -6.744088649749756], 'magnitude': 10.231082916259766, 'cosine_with_motion': 0.580935001373291, 'motion_component': 5.943594455718994, 'motion_component_percent': 58.0935001373291}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.108263969421387, 'force': [0.19433173537254333, -3.524526357650757, 4.005063533782959], 'magnitude': 5.33859395980835, 'cosine_with_motion': -0.6978633999824524, 'motion_component': -3.725609302520752, 'motion_component_percent': 69.78633999824524}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.204665660858154, 'force': [1.7985098361968994, -3.607750654220581, 3.1931893825531006], 'magnitude': 5.142660617828369, 'cosine_with_motion': -0.5141631960868835, 'motion_component': -2.6441667079925537, 'motion_component_percent': 51.416319608688354}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.722692489624023, 'force': [-5.9168829917907715, 3.027146816253662, 2.8412938117980957], 'magnitude': 7.228144645690918, 'cosine_with_motion': -0.5501589775085449, 'motion_component': -3.9766287803649902, 'motion_component_percent': 55.01589775085449}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.113308906555176, 'force': [6.542529582977295, -1.7497735023498535, -3.294235944747925], 'magnitude': 7.531161308288574, 'cosine_with_motion': 0.5929698348045349, 'motion_component': 4.465751647949219, 'motion_component_percent': 59.29698348045349}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.2527875900268555, 'force': [7.63437032699585, -6.52311372756958, -4.633557319641113], 'magnitude': 11.059135437011719, 'cosine_with_motion': 0.5620450377464294, 'motion_component': 6.215732097625732, 'motion_component_percent': 56.204503774642944}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.436313629150391, 'force': [-4.377902507781982, 4.1760382652282715, 3.6738297939300537], 'magnitude': 7.078301429748535, 'cosine_with_motion': -0.6479642391204834, 'motion_component': -4.586486339569092, 'motion_component_percent': 64.79642391204834}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.813601493835449, 'force': [-2.6524696350097656, 2.8659005165100098, 1.3190717697143555], 'magnitude': 4.121763229370117, 'cosine_with_motion': -0.4619663655757904, 'motion_component': -1.9041160345077515, 'motion_component_percent': 46.19663655757904}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.534676551818848, 'force': [6.397800922393799, 4.249890327453613, 8.574560165405273], 'magnitude': 11.511581420898438, 'cosine_with_motion': -0.6547769904136658, 'motion_component': -7.5375189781188965, 'motion_component_percent': 65.47769904136658}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.575444221496582, 'force': [-2.910076379776001, -4.051925182342529, -7.973955154418945], 'magnitude': 9.40588092803955, 'cosine_with_motion': 0.8019247055053711, 'motion_component': 7.542808532714844, 'motion_component_percent': 80.19247055053711}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.497517108917236, 'force': [-9.882165908813477, -1.5354973077774048, -11.29392147064209], 'magnitude': 15.085344314575195, 'cosine_with_motion': 0.6276450157165527, 'motion_component': 9.468240737915039, 'motion_component_percent': 62.76450157165527}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.384892463684082, 'force': [3.943589925765991, -0.5436141490936279, 6.053659439086914], 'magnitude': 7.245288848876953, 'cosine_with_motion': -0.7233178615570068, 'motion_component': -5.240646839141846, 'motion_component_percent': 72.33178615570068}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.9015960693359375, 'force': [4.557895660400391, 0.20560939610004425, 3.578164577484131], 'magnitude': 5.798271179199219, 'cosine_with_motion': -0.47212013602256775, 'motion_component': -2.737480640411377, 'motion_component_percent': 47.212013602256775}]}, 5216: {'frame': 5216, 'motion_vector': [0.49591064453125, 1.3578147888183594, -0.21898651123046875], 'ionic_force': [-1.1580060422420502, -1.9418916404247284, -7.661372423171997], 'ionic_force_magnitude': 7.988025321915354, 'radial_force': 2.2609558016512707, 'axial_force': -7.661372423171997, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-3.7864845395088196, -14.654212445020676, 9.05460637807846], 'asn_force_magnitude': 17.637156919800802, 'residue_force': [-3.7864845395088196, -14.654212445020676, 9.05460637807846], 'residue_force_magnitude': 17.637156919800802, 'total_force': [-4.94449058175087, -16.596104085445404, 1.3932339549064636], 'total_force_magnitude': 17.37296056465521, 'cosine_total_motion': -0.9957362669512017, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.9213599580828115, 'cosine_residue_motion': -0.9213599580828115, 'cosine_ionic_motion': -0.13128610588344053, 'motion_component_total': -17.298886898540218, 'motion_component_glu': None, 'motion_component_asn': -16.250170160327635, 'motion_component_residue': -16.250170160327635, 'motion_component_ionic': -1.0487167382125833, 'motion_component_percent_total': 99.57362669512017, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 92.13599580828115, 'motion_component_percent_residue': 92.13599580828115, 'motion_component_percent_ionic': 13.128610588344053, 'ionic_contributions': [{'ion_id': 1306, 'distance': 10.266419410705566, 'force': [-1.4940450191497803, 1.5567138195037842, -2.294883966445923], 'magnitude': 3.1499240398406982, 'cosine_ionic_motion': 0.40721917152404785, 'motion_component_ionic': 1.2827094793319702, 'motion_component_percent_ionic': 40.721917152404785}, {'ion_id': 1308, 'distance': 12.706043243408203, 'force': [-0.5920225381851196, -1.5384231805801392, -1.2295265197753906], 'magnitude': 2.0564465522766113, 'cosine_ionic_motion': -0.7028663754463196, 'motion_component_ionic': -1.4454071521759033, 'motion_component_percent_ionic': 70.28663754463196}, {'ion_id': 1320, 'distance': 10.449557304382324, 'force': [1.186414122581482, -1.7023833990097046, -2.2223496437072754], 'magnitude': 3.0404810905456543, 'cosine_ionic_motion': -0.27816012501716614, 'motion_component_ionic': -0.845740556716919, 'motion_component_percent_ionic': 27.816012501716614}, {'ion_id': 1403, 'distance': 13.051283836364746, 'force': [-0.2583526074886322, -0.2577988803386688, -1.9146122932434082], 'magnitude': 1.9490886926651, 'cosine_ionic_motion': -0.020665349438786507, 'motion_component_ionic': -0.0402785986661911, 'motion_component_percent_ionic': 2.0665349438786507}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.96173620223999, 'force': [1.6038880348205566, -6.3169097900390625, -1.371645450592041], 'magnitude': 6.660121440887451, 'cosine_with_motion': -0.7683257460594177, 'motion_component': -5.117142677307129, 'motion_component_percent': 76.83257460594177}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.816272258758545, 'force': [-2.506654739379883, 8.01327133178711, 1.2502413988113403], 'magnitude': 8.488753318786621, 'cosine_with_motion': 0.7544751763343811, 'motion_component': 6.4045538902282715, 'motion_component_percent': 75.44751763343811}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.8918938636779785, 'force': [-0.36741095781326294, -3.8968489170074463, -0.8850693106651306], 'magnitude': 4.012950420379639, 'cosine_with_motion': -0.8998672366142273, 'motion_component': -3.6111226081848145, 'motion_component_percent': 89.98672366142273}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.597157955169678, 'force': [-5.129405498504639, 3.937967300415039, -3.9083101749420166], 'magnitude': 7.556009292602539, 'cosine_with_motion': 0.33123233914375305, 'motion_component': 2.5027947425842285, 'motion_component_percent': 33.123233914375305}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.731990814208984, 'force': [6.930484294891357, -3.6226212978363037, 4.022002696990967], 'magnitude': 8.79383373260498, 'cosine_with_motion': -0.18377022445201874, 'motion_component': -1.6160447597503662, 'motion_component_percent': 18.377022445201874}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.536361217498779, 'force': [4.822237014770508, -5.848729133605957, 6.453319072723389], 'magnitude': 9.955246925354004, 'cosine_with_motion': -0.4784146249294281, 'motion_component': -4.762735843658447, 'motion_component_percent': 47.84146249294281}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.722114562988281, 'force': [-2.436523914337158, 3.613025188446045, -4.476563930511475], 'magnitude': 6.247417449951172, 'cosine_with_motion': 0.5121371150016785, 'motion_component': 3.1995344161987305, 'motion_component_percent': 51.21371150016785}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.7144429683685303, 'force': [12.244051933288574, 6.392899036407471, -10.1771879196167], 'magnitude': 17.15695571899414, 'cosine_with_motion': 0.676963746547699, 'motion_component': 11.61463737487793, 'motion_component_percent': 67.6963746547699}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.6490366458892822, 'force': [-17.539894104003906, -14.308707237243652, 16.582679748535156], 'magnitude': 28.06015396118164, 'cosine_with_motion': -0.7741195559501648, 'motion_component': -21.721914291381836, 'motion_component_percent': 77.41195559501648}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.133080005645752, 'force': [-13.984121322631836, -1.2258847951889038, 11.046565055847168], 'magnitude': 17.862951278686523, 'cosine_with_motion': -0.4219001829624176, 'motion_component': -7.536382675170898, 'motion_component_percent': 42.19001829624176}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.625009536743164, 'force': [8.369632720947266, -1.6478105783462524, -6.29440450668335], 'magnitude': 10.601205825805664, 'cosine_with_motion': 0.21236783266067505, 'motion_component': 2.2513551712036133, 'motion_component_percent': 21.236783266067505}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.134454250335693, 'force': [4.2072319984436035, 0.2561364471912384, -3.1870203018188477], 'magnitude': 5.2842698097229, 'cosine_with_motion': 0.4054102599620819, 'motion_component': 2.1422972679138184, 'motion_component_percent': 40.54102599620819}]}, 5217: {'frame': 5217, 'motion_vector': [1.0223388671875, -0.4985237121582031, 2.0433120727539062], 'ionic_force': [-1.6522649973630905, -0.9567364044487476, -8.501810789108276], 'ionic_force_magnitude': 8.713559023895268, 'radial_force': 1.9092732044180507, 'axial_force': -8.501810789108276, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-1.3066682368516922, -0.37906181812286377, 3.6236820220947266], 'asn_force_magnitude': 3.870677090692047, 'residue_force': [-1.3066682368516922, -0.37906181812286377, 3.6236820220947266], 'residue_force_magnitude': 3.870677090692047, 'total_force': [-2.9589332342147827, -1.3357982225716114, -4.87812876701355], 'total_force_magnitude': 5.859674312069858, 'cosine_total_motion': -0.8995479594236555, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.6912923510244952, 'cosine_residue_motion': 0.6912923510244952, 'cosine_ionic_motion': -0.9120070816755999, 'motion_component_total': -5.271058070309653, 'motion_component_glu': None, 'motion_component_asn': 2.675769466081158, 'motion_component_residue': 2.675769466081158, 'motion_component_ionic': -7.946827536390812, 'motion_component_percent_total': 89.95479594236555, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 69.12923510244951, 'motion_component_percent_residue': 69.12923510244951, 'motion_component_percent_ionic': 91.20070816755998, 'ionic_contributions': [{'ion_id': 1306, 'distance': 11.288458824157715, 'force': [-1.082576036453247, 1.5340907573699951, -1.8062469959259033], 'magnitude': 2.6053662300109863, 'cosine_ionic_motion': -0.9129267930984497, 'motion_component_ionic': -2.3785085678100586, 'motion_component_percent_ionic': 91.29267930984497}, {'ion_id': 1308, 'distance': 9.986126899719238, 'force': [-1.6062496900558472, -1.6342322826385498, -2.415165901184082], 'magnitude': 3.329231023788452, 'cosine_ionic_motion': -0.7401330471038818, 'motion_component_ionic': -2.464073896408081, 'motion_component_percent_ionic': 74.01330471038818}, {'ion_id': 1320, 'distance': 10.916261672973633, 'force': [1.2217909097671509, -0.8660487532615662, -2.349320888519287], 'magnitude': 2.7860584259033203, 'cosine_ionic_motion': -0.47880297899246216, 'motion_component_ionic': -1.3339730501174927, 'motion_component_percent_ionic': 47.880297899246216}, {'ion_id': 1403, 'distance': 13.08194351196289, 'force': [-0.18523018062114716, 0.009453874081373215, -1.931077003479004], 'magnitude': 1.939963459968567, 'cosine_ionic_motion': -0.9125285744667053, 'motion_component_ionic': -1.770272135734558, 'motion_component_percent_ionic': 91.25285744667053}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.3549933433532715, 'force': [3.173546075820923, -7.269976615905762, -2.2844626903533936], 'magnitude': 8.254860877990723, 'cosine_with_motion': 0.11400625109672546, 'motion_component': 0.9411057233810425, 'motion_component_percent': 11.400625109672546}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.493684768676758, 'force': [-3.743788242340088, 8.962427139282227, 0.8637454509735107], 'magnitude': 9.751261711120605, 'cosine_with_motion': -0.28637734055519104, 'motion_component': -2.7925403118133545, 'motion_component_percent': 28.637734055519104}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.609076023101807, 'force': [-1.943361520767212, 8.57589340209961, 4.0919671058654785], 'magnitude': 9.698803901672363, 'cosine_with_motion': 0.0925484150648117, 'motion_component': 0.8976089358329773, 'motion_component_percent': 9.25484150648117}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.2177839279174805, 'force': [0.15768615901470184, -4.663626194000244, -2.099456787109375], 'magnitude': 5.1168341636657715, 'cosine_with_motion': -0.15073631703853607, 'motion_component': -0.7712927460670471, 'motion_component_percent': 15.073631703853607}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.941163539886475, 'force': [5.086411952972412, -4.929412841796875, 3.856743812561035], 'magnitude': 8.065058708190918, 'cosine_with_motion': 0.8238353729248047, 'motion_component': 6.644280433654785, 'motion_component_percent': 82.38353729248047}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.714658260345459, 'force': [-1.1342309713363647, 2.9586288928985596, -2.8559513092041016], 'magnitude': 4.265726566314697, 'cosine_with_motion': -0.8490812182426453, 'motion_component': -3.6219482421875, 'motion_component_percent': 84.90812182426453}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.690225601196289, 'force': [4.250235557556152, 4.45625114440918, -3.940310478210449], 'magnitude': 7.310863494873047, 'cosine_with_motion': -0.34671032428741455, 'motion_component': -2.5347518920898438, 'motion_component_percent': 34.671032428741455}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.7684526443481445, 'force': [-4.517857074737549, -6.293577194213867, 3.8695077896118164], 'magnitude': 8.659863471984863, 'cosine_with_motion': 0.3172759711742401, 'motion_component': 2.7475666999816895, 'motion_component_percent': 31.72759711742401}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.785881519317627, 'force': [-5.477853775024414, -3.934474229812622, 6.131738662719727], 'magnitude': 9.115107536315918, 'cosine_with_motion': 0.4170668423175812, 'motion_component': 3.8016090393066406, 'motion_component_percent': 41.70668423175812}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.165782928466797, 'force': [2.842543601989746, 1.7588046789169312, -4.0098395347595215], 'magnitude': 5.220369815826416, 'cosine_with_motion': -0.5049198865890503, 'motion_component': -2.635868549346924, 'motion_component_percent': 50.49198865890503}]}, 5218: {'frame': 5218, 'motion_vector': [-0.7376747131347656, 0.12036895751953125, 5.263938903808594], 'ionic_force': [2.5373760387301445, -1.672971323132515, -10.462154865264893], 'ionic_force_magnitude': 10.894668174604103, 'radial_force': 3.0392614579771906, 'axial_force': -10.462154865264893, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [2.102584421634674, -2.3916987776756287, 2.5022700428962708], 'asn_force_magnitude': 4.049992550710682, 'residue_force': [2.102584421634674, -2.3916987776756287, 2.5022700428962708], 'residue_force_magnitude': 4.049992550710682, '</t>
         </is>
       </c>
     </row>
@@ -643,7 +643,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>{5293: {'frame': 5293, 'ionic_force': [-7.19414022564888, -9.335815489292145, -6.3991100788116455], 'ionic_force_magnitude': 13.411253268697719, 'motion_vector': [3.6029815673828125, -0.9414405822753906, -2.305633544921875], 'ionic_force_x': -7.19414022564888, 'ionic_force_y': -9.335815489292145, 'ionic_force_z': -6.3991100788116455, 'radial_force': 11.786140353669918, 'axial_force': -6.3991100788116455, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-5.293145418167114, 2.4644975066184998, -13.945229291915894], 'asn_force_magnitude': 15.118219352228667, 'residue_force': [-5.293145418167114, 2.4644975066184998, -13.945229291915894], 'residue_force_magnitude': 15.118219352228667, 'total_force': [-12.487285643815994, -6.871317982673645, -20.34433937072754], 'total_force_magnitude': 24.840278943695495, 'motion_component_total': 1.9142044591863385, 'cosine_total_motion': 0.0770605057827729, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.16251661081762375, 'cosine_residue_motion': 0.16251661081762375, 'cosine_ionic_motion': -0.04047029018548834, 'motion_component_glu': None, 'motion_component_asn': 2.4569617707216143, 'motion_component_residue': 2.4569617707216143, 'motion_component_ionic': -0.5427573115352757, 'ionic_contributions': [{'ion_id': 1306, 'distance': 9.595380783081055, 'force': [-2.7549750804901123, 2.149670362472534, -0.8896871209144592], 'magnitude': 3.6058998107910156}, {'ion_id': 1309, 'distance': 7.038130283355713, 'force': [-0.4600997269153595, -6.4237165451049805, -1.8560487031936646], 'magnitude': 6.702293872833252}, {'ion_id': 1320, 'distance': 8.00695514678955, 'force': [-2.2913060188293457, -4.553028583526611, 0.9146720767021179], 'magnitude': 5.178492069244385}, {'ion_id': 1469, 'distance': 10.095939636230469, 'force': [-1.280375599861145, -0.43071743845939636, -2.963862419128418], 'magnitude': 3.2572009563446045}, {'ion_id': 2436, 'distance': 14.155181884765625, 'force': [-0.4073837995529175, -0.0780232846736908, -1.6041839122772217], 'magnitude': 1.656941533088684}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.7163825035095215, 'force': [1.3641202449798584, 4.213038921356201, -4.0867109298706055], 'magnitude': 6.02592134475708}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.1833295822143555, 'force': [-4.183377742767334, 2.830166816711426, 1.1724398136138916], 'magnitude': 5.185084819793701}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.6503655910491943, 'force': [11.936121940612793, 8.980183601379395, 9.615899085998535], 'magnitude': 17.764577865600586}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.822566270828247, 'force': [-11.983016967773438, -10.793547630310059, -18.729280471801758], 'magnitude': 24.715972900390625}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.187878608703613, 'force': [-14.870417594909668, -5.1708245277404785, -7.405556678771973], 'magnitude': 17.398534774780273}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.026407241821289, 'force': [7.773963928222656, 0.5124548077583313, 3.624950408935547], 'magnitude': 8.59286880493164}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.092360496520996, 'force': [4.669460773468018, 1.893025517463684, 1.8630294799804688], 'magnitude': 5.371991157531738}]}, 5294: {'frame': 5294, 'ionic_force': [-3.9219388999044895, -4.9589075446128845, -9.572859406471252], 'ionic_force_magnitude': 11.472227594790288, 'motion_vector': [-1.1986160278320312, 0.10608673095703125, 0.8895950317382812], 'ionic_force_x': -3.9219388999044895, 'ionic_force_y': -4.9589075446128845, 'ionic_force_z': -9.572859406471252, 'radial_force': 6.322370502477898, 'axial_force': -9.572859406471252, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-2.3613901138305664, -2.0234079360961914, -5.287694956175983], 'asn_force_magnitude': 6.134334592694037, 'residue_force': [-2.3613901138305664, -2.0234079360961914, -5.287694956175983], 'residue_force_magnitude': 6.134334592694037, 'total_force': [-6.283329013735056, -6.982315480709076, -14.860554362647235], 'total_force_magnitude': 17.580359180977734, 'motion_component_total': -4.2964192885545724, 'cosine_total_motion': -0.24438745786282773, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.227478088410098, 'cosine_residue_motion': -0.227478088410098, 'cosine_ionic_motion': -0.2528709056520096, 'motion_component_glu': None, 'motion_component_asn': -1.3954267068139767, 'motion_component_residue': -1.3954267068139767, 'motion_component_ionic': -2.9009925817405957, 'ionic_contributions': [{'ion_id': 1306, 'distance': 7.554628372192383, 'force': [-4.087786674499512, 1.854230284690857, -3.7001771926879883], 'magnitude': 5.817171096801758}, {'ion_id': 1309, 'distance': 9.034814834594727, 'force': [1.4283074140548706, -3.2946081161499023, -1.909952163696289], 'magnitude': 4.067237377166748}, {'ion_id': 1320, 'distance': 9.996163368225098, 'force': [-1.2332184314727783, -2.8408944606781006, -1.2032557725906372], 'magnitude': 3.3225491046905518}, {'ion_id': 1469, 'distance': 10.809033393859863, 'force': [-0.029241207987070084, -0.6776352524757385, -2.759474277496338], 'magnitude': 2.841609239578247}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.8706774711608887, 'force': [-13.338183403015137, 7.705677509307861, -3.5144574642181396], 'magnitude': 15.799874305725098}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.3188631534576416, 'force': [16.086706161499023, -4.274590015411377, 6.520899772644043], 'magnitude': 17.876699447631836}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.574234962463379, 'force': [15.354435920715332, -18.03443145751953, 3.0851986408233643], 'magnitude': 23.885517120361328}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.0706281661987305, 'force': [-6.634010314941406, 12.520920753479004, -4.184329032897949], 'magnitude': 14.774713516235352}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.395316123962402, 'force': [-4.284043788909912, 5.80040979385376, 0.01454452145844698], 'magnitude': 7.210963249206543}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.871678113937378, 'force': [14.96583366394043, 3.221412420272827, 3.876132011413574], 'magnitude': 15.791708946228027}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.7660417556762695, 'force': [-22.42108726501465, -7.137618064880371, -10.426596641540527], 'magnitude': 25.736446380615234}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.390989303588867, 'force': [-15.354634284973145, 1.2392737865447998, -3.62868595123291], 'magnitude': 15.826179504394531}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.925269365310669, 'force': [8.349770545959473, -2.6006577014923096, 2.2944328784942627], 'magnitude': 9.041377067565918}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.2881178855896, 'force': [4.913822650909424, -0.4638049602508545, 0.6751663088798523], 'magnitude': 4.981627941131592}]}, 5295: {'frame': 5295, 'ionic_force': [-4.847121506929398, -6.3855297565460205, -10.225951194763184], 'ionic_force_magnitude': 12.993831421576576, 'motion_vector': [1.4610366821289062, 0.4837226867675781, -0.33788299560546875], 'ionic_force_x': -4.847121506929398, 'ionic_force_y': -6.3855297565460205, 'ionic_force_z': -10.225951194763184, 'radial_force': 8.016830868533537, 'axial_force': -10.225951194763184, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-2.7353638410568237, 1.8772039078176022, -16.558398723602295], 'asn_force_magnitude': 16.887471040516424, 'residue_force': [-2.7353638410568237, 1.8772039078176022, -16.558398723602295], 'residue_force_magnitude': 16.887471040516424, 'total_force': [-7.582485347986221, -4.508325848728418, -26.78434991836548], 'total_force_magnitude': 28.199654014902087, 'motion_component_total': -2.6712792367599008, 'cosine_total_motion': -0.09472737627732117, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.09419181356133025, 'cosine_residue_motion': 0.09419181356133025, 'cosine_ionic_motion': -0.32799723362991534, 'motion_component_glu': None, 'motion_component_asn': 1.5906615237706867, 'motion_component_residue': 1.5906615237706867, 'motion_component_ionic': -4.261940760530587, 'ionic_contributions': [{'ion_id': 1306, 'distance': 7.963080883026123, 'force': [-3.9522693157196045, 1.6182080507278442, -3.028805732727051], 'magnitude': 5.235713481903076}, {'ion_id': 1309, 'distance': 8.245342254638672, 'force': [1.2909294366836548, -4.2322163581848145, -2.066220760345459], 'magnitude': 4.883382320404053}, {'ion_id': 1320, 'distance': 9.006513595581055, 'force': [-1.8195945024490356, -3.148383855819702, -1.8783209323883057], 'magnitude': 4.09283971786499}, {'ion_id': 1469, 'distance': 9.98206615447998, 'force': [-0.36618712544441223, -0.6231375932693481, -3.252603769302368], 'magnitude': 3.331940174102783}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.451868057250977, 'force': [-0.9308732748031616, 6.142979145050049, -2.2990808486938477], 'magnitude': 6.624838829040527}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.322166442871094, 'force': [-11.900971412658691, 3.9270126819610596, -1.8734612464904785], 'magnitude': 12.671401023864746}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.7789976596832275, 'force': [13.675838470458984, -0.526833713054657, 1.6771659851074219], 'magnitude': 13.78836441040039}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.9603607654571533, 'force': [15.479023933410645, -10.661806106567383, 5.022245407104492], 'magnitude': 19.455005645751953}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.210261821746826, 'force': [-9.407450675964355, 7.921640396118164, -5.609560012817383], 'magnitude': 13.51738452911377}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.790666103363037, 'force': [-4.324090003967285, 3.947477340698242, -1.601058006286621], 'magnitude': 6.0699028968811035}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.3971450328826904, 'force': [17.317733764648438, 6.5973801612854, 8.791823387145996], 'magnitude': 20.511594772338867}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.571812391281128, 'force': [-19.24126625061035, -12.519775390625, -18.95565414428711], 'magnitude': 29.77058982849121}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.7295291423797607, 'force': [-20.737747192382812, 0.04725603386759758, -7.156125545501709], 'magnitude': 21.937788009643555}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.431196928024292, 'force': [10.592588424682617, -3.138904094696045, 4.237466812133789], 'magnitude': 11.832656860351562}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.509426116943359, 'force': [6.74185037612915, 0.14077745378017426, 1.2078394889831543], 'magnitude': 6.850637912750244}]}, 5296: {'frame': 5296, 'ionic_force': [-3.5437815007171594, -4.856745570898056, -10.527804255485535], 'ionic_force_magnitude': 12.123573207065744, 'motion_vector': [-0.4652824401855469, 0.103912353515625, -2.422882080078125], 'ionic_force_x': -3.5437815007171594, 'ionic_force_y': -4.856745570898056, 'ionic_force_z': -10.527804255485535, 'radial_force': 6.012184699862692, 'axial_force': -10.527804255485535, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-2.572254717350006, -7.467640861868858, -7.545591441914439], 'asn_force_magnitude': 10.9232826833821, 'residue_force': [-2.572254717350006, -7.467640861868858, -7.545591441914439], 'residue_force_magnitude': 10.9232826833821, 'total_force': [-6.1160362180671655, -12.324386432766914, -18.073395697399974], 'total_force_magnitude': 22.714401422878712, 'motion_component_total': 18.367144100508877, 'cosine_total_motion': 0.8086122877976819, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.6933863957561204, 'cosine_residue_motion': 0.6933863957561204, 'cosine_ionic_motion': 0.8902563878249191, 'motion_component_glu': None, 'motion_component_asn': 7.574055609655557, 'motion_component_residue': 7.574055609655557, 'motion_component_ionic': 10.79308849085332, 'ionic_contributions': [{'ion_id': 1306, 'distance': 7.367055416107178, 'force': [-3.8624563217163086, 3.411072015762329, -3.2963201999664307], 'magnitude': 6.1171650886535645}, {'ion_id': 1309, 'distance': 8.020055770874023, 'force': [2.060899019241333, -4.070521354675293, -2.4136157035827637], 'magnitude': 5.161587715148926}, {'ion_id': 1320, 'distance': 8.660042762756348, 'force': [-1.741642713546753, -3.7549068927764893, -1.5699185132980347], 'magnitude': 4.426882743835449}, {'ion_id': 1469, 'distance': 10.063952445983887, 'force': [-0.000581484695430845, -0.4423893392086029, -3.2479498386383057], 'magnitude': 3.2779393196105957}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.475654602050781, 'force': [-3.314055919647217, 5.48734712600708, -1.427195429801941], 'magnitude': 6.56740665435791}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.650543212890625, 'force': [0.9490165114402771, -3.6277644634246826, 2.230506420135498], 'magnitude': 4.363080024719238}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.205751895904541, 'force': [-10.947237014770508, 7.480644702911377, 1.8143311738967896], 'magnitude': 13.38259506225586}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.384101390838623, 'force': [15.3755521774292, -6.260193347930908, -4.476517677307129], 'magnitude': 17.194093704223633}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.154862880706787, 'force': [11.010217666625977, -13.819613456726074, -0.4892059862613678], 'magnitude': 17.67613983154297}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.360344648361206, 'force': [-6.042136192321777, 10.753800392150879, -0.21772125363349915], 'magnitude': 12.336896896362305}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.11579704284668, 'force': [-3.0643396377563477, 4.352277755737305, -0.024219540879130363], 'magnitude': 5.322883129119873}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.543903350830078, 'force': [16.604293823242188, 6.710258960723877, 5.874915599822998], 'magnitude': 18.847938537597656}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.664991855621338, 'force': [-20.179588317871094, -15.57806396484375, -10.899232864379883], 'magnitude': 27.72517204284668}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.811741352081299, 'force': [-19.6517333984375, -0.3746032118797302, -7.398617744445801], 'magnitude': 21.001678466796875}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.3588569164276123, 'force': [10.628477096557617, -2.363619565963745, 5.823884010314941], 'magnitude': 12.347826957702637}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.708967685699463, 'force': [6.05927848815918, -0.22811178863048553, 1.6434818506240845], 'magnitude': 6.282350063323975}]}, 5297: {'frame': 5297, 'ionic_force': [-0.009639695286750793, -1.7626727223396301, -9.943647146224976], 'ionic_force_magnitude': 10.098674498092981, 'motion_vector': [0.11940383911132812, -0.8824501037597656, 1.4705276489257812], 'ionic_force_x': -0.009639695286750793, 'ionic_force_y': -1.7626727223396301, 'ionic_force_z': -9.943647146224976, 'radial_force': 1.7626990808999203, 'axial_force': -9.943647146224976, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [4.436001926660538, -11.630098760128021, -6.283489029854536], 'asn_force_magnitude': 13.943440918653101, 'residue_force': [4.436001926660538, -11.630098760128021, -6.283489029854536], 'residue_force_magnitude': 13.943440918653101, 'total_force': [4.426362231373787, -13.392771482467651, -16.22713617607951], 'total_force_magnitude': 21.500673456009686, 'motion_component_total': -6.698410593287386, 'cosine_total_motion': -0.3115442224166752, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.06477137670010895, 'cosine_residue_motion': 0.06477137670010895, 'cosine_ionic_motion': -0.752727148395628, 'motion_component_glu': None, 'motion_component_asn': 0.9031358642377931, 'motion_component_residue': 0.9031358642377931, 'motion_component_ionic': -7.601546457525179, 'ionic_contributions': [{'ion_id': 1306, 'distance': 8.668022155761719, 'force': [-2.068286657333374, 2.263288974761963, -3.181971549987793], 'magnitude': 4.418736457824707}, {'ion_id': 1309, 'distance': 8.45644760131836, 'force': [2.703697919845581, -1.9296005964279175, -3.2435293197631836], 'magnitude': 4.642609596252441}, {'ion_id': 1320, 'distance': 12.18014144897461, 'force': [-0.5463349223136902, -1.8209863901138306, -1.1804895401000977], 'magnitude': 2.2378625869750977}, {'ion_id': 1469, 'distance': 11.871116638183594, 'force': [-0.09871603548526764, -0.27537471055984497, -2.3376567363739014], 'magnitude': 2.3558895587921143}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.975148677825928, 'force': [2.3363046646118164, -6.196939945220947, 0.3160478174686432], 'magnitude': 6.63025426864624}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.07656192779541, 'force': [-3.1747586727142334, 6.821689605712891, -1.328155755996704], 'magnitude': 7.640584945678711}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.54438591003418, 'force': [0.16415539383888245, -4.528603553771973, 0.04035912826657295], 'magnitude': 4.531757354736328}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.7697625160217285, 'force': [-13.49344253540039, 8.760592460632324, -4.317205905914307], 'magnitude': 16.657108306884766}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.866915464401245, 'force': [22.21710205078125, -8.122876167297363, 3.7904014587402344], 'magnitude': 23.95720863342285}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.8130388259887695, 'force': [11.768106460571289, -15.617859840393066, 7.620014190673828], 'magnitude': 20.987388610839844}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.0839486122131348, 'force': [-5.583521842956543, 12.184574127197266, -5.908089637756348], 'magnitude': 14.647357940673828}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.789551734924316, 'force': [-3.1275062561035156, 4.604251861572266, -2.428496837615967], 'magnitude': 6.072728157043457}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.6329565048217773, 'force': [15.437233924865723, 8.385323524475098, -3.61263108253479], 'magnitude': 17.935243606567383}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.7806921005249023, 'force': [-20.78520965576172, -14.704225540161133, -0.5257099270820618], 'magnitude': 25.46596908569336}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.8929929733276367, 'force': [-18.53752326965332, -3.2374870777130127, 7.159854888916016], 'magnitude': 20.134164810180664}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.2931578159332275, 'force': [11.92614459991455, -0.8451853394508362, -4.696558952331543], 'magnitude': 12.84542465209961}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.871740341186523, 'force': [5.288917064666748, 0.8666471242904663, -2.3933184146881104], 'magnitude': 5.869556427001953}]}, 5298: {'frame': 5298, 'ionic_force': [-0.9545583575963974, -6.526641249656677, -10.410386621952057], 'ionic_force_magnitude': 12.324137993316027, 'motion_vector': [-0.8501853942871094, 0.7801551818847656, 2.5111923217773438], 'ionic_force_x': -0.9545583575963974, 'ionic_force_y': -6.526641249656677, 'ionic_force_z': -10.410386621952057, 'radial_force': 6.596076686923614, 'axial_force': -10.410386621952057, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.4110836982727051, 1.5610126554965973, -9.66257780790329], 'asn_force_magnitude': 9.796487136284682, 'residue_force': [0.4110836982727051, 1.5610126554965973, -9.66257780790329], 'residue_force_magnitude': 9.796487136284682, 'total_force': [-0.5434746593236923, -4.96562859416008, -20.072964429855347], 'total_force_magnitude': 20.685181484403397, 'motion_component_total': -19.474154475480713, 'cosine_total_motion': -0.9414543686824407, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.864169916613226, 'cosine_residue_motion': -0.864169916613226, 'cosine_ionic_motion': -0.8932328581346122, 'motion_component_glu': None, 'motion_component_asn': -8.465829471665675, 'motion_component_residue': -8.465829471665675, 'motion_component_ionic': -11.008325003815038, 'ionic_contributions': [{'ion_id': 1306, 'distance': 7.934369087219238, 'force': [-3.5949900150299072, 2.179809331893921, -3.1837265491485596], 'magnitude': 5.273674011230469}, {'ion_id': 1309, 'distance': 6.483048439025879, 'force': [3.2287416458129883, -6.1072096824646, -3.8306076526641846], 'magnitude': 7.899135589599609}, {'ion_id': 1320, 'distance': 11.889945030212402, 'force': [-0.4978197515010834, -2.0856738090515137, -0.9577496647834778], 'magnitude': 2.3484344482421875}, {'ion_id': 1469, 'distance': 11.539029121398926, 'force': [-0.09049023687839508, -0.5135670900344849, -2.438302755355835], 'magnitude': 2.493443489074707}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.636988878250122, 'force': [-15.984102249145508, 7.385895729064941, -3.1946353912353516], 'magnitude': 17.895492553710938}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.728573799133301, 'force': [25.80952262878418, -5.747241020202637, 0.5831102132797241], 'magnitude': 26.448104858398438}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.764742136001587, 'force': [15.105339050292969, -12.718276977539062, 8.578225135803223], 'magnitude': 21.52932357788086}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.156459331512451, 'force': [-7.374248504638672, 9.16679573059082, -7.55579948425293], 'magnitude': 13.982123374938965}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.715879440307617, 'force': [-4.074628829956055, 4.08638858795166, -2.436366081237793], 'magnitude': 6.263948440551758}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.6370186805725098, 'force': [17.884544372558594, 0.48286235332489014, 0.38473576307296753], 'magnitude': 17.89519691467285}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.664646863937378, 'force': [-26.8710994720459, -0.2557571828365326, -6.852878570556641], 'magnitude': 27.732351303100586}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.254710674285889, 'force': [-16.34813117980957, 3.4516592025756836, 2.2265689373016357], 'magnitude': 16.856243133544922}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.1428914070129395, 'force': [7.3210225105285645, -3.456111431121826, -0.5785969495773315], 'magnitude': 8.116456031799316}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.237150192260742, 'force': [4.942865371704102, -0.8352023363113403, -0.8169413805007935], 'magnitude': 5.079062461853027}]}, 5299: {'frame': 5299, 'ionic_force': [2.9334011897444725, -1.9908200800418854, -12.94955426454544], 'ionic_force_magnitude': 13.426062817576092, 'motion_vector': [-0.3539390563964844, 2.2585983276367188, 2.1390380859375], 'ionic_force_x': 2.9334011897444725, 'ionic_force_y': -1.9908200800418854, 'ionic_force_z': -12.94955426454544, 'radial_force': 3.5451667282502055, 'axial_force': -12.94955426454544, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-9.794504404067993, -4.070549488067627, -5.41352653503418], 'asn_force_magnitude': 11.908314708708119, 'residue_force': [-9.794504404067993, -4.070549488067627, -5.41352653503418], 'residue_force_magnitude': 11.908314708708119, 'total_force': [-6.861103214323521, -6.061369568109512, -18.36308079957962], 'total_force_magnitude': 20.518715232945127, 'motion_component_total': -16.1431002373389, 'cosine_total_motion': -0.7867500500917971, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.4642041777216187, 'cosine_residue_motion': -0.4642041777216187, 'cosine_ionic_motion': -0.7906421222784978, 'motion_component_glu': None, 'motion_component_asn': -5.52788943740611, 'motion_component_residue': -5.52788943740611, 'motion_component_ionic': -10.61521079993279, 'ionic_contributions': [{'ion_id': 1306, 'distance': 6.892374515533447, 'force': [-5.214995384216309, 3.869166851043701, -2.5838310718536377], 'magnitude': 6.988763332366943}, {'ion_id': 1309, 'distance': 5.485037326812744, 'force': [9.771367073059082, -2.351778030395508, -4.5568013191223145], 'magnitude': 11.03516674041748}, {'ion_id': 1320, 'distance': 10.32797622680664, 'force': [-1.1783761978149414, -2.824215888977051, -0.5681673884391785], 'magnitude': 3.11248779296875}, {'ion_id': 1469, 'distance': 9.387465476989746, 'force': [-0.3746396005153656, -0.5283625721931458, -3.711301326751709], 'magnitude': 3.767396926879883}, {'ion_id': 2436, 'distance': 14.687841415405273, 'force': [-0.06995470076799393, -0.1556304395198822, -1.529453158378601], 'magnitude': 1.5389416217803955}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.11881160736084, 'force': [-7.655621528625488, 2.943966865539551, 3.786971092224121], 'magnitude': 9.034192085266113}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.258686065673828, 'force': [5.884469032287598, -0.934746265411377, -3.898850679397583], 'magnitude': 7.120517253875732}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.132544040679932, 'force': [13.78491497039795, -8.946660995483398, -7.013131141662598], 'magnitude': 17.867586135864258}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.4339210987091064, 'force': [-8.266595840454102, 5.208965301513672, 6.6406378746032715], 'magnitude': 11.813889503479004}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.166271209716797, 'force': [-6.170213222503662, 4.930660724639893, 1.4239377975463867], 'magnitude': 8.025617599487305}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.9912071228027344, 'force': [11.061163902282715, 5.122350215911865, 8.498945236206055], 'magnitude': 14.86000919342041}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.855531930923462, 'force': [-16.442785263061523, -10.62416934967041, -14.139192581176758], 'magnitude': 24.14859962463379}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.516100883483887, 'force': [-11.402366638183594, -1.0102370977401733, -9.633813858032227], 'magnitude': 14.961447715759277}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.054115295410156, 'force': [6.0097479820251465, -1.0975724458694458, 5.875173091888428], 'magnitude': 8.475811958312988}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.515574932098389, 'force': [3.4027822017669678, 0.33689355850219727, 3.0457966327667236], 'magnitude': 4.579225063323975}]}, 5302: {'frame': 5302, 'ionic_force': [-6.390175463631749, -3.4052871465682983, -11.440962880849838], 'ionic_force_magnitude': 13.539791528955249, 'motion_vector': [-1.703094482421875, 1.6502799987792969, -1.0469818115234375], 'ionic_force_x': -6.390175463631749, 'ionic_force_y': -3.4052871465682983, 'ionic_force_z': -11.440962880849838, 'radial_force': 7.240878607364199, 'axial_force': -11.440962880849838, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-3.692608594894409, -1.8346710801124573, -7.9459028244018555], 'asn_force_magnitude': 8.952024793426705, 'residue_force': [-3.692608594894409, -1.8346710801124573, -7.9459028244018555], 'residue_force_magnitude': 8.952024793426705, 'total_force': [-10.082784058526158, -5.239958226680756, -19.386865705251694], 'total_force_magnitude': 22.471543303958736, 'motion_component_total': 11.118313330806455, 'cosine_total_motion': 0.4947730193879376, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.49901309913008335, 'cosine_residue_motion': 0.49901309913008335, 'cosine_ionic_motion': 0.4912288110880878, 'motion_component_glu': None, 'motion_component_asn': 4.467177635657205, 'motion_component_residue': 4.467177635657205, 'motion_component_ionic': 6.651135695149249, 'ionic_contributions': [{'ion_id': 1306, 'distance': 4.272507667541504, 'force': [-15.774862289428711, 7.403421878814697, -5.208380699157715], 'magnitude': 18.18747329711914}, {'ion_id': 1309, 'distance': 5.402655601501465, 'force': [9.655634880065918, -6.011810302734375, 0.029120855033397675], 'magnitude': 11.374268531799316}, {'ion_id': 1320, 'distance': 12.33087158203125, 'force': [-0.391956627368927, -2.144749641418457, -0.11846282333135605], 'magnitude': 2.1834867000579834}, {'ion_id': 1469, 'distance': 8.355583190917969, 'force': [0.1119040995836258, -2.1314122676849365, -4.249485492706299], 'magnitude': 4.755372524261475}, {'ion_id': 2436, 'distance': 13.001425743103027, 'force': [0.009104473516345024, -0.520736813545227, -1.8937547206878662], 'magnitude': 1.9640663862228394}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.903573513031006, 'force': [-5.821902275085449, 1.4852484464645386, 7.798557281494141], 'magnitude': 9.844694137573242}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.284696578979492, 'force': [4.755422592163086, -3.5165600776672363, -8.947652816772461], 'magnitude': 10.725704193115234}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.137609958648682, 'force': [5.951892852783203, 0.9972097277641296, -9.860370635986328], 'magnitude': 11.560551643371582}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.868834495544434, 'force': [-2.0706679821014404, -0.9965938329696655, 5.408618450164795], 'magnitude': 5.876565456390381}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.782569885253906, 'force': [-2.4373462200164795, -0.7999602556228638, 3.2826759815216064], 'magnitude': 4.166119575500488}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.277355194091797, 'force': [5.856673240661621, -0.7434579133987427, 6.114627838134766], 'magnitude': 8.499530792236328}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.236225605010986, 'force': [-6.2650322914123535, 1.0024688243865967, -8.95217514038086], 'magnitude': 10.972557067871094}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.966956615447998, 'force': [-6.115854740142822, 2.376171112060547, -5.513607025146484], 'magnitude': 8.570281982421875}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.889759063720703, 'force': [2.4542062282562256, -1.6391971111297607, 2.7234232425689697], 'magnitude': 4.015859603881836}]}, 5303: {'frame': 5303, 'ionic_force': [0.2442486435174942, -4.38072469830513, -19.32172292470932], 'ionic_force_magnitude': 19.813616102605764, 'motion_vector': [2.9986648559570312,</t>
+          <t>{5293: {'frame': 5293, 'motion_vector': [3.6029815673828125, -0.9414405822753906, -2.305633544921875], 'ionic_force': [-7.19414022564888, -9.335815489292145, -6.3991100788116455], 'ionic_force_magnitude': 13.411253268697719, 'radial_force': 11.786140353669918, 'axial_force': -6.3991100788116455, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-5.293145418167114, 2.4644975066184998, -13.945229291915894], 'asn_force_magnitude': 15.118219352228667, 'residue_force': [-5.293145418167114, 2.4644975066184998, -13.945229291915894], 'residue_force_magnitude': 15.118219352228667, 'total_force': [-12.487285643815994, -6.871317982673645, -20.34433937072754], 'total_force_magnitude': 24.840278943695495, 'cosine_total_motion': 0.0770605057827729, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.16251661081762375, 'cosine_residue_motion': 0.16251661081762375, 'cosine_ionic_motion': -0.04047029018548834, 'motion_component_total': 1.9142044591863385, 'motion_component_glu': None, 'motion_component_asn': 2.4569617707216143, 'motion_component_residue': 2.4569617707216143, 'motion_component_ionic': -0.5427573115352757, 'motion_component_percent_total': 7.70605057827729, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 16.251661081762375, 'motion_component_percent_residue': 16.251661081762375, 'motion_component_percent_ionic': 4.047029018548834, 'ionic_contributions': [{'ion_id': 1306, 'distance': 9.595380783081055, 'force': [-2.7549750804901123, 2.149670362472534, -0.8896871209144592], 'magnitude': 3.6058998107910156, 'cosine_ionic_motion': -0.6267500519752502, 'motion_component_ionic': -2.259997844696045, 'motion_component_percent_ionic': 62.675005197525024}, {'ion_id': 1309, 'distance': 7.038130283355713, 'force': [-0.4600997269153595, -6.4237165451049805, -1.8560487031936646], 'magnitude': 6.702293872833252, 'cosine_ionic_motion': 0.2953168451786041, 'motion_component_ionic': 1.9793003797531128, 'motion_component_percent_ionic': 29.531684517860413}, {'ion_id': 1320, 'distance': 8.00695514678955, 'force': [-2.2913060188293457, -4.553028583526611, 0.9146720767021179], 'magnitude': 5.178492069244385, 'cosine_ionic_motion': -0.26797401905059814, 'motion_component_ionic': -1.3877012729644775, 'motion_component_percent_ionic': 26.797401905059814}, {'ion_id': 1469, 'distance': 10.095939636230469, 'force': [-1.280375599861145, -0.43071743845939636, -2.963862419128418], 'magnitude': 3.2572009563446045, 'cosine_ionic_motion': 0.1840636283159256, 'motion_component_ionic': 0.5995322465896606, 'motion_component_percent_ionic': 18.40636283159256}, {'ion_id': 2436, 'distance': 14.155181884765625, 'force': [-0.4073837995529175, -0.0780232846736908, -1.6041839122772217], 'magnitude': 1.656941533088684, 'cosine_ionic_motion': 0.3175182640552521, 'motion_component_ionic': 0.5261092185974121, 'motion_component_percent_ionic': 31.751826405525208}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.7163825035095215, 'force': [1.3641202449798584, 4.213038921356201, -4.0867109298706055], 'magnitude': 6.02592134475708, 'cosine_with_motion': 0.39294517040252686, 'motion_component': 2.367856740951538, 'motion_component_percent': 39.294517040252686}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.1833295822143555, 'force': [-4.183377742767334, 2.830166816711426, 1.1724398136138916], 'magnitude': 5.185084819793701, 'cosine_with_motion': -0.9000455141067505, 'motion_component': -4.666812419891357, 'motion_component_percent': 90.00455141067505}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.6503655910491943, 'force': [11.936121940612793, 8.980183601379395, 9.615899085998535], 'magnitude': 17.764577865600586, 'cosine_with_motion': 0.15911804139614105, 'motion_component': 2.826664924621582, 'motion_component_percent': 15.911804139614105}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.822566270828247, 'force': [-11.983016967773438, -10.793547630310059, -18.729280471801758], 'magnitude': 24.715972900390625, 'cosine_with_motion': 0.09394334256649017, 'motion_component': 2.3219010829925537, 'motion_component_percent': 9.394334256649017}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.187878608703613, 'force': [-14.870417594909668, -5.1708245277404785, -7.405556678771973], 'magnitude': 17.398534774780273, 'cosine_with_motion': -0.41513845324516296, 'motion_component': -7.2228007316589355, 'motion_component_percent': 41.513845324516296}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.026407241821289, 'force': [7.773963928222656, 0.5124548077583313, 3.624950408935547], 'magnitude': 8.59286880493164, 'cosine_with_motion': 0.5093298554420471, 'motion_component': 4.3766045570373535, 'motion_component_percent': 50.93298554420471}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.092360496520996, 'force': [4.669460773468018, 1.893025517463684, 1.8630294799804688], 'magnitude': 5.371991157531738, 'cosine_with_motion': 0.4567294418811798, 'motion_component': 2.4535465240478516, 'motion_component_percent': 45.67294418811798}]}, 5294: {'frame': 5294, 'motion_vector': [-1.1986160278320312, 0.10608673095703125, 0.8895950317382812], 'ionic_force': [-3.9219388999044895, -4.9589075446128845, -9.572859406471252], 'ionic_force_magnitude': 11.472227594790288, 'radial_force': 6.322370502477898, 'axial_force': -9.572859406471252, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-2.3613901138305664, -2.0234079360961914, -5.287694956175983], 'asn_force_magnitude': 6.134334592694037, 'residue_force': [-2.3613901138305664, -2.0234079360961914, -5.287694956175983], 'residue_force_magnitude': 6.134334592694037, 'total_force': [-6.283329013735056, -6.982315480709076, -14.860554362647235], 'total_force_magnitude': 17.580359180977734, 'cosine_total_motion': -0.24438745786282773, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.227478088410098, 'cosine_residue_motion': -0.227478088410098, 'cosine_ionic_motion': -0.2528709056520096, 'motion_component_total': -4.2964192885545724, 'motion_component_glu': None, 'motion_component_asn': -1.3954267068139767, 'motion_component_residue': -1.3954267068139767, 'motion_component_ionic': -2.9009925817405957, 'motion_component_percent_total': 24.438745786282773, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 22.7478088410098, 'motion_component_percent_residue': 22.7478088410098, 'motion_component_percent_ionic': 25.28709056520096, 'ionic_contributions': [{'ion_id': 1306, 'distance': 7.554628372192383, 'force': [-4.087786674499512, 1.854230284690857, -3.7001771926879883], 'magnitude': 5.817171096801758, 'cosine_ionic_motion': 0.20732159912586212, 'motion_component_ionic': 1.206025242805481, 'motion_component_percent_ionic': 20.732159912586212}, {'ion_id': 1309, 'distance': 9.034814834594727, 'force': [1.4283074140548706, -3.2946081161499023, -1.909952163696289], 'magnitude': 4.067237377166748, 'cosine_ionic_motion': -0.6178727149963379, 'motion_component_ionic': -2.5130350589752197, 'motion_component_percent_ionic': 61.78727149963379}, {'ion_id': 1320, 'distance': 9.996163368225098, 'force': [-1.2332184314727783, -2.8408944606781006, -1.2032557725906372], 'magnitude': 3.3225491046905518, 'cosine_ionic_motion': 0.021392682567238808, 'motion_component_ionic': 0.07107824087142944, 'motion_component_percent_ionic': 2.1392682567238808}, {'ion_id': 1469, 'distance': 10.809033393859863, 'force': [-0.029241207987070084, -0.6776352524757385, -2.759474277496338], 'magnitude': 2.841609239578247, 'cosine_ionic_motion': -0.5859571099281311, 'motion_component_ionic': -1.665061116218567, 'motion_component_percent_ionic': 58.59571099281311}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.8706774711608887, 'force': [-13.338183403015137, 7.705677509307861, -3.5144574642181396], 'magnitude': 15.799874305725098, 'cosine_with_motion': 0.5785271525382996, 'motion_component': 9.140656471252441, 'motion_component_percent': 57.852715253829956}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.3188631534576416, 'force': [16.086706161499023, -4.274590015411377, 6.520899772644043], 'magnitude': 17.876699447631836, 'cosine_with_motion': -0.5208832621574402, 'motion_component': -9.311673164367676, 'motion_component_percent': 52.08832621574402}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.574234962463379, 'force': [15.354435920715332, -18.03443145751953, 3.0851986408233643], 'magnitude': 23.885517120361328, 'cosine_with_motion': -0.49163931608200073, 'motion_component': -11.743059158325195, 'motion_component_percent': 49.16393160820007}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.0706281661987305, 'force': [-6.634010314941406, 12.520920753479004, -4.184329032897949], 'magnitude': 14.774713516235352, 'cosine_with_motion': 0.25136736035346985, 'motion_component': 3.7138805389404297, 'motion_component_percent': 25.136736035346985}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.395316123962402, 'force': [-4.284043788909912, 5.80040979385376, 0.01454452145844698], 'magnitude': 7.210963249206543, 'cosine_with_motion': 0.5340889096260071, 'motion_component': 3.8512957096099854, 'motion_component_percent': 53.40889096260071}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.871678113937378, 'force': [14.96583366394043, 3.221412420272827, 3.876132011413574], 'magnitude': 15.791708946228027, 'cosine_with_motion': -0.5987136960029602, 'motion_component': -9.454712867736816, 'motion_component_percent': 59.87136960029602}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.7660417556762695, 'force': [-22.42108726501465, -7.137618064880371, -10.426596641540527], 'magnitude': 25.736446380615234, 'cosine_with_motion': 0.43729832768440247, 'motion_component': 11.254505157470703, 'motion_component_percent': 43.72983276844025}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.390989303588867, 'force': [-15.354634284973145, 1.2392737865447998, -3.62868595123291], 'magnitude': 15.826179504394531, 'cosine_with_motion': 0.6463637351989746, 'motion_component': 10.22946834564209, 'motion_component_percent': 64.63637351989746}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.925269365310669, 'force': [8.349770545959473, -2.6006577014923096, 2.2944328784942627], 'magnitude': 9.041377067565918, 'cosine_with_motion': -0.6092429161071777, 'motion_component': -5.508395195007324, 'motion_component_percent': 60.92429161071777}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.2881178855896, 'force': [4.913822650909424, -0.4638049602508545, 0.6751663088798523], 'magnitude': 4.981627941131592, 'cosine_with_motion': -0.7161096334457397, 'motion_component': -3.567391872406006, 'motion_component_percent': 71.61096334457397}]}, 5295: {'frame': 5295, 'motion_vector': [1.4610366821289062, 0.4837226867675781, -0.33788299560546875], 'ionic_force': [-4.847121506929398, -6.3855297565460205, -10.225951194763184], 'ionic_force_magnitude': 12.993831421576576, 'radial_force': 8.016830868533537, 'axial_force': -10.225951194763184, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-2.7353638410568237, 1.8772039078176022, -16.558398723602295], 'asn_force_magnitude': 16.887471040516424, 'residue_force': [-2.7353638410568237, 1.8772039078176022, -16.558398723602295], 'residue_force_magnitude': 16.887471040516424, 'total_force': [-7.582485347986221, -4.508325848728418, -26.78434991836548], 'total_force_magnitude': 28.199654014902087, 'cosine_total_motion': -0.09472737627732117, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.09419181356133025, 'cosine_residue_motion': 0.09419181356133025, 'cosine_ionic_motion': -0.32799723362991534, 'motion_component_total': -2.6712792367599008, 'motion_component_glu': None, 'motion_component_asn': 1.5906615237706867, 'motion_component_residue': 1.5906615237706867, 'motion_component_ionic': -4.261940760530587, 'motion_component_percent_total': 9.472737627732117, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 9.419181356133025, 'motion_component_percent_residue': 9.419181356133025, 'motion_component_percent_ionic': 32.799723362991536, 'ionic_contributions': [{'ion_id': 1306, 'distance': 7.963080883026123, 'force': [-3.9522693157196045, 1.6182080507278442, -3.028805732727051], 'magnitude': 5.235713481903076, 'cosine_ionic_motion': -0.4810115694999695, 'motion_component_ionic': -2.5184388160705566, 'motion_component_percent_ionic': 48.10115694999695}, {'ion_id': 1309, 'distance': 8.245342254638672, 'force': [1.2909294366836548, -4.2322163581848145, -2.066220760345459], 'magnitude': 4.883382320404053, 'cosine_ionic_motion': 0.0697907879948616, 'motion_component_ionic': 0.34081509709358215, 'motion_component_percent_ionic': 6.97907879948616}, {'ion_id': 1320, 'distance': 9.006513595581055, 'force': [-1.8195945024490356, -3.148383855819702, -1.8783209323883057], 'magnitude': 4.09283971786499, 'cosine_ionic_motion': -0.549972653388977, 'motion_component_ionic': -2.2509498596191406, 'motion_component_percent_ionic': 54.997265338897705}, {'ion_id': 1469, 'distance': 9.98206615447998, 'force': [-0.36618712544441223, -0.6231375932693481, -3.252603769302368], 'magnitude': 3.331940174102783, 'cosine_ionic_motion': 0.05001077428460121, 'motion_component_ionic': 0.16663290560245514, 'motion_component_percent_ionic': 5.001077428460121}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.451868057250977, 'force': [-0.9308732748031616, 6.142979145050049, -2.2990808486938477], 'magnitude': 6.624838829040527, 'cosine_with_motion': 0.22879181802272797, 'motion_component': 1.5157089233398438, 'motion_component_percent': 22.879181802272797}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.322166442871094, 'force': [-11.900971412658691, 3.9270126819610596, -1.8734612464904785], 'magnitude': 12.671401023864746, 'cosine_with_motion': -0.7440180778503418, 'motion_component': -9.427751541137695, 'motion_component_percent': 74.40180778503418}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.7789976596832275, 'force': [13.675838470458984, -0.526833713054657, 1.6771659851074219], 'magnitude': 13.78836441040039, 'cosine_with_motion': 0.8818594217300415, 'motion_component': 12.159399032592773, 'motion_component_percent': 88.18594217300415}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.9603607654571533, 'force': [15.479023933410645, -10.661806106567383, 5.022245407104492], 'magnitude': 19.455005645751953, 'cosine_with_motion': 0.5141465067863464, 'motion_component': 10.00272274017334, 'motion_component_percent': 51.414650678634644}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.210261821746826, 'force': [-9.407450675964355, 7.921640396118164, -5.609560012817383], 'magnitude': 13.51738452911377, 'cosine_with_motion': -0.3764180839061737, 'motion_component': -5.088188171386719, 'motion_component_percent': 37.64180839061737}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.790666103363037, 'force': [-4.324090003967285, 3.947477340698242, -1.601058006286621], 'magnitude': 6.0699028968811035, 'cosine_with_motion': -0.4043390154838562, 'motion_component': -2.454298496246338, 'motion_component_percent': 40.43390154838562}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.3971450328826904, 'force': [17.317733764648438, 6.5973801612854, 8.791823387145996], 'magnitude': 20.511594772338867, 'cosine_with_motion': 0.7896873950958252, 'motion_component': 16.1977481842041, 'motion_component_percent': 78.96873950958252}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.571812391281128, 'force': [-19.24126625061035, -12.519775390625, -18.95565414428711], 'magnitude': 29.77058982849121, 'cosine_with_motion': -0.5918580889701843, 'motion_component': -17.619964599609375, 'motion_component_percent': 59.18580889701843}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.7295291423797607, 'force': [-20.737747192382812, 0.04725603386759758, -7.156125545501709], 'magnitude': 21.937788009643555, 'cosine_with_motion': -0.8059071898460388, 'motion_component': -17.679821014404297, 'motion_component_percent': 80.59071898460388}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.431196928024292, 'force': [10.592588424682617, -3.138904094696045, 4.237466812133789], 'magnitude': 11.832656860351562, 'cosine_with_motion': 0.6718341708183289, 'motion_component': 7.949583053588867, 'motion_component_percent': 67.18341708183289}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.509426116943359, 'force': [6.74185037612915, 0.14077745378017426, 1.2078394889831543], 'magnitude': 6.850637912750244, 'cosine_with_motion': 0.8810162544250488, 'motion_component': 6.035523414611816, 'motion_component_percent': 88.10162544250488}]}, 5296: {'frame': 5296, 'motion_vector': [-0.4652824401855469, 0.103912353515625, -2.422882080078125], 'ionic_force': [-3.5437815007171594, -4.856745570898056, -10.527804255485535], 'ionic_force_magnitude': 12.123573207065744, 'radial_force': 6.012184699862692, 'axial_force': -10.527804255485535, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-2.572254717350006, -7.467640861868858, -7.545591441914439], 'asn_force_magnitude': 10.9232826833821, 'residue_force': [-2.572254717350006, -7.467640861868858, -7.545591441914439], 'residue_force_magnitude': 10.9232826833821, 'total_force': [-6.1160362180671655, -12.324386432766914, -18.073395697399974], 'total_force_magnitude': 22.714401422878712, 'cosine_total_motion': 0.8086122877976819, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.6933863957561204, 'cosine_residue_motion': 0.6933863957561204, 'cosine_ionic_motion': 0.8902563878249191, 'motion_component_total': 18.367144100508877, 'motion_component_glu': None, 'motion_component_asn': 7.574055609655557, 'motion_component_residue': 7.574055609655557, 'motion_component_ionic': 10.79308849085332, 'motion_component_percent_total': 80.8612287797682, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 69.33863957561204, 'motion_component_percent_residue': 69.33863957561204, 'motion_component_percent_ionic': 89.02563878249191, 'ionic_contributions': [{'ion_id': 1306, 'distance': 7.367055416107178, 'force': [-3.8624563217163086, 3.411072015762329, -3.2963201999664307], 'magnitude': 6.1171650886535645, 'cosine_ionic_motion': 0.6711642742156982, 'motion_component_ionic': 4.1056227684021, 'motion_component_percent_ionic': 67.11642742156982}, {'ion_id': 1309, 'distance': 8.020055770874023, 'force': [2.060899019241333, -4.070521354675293, -2.4136157035827637], 'magnitude': 5.161587715148926, 'cosine_ionic_motion': 0.3503943979740143, 'motion_component_ionic': 1.8085914850234985, 'motion_component_percent_ionic': 35.03943979740143}, {'ion_id': 1320, 'distance': 8.660042762756348, 'force': [-1.741642713546753, -3.7549068927764893, -1.5699185132980347], 'magnitude': 4.426882743835449, 'cosine_ionic_motion': 0.38639795780181885, 'motion_component_ionic': 1.710538387298584, 'motion_component_percent_ionic': 38.639795780181885}, {'ion_id': 1469, 'distance': 10.063952445983887, 'force': [-0.000581484695430845, -0.4423893392086029, -3.2479498386383057], 'magnitude': 3.2779393196105957, 'cosine_ionic_motion': 0.96656334400177, 'motion_component_ionic': 3.1683359146118164, 'motion_component_percent_ionic': 96.656334400177}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.475654602050781, 'force': [-3.314055919647217, 5.48734712600708, -1.427195429801941], 'magnitude': 6.56740665435791, 'cosine_with_motion': 0.3434695303440094, 'motion_component': 2.255704164505005, 'motion_component_percent': 34.34695303440094}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.650543212890625, 'force': [0.9490165114402771, -3.6277644634246826, 2.230506420135498], 'magnitude': 4.363080024719238, 'cosine_with_motion': -0.5775778889656067, 'motion_component': -2.5200185775756836, 'motion_component_percent': 57.75778889656067}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.205751895904541, 'force': [-10.947237014770508, 7.480644702911377, 1.8143311738967896], 'magnitude': 13.38259506225586, 'cosine_with_motion': 0.04463384300470352, 'motion_component': 0.5973166227340698, 'motion_component_percent': 4.463384300470352}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.384101390838623, 'force': [15.3755521774292, -6.260193347930908, -4.476517677307129], 'magnitude': 17.194093704223633, 'cosine_with_motion': 0.07163745164871216, 'motion_component': 1.2317410707473755, 'motion_component_percent': 7.163745164871216}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.154862880706787, 'force': [11.010217666625977, -13.819613456726074, -0.4892059862613678], 'magnitude': 17.67613983154297, 'cosine_with_motion': -0.12311103940010071, 'motion_component': -2.1761279106140137, 'motion_component_percent': 12.31110394001007}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.360344648361206, 'force': [-6.042136192321777, 10.753800392150879, -0.21772125363349915], 'magnitude': 12.336896896362305, 'cosine_with_motion': 0.1462797224521637, 'motion_component': 1.8046379089355469, 'motion_component_percent': 14.62797224521637}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.11579704284668, 'force': [-3.0643396377563477, 4.352277755737305, -0.024219540879130363], 'magnitude': 5.322883129119873, 'cosine_with_motion': 0.14734619855880737, 'motion_component': 0.7843065857887268, 'motion_component_percent': 14.734619855880737}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.543903350830078, 'force': [16.604293823242188, 6.710258960723877, 5.874915599822998], 'magnitude': 18.847938537597656, 'cosine_with_motion': -0.45684853196144104, 'motion_component': -8.610652923583984, 'motion_component_percent': 45.684853196144104}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.664991855621338, 'force': [-20.179588317871094, -15.57806396484375, -10.899232864379883], 'magnitude': 27.72517204284668, 'cosine_with_motion': 0.49921947717666626, 'motion_component': 13.840946197509766, 'motion_component_percent': 49.921947717666626}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.811741352081299, 'force': [-19.6517333984375, -0.3746032118797302, -7.398617744445801], 'magnitude': 21.001678466796875, 'cosine_with_motion': 0.5212206840515137, 'motion_component': 10.94650936126709, 'motion_component_percent': 52.12206840515137}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.3588569164276123, 'force': [10.628477096557617, -2.363619565963745, 5.823884010314941], 'magnitude': 12.347826957702637, 'cosine_with_motion': -0.6330209970474243, 'motion_component': -7.816433906555176, 'motion_component_percent': 63.30209970474243}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.708967685699463, 'force': [6.05927848815918, -0.22811178863048553, 1.6434818506240845], 'magnitude': 6.282350063323975, 'cosine_with_motion': -0.43994244933128357, 'motion_component': -2.7638723850250244, 'motion_component_percent': 43.99424493312836}]}, 5297: {'frame': 5297, 'motion_vector': [0.11940383911132812, -0.8824501037597656, 1.4705276489257812], 'ionic_force': [-0.009639695286750793, -1.7626727223396301, -9.943647146224976], 'ionic_force_magnitude': 10.098674498092981, 'radial_force': 1.7626990808999203, 'axial_force': -9.943647146224976, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [4.436001926660538, -11.630098760128021, -6.283489029854536], 'asn_force_magnitude': 13.943440918653101, 'residue_force': [4.436001926660538, -11.630098760128021, -6.283489029854536], 'residue_force_magnitude': 13.943440918653101, 'total_force': [4.426362231373787, -13.392771482467651, -16.22713617607951], 'total_force_magnitude': 21.500673456009686, 'cosine_total_motion': -0.3115442224166752, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.06477137670010895, 'cosine_residue_motion': 0.06477137670010895, 'cosine_ionic_motion': -0.752727148395628, 'motion_component_total': -6.698410593287386, 'motion_component_glu': None, 'motion_component_asn': 0.9031358642377931, 'motion_component_residue': 0.9031358642377931, 'motion_component_ionic': -7.601546457525179, 'motion_component_percent_total': 31.15442224166752, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 6.477137670010895, 'motion_component_percent_residue': 6.477137670010895, 'motion_component_percent_ionic': 75.27271483956281, 'ionic_contributions': [{'ion_id': 1306, 'distance': 8.668022155761719, 'force': [-2.068286657333374, 2.263288974761963, -3.181971549987793], 'magnitude': 4.418736457824707, 'cosine_ionic_motion': -0.9114017486572266, 'motion_component_ionic': -4.0272440910339355, 'motion_component_percent_ionic': 91.14017486572266}, {'ion_id': 1309, 'distance': 8.45644760131836, 'force': [2.703697919845581, -1.9296005964279175, -3.2435293197631836], 'magnitude': 4.642609596252441, 'cosine_ionic_motion': -0.34381619095802307, 'motion_component_ionic': -1.5962042808532715, 'motion_component_percent_ionic': 34.38161909580231}, {'ion_id': 1320, 'distance': 12.18014144897461, 'force': [-0.5463349223136902, -1.8209863901138306, -1.1804895401000977], 'magnitude': 2.2378625869750977, 'cosine_ionic_motion': -0.05049075931310654, 'motion_component_ionic': -0.11299138516187668, 'motion_component_percent_ionic': 5.049075931310654}, {'ion_id': 1469, 'distance': 11.871116638183594, 'force': [-0.09871603548526764, -0.27537471055984497, -2.3376567363739014], 'magnitude': 2.3558895587921143, 'cosine_ionic_motion': -0.7916783690452576, 'motion_component_ionic': -1.8651068210601807, 'motion_component_percent_ionic': 79.16783690452576}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.975148677825928, 'force': [2.3363046646118164, -6.196939945220947, 0.3160478174686432], 'magnitude': 6.63025426864624, 'cosine_with_motion': 0.5450118184089661, 'motion_component': 3.6135668754577637, 'motion_component_percent': 54.501181840896606}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.07656192779541, 'force': [-3.1747586727142334, 6.821689605712891, -1.328155755996704], 'magnitude': 7.640584945678711, 'cosine_with_motion': -0.6358463168144226, 'motion_component': -4.8582377433776855, 'motion_component_percent': 63.58463168144226}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.54438591003418, 'force': [0.16415539383888245, -4.528603553771973, 0.04035912826657295], 'magnitude': 4.531757354736328, 'cosine_with_motion': 0.5230870246887207, 'motion_component': 2.3705034255981445, 'motion_component_percent': 52.30870246887207}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.7697625160217285, 'force': [-13.49344253540039, 8.760592460632324, -4.317205905914307], 'magnitude': 16.657108306884766, 'cosine_with_motion': -0.5479333996772766, 'motion_component': -9.126985549926758, 'motion_component_percent': 54.79333996772766}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.866915464401245, 'force': [22.21710205078125, -8.122876167297363, 3.7904014587402344], 'magnitude': 23.95720863342285, 'cosine_with_motion': 0.37378835678100586, 'motion_component': 8.954925537109375, 'motion_component_percent': 37.378835678100586}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.8130388259887695, 'force': [11.768106460571289, -15.617859840393066, 7.620014190673828], 'magnitude': 20.987388610839844, 'cosine_with_motion': 0.7314983010292053, 'motion_component': 15.352239608764648, 'motion_component_percent': 73.14983010292053}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.0839486122131348, 'force': [-5.583521842956543, 12.184574127197266, -5.908089637756348], 'magnitude': 14.647357940673828, 'cosine_with_motion': -0.7985047101974487, 'motion_component': -11.69598388671875, 'motion_component_percent': 79.85047101974487}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.789551734924316, 'force': [-3.1275062561035156, 4.604251861572266, -2.428496837615967], 'magnitude': 6.072728157043457, 'cosine_with_motion': -0.7670260071754456, 'motion_component': -4.65794038772583, 'motion_component_percent': 76.70260071754456}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.6329565048217773, 'force': [15.437233924865723, 8.385323524475098, -3.61263108253479], 'magnitude': 17.935243606567383, 'cosine_with_motion': -0.3525053858757019, 'motion_component': -6.322269916534424, 'motion_component_percent': 35.25053858757019}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.7806921005249023, 'force': [-20.78520965576172, -14.704225540161133, -0.5257099270820618], 'magnitude': 25.46596908569336, 'cosine_with_motion': 0.22204115986824036, 'motion_component': 5.65449333190918, 'motion_component_percent': 22.204115986824036}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.8929929733276367, 'force': [-18.53752326965332, -3.2374870777130127, 7.159854888916016], 'magnitude': 20.134164810180664, 'cosine_with_motion': 0.3227723240852356, 'motion_component': 6.498751163482666, 'motion_component_percent': 32.27723240852356}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.2931578159332275, 'force': [11.92614459991455, -0.8451853394508362, -4.696558952331543], 'magnitude': 12.84542465209961, 'cosine_with_motion': -0.214488685131073, 'motion_component': -2.7551982402801514, 'motion_component_percent': 21.4488685131073}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.871740341186523, 'force': [5.288917064666748, 0.8666471242904663, -2.3933184146881104], 'magnitude': 5.869556427001953, 'cosine_with_motion': -0.36199134588241577, 'motion_component': -2.1247286796569824, 'motion_component_percent': 36.19913458824158}]}, 5298: {'frame': 5298, 'motion_vector': [-0.8501853942871094, 0.7801551818847656, 2.5111923217773438], 'ionic_force': [-0.9545583575963974, -6.526641249656677, -10.410386621952057], 'ionic_force_magnitude': 12.324137993316027, 'radial_force': 6.596076686923614, 'axial_force': -10.410386621952057, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.4110836982727051, 1.5610126554965973, -9.66257780790329], 'asn_force_magnitude': 9.796487136284682, 'residue_force': [0.4110836982727051, 1.5610126554965973, -9.66257780790329], 'residue_force_magnitude': 9.796487136284682, 'total_force': [-0.5434746593236923, -4.96562859416008, -20.072964429855347], 'total_force_magnitude': 20.685181484403397, 'cosine_total_motion': -0.9414543686824407, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.864169916613226, 'cosine_residue_motion': -0.864169916613226, 'cosine_ionic_motion': -0.8932328581346122, 'motion_component_total': -19.474154475480713, 'motion_component_glu': None, 'motion_component_asn': -8.465829471665675, 'motion_component_residue': -8.465829471665675, 'motion_component_ionic': -11.008325003815038, 'motion_component_percent_total': 94.14543686824408, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 86.4169916613226, 'motion_component_percent_residue': 86.4169916613226, 'motion_component_percent_ionic': 89.32328581346121, 'ionic_contributions': [{'ion_id': 1306, 'distance': 7.934369087219238, 'force': [-3.5949900150299072, 2.179809331893921, -3.1837265491485596], 'magnitude': 5.273674011230469, 'cosine_ionic_motion': -</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>{5347: {'frame': 5347, 'ionic_force': [-1.5767408609390259, -7.108273267745972, -12.609045714139938], 'ionic_force_magnitude': 14.560277964818443, 'motion_vector': [3.316211700439453, -1.65020751953125, -0.9902801513671875], 'ionic_force_x': -1.5767408609390259, 'ionic_force_y': -7.108273267745972, 'ionic_force_z': -12.609045714139938, 'radial_force': 7.281048042109511, 'axial_force': -12.609045714139938, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-2.012432560324669, 9.585110425949097, -5.336213946342468], 'asn_force_magnitude': 11.153448164968214, 'residue_force': [-2.012432560324669, 9.585110425949097, -5.336213946342468], 'residue_force_magnitude': 11.153448164968214, 'total_force': [-3.5891734212636948, 2.476837158203125, -17.945259660482407], 'total_force_magnitude': 18.46751830751221, 'motion_component_total': 0.46452463823756585, 'cosine_total_motion': 0.02515360377623704, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.40235943734978263, 'cosine_residue_motion': -0.40235943734978263, 'cosine_ionic_motion': 0.34011849075752815, 'motion_component_glu': None, 'motion_component_asn': -4.4876951281665765, 'motion_component_residue': -4.4876951281665765, 'motion_component_ionic': 4.952219766404142, 'ionic_contributions': [{'ion_id': 1306, 'distance': 10.253976821899414, 'force': [-2.2620508670806885, 2.0216140747070312, -0.8754827976226807], 'magnitude': 3.1575732231140137}, {'ion_id': 1309, 'distance': 9.169376373291016, 'force': [-3.900376081466675, -0.4288240671157837, -0.44240328669548035], 'magnitude': 3.948739528656006}, {'ion_id': 1320, 'distance': 5.010506629943848, 'force': [5.2017621994018555, -9.052448272705078, -8.116565704345703], 'magnitude': 13.224363327026367}, {'ion_id': 2436, 'distance': 10.102682113647461, 'force': [-0.6160761117935181, 0.3513849973678589, -3.174593925476074], 'magnitude': 3.2528553009033203}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.1278557777404785, 'force': [1.8304100036621094, -9.567811965942383, 9.904873847961426], 'magnitude': 13.89244270324707}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.937706470489502, 'force': [-2.408155679702759, 15.851311683654785, -16.233600616455078], 'magnitude': 22.816509246826172}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.964436054229736, 'force': [1.0552637577056885, 8.436544418334961, -9.000224113464355], 'magnitude': 12.38115119934082}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.741171360015869, 'force': [-1.7530465126037598, -3.939984083175659, 4.450823783874512], 'magnitude': 6.197296142578125}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.957278251647949, 'force': [-0.20133398473262787, -2.687417507171631, 2.854046583175659], 'magnitude': 3.925344467163086}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.68625020980835, 'force': [-2.6577091217041016, 3.119086980819702, 1.330664038658142], 'magnitude': 4.308455467224121}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.918987274169922, 'force': [3.7938876152038574, 8.250432014465332, 3.639465093612671], 'magnitude': 9.783093452453613}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.591378211975098, 'force': [-1.4122247695922852, -8.516304016113281, -3.5674989223480225], 'magnitude': 9.340709686279297}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.47483491897583, 'force': [-8.311904907226562, -10.374906539916992, -7.449184894561768], 'magnitude': 15.23866081237793}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.7777469158172607, 'force': [4.578917503356934, 5.99346399307251, 6.196365833282471], 'magnitude': 9.761303901672363}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.147976398468018, 'force': [3.473463535308838, 3.020695447921753, 2.538055419921875], 'magnitude': 5.2565460205078125}]}, 5348: {'frame': 5348, 'ionic_force': [-6.454585552215576, -0.6436145454645157, -10.31672191619873], 'ionic_force_magnitude': 12.186495206997735, 'motion_vector': [1.4751319885253906, 0.6213607788085938, -1.0232925415039062], 'ionic_force_x': -6.454585552215576, 'ionic_force_y': -0.6436145454645157, 'ionic_force_z': -10.31672191619873, 'radial_force': 6.4865949722488105, 'axial_force': -10.31672191619873, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [9.034229032695293, 4.56985867023468, -0.8264970034360886], 'asn_force_magnitude': 10.157952538666562, 'residue_force': [9.034229032695293, 4.56985867023468, -0.8264970034360886], 'residue_force_magnitude': 10.157952538666562, 'total_force': [2.5796434804797173, 3.9262441247701645, -11.143218919634819], 'total_force_magnitude': 12.093026143384506, 'motion_component_total': 9.289253214061397, 'cosine_total_motion': 0.7681496015902591, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.8815375083814108, 'cosine_residue_motion': 0.8815375083814108, 'cosine_ionic_motion': 0.027459662288833966, 'motion_component_glu': None, 'motion_component_asn': 8.954616171192747, 'motion_component_residue': 8.954616171192747, 'motion_component_ionic': 0.3346370428686516, 'ionic_contributions': [{'ion_id': 1306, 'distance': 7.247408866882324, 'force': [-3.4947903156280518, 3.541504383087158, -3.898306131362915], 'magnitude': 6.320806980133057}, {'ion_id': 1309, 'distance': 7.04019021987915, 'force': [-6.009511947631836, -2.5683140754699707, -1.4689178466796875], 'magnitude': 6.6983723640441895}, {'ion_id': 1320, 'distance': 9.25703239440918, 'force': [2.708761215209961, -1.4557560682296753, -2.3566243648529053], 'magnitude': 3.874311685562134}, {'ion_id': 2436, 'distance': 11.256568908691406, 'force': [0.3409554958343506, -0.1610487848520279, -2.5928735733032227], 'magnitude': 2.6201491355895996}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.968769073486328, 'force': [-3.061173677444458, 3.62992787361145, -2.8287014961242676], 'magnitude': 5.5270891189575195}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.92423677444458, 'force': [-3.5336523056030273, 7.641610622406006, -2.1703529357910156], 'magnitude': 8.694328308105469}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.204074382781982, 'force': [1.4865944385528564, -4.701045036315918, 1.4660147428512573], 'magnitude': 5.143830299377441}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.9277448654174805, 'force': [5.234803676605225, 6.926398277282715, -0.18550346791744232], 'magnitude': 8.684041023254395}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.112987518310547, 'force': [-3.6498842239379883, -3.8784492015838623, 0.17717140913009644], 'magnitude': 5.328734397888184}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.8407797813415527, 'force': [-8.138960838317871, 13.817949295043945, 0.5673233866691589], 'magnitude': 16.046815872192383}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.717693567276001, 'force': [16.912630081176758, -20.566455841064453, 1.3248811960220337], 'magnitude': 26.660297393798828}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.126919269561768, 'force': [3.754265308380127, -17.444454193115234, -1.6097160577774048], 'magnitude': 17.916324615478516}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.5537662506103516, 'force': [0.06863891333341599, 10.972410202026367, 1.1286287307739258], 'magnitude': 11.030516624450684}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.119487762451172, 'force': [-0.9293440580368042, 5.20028018951416, 0.5872605443000793], 'magnitude': 5.315211296081543}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.503318786621094, 'force': [6.718957424163818, 3.816227674484253, 1.1747814416885376], 'magnitude': 7.815887451171875}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.4803242683410645, 'force': [-6.153043270111084, -1.834584355354309, -1.3260352611541748], 'magnitude': 6.556219577789307}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.622708797454834, 'force': [-10.682412147521973, -9.02637004852295, -2.8826956748962402], 'magnitude': 14.279328346252441}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.7758493423461914, 'force': [7.379847049713135, 5.593720436096191, 3.1181576251983643], 'magnitude': 9.771119117736816}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.920180797576904, 'force': [3.626962661743164, 4.422692775726318, 0.6322888135910034], 'magnitude': 5.754551410675049}]}, 5349: {'frame': 5349, 'ionic_force': [-8.160462379455566, -2.827123999595642, -15.069315671920776], 'ionic_force_magnitude': 17.368651391964672, 'motion_vector': [-0.10723876953125, -1.5981407165527344, 3.5609359741210938], 'ionic_force_x': -8.160462379455566, 'ionic_force_y': -2.827123999595642, 'ionic_force_z': -15.069315671920776, 'radial_force': 8.636305712259105, 'axial_force': -15.069315671920776, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [3.8222084045410156, -20.25890064239502, 4.474711656570435], 'asn_force_magnitude': 21.096335623411584, 'residue_force': [3.8222084045410156, -20.25890064239502, 4.474711656570435], 'residue_force_magnitude': 21.096335623411584, 'total_force': [-4.338253974914551, -23.08602464199066, -10.594604015350342], 'total_force_magnitude': 25.768791503746144, 'motion_component_total': -0.09393061142325543, 'cosine_total_motion': -0.003645130638338249, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.5815148384535481, 'cosine_residue_motion': 0.5815148384535481, 'cosine_ionic_motion': -0.7117284200402713, 'motion_component_glu': None, 'motion_component_asn': 12.26783220201002, 'motion_component_residue': 12.26783220201002, 'motion_component_ionic': -12.361762813433275, 'ionic_contributions': [{'ion_id': 1306, 'distance': 7.578710079193115, 'force': [-0.7823565006256104, 3.8195178508758545, -4.267391204833984], 'magnitude': 5.780261993408203}, {'ion_id': 1309, 'distance': 5.037866592407227, 'force': [-10.252406120300293, -4.798220634460449, -6.5559773445129395], 'magnitude': 13.08111572265625}, {'ion_id': 1320, 'distance': 9.588546752929688, 'force': [2.3740317821502686, -1.7368981838226318, -2.094464063644409], 'magnitude': 3.61104154586792}, {'ion_id': 2436, 'distance': 12.25199031829834, 'force': [0.5002684593200684, -0.11152303218841553, -2.1514830589294434], 'magnitude': 2.2116928100585938}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.714705944061279, 'force': [2.5282323360443115, -3.42513370513916, 0.2689163088798523], 'magnitude': 4.265655517578125}, {'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.9969868659973145, 'force': [-3.401597499847412, -5.548208713531494, -0.9848582148551941], 'magnitude': 6.5820536613464355}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.643714427947998, 'force': [4.178359508514404, 4.446136951446533, 0.9957524538040161], 'magnitude': 6.182098865509033}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.181082248687744, 'force': [3.9827682971954346, 10.391151428222656, 2.31917142868042], 'magnitude': 11.367366790771484}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.225279331207275, 'force': [-2.8059706687927246, -6.969738006591797, -2.106276273727417], 'magnitude': 7.803020000457764}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.655406951904297, 'force': [-0.8367324471473694, -4.1805949211120605, -0.8908227682113647], 'magnitude': 4.3555779457092285}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.8687236309051514, 'force': [-0.8066186904907227, 15.26418685913086, -4.061367034912109], 'magnitude': 15.815838813781738}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.62357497215271, 'force': [0.3202016353607178, -27.434558868408203, 8.101126670837402], 'magnitude': 28.60744285583496}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.746272563934326, 'force': [-2.539971113204956, -12.90213394165039, 3.250295877456665], 'magnitude': 13.545513153076172}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.569466590881348, 'force': [2.6129343509674072, 5.93994665145874, -1.549977421760559], 'magnitude': 6.671792984008789}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.698250770568848, 'force': [0.590602695941925, 4.160045623779297, -0.8672493696212769], 'magnitude': 4.290327548980713}]}, 5350: {'frame': 5350, 'ionic_force': [-2.6436456441879272, -5.840722948312759, -5.4077256843447685], 'ionic_force_magnitude': 8.387276311658225, 'motion_vector': [2.5827255249023438, 0.7509269714355469, 2.464935302734375], 'ionic_force_x': -2.6436456441879272, 'ionic_force_y': -5.840722948312759, 'ionic_force_z': -5.4077256843447685, 'radial_force': 6.4111548765398805, 'axial_force': -5.4077256843447685, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-0.9372458755970001, -14.393380880355835, -5.259363174438477], 'asn_force_magnitude': 15.352808993762544, 'residue_force': [-0.9372458755970001, -14.393380880355835, -5.259363174438477], 'residue_force_magnitude': 15.352808993762544, 'total_force': [-3.5808915197849274, -20.234103828668594, -10.667088858783245], 'total_force_magnitude': 23.152289876964357, 'motion_component_total': -13.906790526765015, 'cosine_total_motion': -0.6006658780046521, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.46763204887808907, 'cosine_residue_motion': -0.46763204887808907, 'cosine_ionic_motion': -0.8020869649455775, 'motion_component_glu': None, 'motion_component_asn': -7.179465525787132, 'motion_component_residue': -7.179465525787132, 'motion_component_ionic': -6.727325000977883, 'ionic_contributions': [{'ion_id': 1306, 'distance': 5.389224529266357, 'force': [-2.4985830783843994, 10.913158416748047, -2.3083724975585938], 'magnitude': 11.43103313446045}, {'ion_id': 1309, 'distance': 4.974605083465576, 'force': [-7.1796159744262695, -10.836474418640137, 3.318307876586914], 'magnitude': 13.415931701660156}, {'ion_id': 1320, 'distance': 6.856228351593018, 'force': [5.264742851257324, -4.707367897033691, -0.06457030028104782], 'magnitude': 7.062648296356201}, {'ion_id': 2434, 'distance': 13.50754165649414, 'force': [0.3296545743942261, -0.23305991291999817, -1.7742886543273926], 'magnitude': 1.8196399211883545}, {'ion_id': 2436, 'distance': 8.232723236083984, 'force': [1.4401559829711914, -0.97697913646698, -4.578802108764648], 'magnitude': 4.8983635902404785}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.6037564277648926, 'force': [-1.701090693473816, 13.214588165283203, 12.438122749328613], 'magnitude': 18.227066040039062}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.5839462280273438, 'force': [-0.2818261384963989, -25.29926300048828, -15.153389930725098], 'magnitude': 29.491649627685547}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.383675575256348, 'force': [-2.2130520343780518, -9.805706977844238, -12.292037010192871], 'magnitude': 15.879032135009766}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.1893157958984375, 'force': [2.88234806060791, 4.61500358581543, 5.779166221618652], 'magnitude': 7.937565803527832}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.321555137634277, 'force': [0.3763749301433563, 2.8819973468780518, 3.9687747955322266], 'magnitude': 4.9192214012146}]}, 5357: {'frame': 5357, 'ionic_force': [-8.905019342899323, -7.153529971837997, -3.628664266318083], 'ionic_force_magnitude': 11.984972461922863, 'motion_vector': [1.0815353393554688, -1.1651802062988281, 1.2048263549804688], 'ionic_force_x': -8.905019342899323, 'ionic_force_y': -7.153529971837997, 'ionic_force_z': -3.628664266318083, 'radial_force': 11.42244984910836, 'axial_force': -3.628664266318083, 'glu_force': [-14.458162307739258, -25.77945041656494, 17.271218299865723], 'glu_force_magnitude': 34.23322220677859, 'asn_force': [-0.9490005970001221, 1.3122189715504646, 0.2846684455871582], 'asn_force_magnitude': 1.6442496423343251, 'residue_force': [-15.40716290473938, -24.467231445014477, 17.55588674545288], 'residue_force_magnitude': 33.82654642106183, 'total_force': [-24.312182247638702, -31.620761416852474, 13.927222479134798], 'total_force_magnitude': 42.24834060891886, 'motion_component_total': 13.700706003078228, 'cosine_total_motion': 0.3242898018149838, 'cosine_glu_motion': 0.5156165811506185, 'cosine_asn_motion': -0.6745362784715716, 'cosine_residue_motion': 0.48902748614946956, 'cosine_ionic_motion': -0.2370806413914865, 'motion_component_glu': 17.65121699602861, 'motion_component_asn': -1.1091060346184083, 'motion_component_residue': 16.542110961410202, 'motion_component_ionic': -2.8414049583319754, 'ionic_contributions': [{'ion_id': 1306, 'distance': 11.257436752319336, 'force': [-2.544297695159912, 0.6225996017456055, -0.04454083368182182], 'magnitude': 2.6197452545166016}, {'ion_id': 1309, 'distance': 12.459333419799805, 'force': [-1.7606245279312134, -0.44900551438331604, 1.1280972957611084], 'magnitude': 2.13869309425354}, {'ion_id': 1320, 'distance': 7.310723304748535, 'force': [-1.3347965478897095, -6.032811641693115, -0.6402768492698669], 'magnitude': 6.211799621582031}, {'ion_id': 2434, 'distance': 12.882223129272461, 'force': [-0.9485629200935364, -0.36116552352905273, -1.7239831686019897], 'magnitude': 2.000582456588745}, {'ion_id': 2436, 'distance': 9.84126091003418, 'force': [-2.316737651824951, -0.9331468939781189, -2.3479607105255127], 'magnitude': 3.427966594696045}], 'glu_contributions': [{'resid': 1073, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.6488587856292725, 'force': [9.130406379699707, 13.733925819396973, -11.461014747619629], 'magnitude': 20.083324432373047}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 3.767866611480713, 'force': [-12.514763832092285, -8.214937210083008, 11.939172744750977], 'magnitude': 19.14806365966797}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.703062057495117, 'force': [-11.07380485534668, -31.298439025878906, 16.793060302734375], 'magnitude': 37.20521926879883}], 'asn_contributions': [{'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.690690040588379, 'force': [-4.285954475402832, 0.1079070046544075, 5.920322418212891], 'magnitude': 7.309669494628906}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.437745094299316, 'force': [3.33695387840271, 1.2043119668960571, -5.635653972625732], 'magnitude': 6.659296035766602}]}, 5358: {'frame': 5358, 'ionic_force': [-11.324523270130157, -9.701948136091232, -1.8851598501205444], 'ionic_force_magnitude': 15.030850028911543, 'motion_vector': [-0.13986587524414062, 0.56707763671875, 0.13983154296875], 'ionic_force_x': -11.324523270130157, 'ionic_force_y': -9.701948136091232, 'ionic_force_z': -1.8851598501205444, 'radial_force': 14.912163656932, 'axial_force': -1.8851598501205444, 'glu_force': [-21.786322593688965, -22.081520557403564, 0.5893383026123047], 'glu_force_magnitude': 31.025549502277062, 'asn_force': [-0.42053282260894775, 1.0421932339668274, 1.0245709419250488], 'asn_force_magnitude': 1.5207761856548336, 'residue_force': [-22.206855416297913, -21.039327323436737, 1.6139092445373535], 'residue_force_magnitude': 30.633354774700642, 'total_force': [-33.53137868642807, -30.74127545952797, -0.2712506055831909], 'total_force_magnitude': 45.49124036979261, 'motion_component_total': -21.28075185600639, 'cosine_total_motion': -0.4677988923365865, 'cosine_glu_motion': -0.5040655535571943, 'cosine_asn_motion': 0.8683377820398746, 'cosine_residue_motion': -0.46741088168626044, 'cosine_ionic_motion': -0.46320657037782487, 'motion_component_glu': -15.638910784281421, 'motion_component_asn': 1.3205474200305787, 'motion_component_residue': -14.318363364250843, 'motion_component_ionic': -6.962388491755545, 'ionic_contributions': [{'ion_id': 1306, 'distance': 10.533956527709961, 'force': [-2.950573682785034, 0.41228511929512024, 0.27555233240127563], 'magnitude': 2.9919545650482178}, {'ion_id': 1309, 'distance': 8.590034484863281, 'force': [-2.585419178009033, -2.5263538360595703, 2.679021120071411], 'magnitude': 4.499334335327148}, {'ion_id': 1320, 'distance': 7.956185340881348, 'force': [-1.769490361213684, -4.937245845794678, 0.018840014934539795], 'magnitude': 5.244792461395264}, {'ion_id': 2434, 'distance': 12.551528930664062, 'force': [-0.9104146361351013, -0.6412608623504639, -1.7891393899917603], 'magnitude': 2.107389450073242}, {'ion_id': 2436, 'distance': 8.309216499328613, 'force': [-3.1086254119873047, -2.0093727111816406, -3.0694339275360107], 'magnitude': 4.808591842651367}], 'glu_contributions': [{'resid': 1073, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.5416152477264404, 'force': [15.885651588439941, 13.243943214416504, -5.167411804199219], 'magnitude': 21.318023681640625}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 3.76960825920105, 'force': [-17.6264705657959, -6.562671184539795, 3.4942963123321533], 'magnitude': 19.130374908447266}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.7816860675811768, 'force': [-20.045503616333008, -28.762792587280273, 2.26245379447937], 'magnitude': 35.13174057006836}], 'asn_contributions': [{'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.960376262664795, 'force': [-1.8748300075531006, -0.879643976688385, 6.3331618309021], 'magnitude': 6.6631598472595215}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.811611175537109, 'force': [1.4542971849441528, 1.9218372106552124, -5.308590888977051], 'magnitude': 5.830057621002197}]}, 5359: {'frame': 5359, 'ionic_force': [-10.53284615278244, -8.8823823928833, -3.6715437918901443], 'ionic_force_magnitude': 14.25895504121372, 'motion_vector': [-0.3754844665527344, 0.34723663330078125, 0.0055084228515625], 'ionic_force_x': -10.53284615278244, 'ionic_force_y': -8.8823823928833, 'ionic_force_z': -3.6715437918901443, 'radial_force': 13.778155357361417, 'axial_force': -3.6715437918901443, 'glu_force': [-23.447912216186523, -20.212891578674316, 1.183917723596096], 'glu_force_magnitude': 30.980110303959172, 'asn_force': [-1.0798755884170532, 1.0870248824357986, 1.4386496543884277], 'asn_force_magnitude': 2.101777155067963, 'residue_force': [-24.527787804603577, -19.125866696238518, 2.6225673779845238], 'residue_force_magnitude': 31.213602982065595, 'total_force': [-35.06063395738602, -28.00824908912182, -1.0489764139056206], 'total_force_magnitude': 44.88663968319563, 'motion_component_total': 6.713036481960517, 'cosine_total_motion': 0.14955533604966423, 'cosine_glu_motion': 0.11310692527907534, 'cosine_asn_motion': 0.7356959750651075, 'cosine_residue_motion': 0.1617991366666798, 'cosine_ionic_motion': 0.11660759588623211, 'motion_component_glu': 3.5040650212874223, 'motion_component_asn': 1.5462689934672929, 'motion_component_residue': 5.050334014754715, 'motion_component_ionic': 1.6627024672058017, 'ionic_contributions': [{'ion_id': 1306, 'distance': 10.268025398254395, 'force': [-3.0441882610321045, 0.7864692211151123, 0.17377707362174988], 'magnitude': 3.1489386558532715}, {'ion_id': 1309, 'distance': 8.95406723022461, 'force': [-3.55322265625, -1.968692660331726, 0.8038131594657898], 'magnitude': 4.140924453735352}, {'ion_id': 1320, 'distance': 7.730974197387695, 'force': [-0.5556600689888, -5.521777629852295, -0.23913930356502533], 'magnitude': 5.554815292358398}, {'ion_id': 2434, 'distance': 12.37110710144043, 'force': [-0.9361525774002075, -0.5566215515136719, -1.8760818243026733], 'magnitude': 2.169306993484497}, {'ion_id': 2436, 'distance': 9.255210876464844, 'force': [-2.443622589111328, -1.6217597723007202, -2.5339128971099854], 'magnitude': 3.8758368492126465}], 'glu_contributions': [{'resid': 1073, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.4769842624664307, 'force': [16.11248207092285, 13.749393463134766, -6.367447853088379], 'magnitude': 22.117918014526367}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 3.6871957778930664, 'force': [-17.459463119506836, -6.3013410568237305, 7.433990478515625], 'magnitude': 19.995098114013672}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.7708871364593506, 'force': [-22.10093116760254, -27.66094398498535, 0.11737509816884995], 'magnitude': 35.40611267089844}], 'asn_contributions': [{'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.7145185470581055, 'force': [-2.8509726524353027, -0.19972173869609833, 6.661658763885498], 'magnitude': 7.248836517333984}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.89658260345459, 'force': [1.7710970640182495, 1.286746621131897, -5.22300910949707], 'magnitude': 5.663243293762207}]}, 5360: {'frame': 5360, 'ionic_force': [-9.028356164693832, -11.008867591619492, -3.8418196588754654], 'ionic_force_magnitude': 14.746727059849487, 'motion_vector': [0.4962959289550781, -1.1936683654785156, -0.0410003662109375], 'ionic_force_x': -9.028356164693832, 'ionic_force_y': -11.008867591619492, 'ionic_force_z': -3.8418196588754654, 'radial_force': 14.23749910224317, 'axial_force': -3.8418196588754654, 'glu_force': [-25.60232162475586, -21.104600429534912, 2.789428234100342], 'glu_force_magnitude': 33.29660555883982, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [-25.60232162475586, -21.104600429534912, 2.789428234100342], 'residue_force_magnitude': 33.29660555883982, 'total_force': [-34.63067778944969, -32.113468021154404, -1.0523914247751236], 'total_force_magnitude': 47.24051439403821, 'motion_component_total': 16.38257392366342, 'cosine_total_motion': 0.34679076072319215, 'cosine_glu_motion': 0.2872666576447246, 'cosine_asn_motion': None, 'cosine_residue_motion': 0.2872666576447246, 'cosine_ionic_motion': 0.462310674510465, 'motion_component_glu': 9.565004589802673, 'motion_component_asn': None, 'motion_component_residue': 9.565004589802673, 'motion_component_ionic': 6.817569333860742, 'ionic_contributions': [{'ion_id': 1306, 'distance': 10.124517440795898, 'force': [-3.037724494934082, 1.0906109809875488, 0.26996007561683655], 'magnitude': 3.2388393878936768}, {'ion_id': 1309, 'distance': 12.860404014587402, 'force': [-1.7648735046386719, -0.8681292533874512, 0.4014160633087158], 'magnitude': 2.0073769092559814}, {'ion_id': 1320, 'distance': 6.024328708648682, 'force': [-0.222377210855484, -9.145050048828125, 0.049248531460762024], 'magnitude': 9.147886276245117}, {'ion_id': 2434, 'distance': 13.161803245544434, 'force': [-0.8280560374259949, -0.4974512755870819, -1.6552377939224243], 'magnitude': 1.91649329662323}, {'ion_id': 2436, 'distance': 8.505693435668945, 'force': [-3.1753249168395996, -1.5888479948043823, -2.9072065353393555], 'magnitude': 4.589005947113037}], 'glu_contributions': [{'resid': 1073, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.414323329925537, 'force': [16.867462158203125, 13.998327255249023, -6.756528377532959], 'magnitude': 22.937198638916016}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 3.596926212310791, 'force': [-18.054765701293945, -6.262147426605225, 8.734156608581543], 'magnitude': 21.011295318603516}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.6818509101867676, 'force': [-24.41501808166504, -28.84078025817871, 0.8118000030517578], 'magnitude': 37.79606628417969}], 'asn_contributions': []}, 5361: {'frame': 5361, 'ionic_force': [-7.815921291708946, -18.790564686059952, -0.12370511889457703], 'ionic_force_magnitude': 20.351639978528347, 'motion_vector': [-0.574737548828125, 0.9560508728027344, -0.38732147216796875], 'ionic_force_x': -7.815921291708946, 'ionic_force_y': -18.790564686059952, 'ionic_force_z': -0.12370511889457703, 'radial_force': 20.351264011338277, 'axial_force': -0.12370511889457703, 'glu_force': [-31.51246452331543, -16.46138310432434, 1.369075059890747], 'glu_force_magnitude': 35.57930466661993, 'asn_force': [-0.19230318069458008, 0.3716185688972473, -1.0902862548828125], 'asn_force_magnitude': 1.1678206162081912, 'residue_force': [-31.70476770401001, -16.089764535427094, 0.27878880500793457], 'residue_force_magnitude': 35.55489475681964, 'total_force': [-39.520688995718956, -34.880329221487045, 0.15508368611335754], 'total_force_magnitude': 52.71191778189599, 'motion_component_total': -9.055796019138132, 'cosine_total_motion': -0.1717978855675094, 'cosine_glu_motion': 0.04387189918863489, 'cosine_asn_motion': 0.6440160851360817, 'cosine_residue_motion': 0.06505509142264104, 'cosine_ionic_motion': -0.5586194999547898, 'motion_component_glu': 1.5609316675356766, 'motion_component_asn': 0.7520952613916059, 'motion_component_residue': 2.3130269289272825, 'motion_component_ionic': -11.368822948065414, 'ionic_contributions': [{'ion_id': 1306, 'distance': 11.069668769836426, 'force': [-2.695746898651123, 0.2362404763698578, 0.13357296586036682], 'magnitude': 2.7093729972839355}, {'ion_id': 1309, 'distance': 13.667428970336914, 'force': [-1.4405096769332886, -0.9803712368011475, 0.35021817684173584], 'magnitude': 1.7773150205612183}, {'ion_id': 1320, 'distance': 4.601624011993408, 'force': [0.1950037032365799, -15.115640640258789, 4.1602349281311035], 'magnitude': 15.678908348083496}, {'ion_id': 2434, 'distance': 11.943093299865723, 'force': [-0.9663851857185364, -0.6437287330627441, -2.0172598361968994], 'magnitude': 2.3275790214538574}, {'ion_id': 2436, 'distance': 8.486127853393555, 'force': [-2.908283233642578, -2.287064552307129, -2.750471353530884], 'magnitude': 4.610191822052002}], 'glu_contributions': [{'resid': 1073, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.522725820541382, 'force': [18.8028507232666, 8.688213348388672, -5.937351703643799], 'magnitude': 21.547258377075195}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 3.9435465335845947, 'force': [-16.803157806396484, -1.5786983966827393, 4.55112886428833], 'magnitude': 17.48002052307129}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.5729293823242188, 'force': [-33.51215744018555, -23.570898056030273, 2.755297899246216], 'magnitude': 41.06389617919922}], 'asn_contributions': [{'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.671150207519531, 'force': [4.405974388122559, 1.7179784774780273, -8.225048065185547], 'magnitude': 9.487648010253906}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.992292404174805, 'force': [-2.012876033782959, -1.2323555946350098, 3.079118251800537], 'magnitude': 3.879605770111084}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.3810858726501465, 'force': [-2.5854015350341797, -0.11400431394577026, 4.055643558502197], 'magnitude': 4.810981273651123}]}, 5362: {'frame': 5362, 'ionic_force': [-5.433648765087128, -16.242994844913483, 4.414413258433342], 'ionic_force_magnitude': 17.68746632082874, 'motion_vector': [0.4037361145019531, -0.2184600830078125, -0.226226806640625], 'ionic_force_x': -5.433648765087128, 'ionic_force_y': -16.242994844913483, 'ionic_force_z': 4.414413258433342, 'radial_force': 17.127738333890406, 'axial_force': 4.414413258433342, 'glu_force': [-22.37955665588379, -21.767789840698242, 0.5034797191619873], 'glu_force_magnitude': 31.22394469778483, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [-22.37955665588379, -21.767789840698242, 0.5034797191619873], 'residue_force</t>
+          <t>{5347: {'frame': 5347, 'motion_vector': [3.316211700439453, -1.65020751953125, -0.9902801513671875], 'ionic_force': [-1.5767408609390259, -7.108273267745972, -12.609045714139938], 'ionic_force_magnitude': 14.560277964818443, 'radial_force': 7.281048042109511, 'axial_force': -12.609045714139938, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-2.012432560324669, 9.585110425949097, -5.336213946342468], 'asn_force_magnitude': 11.153448164968214, 'residue_force': [-2.012432560324669, 9.585110425949097, -5.336213946342468], 'residue_force_magnitude': 11.153448164968214, 'total_force': [-3.5891734212636948, 2.476837158203125, -17.945259660482407], 'total_force_magnitude': 18.46751830751221, 'cosine_total_motion': 0.02515360377623704, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.40235943734978263, 'cosine_residue_motion': -0.40235943734978263, 'cosine_ionic_motion': 0.34011849075752815, 'motion_component_total': 0.46452463823756585, 'motion_component_glu': None, 'motion_component_asn': -4.4876951281665765, 'motion_component_residue': -4.4876951281665765, 'motion_component_ionic': 4.952219766404142, 'motion_component_percent_total': 2.515360377623704, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 40.235943734978264, 'motion_component_percent_residue': 40.235943734978264, 'motion_component_percent_ionic': 34.011849075752814, 'ionic_contributions': [{'ion_id': 1306, 'distance': 10.253976821899414, 'force': [-2.2620508670806885, 2.0216140747070312, -0.8754827976226807], 'magnitude': 3.1575732231140137, 'cosine_ionic_motion': -0.8235514760017395, 'motion_component_ionic': -2.60042405128479, 'motion_component_percent_ionic': 82.35514760017395}, {'ion_id': 1309, 'distance': 9.169376373291016, 'force': [-3.900376081466675, -0.4288240671157837, -0.44240328669548035], 'magnitude': 3.948739528656006, 'cosine_ionic_motion': -0.7786338925361633, 'motion_component_ionic': -3.074622392654419, 'motion_component_percent_ionic': 77.86338925361633}, {'ion_id': 1320, 'distance': 5.010506629943848, 'force': [5.2017621994018555, -9.052448272705078, -8.116565704345703], 'magnitude': 13.224363327026367, 'cosine_ionic_motion': 0.7933406829833984, 'motion_component_ionic': 10.491425514221191, 'motion_component_percent_ionic': 79.33406829833984}, {'ion_id': 2436, 'distance': 10.102682113647461, 'force': [-0.6160761117935181, 0.3513849973678589, -3.174593925476074], 'magnitude': 3.2528553009033203, 'cosine_ionic_motion': 0.04176044464111328, 'motion_component_ionic': 0.13584068417549133, 'motion_component_percent_ionic': 4.176044464111328}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.1278557777404785, 'force': [1.8304100036621094, -9.567811965942383, 9.904873847961426], 'magnitude': 13.89244270324707, 'cosine_with_motion': 0.22622698545455933, 'motion_component': 3.142845392227173, 'motion_component_percent': 22.622698545455933}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.937706470489502, 'force': [-2.408155679702759, 15.851311683654785, -16.233600616455078], 'magnitude': 22.816509246826172, 'cosine_with_motion': -0.20653241872787476, 'motion_component': -4.712348937988281, 'motion_component_percent': 20.653241872787476}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.964436054229736, 'force': [1.0552637577056885, 8.436544418334961, -9.000224113464355], 'magnitude': 12.38115119934082, 'cosine_with_motion': -0.03180469945073128, 'motion_component': -0.39377880096435547, 'motion_component_percent': 3.1804699450731277}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.741171360015869, 'force': [-1.7530465126037598, -3.939984083175659, 4.450823783874512], 'magnitude': 6.197296142578125, 'cosine_with_motion': -0.15652279555797577, 'motion_component': -0.9700181484222412, 'motion_component_percent': 15.652279555797577}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.957278251647949, 'force': [-0.20133398473262787, -2.687417507171631, 2.854046583175659], 'magnitude': 3.925344467163086, 'cosine_with_motion': 0.06251095235347748, 'motion_component': 0.24537703394889832, 'motion_component_percent': 6.251095235347748}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.68625020980835, 'force': [-2.6577091217041016, 3.119086980819702, 1.330664038658142], 'magnitude': 4.308455467224121, 'cosine_with_motion': -0.9248712062835693, 'motion_component': -3.9847664833068848, 'motion_component_percent': 92.48712062835693}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.918987274169922, 'force': [3.7938876152038574, 8.250432014465332, 3.639465093612671], 'magnitude': 9.783093452453613, 'cosine_with_motion': -0.1236373633146286, 'motion_component': -1.2095558643341064, 'motion_component_percent': 12.36373633146286}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.591378211975098, 'force': [-1.4122247695922852, -8.516304016113281, -3.5674989223480225], 'magnitude': 9.340709686279297, 'cosine_with_motion': 0.36028361320495605, 'motion_component': 3.365304708480835, 'motion_component_percent': 36.028361320495605}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.47483491897583, 'force': [-8.311904907226562, -10.374906539916992, -7.449184894561768], 'magnitude': 15.23866081237793, 'cosine_with_motion': -0.05248343572020531, 'motion_component': -0.7997772693634033, 'motion_component_percent': 5.248343572020531}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.7777469158172607, 'force': [4.578917503356934, 5.99346399307251, 6.196365833282471], 'magnitude': 9.761303901672363, 'cosine_with_motion': -0.022495586425065994, 'motion_component': -0.21958625316619873, 'motion_component_percent': 2.2495586425065994}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.147976398468018, 'force': [3.473463535308838, 3.020695447921753, 2.538055419921875], 'magnitude': 5.2565460205078125, 'cosine_with_motion': 0.19948643445968628, 'motion_component': 1.0486096143722534, 'motion_component_percent': 19.948643445968628}]}, 5348: {'frame': 5348, 'motion_vector': [1.4751319885253906, 0.6213607788085938, -1.0232925415039062], 'ionic_force': [-6.454585552215576, -0.6436145454645157, -10.31672191619873], 'ionic_force_magnitude': 12.186495206997735, 'radial_force': 6.4865949722488105, 'axial_force': -10.31672191619873, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [9.034229032695293, 4.56985867023468, -0.8264970034360886], 'asn_force_magnitude': 10.157952538666562, 'residue_force': [9.034229032695293, 4.56985867023468, -0.8264970034360886], 'residue_force_magnitude': 10.157952538666562, 'total_force': [2.5796434804797173, 3.9262441247701645, -11.143218919634819], 'total_force_magnitude': 12.093026143384506, 'cosine_total_motion': 0.7681496015902591, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.8815375083814108, 'cosine_residue_motion': 0.8815375083814108, 'cosine_ionic_motion': 0.027459662288833966, 'motion_component_total': 9.289253214061397, 'motion_component_glu': None, 'motion_component_asn': 8.954616171192747, 'motion_component_residue': 8.954616171192747, 'motion_component_ionic': 0.3346370428686516, 'motion_component_percent_total': 76.81496015902592, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 88.15375083814108, 'motion_component_percent_residue': 88.15375083814108, 'motion_component_percent_ionic': 2.745966228883397, 'ionic_contributions': [{'ion_id': 1306, 'distance': 7.247408866882324, 'force': [-3.4947903156280518, 3.541504383087158, -3.898306131362915], 'magnitude': 6.320806980133057, 'cosine_ionic_motion': 0.08613929152488708, 'motion_component_ionic': 0.5444698333740234, 'motion_component_percent_ionic': 8.613929152488708}, {'ion_id': 1309, 'distance': 7.04019021987915, 'force': [-6.009511947631836, -2.5683140754699707, -1.4689178466796875], 'magnitude': 6.6983723640441895, 'cosine_ionic_motion': -0.7039017677307129, 'motion_component_ionic': -4.714996337890625, 'motion_component_percent_ionic': 70.39017677307129}, {'ion_id': 1320, 'distance': 9.25703239440918, 'force': [2.708761215209961, -1.4557560682296753, -2.3566243648529053], 'magnitude': 3.874311685562134, 'cosine_ionic_motion': 0.7476143836975098, 'motion_component_ionic': 2.896491050720215, 'motion_component_percent_ionic': 74.76143836975098}, {'ion_id': 2436, 'distance': 11.256568908691406, 'force': [0.3409554958343506, -0.1610487848520279, -2.5928735733032227], 'magnitude': 2.6201491355895996, 'cosine_ionic_motion': 0.6139623522758484, 'motion_component_ionic': 1.6086729764938354, 'motion_component_percent_ionic': 61.39623522758484}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.968769073486328, 'force': [-3.061173677444458, 3.62992787361145, -2.8287014961242676], 'magnitude': 5.5270891189575195, 'cosine_with_motion': 0.06042170152068138, 'motion_component': 0.33395612239837646, 'motion_component_percent': 6.042170152068138}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.92423677444458, 'force': [-3.5336523056030273, 7.641610622406006, -2.1703529357910156], 'magnitude': 8.694328308105469, 'cosine_with_motion': 0.10634195804595947, 'motion_component': 0.9245718717575073, 'motion_component_percent': 10.634195804595947}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.204074382781982, 'force': [1.4865944385528564, -4.701045036315918, 1.4660147428512573], 'magnitude': 5.143830299377441, 'cosine_with_motion': -0.22802188992500305, 'motion_component': -1.1729059219360352, 'motion_component_percent': 22.802188992500305}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.9277448654174805, 'force': [5.234803676605225, 6.926398277282715, -0.18550346791744232], 'magnitude': 8.684041023254395, 'cosine_with_motion': 0.7404352426528931, 'motion_component': 6.4299702644348145, 'motion_component_percent': 74.0435242652893}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.112987518310547, 'force': [-3.6498842239379883, -3.8784492015838623, 0.17717140913009644], 'magnitude': 5.328734397888184, 'cosine_with_motion': -0.7877969145774841, 'motion_component': -4.197960376739502, 'motion_component_percent': 78.77969145774841}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.8407797813415527, 'force': [-8.138960838317871, 13.817949295043945, 0.5673233866691589], 'magnitude': 16.046815872192383, 'cosine_with_motion': -0.13123029470443726, 'motion_component': -2.105828285217285, 'motion_component_percent': 13.123029470443726}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.717693567276001, 'force': [16.912630081176758, -20.566455841064453, 1.3248811960220337], 'magnitude': 26.660297393798828, 'cosine_with_motion': 0.21349669992923737, 'motion_component': 5.691885471343994, 'motion_component_percent': 21.349669992923737}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.126919269561768, 'force': [3.754265308380127, -17.444454193115234, -1.6097160577774048], 'magnitude': 17.916324615478516, 'cosine_with_motion': -0.107354074716568, 'motion_component': -1.9233903884887695, 'motion_component_percent': 10.7354074716568}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.5537662506103516, 'force': [0.06863891333341599, 10.972410202026367, 1.1286287307739258], 'magnitude': 11.030516624450684, 'cosine_with_motion': 0.2750633955001831, 'motion_component': 3.0340912342071533, 'motion_component_percent': 27.50633955001831}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.119487762451172, 'force': [-0.9293440580368042, 5.20028018951416, 0.5872605443000793], 'magnitude': 5.315211296081543, 'cosine_with_motion': 0.12472046911716461, 'motion_component': 0.6629156470298767, 'motion_component_percent': 12.472046911716461}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.503318786621094, 'force': [6.718957424163818, 3.816227674484253, 1.1747814416885376], 'magnitude': 7.815887451171875, 'cosine_with_motion': 0.7462288737297058, 'motion_component': 5.8324408531188965, 'motion_component_percent': 74.62288737297058}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.4803242683410645, 'force': [-6.153043270111084, -1.834584355354309, -1.3260352611541748], 'magnitude': 6.556219577789307, 'cosine_with_motion': -0.7112981677055359, 'motion_component': -4.663426876068115, 'motion_component_percent': 71.12981677055359}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.622708797454834, 'force': [-10.682412147521973, -9.02637004852295, -2.8826956748962402], 'magnitude': 14.279328346252441, 'cosine_with_motion': -0.6788879036903381, 'motion_component': -9.694063186645508, 'motion_component_percent': 67.88879036903381}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.7758493423461914, 'force': [7.379847049713135, 5.593720436096191, 3.1181576251983643], 'magnitude': 9.771119117736816, 'cosine_with_motion': 0.6017932891845703, 'motion_component': 5.880194187164307, 'motion_component_percent': 60.17932891845703}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.920180797576904, 'force': [3.626962661743164, 4.422692775726318, 0.6322888135910034], 'magnitude': 5.754551410675049, 'cosine_with_motion': 0.681576132774353, 'motion_component': 3.9221649169921875, 'motion_component_percent': 68.1576132774353}]}, 5349: {'frame': 5349, 'motion_vector': [-0.10723876953125, -1.5981407165527344, 3.5609359741210938], 'ionic_force': [-8.160462379455566, -2.827123999595642, -15.069315671920776], 'ionic_force_magnitude': 17.368651391964672, 'radial_force': 8.636305712259105, 'axial_force': -15.069315671920776, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [3.8222084045410156, -20.25890064239502, 4.474711656570435], 'asn_force_magnitude': 21.096335623411584, 'residue_force': [3.8222084045410156, -20.25890064239502, 4.474711656570435], 'residue_force_magnitude': 21.096335623411584, 'total_force': [-4.338253974914551, -23.08602464199066, -10.594604015350342], 'total_force_magnitude': 25.768791503746144, 'cosine_total_motion': -0.003645130638338249, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.5815148384535481, 'cosine_residue_motion': 0.5815148384535481, 'cosine_ionic_motion': -0.7117284200402713, 'motion_component_total': -0.09393061142325543, 'motion_component_glu': None, 'motion_component_asn': 12.26783220201002, 'motion_component_residue': 12.26783220201002, 'motion_component_ionic': -12.361762813433275, 'motion_component_percent_total': 0.36451306383382487, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 58.15148384535481, 'motion_component_percent_residue': 58.15148384535481, 'motion_component_percent_ionic': 71.17284200402713, 'ionic_contributions': [{'ion_id': 1306, 'distance': 7.578710079193115, 'force': [-0.7823565006256104, 3.8195178508758545, -4.267391204833984], 'magnitude': 5.780261993408203, 'cosine_ionic_motion': -0.9400336146354675, 'motion_component_ionic': -5.433640480041504, 'motion_component_percent_ionic': 94.00336146354675}, {'ion_id': 1309, 'distance': 5.037866592407227, 'force': [-10.252406120300293, -4.798220634460449, -6.5559773445129395], 'magnitude': 13.08111572265625, 'cosine_ionic_motion': -0.2854103446006775, 'motion_component_ionic': -3.733485698699951, 'motion_component_percent_ionic': 28.54103446006775}, {'ion_id': 1320, 'distance': 9.588546752929688, 'force': [2.3740317821502686, -1.7368981838226318, -2.094464063644409], 'magnitude': 3.61104154586792, 'cosine_ionic_motion': -0.35015326738357544, 'motion_component_ionic': -1.2644180059432983, 'motion_component_percent_ionic': 35.015326738357544}, {'ion_id': 2436, 'distance': 12.25199031829834, 'force': [0.5002684593200684, -0.11152303218841553, -2.1514830589294434], 'magnitude': 2.2116928100585938, 'cosine_ionic_motion': -0.8727337121963501, 'motion_component_ionic': -1.9302188158035278, 'motion_component_percent_ionic': 87.27337121963501}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.714705944061279, 'force': [2.5282323360443115, -3.42513370513916, 0.2689163088798523], 'magnitude': 4.265655517578125, 'cosine_with_motion': 0.36986374855041504, 'motion_component': 1.5777113437652588, 'motion_component_percent': 36.986374855041504}, {'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.9969868659973145, 'force': [-3.401597499847412, -5.548208713531494, -0.9848582148551941], 'magnitude': 6.5820536613464355, 'cosine_with_motion': 0.22274459898471832, 'motion_component': 1.4661169052124023, 'motion_component_percent': 22.274459898471832}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.643714427947998, 'force': [4.178359508514404, 4.446136951446533, 0.9957524538040161], 'magnitude': 6.182098865509033, 'cosine_with_motion': -0.16603411734104156, 'motion_component': -1.0264393091201782, 'motion_component_percent': 16.603411734104156}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.181082248687744, 'force': [3.9827682971954346, 10.391151428222656, 2.31917142868042], 'magnitude': 11.367366790771484, 'cosine_with_motion': -0.19770710170269012, 'motion_component': -2.2474091053009033, 'motion_component_percent': 19.770710170269012}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.225279331207275, 'force': [-2.8059706687927246, -6.969738006591797, -2.106276273727417], 'magnitude': 7.803020000457764, 'cosine_with_motion': 0.12929202616214752, 'motion_component': 1.0088682174682617, 'motion_component_percent': 12.929202616214752}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.655406951904297, 'force': [-0.8367324471473694, -4.1805949211120605, -0.8908227682113647], 'magnitude': 4.3555779457092285, 'cosine_with_motion': 0.21160702407360077, 'motion_component': 0.9216709136962891, 'motion_component_percent': 21.160702407360077}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.8687236309051514, 'force': [-0.8066186904907227, 15.26418685913086, -4.061367034912109], 'magnitude': 15.815838813781738, 'cosine_with_motion': -0.6278113722801208, 'motion_component': -9.929363250732422, 'motion_component_percent': 62.781137228012085}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.62357497215271, 'force': [0.3202016353607178, -27.434558868408203, 8.101126670837402], 'magnitude': 28.60744285583496, 'cosine_with_motion': 0.6504685282707214, 'motion_component': 18.60824203491211, 'motion_component_percent': 65.04685282707214}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.746272563934326, 'force': [-2.539971113204956, -12.90213394165039, 3.250295877456665], 'magnitude': 13.545513153076172, 'cosine_with_motion': 0.6138420701026917, 'motion_component': 8.31480598449707, 'motion_component_percent': 61.384207010269165}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.569466590881348, 'force': [2.6129343509674072, 5.93994665145874, -1.549977421760559], 'magnitude': 6.671792984008789, 'cosine_with_motion': -0.5870283842086792, 'motion_component': -3.916531801223755, 'motion_component_percent': 58.70283842086792}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.698250770568848, 'force': [0.590602695941925, 4.160045623779297, -0.8672493696212769], 'magnitude': 4.290327548980713, 'cosine_with_motion': -0.5849995613098145, 'motion_component': -2.5098397731781006, 'motion_component_percent': 58.499956130981445}]}, 5350: {'frame': 5350, 'motion_vector': [2.5827255249023438, 0.7509269714355469, 2.464935302734375], 'ionic_force': [-2.6436456441879272, -5.840722948312759, -5.4077256843447685], 'ionic_force_magnitude': 8.387276311658225, 'radial_force': 6.4111548765398805, 'axial_force': -5.4077256843447685, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-0.9372458755970001, -14.393380880355835, -5.259363174438477], 'asn_force_magnitude': 15.352808993762544, 'residue_force': [-0.9372458755970001, -14.393380880355835, -5.259363174438477], 'residue_force_magnitude': 15.352808993762544, 'total_force': [-3.5808915197849274, -20.234103828668594, -10.667088858783245], 'total_force_magnitude': 23.152289876964357, 'cosine_total_motion': -0.6006658780046521, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.46763204887808907, 'cosine_residue_motion': -0.46763204887808907, 'cosine_ionic_motion': -0.8020869649455775, 'motion_component_total': -13.906790526765015, 'motion_component_glu': None, 'motion_component_asn': -7.179465525787132, 'motion_component_residue': -7.179465525787132, 'motion_component_ionic': -6.727325000977883, 'motion_component_percent_total': 60.06658780046521, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 46.763204887808904, 'motion_component_percent_residue': 46.763204887808904, 'motion_component_percent_ionic': 80.20869649455776, 'ionic_contributions': [{'ion_id': 1306, 'distance': 5.389224529266357, 'force': [-2.4985830783843994, 10.913158416748047, -2.3083724975585938], 'magnitude': 11.43103313446045, 'cosine_ionic_motion': -0.09467071294784546, 'motion_component_ionic': -1.082184076309204, 'motion_component_percent_ionic': 9.467071294784546}, {'ion_id': 1309, 'distance': 4.974605083465576, 'force': [-7.1796159744262695, -10.836474418640137, 3.318307876586914], 'magnitude': 13.415931701660156, 'cosine_ionic_motion': -0.37798985838890076, 'motion_component_ionic': -5.0710859298706055, 'motion_component_percent_ionic': 37.798985838890076}, {'ion_id': 1320, 'distance': 6.856228351593018, 'force': [5.264742851257324, -4.707367897033691, -0.06457030028104782], 'magnitude': 7.062648296356201, 'cosine_ionic_motion': 0.38434430956840515, 'motion_component_ionic': 2.7144887447357178, 'motion_component_percent_ionic': 38.434430956840515}, {'ion_id': 2434, 'distance': 13.50754165649414, 'force': [0.3296545743942261, -0.23305991291999817, -1.7742886543273926], 'magnitude': 1.8196399211883545, 'cosine_ionic_motion': -0.556908130645752, 'motion_component_ionic': -1.0133723020553589, 'motion_component_percent_ionic': 55.690813064575195}, {'ion_id': 2436, 'distance': 8.232723236083984, 'force': [1.4401559829711914, -0.97697913646698, -4.578802108764648], 'magnitude': 4.8983635902404785, 'cosine_ionic_motion': -0.4644758403301239, 'motion_component_ionic': -2.2751715183258057, 'motion_component_percent_ionic': 46.44758403301239}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.6037564277648926, 'force': [-1.701090693473816, 13.214588165283203, 12.438122749328613], 'magnitude': 18.227066040039062, 'cosine_with_motion': 0.5442085266113281, 'motion_component': 9.91932487487793, 'motion_component_percent': 54.42085266113281}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.5839462280273438, 'force': [-0.2818261384963989, -25.29926300048828, -15.153389930725098], 'magnitude': 29.491649627685547, 'cosine_with_motion': -0.5304880142211914, 'motion_component': -15.644966125488281, 'motion_component_percent': 53.04880142211914}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.383675575256348, 'force': [-2.2130520343780518, -9.805706977844238, -12.292037010192871], 'magnitude': 15.879032135009766, 'cosine_with_motion': -0.7487788796424866, 'motion_component': -11.889883995056152, 'motion_component_percent': 74.87788796424866}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.1893157958984375, 'force': [2.88234806060791, 4.61500358581543, 5.779166221618652], 'magnitude': 7.937565803527832, 'cosine_with_motion': 0.8686515092849731, 'motion_component': 6.8949785232543945, 'motion_component_percent': 86.86515092849731}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.321555137634277, 'force': [0.3763749301433563, 2.8819973468780518, 3.9687747955322266], 'magnitude': 4.9192214012146, 'cosine_with_motion': 0.7198460698127747, 'motion_component': 3.5410821437835693, 'motion_component_percent': 71.98460698127747}]}, 5357: {'frame': 5357, 'motion_vector': [1.0815353393554688, -1.1651802062988281, 1.2048263549804688], 'ionic_force': [-8.905019342899323, -7.153529971837997, -3.628664266318083], 'ionic_force_magnitude': 11.984972461922863, 'radial_force': 11.42244984910836, 'axial_force': -3.628664266318083, 'glu_force': [-14.458162307739258, -25.77945041656494, 17.271218299865723], 'glu_force_magnitude': 34.23322220677859, 'asn_force': [-0.9490005970001221, 1.3122189715504646, 0.2846684455871582], 'asn_force_magnitude': 1.6442496423343251, 'residue_force': [-15.40716290473938, -24.467231445014477, 17.55588674545288], 'residue_force_magnitude': 33.82654642106183, 'total_force': [-24.312182247638702, -31.620761416852474, 13.927222479134798], 'total_force_magnitude': 42.24834060891886, 'cosine_total_motion': 0.3242898018149838, 'cosine_glu_motion': 0.5156165811506185, 'cosine_asn_motion': -0.6745362784715716, 'cosine_residue_motion': 0.48902748614946956, 'cosine_ionic_motion': -0.2370806413914865, 'motion_component_total': 13.700706003078228, 'motion_component_glu': 17.65121699602861, 'motion_component_asn': -1.1091060346184083, 'motion_component_residue': 16.542110961410202, 'motion_component_ionic': -2.8414049583319754, 'motion_component_percent_total': 32.42898018149838, 'motion_component_percent_glu': 51.561658115061846, 'motion_component_percent_asn': 67.45362784715716, 'motion_component_percent_residue': 48.90274861494696, 'motion_component_percent_ionic': 23.70806413914865, 'ionic_contributions': [{'ion_id': 1306, 'distance': 11.257436752319336, 'force': [-2.544297695159912, 0.6225996017456055, -0.04454083368182182], 'magnitude': 2.6197452545166016, 'cosine_ionic_motion': -0.6756708025932312, 'motion_component_ionic': -1.7700854539871216, 'motion_component_percent_ionic': 67.56708025932312}, {'ion_id': 1309, 'distance': 12.459333419799805, 'force': [-1.7606245279312134, -0.44900551438331604, 1.1280972957611084], 'magnitude': 2.13869309425354, 'cosine_ionic_motion': -0.005120324902236462, 'motion_component_ionic': -0.010950803756713867, 'motion_component_percent_ionic': 0.5120324902236462}, {'ion_id': 1320, 'distance': 7.310723304748535, 'force': [-1.3347965478897095, -6.032811641693115, -0.6402768492698669], 'magnitude': 6.211799621582031, 'cosine_ionic_motion': 0.3885320723056793, 'motion_component_ionic': 2.4134833812713623, 'motion_component_percent_ionic': 38.85320723056793}, {'ion_id': 2434, 'distance': 12.882223129272461, 'force': [-0.9485629200935364, -0.36116552352905273, -1.7239831686019897], 'magnitude': 2.000582456588745, 'cosine_ionic_motion': -0.6721193194389343, 'motion_component_ionic': -1.3446301221847534, 'motion_component_percent_ionic': 67.21193194389343}, {'ion_id': 2436, 'distance': 9.84126091003418, 'force': [-2.316737651824951, -0.9331468939781189, -2.3479607105255127], 'magnitude': 3.427966594696045, 'cosine_ionic_motion': -0.6211325526237488, 'motion_component_ionic': -2.1292216777801514, 'motion_component_percent_ionic': 62.11325526237488}], 'glu_contributions': [{'resid': 1073, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.6488587856292725, 'force': [9.130406379699707, 13.733925819396973, -11.461014747619629], 'magnitude': 20.083324432373047, 'cosine_with_motion': -0.49764636158943176, 'motion_component': -9.994393348693848, 'motion_component_percent': 49.764636158943176}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 3.767866611480713, 'force': [-12.514763832092285, -8.214937210083008, 11.939172744750977], 'magnitude': 19.14806365966797, 'cosine_with_motion': 0.2728436589241028, 'motion_component': 5.224427700042725, 'motion_component_percent': 27.28436589241028}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.703062057495117, 'force': [-11.07380485534668, -31.298439025878906, 16.793060302734375], 'magnitude': 37.20521926879883, 'cosine_with_motion': 0.602635383605957, 'motion_component': 22.42118263244629, 'motion_component_percent': 60.2635383605957}], 'asn_contributions': [{'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.690690040588379, 'force': [-4.285954475402832, 0.1079070046544075, 5.920322418212891], 'magnitude': 7.309669494628906, 'cosine_with_motion': 0.16266655921936035, 'motion_component': 1.1890387535095215, 'motion_component_percent': 16.266655921936035}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.437745094299316, 'force': [3.33695387840271, 1.2043119668960571, -5.635653972625732], 'magnitude': 6.659296035766602, 'cosine_with_motion': -0.3451032340526581, 'motion_component': -2.298144578933716, 'motion_component_percent': 34.51032340526581}]}, 5358: {'frame': 5358, 'motion_vector': [-0.13986587524414062, 0.56707763671875, 0.13983154296875], 'ionic_force': [-11.324523270130157, -9.701948136091232, -1.8851598501205444], 'ionic_force_magnitude': 15.030850028911543, 'radial_force': 14.912163656932, 'axial_force': -1.8851598501205444, 'glu_force': [-21.786322593688965, -22.081520557403564, 0.5893383026123047], 'glu_force_magnitude': 31.025549502277062, 'asn_force': [-0.42053282260894775, 1.0421932339668274, 1.0245709419250488], 'asn_force_magnitude': 1.5207761856548336, 'residue_force': [-22.206855416297913, -21.039327323436737, 1.6139092445373535], 'residue_force_magnitude': 30.633354774700642, 'total_force': [-33.53137868642807, -30.74127545952797, -0.2712506055831909], 'total_force_magnitude': 45.49124036979261, 'cosine_total_motion': -0.4677988923365865, 'cosine_glu_motion': -0.5040655535571943, 'cosine_asn_motion': 0.8683377820398746, 'cosine_residue_motion': -0.46741088168626044, 'cosine_ionic_motion': -0.46320657037782487, 'motion_component_total': -21.28075185600639, 'motion_component_glu': -15.638910784281421, 'motion_component_asn': 1.3205474200305787, 'motion_component_residue': -14.318363364250843, 'motion_component_ionic': -6.962388491755545, 'motion_component_percent_total': 46.77988923365865, 'motion_component_percent_glu': 50.406555355719426, 'motion_component_percent_asn': 86.83377820398745, 'motion_component_percent_residue': 46.74108816862604, 'motion_component_percent_ionic': 46.32065703778249, 'ionic_contributions': [{'ion_id': 1306, 'distance': 10.533956527709961, 'force': [-2.950573682785034, 0.41228511929512024, 0.27555233240127563], 'magnitude': 2.9919545650482178, 'cosine_ionic_motion': 0.3812198042869568, 'motion_component_ionic': 1.140592336654663, 'motion_component_percent_ionic': 38.12198042869568}, {'ion_id': 1309, 'distance': 8.590034484863281, 'force': [-2.585419178009033, -2.5263538360595703, 2.679021120071411], 'magnitude': 4.499334335327148, 'cosine_ionic_motion': -0.25772199034690857, 'motion_component_ionic': -1.1595773696899414, 'motion_component_percent_ionic': 25.772199034690857}, {'ion_id': 1320, 'distance': 7.956185340881348, 'force': [-1.769490361213684, -4.937245845794678, 0.018840014934539795], 'magnitude': 5.244792461395264, 'cosine_ionic_motion': -0.8094466328620911, 'motion_component_ionic': -4.245379447937012, 'motion_component_percent_ionic': 80.9446632862091}, {'ion_id': 2434, 'distance': 12.551528930664062, 'force': [-0.9104146361351013, -0.6412608623504639, -1.7891393899917603], 'magnitude': 2.107389450073242, 'cosine_ionic_motion': -0.3843774199485779, 'motion_component_ionic': -0.8100329041481018, 'motion_component_percent_ionic': 38.43774199485779}, {'ion_id': 2436, 'distance': 8.309216499328613, 'force': [-3.1086254119873047, -2.0093727111816406, -3.0694339275360107], 'magnitude': 4.808591842651367, 'cosine_ionic_motion': -0.39262866973876953, 'motion_component_ionic': -1.887990951538086, 'motion_component_percent_ionic': 39.26286697387695}], 'glu_contributions': [{'resid': 1073, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.5416152477264404, 'force': [15.885651588439941, 13.243943214416</t>
         </is>
       </c>
     </row>
@@ -675,7 +675,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>{5416: {'frame': 5416, 'ionic_force': [-4.081433027982712, 10.87008786201477, -3.291440822184086], 'ionic_force_magnitude': 12.068574413565539, 'motion_vector': [-2.1743736267089844, -0.24370956420898438, 0.42597198486328125], 'ionic_force_x': -4.081433027982712, 'ionic_force_y': 10.87008786201477, 'ionic_force_z': -3.291440822184086, 'radial_force': 11.611068240684359, 'axial_force': -3.291440822184086, 'glu_force': [-21.39911460876465, 19.285168170928955, -4.4350786209106445], 'glu_force_magnitude': 29.14635036833453, 'asn_force': [1.2253453731536865, -1.2446757555007935, -6.62385368347168], 'asn_force_magnitude': 6.850264713124739, 'residue_force': [-20.173769235610962, 18.04049241542816, -11.058932304382324], 'residue_force_magnitude': 29.235942185531073, 'total_force': [-24.255202263593674, 28.910580277442932, -14.35037312656641], 'total_force_magnitude': 40.37412163376426, 'motion_component_total': 17.756845945458085, 'cosine_total_motion': 0.43980761009567837, 'cosine_glu_motion': 0.6147599144253062, 'cosine_asn_motion': -0.3394036329064777, 'cosine_residue_motion': 0.5333504570945126, 'cosine_ionic_motion': 0.179295643633278, 'motion_component_glu': 17.91800785824733, 'motion_component_asn': -2.3250047300055865, 'motion_component_residue': 15.59300312824174, 'motion_component_ionic': 2.1638428172163438, 'ionic_contributions': [{'ion_id': 1306, 'distance': 13.629586219787598, 'force': [-1.1908079385757446, 1.3305332660675049, 0.07573240250349045], 'magnitude': 1.7871983051300049}, {'ion_id': 1309, 'distance': 10.115814208984375, 'force': [-1.7372729778289795, 1.9497443437576294, 1.9252551794052124], 'magnitude': 3.244414806365967}, {'ion_id': 1469, 'distance': 9.103331565856934, 'force': [1.0098694562911987, 3.874903678894043, -0.12357929348945618], 'magnitude': 4.0062432289123535}, {'ion_id': 2434, 'distance': 8.181844711303711, 'force': [-1.7631807327270508, 3.0347986221313477, -3.503937005996704], 'magnitude': 4.959474086761475}, {'ion_id': 2444, 'distance': 13.423776626586914, 'force': [-0.4000408351421356, 0.6801079511642456, -1.6649121046066284], 'magnitude': 1.8424201011657715}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.471595287322998, 'force': [17.139673233032227, -13.486157417297363, -4.074573040008545], 'magnitude': 22.1866397857666}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 4.065815448760986, 'force': [-15.189096450805664, 5.82362699508667, 2.4079465866088867], 'magnitude': 16.444496154785156}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.75699520111084, 'force': [-23.34969139099121, 26.94769859313965, -2.7684521675109863], 'magnitude': 35.76382064819336}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.361413955688477, 'force': [1.2253453731536865, -1.2446757555007935, -6.62385368347168], 'magnitude': 6.850265026092529}]}, 5417: {'frame': 5417, 'ionic_force': [-5.814258098602295, 10.77547174692154, -1.0274325460195541], 'ionic_force_magnitude': 12.287066624808661, 'motion_vector': [0.7505950927734375, 1.0793838500976562, -1.4337081909179688], 'ionic_force_x': -5.814258098602295, 'ionic_force_y': 10.77547174692154, 'ionic_force_z': -1.0274325460195541, 'radial_force': 12.244034817243321, 'axial_force': -1.0274325460195541, 'glu_force': [-19.86545753479004, 30.29177474975586, -1.7698564529418945], 'glu_force_magnitude': 36.267897821910125, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [-19.86545753479004, 30.29177474975586, -1.7698564529418945], 'residue_force_magnitude': 36.267897821910125, 'total_force': [-25.679715633392334, 41.0672464966774, -2.7972889989614487], 'total_force_magnitude': 48.515887661409096, 'motion_component_total': 14.940399584679348, 'cosine_total_motion': 0.30794859797161583, 'cosine_glu_motion': 0.28806522520928557, 'cosine_asn_motion': None, 'cosine_residue_motion': 0.28806522520928557, 'cosine_ionic_motion': 0.3656592389327437, 'motion_component_glu': 10.447520153935898, 'motion_component_asn': None, 'motion_component_residue': 10.447520153935898, 'motion_component_ionic': 4.492879430743451, 'ionic_contributions': [{'ion_id': 1306, 'distance': 13.446145057678223, 'force': [-1.2127642631530762, 1.3744667768478394, 0.10965488851070404], 'magnitude': 1.836295247077942}, {'ion_id': 1309, 'distance': 8.976375579833984, 'force': [-1.6386932134628296, 1.689590573310852, 3.3819234371185303], 'magnitude': 4.120368480682373}, {'ion_id': 1469, 'distance': 8.527118682861328, 'force': [0.2765955328941345, 4.555323600769043, -0.1436668336391449], 'magnitude': 4.56597375869751}, {'ion_id': 2434, 'distance': 8.563232421875, 'force': [-2.509505271911621, 2.4902234077453613, -2.8283956050872803], 'magnitude': 4.527543544769287}, {'ion_id': 2444, 'distance': 13.448948860168457, 'force': [-0.7298908829689026, 0.6658673882484436, -1.5469484329223633], 'magnitude': 1.8355298042297363}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 2.9978244304656982, 'force': [13.858800888061523, -25.350576400756836, -7.109826564788818], 'magnitude': 29.753448486328125}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 2.9384243488311768, 'force': [-23.838666915893555, 17.966581344604492, 10.007415771484375], 'magnitude': 31.483779907226562}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.632389545440674, 'force': [-9.885591506958008, 37.6757698059082, -4.667445659637451], 'magnitude': 39.22975540161133}], 'asn_contributions': []}, 5418: {'frame': 5418, 'ionic_force': [-3.0948960185050964, 8.432614922523499, -0.9114571809768677], 'ionic_force_magnitude': 9.028739114055682, 'motion_vector': [0.6279106140136719, 0.4439239501953125, -0.27136993408203125], 'ionic_force_x': -3.0948960185050964, 'ionic_force_y': 8.432614922523499, 'ionic_force_z': -0.9114571809768677, 'radial_force': 8.982615198088176, 'axial_force': -0.9114571809768677, 'glu_force': [-11.208107233047485, 22.827584266662598, 28.53571891784668], 'glu_force_magnitude': 38.223128147202004, 'asn_force': [-3.8814868927001953, 3.422593593597412, 6.517432689666748], 'asn_force_magnitude': 8.322080044644741, 'residue_force': [-15.08959412574768, 26.25017786026001, 35.05315160751343], 'residue_force_magnitude': 46.319446522971376, 'total_force': [-18.184490144252777, 34.68279278278351, 34.14169442653656], 'total_force_magnitude': 51.95408641613212, 'motion_component_total': -6.483106412225347, 'cosine_total_motion': -0.12478530293648461, 'cosine_glu_motion': -0.14911051997366015, 'cosine_asn_motion': -0.39586634066962845, 'cosine_residue_motion': -0.1941711864502096, 'cosine_ionic_motion': 0.2780892706212218, 'motion_component_glu': -5.699470513049135, 'motion_component_asn': -3.294431374033252, 'motion_component_residue': -8.993901887082387, 'motion_component_ionic': 2.5107954748570407, 'ionic_contributions': [{'ion_id': 1306, 'distance': 13.538542747497559, 'force': [-1.2676705121994019, 1.2841308116912842, -0.15775233507156372], 'magnitude': 1.8113162517547607}, {'ion_id': 1309, 'distance': 10.023154258728027, 'force': [-1.2601678371429443, 2.125608205795288, 2.1942358016967773], 'magnitude': 3.3046791553497314}, {'ion_id': 1469, 'distance': 9.518566131591797, 'force': [0.4336826205253601, 3.54756498336792, -0.8087297081947327], 'magnitude': 3.6643335819244385}, {'ion_id': 2434, 'distance': 10.919032096862793, 'force': [-1.0007402896881104, 1.4753109216690063, -2.1392109394073486], 'magnitude': 2.784644842147827}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.1398327350616455, 'force': [7.858447074890137, -17.051971435546875, -19.573671340942383], 'magnitude': 27.122934341430664}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 2.75374436378479, 'force': [-22.12091636657715, 14.096833229064941, 24.434518814086914], 'magnitude': 35.84830856323242}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.7814955711364746, 'force': [3.0543620586395264, 25.78272247314453, 23.67487144470215], 'magnitude': 35.13655471801758}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.295187950134277, 'force': [-2.860029458999634, 3.017911195755005, 7.347530364990234], 'magnitude': 8.442378997802734}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.961963176727295, 'force': [6.7524518966674805, -4.665207862854004, -9.286492347717285], 'magnitude': 12.393494606018066}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.774838447570801, 'force': [-2.589862108230591, 1.6945786476135254, 2.805478572845459], 'magnitude': 4.177282810211182}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.077581405639648, 'force': [-5.184047222137451, 3.3753116130828857, 5.65091609954834], 'magnitude': 8.3785400390625}]}, 5419: {'frame': 5419, 'ionic_force': [-3.6241090893745422, 8.350408673286438, -1.4899036781862378], 'ionic_force_magnitude': 9.224061181109839, 'motion_vector': [-0.07321548461914062, -1.4095268249511719, 1.3923492431640625], 'ionic_force_x': -3.6241090893745422, 'ionic_force_y': 8.350408673286438, 'ionic_force_z': -1.4899036781862378, 'radial_force': 9.102938630057029, 'axial_force': -1.4899036781862378, 'glu_force': [-29.96388816833496, 8.629873633384705, 5.891890525817871], 'glu_force_magnitude': 31.733636524371025, 'asn_force': [-1.8064911365509033, 2.3654412031173706, 7.011445045471191], 'asn_force_magnitude': 7.617025924696912, 'residue_force': [-31.770379304885864, 10.995314836502075, 12.903335571289062], 'residue_force_magnitude': 36.01041541547968, 'total_force': [-35.39448839426041, 19.345723509788513, 11.413431893102825], 'total_force_magnitude': 41.920081755491786, 'motion_component_total': -4.431221780922817, 'cosine_total_motion': -0.10570642029681394, 'cosine_glu_motion': -0.028079654964546685, 'cosine_asn_motion': 0.43442266831689863, 'cosine_residue_motion': 0.0671455503796204, 'cosine_ionic_motion': -0.7425320375606914, 'motion_component_glu': -0.8910695643746749, 'motion_component_asn': 3.309008726845825, 'motion_component_residue': 2.41793916247115, 'motion_component_ionic': -6.849160943393967, 'ionic_contributions': [{'ion_id': 1306, 'distance': 13.959966659545898, 'force': [-1.068015694618225, 1.3272424936294556, 0.00673897098749876], 'magnitude': 1.7036066055297852}, {'ion_id': 1309, 'distance': 9.966863632202148, 'force': [-2.2032456398010254, 2.115774631500244, 1.356068730354309], 'magnitude': 3.3421125411987305}, {'ion_id': 1469, 'distance': 10.095869064331055, 'force': [0.5705264210700989, 3.1289117336273193, -0.7028989195823669], 'magnitude': 3.257246732711792}, {'ion_id': 2434, 'distance': 10.628561973571777, 'force': [-0.9233741760253906, 1.778479814529419, -2.1498124599456787], 'magnitude': 2.9389290809631348}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.634676456451416, 'force': [16.686546325683594, -6.239892482757568, -9.607030868530273], 'magnitude': 20.240358352661133}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 4.568996906280518, 'force': [-11.584787368774414, 1.6108101606369019, 5.724312782287598], 'magnitude': 13.021896362304688}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.6489083766937256, 'force': [-35.06564712524414, 13.258955955505371, 9.774608612060547], 'magnitude': 38.742000579833984}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.565687656402588, 'force': [-0.8570419549942017, 2.804591178894043, 7.056579113006592], 'magnitude': 7.641698837280273}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.063930034637451, 'force': [3.914184331893921, -3.9346847534179688, -10.52584457397461], 'magnitude': 11.89941120147705}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.882103443145752, 'force': [-1.7019652128219604, 1.421000361442566, 3.360851287841797], 'magnitude': 4.02631950378418}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.156917572021484, 'force': [-3.161668300628662, 2.0745344161987305, 7.119859218597412], 'magnitude': 8.061776161193848}]}, 5420: {'frame': 5420, 'ionic_force': [-4.995375692844391, 9.29425859451294, -4.6483332216739655], 'ionic_force_magnitude': 11.530135423057965, 'motion_vector': [1.37384033203125, 0.6198310852050781, 1.271148681640625], 'ionic_force_x': -4.995375692844391, 'ionic_force_y': 9.29425859451294, 'ionic_force_z': -4.6483332216739655, 'radial_force': 10.551635945877692, 'axial_force': -4.6483332216739655, 'glu_force': [-14.163765907287598, 16.9093017578125, -2.9894802570343018], 'glu_force_magnitude': 22.25923949330707, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [-14.163765907287598, 16.9093017578125, -2.9894802570343018], 'residue_force_magnitude': 22.25923949330707, 'total_force': [-19.15914160013199, 26.20356035232544, -7.637813478708267], 'total_force_magnitude': 33.347195935001906, 'motion_component_total': -10.036521124171347, 'cosine_total_motion': -0.3009704667143185, 'cosine_glu_motion': -0.2911504486400682, 'cosine_asn_motion': None, 'cosine_residue_motion': -0.2911504486400682, 'cosine_ionic_motion': -0.3083861055263508, 'motion_component_glu': -6.480787564863078, 'motion_component_asn': None, 'motion_component_residue': -6.480787564863078, 'motion_component_ionic': -3.555733559308269, 'ionic_contributions': [{'ion_id': 1306, 'distance': 14.215216636657715, 'force': [-0.9783754944801331, 1.3178855180740356, 0.07299147546291351], 'magnitude': 1.6429754495620728}, {'ion_id': 1309, 'distance': 11.428321838378906, 'force': [-2.296131134033203, 1.0717114210128784, 0.202259823679924], 'magnitude': 2.5419859886169434}, {'ion_id': 1469, 'distance': 8.802873611450195, 'force': [0.5067126154899597, 4.24498176574707, -0.2817506194114685], 'magnitude': 4.2843918800354}, {'ion_id': 2434, 'distance': 9.167643547058105, 'force': [-1.693018913269043, 2.0171566009521484, -2.944333791732788], 'magnitude': 3.9502322673797607}, {'ion_id': 2444, 'distance': 13.246319770812988, 'force': [-0.5345627665519714, 0.6425232887268066, -1.6975001096725464], 'magnitude': 1.8921153545379639}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.7301101684570312, 'force': [11.731582641601562, -14.838068962097168, -3.395612955093384], 'magnitude': 19.21792221069336}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 3.9945478439331055, 'force': [-13.951499938964844, 9.3285493850708, 2.92856764793396], 'magnitude': 17.036510467529297}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 3.263315439224243, 'force': [-11.943848609924316, 22.418821334838867, -2.522434949874878], 'magnitude': 25.526884078979492}], 'asn_contributions': []}, 5421: {'frame': 5421, 'ionic_force': [-5.303912997245789, 10.99374771118164, -2.734027996659279], 'ionic_force_magnitude': 12.508752571938622, 'motion_vector': [-0.43817138671875, 0.11849594116210938, -1.432342529296875], 'ionic_force_x': -5.303912997245789, 'ionic_force_y': 10.99374771118164, 'ionic_force_z': -2.734027996659279, 'radial_force': 12.206309098964534, 'axial_force': -2.734027996659279, 'glu_force': [-24.575862884521484, 9.054282903671265, -13.014705747365952], 'glu_force_magnitude': 29.246121813140196, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [-24.575862884521484, 9.054282903671265, -13.014705747365952], 'residue_force_magnitude': 29.246121813140196, 'total_force': [-29.879775881767273, 20.048030614852905, -15.74873374402523], 'total_force_magnitude': 39.27782011286929, 'motion_component_total': 25.30750121074543, 'cosine_total_motion': 0.6443204113166525, 'cosine_glu_motion': 0.6936811414343523, 'cosine_asn_motion': None, 'cosine_residue_motion': 0.6936811414343523, 'cosine_ionic_motion': 0.4013204370306142, 'motion_component_glu': 20.2874831618672, 'motion_component_asn': None, 'motion_component_residue': 20.2874831618672, 'motion_component_ionic': 5.020018048878227, 'ionic_contributions': [{'ion_id': 1306, 'distance': 13.276257514953613, 'force': [-0.9376237988471985, 1.6168675422668457, 0.2334917038679123], 'magnitude': 1.883591651916504}, {'ion_id': 1309, 'distance': 8.914875984191895, 'force': [-3.586841344833374, 1.4117411375045776, 1.6100742816925049], 'magnitude': 4.177413463592529}, {'ion_id': 1469, 'distance': 9.480932235717773, 'force': [1.202595829963684, 3.48968505859375, 0.13294559717178345], 'magnitude': 3.6934826374053955}, {'ion_id': 2434, 'distance': 8.310657501220703, 'force': [-1.507516622543335, 3.459397077560425, -2.9776651859283447], 'magnitude': 4.806924819946289}, {'ion_id': 2444, 'distance': 12.682544708251953, 'force': [-0.4745270609855652, 1.0160568952560425, -1.7328743934631348], 'magnitude': 2.0640740394592285}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.2050793170928955, 'force': [23.994768142700195, -10.068934440612793, 0.6498544812202454], 'magnitude': 26.029878616333008}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 3.727823257446289, 'force': [-19.498056411743164, 1.5375049114227295, 0.3459826409816742], 'magnitude': 19.561641693115234}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.719648838043213, 'force': [-29.072574615478516, 17.585712432861328, -14.010542869567871], 'magnitude': 36.752784729003906}], 'asn_contributions': []}, 5422: {'frame': 5422, 'ionic_force': [-4.211169719696045, 10.116018772125244, -4.300447233021259], 'ionic_force_magnitude': 11.771220523381396, 'motion_vector': [0.1480560302734375, -0.8996047973632812, 0.5749053955078125], 'ionic_force_x': -4.211169719696045, 'ionic_force_y': 10.116018772125244, 'ionic_force_z': -4.300447233021259, 'radial_force': 10.957544716133956, 'axial_force': -4.300447233021259, 'glu_force': [-25.784714698791504, 17.801549434661865, -1.6186452209949493], 'glu_force_magnitude': 31.374618511214358, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [-25.784714698791504, 17.801549434661865, -1.6186452209949493], 'residue_force_magnitude': 31.374618511214358, 'total_force': [-29.99588441848755, 27.91756820678711, -5.919092454016209], 'total_force_magnitude': 41.40264909528213, 'motion_component_total': -30.57871196348129, 'cosine_total_motion': -0.7385689715918627, 'cosine_glu_motion': -0.6139734756369628, 'cosine_asn_motion': None, 'cosine_residue_motion': -0.6139734756369628, 'cosine_ionic_motion': -0.9612876053839085, 'motion_component_glu': -19.26318357411407, 'motion_component_asn': None, 'motion_component_residue': -19.26318357411407, 'motion_component_ionic': -11.31552838936722, 'ionic_contributions': [{'ion_id': 1306, 'distance': 13.448433876037598, 'force': [-0.8739737868309021, 1.613553762435913, -0.04794659465551376], 'magnitude': 1.8356701135635376}, {'ion_id': 1309, 'distance': 10.17707633972168, 'force': [-2.566864252090454, 1.8449293375015259, 0.5315044522285461], 'magnitude': 3.205472469329834}, {'ion_id': 1469, 'distance': 10.020413398742676, 'force': [1.0937838554382324, 3.111398458480835, -0.23599140346050262], 'magnitude': 3.3064868450164795}, {'ion_id': 2434, 'distance': 8.782258033752441, 'force': [-1.3929810523986816, 2.763676643371582, -2.991767168045044], 'magnitude': 4.304529666900635}, {'ion_id': 2444, 'distance': 13.564197540283203, 'force': [-0.4711344838142395, 0.7824605703353882, -1.5562465190887451], 'magnitude': 1.8044710159301758}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.6099252700805664, 'force': [16.747026443481445, -10.924179077148438, -4.606855392456055], 'magnitude': 20.518861770629883}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 4.096811771392822, 'force': [-15.286845207214355, 4.196801662445068, 3.321016788482666], 'magnitude': 16.19660186767578}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.7230336666107178, 'force': [-27.244895935058594, 24.528926849365234, -0.33280661702156067], 'magnitude': 36.661468505859375}], 'asn_contributions': []}, 5423: {'frame': 5423, 'ionic_force': [-8.426977157592773, 12.587924428284168, -3.720699816942215], 'ionic_force_magnitude': 15.598506100091043, 'motion_vector': [-0.2519950866699219, 0.5466041564941406, 0.0637054443359375], 'ionic_force_x': -8.426977157592773, 'ionic_force_y': 12.587924428284168, 'ionic_force_z': -3.720699816942215, 'radial_force': 15.148260145204256, 'axial_force': -3.720699816942215, 'glu_force': [-11.985785484313965, 10.626004219055176, -3.2562605142593384], 'glu_force_magnitude': 16.345465789511604, 'asn_force': [0.01022881269454956, 0.8976959884166718, 6.308809280395508], 'asn_force_magnitude': 6.372365122357084, 'residue_force': [-11.975556671619415, 11.523700207471848, 3.0525487661361694], 'residue_force_magnitude': 16.897564263422538, 'total_force': [-20.40253382921219, 24.111624635756016, -0.6681510508060455], 'total_force_magnitude': 31.592408187006534, 'motion_component_total': 30.1992184117698, 'cosine_total_motion': 0.9559011213393435, 'cosine_glu_motion': 0.8714196926836075, 'cosine_asn_motion': 0.23075734057105896, 'cosine_residue_motion': 0.9299701755160927, 'cosine_ionic_motion': 0.9286137733302382, 'motion_component_glu': 14.243760775066622, 'motion_component_asn': 1.4704700287828913, 'motion_component_residue': 15.714230803849514, 'motion_component_ionic': 14.484987607920282, 'ionic_contributions': [{'ion_id': 1306, 'distance': 12.553146362304688, 'force': [-1.232452630996704, 1.7019360065460205, 0.152567058801651], 'magnitude': 2.106846570968628}, {'ion_id': 1309, 'distance': 6.604099273681641, 'force': [-7.53367280960083, -0.03545748442411423, 1.090088963508606], 'magnitude': 7.612212181091309}, {'ion_id': 1469, 'distance': 6.873001575469971, 'force': [3.078547954559326, 6.243687152862549, 0.9668325781822205], 'magnitude': 7.0282182693481445}, {'ion_id': 2434, 'distance': 7.4333624839782715, 'force': [-2.2350199222564697, 3.7992143630981445, -4.083253383636475], 'magnitude': 6.008519172668457}, {'ion_id': 2444, 'distance': 12.554132461547852, 'force': [-0.5043797492980957, 0.8785443902015686, -1.8469350337982178], 'magnitude': 2.106515645980835}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 4.465732097625732, 'force': [9.682783126831055, -9.209187507629395, -1.0997029542922974], 'magnitude': 13.408011436462402}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 5.089153289794922, 'force': [-9.014503479003906, 5.310901641845703, 0.8364148139953613], 'magnitude': 10.496025085449219}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 3.7342305183410645, 'force': [-12.654065132141113, 14.524290084838867, -2.9929723739624023], 'magnitude': 19.494569778442383}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.82766056060791, 'force': [-0.39081647992134094, 0.1555226743221283, 6.957398414611816], 'magnitude': 6.970101833343506}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.047962665557861, 'force': [1.2929837703704834, -2.605830669403076, -11.616104125976562], 'magnitude': 11.974807739257812}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.433774471282959, 'force': [-1.253646731376648, 1.3427573442459106, 4.345821857452393], 'magnitude': 4.718134880065918}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.484143257141113, 'force': [0.36170825362205505, 2.005246639251709, 6.621693134307861], 'magnitude': 6.928107261657715}]}, 5424: {'frame': 5424, 'ionic_force': [-10.658977925777435, 9.611903131008148, -3.6862301863729954], 'ionic_force_magnitude': 14.818595925694929, 'motion_vector': [-1.8115425109863281, -1.1403274536132812, 0.10491180419921875], 'ionic_force_x': -10.658977925777435, 'ionic_force_y': 9.611903131008148, 'ionic_force_z': -3.6862301863729954, 'radial_force': 14.352786914815354, 'axial_force': -3.6862301863729954, 'glu_force': [-20.872244834899902, 17.029710292816162, -2.6130096912384033], 'glu_force_magnitude': 27.064542426425025, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [-20.872244834899902, 17.029710292816162, -2.6130096912384033], 'residue_force_magnitude': 27.064542426425025, 'total_force': [-31.531222760677338, 26.64161342382431, -6.299239877611399], 'total_force_magnitude': 41.757322682897694, 'motion_component_total': 12.16866333605682, 'cosine_total_motion': 0.29141387795536683, 'cosine_glu_motion': 0.3123521756128088, 'cosine_asn_motion': None, 'cosine_residue_motion': 0.3123521756128088, 'cosine_ionic_motion': 0.2506981529036854, 'motion_component_glu': 8.453668708859023, 'motion_component_asn': None, 'motion_component_residue': 8.453668708859023, 'motion_component_ionic': 3.714994627197797, 'ionic_contributions': [{'ion_id': 1306, 'distance': 13.732420921325684, 'force': [-0.8292531967163086, 1.547203540802002, 0.13406047224998474], 'magnitude': 1.7605317831039429}, {'ion_id': 1309, 'distance': 6.30421781539917, 'force': [-8.29712200164795, 0.1777876615524292, 0.9536499381065369], 'magnitude': 8.353639602661133}, {'ion_id': 1469, 'distance': 9.281245231628418, 'force': [0.7835202217102051, 3.773498058319092, -0.03277162089943886], 'magnitude': 3.854123115539551}, {'ion_id': 2434, 'distance': 8.33357048034668, 'force': [-1.8014920949935913, 3.1987240314483643, -3.0620651245117188], 'magnitude': 4.7805280685424805}, {'ion_id': 2444, 'distance': 12.948599815368652, 'force': [-0.5146308541297913, 0.914689838886261, -1.6791038513183594], 'magnitude': 1.9801243543624878}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.613959550857544, 'force': [15.623372077941895, -12.766215324401855, -3.47575044631958], 'magnitude': 20.47307586669922}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 3.7978475093841553, 'force': [-17.549972534179688, 6.209715366363525, 2.9402565956115723], 'magnitude': 18.846940994262695}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.994074583053589, 'force': [-18.94564437866211, 23.586210250854492, -2.0775158405303955], 'magnitude': 30.324295043945312}], 'asn_contributions': []}, 5425: {'frame': 5425, 'ionic_force': [-8.817112369462848, 4.628080368041992, -5.053674541413784], 'ionic_force_magnitude': 11.16692548552753, 'motion_vector': [0.7701644897460938, 1.122161865234375, -0.6427230834960938], 'ionic_force_x': -8.817112369462848, 'ionic_force_y': 4.628080368041992, 'ionic_force_z': -5.053674541413784, 'radial_force': 9.957941475465221, 'axial_force': -5.053674541413784, 'glu_force': [-11.757940769195557, 38.20547676086426, -4.833729267120361], 'glu_force_magnitude': 40.265029048600795, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [-11.757940769195557, 38.20547676086426, -4.833729267120361], 'residue_force_magnitude': 40.265029048600795, 'total_force': [-20.575053138658404, 42.83355712890625, -9.887403808534145], 'total_force_magnitude': 48.536658126069085, 'motion_component_total': 25.628492624868933, 'cosine_total_motion': 0.5280234283600964, 'cosine_glu_motion': 0.6092541254283386, 'cosine_asn_motion': None, 'cosine_residue_motion': 0.6092541254283386, 'cosine_ionic_motion': 0.09822377412104595, 'motion_component_glu': 24.531635058351924, 'motion_component_asn': None, 'motion_component_residue': 24.531635058351924, 'motion_component_ionic': 1.0968575665170075, 'ionic_contributions': [{'ion_id': 1306, 'distance': 12.973211288452148, 'force': [-1.4571207761764526, 1.3220487833023071, 0.14216242730617523], 'magnitude': 1.972618579864502}, {'ion_id': 1309, 'distance': 8.255983352661133, 'force': [-4.172080993652344, -2.511462926864624, -0.10490787774324417], 'magnitude': 4.87080192565918}, {'ion_id': 1469, 'distance': 10.572911262512207, 'force': [0.024452881887555122, 2.9648444652557373, -0.17231887578964233], 'magnitude': 2.9699485301971436}, {'ion_id': 2434, 'distance': 8.574973106384277, 'force': [-2.4676637649536133, 2.1257126331329346, -3.127074718475342], 'magnitude': 4.515153884887695}, {'ion_id': 2444, 'distance': 12.658683776855469, 'force': [-0.7446997165679932, 0.7269374132156372, -1.791535496711731], 'magnitude': 2.0718626976013184}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 2.86383318901062, 'force': [6.259057521820068, -31.7213134765625, -4.185907363891602], 'magnitude': 32.60274887084961}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 2.6228954792022705, 'force': [-23.76770782470703, 30.987585067749023, 6.020213603973389], 'magnitude': 39.51426696777344}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.609455108642578, 'force': [5.750709533691406, 38.939205169677734, -6.668035507202148], 'magnitude': 39.92236328125}], 'asn_contributions': []}, 5426: {'frame': 5426, 'ionic_force': [-6.718421280384064, 6.112494587898254, -4.578008808195591], 'ionic_force_magnitude': 10.17142759084089, 'motion_vector': [0.9683570861816406, -1.1876640319824219, -1.7886962890625], 'ionic_force_x': -6.718421280384064, 'ionic_force_y': 6.112494587898254, 'ionic_force_z': -4.578008808195591, 'radial_force': 9.082938653750938, 'axial_force': -4.578008808195591, 'glu_force': [-20.334662437438965, 20.99546241760254, -0.7494313716888428], 'glu_force_magnitude': 29.238152916256922, 'asn_force': [0.5758064985275269, -1.1249361038208008, 0.5951805114746094], 'asn_force_magnitude': 1.396880167611106, 'residue_force': [-19.758855938911438, 19.87052631378174, -0.1542508602142334], 'residue_force_magnitude': 28.02274071766045, 'total_force': [-26.4772772192955, 25.983020901679993, -4.732259668409824], 'total_force_magnitude': 37.397297572068254, 'motion_component_total': -20.39352376569765, 'cosine_total_motion': -0.545320787588925, 'cosine_glu_motion': -0.6285558204921825, 'cosine_asn_motion': 0.2519750443968476, 'cosine_residue_motion': -0.6432572900459615, 'cosine_ionic_motion': -0.23277868232840937, 'motion_component_glu': -18.377811195953768, 'motion_component_asn': 0.35197894225088433, 'motion_component_residue': -18.025832253702884, 'motion_component_ionic': -2.36769151199477, 'ionic_contributions': [{'ion_id': 1306, 'distance': 14.053243637084961, 'force': [-1.0048154592514038, 1.347147822380066, 0.03903442621231079], 'magnitude': 1.681066632270813}, {'ion_id': 1309, 'distance': 9.073514938354492, 'force': [-3.82336688041687, -1.281545877456665, 0.038811035454273224], 'magnitude': 4.032617092132568}, {'ion_id': 1469, 'distance': 10.299788475036621, 'force': [0.3030494451522827, 3.1069347858428955, -0.22176901996135712], 'magnitude': 3.129547119140625}, {'ion_id': 2434, 'distance': 9.169970512390137, 'force': [-1.6431152820587158, 2.2570924758911133, -2.791811227798462], 'magnitude': 3.948227882385254}, {'ion_id': 2444, 'distance': 13.353959083557129, 'force': [-0.5501731038093567, 0.6828653812408447, -1.642274022102356], 'magnitude': 1.8617355823516846}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.304647922515869, 'force': [15.96073055267334, -17.349992752075195, -6.614067077636719], 'magnitude': 24.484956741333008}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 3.4781577587127686, 'force': [-19.24537467956543, 9.29733657836914, 6.936078071594238], 'magnitude': 22.470739364624023}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.8401899337768555, 'force': [-17.050018310546875, 29.048118591308594, -1.0714423656463623], 'magnitude': 33.69932174682617}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.826351165771484, 'force': [-1.3223525285720825, 2.2006185054779053, 6.483415126800537], 'magnitude': 6.973235130310059}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.294771671295166, 'force': [1.8981590270996094, -3.325554609298706, -5.888234615325928], 'magnitude': 7.02379035949707}]}, 5427: {'frame': 5427, 'ionic_force': [-9.</t>
+          <t>{5416: {'frame': 5416, 'motion_vector': [-2.1743736267089844, -0.24370956420898438, 0.42597198486328125], 'ionic_force': [-4.081433027982712, 10.87008786201477, -3.291440822184086], 'ionic_force_magnitude': 12.068574413565539, 'radial_force': 11.611068240684359, 'axial_force': -3.291440822184086, 'glu_force': [-21.39911460876465, 19.285168170928955, -4.4350786209106445], 'glu_force_magnitude': 29.14635036833453, 'asn_force': [1.2253453731536865, -1.2446757555007935, -6.62385368347168], 'asn_force_magnitude': 6.850264713124739, 'residue_force': [-20.173769235610962, 18.04049241542816, -11.058932304382324], 'residue_force_magnitude': 29.235942185531073, 'total_force': [-24.255202263593674, 28.910580277442932, -14.35037312656641], 'total_force_magnitude': 40.37412163376426, 'cosine_total_motion': 0.43980761009567837, 'cosine_glu_motion': 0.6147599144253062, 'cosine_asn_motion': -0.3394036329064777, 'cosine_residue_motion': 0.5333504570945126, 'cosine_ionic_motion': 0.179295643633278, 'motion_component_total': 17.756845945458085, 'motion_component_glu': 17.91800785824733, 'motion_component_asn': -2.3250047300055865, 'motion_component_residue': 15.59300312824174, 'motion_component_ionic': 2.1638428172163438, 'motion_component_percent_total': 43.980761009567836, 'motion_component_percent_glu': 61.47599144253062, 'motion_component_percent_asn': 33.94036329064777, 'motion_component_percent_residue': 53.33504570945126, 'motion_component_percent_ionic': 17.9295643633278, 'ionic_contributions': [{'ion_id': 1306, 'distance': 13.629586219787598, 'force': [-1.1908079385757446, 1.3305332660675049, 0.07573240250349045], 'magnitude': 1.7871983051300049, 'cosine_ionic_motion': 0.5766515135765076, 'motion_component_ionic': 1.0305906534194946, 'motion_component_percent_ionic': 57.66515135765076}, {'ion_id': 1309, 'distance': 10.115814208984375, 'force': [-1.7372729778289795, 1.9497443437576294, 1.9252551794052124], 'magnitude': 3.244414806365967, 'cosine_ionic_motion': 0.5700222253799438, 'motion_component_ionic': 1.8493884801864624, 'motion_component_percent_ionic': 57.002222537994385}, {'ion_id': 1469, 'distance': 9.103331565856934, 'force': [1.0098694562911987, 3.874903678894043, -0.12357929348945618], 'magnitude': 4.0062432289123535, 'cosine_ionic_motion': -0.3575316071510315, 'motion_component_ionic': -1.4323586225509644, 'motion_component_percent_ionic': 35.75316071510315}, {'ion_id': 2434, 'distance': 8.181844711303711, 'force': [-1.7631807327270508, 3.0347986221313477, -3.503937005996704], 'magnitude': 4.959474086761475, 'cosine_ionic_motion': 0.14487779140472412, 'motion_component_ionic': 0.7185176610946655, 'motion_component_percent_ionic': 14.487779140472412}, {'ion_id': 2444, 'distance': 13.423776626586914, 'force': [-0.4000408351421356, 0.6801079511642456, -1.6649121046066284], 'magnitude': 1.8424201011657715, 'cosine_ionic_motion': -0.0012458193814381957, 'motion_component_ionic': -0.0022953227162361145, 'motion_component_percent_ionic': 0.12458193814381957}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.471595287322998, 'force': [17.139673233032227, -13.486157417297363, -4.074573040008545], 'magnitude': 22.1866397857666, 'cosine_with_motion': -0.7222042083740234, 'motion_component': -16.023284912109375, 'motion_component_percent': 72.22042083740234}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 4.065815448760986, 'force': [-15.189096450805664, 5.82362699508667, 2.4079465866088867], 'magnitude': 16.444496154785156, 'cosine_with_motion': 0.8902578353881836, 'motion_component': 14.63984203338623, 'motion_component_percent': 89.02578353881836}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.75699520111084, 'force': [-23.34969139099121, 26.94769859313965, -2.7684521675109863], 'magnitude': 35.76382064819336, 'cosine_with_motion': 0.5396920442581177, 'motion_component': 19.301448822021484, 'motion_component_percent': 53.96920442581177}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.361413955688477, 'force': [1.2253453731536865, -1.2446757555007935, -6.62385368347168], 'magnitude': 6.850265026092529, 'cosine_with_motion': -0.3394036293029785, 'motion_component': -2.325004816055298, 'motion_component_percent': 33.94036293029785}]}, 5417: {'frame': 5417, 'motion_vector': [0.7505950927734375, 1.0793838500976562, -1.4337081909179688], 'ionic_force': [-5.814258098602295, 10.77547174692154, -1.0274325460195541], 'ionic_force_magnitude': 12.287066624808661, 'radial_force': 12.244034817243321, 'axial_force': -1.0274325460195541, 'glu_force': [-19.86545753479004, 30.29177474975586, -1.7698564529418945], 'glu_force_magnitude': 36.267897821910125, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [-19.86545753479004, 30.29177474975586, -1.7698564529418945], 'residue_force_magnitude': 36.267897821910125, 'total_force': [-25.679715633392334, 41.0672464966774, -2.7972889989614487], 'total_force_magnitude': 48.515887661409096, 'cosine_total_motion': 0.30794859797161583, 'cosine_glu_motion': 0.28806522520928557, 'cosine_asn_motion': None, 'cosine_residue_motion': 0.28806522520928557, 'cosine_ionic_motion': 0.3656592389327437, 'motion_component_total': 14.940399584679348, 'motion_component_glu': 10.447520153935898, 'motion_component_asn': None, 'motion_component_residue': 10.447520153935898, 'motion_component_ionic': 4.492879430743451, 'motion_component_percent_total': 30.794859797161582, 'motion_component_percent_glu': 28.806522520928556, 'motion_component_percent_asn': None, 'motion_component_percent_residue': 28.806522520928556, 'motion_component_percent_ionic': 36.56592389327437, 'ionic_contributions': [{'ion_id': 1306, 'distance': 13.446145057678223, 'force': [-1.2127642631530762, 1.3744667768478394, 0.10965488851070404], 'magnitude': 1.836295247077942, 'cosine_ionic_motion': 0.11647925525903702, 'motion_component_ionic': 0.21389029920101166, 'motion_component_percent_ionic': 11.647925525903702}, {'ion_id': 1309, 'distance': 8.976375579833984, 'force': [-1.6386932134628296, 1.689590573310852, 3.3819234371185303], 'magnitude': 4.120368480682373, 'cosine_ionic_motion': -0.5308672189712524, 'motion_component_ionic': -2.187368631362915, 'motion_component_percent_ionic': 53.086721897125244}, {'ion_id': 1469, 'distance': 8.527118682861328, 'force': [0.2765955328941345, 4.555323600769043, -0.1436668336391449], 'magnitude': 4.56597375869751, 'cosine_ionic_motion': 0.6001537442207336, 'motion_component_ionic': 2.740286111831665, 'motion_component_percent_ionic': 60.015374422073364}, {'ion_id': 2434, 'distance': 8.563232421875, 'force': [-2.509505271911621, 2.4902234077453613, -2.8283956050872803], 'magnitude': 4.527543544769287, 'cosine_ionic_motion': 0.5517515540122986, 'motion_component_ionic': 2.498079299926758, 'motion_component_percent_ionic': 55.17515540122986}, {'ion_id': 2444, 'distance': 13.448948860168457, 'force': [-0.7298908829689026, 0.6658673882484436, -1.5469484329223633], 'magnitude': 1.8355298042297363, 'cosine_ionic_motion': 0.6690123677253723, 'motion_component_ionic': 1.2279921770095825, 'motion_component_percent_ionic': 66.90123677253723}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 2.9978244304656982, 'force': [13.858800888061523, -25.350576400756836, -7.109826564788818], 'magnitude': 29.753448486328125, 'cosine_with_motion': -0.11692290008068085, 'motion_component': -3.4788594245910645, 'motion_component_percent': 11.692290008068085}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 2.9384243488311768, 'force': [-23.838666915893555, 17.966581344604492, 10.007415771484375], 'magnitude': 31.483779907226562, 'cosine_with_motion': -0.20978590846061707, 'motion_component': -6.60485315322876, 'motion_component_percent': 20.978590846061707}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.632389545440674, 'force': [-9.885591506958008, 37.6757698059082, -4.667445659637451], 'magnitude': 39.22975540161133, 'cosine_with_motion': 0.5233587026596069, 'motion_component': 20.531232833862305, 'motion_component_percent': 52.33587026596069}], 'asn_contributions': []}, 5418: {'frame': 5418, 'motion_vector': [0.6279106140136719, 0.4439239501953125, -0.27136993408203125], 'ionic_force': [-3.0948960185050964, 8.432614922523499, -0.9114571809768677], 'ionic_force_magnitude': 9.028739114055682, 'radial_force': 8.982615198088176, 'axial_force': -0.9114571809768677, 'glu_force': [-11.208107233047485, 22.827584266662598, 28.53571891784668], 'glu_force_magnitude': 38.223128147202004, 'asn_force': [-3.8814868927001953, 3.422593593597412, 6.517432689666748], 'asn_force_magnitude': 8.322080044644741, 'residue_force': [-15.08959412574768, 26.25017786026001, 35.05315160751343], 'residue_force_magnitude': 46.319446522971376, 'total_force': [-18.184490144252777, 34.68279278278351, 34.14169442653656], 'total_force_magnitude': 51.95408641613212, 'cosine_total_motion': -0.12478530293648461, 'cosine_glu_motion': -0.14911051997366015, 'cosine_asn_motion': -0.39586634066962845, 'cosine_residue_motion': -0.1941711864502096, 'cosine_ionic_motion': 0.2780892706212218, 'motion_component_total': -6.483106412225347, 'motion_component_glu': -5.699470513049135, 'motion_component_asn': -3.294431374033252, 'motion_component_residue': -8.993901887082387, 'motion_component_ionic': 2.5107954748570407, 'motion_component_percent_total': 12.478530293648461, 'motion_component_percent_glu': 14.911051997366014, 'motion_component_percent_asn': 39.586634066962844, 'motion_component_percent_residue': 19.41711864502096, 'motion_component_percent_ionic': 27.80892706212218, 'ionic_contributions': [{'ion_id': 1306, 'distance': 13.538542747497559, 'force': [-1.2676705121994019, 1.2841308116912842, -0.15775233507156372], 'magnitude': 1.8113162517547607, 'cosine_ionic_motion': -0.12397442013025284, 'motion_component_ionic': -0.22455687820911407, 'motion_component_percent_ionic': 12.397442013025284}, {'ion_id': 1309, 'distance': 10.023154258728027, 'force': [-1.2601678371429443, 2.125608205795288, 2.1942358016967773], 'magnitude': 3.3046791553497314, 'cosine_ionic_motion': -0.16443008184432983, 'motion_component_ionic': -0.5433886647224426, 'motion_component_percent_ionic': 16.443008184432983}, {'ion_id': 1469, 'distance': 9.518566131591797, 'force': [0.4336826205253601, 3.54756498336792, -0.8087297081947327], 'magnitude': 3.6643335819244385, 'cosine_ionic_motion': 0.6916117668151855, 'motion_component_ionic': 2.5342962741851807, 'motion_component_percent_ionic': 69.16117668151855}, {'ion_id': 2434, 'distance': 10.919032096862793, 'force': [-1.0007402896881104, 1.4753109216690063, -2.1392109394073486], 'magnitude': 2.784644842147827, 'cosine_ionic_motion': 0.26733916997909546, 'motion_component_ionic': 0.7444446682929993, 'motion_component_percent_ionic': 26.733916997909546}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.1398327350616455, 'force': [7.858447074890137, -17.051971435546875, -19.573671340942383], 'magnitude': 27.122934341430664, 'cosine_with_motion': 0.12100353837013245, 'motion_component': 3.281970977783203, 'motion_component_percent': 12.100353837013245}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 2.75374436378479, 'force': [-22.12091636657715, 14.096833229064941, 24.434518814086914], 'magnitude': 35.84830856323242, 'cosine_with_motion': -0.4879014790058136, 'motion_component': -17.490442276000977, 'motion_component_percent': 48.79014790058136}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.7814955711364746, 'force': [3.0543620586395264, 25.78272247314453, 23.67487144470215], 'magnitude': 35.13655471801758, 'cosine_with_motion': 0.24216952919960022, 'motion_component': 8.509002685546875, 'motion_component_percent': 24.216952919960022}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.295187950134277, 'force': [-2.860029458999634, 3.017911195755005, 7.347530364990234], 'magnitude': 8.442378997802734, 'cosine_with_motion': -0.35587677359580994, 'motion_component': -3.004446506500244, 'motion_component_percent': 35.587677359580994}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.961963176727295, 'force': [6.7524518966674805, -4.665207862854004, -9.286492347717285], 'magnitude': 12.393494606018066, 'cosine_with_motion': 0.4639624059200287, 'motion_component': 5.750115394592285, 'motion_component_percent': 46.39624059200287}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.774838447570801, 'force': [-2.589862108230591, 1.6945786476135254, 2.805478572845459], 'magnitude': 4.177282810211182, 'cosine_with_motion': -0.48005181550979614, 'motion_component': -2.005312204360962, 'motion_component_percent': 48.005181550979614}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.077581405639648, 'force': [-5.184047222137451, 3.3753116130828857, 5.65091609954834], 'magnitude': 8.3785400390625, 'cosine_with_motion': -0.48156219720840454, 'motion_component': -4.034788131713867, 'motion_component_percent': 48.156219720840454}]}, 5419: {'frame': 5419, 'motion_vector': [-0.07321548461914062, -1.4095268249511719, 1.3923492431640625], 'ionic_force': [-3.6241090893745422, 8.350408673286438, -1.4899036781862378], 'ionic_force_magnitude': 9.224061181109839, 'radial_force': 9.102938630057029, 'axial_force': -1.4899036781862378, 'glu_force': [-29.96388816833496, 8.629873633384705, 5.891890525817871], 'glu_force_magnitude': 31.733636524371025, 'asn_force': [-1.8064911365509033, 2.3654412031173706, 7.011445045471191], 'asn_force_magnitude': 7.617025924696912, 'residue_force': [-31.770379304885864, 10.995314836502075, 12.903335571289062], 'residue_force_magnitude': 36.01041541547968, 'total_force': [-35.39448839426041, 19.345723509788513, 11.413431893102825], 'total_force_magnitude': 41.920081755491786, 'cosine_total_motion': -0.10570642029681394, 'cosine_glu_motion': -0.028079654964546685, 'cosine_asn_motion': 0.43442266831689863, 'cosine_residue_motion': 0.0671455503796204, 'cosine_ionic_motion': -0.7425320375606914, 'motion_component_total': -4.431221780922817, 'motion_component_glu': -0.8910695643746749, 'motion_component_asn': 3.309008726845825, 'motion_component_residue': 2.41793916247115, 'motion_component_ionic': -6.849160943393967, 'motion_component_percent_total': 10.570642029681395, 'motion_component_percent_glu': 2.8079654964546683, 'motion_component_percent_asn': 43.442266831689864, 'motion_component_percent_residue': 6.7145550379620405, 'motion_component_percent_ionic': 74.25320375606914, 'ionic_contributions': [{'ion_id': 1306, 'distance': 13.959966659545898, 'force': [-1.068015694618225, 1.3272424936294556, 0.00673897098749876], 'magnitude': 1.7036066055297852, 'cosine_ionic_motion': -0.5279510617256165, 'motion_component_ionic': -0.8994209170341492, 'motion_component_percent_ionic': 52.795106172561646}, {'ion_id': 1309, 'distance': 9.966863632202148, 'force': [-2.2032456398010254, 2.115774631500244, 1.356068730354309], 'magnitude': 3.3421125411987305, 'cosine_ionic_motion': -0.1407773643732071, 'motion_component_ionic': -0.47049379348754883, 'motion_component_percent_ionic': 14.07773643732071}, {'ion_id': 1469, 'distance': 10.095869064331055, 'force': [0.5705264210700989, 3.1289117336273193, -0.7028989195823669], 'magnitude': 3.257246732711792, 'cosine_ionic_motion': -0.8409490585327148, 'motion_component_ionic': -2.7391786575317383, 'motion_component_percent_ionic': 84.09490585327148}, {'ion_id': 2434, 'distance': 10.628561973571777, 'force': [-0.9233741760253906, 1.778479814529419, -2.1498124599456787], 'magnitude': 2.9389290809631348, 'cosine_ionic_motion': -0.9323354363441467, 'motion_component_ionic': -2.740067720413208, 'motion_component_percent_ionic': 93.23354363441467}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.634676456451416, 'force': [16.686546325683594, -6.239892482757568, -9.607030868530273], 'magnitude': 20.240358352661133, 'cosine_with_motion': -0.14460325241088867, 'motion_component': -2.926821708679199, 'motion_component_percent': 14.460325241088867}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 4.568996906280518, 'force': [-11.584787368774414, 1.6108101606369019, 5.724312782287598], 'magnitude': 13.021896362304688, 'cosine_with_motion': 0.2536253035068512, 'motion_component': 3.302682399749756, 'motion_component_percent': 25.36253035068512}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.6489083766937256, 'force': [-35.06564712524414, 13.258955955505371, 9.774608612060547], 'magnitude': 38.742000579833984, 'cosine_with_motion': -0.03270173817873001, 'motion_component': -1.2669308185577393, 'motion_component_percent': 3.270173817873001}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.565687656402588, 'force': [-0.8570419549942017, 2.804591178894043, 7.056579113006592], 'magnitude': 7.641698837280273, 'cosine_with_motion': 0.39172348380088806, 'motion_component': 2.9934329986572266, 'motion_component_percent': 39.172348380088806}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.063930034637451, 'force': [3.914184331893921, -3.9346847534179688, -10.52584457397461], 'magnitude': 11.89941120147705, 'cosine_with_motion': -0.3982793390750885, 'motion_component': -4.7392897605896, 'motion_component_percent': 39.82793390750885}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.882103443145752, 'force': [-1.7019652128219604, 1.421000361442566, 3.360851287841797], 'magnitude': 4.02631950378418, 'cosine_with_motion': 0.35090523958206177, 'motion_component': 1.4128565788269043, 'motion_component_percent': 35.09052395820618}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.156917572021484, 'force': [-3.161668300628662, 2.0745344161987305, 7.119859218597412], 'magnitude': 8.061776161193848, 'cosine_with_motion': 0.4517626166343689, 'motion_component': 3.6420090198516846, 'motion_component_percent': 45.17626166343689}]}, 5420: {'frame': 5420, 'motion_vector': [1.37384033203125, 0.6198310852050781, 1.271148681640625], 'ionic_force': [-4.995375692844391, 9.29425859451294, -4.6483332216739655], 'ionic_force_magnitude': 11.530135423057965, 'radial_force': 10.551635945877692, 'axial_force': -4.6483332216739655, 'glu_force': [-14.163765907287598, 16.9093017578125, -2.9894802570343018], 'glu_force_magnitude': 22.25923949330707, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [-14.163765907287598, 16.9093017578125, -2.9894802570343018], 'residue_force_magnitude': 22.25923949330707, 'total_force': [-19.15914160013199, 26.20356035232544, -7.637813478708267], 'total_force_magnitude': 33.347195935001906, 'cosine_total_motion': -0.3009704667143185, 'cosine_glu_motion': -0.2911504486400682, 'cosine_asn_motion': None, 'cosine_residue_motion': -0.2911504486400682, 'cosine_ionic_motion': -0.3083861055263508, 'motion_component_total': -10.036521124171347, 'motion_component_glu': -6.480787564863078, 'motion_component_asn': None, 'motion_component_residue': -6.480787564863078, 'motion_component_ionic': -3.555733559308269, 'motion_component_percent_total': 30.097046671431848, 'motion_component_percent_glu': 29.115044864006823, 'motion_component_percent_asn': None, 'motion_component_percent_residue': 29.115044864006823, 'motion_component_percent_ionic': 30.83861055263508, 'ionic_contributions': [{'ion_id': 1306, 'distance': 14.215216636657715, 'force': [-0.9783754944801331, 1.3178855180740356, 0.07299147546291351], 'magnitude': 1.6429754495620728, 'cosine_ionic_motion': -0.13412469625473022, 'motion_component_ionic': -0.2203635722398758, 'motion_component_percent_ionic': 13.412469625473022}, {'ion_id': 1309, 'distance': 11.428321838378906, 'force': [-2.296131134033203, 1.0717114210128784, 0.202259823679924], 'magnitude': 2.5419859886169434, 'cosine_ionic_motion': -0.44556349515914917, 'motion_component_ionic': -1.1326161623001099, 'motion_component_percent_ionic': 44.55634951591492}, {'ion_id': 1469, 'distance': 8.802873611450195, 'force': [0.5067126154899597, 4.24498176574707, -0.2817506194114685], 'magnitude': 4.2843918800354, 'cosine_ionic_motion': 0.35149016976356506, 'motion_component_ionic': 1.5059216022491455, 'motion_component_percent_ionic': 35.149016976356506}, {'ion_id': 2434, 'distance': 9.167643547058105, 'force': [-1.693018913269043, 2.0171566009521484, -2.944333791732788], 'magnitude': 3.9502322673797607, 'cosine_ionic_motion': -0.6186449527740479, 'motion_component_ionic': -2.443791151046753, 'motion_component_percent_ionic': 61.864495277404785}, {'ion_id': 2444, 'distance': 13.246319770812988, 'force': [-0.5345627665519714, 0.6425232887268066, -1.6975001096725464], 'magnitude': 1.8921153545379639, 'cosine_ionic_motion': -0.6685027480125427, 'motion_component_ionic': -1.264884352684021, 'motion_component_percent_ionic': 66.85027480125427}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.7301101684570312, 'force': [11.731582641601562, -14.838068962097168, -3.395612955093384], 'magnitude': 19.21792221069336, 'cosine_with_motion': 0.06872028112411499, 'motion_component': 1.3206610679626465, 'motion_component_percent': 6.872028112411499}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 3.9945478439331055, 'force': [-13.951499938964844, 9.3285493850708, 2.92856764793396], 'magnitude': 17.036510467529297, 'cosine_with_motion': -0.28765401244163513, 'motion_component': -4.900620460510254, 'motion_component_percent': 28.765401244163513}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 3.263315439224243, 'force': [-11.943848609924316, 22.418821334838867, -2.522434949874878], 'magnitude': 25.526884078979492, 'cosine_with_motion': -0.11363813281059265, 'motion_component': -2.900827407836914, 'motion_component_percent': 11.363813281059265}], 'asn_contributions': []}, 5421: {'frame': 5421, 'motion_vector': [-0.43817138671875, 0.11849594116210938, -1.432342529296875], 'ionic_force': [-5.303912997245789, 10.99374771118164, -2.734027996659279], 'ionic_force_magnitude': 12.508752571938622, 'radial_force': 12.206309098964534, 'axial_force': -2.734027996659279, 'glu_force': [-24.575862884521484, 9.054282903671265, -13.014705747365952], 'glu_force_magnitude': 29.246121813140196, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [-24.575862884521484, 9.054282903671265, -13.014705747365952], 'residue_force_magnitude': 29.246121813140196, 'total_force': [-29.879775881767273, 20.048030614852905, -15.74873374402523], 'total_force_magnitude': 39.27782011286929, 'cosine_total_motion': 0.6443204113166525, 'cosine_glu_motion': 0.6936811414343523, 'cosine_asn_motion': None, 'cosine_residue_motion': 0.6936811414343523, 'cosine_ionic_motion': 0.4013204370306142, 'motion_component_total': 25.30750121074543, 'motion_component_glu': 20.2874831618672, 'motion_component_asn': None, 'motion_component_residue': 20.2874831618672, 'motion_component_ionic': 5.020018048878227, 'motion_component_percent_total': 64.43204113166526, 'motion_component_percent_glu': 69.36811414343524, 'motion_component_percent_asn': None, 'motion_component_percent_residue': 69.36811414343524, 'motion_component_percent_ionic': 40.13204370306142, 'ionic_contributions': [{'ion_id': 1306, 'distance': 13.276257514953613, 'force': [-0.9376237988471985, 1.6168675422668457, 0.2334917038679123], 'magnitude': 1.883591651916504, 'cosine_ionic_motion': 0.09469078481197357, 'motion_component_ionic': 0.1783587783575058, 'motion_component_percent_ionic': 9.469078481197357}, {'ion_id': 1309, 'distance': 8.914875984191895, 'force': [-3.586841344833374, 1.4117411375045776, 1.6100742816925049], 'magnitude': 4.177413463592529, 'cosine_ionic_motion': -0.0903717428445816, 'motion_component_ionic': -0.3775201439857483, 'motion_component_percent_ionic': 9.03717428445816}, {'ion_id': 1469, 'distance': 9.480932235717773, 'force': [1.202595829963684, 3.48968505859375, 0.13294559717178345], 'magnitude': 3.6934826374053955, 'cosine_ionic_motion': -0.05475204065442085, 'motion_component_ionic': -0.2022257149219513, 'motion_component_percent_ionic': 5.475204065442085}, {'ion_id': 2434, 'distance': 8.310657501220703, 'force': [-1.507516622543335, 3.459397077560425, -2.9776651859283447], 'magnitude': 4.806924819946289, 'cosine_ionic_motion': 0.7387225031852722, 'motion_component_ionic': 3.550983428955078, 'motion_component_percent_ionic': 73.87225031852722}, {'ion_id': 2444, 'distance': 12.682544708251953, 'force': [-0.4745270609855652, 1.0160568952560425, -1.7328743934631348], 'magnitude': 2.0640740394592285, 'cosine_ionic_motion': 0.9061796069145203, 'motion_component_ionic': 1.8704217672348022, 'motion_component_percent_ionic': 90.61796069145203}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.2050793170928955, 'force': [23.994768142700195, -10.068934440612793, 0.6498544812202454], 'magnitude': 26.029878616333008, 'cosine_with_motion': -0.32312506437301636, 'motion_component': -8.410905838012695, 'motion_component_percent': 32.312506437301636}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 3.727823257446289, 'force': [-19.498056411743164, 1.5375049114227295, 0.3459826409816742], 'magnitude': 19.561641693115234, 'cosine_with_motion': 0.2800096869468689, 'motion_component': 5.4774489402771, 'motion_component_percent': 28.00096869468689}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.719648838043213, 'force': [-29.072574615478516, 17.585712432861328, -14.010542869567871], 'magnitude': 36.752784729003906, 'cosine_with_motion': 0.6318144202232361, 'motion_component': 23.22093963623047, 'motion_component_percent': 63.18144202232361}], 'asn_contributions': []}, 5422: {'frame': 5422, 'motion_vector': [0.1480560302734375, -0.8996047973632812, 0.5749053955078125], 'ionic_force': [-4.211169719696045, 10.116018772125244, -4.300447233021259], 'ionic_force_magnitude': 11.771220523381396, 'radial_force': 10.957544716133956, 'axial_force': -4.300447233021259, 'glu_force': [-25.784714698791504, 17.801549434661865, -1.6186452209949493], 'glu_force_magnitude': 31.374618511214358, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [-25.784714698791504, 17.801549434661865, -1.6186452209949493], 'residue_force_magnitude': 31.374618511214358, 'total_force': [-29.99588441848755, 27.91756820678711, -5.919092454016209], 'total_force_magnitude': 41.40264909528213, 'cosine_total_motion': -0.7385689715918627, 'cosine_glu_motion': -0.6139734756369628, 'cosine_asn_motion': None, 'cosine_residue_motion': -0.6139734756369628, 'cosine_ionic_motion': -0.9612876053839085, 'motion_component_total': -30.57871196348129, 'motion_component_glu': -19.26318357411407, 'motion_component_asn': None, 'motion_component_residue': -19.26318357411407, 'motion_component_ionic': -11.31552838936722, 'motion_component_percent_total': 73.85689715918627, 'motion_component_percent_glu': 61.39734756369628, 'motion_component_percent_asn': None, 'motion_component_percent_residue': 61.39734756369628, 'motion_component_percent_ionic': 96.12876053839085, 'ionic_contributions': [{'ion_id': 1306, 'distance': 13.448433876037598, 'force': [-0.8739737868309021, 1.613553762435913, -0.04794659465551376], 'magnitude': 1.8356701135635376, 'cosine_ionic_motion': -0.8129816055297852, 'motion_component_ionic': -1.492366075515747, 'motion_component_percent_ionic': 81.29816055297852}, {'ion_id': 1309, 'distance': 10.17707633972168, 'force': [-2.566864252090454, 1.8449293375015259, 0.5315044522285461], 'magnitude': 3.205472469329834, 'cosine_ionic_motion': -0.5019389390945435, 'motion_component_ionic': -1.608951449394226, 'motion_component_percent_ionic': 50.193893909454346}, {'ion_id': 1469, 'distance': 10.020413398742676, 'force': [1.0937838554382324, 3.111398458480835, -0.23599140346050262], 'magnitude': 3.3064868450164795, 'cosine_ionic_motion': -0.7780253887176514, 'motion_component_ionic': -2.572530746459961, 'motion_component_percent_ionic': 77.80253887176514}, {'ion_id': 2434, 'distance': 8.782258033752441, 'force': [-1.3929810523986816, 2.763676643371582, -2.991767168045044], 'magnitude': 4.304529666900635, 'cosine_ionic_motion': -0.9510453343391418, 'motion_component_ionic': -4.0938029289245605, 'motion_component_percent_ionic': 95.10453343391418}, {'ion_id': 2444, 'distance': 13.564197540283203, 'force': [-0.4711344838142395, 0.7824605703353882, -1.5562465190887451], 'magnitude': 1.8044710159301758, 'cosine_ionic_motion': -0.8578010201454163, 'motion_component_ionic': -1.5478770732879639, 'motion_component_percent_ionic': 85.78010201454163}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.6099252700805664, 'force': [16.747026443481445, -10.924179077148438, -4.606855392456055], 'magnitude': 20.518861770629883, 'cosine_with_motion': 0.4367186725139618, 'motion_component': 8.960969924926758, 'motion_component_percent': 43.67186725139618}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 4.096811771392822, 'force': [-15.286845207214355, 4.196801662445068, 3.321016788482666], 'magnitude': 16.19660186767578, 'cosine_with_motion': -0.2365494668483734, 'motion_component': -3.8312976360321045, 'motion_component_percent': 23.65494668483734}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.7230336666107178, 'force': [-27.244895935058594, 24.528926849365234, -0.33280661702156067], 'magnitude': 36.661468505859375, 'cosine_with_motion': -0.6653540134429932, 'motion_component': -24.392854690551758, 'motion_component_percent': 66.53540134429932}], 'asn_contributions': []}, 5423: {'frame': 5423, 'motion_vector': [-0.2519950866699219, 0.5466041564941406, 0.0637054443359375], 'ionic_force': [-8.426977157592773, 12.587924428284168, -3.720699816942215], 'ionic_force_magnitude': 15.598506100091043, 'radial_force': 15.148260145204256, 'axial_force': -3.720699816942215, 'glu_force': [-11.985785484313965, 10.626004219055176, -3.2562605142593384], 'glu_force_magnitude': 16.345465789511604, 'asn_force': [0.01022881269454956, 0.8976959884166718, 6.308809280395508], 'asn_force_magnitude': 6.372365122357084, 'residue_force': [-11.975556671619415, 11.523700207471848, 3.0525487661361694], 'residue_force_magnitude': 16.897564263422538, 'total_force': [-20.40253382921219, 24.111624635756016, -0.6681510508060455], 'total_force_magnitude': 31.592408187006534, 'cosine_total_motion': 0.9559011213393435, 'cosine_glu_motion': 0.8714196926836075, 'cosine_asn_motion': 0.23075734057105896, 'cosine_residue_motion': 0.9299701755160927, 'cosine_ionic_motion': 0.9286137733302382, 'motion_component_total': 30.1992184117698, 'motion_component_glu': 14.243760775066622, 'motion_component_asn': 1.4704700287828913, 'motion_component_residue': 15.714230803849514, 'motion_component_ionic': 14.484987607920282, 'motion_component_percent_total': 95.59011213393434, 'motion_component_percent_glu': 87.14196926836075, 'motion_component_percent_asn': 23.075734057105894, 'motion_component_percent_residue': 92.99701755160928, 'motion_component_percent_ionic': 92.86137733302382, 'ionic_contributions': [{'ion_id': 1306, 'distance': 12.553146362304688, 'force': [-1.232452630996704, 1.7019360065460205, 0.152567058801651], 'magnitude': 2.106846570968628, 'cosine_ionic_motion': 0.9807032346725464, 'motion_component_ionic': 2.0661911964416504, 'motion_component_percent_ionic': 98.07032346725464}, {'ion_id': 1309, 'distance': 6.604099273681641, 'force': [-7.53367280960083, -0.03545748442411423, 1.090088963508606], 'magnitude': 7.612212181091309, 'cosine_ionic_motion': 0.4229142963886261, 'motion_component_ionic': 3.219313383102417, 'motion_component_percent_ionic': 42.29142963886261}, {'ion_id': 1469, 'distance': 6.873001575469971, 'force': [3.078547954559326, 6.243687152862549, 0.9668325781822205], 'magnitude': 7.0282182693481445, 'cosine_ionic_motion': 0.6343949437141418, 'motion_component_ionic': 4.4586663246154785, 'motion_component_percent_ionic': 63.439494371414185}, {'ion_id': 2434, 'distance': 7.4333624839782715, 'force': [-2.2350199222564697, 3.7992143630981445, -4</t>
         </is>
       </c>
     </row>
@@ -691,7 +691,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>{5477: {'frame': 5477, 'ionic_force': [-0.44713205099105835, -1.720797836780548, -10.73732876777649], 'ionic_force_magnitude': 10.883533494844983, 'motion_vector': [-0.5623664855957031, 0.9072761535644531, 0.3484649658203125], 'ionic_force_x': -0.44713205099105835, 'ionic_force_y': -1.720797836780548, 'ionic_force_z': -10.73732876777649, 'radial_force': 1.7779404562842043, 'axial_force': -10.73732876777649, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-4.5958311557769775, 4.517671346664429, -9.459369152784348], 'asn_force_magnitude': 11.445989829522443, 'residue_force': [-4.5958311557769775, 4.517671346664429, -9.459369152784348], 'residue_force_magnitude': 11.445989829522443, 'total_force': [-5.042963206768036, 2.7968735098838806, -20.196697920560837], 'total_force_magnitude': 21.003823133646236, 'motion_component_total': -1.482195750316329, 'cosine_total_motion': -0.0705679028472671, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.26353625500195504, 'cosine_residue_motion': 0.26353625500195504, 'cosine_ionic_motion': -0.41334269306102916, 'motion_component_glu': None, 'motion_component_asn': 3.0164332944628107, 'motion_component_residue': 3.0164332944628107, 'motion_component_ionic': -4.49862904477914, 'ionic_contributions': [{'ion_id': 1306, 'distance': 9.458476066589355, 'force': [-1.8695889711380005, 2.9205055236816406, -1.3217833042144775], 'magnitude': 3.71104097366333}, {'ion_id': 1309, 'distance': 6.1396098136901855, 'force': [-0.14590446650981903, -7.744018077850342, -4.193130970001221], 'magnitude': 8.807579040527344}, {'ion_id': 1469, 'distance': 10.075268745422363, 'force': [1.5043941736221313, 2.458629608154297, -1.5455207824707031], 'magnitude': 3.270580291748047}, {'ion_id': 2444, 'distance': 9.430074691772461, 'force': [0.06396721303462982, 0.6440851092338562, -3.676893711090088], 'magnitude': 3.7334280014038086}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.793630361557007, 'force': [11.624513626098633, -10.297250747680664, 5.420295238494873], 'magnitude': 16.448169708251953}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.815434694290161, 'force': [-13.746847152709961, 16.928144454956055, -11.89767074584961], 'magnitude': 24.841344833374023}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.118040561676025, 'force': [-13.543807029724121, 11.842682838439941, -0.2968275547027588], 'magnitude': 17.993663787841797}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.5625646114349365, 'force': [7.083231449127197, -8.214049339294434, -1.682852029800415], 'magnitude': 10.976099967956543}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.119686126708984, 'force': [4.05751895904541, -3.4325551986694336, -0.03470611572265625], 'magnitude': 5.314800262451172}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.418187141418457, 'force': [9.146876335144043, 4.849287033081055, -0.9270142316818237], 'magnitude': 10.394243240356445}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.823740482330322, 'force': [-5.628729343414307, -1.9206788539886475, 0.6870071291923523], 'magnitude': 5.986950874328613}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.228281021118164, 'force': [-3.95939302444458, -3.1348214149475098, 0.6844471096992493], 'magnitude': 5.096309185028076}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.738805294036865, 'force': [-3.6168277263641357, -4.4709858894348145, -1.6359606981277466], 'magnitude': 5.978923320770264}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.47750997543335, 'force': [3.9876327514648438, 2.367898464202881, 0.22391274571418762], 'magnitude': 4.643091201782227}]}, 5478: {'frame': 5478, 'ionic_force': [1.7842273004353046, -1.3310573995113373, -13.13483214378357], 'ionic_force_magnitude': 13.322124316556373, 'motion_vector': [5.6822967529296875, -1.4546623229980469, 1.581939697265625], 'ionic_force_x': 1.7842273004353046, 'ionic_force_y': -1.3310573995113373, 'ionic_force_z': -13.13483214378357, 'radial_force': 2.226023553427173, 'axial_force': -13.13483214378357, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [4.776796340942383, 5.489965319633484, -0.3961131274700165], 'asn_force_magnitude': 7.287963234222096, 'residue_force': [4.776796340942383, 5.489965319633484, -0.3961131274700165], 'residue_force_magnitude': 7.287963234222096, 'total_force': [6.5610236413776875, 4.158907920122147, -13.530945271253586], 'total_force_magnitude': 15.602244269477113, 'motion_component_total': 1.6175383380477966, 'cosine_total_motion': 0.103673440186564, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.4185296249625578, 'cosine_residue_motion': 0.4185296249625578, 'cosine_ionic_motion': -0.1075421717339463, 'motion_component_glu': None, 'motion_component_asn': 3.0502285191598837, 'motion_component_residue': 3.0502285191598837, 'motion_component_ionic': -1.4326901811120873, 'ionic_contributions': [{'ion_id': 1306, 'distance': 9.401440620422363, 'force': [-1.9984097480773926, 2.8898801803588867, -1.3281662464141846], 'magnitude': 3.756204843521118}, {'ion_id': 1309, 'distance': 5.802047252655029, 'force': [2.848625421524048, -7.680440902709961, -5.491806507110596], 'magnitude': 9.862239837646484}, {'ion_id': 1469, 'distance': 11.164752006530762, 'force': [1.1187093257904053, 2.1294939517974854, -1.1434855461120605], 'magnitude': 2.663421392440796}, {'ion_id': 2443, 'distance': 14.983959197998047, 'force': [-0.03920864686369896, 0.29816392064094543, -1.4478132724761963], 'magnitude': 1.478716492652893}, {'ion_id': 2444, 'distance': 9.266230583190918, 'force': [-0.14548905193805695, 1.0318454504013062, -3.7235605716705322], 'magnitude': 3.8666231632232666}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.346997261047363, 'force': [8.600956916809082, -8.802119255065918, 2.3395042419433594], 'magnitude': 12.527052879333496}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.540380477905273, 'force': [-4.551881313323975, 8.276850700378418, -1.4175502061843872], 'magnitude': 9.551718711853027}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.867973804473877, 'force': [-16.598386764526367, 11.808831214904785, 1.010152816772461], 'magnitude': 20.39547348022461}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.704692840576172, 'force': [7.034178733825684, -6.805782794952393, -2.6880531311035156], 'magnitude': 10.150073051452637}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.167927265167236, 'force': [7.445319175720215, -2.9503414630889893, -0.413440465927124], 'magnitude': 8.019241333007812}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.4427409172058105, 'force': [9.58101749420166, 2.6851537227630615, -2.6641883850097656], 'magnitude': 10.30067253112793}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.947059631347656, 'force': [-5.449575424194336, -0.5346041917800903, 1.554775595664978], 'magnitude': 5.692187786102295}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.192211151123047, 'force': [-4.405142784118652, -2.161324977874756, 1.6201916933059692], 'magnitude': 5.167361736297607}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.2475810050964355, 'force': [3.1203103065490723, 3.9733023643493652, 0.2624947130680084], 'magnitude': 5.058890342712402}]}, 5479: {'frame': 5479, 'ionic_force': [8.564183592796326, 7.061019524931908, -8.43285158276558], 'ionic_force_magnitude': 13.939735404933026, 'motion_vector': [-0.8315162658691406, 0.4536933898925781, 0.4904327392578125], 'ionic_force_x': 8.564183592796326, 'ionic_force_y': 7.061019524931908, 'ionic_force_z': -8.43285158276558, 'radial_force': 11.099695371612295, 'axial_force': -8.43285158276558, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [4.034980535507202, 0.3665037155151367, -0.8855640888214111], 'asn_force_magnitude': 4.147242053560231, 'residue_force': [4.034980535507202, 0.3665037155151367, -0.8855640888214111], 'residue_force_magnitude': 4.147242053560231, 'total_force': [12.599164128303528, 7.427523240447044, -9.31841567158699], 'total_force_magnitude': 17.341854250563557, 'motion_component_total': -10.946840587043383, 'cosine_total_motion': -0.6312381841571321, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.8190327924920568, 'cosine_residue_motion': -0.8190327924920568, 'cosine_ionic_motion': -0.5416252982896361, 'motion_component_glu': None, 'motion_component_asn': -3.3967272402679285, 'motion_component_residue': -3.3967272402679285, 'motion_component_ionic': -7.550113346775452, 'ionic_contributions': [{'ion_id': 1306, 'distance': 6.694813251495361, 'force': [0.8983935117721558, 7.096762180328369, -1.9228250980377197], 'magnitude': 7.407320976257324}, {'ion_id': 1309, 'distance': 9.535407066345215, 'force': [2.8427734375, -2.1192972660064697, -0.8717526197433472], 'magnitude': 3.6514017581939697}, {'ion_id': 1469, 'distance': 12.905256271362305, 'force': [1.5580865144729614, 1.1739774942398071, -0.4098491966724396], 'magnitude': 1.9934475421905518}, {'ion_id': 2443, 'distance': 13.859634399414062, 'force': [0.5962351560592651, 0.1816510409116745, -1.6120604276657104], 'magnitude': 1.7283612489700317}, {'ion_id': 2444, 'distance': 8.539250373840332, 'force': [2.6686949729919434, 0.7279260754585266, -3.6163642406463623], 'magnitude': 4.553009986877441}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.292919635772705, 'force': [-1.668077826499939, -11.140223503112793, 6.172342777252197], 'magnitude': 12.844643592834473}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.100113868713379, 'force': [4.060624599456787, 8.442559242248535, -7.030838489532471], 'magnitude': 11.713162422180176}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.018746852874756, 'force': [-3.56195068359375, 16.02308464050293, -9.356781005859375], 'magnitude': 18.893810272216797}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.5947213172912598, 'force': [3.3128061294555664, -7.549646854400635, 6.946192741394043], 'magnitude': 10.78060531616211}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.737691879272461, 'force': [1.8915783166885376, -5.4092698097229, 2.3835198879241943], 'magnitude': 6.206402778625488}]}, 5480: {'frame': 5480, 'ionic_force': [8.845621451735497, 5.174365371465683, -6.945133060216904], 'ionic_force_magnitude': 12.379577904312578, 'motion_vector': [-2.4467201232910156, 2.9426307678222656, 1.0514373779296875], 'ionic_force_x': 8.845621451735497, 'ionic_force_y': 5.174365371465683, 'ionic_force_z': -6.945133060216904, 'radial_force': 10.247881530581157, 'axial_force': -6.945133060216904, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [3.2695456594228745, 0.8918981552124023, -0.8600523471832275], 'asn_force_magnitude': 3.4964412161821947, 'residue_force': [3.2695456594228745, 0.8918981552124023, -0.8600523471832275], 'residue_force_magnitude': 3.4964412161821947, 'total_force': [12.115167111158371, 6.066263526678085, -7.805185407400131], 'total_force_magnitude': 15.636423713569872, 'motion_component_total': -5.038935618007108, 'cosine_total_motion': -0.32225627229800197, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.4525215385641118, 'cosine_residue_motion': -0.4525215385641118, 'cosine_ionic_motion': -0.2792276672177309, 'motion_component_glu': None, 'motion_component_asn': -1.582214958645741, 'motion_component_residue': -1.582214958645741, 'motion_component_ionic': -3.456720659361367, 'ionic_contributions': [{'ion_id': 1306, 'distance': 7.943610668182373, 'force': [0.21233676373958588, 5.167843818664551, -0.9647490382194519], 'magnitude': 5.261410236358643}, {'ion_id': 1309, 'distance': 7.917448043823242, 'force': [4.6044087409973145, -2.470323085784912, -0.8643374443054199], 'magnitude': 5.296239852905273}, {'ion_id': 1469, 'distance': 12.11471939086914, 'force': [1.6390438079833984, 1.4995357990264893, -0.4266315996646881], 'magnitude': 2.2620978355407715}, {'ion_id': 2443, 'distance': 13.938857078552246, 'force': [0.6318773031234741, 0.20215561985969543, -1.57472562789917], 'magnitude': 1.708770513534546}, {'ion_id': 2444, 'distance': 9.524741172790527, 'force': [1.7579548358917236, 0.7751532196998596, -3.114689350128174], 'magnitude': 3.6595845222473145}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.656192302703857, 'force': [-2.944319009780884, -7.897385597229004, 6.9409990310668945], 'magnitude': 10.918570518493652}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.206221103668213, 'force': [5.27993631362915, 6.390595436096191, -7.426429748535156], 'magnitude': 11.129658699035645}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.523441314697266, 'force': [0.022058889269828796, 10.369463920593262, -10.717702865600586], 'magnitude': 14.912927627563477}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.082260608673096, 'force': [0.4331759512424469, -4.46119499206543, 7.056110858917236], 'magnitude': 8.359342575073242}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.3692402839660645, 'force': [0.47869351506233215, -3.509580612182617, 3.286970376968384], 'magnitude': 4.83223295211792}]}, 5481: {'frame': 5481, 'ionic_force': [10.121144622564316, 6.428409576416016, -5.320772521197796], 'ionic_force_magnitude': 13.11764606838259, 'motion_vector': [1.9404220581054688, -4.451213836669922, 0.8924026489257812], 'ionic_force_x': 10.121144622564316, 'ionic_force_y': 6.428409576416016, 'ionic_force_z': -5.320772521197796, 'radial_force': 11.990079989433752, 'axial_force': -5.320772521197796, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-3.4476019144058228, -0.01515108346939087, 4.744694709777832], 'asn_force_magnitude': 5.865007792368117, 'residue_force': [-3.4476019144058228, -0.01515108346939087, 4.744694709777832], 'residue_force_magnitude': 5.865007792368117, 'total_force': [6.673542708158493, 6.413258492946625, -0.5760778114199638], 'total_force_magnitude': 9.273506479200725, 'motion_component_total': -3.263332301931266, 'cosine_total_motion': -0.351898422592414, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.08247598576067056, 'cosine_residue_motion': -0.08247598576067056, 'cosine_ionic_motion': -0.2118985363891906, 'motion_component_glu': None, 'motion_component_asn': -0.48372229916957465, 'motion_component_residue': -0.48372229916957465, 'motion_component_ionic': -2.7796100027616912, 'ionic_contributions': [{'ion_id': 1306, 'distance': 10.731383323669434, 'force': [-0.6012338399887085, 2.818525791168213, -0.07370224595069885], 'magnitude': 2.882880926132202}, {'ion_id': 1309, 'distance': 6.173717498779297, 'force': [8.690352439880371, -0.589633584022522, -0.05870877951383591], 'magnitude': 8.710530281066895}, {'ion_id': 1469, 'distance': 13.34061336517334, 'force': [0.9652875065803528, 1.5830146074295044, -0.20551034808158875], 'magnitude': 1.865462303161621}, {'ion_id': 2443, 'distance': 12.948829650878906, 'force': [0.3752489387989044, 0.6354923248291016, -1.8373764753341675], 'magnitude': 1.9800541400909424}, {'ion_id': 2444, 'distance': 9.370463371276855, 'force': [0.691489577293396, 1.9810104370117188, -3.145474672317505], 'magnitude': 3.781080722808838}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.794651508331299, 'force': [-4.679443359375, -0.1746199131011963, 5.26983118057251], 'magnitude': 7.049737930297852}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.264755725860596, 'force': [5.481466770172119, -0.6339924931526184, -9.52616024017334], 'magnitude': 11.008912086486816}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.354150772094727, 'force': [-2.290189266204834, 1.1873915195465088, 4.1182475090026855], 'magnitude': 4.859508991241455}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.138481616973877, 'force': [-1.959436058998108, -0.39393019676208496, 4.882776260375977], 'magnitude': 5.275990009307861}]}, 5483: {'frame': 5483, 'ionic_force': [13.281899441033602, -1.611535370349884, -14.18665498495102], 'ionic_force_magnitude': 19.500437909792, 'motion_vector': [-1.0512886047363281, -1.1198539733886719, -3.1050186157226562], 'ionic_force_x': 13.281899441033602, 'ionic_force_y': -1.611535370349884, 'ionic_force_z': -14.18665498495102, 'radial_force': 13.379308614858147, 'axial_force': -14.18665498495102, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-1.1116523742675781, -0.5470233708620071, -1.6721093654632568], 'asn_force_magnitude': 2.081094735843112, 'residue_force': [-1.1116523742675781, -0.5470233708620071, -1.6721093654632568], 'residue_force_magnitude': 2.081094735843112, 'total_force': [12.170247066766024, -2.158558741211891, -15.858764350414276], 'total_force_magnitude': 20.106583405127783, 'motion_component_total': 11.219043094478927, 'cosine_total_motion': 0.5579785918087772, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.9672551795401328, 'cosine_residue_motion': 0.9672551795401328, 'cosine_ionic_motion': 0.47209675365793713, 'motion_component_glu': None, 'motion_component_asn': 2.0129496623579546, 'motion_component_residue': 2.0129496623579546, 'motion_component_ionic': 9.206093432120973, 'ionic_contributions': [{'ion_id': 1306, 'distance': 9.658601760864258, 'force': [-1.4231153726577759, 3.2190465927124023, -0.5271512866020203], 'magnitude': 3.5588490962982178}, {'ion_id': 1309, 'distance': 4.376565933227539, 'force': [12.95172119140625, -9.656329154968262, -6.279929161071777], 'magnitude': 17.332895278930664}, {'ion_id': 1469, 'distance': 10.299714088439941, 'force': [1.47786545753479, 2.6548736095428467, -0.7496045827865601], 'magnitude': 3.129592180252075}, {'ion_id': 2443, 'distance': 13.630022048950195, 'force': [0.023254413157701492, 0.36658936738967896, -1.7489255666732788], 'magnitude': 1.7870839834213257}, {'ion_id': 2444, 'distance': 7.982741832733154, 'force': [0.2521737515926361, 1.8042842149734497, -4.881044387817383], 'magnitude': 5.209954738616943}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.441762924194336, 'force': [4.711716175079346, -1.0550556182861328, 6.370713233947754], 'magnitude': 7.993710041046143}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.3333330154418945, 'force': [-6.330883502960205, 0.2161678522825241, -8.356761932373047], 'magnitude': 10.48629093170166}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.463705062866211, 'force': [7.841887474060059, 3.829061985015869, -5.322386741638184], 'magnitude': 10.221776008605957}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.135146141052246, 'force': [-4.220770359039307, -1.072511911392212, 2.9905319213867188], 'magnitude': 5.282846450805664}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.403172016143799, 'force': [-3.1136021614074707, -2.4646856784820557, 2.645794153213501], 'magnitude': 4.771731376647949}]}, 5484: {'frame': 5484, 'ionic_force': [2.082847408950329, 0.5381690561771393, -11.26388955116272], 'ionic_force_magnitude': 11.467479543595898, 'motion_vector': [-1.2701416015625, -1.1113739013671875, -2.5788192749023438], 'ionic_force_x': 2.082847408950329, 'ionic_force_y': 0.5381690561771393, 'ionic_force_z': -11.26388955116272, 'radial_force': 2.151250627425287, 'axial_force': -11.26388955116272, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-5.776663586497307, -0.6191740036010742, -10.50797963142395], 'asn_force_magnitude': 12.007116830143692, 'residue_force': [-5.776663586497307, -0.6191740036010742, -10.50797963142395], 'residue_force_magnitude': 12.007116830143692, 'total_force': [-3.693816177546978, -0.08100494742393494, -21.77186918258667], 'total_force_magnitude': 22.083141249801443, 'motion_component_total': 19.768793608390794, 'cosine_total_motion': 0.8951984405102938, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.9491315711435183, 'cosine_residue_motion': 0.9491315711435183, 'cosine_ionic_motion': 0.7301046332512008, 'motion_component_glu': None, 'motion_component_asn': 11.396333661898064, 'motion_component_residue': 11.396333661898064, 'motion_component_ionic': 8.37245994649273, 'ionic_contributions': [{'ion_id': 1306, 'distance': 10.203856468200684, 'force': [-1.2755056619644165, 2.3901894092559814, -1.6815731525421143], 'magnitude': 3.188668727874756}, {'ion_id': 1309, 'distance': 6.766260623931885, 'force': [2.1952145099639893, -4.486453056335449, -5.257387638092041], 'magnitude': 7.251713752746582}, {'ion_id': 1469, 'distance': 10.19710636138916, 'force': [1.2880535125732422, 2.27970814704895, -1.8271305561065674], 'magnitude': 3.1928915977478027}, {'ion_id': 2444, 'distance': 11.46453857421875, 'force': [-0.12491495162248611, 0.35472455620765686, -2.497798204421997], 'magnitude': 2.5259511470794678}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.298002004623413, 'force': [12.503654479980469, -16.719730377197266, 6.1443257331848145], 'magnitude': 21.763351440429688}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.7381234169006348, 'force': [-16.12070083618164, 14.657597541809082, -14.665353775024414], 'magnitude': 26.263944625854492}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.4153730869293213, 'force': [-6.831456184387207, 24.97312355041504, -3.7387590408325195], 'magnitude': 26.159204483032227}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.094322919845581, 'force': [-0.14636151492595673, -14.058687210083008, 3.7435548305511475], 'magnitude': 14.54930591583252}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.016315937042236, 'force': [2.039274215698242, -8.367271423339844, -0.6421957612037659], 'magnitude': 8.636103630065918}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.3982744216918945, 'force': [3.9998672008514404, -5.398072242736816, -0.7206801176071167], 'magnitude': 6.757033348083496}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.558880805969238, 'force': [-1.2209409475326538, 4.293866157531738, -0.628871500492096], 'magnitude': 4.508155345916748}]}, 5485: {'frame': 5485, 'ionic_force': [0.2769479751586914, 0.9982298463582993, -7.456764340400696], 'ionic_force_magnitude': 7.528379469406177, 'motion_vector': [4.385654449462891, -1.0877685546875, 2.3917007446289062], 'ionic_force_x': 0.2769479751586914, 'ionic_force_y': 0.9982298463582993, 'ionic_force_z': -7.456764340400696, 'radial_force': 1.0359358122514217, 'axial_force': -7.456764340400696, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-3.806230127811432, 11.06399917602539, -2.2032819986343384], 'asn_force_magnitude': 11.906045402166752, 'residue_force': [-3.806230127811432, 11.06399917602539, -2.2032819986343384], 'residue_force_magnitude': 11.906045402166752, 'total_force': [-3.5292821526527405, 12.06222902238369, -9.660046339035034], 'total_force_magnitude': 15.851488787296061, 'motion_component_total': -10.113110895878725, 'cosine_total_motion': -0.637991234235596, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.5585313602891084, 'cosine_residue_motion': -0.5585313602891084, 'cosine_ionic_motion': -0.46002080206190965, 'motion_component_glu': None, 'motion_component_asn': -6.649899734136081, 'motion_component_residue': -6.649899734136081, 'motion_component_ionic': -3.4632111617426435, 'ionic_contributions': [{'ion_id': 1306, 'distance': 11.38329792022705, 'force': [-1.2062158584594727, 1.471609354019165, -1.7157915830612183], 'magnitude': 2.562134027481079}, {'ion_id': 1309, 'distance': 9.005099296569824, 'force': [0.5064878463745117, -2.087893009185791, -3.4851157665252686], 'magnitude': 4.094125270843506}, {'ion_id': 1469, 'distance': 11.275890350341797, 'force': [0.7889192700386047, 1.6113115549087524, -1.897242546081543], 'magnitude': 2.611177444458008}, {'ion_id': 2436, 'distance': 14.687723159790039, 'force': [0.3979494571685791, -0.12599879503250122, 1.4812759160995483], 'magnitude': 1.538966417312622}, {'ion_id': 2444, 'distance': 13.373282432556152, 'force': [-0.2101927399635315, 0.129200741648674, -1.8398903608322144], 'magnitude': 1.8563593626022339}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.6561150550842285, 'force': [4.050293922424316, -16.094636917114258, -6.177183151245117], 'magnitude': 17.708749771118164}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.6600563526153564, 'force': [-8.526857376098633, 26.200334548950195, 3.903982639312744], 'magnitude': 27.828149795532227}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.027401447296143, 'force': [1.176471471786499, 16.352994918823242, 9.225669860839844], 'magnitude': 18.812694549560547}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.5700936317443848, 'force': [-3.221045970916748, -8.954358100891113, -5.376433849334717], 'magnitude': 10.929853439331055}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.924551486968994, 'force': [-0.3331156373023987, -4.674124717712402, -3.3225059509277344], 'magnitude': 5.7443413734436035}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.339736461639404, 'force': [4.47689962387085, -5.004852771759033, 1.6129518747329712], 'magnitude': 6.905996799468994}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.8286285400390625, 'force': [-1.4288761615753174, 3.2386422157287598, -2.069763422012329], 'magnitude': 4.1005377769470215}]}, 5486: {'frame': 5486, 'ionic_force': [3.3664588928222656, 2.9159571398049593, -8.914527297019958], 'ionic_force_magnitude': 9.965171772104863, 'motion_vector': [-1.728607177734375, 5.325992584228516, 4.6172027587890625], 'ionic_force_x': 3.3664588928222656, 'ionic_force_y': 2.9159571398049593, 'ionic_force_z': -8.914527297019958, 'radial_force': 4.453745785093894, 'axial_force': -8.914527297019958, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-1.8950878083705902, -10.64593243598938, 6.008089393377304], 'asn_force_magnitude': 12.37030207359135, 'residue_force': [-1.8950878083705902, -10.64593243598938, 6.008089393377304], 'residue_force_magnitude': 12.37030207359135, 'total_force': [1.4713710844516754, -7.729975296184421, -2.9064379036426544], 'total_force_magnitude': 8.388374826836998, 'motion_component_total': -7.872131149663212, 'cosine_total_motion': -0.938457247341623, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.286077911386587, 'cosine_residue_motion': -0.286077911386587, 'cosine_ionic_motion': -0.43484056956840117, 'motion_component_glu': None, 'motion_component_asn': -3.53887018043418, 'motion_component_residue': -3.53887018043418, 'motion_component_ionic': -4.333260969229032, 'ionic_contributions': [{'ion_id': 1306, 'distance': 7.911111354827881, 'force': [-0.8589418530464172, 4.029123783111572, -3.341933012008667], 'magnitude': 5.304727554321289}, {'ion_id': 1309, 'distance': 9.57223129272461, 'force': [2.1206986904144287, -2.4510836601257324, -1.6197460889816284], 'magnitude': 3.623361825942993}, {'ion_id': 1469, 'distance': 11.634034156799316, 'force': [1.5200526714324951, 1.3517338037490845, -1.3707325458526611], 'magnitude': 2.4528865814208984}, {'ion_id': 2444, 'distance': 11.19824504852295, 'force': [0.584649384021759, -0.01381678692996502, -2.582115650177002], 'magnitude': 2.6475133895874023}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.612143039703369, 'force': [-1.8252153396606445, -3.661539316177368, -1.6806464195251465], 'magnitude': 4.4229912757873535}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.7498786449432373, 'force': [-0.45775699615478516, 16.191463470458984, -4.584557056427002], 'magnitude': 16.834226608276367}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.9197967052459717, 'force': [-0.3881295621395111, -20.042327880859375, 11.473390579223633], 'magnitude': 23.097278594970703}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.484484672546387, 'force': [-3.4142470359802246, -14.56297779083252, 2.546977996826172], 'magnitude': 15.173151016235352}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.302166938781738, 'force': [3.276872396469116, 6.6223249435424805, -1.4341151714324951], 'magnitude': 7.526603698730469}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.330281734466553, 'force': [0.913388729095459, 4.807124137878418, -0.31296053528785706], 'magnitude': 4.903128147125244}]}, 5487: {'frame': 5487, 'ionic_force': [14.640848532319069, 6.408383667469025, -6.467983774840832], 'ionic_force_magnitude': 17.24113224493674, 'motion_vector': [0.3015022277832031, -3.9131088256835938, 0.8899307250976562], 'ionic_force_x': 14.640848532319069, 'ionic_force_y': 6.408383667469025, 'ionic_force_z': -6.467983774840832, 'radial_force': 15.981921879917733, 'axial_force': -6.467983774840832, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-8.309809863567352, -1.2385395541787148, 4.190282344818115], 'asn_force_magnitude': 9.388577438845614, 'residue_force': [-8.309809863567352, -1.2385395541787148, 4.190282344818115], 'residue_force_magnitude': 9.388577438845614, 'total_force': [6.331038668751717, 5.16984411329031, -2.2777014300227165], 'total_force_magnitude': 8.485120068996048, 'motion_component_total': -5.056318293749003, 'cosine_total_motion': -0.5959041536989426, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.16065968113555476, 'cosine_residue_motion': 0.16065968113555476, 'cosine_ionic_motion': -0.38075713695185387, 'motion_component_glu': None, 'motion_component_asn': 1.5083658576413996, 'motion_component_residue': 1.5083658576413996, 'motion_component_ionic': -6.564684151390402, 'ionic_contributions': [{'ion_id': 1306, 'distance': 11.268638610839844, 'force': [-0.8415454030036926, 2.4747672080993652, -0.05607883632183075], 'magnitude': 2.614539384841919}, {'ion_id': 1309, 'distance': 4.883230686187744, 'force': [13.761055946350098, -2.1138620376586914, -0.08146259933710098], 'magnitude': 13.922704696655273}, {'ion_id': 1469, 'distance': 12.495586395263672, 'force': [0.9084755182266235, 1.9054216146469116, -0.2553384602069855], 'magnitude': 2.1263012886047363}, {'ion_id': 2443, 'distance': 13.029350280761719, 'force': [0.1551320105791092, 0.6592459082603455, -1.8346444368362427], 'magnitude': 1.9556562900543213}, {'ion_id': 2444, 'distance': 7.750635147094727, 'force': [0.6577304601669312, 3.4828109741210938, -4.240459442138672], 'magnitude': 5.526669979095459}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.877341270446777, 'force': [-3.435832977294922, 0.626846969127655, -8.11388111114502], 'magnitude': 8.833625793457031}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.894800662994385, 'force': [0.9960408806800842, 0.055521391332149506, 3.8828914165496826], 'magnitude': 4.008993148803711}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.525697708129883, 'force': [1.8769385814666748, -1.0556988716125488, 4.022271156311035], 'magnitude': 4.562462329864502}, {'resid': 455, 'resname': 'ASN</t>
+          <t>{5477: {'frame': 5477, 'motion_vector': [-0.5623664855957031, 0.9072761535644531, 0.3484649658203125], 'ionic_force': [-0.44713205099105835, -1.720797836780548, -10.73732876777649], 'ionic_force_magnitude': 10.883533494844983, 'radial_force': 1.7779404562842043, 'axial_force': -10.73732876777649, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-4.5958311557769775, 4.517671346664429, -9.459369152784348], 'asn_force_magnitude': 11.445989829522443, 'residue_force': [-4.5958311557769775, 4.517671346664429, -9.459369152784348], 'residue_force_magnitude': 11.445989829522443, 'total_force': [-5.042963206768036, 2.7968735098838806, -20.196697920560837], 'total_force_magnitude': 21.003823133646236, 'cosine_total_motion': -0.0705679028472671, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.26353625500195504, 'cosine_residue_motion': 0.26353625500195504, 'cosine_ionic_motion': -0.41334269306102916, 'motion_component_total': -1.482195750316329, 'motion_component_glu': None, 'motion_component_asn': 3.0164332944628107, 'motion_component_residue': 3.0164332944628107, 'motion_component_ionic': -4.49862904477914, 'motion_component_percent_total': 7.056790284726711, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 26.353625500195506, 'motion_component_percent_residue': 26.353625500195506, 'motion_component_percent_ionic': 41.33426930610292, 'ionic_contributions': [{'ion_id': 1306, 'distance': 9.458476066589355, 'force': [-1.8695889711380005, 2.9205055236816406, -1.3217833042144775], 'magnitude': 3.71104097366333, 'cosine_ionic_motion': 0.7776566743850708, 'motion_component_ionic': 2.885915756225586, 'motion_component_percent_ionic': 77.76566743850708}, {'ion_id': 1309, 'distance': 6.1396098136901855, 'force': [-0.14590446650981903, -7.744018077850342, -4.193130970001221], 'magnitude': 8.807579040527344, 'cosine_ionic_motion': -0.8498765230178833, 'motion_component_ionic': -7.485354900360107, 'motion_component_percent_ionic': 84.98765230178833}, {'ion_id': 1469, 'distance': 10.075268745422363, 'force': [1.5043941736221313, 2.458629608154297, -1.5455207824707031], 'magnitude': 3.270580291748047, 'cosine_ionic_motion': 0.23038555681705475, 'motion_component_ionic': 0.7534944415092468, 'motion_component_percent_ionic': 23.038555681705475}, {'ion_id': 2444, 'distance': 9.430074691772461, 'force': [0.06396721303462982, 0.6440851092338562, -3.676893711090088], 'magnitude': 3.7334280014038086, 'cosine_ionic_motion': -0.1748216599225998, 'motion_component_ionic': -0.6526840925216675, 'motion_component_percent_ionic': 17.48216599225998}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.793630361557007, 'force': [11.624513626098633, -10.297250747680664, 5.420295238494873], 'magnitude': 16.448169708251953, 'cosine_with_motion': -0.7575289607048035, 'motion_component': -12.459964752197266, 'motion_component_percent': 75.75289607048035}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.815434694290161, 'force': [-13.746847152709961, 16.928144454956055, -11.89767074584961], 'magnitude': 24.841344833374023, 'cosine_with_motion': 0.6791295409202576, 'motion_component': 16.87049102783203, 'motion_component_percent': 67.91295409202576}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.118040561676025, 'force': [-13.543807029724121, 11.842682838439941, -0.2968275547027588], 'magnitude': 17.993663787841797, 'cosine_with_motion': 0.903645932674408, 'motion_component': 16.25990104675293, 'motion_component_percent': 90.3645932674408}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.5625646114349365, 'force': [7.083231449127197, -8.214049339294434, -1.682852029800415], 'magnitude': 10.976099967956543, 'cosine_with_motion': -0.9754542112350464, 'motion_component': -10.706683158874512, 'motion_component_percent': 97.54542112350464}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.119686126708984, 'force': [4.05751895904541, -3.4325551986694336, -0.03470611572265625], 'magnitude': 5.314800262451172, 'cosine_with_motion': -0.9062236547470093, 'motion_component': -4.816397666931152, 'motion_component_percent': 90.62236547470093}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.418187141418457, 'force': [9.146876335144043, 4.849287033081055, -0.9270142316818237], 'magnitude': 10.394243240356445, 'cosine_with_motion': -0.09144483506679535, 'motion_component': -0.9504998922348022, 'motion_component_percent': 9.144483506679535}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.823740482330322, 'force': [-5.628729343414307, -1.9206788539886475, 0.6870071291923523], 'magnitude': 5.986950874328613, 'cosine_with_motion': 0.24726004898548126, 'motion_component': 1.4803338050842285, 'motion_component_percent': 24.726004898548126}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.228281021118164, 'force': [-3.95939302444458, -3.1348214149475098, 0.6844471096992493], 'magnitude': 5.096309185028076, 'cosine_with_motion': -0.06623220443725586, 'motion_component': -0.33753979206085205, 'motion_component_percent': 6.623220443725586}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.738805294036865, 'force': [-3.6168277263641357, -4.4709858894348145, -1.6359606981277466], 'magnitude': 5.978923320770264, 'cosine_with_motion': -0.3861612379550934, 'motion_component': -2.308828353881836, 'motion_component_percent': 38.61612379550934}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.47750997543335, 'force': [3.9876327514648438, 2.367898464202881, 0.22391274571418762], 'magnitude': 4.643091201782227, 'cosine_with_motion': -0.003097212640568614, 'motion_component': -0.014380641281604767, 'motion_component_percent': 0.3097212640568614}]}, 5478: {'frame': 5478, 'motion_vector': [5.6822967529296875, -1.4546623229980469, 1.581939697265625], 'ionic_force': [1.7842273004353046, -1.3310573995113373, -13.13483214378357], 'ionic_force_magnitude': 13.322124316556373, 'radial_force': 2.226023553427173, 'axial_force': -13.13483214378357, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [4.776796340942383, 5.489965319633484, -0.3961131274700165], 'asn_force_magnitude': 7.287963234222096, 'residue_force': [4.776796340942383, 5.489965319633484, -0.3961131274700165], 'residue_force_magnitude': 7.287963234222096, 'total_force': [6.5610236413776875, 4.158907920122147, -13.530945271253586], 'total_force_magnitude': 15.602244269477113, 'cosine_total_motion': 0.103673440186564, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.4185296249625578, 'cosine_residue_motion': 0.4185296249625578, 'cosine_ionic_motion': -0.1075421717339463, 'motion_component_total': 1.6175383380477966, 'motion_component_glu': None, 'motion_component_asn': 3.0502285191598837, 'motion_component_residue': 3.0502285191598837, 'motion_component_ionic': -1.4326901811120873, 'motion_component_percent_total': 10.3673440186564, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 41.85296249625578, 'motion_component_percent_residue': 41.85296249625578, 'motion_component_percent_ionic': 10.754217173394629, 'ionic_contributions': [{'ion_id': 1306, 'distance': 9.401440620422363, 'force': [-1.9984097480773926, 2.8898801803588867, -1.3281662464141846], 'magnitude': 3.756204843521118, 'cosine_ionic_motion': -0.7739222645759583, 'motion_component_ionic': -2.907010555267334, 'motion_component_percent_ionic': 77.39222645759583}, {'ion_id': 1309, 'distance': 5.802047252655029, 'force': [2.848625421524048, -7.680440902709961, -5.491806507110596], 'magnitude': 9.862239837646484, 'cosine_ionic_motion': 0.3116365075111389, 'motion_component_ionic': 3.0734338760375977, 'motion_component_percent_ionic': 31.16365075111389}, {'ion_id': 1469, 'distance': 11.164752006530762, 'force': [1.1187093257904053, 2.1294939517974854, -1.1434855461120605], 'magnitude': 2.663421392440796, 'cosine_ionic_motion': 0.0896269828081131, 'motion_component_ionic': 0.23871442675590515, 'motion_component_percent_ionic': 8.96269828081131}, {'ion_id': 2443, 'distance': 14.983959197998047, 'force': [-0.03920864686369896, 0.29816392064094543, -1.4478132724761963], 'magnitude': 1.478716492652893, 'cosine_ionic_motion': -0.32803651690483093, 'motion_component_ionic': -0.4850730001926422, 'motion_component_percent_ionic': 32.80365169048309}, {'ion_id': 2444, 'distance': 9.266230583190918, 'force': [-0.14548905193805695, 1.0318454504013062, -3.7235605716705322], 'magnitude': 3.8666231632232666, 'cosine_ionic_motion': -0.34985432028770447, 'motion_component_ionic': -1.352754831314087, 'motion_component_percent_ionic': 34.98543202877045}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.346997261047363, 'force': [8.600956916809082, -8.802119255065918, 2.3395042419433594], 'magnitude': 12.527052879333496, 'cosine_with_motion': 0.8590721487998962, 'motion_component': 10.761642456054688, 'motion_component_percent': 85.90721487998962}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.540380477905273, 'force': [-4.551881313323975, 8.276850700378418, -1.4175502061843872], 'magnitude': 9.551718711853027, 'cosine_with_motion': -0.691868782043457, 'motion_component': -6.6085357666015625, 'motion_component_percent': 69.1868782043457}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.867973804473877, 'force': [-16.598386764526367, 11.808831214904785, 1.010152816772461], 'magnitude': 20.39547348022461, 'cosine_with_motion': -0.8869447112083435, 'motion_component': -18.089656829833984, 'motion_component_percent': 88.69447112083435}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.704692840576172, 'force': [7.034178733825684, -6.805782794952393, -2.6880531311035156], 'magnitude': 10.150073051452637, 'cosine_with_motion': 0.7397975921630859, 'motion_component': 7.508999824523926, 'motion_component_percent': 73.9797592163086}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.167927265167236, 'force': [7.445319175720215, -2.9503414630889893, -0.413440465927124], 'magnitude': 8.019241333007812, 'cosine_with_motion': 0.9430676698684692, 'motion_component': 7.562687397003174, 'motion_component_percent': 94.30676698684692}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.4427409172058105, 'force': [9.58101749420166, 2.6851537227630615, -2.6641883850097656], 'magnitude': 10.30067253112793, 'cosine_with_motion': 0.7402241826057434, 'motion_component': 7.624806880950928, 'motion_component_percent': 74.02241826057434}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.947059631347656, 'force': [-5.449575424194336, -0.5346041917800903, 1.554775595664978], 'magnitude': 5.692187786102295, 'cosine_with_motion': -0.801859438419342, 'motion_component': -4.564334392547607, 'motion_component_percent': 80.1859438419342}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.192211151123047, 'force': [-4.405142784118652, -2.161324977874756, 1.6201916933059692], 'magnitude': 5.167361736297607, 'cosine_with_motion': -0.6155733466148376, 'motion_component': -3.1808900833129883, 'motion_component_percent': 61.557334661483765}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.2475810050964355, 'force': [3.1203103065490723, 3.9733023643493652, 0.2624947130680084], 'magnitude': 5.058890342712402, 'cosine_with_motion': 0.4023629426956177, 'motion_component': 2.0355100631713867, 'motion_component_percent': 40.23629426956177}]}, 5479: {'frame': 5479, 'motion_vector': [-0.8315162658691406, 0.4536933898925781, 0.4904327392578125], 'ionic_force': [8.564183592796326, 7.061019524931908, -8.43285158276558], 'ionic_force_magnitude': 13.939735404933026, 'radial_force': 11.099695371612295, 'axial_force': -8.43285158276558, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [4.034980535507202, 0.3665037155151367, -0.8855640888214111], 'asn_force_magnitude': 4.147242053560231, 'residue_force': [4.034980535507202, 0.3665037155151367, -0.8855640888214111], 'residue_force_magnitude': 4.147242053560231, 'total_force': [12.599164128303528, 7.427523240447044, -9.31841567158699], 'total_force_magnitude': 17.341854250563557, 'cosine_total_motion': -0.6312381841571321, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.8190327924920568, 'cosine_residue_motion': -0.8190327924920568, 'cosine_ionic_motion': -0.5416252982896361, 'motion_component_total': -10.946840587043383, 'motion_component_glu': None, 'motion_component_asn': -3.3967272402679285, 'motion_component_residue': -3.3967272402679285, 'motion_component_ionic': -7.550113346775452, 'motion_component_percent_total': 63.12381841571321, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 81.90327924920568, 'motion_component_percent_residue': 81.90327924920568, 'motion_component_percent_ionic': 54.16252982896361, 'ionic_contributions': [{'ion_id': 1306, 'distance': 6.694813251495361, 'force': [0.8983935117721558, 7.096762180328369, -1.9228250980377197], 'magnitude': 7.407320976257324, 'cosine_ionic_motion': 0.19360578060150146, 'motion_component_ionic': 1.4341001510620117, 'motion_component_percent_ionic': 19.360578060150146}, {'ion_id': 1309, 'distance': 9.535407066345215, 'force': [2.8427734375, -2.1192972660064697, -0.8717526197433472], 'magnitude': 3.6514017581939697, 'cosine_ionic_motion': -0.9635478854179382, 'motion_component_ionic': -3.5183005332946777, 'motion_component_percent_ionic': 96.35478854179382}, {'ion_id': 1469, 'distance': 12.905256271362305, 'force': [1.5580865144729614, 1.1739774942398071, -0.4098491966724396], 'magnitude': 1.9934475421905518, 'cosine_ionic_motion': -0.4533369839191437, 'motion_component_ionic': -0.903703510761261, 'motion_component_percent_ionic': 45.33369839191437}, {'ion_id': 2443, 'distance': 13.859634399414062, 'force': [0.5962351560592651, 0.1816510409116745, -1.6120604276657104], 'magnitude': 1.7283612489700317, 'cosine_ionic_motion': -0.6530594229698181, 'motion_component_ionic': -1.1287225484848022, 'motion_component_percent_ionic': 65.30594229698181}, {'ion_id': 2444, 'distance': 8.539250373840332, 'force': [2.6686949729919434, 0.7279260754585266, -3.6163642406463623], 'magnitude': 4.553009986877441, 'cosine_ionic_motion': -0.7541136145591736, 'motion_component_ionic': -3.4334869384765625, 'motion_component_percent_ionic': 75.41136145591736}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.292919635772705, 'force': [-1.668077826499939, -11.140223503112793, 6.172342777252197], 'magnitude': 12.844643592834473, 'cosine_with_motion': -0.046718817204236984, 'motion_component': -0.6000865697860718, 'motion_component_percent': 4.671881720423698}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.100113868713379, 'force': [4.060624599456787, 8.442559242248535, -7.030838489532471], 'magnitude': 11.713162422180176, 'cosine_with_motion': -0.23965755105018616, 'motion_component': -2.807147741317749, 'motion_component_percent': 23.965755105018616}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.018746852874756, 'force': [-3.56195068359375, 16.02308464050293, -9.356781005859375], 'magnitude': 18.893810272216797, 'cosine_with_motion': 0.2799779772758484, 'motion_component': 5.28985071182251, 'motion_component_percent': 27.99779772758484}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.5947213172912598, 'force': [3.3128061294555664, -7.549646854400635, 6.946192741394043], 'magnitude': 10.78060531616211, 'cosine_with_motion': -0.24116507172584534, 'motion_component': -2.599905490875244, 'motion_component_percent': 24.116507172584534}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.737691879272461, 'force': [1.8915783166885376, -5.4092698097229, 2.3835198879241943], 'magnitude': 6.206402778625488, 'cosine_with_motion': -0.43172162771224976, 'motion_component': -2.679438352584839, 'motion_component_percent': 43.172162771224976}]}, 5480: {'frame': 5480, 'motion_vector': [-2.4467201232910156, 2.9426307678222656, 1.0514373779296875], 'ionic_force': [8.845621451735497, 5.174365371465683, -6.945133060216904], 'ionic_force_magnitude': 12.379577904312578, 'radial_force': 10.247881530581157, 'axial_force': -6.945133060216904, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [3.2695456594228745, 0.8918981552124023, -0.8600523471832275], 'asn_force_magnitude': 3.4964412161821947, 'residue_force': [3.2695456594228745, 0.8918981552124023, -0.8600523471832275], 'residue_force_magnitude': 3.4964412161821947, 'total_force': [12.115167111158371, 6.066263526678085, -7.805185407400131], 'total_force_magnitude': 15.636423713569872, 'cosine_total_motion': -0.32225627229800197, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.4525215385641118, 'cosine_residue_motion': -0.4525215385641118, 'cosine_ionic_motion': -0.2792276672177309, 'motion_component_total': -5.038935618007108, 'motion_component_glu': None, 'motion_component_asn': -1.582214958645741, 'motion_component_residue': -1.582214958645741, 'motion_component_ionic': -3.456720659361367, 'motion_component_percent_total': 32.225627229800196, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 45.252153856411184, 'motion_component_percent_residue': 45.252153856411184, 'motion_component_percent_ionic': 27.92276672177309, 'ionic_contributions': [{'ion_id': 1306, 'distance': 7.943610668182373, 'force': [0.21233676373958588, 5.167843818664551, -0.9647490382194519], 'magnitude': 5.261410236358643, 'cosine_ionic_motion': 0.6548050045967102, 'motion_component_ionic': 3.445197820663452, 'motion_component_percent_ionic': 65.48050045967102}, {'ion_id': 1309, 'distance': 7.917448043823242, 'force': [4.6044087409973145, -2.470323085784912, -0.8643374443054199], 'magnitude': 5.296239852905273, 'cosine_ionic_motion': -0.9250341057777405, 'motion_component_ionic': -4.899202346801758, 'motion_component_percent_ionic': 92.50341057777405}, {'ion_id': 1469, 'distance': 12.11471939086914, 'force': [1.6390438079833984, 1.4995357990264893, -0.4266315996646881], 'magnitude': 2.2620978355407715, 'cosine_ionic_motion': -0.005154735408723354, 'motion_component_ionic': -0.011660516262054443, 'motion_component_percent_ionic': 0.5154735408723354}, {'ion_id': 2443, 'distance': 13.938857078552246, 'force': [0.6318773031234741, 0.20215561985969543, -1.57472562789917], 'magnitude': 1.708770513534546, 'cosine_ionic_motion': -0.3843998610973358, 'motion_component_ionic': -0.6568511724472046, 'motion_component_percent_ionic': 38.43998610973358}, {'ion_id': 2444, 'distance': 9.524741172790527, 'force': [1.7579548358917236, 0.7751532196998596, -3.114689350128174], 'magnitude': 3.6595845222473145, 'cosine_ionic_motion': -0.3645781874656677, 'motion_component_ionic': -1.3342046737670898, 'motion_component_percent_ionic': 36.45781874656677}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.656192302703857, 'force': [-2.944319009780884, -7.897385597229004, 6.9409990310668945], 'magnitude': 10.918570518493652, 'cosine_with_motion': -0.20162712037563324, 'motion_component': -2.201479911804199, 'motion_component_percent': 20.162712037563324}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.206221103668213, 'force': [5.27993631362915, 6.390595436096191, -7.426429748535156], 'magnitude': 11.129658699035645, 'cosine_with_motion': -0.04350803419947624, 'motion_component': -0.48422956466674805, 'motion_component_percent': 4.350803419947624}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.523441314697266, 'force': [0.022058889269828796, 10.369463920593262, -10.717702865600586], 'magnitude': 14.912927627563477, 'cosine_with_motion': 0.3242422938346863, 'motion_component': 4.835402011871338, 'motion_component_percent': 32.42422938346863}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.082260608673096, 'force': [0.4331759512424469, -4.46119499206543, 7.056110858917236], 'magnitude': 8.359342575073242, 'cosine_with_motion': -0.20401525497436523, 'motion_component': -1.7054333686828613, 'motion_component_percent': 20.401525497436523}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.3692402839660645, 'force': [0.47869351506233215, -3.509580612182617, 3.286970376968384], 'magnitude': 4.83223295211792, 'cosine_with_motion': -0.4193660020828247, 'motion_component': -2.0264742374420166, 'motion_component_percent': 41.93660020828247}]}, 5481: {'frame': 5481, 'motion_vector': [1.9404220581054688, -4.451213836669922, 0.8924026489257812], 'ionic_force': [10.121144622564316, 6.428409576416016, -5.320772521197796], 'ionic_force_magnitude': 13.11764606838259, 'radial_force': 11.990079989433752, 'axial_force': -5.320772521197796, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-3.4476019144058228, -0.01515108346939087, 4.744694709777832], 'asn_force_magnitude': 5.865007792368117, 'residue_force': [-3.4476019144058228, -0.01515108346939087, 4.744694709777832], 'residue_force_magnitude': 5.865007792368117, 'total_force': [6.673542708158493, 6.413258492946625, -0.5760778114199638], 'total_force_magnitude': 9.273506479200725, 'cosine_total_motion': -0.351898422592414, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.08247598576067056, 'cosine_residue_motion': -0.08247598576067056, 'cosine_ionic_motion': -0.2118985363891906, 'motion_component_total': -3.263332301931266, 'motion_component_glu': None, 'motion_component_asn': -0.48372229916957465, 'motion_component_residue': -0.48372229916957465, 'motion_component_ionic': -2.7796100027616912, 'motion_component_percent_total': 35.1898422592414, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 8.247598576067055, 'motion_component_percent_residue': 8.247598576067055, 'motion_component_percent_ionic': 21.18985363891906, 'ionic_contributions': [{'ion_id': 1306, 'distance': 10.731383323669434, 'force': [-0.6012338399887085, 2.818525791168213, -0.07370224595069885], 'magnitude': 2.882880926132202, 'cosine_ionic_motion': -0.9680474400520325, 'motion_component_ionic': -2.7907655239105225, 'motion_component_percent_ionic': 96.80474400520325}, {'ion_id': 1309, 'distance': 6.173717498779297, 'force': [8.690352439880371, -0.589633584022522, -0.05870877951383591], 'magnitude': 8.710530281066895, 'cosine_ionic_motion': 0.45193034410476685, 'motion_component_ionic': 3.9365530014038086, 'motion_component_percent_ionic': 45.193034410476685}, {'ion_id': 1469, 'distance': 13.34061336517334, 'force': [0.9652875065803528, 1.5830146074295044, -0.20551034808158875], 'magnitude': 1.865462303161621, 'cosine_ionic_motion': -0.5816164612770081, 'motion_component_ionic': -1.0849835872650146, 'motion_component_percent_ionic': 58.161646127700806}, {'ion_id': 2443, 'distance': 12.948829650878906, 'force': [0.3752489387989044, 0.6354923248291016, -1.8373764753341675], 'magnitude': 1.9800541400909424, 'cosine_ionic_motion': -0.38260617852211, 'motion_component_ionic': -0.7575809359550476, 'motion_component_percent_ionic': 38.260617852211}, {'ion_id': 2444, 'distance': 9.370463371276855, 'force': [0.691489577293396, 1.9810104370117188, -3.145474672317505], 'magnitude': 3.781080722808838, 'cosine_ionic_motion': -0.5508565306663513, 'motion_component_ionic': -2.0828330516815186, 'motion_component_percent_ionic': 55.08565306663513}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.794651508331299, 'force': [-4.679443359375, -0.1746199131011963, 5.26983118057251], 'magnitude': 7.049737930297852, 'cosine_with_motion': -0.10343307256698608, 'motion_component': -0.7291760444641113, 'motion_component_percent': 10.343307256698608}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.264755725860596, 'force': [5.481466770172119, -0.6339924931526184, -9.52616024017334], 'magnitude': 11.008912086486816, 'cosine_with_motion': 0.09120580554008484, 'motion_component': 1.0040767192840576, 'motion_component_percent': 9.120580554008484}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.354150772094727, 'force': [-2.290189266204834, 1.1873915195465088, 4.1182475090026855], 'magnitude': 4.859508991241455, 'cosine_with_motion': -0.25234100222587585, 'motion_component': -1.2262533903121948, 'motion_component_percent': 25.234100222587585}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.138481616973877, 'force': [-1.959436058998108, -0.39393019676208496, 4.882776260375977], 'magnitude': 5.275990009307861, 'cosine_with_motion': 0.088633693754673, 'motion_component': 0.4676304757595062, 'motion_component_percent': 8.8633693754673}]}, 5483: {'frame': 5483, 'motion_vector': [-1.0512886047363281, -1.1198539733886719, -3.1050186157226562], 'ionic_force': [13.281899441033602, -1.611535370349884, -14.18665498495102], 'ionic_force_magnitude': 19.500437909792, 'radial_force': 13.379308614858147, 'axial_force': -14.18665498495102, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-1.1116523742675781, -0.5470233708620071, -1.6721093654632568], 'asn_force_magnitude': 2.081094735843112, 'residue_force': [-1.1116523742675781, -0.5470233708620071, -1.6721093654632568], 'residue_force_magnitude': 2.081094735843112, 'total_force': [12.170247066766024, -2.158558741211891, -15.858764350414276], 'total_force_magnitude': 20.106583405127783, 'cosine_total_motion': 0.5579785918087772, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.9672551795401328, 'cosine_residue_motion': 0.9672551795401328, 'cosine_ionic_motion': 0.47209675365793713, 'motion_component_total': 11.219043094478927, 'motion_component_glu': None, 'motion_component_asn': 2.0129496623579546, 'motion_component_residue': 2.0129496623579546, 'motion_component_ionic': 9.206093432120973, 'motion_component_percent_total': 55.797859180877715, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 96.72551795401328, 'motion_component_percent_residue': 96.72551795401328, 'motion_component_percent_ionic': 47.209675365793714, 'ionic_contributions': [{'ion_id': 1306, 'distance': 9.658601760864258, 'force': [-1.4231153726577759, 3.2190465927124023, -0.5271512866020203], 'magnitude': 3.5588490962982178, 'cosine_ionic_motion': -0.038280826061964035, 'motion_component_ionic': -0.13623568415641785, 'motion_component_percent_ionic': 3.8280826061964035}, {'ion_id': 1309, 'distance': 4.376565933227539, 'force': [12.95172119140625, -9.656329154968262, -6.279929161071777], 'magnitude': 17.332895278930664, 'cosine_ionic_motion': 0.27807921171188354, 'motion_component_ionic': 4.819917678833008, 'motion_component_percent_ionic': 27.807921171188354}, {'ion_id': 1469, 'distance': 10.299714088439941, 'force': [1.47786545753479, 2.6548736095428467, -0.7496045827865601], 'magnitude': 3.129592180252075, 'cosine_ionic_motion': -0.2028515338897705, 'motion_component_ionic': -0.634842574596405, 'motion_component_percent_ionic': 20.28515338897705}, {'ion_id': 2443, 'distance': 13.630022048950195, 'force': [0.023254413157701492, 0.36658936738967896, -1.7489255666732788], 'magnitude': 1.7870839834213257, 'cosine_ionic_motion': 0.8069254755973816, 'motion_component_ionic': 1.4420435428619385, 'motion_component_percent_ionic': 80.69254755973816}, {'ion_id': 2444, 'distance': 7.982741832733154, 'force': [0.2521737515926361, 1.8042842149734497, -4.881044387817383], 'magnitude': 5.209954738616943, 'cosine_ionic_motion': 0.7130983471870422, 'motion_component_ionic': 3.715210199356079, 'motion_component_percent_ionic': 71.30983471870422}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.441762924194336, 'force': [4.711716175079346, -1.0550556182861328, 6.370713233947754], 'magnitude': 7.993710041046143, 'cosine_with_motion': -0.8505513072013855, 'motion_component': -6.799060344696045, 'motion_component_percent': 85.05513072013855}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.3333330154418945, 'force': [-6.330883502960205, 0.2161678522825241, -8.356761932373047], 'magnitude': 10.48629093170166, 'cosine_with_motion': 0.890855610370636, 'motion_component': 9.341771125793457, 'motion_component_percent': 89.0855610370636}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.463705062866211, 'force': [7.841887474060059, 3.829061985015869, -5.322386741638184], 'magnitude': 10.221776008605957, 'cosine_with_motion': 0.11279423534870148, 'motion_component': 1.1529574394226074, 'motion_component_percent': 11.279423534870148}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.135146141052246, 'force': [-4.220770359039307, -1.072511911392212, 2.9905319213867188], 'magnitude': 5.282846450805664, 'cosine_with_motion': -0.19930197298526764, 'motion_component': -1.0528817176818848, 'motion_component_percent': 19.930197298526764}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.403172016143799, 'force': [-3.1136021614074707, -2.4646856784820557, 2.645794153213501], 'magnitude': 4.771731376647949, 'cosine_with_motion': -0.1319933980703354, 'motion_component': -0.6298370361328125, 'motion_component_percent': 13.199339807033539}]}, 5484: {'frame': 5484, 'motion_vector': [-1.2701416015625, -1.1113739013671875, -2.5788192749023438], 'ionic_force': [2.082847408950329, 0.5381690561771393, -11.26388955116272], 'ionic_force_magnitude': 11.467479543595898, 'radial_force': 2.151250627425287, 'axial_force': -11.26388955116272, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-5.776663586497307, -0.6191740036010742, -10.50797963142395], 'asn_force_magnitude': 12.007116830143692, 'residue_force': [-5.776663586497307, -0.6191740036010742, -10.50797963142395], 'residue_force_magnitude': 12.007116830143692, 'total_force': [-3.693816177546978, -0.08100494742393494, -21.77186918258667], 'total_force_magnitude': 22.083141249801443, 'cosine_total_motion': 0.8951984405102938, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.9491315711435183, 'cosine_residue_motion': 0.9491315711435183, 'cosine_ionic_motion': 0.7301046332512008, 'motion_component_total': 19.768793608390794, 'motion_component_glu': None, 'motion_component_asn': 11.396333661898064, 'motion_component_residue': 11.396333661898064, 'motion_component_ionic': 8.37245994649273, 'motion_component_percent_total': 89.51984405102938, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 94.91315711435183, 'motion_component_percent_residue': 94.91315711435183, 'motion_component_percent_ionic': 73.01046332512009, 'ionic_contributions': [{'ion_id': 1306, 'distance': 10.203856468200684, 'force': [-1.2755056619644165, 2.3901894092559814, -1.6815731525421143], 'magnitude': 3.188668727874756, 'cosine_ionic_motion': 0.33580875396728516, 'motion_component_ionic': 1.0707828998565674, 'motion_component_percent_ionic': 33.580875396728516}, {'ion_id': 1309, 'distance': 6.766260623931885, 'force': [2.1952145099639893, -4.486453056335449, -5.257387638092041], 'magnitude': 7.251713752746582, 'cosine_ionic_motion': 0.7049621343612671, 'motion_component_ionic': 5.112183570861816, 'motion_component_percent_ionic': 70.49621343612671}, {'ion_id': 1469, 'distance': 10.19710636138916, 'force': [1.2880535125732422, 2.27970814704895, -1.8271305561065674], 'magnitude': 3.1928915977478027, 'cosine_ionic_motion': 0.05510101839900017, 'motion_component_ionic': 0.17593157291412354, 'motion_component_percent_ionic': 5.510101839900017}, {'ion_id': 2444, 'distance': 11.46453857421875, 'force': [-0.12491495162248611, 0.35472455620765686, -2.497798204421997], 'magnitude': 2.5259511470794678, 'cosine_ionic_motion': 0.7971500754356384, 'motion_component_ionic': 2.0135622024536133, 'motion_component_percent_ionic': 79.71500754356384}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.298002004623413, 'force': [12.503654479980469, -1</t>
         </is>
       </c>
     </row>
@@ -707,7 +707,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>{5576: {'frame': 5576, 'ionic_force': [-5.12838389724493, -9.299570322036743, -7.61335426568985], 'ionic_force_magnitude': 13.066961878987996, 'motion_vector': [0.9404220581054688, -0.198822021484375, -0.6372222900390625], 'ionic_force_x': -5.12838389724493, 'ionic_force_y': -9.299570322036743, 'ionic_force_z': -7.61335426568985, 'radial_force': 10.619902521776162, 'axial_force': -7.61335426568985, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [1.534182071685791, -1.9800267219543457, -0.23618412017822266], 'asn_force_magnitude': 2.515949798259047, 'residue_force': [1.534182071685791, -1.9800267219543457, -0.23618412017822266], 'residue_force_magnitude': 2.515949798259047, 'total_force': [-3.5942018255591393, -11.279597043991089, -7.8495383858680725], 'total_force_magnitude': 14.204325014194849, 'motion_component_total': 3.350947342129791, 'cosine_total_motion': 0.23591035397888171, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.6848000184159503, 'cosine_residue_motion': 0.6848000184159503, 'cosine_ionic_motion': 0.12459092549786145, 'motion_component_glu': None, 'motion_component_asn': 1.7229224681814017, 'motion_component_residue': 1.7229224681814017, 'motion_component_ionic': 1.6280248739483891, 'ionic_contributions': [{'ion_id': 1309, 'distance': 6.352936267852783, 'force': [6.9591827392578125, -4.298310279846191, -0.8726447224617004], 'magnitude': 8.226007461547852}, {'ion_id': 1380, 'distance': 14.568533897399902, 'force': [-0.09576242417097092, -0.6451082229614258, -1.4218106269836426], 'magnitude': 1.5642507076263428}, {'ion_id': 1469, 'distance': 5.2329535484313965, 'force': [-11.656188011169434, -2.1556320190429688, -2.5449581146240234], 'magnitude': 12.123954772949219}, {'ion_id': 2443, 'distance': 9.661603927612305, 'force': [-0.33561620116233826, -2.2005198001861572, -2.7739408016204834], 'magnitude': 3.55663800239563}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.452768325805664, 'force': [-4.987297534942627, -3.4656054973602295, 5.147963047027588], 'magnitude': 7.961474895477295}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.264543056488037, 'force': [6.568163871765137, 4.007881164550781, -7.6175456047058105], 'magnitude': 10.82732105255127}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.885590553283691, 'force': [-1.3890328407287598, -2.6289796829223633, 2.707751750946045], 'magnitude': 4.021550178527832}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.840651512145996, 'force': [4.195528984069824, -3.768968105316162, 4.042763710021973], 'magnitude': 6.939129829406738}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.461941719055176, 'force': [-2.853180408477783, 3.875645399093628, -4.517117023468018], 'magnitude': 6.6004252433776855}]}, 5577: {'frame': 5577, 'ionic_force': [-5.55037547647953, -9.919090867042542, -9.448231399059296], 'ionic_force_magnitude': 14.780531388577412, 'motion_vector': [1.2938232421875, 4.777435302734375, -1.3350448608398438], 'ionic_force_x': -5.55037547647953, 'ionic_force_y': -9.919090867042542, 'ionic_force_z': -9.448231399059296, 'radial_force': 11.366399234522433, 'axial_force': -9.448231399059296, 'glu_force': [7.344610214233398, -0.7519962191581726, 2.9800832271575928], 'glu_force_magnitude': 7.961764474878402, 'asn_force': [-0.9773849248886108, 5.0761494636535645, -9.112831115722656], 'asn_force_magnitude': 10.47693970644257, 'residue_force': [6.367225289344788, 4.324153244495392, -6.1327478885650635], 'residue_force_magnitude': 9.841262918541048, 'total_force': [0.8168498128652573, -5.59493762254715, -15.58097928762436], 'total_force_magnitude': 16.57520697241367, 'motion_component_total': -0.9502310940700767, 'cosine_total_motion': -0.05732846025099768, 'cosine_glu_motion': 0.04732209463631694, 'cosine_asn_motion': 0.6544955989926504, 'cosine_residue_motion': 0.7350558927860334, 'cosine_ionic_motion': -0.5537087388566516, 'motion_component_glu': 0.37676737195226195, 'motion_component_asn': 6.857110928778013, 'motion_component_residue': 7.233878300730275, 'motion_component_ionic': -8.184109394800352, 'ionic_contributions': [{'ion_id': 1309, 'distance': 7.8708953857421875, 'force': [4.450619697570801, -1.8525863885879517, -2.3408517837524414], 'magnitude': 5.359074592590332}, {'ion_id': 1469, 'distance': 5.398885250091553, 'force': [-9.812492370605469, -4.156482219696045, -4.021743297576904], 'magnitude': 11.39016056060791}, {'ion_id': 2434, 'distance': 13.089409828186035, 'force': [-0.3545006811618805, -1.8371081352233887, -0.5042237639427185], 'magnitude': 1.9377509355545044}, {'ion_id': 2443, 'distance': 10.007767677307129, 'force': [0.16599787771701813, -2.0729141235351562, -2.5814125537872314], 'magnitude': 3.3148481845855713}], 'glu_contributions': [{'resid': 748, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 5.843234062194824, 'force': [7.344610214233398, -0.7519962191581726, 2.9800832271575928], 'magnitude': 7.961764335632324}], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.415275573730469, 'force': [-6.848346710205078, -7.028812408447266, 7.151146411895752], 'magnitude': 12.142608642578125}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.4983105659484863, 'force': [7.741075038909912, 7.512360095977783, -11.93818473815918], 'magnitude': 16.089750289916992}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.94879150390625, 'force': [5.295975208282471, 9.519482612609863, -6.047527313232422], 'magnitude': 12.459554672241211}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.810720920562744, 'force': [-1.3970375061035156, -4.888218402862549, 3.2228546142578125], 'magnitude': 6.019400596618652}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.8562092781066895, 'force': [-1.8843098878860474, -3.1789588928222656, 1.6862621307373047], 'magnitude': 4.062005043029785}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.764595985412598, 'force': [-3.8847410678863525, 3.140296459197998, -3.187382221221924], 'magnitude': 5.925544738769531}]}, 5578: {'frame': 5578, 'ionic_force': [1.3535993099212646, 2.408291459083557, -11.13271152973175], 'ionic_force_magnitude': 11.470368993538804, 'motion_vector': [-3.8603553771972656, 0.4764251708984375, -2.4455490112304688], 'ionic_force_x': 1.3535993099212646, 'ionic_force_y': 2.408291459083557, 'ionic_force_z': -11.13271152973175, 'radial_force': 2.762625353484278, 'axial_force': -11.13271152973175, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-8.662565410137177, -2.981669306755066, 1.2691880613565445], 'asn_force_magnitude': 9.248850181230113, 'residue_force': [-8.662565410137177, -2.981669306755066, 1.2691880613565445], 'residue_force_magnitude': 9.248850181230113, 'total_force': [-7.308966100215912, -0.5733778476715088, -9.863523468375206], 'total_force_magnitude': 12.28978611780914, 'motion_component_total': 11.331596335961567, 'cosine_total_motion': 0.9220336487012529, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.6804694713337368, 'cosine_residue_motion': 0.6804694713337368, 'cosine_ionic_motion': 0.43922180232674957, 'motion_component_glu': None, 'motion_component_asn': 6.2935601932665906, 'motion_component_residue': 6.2935601932665906, 'motion_component_ionic': 5.038036142694978, 'ionic_contributions': [{'ion_id': 1309, 'distance': 8.761899948120117, 'force': [3.6393582820892334, 1.2222265005111694, -1.990733027458191], 'magnitude': 4.32455587387085}, {'ion_id': 1469, 'distance': 7.00886344909668, 'force': [-2.00545072555542, 5.622910022735596, -3.1680915355682373], 'magnitude': 6.7583842277526855}, {'ion_id': 2434, 'distance': 8.5108642578125, 'force': [-1.0407629013061523, -3.8392817974090576, -2.276965618133545], 'magnitude': 4.583431720733643}, {'ion_id': 2443, 'distance': 9.320978164672852, 'force': [0.7604546546936035, -0.5975632667541504, -3.6969213485717773], 'magnitude': 3.8213350772857666}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.739819526672363, 'force': [-2.376432180404663, -3.4947781562805176, 0.136177197098732], 'magnitude': 4.228409767150879}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.699294567108154, 'force': [-4.322408199310303, 9.774972915649414, 0.8172364830970764], 'magnitude': 10.719197273254395}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.974052429199219, 'force': [3.2886385917663574, -7.10646390914917, 1.4229737520217896], 'magnitude': 7.9587578773498535}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.528311252593994, 'force': [2.427645683288574, -14.384419441223145, -2.9385924339294434], 'magnitude': 14.880870819091797}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.446437358856201, 'force': [0.21913164854049683, 7.014721393585205, 0.6271215081214905], 'magnitude': 7.046106338500977}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.214537620544434, 'force': [-1.29389488697052, 7.04803991317749, 3.1876654624938965], 'magnitude': 7.842846393585205}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.252894401550293, 'force': [-6.605246067047119, -1.8337420225143433, -1.983393907546997], 'magnitude': 7.136227130889893}]}, 5579: {'frame': 5579, 'ionic_force': [-1.6814625263214111, 1.4262338280677795, -10.292737245559692], 'ionic_force_magnitude': 10.526248104898524, 'motion_vector': [2.0666732788085938, -1.3358840942382812, 0.7496261596679688], 'ionic_force_x': -1.6814625263214111, 'ionic_force_y': 1.4262338280677795, 'ionic_force_z': -10.292737245559692, 'radial_force': 2.20487168781951, 'axial_force': -10.292737245559692, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [5.065872430801392, -10.121050894260406, 7.583192825317383], 'asn_force_magnitude': 13.623639312434397, 'residue_force': [5.065872430801392, -10.121050894260406, 7.583192825317383], 'residue_force_magnitude': 13.623639312434397, 'total_force': [3.3844099044799805, -8.694817066192627, -2.7095444202423096], 'total_force_magnitude': 9.71574522007257, 'motion_component_total': 6.444589885188144, 'cosine_total_motion': 0.6633140062044574, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.846719535473441, 'cosine_residue_motion': 0.846719535473441, 'cosine_ionic_motion': -0.48363021792398614, 'motion_component_glu': None, 'motion_component_asn': 11.535401550082163, 'motion_component_residue': 11.535401550082163, 'motion_component_ionic': -5.090811664894019, 'ionic_contributions': [{'ion_id': 1309, 'distance': 8.065214157104492, 'force': [2.5060808658599854, 1.78612220287323, -4.071807861328125], 'magnitude': 5.103948593139648}, {'ion_id': 1469, 'distance': 9.613414764404297, 'force': [-2.498354911804199, 1.540704369544983, -2.071153163909912], 'magnitude': 3.592384099960327}, {'ion_id': 2434, 'distance': 11.22485637664795, 'force': [-1.2354334592819214, -1.6161770820617676, -1.6747441291809082], 'magnitude': 2.634974718093872}, {'ion_id': 2443, 'distance': 11.450145721435547, 'force': [-0.4537550210952759, -0.28441566228866577, -2.475032091140747], 'magnitude': 2.5323052406311035}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.995687961578369, 'force': [-0.5305469036102295, 7.846015930175781, -0.6404566764831543], 'magnitude': 7.889970302581787}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.552929878234863, 'force': [5.089491844177246, -3.5420284271240234, 1.5266737937927246], 'magnitude': 6.385892868041992}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.397833824157715, 'force': [10.111968994140625, -2.2511208057403564, 1.53609037399292], 'magnitude': 10.47277545928955}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.456086158752441, 'force': [-6.790855884552002, 1.110723853111267, -1.3673229217529297], 'magnitude': 7.015625476837158}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.294404983520508, 'force': [16.978822708129883, 10.63389778137207, -8.622949600219727], 'magnitude': 21.810901641845703}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.6203229427337646, 'force': [-15.075602531433105, -19.17746353149414, 15.08002758026123], 'magnitude': 28.678495407104492}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.340435266494751, 'force': [-25.120458602905273, -3.575512170791626, 10.197306632995605], 'magnitude': 27.34605598449707}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.000636100769043, 'force': [13.117599487304688, -1.9181121587753296, -7.977011203765869], 'magnitude': 15.472015380859375}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.27207088470459, 'force': [7.2854533195495605, 0.7525486350059509, -2.149165153503418], 'magnitude': 7.633025169372559}]}, 5580: {'frame': 5580, 'ionic_force': [-0.7721650202292949, 0.8433377742767334, -11.557860493659973], 'ionic_force_magnitude': 11.614284162654782, 'motion_vector': [-1.6046180725097656, 1.9312629699707031, -1.8199996948242188], 'ionic_force_x': -0.7721650202292949, 'ionic_force_y': 0.8433377742767334, 'ionic_force_z': -11.557860493659973, 'radial_force': 1.1434410435119695, 'axial_force': -11.557860493659973, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-3.86629581451416, -10.708865348249674, 3.0412516593933105], 'asn_force_magnitude': 11.784619299240637, 'residue_force': [-3.86629581451416, -10.708865348249674, 3.0412516593933105], 'residue_force_magnitude': 11.784619299240637, 'total_force': [-4.638460834743455, -9.86552757397294, -8.516608834266663], 'total_force_magnitude': 13.833892411905563, 'motion_component_total': 1.254466118825686, 'cosine_total_motion': 0.09068063285977865, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.5476116662464738, 'cosine_residue_motion': -0.5476116662464738, 'cosine_ionic_motion': 0.6636535684349356, 'motion_component_glu': None, 'motion_component_asn': -6.453395010537518, 'motion_component_residue': -6.453395010537518, 'motion_component_ionic': 7.707861129363204, 'ionic_contributions': [{'ion_id': 1309, 'distance': 8.492998123168945, 'force': [3.384483575820923, 0.7182776927947998, -3.0355429649353027], 'magnitude': 4.60273551940918}, {'ion_id': 1469, 'distance': 7.310606479644775, 'force': [-3.7529938220977783, 2.630032777786255, -4.193670749664307], 'magnitude': 6.211997032165527}, {'ion_id': 2434, 'distance': 11.535965919494629, 'force': [-0.40012770891189575, -1.974854826927185, -1.4709564447402954], 'magnitude': 2.494767904281616}, {'ion_id': 2443, 'distance': 10.687788963317871, 'force': [-0.0035270650405436754, -0.5301178693771362, -2.8576903343200684], 'magnitude': 2.9064464569091797}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.049490451812744, 'force': [-9.586258888244629, 10.096769332885742, -3.8128442764282227], 'magnitude': 14.435335159301758}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.8729913234710693, 'force': [14.967676162719727, -17.172510147094727, 7.083902835845947], 'magnitude': 23.855985641479492}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.991913795471191, 'force': [5.9453511238098145, -9.965107917785645, 3.910872220993042], 'magnitude': 12.245223045349121}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.011364459991455, 'force': [-1.706739902496338, 4.78489351272583, -2.227449655532837], 'magnitude': 5.547044277191162}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.914214611053467, 'force': [-2.1904101371765137, 3.107361078262329, -1.1867775917053223], 'magnitude': 3.9827163219451904}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.108897686004639, 'force': [13.608816146850586, 2.2836806774139404, -2.4842469692230225], 'magnitude': 14.0209321975708}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.94612455368042, 'force': [-22.468996047973633, -2.854041337966919, 1.2911922931671143], 'magnitude': 22.68630599975586}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.816590785980225, 'force': [-12.67530345916748, 0.8918702602386475, 3.397038459777832], 'magnitude': 13.152894020080566}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.553234100341797, 'force': [6.23122501373291, -1.8331278562545776, -1.721178650856018], 'magnitude': 6.719448089599609}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.768090724945068, 'force': [4.0083441734313965, -0.048652950674295425, -1.2092570066452026], 'magnitude': 4.187062740325928}]}, 5581: {'frame': 5581, 'ionic_force': [-1.0563013553619385, 1.5127899050712585, -8.483844637870789], 'ionic_force_magnitude': 8.682161348981825, 'motion_vector': [0.801727294921875, 2.2831573486328125, -1.9393539428710938], 'ionic_force_x': -1.0563013553619385, 'ionic_force_y': 1.5127899050712585, 'ionic_force_z': -8.483844637870789, 'radial_force': 1.8450761096022505, 'axial_force': -8.483844637870789, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-4.091072916984558, -0.5949215888977051, 7.045930489897728], 'asn_force_magnitude': 8.169207169456016, 'residue_force': [-4.091072916984558, -0.5949215888977051, 7.045930489897728], 'residue_force_magnitude': 8.169207169456016, 'total_force': [-5.147374272346497, 0.9178683161735535, -1.4379141479730606], 'total_force_magnitude': 5.422687640127448, 'motion_component_total': 0.2442610229680886, 'cosine_total_motion': 0.04504427309450334, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.7224783062472008, 'cosine_residue_motion': -0.7224783062472008, 'cosine_ionic_motion': 0.7079269475750936, 'motion_component_glu': None, 'motion_component_asn': -5.902074959171071, 'motion_component_residue': -5.902074959171071, 'motion_component_ionic': 6.14633598213916, 'ionic_contributions': [{'ion_id': 1309, 'distance': 9.217119216918945, 'force': [1.5847398042678833, 1.608560562133789, -3.1895318031311035], 'magnitude': 3.907938003540039}, {'ion_id': 1469, 'distance': 10.581854820251465, 'force': [-1.8289650678634644, 1.3348606824874878, -1.9141175746917725], 'magnitude': 2.964930534362793}, {'ion_id': 2434, 'distance': 13.097936630249023, 'force': [-0.5441734194755554, -1.361169457435608, -1.2634094953536987], 'magnitude': 1.9352288246154785}, {'ion_id': 2443, 'distance': 12.470683097839355, 'force': [-0.267902672290802, -0.0694618821144104, -2.116785764694214], 'magnitude': 2.1348018646240234}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.14915132522583, 'force': [1.1958789825439453, -13.484228134155273, -2.4111251831054688], 'magnitude': 13.750202178955078}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.0121681690216064, 'force': [-5.087360382080078, 20.721418380737305, 3.9667885303497314], 'magnitude': 21.702392578125}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.44619083404541, 'force': [2.8244411945343018, 15.098342895507812, 1.5236696004867554], 'magnitude': 15.435640335083008}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.8720946311950684, 'force': [-3.347208261489868, -8.666054725646973, -0.16123293340206146], 'magnitude': 9.291410446166992}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.43958044052124, 'force': [-1.0241671800613403, -4.57720422744751, -0.4076673090457916], 'magnitude': 4.708068370819092}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.308557987213135, 'force': [5.8510541915893555, -3.5571577548980713, 1.3910175561904907], 'magnitude': 6.9873552322387695}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.618579864501953, 'force': [-2.400791883468628, 3.0406863689422607, -2.1127662658691406], 'magnitude': 4.412862777709961}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.9893813133239746, 'force': [9.230582237243652, 8.277998924255371, -8.21556282043457], 'magnitude': 14.873614311218262}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.9905595779418945, 'force': [-10.00835132598877, -14.792145729064941, 12.875567436218262], 'magnitude': 22.01715087890625}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.267385005950928, 'force': [-12.618948936462402, -4.7344818115234375, 9.955862998962402], 'magnitude': 16.756263732910156}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.767609119415283, 'force': [7.267451763153076, 0.753171443939209, -6.552069187164307], 'magnitude': 9.813905715942383}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.234805583953857, 'force': [4.026346683502197, 1.324732780456543, -2.806551933288574], 'magnitude': 5.08361291885376}]}, 5582: {'frame': 5582, 'ionic_force': [-0.011387579143047333, 0.7488982081413269, -5.534487962722778], 'ionic_force_magnitude': 5.584938246090046, 'motion_vector': [1.6045913696289062, -2.307353973388672, -3.4020919799804688], 'ionic_force_x': -0.011387579143047333, 'ionic_force_y': 0.7488982081413269, 'ionic_force_z': -5.534487962722778, 'radial_force': 0.7489847816317962, 'axial_force': -5.534487962722778, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-7.578532576560974, 7.799448370933533, 8.200879573822021], 'asn_force_magnitude': 13.620571819464296, 'residue_force': [-7.578532576560974, 7.799448370933533, 8.200879573822021], 'residue_force_magnitude': 13.620571819464296, 'total_force': [-7.5899201557040215, 8.54834657907486, 2.666391611099243], 'total_force_magnitude': 11.738430961149936, 'motion_component_total': -9.285276102306533, 'cosine_total_motion': -0.7910150967397193, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.9659226805711397, 'cosine_residue_motion': -0.9659226805711397, 'cosine_ionic_motion': 0.6931398289268983, 'motion_component_glu': None, 'motion_component_asn': -13.156419242768678, 'motion_component_residue': -13.156419242768678, 'motion_component_ionic': 3.871143140462146, 'ionic_contributions': [{'ion_id': 1306, 'distance': 14.375834465026855, 'force': [0.44565045833587646, 0.22126013040542603, 1.527474284172058], 'magnitude': 1.606467604637146}, {'ion_id': 1309, 'distance': 11.71274471282959, 'force': [0.9512708783149719, 0.9681544303894043, -2.003573179244995], 'magnitude': 2.420029878616333}, {'ion_id': 1469, 'distance': 12.449092864990234, 'force': [-1.059220314025879, 0.999154806137085, -1.5712475776672363], 'magnitude': 2.1422131061553955}, {'ion_id': 2434, 'distance': 11.498509407043457, 'force': [-0.2705686688423157, -1.578347086906433, -1.934159755706787], 'magnitude': 2.511047840118408}, {'ion_id': 2443, 'distance': 14.58305549621582, 'force': [-0.07851993292570114, 0.13867592811584473, -1.5529817342758179], 'magnitude': 1.5611369609832764}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.8710620403289795, 'force': [6.05463171005249, -10.261305809020996, -10.372265815734863], 'magnitude': 15.796735763549805}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.6831188201904297, 'force': [-12.05867862701416, 18.463668823242188, 16.180330276489258], 'magnitude': 27.351816177368164}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.444665908813477, 'force': [-1.9319086074829102, 9.833566665649414, 11.753928184509277], 'magnitude': 15.446233749389648}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.170926570892334, 'force': [-0.7441778182983398, -4.746197700500488, -6.406501770019531], 'magnitude': 8.007712364196777}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.4331183433532715, 'force': [0.7702282667160034, -2.924844264984131, -3.6226491928100586], 'magnitude': 4.719274520874023}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.806340217590332, 'force': [-1.9977385997772217, -4.124251365661621, 3.621154546737671], 'magnitude': 5.840648174285889}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.849514007568359, 'force': [2.329111099243164, 1.5588120222091675, -2.9531166553497314], 'magnitude': 4.071308135986328}]}}</t>
+          <t>{5576: {'frame': 5576, 'motion_vector': [0.9404220581054688, -0.198822021484375, -0.6372222900390625], 'ionic_force': [-5.12838389724493, -9.299570322036743, -7.61335426568985], 'ionic_force_magnitude': 13.066961878987996, 'radial_force': 10.619902521776162, 'axial_force': -7.61335426568985, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [1.534182071685791, -1.9800267219543457, -0.23618412017822266], 'asn_force_magnitude': 2.515949798259047, 'residue_force': [1.534182071685791, -1.9800267219543457, -0.23618412017822266], 'residue_force_magnitude': 2.515949798259047, 'total_force': [-3.5942018255591393, -11.279597043991089, -7.8495383858680725], 'total_force_magnitude': 14.204325014194849, 'cosine_total_motion': 0.23591035397888171, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.6848000184159503, 'cosine_residue_motion': 0.6848000184159503, 'cosine_ionic_motion': 0.12459092549786145, 'motion_component_total': 3.350947342129791, 'motion_component_glu': None, 'motion_component_asn': 1.7229224681814017, 'motion_component_residue': 1.7229224681814017, 'motion_component_ionic': 1.6280248739483891, 'motion_component_percent_total': 23.59103539788817, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 68.48000184159503, 'motion_component_percent_residue': 68.48000184159503, 'motion_component_percent_ionic': 12.459092549786146, 'ionic_contributions': [{'ion_id': 1309, 'distance': 6.352936267852783, 'force': [6.9591827392578125, -4.298310279846191, -0.8726447224617004], 'magnitude': 8.226007461547852, 'cosine_ionic_motion': 0.8385752439498901, 'motion_component_ionic': 6.898126125335693, 'motion_component_percent_ionic': 83.85752439498901}, {'ion_id': 1380, 'distance': 14.568533897399902, 'force': [-0.09576242417097092, -0.6451082229614258, -1.4218106269836426], 'magnitude': 1.5642507076263428, 'cosine_ionic_motion': 0.5234101414680481, 'motion_component_ionic': 0.8187447190284729, 'motion_component_percent_ionic': 52.34101414680481}, {'ion_id': 1469, 'distance': 5.2329535484313965, 'force': [-11.656188011169434, -2.1556320190429688, -2.5449581146240234], 'magnitude': 12.123954772949219, 'cosine_ionic_motion': -0.6373556852340698, 'motion_component_ionic': -7.727271556854248, 'motion_component_percent_ionic': 63.73556852340698}, {'ion_id': 2443, 'distance': 9.661603927612305, 'force': [-0.33561620116233826, -2.2005198001861572, -2.7739408016204834], 'magnitude': 3.55663800239563, 'cosine_ionic_motion': 0.4606669843196869, 'motion_component_ionic': 1.6384257078170776, 'motion_component_percent_ionic': 46.06669843196869}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.452768325805664, 'force': [-4.987297534942627, -3.4656054973602295, 5.147963047027588], 'magnitude': 7.961474895477295, 'cosine_with_motion': -0.7930613160133362, 'motion_component': -6.313937664031982, 'motion_component_percent': 79.30613160133362}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.264543056488037, 'force': [6.568163871765137, 4.007881164550781, -7.6175456047058105], 'magnitude': 10.82732105255127, 'cosine_with_motion': 0.8196058869361877, 'motion_component': 8.874135971069336, 'motion_component_percent': 81.96058869361877}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.885590553283691, 'force': [-1.3890328407287598, -2.6289796829223633, 2.707751750946045], 'magnitude': 4.021550178527832, 'cosine_with_motion': -0.5409888625144958, 'motion_component': -2.1756138801574707, 'motion_component_percent': 54.098886251449585}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.840651512145996, 'force': [4.195528984069824, -3.768968105316162, 4.042763710021973], 'magnitude': 6.939129829406738, 'cosine_with_motion': 0.26476433873176575, 'motion_component': 1.8372341394424438, 'motion_component_percent': 26.476433873176575}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.461941719055176, 'force': [-2.853180408477783, 3.875645399093628, -4.517117023468018], 'magnitude': 6.6004252433776855, 'cosine_with_motion': -0.07558543235063553, 'motion_component': -0.4988960027694702, 'motion_component_percent': 7.558543235063553}]}, 5577: {'frame': 5577, 'motion_vector': [1.2938232421875, 4.777435302734375, -1.3350448608398438], 'ionic_force': [-5.55037547647953, -9.919090867042542, -9.448231399059296], 'ionic_force_magnitude': 14.780531388577412, 'radial_force': 11.366399234522433, 'axial_force': -9.448231399059296, 'glu_force': [7.344610214233398, -0.7519962191581726, 2.9800832271575928], 'glu_force_magnitude': 7.961764474878402, 'asn_force': [-0.9773849248886108, 5.0761494636535645, -9.112831115722656], 'asn_force_magnitude': 10.47693970644257, 'residue_force': [6.367225289344788, 4.324153244495392, -6.1327478885650635], 'residue_force_magnitude': 9.841262918541048, 'total_force': [0.8168498128652573, -5.59493762254715, -15.58097928762436], 'total_force_magnitude': 16.57520697241367, 'cosine_total_motion': -0.05732846025099768, 'cosine_glu_motion': 0.04732209463631694, 'cosine_asn_motion': 0.6544955989926504, 'cosine_residue_motion': 0.7350558927860334, 'cosine_ionic_motion': -0.5537087388566516, 'motion_component_total': -0.9502310940700767, 'motion_component_glu': 0.37676737195226195, 'motion_component_asn': 6.857110928778013, 'motion_component_residue': 7.233878300730275, 'motion_component_ionic': -8.184109394800352, 'motion_component_percent_total': 5.732846025099768, 'motion_component_percent_glu': 4.732209463631694, 'motion_component_percent_asn': 65.44955989926504, 'motion_component_percent_residue': 73.50558927860334, 'motion_component_percent_ionic': 55.37087388566516, 'ionic_contributions': [{'ion_id': 1309, 'distance': 7.8708953857421875, 'force': [4.450619697570801, -1.8525863885879517, -2.3408517837524414], 'magnitude': 5.359074592590332, 'cosine_ionic_motion': 0.0011955687077715993, 'motion_component_ionic': 0.00640714168548584, 'motion_component_percent_ionic': 0.11955687077715993}, {'ion_id': 1469, 'distance': 5.398885250091553, 'force': [-9.812492370605469, -4.156482219696045, -4.021743297576904], 'magnitude': 11.39016056060791, 'cosine_ionic_motion': -0.4655486047267914, 'motion_component_ionic': -5.30267333984375, 'motion_component_percent_ionic': 46.55486047267914}, {'ion_id': 2434, 'distance': 13.089409828186035, 'force': [-0.3545006811618805, -1.8371081352233887, -0.5042237639427185], 'magnitude': 1.9377509355545044, 'cosine_ionic_motion': -0.861928403377533, 'motion_component_ionic': -1.670202612876892, 'motion_component_percent_ionic': 86.1928403377533}, {'ion_id': 2443, 'distance': 10.007767677307129, 'force': [0.16599787771701813, -2.0729141235351562, -2.5814125537872314], 'magnitude': 3.3148481845855713, 'cosine_ionic_motion': -0.3673291504383087, 'motion_component_ionic': -1.2176403999328613, 'motion_component_percent_ionic': 36.73291504383087}], 'glu_contributions': [{'resid': 748, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 5.843234062194824, 'force': [7.344610214233398, -0.7519962191581726, 2.9800832271575928], 'magnitude': 7.961764335632324, 'cosine_with_motion': 0.04732208326458931, 'motion_component': 0.37676727771759033, 'motion_component_percent': 4.732208326458931}], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.415275573730469, 'force': [-6.848346710205078, -7.028812408447266, 7.151146411895752], 'magnitude': 12.142608642578125, 'cosine_with_motion': -0.8351629376411438, 'motion_component': -10.141057014465332, 'motion_component_percent': 83.51629376411438}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.4983105659484863, 'force': [7.741075038909912, 7.512360095977783, -11.93818473815918], 'magnitude': 16.089750289916992, 'cosine_with_motion': 0.749772846698761, 'motion_component': 12.063657760620117, 'motion_component_percent': 74.9772846698761}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.94879150390625, 'force': [5.295975208282471, 9.519482612609863, -6.047527313232422], 'magnitude': 12.459554672241211, 'cosine_with_motion': 0.945697546005249, 'motion_component': 11.782970428466797, 'motion_component_percent': 94.5697546005249}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.810720920562744, 'force': [-1.3970375061035156, -4.888218402862549, 3.2228546142578125], 'magnitude': 6.019400596618652, 'cosine_with_motion': -0.9548035264015198, 'motion_component': -5.747344970703125, 'motion_component_percent': 95.48035264015198}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.8562092781066895, 'force': [-1.8843098878860474, -3.1789588928222656, 1.6862621307373047], 'magnitude': 4.062005043029785, 'cosine_with_motion': -0.9545184969902039, 'motion_component': -3.8772590160369873, 'motion_component_percent': 95.45184969902039}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.764595985412598, 'force': [-3.8847410678863525, 3.140296459197998, -3.187382221221924], 'magnitude': 5.925544738769531, 'cosine_with_motion': 0.4685046076774597, 'motion_component': 2.7761449813842773, 'motion_component_percent': 46.85046076774597}]}, 5578: {'frame': 5578, 'motion_vector': [-3.8603553771972656, 0.4764251708984375, -2.4455490112304688], 'ionic_force': [1.3535993099212646, 2.408291459083557, -11.13271152973175], 'ionic_force_magnitude': 11.470368993538804, 'radial_force': 2.762625353484278, 'axial_force': -11.13271152973175, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-8.662565410137177, -2.981669306755066, 1.2691880613565445], 'asn_force_magnitude': 9.248850181230113, 'residue_force': [-8.662565410137177, -2.981669306755066, 1.2691880613565445], 'residue_force_magnitude': 9.248850181230113, 'total_force': [-7.308966100215912, -0.5733778476715088, -9.863523468375206], 'total_force_magnitude': 12.28978611780914, 'cosine_total_motion': 0.9220336487012529, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.6804694713337368, 'cosine_residue_motion': 0.6804694713337368, 'cosine_ionic_motion': 0.43922180232674957, 'motion_component_total': 11.331596335961567, 'motion_component_glu': None, 'motion_component_asn': 6.2935601932665906, 'motion_component_residue': 6.2935601932665906, 'motion_component_ionic': 5.038036142694978, 'motion_component_percent_total': 92.2033648701253, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 68.04694713337368, 'motion_component_percent_residue': 68.04694713337368, 'motion_component_percent_ionic': 43.922180232674954, 'ionic_contributions': [{'ion_id': 1309, 'distance': 8.761899948120117, 'force': [3.6393582820892334, 1.2222265005111694, -1.990733027458191], 'magnitude': 4.32455587387085, 'cosine_ionic_motion': -0.4327487051486969, 'motion_component_ionic': -1.8714460134506226, 'motion_component_percent_ionic': 43.27487051486969}, {'ion_id': 1469, 'distance': 7.00886344909668, 'force': [-2.00545072555542, 5.622910022735596, -3.1680915355682373], 'magnitude': 6.7583842277526855, 'cosine_ionic_motion': 0.5850980281829834, 'motion_component_ionic': 3.954317331314087, 'motion_component_percent_ionic': 58.50980281829834}, {'ion_id': 2434, 'distance': 8.5108642578125, 'force': [-1.0407629013061523, -3.8392817974090576, -2.276965618133545], 'magnitude': 4.583431720733643, 'cosine_ionic_motion': 0.3683488965034485, 'motion_component_ionic': 1.6883020401000977, 'motion_component_percent_ionic': 36.83488965034485}, {'ion_id': 2443, 'distance': 9.320978164672852, 'force': [0.7604546546936035, -0.5975632667541504, -3.6969213485717773], 'magnitude': 3.8213350772857666, 'cosine_ionic_motion': 0.3315235376358032, 'motion_component_ionic': 1.2668625116348267, 'motion_component_percent_ionic': 33.15235376358032}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.739819526672363, 'force': [-2.376432180404663, -3.4947781562805176, 0.136177197098732], 'magnitude': 4.228409767150879, 'cosine_with_motion': 0.36936137080192566, 'motion_component': 1.5618112087249756, 'motion_component_percent': 36.936137080192566}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.699294567108154, 'force': [-4.322408199310303, 9.774972915649414, 0.8172364830970764], 'magnitude': 10.719197273254395, 'cosine_with_motion': 0.39278092980384827, 'motion_component': 4.210296154022217, 'motion_component_percent': 39.27809298038483}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.974052429199219, 'force': [3.2886385917663574, -7.10646390914917, 1.4229737520217896], 'magnitude': 7.9587578773498535, 'cosine_with_motion': -0.5349343419075012, 'motion_component': -4.257412910461426, 'motion_component_percent': 53.49343419075012}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.528311252593994, 'force': [2.427645683288574, -14.384419441223145, -2.9385924339294434], 'magnitude': 14.880870819091797, 'cosine_with_motion': -0.13219323754310608, 'motion_component': -1.9671505689620972, 'motion_component_percent': 13.219323754310608}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.446437358856201, 'force': [0.21913164854049683, 7.014721393585205, 0.6271215081214905], 'magnitude': 7.046106338500977, 'cosine_with_motion': 0.02972797490656376, 'motion_component': 0.20946647226810455, 'motion_component_percent': 2.972797490656376}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.214537620544434, 'force': [-1.29389488697052, 7.04803991317749, 3.1876654624938965], 'magnitude': 7.842846393585205, 'cosine_with_motion': 0.015462012030184269, 'motion_component': 0.1212661862373352, 'motion_component_percent': 1.546201203018427}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.252894401550293, 'force': [-6.605246067047119, -1.8337420225143433, -1.983393907546997], 'magnitude': 7.136227130889893, 'cosine_with_motion': 0.8989741206169128, 'motion_component': 6.415283679962158, 'motion_component_percent': 89.89741206169128}]}, 5579: {'frame': 5579, 'motion_vector': [2.0666732788085938, -1.3358840942382812, 0.7496261596679688], 'ionic_force': [-1.6814625263214111, 1.4262338280677795, -10.292737245559692], 'ionic_force_magnitude': 10.526248104898524, 'radial_force': 2.20487168781951, 'axial_force': -10.292737245559692, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [5.065872430801392, -10.121050894260406, 7.583192825317383], 'asn_force_magnitude': 13.623639312434397, 'residue_force': [5.065872430801392, -10.121050894260406, 7.583192825317383], 'residue_force_magnitude': 13.623639312434397, 'total_force': [3.3844099044799805, -8.694817066192627, -2.7095444202423096], 'total_force_magnitude': 9.71574522007257, 'cosine_total_motion': 0.6633140062044574, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.846719535473441, 'cosine_residue_motion': 0.846719535473441, 'cosine_ionic_motion': -0.48363021792398614, 'motion_component_total': 6.444589885188144, 'motion_component_glu': None, 'motion_component_asn': 11.535401550082163, 'motion_component_residue': 11.535401550082163, 'motion_component_ionic': -5.090811664894019, 'motion_component_percent_total': 66.33140062044573, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 84.6719535473441, 'motion_component_percent_residue': 84.6719535473441, 'motion_component_percent_ionic': 48.36302179239861, 'ionic_contributions': [{'ion_id': 1309, 'distance': 8.065214157104492, 'force': [2.5060808658599854, 1.78612220287323, -4.071807861328125], 'magnitude': 5.103948593139648, 'cosine_ionic_motion': -0.019736401736736298, 'motion_component_ionic': -0.10073357820510864, 'motion_component_percent_ionic': 1.9736401736736298}, {'ion_id': 1469, 'distance': 9.613414764404297, 'force': [-2.498354911804199, 1.540704369544983, -2.071153163909912], 'magnitude': 3.592384099960327, 'cosine_ionic_motion': -0.9494373798370361, 'motion_component_ionic': -3.4107437133789062, 'motion_component_percent_ionic': 94.94373798370361}, {'ion_id': 2434, 'distance': 11.22485637664795, 'force': [-1.2354334592819214, -1.6161770820617676, -1.6747441291809082], 'magnitude': 2.634974718093872, 'cosine_ionic_motion': -0.24336685240268707, 'motion_component_ionic': -0.6412655115127563, 'motion_component_percent_ionic': 24.336685240268707}, {'ion_id': 2443, 'distance': 11.450145721435547, 'force': [-0.4537550210952759, -0.28441566228866577, -2.475032091140747], 'magnitude': 2.5323052406311035, 'cosine_ionic_motion': -0.3704407215118408, 'motion_component_ionic': -0.9380689859390259, 'motion_component_percent_ionic': 37.04407215118408}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.995687961578369, 'force': [-0.5305469036102295, 7.846015930175781, -0.6404566764831543], 'magnitude': 7.889970302581787, 'cosine_with_motion': -0.5940805077552795, 'motion_component': -4.687277793884277, 'motion_component_percent': 59.408050775527954}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.552929878234863, 'force': [5.089491844177246, -3.5420284271240234, 1.5266737937927246], 'magnitude': 6.385892868041992, 'cosine_with_motion': 0.9979848861694336, 'motion_component': 6.3730244636535645, 'motion_component_percent': 99.79848861694336}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.397833824157715, 'force': [10.111968994140625, -2.2511208057403564, 1.53609037399292], 'magnitude': 10.47277545928955, 'cosine_with_motion': 0.9300635457038879, 'motion_component': 9.740346908569336, 'motion_component_percent': 93.0063545703888}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.456086158752441, 'force': [-6.790855884552002, 1.110723853111267, -1.3673229217529297], 'magnitude': 7.015625476837158, 'cosine_with_motion': -0.9166474342346191, 'motion_component': -6.4308552742004395, 'motion_component_percent': 91.66474342346191}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.294404983520508, 'force': [16.978822708129883, 10.63389778137207, -8.622949600219727], 'magnitude': 21.810901641845703, 'cosine_with_motion': 0.2570042610168457, 'motion_component': 5.605494976043701, 'motion_component_percent': 25.70042610168457}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.6203229427337646, 'force': [-15.075602531433105, -19.17746353149414, 15.08002758026123], 'magnitude': 28.678495407104492, 'cosine_with_motion': 0.07816889882087708, 'motion_component': 2.2417664527893066, 'motion_component_percent': 7.8168898820877075}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.340435266494751, 'force': [-25.120458602905273, -3.575512170791626, 10.197306632995605], 'magnitude': 27.34605598449707, 'cosine_with_motion': -0.5614312887191772, 'motion_component': -15.35293197631836, 'motion_component_percent': 56.143128871917725}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.000636100769043, 'force': [13.117599487304688, -1.9181121587753296, -7.977011203765869], 'magnitude': 15.472015380859375, 'cosine_with_motion': 0.5952640771865845, 'motion_component': 9.209935188293457, 'motion_component_percent': 59.52640771865845}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.27207088470459, 'force': [7.2854533195495605, 0.7525486350059509, -2.149165153503418], 'magnitude': 7.633025169372559, 'cosine_with_motion': 0.6335495114326477, 'motion_component': 4.835899353027344, 'motion_component_percent': 63.35495114326477}]}, 5580: {'frame': 5580, 'motion_vector': [-1.6046180725097656, 1.9312629699707031, -1.8199996948242188], 'ionic_force': [-0.7721650202292949, 0.8433377742767334, -11.557860493659973], 'ionic_force_magnitude': 11.614284162654782, 'radial_force': 1.1434410435119695, 'axial_force': -11.557860493659973, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-3.86629581451416, -10.708865348249674, 3.0412516593933105], 'asn_force_magnitude': 11.784619299240637, 'residue_force': [-3.86629581451416, -10.708865348249674, 3.0412516593933105], 'residue_force_magnitude': 11.784619299240637, 'total_force': [-4.638460834743455, -9.86552757397294, -8.516608834266663], 'total_force_magnitude': 13.833892411905563, 'cosine_total_motion': 0.09068063285977865, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.5476116662464738, 'cosine_residue_motion': -0.5476116662464738, 'cosine_ionic_motion': 0.6636535684349356, 'motion_component_total': 1.254466118825686, 'motion_component_glu': None, 'motion_component_asn': -6.453395010537518, 'motion_component_residue': -6.453395010537518, 'motion_component_ionic': 7.707861129363204, 'motion_component_percent_total': 9.068063285977864, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 54.76116662464739, 'motion_component_percent_residue': 54.76116662464739, 'motion_component_percent_ionic': 66.36535684349356, 'ionic_contributions': [{'ion_id': 1309, 'distance': 8.492998123168945, 'force': [3.384483575820923, 0.7182776927947998, -3.0355429649353027], 'magnitude': 4.60273551940918, 'cosine_ionic_motion': 0.10376221686601639, 'motion_component_ionic': 0.47759002447128296, 'motion_component_percent_ionic': 10.376221686601639}, {'ion_id': 1469, 'distance': 7.310606479644775, 'force': [-3.7529938220977783, 2.630032777786255, -4.193670749664307], 'magnitude': 6.211997032165527, 'cosine_ionic_motion': 0.9724726676940918, 'motion_component_ionic': 6.040997505187988, 'motion_component_percent_ionic': 97.24726676940918}, {'ion_id': 2434, 'distance': 11.535965919494629, 'force': [-0.40012770891189575, -1.974854826927185, -1.4709564447402954], 'magnitude': 2.494767904281616, 'cosine_ionic_motion': -0.06395216286182404, 'motion_component_ionic': -0.15954580903053284, 'motion_component_percent_ionic': 6.395216286182404}, {'ion_id': 2443, 'distance': 10.687788963317871, 'force': [-0.0035270650405436754, -0.5301178693771362, -2.8576903343200684], 'magnitude': 2.9064464569091797, 'cosine_ionic_motion': 0.4640786051750183, 'motion_component_ionic': 1.348819613456726, 'motion_component_percent_ionic': 46.40786051750183}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.049490451812744, 'force': [-9.586258888244629, 10.096769332885742, -3.8128442764282227], 'magnitude': 14.435335159301758, 'cosine_with_motion': 0.9342221021652222, 'motion_component': 13.485809326171875, 'motion_component_percent': 93.42221021652222}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.8729913234710693, 'force': [14.967676162719727, -17.172510147094727, 7.083902835845947], 'magnitude': 23.855985641479492, 'cosine_with_motion': -0.947206974029541, 'motion_component': -22.596555709838867, 'motion_component_percent': 94.7206974029541}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.991913795471191, 'force': [5.9453511238098145, -9.965107917785645, 3.910872220993042], 'magnitude': 12.245223045349121, 'cosine_with_motion': -0.9454648494720459, 'motion_component': -11.577427864074707, 'motion_component_percent': 94.54648494720459}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.011364459991455, 'force': [-1.706739902496338, 4.78489351272583, -2.227449655532837], 'magnitude': 5.547044277191162, 'cosine_with_motion': 0.9320682883262634, 'motion_component': 5.170224189758301, 'motion_component_percent': 93.20682883262634}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.914214611053467, 'force': [-2.1904101371765137, 3.107361078262329, -1.1867775917053223], 'magnitude': 3.9827163219451904, 'cosine_with_motion': 0.9453430771827698, 'motion_component': 3.76503324508667, 'motion_component_percent': 94.53430771827698}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.108897686004639, 'force': [13.608816146850586, 2.2836806774139404, -2.4842469692230225], 'magnitude': 14.0209321975708, 'cosine_with_motion': -0.2968040704727173, 'motion_component': -4.16146993637085, 'motion_component_percent': 29.68040704727173}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.94612455368042, 'force': [-22.468996047973633, -2.854041337966919, 1.2911922931671143], 'magnitude': 22.68630599975586, 'cosine_with_motion': 0.40072575211524963, 'motion_component': 9.090987205505371, 'motion_component_percent': 40.07257521152496}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.816590785980225, 'force': [-12.67530345916748, 0.8918702602386475, 3.397038459777832], 'magnitude': 13.152894020080566, 'cosine_with_motion': 0.38929468393325806, 'motion_component': 5.120351791381836, 'motion_component_percent': 38.929468393325806}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.553234100341797, 'force': [6.23122501373291, -1.8331278562545776, -1.721178650856018], 'magnitude': 6.719448089599609, 'cosine_with_motion': -0.49940112233161926, 'motion_component': -3.3557000160217285, 'motion_component_percent': 49.940112233161926}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.768090724945068, 'force': [4.0083441734313965, -0.048652950674295425, -1.2092570066452026], 'magnitude': 4.187062740325928, 'cosine_with_motion': -0.33308494091033936, 'motion_component': -1.3946475982666016, 'motion_component_percent': 33.308494091033936}]}, 5581: {'frame': 5581, 'motion_vector': [0.801727294921875, 2.2831573486328125, -1.9393539428710938], 'ionic_force': [-1.0563013553619385, 1.5127899050712585, -8.483844637870789], 'ionic_force_magnitude': 8.682161348981825, 'radial_force': 1.8450761096022505, 'axial_force': -8.483844637870789, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-4.091072916984558, -0.5949215888977051, 7.045930489897728], 'asn_force_magnitude': 8.169207169456016, 'residue_force': [-4.091072916984558, -0.5949215888977051, 7.045930489897728], 'residue_force_magnitude': 8.169207169456016, 'total_force': [-5.147374272346497, 0.9178683161735535, -1.4379141479730606], 'total_force_magnitude': 5.422687640127448, 'cosine_total_motion': 0.04504427309450334, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.7224783062472008, 'cosine_residue_motion': -0.7224783062472008, 'cosine_ionic_motion': 0.7079269475750936, 'motion_component_total': 0.2442610229680886, 'motion_component_glu': None, 'motion_component_asn': -5.902074959171071, 'motion_component_residue': -5.902074959171071, 'motion_component_ionic': 6.14633598213916, 'motion_component_percent_total': 4.5044273094503335, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 72.24783062472008, 'motion_component_percent_residue': 72.24783062472008, 'motion_component_percent_ionic': 70.79269475750935, 'ionic_contributions': [{'ion_id': 1309, 'distance': 9.217119216918945, 'force': [1.5847398042678833, 1.608560562133789, -3.1895318031311035], 'magnitude': 3.907938003540039, 'cosine_ionic_motion': 0.9183045029640198, 'motion_component_ionic': 3.588677167892456, 'motion_component_percent_ionic': 91.83045029640198}, {'ion_id': 1469, 'distance': 10.581854820251465, 'force': [-1.8289650678634644, 1.3348606824874878, -1.9141175746917725], 'magnitude': 2.964930534362793, 'cosine_ionic_motion': 0.5757282376289368, 'motion_component_ionic': 1.7069941759109497, 'motion_component_percent_ionic': 57.57282376289368}, {'ion_id': 2434, 'distance': 13.097936630249023, 'force': [-0.5441734194755554, -1.361169457435608, -1.2634094953536987], 'magnitude': 1.9352288246154785, 'cosine_ionic_motion': -0.18226824700832367, 'motion_component_ionic': -0.35273075103759766, 'motion_component_percent_ionic': 18.226824700832367}, {'ion_id': 2443, 'distance': 12.470683097839355, 'force': [-0.267902672290802, -0.0694618821144104, -2.116785764694214], 'magnitude': 2.1348018646240234, 'cosine_ionic_motion': 0.5637035369873047, 'motion_component_ionic': 1.2033953666687012, 'motion_component_percent_ionic': 56.37035369873047}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.14915132522583, 'force': [1.1958789825439453, -13.484228134155273, -2.4111251831054688], 'magnitude': 13.750202178955078, 'cosine_with_motion': -0.5898587703704834, 'motion_component': -8.110677719116211, 'motion_component_percent': 58.98587703704834}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.0121681690216064, 'force': [-5.087360382080078, 20.721418380737305, 3.9667885303497314], 'magnitude': 21.702392578125, 'cosine_with_motion': 0.5280561447143555, 'motion_component': 11.460082054138184, 'motion_component_percent': 52.80561447143555}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.44619083404541, 'force': [2.8244411945343018, 15.098342895507812, 1.5236696004867554], 'magnitude': 15.435640335083008, 'cosine_with_motion': 0.7057332396507263, 'motion_component': 10.893444061279297, 'motion_component_percent': 70.57332396507263}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.8720946311950684, 'force': [-3.347208261489868, -8.666054725646973, -0.16123293340206146], 'magnitude': 9.291410446166992, 'cosine_with_motion': -0.7689775228500366, 'motion_component': -7.144885540008545, 'motion_component_percent': 76.89775228500366}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.43958044052124, 'force': [-1.0241671800613403, -4.57720422744751, -0.4076673090457916], 'magnitude': 4.708068370819092, 'cosine_with_motion': -0.7178709506988525, 'motion_component': -3.3797855377197266, 'motion_component_percent': 71.78709506988525}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.308557987213135, 'force': [5.8510541915893555, -3.5571577548980713, 1.3910175561904907], 'magnitude': 6.9873552322387695, 'cosine_with_motion': -0.28282201290130615, 'motion_component': -1.9761779308319092, 'motion_component_percent': 28.282201290130615}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.618579864501953, 'force': [-2.400791883468628, 3.0406863689422607, -2.1127662658691406], 'magnitude': 4.412862777709961, 'cosine_with_motion': 0.6660753488540649, 'motion_component': 2.9392991065979004, 'motion_component_percent': 66.6075348854065}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.9893813133239746, 'force': [9.230582237243652, 8.277998924255371, -8.21556282043457], 'magnitude': 14.873614311218262, 'cosine_with_motion': 0.9156423807144165, 'motion_component': 13.618911743164062, 'motion_component_percent': 91.56423807144165}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.9905595779418945, 'force': [-10.00835132598877, -14.792145729064941, 12.875567436218262], 'magnitude': 22.01715087890625, 'cosine_with_motion': -0.9778871536254883, 'motion_component': -21.530288696289062, 'motion_component_percent': 97.78871536254883}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.267385005950928, 'force': [-12.618948936462402, -4.7344818115234375, 9.955862998962402], 'magnitude': 16.756263732910156, 'cosine_with_motion': -0.7742990851402283, 'motion_component': -12.974359512329102, 'motion_component_percent': 77.42990851402283}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.767609119415283, 'force': [7.267451763153076, 0.753171443939209, -6.552069187164307], 'magnitude': 9.813905715942383, 'cosine_with_motion': 0.6654771566390991, 'motion_component': 6.530930042266846, 'motion_component_percent': 66.54771566390991}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.234805583953857, 'force': [4.026346683502197, 1.324732780456543, -2.806551933288574], 'magnitude': 5.08361291885376, 'cosine_with_motion': 0.7418808341026306, 'motion_component': 3.771435022354126, 'motion_component_percent': 74.18808341026306}]}, 5582: {'frame': 5582, 'motion_vector': [1.6045913696289062, -2.307353973388672, -3.4020919799804688], 'ionic_force': [-0.011387579143047333, 0.7488982081413269, -5.534487962722778], 'ionic_force_mag</t>
         </is>
       </c>
     </row>
@@ -723,7 +723,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>{5599: {'frame': 5599, 'ionic_force': [-1.9013180434703827, -9.60105836391449, -11.383936129510403], 'ionic_force_magnitude': 15.012972184430726, 'motion_vector': [-3.3165664672851562, 2.1229324340820312, -0.15932464599609375], 'ionic_force_x': -1.9013180434703827, 'ionic_force_y': -9.60105836391449, 'ionic_force_z': -11.383936129510403, 'radial_force': 9.787508978780986, 'axial_force': -11.383936129510403, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-10.478373050689697, -0.794865264557302, -0.7303848266601562], 'asn_force_magnitude': 10.533830004952389, 'residue_force': [-10.478373050689697, -0.794865264557302, -0.7303848266601562], 'residue_force_magnitude': 10.533830004952389, 'total_force': [-12.37969109416008, -10.395923628471792, -12.114320956170559], 'total_force_magnitude': 20.20120669427838, 'motion_component_total': 5.307813394954503, 'cosine_total_motion': 0.26274734352665396, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.7992701343413963, 'cosine_residue_motion': 0.7992701343413963, 'cosine_ionic_motion': -0.20725824906676935, 'motion_component_glu': None, 'motion_component_asn': 8.419375723187727, 'motion_component_residue': 8.419375723187727, 'motion_component_ionic': -3.111562328233224, 'ionic_contributions': [{'ion_id': 1309, 'distance': 8.083805084228516, 'force': [3.44903564453125, 3.2919468879699707, -1.7546262741088867], 'magnitude': 5.080499172210693}, {'ion_id': 1380, 'distance': 10.135680198669434, 'force': [0.5980334877967834, 1.709892749786377, -2.676297664642334], 'magnitude': 3.2317094802856445}, {'ion_id': 1469, 'distance': 11.055704116821289, 'force': [-0.6552402973175049, 2.634486198425293, -0.08947023004293442], 'magnitude': 2.716222047805786}, {'ion_id': 1476, 'distance': 13.930360794067383, 'force': [0.27780506014823914, 0.6250635385513306, -1.5681666135787964], 'magnitude': 1.710855484008789}, {'ion_id': 2434, 'distance': 4.131947994232178, 'force': [-5.57095193862915, -17.86244773864746, -5.295375347137451], 'magnitude': 19.445913314819336}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.984648704528809, 'force': [-4.895257949829102, -1.0194158554077148, -6.148347854614258], 'magnitude': 7.924956798553467}, {'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.503798007965088, 'force': [-6.254924297332764, -0.015604271553456783, 4.684281826019287], 'magnitude': 7.814526081085205}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.844854831695557, 'force': [8.499029159545898, -0.5871928334236145, -9.819294929504395], 'magnitude': 12.999878883361816}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.637355327606201, 'force': [-4.003154754638672, 1.6218104362487793, 4.827773094177246], 'magnitude': 6.477878570556641}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.483351230621338, 'force': [-3.8240652084350586, -0.7944627404212952, 5.725203037261963], 'magnitude': 6.93055534362793}]}, 5600: {'frame': 5600, 'ionic_force': [-18.553392615169287, 5.5990365743637085, -7.359938099980354], 'ionic_force_magnitude': 20.7303226441178, 'motion_vector': [-2.751720428466797, -2.4600486755371094, 0.600830078125], 'ionic_force_x': -18.553392615169287, 'ionic_force_y': 5.5990365743637085, 'ionic_force_z': -7.359938099980354, 'radial_force': 19.379824253426055, 'axial_force': -7.359938099980354, 'glu_force': [-34.1942024230957, 6.112398624420166, 16.177690505981445], 'glu_force_magnitude': 38.318697347414876, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [-34.1942024230957, 6.112398624420166, 16.177690505981445], 'residue_force_magnitude': 38.318697347414876, 'total_force': [-52.74759503826499, 11.711435198783875, 8.817752406001091], 'total_force_magnitude': 54.74686524568918, 'motion_component_total': 32.52568909929408, 'cosine_total_motion': 0.5941105294947491, 'cosine_glu_motion': 0.6195228479127445, 'cosine_asn_motion': None, 'cosine_residue_motion': 0.6195228479127445, 'cosine_ionic_motion': 0.4238419604535297, 'motion_component_glu': 23.73930850897699, 'motion_component_asn': None, 'motion_component_residue': 23.73930850897699, 'motion_component_ionic': 8.786380590317087, 'ionic_contributions': [{'ion_id': 1309, 'distance': 7.418415546417236, 'force': [-0.036227066069841385, 5.730989933013916, -1.8837703466415405], 'magnitude': 6.032756328582764}, {'ion_id': 1380, 'distance': 11.569257736206055, 'force': [-0.34478411078453064, 1.6263123750686646, -1.8408604860305786], 'magnitude': 2.4804306030273438}, {'ion_id': 1469, 'distance': 14.104735374450684, 'force': [-0.7819127440452576, 1.468832015991211, -0.126841738820076], 'magnitude': 1.6688151359558105}, {'ion_id': 1476, 'distance': 14.7647123336792, 'force': [-0.10772905498743057, 0.7481944561004639, -1.3221204280853271], 'magnitude': 1.5229586362838745}, {'ion_id': 2434, 'distance': 4.310497760772705, 'force': [-17.282739639282227, -3.975292205810547, -2.186345100402832], 'magnitude': 17.86829948425293}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.160724401473999, 'force': [24.515661239624023, -4.078901290893555, -9.936822891235352], 'magnitude': 26.765565872192383}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 2.6899526119232178, 'force': [-26.513227462768555, 14.984768867492676, 21.998085021972656], 'magnitude': 37.56874084472656}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.8783912658691406, 'force': [-32.19663619995117, -4.793468952178955, 4.116428375244141], 'magnitude': 32.81075668334961}], 'asn_contributions': []}, 5601: {'frame': 5601, 'ionic_force': [-9.747690379619598, 9.922138929367065, -7.001989342272282], 'ionic_force_magnitude': 15.572224099976358, 'motion_vector': [-0.6682701110839844, -0.8040084838867188, 0.39972686767578125], 'ionic_force_x': -9.747690379619598, 'ionic_force_y': 9.922138929367065, 'ionic_force_z': -7.001989342272282, 'radial_force': 13.909216680697368, 'axial_force': -7.001989342272282, 'glu_force': [-20.76607894897461, 27.381933212280273, 0.22750675678253174], 'glu_force_magnitude': 34.36643799815753, 'asn_force': [-1.7546709775924683, 1.6305269002914429, 8.389400959014893], 'asn_force_magnitude': 8.72465109120699, 'residue_force': [-22.520749926567078, 29.012460112571716, 8.616907715797424], 'residue_force_magnitude': 37.72476795980467, 'total_force': [-32.268440306186676, 38.93459904193878, 1.6149183735251427], 'total_force_magnitude': 50.59410245970989, 'motion_component_total': -8.12500526013541, 'cosine_total_motion': -0.1605919438259761, 'cosine_glu_motion': -0.20919924373673454, 'cosine_asn_motion': 0.32923574729680877, 'cosine_residue_motion': -0.114433197357825, 'cosine_ionic_motion': -0.2445404984197928, 'motion_component_glu': -7.189432839139933, 'motion_component_asn': 2.8724670219174513, 'motion_component_residue': -4.316965817222481, 'motion_component_ionic': -3.808039442912928, 'ionic_contributions': [{'ion_id': 1309, 'distance': 6.409053802490234, 'force': [-1.464813470840454, 7.521646022796631, -2.570472478866577], 'magnitude': 8.082584381103516}, {'ion_id': 1380, 'distance': 10.99662971496582, 'force': [-1.123779535293579, 1.281681776046753, -2.1522297859191895], 'magnitude': 2.745483875274658}, {'ion_id': 1469, 'distance': 13.696661949157715, 'force': [-1.2938627004623413, 1.2048321962356567, -0.07915589958429337], 'magnitude': 1.769736409187317}, {'ion_id': 1476, 'distance': 14.374396324157715, 'force': [-0.5480816960334778, 0.5199006199836731, -1.4181257486343384], 'magnitude': 1.606788992881775}, {'ion_id': 2434, 'distance': 7.834921360015869, 'force': [-5.317152976989746, -0.6059216856956482, -0.7820054292678833], 'magnitude': 5.408400058746338}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.2818381786346436, 'force': [14.98430061340332, -18.21042251586914, -7.759255409240723], 'magnitude': 24.826494216918945}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 2.618565559387207, 'force': [-17.718032836914062, 35.45824432373047, 0.7173105478286743], 'magnitude': 39.64505386352539}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 3.521170139312744, 'force': [-18.032346725463867, 10.134111404418945, 7.26945161819458], 'magnitude': 21.92511558532715}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.179820537567139, 'force': [-2.1817688941955566, 0.38443517684936523, 8.539961814880371], 'magnitude': 8.822632789611816}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.6257147789001465, 'force': [4.295049667358398, -3.9265239238739014, -13.01939582824707], 'magnitude': 14.260774612426758}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.978527069091797, 'force': [-2.5541765689849854, 1.991648554801941, 4.593373775482178], 'magnitude': 5.62045955657959}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 3.9424872398376465, 'force': [-1.3137751817703247, 3.180967092514038, 8.275461196899414], 'magnitude': 8.962578773498535}]}, 5602: {'frame': 5602, 'ionic_force': [-9.748128592967987, 11.87373073399067, -8.434279189445078], 'ionic_force_magnitude': 17.525654283189, 'motion_vector': [1.2005729675292969, 0.9844474792480469, -0.0977783203125], 'ionic_force_x': -9.748128592967987, 'ionic_force_y': 11.87373073399067, 'ionic_force_z': -8.434279189445078, 'radial_force': 15.362665543724976, 'axial_force': -8.434279189445078, 'glu_force': [-13.67834460735321, 34.34225273132324, -5.655503749847412], 'glu_force_magnitude': 37.39615162719455, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [-13.67834460735321, 34.34225273132324, -5.655503749847412], 'residue_force_magnitude': 37.39615162719455, 'total_force': [-23.426473200321198, 46.21598346531391, -14.08978293929249], 'total_force_magnitude': 53.69579832303375, 'motion_component_total': 12.05257716100193, 'cosine_total_motion': 0.22446034023916853, 'cosine_glu_motion': 0.3083641148932268, 'cosine_asn_motion': None, 'cosine_residue_motion': 0.3083641148932268, 'cosine_ionic_motion': 0.029724765515252854, 'motion_component_glu': 11.53163119693275, 'motion_component_asn': None, 'motion_component_residue': 11.53163119693275, 'motion_component_ionic': 0.5209459640691798, 'ionic_contributions': [{'ion_id': 1309, 'distance': 5.589580535888672, 'force': [-2.806483507156372, 9.153647422790527, -4.609921932220459], 'magnitude': 10.626240730285645}, {'ion_id': 1380, 'distance': 10.90501594543457, 'force': [-1.2517857551574707, 1.1912050247192383, -2.192772626876831], 'magnitude': 2.7918074131011963}, {'ion_id': 1469, 'distance': 13.315174102783203, 'force': [-1.356601595878601, 1.2908194065093994, -0.006111637689173222], 'magnitude': 1.872597098350525}, {'ion_id': 1476, 'distance': 14.112052917480469, 'force': [-0.6084700226783752, 0.47949525713920593, -1.4761505126953125], 'magnitude': 1.667084813117981}, {'ion_id': 2434, 'distance': 9.427346229553223, 'force': [-3.724787712097168, -0.24143637716770172, -0.1493224799633026], 'magnitude': 3.7355899810791016}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 2.9619991779327393, 'force': [9.577141761779785, -28.668466567993164, -3.9086532592773438], 'magnitude': 30.477535247802734}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 2.6011602878570557, 'force': [-1.2337597608566284, 39.29288101196289, -8.292745590209961], 'magnitude': 40.17738342285156}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.8692431449890137, 'force': [-22.021726608276367, 23.717838287353516, 6.545895099639893], 'magnitude': 33.02031326293945}], 'asn_contributions': []}, 5603: {'frame': 5603, 'ionic_force': [-17.560770630836487, 16.140983641147614, -9.764761259779334], 'ionic_force_magnitude': 25.773291999919827, 'motion_vector': [-1.2378005981445312, -0.32138824462890625, 0.05432891845703125], 'ionic_force_x': -17.560770630836487, 'ionic_force_y': 16.140983641147614, 'ionic_force_z': -9.764761259779334, 'radial_force': 23.851876614904835, 'axial_force': -9.764761259779334, 'glu_force': [-8.688776016235352, 18.961535453796387, -3.2987524271011353], 'glu_force_magnitude': 21.11673324643728, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [-8.688776016235352, 18.961535453796387, -3.2987524271011353], 'residue_force_magnitude': 21.11673324643728, 'total_force': [-26.24954664707184, 35.102519094944, -13.06351368688047], 'total_force_magnitude': 45.7370849074908, 'motion_component_total': 16.016006731139502, 'cosine_total_motion': 0.35017550339148107, 'cosine_glu_motion': 0.165810085529384, 'cosine_asn_motion': None, 'cosine_residue_motion': 0.165810085529384, 'cosine_ionic_motion': 0.4855661971891475, 'motion_component_glu': 3.501367345692952, 'motion_component_asn': None, 'motion_component_residue': 3.501367345692952, 'motion_component_ionic': 12.514639385446548, 'ionic_contributions': [{'ion_id': 1309, 'distance': 4.739724159240723, 'force': [-7.167101860046387, 12.286242485046387, -4.010806083679199], 'magnitude': 14.77855396270752}, {'ion_id': 1380, 'distance': 9.010942459106445, 'force': [-1.6355546712875366, 2.433621406555176, -2.8497138023376465], 'magnitude': 4.0888166427612305}, {'ion_id': 1469, 'distance': 13.02607250213623, 'force': [-1.2709964513778687, 1.487382173538208, -0.02657478116452694], 'magnitude': 1.9566409587860107}, {'ion_id': 1476, 'distance': 13.13216495513916, 'force': [-0.5827058553695679, 0.6906329989433289, -1.6999109983444214], 'magnitude': 1.9251538515090942}, {'ion_id': 2434, 'distance': 6.864849090576172, 'force': [-6.904411792755127, -0.7568954229354858, -1.17775559425354], 'magnitude': 7.044920444488525}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.8883092403411865, 'force': [7.783102989196777, -15.684765815734863, -2.4907524585723877], 'magnitude': 17.685937881469727}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 3.3359897136688232, 'force': [-5.854516983032227, 23.5977840423584, -2.3532145023345947], 'magnitude': 24.426795959472656}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 4.201320171356201, 'force': [-10.617362022399902, 11.048517227172852, 1.5452145338058472], 'magnitude': 15.400837898254395}], 'asn_contributions': []}, 5604: {'frame': 5604, 'ionic_force': [-14.2177032828331, 19.06482544541359, -2.1827616719529033], 'ionic_force_magnitude': 23.882527178238888, 'motion_vector': [0.9648094177246094, 0.07035064697265625, 0.3220977783203125], 'ionic_force_x': -14.2177032828331, 'ionic_force_y': 19.06482544541359, 'ionic_force_z': -2.1827616719529033, 'radial_force': 23.782570422533652, 'axial_force': -2.1827616719529033, 'glu_force': [-9.147841453552246, 32.45199394226074, -0.4819430708885193], 'glu_force_magnitude': 33.72013023716596, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [-9.147841453552246, 32.45199394226074, -0.4819430708885193], 'residue_force_magnitude': 33.72013023716596, 'total_force': [-23.365544736385345, 51.51681938767433, -2.6647047428414226], 'total_force_magnitude': 56.6306631783242, 'motion_component_total': -19.397453722912054, 'cosine_total_motion': -0.3425256324799066, 'cosine_glu_motion': -0.19482353079901096, 'cosine_asn_motion': None, 'cosine_residue_motion': -0.19482353079901096, 'cosine_ionic_motion': -0.5371282023618255, 'motion_component_glu': -6.569474831807163, 'motion_component_asn': None, 'motion_component_residue': -6.569474831807163, 'motion_component_ionic': -12.827978891104895, 'ionic_contributions': [{'ion_id': 1309, 'distance': 4.387622833251953, 'force': [-7.5053019523620605, 15.458601951599121, 1.4540939331054688], 'magnitude': 17.245647430419922}, {'ion_id': 1380, 'distance': 10.315604209899902, 'force': [-1.4976059198379517, 1.5437307357788086, -2.2601349353790283], 'magnitude': 3.1199581623077393}, {'ion_id': 1469, 'distance': 13.825953483581543, 'force': [-1.2702255249023438, 1.183520793914795, 0.04746720567345619], 'magnitude': 1.7367923259735107}, {'ion_id': 1476, 'distance': 14.050297737121582, 'force': [-0.6734047532081604, 0.5765787363052368, -1.429139256477356], 'magnitude': 1.6817716360092163}, {'ion_id': 2434, 'distance': 10.052953720092773, 'force': [-3.271165132522583, 0.30239322781562805, 0.004951381124556065], 'magnitude': 3.285115957260132}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.1217877864837646, 'force': [6.149357795715332, -25.953346252441406, -6.435849666595459], 'magnitude': 27.437400817871094}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 2.816182851791382, 'force': [3.228656768798828, 34.113380432128906, -0.8480800986289978], 'magnitude': 34.27632141113281}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.9471259117126465, 'force': [-18.525856018066406, 24.291959762573242, 6.8019866943359375], 'magnitude': 31.298141479492188}], 'asn_contributions': []}, 5605: {'frame': 5605, 'ionic_force': [-18.65671706199646, 11.948305934667587, -10.66128496825695], 'ionic_force_magnitude': 24.586543136727947, 'motion_vector': [-0.040676116943359375, 0.6826667785644531, -0.5590362548828125], 'ionic_force_x': -18.65671706199646, 'ionic_force_y': 11.948305934667587, 'ionic_force_z': -10.66128496825695, 'radial_force': 22.154798718106253, 'axial_force': -10.66128496825695, 'glu_force': [-10.341562330722809, 32.2280387878418, 1.596648931503296], 'glu_force_magnitude': 33.884268966016236, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [-10.341562330722809, 32.2280387878418, 1.596648931503296], 'residue_force_magnitude': 33.884268966016236, 'total_force': [-28.99827939271927, 44.176344722509384, -9.064636036753654], 'total_force_magnitude': 53.61545735381731, 'motion_component_total': 41.21468010136568, 'cosine_total_motion': 0.7687089159639758, 'cosine_glu_motion': 0.7193191344814241, 'cosine_asn_motion': None, 'cosine_residue_motion': 0.7193191344814241, 'cosine_ionic_motion': 0.6849713268978227, 'motion_component_glu': 24.37360302517058, 'motion_component_asn': None, 'motion_component_residue': 24.37360302517058, 'motion_component_ionic': 16.8410770761951, 'ionic_contributions': [{'ion_id': 1309, 'distance': 4.6242804527282715, 'force': [-11.117942810058594, 8.545702934265137, -6.663941860198975], 'magnitude': 15.525650024414062}, {'ion_id': 1380, 'distance': 10.08809757232666, 'force': [-1.4706867933273315, 1.5739147663116455, -2.449951410293579], 'magnitude': 3.262267589569092}, {'ion_id': 1469, 'distance': 13.289344787597656, 'force': [-1.0578231811523438, 1.5526583194732666, 0.06499066203832626], 'magnitude': 1.8798832893371582}, {'ion_id': 1476, 'distance': 13.405807495117188, 'force': [-0.48204028606414795, 0.6503790020942688, -1.660539984703064], 'magnitude': 1.8473626375198364}, {'ion_id': 2434, 'distance': 8.547780990600586, 'force': [-4.528223991394043, -0.37434908747673035, 0.048157624900341034], 'magnitude': 4.54392671585083}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.267085552215576, 'force': [7.773112773895264, -22.777538299560547, -6.951651573181152], 'magnitude': 25.051206588745117}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 2.757434368133545, 'force': [-0.8180308938026428, 35.714202880859375, 1.4362404346466064], 'magnitude': 35.7524299621582}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 3.1808032989501953, 'force': [-17.29664421081543, 19.29137420654297, 7.112060070037842], 'magnitude': 26.868427276611328}], 'asn_contributions': []}, 5606: {'frame': 5606, 'ionic_force': [-21.41411665081978, 2.977629542350769, -6.465997515246272], 'ionic_force_magnitude': 22.566342049467565, 'motion_vector': [-0.3365478515625, -0.6044425964355469, 0.14295196533203125], 'ionic_force_x': -21.41411665081978, 'ionic_force_y': 2.977629542350769, 'ionic_force_z': -6.465997515246272, 'radial_force': 21.62014499549892, 'axial_force': -6.465997515246272, 'glu_force': [-15.111041069030762, 33.415127754211426, -0.8798074722290039], 'glu_force_magnitude': 36.68362558701627, 'asn_force': [1.0994532108306885, 0.4009546935558319, 0.7341213226318359], 'asn_force_magnitude': 1.3814833134834013, 'residue_force': [-14.011587858200073, 33.81608244776726, -0.14568614959716797], 'residue_force_magnitude': 36.60427913340784, 'total_force': [-35.42570450901985, 36.79371199011803, -6.61168366484344], 'total_force_magnitude': 51.502156681600255, 'motion_component_total': -15.942577150333303, 'cosine_total_motion': -0.3095516416699686, 'cosine_glu_motion': -0.5879970714475303, 'cosine_asn_motion': -0.5199445990274864, 'cosine_residue_motion': -0.6088949087483513, 'cosine_ionic_motion': 0.2811967503856907, 'motion_component_glu': -21.56986441524326, 'motion_component_asn': -0.7182947874922903, 'motion_component_residue': -22.28815920273555, 'motion_component_ionic': 6.345582052402246, 'ionic_contributions': [{'ion_id': 1309, 'distance': 5.460677623748779, 'force': [-7.701904296875, 6.24114990234375, -5.068641662597656], 'magnitude': 11.133840560913086}, {'ion_id': 1380, 'distance': 10.715598106384277, 'force': [-1.0523978471755981, 1.6155245304107666, -2.1546742916107178], 'magnitude': 2.891380786895752}, {'ion_id': 1469, 'distance': 14.11843490600586, 'force': [-1.061071753501892, 1.283768892288208, -0.014648376032710075], 'magnitude': 1.6655781269073486}, {'ion_id': 1476, 'distance': 13.845550537109375, 'force': [-0.44619205594062805, 0.6866577863693237, -1.5260471105575562], 'magnitude': 1.7318793535232544}, {'ion_id': 2434, 'distance': 4.998462200164795, 'force': [-11.15255069732666, -6.849471569061279, 2.298013925552368], 'magnitude': 13.288171768188477}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.3145811557769775, 'force': [11.498557090759277, -20.02912712097168, -7.67957878112793], 'magnitude': 24.33841896057129}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 2.503218412399292, 'force': [-12.867231369018555, 41.36821365356445, 2.2759690284729004], 'magnitude': 43.38288497924805}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 3.7980051040649414, 'force': [-13.742366790771484, 12.076041221618652, 4.523802280426025], 'magnitude': 18.845375061035156}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.950682163238525, 'force': [-1.9842679500579834, 0.8550195693969727, 6.326084613800049], 'magnitude': 6.684887886047363}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.545941352844238, 'force': [3.083721160888672, -0.45406487584114075, -5.591963291168213], 'magnitude': 6.401997089385986}]}, 5607: {'frame': 5607, 'ionic_force': [-23.770193874835968, 13.231722950935364, -0.08699758723378181], 'ionic_force_magnitude': 27.204929290071377, 'motion_vector': [-0.3793296813964844, -0.6377906799316406, 0.31902313232421875], 'ionic_force_x': -23.770193874835968, 'ionic_force_y': 13.231722950935364, 'ionic_force_z': -0.08699758723378181, 'radial_force': 27.20479018661234, 'axial_force': -0.08699758723378181, 'glu_force': [-10.55739164352417, 24.778688430786133, 0.6941158771514893], 'glu_force_magnitude': 26.942971542048628, 'asn_force': [-2.1632673740386963, -0.7775283455848694, 3.4888997077941895], 'asn_force_magnitude': 4.178121256116749, 'residue_force': [-12.720659017562866, 24.001160085201263, 4.183015584945679], 'residue_force_magnitude': 27.483967520364672, 'total_force': [-36.490852892398834, 37.23288303613663, 4.096017997711897], 'total_force_magnitude': 52.29385515942483, 'motion_component_total': -10.644513601928445, 'cosine_total_motion': -0.20355190049533003, 'cosine_glu_motion': -0.5319805362843553, 'cosine_asn_motion': 0.7198963924990891, 'cosine_residue_motion': -0.41207012859185155, 'cosine_ionic_motion': 0.0250251864705622, 'motion_component_glu': -14.333136450033152, 'motion_component_asn': 3.0078144197022105, 'motion_component_residue': -11.325322030330941, 'motion_component_ionic': 0.6808084284024956, 'ionic_contributions': [{'ion_id': 1309, 'distance': 5.314762592315674, 'force': [-8.924793243408203, 5.3618340492248535, -5.453948497772217], 'magnitude': 11.753583908081055}, {'ion_id': 1380, 'distance': 9.945533752441406, 'force': [-1.5038363933563232, 1.5769492387771606, -2.552949905395508], 'magnitude': 3.3564634323120117}, {'ion_id': 1469, 'distance': 12.824362754821777, 'force': [-1.4209312200546265, 1.4332846403121948, 0.041228216141462326], 'magnitude': 2.0186753273010254}, {'ion_id': 1476, 'distance': 13.836520195007324, 'force': [-0.508072555065155, 0.625862717628479, -1.5353832244873047], 'magnitude': 1.7341405153274536}, {'ion_id': 2434, 'distance': 4.644890308380127, 'force': [-11.41256046295166, 4.233792304992676, 9.414055824279785], 'magnitude': 15.388176918029785}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.4388439655303955, 'force': [8.377961158752441, -20.170866012573242, -5.84935998916626], 'magnitude': 22.61125946044922}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 3.12336802482605, 'force': [-2.1286587715148926, 27.75999641418457, 1.1607463359832764], 'magnitude': 27.865676879882812}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 3.321812868118286, 'force': [-16.80669403076172, 17.189558029174805, 5.382729530334473], 'magnitude': 24.635738372802734}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.774259090423584, 'force': [-2.1632673740386963, -0.7775283455848694, 3.4888997077941895], 'magnitude': 4.178121089935303}]}, 5608: {'frame': 5608, 'ionic_force': [-18.901110351085663, 10.239649832248688, -9.298373874276876], 'ionic_force_magnitude': 23.42140384129062, 'motion_vector': [-1.0680618286132812, 0.4606742858886719, 1.07733154296875], 'ionic_force_x': -18.901110351085663, 'ionic_force_y': 10.239649832248688, 'ionic_force_z': -9.298373874276876, 'radial_force': 21.496567195507943, 'axial_force': -9.298373874276876, 'glu_force': [-3.8896929025650024, 9.817646026611328, -1.464644730091095], 'glu_force_magnitude': 10.66119451869655, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [-3.8896929025650024, 9.817646026611328, -1.464644730091095], 'residue_force_magnitude': 10.66119451869655, 'total_force': [-22.790803253650665, 20.057295858860016, -10.763018604367971], 'total_force_magnitude': 32.21115334157453, 'motion_component_total': 13.867777388868902, 'cosine_total_motion': 0.43052719167835374, 'cosine_glu_motion': 0.4200079536096653, 'cosine_asn_motion': None, 'cosine_residue_motion': 0.4200079536096653, 'cosine_ionic_motion': 0.40091494769765074, 'motion_component_glu': 4.477786492832319, 'motion_component_asn': None, 'motion_component_residue': 4.477786492832319, 'motion_component_ionic': 9.389990896036585, 'ionic_contributions': [{'ion_id': 1309, 'distance': 4.78732442855835, 'force': [-12.437792778015137, 5.437849521636963, -5.057575702667236], 'magnitude': 14.486129760742188}, {'ion_id': 1380, 'distance': 9.245156288146973, 'force': [-1.8392237424850464, 1.9834181070327759, -2.787628412246704], 'magnitude': 3.8842713832855225}, {'ion_id': 1469, 'distance': 13.138921737670898, 'force': [-1.3467543125152588, 1.3719929456710815, 0.04987660422921181], 'magnitude': 1.9231743812561035}, {'ion_id': 1476, 'distance': 12.785204887390137, 'force': [-0.6551981568336487, 0.6240441799163818, -1.8183751106262207], 'magnitude': 2.031059741973877}, {'ion_id': 2434, 'distance': 10.955573081970215, 'force': [-2.6221413612365723, 0.8223450779914856, 0.3153287470340729], 'magnitude': 2.7660999298095703}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 4.9567389488220215, 'force': [2.9764342308044434, -10.428354263305664, -0.9137062430381775], 'magnitude': 10.883225440979004}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 4.885817527770996, 'force': [-1.5794025659561157, 11.183220863342285, -1.4574053287506104], 'magnitude': 11.387843132019043}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 5.08065938949585, 'force': [-5.28672456741333, 9.062779426574707, 0.9064668416976929], 'magnitude': 10.531149864196777}], 'asn_contributions': []}, 5609: {'frame': 5609, 'ionic_force': [-12.13606995344162, 7.872880041599274, 1.560283213853836], 'ionic_force_magnitude': 14.54994562779101, 'motion_vector': [1.0545501708984375, 1.109100341796875, -1.9637222290039062], 'ionic_force_x': -12.13606995344162, 'ionic_force_y': 7.872880041599274, 'ionic_force_z': 1.560283213853836, 'radial_force': 14.466044174695467, 'axial_force': 1.560283213853836, 'glu_force': [-9.246035397052765, 33.05647277832031, -10.786303043365479], 'glu_force_magnitude': 35.98004858877625, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [-9.246035397052765, 33.05647277832031, -10.786303043365479], 'residue_force_magnitude': 35.98004858877625, 'total_force': [-21.382105350494385, 40.929352819919586, -9.226019829511642], 'total_force_magnitude': 47.09061258225085, 'motion_component_total': 16.45351990913612, 'cosine_total_motion': 0.3494012714401956, 'cosine_glu_motion': 0.5368938773038957, 'cosine_asn_motion': None, 'cosine_residue_motion': 0.5368938773038957, 'cosine_ionic_motion': -0.1968356416263346, 'motion_component_glu': 19.317467792410643, 'motion_component_asn': None, 'motion_component_residue': 19.317467792410643, 'motion_component_ionic': -2.863947883274525, 'ionic_contributions': [{'ion_id': 1309, 'distance': 6.845191478729248, 'force': [-4.694593906402588, 2.2950472831726074, 4.785083293914795], 'magnitude': 7.0854411125183105}, {'ion_id': 1380, 'distance': 8.868368148803711, 'force': [-2.6745073795318604, 2.1261026859283447, -2.479200601577759], 'magnitude': 4.221343040466309}, {'ion_id': 1469, 'distance': 13.73509407043457, 'force': [-1.283077597618103, 1.198951244354248, 0.1152741014957428], 'magnitude': 1.7598466873168945}, {'ion_id': 1476, 'distance': 12.844072341918945, 'force': [-0.8566756844520569, 0.700995147228241, -1.6807165145874023], 'magnitude': 2.0124850273132324}, {'ion_id': 2434, 'distance': 10.250850677490234, 'force': [-2.6272153854370117, 1.5517836809158325, 0.8198429346084595], 'magnitude': 3.159499406814575}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.280378580093384, 'force': [-0.3767750859260559, -24.366588592529297, 4.855916500091553], 'magnitude': 24.848590850830078}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 3.4607982635498047, 'force': [5.027754306793213, 19.39040756225586, -10.671244621276855], 'magnitude': 22.696733474731445}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.5813608169555664, 'force': [-13.897014617919922, 38.03265380859375, -4.970974922180176], 'magnitude': 40.796085357666016}], 'asn_contributions': []}, 5610: {'frame': 5610, 'ionic_force': [-9.932288229465485, 6.841108322143555, -1.9635789394378662], 'ionic_force_magnitude': 12.219114321418077, 'motion_vector': [-1.6703529357910156, -1.2484626770019531, 1.5174026489257812], 'ionic_force_x': -9.932288229465485, 'ionic_force_y': 6.841108322143555, 'ionic_force_z': -1.9635789394378662, 'radial_force': 12.06031146150382, 'axial_force': -1.9635789394378662, 'glu_force': [-13.192487955093384, 33.60896301269531, 4.265116627328098], 'glu_force_magnitude': 36.356503587098636, 'asn_force': [-0.5195410251617432, 0.018864214420318604, 2.868495464324951], 'asn_force_magnitude': 2.9152264001728283, 'residue_force': [-13.712028980255127, 33.62782722711563, 7.133612091653049], 'residue_force_magnitude': 37.00998411572578, 'total_force': [-23.64431720972061, 40.468935549259186, 5.170033152215183], 'total_force_magnitude': 47.15419094416729, 'motion_component_total': -1.234809820156706, 'cosine_total_motion': -0.0261866399450852, 'cosine_glu_motion': -0.1434623017867572, 'cosine_asn_motion': 0.6912304439874805, 'cosine_residue_motion': -0.0864819190573</t>
+          <t>{5599: {'frame': 5599, 'motion_vector': [-3.3165664672851562, 2.1229324340820312, -0.15932464599609375], 'ionic_force': [-1.9013180434703827, -9.60105836391449, -11.383936129510403], 'ionic_force_magnitude': 15.012972184430726, 'radial_force': 9.787508978780986, 'axial_force': -11.383936129510403, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-10.478373050689697, -0.794865264557302, -0.7303848266601562], 'asn_force_magnitude': 10.533830004952389, 'residue_force': [-10.478373050689697, -0.794865264557302, -0.7303848266601562], 'residue_force_magnitude': 10.533830004952389, 'total_force': [-12.37969109416008, -10.395923628471792, -12.114320956170559], 'total_force_magnitude': 20.20120669427838, 'cosine_total_motion': 0.26274734352665396, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.7992701343413963, 'cosine_residue_motion': 0.7992701343413963, 'cosine_ionic_motion': -0.20725824906676935, 'motion_component_total': 5.307813394954503, 'motion_component_glu': None, 'motion_component_asn': 8.419375723187727, 'motion_component_residue': 8.419375723187727, 'motion_component_ionic': -3.111562328233224, 'motion_component_percent_total': 26.274734352665398, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 79.92701343413962, 'motion_component_percent_residue': 79.92701343413962, 'motion_component_percent_ionic': 20.725824906676934, 'ionic_contributions': [{'ion_id': 1309, 'distance': 8.083805084228516, 'force': [3.44903564453125, 3.2919468879699707, -1.7546262741088867], 'magnitude': 5.080499172210693, 'cosine_ionic_motion': -0.20830686390399933, 'motion_component_ionic': -1.058302879333496, 'motion_component_percent_ionic': 20.830686390399933}, {'ion_id': 1380, 'distance': 10.135680198669434, 'force': [0.5980334877967834, 1.709892749786377, -2.676297664642334], 'magnitude': 3.2317094802856445, 'cosine_ionic_motion': 0.16276052594184875, 'motion_component_ionic': 0.5259947180747986, 'motion_component_percent_ionic': 16.276052594184875}, {'ion_id': 1469, 'distance': 11.055704116821289, 'force': [-0.6552402973175049, 2.634486198425293, -0.08947023004293442], 'magnitude': 2.716222047805786, 'cosine_ionic_motion': 0.7268021702766418, 'motion_component_ionic': 1.9741560220718384, 'motion_component_percent_ionic': 72.68021702766418}, {'ion_id': 1476, 'distance': 13.930360794067383, 'force': [0.27780506014823914, 0.6250635385513306, -1.5681666135787964], 'magnitude': 1.710855484008789, 'cosine_ionic_motion': 0.09721178561449051, 'motion_component_ionic': 0.16631531715393066, 'motion_component_percent_ionic': 9.721178561449051}, {'ion_id': 2434, 'distance': 4.131947994232178, 'force': [-5.57095193862915, -17.86244773864746, -5.295375347137451], 'magnitude': 19.445913314819336, 'cosine_ionic_motion': -0.2427104115486145, 'motion_component_ionic': -4.719725608825684, 'motion_component_percent_ionic': 24.27104115486145}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.984648704528809, 'force': [-4.895257949829102, -1.0194158554077148, -6.148347854614258], 'magnitude': 7.924956798553467, 'cosine_with_motion': 0.4818962514400482, 'motion_component': 3.81900691986084, 'motion_component_percent': 48.18962514400482}, {'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.503798007965088, 'force': [-6.254924297332764, -0.015604271553456783, 4.684281826019287], 'magnitude': 7.814526081085205, 'cosine_with_motion': 0.6482827067375183, 'motion_component': 5.066021919250488, 'motion_component_percent': 64.82827067375183}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.844854831695557, 'force': [8.499029159545898, -0.5871928334236145, -9.819294929504395], 'magnitude': 12.999878883361816, 'cosine_with_motion': -0.5439784526824951, 'motion_component': -7.071653842926025, 'motion_component_percent': 54.39784526824951}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.637355327606201, 'force': [-4.003154754638672, 1.6218104362487793, 4.827773094177246], 'magnitude': 6.477878570556641, 'cosine_with_motion': 0.6247857213020325, 'motion_component': 4.047286033630371, 'motion_component_percent': 62.47857213020325}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.483351230621338, 'force': [-3.8240652084350586, -0.7944627404212952, 5.725203037261963], 'magnitude': 6.93055534362793, 'cosine_with_motion': 0.36919325590133667, 'motion_component': 2.5587143898010254, 'motion_component_percent': 36.91932559013367}]}, 5600: {'frame': 5600, 'motion_vector': [-2.751720428466797, -2.4600486755371094, 0.600830078125], 'ionic_force': [-18.553392615169287, 5.5990365743637085, -7.359938099980354], 'ionic_force_magnitude': 20.7303226441178, 'radial_force': 19.379824253426055, 'axial_force': -7.359938099980354, 'glu_force': [-34.1942024230957, 6.112398624420166, 16.177690505981445], 'glu_force_magnitude': 38.318697347414876, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [-34.1942024230957, 6.112398624420166, 16.177690505981445], 'residue_force_magnitude': 38.318697347414876, 'total_force': [-52.74759503826499, 11.711435198783875, 8.817752406001091], 'total_force_magnitude': 54.74686524568918, 'cosine_total_motion': 0.5941105294947491, 'cosine_glu_motion': 0.6195228479127445, 'cosine_asn_motion': None, 'cosine_residue_motion': 0.6195228479127445, 'cosine_ionic_motion': 0.4238419604535297, 'motion_component_total': 32.52568909929408, 'motion_component_glu': 23.73930850897699, 'motion_component_asn': None, 'motion_component_residue': 23.73930850897699, 'motion_component_ionic': 8.786380590317087, 'motion_component_percent_total': 59.41105294947491, 'motion_component_percent_glu': 61.95228479127445, 'motion_component_percent_asn': None, 'motion_component_percent_residue': 61.95228479127445, 'motion_component_percent_ionic': 42.384196045352965, 'ionic_contributions': [{'ion_id': 1309, 'distance': 7.418415546417236, 'force': [-0.036227066069841385, 5.730989933013916, -1.8837703466415405], 'magnitude': 6.032756328582764, 'cosine_ionic_motion': -0.6706774830818176, 'motion_component_ionic': -4.04603385925293, 'motion_component_percent_ionic': 67.06774830818176}, {'ion_id': 1380, 'distance': 11.569257736206055, 'force': [-0.34478411078453064, 1.6263123750686646, -1.8408604860305786], 'magnitude': 2.4804306030273438, 'cosine_ionic_motion': -0.4482702612876892, 'motion_component_ionic': -1.1119033098220825, 'motion_component_percent_ionic': 44.82702612876892}, {'ion_id': 1469, 'distance': 14.104735374450684, 'force': [-0.7819127440452576, 1.468832015991211, -0.126841738820076], 'magnitude': 1.6688151359558105, 'cosine_ionic_motion': -0.2464454621076584, 'motion_component_ionic': -0.41127192974090576, 'motion_component_percent_ionic': 24.64454621076584}, {'ion_id': 1476, 'distance': 14.7647123336792, 'force': [-0.10772905498743057, 0.7481944561004639, -1.3221204280853271], 'magnitude': 1.5229586362838745, 'cosine_ionic_motion': -0.4106062948703766, 'motion_component_ionic': -0.6253364086151123, 'motion_component_percent_ionic': 41.06062948703766}, {'ion_id': 2434, 'distance': 4.310497760772705, 'force': [-17.282739639282227, -3.975292205810547, -2.186345100402832], 'magnitude': 17.86829948425293, 'cosine_ionic_motion': 0.8384079933166504, 'motion_component_ionic': 14.980925559997559, 'motion_component_percent_ionic': 83.84079933166504}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.160724401473999, 'force': [24.515661239624023, -4.078901290893555, -9.936822891235352], 'magnitude': 26.765565872192383, 'cosine_with_motion': -0.6333726048469543, 'motion_component': -16.95257568359375, 'motion_component_percent': 63.337260484695435}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 2.6899526119232178, 'force': [-26.513227462768555, 14.984768867492676, 21.998085021972656], 'magnitude': 37.56874084472656, 'cosine_with_motion': 0.35098427534103394, 'motion_component': 13.186037063598633, 'motion_component_percent': 35.098427534103394}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.8783912658691406, 'force': [-32.19663619995117, -4.793468952178955, 4.116428375244141], 'magnitude': 32.81075668334961, 'cosine_with_motion': 0.8383179903030396, 'motion_component': 27.505847930908203, 'motion_component_percent': 83.83179903030396}], 'asn_contributions': []}, 5601: {'frame': 5601, 'motion_vector': [-0.6682701110839844, -0.8040084838867188, 0.39972686767578125], 'ionic_force': [-9.747690379619598, 9.922138929367065, -7.001989342272282], 'ionic_force_magnitude': 15.572224099976358, 'radial_force': 13.909216680697368, 'axial_force': -7.001989342272282, 'glu_force': [-20.76607894897461, 27.381933212280273, 0.22750675678253174], 'glu_force_magnitude': 34.36643799815753, 'asn_force': [-1.7546709775924683, 1.6305269002914429, 8.389400959014893], 'asn_force_magnitude': 8.72465109120699, 'residue_force': [-22.520749926567078, 29.012460112571716, 8.616907715797424], 'residue_force_magnitude': 37.72476795980467, 'total_force': [-32.268440306186676, 38.93459904193878, 1.6149183735251427], 'total_force_magnitude': 50.59410245970989, 'cosine_total_motion': -0.1605919438259761, 'cosine_glu_motion': -0.20919924373673454, 'cosine_asn_motion': 0.32923574729680877, 'cosine_residue_motion': -0.114433197357825, 'cosine_ionic_motion': -0.2445404984197928, 'motion_component_total': -8.12500526013541, 'motion_component_glu': -7.189432839139933, 'motion_component_asn': 2.8724670219174513, 'motion_component_residue': -4.316965817222481, 'motion_component_ionic': -3.808039442912928, 'motion_component_percent_total': 16.05919438259761, 'motion_component_percent_glu': 20.919924373673453, 'motion_component_percent_asn': 32.92357472968088, 'motion_component_percent_residue': 11.4433197357825, 'motion_component_percent_ionic': 24.45404984197928, 'ionic_contributions': [{'ion_id': 1309, 'distance': 6.409053802490234, 'force': [-1.464813470840454, 7.521646022796631, -2.570472478866577], 'magnitude': 8.082584381103516, 'cosine_ionic_motion': -0.6738434433937073, 'motion_component_ionic': -5.446396350860596, 'motion_component_percent_ionic': 67.38434433937073}, {'ion_id': 1380, 'distance': 10.99662971496582, 'force': [-1.123779535293579, 1.281681776046753, -2.1522297859191895], 'magnitude': 2.745483875274658, 'cosine_ionic_motion': -0.3709104657173157, 'motion_component_ionic': -1.0183286666870117, 'motion_component_percent_ionic': 37.09104657173157}, {'ion_id': 1469, 'distance': 13.696661949157715, 'force': [-1.2938627004623413, 1.2048321962356567, -0.07915589958429337], 'magnitude': 1.769736409187317, 'cosine_ionic_motion': -0.06849946826696396, 'motion_component_ionic': -0.1212259978055954, 'motion_component_percent_ionic': 6.849946826696396}, {'ion_id': 1476, 'distance': 14.374396324157715, 'force': [-0.5480816960334778, 0.5199006199836731, -1.4181257486343384], 'magnitude': 1.606788992881775, 'cosine_ionic_motion': -0.34396278858184814, 'motion_component_ionic': -0.5526756048202515, 'motion_component_percent_ionic': 34.396278858184814}, {'ion_id': 2434, 'distance': 7.834921360015869, 'force': [-5.317152976989746, -0.6059216856956482, -0.7820054292678833], 'magnitude': 5.408400058746338, 'cosine_ionic_motion': 0.6158174276351929, 'motion_component_ionic': 3.3305869102478027, 'motion_component_percent_ionic': 61.58174276351929}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.2818381786346436, 'force': [14.98430061340332, -18.21042251586914, -7.759255409240723], 'magnitude': 24.826494216918945, 'cosine_with_motion': 0.05492289736866951, 'motion_component': 1.3635430335998535, 'motion_component_percent': 5.492289736866951}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 2.618565559387207, 'force': [-17.718032836914062, 35.45824432373047, 0.7173105478286743], 'magnitude': 39.64505386352539, 'cosine_with_motion': -0.3691698908805847, 'motion_component': -14.635760307312012, 'motion_component_percent': 36.91698908805847}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 3.521170139312744, 'force': [-18.032346725463867, 10.134111404418945, 7.26945161819458], 'magnitude': 21.92511558532715, 'cosine_with_motion': 0.2774345576763153, 'motion_component': 6.082784652709961, 'motion_component_percent': 27.74345576763153}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.179820537567139, 'force': [-2.1817688941955566, 0.38443517684936523, 8.539961814880371], 'magnitude': 8.822632789611816, 'cosine_with_motion': 0.46203142404556274, 'motion_component': 4.076333522796631, 'motion_component_percent': 46.203142404556274}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.6257147789001465, 'force': [4.295049667358398, -3.9265239238739014, -13.01939582824707], 'magnitude': 14.260774612426758, 'cosine_with_motion': -0.3080780506134033, 'motion_component': -4.393431663513184, 'motion_component_percent': 30.807805061340332}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.978527069091797, 'force': [-2.5541765689849854, 1.991648554801941, 4.593373775482178], 'magnitude': 5.62045955657959, 'cosine_with_motion': 0.30864834785461426, 'motion_component': 1.7347455024719238, 'motion_component_percent': 30.864834785461426}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 3.9424872398376465, 'force': [-1.3137751817703247, 3.180967092514038, 8.275461196899414], 'magnitude': 8.962578773498535, 'cosine_with_motion': 0.16232159733772278, 'motion_component': 1.4548200368881226, 'motion_component_percent': 16.232159733772278}]}, 5602: {'frame': 5602, 'motion_vector': [1.2005729675292969, 0.9844474792480469, -0.0977783203125], 'ionic_force': [-9.748128592967987, 11.87373073399067, -8.434279189445078], 'ionic_force_magnitude': 17.525654283189, 'radial_force': 15.362665543724976, 'axial_force': -8.434279189445078, 'glu_force': [-13.67834460735321, 34.34225273132324, -5.655503749847412], 'glu_force_magnitude': 37.39615162719455, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [-13.67834460735321, 34.34225273132324, -5.655503749847412], 'residue_force_magnitude': 37.39615162719455, 'total_force': [-23.426473200321198, 46.21598346531391, -14.08978293929249], 'total_force_magnitude': 53.69579832303375, 'cosine_total_motion': 0.22446034023916853, 'cosine_glu_motion': 0.3083641148932268, 'cosine_asn_motion': None, 'cosine_residue_motion': 0.3083641148932268, 'cosine_ionic_motion': 0.029724765515252854, 'motion_component_total': 12.05257716100193, 'motion_component_glu': 11.53163119693275, 'motion_component_asn': None, 'motion_component_residue': 11.53163119693275, 'motion_component_ionic': 0.5209459640691798, 'motion_component_percent_total': 22.44603402391685, 'motion_component_percent_glu': 30.83641148932268, 'motion_component_percent_asn': None, 'motion_component_percent_residue': 30.83641148932268, 'motion_component_percent_ionic': 2.9724765515252853, 'ionic_contributions': [{'ion_id': 1309, 'distance': 5.589580535888672, 'force': [-2.806483507156372, 9.153647422790527, -4.609921932220459], 'magnitude': 10.626240730285645, 'cosine_ionic_motion': 0.36856338381767273, 'motion_component_ionic': 3.916443109512329, 'motion_component_percent_ionic': 36.85633838176727}, {'ion_id': 1380, 'distance': 10.90501594543457, 'force': [-1.2517857551574707, 1.1912050247192383, -2.192772626876831], 'magnitude': 2.7918074131011963, 'cosine_ionic_motion': -0.02665742300450802, 'motion_component_ionic': -0.07442238926887512, 'motion_component_percent_ionic': 2.665742300450802}, {'ion_id': 1469, 'distance': 13.315174102783203, 'force': [-1.356601595878601, 1.2908194065093994, -0.006111637689173222], 'magnitude': 1.872597098350525, 'cosine_ionic_motion': -0.12267178297042847, 'motion_component_ionic': -0.22971482574939728, 'motion_component_percent_ionic': 12.267178297042847}, {'ion_id': 1476, 'distance': 14.112052917480469, 'force': [-0.6084700226783752, 0.47949525713920593, -1.4761505126953125], 'magnitude': 1.667084813117981, 'cosine_ionic_motion': -0.044011190533638, 'motion_component_ionic': -0.07337038964033127, 'motion_component_percent_ionic': 4.4011190533638}, {'ion_id': 2434, 'distance': 9.427346229553223, 'force': [-3.724787712097168, -0.24143637716770172, -0.1493224799633026], 'magnitude': 3.7355899810791016, 'cosine_ionic_motion': -0.8079016804695129, 'motion_component_ionic': -3.01798939704895, 'motion_component_percent_ionic': 80.7901680469513}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 2.9619991779327393, 'force': [9.577141761779785, -28.668466567993164, -3.9086532592773438], 'magnitude': 30.477535247802734, 'cosine_with_motion': -0.3446836769580841, 'motion_component': -10.505108833312988, 'motion_component_percent': 34.46836769580841}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 2.6011602878570557, 'force': [-1.2337597608566284, 39.29288101196289, -8.292745590209961], 'magnitude': 40.17738342285156, 'cosine_with_motion': 0.6081603765487671, 'motion_component': 24.43429183959961, 'motion_component_percent': 60.81603765487671}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.8692431449890137, 'force': [-22.021726608276367, 23.717838287353516, 6.545895099639893], 'magnitude': 33.02031326293945, 'cosine_with_motion': -0.07260838150978088, 'motion_component': -2.3975515365600586, 'motion_component_percent': 7.260838150978088}], 'asn_contributions': []}, 5603: {'frame': 5603, 'motion_vector': [-1.2378005981445312, -0.32138824462890625, 0.05432891845703125], 'ionic_force': [-17.560770630836487, 16.140983641147614, -9.764761259779334], 'ionic_force_magnitude': 25.773291999919827, 'radial_force': 23.851876614904835, 'axial_force': -9.764761259779334, 'glu_force': [-8.688776016235352, 18.961535453796387, -3.2987524271011353], 'glu_force_magnitude': 21.11673324643728, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [-8.688776016235352, 18.961535453796387, -3.2987524271011353], 'residue_force_magnitude': 21.11673324643728, 'total_force': [-26.24954664707184, 35.102519094944, -13.06351368688047], 'total_force_magnitude': 45.7370849074908, 'cosine_total_motion': 0.35017550339148107, 'cosine_glu_motion': 0.165810085529384, 'cosine_asn_motion': None, 'cosine_residue_motion': 0.165810085529384, 'cosine_ionic_motion': 0.4855661971891475, 'motion_component_total': 16.016006731139502, 'motion_component_glu': 3.501367345692952, 'motion_component_asn': None, 'motion_component_residue': 3.501367345692952, 'motion_component_ionic': 12.514639385446548, 'motion_component_percent_total': 35.01755033914811, 'motion_component_percent_glu': 16.5810085529384, 'motion_component_percent_asn': None, 'motion_component_percent_residue': 16.5810085529384, 'motion_component_percent_ionic': 48.55661971891475, 'ionic_contributions': [{'ion_id': 1309, 'distance': 4.739724159240723, 'force': [-7.167101860046387, 12.286242485046387, -4.010806083679199], 'magnitude': 14.77855396270752, 'cosine_ionic_motion': 0.24871857464313507, 'motion_component_ionic': 3.6757009029388428, 'motion_component_percent_ionic': 24.871857464313507}, {'ion_id': 1380, 'distance': 9.010942459106445, 'force': [-1.6355546712875366, 2.433621406555176, -2.8497138023376465], 'magnitude': 4.0888166427612305, 'cosine_ionic_motion': 0.20779502391815186, 'motion_component_ionic': 0.8496357798576355, 'motion_component_percent_ionic': 20.779502391815186}, {'ion_id': 1469, 'distance': 13.02607250213623, 'force': [-1.2709964513778687, 1.487382173538208, -0.02657478116452694], 'magnitude': 1.9566409587860107, 'cosine_ionic_motion': 0.4367225468158722, 'motion_component_ionic': 0.8545092344284058, 'motion_component_percent_ionic': 43.67225468158722}, {'ion_id': 1476, 'distance': 13.13216495513916, 'force': [-0.5827058553695679, 0.6906329989433289, -1.6999109983444214], 'magnitude': 1.9251538515090942, 'cosine_ionic_motion': 0.16514870524406433, 'motion_component_ionic': 0.31793665885925293, 'motion_component_percent_ionic': 16.514870524406433}, {'ion_id': 2434, 'distance': 6.864849090576172, 'force': [-6.904411792755127, -0.7568954229354858, -1.17775559425354], 'magnitude': 7.044920444488525, 'cosine_ionic_motion': 0.9676271677017212, 'motion_component_ionic': 6.816856384277344, 'motion_component_percent_ionic': 96.76271677017212}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.8883092403411865, 'force': [7.783102989196777, -15.684765815734863, -2.4907524585723877], 'magnitude': 17.685937881469727, 'cosine_with_motion': -0.20886830985546112, 'motion_component': -3.6940319538116455, 'motion_component_percent': 20.886830985546112}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 3.3359897136688232, 'force': [-5.854516983032227, 23.5977840423584, -2.3532145023345947], 'magnitude': 24.426795959472656, 'cosine_with_motion': -0.014877845533192158, 'motion_component': -0.3634181022644043, 'motion_component_percent': 1.4877845533192158}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 4.201320171356201, 'force': [-10.617362022399902, 11.048517227172852, 1.5452145338058472], 'magnitude': 15.400837898254395, 'cosine_with_motion': 0.49080559611320496, 'motion_component': 7.558817386627197, 'motion_component_percent': 49.080559611320496}], 'asn_contributions': []}, 5604: {'frame': 5604, 'motion_vector': [0.9648094177246094, 0.07035064697265625, 0.3220977783203125], 'ionic_force': [-14.2177032828331, 19.06482544541359, -2.1827616719529033], 'ionic_force_magnitude': 23.882527178238888, 'radial_force': 23.782570422533652, 'axial_force': -2.1827616719529033, 'glu_force': [-9.147841453552246, 32.45199394226074, -0.4819430708885193], 'glu_force_magnitude': 33.72013023716596, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [-9.147841453552246, 32.45199394226074, -0.4819430708885193], 'residue_force_magnitude': 33.72013023716596, 'total_force': [-23.365544736385345, 51.51681938767433, -2.6647047428414226], 'total_force_magnitude': 56.6306631783242, 'cosine_total_motion': -0.3425256324799066, 'cosine_glu_motion': -0.19482353079901096, 'cosine_asn_motion': None, 'cosine_residue_motion': -0.19482353079901096, 'cosine_ionic_motion': -0.5371282023618255, 'motion_component_total': -19.397453722912054, 'motion_component_glu': -6.569474831807163, 'motion_component_asn': None, 'motion_component_residue': -6.569474831807163, 'motion_component_ionic': -12.827978891104895, 'motion_component_percent_total': 34.25256324799066, 'motion_component_percent_glu': 19.482353079901095, 'motion_component_percent_asn': None, 'motion_component_percent_residue': 19.482353079901095, 'motion_component_percent_ionic': 53.712820236182544, 'ionic_contributions': [{'ion_id': 1309, 'distance': 4.387622833251953, 'force': [-7.5053019523620605, 15.458601951599121, 1.4540939331054688], 'magnitude': 17.245647430419922, 'cosine_ionic_motion': -0.3233335018157959, 'motion_component_ionic': -5.5760955810546875, 'motion_component_percent_ionic': 32.33335018157959}, {'ion_id': 1380, 'distance': 10.315604209899902, 'force': [-1.4976059198379517, 1.5437307357788086, -2.2601349353790283], 'magnitude': 3.1199581623077393, 'cosine_ionic_motion': -0.6489298939704895, 'motion_component_ionic': -2.0246341228485107, 'motion_component_percent_ionic': 64.89298939704895}, {'ion_id': 1469, 'distance': 13.825953483581543, 'force': [-1.2702255249023438, 1.183520793914795, 0.04746720567345619], 'magnitude': 1.7367923259735107, 'cosine_ionic_motion': -0.6364187598228455, 'motion_component_ionic': -1.1053272485733032, 'motion_component_percent_ionic': 63.641875982284546}, {'ion_id': 1476, 'distance': 14.050297737121582, 'force': [-0.6734047532081604, 0.5765787363052368, -1.429139256477356], 'magnitude': 1.6817716360092163, 'cosine_ionic_motion': -0.6237018704414368, 'motion_component_ionic': -1.0489240884780884, 'motion_component_percent_ionic': 62.37018704414368}, {'ion_id': 2434, 'distance': 10.052953720092773, 'force': [-3.271165132522583, 0.30239322781562805, 0.004951381124556065], 'magnitude': 3.285115957260132, 'cosine_ionic_motion': -0.935430645942688, 'motion_component_ionic': -3.072998046875, 'motion_component_percent_ionic': 93.5430645942688}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.1217877864837646, 'force': [6.149357795715332, -25.953346252441406, -6.435849666595459], 'magnitude': 27.437400817871094, 'cosine_with_motion': 0.07271376997232437, 'motion_component': 1.9950768947601318, 'motion_component_percent': 7.271376997232437}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 2.816182851791382, 'force': [3.228656768798828, 34.113380432128906, -0.8480800986289978], 'magnitude': 34.27632141113281, 'cosine_with_motion': 0.14998939633369446, 'motion_component': 5.141084671020508, 'motion_component_percent': 14.998939633369446}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.9471259117126465, 'force': [-18.525856018066406, 24.291959762573242, 6.8019866943359375], 'magnitude': 31.298141479492188, 'cosine_with_motion': -0.4379057288169861, 'motion_component': -13.705635070800781, 'motion_component_percent': 43.79057288169861}], 'asn_contributions': []}, 5605: {'frame': 5605, 'motion_vector': [-0.040676116943359375, 0.6826667785644531, -0.5590362548828125], 'ionic_force': [-18.65671706199646, 11.948305934667587, -10.66128496825695], 'ionic_force_magnitude': 24.586543136727947, 'radial_force': 22.154798718106253, 'axial_force': -10.66128496825695, 'glu_force': [-10.341562330722809, 32.2280387878418, 1.596648931503296], 'glu_force_magnitude': 33.884268966016236, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [-10.341562330722809, 32.2280387878418, 1.596648931503296], 'residue_force_magnitude': 33.884268966016236, 'total_force': [-28.99827939271927, 44.176344722509384, -9.064636036753654], 'total_force_magnitude': 53.61545735381731, 'cosine_total_motion': 0.7687089159639758, 'cosine_glu_motion': 0.7193191344814241, 'cosine_asn_motion': None, 'cosine_residue_motion': 0.7193191344814241, 'cosine_ionic_motion': 0.6849713268978227, 'motion_component_total': 41.21468010136568, 'motion_component_glu': 24.37360302517058, 'motion_component_asn': None, 'motion_component_residue': 24.37360302517058, 'motion_component_ionic': 16.8410770761951, 'motion_component_percent_total': 76.87089159639758, 'motion_component_percent_glu': 71.93191344814241, 'motion_component_percent_asn': None, 'motion_component_percent_residue': 71.93191344814241, 'motion_component_percent_ionic': 68.49713268978228, 'ionic_contributions': [{'ion_id': 1309, 'distance': 4.6242804527282715, 'force': [-11.117942810058594, 8.545702934265137, -6.663941860198975], 'magnitude': 15.525650024414062, 'cosine_ionic_motion': 0.7300338745117188, 'motion_component_ionic': 11.334250450134277, 'motion_component_percent_ionic': 73.00338745117188}, {'ion_id': 1380, 'distance': 10.08809757232666, 'force': [-1.4706867933273315, 1.5739147663116455, -2.449951410293579], 'magnitude': 3.262267589569092, 'cosine_ionic_motion': 0.8689411878585815, 'motion_component_ionic': 2.834718704223633, 'motion_component_percent_ionic': 86.89411878585815}, {'ion_id': 1469, 'distance': 13.289344787597656, 'force': [-1.0578231811523438, 1.5526583194732666, 0.06499066203832626], 'magnitude': 1.8798832893371582, 'cosine_ionic_motion': 0.6423665881156921, 'motion_component_ionic': 1.2075742483139038, 'motion_component_percent_ionic': 64.23665881156921}, {'ion_id': 1476, 'distance': 13.405807495117188, 'force': [-0.48204028606414795, 0.6503790020942688, -1.660539984703064], 'magnitude': 1.8473626375198364, 'cosine_ionic_motion': 0.853003203868866, 'motion_component_ionic': 1.5758062601089478, 'motion_component_percent_ionic': 85.3003203868866}, {'ion_id': 2434, 'distance': 8.547780990600586, 'force': [-4.528223991394043, -0.37434908747673035, 0.048157624900341034], 'magnitude': 4.54392671585083, 'cosine_ionic_motion': -0.024488314986228943, 'motion_component_ionic': -0.11127310991287231, 'motion_component_percent_ionic': 2.4488314986228943}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.267085552215576, 'force': [7.773112773895264, -22.777538299560547, -6.951651573181152], 'magnitude': 25.051206588745117, 'cosine_with_motion': -0.5413791537284851, 'motion_component': -13.562201499938965, 'motion_component_percent': 54.13791537284851}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 2.757434368133545, 'force': [-0.8180308938026428, 35.714202880859375, 1.4362404346466064], 'magnitude': 35.7524299621582, 'cosine_with_motion': 0.7476664185523987, 'motion_component': 26.730892181396484, 'motion_component_percent': 74.76664185523987}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 3.1808032989501953, 'force': [-17.29664421081543, 19.29137420654297, 7.112060070037842], 'magnitude': 26.868427276611328, 'cosine_with_motion': 0.41702887415885925, 'motion_component': 11.204910278320312, 'motion_component_percent': 41.702887415885925}], 'asn_contributions': []}, 5606: {'frame': 5606, 'motion_vector': [-0.3365478515625, -0.6044425964355469, 0.14295196533203125], 'ionic_force': [-21.41411665081978, 2.977629542350769, -6.465997515246272], 'ionic_force_magnitude': 22.566342049467565, 'radial_force': 21.62014499549892, 'axial_force': -6.465997515246272, 'glu_force': [-15.111041069030762, 33.415127754211426, -0.8798074722290039], 'glu_force_magnitude': 36.68362558701627, 'asn_force': [1.0994532108306885, 0.4009546935558319, 0.7341213226318359], 'asn_force_magnitude': 1.3814833134834013, 'residue_force': [-14.011587858200073, 33.81608244776726, -0.14568614959716797], 'residue_force_magnitude': 36.60427913340784, 'total_force': [-35.42570450901985, 36.79371199011803, -6.61168366484344], 'total_force_magnitude': 51.502156681600255, 'cosine_total_motion': -0.3095516416699686, 'cosine_glu_motion': -0.5879970714475303, 'cosine_asn_motion': -0.5199445990274864, 'cosine_residue_motion': -0.6088949087483513, 'cosine_ionic_motion': 0.2811967503856907, 'motion_component_total': -15.942577150333303, 'motion_component_glu': -21.56986441524326, 'motion_component_asn': -0.7182947874922903, 'motion_component_residue': -22.28815920273555, 'motion_component_ionic': 6.345582052402246, 'motion_component_percent_total': 30.955164166996862, 'motion_component_percent_glu': 58.799707144753036, 'motion_component_percent_asn': 51.99445990274864, 'motion_component_percent_residue': 60.889490874835126, 'motion_component_percent_ionic': 28.11967503856907, 'ionic_contributions': [{'ion_id': 1309, 'distance': 5.460677623748779, 'force': [-7.701904296875, 6.24114990234375, -5.068641662597656], 'magnitude': 11.133840560913086, 'cosine_ionic_motion': -0.2421931028366089, 'motion_component_ionic': -2.6965394020080566, 'motion_component_percent_ionic': 24.21931028366089}, {'ion_id': 1380, 'distance': 10.715598106384277, 'force': [-1.0523978471755981, 1.6155245304107666, -2.1546742916107178], 'magnitude': 2.891380786895752, 'cosine_ionic_motion': -0.45546698570251465, 'motion_component_ionic': -1.316928505897522, 'motion_component_percent_ionic': 45.546698570251465}, {'ion_id': 1469, 'distance': 14.11843490600586, 'force': [-1.061071753501892, 1.283768892288208, -0.014648376032710075], 'magnitude': 1.6655781269073486, 'cosine_ionic_motion': -0.35776734352111816, 'motion_component_ionic': -0.5958894491195679, 'motion_component_percent_ionic': 35.776734352111816}, {'ion_id': 1476, 'distance': 13.845550537109375, 'force': [-0.44619205594062805, 0.6866577863693237, -1.5260471105575562], 'magnitude': 1.7318793535232544, 'cosine_ionic_motion': -0.3948078155517578, 'motion_component_ionic': -0.6837595105171204, 'motion_component_percent_ionic': 39.48078155517578}, {'ion_id': 2434, 'distance': 4.998462200164795, 'force': [-11.15255069732666, -6.849471569061279, 2.298013925552368], 'magnitude': 13.288171768188477, 'cosine_ionic_motion': 0.8758690357208252, 'motion_component_ionic': 11.63869857788086, 'motion_component_percent_ionic': 87.58690357208252}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.3145811557769775, '</t>
         </is>
       </c>
     </row>
@@ -739,7 +739,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>{5689: {'frame': 5689, 'ionic_force': [-10.846781343221664, 1.6348312199115753, -4.6059174835681915], 'ionic_force_magnitude': 11.897050663534147, 'motion_vector': [1.6955833435058594, -2.072643280029297, 4.204833984375], 'ionic_force_x': -10.846781343221664, 'ionic_force_y': 1.6348312199115753, 'ionic_force_z': -4.6059174835681915, 'radial_force': 10.969290707482374, 'axial_force': -4.6059174835681915, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.057557977735996246, -1.561832070350647, -1.0622444152832031], 'asn_force_magnitude': 1.889707790791264, 'residue_force': [0.057557977735996246, -1.561832070350647, -1.0622444152832031], 'residue_force_magnitude': 1.889707790791264, 'total_force': [-10.789223365485668, 0.07299914956092834, -5.668161898851395], 'total_force_magnitude': 12.187728624225647, 'motion_component_total': -8.481030857452163, 'cosine_total_motion': -0.6958664012746681, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.12014802608635168, 'cosine_residue_motion': -0.12014802608635168, 'cosine_ionic_motion': -0.6937842352649658, 'motion_component_glu': None, 'motion_component_asn': -0.2270446609435708, 'motion_component_residue': -0.2270446609435708, 'motion_component_ionic': -8.253986196508592, 'ionic_contributions': [{'ion_id': 1355, 'distance': 12.842514038085938, 'force': [-0.2695693075656891, 0.3014860451221466, -1.9719277620315552], 'magnitude': 2.0129730701446533}, {'ion_id': 1469, 'distance': 9.714579582214355, 'force': [-2.6125478744506836, 2.329728126525879, -0.3506489098072052], 'magnitude': 3.5179531574249268}, {'ion_id': 1476, 'distance': 7.228488922119141, 'force': [-1.3893324136734009, 1.863111972808838, -5.913637638092041], 'magnitude': 6.353939056396484}, {'ion_id': 2434, 'distance': 7.680809497833252, 'force': [-0.631294310092926, -5.49688720703125, -1.0274757146835327], 'magnitude': 5.62761116027832}, {'ion_id': 2443, 'distance': 6.442495822906494, 'force': [-5.944037437438965, 2.637392282485962, 4.657772541046143], 'magnitude': 7.998891353607178}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.862374305725098, 'force': [1.5012428760528564, -4.139888286590576, 8.99179458618164], 'magnitude': 10.01223087310791}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.928593635559082, 'force': [0.669931948184967, 3.9480724334716797, -7.0480637550354], 'magnitude': 8.106249809265137}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.005432605743408, 'force': [-2.076143741607666, 2.082576036453247, -11.818824768066406], 'magnitude': 12.179166793823242}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.1369948387146, 'force': [-0.034623049199581146, -0.46103692054748535, 5.258759498596191], 'magnitude': 5.279044151306152}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.172613143920898, 'force': [1.7645483016967773, -0.3997570276260376, 4.882126808166504], 'magnitude': 5.206592082977295}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.840487003326416, 'force': [-4.325311660766602, -6.203693866729736, -4.77777624130249], 'magnitude': 8.945462226867676}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.982481002807617, 'force': [2.557913303375244, 3.6118955612182617, 3.449739456176758], 'magnitude': 5.611542701721191}]}, 5692: {'frame': 5692, 'ionic_force': [-2.2680077254772186, -15.304942309856415, -10.105775147676468], 'ionic_force_magnitude': 18.48003813541121, 'motion_vector': [5.063621520996094, 4.651702880859375, -0.6800384521484375], 'ionic_force_x': -2.2680077254772186, 'ionic_force_y': -15.304942309856415, 'ionic_force_z': -10.105775147676468, 'radial_force': 15.472075431268339, 'axial_force': -10.105775147676468, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [2.5782699584960938, 3.2258684039115906, -0.9870598316192627], 'asn_force_magnitude': 4.245938064719598, 'residue_force': [2.5782699584960938, 3.2258684039115906, -0.9870598316192627], 'residue_force_magnitude': 4.245938064719598, 'total_force': [0.3102622330188751, -12.079073905944824, -11.09283497929573], 'total_force_magnitude': 16.4027825979741, 'motion_component_total': -6.8128987085620665, 'cosine_total_motion': -0.4153501802434134, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.9793823974703162, 'cosine_residue_motion': 0.9793823974703162, 'cosine_ionic_motion': -0.5936836076585019, 'motion_component_glu': None, 'motion_component_asn': 4.158397001335555, 'motion_component_residue': 4.158397001335555, 'motion_component_ionic': -10.971295709897621, 'ionic_contributions': [{'ion_id': 1355, 'distance': 13.362324714660645, 'force': [-0.16544833779335022, -0.5105010867118835, -1.7802817821502686], 'magnitude': 1.859405279159546}, {'ion_id': 1469, 'distance': 6.331493854522705, 'force': [-8.14029312133789, 1.124986171722412, -1.0288584232330322], 'magnitude': 8.281818389892578}, {'ion_id': 1476, 'distance': 8.040470123291016, 'force': [-0.7527567744255066, -2.250356912612915, -4.554305553436279], 'magnitude': 5.135411262512207}, {'ion_id': 2434, 'distance': 11.164103507995605, 'force': [-0.9204217195510864, -2.4938366413116455, -0.17049100995063782], 'magnitude': 2.663731336593628}, {'ion_id': 2443, 'distance': 4.901560306549072, 'force': [7.710912227630615, -11.175233840942383, -2.57183837890625], 'magnitude': 13.818768501281738}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.955214023590088, 'force': [-7.112100124359131, 0.5117895007133484, 6.488199234008789], 'magnitude': 9.640571594238281}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.565440654754639, 'force': [6.408121585845947, 1.6682206392288208, -6.738068580627441], 'magnitude': 9.447145462036133}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.608523845672607, 'force': [9.413819313049316, -4.310042858123779, -9.961161613464355], 'magnitude': 14.367365837097168}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.879380702972412, 'force': [-4.83558988571167, 3.2670257091522217, 7.185204982757568], 'magnitude': 9.25654125213623}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.195611476898193, 'force': [-3.49900484085083, 2.236114978790283, 3.0640740394592285], 'magnitude': 5.160600185394287}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.786916732788086, 'force': [5.836784839630127, -2.088743209838867, 8.26351261138916], 'magnitude': 10.33036994934082}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.929454326629639, 'force': [-2.7333264350891113, 1.915501356124878, -7.384117126464844], 'magnitude': 8.103419303894043}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.011087894439697, 'force': [-8.006246566772461, 4.756603240966797, -7.806305408477783], 'magnitude': 12.151694297790527}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.242641925811768, 'force': [2.7847952842712402, -2.780026912689209, 3.1945762634277344], 'magnitude': 5.068427085876465}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.051477909088135, 'force': [4.321016788482666, -1.9505740404129028, 2.7070257663726807], 'magnitude': 5.459296226501465}]}, 5693: {'frame': 5693, 'ionic_force': [14.037217020988464, 0.7251570634543896, -12.502707362174988], 'ionic_force_magnitude': 18.811884696786514, 'motion_vector': [0.5311241149902344, 0.9281234741210938, 2.3688735961914062], 'ionic_force_x': 14.037217020988464, 'ionic_force_y': 0.7251570634543896, 'ionic_force_z': -12.502707362174988, 'radial_force': 14.055935204069705, 'axial_force': -12.502707362174988, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [1.5051481127738953, -1.2537007331848145, -0.4803304672241211], 'asn_force_magnitude': 2.016916886616477, 'residue_force': [1.5051481127738953, -1.2537007331848145, -0.4803304672241211], 'residue_force_magnitude': 2.016916886616477, 'total_force': [15.54236513376236, -0.5285436697304249, -12.983037829399109], 'total_force_magnitude': 20.258424016729737, 'motion_component_total': -8.84584423483109, 'cosine_total_motion': -0.43665016723542005, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.28653004267432075, 'cosine_residue_motion': -0.28653004267432075, 'cosine_ionic_motion': -0.4395060402773284, 'motion_component_glu': None, 'motion_component_asn': -0.5779072815927773, 'motion_component_residue': -0.5779072815927773, 'motion_component_ionic': -8.267936953238312, 'ionic_contributions': [{'ion_id': 1355, 'distance': 14.424660682678223, 'force': [0.4393165409564972, 0.04694287106394768, -1.5332221984863281], 'magnitude': 1.595610499382019}, {'ion_id': 1469, 'distance': 6.90531063079834, 'force': [-0.2973380386829376, 6.702067852020264, -1.863255262374878], 'magnitude': 6.9626030921936035}, {'ion_id': 1476, 'distance': 9.697990417480469, 'force': [1.3921409845352173, 0.3217581510543823, -3.227895498275757], 'magnitude': 3.529999256134033}, {'ion_id': 2434, 'distance': 6.285351276397705, 'force': [2.518434524536133, -7.808837413787842, -1.8178147077560425], 'magnitude': 8.403862953186035}, {'ion_id': 2443, 'distance': 5.524619102478027, 'force': [9.984663009643555, 1.4632256031036377, -4.060519695281982], 'magnitude': 10.877607345581055}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.116811752319336, 'force': [-3.8710646629333496, -6.429830074310303, 5.041471004486084], 'magnitude': 9.041254997253418}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.730896472930908, 'force': [5.400066375732422, 5.145687103271484, -4.665219783782959], 'magnitude': 8.797903060913086}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.740130424499512, 'force': [2.9290695190429688, 9.451510429382324, -9.301790237426758], 'magnitude': 13.58064079284668}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.183035850524902, 'force': [-1.4411402940750122, -4.443267822265625, 6.447065353393555], 'magnitude': 7.961417198181152}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.227376461029053, 'force': [-0.31844228506088257, -3.9280471801757812, 3.2340965270996094], 'magnitude': 5.098072528839111}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.659245491027832, 'force': [1.005800485610962, 6.544600963592529, 3.2840981483459473], 'magnitude': 7.391125679016113}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.649864196777344, 'force': [-2.199141025543213, -7.594354152679443, -4.5200514793396], 'magnitude': 9.107211112976074}]}, 5694: {'frame': 5694, 'ionic_force': [15.186673760414124, -2.523807108402252, -6.381444334983826], 'ionic_force_magnitude': 16.66515808584394, 'motion_vector': [-6.16156005859375, -6.210399627685547, -0.5569686889648438], 'ionic_force_x': 15.186673760414124, 'ionic_force_y': -2.523807108402252, 'ionic_force_z': -6.381444334983826, 'radial_force': 15.39495573964643, 'axial_force': -6.381444334983826, 'glu_force': [4.446905136108398, 5.983371257781982, 1.298695683479309], 'glu_force_magnitude': 7.567186225823082, 'asn_force': [1.872458316385746, -0.19104492664337158, -0.5029773712158203], 'asn_force_magnitude': 1.9482259998659013, 'residue_force': [6.319363452494144, 5.792326331138611, 0.7957183122634888], 'residue_force_magnitude': 8.609214040990725, 'total_force': [21.506037212908268, 3.2685192227363586, -5.585726022720337], 'total_force_magnitude': 22.45869964430905, 'motion_component_total': -17.07702021107542, 'cosine_total_motion': -0.7603743975178311, 'cosine_glu_motion': -0.9841378927108955, 'cosine_asn_motion': -0.5896755991616716, 'cosine_residue_motion': -0.9984623449803918, 'cosine_ionic_motion': -0.5089087140717763, 'motion_component_glu': -7.447154706032443, 'motion_component_asn': -1.148821333773272, 'motion_component_residue': -8.595976039805715, 'motion_component_ionic': -8.481044171269705, 'ionic_contributions': [{'ion_id': 1355, 'distance': 12.02578067779541, 'force': [0.7672042846679688, 0.321216881275177, -2.13971209526062], 'magnitude': 2.2956807613372803}, {'ion_id': 1469, 'distance': 7.6157989501953125, 'force': [0.36691606044769287, 5.6577959060668945, 0.787419319152832], 'magnitude': 5.724099159240723}, {'ion_id': 1476, 'distance': 7.09453010559082, 'force': [4.058429718017578, 1.9305769205093384, -4.828175067901611], 'magnitude': 6.596154689788818}, {'ion_id': 2434, 'distance': 5.142002105712891, 'force': [3.7240912914276123, -11.90422248840332, -1.445675253868103], 'magnitude': 12.556645393371582}, {'ion_id': 2443, 'distance': 7.114371299743652, 'force': [6.2700324058532715, 1.4708256721496582, 1.2446987628936768], 'magnitude': 6.559413909912109}], 'glu_contributions': [{'resid': 423, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 5.993641376495361, 'force': [4.446905136108398, 5.983371257781982, 1.298695683479309], 'magnitude': 7.56718635559082}], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.322994709014893, 'force': [-2.409579277038574, -3.641601324081421, 7.12241268157959], 'magnitude': 8.354405403137207}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.167766094207764, 'force': [3.4821557998657227, 2.2395565509796143, -6.101158618927002], 'magnitude': 7.3732733726501465}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.217445373535156, 'force': [0.6987098455429077, 4.0230584144592285, -10.439300537109375], 'magnitude': 11.209468841552734}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.1344733238220215, 'force': [-0.11744511872529984, -0.9304448366165161, 5.200343132019043], 'magnitude': 5.2842302322387695}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.779999256134033, 'force': [0.21861706674098969, -1.8816137313842773, 3.714725971221924], 'magnitude': 4.169826507568359}]}, 5695: {'frame': 5695, 'ionic_force': [-17.885726302862167, -13.695586919784546, -6.164025843143463], 'ionic_force_magnitude': 23.35516048014249, 'motion_vector': [2.018024444580078, -2.0229759216308594, -1.58453369140625], 'ionic_force_x': -17.885726302862167, 'ionic_force_y': -13.695586919784546, 'ionic_force_z': -6.164025843143463, 'radial_force': 22.527057208127943, 'axial_force': -6.164025843143463, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [6.174872726202011, -0.7085607051849365, -5.937305212020874], 'asn_force_magnitude': 8.595504908870442, 'residue_force': [6.174872726202011, -0.7085607051849365, -5.937305212020874], 'residue_force_magnitude': 8.595504908870442, 'total_force': [-11.710853576660156, -14.404147624969482, -12.101331055164337], 'total_force_magnitude': 22.160003917025215, 'motion_component_total': 7.553948628901599, 'cosine_total_motion': 0.3408820980892521, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.8297195954635821, 'cosine_residue_motion': 0.8297195954635821, 'cosine_ionic_motion': 0.018072655654293633, 'motion_component_glu': None, 'motion_component_asn': 7.131858855793217, 'motion_component_residue': 7.131858855793217, 'motion_component_ionic': 0.42208977310838236, 'ionic_contributions': [{'ion_id': 1355, 'distance': 12.444255828857422, 'force': [-0.28277072310447693, -0.719104528427124, -1.999786376953125], 'magnitude': 2.143878698348999}, {'ion_id': 1469, 'distance': 5.576650142669678, 'force': [-9.842928886413574, 4.126557350158691, -0.23699882626533508], 'magnitude': 10.67557430267334}, {'ion_id': 1476, 'distance': 7.306352615356445, 'force': [-1.4224494695663452, -3.3690109252929688, -5.0304341316223145], 'magnitude': 6.219233512878418}, {'ion_id': 2434, 'distance': 11.169254302978516, 'force': [-1.0529464483261108, -2.425291061401367, -0.3027394115924835], 'magnitude': 2.6612749099731445}, {'ion_id': 2443, 'distance': 5.141005992889404, 'force': [-5.28463077545166, -11.308737754821777, 1.405932903289795], 'magnitude': 12.561509132385254}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.290620803833008, 'force': [4.5950398445129395, -0.5332372188568115, -5.299990653991699], 'magnitude': 7.034815788269043}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.208616733551025, 'force': [2.3981988430023193, -2.072134256362915, 8.12936782836914], 'magnitude': 8.725349426269531}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.3863396644592285, 'force': [-0.35104599595069885, 1.4455454349517822, -6.621984958648682], 'magnitude': 6.78701114654541}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.305342674255371, 'force': [-3.8804843425750732, 4.840791702270508, -8.890351295471191], 'magnitude': 10.84111499786377}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.697933673858643, 'force': [1.0434727668762207, -2.4309587478637695, 3.3782551288604736], 'magnitude': 4.290804386138916}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.5273756980896, 'force': [2.3696916103363037, -1.9585676193237305, 3.367398738861084], 'magnitude': 4.559692859649658}]}, 5696: {'frame': 5696, 'ionic_force': [-15.213935688138008, -14.176376223564148, -12.65572875738144], 'ionic_force_magnitude': 24.3433964831378, 'motion_vector': [-0.21909713745117188, -0.3765602111816406, 0.164337158203125], 'ionic_force_x': -15.213935688138008, 'ionic_force_y': -14.176376223564148, 'ionic_force_z': -12.65572875738144, 'radial_force': 20.79503503134424, 'axial_force': -12.65572875738144, 'glu_force': [6.629117012023926, -1.965427279472351, 3.735133409500122], 'glu_force_magnitude': 7.858709711954191, 'asn_force': [1.0297255516052246, 2.3191022872924805, -2.3139519691467285], 'asn_force_magnitude': 3.43408559096478, 'residue_force': [7.65884256362915, 0.3536750078201294, 1.4211814403533936], 'residue_force_magnitude': 7.797609384421552, 'total_force': [-7.555093124508858, -13.822701215744019, -11.234547317028046], 'total_force_magnitude': 19.34842511519411, 'motion_component_total': 10.768560674011754, 'cosine_total_motion': 0.5565600616018778, 'cosine_glu_motion': -0.0269176470304038, 'cosine_asn_motion': -0.9250527483988816, 'cosine_residue_motion': -0.43452398309012064, 'cosine_ionic_motion': 0.5815461688806515, 'motion_component_glu': -0.21153797414078923, 'motion_component_asn': -3.176710314158967, 'motion_component_residue': -3.3882482882997564, 'motion_component_ionic': 14.156808962311512, 'ionic_contributions': [{'ion_id': 1355, 'distance': 14.936958312988281, 'force': [0.09340129792690277, -0.6584328413009644, -1.331163763999939], 'magnitude': 1.4880372285842896}, {'ion_id': 1469, 'distance': 4.184452533721924, 'force': [-16.17984390258789, -5.707157611846924, -8.072161674499512], 'magnitude': 18.960981369018555}, {'ion_id': 1476, 'distance': 10.000617980957031, 'force': [0.16498154401779175, -2.0770199298858643, -2.584268808364868], 'magnitude': 3.319589853286743}, {'ion_id': 2434, 'distance': 9.450231552124023, 'force': [-0.31412482261657715, -3.6910321712493896, -0.3123330771923065], 'magnitude': 3.7175185680389404}, {'ion_id': 2443, 'distance': 11.98450756072998, 'force': [1.0216501951217651, -2.042733669281006, -0.35580143332481384], 'magnitude': 2.3115200996398926}], 'glu_contributions': [{'resid': 748, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 5.88142204284668, 'force': [6.629117012023926, -1.965427279472351, 3.735133409500122], 'magnitude': 7.858709812164307}], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.225194931030273, 'force': [-4.542599201202393, -4.742160797119141, 5.660992622375488], 'magnitude': 8.670071601867676}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.047222137451172, 'force': [5.572324752807617, 7.061263084411621, -7.974944591522217], 'magnitude': 12.021313667297363}]}, 5697: {'frame': 5697, 'ionic_force': [-14.388794315978885, -13.769953429698944, -10.123002961277962], 'ionic_force_magnitude': 22.341087893781413, 'motion_vector': [-1.5983009338378906, 3.4348678588867188, 0.1610565185546875], 'ionic_force_x': -14.388794315978885, 'ionic_force_y': -13.769953429698944, 'ionic_force_z': -10.123002961277962, 'radial_force': 19.916049290048065, 'axial_force': -10.123002961277962, 'glu_force': [14.417499542236328, -2.0770235806703568, 5.661137580871582], 'glu_force_magnitude': 15.627757315578009, 'asn_force': [1.2730975151062012, 1.467081069946289, -1.7679595947265625], 'asn_force_magnitude': 2.6265538786307134, 'residue_force': [15.69059705734253, -0.6099425107240677, 3.8931779861450195], 'residue_force_magnitude': 16.177876891424248, 'total_force': [1.3018027413636446, -14.379895940423012, -6.229824975132942], 'total_force_magnitude': 15.72535585783693, 'motion_component_total': -13.839101785419329, 'cosine_total_motion': -0.880050150249696, 'cosine_glu_motion': -0.49386203951895075, 'cosine_asn_motion': 0.27306892439713226, 'cosine_residue_motion': -0.4327345241563049, 'cosine_ionic_motion': -0.3060896568449122, 'motion_component_glu': -7.717956100978558, 'motion_component_asn': 0.7172302425088048, 'motion_component_residue': -7.000725858469753, 'motion_component_ionic': -6.838375926949575, 'ionic_contributions': [{'ion_id': 1355, 'distance': 14.766557693481445, 'force': [0.01840483583509922, -0.6926707625389099, -1.3557699918746948], 'magnitude': 1.5225780010223389}, {'ion_id': 1469, 'distance': 4.3431806564331055, 'force': [-15.130455017089844, -6.483215808868408, -6.229846477508545], 'magnitude': 17.60038948059082}, {'ion_id': 1476, 'distance': 9.86992359161377, 'force': [0.08019865304231644, -2.2278919219970703, -2.5778114795684814], 'magnitude': 3.408085346221924}, {'ion_id': 2434, 'distance': 12.017027854919434, 'force': [-0.08338899910449982, -2.282119035720825, 0.2655191719532013], 'magnitude': 2.2990262508392334}, {'ion_id': 2443, 'distance': 12.233217239379883, 'force': [0.7264462113380432, -2.0840559005737305, -0.22509418427944183], 'magnitude': 2.2184860706329346}], 'glu_contributions': [{'resid': 748, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 5.904326438903809, 'force': [7.589880466461182, -0.039861276745796204, 1.7884876728057861], 'magnitude': 7.797856330871582}, {'resid': 748, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 5.789768218994141, 'force': [6.8276190757751465, -2.0371623039245605, 3.872649908065796], 'magnitude': 8.109490394592285}], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.585978031158447, 'force': [-4.363496780395508, -3.7959542274475098, 4.909414768218994], 'magnitude': 7.586285591125488}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.3935346603393555, 'force': [5.636594295501709, 5.263035297393799, -6.677374362945557], 'magnitude': 10.200885772705078}]}, 5698: {'frame': 5698, 'ionic_force': [-9.738676965236664, -11.330120891332626, -6.976988285779953], 'ionic_force_magnitude': 16.48914291239402, 'motion_vector': [-2.993671417236328, -2.5537109375, 1.6241912841796875], 'ionic_force_x': -9.738676965236664, 'ionic_force_y': -11.330120891332626, 'ionic_force_z': -6.976988285779953, 'radial_force': 14.940330265608027, 'axial_force': -6.976988285779953, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [1.6149744987487793, -2.038796864449978, 2.790360927581787], 'asn_force_magnitude': 3.8145706694561348, 'residue_force': [1.6149744987487793, -2.038796864449978, 2.790360927581787], 'residue_force_magnitude': 3.8145706694561348, 'total_force': [-8.123702466487885, -13.368917755782604, -4.186627358198166], 'total_force_magnitude': 16.19414561998607, 'motion_component_total': 12.1355271455568, 'cosine_total_motion': 0.7493774250479562, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.30199277216950493, 'cosine_residue_motion': 0.30199277216950493, 'cosine_ionic_motion': 0.6661082648629056, 'motion_component_glu': None, 'motion_component_asn': 1.1519727711055423, 'motion_component_residue': 1.1519727711055423, 'motion_component_ionic': 10.98355437445126, 'ionic_contributions': [{'ion_id': 1355, 'distance': 13.537941932678223, 'force': [-0.1521759033203125, -0.4667292535305023, -1.7436898946762085], 'magnitude': 1.8114768266677856}, {'ion_id': 1469, 'distance': 7.151844024658203, 'force': [-6.2060546875, 1.8714954853057861, -0.3370665907859802], 'magnitude': 6.490856647491455}, {'ion_id': 1476, 'distance': 8.102265357971191, 'force': [-0.9171950221061707, -2.0580520629882812, -4.527716159820557], 'magnitude': 5.057374477386475}, {'ion_id': 2434, 'distance': 6.5624518394470215, 'force': [-3.975003957748413, -6.597219944000244, 0.32685384154319763], 'magnitude': 7.709137439727783}, {'ion_id': 2443, 'distance': 8.680612564086914, 'force': [1.5117526054382324, -4.079615116119385, -0.6953694820404053], 'magnitude': 4.4059271812438965}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.989780902862549, 'force': [-5.10177755355835, 1.2264975309371948, 3.9999825954437256], 'magnitude': 6.597900390625}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.934056282043457, 'force': [6.173290729522705, -2.4099342823028564, -4.63718318939209], 'magnitude': 8.088310241699219}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.815628528594971, 'force': [-2.4016177654266357, -0.08513995260000229, 3.345181703567505], 'magnitude': 4.118890285491943}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.526407718658447, 'force': [5.539077281951904, 0.19701914489269257, 10.137420654296875], 'magnitude': 11.553678512573242}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.125009059906006, 'force': [-2.065647840499878, -0.12887804210186005, -7.205463409423828], 'magnitude': 7.496813774108887}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.123382568359375, 'force': [-10.020918846130371, 4.287226676940918, -14.258268356323242], 'magnitude': 17.947071075439453}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.470301628112793, 'force': [2.8273348808288574, -2.758668899536133, 5.7438530921936035], 'magnitude': 6.971077919006348}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 3.9208221435546875, 'force': [6.665233612060547, -2.3669190406799316, 5.664837837219238], 'magnitude': 9.06190013885498}]}, 5699: {'frame': 5699, 'ionic_force': [-7.502817556262016, -9.551654130220413, -3.1742424368858337], 'ionic_force_magnitude': 12.553970804253016, 'motion_vector': [-0.2769050598144531, -0.16832733154296875, 0.20163726806640625], 'ionic_force_x': -7.502817556262016, 'ionic_force_y': -9.551654130220413, 'ionic_force_z': -3.1742424368858337, 'radial_force': 12.14604330248786, 'axial_force': -3.1742424368858337, 'glu_force': [-34.038984298706055, -13.682983309030533, -3.127213954925537], 'glu_force_magnitude': 36.81923344452796, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [-34.038984298706055, -13.682983309030533, -3.127213954925537], 'residue_force_magnitude': 36.81923344452796, 'total_force': [-41.54180185496807, -23.234637439250946, -6.301456391811371], 'total_force_magnitude': 48.013310976736136, 'motion_component_total': 37.057511765974226, 'cosine_total_motion': 0.7718174608689179, 'cosine_glu_motion': 0.78976255678907, 'cosine_asn_motion': None, 'cosine_residue_motion': 0.78976255678907, 'cosine_ionic_motion': 0.6355805622159841, 'motion_component_glu': 29.07845194416404, 'motion_component_asn': None, 'motion_component_residue': 29.07845194416404, 'motion_component_ionic': 7.979059821810182, 'ionic_contributions': [{'ion_id': 1355, 'distance': 13.017755508422852, 'force': [-0.6258348226547241, -0.9120814800262451, -1.6169955730438232], 'magnitude': 1.959141731262207}, {'ion_id': 1469, 'distance': 9.91153335571289, 'force': [-3.346435785293579, -0.3936164677143097, 0.2601182758808136], 'magnitude': 3.379530668258667}, {'ion_id': 1476, 'distance': 9.026442527770996, 'force': [-2.058412790298462, -2.6242835521698, -2.340930461883545], 'magnitude': 4.074786186218262}, {'ion_id': 2434, 'distance': 10.497147560119629, 'force': [-1.4498467445373535, -2.6175620555877686, 0.3526051938533783], 'magnitude': 3.012974739074707}, {'ion_id': 2443, 'distance': 10.503984451293945, 'force': [-0.022287413477897644, -3.00411057472229, 0.17096012830734253], 'magnitude': 3.0090537071228027}], 'glu_contributions': [{'resid': 1073, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 2.99222731590271, 'force': [27.9241886138916, 9.012788772583008, -5.560523986816406], 'magnitude': 29.864864349365234}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 2.710928440093994, 'force': [-36.79689407348633, 0.32354363799095154, -3.757082939147949], 'magnitude': 36.98961639404297}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.800414800643921, 'force': [-25.166278839111328, -23.019315719604492, 6.190392971038818], 'magnitude': 34.66340255737305}], 'asn_contributions': []}, 5700: {'frame': 5700, 'ionic_force': [-7.085268452763557, -8.294093906879425, -2.452709883451462], 'ionic_force_magnitude': 11.180733811170061, 'motion_vector': [0.4935493469238281, -0.46282196044921875, 0.6883697509765625], 'ionic_force_x': -7.085268452763557, 'ionic_force_y': -8.294093906879425, 'ionic_force_z': -2.452709883451462, 'radial_force': 10.908392309770532, 'axial_force': -2.452709883451462, 'glu_force': [-39.5418701171875, -4.393214702606201, -0.0832822322845459], 'glu_force_magnitude': 39.78525812053926, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [-39.5418701171875, -4.393214702606201, -0.0832822322845459], 'residue_force_magnitude': 39.78525812053926, 'total_force': [-46.62713856995106, -12.687308609485626, -2.5359921157360077], 'total_force_magnitude': 48.38893579099277, 'motion_component_total': -19.567090000053497, 'cosine_total_motion': -0.4043711579971503, 'cosine_glu_motion': -0.4567509334447507, 'cosine_asn_motion': None, 'cosine_residue_motion': -0.4567509334447507, 'cosine_ionic_motion': -0.12478038022540532, 'motion_component_glu': -18.171953783896654, 'motion_component_asn': None, 'motion_component_residue': -18.171953783896654, 'motion_component_ionic': -1.3951362161568452, 'ionic_contributions': [{'ion_id': 1355, 'distance': 13.742049217224121, 'force': [-0.5744865536689758, -0.7606053352355957, -1.4772404432296753], 'magnitude': 1.7580655813217163}, {'ion_id': 1469, 'distance': 9.510303497314453, 'force': [-3.6154754161834717, -0.5478944182395935, 0.3197089731693268], 'magnitude': 3.670703649520874}, {'ion_id': 1476, 'distance': 9.531294822692871, 'force': [-1.7856495380401611, -2.236912727355957, -2.2723193168640137], 'magnitude': 3.654552936553955}, {'ion_id': 2434, 'distance': 12.39127254486084, 'force': [-0.9666056632995605, -1.7378770112991333, 0.8489934206008911], 'magnitude': 2.1622519493103027}, {'ion_id': 2443, 'distance': 10.490275382995605, 'force': [-0.14305128157138824, -3.0108044147491455, 0.12814748287200928], 'magnitude': 3.016923666000366}], 'glu_contributions': [{'resid': 1073, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 2.974531888961792, 'force': [29.787803649902344, -0.2881608009338379, -5.091938495635986], 'magnitude': 30.22125244140625}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 2.804795503616333, 'force': [-32.11030197143555, 12.47452449798584, -2.716064691543579], 'magnitude': 34.555206298828125}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.5602729320526123, 'force': [-37.2193717956543, -16.579578399658203, 7.7247209548950195], 'magnitude': 41.47089767456055}], 'asn_contributions': []}, 5701: {'frame': 5701, 'ionic_force': [-7.92530158162117, -8.08792930841446, -1.2593768686056137], 'ionic_force_mag</t>
+          <t>{5689: {'frame': 5689, 'motion_vector': [1.6955833435058594, -2.072643280029297, 4.204833984375], 'ionic_force': [-10.846781343221664, 1.6348312199115753, -4.6059174835681915], 'ionic_force_magnitude': 11.897050663534147, 'radial_force': 10.969290707482374, 'axial_force': -4.6059174835681915, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.057557977735996246, -1.561832070350647, -1.0622444152832031], 'asn_force_magnitude': 1.889707790791264, 'residue_force': [0.057557977735996246, -1.561832070350647, -1.0622444152832031], 'residue_force_magnitude': 1.889707790791264, 'total_force': [-10.789223365485668, 0.07299914956092834, -5.668161898851395], 'total_force_magnitude': 12.187728624225647, 'cosine_total_motion': -0.6958664012746681, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.12014802608635168, 'cosine_residue_motion': -0.12014802608635168, 'cosine_ionic_motion': -0.6937842352649658, 'motion_component_total': -8.481030857452163, 'motion_component_glu': None, 'motion_component_asn': -0.2270446609435708, 'motion_component_residue': -0.2270446609435708, 'motion_component_ionic': -8.253986196508592, 'motion_component_percent_total': 69.58664012746681, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 12.014802608635168, 'motion_component_percent_residue': 12.014802608635168, 'motion_component_percent_ionic': 69.37842352649658, 'ionic_contributions': [{'ion_id': 1355, 'distance': 12.842514038085938, 'force': [-0.2695693075656891, 0.3014860451221466, -1.9719277620315552], 'magnitude': 2.0129730701446533, 'cosine_ionic_motion': -0.934095561504364, 'motion_component_ionic': -1.8803092241287231, 'motion_component_percent_ionic': 93.4095561504364}, {'ion_id': 1469, 'distance': 9.714579582214355, 'force': [-2.6125478744506836, 2.329728126525879, -0.3506489098072052], 'magnitude': 3.5179531574249268, 'cosine_ionic_motion': -0.6119996905326843, 'motion_component_ionic': -2.1529862880706787, 'motion_component_percent_ionic': 61.19996905326843}, {'ion_id': 1476, 'distance': 7.228488922119141, 'force': [-1.3893324136734009, 1.863111972808838, -5.913637638092041], 'magnitude': 6.353939056396484, 'cosine_ionic_motion': -0.9813093543052673, 'motion_component_ionic': -6.235179901123047, 'motion_component_percent_ionic': 98.13093543052673}, {'ion_id': 2434, 'distance': 7.680809497833252, 'force': [-0.631294310092926, -5.49688720703125, -1.0274757146835327], 'magnitude': 5.62761116027832, 'cosine_ionic_motion': 0.21395288407802582, 'motion_component_ionic': 1.2040436267852783, 'motion_component_percent_ionic': 21.395288407802582}, {'ion_id': 2443, 'distance': 6.442495822906494, 'force': [-5.944037437438965, 2.637392282485962, 4.657772541046143], 'magnitude': 7.998891353607178, 'cosine_ionic_motion': 0.1013197973370552, 'motion_component_ionic': 0.81044602394104, 'motion_component_percent_ionic': 10.13197973370552}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.862374305725098, 'force': [1.5012428760528564, -4.139888286590576, 8.99179458618164], 'magnitude': 10.01223087310791, 'cosine_with_motion': 0.9804208874702454, 'motion_component': 9.816200256347656, 'motion_component_percent': 98.04208874702454}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.928593635559082, 'force': [0.669931948184967, 3.9480724334716797, -7.0480637550354], 'magnitude': 8.106249809265137, 'cosine_with_motion': -0.907754123210907, 'motion_component': -7.3584818840026855, 'motion_component_percent': 90.7754123210907}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.005432605743408, 'force': [-2.076143741607666, 2.082576036453247, -11.818824768066406], 'magnitude': 12.179166793823242, 'cosine_with_motion': -0.9475945830345154, 'motion_component': -11.540912628173828, 'motion_component_percent': 94.75945830345154}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.1369948387146, 'force': [-0.034623049199581146, -0.46103692054748535, 5.258759498596191], 'magnitude': 5.279044151306152, 'cosine_with_motion': 0.8743143081665039, 'motion_component': 4.615543842315674, 'motion_component_percent': 87.43143081665039}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.172613143920898, 'force': [1.7645483016967773, -0.3997570276260376, 4.882126808166504], 'magnitude': 5.206592082977295, 'cosine_with_motion': 0.9381059408187866, 'motion_component': 4.884335041046143, 'motion_component_percent': 93.81059408187866}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.840487003326416, 'force': [-4.325311660766602, -6.203693866729736, -4.77777624130249], 'magnitude': 8.945462226867676, 'cosine_with_motion': -0.32662585377693176, 'motion_component': -2.9218192100524902, 'motion_component_percent': 32.662585377693176}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.982481002807617, 'force': [2.557913303375244, 3.6118955612182617, 3.449739456176758], 'magnitude': 5.611542701721191, 'cosine_with_motion': 0.4059649705886841, 'motion_component': 2.278089761734009, 'motion_component_percent': 40.59649705886841}]}, 5692: {'frame': 5692, 'motion_vector': [5.063621520996094, 4.651702880859375, -0.6800384521484375], 'ionic_force': [-2.2680077254772186, -15.304942309856415, -10.105775147676468], 'ionic_force_magnitude': 18.48003813541121, 'radial_force': 15.472075431268339, 'axial_force': -10.105775147676468, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [2.5782699584960938, 3.2258684039115906, -0.9870598316192627], 'asn_force_magnitude': 4.245938064719598, 'residue_force': [2.5782699584960938, 3.2258684039115906, -0.9870598316192627], 'residue_force_magnitude': 4.245938064719598, 'total_force': [0.3102622330188751, -12.079073905944824, -11.09283497929573], 'total_force_magnitude': 16.4027825979741, 'cosine_total_motion': -0.4153501802434134, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.9793823974703162, 'cosine_residue_motion': 0.9793823974703162, 'cosine_ionic_motion': -0.5936836076585019, 'motion_component_total': -6.8128987085620665, 'motion_component_glu': None, 'motion_component_asn': 4.158397001335555, 'motion_component_residue': 4.158397001335555, 'motion_component_ionic': -10.971295709897621, 'motion_component_percent_total': 41.53501802434134, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 97.93823974703162, 'motion_component_percent_residue': 97.93823974703162, 'motion_component_percent_ionic': 59.36836076585019, 'ionic_contributions': [{'ion_id': 1355, 'distance': 13.362324714660645, 'force': [-0.16544833779335022, -0.5105010867118835, -1.7802817821502686], 'magnitude': 1.859405279159546, 'cosine_ionic_motion': -0.15581244230270386, 'motion_component_ionic': -0.28971847891807556, 'motion_component_percent_ionic': 15.581244230270386}, {'ion_id': 1469, 'distance': 6.331493854522705, 'force': [-8.14029312133789, 1.124986171722412, -1.0288584232330322], 'magnitude': 8.281818389892578, 'cosine_ionic_motion': -0.6166490912437439, 'motion_component_ionic': -5.106975555419922, 'motion_component_percent_ionic': 61.66490912437439}, {'ion_id': 1476, 'distance': 8.040470123291016, 'force': [-0.7527567744255066, -2.250356912612915, -4.554305553436279], 'magnitude': 5.135411262512207, 'cosine_ionic_motion': -0.31515204906463623, 'motion_component_ionic': -1.6184353828430176, 'motion_component_percent_ionic': 31.515204906463623}, {'ion_id': 2434, 'distance': 11.164103507995605, 'force': [-0.9204217195510864, -2.4938366413116455, -0.17049100995063782], 'magnitude': 2.663731336593628, 'cosine_ionic_motion': -0.8772230744361877, 'motion_component_ionic': -2.336686611175537, 'motion_component_percent_ionic': 87.72230744361877}, {'ion_id': 2443, 'distance': 4.901560306549072, 'force': [7.710912227630615, -11.175233840942383, -2.57183837890625], 'magnitude': 13.818768501281738, 'cosine_ionic_motion': -0.11719417572021484, 'motion_component_ionic': -1.6194791793823242, 'motion_component_percent_ionic': 11.719417572021484}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.955214023590088, 'force': [-7.112100124359131, 0.5117895007133484, 6.488199234008789], 'magnitude': 9.640571594238281, 'cosine_with_motion': -0.5711409449577332, 'motion_component': -5.506124973297119, 'motion_component_percent': 57.114094495773315}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.565440654754639, 'force': [6.408121585845947, 1.6682206392288208, -6.738068580627441], 'magnitude': 9.447145462036133, 'cosine_with_motion': 0.6861822605133057, 'motion_component': 6.482463359832764, 'motion_component_percent': 68.61822605133057}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.608523845672607, 'force': [9.413819313049316, -4.310042858123779, -9.961161613464355], 'magnitude': 14.367365837097168, 'cosine_with_motion': 0.3464546203613281, 'motion_component': 4.977640151977539, 'motion_component_percent': 34.64546203613281}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.879380702972412, 'force': [-4.83558988571167, 3.2670257091522217, 7.185204982757568], 'magnitude': 9.25654125213623, 'cosine_with_motion': -0.22162330150604248, 'motion_component': -2.0514652729034424, 'motion_component_percent': 22.162330150604248}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.195611476898193, 'force': [-3.49900484085083, 2.236114978790283, 3.0640740394592285], 'magnitude': 5.160600185394287, 'cosine_with_motion': -0.263610303401947, 'motion_component': -1.3603873252868652, 'motion_component_percent': 26.361030340194702}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.786916732788086, 'force': [5.836784839630127, -2.088743209838867, 8.26351261138916], 'magnitude': 10.33036994934082, 'cosine_with_motion': 0.19921588897705078, 'motion_component': 2.057973861694336, 'motion_component_percent': 19.921588897705078}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.929454326629639, 'force': [-2.7333264350891113, 1.915501356124878, -7.384117126464844], 'magnitude': 8.103419303894043, 'cosine_with_motion': 0.0016305509489029646, 'motion_component': 0.013213038444519043, 'motion_component_percent': 0.16305509489029646}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.011087894439697, 'force': [-8.006246566772461, 4.756603240966797, -7.806305408477783], 'magnitude': 12.151694297790527, 'cosine_with_motion': -0.15609093010425568, 'motion_component': -1.8967692852020264, 'motion_component_percent': 15.609093010425568}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.242641925811768, 'force': [2.7847952842712402, -2.780026912689209, 3.1945762634277344], 'magnitude': 5.068427085876465, 'cosine_with_motion': -0.028644675388932228, 'motion_component': -0.14518344402313232, 'motion_component_percent': 2.864467538893223}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.051477909088135, 'force': [4.321016788482666, -1.9505740404129028, 2.7070257663726807], 'magnitude': 5.459296226501465, 'cosine_with_motion': 0.2907037138938904, 'motion_component': 1.5870376825332642, 'motion_component_percent': 29.070371389389038}]}, 5693: {'frame': 5693, 'motion_vector': [0.5311241149902344, 0.9281234741210938, 2.3688735961914062], 'ionic_force': [14.037217020988464, 0.7251570634543896, -12.502707362174988], 'ionic_force_magnitude': 18.811884696786514, 'radial_force': 14.055935204069705, 'axial_force': -12.502707362174988, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [1.5051481127738953, -1.2537007331848145, -0.4803304672241211], 'asn_force_magnitude': 2.016916886616477, 'residue_force': [1.5051481127738953, -1.2537007331848145, -0.4803304672241211], 'residue_force_magnitude': 2.016916886616477, 'total_force': [15.54236513376236, -0.5285436697304249, -12.983037829399109], 'total_force_magnitude': 20.258424016729737, 'cosine_total_motion': -0.43665016723542005, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.28653004267432075, 'cosine_residue_motion': -0.28653004267432075, 'cosine_ionic_motion': -0.4395060402773284, 'motion_component_total': -8.84584423483109, 'motion_component_glu': None, 'motion_component_asn': -0.5779072815927773, 'motion_component_residue': -0.5779072815927773, 'motion_component_ionic': -8.267936953238312, 'motion_component_percent_total': 43.665016723542, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 28.653004267432074, 'motion_component_percent_residue': 28.653004267432074, 'motion_component_percent_ionic': 43.950604027732844, 'ionic_contributions': [{'ion_id': 1355, 'distance': 14.424660682678223, 'force': [0.4393165409564972, 0.04694287106394768, -1.5332221984863281], 'magnitude': 1.595610499382019, 'cosine_ionic_motion': -0.8090305328369141, 'motion_component_ionic': -1.2908976078033447, 'motion_component_percent_ionic': 80.9030532836914}, {'ion_id': 1469, 'distance': 6.90531063079834, 'force': [-0.2973380386829376, 6.702067852020264, -1.863255262374878], 'magnitude': 6.9626030921936035, 'cosine_ionic_motion': 0.09110256284475327, 'motion_component_ionic': 0.6343109607696533, 'motion_component_percent_ionic': 9.110256284475327}, {'ion_id': 1476, 'distance': 9.697990417480469, 'force': [1.3921409845352173, 0.3217581510543823, -3.227895498275757], 'magnitude': 3.529999256134033, 'cosine_ionic_motion': -0.7202940583229065, 'motion_component_ionic': -2.542637586593628, 'motion_component_percent_ionic': 72.02940583229065}, {'ion_id': 2434, 'distance': 6.285351276397705, 'force': [2.518434524536133, -7.808837413787842, -1.8178147077560425], 'magnitude': 8.403862953186035, 'cosine_ionic_motion': -0.4677274823188782, 'motion_component_ionic': -3.930717706680298, 'motion_component_percent_ionic': 46.77274823188782}, {'ion_id': 2443, 'distance': 5.524619102478027, 'force': [9.984663009643555, 1.4632256031036377, -4.060519695281982], 'magnitude': 10.877607345581055, 'cosine_ionic_motion': -0.10461817681789398, 'motion_component_ionic': -1.1379954814910889, 'motion_component_percent_ionic': 10.461817681789398}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.116811752319336, 'force': [-3.8710646629333496, -6.429830074310303, 5.041471004486084], 'magnitude': 9.041254997253418, 'cosine_with_motion': 0.16677168011665344, 'motion_component': 1.507825255393982, 'motion_component_percent': 16.677168011665344}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.730896472930908, 'force': [5.400066375732422, 5.145687103271484, -4.665219783782959], 'magnitude': 8.797903060913086, 'cosine_with_motion': -0.1490137130022049, 'motion_component': -1.3110082149505615, 'motion_component_percent': 14.90137130022049}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.740130424499512, 'force': [2.9290695190429688, 9.451510429382324, -9.301790237426758], 'magnitude': 13.58064079284668, 'cosine_with_motion': -0.331670343875885, 'motion_component': -4.504295825958252, 'motion_component_percent': 33.1670343875885}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.183035850524902, 'force': [-1.4411402940750122, -4.443267822265625, 6.447065353393555], 'magnitude': 7.961417198181152, 'cosine_with_motion': 0.5017828345298767, 'motion_component': 3.9949026107788086, 'motion_component_percent': 50.17828345298767}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.227376461029053, 'force': [-0.31844228506088257, -3.9280471801757812, 3.2340965270996094], 'magnitude': 5.098072528839111, 'cosine_with_motion': 0.29028499126434326, 'motion_component': 1.4798939228057861, 'motion_component_percent': 29.028499126434326}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.659245491027832, 'force': [1.005800485610962, 6.544600963592529, 3.2840981483459473], 'magnitude': 7.391125679016113, 'cosine_with_motion': 0.7489890456199646, 'motion_component': 5.535871982574463, 'motion_component_percent': 74.89890456199646}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.649864196777344, 'force': [-2.199141025543213, -7.594354152679443, -4.5200514793396], 'magnitude': 9.107211112976074, 'cosine_with_motion': -0.7994870543479919, 'motion_component': -7.281097412109375, 'motion_component_percent': 79.9487054347992}]}, 5694: {'frame': 5694, 'motion_vector': [-6.16156005859375, -6.210399627685547, -0.5569686889648438], 'ionic_force': [15.186673760414124, -2.523807108402252, -6.381444334983826], 'ionic_force_magnitude': 16.66515808584394, 'radial_force': 15.39495573964643, 'axial_force': -6.381444334983826, 'glu_force': [4.446905136108398, 5.983371257781982, 1.298695683479309], 'glu_force_magnitude': 7.567186225823082, 'asn_force': [1.872458316385746, -0.19104492664337158, -0.5029773712158203], 'asn_force_magnitude': 1.9482259998659013, 'residue_force': [6.319363452494144, 5.792326331138611, 0.7957183122634888], 'residue_force_magnitude': 8.609214040990725, 'total_force': [21.506037212908268, 3.2685192227363586, -5.585726022720337], 'total_force_magnitude': 22.45869964430905, 'cosine_total_motion': -0.7603743975178311, 'cosine_glu_motion': -0.9841378927108955, 'cosine_asn_motion': -0.5896755991616716, 'cosine_residue_motion': -0.9984623449803918, 'cosine_ionic_motion': -0.5089087140717763, 'motion_component_total': -17.07702021107542, 'motion_component_glu': -7.447154706032443, 'motion_component_asn': -1.148821333773272, 'motion_component_residue': -8.595976039805715, 'motion_component_ionic': -8.481044171269705, 'motion_component_percent_total': 76.03743975178311, 'motion_component_percent_glu': 98.41378927108954, 'motion_component_percent_asn': 58.967559916167154, 'motion_component_percent_residue': 99.84623449803918, 'motion_component_percent_ionic': 50.89087140717763, 'ionic_contributions': [{'ion_id': 1355, 'distance': 12.02578067779541, 'force': [0.7672042846679688, 0.321216881275177, -2.13971209526062], 'magnitude': 2.2956807613372803, 'cosine_ionic_motion': -0.27480998635292053, 'motion_component_ionic': -0.6308760046958923, 'motion_component_percent_ionic': 27.480998635292053}, {'ion_id': 1469, 'distance': 7.6157989501953125, 'force': [0.36691606044769287, 5.6577959060668945, 0.787419319152832], 'magnitude': 5.724099159240723, 'cosine_ionic_motion': -0.7540475130081177, 'motion_component_ionic': -4.316242694854736, 'motion_component_percent_ionic': 75.40475130081177}, {'ion_id': 1476, 'distance': 7.09453010559082, 'force': [4.058429718017578, 1.9305769205093384, -4.828175067901611], 'magnitude': 6.596154689788818, 'cosine_ionic_motion': -0.5933127999305725, 'motion_component_ionic': -3.9135830402374268, 'motion_component_percent_ionic': 59.33127999305725}, {'ion_id': 2434, 'distance': 5.142002105712891, 'force': [3.7240912914276123, -11.90422248840332, -1.445675253868103], 'magnitude': 12.556645393371582, 'cosine_ionic_motion': 0.47049853205680847, 'motion_component_ionic': 5.907883167266846, 'motion_component_percent_ionic': 47.04985320568085}, {'ion_id': 2443, 'distance': 7.114371299743652, 'force': [6.2700324058532715, 1.4708256721496582, 1.2446987628936768], 'magnitude': 6.559413909912109, 'cosine_ionic_motion': -0.8427926898002625, 'motion_component_ionic': -5.528225898742676, 'motion_component_percent_ionic': 84.27926898002625}], 'glu_contributions': [{'resid': 423, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 5.993641376495361, 'force': [4.446905136108398, 5.983371257781982, 1.298695683479309], 'magnitude': 7.56718635559082, 'cosine_with_motion': -0.9841378331184387, 'motion_component': -7.447154521942139, 'motion_component_percent': 98.41378331184387}], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.322994709014893, 'force': [-2.409579277038574, -3.641601324081421, 7.12241268157959], 'magnitude': 8.354405403137207, 'cosine_with_motion': 0.45736929774284363, 'motion_component': 3.8210484981536865, 'motion_component_percent': 45.73692977428436}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.167766094207764, 'force': [3.4821557998657227, 2.2395565509796143, -6.101158618927002], 'magnitude': 7.3732733726501465, 'cosine_with_motion': -0.49456262588500977, 'motion_component': -3.64654541015625, 'motion_component_percent': 49.45626258850098}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.217445373535156, 'force': [0.6987098455429077, 4.0230584144592285, -10.439300537109375], 'magnitude': 11.209468841552734, 'cosine_with_motion': -0.2389054149389267, 'motion_component': -2.6780028343200684, 'motion_component_percent': 23.89054149389267}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.1344733238220215, 'force': [-0.11744511872529984, -0.9304448366165161, 5.200343132019043], 'magnitude': 5.2842302322387695, 'cosine_with_motion': 0.07783889025449753, 'motion_component': 0.4113186299800873, 'motion_component_percent': 7.783889025449753}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.779999256134033, 'force': [0.21861706674098969, -1.8816137313842773, 3.714725971221924], 'magnitude': 4.169826507568359, 'cosine_with_motion': 0.2262347936630249, 'motion_component': 0.9433598518371582, 'motion_component_percent': 22.62347936630249}]}, 5695: {'frame': 5695, 'motion_vector': [2.018024444580078, -2.0229759216308594, -1.58453369140625], 'ionic_force': [-17.885726302862167, -13.695586919784546, -6.164025843143463], 'ionic_force_magnitude': 23.35516048014249, 'radial_force': 22.527057208127943, 'axial_force': -6.164025843143463, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [6.174872726202011, -0.7085607051849365, -5.937305212020874], 'asn_force_magnitude': 8.595504908870442, 'residue_force': [6.174872726202011, -0.7085607051849365, -5.937305212020874], 'residue_force_magnitude': 8.595504908870442, 'total_force': [-11.710853576660156, -14.404147624969482, -12.101331055164337], 'total_force_magnitude': 22.160003917025215, 'cosine_total_motion': 0.3408820980892521, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.8297195954635821, 'cosine_residue_motion': 0.8297195954635821, 'cosine_ionic_motion': 0.018072655654293633, 'motion_component_total': 7.553948628901599, 'motion_component_glu': None, 'motion_component_asn': 7.131858855793217, 'motion_component_residue': 7.131858855793217, 'motion_component_ionic': 0.42208977310838236, 'motion_component_percent_total': 34.08820980892521, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 82.9719595463582, 'motion_component_percent_residue': 82.9719595463582, 'motion_component_percent_ionic': 1.8072655654293632, 'ionic_contributions': [{'ion_id': 1355, 'distance': 12.444255828857422, 'force': [-0.28277072310447693, -0.719104528427124, -1.999786376953125], 'magnitude': 2.143878698348999, 'cosine_ionic_motion': 0.5785769820213318, 'motion_component_ionic': 1.24039888381958, 'motion_component_percent_ionic': 57.85769820213318}, {'ion_id': 1469, 'distance': 5.576650142669678, 'force': [-9.842928886413574, 4.126557350158691, -0.23699882626533508], 'magnitude': 10.67557430267334, 'cosine_ionic_motion': -0.7980207800865173, 'motion_component_ionic': -8.519330024719238, 'motion_component_percent_ionic': 79.80207800865173}, {'ion_id': 1476, 'distance': 7.306352615356445, 'force': [-1.4224494695663452, -3.3690109252929688, -5.0304341316223145], 'magnitude': 6.219233512878418, 'cosine_ionic_motion': 0.5863940119743347, 'motion_component_ionic': 3.646921396255493, 'motion_component_percent_ionic': 58.63940119743347}, {'ion_id': 2434, 'distance': 11.169254302978516, 'force': [-1.0529464483261108, -2.425291061401367, -0.3027394115924835], 'magnitude': 2.6612749099731445, 'cosine_ionic_motion': 0.3750445544719696, 'motion_component_ionic': 0.9980966448783875, 'motion_component_percent_ionic': 37.50445544719696}, {'ion_id': 2443, 'distance': 5.141005992889404, 'force': [-5.28463077545166, -11.308737754821777, 1.405932903289795], 'magnitude': 12.561509132385254, 'cosine_ionic_motion': 0.24328312277793884, 'motion_component_ionic': 3.0560030937194824, 'motion_component_percent_ionic': 24.328312277793884}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.290620803833008, 'force': [4.5950398445129395, -0.5332372188568115, -5.299990653991699], 'magnitude': 7.034815788269043, 'cosine_with_motion': 0.8157256245613098, 'motion_component': 5.7384796142578125, 'motion_component_percent': 81.57256245613098}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.208616733551025, 'force': [2.3981988430023193, -2.072134256362915, 8.12936782836914], 'magnitude': 8.725349426269531, 'cosine_with_motion': -0.13503743708133698, 'motion_component': -1.1782488822937012, 'motion_component_percent': 13.503743708133698}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.3863396644592285, 'force': [-0.35104599595069885, 1.4455454349517822, -6.621984958648682], 'magnitude': 6.78701114654541, 'cosine_with_motion': 0.3093510568141937, 'motion_component': 2.099569082260132, 'motion_component_percent': 30.935105681419373}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.305342674255371, 'force': [-3.8804843425750732, 4.840791702270508, -8.890351295471191], 'magnitude': 10.84111499786377, 'cosine_with_motion': -0.09984415769577026, 'motion_component': -1.0824220180511475, 'motion_component_percent': 9.984415769577026}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.697933673858643, 'force': [1.0434727668762207, -2.4309587478637695, 3.3782551288604736], 'magnitude': 4.290804386138916, 'cosine_with_motion': 0.1191595047712326, 'motion_component': 0.5112901329994202, 'motion_component_percent': 11.91595047712326}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.5273756980896, 'force': [2.3696916103363037, -1.9585676193237305, 3.367398738861084], 'magnitude': 4.559692859649658, 'cosine_with_motion': 0.22878538072109222, 'motion_component': 1.0431910753250122, 'motion_component_percent': 22.878538072109222}]}, 5696: {'frame': 5696, 'motion_vector': [-0.21909713745117188, -0.3765602111816406, 0.164337158203125], 'ionic_force': [-15.213935688138008, -14.176376223564148, -12.65572875738144], 'ionic_force_magnitude': 24.3433964831378, 'radial_force': 20.79503503134424, 'axial_force': -12.65572875738144, 'glu_force': [6.629117012023926, -1.965427279472351, 3.735133409500122], 'glu_force_magnitude': 7.858709711954191, 'asn_force': [1.0297255516052246, 2.3191022872924805, -2.3139519691467285], 'asn_force_magnitude': 3.43408559096478, 'residue_force': [7.65884256362915, 0.3536750078201294, 1.4211814403533936], 'residue_force_magnitude': 7.797609384421552, 'total_force': [-7.555093124508858, -13.822701215744019, -11.234547317028046], 'total_force_magnitude': 19.34842511519411, 'cosine_total_motion': 0.5565600616018778, 'cosine_glu_motion': -0.0269176470304038, 'cosine_asn_motion': -0.9250527483988816, 'cosine_residue_motion': -0.43452398309012064, 'cosine_ionic_motion': 0.5815461688806515, 'motion_component_total': 10.768560674011754, 'motion_component_glu': -0.21153797414078923, 'motion_component_asn': -3.176710314158967, 'motion_component_residue': -3.3882482882997564, 'motion_component_ionic': 14.156808962311512, 'motion_component_percent_total': 55.65600616018778, 'motion_component_percent_glu': 2.69176470304038, 'motion_component_percent_asn': 92.50527483988816, 'motion_component_percent_residue': 43.45239830901206, 'motion_component_percent_ionic': 58.15461688806515, 'ionic_contributions': [{'ion_id': 1355, 'distance': 14.936958312988281, 'force': [0.09340129792690277, -0.6584328413009644, -1.331163763999939], 'magnitude': 1.4880372285842896, 'cosine_ionic_motion': 0.012579542584717274, 'motion_component_ionic': 0.01871882751584053, 'motion_component_percent_ionic': 1.2579542584717274}, {'ion_id': 1469, 'distance': 4.184452533721924, 'force': [-16.17984390258789, -5.707157611846924, -8.072161674499512], 'magnitude': 18.960981369018555, 'cosine_ionic_motion': 0.49469053745269775, 'motion_component_ionic': 9.379817962646484, 'motion_component_percent_ionic': 49.469053745269775}, {'ion_id': 1476, 'distance': 10.000617980957031, 'force': [0.16498154401779175, -2.0770199298858643, -2.584268808364868], 'magnitude': 3.319589853286743, 'cosine_ionic_motion': 0.2078586369752884, 'motion_component_ionic': 0.6900054216384888, 'motion_component_percent_ionic': 20.78586369752884}, {'ion_id': 2434, 'distance': 9.450231552124023, 'force': [-0.31412482261657715, -3.6910321712493896, -0.3123330771923065], 'magnitude': 3.7175185680389404, 'cosine_ionic_motion': 0.8130633234977722, 'motion_component_ionic': 3.022578001022339, 'motion_component_percent_ionic': 81.30633234977722}, {'ion_id': 2443, 'distance': 11.98450756072998, 'force': [1.0216501951217651, -2.042733669281006, -0.35580143332481384], 'magnitude': 2.3115200996398926, 'cosine_ionic_motion': 0.452381432056427, 'motion_component_ionic': 1.0456887483596802, 'motion_component_percent_ionic': 45.2381432056427}], 'glu_contributions': [{'resid': 748, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 5.88142204284668, 'force': [6.629117012023926, -1.965427279472351, 3.735133409500122], 'magnitude': 7.858709812164307, 'cosine_with_motion': -0.026917660608887672, 'motion_component': -0.21153807640075684, 'motion_component_percent': 2.6917660608887672}], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.225194931030273, 'force': [-4.542599201202393, -4.742160797119141, 5.660992622375488], 'magnitude': 8.670071601867676, 'cosine_with_motion': 0.9193159937858582, 'motion_component': 7.9705352783203125, 'motion_component_percent': 91.93159937858582}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.047222137451172, 'force': [5.572324752807617, 7.061263084411621, -7.974944591522217], 'magnitude': 12.021313667297363, 'cosine_with_motion': -0.9272902011871338, 'motion_component': -11.147246360778809, 'motion_component_percent': 92.72902011871338}]}, 5697: {'frame': 5697, 'motion_vector': [-1.5983009338378906, 3.4348678588867188, 0.1610565185546875], 'ionic_force': [-14.388794315978885, -13.769953429698944, -10.123002961277962], 'ionic_force_magnitude': 22.341087893781413, 'radial_force': 19.916049290048065, 'axial_force': -10.123002961277962, 'glu_force': [14.417499542236328, -2.0770235806703568, 5.661137580871582], 'glu_force_magnitude': 15.627757315578009, 'asn_force': [1.2730975151062012, 1.467081069946289, -1.7679595947265625], 'asn_force_magnitude': 2.6265538786307134, 'residue_force': [15.69059705734253, -0.6099425107240677, 3.8931779861450195], 'residue_force_magnitude': 16.177876891424248, 'total_force': [1.3018027413636446, -14.379895940423012, -6.229824975132942], 'total_force_magnitude': 15.72535585783693, 'cosine_total_motion': -0.880050150249696, 'cosine_glu_motion': -0.49386203951895075, 'cosine_asn_motion': 0.27306892439713226, 'cosine_residue_motion': -0.4327345241563049, 'cosine_ionic_motion': -0.3060896568449122, 'motion_component_total': -13.839101785419329, 'motion_component_glu': -7.717956100978558, 'motion_component_asn': 0.7172302425088048, 'motion_component_residue': -7.000725858469753, 'motion_component_ionic': -6.838375926949575, 'motion_component_percent_total': 88.0050150249696, 'motion_component_percent_glu': 49.38620395189508, 'motion_component_percent_asn': 27.306892439713227, 'motion_component_percent_residue': 43.273452415630494, 'motion_component_percent_ionic': 30.608965684491217, 'ionic_contributions': [{'ion_id': 1355, 'distance': 14.766557693481445, 'force': [0.01840483583509922, -0.6926707625389099, -1.3557699918746948], 'magnitude': 1.5225780010223389, 'cosine_ionic_motion': -0.4550085961818695, 'motion_component_ionic': -0.6927860975265503, 'motion_component_percent_ionic': 45.50085961818695}, {'ion_id': 1469, 'distance': 4.3431806564331055, 'force': [-15.130455017089844, -6.483215808868408, -6.229846477508545], 'magnitude': 17.60038948059082, 'cosine_i</t>
         </is>
       </c>
     </row>
@@ -755,7 +755,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>{5892: {'frame': 5892, 'ionic_force': [-2.49815434217453, 7.7181031331419945, -11.375910818576813], 'ionic_force_magnitude': 13.972159390851319, 'motion_vector': [1.8442268371582031, 0.5494155883789062, -1.9481353759765625], 'ionic_force_x': -2.49815434217453, 'ionic_force_y': 7.7181031331419945, 'ionic_force_z': -11.375910818576813, 'radial_force': 8.112329572394216, 'axial_force': -11.375910818576813, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [2.0721981301903725, 7.206418514251709, -10.358462810516357], 'asn_force_magnitude': 12.787659077804847, 'residue_force': [2.0721981301903725, 7.206418514251709, -10.358462810516357], 'residue_force_magnitude': 12.787659077804847, 'total_force': [-0.42595621198415756, 14.924521647393703, -21.73437362909317], 'total_force_magnitude': 26.368651504145443, 'motion_component_total': 18.170321549772634, 'cosine_total_motion': 0.6890880084222759, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.7985007052174479, 'cosine_residue_motion': 0.7985007052174479, 'cosine_ionic_motion': 0.5696590294608859, 'motion_component_glu': None, 'motion_component_asn': 10.210954791707469, 'motion_component_residue': 10.210954791707469, 'motion_component_ionic': 7.959366758065165, 'ionic_contributions': [{'ion_id': 1355, 'distance': 8.86598014831543, 'force': [-1.323460340499878, 0.5493678450584412, -3.9731087684631348], 'magnitude': 4.2236175537109375}, {'ion_id': 1380, 'distance': 6.224255084991455, 'force': [4.6296796798706055, 6.161921977996826, -3.7464330196380615], 'magnitude': 8.56965446472168}, {'ion_id': 1443, 'distance': 14.482345581054688, 'force': [-0.2683507800102234, 0.09991147369146347, -1.5568095445632935], 'magnitude': 1.582924723625183}, {'ion_id': 2434, 'distance': 8.72790813446045, 'force': [-3.6428050994873047, -2.0931317806243896, -1.1591386795043945], 'magnitude': 4.358306407928467}, {'ion_id': 2443, 'distance': 9.511220932006836, 'force': [-1.8932178020477295, 3.0000336170196533, -0.9404208064079285], 'magnitude': 3.6699955463409424}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.281759738922119, 'force': [-0.11318054050207138, -7.720134735107422, 10.348835945129395], 'magnitude': 12.911688804626465}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.179053544998169, 'force': [2.0918679237365723, 11.468158721923828, -15.611472129821777], 'magnitude': 19.48365020751953}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.282458782196045, 'force': [1.7491469383239746, 5.639178276062012, -9.20433521270752], 'magnitude': 10.935247421264648}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.311811447143555, 'force': [-1.655636191368103, -2.180783748626709, 4.108508586883545], 'magnitude': 4.937285900115967}]}, 5893: {'frame': 5893, 'ionic_force': [-2.40166874229908, 3.821544498205185, -9.344871044158936], 'ionic_force_magnitude': 10.377804677842944, 'motion_vector': [1.5363502502441406, -0.806884765625, 5.4425048828125], 'ionic_force_x': -2.40166874229908, 'ionic_force_y': 3.821544498205185, 'ionic_force_z': -9.344871044158936, 'radial_force': 4.513559028028632, 'axial_force': -9.344871044158936, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [5.75072717666626, 6.16840672492981, -0.7180404663085938], 'asn_force_magnitude': 8.463786782278005, 'residue_force': [5.75072717666626, 6.16840672492981, -0.7180404663085938], 'residue_force_magnitude': 8.463786782278005, 'total_force': [3.34905843436718, 9.989951223134995, -10.06291151046753], 'total_force_magnitude': 14.569746253964832, 'motion_component_total': -10.09771182962446, 'cosine_total_motion': -0.6930602395959088, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.0010341729765157542, 'cosine_residue_motion': -0.0010341729765157542, 'cosine_ionic_motion': -0.9721669585471766, 'motion_component_glu': None, 'motion_component_asn': -0.008753019569223142, 'motion_component_residue': -0.008753019569223142, 'motion_component_ionic': -10.088958810055237, 'ionic_contributions': [{'ion_id': 1355, 'distance': 10.92094898223877, 'force': [-0.15968115627765656, 0.468254417181015, -2.7393507957458496], 'magnitude': 2.7836670875549316}, {'ion_id': 1380, 'distance': 8.750675201416016, 'force': [2.5271170139312744, 2.5101613998413086, -2.471982479095459], 'magnitude': 4.335657596588135}, {'ion_id': 2434, 'distance': 8.478754997253418, 'force': [-3.2794134616851807, -2.170670509338379, -2.4210591316223145], 'magnitude': 4.618212699890137}, {'ion_id': 2443, 'distance': 9.380620956420898, 'force': [-1.489691138267517, 3.0137991905212402, -1.7124786376953125], 'magnitude': 3.7728965282440186}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.5242350101470947, 'force': [11.313807487487793, -12.524626731872559, 8.85286808013916], 'magnitude': 19.058902740478516}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.5148048400878906, 'force': [-4.444352626800537, 11.89638900756836, -9.632149696350098], 'magnitude': 15.939091682434082}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.015230417251587, 'force': [-26.79184341430664, 11.911879539489746, -16.333223342895508], 'magnitude': 33.562923431396484}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 2.6753408908843994, 'force': [13.974332809448242, -1.9521121978759766, 13.406163215637207], 'magnitude': 19.463245391845703}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 3.3407742977142334, 'force': [11.698782920837402, -3.1631228923797607, 2.9883012771606445], 'magnitude': 12.48185920715332}]}, 5895: {'frame': 5895, 'ionic_force': [5.1735977828502655, -3.9379420280456543, -22.839519739151], 'ionic_force_magnitude': 23.746940083935648, 'motion_vector': [-0.4307060241699219, 1.0893287658691406, 5.436920166015625], 'ionic_force_x': 5.1735977828502655, 'ionic_force_y': -3.9379420280456543, 'ionic_force_z': -22.839519739151, 'radial_force': 6.5018075513630444, 'axial_force': -22.839519739151, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-1.2915751449763775, -2.572007179260254, 0.15658342093229294], 'asn_force_magnitude': 2.8823437777263656, 'residue_force': [-1.2915751449763775, -2.572007179260254, 0.15658342093229294], 'residue_force_magnitude': 2.8823437777263656, 'total_force': [3.882022637873888, -6.509949207305908, -22.682936318218708], 'total_force_magnitude': 23.915792657970453, 'motion_component_total': -23.749816872599165, 'cosine_total_motion': -0.9930599922927509, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.0869671210202065, 'cosine_residue_motion': -0.0869671210202065, 'cosine_ionic_motion': -0.9895652934399124, 'motion_component_glu': None, 'motion_component_asn': -0.25066914013936803, 'motion_component_residue': -0.25066914013936803, 'motion_component_ionic': -23.499147732459797, 'ionic_contributions': [{'ion_id': 1355, 'distance': 11.54110336303711, 'force': [-0.23459890484809875, -0.226188063621521, -2.4711523056030273], 'magnitude': 2.4925472736358643}, {'ion_id': 1380, 'distance': 8.790602684020996, 'force': [2.8447628021240234, 1.016716718673706, -3.0548858642578125], 'magnitude': 4.296360492706299}, {'ion_id': 2434, 'distance': 10.765507698059082, 'force': [-1.8455193042755127, -1.5154215097427368, -1.5823023319244385], 'magnitude': 2.864633321762085}, {'ion_id': 2443, 'distance': 4.4653754234313965, 'force': [4.4089531898498535, -3.2130491733551025, -15.731179237365723], 'magnitude': 16.650300979614258}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.85567569732666, 'force': [2.235358238220215, -6.513691425323486, -0.4839867651462555], 'magnitude': 6.903567790985107}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.741044998168945, 'force': [-3.4772939682006836, 8.009230613708496, 0.7093163728713989], 'magnitude': 8.760278701782227}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.8515825271606445, 'force': [-0.04963941499590874, -4.067546367645264, -0.0687461867928505], 'magnitude': 4.068429946899414}]}, 5897: {'frame': 5897, 'ionic_force': [1.8552783280611038, -2.173237666487694, -12.846055001020432], 'ionic_force_magnitude': 13.160020847964342, 'motion_vector': [-2.82208251953125, 5.449005126953125, 2.03216552734375], 'ionic_force_x': 1.8552783280611038, 'ionic_force_y': -2.173237666487694, 'ionic_force_z': -12.846055001020432, 'radial_force': 2.8574498472613796, 'axial_force': -12.846055001020432, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [5.754067823290825, 3.725393295288086, 0.30819422006607056], 'asn_force_magnitude': 6.861693333054923, 'residue_force': [5.754067823290825, 3.725393295288086, 0.30819422006607056], 'residue_force_magnitude': 6.861693333054923, 'total_force': [7.609346151351929, 1.5521556288003922, -12.537860780954361], 'total_force_magnitude': 14.748196123923245, 'motion_component_total': -5.955211810474433, 'cosine_total_motion': -0.40379255608178444, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.10568184370924465, 'cosine_residue_motion': 0.10568184370924465, 'cosine_ionic_motion': -0.5076259597196963, 'motion_component_glu': None, 'motion_component_asn': 0.7251564024046764, 'motion_component_residue': 0.7251564024046764, 'motion_component_ionic': -6.6803682128791095, 'ionic_contributions': [{'ion_id': 1355, 'distance': 8.73934555053711, 'force': [-0.9138748049736023, -0.6297469139099121, -4.202837944030762], 'magnitude': 4.346906661987305}, {'ion_id': 1380, 'distance': 5.286211967468262, 'force': [9.447088241577148, 4.048842430114746, -5.9594407081604], 'magnitude': 11.880888938903809}, {'ion_id': 1443, 'distance': 14.335472106933594, 'force': [-0.18578504025936127, -0.21087370812892914, -1.5908935070037842], 'magnitude': 1.615526556968689}, {'ion_id': 2434, 'distance': 10.152715682983398, 'force': [-1.8904106616973877, -2.4841415882110596, -0.7933556437492371], 'magnitude': 3.2208733558654785}, {'ion_id': 2443, 'distance': 7.807744979858398, 'force': [-4.601739406585693, -2.897317886352539, -0.29952719807624817], 'magnitude': 5.446115493774414}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.90973424911499, 'force': [-0.4573526382446289, 7.55396842956543, -4.366289138793945], 'magnitude': 8.737052917480469}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.805153846740723, 'force': [-0.3889302909374237, -3.3646371364593506, 2.369807720184326], 'magnitude': 4.133768081665039}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.974772930145264, 'force': [0.23733748495578766, -3.653355598449707, 1.35104238986969], 'magnitude': 3.902390480041504}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.741364002227783, 'force': [6.36301326751709, 3.189417600631714, 0.9536332488059998], 'magnitude': 7.181207656860352}]}, 5898: {'frame': 5898, 'ionic_force': [-8.504436016082764, 11.964142084121704, -4.874931126832962], 'ionic_force_magnitude': 15.467096729899332, 'motion_vector': [1.28692626953125, 1.0255928039550781, -0.0074005126953125], 'ionic_force_x': -8.504436016082764, 'ionic_force_y': 11.964142084121704, 'ionic_force_z': -4.874931126832962, 'radial_force': 14.678764517516374, 'axial_force': -4.874931126832962, 'glu_force': [-6.0847327709198, 27.38208770751953, 0.3657366633415222], 'glu_force_magnitude': 28.0523878381629, 'asn_force': [-0.9865337014198303, 1.5351793766021729, 3.704575300216675], 'asn_force_magnitude': 4.129637104801972, 'residue_force': [-7.07126647233963, 28.917267084121704, 4.070311963558197], 'residue_force_magnitude': 30.0462740554956, 'total_force': [-15.575702488422394, 40.88140916824341, -0.804619163274765], 'total_force_magnitude': 43.75545149563757, 'motion_component_total': 13.301255936647456, 'cosine_total_motion': 0.30399082815940304, 'cosine_glu_motion': 0.4386473239877334, 'cosine_asn_motion': 0.0408275550169387, 'cosine_residue_motion': 0.4151499057664685, 'cosine_ionic_motion': 0.053503776974203714, 'motion_component_glu': 12.305104856676193, 'motion_component_asn': 0.16860298609629398, 'motion_component_residue': 12.473707842772486, 'motion_component_ionic': 0.8275480938749694, 'ionic_contributions': [{'ion_id': 1355, 'distance': 8.775650978088379, 'force': [-2.246494770050049, 1.9543259143829346, -3.1174850463867188], 'magnitude': 4.311013698577881}, {'ion_id': 1380, 'distance': 6.865221977233887, 'force': [1.3024711608886719, 6.837247848510742, -1.0843136310577393], 'magnitude': 7.044155597686768}, {'ion_id': 1443, 'distance': 13.32459545135498, 'force': [-0.6266984939575195, 0.5076103806495667, -1.6870962381362915], 'magnitude': 1.8699499368667603}, {'ion_id': 2434, 'distance': 9.414612770080566, 'force': [-3.711239814758301, -0.4314489960670471, -0.2661377489566803], 'magnitude': 3.745701313018799}, {'ion_id': 2443, 'distance': 8.450874328613281, 'force': [-3.2224740982055664, 3.096406936645508, 1.2801015377044678], 'magnitude': 4.6487345695495605}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.7421162128448486, 'force': [4.402163028717041, -18.31712532043457, -3.1169562339782715], 'magnitude': 19.094804763793945}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 3.1276965141296387, 'force': [1.2825896739959717, 27.75776481628418, -0.26049691438674927], 'magnitude': 27.788602828979492}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 3.5327703952789307, 'force': [-11.769485473632812, 17.941448211669922, 3.743189811706543], 'magnitude': 21.78136444091797}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.808056354522705, 'force': [-0.9865337014198303, 1.5351793766021729, 3.704575300216675], 'magnitude': 4.129636764526367}]}, 5899: {'frame': 5899, 'ionic_force': [-6.799471914768219, 9.492137521505356, -5.600397616624832], 'ionic_force_magnitude': 12.949824188427762, 'motion_vector': [-1.2925643920898438, 0.4482421875, -0.7178955078125], 'ionic_force_x': -6.799471914768219, 'ionic_force_y': 9.492137521505356, 'ionic_force_z': -5.600397616624832, 'radial_force': 11.676193431375298, 'axial_force': -5.600397616624832, 'glu_force': [-14.378485679626465, 17.21088981628418, -0.5976857244968414], 'glu_force_magnitude': 22.43463409402447, 'asn_force': [0.1363511085510254, 2.1622188091278076, 3.2376694679260254], 'asn_force_magnitude': 3.8956752157860337, 'residue_force': [-14.24213457107544, 19.373108625411987, 2.639983743429184], 'residue_force_magnitude': 24.18936231317818, 'total_force': [-21.04160648584366, 28.865246146917343, -2.960413873195648], 'total_force_magnitude': 35.84293080828957, 'motion_component_total': 27.35377618262949, 'cosine_total_motion': 0.7631567945415682, 'cosine_glu_motion': 0.7711401530138393, 'cosine_asn_motion': -0.2544279520088098, 'cosine_residue_motion': 0.6742252354600744, 'cosine_ionic_motion': 0.8528839867391913, 'motion_component_glu': 17.300247168075526, 'motion_component_asn': -0.9911686668439188, 'motion_component_residue': 16.309078501231607, 'motion_component_ionic': 11.044697681397881, 'ionic_contributions': [{'ion_id': 1355, 'distance': 8.837882995605469, 'force': [-1.5860280990600586, 2.484849214553833, -3.0621752738952637], 'magnitude': 4.250514984130859}, {'ion_id': 1380, 'distance': 8.98376750946045, 'force': [1.502514123916626, 3.8119521141052246, -0.36482638120651245], 'magnitude': 4.113590717315674}, {'ion_id': 1443, 'distance': 13.691761016845703, 'force': [-0.44899803400039673, 0.7380704879760742, -1.5459970235824585], 'magnitude': 1.7710037231445312}, {'ion_id': 2434, 'distance': 7.952696323394775, 'force': [-5.232437610626221, -0.4004041254520416, -0.13199836015701294], 'magnitude': 5.249395370483398}, {'ion_id': 2443, 'distance': 10.383524894714355, 'force': [-1.034522294998169, 2.8576698303222656, -0.4954005777835846], 'magnitude': 3.079274892807007}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.9437255859375, 'force': [11.095504760742188, -12.466623306274414, -4.129337787628174], 'magnitude': 17.192392349243164}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 3.2568912506103516, 'force': [-13.083478927612305, 22.031465530395508, 0.4641817510128021], 'magnitude': 25.627687454223633}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 4.274304389953613, 'force': [-12.390511512756348, 7.646047592163086, 3.0674703121185303], 'magnitude': 14.879387855529785}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.979920387268066, 'force': [0.1363511085510254, 2.1622188091278076, 3.2376694679260254], 'magnitude': 3.8956751823425293}]}, 5900: {'frame': 5900, 'ionic_force': [-6.1381120681762695, 8.840319886803627, -5.065477430820465], 'ionic_force_magnitude': 11.894819757552376, 'motion_vector': [1.6382980346679688, 0.11060333251953125, 0.5860443115234375], 'ionic_force_x': -6.1381120681762695, 'ionic_force_y': 8.840319886803627, 'ionic_force_z': -5.065477430820465, 'radial_force': 10.762326675143571, 'axial_force': -5.065477430820465, 'glu_force': [-13.204449653625488, 35.04855918884277, 7.875988960266113], 'glu_force_magnitude': 38.27257757156133, 'asn_force': [-0.1663786768913269, 1.9670840501785278, 3.335846185684204], 'asn_force_magnitude': 3.876205786479186, 'residue_force': [-13.370828330516815, 37.0156432390213, 11.211835145950317], 'residue_force_magnitude': 40.92239169431109, 'total_force': [-19.508940398693085, 45.85596312582493, 6.146357715129852], 'total_force_magnitude': 50.21101296368269, 'motion_component_total': -13.357009560779273, 'cosine_total_motion': -0.26601752827492875, 'cosine_glu_motion': -0.1969309319969785, 'cosine_asn_motion': 0.28113699634928935, 'cosine_residue_motion': -0.15754967518059365, 'cosine_ionic_motion': -0.580899936490451, 'motion_component_glu': -7.537054371094229, 'motion_component_asn': 1.089744852042493, 'motion_component_residue': -6.4473095190517355, 'motion_component_ionic': -6.909700041727537, 'ionic_contributions': [{'ion_id': 1355, 'distance': 9.429265022277832, 'force': [-1.8010727167129517, 2.0751216411590576, -2.528494358062744], 'magnitude': 3.734069585800171}, {'ion_id': 1380, 'distance': 9.132181167602539, 'force': [0.7935147881507874, 3.8666439056396484, -0.5172351598739624], 'magnitude': 3.980971336364746}, {'ion_id': 1443, 'distance': 14.607885360717773, 'force': [-0.539768397808075, 0.6087048649787903, -1.3261784315109253], 'magnitude': 1.555834412574768}, {'ion_id': 2434, 'distance': 9.848250389099121, 'force': [-3.400973320007324, 0.1036798506975174, -0.37451714277267456], 'magnitude': 3.423102617263794}, {'ion_id': 2443, 'distance': 11.502422332763672, 'force': [-1.189812421798706, 2.1861696243286133, -0.3190523386001587], 'magnitude': 2.5093395709991455}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.0938239097595215, 'force': [9.60705280303955, -24.070093154907227, -10.427596092224121], 'magnitude': 27.935632705688477}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 2.6615397930145264, 'force': [-0.44991493225097656, 37.92254638671875, 5.859124183654785], 'magnitude': 38.37513732910156}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.860210418701172, 'force': [-22.361587524414062, 21.19610595703125, 12.44446086883545], 'magnitude': 33.22920608520508}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.994919776916504, 'force': [-0.1663786768913269, 1.9670840501785278, 3.335846185684204], 'magnitude': 3.8762056827545166}]}, 5901: {'frame': 5901, 'ionic_force': [-7.439622104167938, 9.131087750196457, -4.992527484893799], 'ionic_force_magnitude': 12.792578756530364, 'motion_vector': [-0.2744865417480469, -0.7472152709960938, 0.6619415283203125], 'ionic_force_x': -7.439622104167938, 'ionic_force_y': 9.131087750196457, 'ionic_force_z': -4.992527484893799, 'radial_force': 11.77814673684328, 'axial_force': -4.992527484893799, 'glu_force': [-17.11140537261963, 17.92721128463745, 0.5718311071395874], 'glu_force_magnitude': 24.789354349906752, 'asn_force': [1.2753161489963531, 0.5340880155563354, 0.8194022178649902], 'asn_force_magnitude': 1.6072029376820645, 'residue_force': [-15.836089223623276, 18.461299300193787, 1.3912333250045776], 'residue_force_magnitude': 24.362611188345475, 'total_force': [-23.275711327791214, 27.592387050390244, -3.601294159889221], 'total_force_magnitude': 36.277649876739034, 'motion_component_total': -16.046052413357938, 'cosine_total_motion': -0.44231234569708305, 'cosine_glu_motion': -0.32418974116579324, 'cosine_asn_motion': -0.12424751672783133, 'cosine_residue_motion': -0.33806496686972776, 'cosine_ionic_motion': -0.6105029500110021, 'motion_component_glu': -8.036454370363401, 'motion_component_asn': -0.19969097388467194, 'motion_component_residue': -8.236145344248072, 'motion_component_ionic': -7.8099070691098635, 'ionic_contributions': [{'ion_id': 1355, 'distance': 8.822335243225098, 'force': [-1.4037278890609741, 2.735112428665161, -2.956904888153076], 'magnitude': 4.265510082244873}, {'ion_id': 1380, 'distance': 9.430712699890137, 'force': [1.2992652654647827, 3.4894778728485107, -0.26489782333374023], 'magnitude': 3.7329232692718506}, {'ion_id': 1443, 'distance': 14.058492660522461, 'force': [-0.41779905557632446, 0.741924524307251, -1.4480189085006714], 'magnitude': 1.6798115968704224}, {'ion_id': 2434, 'distance': 8.001550674438477, 'force': [-5.164675235748291, 0.30420610308647156, -0.35055652260780334], 'magnitude': 5.185489654541016}, {'ion_id': 2443, 'distance': 11.396726608276367, 'force': [-1.7526851892471313, 1.8603668212890625, 0.02785065770149231], 'magnitude': 2.5560996532440186}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.7720160484313965, 'force': [13.748322486877441, -11.805517196655273, -4.980049133300781], 'magnitude': 18.793283462524414}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 3.0480844974517822, 'force': [-16.925514221191406, 23.783924102783203, 1.9876269102096558], 'magnitude': 29.259164810180664}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 4.179169654846191, 'force': [-13.934213638305664, 5.9488043785095215, 3.564253330230713], 'magnitude': 15.564526557922363}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.706557750701904, 'force': [-0.3456059396266937, 2.0732614994049072, 6.958563327789307], 'magnitude': 7.269075870513916}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.489872932434082, 'force': [1.6209220886230469, -1.5391734838485718, -6.139161109924316], 'magnitude': 6.533432960510254}]}, 5902: {'frame': 5902, 'ionic_force': [-7.47670590877533, 10.180595852434635, -5.091444402933121], 'ionic_force_magnitude': 13.618680892989754, 'motion_vector': [-0.6989402770996094, 0.07197189331054688, -0.5127105712890625], 'ionic_force_x': -7.47670590877533, 'ionic_force_y': 10.180595852434635, 'ionic_force_z': -5.091444402933121, 'radial_force': 12.631138632638201, 'axial_force': -5.091444402933121, 'glu_force': [-21.30510711669922, 25.9502592086792, -5.566610872745514], 'glu_force_magnitude': 34.033963901670866, 'asn_force': [1.2503969967365265, 0.6573889255523682, -0.4454002380371094], 'asn_force_magnitude': 1.4812272684939796, 'residue_force': [-20.054710119962692, 26.607648134231567, -6.012011110782623], 'residue_force_magnitude': 33.8570910567784, 'total_force': [-27.531416028738022, 36.7882439866662, -11.103455513715744], 'total_force_magnitude': 47.27198418212419, 'motion_component_total': 31.71197202788742, 'cosine_total_motion': 0.6708407226087887, 'cosine_glu_motion': 0.6625237287437387, 'cosine_asn_motion': -0.46436213865074233, 'cosine_residue_motion': 0.6456692563805629, 'cosine_ionic_motion': 0.72338057550929, 'motion_component_glu': 22.54830866806478, 'motion_component_asn': -0.6878258622256617, 'motion_component_residue': 21.86048280583912, 'motion_component_ionic': 9.8514892220483, 'ionic_contributions': [{'ion_id': 1355, 'distance': 7.728732109069824, 'force': [-2.3436784744262695, 3.635133743286133, -3.490668773651123], 'magnitude': 5.558038711547852}, {'ion_id': 1380, 'distance': 8.802467346191406, 'force': [1.7799241542816162, 3.8899707794189453, -0.24371981620788574], 'magnitude': 4.284787178039551}, {'ion_id': 1443, 'distance': 12.639395713806152, 'force': [-0.6318591833114624, 0.8132873177528381, -1.8050473928451538], 'magnitude': 2.078191041946411}, {'ion_id': 2434, 'distance': 9.059673309326172, 'force': [-4.041162490844727, 0.0778370276093483, 0.15670618414878845], 'magnitude': 4.044948577880859}, {'ion_id': 2443, 'distance': 10.762557983398438, 'force': [-2.2399299144744873, 1.7643669843673706, 0.2912853956222534], 'magnitude': 2.866203784942627}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.519524574279785, 'force': [14.935579299926758, -15.490436553955078, -1.717751383781433], 'magnitude': 21.58647346496582}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 2.638275623321533, 'force': [-20.212709426879883, 33.11326599121094, -4.499279975891113], 'magnitude': 39.05490493774414}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 3.878218173980713, 'force': [-16.027976989746094, 8.32742977142334, 0.6504204869270325], 'magnitude': 18.073881149291992}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.74351692199707, 'force': [-0.4163481891155243, 1.2797852754592896, 7.0484938621521], 'magnitude': 7.1758246421813965}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.056216239929199, 'force': [1.6667451858520508, -0.6223963499069214, -7.493894100189209], 'magnitude': 7.702198505401611}]}, 5903: {'frame': 5903, 'ionic_force': [-7.226976692676544, 9.150095321238041, -4.231179058551788], 'ionic_force_magnitude': 12.403882969850992, 'motion_vector': [-2.064189910888672, -0.9773674011230469, 0.5256500244140625], 'ionic_force_x': -7.226976692676544, 'ionic_force_y': 9.150095321238041, 'ionic_force_z': -4.231179058551788, 'radial_force': 11.65990722536986, 'axial_force': -4.231179058551788, 'glu_force': [-21.258756637573242, 30.960488319396973, -2.6409695148468018], 'glu_force_magnitude': 37.64918711910565, 'asn_force': [-2.484264612197876, 0.550076425075531, 4.405158042907715], 'asn_force_magnitude': 5.087196882354473, 'residue_force': [-23.743021249771118, 31.510564744472504, 1.764188528060913], 'residue_force_magnitude': 39.49378571047878, 'total_force': [-30.969997942447662, 40.660660065710545, -2.4669905304908752], 'total_force_magnitude': 51.17143824255883, 'motion_component_total': 9.767380424322951, 'cosine_total_motion': 0.1908756282757655, 'cosine_glu_motion': 0.13865463808292292, 'cosine_asn_motion': 0.5792441905647682, 'cosine_residue_motion': 0.20679110669079126, 'cosine_ionic_motion': 0.12902546514942756, 'motion_component_glu': 5.220234414115836, 'motion_component_asn': 2.9467292403630285, 'motion_component_residue': 8.166963654478865, 'motion_component_ionic': 1.6004167698440872, 'ionic_contributions': [{'ion_id': 1355, 'distance': 8.847192764282227, 'force': [-1.8546229600906372, 2.477461338043213, -2.9006059169769287], 'magnitude': 4.241574764251709}, {'ion_id': 1380, 'distance': 8.467968940734863, 'force': [1.4170900583267212, 4.401101589202881, -0.24274271726608276], 'magnitude': 4.629985332489014}, {'ion_id': 1443, 'distance': 13.62232780456543, 'force': [-0.5996553301811218, 0.7718545794487, -1.4985142946243286], 'magnitude': 1.7891035079956055}, {'ion_id': 2434, 'distance': 8.815616607666016, 'force': [-4.2714080810546875, 0.0717788115143776, 0.005224108695983887], 'magnitude': 4.272014141082764}, {'ion_id': 2443, 'distance': 11.69931697845459, 'force': [-1.9183803796768188, 1.4278990030288696, 0.40545976161956787], 'magnitude': 2.4255878925323486}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.1204171180725098, 'force': [15.473880767822266, -21.63675308227539, -6.82235050201416], 'magnitude': 27.461509704589844}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 2.5072312355041504, 'force': [-16.3488712310791, 39.954471588134766, -2.5316598415374756], 'magnitude': 43.2441291809082}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 3.3036160469055176, 'force': [-20.383766174316406, 12.642769813537598, 6.713040828704834], 'magnitude': 24.907878875732422}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.232961177825928, 'force': [-2.484264612197876, 0.550076425075531, 4.405158042907715], 'magnitude': 5.0871968269348145}]}, 5904: {'frame': 5904, 'ionic_force': [-9.568521454930305, 7.556034505367279, -3.6204235684126616], 'ionic_force_magnitude': 12.718401121779435, 'motion_vector': [0.26805877685546875, -0.65460205078125, 0.54949951171875], 'ionic_force_x': -9.568521454930305, 'ionic_force_y': 7.556034505367279, 'ionic_force_z': -3.6204235684126616, 'radial_force': 12.192221302115644, 'axial_force': -3.6204235684126616, 'glu_force': [-6.736070156097412, 32.19764709472656, -4.970304608345032], 'glu_force_magnitude': 33.26810856487269, 'asn_force': [-1.2161200046539307, 1.3885096311569214, 3.4054620265960693], 'asn_force_magnitude': 3.8735098394250675, 'residue_force': [-7.952190160751343, 33.586156725883484, -1.5648425817489624], 'residue_force_magnitude': 34.55019514089629, 'total_force': [-17.52071161568165, 41.14219123125076, -5.185266150161624], 'total_force_magnitude': 45.01713251504032, 'motion_component_total': -38.49167003972468, 'cosine_total_motion': -0.8550449104430303, 'cosine_glu_motion': -0.859547315378275, 'cosine_asn_motion': 0.18341955773818241, 'cosine_residue_motion': -0.8070876540433944, 'cosine_ionic_motion': -0.8339597088626205, 'motion_component_glu': -28.595513404649317, 'motion_component_asn': 0.7104774616418439, 'motion_component_residue': -27.885035943007473, 'motion_component_ionic': -10.606634096717203, 'ionic_contributions': [{'ion_id': 1355, 'distance': 8.908178329467773, 'force': [-2.7520177364349365, 2.0397398471832275, -2.4019126892089844], 'magnitude': 4.183697700500488}, {'ion_id': 1380, 'distance': 8.066484451293945, 'force': [-0.21680445969104767, 5.097675800323486, -0.02414863370358944], 'magnitude': 5.102341175079346}, {'ion_id': 1443, 'distance': 13.487966537475586, 'force': [-0.8819059133529663, 0.5921956896781921, -1.4838796854019165], 'magnitude': 1.8249253034591675}, {'ion_id': 2434, 'distance': 9.327481269836426, 'force': [-3.755582809448242, -0.6733697652816772, -0.06396784633398056], 'magnitude': 3.8160085678100586}, {'ion_id': 2443, 'distance': 12.709017753601074, 'force': [-1.9622105360031128, 0.4997929334640503, 0.3534852862358093], 'magnitude': 2.0554840564727783}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.059662103652954, 'force': [1.2786283493041992, -28.47112274169922, -1.8977328538894653], 'magnitude': 28.56293296813965}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 2.9579639434814453, 'force': [7.892388820648193, 29.26656723022461, -6.817164421081543], 'magnitude': 31.06920623779297}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.7711286544799805, 'force': [-15.907087326049805, 31.402202606201172, 3.7445926666259766], 'magnitude': 35.399940490722656}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.997005462646484, 'force': [-1.2161200046539307, 1.3885096311569214, 3.4054620265960693], 'magnitude': 3.8735098838806152}]}, 5905: {'frame': 5905, 'ionic_force': [-9.992130100727081, 6.58165055513382, -3.931290879845619], 'ionic_force_magnitude': 12.594277905529433, 'motion_vector': [0.7903480529785156, -0.9876708984375, -0.41739654541015625], 'ionic_force_x': -9.992130</t>
+          <t>{5892: {'frame': 5892, 'motion_vector': [1.8442268371582031, 0.5494155883789062, -1.9481353759765625], 'ionic_force': [-2.49815434217453, 7.7181031331419945, -11.375910818576813], 'ionic_force_magnitude': 13.972159390851319, 'radial_force': 8.112329572394216, 'axial_force': -11.375910818576813, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [2.0721981301903725, 7.206418514251709, -10.358462810516357], 'asn_force_magnitude': 12.787659077804847, 'residue_force': [2.0721981301903725, 7.206418514251709, -10.358462810516357], 'residue_force_magnitude': 12.787659077804847, 'total_force': [-0.42595621198415756, 14.924521647393703, -21.73437362909317], 'total_force_magnitude': 26.368651504145443, 'cosine_total_motion': 0.6890880084222759, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.7985007052174479, 'cosine_residue_motion': 0.7985007052174479, 'cosine_ionic_motion': 0.5696590294608859, 'motion_component_total': 18.170321549772634, 'motion_component_glu': None, 'motion_component_asn': 10.210954791707469, 'motion_component_residue': 10.210954791707469, 'motion_component_ionic': 7.959366758065165, 'motion_component_percent_total': 68.90880084222759, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 79.85007052174478, 'motion_component_percent_residue': 79.85007052174478, 'motion_component_percent_ionic': 56.96590294608859, 'ionic_contributions': [{'ion_id': 1355, 'distance': 8.86598014831543, 'force': [-1.323460340499878, 0.5493678450584412, -3.9731087684631348], 'magnitude': 4.2236175537109375, 'cosine_ionic_motion': 0.4843039810657501, 'motion_component_ionic': 2.0455148220062256, 'motion_component_percent_ionic': 48.43039810657501}, {'ion_id': 1380, 'distance': 6.224255084991455, 'force': [4.6296796798706055, 6.161921977996826, -3.7464330196380615], 'magnitude': 8.56965446472168, 'cosine_ionic_motion': 0.8191423416137695, 'motion_component_ionic': 7.019766807556152, 'motion_component_percent_ionic': 81.91423416137695}, {'ion_id': 1443, 'distance': 14.482345581054688, 'force': [-0.2683507800102234, 0.09991147369146347, -1.5568095445632935], 'magnitude': 1.582924723625183, 'cosine_ionic_motion': 0.5981912016868591, 'motion_component_ionic': 0.9468916654586792, 'motion_component_percent_ionic': 59.81912016868591}, {'ion_id': 2434, 'distance': 8.72790813446045, 'force': [-3.6428050994873047, -2.0931317806243896, -1.1591386795043945], 'magnitude': 4.358306407928467, 'cosine_ionic_motion': -0.47007235884666443, 'motion_component_ionic': -2.0487194061279297, 'motion_component_percent_ionic': 47.00723588466644}, {'ion_id': 2443, 'distance': 9.511220932006836, 'force': [-1.8932178020477295, 3.0000336170196533, -0.9404208064079285], 'magnitude': 3.6699955463409424, 'cosine_ionic_motion': -0.0011135850800201297, 'motion_component_ionic': -0.004086852073669434, 'motion_component_percent_ionic': 0.11135850800201297}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.281759738922119, 'force': [-0.11318054050207138, -7.720134735107422, 10.348835945129395], 'magnitude': 12.911688804626465, 'cosine_with_motion': -0.6960972547531128, 'motion_component': -8.987791061401367, 'motion_component_percent': 69.60972547531128}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.179053544998169, 'force': [2.0918679237365723, 11.468158721923828, -15.611472129821777], 'magnitude': 19.48365020751953, 'cosine_with_motion': 0.7604576349258423, 'motion_component': 14.816490173339844, 'motion_component_percent': 76.04576349258423}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.282458782196045, 'force': [1.7491469383239746, 5.639178276062012, -9.20433521270752], 'magnitude': 10.935247421264648, 'cosine_with_motion': 0.8100259900093079, 'motion_component': 8.857834815979004, 'motion_component_percent': 81.00259900093079}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.311811447143555, 'force': [-1.655636191368103, -2.180783748626709, 4.108508586883545], 'magnitude': 4.937285900115967, 'cosine_with_motion': -0.9064856171607971, 'motion_component': -4.475578784942627, 'motion_component_percent': 90.64856171607971}]}, 5893: {'frame': 5893, 'motion_vector': [1.5363502502441406, -0.806884765625, 5.4425048828125], 'ionic_force': [-2.40166874229908, 3.821544498205185, -9.344871044158936], 'ionic_force_magnitude': 10.377804677842944, 'radial_force': 4.513559028028632, 'axial_force': -9.344871044158936, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [5.75072717666626, 6.16840672492981, -0.7180404663085938], 'asn_force_magnitude': 8.463786782278005, 'residue_force': [5.75072717666626, 6.16840672492981, -0.7180404663085938], 'residue_force_magnitude': 8.463786782278005, 'total_force': [3.34905843436718, 9.989951223134995, -10.06291151046753], 'total_force_magnitude': 14.569746253964832, 'cosine_total_motion': -0.6930602395959088, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.0010341729765157542, 'cosine_residue_motion': -0.0010341729765157542, 'cosine_ionic_motion': -0.9721669585471766, 'motion_component_total': -10.09771182962446, 'motion_component_glu': None, 'motion_component_asn': -0.008753019569223142, 'motion_component_residue': -0.008753019569223142, 'motion_component_ionic': -10.088958810055237, 'motion_component_percent_total': 69.30602395959087, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 0.10341729765157542, 'motion_component_percent_residue': 0.10341729765157542, 'motion_component_percent_ionic': 97.21669585471766, 'ionic_contributions': [{'ion_id': 1355, 'distance': 10.92094898223877, 'force': [-0.15968115627765656, 0.468254417181015, -2.7393507957458496], 'magnitude': 2.7836670875549316, 'cosine_ionic_motion': -0.9767616987228394, 'motion_component_ionic': -2.7189793586730957, 'motion_component_percent_ionic': 97.67616987228394}, {'ion_id': 1380, 'distance': 8.750675201416016, 'force': [2.5271170139312744, 2.5101613998413086, -2.471982479095459], 'magnitude': 4.335657596588135, 'cosine_ionic_motion': -0.4682241380214691, 'motion_component_ionic': -2.030059576034546, 'motion_component_percent_ionic': 46.82241380214691}, {'ion_id': 2434, 'distance': 8.478754997253418, 'force': [-3.2794134616851807, -2.170670509338379, -2.4210591316223145], 'magnitude': 4.618212699890137, 'cosine_ionic_motion': -0.6240562796592712, 'motion_component_ionic': -2.8820245265960693, 'motion_component_percent_ionic': 62.405627965927124}, {'ion_id': 2443, 'distance': 9.380620956420898, 'force': [-1.489691138267517, 3.0137991905212402, -1.7124786376953125], 'magnitude': 3.7728965282440186, 'cosine_ionic_motion': -0.6514610648155212, 'motion_component_ionic': -2.457895278930664, 'motion_component_percent_ionic': 65.14610648155212}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.5242350101470947, 'force': [11.313807487487793, -12.524626731872559, 8.85286808013916], 'magnitude': 19.058902740478516, 'cosine_with_motion': 0.6950246691703796, 'motion_component': 13.246407508850098, 'motion_component_percent': 69.50246691703796}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.5148048400878906, 'force': [-4.444352626800537, 11.89638900756836, -9.632149696350098], 'magnitude': 15.939091682434082, 'cosine_with_motion': -0.7561663389205933, 'motion_component': -12.052604675292969, 'motion_component_percent': 75.61663389205933}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.015230417251587, 'force': [-26.79184341430664, 11.911879539489746, -16.333223342895508], 'magnitude': 33.562923431396484, 'cosine_with_motion': -0.7284665703773499, 'motion_component': -24.4494686126709, 'motion_component_percent': 72.84665703773499}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 2.6753408908843994, 'force': [13.974332809448242, -1.9521121978759766, 13.406163215637207], 'magnitude': 19.463245391845703, 'cosine_with_motion': 0.8635093569755554, 'motion_component': 16.80669403076172, 'motion_component_percent': 86.35093569755554}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 3.3407742977142334, 'force': [11.698782920837402, -3.1631228923797607, 2.9883012771606445], 'magnitude': 12.48185920715332, 'cosine_with_motion': 0.5159663558006287, 'motion_component': 6.440219402313232, 'motion_component_percent': 51.596635580062866}]}, 5895: {'frame': 5895, 'motion_vector': [-0.4307060241699219, 1.0893287658691406, 5.436920166015625], 'ionic_force': [5.1735977828502655, -3.9379420280456543, -22.839519739151], 'ionic_force_magnitude': 23.746940083935648, 'radial_force': 6.5018075513630444, 'axial_force': -22.839519739151, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-1.2915751449763775, -2.572007179260254, 0.15658342093229294], 'asn_force_magnitude': 2.8823437777263656, 'residue_force': [-1.2915751449763775, -2.572007179260254, 0.15658342093229294], 'residue_force_magnitude': 2.8823437777263656, 'total_force': [3.882022637873888, -6.509949207305908, -22.682936318218708], 'total_force_magnitude': 23.915792657970453, 'cosine_total_motion': -0.9930599922927509, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.0869671210202065, 'cosine_residue_motion': -0.0869671210202065, 'cosine_ionic_motion': -0.9895652934399124, 'motion_component_total': -23.749816872599165, 'motion_component_glu': None, 'motion_component_asn': -0.25066914013936803, 'motion_component_residue': -0.25066914013936803, 'motion_component_ionic': -23.499147732459797, 'motion_component_percent_total': 99.30599922927509, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 8.69671210202065, 'motion_component_percent_residue': 8.69671210202065, 'motion_component_percent_ionic': 98.95652934399124, 'ionic_contributions': [{'ion_id': 1355, 'distance': 11.54110336303711, 'force': [-0.23459890484809875, -0.226188063621521, -2.4711523056030273], 'magnitude': 2.4925472736358643, 'cosine_ionic_motion': -0.9796624183654785, 'motion_component_ionic': -2.441854953765869, 'motion_component_percent_ionic': 97.96624183654785}, {'ion_id': 1380, 'distance': 8.790602684020996, 'force': [2.8447628021240234, 1.016716718673706, -3.0548858642578125], 'magnitude': 4.296360492706299, 'cosine_ionic_motion': -0.7000171542167664, 'motion_component_ionic': -3.007526159286499, 'motion_component_percent_ionic': 70.00171542167664}, {'ion_id': 2434, 'distance': 10.765507698059082, 'force': [-1.8455193042755127, -1.5154215097427368, -1.5823023319244385], 'magnitude': 2.864633321762085, 'cosine_ionic_motion': -0.593690037727356, 'motion_component_ionic': -1.7007043361663818, 'motion_component_percent_ionic': 59.369003772735596}, {'ion_id': 2443, 'distance': 4.4653754234313965, 'force': [4.4089531898498535, -3.2130491733551025, -15.731179237365723], 'magnitude': 16.650300979614258, 'cosine_ionic_motion': -0.9819079041481018, 'motion_component_ionic': -16.349061965942383, 'motion_component_percent_ionic': 98.19079041481018}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.85567569732666, 'force': [2.235358238220215, -6.513691425323486, -0.4839867651462555], 'magnitude': 6.903567790985107, 'cosine_with_motion': -0.2784116864204407, 'motion_component': -1.9220340251922607, 'motion_component_percent': 27.841168642044067}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.741044998168945, 'force': [-3.4772939682006836, 8.009230613708496, 0.7093163728713989], 'magnitude': 8.760278701782227, 'cosine_with_motion': 0.28896433115005493, 'motion_component': 2.5314080715179443, 'motion_component_percent': 28.896433115005493}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.8515825271606445, 'force': [-0.04963941499590874, -4.067546367645264, -0.0687461867928505], 'magnitude': 4.068429946899414, 'cosine_with_motion': -0.21139441430568695, 'motion_component': -0.8600433468818665, 'motion_component_percent': 21.139441430568695}]}, 5897: {'frame': 5897, 'motion_vector': [-2.82208251953125, 5.449005126953125, 2.03216552734375], 'ionic_force': [1.8552783280611038, -2.173237666487694, -12.846055001020432], 'ionic_force_magnitude': 13.160020847964342, 'radial_force': 2.8574498472613796, 'axial_force': -12.846055001020432, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [5.754067823290825, 3.725393295288086, 0.30819422006607056], 'asn_force_magnitude': 6.861693333054923, 'residue_force': [5.754067823290825, 3.725393295288086, 0.30819422006607056], 'residue_force_magnitude': 6.861693333054923, 'total_force': [7.609346151351929, 1.5521556288003922, -12.537860780954361], 'total_force_magnitude': 14.748196123923245, 'cosine_total_motion': -0.40379255608178444, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.10568184370924465, 'cosine_residue_motion': 0.10568184370924465, 'cosine_ionic_motion': -0.5076259597196963, 'motion_component_total': -5.955211810474433, 'motion_component_glu': None, 'motion_component_asn': 0.7251564024046764, 'motion_component_residue': 0.7251564024046764, 'motion_component_ionic': -6.6803682128791095, 'motion_component_percent_total': 40.37925560817845, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 10.568184370924465, 'motion_component_percent_residue': 10.568184370924465, 'motion_component_percent_ionic': 50.762595971969624, 'ionic_contributions': [{'ion_id': 1355, 'distance': 8.73934555053711, 'force': [-0.9138748049736023, -0.6297469139099121, -4.202837944030762], 'magnitude': 4.346906661987305, 'cosine_ionic_motion': -0.3342922329902649, 'motion_component_ionic': -1.4531371593475342, 'motion_component_percent_ionic': 33.42922329902649}, {'ion_id': 1380, 'distance': 5.286211967468262, 'force': [9.447088241577148, 4.048842430114746, -5.9594407081604], 'magnitude': 11.880888938903809, 'cosine_ionic_motion': -0.21756315231323242, 'motion_component_ionic': -2.584843635559082, 'motion_component_percent_ionic': 21.756315231323242}, {'ion_id': 1443, 'distance': 14.335472106933594, 'force': [-0.18578504025936127, -0.21087370812892914, -1.5908935070037842], 'magnitude': 1.615526556968689, 'cosine_ionic_motion': -0.3694048821926117, 'motion_component_ionic': -0.5967833995819092, 'motion_component_percent_ionic': 36.94048821926117}, {'ion_id': 2434, 'distance': 10.152715682983398, 'force': [-1.8904106616973877, -2.4841415882110596, -0.7933556437492371], 'magnitude': 3.2208733558654785, 'cosine_ionic_motion': -0.4713403582572937, 'motion_component_ionic': -1.5181275606155396, 'motion_component_percent_ionic': 47.13403582572937}, {'ion_id': 2443, 'distance': 7.807744979858398, 'force': [-4.601739406585693, -2.897317886352539, -0.29952719807624817], 'magnitude': 5.446115493774414, 'cosine_ionic_motion': -0.0968538224697113, 'motion_component_ionic': -0.5274770855903625, 'motion_component_percent_ionic': 9.68538224697113}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.90973424911499, 'force': [-0.4573526382446289, 7.55396842956543, -4.366289138793945], 'magnitude': 8.737052917480469, 'cosine_with_motion': 0.5945570468902588, 'motion_component': 5.194676399230957, 'motion_component_percent': 59.45570468902588}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.805153846740723, 'force': [-0.3889302909374237, -3.3646371364593506, 2.369807720184326], 'magnitude': 4.133768081665039, 'cosine_with_motion': -0.4648146331310272, 'motion_component': -1.921435832977295, 'motion_component_percent': 46.48146331310272}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.974772930145264, 'force': [0.23733748495578766, -3.653355598449707, 1.35104238986969], 'magnitude': 3.902390480041504, 'cosine_with_motion': -0.7068737149238586, 'motion_component': -2.7584972381591797, 'motion_component_percent': 70.68737149238586}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.741364002227783, 'force': [6.36301326751709, 3.189417600631714, 0.9536332488059998], 'magnitude': 7.181207656860352, 'cosine_with_motion': 0.029300492256879807, 'motion_component': 0.2104129195213318, 'motion_component_percent': 2.9300492256879807}]}, 5898: {'frame': 5898, 'motion_vector': [1.28692626953125, 1.0255928039550781, -0.0074005126953125], 'ionic_force': [-8.504436016082764, 11.964142084121704, -4.874931126832962], 'ionic_force_magnitude': 15.467096729899332, 'radial_force': 14.678764517516374, 'axial_force': -4.874931126832962, 'glu_force': [-6.0847327709198, 27.38208770751953, 0.3657366633415222], 'glu_force_magnitude': 28.0523878381629, 'asn_force': [-0.9865337014198303, 1.5351793766021729, 3.704575300216675], 'asn_force_magnitude': 4.129637104801972, 'residue_force': [-7.07126647233963, 28.917267084121704, 4.070311963558197], 'residue_force_magnitude': 30.0462740554956, 'total_force': [-15.575702488422394, 40.88140916824341, -0.804619163274765], 'total_force_magnitude': 43.75545149563757, 'cosine_total_motion': 0.30399082815940304, 'cosine_glu_motion': 0.4386473239877334, 'cosine_asn_motion': 0.0408275550169387, 'cosine_residue_motion': 0.4151499057664685, 'cosine_ionic_motion': 0.053503776974203714, 'motion_component_total': 13.301255936647456, 'motion_component_glu': 12.305104856676193, 'motion_component_asn': 0.16860298609629398, 'motion_component_residue': 12.473707842772486, 'motion_component_ionic': 0.8275480938749694, 'motion_component_percent_total': 30.399082815940304, 'motion_component_percent_glu': 43.864732398773334, 'motion_component_percent_asn': 4.08275550169387, 'motion_component_percent_residue': 41.51499057664685, 'motion_component_percent_ionic': 5.350377697420371, 'ionic_contributions': [{'ion_id': 1355, 'distance': 8.775650978088379, 'force': [-2.246494770050049, 1.9543259143829346, -3.1174850463867188], 'magnitude': 4.311013698577881, 'cosine_ionic_motion': -0.12173992395401001, 'motion_component_ionic': -0.524822473526001, 'motion_component_percent_ionic': 12.173992395401001}, {'ion_id': 1380, 'distance': 6.865221977233887, 'force': [1.3024711608886719, 6.837247848510742, -1.0843136310577393], 'magnitude': 7.044155597686768, 'cosine_ionic_motion': 0.7502090334892273, 'motion_component_ionic': 5.2845892906188965, 'motion_component_percent_ionic': 75.02090334892273}, {'ion_id': 1443, 'distance': 13.32459545135498, 'force': [-0.6266984939575195, 0.5076103806495667, -1.6870962381362915], 'magnitude': 1.8699499368667603, 'cosine_ionic_motion': -0.08885513246059418, 'motion_component_ionic': -0.1661546528339386, 'motion_component_percent_ionic': 8.885513246059418}, {'ion_id': 2434, 'distance': 9.414612770080566, 'force': [-3.711239814758301, -0.4314489960670471, -0.2661377489566803], 'magnitude': 3.745701313018799, 'cosine_ionic_motion': -0.8463016748428345, 'motion_component_ionic': -3.1699934005737305, 'motion_component_percent_ionic': 84.63016748428345}, {'ion_id': 2443, 'distance': 8.450874328613281, 'force': [-3.2224740982055664, 3.096406936645508, 1.2801015377044678], 'magnitude': 4.6487345695495605, 'cosine_ionic_motion': -0.12822215259075165, 'motion_component_ionic': -0.5960707664489746, 'motion_component_percent_ionic': 12.822215259075165}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.7421162128448486, 'force': [4.402163028717041, -18.31712532043457, -3.1169562339782715], 'magnitude': 19.094804763793945, 'cosine_with_motion': -0.4168172776699066, 'motion_component': -7.959044456481934, 'motion_component_percent': 41.68172776699066}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 3.1276965141296387, 'force': [1.2825896739959717, 27.75776481628418, -0.26049691438674927], 'magnitude': 27.788602828979492, 'cosine_with_motion': 0.6586699485778809, 'motion_component': 18.303518295288086, 'motion_component_percent': 65.86699485778809}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 3.5327703952789307, 'force': [-11.769485473632812, 17.941448211669922, 3.743189811706543], 'magnitude': 21.78136444091797, 'cosine_with_motion': 0.09001407027244568, 'motion_component': 1.9606293439865112, 'motion_component_percent': 9.001407027244568}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.808056354522705, 'force': [-0.9865337014198303, 1.5351793766021729, 3.704575300216675], 'magnitude': 4.129636764526367, 'cosine_with_motion': 0.04082755744457245, 'motion_component': 0.16860298812389374, 'motion_component_percent': 4.082755744457245}]}, 5899: {'frame': 5899, 'motion_vector': [-1.2925643920898438, 0.4482421875, -0.7178955078125], 'ionic_force': [-6.799471914768219, 9.492137521505356, -5.600397616624832], 'ionic_force_magnitude': 12.949824188427762, 'radial_force': 11.676193431375298, 'axial_force': -5.600397616624832, 'glu_force': [-14.378485679626465, 17.21088981628418, -0.5976857244968414], 'glu_force_magnitude': 22.43463409402447, 'asn_force': [0.1363511085510254, 2.1622188091278076, 3.2376694679260254], 'asn_force_magnitude': 3.8956752157860337, 'residue_force': [-14.24213457107544, 19.373108625411987, 2.639983743429184], 'residue_force_magnitude': 24.18936231317818, 'total_force': [-21.04160648584366, 28.865246146917343, -2.960413873195648], 'total_force_magnitude': 35.84293080828957, 'cosine_total_motion': 0.7631567945415682, 'cosine_glu_motion': 0.7711401530138393, 'cosine_asn_motion': -0.2544279520088098, 'cosine_residue_motion': 0.6742252354600744, 'cosine_ionic_motion': 0.8528839867391913, 'motion_component_total': 27.35377618262949, 'motion_component_glu': 17.300247168075526, 'motion_component_asn': -0.9911686668439188, 'motion_component_residue': 16.309078501231607, 'motion_component_ionic': 11.044697681397881, 'motion_component_percent_total': 76.31567945415682, 'motion_component_percent_glu': 77.11401530138393, 'motion_component_percent_asn': 25.44279520088098, 'motion_component_percent_residue': 67.42252354600744, 'motion_component_percent_ionic': 85.28839867391913, 'ionic_contributions': [{'ion_id': 1355, 'distance': 8.837882995605469, 'force': [-1.5860280990600586, 2.484849214553833, -3.0621752738952637], 'magnitude': 4.250514984130859, 'cosine_ionic_motion': 0.8165296912193298, 'motion_component_ionic': 3.4706716537475586, 'motion_component_percent_ionic': 81.65296912193298}, {'ion_id': 1380, 'distance': 8.98376750946045, 'force': [1.502514123916626, 3.8119521141052246, -0.36482638120651245], 'magnitude': 4.113590717315674, 'cosine_ionic_motion': 0.004482547752559185, 'motion_component_ionic': 0.018439367413520813, 'motion_component_percent_ionic': 0.4482547752559185}, {'ion_id': 1443, 'distance': 13.691761016845703, 'force': [-0.44899803400039673, 0.7380704879760742, -1.5459970235824585], 'magnitude': 1.7710037231445312, 'cosine_ionic_motion': 0.7386375069618225, 'motion_component_ionic': 1.3081297874450684, 'motion_component_percent_ionic': 73.86375069618225}, {'ion_id': 2434, 'distance': 7.952696323394775, 'force': [-5.232437610626221, -0.4004041254520416, -0.13199836015701294], 'magnitude': 5.249395370483398, 'cosine_ionic_motion': 0.8234643340110779, 'motion_component_ionic': 4.322690010070801, 'motion_component_percent_ionic': 82.34643340110779}, {'ion_id': 2443, 'distance': 10.383524894714355, 'force': [-1.034522294998169, 2.8576698303222656, -0.4954005777835846], 'magnitude': 3.079274892807007, 'cosine_ionic_motion': 0.6250715255737305, 'motion_component_ionic': 1.9247671365737915, 'motion_component_percent_ionic': 62.50715255737305}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.9437255859375, 'force': [11.095504760742188, -12.466623306274414, -4.129337787628174], 'magnitude': 17.192392349243164, 'cosine_with_motion': -0.6387002468109131, 'motion_component': -10.980785369873047, 'motion_component_percent': 63.87002468109131}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 3.2568912506103516, 'force': [-13.083478927612305, 22.031465530395508, 0.4641817510128021], 'magnitude': 25.627687454223633, 'cosine_with_motion': 0.6681052446365356, 'motion_component': 17.121992111206055, 'motion_component_percent': 66.81052446365356}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 4.274304389953613, 'force': [-12.390511512756348, 7.646047592163086, 3.0674703121185303], 'magnitude': 14.879387855529785, 'cosine_with_motion': 0.7499664425849915, 'motion_component': 11.159041404724121, 'motion_component_percent': 74.99664425849915}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.979920387268066, 'force': [0.1363511085510254, 2.1622188091278076, 3.2376694679260254], 'magnitude': 3.8956751823425293, 'cosine_with_motion': -0.2544279396533966, 'motion_component': -0.9911686182022095, 'motion_component_percent': 25.44279396533966}]}, 5900: {'frame': 5900, 'motion_vector': [1.6382980346679688, 0.11060333251953125, 0.5860443115234375], 'ionic_force': [-6.1381120681762695, 8.840319886803627, -5.065477430820465], 'ionic_force_magnitude': 11.894819757552376, 'radial_force': 10.762326675143571, 'axial_force': -5.065477430820465, 'glu_force': [-13.204449653625488, 35.04855918884277, 7.875988960266113], 'glu_force_magnitude': 38.27257757156133, 'asn_force': [-0.1663786768913269, 1.9670840501785278, 3.335846185684204], 'asn_force_magnitude': 3.876205786479186, 'residue_force': [-13.370828330516815, 37.0156432390213, 11.211835145950317], 'residue_force_magnitude': 40.92239169431109, 'total_force': [-19.508940398693085, 45.85596312582493, 6.146357715129852], 'total_force_magnitude': 50.21101296368269, 'cosine_total_motion': -0.26601752827492875, 'cosine_glu_motion': -0.1969309319969785, 'cosine_asn_motion': 0.28113699634928935, 'cosine_residue_motion': -0.15754967518059365, 'cosine_ionic_motion': -0.580899936490451, 'motion_component_total': -13.357009560779273, 'motion_component_glu': -7.537054371094229, 'motion_component_asn': 1.089744852042493, 'motion_component_residue': -6.4473095190517355, 'motion_component_ionic': -6.909700041727537, 'motion_component_percent_total': 26.601752827492874, 'motion_component_percent_glu': 19.69309319969785, 'motion_component_percent_asn': 28.113699634928935, 'motion_component_percent_residue': 15.754967518059365, 'motion_component_percent_ionic': 58.0899936490451, 'ionic_contributions': [{'ion_id': 1355, 'distance': 9.429265022277832, 'force': [-1.8010727167129517, 2.0751216411590576, -2.528494358062744], 'magnitude': 3.734069585800171, 'cosine_ionic_motion': -0.6455951929092407, 'motion_component_ionic': -2.4106974601745605, 'motion_component_percent_ionic': 64.55951929092407}, {'ion_id': 1380, 'distance': 9.132181167602539, 'force': [0.7935147881507874, 3.8666439056396484, -0.5172351598739624], 'magnitude': 3.980971336364746, 'cosine_ionic_motion': 0.2052459418773651, 'motion_component_ionic': 0.8170782327651978, 'motion_component_percent_ionic': 20.52459418773651}, {'ion_id': 1443, 'distance': 14.607885360717773, 'force': [-0.539768397808075, 0.6087048649787903, -1.3261784315109253], 'magnitude': 1.555834412574768, 'cosine_ionic_motion': -0.5877023339271545, 'motion_component_ionic': -0.9143675565719604, 'motion_component_percent_ionic': 58.770233392715454}, {'ion_id': 2434, 'distance': 9.848250389099121, 'force': [-3.400973320007324, 0.1036798506975174, -0.37451714277267456], 'magnitude': 3.423102617263794, 'cosine_ionic_motion': -0.9684545397758484, 'motion_component_ionic': -3.3151192665100098, 'motion_component_percent_ionic': 96.84545397758484}, {'ion_id': 2443, 'distance': 11.502422332763672, 'force': [-1.189812421798706, 2.1861696243286133, -0.3190523386001587], 'magnitude': 2.5093395709991455, 'cosine_ionic_motion': -0.4330199658870697, 'motion_component_ionic': -1.0865941047668457, 'motion_component_percent_ionic': 43.30199658870697}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.0938239097595215, 'force': [9.60705280303955, -24.070093154907227, -10.427596092224121], 'magnitude': 27.935632705688477, 'cosine_with_motion': 0.14302313327789307, 'motion_component': 3.9954419136047363, 'motion_component_percent': 14.302313327789307}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 2.6615397930145264, 'force': [-0.44991493225097656, 37.92254638671875, 5.859124183654785], 'magnitude': 38.37513732910156, 'cosine_with_motion': 0.10299474000930786, 'motion_component': 3.952437400817871, 'motion_component_percent': 10.299474000930786}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 2.860210418701172, 'force': [-22.361587524414062, 21.19610595703125, 12.44446086883545], 'magnitude': 33.22920608520508, 'cosine_with_motion': -0.4660037159919739, 'motion_component': -15.484933853149414, 'motion_component_percent': 46.60037159919739}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.994919776916504, 'force': [-0.1663786768913269, 1.9670840501785278, 3.335846185684204], 'magnitude': 3.8762056827545166, 'cosine_with_motion': 0.28113698959350586, 'motion_component': 1.0897448062896729, 'motion_component_percent': 28.113698959350586}]}, 5901: {'frame': 5901, 'motion_vector': [-0.2744865417480469, -0.7472152709960938, 0.6619415283203125], 'ionic_force': [-7.439622104167938, 9.131087750196457, -4.992527484893799], 'ionic_force_magnitude': 12.792578756530364, 'radial_force': 11.77814673684328, 'axial_force': -4.992527484893799, 'glu_force': [-17.11140537261963, 17.92721128463745, 0.5718311071395874], 'glu_force_magnitude': 24.789354349906752, 'asn_force': [1.2753161489963531, 0.5340880155563354, 0.8194022178649902], 'asn_force_magnitude': 1.6072029376820645, 'residue_force': [-15.836089223623276, 18.461299300193787, 1.3912333250045776], 'residue_force_magnitude': 24.362611188345475, 'total_force': [-23.275711327791214, 27.592387050390244, -3.601294159889221], 'total_force_magnitude': 36.277649876739034, 'cosine_total_motion': -0.44231234569708305, 'cosine_glu_motion': -0.32418974116579324, 'cosine_asn_motion': -0.12424751672783133, 'cosine_residue_motion': -0.33806496686972776, 'cosine_ionic_motion': -0.6105029500110021, 'motion_component_total': -16.046052413357938, 'motion_component_glu': -8.036454370363401, 'motion_component_asn': -0.19969097388467194, 'motion_component_residue': -8.236145344248072, 'motion_component_ionic': -7.8099070691098635, 'motion_component_percent_total': 44.231234569708306, 'motion_component_percent_glu': 32.41897411657932, 'motion_component_percent_asn': 12.424751672783133, 'motion_component_percent_residue': 33.80649668697278, 'motion_component_percent_ionic': 61.05029500110021, 'ionic_contributions': [{'ion_id': 1355, 'distance': 8.822335243225098, 'force': [-1.4037278890609741, 2.735112428665161, -2.956904888153076], 'magnitude': 4.265510082244873, 'cosine_ionic_motion': -0.8187623023986816, 'motion_component_ionic': -3.492438793182373, 'motion_component_percent_ionic': 81.87623023986816}, {'ion_id': 1380, 'distance': 9.430712699890137, 'force': [1.2992652654647827, 3.4894778728485107, -0.26489782333374023], 'magnitude': 3.7329232692718506, 'cosine_ionic_motion': -0.812322199344635, 'motion_component_ionic': -3.032336473464966, 'motion_component_percent_ionic': 81.2322199344635}, {'ion_id': 1443, 'distance': 14.058492660522461, 'force': [-0.41779905557632446, 0.741924524307251, -1.4480189085006714], 'magnitude': 1.6798115968704224, 'cosine_ionic_motion': -0.8039778470993042, 'motion_component_ionic': -1.3505313396453857, 'motion_component_percent_ionic': 80.39778470993042}, {'ion_id': 2434, 'distance': 8.001550674438477, 'force': [-5.164675235748291, 0.30420610308647156, -0.35055652260780334], 'magnitude': 5.185489654541016, 'cosine_ionic_motion': 0.1784994751214981, 'motion_component_ionic': 0.9256071448326111, 'motion_component_percent_ionic': 17.84994751214981}, {'ion_id': 2443, 'distance': 11.396726608276367, 'force': [-1.7526851892471313, 1.8603668212890625, 0.02785065770149231], 'magnitude': 2.5560996532440186, 'cosine_ionic_motion': -0.336531400680542, 'motion_component_ionic': -0.8602077960968018, 'motion_component_percent_ionic': 33.6531400680542}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 3.7720160484313965, 'force': [13.748322486877441, -11</t>
         </is>
       </c>
     </row>
@@ -771,7 +771,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>{5997: {'frame': 5997, 'ionic_force': [9.381639122962952, 3.428868383169174, -11.025252528488636], 'ionic_force_magnitude': 14.877112768933067, 'motion_vector': [0.7771873474121094, 0.3831329345703125, 0.82928466796875], 'ionic_force_x': 9.381639122962952, 'ionic_force_y': 3.428868383169174, 'ionic_force_z': -11.025252528488636, 'radial_force': 9.988608062318105, 'axial_force': -11.025252528488636, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-0.08171731978654861, -3.155369997024536, 3.1179258823394775], 'asn_force_magnitude': 4.436721689067067, 'residue_force': [-0.08171731978654861, -3.155369997024536, 3.1179258823394775], 'residue_force_magnitude': 4.436721689067067, 'total_force': [9.299921803176403, 0.27349838614463806, -7.9073266461491585], 'total_force_magnitude': 12.210207271022064, 'motion_component_total': 0.646283733426138, 'cosine_total_motion': 0.0529297921878799, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.24678240547398328, 'cosine_residue_motion': 0.24678240547398328, 'cosine_ionic_motion': -0.03015511977278639, 'motion_component_glu': None, 'motion_component_asn': 1.0949048508465649, 'motion_component_residue': 1.0949048508465649, 'motion_component_ionic': -0.44862111742042643, 'ionic_contributions': [{'ion_id': 1327, 'distance': 13.469212532043457, 'force': [0.5210571885108948, -0.15596595406532288, -1.7473162412643433], 'magnitude': 1.8300108909606934}, {'ion_id': 1380, 'distance': 10.161314010620117, 'force': [3.0363898277282715, 0.8332290053367615, -0.6519385576248169], 'magnitude': 3.2154250144958496}, {'ion_id': 1443, 'distance': 8.256528854370117, 'force': [2.586791753768921, -0.8877150416374207, -4.0297532081604], 'magnitude': 4.8701581954956055}, {'ion_id': 1476, 'distance': 12.340150833129883, 'force': [1.3487483263015747, -1.712496280670166, -0.039044089615345], 'magnitude': 2.180204153060913}, {'ion_id': 2434, 'distance': 6.7822136878967285, 'force': [-0.48151785135269165, -7.0847249031066895, -1.291944980621338], 'magnitude': 7.217638969421387}, {'ion_id': 2443, 'distance': 5.039106845855713, 'force': [2.3701698780059814, 12.436541557312012, -3.2652554512023926], 'magnitude': 13.074676513671875}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.603452205657959, 'force': [-0.08171731978654861, -3.155369997024536, 3.1179258823394775], 'magnitude': 4.4367218017578125}]}, 5998: {'frame': 5998, 'ionic_force': [10.780787527561188, 0.28440017998218536, -7.232492357492447], 'ionic_force_magnitude': 12.985191907629991, 'motion_vector': [-0.7672195434570312, 2.2775001525878906, -1.0481185913085938], 'ionic_force_x': 10.780787527561188, 'ionic_force_y': 0.28440017998218536, 'ionic_force_z': -7.232492357492447, 'radial_force': 10.784538153152075, 'axial_force': -7.232492357492447, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.5282077789306641, 5.127721786499023, -4.209736347198486], 'asn_force_magnitude': 6.655404893046227, 'residue_force': [0.5282077789306641, 5.127721786499023, -4.209736347198486], 'residue_force_magnitude': 6.655404893046227, 'total_force': [11.308995306491852, 5.412121966481209, -11.442228704690933], 'total_force_magnitude': 16.973774970606165, 'motion_component_total': 5.966145995714864, 'cosine_total_motion': 0.3514919931509969, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.8989004348307543, 'cosine_residue_motion': 0.8989004348307543, 'cosine_ionic_motion': -0.0012630045621029582, 'motion_component_glu': None, 'motion_component_asn': 5.9825463523339835, 'motion_component_residue': 5.9825463523339835, 'motion_component_ionic': -0.016400356619119094, 'ionic_contributions': [{'ion_id': 1327, 'distance': 13.114724159240723, 'force': [0.6711025238037109, -0.13265840709209442, -1.804991602897644], 'magnitude': 1.9302775859832764}, {'ion_id': 1380, 'distance': 10.606010437011719, 'force': [2.8374791145324707, 0.6517823338508606, -0.4846545159816742], 'magnitude': 2.95143985748291}, {'ion_id': 1443, 'distance': 8.347920417785645, 'force': [3.076692581176758, -0.8291545510292053, -3.541635036468506], 'magnitude': 4.764106750488281}, {'ion_id': 1476, 'distance': 12.868345260620117, 'force': [1.263065218925476, -1.5566960573196411, 0.03140932321548462], 'magnitude': 2.004899740219116}, {'ion_id': 2434, 'distance': 6.327516555786133, 'force': [-0.50923091173172, -8.268269538879395, -0.3708587884902954], 'magnitude': 8.29223346710205}, {'ion_id': 2443, 'distance': 5.487727642059326, 'force': [3.441679000854492, 10.41939640045166, -1.061761736869812], 'magnitude': 11.024351119995117}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.439334392547607, 'force': [0.5282077789306641, 5.127721786499023, -4.209736347198486], 'magnitude': 6.655405044555664}]}, 5999: {'frame': 5999, 'ionic_force': [6.903971970081329, -9.943094223737717, -11.683605313301086], 'ionic_force_magnitude': 16.8236911771107, 'motion_vector': [-1.3753700256347656, -4.601753234863281, -0.27584075927734375], 'ionic_force_x': 6.903971970081329, 'ionic_force_y': -9.943094223737717, 'ionic_force_z': -11.683605313301086, 'radial_force': 12.104955667237903, 'axial_force': -11.683605313301086, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.3626566529273987, 14.090182542800903, -4.2385945320129395], 'asn_force_magnitude': 14.71837109004165, 'residue_force': [0.3626566529273987, 14.090182542800903, -4.2385945320129395], 'residue_force_magnitude': 14.71837109004165, 'total_force': [7.266628623008728, 4.147088319063187, -15.922199845314026], 'total_force_magnitude': 17.986625058219175, 'motion_component_total': -5.13140303229955, 'cosine_total_motion': -0.28528993158473065, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.906251286651912, 'cosine_residue_motion': -0.906251286651912, 'cosine_ionic_motion': 0.48783228478641716, 'motion_component_glu': None, 'motion_component_asn': -13.33854273777055, 'motion_component_residue': -13.33854273777055, 'motion_component_ionic': 8.207139705471, 'ionic_contributions': [{'ion_id': 1327, 'distance': 13.49657154083252, 'force': [0.45604217052459717, 0.1768944263458252, -1.7557339668273926], 'magnitude': 1.822599172592163}, {'ion_id': 1380, 'distance': 11.447005271911621, 'force': [2.0143558979034424, 1.382273554801941, -0.6717885732650757], 'magnitude': 2.5336947441101074}, {'ion_id': 1443, 'distance': 8.888298988342285, 'force': [2.022075653076172, 0.4375012218952179, -3.6579012870788574], 'magnitude': 4.202432632446289}, {'ion_id': 1476, 'distance': 10.855681419372559, 'force': [2.0586459636688232, -1.9142779111862183, -0.18536603450775146], 'magnitude': 2.8172404766082764}, {'ion_id': 2434, 'distance': 4.453519821166992, 'force': [0.3335014283657074, -16.288362503051758, -3.843754291534424], 'magnitude': 16.73906898498535}, {'ion_id': 2443, 'distance': 7.170866012573242, 'force': [0.01935085654258728, 6.262876987457275, -1.5690611600875854], 'magnitude': 6.456466197967529}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.693239450454712, 'force': [-2.7312347888946533, -12.222817420959473, 12.013432502746582], 'magnitude': 17.354522705078125}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.659578561782837, 'force': [2.1643474102020264, 23.001497268676758, -15.530914306640625], 'magnitude': 27.83814811706543}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.045992851257324, 'force': [2.8511462211608887, 8.098589897155762, -16.545122146606445], 'magnitude': 18.64020538330078}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.5204715728759766, 'force': [-1.0469173192977905, -2.5786657333374023, 10.890146255493164], 'magnitude': 11.240143775939941}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.043825149536133, 'force': [-0.8746848702430725, -2.208421468734741, 4.933863162994385], 'magnitude': 5.475874900817871}]}, 6000: {'frame': 6000, 'ionic_force': [5.517950534820557, 7.6139421463012695, -19.801055759191513], 'ionic_force_magnitude': 21.920349045819517, 'motion_vector': [-4.781524658203125, 2.4392776489257812, 0.5065383911132812], 'ionic_force_x': 5.517950534820557, 'ionic_force_y': 7.6139421463012695, 'ionic_force_z': -19.801055759191513, 'radial_force': 9.403185264151146, 'axial_force': -19.801055759191513, 'glu_force': [5.4703192710876465, -5.7910475730896, 4.048490047454834], 'glu_force_magnitude': 8.935932888387237, 'asn_force': [-3.052062064409256, -1.6076116561889648, 2.321760445833206], 'asn_force_magnitude': 4.158132952414619, 'residue_force': [2.4182572066783905, -7.3986592292785645, 6.37025049328804], 'residue_force_magnitude': 10.058241280456409, 'total_force': [7.936207741498947, 0.21528291702270508, -13.430805265903473], 'total_force_magnitude': 15.60180342592516, 'motion_component_total': -8.202581793157563, 'cosine_total_motion': -0.5257457467722944, 'cosine_glu_motion': -0.7935315382180069, 'cosine_asn_motion': 0.5284850823239703, 'cosine_residue_motion': -0.48650983787514596, 'cosine_ionic_motion': -0.1509623980702402, 'motion_component_glu': -7.090944570334802, 'motion_component_asn': 2.197511235670854, 'motion_component_residue': -4.893433334663948, 'motion_component_ionic': -3.309148458493616, 'ionic_contributions': [{'ion_id': 1327, 'distance': 14.055419921875, 'force': [0.27228718996047974, -0.34001588821411133, -1.6231095790863037], 'magnitude': 1.6805462837219238}, {'ion_id': 1380, 'distance': 8.973416328430176, 'force': [3.8357651233673096, 0.6248253583908081, -1.3770771026611328], 'magnitude': 4.123086452484131}, {'ion_id': 1443, 'distance': 8.977163314819336, 'force': [1.5023193359375, -1.549290657043457, -3.5091614723205566], 'magnitude': 4.119645595550537}, {'ion_id': 1476, 'distance': 12.293431282043457, 'force': [1.1409306526184082, -1.8393505811691284, -0.37553462386131287], 'magnitude': 2.1968066692352295}, {'ion_id': 2434, 'distance': 8.713654518127441, 'force': [-0.8899776935577393, -4.16619348526001, -0.9849853515625], 'magnitude': 4.3725762367248535}, {'ion_id': 2443, 'distance': 4.17150354385376, 'force': [-0.3433740735054016, 14.883967399597168, -11.931187629699707], 'magnitude': 19.07887840270996}], 'glu_contributions': [{'resid': 748, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 5.515539646148682, 'force': [5.4703192710876465, -5.7910475730896, 4.048490047454834], 'magnitude': 8.935933113098145}], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.959725856781006, 'force': [-1.3925870656967163, -3.071686267852783, 2.0021188259124756], 'magnitude': 3.922121286392212}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.887828350067139, 'force': [-1.1611191034317017, 9.759984016418457, 1.2519491910934448], 'magnitude': 9.908222198486328}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.66547966003418, 'force': [-0.33897170424461365, -6.09545373916626, -0.6041290163993835], 'magnitude': 6.134690761566162}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.179264545440674, 'force': [3.3775413036346436, -10.843356132507324, 0.6421475410461426], 'magnitude': 11.375347137451172}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.829558849334717, 'force': [-0.9659819006919861, 3.9124884605407715, -0.7503260970115662], 'magnitude': 4.099228858947754}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.084596633911133, 'force': [-2.570943593978882, 4.730412006378174, -0.2199999988079071], 'magnitude': 5.388408660888672}]}, 6004: {'frame': 6004, 'ionic_force': [-13.262407958507538, 11.088155046105385, -8.382136479020119], 'ionic_force_magnitude': 19.2119457405354, 'motion_vector': [-0.223419189453125, 2.570514678955078, -0.7060775756835938], 'ionic_force_x': -13.262407958507538, 'ionic_force_y': 11.088155046105385, 'ionic_force_z': -8.382136479020119, 'radial_force': 17.28695019904773, 'axial_force': -8.382136479020119, 'glu_force': [-1.8934214115142822, -5.6408562660217285, 2.6732892990112305], 'glu_force_magnitude': 6.5230958701911845, 'asn_force': [7.777035713195801, -11.803484916687012, -4.9318801164627075], 'asn_force_magnitude': 14.970904519966084, 'residue_force': [5.8836143016815186, -17.44434118270874, -2.258590817451477], 'residue_force_magnitude': 18.547862114820013, 'total_force': [-7.378793656826019, -6.356186136603355, -10.640727296471596], 'total_force_magnitude': 14.424727915320979, 'motion_component_total': -2.682891392198875, 'cosine_total_motion': -0.18599251285352061, 'cosine_glu_motion': -0.9148800802838679, 'cosine_asn_motion': -0.7140458572334746, 'cosine_residue_motion': -0.8980961105824571, 'cosine_ionic_motion': 0.7274053144578178, 'motion_component_glu': -5.967850473419878, 'motion_component_asn': -10.68991235151968, 'motion_component_residue': -16.65776282493956, 'motion_component_ionic': 13.974871432740684, 'ionic_contributions': [{'ion_id': 1327, 'distance': 14.805962562561035, 'force': [-0.7501986622810364, -0.13029859960079193, -1.3091551065444946], 'magnitude': 1.5144842863082886}, {'ion_id': 1380, 'distance': 4.653715133666992, 'force': [-4.599451065063477, 13.990073204040527, -4.257678985595703], 'magnitude': 15.329870223999023}, {'ion_id': 1443, 'distance': 9.613933563232422, 'force': [-2.4518744945526123, -0.6125720739364624, -2.5525479316711426], 'magnitude': 3.59199595451355}, {'ion_id': 1476, 'distance': 11.188375473022461, 'force': [-1.4830362796783447, -2.197493553161621, 0.07560582458972931], 'magnitude': 2.652186155319214}, {'ion_id': 2434, 'distance': 13.317967414855957, 'force': [-1.6397267580032349, -0.897940993309021, -0.09315349161624908], 'magnitude': 1.8718117475509644}, {'ion_id': 2443, 'distance': 11.454083442687988, 'force': [-2.338120698928833, 0.9363870620727539, -0.2452067881822586], 'magnitude': 2.530564308166504}], 'glu_contributions': [{'resid': 1073, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 5.350562572479248, 'force': [1.9671130180358887, 7.572391033172607, -5.101621627807617], 'magnitude': 9.34008502960205}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 4.146653652191162, 'force': [-3.860534429550171, -13.213247299194336, 7.774910926818848], 'magnitude': 15.809581756591797}], 'asn_contributions': [{'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.5101473331451416, 'force': [-0.8161220550537109, 17.44001579284668, 8.017990112304688], 'magnitude': 19.21219253540039}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.610398530960083, 'force': [8.503637313842773, -25.7799072265625, -9.905538558959961], 'magnitude': 28.896974563598633}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.922837495803833, 'force': [-4.029259204864502, -19.039121627807617, -3.8032891750335693], 'magnitude': 19.82897186279297}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.649535655975342, 'force': [2.6498820781707764, 10.098359107971191, -0.6293421983718872], 'magnitude': 10.459197044372559}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.8848114013671875, 'force': [1.4688975811004639, 5.477169036865234, 1.3882997035980225], 'magnitude': 5.838185787200928}]}, 6005: {'frame': 6005, 'ionic_force': [-11.751091122627258, 3.513936460018158, -5.2574396431446075], 'ionic_force_magnitude': 13.344533098562968, 'motion_vector': [-0.2879486083984375, 0.21361923217773438, 0.6275177001953125], 'ionic_force_x': -11.751091122627258, 'ionic_force_y': 3.513936460018158, 'ionic_force_z': -5.2574396431446075, 'radial_force': 12.265231021767756, 'axial_force': -5.2574396431446075, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-2.13910374045372, -4.090269088745117, 1.7995737791061401], 'asn_force_magnitude': 4.954243818910537, 'residue_force': [-2.13910374045372, -4.090269088745117, 1.7995737791061401], 'residue_force_magnitude': 4.954243818910537, 'total_force': [-13.890194863080978, -0.5763326287269592, -3.4578658640384674], 'total_force_magnitude': 14.325728915729874, 'motion_component_total': 2.3614557737812616, 'cosine_total_motion': 0.16484018283972596, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.2433869696212026, 'cosine_residue_motion': 0.2433869696212026, 'cosine_ionic_motion': 0.08660156000935704, 'motion_component_glu': None, 'motion_component_asn': 1.2057983898492095, 'motion_component_residue': 1.2057983898492095, 'motion_component_ionic': 1.155657383932052, 'ionic_contributions': [{'ion_id': 1380, 'distance': 7.387109279632568, 'force': [-1.5290939807891846, 5.18525505065918, -2.7910616397857666], 'magnitude': 6.0839972496032715}, {'ion_id': 1443, 'distance': 10.215596199035645, 'force': [-2.1018567085266113, 0.29880401492118835, -2.3693599700927734], 'magnitude': 3.181344509124756}, {'ion_id': 1476, 'distance': 10.20903491973877, 'force': [-1.9276835918426514, -2.4968819618225098, -0.44340747594833374], 'magnitude': 3.185434579849243}, {'ion_id': 2434, 'distance': 8.538402557373047, 'force': [-4.488006591796875, -0.4852888882160187, 0.6003507971763611], 'magnitude': 4.553913593292236}, {'ion_id': 2443, 'distance': 12.88902473449707, 'force': [-1.704450249671936, 1.0120482444763184, -0.25396135449409485], 'magnitude': 1.9984716176986694}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.525741100311279, 'force': [-4.685890197753906, -4.98834228515625, 3.641629219055176], 'magnitude': 7.7525858879089355}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.655789375305176, 'force': [5.722832679748535, 7.2156758308410645, -2.4860730171203613], 'magnitude': 9.539253234863281}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.459854602813721, 'force': [-2.216416835784912, -4.019174098968506, 0.8787698149681091], 'magnitude': 4.673168182373047}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.66311502456665, 'force': [0.4617593586444855, 7.302806854248047, 0.9671420454978943], 'magnitude': 7.381028175354004}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.487074851989746, 'force': [-1.4213887453079224, -9.601235389709473, -1.2018942832946777], 'magnitude': 9.780011177062988}]}, 6006: {'frame': 6006, 'ionic_force': [-11.669181168079376, 5.09692008793354, -6.636843234300613], 'ionic_force_magnitude': 14.35952894885207, 'motion_vector': [3.3086013793945312, -2.3047142028808594, -0.0504608154296875], 'ionic_force_x': -11.669181168079376, 'ionic_force_y': 5.09692008793354, 'ionic_force_z': -6.636843234300613, 'radial_force': 12.733749782221999, 'axial_force': -6.636843234300613, 'glu_force': [1.9968379735946655, 7.997310161590576, 2.0858542919158936], 'glu_force_magnitude': 8.502653694028323, 'asn_force': [-1.1865164488554, -2.8178770542144775, -0.6750527620315552], 'asn_force_magnitude': 3.1311257732003233, 'residue_force': [0.8103215247392654, 5.179433107376099, 1.4108015298843384], 'residue_force_magnitude': 5.4289510261157625, 'total_force': [-10.85885964334011, 10.276353195309639, -5.226041704416275], 'total_force_magnitude': 15.83760649987268, 'motion_component_total': -14.717398847824802, 'cosine_total_motion': -0.9292691321724098, 'cosine_glu_motion': -0.34794612235353367, 'cosine_asn_motion': 0.20613788133289312, 'cosine_residue_motion': -0.4260531617159685, 'cosine_ionic_motion': -0.863842897808891, 'motion_component_glu': -2.958465382552104, 'motion_component_asn': 0.6454436330743315, 'motion_component_residue': -2.3130217494777723, 'motion_component_ionic': -12.40437709834703, 'ionic_contributions': [{'ion_id': 1327, 'distance': 14.995388984680176, 'force': [-0.7694267630577087, 0.20096524059772491, -1.2440012693405151], 'magnitude': 1.4764631986618042}, {'ion_id': 1380, 'distance': 7.06876802444458, 'force': [-1.6209291219711304, 5.998019695281982, -2.354433298110962], 'magnitude': 6.644321918487549}, {'ion_id': 1443, 'distance': 10.300626754760742, 'force': [-2.171865224838257, 0.4668664336204529, -2.2036139965057373], 'magnitude': 3.129037857055664}, {'ion_id': 1476, 'distance': 8.93224811553955, 'force': [-3.098361015319824, -2.754167318344116, -0.36075103282928467], 'magnitude': 4.161180019378662}, {'ion_id': 2434, 'distance': 11.276430130004883, 'force': [-2.578646183013916, 0.22548645734786987, -0.3415878117084503], 'magnitude': 2.6109275817871094}, {'ion_id': 2443, 'distance': 13.864049911499023, 'force': [-1.42995285987854, 0.9597495794296265, -0.13245582580566406], 'magnitude': 1.7272605895996094}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 5.654324531555176, 'force': [1.9968379735946655, 7.997310161590576, 2.0858542919158936], 'magnitude': 8.502654075622559}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.498685359954834, 'force': [5.774613857269287, 7.766817569732666, -2.8603482246398926], 'magnitude': 10.09213638305664}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.6935200691223145, 'force': [-2.679769992828369, -3.323723077774048, 0.48975634574890137], 'magnitude': 4.297460079193115}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.597736835479736, 'force': [-3.3127877712249756, -5.251379013061523, 2.2082884311676025], 'magnitude': 6.589998722076416}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.6094465255737305, 'force': [-0.1876792162656784, 7.33982515335083, 1.6390122175216675], 'magnitude': 7.522939205169678}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.52293062210083, 'force': [-0.7808933258056641, -9.349417686462402, -2.151761531829834], 'magnitude': 9.625564575195312}]}, 6007: {'frame': 6007, 'ionic_force': [-8.5225989818573, 11.005497053265572, -12.623888924717903], 'ionic_force_magnitude': 18.7914403486962, 'motion_vector': [2.3887977600097656, 0.3354644775390625, 2.6361465454101562], 'ionic_force_x': -8.5225989818573, 'ionic_force_y': 11.005497053265572, 'ionic_force_z': -12.623888924717903, 'radial_force': 13.919614175507604, 'axial_force': -12.623888924717903, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-6.5108597001526505, -8.863329410552979, 0.8051426857709885], 'asn_force_magnitude': 11.02715543644397, 'residue_force': [-6.5108597001526505, -8.863329410552979, 0.8051426857709885], 'residue_force_magnitude': 11.02715543644397, 'total_force': [-15.03345868200995, 2.142167642712593, -11.818746238946915], 'total_force_magnitude': 19.242570639439187, 'motion_component_total': -18.568279293441314, 'cosine_total_motion': -0.9649583541288471, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.41631468010525446, 'cosine_residue_motion': -0.41631468010525446, 'cosine_ionic_motion': -0.7438233762861622, 'motion_component_glu': None, 'motion_component_asn': -4.590766687994089, 'motion_component_residue': -4.590766687994089, 'motion_component_ionic': -13.977512605447224, 'ionic_contributions': [{'ion_id': 1327, 'distance': 13.203627586364746, 'force': [-0.6066397428512573, -0.07653407752513885, -1.803540825843811], 'magnitude': 1.904370903968811}, {'ion_id': 1380, 'distance': 4.676848411560059, 'force': [3.8302056789398193, 13.930157661437988, -4.655093669891357], 'magnitude': 15.178592681884766}, {'ion_id': 1443, 'distance': 8.234951972961426, 'force': [-2.181785821914673, -0.8094444274902344, -4.307274341583252], 'magnitude': 4.895712852478027}, {'ion_id': 1476, 'distance': 9.530322074890137, 'force': [-1.5309606790542603, -3.3161826133728027, -0.14249469339847565], 'magnitude': 3.655299186706543}, {'ion_id': 2434, 'distance': 8.400443077087402, 'force': [-4.577861785888672, -0.5349699258804321, -0.9441246390342712], 'magnitude': 4.704719066619873}, {'ion_id': 2443, 'distance': 9.13610553741455, 'force': [-3.455556631088257, 1.8124704360961914, -0.7713607549667358], 'magnitude': 3.9775516986846924}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.860510349273682, 'force': [-0.6983756422996521, -5.7327985763549805, 3.7615768909454346], 'magnitude': 6.892181396484375}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.1887969970703125, 'force': [-0.4211355745792389, 10.303326606750488, -4.702589988708496], 'magnitude': 11.333588600158691}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.051659107208252, 'force': [-0.003207089612260461, -5.307527542114258, 1.276627779006958], 'magnitude': 5.45890474319458}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.457014083862305, 'force': [1.002776861190796, -4.077197074890137, 2.062742233276367], 'magnitude': 4.678033828735352}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.595729351043701, 'force': [7.024986743927002, 7.913211822509766, 3.6938416957855225], 'magnitude': 11.207757949829102}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.911944627761841, 'force': [-10.114625930786133, -7.043038368225098, -3.6948840618133545], 'magnitude': 12.867097854614258}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.37458610534668, 'force': [-6.267003059387207, -8.382468223571777, -1.4310636520385742], 'magnitude': 10.563570976257324}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.525770664215088, 'force': [2.965723991394043, 3.4631619453430176, -0.16110821068286896], 'magnitude': 4.562342166900635}]}, 6009: {'frame': 6009, 'ionic_force': [-7.961302757263184, 8.177349001169205, -15.085426807403564], 'ionic_force_magnitude': 18.916169808956028, 'motion_vector': [3.8805274963378906, 4.743255615234375, -1.0284576416015625], 'ionic_force_x': -7.961302757263184, 'ionic_force_y': 8.177349001169205, 'ionic_force_z': -15.085426807403564, 'radial_force': 11.41277259388486, 'axial_force': -15.085426807403564, 'glu_force': [-5.527263164520264, -6.202527046203613, 5.248671531677246], 'glu_force_magnitude': 9.827030716151702, 'asn_force': [-13.272437572479248, -4.027345180511475, -2.84513857960701], 'asn_force_magnitude': 14.158810750042393, 'residue_force': [-18.79970073699951, -10.229872226715088, 2.403532952070236], 'residue_force_magnitude': 21.537316551217426, 'total_force': [-26.761003494262695, -2.052523225545883, -12.681893855333328], 'total_force_magnitude': 29.684921953228827, 'motion_component_total': -16.179352335761717, 'cosine_total_motion': -0.5450360408982612, 'cosine_glu_motion': -0.9214131879107607, 'cosine_asn_motion': -0.7692396552437373, 'cosine_residue_motion': -0.9261262586941338, 'cosine_ionic_motion': 0.19913767439035357, 'motion_component_glu': -9.054755699866305, 'motion_component_asn': -10.891518700023932, 'motion_component_residue': -19.94627439989024, 'motion_component_ionic': 3.766922064128522, 'ionic_contributions': [{'ion_id': 1327, 'distance': 14.167987823486328, 'force': [-0.591535210609436, -0.1539454162120819, -1.536857008934021], 'magnitude': 1.6539475917816162}, {'ion_id': 1380, 'distance': 4.695187568664551, 'force': [0.541907787322998, 12.025218963623047, -9.050501823425293], 'magnitude': 15.060250282287598}, {'ion_id': 1443, 'distance': 8.826412200927734, 'force': [-2.206110715866089, -0.993217945098877, -3.5082154273986816], 'magnitude': 4.261570453643799}, {'ion_id': 1476, 'distance': 10.639166831970215, 'force': [-0.4248296022415161, -2.8931193351745605, -0.22868134081363678], 'magnitude': 2.933072566986084}, {'ion_id': 2434, 'distance': 11.543355941772461, 'force': [-2.3827462196350098, -0.7271773219108582, -0.04096989333629608], 'magnitude': 2.491574764251709}, {'ion_id': 2443, 'distance': 10.30805778503418, 'force': [-2.897988796234131, 0.9195900559425354, -0.720201313495636], 'magnitude': 3.124527931213379}], 'glu_contributions': [{'resid': 1073, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 5.259528160095215, 'force': [-5.527263164520264, -6.202527046203613, 5.248671531677246], 'magnitude': 9.827031135559082}], 'asn_contributions': [{'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.4478089809417725, 'force': [11.730192184448242, 15.527929306030273, 4.221592426300049], 'magnitude': 19.9132080078125}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.6283836364746094, 'force': [-22.68062973022461, -16.212852478027344, -5.928383827209473], 'magnitude': 28.502864837646484}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.3446478843688965, 'force': [-9.240912437438965, -13.260483741760254, 0.3025539815425873], 'magnitude': 16.16559410095215}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.408743858337402, 'force': [4.383737564086914, 5.412045955657959, -1.691156268119812], 'magnitude': 7.167105674743652}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.187734603881836, 'force': [2.53517484664917, 4.506015777587891, 0.25025510787963867], 'magnitude': 5.176283836364746}]}, 6010: {'frame': 6010, 'ionic_force': [-3.6213796138763428, 1.774631679058075, -10.690930426120758], 'ionic_force_magnitude': 11.426272414058323, 'motion_vector': [1.1203804016113281, -1.3056755065917969, -0.7982025146484375], 'ionic_force_x': -3.6213796138763428, 'ionic_force_y': 1.774631679058075, 'ionic_force_z': -10.690930426120758, 'radial_force': 4.032828771980736, 'axial_force': -10.690930426120758, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-2.0518531799316406, 8.38363516330719, 0.9321974515914917], 'asn_force_magnitude': 8.68126903811822, 'residue_force': [-2.0518531799316406, 8.38363516330719, 0.9321974515914917], 'residue_force_magnitude': 8.68126903811822, 'total_force': [-5.673232793807983, 10.158266842365265, -9.758732974529266], 'total_force_magnitude': 15.185809983059867, 'motion_component_total': -6.23748206904564, 'cosine_total_motion': -0.41074411414364465, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.8496317291117762, 'cosine_residue_motion': -0.8496317291117762, 'cosine_ionic_motion': 0.0996300029828309, 'motion_component_glu': None, 'motion_component_asn': -7.375881623740909, 'motion_component_residue': -7.375881623740909, 'motion_component_ionic': 1.138399554695269, 'ionic_contributions': [{'ion_id': 1327, 'distance': 14.576889038085938, 'force': [-0.1575925350189209, 0.3570076823234558, -1.512939453125], 'magnitude': 1.5624581575393677}, {'ion_id': 1380, 'distance': 9.456782341003418, 'force': [1.4782865047454834, 3.0387051105499268, -1.537086009979248], 'magnitude': 3.7123701572418213}, {'ion_id': 1443, 'distance': 9.319299697875977, 'force': [-0.25140249729156494, 0.9879297614097595, -3.684279203414917], 'magnitude': 3.822711229324341}, {'ion_id': 1476, 'distance': 6.902045249938965, 'force': [2.1201860904693604, -6.282724380493164, -2.145188093185425], 'magnitude': 6.969192981719971}, {'ion_id': 2434, 'distance': 7.881553649902344, 'force': [-5.255415439605713, 0.688380777835846, -0.6865726113319397], 'magnitude': 5.344590187072754}, {'ion_id': 2443, 'distance': 9.671700477600098, 'force': [-1.5554417371749878, 2.985332727432251, -1.1248650550842285], 'magnitude': 3.54921555519104}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.6212244033813477, 'force': [10.093687057495117, -9.033501625061035, 11.932106018066406], 'magnitude': 18.05164337158203}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.126033067703247, 'force': [-7.931264400482178, 15.314237594604492, -10.421074867248535], 'magnitude': 20.150177001953125}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.5542259216308594, 'force': [-11.255677223205566, 5.027613162994385, -20.772743225097656], 'magnitude': 24.15520668029785}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.0041399002075195, 'force': [3.62773060798645, -2.2740817070007324, 14.8302583694458], 'magnitude': 15.435946464538574}, {'resid': 130, 'resname': 'ASN', 'at</t>
+          <t>{5997: {'frame': 5997, 'motion_vector': [0.7771873474121094, 0.3831329345703125, 0.82928466796875], 'ionic_force': [9.381639122962952, 3.428868383169174, -11.025252528488636], 'ionic_force_magnitude': 14.877112768933067, 'radial_force': 9.988608062318105, 'axial_force': -11.025252528488636, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-0.08171731978654861, -3.155369997024536, 3.1179258823394775], 'asn_force_magnitude': 4.436721689067067, 'residue_force': [-0.08171731978654861, -3.155369997024536, 3.1179258823394775], 'residue_force_magnitude': 4.436721689067067, 'total_force': [9.299921803176403, 0.27349838614463806, -7.9073266461491585], 'total_force_magnitude': 12.210207271022064, 'cosine_total_motion': 0.0529297921878799, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.24678240547398328, 'cosine_residue_motion': 0.24678240547398328, 'cosine_ionic_motion': -0.03015511977278639, 'motion_component_total': 0.646283733426138, 'motion_component_glu': None, 'motion_component_asn': 1.0949048508465649, 'motion_component_residue': 1.0949048508465649, 'motion_component_ionic': -0.44862111742042643, 'motion_component_percent_total': 5.29297921878799, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 24.678240547398328, 'motion_component_percent_residue': 24.678240547398328, 'motion_component_percent_ionic': 3.015511977278639, 'ionic_contributions': [{'ion_id': 1327, 'distance': 13.469212532043457, 'force': [0.5210571885108948, -0.15596595406532288, -1.7473162412643433], 'magnitude': 1.8300108909606934, 'cosine_ionic_motion': -0.5029047131538391, 'motion_component_ionic': -0.9203211069107056, 'motion_component_percent_ionic': 50.29047131538391}, {'ion_id': 1380, 'distance': 10.161314010620117, 'force': [3.0363898277282715, 0.8332290053367615, -0.6519385576248169], 'magnitude': 3.2154250144958496, 'cosine_ionic_motion': 0.5544977784156799, 'motion_component_ionic': 1.782945990562439, 'motion_component_percent_ionic': 55.44977784156799}, {'ion_id': 1443, 'distance': 8.256528854370117, 'force': [2.586791753768921, -0.8877150416374207, -4.0297532081604], 'magnitude': 4.8701581954956055, 'cosine_ionic_motion': -0.28615787625312805, 'motion_component_ionic': -1.3936340808868408, 'motion_component_percent_ionic': 28.615787625312805}, {'ion_id': 1476, 'distance': 12.340150833129883, 'force': [1.3487483263015747, -1.712496280670166, -0.039044089615345], 'magnitude': 2.180204153060913, 'cosine_ionic_motion': 0.13757206499576569, 'motion_component_ionic': 0.2999351918697357, 'motion_component_percent_ionic': 13.757206499576569}, {'ion_id': 2434, 'distance': 6.7822136878967285, 'force': [-0.48151785135269165, -7.0847249031066895, -1.291944980621338], 'magnitude': 7.217638969421387, 'cosine_ionic_motion': -0.48055243492126465, 'motion_component_ionic': -3.468453884124756, 'motion_component_percent_ionic': 48.055243492126465}, {'ion_id': 2443, 'distance': 5.039106845855713, 'force': [2.3701698780059814, 12.436541557312012, -3.2652554512023926], 'magnitude': 13.074676513671875, 'cosine_ionic_motion': 0.24864144623279572, 'motion_component_ionic': 3.250906467437744, 'motion_component_percent_ionic': 24.86414462327957}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.603452205657959, 'force': [-0.08171731978654861, -3.155369997024536, 3.1179258823394775], 'magnitude': 4.4367218017578125, 'cosine_with_motion': 0.24678240716457367, 'motion_component': 1.094904899597168, 'motion_component_percent': 24.678240716457367}]}, 5998: {'frame': 5998, 'motion_vector': [-0.7672195434570312, 2.2775001525878906, -1.0481185913085938], 'ionic_force': [10.780787527561188, 0.28440017998218536, -7.232492357492447], 'ionic_force_magnitude': 12.985191907629991, 'radial_force': 10.784538153152075, 'axial_force': -7.232492357492447, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.5282077789306641, 5.127721786499023, -4.209736347198486], 'asn_force_magnitude': 6.655404893046227, 'residue_force': [0.5282077789306641, 5.127721786499023, -4.209736347198486], 'residue_force_magnitude': 6.655404893046227, 'total_force': [11.308995306491852, 5.412121966481209, -11.442228704690933], 'total_force_magnitude': 16.973774970606165, 'cosine_total_motion': 0.3514919931509969, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.8989004348307543, 'cosine_residue_motion': 0.8989004348307543, 'cosine_ionic_motion': -0.0012630045621029582, 'motion_component_total': 5.966145995714864, 'motion_component_glu': None, 'motion_component_asn': 5.9825463523339835, 'motion_component_residue': 5.9825463523339835, 'motion_component_ionic': -0.016400356619119094, 'motion_component_percent_total': 35.149199315099686, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 89.89004348307543, 'motion_component_percent_residue': 89.89004348307543, 'motion_component_percent_ionic': 0.12630045621029581, 'ionic_contributions': [{'ion_id': 1327, 'distance': 13.114724159240723, 'force': [0.6711025238037109, -0.13265840709209442, -1.804991602897644], 'magnitude': 1.9302775859832764, 'cosine_ionic_motion': 0.21237851679325104, 'motion_component_ionic': 0.40994948148727417, 'motion_component_percent_ionic': 21.237851679325104}, {'ion_id': 1380, 'distance': 10.606010437011719, 'force': [2.8374791145324707, 0.6517823338508606, -0.4846545159816742], 'magnitude': 2.95143985748291, 'cosine_ionic_motion': -0.0238502100110054, 'motion_component_ionic': -0.07039245963096619, 'motion_component_percent_ionic': 2.38502100110054}, {'ion_id': 1443, 'distance': 8.347920417785645, 'force': [3.076692581176758, -0.8291545510292053, -3.541635036468506], 'magnitude': 4.764106750488281, 'cosine_ionic_motion': -0.04297903925180435, 'motion_component_ionic': -0.2047567367553711, 'motion_component_percent_ionic': 4.297903925180435}, {'ion_id': 1476, 'distance': 12.868345260620117, 'force': [1.263065218925476, -1.5566960573196411, 0.03140932321548462], 'magnitude': 2.004899740219116, 'cosine_ionic_motion': -0.8650766611099243, 'motion_component_ionic': -1.7343919277191162, 'motion_component_percent_ionic': 86.50766611099243}, {'ion_id': 2434, 'distance': 6.327516555786133, 'force': [-0.50923091173172, -8.268269538879395, -0.3708587884902954], 'magnitude': 8.29223346710205, 'cosine_ionic_motion': -0.8302967548370361, 'motion_component_ionic': -6.885014533996582, 'motion_component_percent_ionic': 83.02967548370361}, {'ion_id': 2443, 'distance': 5.487727642059326, 'force': [3.441679000854492, 10.41939640045166, -1.061761736869812], 'magnitude': 11.024351119995117, 'cosine_ionic_motion': 0.7681363821029663, 'motion_component_ionic': 8.468205451965332, 'motion_component_percent_ionic': 76.81363821029663}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.439334392547607, 'force': [0.5282077789306641, 5.127721786499023, -4.209736347198486], 'magnitude': 6.655405044555664, 'cosine_with_motion': 0.8989003896713257, 'motion_component': 5.982546329498291, 'motion_component_percent': 89.89003896713257}]}, 5999: {'frame': 5999, 'motion_vector': [-1.3753700256347656, -4.601753234863281, -0.27584075927734375], 'ionic_force': [6.903971970081329, -9.943094223737717, -11.683605313301086], 'ionic_force_magnitude': 16.8236911771107, 'radial_force': 12.104955667237903, 'axial_force': -11.683605313301086, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.3626566529273987, 14.090182542800903, -4.2385945320129395], 'asn_force_magnitude': 14.71837109004165, 'residue_force': [0.3626566529273987, 14.090182542800903, -4.2385945320129395], 'residue_force_magnitude': 14.71837109004165, 'total_force': [7.266628623008728, 4.147088319063187, -15.922199845314026], 'total_force_magnitude': 17.986625058219175, 'cosine_total_motion': -0.28528993158473065, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.906251286651912, 'cosine_residue_motion': -0.906251286651912, 'cosine_ionic_motion': 0.48783228478641716, 'motion_component_total': -5.13140303229955, 'motion_component_glu': None, 'motion_component_asn': -13.33854273777055, 'motion_component_residue': -13.33854273777055, 'motion_component_ionic': 8.207139705471, 'motion_component_percent_total': 28.528993158473064, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 90.6251286651912, 'motion_component_percent_residue': 90.6251286651912, 'motion_component_percent_ionic': 48.78322847864172, 'ionic_contributions': [{'ion_id': 1327, 'distance': 13.49657154083252, 'force': [0.45604217052459717, 0.1768944263458252, -1.7557339668273926], 'magnitude': 1.822599172592163, 'cosine_ionic_motion': -0.1091388463973999, 'motion_component_ionic': -0.19891637563705444, 'motion_component_percent_ionic': 10.91388463973999}, {'ion_id': 1380, 'distance': 11.447005271911621, 'force': [2.0143558979034424, 1.382273554801941, -0.6717885732650757], 'magnitude': 2.5336947441101074, 'cosine_ionic_motion': -0.7339383959770203, 'motion_component_ionic': -1.859575867652893, 'motion_component_percent_ionic': 73.39383959770203}, {'ion_id': 1443, 'distance': 8.888298988342285, 'force': [2.022075653076172, 0.4375012218952179, -3.6579012870788574], 'magnitude': 4.202432632446289, 'cosine_ionic_motion': -0.1872364580631256, 'motion_component_ionic': -0.7868486046791077, 'motion_component_percent_ionic': 18.72364580631256}, {'ion_id': 1476, 'distance': 10.855681419372559, 'force': [2.0586459636688232, -1.9142779111862183, -0.18536603450775146], 'magnitude': 2.8172404766082764, 'cosine_ionic_motion': 0.44482237100601196, 'motion_component_ionic': 1.2531715631484985, 'motion_component_percent_ionic': 44.482237100601196}, {'ion_id': 2434, 'distance': 4.453519821166992, 'force': [0.3335014283657074, -16.288362503051758, -3.843754291534424], 'magnitude': 16.73906898498535, 'cosine_ionic_motion': 0.938260018825531, 'motion_component_ionic': 15.705598831176758, 'motion_component_percent_ionic': 93.8260018825531}, {'ion_id': 2443, 'distance': 7.170866012573242, 'force': [0.01935085654258728, 6.262876987457275, -1.5690611600875854], 'magnitude': 6.456466197967529, 'cosine_ionic_motion': -0.9147867560386658, 'motion_component_ionic': -5.906289577484131, 'motion_component_percent_ionic': 91.47867560386658}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.693239450454712, 'force': [-2.7312347888946533, -12.222817420959473, 12.013432502746582], 'magnitude': 17.354522705078125, 'cosine_with_motion': 0.6789981722831726, 'motion_component': 11.783689498901367, 'motion_component_percent': 67.89981722831726}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.659578561782837, 'force': [2.1643474102020264, 23.001497268676758, -15.530914306640625], 'magnitude': 27.83814811706543, 'cosine_with_motion': -0.7805917263031006, 'motion_component': -21.730228424072266, 'motion_component_percent': 78.05917263031006}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.045992851257324, 'force': [2.8511462211608887, 8.098589897155762, -16.545122146606445], 'magnitude': 18.64020538330078, 'cosine_with_motion': -0.4084249436855316, 'motion_component': -7.613124847412109, 'motion_component_percent': 40.84249436855316}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.5204715728759766, 'force': [-1.0469173192977905, -2.5786657333374023, 10.890146255493164], 'magnitude': 11.240143775939941, 'cosine_with_motion': 0.19052234292030334, 'motion_component': 2.141498565673828, 'motion_component_percent': 19.052234292030334}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.043825149536133, 'force': [-0.8746848702430725, -2.208421468734741, 4.933863162994385], 'magnitude': 5.475874900817871, 'cosine_with_motion': 0.3797791302204132, 'motion_component': 2.079622983932495, 'motion_component_percent': 37.97791302204132}]}, 6000: {'frame': 6000, 'motion_vector': [-4.781524658203125, 2.4392776489257812, 0.5065383911132812], 'ionic_force': [5.517950534820557, 7.6139421463012695, -19.801055759191513], 'ionic_force_magnitude': 21.920349045819517, 'radial_force': 9.403185264151146, 'axial_force': -19.801055759191513, 'glu_force': [5.4703192710876465, -5.7910475730896, 4.048490047454834], 'glu_force_magnitude': 8.935932888387237, 'asn_force': [-3.052062064409256, -1.6076116561889648, 2.321760445833206], 'asn_force_magnitude': 4.158132952414619, 'residue_force': [2.4182572066783905, -7.3986592292785645, 6.37025049328804], 'residue_force_magnitude': 10.058241280456409, 'total_force': [7.936207741498947, 0.21528291702270508, -13.430805265903473], 'total_force_magnitude': 15.60180342592516, 'cosine_total_motion': -0.5257457467722944, 'cosine_glu_motion': -0.7935315382180069, 'cosine_asn_motion': 0.5284850823239703, 'cosine_residue_motion': -0.48650983787514596, 'cosine_ionic_motion': -0.1509623980702402, 'motion_component_total': -8.202581793157563, 'motion_component_glu': -7.090944570334802, 'motion_component_asn': 2.197511235670854, 'motion_component_residue': -4.893433334663948, 'motion_component_ionic': -3.309148458493616, 'motion_component_percent_total': 52.574574677229435, 'motion_component_percent_glu': 79.35315382180069, 'motion_component_percent_asn': 52.84850823239703, 'motion_component_percent_residue': 48.6509837875146, 'motion_component_percent_ionic': 15.09623980702402, 'ionic_contributions': [{'ion_id': 1327, 'distance': 14.055419921875, 'force': [0.27228718996047974, -0.34001588821411133, -1.6231095790863037], 'magnitude': 1.6805462837219238, 'cosine_ionic_motion': -0.32596269249916077, 'motion_component_ionic': -0.5477954149246216, 'motion_component_percent_ionic': 32.59626924991608}, {'ion_id': 1380, 'distance': 8.973416328430176, 'force': [3.8357651233673096, 0.6248253583908081, -1.3770771026611328], 'magnitude': 4.123086452484131, 'cosine_ionic_motion': -0.7878593802452087, 'motion_component_ionic': -3.2484123706817627, 'motion_component_percent_ionic': 78.78593802452087}, {'ion_id': 1443, 'distance': 8.977163314819336, 'force': [1.5023193359375, -1.549290657043457, -3.5091614723205566], 'magnitude': 4.119645595550537, 'cosine_ionic_motion': -0.5735767483711243, 'motion_component_ionic': -2.3629329204559326, 'motion_component_percent_ionic': 57.35767483711243}, {'ion_id': 1476, 'distance': 12.293431282043457, 'force': [1.1409306526184082, -1.8393505811691284, -0.37553462386131287], 'magnitude': 2.1968066692352295, 'cosine_ionic_motion': -0.8554533123970032, 'motion_component_ionic': -1.879265546798706, 'motion_component_percent_ionic': 85.54533123970032}, {'ion_id': 2434, 'distance': 8.713654518127441, 'force': [-0.8899776935577393, -4.16619348526001, -0.9849853515625], 'magnitude': 4.3725762367248535, 'cosine_ionic_motion': -0.27172449231147766, 'motion_component_ionic': -1.188136100769043, 'motion_component_percent_ionic': 27.172449231147766}, {'ion_id': 2443, 'distance': 4.17150354385376, 'force': [-0.3433740735054016, 14.883967399597168, -11.931187629699707], 'magnitude': 19.07887840270996, 'cosine_ionic_motion': 0.31015416979789734, 'motion_component_ionic': 5.917393684387207, 'motion_component_percent_ionic': 31.015416979789734}], 'glu_contributions': [{'resid': 748, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 5.515539646148682, 'force': [5.4703192710876465, -5.7910475730896, 4.048490047454834], 'magnitude': 8.935933113098145, 'cosine_with_motion': -0.7935314774513245, 'motion_component': -7.090944290161133, 'motion_component_percent': 79.35314774513245}], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.959725856781006, 'force': [-1.3925870656967163, -3.071686267852783, 2.0021188259124756], 'magnitude': 3.922121286392212, 'cosine_with_motion': 0.008518793620169163, 'motion_component': 0.03341174125671387, 'motion_component_percent': 0.8518793620169163}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.887828350067139, 'force': [-1.1611191034317017, 9.759984016418457, 1.2519491910934448], 'magnitude': 9.908222198486328, 'cosine_with_motion': 0.5614486336708069, 'motion_component': 5.562957763671875, 'motion_component_percent': 56.14486336708069}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.66547966003418, 'force': [-0.33897170424461365, -6.09545373916626, -0.6041290163993835], 'magnitude': 6.134690761566162, 'cosine_with_motion': -0.4097754955291748, 'motion_component': -2.513845920562744, 'motion_component_percent': 40.97754955291748}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.179264545440674, 'force': [3.3775413036346436, -10.843356132507324, 0.6421475410461426], 'magnitude': 11.375347137451172, 'cosine_with_motion': -0.6892771124839783, 'motion_component': -7.840766429901123, 'motion_component_percent': 68.92771124839783}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.829558849334717, 'force': [-0.9659819006919861, 3.9124884605407715, -0.7503260970115662], 'magnitude': 4.099228858947754, 'cosine_with_motion': 0.6235973238945007, 'motion_component': 2.5562682151794434, 'motion_component_percent': 62.35973238945007}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.084596633911133, 'force': [-2.570943593978882, 4.730412006378174, -0.2199999988079071], 'magnitude': 5.388408660888672, 'cosine_with_motion': 0.816472053527832, 'motion_component': 4.399485111236572, 'motion_component_percent': 81.6472053527832}]}, 6004: {'frame': 6004, 'motion_vector': [-0.223419189453125, 2.570514678955078, -0.7060775756835938], 'ionic_force': [-13.262407958507538, 11.088155046105385, -8.382136479020119], 'ionic_force_magnitude': 19.2119457405354, 'radial_force': 17.28695019904773, 'axial_force': -8.382136479020119, 'glu_force': [-1.8934214115142822, -5.6408562660217285, 2.6732892990112305], 'glu_force_magnitude': 6.5230958701911845, 'asn_force': [7.777035713195801, -11.803484916687012, -4.9318801164627075], 'asn_force_magnitude': 14.970904519966084, 'residue_force': [5.8836143016815186, -17.44434118270874, -2.258590817451477], 'residue_force_magnitude': 18.547862114820013, 'total_force': [-7.378793656826019, -6.356186136603355, -10.640727296471596], 'total_force_magnitude': 14.424727915320979, 'cosine_total_motion': -0.18599251285352061, 'cosine_glu_motion': -0.9148800802838679, 'cosine_asn_motion': -0.7140458572334746, 'cosine_residue_motion': -0.8980961105824571, 'cosine_ionic_motion': 0.7274053144578178, 'motion_component_total': -2.682891392198875, 'motion_component_glu': -5.967850473419878, 'motion_component_asn': -10.68991235151968, 'motion_component_residue': -16.65776282493956, 'motion_component_ionic': 13.974871432740684, 'motion_component_percent_total': 18.59925128535206, 'motion_component_percent_glu': 91.48800802838679, 'motion_component_percent_asn': 71.40458572334745, 'motion_component_percent_residue': 89.80961105824571, 'motion_component_percent_ionic': 72.74053144578177, 'ionic_contributions': [{'ion_id': 1327, 'distance': 14.805962562561035, 'force': [-0.7501986622810364, -0.13029859960079193, -1.3091551065444946], 'magnitude': 1.5144842863082886, 'cosine_ionic_motion': 0.1868608444929123, 'motion_component_ionic': 0.28299781680107117, 'motion_component_percent_ionic': 18.68608444929123}, {'ion_id': 1380, 'distance': 4.653715133666992, 'force': [-4.599451065063477, 13.990073204040527, -4.257678985595703], 'magnitude': 15.329870223999023, 'cosine_ionic_motion': 0.9752989411354065, 'motion_component_ionic': 14.95120620727539, 'motion_component_percent_ionic': 97.52989411354065}, {'ion_id': 1443, 'distance': 9.613933563232422, 'force': [-2.4518744945526123, -0.6125720739364624, -2.5525479316711426], 'magnitude': 3.59199595451355, 'cosine_ionic_motion': 0.08070346713066101, 'motion_component_ionic': 0.2898865342140198, 'motion_component_percent_ionic': 8.070346713066101}, {'ion_id': 1476, 'distance': 11.188375473022461, 'force': [-1.4830362796783447, -2.197493553161621, 0.07560582458972931], 'magnitude': 2.652186155319214, 'cosine_ionic_motion': -0.7569971680641174, 'motion_component_ionic': -2.007697343826294, 'motion_component_percent_ionic': 75.69971680641174}, {'ion_id': 2434, 'distance': 13.317967414855957, 'force': [-1.6397267580032349, -0.897940993309021, -0.09315349161624908], 'magnitude': 1.8718117475509644, 'cosine_ionic_motion': -0.37466830015182495, 'motion_component_ionic': -0.70130854845047, 'motion_component_percent_ionic': 37.466830015182495}, {'ion_id': 2443, 'distance': 11.454083442687988, 'force': [-2.338120698928833, 0.9363870620727539, -0.2452067881822586], 'magnitude': 2.530564308166504, 'cosine_ionic_motion': 0.458311527967453, 'motion_component_ionic': 1.1597868204116821, 'motion_component_percent_ionic': 45.8311527967453}], 'glu_contributions': [{'resid': 1073, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 5.350562572479248, 'force': [1.9671130180358887, 7.572391033172607, -5.101621627807617], 'magnitude': 9.34008502960205, 'cosine_with_motion': 0.905632734298706, 'motion_component': 8.458686828613281, 'motion_component_percent': 90.5632734298706}, {'resid': 1073, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 4.146653652191162, 'force': [-3.860534429550171, -13.213247299194336, 7.774910926818848], 'magnitude': 15.809581756591797, 'cosine_with_motion': -0.9125186204910278, 'motion_component': -14.42653751373291, 'motion_component_percent': 91.25186204910278}], 'asn_contributions': [{'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.5101473331451416, 'force': [-0.8161220550537109, 17.44001579284668, 8.017990112304688], 'magnitude': 19.21219253540039, 'cosine_with_motion': 0.7656698822975159, 'motion_component': 14.710197448730469, 'motion_component_percent': 76.56698822975159}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.610398530960083, 'force': [8.503637313842773, -25.7799072265625, -9.905538558959961], 'magnitude': 28.896974563598633, 'cosine_with_motion': -0.7913617491722107, 'motion_component': -22.86795997619629, 'motion_component_percent': 79.13617491722107}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.922837495803833, 'force': [-4.029259204864502, -19.039121627807617, -3.8032891750335693], 'magnitude': 19.82897186279297, 'cosine_with_motion': -0.8550407290458679, 'motion_component': -16.954578399658203, 'motion_component_percent': 85.50407290458679}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.649535655975342, 'force': [2.6498820781707764, 10.098359107971191, -0.6293421983718872], 'magnitude': 10.459197044372559, 'cosine_with_motion': 0.9224852919578552, 'motion_component': 9.648455619812012, 'motion_component_percent': 92.24852919578552}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.8848114013671875, 'force': [1.4688975811004639, 5.477169036865234, 1.3882997035980225], 'magnitude': 5.838185787200928, 'cosine_with_motion': 0.8177149891853333, 'motion_component': 4.773972034454346, 'motion_component_percent': 81.77149891853333}]}, 6005: {'frame': 6005, 'motion_vector': [-0.2879486083984375, 0.21361923217773438, 0.6275177001953125], 'ionic_force': [-11.751091122627258, 3.513936460018158, -5.2574396431446075], 'ionic_force_magnitude': 13.344533098562968, 'radial_force': 12.265231021767756, 'axial_force': -5.2574396431446075, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-2.13910374045372, -4.090269088745117, 1.7995737791061401], 'asn_force_magnitude': 4.954243818910537, 'residue_force': [-2.13910374045372, -4.090269088745117, 1.7995737791061401], 'residue_force_magnitude': 4.954243818910537, 'total_force': [-13.890194863080978, -0.5763326287269592, -3.4578658640384674], 'total_force_magnitude': 14.325728915729874, 'cosine_total_motion': 0.16484018283972596, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.2433869696212026, 'cosine_residue_motion': 0.2433869696212026, 'cosine_ionic_motion': 0.08660156000935704, 'motion_component_total': 2.3614557737812616, 'motion_component_glu': None, 'motion_component_asn': 1.2057983898492095, 'motion_component_residue': 1.2057983898492095, 'motion_component_ionic': 1.155657383932052, 'motion_component_percent_total': 16.484018283972595, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 24.33869696212026, 'motion_component_percent_residue': 24.33869696212026, 'motion_component_percent_ionic': 8.660156000935704, 'ionic_contributions': [{'ion_id': 1380, 'distance': 7.387109279632568, 'force': [-1.5290939807891846, 5.18525505065918, -2.7910616397857666], 'magnitude': 6.0839972496032715, 'cosine_ionic_motion': -0.04627435654401779, 'motion_component_ionic': -0.28153306245803833, 'motion_component_percent_ionic': 4.627435654401779}, {'ion_id': 1443, 'distance': 10.215596199035645, 'force': [-2.1018567085266113, 0.29880401492118835, -2.3693599700927734], 'magnitude': 3.181344509124756, 'cosine_ionic_motion': -0.355666846036911, 'motion_component_ionic': -1.1314988136291504, 'motion_component_percent_ionic': 35.5666846036911}, {'ion_id': 1476, 'distance': 10.20903491973877, 'force': [-1.9276835918426514, -2.4968819618225098, -0.44340747594833374], 'magnitude': 3.185434579849243, 'cosine_ionic_motion': -0.11143966019153595, 'motion_component_ionic': -0.35498374700546265, 'motion_component_percent_ionic': 11.143966019153595}, {'ion_id': 2434, 'distance': 8.538402557373047, 'force': [-4.488006591796875, -0.4852888882160187, 0.6003507971763611], 'magnitude': 4.553913593292236, 'cosine_ionic_motion': 0.47562408447265625, 'motion_component_ionic': 2.1659510135650635, 'motion_component_percent_ionic': 47.562408447265625}, {'ion_id': 2443, 'distance': 12.88902473449707, 'force': [-1.704450249671936, 1.0120482444763184, -0.25396135449409485], 'magnitude': 1.9984716176986694, 'cosine_ionic_motion': 0.37915071845054626, 'motion_component_ionic': 0.7577219605445862, 'motion_component_percent_ionic': 37.91507184505463}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.525741100311279, 'force': [-4.685890197753906, -4.98834228515625, 3.641629219055176], 'magnitude': 7.7525858879089355, 'cosine_with_motion': 0.4584856629371643, 'motion_component': 3.5544495582580566, 'motion_component_percent': 45.84856629371643}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.655789375305176, 'force': [5.722832679748535, 7.2156758308410645, -2.4860730171203613], 'magnitude': 9.539253234863281, 'cosine_with_motion': -0.24172842502593994, 'motion_component': -2.305908679962158, 'motion_component_percent': 24.172842502593994}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.459854602813721, 'force': [-2.216416835784912, -4.019174098968506, 0.8787698149681091], 'magnitude': 4.673168182373047, 'cosine_with_motion': 0.09802954643964767, 'motion_component': 0.4581085443496704, 'motion_component_percent': 9.802954643964767}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.66311502456665, 'force': [0.4617593586444855, 7.302806854248047, 0.9671420454978943], 'magnitude': 7.381028175354004, 'cosine_with_motion': 0.38128861784935, 'motion_component': 2.8143019676208496, 'motion_component_percent': 38.128861784935}, {'resid': 1105, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.487074851989746, 'force': [-1.4213887453079224, -9.601235389709473, -1.2018942832946777], 'magnitude': 9.780011177062988, 'cosine_with_motion': -0.3389723300933838, 'motion_component': -3.315153121948242, 'motion_component_percent': 33.89723300933838}]}, 6006: {'frame': 6006, 'motion_vector': [3.3086013793945312, -2.3047142028808594, -0.0504608154296875], 'ionic_force': [-11.669181168079376, 5.09692008793354, -6.636843234300613], 'ionic_force_magnitude': 14.35952894885207, 'radial_force': 12.733749782221999, 'axial_force': -6.636843234300613, 'glu_force': [1.9968379735946655, 7.997310161590576, 2.0858542919158936], 'glu_force_magnitude': 8.502653694028323, 'asn_force': [-1.1865164488554, -2.8178770542144775, -0.6750527620315552], 'asn_force_magnitude': 3.1311257732003233, 'residue_force': [0.8103215247392654, 5.179433107376099, 1.4108015298843384], 'residue_force_magnitude': 5.4289510261157625, 'total_force': [-10.85885964334011, 10.276353195309639, -5.226041704416275], 'total_force_magnitude': 15.83760649987268, 'cosine_total_motion': -0.9292691321724098, 'cosine_glu_motion': -0.34794612235353367, 'cosine_asn_motion': 0.20613788133289312, 'cosine_residue_motion': -0.4260531617159685, 'cosine_ionic_motion': -0.863842897808891, 'motion_component_total': -14.717398847824802, 'motion_component_glu': -2.958465382552104, 'motion_component_asn': 0.6454436330743315, 'motion_component_residue': -2.3130217494777723, 'motion_component_ionic': -12.40437709834703, 'motion_component_percent_total': 92.92691321724098, 'motion_component_percent_glu': 34.79461223535337, 'motion_component_percent_asn': 20.61378813328931, 'motion_component_percent_residue': 42.605316171596854, 'motion_component_percent_ionic': 86.3842897808891, 'ionic_contributions': [{'ion_id': 1327, 'distance': 14.995388984680176, 'force': [-0.7694267630577087, 0.20096524059772491, -1.2440012693405151], 'magnitude': 1.4764631986618042, 'cosine_ionic_motion': -0.4948265552520752, 'motion_component_ionic': -0.730593204498291, 'motion_component_percent_ionic': 49.48265552520752}, {'ion_id': 1380, 'distance': 7.06876802444458, 'force': [-1.6209291219711304, 5.998019695281982, -2.354433298110962], 'magnitude': 6.644321918487549, 'cosine_ionic_motion': -0.7116686105728149, 'motion_component_ionic': -4.728555202484131, 'motion_component_percent_ionic': 71.1668610572815}, {'ion_id': 1443, 'distance': 10.300626754760742, 'force': [-2.171865224838257, 0.4668664336204529, -2.2036139965057373], 'magnitude': 3.129037857055664, 'cosine_ionic_motion': -0.6459600329399109, 'motion_component_ionic': -2.021233320236206, 'motion_component_percent_ionic': 64.59600329399109}, {'ion_id': 1476, 'distance': 8.93224811553955, 'force': [-3.098361015319824, -2.754167318344116, -0.36075103282928467], 'magnitude': 4.161180019378662, 'cosine_ionic_motion': -0.23155388236045837, 'motion_component_ionic': -0.9635373950004578, 'motion_component_percent_ionic': 23.155388236045837}, {'ion_id': 2434, 'distance': 11.276430130004883, 'force': [-2.578646183013916, 0.22548645734786987, -0.3415878117084503], 'magnitude': 2.6109275817871094, 'cosine_ionic_motion': -0.8580604791641235, 'motion_component_ionic': -2.2403337955474854, 'motion_component_percent_ionic': 85.80604791641235}, {'ion_id': 2443, 'distance': 13.864049911499023, 'force': [-1.42995285987854, 0.9597495794296265, -0.13245582580566406], 'magnitude': 1.7272605895996094, 'cosine_ionic_motion': -0.9958682656288147, 'motion_component_ionic': -1.7201240062713623, 'motion_component_percent_ionic': 99.58682656288147}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 5.654324531555176, 'force': [1.9968379735946655, 7.997310161590576, 2.0858542919158936], 'magnitude': 8.502654075622559, 'cosine_with_motion': -0.3479461073875427, 'motion_component': -2.958465337753296, 'motion_component_percent': 34.79461073875427}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.498685359954834, 'force': [5.774613857269287, 7.766817569732666, -2.8603482246398926], 'magnitude': 10.09213638305664, 'cosine_with_motion': 0.03317074850201607, 'motion_component': 0.33476370573043823, 'motion_component_percent': 3.3170748502016068}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.6935200691223145, 'force': [-2.679769992828369, -3.323723077774048, 0.48975634574890137], 'magnitude': 4.297460079193115, 'cosine_with_motion': -0.07102172076702118, 'motion_component': -0.30521300435066223, 'motion_component_percent': 7.102172076702118}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.597736835479736, 'force': [-3.3127877712249756, -5.251379013061523, 2.2082884311676025], 'magnitude': 6.589998722076416, 'cosine_with_motion': 0.03878951072692871, 'motion_component': 0.25562283396720886, 'motion_component_percent': 3.878951072692871}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.6094465255737305, 'force': [-0</t>
         </is>
       </c>
     </row>
@@ -787,7 +787,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>{6161: {'frame': 6161, 'ionic_force': [2.045816570520401, 2.513314615935087, -12.963244438171387], 'ionic_force_magnitude': 13.362178795491031, 'motion_vector': [4.460853576660156, 2.02520751953125, 0.9477462768554688], 'ionic_force_x': 2.045816570520401, 'ionic_force_y': 2.513314615935087, 'ionic_force_z': -12.963244438171387, 'radial_force': 3.2406968076154223, 'axial_force': -12.963244438171387, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [5.636149525642395, -11.620142102241516, 1.9752273261547089], 'asn_force_magnitude': 13.06504523305117, 'residue_force': [5.636149525642395, -11.620142102241516, 1.9752273261547089], 'residue_force_magnitude': 13.06504523305117, 'total_force': [7.681966096162796, -9.106827486306429, -10.988017112016678], 'total_force_magnitude': 16.20751153082768, 'motion_component_total': 1.0844067892659779, 'cosine_total_motion': 0.0669076673000275, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.05339305783568137, 'cosine_residue_motion': 0.05339305783568137, 'cosine_ionic_motion': 0.028949176585065187, 'motion_component_glu': None, 'motion_component_asn': 0.6975827157540944, 'motion_component_residue': 0.6975827157540944, 'motion_component_ionic': 0.3868240735118835, 'ionic_contributions': [{'ion_id': 1327, 'distance': 9.253506660461426, 'force': [0.9507448077201843, 0.019289210438728333, -3.7588417530059814], 'magnitude': 3.8772642612457275}, {'ion_id': 1341, 'distance': 14.722437858581543, 'force': [0.26577094197273254, -0.029373470693826675, -1.5081979036331177], 'magnitude': 1.531717300415039}, {'ion_id': 1355, 'distance': 9.555658340454102, 'force': [-0.5799313187599182, -3.2436165809631348, -1.537106990814209], 'magnitude': 3.6359410285949707}, {'ion_id': 1380, 'distance': 10.345450401306152, 'force': [2.139223337173462, 1.9624422788619995, -1.0930858850479126], 'magnitude': 3.1019821166992188}, {'ion_id': 1476, 'distance': 6.429809093475342, 'force': [-4.092360019683838, 5.589524745941162, -4.061839580535889], 'magnitude': 8.030488014221191}, {'ion_id': 2443, 'distance': 9.1830415725708, 'force': [3.3623688220977783, -1.7849515676498413, -1.0041723251342773], 'magnitude': 3.9369959831237793}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.937707424163818, 'force': [3.445258140563965, -1.7017422914505005, 0.92019122838974], 'magnitude': 3.951263427734375}, {'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.288460731506348, 'force': [-5.059122085571289, -6.626802921295166, 1.4587273597717285], 'magnitude': 8.463871002197266}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.338872909545898, 'force': [5.106224060058594, 4.332803249359131, -1.69615638256073], 'magnitude': 6.908230781555176}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.25961446762085, 'force': [7.841231346130371, 14.6804780960083, -2.4135947227478027], 'magnitude': 16.817455291748047}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.332993984222412, 'force': [-6.791555881500244, -10.254345893859863, 2.445364475250244], 'magnitude': 12.540201187133789}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.605200290679932, 'force': [-1.9009085893630981, -6.2771172523498535, 0.3627375066280365], 'magnitude': 6.568655490875244}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.476353645324707, 'force': [2.9950225353240967, -5.7734150886535645, 0.8979578614234924], 'magnitude': 6.565730094909668}]}, 6162: {'frame': 6162, 'ionic_force': [7.763323903083801, 2.8181435465812683, -6.318853139877319], 'ionic_force_magnitude': 10.398992070228124, 'motion_vector': [-1.7015113830566406, -2.5169944763183594, 0.5141983032226562], 'ionic_force_x': 7.763323903083801, 'ionic_force_y': 2.8181435465812683, 'ionic_force_z': -6.318853139877319, 'radial_force': 8.259003031439688, 'axial_force': -6.318853139877319, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [2.2658984661102295, 6.250769853591919, -11.89534592628479], 'asn_force_magnitude': 13.627386922197314, 'residue_force': [2.2658984661102295, 6.250769853591919, -11.89534592628479], 'residue_force_magnitude': 13.627386922197314, 'total_force': [10.02922236919403, 9.068913400173187, -18.21419906616211], 'total_force_magnitude': 22.684522018600333, 'motion_component_total': -15.98543933181385, 'cosine_total_motion': -0.7046848648036964, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.6121600336023413, 'cosine_residue_motion': -0.6121600336023413, 'cosine_ionic_motion': -0.7350037045890127, 'motion_component_glu': None, 'motion_component_asn': -8.342141636204413, 'motion_component_residue': -8.342141636204413, 'motion_component_ionic': -7.643297695609437, 'ionic_contributions': [{'ion_id': 1327, 'distance': 10.584158897399902, 'force': [1.9486887454986572, 0.7575831413269043, -2.100437641143799], 'magnitude': 2.963639259338379}, {'ion_id': 1355, 'distance': 8.435245513916016, 'force': [1.829471230506897, -3.8013644218444824, -1.9934921264648438], 'magnitude': 4.665977478027344}, {'ion_id': 1380, 'distance': 14.387797355651855, 'force': [1.3906784057617188, 0.7438085079193115, -0.29142385721206665], 'magnitude': 1.603797197341919}, {'ion_id': 1476, 'distance': 7.511940956115723, 'force': [0.6493955850601196, 5.551018238067627, -1.8384053707122803], 'magnitude': 5.883472919464111}, {'ion_id': 2443, 'distance': 12.900399208068848, 'force': [1.9450899362564087, -0.43290191888809204, -0.09509414434432983], 'magnitude': 1.9949489831924438}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.1263973712921143, 'force': [8.836230278015137, -18.055543899536133, 13.506759643554688], 'magnitude': 24.218053817749023}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.620124578475952, 'force': [-2.554917097091675, 17.166858673095703, -22.835859298706055], 'magnitude': 28.682836532592773}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.2906246185302734, 'force': [-19.775497436523438, 15.2301025390625, -13.08043384552002], 'magnitude': 28.180208206176758}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.2818853855133057, 'force': [9.693719863891602, -3.504816770553589, 7.812277793884277], 'magnitude': 12.933816909790039}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.154703140258789, 'force': [6.0663628578186035, -4.5858306884765625, 2.7019097805023193], 'magnitude': 8.070372581481934}]}, 6163: {'frame': 6163, 'ionic_force': [5.693150162696838, 11.41169948130846, -10.106098487973213], 'ionic_force_magnitude': 16.271818290385536, 'motion_vector': [-5.470054626464844, -0.9522628784179688, -5.482391357421875], 'ionic_force_x': 5.693150162696838, 'ionic_force_y': 11.41169948130846, 'ionic_force_z': -10.106098487973213, 'radial_force': 12.752993524138198, 'axial_force': -10.106098487973213, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [1.3283605575561523, 1.9260282516479492, -3.0279898643493652], 'asn_force_magnitude': 3.8265976030436537, 'residue_force': [1.3283605575561523, 1.9260282516479492, -3.0279898643493652], 'residue_force_magnitude': 3.8265976030436537, 'total_force': [7.021510720252991, 13.33772773295641, -13.134088352322578], 'total_force_magnitude': 19.99252036937109, 'motion_component_total': 2.6781326217801196, 'cosine_total_motion': 0.1339567284314522, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.25119619538697685, 'cosine_residue_motion': 0.25119619538697685, 'cosine_ionic_motion': 0.10551407543882721, 'motion_component_glu': None, 'motion_component_asn': 0.9612267591614909, 'motion_component_residue': 0.9612267591614909, 'motion_component_ionic': 1.7169058626186278, 'ionic_contributions': [{'ion_id': 1327, 'distance': 8.839310646057129, 'force': [2.395063638687134, 0.08514890819787979, -3.508793830871582], 'magnitude': 4.249142646789551}, {'ion_id': 1341, 'distance': 13.962050437927246, 'force': [0.5789742469787598, -0.06532517075538635, -1.6003326177597046], 'magnitude': 1.7030980587005615}, {'ion_id': 1355, 'distance': 9.791486740112305, 'force': [0.5200189352035522, -3.328923225402832, -0.7997344136238098], 'magnitude': 3.462907075881958}, {'ion_id': 1380, 'distance': 11.607020378112793, 'force': [2.3475747108459473, 0.65799880027771, -0.3588736653327942], 'magnitude': 2.4643173217773438}, {'ion_id': 1476, 'distance': 4.583294868469238, 'force': [-2.214129686355591, 15.15945053100586, -3.8823859691619873], 'magnitude': 15.804563522338867}, {'ion_id': 2443, 'distance': 11.913593292236328, 'force': [2.065648317337036, -1.0966503620147705, 0.044022008776664734], 'magnitude': 2.3391201496124268}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.494832992553711, 'force': [-1.025095820426941, -6.225288391113281, 4.654168128967285], 'magnitude': 7.840045928955078}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.997812747955322, 'force': [2.575059652328491, 5.630373001098633, -4.879940032958984], 'magnitude': 7.88326358795166}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.319039344787598, 'force': [-1.1120789051055908, 8.198407173156738, -6.919050693511963], 'magnitude': 10.785354614257812}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.033473014831543, 'force': [0.680869460105896, -3.440354824066162, 4.234739780426025], 'magnitude': 5.498422145843506}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.729037761688232, 'force': [0.7276909351348877, 6.655938625335693, 2.680285930633545], 'magnitude': 7.212141513824463}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.59222412109375, 'force': [-0.5180847644805908, -8.893047332763672, -2.7981929779052734], 'magnitude': 9.337268829345703}]}, 6164: {'frame': 6164, 'ionic_force': [0.7338058315217495, -0.6169207841157913, -9.97306752204895], 'ionic_force_magnitude': 10.019038778824891, 'motion_vector': [0.8026161193847656, -1.9557952880859375, 2.9555435180664062], 'ionic_force_x': 0.7338058315217495, 'ionic_force_y': -0.6169207841157913, 'ionic_force_z': -9.97306752204895, 'radial_force': 0.9586773452258945, 'axial_force': -9.97306752204895, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [0.0, 0.0, 0.0], 'residue_force_magnitude': 0.0, 'total_force': [0.7338058315217495, -0.6169207841157913, -9.97306752204895], 'total_force_magnitude': 10.019038778824891, 'motion_component_total': -7.617434904944093, 'cosine_total_motion': -0.7602959797943335, 'cosine_glu_motion': None, 'cosine_asn_motion': None, 'cosine_residue_motion': None, 'cosine_ionic_motion': -0.7602959797943335, 'motion_component_glu': None, 'motion_component_asn': None, 'motion_component_residue': None, 'motion_component_ionic': -7.617434904944093, 'ionic_contributions': [{'ion_id': 1327, 'distance': 13.327520370483398, 'force': [-0.05467653647065163, -0.15348537266254425, -1.8620142936706543], 'magnitude': 1.8691293001174927}, {'ion_id': 1355, 'distance': 13.564136505126953, 'force': [-0.5475013852119446, -1.3620316982269287, -1.0494215488433838], 'magnitude': 1.8044871091842651}, {'ion_id': 1380, 'distance': 9.610234260559082, 'force': [1.875036597251892, 1.458633303642273, -2.697950601577759], 'magnitude': 3.594761610031128}, {'ion_id': 1476, 'distance': 9.47956657409668, 'force': [-2.0720303058624268, 1.2611353397369385, -2.7867367267608643], 'magnitude': 3.6945464611053467}, {'ion_id': 2443, 'distance': 10.782855987548828, 'force': [1.5329774618148804, -1.8211723566055298, -1.576944351196289], 'magnitude': 2.8554232120513916}], 'glu_contributions': [], 'asn_contributions': []}, 6165: {'frame': 6165, 'ionic_force': [0.8527390398085117, -2.051217794418335, -13.607491910457611], 'ionic_force_magnitude': 13.78762105670595, 'motion_vector': [-0.4117393493652344, 4.247417449951172, -2.2331161499023438], 'ionic_force_x': 0.8527390398085117, 'ionic_force_y': -2.051217794418335, 'ionic_force_z': -13.607491910457611, 'radial_force': 2.221409082126019, 'axial_force': -13.607491910457611, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [2.341707944869995, -0.19888710975646973, 2.5418634712696075], 'asn_force_magnitude': 3.4618235206418766, 'residue_force': [2.341707944869995, -0.19888710975646973, 2.5418634712696075], 'residue_force_magnitude': 3.4618235206418766, 'total_force': [3.194446984678507, -2.2501049041748047, -11.065628439188004], 'total_force_magnitude': 11.735228858947723, 'motion_component_total': 2.8732380160282083, 'cosine_total_motion': 0.24483868619549415, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.4489355041013871, 'cosine_residue_motion': -0.4489355041013871, 'cosine_ionic_motion': 0.3211122125541915, 'motion_component_glu': None, 'motion_component_asn': -1.5541354873493995, 'motion_component_residue': -1.5541354873493995, 'motion_component_ionic': 4.427373503377607, 'ionic_contributions': [{'ion_id': 1327, 'distance': 11.319201469421387, 'force': [0.062102917581796646, -0.7361721992492676, -2.4836835861206055], 'magnitude': 2.591233491897583}, {'ion_id': 1355, 'distance': 13.651247024536133, 'force': [-0.45634692907333374, -1.6045798063278198, -0.6252397894859314], 'magnitude': 1.7815312147140503}, {'ion_id': 1380, 'distance': 7.018681526184082, 'force': [4.697567462921143, 1.9251720905303955, -4.4325270652771], 'magnitude': 6.739490032196045}, {'ion_id': 1476, 'distance': 6.703571796417236, 'force': [-5.758725166320801, 1.1061946153640747, -4.493953704833984], 'magnitude': 7.38797664642334}, {'ion_id': 2443, 'distance': 9.210395812988281, 'force': [2.308140754699707, -2.7418324947357178, -1.5720877647399902], 'magnitude': 3.9136452674865723}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.529760837554932, 'force': [-10.259325981140137, 4.805561065673828, -2.178412437438965], 'magnitude': 11.536579132080078}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.9075493812561035, 'force': [7.5509419441223145, -1.7516062259674072, 2.6001579761505127], 'magnitude': 8.175920486450195}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.285310745239258, 'force': [8.399792671203613, -6.517972469329834, 2.5062448978424072], 'magnitude': 10.923449516296387}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.447909355163574, 'force': [-3.349700689315796, 3.2651305198669434, -0.38612696528434753], 'magnitude': 4.693683624267578}]}, 6166: {'frame': 6166, 'ionic_force': [1.4523009806871414, 1.297539383172989, -11.587992548942566], 'ionic_force_magnitude': 11.750504580814315, 'motion_vector': [2.0425567626953125, -2.522167205810547, 0.7178115844726562], 'ionic_force_x': 1.4523009806871414, 'ionic_force_y': 1.297539383172989, 'ionic_force_z': -11.587992548942566, 'radial_force': 1.9475077893014379, 'axial_force': -11.587992548942566, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.6397826671600342, 0.49869585037231445, -0.6913818120956421], 'asn_force_magnitude': 1.0658462471077275, 'residue_force': [0.6397826671600342, 0.49869585037231445, -0.6913818120956421], 'residue_force_magnitude': 1.0658462471077275, 'total_force': [2.0920836478471756, 1.7962352335453033, -12.279374361038208], 'total_force_magnitude': 12.585162283512343, 'motion_component_total': -2.7291304462645094, 'cosine_total_motion': -0.2168530198327206, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.12625091430709678, 'cosine_residue_motion': -0.12625091430709678, 'cosine_ionic_motion': -0.22080467823421474, 'motion_component_glu': None, 'motion_component_asn': -0.1345640632081384, 'motion_component_residue': -0.1345640632081384, 'motion_component_ionic': -2.594566383056371, 'ionic_contributions': [{'ion_id': 1327, 'distance': 11.323769569396973, 'force': [0.08723576366901398, 0.26207712292671204, -2.5743675231933594], 'magnitude': 2.5891432762145996}, {'ion_id': 1355, 'distance': 10.770421981811523, 'force': [-0.8347313404083252, -2.0121395587921143, -1.8562531471252441], 'magnitude': 2.8620200157165527}, {'ion_id': 1380, 'distance': 10.39759635925293, 'force': [1.436957836151123, 2.019728899002075, -1.8128858804702759], 'magnitude': 3.0709457397460938}, {'ion_id': 1476, 'distance': 9.792675018310547, 'force': [-1.8430176973342896, 1.9066798686981201, -2.2257046699523926], 'magnitude': 3.462066411972046}, {'ion_id': 2443, 'distance': 8.935583114624023, 'force': [2.605856418609619, -0.8788069486618042, -3.118781328201294], 'magnitude': 4.158074855804443}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.566076755523682, 'force': [5.6690168380737305, -4.858895778656006, -1.622536301612854], 'magnitude': 7.640631198883057}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.915214538574219, 'force': [-3.328258514404297, 4.29303503036499, 1.470607876777649], 'magnitude': 5.627623081207275}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.352017402648926, 'force': [-8.489718437194824, 5.058170318603516, 3.977790117263794], 'magnitude': 10.652850151062012}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.660675525665283, 'force': [3.091325283050537, -2.0316126346588135, -2.2840301990509033], 'magnitude': 4.347474575042725}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.47129487991333, 'force': [4.145976543426514, -1.5143561363220215, -1.4744571447372437], 'magnitude': 4.653645992279053}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.0422515869140625, 'force': [8.858025550842285, 6.583568572998047, 4.715805530548096], 'magnitude': 12.00195026397705}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.265072345733643, 'force': [-6.051389694213867, -3.277486562728882, -3.359344244003296], 'magnitude': 7.658095359802246}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.079097270965576, 'force': [-3.255194902420044, -3.7537269592285156, -2.115217447280884], 'magnitude': 5.400083541870117}]}, 6167: {'frame': 6167, 'ionic_force': [1.0688188672065735, 1.0091578364372253, -11.419165134429932], 'ionic_force_magnitude': 11.513388105901736, 'motion_vector': [-0.13602447509765625, -1.4195594787597656, 3.152008056640625], 'ionic_force_x': 1.0688188672065735, 'ionic_force_y': 1.0091578364372253, 'ionic_force_z': -11.419165134429932, 'radial_force': 1.4699569074430054, 'axial_force': -11.419165134429932, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-0.5007350444793701, 1.4731664657592773, 0.6470582485198975], 'asn_force_magnitude': 1.6851229621558999, 'residue_force': [-0.5007350444793701, 1.4731664657592773, 0.6470582485198975], 'residue_force_magnitude': 1.6851229621558999, 'total_force': [0.5680838227272034, 2.4823243021965027, -10.772106885910034], 'total_force_magnitude': 11.06900808258762, 'motion_component_total': -10.855269310537563, 'cosine_total_motion': -0.9806903409541923, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.002812700470559097, 'cosine_residue_motion': 0.002812700470559097, 'cosine_ionic_motion': -0.9432504973161943, 'motion_component_glu': None, 'motion_component_asn': 0.004739746148605839, 'motion_component_residue': 0.004739746148605839, 'motion_component_ionic': -10.860009056686168, 'ionic_contributions': [{'ion_id': 1327, 'distance': 12.285541534423828, 'force': [0.37463992834091187, -0.28571516275405884, -2.148576259613037], 'magnitude': 2.199629068374634}, {'ion_id': 1355, 'distance': 12.605382919311523, 'force': [-0.322290301322937, -1.734464168548584, -1.1195731163024902], 'magnitude': 2.089421033859253}, {'ion_id': 1380, 'distance': 9.691065788269043, 'force': [2.3296315670013428, 1.3743340969085693, -2.2760865688323975], 'magnitude': 3.535045623779297}, {'ion_id': 1476, 'distance': 7.381692886352539, 'force': [-3.17857027053833, 2.7836079597473145, -4.389988899230957], 'magnitude': 6.092929363250732}, {'ion_id': 2443, 'distance': 11.218620300292969, 'force': [1.865407943725586, -1.1286048889160156, -1.4849402904510498], 'magnitude': 2.6379051208496094}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.799045562744141, 'force': [-2.612501859664917, 5.787351608276367, -3.0380492210388184], 'magnitude': 7.039058685302734}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.70307731628418, 'force': [2.111766815185547, -4.31418514251709, 3.685107469558716], 'magnitude': 6.054070472717285}]}, 6168: {'frame': 6168, 'ionic_force': [-7.520926967263222, 6.472836136817932, -23.5761159658432], 'ionic_force_magnitude': 25.579194556042808, 'motion_vector': [-0.9997520446777344, 3.4777908325195312, -1.7257232666015625], 'ionic_force_x': -7.520926967263222, 'ionic_force_y': 6.472836136817932, 'ionic_force_z': -23.5761159658432, 'radial_force': 9.922799509261651, 'axial_force': -23.5761159658432, 'glu_force': [4.036025524139404, -6.077040672302246, 2.879143238067627], 'glu_force_magnitude': 7.842792305654347, 'asn_force': [10.653934240341187, -4.135525226593018, 1.371400237083435], 'asn_force_magnitude': 11.510413646241132, 'residue_force': [14.68995976448059, -10.212565898895264, 4.250543475151062], 'residue_force_magnitude': 18.389087523732282, 'total_force': [7.169032797217369, -3.7397297620773315, -19.32557249069214], 'total_force_magnitude': 20.948946561436976, 'motion_component_total': 3.2868800400238314, 'cosine_total_motion': 0.15689953814070784, 'cosine_glu_motion': -0.9585269572055755, 'cosine_asn_motion': -0.593776284742608, 'cosine_residue_motion': -0.7804704000091083, 'cosine_ionic_motion': 0.6895845956692425, 'motion_component_glu': -7.517527844734161, 'motion_component_asn': -6.834610650715675, 'motion_component_residue': -14.352138495449836, 'motion_component_ionic': 17.639018535473667, 'ionic_contributions': [{'ion_id': 1327, 'distance': 8.464936256408691, 'force': [1.1435531377792358, -1.7503900527954102, -4.134721279144287], 'magnitude': 4.633303165435791}, {'ion_id': 1341, 'distance': 14.111098289489746, 'force': [0.19866521656513214, -0.4084584712982178, -1.6042498350143433], 'magnitude': 1.667310357093811}, {'ion_id': 1355, 'distance': 12.560206413269043, 'force': [-0.2531542479991913, -2.0059866905212402, -0.5837475061416626], 'magnitude': 2.104478597640991}, {'ion_id': 1380, 'distance': 7.985230922698975, 'force': [4.757066249847412, 1.4454026222229004, -1.5462619066238403], 'magnitude': 5.206706523895264}, {'ion_id': 1476, 'distance': 3.702267646789551, 'force': [-15.625587463378906, 11.02933120727539, -14.86202335357666], 'magnitude': 24.22157859802246}, {'ion_id': 2443, 'distance': 10.465030670166016, 'force': [2.2585301399230957, -1.8370624780654907, -0.8451120853424072], 'magnitude': 3.031496524810791}], 'glu_contributions': [{'resid': 748, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 5.887387275695801, 'force': [4.036025524139404, -6.077040672302246, 2.879143238067627], 'magnitude': 7.842792510986328}], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.675126552581787, 'force': [-11.261908531188965, 12.583945274353027, 4.687719821929932], 'magnitude': 17.52600860595703}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.862881898880005, 'force': [19.568429946899414, -13.747295379638672, -2.2973248958587646], 'magnitude': 24.024763107299805}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.6068854331970215, 'force': [7.704651832580566, -12.040438652038574, -1.5431114435195923], 'magnitude': 14.37758731842041}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.917903423309326, 'force': [-3.1650025844573975, 4.7818498611450195, -0.5412113666534424], 'magnitude': 5.759881973266602}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.315228462219238, 'force': [-2.1922364234924316, 4.286413669586182, 1.0653281211853027], 'magnitude': 4.930939674377441}]}, 6169: {'frame': 6169, 'ionic_force': [3.391502261161804, 2.702711671590805, -11.971076011657715], 'ionic_force_magnitude': 12.732383863366104, 'motion_vector': [0.38364410400390625, 1.7301025390625, 2.6249771118164062], 'ionic_force_x': 3.391502261161804, 'ionic_force_y': 2.702711671590805, 'ionic_force_z': -11.971076011657715, 'radial_force': 4.336696665345501, 'axial_force': -11.971076011657715, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-5.452151775360107, -3.9008262157440186, 0.9572838507592678], 'asn_force_magnitude': 6.771912323555486, 'residue_force': [-5.452151775360107, -3.9008262157440186, 0.9572838507592678], 'residue_force_magnitude': 6.771912323555486, 'total_force': [-2.0606495141983032, -1.1981145441532135, -11.013792160898447], 'total_force_magnitude': 11.268778666951679, 'motion_component_total': -10.03242788635822, 'cosine_total_motion': -0.8902852902578213, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.2950267622208909, 'cosine_residue_motion': -0.2950267622208909, 'cosine_ionic_motion': -0.63103128257176, 'motion_component_glu': None, 'motion_component_asn': -1.9978953668623254, 'motion_component_residue': -1.9978953668623254, 'motion_component_ionic': -8.034532519495894, 'ionic_contributions': [{'ion_id': 1327, 'distance': 8.871306419372559, 'force': [0.43922919034957886, 0.3048649728298187, -4.18452787399292], 'magnitude': 4.2185468673706055}, {'ion_id': 1355, 'distance': 9.382793426513672, 'force': [-1.1267592906951904, -3.0149948596954346, -1.965143084526062], 'magnitude': 3.7711493968963623}, {'ion_id': 1380, 'distance': 9.77778434753418, 'force': [1.8862299919128418, 2.4746272563934326, -1.5418955087661743], 'magnitude': 3.4726195335388184}, {'ion_id': 1476, 'distance': 8.223102569580078, 'force': [-0.951141893863678, 4.275298595428467, -2.218920946121216], 'magnitude': 4.909832954406738}, {'ion_id': 2443, 'distance': 9.122114181518555, 'force': [3.143944263458252, -1.3370842933654785, -2.0605885982513428], 'magnitude': 3.989762544631958}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.995276927947998, 'force': [-6.935718059539795, 4.872714996337891, 0.47344037890434265], 'magnitude': 8.489503860473633}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.97440242767334, 'force': [2.9724650382995605, -2.392317056655884, -0.8207941651344299], 'magnitude': 3.9028749465942383}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.421607971191406, 'force': [4.215058326721191, -2.1664304733276367, -0.033939991146326065], 'magnitude': 4.7393341064453125}, {'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.920722961425781, 'force': [-5.378741264343262, -4.046887397766113, 0.5393877029418945], 'magnitude': 6.752710342407227}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.9423394203186035, 'force': [9.104782104492188, 8.14169979095459, -2.6207685470581055], 'magnitude': 12.492108345031738}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.236535549163818, 'force': [-6.2823357582092285, -4.082765579223633, 2.0262975692749023], 'magnitude': 7.761610507965088}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.055199146270752, 'force': [-3.1476621627807617, -4.226840496063232, 1.3936609029769897], 'magnitude': 5.451261043548584}]}, 6170: {'frame': 6170, 'ionic_force': [5.667690142989159, 1.7710587978363037, -13.184255957603455], 'ionic_force_magnitude': 14.459736027256238, 'motion_vector': [3.7403221130371094, -1.5651435852050781, 1.4440078735351562], 'ionic_force_x': 5.667690142989159, 'ionic_force_y': 1.7710587978363037, 'ionic_force_z': -13.184255957603455, 'radial_force': 5.9379593146408345, 'axial_force': -13.184255957603455, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.2521066665649414, -1.8338649272918701, 3.0910134315490723], 'asn_force_magnitude': 3.6029130404291574, 'residue_force': [0.2521066665649414, -1.8338649272918701, 3.0910134315490723], 'residue_force_magnitude': 3.6029130404291574, 'total_force': [5.9197968095541, -0.0628061294555664, -10.093242526054382], 'total_force_magnitude': 11.701345374189104, 'motion_component_total': 1.78100339325177, 'cosine_total_motion': 0.15220501030422687, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.533733655568447, 'cosine_residue_motion': 0.533733655568447, 'cosine_ionic_motion': -0.009819858000454493, 'motion_component_glu': None, 'motion_component_asn': 1.9229959477634821, 'motion_component_residue': 1.9229959477634821, 'motion_component_ionic': -0.14199255451171222, 'ionic_contributions': [{'ion_id': 1327, 'distance': 7.1115241050720215, 'force': [1.4770755767822266, 2.068378448486328, -6.052678108215332], 'magnitude': 6.564666748046875}, {'ion_id': 1341, 'distance': 12.754508018493652, 'force': [0.2155987173318863, 0.3436358571052551, -2.0001230239868164], 'magnitude': 2.0408480167388916}, {'ion_id': 1355, 'distance': 6.782222270965576, 'force': [-2.284257650375366, -6.364039421081543, -2.5249183177948], 'magnitude': 7.217620372772217}, {'ion_id': 1380, 'distance': 10.311996459960938, 'force': [1.8270621299743652, 2.4519355297088623, -0.6305731534957886], 'magnitude': 3.1221413612365723}, {'ion_id': 1476, 'distance': 8.861822128295898, 'force': [-0.3435497581958771, 4.183430194854736, -0.503319263458252], 'magnitude': 4.22758150100708}, {'ion_id': 2443, 'distance': 8.084012031555176, 'force': [4.775761127471924, -0.9122818112373352, -1.4726440906524658], 'magnitude': 5.080239295959473}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.851452827453613, 'force': [-7.37550687789917, -3.1824967861175537, 6.051785469055176], 'magnitude': 10.057360649108887}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.4596381187438965, 'force': [5.479697227478027, 0.9727195501327515, -3.5589194297790527], 'magnitude': 6.605995178222656}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.063913345336914, 'force': [10.63857364654541, 5.091320037841797, -14.222100257873535], 'magnitude': 18.476171493530273}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.9458069801330566, 'force': [-4.660987377166748, -0.4075368642807007, 7.626725673675537], 'magnitude': 8.947504043579102}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 3.8874897956848145, 'force': [-3.829669952392578, -4.307870864868164, 7.193521976470947], 'magnitude': 9.217965126037598}]}, 6171: {'frame': 6171, 'ionic_force': [10.627623319625854, -0.529610387980938, -5.966325297951698], 'ionic_force_magnitude': 12.19934023412295, 'motion_vector': [-1.0708656311035156, 1.0283088684082031, -2.1849288940429688], 'ionic_force_x': 10.627623319625854, 'ionic_force_y': -0.529610387980938, 'ionic_force_z': -5.966325297951698, 'radial_force': 10.640811274847072, 'axial_force': -5.966325297951698, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [1.794920027256012, 3.4204158782958984, -4.735507488250732], 'asn_force_magnitude': 6.111138507350507, 'residue_force': [1.794920027256012, 3.4204158782958984, -4.735507488250732], 'residue_force_magnitude': 6.111138507350507, 'total_force': [12.422543346881866, 2.8908054903149605, -10.70183278620243], 'total_force_magnitude': 16.649491420816172, 'motion_component_total': 4.9411249540291715, 'cosine_total_motion': 0.29677332653245414, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.7397451597167899, 'cosine_residue_motion': 0.7397451597167899, 'cosine_ionic_motion': 0.034464144354440354, 'motion_component_glu': None, 'motion_component_asn': 4.520685131171426, 'motion_component_residue': 4.520685131171426, 'motion_component_ionic': 0.4204398228577455, 'ionic_contribut</t>
+          <t>{6161: {'frame': 6161, 'motion_vector': [4.460853576660156, 2.02520751953125, 0.9477462768554688], 'ionic_force': [2.045816570520401, 2.513314615935087, -12.963244438171387], 'ionic_force_magnitude': 13.362178795491031, 'radial_force': 3.2406968076154223, 'axial_force': -12.963244438171387, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [5.636149525642395, -11.620142102241516, 1.9752273261547089], 'asn_force_magnitude': 13.06504523305117, 'residue_force': [5.636149525642395, -11.620142102241516, 1.9752273261547089], 'residue_force_magnitude': 13.06504523305117, 'total_force': [7.681966096162796, -9.106827486306429, -10.988017112016678], 'total_force_magnitude': 16.20751153082768, 'cosine_total_motion': 0.0669076673000275, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.05339305783568137, 'cosine_residue_motion': 0.05339305783568137, 'cosine_ionic_motion': 0.028949176585065187, 'motion_component_total': 1.0844067892659779, 'motion_component_glu': None, 'motion_component_asn': 0.6975827157540944, 'motion_component_residue': 0.6975827157540944, 'motion_component_ionic': 0.3868240735118835, 'motion_component_percent_total': 6.690766730002751, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 5.339305783568137, 'motion_component_percent_residue': 5.339305783568137, 'motion_component_percent_ionic': 2.8949176585065186, 'ionic_contributions': [{'ion_id': 1327, 'distance': 9.253506660461426, 'force': [0.9507448077201843, 0.019289210438728333, -3.7588417530059814], 'magnitude': 3.8772642612457275, 'cosine_ionic_motion': 0.037099648267030716, 'motion_component_ionic': 0.14384514093399048, 'motion_component_percent_ionic': 3.7099648267030716}, {'ion_id': 1341, 'distance': 14.722437858581543, 'force': [0.26577094197273254, -0.029373470693826675, -1.5081979036331177], 'magnitude': 1.531717300415039, 'cosine_ionic_motion': -0.03968436270952225, 'motion_component_ionic': -0.06078522279858589, 'motion_component_percent_ionic': 3.9684362709522247}, {'ion_id': 1355, 'distance': 9.555658340454102, 'force': [-0.5799313187599182, -3.2436165809631348, -1.537106990814209], 'magnitude': 3.6359410285949707, 'cosine_ionic_motion': -0.5849542617797852, 'motion_component_ionic': -2.126859188079834, 'motion_component_percent_ionic': 58.495426177978516}, {'ion_id': 1380, 'distance': 10.345450401306152, 'force': [2.139223337173462, 1.9624422788619995, -1.0930858850479126], 'magnitude': 3.1019821166992188, 'cosine_ionic_motion': 0.8063527941703796, 'motion_component_ionic': 2.5012919902801514, 'motion_component_percent_ionic': 80.63527941703796}, {'ion_id': 1476, 'distance': 6.429809093475342, 'force': [-4.092360019683838, 5.589524745941162, -4.061839580535889], 'magnitude': 8.030488014221191, 'cosine_ionic_motion': -0.26914769411087036, 'motion_component_ionic': -2.1613874435424805, 'motion_component_percent_ionic': 26.914769411087036}, {'ion_id': 2443, 'distance': 9.1830415725708, 'force': [3.3623688220977783, -1.7849515676498413, -1.0041723251342773], 'magnitude': 3.9369959831237793, 'cosine_ionic_motion': 0.5310443043708801, 'motion_component_ionic': 2.090719223022461, 'motion_component_percent_ionic': 53.10443043708801}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.937707424163818, 'force': [3.445258140563965, -1.7017422914505005, 0.92019122838974], 'magnitude': 3.951263427734375, 'cosine_with_motion': 0.648930013179779, 'motion_component': 2.5640933513641357, 'motion_component_percent': 64.8930013179779}, {'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.288460731506348, 'force': [-5.059122085571289, -6.626802921295166, 1.4587273597717285], 'magnitude': 8.463871002197266, 'cosine_with_motion': -0.8193965554237366, 'motion_component': -6.935266971588135, 'motion_component_percent': 81.93965554237366}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.338872909545898, 'force': [5.106224060058594, 4.332803249359131, -1.69615638256073], 'magnitude': 6.908230781555176, 'cosine_with_motion': 0.8687071800231934, 'motion_component': 6.001229763031006, 'motion_component_percent': 86.87071800231934}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.25961446762085, 'force': [7.841231346130371, 14.6804780960083, -2.4135947227478027], 'magnitude': 16.817455291748047, 'cosine_with_motion': 0.7438547611236572, 'motion_component': 12.509744644165039, 'motion_component_percent': 74.38547611236572}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.332993984222412, 'force': [-6.791555881500244, -10.254345893859863, 2.445364475250244], 'magnitude': 12.540201187133789, 'cosine_with_motion': -0.7790080904960632, 'motion_component': -9.76891803741455, 'motion_component_percent': 77.90080904960632}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.605200290679932, 'force': [-1.9009085893630981, -6.2771172523498535, 0.3627375066280365], 'magnitude': 6.568655490875244, 'cosine_with_motion': -0.6360704898834229, 'motion_component': -4.178127765655518, 'motion_component_percent': 63.607048988342285}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.476353645324707, 'force': [2.9950225353240967, -5.7734150886535645, 0.8979578614234924], 'magnitude': 6.565730094909668, 'cosine_with_motion': 0.0768883153796196, 'motion_component': 0.5048279166221619, 'motion_component_percent': 7.68883153796196}]}, 6162: {'frame': 6162, 'motion_vector': [-1.7015113830566406, -2.5169944763183594, 0.5141983032226562], 'ionic_force': [7.763323903083801, 2.8181435465812683, -6.318853139877319], 'ionic_force_magnitude': 10.398992070228124, 'radial_force': 8.259003031439688, 'axial_force': -6.318853139877319, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [2.2658984661102295, 6.250769853591919, -11.89534592628479], 'asn_force_magnitude': 13.627386922197314, 'residue_force': [2.2658984661102295, 6.250769853591919, -11.89534592628479], 'residue_force_magnitude': 13.627386922197314, 'total_force': [10.02922236919403, 9.068913400173187, -18.21419906616211], 'total_force_magnitude': 22.684522018600333, 'cosine_total_motion': -0.7046848648036964, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.6121600336023413, 'cosine_residue_motion': -0.6121600336023413, 'cosine_ionic_motion': -0.7350037045890127, 'motion_component_total': -15.98543933181385, 'motion_component_glu': None, 'motion_component_asn': -8.342141636204413, 'motion_component_residue': -8.342141636204413, 'motion_component_ionic': -7.643297695609437, 'motion_component_percent_total': 70.46848648036963, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 61.216003360234126, 'motion_component_percent_residue': 61.216003360234126, 'motion_component_percent_ionic': 73.50037045890126, 'ionic_contributions': [{'ion_id': 1327, 'distance': 10.584158897399902, 'force': [1.9486887454986572, 0.7575831413269043, -2.100437641143799], 'magnitude': 2.963639259338379, 'cosine_ionic_motion': -0.6901615858078003, 'motion_component_ionic': -2.0453898906707764, 'motion_component_percent_ionic': 69.01615858078003}, {'ion_id': 1355, 'distance': 8.435245513916016, 'force': [1.829471230506897, -3.8013644218444824, -1.9934921264648438], 'magnitude': 4.665977478027344, 'cosine_ionic_motion': 0.377678245306015, 'motion_component_ionic': 1.7622381448745728, 'motion_component_percent_ionic': 37.7678245306015}, {'ion_id': 1380, 'distance': 14.387797355651855, 'force': [1.3906784057617188, 0.7438085079193115, -0.29142385721206665], 'magnitude': 1.603797197341919, 'cosine_ionic_motion': -0.887974739074707, 'motion_component_ionic': -1.4241313934326172, 'motion_component_percent_ionic': 88.7974739074707}, {'ion_id': 1476, 'distance': 7.511940956115723, 'force': [0.6493955850601196, 5.551018238067627, -1.8384053707122803], 'magnitude': 5.883472919464111, 'cosine_ionic_motion': -0.8837793469429016, 'motion_component_ionic': -5.1996917724609375, 'motion_component_percent_ionic': 88.37793469429016}, {'ion_id': 2443, 'distance': 12.900399208068848, 'force': [1.9450899362564087, -0.43290191888809204, -0.09509414434432983], 'magnitude': 1.9949489831924438, 'cosine_ionic_motion': -0.36909356713294983, 'motion_component_ionic': -0.736322820186615, 'motion_component_percent_ionic': 36.90935671329498}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.1263973712921143, 'force': [8.836230278015137, -18.055543899536133, 13.506759643554688], 'magnitude': 24.218053817749023, 'cosine_with_motion': 0.5005841851234436, 'motion_component': 12.123174667358398, 'motion_component_percent': 50.05841851234436}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.620124578475952, 'force': [-2.554917097091675, 17.166858673095703, -22.835859298706055], 'magnitude': 28.682836532592773, 'cosine_with_motion': -0.5725564360618591, 'motion_component': -16.422542572021484, 'motion_component_percent': 57.25564360618591}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.2906246185302734, 'force': [-19.775497436523438, 15.2301025390625, -13.08043384552002], 'magnitude': 28.180208206176758, 'cosine_with_motion': -0.1314215064048767, 'motion_component': -3.7034854888916016, 'motion_component_percent': 13.142150640487671}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.2818853855133057, 'force': [9.693719863891602, -3.504816770553589, 7.812277793884277], 'magnitude': 12.933816909790039, 'cosine_with_motion': -0.09171803295612335, 'motion_component': -1.1862642765045166, 'motion_component_percent': 9.171803295612335}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.154703140258789, 'force': [6.0663628578186035, -4.5858306884765625, 2.7019097805023193], 'magnitude': 8.070372581481934, 'cosine_with_motion': 0.10494884848594666, 'motion_component': 0.8469762802124023, 'motion_component_percent': 10.494884848594666}]}, 6163: {'frame': 6163, 'motion_vector': [-5.470054626464844, -0.9522628784179688, -5.482391357421875], 'ionic_force': [5.693150162696838, 11.41169948130846, -10.106098487973213], 'ionic_force_magnitude': 16.271818290385536, 'radial_force': 12.752993524138198, 'axial_force': -10.106098487973213, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [1.3283605575561523, 1.9260282516479492, -3.0279898643493652], 'asn_force_magnitude': 3.8265976030436537, 'residue_force': [1.3283605575561523, 1.9260282516479492, -3.0279898643493652], 'residue_force_magnitude': 3.8265976030436537, 'total_force': [7.021510720252991, 13.33772773295641, -13.134088352322578], 'total_force_magnitude': 19.99252036937109, 'cosine_total_motion': 0.1339567284314522, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.25119619538697685, 'cosine_residue_motion': 0.25119619538697685, 'cosine_ionic_motion': 0.10551407543882721, 'motion_component_total': 2.6781326217801196, 'motion_component_glu': None, 'motion_component_asn': 0.9612267591614909, 'motion_component_residue': 0.9612267591614909, 'motion_component_ionic': 1.7169058626186278, 'motion_component_percent_total': 13.39567284314522, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 25.119619538697684, 'motion_component_percent_residue': 25.119619538697684, 'motion_component_percent_ionic': 10.551407543882721, 'ionic_contributions': [{'ion_id': 1327, 'distance': 8.839310646057129, 'force': [2.395063638687134, 0.08514890819787979, -3.508793830871582], 'magnitude': 4.249142646789551, 'cosine_ionic_motion': 0.18260499835014343, 'motion_component_ionic': 0.7759146690368652, 'motion_component_percent_ionic': 18.260499835014343}, {'ion_id': 1341, 'distance': 13.962050437927246, 'force': [0.5789742469787598, -0.06532517075538635, -1.6003326177597046], 'magnitude': 1.7030980587005615, 'cosine_ionic_motion': 0.42657893896102905, 'motion_component_ionic': 0.7265057563781738, 'motion_component_percent_ionic': 42.657893896102905}, {'ion_id': 1355, 'distance': 9.791486740112305, 'force': [0.5200189352035522, -3.328923225402832, -0.7997344136238098], 'magnitude': 3.462907075881958, 'cosine_ionic_motion': 0.17430876195430756, 'motion_component_ionic': 0.6036150455474854, 'motion_component_percent_ionic': 17.430876195430756}, {'ion_id': 1380, 'distance': 11.607020378112793, 'force': [2.3475747108459473, 0.65799880027771, -0.3588736653327942], 'magnitude': 2.4643173217773438, 'cosine_ionic_motion': -0.5980862975120544, 'motion_component_ionic': -1.4738744497299194, 'motion_component_percent_ionic': 59.808629751205444}, {'ion_id': 1476, 'distance': 4.583294868469238, 'force': [-2.214129686355591, 15.15945053100586, -3.8823859691619873], 'magnitude': 15.804563522338867, 'cosine_ionic_motion': 0.15374812483787537, 'motion_component_ionic': 2.429922103881836, 'motion_component_percent_ionic': 15.374812483787537}, {'ion_id': 2443, 'distance': 11.913593292236328, 'force': [2.065648317337036, -1.0966503620147705, 0.044022008776664734], 'magnitude': 2.3391201496124268, 'cosine_ionic_motion': -0.5750783085823059, 'motion_component_ionic': -1.3451772928237915, 'motion_component_percent_ionic': 57.50783085823059}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.494832992553711, 'force': [-1.025095820426941, -6.225288391113281, 4.654168128967285], 'magnitude': 7.840045928955078, 'cosine_with_motion': -0.22853367030620575, 'motion_component': -1.7917144298553467, 'motion_component_percent': 22.853367030620575}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.997812747955322, 'force': [2.575059652328491, 5.630373001098633, -4.879940032958984], 'magnitude': 7.88326358795166, 'cosine_with_motion': 0.11878027021884918, 'motion_component': 0.93637615442276, 'motion_component_percent': 11.878027021884918}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.319039344787598, 'force': [-1.1120789051055908, 8.198407173156738, -6.919050693511963], 'magnitude': 10.785354614257812, 'cosine_with_motion': 0.43025678396224976, 'motion_component': 4.640471935272217, 'motion_component_percent': 43.025678396224976}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.033473014831543, 'force': [0.680869460105896, -3.440354824066162, 4.234739780426025], 'magnitude': 5.498422145843506, 'cosine_with_motion': -0.551581084728241, 'motion_component': -3.0328257083892822, 'motion_component_percent': 55.1581084728241}, {'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.729037761688232, 'force': [0.7276909351348877, 6.655938625335693, 2.680285930633545], 'magnitude': 7.212141513824463, 'cosine_with_motion': -0.444475919008255, 'motion_component': -3.205623149871826, 'motion_component_percent': 44.4475919008255}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.59222412109375, 'force': [-0.5180847644805908, -8.893047332763672, -2.7981929779052734], 'magnitude': 9.337268829345703, 'cosine_with_motion': 0.36568963527679443, 'motion_component': 3.4145424365997314, 'motion_component_percent': 36.56896352767944}]}, 6164: {'frame': 6164, 'motion_vector': [0.8026161193847656, -1.9557952880859375, 2.9555435180664062], 'ionic_force': [0.7338058315217495, -0.6169207841157913, -9.97306752204895], 'ionic_force_magnitude': 10.019038778824891, 'radial_force': 0.9586773452258945, 'axial_force': -9.97306752204895, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [0.0, 0.0, 0.0], 'residue_force_magnitude': 0.0, 'total_force': [0.7338058315217495, -0.6169207841157913, -9.97306752204895], 'total_force_magnitude': 10.019038778824891, 'cosine_total_motion': -0.7602959797943335, 'cosine_glu_motion': None, 'cosine_asn_motion': None, 'cosine_residue_motion': None, 'cosine_ionic_motion': -0.7602959797943335, 'motion_component_total': -7.617434904944093, 'motion_component_glu': None, 'motion_component_asn': None, 'motion_component_residue': None, 'motion_component_ionic': -7.617434904944093, 'motion_component_percent_total': 76.02959797943335, 'motion_component_percent_glu': None, 'motion_component_percent_asn': None, 'motion_component_percent_residue': None, 'motion_component_percent_ionic': 76.02959797943335, 'ionic_contributions': [{'ion_id': 1327, 'distance': 13.327520370483398, 'force': [-0.05467653647065163, -0.15348537266254425, -1.8620142936706543], 'magnitude': 1.8691293001174927, 'cosine_ionic_motion': -0.7725144028663635, 'motion_component_ionic': -1.4439293146133423, 'motion_component_percent_ionic': 77.25144028663635}, {'ion_id': 1355, 'distance': 13.564136505126953, 'force': [-0.5475013852119446, -1.3620316982269287, -1.0494215488433838], 'magnitude': 1.8044871091842651, 'cosine_ionic_motion': -0.13377580046653748, 'motion_component_ionic': -0.2413966953754425, 'motion_component_percent_ionic': 13.377580046653748}, {'ion_id': 1380, 'distance': 9.610234260559082, 'force': [1.875036597251892, 1.458633303642273, -2.697950601577759], 'magnitude': 3.594761610031128, 'cosine_ionic_motion': -0.713618278503418, 'motion_component_ionic': -2.5652875900268555, 'motion_component_percent_ionic': 71.3618278503418}, {'ion_id': 1476, 'distance': 9.47956657409668, 'force': [-2.0720303058624268, 1.2611353397369385, -2.7867367267608643], 'magnitude': 3.6945464611053467, 'cosine_ionic_motion': -0.9210902452468872, 'motion_component_ionic': -3.403010606765747, 'motion_component_percent_ionic': 92.10902452468872}, {'ion_id': 2443, 'distance': 10.782855987548828, 'force': [1.5329774618148804, -1.8211723566055298, -1.576944351196289], 'magnitude': 2.8554232120513916, 'cosine_ionic_motion': 0.01267388928681612, 'motion_component_ionic': 0.03618931770324707, 'motion_component_percent_ionic': 1.267388928681612}], 'glu_contributions': [], 'asn_contributions': []}, 6165: {'frame': 6165, 'motion_vector': [-0.4117393493652344, 4.247417449951172, -2.2331161499023438], 'ionic_force': [0.8527390398085117, -2.051217794418335, -13.607491910457611], 'ionic_force_magnitude': 13.78762105670595, 'radial_force': 2.221409082126019, 'axial_force': -13.607491910457611, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [2.341707944869995, -0.19888710975646973, 2.5418634712696075], 'asn_force_magnitude': 3.4618235206418766, 'residue_force': [2.341707944869995, -0.19888710975646973, 2.5418634712696075], 'residue_force_magnitude': 3.4618235206418766, 'total_force': [3.194446984678507, -2.2501049041748047, -11.065628439188004], 'total_force_magnitude': 11.735228858947723, 'cosine_total_motion': 0.24483868619549415, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.4489355041013871, 'cosine_residue_motion': -0.4489355041013871, 'cosine_ionic_motion': 0.3211122125541915, 'motion_component_total': 2.8732380160282083, 'motion_component_glu': None, 'motion_component_asn': -1.5541354873493995, 'motion_component_residue': -1.5541354873493995, 'motion_component_ionic': 4.427373503377607, 'motion_component_percent_total': 24.483868619549416, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 44.89355041013871, 'motion_component_percent_residue': 44.89355041013871, 'motion_component_percent_ionic': 32.111221255419146, 'ionic_contributions': [{'ion_id': 1327, 'distance': 11.319201469421387, 'force': [0.062102917581796646, -0.7361721992492676, -2.4836835861206055], 'magnitude': 2.591233491897583, 'cosine_ionic_motion': 0.1918201744556427, 'motion_component_ionic': 0.49705085158348083, 'motion_component_percent_ionic': 19.18201744556427}, {'ion_id': 1355, 'distance': 13.651247024536133, 'force': [-0.45634692907333374, -1.6045798063278198, -0.6252397894859314], 'magnitude': 1.7815312147140503, 'cosine_ionic_motion': -0.6096663475036621, 'motion_component_ionic': -1.0861396789550781, 'motion_component_percent_ionic': 60.96663475036621}, {'ion_id': 1380, 'distance': 7.018681526184082, 'force': [4.697567462921143, 1.9251720905303955, -4.4325270652771], 'magnitude': 6.739490032196045, 'cosine_ionic_motion': 0.4972713589668274, 'motion_component_ionic': 3.3513553142547607, 'motion_component_percent_ionic': 49.72713589668274}, {'ion_id': 1476, 'distance': 6.703571796417236, 'force': [-5.758725166320801, 1.1061946153640747, -4.493953704833984], 'magnitude': 7.38797664642334, 'cosine_ionic_motion': 0.48071181774139404, 'motion_component_ionic': 3.551487684249878, 'motion_component_percent_ionic': 48.071181774139404}, {'ion_id': 2443, 'distance': 9.210395812988281, 'force': [2.308140754699707, -2.7418324947357178, -1.5720877647399902], 'magnitude': 3.9136452674865723, 'cosine_ionic_motion': -0.48200100660324097, 'motion_component_ionic': -1.886380910873413, 'motion_component_percent_ionic': 48.2001006603241}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.529760837554932, 'force': [-10.259325981140137, 4.805561065673828, -2.178412437438965], 'magnitude': 11.536579132080078, 'cosine_with_motion': 0.5309219360351562, 'motion_component': 6.125022888183594, 'motion_component_percent': 53.092193603515625}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.9075493812561035, 'force': [7.5509419441223145, -1.7516062259674072, 2.6001579761505127], 'magnitude': 8.175920486450195, 'cosine_with_motion': -0.4153425097465515, 'motion_component': -3.3958072662353516, 'motion_component_percent': 41.53425097465515}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.285310745239258, 'force': [8.399792671203613, -6.517972469329834, 2.5062448978424072], 'magnitude': 10.923449516296387, 'cosine_with_motion': -0.6983324289321899, 'motion_component': -7.628199100494385, 'motion_component_percent': 69.833242893219}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.447909355163574, 'force': [-3.349700689315796, 3.2651305198669434, -0.38612696528434753], 'magnitude': 4.693683624267578, 'cosine_with_motion': 0.7126275300979614, 'motion_component': 3.344848155975342, 'motion_component_percent': 71.26275300979614}]}, 6166: {'frame': 6166, 'motion_vector': [2.0425567626953125, -2.522167205810547, 0.7178115844726562], 'ionic_force': [1.4523009806871414, 1.297539383172989, -11.587992548942566], 'ionic_force_magnitude': 11.750504580814315, 'radial_force': 1.9475077893014379, 'axial_force': -11.587992548942566, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.6397826671600342, 0.49869585037231445, -0.6913818120956421], 'asn_force_magnitude': 1.0658462471077275, 'residue_force': [0.6397826671600342, 0.49869585037231445, -0.6913818120956421], 'residue_force_magnitude': 1.0658462471077275, 'total_force': [2.0920836478471756, 1.7962352335453033, -12.279374361038208], 'total_force_magnitude': 12.585162283512343, 'cosine_total_motion': -0.2168530198327206, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.12625091430709678, 'cosine_residue_motion': -0.12625091430709678, 'cosine_ionic_motion': -0.22080467823421474, 'motion_component_total': -2.7291304462645094, 'motion_component_glu': None, 'motion_component_asn': -0.1345640632081384, 'motion_component_residue': -0.1345640632081384, 'motion_component_ionic': -2.594566383056371, 'motion_component_percent_total': 21.68530198327206, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 12.625091430709679, 'motion_component_percent_residue': 12.625091430709679, 'motion_component_percent_ionic': 22.080467823421472, 'ionic_contributions': [{'ion_id': 1327, 'distance': 11.323769569396973, 'force': [0.08723576366901398, 0.26207712292671204, -2.5743675231933594], 'magnitude': 2.5891432762145996, 'cosine_ionic_motion': -0.27082061767578125, 'motion_component_ionic': -0.7011933922767639, 'motion_component_percent_ionic': 27.082061767578125}, {'ion_id': 1355, 'distance': 10.770421981811523, 'force': [-0.8347313404083252, -2.0121395587921143, -1.8562531471252441], 'magnitude': 2.8620200157165527, 'cosine_ionic_motion': 0.21417881548404694, 'motion_component_ionic': 0.6129840612411499, 'motion_component_percent_ionic': 21.417881548404694}, {'ion_id': 1380, 'distance': 10.39759635925293, 'force': [1.436957836151123, 2.019728899002075, -1.8128858804702759], 'magnitude': 3.0709457397460938, 'cosine_ionic_motion': -0.3389941155910492, 'motion_component_ionic': -1.0410325527191162, 'motion_component_percent_ionic': 33.89941155910492}, {'ion_id': 1476, 'distance': 9.792675018310547, 'force': [-1.8430176973342896, 1.9066798686981201, -2.2257046699523926], 'magnitude': 3.462066411972046, 'cosine_ionic_motion': -0.8838473558425903, 'motion_component_ionic': -3.0599381923675537, 'motion_component_percent_ionic': 88.38473558425903}, {'ion_id': 2443, 'distance': 8.935583114624023, 'force': [2.605856418609619, -0.8788069486618042, -3.118781328201294], 'magnitude': 4.158074855804443, 'cosine_ionic_motion': 0.38349810242652893, 'motion_component_ionic': 1.594613790512085, 'motion_component_percent_ionic': 38.34981024265289}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.566076755523682, 'force': [5.6690168380737305, -4.858895778656006, -1.622536301612854], 'magnitude': 7.640631198883057, 'cosine_with_motion': 0.8926060795783997, 'motion_component': 6.820074081420898, 'motion_component_percent': 89.26060795783997}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.915214538574219, 'force': [-3.328258514404297, 4.29303503036499, 1.470607876777649], 'magnitude': 5.627623081207275, 'cosine_with_motion': -0.8858314752578735, 'motion_component': -4.985125541687012, 'motion_component_percent': 88.58314752578735}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.352017402648926, 'force': [-8.489718437194824, 5.058170318603516, 3.977790117263794], 'magnitude': 10.652850151062012, 'cosine_with_motion': -0.7693691849708557, 'motion_component': -8.195974349975586, 'motion_component_percent': 76.93691849708557}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.660675525665283, 'force': [3.091325283050537, -2.0316126346588135, -2.2840301990509033], 'magnitude': 4.347474575042725, 'cosine_with_motion': 0.6780794262886047, 'motion_component': 2.9479329586029053, 'motion_component_percent': 67.80794262886047}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.47129487991333, 'force': [4.145976543426514, -1.5143561363220215, -1.4744571447372437], 'magnitude': 4.653645992279053, 'cosine_with_motion': 0.7259586453437805, 'motion_component': 3.378354549407959, 'motion_component_percent': 72.59586453437805}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.0422515869140625, 'force': [8.858025550842285, 6.583568572998047, 4.715805530548096], 'magnitude': 12.00195026397705, 'cosine_with_motion': 0.12215469032526016, 'motion_component': 1.4660944938659668, 'motion_component_percent': 12.215469032526016}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.265072345733643, 'force': [-6.051389694213867, -3.277486562728882, -3.359344244003296], 'magnitude': 7.658095359802246, 'cosine_with_motion': -0.25556036829948425, 'motion_component': -1.9571056365966797, 'motion_component_percent': 25.556036829948425}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.079097270965576, 'force': [-3.255194902420044, -3.7537269592285156, -2.115217447280884], 'magnitude': 5.400083541870117, 'cosine_with_motion': 0.07244061678647995, 'motion_component': 0.39118537306785583, 'motion_component_percent': 7.244061678647995}]}, 6167: {'frame': 6167, 'motion_vector': [-0.13602447509765625, -1.4195594787597656, 3.152008056640625], 'ionic_force': [1.0688188672065735, 1.0091578364372253, -11.419165134429932], 'ionic_force_magnitude': 11.513388105901736, 'radial_force': 1.4699569074430054, 'axial_force': -11.419165134429932, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-0.5007350444793701, 1.4731664657592773, 0.6470582485198975], 'asn_force_magnitude': 1.6851229621558999, 'residue_force': [-0.5007350444793701, 1.4731664657592773, 0.6470582485198975], 'residue_force_magnitude': 1.6851229621558999, 'total_force': [0.5680838227272034, 2.4823243021965027, -10.772106885910034], 'total_force_magnitude': 11.06900808258762, 'cosine_total_motion': -0.9806903409541923, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.002812700470559097, 'cosine_residue_motion': 0.002812700470559097, 'cosine_ionic_motion': -0.9432504973161943, 'motion_component_total': -10.855269310537563, 'motion_component_glu': None, 'motion_component_asn': 0.004739746148605839, 'motion_component_residue': 0.004739746148605839, 'motion_component_ionic': -10.860009056686168, 'motion_component_percent_total': 98.06903409541923, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 0.2812700470559097, 'motion_component_percent_residue': 0.2812700470559097, 'motion_component_percent_ionic': 94.32504973161943, 'ionic_contributions': [{'ion_id': 1327, 'distance': 12.285541534423828, 'force': [0.37463992834091187, -0.28571516275405884, -2.148576259613037], 'magnitude': 2.199629068374634, 'cosine_ionic_motion': -0.8433436155319214, 'motion_component_ionic': -1.8550431728363037, 'motion_component_percent_ionic': 84.33436155319214}, {'ion_id': 1355, 'distance': 12.605382919311523, 'force': [-0.322290301322937, -1.734464168548584, -1.1195731163024902], 'magnitude': 2.089421033859253, 'cosine_ionic_motion': -0.14150674641132355, 'motion_component_ionic': -0.2956671714782715, 'motion_component_percent_ionic': 14.150674641132355}, {'ion_id': 1380, 'distance': 9.691065788269043, 'force': [2.3296315670013428, 1.3743340969085693, -2.2760865688323975], 'magnitude': 3.535045623779297, 'cosine_ionic_motion': -0.7720531821250916, 'motion_component_ionic': -2.729243278503418, 'motion_component_percent_ionic': 77.20531821250916}, {'ion_id': 1476, 'distance': 7.381692886352539, 'force': [-3.17857027053833, 2.7836079597473145, -4.389988899230957], 'magnitude': 6.092929363250732, 'cosine_ionic_motion': -0.8233954310417175, 'motion_component_ionic': -5.016890048980713, 'motion_component_percent_ionic': 82.33954310417175}, {'ion_id': 2443, 'distance': 11.218620300292969, 'force': [1.865407943725586, -1.1286048889160156, -1.4849402904510498], 'magnitude': 2.6379051208496094, 'cosine_ionic_motion': -0.3651250898838043, 'motion_component_ionic': -0.9631653428077698, 'motion_component_percent_ionic': 36.51250898838043}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.799045562744141, 'force': [-2.612501859664917, 5.787351608276367, -3.0380492210388184], 'magnitude': 7.039058685302734, 'cosine_with_motion': -0.7159931659698486, 'motion_component': -5.039917945861816, 'motion_component_percent': 71.59931659698486}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.70307731628418, 'force': [2.111766815185547, -4.31418514251709, 3.685107469558716], 'magnitude': 6.054070472717285, 'cosine_with_motion': 0.833267092704773, 'motion_component': 5.0446577072143555, 'motion_component_percent': 83.3267092704773}]}, 6168: {'frame': 6168, 'motion_vector': [-0.9997520446777344, 3.4777908325195312, -1.7257232666015625], 'ionic_force': [-7.520926967263222, 6.472836136817932, -23.5761159658432], 'ionic_force_magnitude': 25.579194556042808, 'radial_force': 9.922799509261651, 'axial_force': -23.5761159658432, 'glu_force': [4.036025524139404, -6.077040672302246, 2.879143238067627], 'glu_force_magnitude': 7.842792305654347, 'asn_force': [10.653934240341187, -4.135525226593018, 1.371400237083435], 'asn_force_magnitude': 11.510413646241132, 'residue_force': [14.68995976448059, -10.212565898895264, 4.250543475151062], 'residue_force_magnitude': 18.389087523732282, 'total_force': [7.169032797217369, -3.7397297620773315, -19.32557249069214], 'total_force_magnitude': 20.948946561436976, 'cosine_total_motion': 0.15689953814070784, 'cosine_glu_motion': -0.9585269572055755, 'cosine_asn_motion': -0.593776284742608, 'cosine_residue_motion': -0.7804704000091083, 'cosine_ionic_motion': 0.6895845956692425, 'motion_component_total': 3.2868800400238314, 'motion_component_glu': -7.517527844734161, 'motion_component_asn': -6.8346106</t>
         </is>
       </c>
     </row>
@@ -803,7 +803,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>{6449: {'frame': 6449, 'ionic_force': [11.088144078850746, 3.661605954170227, -9.956974852830172], 'ionic_force_magnitude': 15.345867375188023, 'motion_vector': [4.9669189453125, 1.6391181945800781, 0.8033828735351562], 'ionic_force_x': 11.088144078850746, 'ionic_force_y': 3.661605954170227, 'ionic_force_z': -9.956974852830172, 'radial_force': 11.67708427977497, 'axial_force': -9.956974852830172, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [2.4526870250701904, 6.051830530166626, -0.10775279998779297], 'asn_force_magnitude': 6.530845050581872, 'residue_force': [2.4526870250701904, 6.051830530166626, -0.10775279998779297], 'residue_force_magnitude': 6.530845050581872, 'total_force': [13.540831103920937, 9.713436484336853, -10.064727652817965], 'total_force_magnitude': 19.468017311620553, 'motion_component_total': 14.190413742165958, 'cosine_total_motion': 0.728909036550714, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.6370292535217775, 'cosine_residue_motion': 0.6370292535217775, 'cosine_ionic_motion': 0.6536010086301492, 'motion_component_glu': None, 'motion_component_asn': 4.1603393474385655, 'motion_component_residue': 4.1603393474385655, 'motion_component_ionic': 10.030074394727393, 'ionic_contributions': [{'ion_id': 1327, 'distance': 8.776840209960938, 'force': [3.5316085815429688, 2.2948412895202637, -0.9144463539123535], 'magnitude': 4.309845447540283}, {'ion_id': 1330, 'distance': 7.018555641174316, 'force': [0.982691764831543, 1.5302084684371948, -6.489742279052734], 'magnitude': 6.739731311798096}, {'ion_id': 1355, 'distance': 7.212211608886719, 'force': [4.765550136566162, -4.245543003082275, 0.05606735870242119], 'magnitude': 6.3826518058776855}, {'ion_id': 1465, 'distance': 13.133724212646484, 'force': [0.14122642576694489, 0.30911684036254883, -1.894454836845398], 'magnitude': 1.924696683883667}, {'ion_id': 1476, 'distance': 8.905438423156738, 'force': [1.6670671701431274, 3.772982358932495, -0.7143987417221069], 'magnitude': 4.186272144317627}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.108480930328369, 'force': [-8.40830135345459, 6.2936530113220215, -5.1391825675964355], 'magnitude': 11.692767143249512}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.946959972381592, 'force': [4.270160675048828, -3.4683640003204346, 1.462803602218628], 'magnitude': 5.692417144775391}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.85023307800293, 'force': [4.502490520477295, -2.196474075317383, 3.157519578933716], 'magnitude': 5.921726703643799}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.804171562194824, 'force': [6.257778167724609, 3.50447678565979, -5.5318803787231445], 'magnitude': 9.057750701904297}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.483778953552246, 'force': [-3.3062853813171387, -1.051046371459961, 3.069798707962036], 'magnitude': 4.632481575012207}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.744706630706787, 'force': [-0.8631556034088135, 2.9695851802825928, 2.8731882572174072], 'magnitude': 4.221218109130859}]}, 6450: {'frame': 6450, 'ionic_force': [11.005028426647186, 3.282705068588257, -4.414879508316517], 'ionic_force_magnitude': 12.303575265409675, 'motion_vector': [1.8098068237304688, -1.3127899169921875, -0.8244171142578125], 'ionic_force_x': 11.005028426647186, 'ionic_force_y': 3.282705068588257, 'ionic_force_z': -4.414879508316517, 'radial_force': 11.484197979774107, 'axial_force': -4.414879508316517, 'glu_force': [3.1059458255767822, 8.62153148651123, 2.919323444366455], 'glu_force_magnitude': 9.617700037802697, 'asn_force': [6.720531940460205, 0.33734792470932007, -5.030340194702148], 'asn_force_magnitude': 8.401409147249499, 'residue_force': [9.826477766036987, 8.95887941122055, -2.1110167503356934], 'residue_force_magnitude': 13.463936174514814, 'total_force': [20.831506192684174, 12.241584479808807, -6.52589625865221], 'total_force_magnitude': 25.027891697280975, 'motion_component_total': 11.334841517085232, 'cosine_total_motion': 0.4528883876509921, 'cosine_glu_motion': -0.3535927756896398, 'cosine_asn_motion': 0.7925546217684223, 'cosine_residue_motion': 0.24196686278635599, 'cosine_ionic_motion': 0.6564770764551591, 'motion_component_glu': -3.4007492521170093, 'motion_component_asn': 6.65857564902009, 'motion_component_residue': 3.2578263969030807, 'motion_component_ionic': 8.077015120182152, 'ionic_contributions': [{'ion_id': 1327, 'distance': 13.44346809387207, 'force': [1.6276063919067383, 0.8470562100410461, -0.08977655321359634], 'magnitude': 1.8370264768600464}, {'ion_id': 1330, 'distance': 8.71585750579834, 'force': [3.048281192779541, 1.3634477853775024, -2.819413661956787], 'magnitude': 4.370366096496582}, {'ion_id': 1355, 'distance': 10.259184837341309, 'force': [2.8688948154449463, -1.2304490804672241, 0.45329388976097107], 'magnitude': 3.1543681621551514}, {'ion_id': 1465, 'distance': 13.79960823059082, 'force': [0.7390469908714294, 0.3952198624610901, -1.5287773609161377], 'magnitude': 1.7434303760528564}, {'ion_id': 1476, 'distance': 9.953839302062988, 'force': [2.7211990356445312, 1.9074302911758423, -0.4302058219909668], 'magnitude': 3.3508644104003906}], 'glu_contributions': [{'resid': 423, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 5.316457271575928, 'force': [3.1059458255767822, 8.62153148651123, 2.919323444366455], 'magnitude': 9.61769962310791}], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.4382638931274414, 'force': [-0.9484546184539795, -7.306424140930176, 18.619186401367188], 'magnitude': 20.023921966552734}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.1025466918945312, 'force': [7.568514347076416, 4.213474750518799, -18.53183364868164], 'magnitude': 20.45640754699707}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.579256534576416, 'force': [-6.583146095275879, 4.72232723236084, -22.398319244384766], 'magnitude': 23.818540573120117}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.5232129096984863, 'force': [3.385124683380127, 0.9476186633110046, 10.657909393310547], 'magnitude': 11.22265911102295}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.245125770568848, 'force': [3.2984936237335205, -2.2396485805511475, 6.622716903686523], 'magnitude': 7.730230331420898}]}, 6451: {'frame': 6451, 'ionic_force': [8.739684104919434, 0.469412237405777, -2.0718104019761086], 'ionic_force_magnitude': 8.994155015572286, 'motion_vector': [-1.5418739318847656, -2.056304931640625, -0.31626129150390625], 'ionic_force_x': 8.739684104919434, 'ionic_force_y': 0.469412237405777, 'ionic_force_z': -2.0718104019761086, 'radial_force': 8.75228119420347, 'axial_force': -2.0718104019761086, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [3.775687575340271, 6.209000110626221, -9.062820196151733], 'asn_force_magnitude': 11.616462841506921, 'residue_force': [3.775687575340271, 6.209000110626221, -9.062820196151733], 'residue_force_magnitude': 11.616462841506921, 'total_force': [12.515371680259705, 6.678412348031998, -11.134630598127842], 'total_force_magnitude': 18.033738335191558, 'motion_component_total': -11.395217466539313, 'cosine_total_motion': -0.6318832653960802, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.5226813089167416, 'cosine_residue_motion': -0.5226813089167416, 'cosine_ionic_motion': -0.5918854471977383, 'motion_component_glu': None, 'motion_component_asn': -6.071708002981529, 'motion_component_residue': -6.071708002981529, 'motion_component_ionic': -5.323509463557783, 'ionic_contributions': [{'ion_id': 1327, 'distance': 14.782349586486816, 'force': [1.4240713119506836, 0.4835692346096039, -0.21571895480155945], 'magnitude': 1.5193264484405518}, {'ion_id': 1330, 'distance': 10.166635513305664, 'force': [2.4229938983917236, 0.5128621459007263, -2.0453357696533203], 'magnitude': 3.212059259414673}, {'ion_id': 1355, 'distance': 10.030377388000488, 'force': [2.7083451747894287, -1.8824938535690308, -0.10277257114648819], 'magnitude': 3.2999210357666016}, {'ion_id': 1476, 'distance': 11.328006744384766, 'force': [2.1842737197875977, 1.3554747104644775, 0.2920168936252594], 'magnitude': 2.5872063636779785}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.6995091438293457, 'force': [5.416232585906982, -11.804396629333496, 11.422066688537598], 'magnitude': 17.29574966430664}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.8317983150482178, 'force': [-1.9182919263839722, 15.030738830566406, -19.322242736816406], 'magnitude': 24.555082321166992}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.0421013832092285, 'force': [-11.055981636047363, 9.408076286315918, -11.74948787689209], 'magnitude': 18.676109313964844}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.5425302982330322, 'force': [7.50039005279541, -3.2488973140716553, 7.510800838470459], 'magnitude': 11.10059928894043}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.8790106773376465, 'force': [3.833338499069214, -3.176521062850952, 3.076042890548706], 'magnitude': 5.852077484130859}]}, 6452: {'frame': 6452, 'ionic_force': [10.327910542488098, 1.1043216735124588, -5.13695291057229], 'ionic_force_magnitude': 11.58764634158565, 'motion_vector': [-0.060070037841796875, 3.2151107788085938, 1.4912796020507812], 'ionic_force_x': 10.327910542488098, 'ionic_force_y': 1.1043216735124588, 'ionic_force_z': -5.13695291057229, 'radial_force': 10.386783069469882, 'axial_force': -5.13695291057229, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [2.5758535265922546, -2.32772159576416, -1.2732272446155548], 'asn_force_magnitude': 3.6978935671914517, 'residue_force': [2.5758535265922546, -2.32772159576416, -1.2732272446155548], 'residue_force_magnitude': 3.6978935671914517, 'total_force': [12.903764069080353, -1.2233999222517014, -6.410180155187845], 'total_force_magnitude': 14.460091429248248, 'motion_component_total': -4.02519699738862, 'cosine_total_motion': -0.2783659437482466, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.7276147828058505, 'cosine_residue_motion': -0.7276147828058505, 'cosine_ionic_motion': -0.11517049565691527, 'motion_component_glu': None, 'motion_component_asn': -2.6906420247311598, 'motion_component_residue': -2.6906420247311598, 'motion_component_ionic': -1.3345549726574601, 'ionic_contributions': [{'ion_id': 1327, 'distance': 13.44875717163086, 'force': [1.7840296030044556, 0.277847021818161, -0.3307577669620514], 'magnitude': 1.8355820178985596}, {'ion_id': 1330, 'distance': 9.372391700744629, 'force': [2.474438190460205, -0.39485305547714233, -2.829497814178467], 'magnitude': 3.7795252799987793}, {'ion_id': 1355, 'distance': 11.513007164001465, 'force': [2.0291547775268555, -1.468042254447937, -0.032318416982889175], 'magnitude': 2.504727840423584}, {'ion_id': 1465, 'distance': 14.323189735412598, 'force': [0.6779139041900635, -0.06925506889820099, -1.4678304195404053], 'magnitude': 1.6182984113693237}, {'ion_id': 1476, 'distance': 8.711008071899414, 'force': [3.3623740673065186, 2.758625030517578, -0.4765484929084778], 'magnitude': 4.3752336502075195}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.110825061798096, 'force': [-0.39502090215682983, -8.049195289611816, 4.145165920257568], 'magnitude': 9.06244945526123}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.403731822967529, 'force': [2.482687473297119, 8.37047004699707, -5.183540344238281], 'magnitude': 10.153698921203613}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.945854663848877, 'force': [-2.5302085876464844, 10.595436096191406, -6.078184604644775], 'magnitude': 12.474355697631836}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.133551597595215, 'force': [2.389244794845581, -6.350554466247559, 4.520648002624512], 'magnitude': 8.153176307678223}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.617127418518066, 'force': [1.3637722730636597, -3.8248510360717773, 1.733247995376587], 'magnitude': 4.415145397186279}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.63272762298584, 'force': [-2.844557285308838, -9.159859657287598, -0.7087050080299377], 'magnitude': 9.617525100708008}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.64634895324707, 'force': [2.109935760498047, 6.090832710266113, 0.2981407940387726], 'magnitude': 6.452826023101807}]}, 6453: {'frame': 6453, 'ionic_force': [9.139528214931488, 2.8800260424613953, -3.7206843197345734], 'ionic_force_magnitude': 10.279543657376202, 'motion_vector': [-0.720062255859375, 0.6362991333007812, 0.15360260009765625], 'ionic_force_x': 9.139528214931488, 'ionic_force_y': 2.8800260424613953, 'ionic_force_z': -3.7206843197345734, 'radial_force': 9.582563644285624, 'axial_force': -3.7206843197345734, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [5.423488736152649, -1.7666098177433014, -5.046192169189453], 'asn_force_magnitude': 7.615720302618173, 'residue_force': [5.423488736152649, -1.7666098177433014, -5.046192169189453], 'residue_force_magnitude': 7.615720302618173, 'total_force': [14.563016951084137, 1.1134162247180939, -8.766876488924026], 'total_force_magnitude': 17.034649446909036, 'motion_component_total': -11.431727738411956, 'cosine_total_motion': -0.6710867619577732, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.7832209129157407, 'cosine_residue_motion': -0.7832209129157407, 'cosine_ionic_motion': -0.5318267534728109, 'motion_component_glu': None, 'motion_component_asn': -5.964791407927546, 'motion_component_residue': -5.964791407927546, 'motion_component_ionic': -5.46693633048441, 'ionic_contributions': [{'ion_id': 1327, 'distance': 13.891127586364746, 'force': [1.5509934425354004, 0.7286680340766907, -0.15393760800361633], 'magnitude': 1.7205332517623901}, {'ion_id': 1330, 'distance': 8.939528465270996, 'force': [2.758227825164795, 1.1968661546707153, -2.8668406009674072], 'magnitude': 4.15440559387207}, {'ion_id': 1355, 'distance': 9.75930118560791, 'force': [3.0123891830444336, -1.6359062194824219, 0.6324722766876221], 'magnitude': 3.4857852458953857}, {'ion_id': 1465, 'distance': 12.989046096801758, 'force': [0.8180946707725525, 0.47484707832336426, -1.7255505323410034], 'magnitude': 1.9678118228912354}, {'ion_id': 1476, 'distance': 11.828947067260742, 'force': [0.9998230934143066, 2.115550994873047, 0.39317214488983154], 'magnitude': 2.3727171421051025}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.734044075012207, 'force': [-1.2577698230743408, -6.357444763183594, 15.691710472106934], 'magnitude': 16.977304458618164}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.233038902282715, 'force': [5.917219161987305, 2.8648087978363037, -17.654033660888672], 'magnitude': 18.83840560913086}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.254058837890625, 'force': [-3.3643405437469482, 4.150124549865723, -15.992646217346191], 'magnitude': 16.861408233642578}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.1967878341674805, 'force': [2.176051616668701, -0.1592055857181549, 7.6024274826049805], 'magnitude': 7.909327030181885}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.782413959503174, 'force': [1.9523283243179321, -2.264892816543579, 5.306349754333496], 'magnitude': 6.09086799621582}]}, 6454: {'frame': 6454, 'ionic_force': [11.519911527633667, 2.6967788338661194, -4.047921255230904], 'ionic_force_magnitude': 12.504664896423474, 'motion_vector': [1.3884010314941406, -1.9174156188964844, -1.4060287475585938], 'ionic_force_x': 11.519911527633667, 'ionic_force_y': 2.6967788338661194, 'ionic_force_z': -4.047921255230904, 'radial_force': 11.831355699297328, 'axial_force': -4.047921255230904, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [3.341969609260559, -3.037167191505432, 2.5321836471557617], 'asn_force_magnitude': 5.177364140303561, 'residue_force': [3.341969609260559, -3.037167191505432, 2.5321836471557617], 'residue_force_magnitude': 5.177364140303561, 'total_force': [14.861881136894226, -0.34038835763931274, -1.515737608075142], 'total_force_magnitude': 14.942852326705305, 'motion_component_total': 8.505239636463802, 'cosine_total_motion': 0.5691844803460687, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.4842568961455796, 'cosine_residue_motion': 0.4842568961455796, 'cosine_ionic_motion': 0.47966622035433437, 'motion_component_glu': None, 'motion_component_asn': 2.5071742887988293, 'motion_component_residue': 2.5071742887988293, 'motion_component_ionic': 5.998065347664972, 'ionic_contributions': [{'ion_id': 1327, 'distance': 13.535551071166992, 'force': [1.6504477262496948, 0.7416374683380127, -0.09881125390529633], 'magnitude': 1.8121168613433838}, {'ion_id': 1330, 'distance': 8.305804252624512, 'force': [3.0074729919433594, 1.765475869178772, -3.316441059112549], 'magnitude': 4.812543869018555}, {'ion_id': 1355, 'distance': 9.316579818725586, 'force': [3.105611801147461, -2.121004343032837, 0.69764643907547], 'magnitude': 3.824943780899048}, {'ion_id': 1465, 'distance': 12.854605674743652, 'force': [0.7477613687515259, 0.573081910610199, -1.774617314338684], 'magnitude': 2.009187936782837}, {'ion_id': 1476, 'distance': 9.735810279846191, 'force': [3.008617639541626, 1.7375879287719727, 0.44430193305015564], 'magnitude': 3.502626895904541}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.6618900299072266, 'force': [-5.3170342445373535, -5.837937355041504, 15.788410186767578], 'magnitude': 17.652938842773438}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.04592752456665, 'force': [5.475624084472656, 0.8606522679328918, -10.675853729248047], 'magnitude': 12.029007911682129}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.11773943901062, 'force': [-1.5295913219451904, 9.564910888671875, -29.8603515625], 'magnitude': 31.392160415649414}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.001457452774048, 'force': [1.4020322561264038, 0.27101999521255493, 15.39747428894043], 'magnitude': 15.463549613952637}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 3.0841104984283447, 'force': [3.310938835144043, -7.89581298828125, 11.8825044631958], 'magnitude': 14.645821571350098}]}, 6455: {'frame': 6455, 'ionic_force': [12.358292996883392, 6.324190944433212, -5.279603046365082], 'ionic_force_magnitude': 14.852508381605297, 'motion_vector': [-0.5884780883789062, -1.5783882141113281, 0.5686721801757812], 'ionic_force_x': 12.358292996883392, 'ionic_force_y': 6.324190944433212, 'ionic_force_z': -5.279603046365082, 'radial_force': 13.882463646574701, 'axial_force': -5.279603046365082, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [4.977549195289612, 2.205629825592041, -6.2864439487457275], 'asn_force_magnitude': 8.316259762645178, 'residue_force': [4.977549195289612, 2.205629825592041, -6.2864439487457275], 'residue_force_magnitude': 8.316259762645178, 'total_force': [17.335842192173004, 8.529820770025253, -11.56604699511081], 'total_force_magnitude': 22.51805297919409, 'motion_component_total': -17.009989276035675, 'cosine_total_motion': -0.7553934299627203, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.6753467944800056, 'cosine_residue_motion': -0.6753467944800056, 'cosine_ionic_motion': -0.7671182274760481, 'motion_component_glu': None, 'motion_component_asn': -5.616359372765473, 'motion_component_residue': -5.616359372765473, 'motion_component_ionic': -11.393629903270202, 'ionic_contributions': [{'ion_id': 1327, 'distance': 14.966226577758789, 'force': [1.4005006551742554, 0.43182238936424255, -0.22161030769348145], 'magnitude': 1.482222557067871}, {'ion_id': 1330, 'distance': 9.79718017578125, 'force': [2.4547295570373535, 0.45704543590545654, -2.393592596054077], 'magnitude': 3.458883285522461}, {'ion_id': 1355, 'distance': 11.781282424926758, 'force': [2.053807497024536, -1.2260771989822388, 0.0074832020327448845], 'magnitude': 2.3919544219970703}, {'ion_id': 1465, 'distance': 14.574193954467773, 'force': [0.7318766713142395, 0.13336181640625, -1.374646544456482], 'magnitude': 1.5630360841751099}, {'ion_id': 1476, 'distance': 6.151278018951416, 'force': [5.717378616333008, 6.528038501739502, -1.2972368001937866], 'magnitude': 8.77419662475586}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.764723062515259, 'force': [1.9649971723556519, -12.073247909545898, 11.372041702270508], 'magnitude': 16.701732635498047}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.094618082046509, 'force': [2.055894136428833, 11.745518684387207, -16.75069236755371], 'magnitude': 20.561363220214844}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.075950622558594, 'force': [-7.7393717765808105, 11.2623291015625, -12.272581100463867], 'magnitude': 18.367204666137695}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.5755672454833984, 'force': [5.694140911102295, -4.580869197845459, 8.082343101501465], 'magnitude': 10.896415710449219}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.785841464996338, 'force': [3.0018887519836426, -4.148100852966309, 3.282444715499878], 'magnitude': 6.08214807510376}]}, 6456: {'frame': 6456, 'ionic_force': [9.233830749988556, 1.1224905923008919, -4.864724556449801], 'ionic_force_magnitude': 10.497102479225585, 'motion_vector': [0.4046783447265625, 0.90826416015625, -0.1713714599609375], 'ionic_force_x': 9.233830749988556, 'ionic_force_y': 1.1224905923008919, 'ionic_force_z': -4.864724556449801, 'radial_force': 9.301807106645365, 'axial_force': -4.864724556449801, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [2.678393017500639, -0.3087630271911621, -0.3737959861755371], 'asn_force_magnitude': 2.721919764143934, 'residue_force': [2.678393017500639, -0.3087630271911621, -0.3737959861755371], 'residue_force_magnitude': 2.721919764143934, 'total_force': [11.912223767489195, 0.8137275651097298, -5.238520542625338], 'total_force_magnitude': 13.038609017547138, 'motion_component_total': 6.399847066344051, 'cosine_total_motion': 0.49083817589217116, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.3158694143775923, 'cosine_residue_motion': 0.3158694143775923, 'cosine_ionic_motion': 0.5277719137662288, 'motion_component_glu': None, 'motion_component_asn': 0.8597712018829387, 'motion_component_residue': 0.8597712018829387, 'motion_component_ionic': 5.540075864461112, 'ionic_contributions': [{'ion_id': 1327, 'distance': 13.006216049194336, 'force': [1.8978043794631958, 0.4435109794139862, -0.23132824897766113], 'magnitude': 1.9626197814941406}, {'ion_id': 1330, 'distance': 8.951516151428223, 'force': [2.841651201248169, -0.0774279534816742, -3.014273166656494], 'magnitude': 4.143286228179932}, {'ion_id': 1355, 'distance': 11.984643936157227, 'force': [1.5171762704849243, -1.7436965703964233, -0.024102753028273582], 'magnitude': 2.3114676475524902}, {'ion_id': 1465, 'distance': 13.629975318908691, 'force': [0.7945194840431213, 0.04755014926195145, -1.6000595092773438], 'magnitude': 1.7870961427688599}, {'ion_id': 1476, 'distance': 10.055949211120605, 'force': [2.1826794147491455, 2.4525539875030518, 0.005039121489971876], 'magnitude': 3.2831594944000244}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.325569152832031, 'force': [0.010892760008573532, -6.21052360534668, 5.575885772705078], 'magnitude': 8.346329689025879}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.952286243438721, 'force': [1.4998239278793335, 5.075260639190674, -6.037801265716553], 'magnitude': 8.028871536254883}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.847168445587158, 'force': [-3.1245315074920654, 9.281523704528809, -8.530243873596191], 'magnitude': 12.987472534179688}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.1708269119262695, 'force': [2.495086908340454, -4.735126972198486, 5.956734657287598], 'magnitude': 8.008094787597656}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.324153423309326, 'force': [1.7971209287643433, -3.7198967933654785, 2.6616287231445312], 'magnitude': 4.914422035217285}]}, 6457: {'frame': 6457, 'ionic_force': [9.096073269844055, 2.163865104317665, -4.737605880945921], 'ionic_force_magnitude': 10.481687392935767, 'motion_vector': [-0.11692047119140625, 0.4889183044433594, -0.9179763793945312], 'ionic_force_x': 9.096073269844055, 'ionic_force_y': 2.163865104317665, 'ionic_force_z': -4.737605880945921, 'radial_force': 9.349912358950496, 'axial_force': -4.737605880945921, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [3.6196987479925156, 0.9866251945495605, -2.1217710971832275], 'asn_force_magnitude': 4.310169473417567, 'residue_force': [3.6196987479925156, 0.9866251945495605, -2.1217710971832275], 'residue_force_magnitude': 4.310169473417567, 'total_force': [12.71577201783657, 3.1504902988672256, -6.8593769781291485], 'total_force_magnitude': 14.787410174230653, 'motion_component_total': 6.067537726993285, 'cosine_total_motion': 0.4103178078854475, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.4448833566328734, 'cosine_residue_motion': 0.4448833566328734, 'cosine_ionic_motion': 0.3959300548115636, 'motion_component_glu': None, 'motion_component_asn': 1.9175226629905513, 'motion_component_residue': 1.9175226629905513, 'motion_component_ionic': 4.150015064002734, 'ionic_contributions': [{'ion_id': 1327, 'distance': 13.356212615966797, 'force': [1.7632050514221191, 0.5160462856292725, -0.29753151535987854], 'magnitude': 1.8611074686050415}, {'ion_id': 1330, 'distance': 9.433257102966309, 'force': [2.496544122695923, 0.2790150046348572, -2.758460760116577], 'magnitude': 3.730909824371338}, {'ion_id': 1355, 'distance': 11.953140258789062, 'force': [1.7096211910247803, -1.5737277269363403, -0.002807583659887314], 'magnitude': 2.3236677646636963}, {'ion_id': 1465, 'distance': 14.086824417114258, 'force': [0.7106510400772095, 0.08507032692432404, -1.5122408866882324], 'magnitude': 1.6730613708496094}, {'ion_id': 1476, 'distance': 9.414636611938477, 'force': [2.4160518646240234, 2.8574612140655518, -0.16656513512134552], 'magnitude': 3.7456822395324707}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.432066917419434, 'force': [0.1876840442419052, -8.85480785369873, 8.171801567077637], 'magnitude': 12.050775527954102}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.074004650115967, 'force': [2.337883472442627, 6.998097896575928, -9.290325164794922], 'magnitude': 11.863778114318848}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.163885593414307, 'force': [-5.59630823135376, 12.156975746154785, -11.42960262298584], 'magnitude': 17.59961700439453}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.773740768432617, 'force': [4.213186264038086, -4.972995758056641, 7.294291019439697], 'magnitude': 9.782039642333984}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.859930038452148, 'force': [2.4772531986236572, -4.340644836425781, 3.1320641040802], 'magnitude': 5.89811897277832}]}, 6458: {'frame': 6458, 'ionic_force': [7.916607975959778, 2.0578590631484985, -4.374101959168911], 'ionic_force_magnitude': 9.27578749853713, 'motion_vector': [1.0696640014648438, -0.24401092529296875, -0.6402435302734375], 'ionic_force_x': 7.916607975959778, 'ionic_force_y': 2.0578590631484985, 'ionic_force_z': -4.374101959168911, 'radial_force': 8.179698391066285, 'axial_force': -4.374101959168911, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [6.513012155890465, 6.821474075317383, -8.224840879440308], 'asn_force_magnitude': 12.513985911575757, 'residue_force': [6.513012155890465, 6.821474075317383, -8.224840879440308], 'residue_force_magnitude': 12.513985911575757, 'total_force': [14.429620131850243, 8.879333138465881, -12.598942838609219], 'total_force_magnitude': 21.113736163547625, 'motion_component_total': 16.795061938220684, 'cosine_total_motion': 0.7954566547637821, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.6648131511804719, 'cosine_residue_motion': 0.6648131511804719, 'cosine_ionic_motion': 0.9137336891185409, 'motion_component_glu': None, 'motion_component_asn': 8.319462407702709, 'motion_component_residue': 8.319462407702709, 'motion_component_ionic': 8.475599530517973, 'ionic_contributions': [{'ion_id': 1327, 'distance': 13.499906539916992, 'force': [1.6573450565338135, 0.6732655763626099, -0.3442486822605133], 'magnitude': 1.821698784828186}, {'ion_id': 1330, 'distance': 10.188179969787598, 'force': [2.1297972202301025, 0.3772757053375244, -2.3562591075897217], 'magnitude': 3.198488712310791}, {'ion_id': 1355, 'distance': 11.447684288024902, 'force': [1.8750309944152832, -1.692273497581482, -0.19635580480098724], 'magnitude': 2.5333943367004395}, {'ion_id': 1465, 'distance': 14.686171531677246, 'force': [0.6408071517944336, 0.15025389194488525, -1.3914772272109985], 'magnitude': 1.5392916202545166}, {'ion_id': 1476, 'distance': 10.487844467163086, 'force': [1.613627552986145, 2.549337387084961, -0.08576113730669022], 'magnitude': 3.018322229385376}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.53127121925354, 'force': [0.14992402493953705, -14.690401077270508, 12.021852493286133], 'magnitude': 18.9830265045166}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.75795316696167, 'force': [6.736653804779053, 16.811969757080078, -18.49714469909668], 'magnitude': 25.88762664794922}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.82559871673584, 'force': [-6.80995512008667, 13.276577949523926, -14.562671661376953], 'magnitude': 20.84980583190918}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.6177797317504883, 'force': [3.8591253757476807, -4.387569904327393, 8.896235466003418], 'magnitude': 10.6436185836792}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.707032203674316, 'force': [2.5772640705108643, -4.189102649688721, 3.9168875217437744], 'magnitude': 6.287517547607422}]}, 6459: {'frame': 6459, 'ionic_force': [10.070922791957855, -0.5866779759526253, -2.2287999242544174], 'ionic_force_magnitude': 10.33127417269528, 'motion_vector': [-1.1145095825195312, -2.0631027221679688, 1.3752975463867188], 'ionic_force_x': 10.070922791957855, 'ionic_force_y': -0.5866779759526253, 'ionic_force_z': -2.2287999242544174, 'radial_force': 10.087996675705444, 'axial_force': -2.2287999242544174, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [2.9267947673797607, 12.591713905334473, -8.047246754169464], 'asn_force_magnitude': 15.227460950750983, 'residue_force': [2.9267947673797607, 12.591713905334473, -8.047246754169464], 'residue_force_magnitude': 15.227460950750983, 'total_force': [12.997717559337616, 12.005035929381847, -10.276046678423882], 'total_force_magnitude': 20.46115062148776, 'motion_component_total': -19.63851903610197, 'cosine_total_motion': -0.9597954386532943, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.9737218344617912, 'cosine_residue_motion': -0.9737218344617912, 'cosine_ionic_motion': -0.4656935576888537, 'motion_component_glu': None, 'motion_compone</t>
+          <t>{6449: {'frame': 6449, 'motion_vector': [4.9669189453125, 1.6391181945800781, 0.8033828735351562], 'ionic_force': [11.088144078850746, 3.661605954170227, -9.956974852830172], 'ionic_force_magnitude': 15.345867375188023, 'radial_force': 11.67708427977497, 'axial_force': -9.956974852830172, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [2.4526870250701904, 6.051830530166626, -0.10775279998779297], 'asn_force_magnitude': 6.530845050581872, 'residue_force': [2.4526870250701904, 6.051830530166626, -0.10775279998779297], 'residue_force_magnitude': 6.530845050581872, 'total_force': [13.540831103920937, 9.713436484336853, -10.064727652817965], 'total_force_magnitude': 19.468017311620553, 'cosine_total_motion': 0.728909036550714, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.6370292535217775, 'cosine_residue_motion': 0.6370292535217775, 'cosine_ionic_motion': 0.6536010086301492, 'motion_component_total': 14.190413742165958, 'motion_component_glu': None, 'motion_component_asn': 4.1603393474385655, 'motion_component_residue': 4.1603393474385655, 'motion_component_ionic': 10.030074394727393, 'motion_component_percent_total': 72.8909036550714, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 63.70292535217775, 'motion_component_percent_residue': 63.70292535217775, 'motion_component_percent_ionic': 65.36010086301492, 'ionic_contributions': [{'ion_id': 1327, 'distance': 8.776840209960938, 'force': [3.5316085815429688, 2.2948412895202637, -0.9144463539123535], 'magnitude': 4.309845447540283, 'cosine_ionic_motion': 0.9018499255180359, 'motion_component_ionic': 3.886833906173706, 'motion_component_percent_ionic': 90.18499255180359}, {'ion_id': 1330, 'distance': 7.018555641174316, 'force': [0.982691764831543, 1.5302084684371948, -6.489742279052734], 'magnitude': 6.739731311798096, 'cosine_ionic_motion': 0.060995496809482574, 'motion_component_ionic': 0.41109326481819153, 'motion_component_percent_ionic': 6.0995496809482574}, {'ion_id': 1355, 'distance': 7.212211608886719, 'force': [4.765550136566162, -4.245543003082275, 0.05606735870242119], 'magnitude': 6.3826518058776855, 'cosine_ionic_motion': 0.49610841274261475, 'motion_component_ionic': 3.166487216949463, 'motion_component_percent_ionic': 49.610841274261475}, {'ion_id': 1465, 'distance': 13.133724212646484, 'force': [0.14122642576694489, 0.30911684036254883, -1.894454836845398], 'magnitude': 1.924696683883667, 'cosine_ionic_motion': -0.03081335499882698, 'motion_component_ionic': -0.05930636078119278, 'motion_component_percent_ionic': 3.081335499882698}, {'ion_id': 1476, 'distance': 8.905438423156738, 'force': [1.6670671701431274, 3.772982358932495, -0.7143987417221069], 'magnitude': 4.186272144317627, 'cosine_ionic_motion': 0.6270415186882019, 'motion_component_ionic': 2.6249663829803467, 'motion_component_percent_ionic': 62.70415186882019}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.108480930328369, 'force': [-8.40830135345459, 6.2936530113220215, -5.1391825675964355], 'magnitude': 11.692767143249512, 'cosine_with_motion': -0.5749664902687073, 'motion_component': -6.722949504852295, 'motion_component_percent': 57.49664902687073}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.946959972381592, 'force': [4.270160675048828, -3.4683640003204346, 1.462803602218628], 'magnitude': 5.692417144775391, 'cosine_with_motion': 0.5543876886367798, 'motion_component': 3.155805826187134, 'motion_component_percent': 55.43876886367798}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.85023307800293, 'force': [4.502490520477295, -2.196474075317383, 3.157519578933716], 'magnitude': 5.921726703643799, 'cosine_with_motion': 0.6797229051589966, 'motion_component': 4.02513313293457, 'motion_component_percent': 67.97229051589966}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.804171562194824, 'force': [6.257778167724609, 3.50447678565979, -5.5318803787231445], 'magnitude': 9.057750701904297, 'cosine_with_motion': 0.675591766834259, 'motion_component': 6.119341850280762, 'motion_component_percent': 67.5591766834259}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.483778953552246, 'force': [-3.3062853813171387, -1.051046371459961, 3.069798707962036], 'magnitude': 4.632481575012207, 'cosine_with_motion': -0.639582097530365, 'motion_component': -2.9628522396087646, 'motion_component_percent': 63.9582097530365}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.744706630706787, 'force': [-0.8631556034088135, 2.9695851802825928, 2.8731882572174072], 'magnitude': 4.221218109130859, 'cosine_with_motion': 0.12931354343891144, 'motion_component': 0.5458606481552124, 'motion_component_percent': 12.931354343891144}]}, 6450: {'frame': 6450, 'motion_vector': [1.8098068237304688, -1.3127899169921875, -0.8244171142578125], 'ionic_force': [11.005028426647186, 3.282705068588257, -4.414879508316517], 'ionic_force_magnitude': 12.303575265409675, 'radial_force': 11.484197979774107, 'axial_force': -4.414879508316517, 'glu_force': [3.1059458255767822, 8.62153148651123, 2.919323444366455], 'glu_force_magnitude': 9.617700037802697, 'asn_force': [6.720531940460205, 0.33734792470932007, -5.030340194702148], 'asn_force_magnitude': 8.401409147249499, 'residue_force': [9.826477766036987, 8.95887941122055, -2.1110167503356934], 'residue_force_magnitude': 13.463936174514814, 'total_force': [20.831506192684174, 12.241584479808807, -6.52589625865221], 'total_force_magnitude': 25.027891697280975, 'cosine_total_motion': 0.4528883876509921, 'cosine_glu_motion': -0.3535927756896398, 'cosine_asn_motion': 0.7925546217684223, 'cosine_residue_motion': 0.24196686278635599, 'cosine_ionic_motion': 0.6564770764551591, 'motion_component_total': 11.334841517085232, 'motion_component_glu': -3.4007492521170093, 'motion_component_asn': 6.65857564902009, 'motion_component_residue': 3.2578263969030807, 'motion_component_ionic': 8.077015120182152, 'motion_component_percent_total': 45.28883876509921, 'motion_component_percent_glu': 35.35927756896398, 'motion_component_percent_asn': 79.25546217684223, 'motion_component_percent_residue': 24.1966862786356, 'motion_component_percent_ionic': 65.64770764551591, 'ionic_contributions': [{'ion_id': 1327, 'distance': 13.44346809387207, 'force': [1.6276063919067383, 0.8470562100410461, -0.08977655321359634], 'magnitude': 1.8370264768600464, 'cosine_ionic_motion': 0.4357820749282837, 'motion_component_ionic': 0.8005431890487671, 'motion_component_percent_ionic': 43.57820749282837}, {'ion_id': 1330, 'distance': 8.71585750579834, 'force': [3.048281192779541, 1.3634477853775024, -2.819413661956787], 'magnitude': 4.370366096496582, 'cosine_ionic_motion': 0.5810471177101135, 'motion_component_ionic': 2.539388656616211, 'motion_component_percent_ionic': 58.10471177101135}, {'ion_id': 1355, 'distance': 10.259184837341309, 'force': [2.8688948154449463, -1.2304490804672241, 0.45329388976097107], 'magnitude': 3.1543681621551514, 'cosine_ionic_motion': 0.8559267520904541, 'motion_component_ionic': 2.6999080181121826, 'motion_component_percent_ionic': 85.59267520904541}, {'ion_id': 1465, 'distance': 13.79960823059082, 'force': [0.7390469908714294, 0.3952198624610901, -1.5287773609161377], 'magnitude': 1.7434303760528564, 'cosine_ionic_motion': 0.5004290342330933, 'motion_component_ionic': 0.8724632263183594, 'motion_component_percent_ionic': 50.042903423309326}, {'ion_id': 1476, 'distance': 9.953839302062988, 'force': [2.7211990356445312, 1.9074302911758423, -0.4302058219909668], 'magnitude': 3.3508644104003906, 'cosine_ionic_motion': 0.3475855886936188, 'motion_component_ionic': 1.1647121906280518, 'motion_component_percent_ionic': 34.75855886936188}], 'glu_contributions': [{'resid': 423, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 5.316457271575928, 'force': [3.1059458255767822, 8.62153148651123, 2.919323444366455], 'magnitude': 9.61769962310791, 'cosine_with_motion': -0.35359278321266174, 'motion_component': -3.4007492065429688, 'motion_component_percent': 35.359278321266174}], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.4382638931274414, 'force': [-0.9484546184539795, -7.306424140930176, 18.619186401367188], 'magnitude': 20.023921966552734, 'cosine_with_motion': -0.15664923191070557, 'motion_component': -3.1367318630218506, 'motion_component_percent': 15.664923191070557}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.1025466918945312, 'force': [7.568514347076416, 4.213474750518799, -18.53183364868164], 'magnitude': 20.45640754699707, 'cosine_with_motion': 0.4809369146823883, 'motion_component': 9.838241577148438, 'motion_component_percent': 48.09369146823883}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.579256534576416, 'force': [-6.583146095275879, 4.72232723236084, -22.398319244384766], 'magnitude': 23.818540573120117, 'cosine_with_motion': 0.006200173869729042, 'motion_component': 0.14767909049987793, 'motion_component_percent': 0.6200173869729042}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.5232129096984863, 'force': [3.385124683380127, 0.9476186633110046, 10.657909393310547], 'magnitude': 11.22265911102295, 'cosine_with_motion': -0.14598771929740906, 'motion_component': -1.638370394706726, 'motion_component_percent': 14.598771929740906}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.245125770568848, 'force': [3.2984936237335205, -2.2396485805511475, 6.622716903686523], 'magnitude': 7.730230331420898, 'cosine_with_motion': 0.1872851550579071, 'motion_component': 1.447757363319397, 'motion_component_percent': 18.72851550579071}]}, 6451: {'frame': 6451, 'motion_vector': [-1.5418739318847656, -2.056304931640625, -0.31626129150390625], 'ionic_force': [8.739684104919434, 0.469412237405777, -2.0718104019761086], 'ionic_force_magnitude': 8.994155015572286, 'radial_force': 8.75228119420347, 'axial_force': -2.0718104019761086, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [3.775687575340271, 6.209000110626221, -9.062820196151733], 'asn_force_magnitude': 11.616462841506921, 'residue_force': [3.775687575340271, 6.209000110626221, -9.062820196151733], 'residue_force_magnitude': 11.616462841506921, 'total_force': [12.515371680259705, 6.678412348031998, -11.134630598127842], 'total_force_magnitude': 18.033738335191558, 'cosine_total_motion': -0.6318832653960802, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.5226813089167416, 'cosine_residue_motion': -0.5226813089167416, 'cosine_ionic_motion': -0.5918854471977383, 'motion_component_total': -11.395217466539313, 'motion_component_glu': None, 'motion_component_asn': -6.071708002981529, 'motion_component_residue': -6.071708002981529, 'motion_component_ionic': -5.323509463557783, 'motion_component_percent_total': 63.18832653960802, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 52.26813089167416, 'motion_component_percent_residue': 52.26813089167416, 'motion_component_percent_ionic': 59.18854471977383, 'ionic_contributions': [{'ion_id': 1327, 'distance': 14.782349586486816, 'force': [1.4240713119506836, 0.4835692346096039, -0.21571895480155945], 'magnitude': 1.5193264484405518, 'cosine_ionic_motion': -0.7934879660606384, 'motion_component_ionic': -1.2055672407150269, 'motion_component_percent_ionic': 79.34879660606384}, {'ion_id': 1330, 'distance': 10.166635513305664, 'force': [2.4229938983917236, 0.5128621459007263, -2.0453357696533203], 'magnitude': 3.212059259414673, 'cosine_ionic_motion': -0.4981716275215149, 'motion_component_ionic': -1.6001567840576172, 'motion_component_percent_ionic': 49.81716275215149}, {'ion_id': 1355, 'distance': 10.030377388000488, 'force': [2.7083451747894287, -1.8824938535690308, -0.10277257114648819], 'magnitude': 3.2999210357666016, 'cosine_ionic_motion': -0.03188204765319824, 'motion_component_ionic': -0.10520824044942856, 'motion_component_percent_ionic': 3.188204765319824}, {'ion_id': 1476, 'distance': 11.328006744384766, 'force': [2.1842737197875977, 1.3554747104644775, 0.2920168936252594], 'magnitude': 2.5872063636779785, 'cosine_ionic_motion': -0.932502806186676, 'motion_component_ionic': -2.4125771522521973, 'motion_component_percent_ionic': 93.2502806186676}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.6995091438293457, 'force': [5.416232585906982, -11.804396629333496, 11.422066688537598], 'magnitude': 17.29574966430664, 'cosine_with_motion': 0.27484723925590515, 'motion_component': 4.753689289093018, 'motion_component_percent': 27.484723925590515}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.8317983150482178, 'force': [-1.9182919263839722, 15.030738830566406, -19.322242736816406], 'magnitude': 24.555082321166992, 'cosine_with_motion': -0.3434545397758484, 'motion_component': -8.433554649353027, 'motion_component_percent': 34.34545397758484}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.0421013832092285, 'force': [-11.055981636047363, 9.408076286315918, -11.74948787689209], 'magnitude': 18.676109313964844, 'cosine_with_motion': 0.02929864637553692, 'motion_component': 0.5471847057342529, 'motion_component_percent': 2.929864637553692}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.5425302982330322, 'force': [7.50039005279541, -3.2488973140716553, 7.510800838470459], 'magnitude': 11.10059928894043, 'cosine_with_motion': -0.2525363564491272, 'motion_component': -2.80330491065979, 'motion_component_percent': 25.25363564491272}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.8790106773376465, 'force': [3.833338499069214, -3.176521062850952, 3.076042890548706], 'magnitude': 5.852077484130859, 'cosine_with_motion': -0.023192286491394043, 'motion_component': -0.1357230544090271, 'motion_component_percent': 2.3192286491394043}]}, 6452: {'frame': 6452, 'motion_vector': [-0.060070037841796875, 3.2151107788085938, 1.4912796020507812], 'ionic_force': [10.327910542488098, 1.1043216735124588, -5.13695291057229], 'ionic_force_magnitude': 11.58764634158565, 'radial_force': 10.386783069469882, 'axial_force': -5.13695291057229, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [2.5758535265922546, -2.32772159576416, -1.2732272446155548], 'asn_force_magnitude': 3.6978935671914517, 'residue_force': [2.5758535265922546, -2.32772159576416, -1.2732272446155548], 'residue_force_magnitude': 3.6978935671914517, 'total_force': [12.903764069080353, -1.2233999222517014, -6.410180155187845], 'total_force_magnitude': 14.460091429248248, 'cosine_total_motion': -0.2783659437482466, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.7276147828058505, 'cosine_residue_motion': -0.7276147828058505, 'cosine_ionic_motion': -0.11517049565691527, 'motion_component_total': -4.02519699738862, 'motion_component_glu': None, 'motion_component_asn': -2.6906420247311598, 'motion_component_residue': -2.6906420247311598, 'motion_component_ionic': -1.3345549726574601, 'motion_component_percent_total': 27.836594374824656, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 72.76147828058505, 'motion_component_percent_residue': 72.76147828058505, 'motion_component_percent_ionic': 11.517049565691527, 'ionic_contributions': [{'ion_id': 1327, 'distance': 13.44875717163086, 'force': [1.7840296030044556, 0.277847021818161, -0.3307577669620514], 'magnitude': 1.8355820178985596, 'cosine_ionic_motion': 0.04501514881849289, 'motion_component_ionic': 0.08262899518013, 'motion_component_percent_ionic': 4.501514881849289}, {'ion_id': 1330, 'distance': 9.372391700744629, 'force': [2.474438190460205, -0.39485305547714233, -2.829497814178467], 'magnitude': 3.7795252799987793, 'cosine_ionic_motion': -0.42081713676452637, 'motion_component_ionic': -1.5904890298843384, 'motion_component_percent_ionic': 42.08171367645264}, {'ion_id': 1355, 'distance': 11.513007164001465, 'force': [2.0291547775268555, -1.468042254447937, -0.032318416982889175], 'magnitude': 2.504727840423584, 'cosine_ionic_motion': -0.5507784485816956, 'motion_component_ionic': -1.3795500993728638, 'motion_component_percent_ionic': 55.077844858169556}, {'ion_id': 1465, 'distance': 14.323189735412598, 'force': [0.6779139041900635, -0.06925506889820099, -1.4678304195404053], 'magnitude': 1.6182984113693237, 'cosine_ionic_motion': -0.42751216888427734, 'motion_component_ionic': -0.691842257976532, 'motion_component_percent_ionic': 42.751216888427734}, {'ion_id': 1476, 'distance': 8.711008071899414, 'force': [3.3623740673065186, 2.758625030517578, -0.4765484929084778], 'magnitude': 4.3752336502075195, 'cosine_ionic_motion': 0.5130462646484375, 'motion_component_ionic': 2.244697332382202, 'motion_component_percent_ionic': 51.30462646484375}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.110825061798096, 'force': [-0.39502090215682983, -8.049195289611816, 4.145165920257568], 'magnitude': 9.06244945526123, 'cosine_with_motion': -0.6124477982521057, 'motion_component': -5.550277233123779, 'motion_component_percent': 61.24477982521057}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.403731822967529, 'force': [2.482687473297119, 8.37047004699707, -5.183540344238281], 'magnitude': 10.153698921203613, 'cosine_with_motion': 0.5288168787956238, 'motion_component': 5.369447231292725, 'motion_component_percent': 52.88168787956238}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.945854663848877, 'force': [-2.5302085876464844, 10.595436096191406, -6.078184604644775], 'magnitude': 12.474355697631836, 'cosine_with_motion': 0.5688576102256775, 'motion_component': 7.096131801605225, 'motion_component_percent': 56.88576102256775}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.133551597595215, 'force': [2.389244794845581, -6.350554466247559, 4.520648002624512], 'magnitude': 8.153176307678223, 'cosine_with_motion': -0.478189617395401, 'motion_component': -3.8987643718719482, 'motion_component_percent': 47.8189617395401}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.617127418518066, 'force': [1.3637722730636597, -3.8248510360717773, 1.733247995376587], 'magnitude': 4.415145397186279, 'cosine_with_motion': -0.6258419752120972, 'motion_component': -2.763183355331421, 'motion_component_percent': 62.58419752120972}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.63272762298584, 'force': [-2.844557285308838, -9.159859657287598, -0.7087050080299377], 'magnitude': 9.617525100708008, 'cosine_with_motion': -0.8898619413375854, 'motion_component': -8.558269500732422, 'motion_component_percent': 88.98619413375854}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.64634895324707, 'force': [2.109935760498047, 6.090832710266113, 0.2981407940387726], 'magnitude': 6.452826023101807, 'cosine_with_motion': 0.8700488805770874, 'motion_component': 5.614274024963379, 'motion_component_percent': 87.00488805770874}]}, 6453: {'frame': 6453, 'motion_vector': [-0.720062255859375, 0.6362991333007812, 0.15360260009765625], 'ionic_force': [9.139528214931488, 2.8800260424613953, -3.7206843197345734], 'ionic_force_magnitude': 10.279543657376202, 'radial_force': 9.582563644285624, 'axial_force': -3.7206843197345734, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [5.423488736152649, -1.7666098177433014, -5.046192169189453], 'asn_force_magnitude': 7.615720302618173, 'residue_force': [5.423488736152649, -1.7666098177433014, -5.046192169189453], 'residue_force_magnitude': 7.615720302618173, 'total_force': [14.563016951084137, 1.1134162247180939, -8.766876488924026], 'total_force_magnitude': 17.034649446909036, 'cosine_total_motion': -0.6710867619577732, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.7832209129157407, 'cosine_residue_motion': -0.7832209129157407, 'cosine_ionic_motion': -0.5318267534728109, 'motion_component_total': -11.431727738411956, 'motion_component_glu': None, 'motion_component_asn': -5.964791407927546, 'motion_component_residue': -5.964791407927546, 'motion_component_ionic': -5.46693633048441, 'motion_component_percent_total': 67.10867619577732, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 78.32209129157407, 'motion_component_percent_residue': 78.32209129157407, 'motion_component_percent_ionic': 53.18267534728109, 'ionic_contributions': [{'ion_id': 1327, 'distance': 13.891127586364746, 'force': [1.5509934425354004, 0.7286680340766907, -0.15393760800361633], 'magnitude': 1.7205332517623901, 'cosine_ionic_motion': -0.40423643589019775, 'motion_component_ionic': -0.6955022215843201, 'motion_component_percent_ionic': 40.423643589019775}, {'ion_id': 1330, 'distance': 8.939528465270996, 'force': [2.758227825164795, 1.1968661546707153, -2.8668406009674072], 'magnitude': 4.15440559387207, 'cosine_ionic_motion': -0.41182196140289307, 'motion_component_ionic': -1.7108755111694336, 'motion_component_percent_ionic': 41.18219614028931}, {'ion_id': 1355, 'distance': 9.75930118560791, 'force': [3.0123891830444336, -1.6359062194824219, 0.6324722766876221], 'magnitude': 3.4857852458953857, 'cosine_ionic_motion': -0.9176909923553467, 'motion_component_ionic': -3.19887375831604, 'motion_component_percent_ionic': 91.76909923553467}, {'ion_id': 1465, 'distance': 12.989046096801758, 'force': [0.8180946707725525, 0.47484707832336426, -1.7255505323410034], 'magnitude': 1.9678118228912354, 'cosine_ionic_motion': -0.28825485706329346, 'motion_component_ionic': -0.567231297492981, 'motion_component_percent_ionic': 28.825485706329346}, {'ion_id': 1476, 'distance': 11.828947067260742, 'force': [0.9998230934143066, 2.115550994873047, 0.39317214488983154], 'magnitude': 2.3727171421051025, 'cosine_ionic_motion': 0.29735809564590454, 'motion_component_ionic': 0.7055466771125793, 'motion_component_percent_ionic': 29.735809564590454}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.734044075012207, 'force': [-1.2577698230743408, -6.357444763183594, 15.691710472106934], 'magnitude': 16.977304458618164, 'cosine_with_motion': -0.044142596423625946, 'motion_component': -0.7494223117828369, 'motion_component_percent': 4.414259642362595}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.233038902282715, 'force': [5.917219161987305, 2.8648087978363037, -17.654033660888672], 'magnitude': 18.83840560913086, 'cosine_with_motion': -0.28090742230415344, 'motion_component': -5.291848182678223, 'motion_component_percent': 28.090742230415344}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.254058837890625, 'force': [-3.3643405437469482, 4.150124549865723, -15.992646217346191], 'magnitude': 16.861408233642578, 'cosine_with_motion': 0.15886881947517395, 'motion_component': 2.6787519454956055, 'motion_component_percent': 15.886881947517395}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.1967878341674805, 'force': [2.176051616668701, -0.1592055857181549, 7.6024274826049805], 'magnitude': 7.909327030181885, 'cosine_with_motion': -0.06502027809619904, 'motion_component': -0.5142666697502136, 'motion_component_percent': 6.502027809619904}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.782413959503174, 'force': [1.9523283243179321, -2.264892816543579, 5.306349754333496], 'magnitude': 6.09086799621582, 'cosine_with_motion': -0.3428093492984772, 'motion_component': -2.0880064964294434, 'motion_component_percent': 34.28093492984772}]}, 6454: {'frame': 6454, 'motion_vector': [1.3884010314941406, -1.9174156188964844, -1.4060287475585938], 'ionic_force': [11.519911527633667, 2.6967788338661194, -4.047921255230904], 'ionic_force_magnitude': 12.504664896423474, 'radial_force': 11.831355699297328, 'axial_force': -4.047921255230904, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [3.341969609260559, -3.037167191505432, 2.5321836471557617], 'asn_force_magnitude': 5.177364140303561, 'residue_force': [3.341969609260559, -3.037167191505432, 2.5321836471557617], 'residue_force_magnitude': 5.177364140303561, 'total_force': [14.861881136894226, -0.34038835763931274, -1.515737608075142], 'total_force_magnitude': 14.942852326705305, 'cosine_total_motion': 0.5691844803460687, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.4842568961455796, 'cosine_residue_motion': 0.4842568961455796, 'cosine_ionic_motion': 0.47966622035433437, 'motion_component_total': 8.505239636463802, 'motion_component_glu': None, 'motion_component_asn': 2.5071742887988293, 'motion_component_residue': 2.5071742887988293, 'motion_component_ionic': 5.998065347664972, 'motion_component_percent_total': 56.918448034606875, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 48.42568961455796, 'motion_component_percent_residue': 48.42568961455796, 'motion_component_percent_ionic': 47.96662203543344, 'ionic_contributions': [{'ion_id': 1327, 'distance': 13.535551071166992, 'force': [1.6504477262496948, 0.7416374683380127, -0.09881125390529633], 'magnitude': 1.8121168613433838, 'cosine_ionic_motion': 0.20210470259189606, 'motion_component_ionic': 0.3662373423576355, 'motion_component_percent_ionic': 20.210470259189606}, {'ion_id': 1330, 'distance': 8.305804252624512, 'force': [3.0074729919433594, 1.765475869178772, -3.316441059112549], 'magnitude': 4.812543869018555, 'cosine_ionic_motion': 0.4115578532218933, 'motion_component_ionic': 1.980640172958374, 'motion_component_percent_ionic': 41.15578532218933}, {'ion_id': 1355, 'distance': 9.316579818725586, 'force': [3.105611801147461, -2.121004343032837, 0.69764643907547], 'magnitude': 3.824943780899048, 'cosine_ionic_motion': 0.7024427056312561, 'motion_component_ionic': 2.6868038177490234, 'motion_component_percent_ionic': 70.24427056312561}, {'ion_id': 1465, 'distance': 12.854605674743652, 'force': [0.7477613687515259, 0.573081910610199, -1.774617314338684], 'magnitude': 2.009187936782837, 'cosine_ionic_motion': 0.44007608294487, 'motion_component_ionic': 0.8841955661773682, 'motion_component_percent_ionic': 44.007608294487}, {'ion_id': 1476, 'distance': 9.735810279846191, 'force': [3.008617639541626, 1.7375879287719727, 0.44430193305015564], 'magnitude': 3.502626895904541, 'cosine_ionic_motion': 0.022893792018294334, 'motion_component_ionic': 0.08018840849399567, 'motion_component_percent_ionic': 2.2893792018294334}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.6618900299072266, 'force': [-5.3170342445373535, -5.837937355041504, 15.788410186767578], 'magnitude': 17.652938842773438, 'cosine_with_motion': -0.3783014416694641, 'motion_component': -6.678132057189941, 'motion_component_percent': 37.83014416694641}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.04592752456665, 'force': [5.475624084472656, 0.8606522679328918, -10.675853729248047], 'magnitude': 12.029007911682129, 'cosine_with_motion': 0.6329251527786255, 'motion_component': 7.613461494445801, 'motion_component_percent': 63.29251527786255}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.11773943901062, 'force': [-1.5295913219451904, 9.564910888671875, -29.8603515625], 'magnitude': 31.392160415649414, 'cosine_with_motion': 0.24898582696914673, 'motion_component': 7.8162031173706055, 'motion_component_percent': 24.898582696914673}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.001457452774048, 'force': [1.4020322561264038, 0.27101999521255493, 15.39747428894043], 'magnitude': 15.463549613952637, 'cosine_with_motion': -0.47496092319488525, 'motion_component': -7.344581604003906, 'motion_component_percent': 47.496092319488525}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 3.0841104984283447, 'force': [3.310938835144043, -7.89581298828125, 11.8825044631958], 'magnitude': 14.645821571350098, 'cosine_with_motion': 0.07512199133634567, 'motion_component': 1.1002233028411865, 'motion_component_percent': 7.512199133634567}]}, 6455: {'frame': 6455, 'motion_vector': [-0.5884780883789062, -1.5783882141113281, 0.5686721801757812], 'ionic_force': [12.358292996883392, 6.324190944433212, -5.279603046365082], 'ionic_force_magnitude': 14.852508381605297, 'radial_force': 13.882463646574701, 'axial_force': -5.279603046365082, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [4.977549195289612, 2.205629825592041, -6.2864439487457275], 'asn_force_magnitude': 8.316259762645178, 'residue_force': [4.977549195289612, 2.205629825592041, -6.2864439487457275], 'residue_force_magnitude': 8.316259762645178, 'total_force': [17.335842192173004, 8.529820770025253, -11.56604699511081], 'total_force_magnitude': 22.51805297919409, 'cosine_total_motion': -0.7553934299627203, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.6753467944800056, 'cosine_residue_motion': -0.6753467944800056, 'cosine_ionic_motion': -0.7671182274760481, 'motion_component_total': -17.009989276035675, 'motion_component_glu': None, 'motion_component_asn': -5.616359372765473, 'motion_component_residue': -5.616359372765473, 'motion_component_ionic': -11.393629903270202, 'motion_component_percent_total': 75.53934299627203, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 67.53467944800056, 'motion_component_percent_residue': 67.53467944800056, 'motion_component_percent_ionic': 76.71182274760481, 'ionic_contributions': [{'ion_id': 1327, 'distance': 14.966226577758789, 'force': [1.4005006551742554, 0.43182238936424255, -0.22161030769348145], 'magnitude': 1.482222557067871, 'cosine_ionic_motion': -0.6192032694816589, 'motion_component_ionic': -0.9177970886230469, 'motion_component_percent_ionic': 61.920326948165894}, {'ion_id': 1330, 'distance': 9.79718017578125, 'force': [2.4547295570373535, 0.45704543590545654, -2.393592596054077], 'magnitude': 3.458883285522461, 'cosine_ionic_motion': -0.5735505819320679, 'motion_component_ionic': -1.983844518661499, 'motion_component_percent_ionic': 57.35505819320679}, {'ion_id': 1355, 'distance': 11.781282424926758, 'force': [2.053807497024536, -1.2260771989822388, 0.0074832020327448845], 'magnitude': 2.3919544219970703, 'cosine_ionic_motion': 0.17185772955417633, 'motion_component_ionic': 0.4110758602619171, 'motion_component_percent_ionic': 17.185772955417633}, {'ion_id': 1465, 'distance': 14.574193954467773, 'force': [0.7318766713142395, 0.13336181640625, -1.374646544456482], 'magnitude': 1.5630360841751099, 'cosine_ionic_motion': -0.5120317935943604, 'motion_component_ionic': -0.8003242015838623, 'motion_component_percent_ionic': 51.203179359436035}, {'ion_id': 1476, 'distance': 6.151278018951416, 'force': [5.717378616333008, 6.528038501739502, -1.2972368001937866], 'magnitude': 8.77419662475586, 'cosine_ionic_motion': -0.9234737753868103, 'motion_component_ionic': -8.102740287780762, 'motion_component_percent_ionic': 92.34737753868103}], 'glu_contributions': [], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.764723062515259, 'force': [1.9649971723556519, -12.073247909545898, 11.372041702270508], 'magnitude': 16.701732635498047, 'cosine_with_motion': 0.8205893039703369, 'motion_component': 13.705263137817383, 'motion_component_percent': 82.05893039703369}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 3.094618082046509, 'force': [2.055894136428833, 11.745518684387207, -16.75069236755371], 'magnitude': 20.561363220214844, 'cosine_with_motion': -0.8008015751838684, 'motion_component': -16.465572357177734, 'motion_component_percent': 80.08015751838684}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.075950622558594, 'force': [-7.7393717765808105, 11.2623291015625, -12.272581100463867], 'magnitude': 18.367204666137695, 'cosine_with_motion': -0.6186090111732483, 'motion_component': -11.3621187210083, 'motion_component_percent': 61.86090111732483}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.5755672454833984, 'force': [5.69414091</t>
         </is>
       </c>
     </row>
@@ -819,7 +819,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>{6569: {'frame': 6569, 'ionic_force': [8.93659296631813, 4.198592029511929, -11.964962244033813], 'ionic_force_magnitude': 15.51293622681027, 'motion_vector': [0.9375572204589844, 4.542621612548828, 3.9090347290039062], 'ionic_force_x': 8.93659296631813, 'ionic_force_y': 4.198592029511929, 'ionic_force_z': -11.964962244033813, 'radial_force': 9.87374644579897, 'axial_force': -11.964962244033813, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.24319716542959213, -5.893840670585632, -0.811901792883873], 'asn_force_magnitude': 5.954467837918879, 'residue_force': [0.24319716542959213, -5.893840670585632, -0.811901792883873], 'residue_force_magnitude': 5.954467837918879, 'total_force': [9.179790131747723, -1.6952486410737038, -12.776864036917686], 'total_force_magnitude': 15.823737530554393, 'motion_component_total': -8.084474507913425, 'cosine_total_motion': -0.5109080261412919, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.822811478701697, 'cosine_residue_motion': -0.822811478701697, 'cosine_ionic_motion': -0.20531703184656236, 'motion_component_glu': None, 'motion_component_asn': -4.89940448659973, 'motion_component_residue': -4.89940448659973, 'motion_component_ionic': -3.1850700213136953, 'ionic_contributions': [{'ion_id': 1327, 'distance': 10.281067848205566, 'force': [2.5776994228363037, 1.23420250415802, -1.3029985427856445], 'magnitude': 3.1409544944763184}, {'ion_id': 1330, 'distance': 7.982583522796631, 'force': [3.5478971004486084, -3.1198573112487793, -2.1965181827545166], 'magnitude': 5.210160732269287}, {'ion_id': 1341, 'distance': 6.964383125305176, 'force': [1.5748634338378906, 5.740958213806152, -3.378621816635132], 'magnitude': 6.844989776611328}, {'ion_id': 1359, 'distance': 9.398062705993652, 'force': [1.0105098485946655, 0.24263377487659454, -3.6123909950256348], 'magnitude': 3.7589054107666016}, {'ion_id': 1374, 'distance': 14.902193069458008, 'force': [0.22562316060066223, 0.10065484791994095, -1.4744327068328857], 'magnitude': 1.494987964630127}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.862966537475586, 'force': [-3.78678035736084, 3.9053030014038086, -1.7953109741210938], 'magnitude': 5.728371620178223}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.223381042480469, 'force': [4.336669921875, -1.6977781057357788, 2.0930356979370117], 'magnitude': 5.105874538421631}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.000786304473877, 'force': [7.137111663818359, 9.86938190460205, -0.7356123328208923], 'magnitude': 12.201810836791992}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.115147590637207, 'force': [-5.323076248168945, -6.185309886932373, 1.0383859872817993], 'magnitude': 8.226264953613281}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.198151111602783, 'force': [-2.1941421031951904, -4.665300369262695, 0.022443369030952454], 'magnitude': 5.155559539794922}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.206618309020996, 'force': [0.07341428846120834, -7.1201372146606445, -1.4348435401916504], 'magnitude': 7.263643741607666}]}, 6570: {'frame': 6570, 'ionic_force': [12.369088254868984, 9.554802000522614, -1.3525469191372395], 'ionic_force_magnitude': 15.688147395227915, 'motion_vector': [0.08165740966796875, 0.8572654724121094, 0.46636962890625], 'ionic_force_x': 12.369088254868984, 'ionic_force_y': 9.554802000522614, 'ionic_force_z': -1.3525469191372395, 'radial_force': 15.629734019679567, 'axial_force': -1.3525469191372395, 'glu_force': [1.7606010437011719, 2.221771240234375, -0.6299586296081543], 'glu_force_magnitude': 2.903933772321957, 'asn_force': [0.8742416501045227, -0.7024664878845215, 2.305647373199463], 'asn_force_magnitude': 2.5639359272259274, 'residue_force': [2.6348426938056946, 1.5193047523498535, 1.6756887435913086], 'residue_force_magnitude': 3.4725517587233625, 'total_force': [15.003930948674679, 11.074106752872467, 0.32314182445406914], 'total_force_magnitude': 18.650957212039412, 'motion_component_total': 11.09883040431671, 'cosine_total_motion': 0.5950810072714275, 'cosine_glu_motion': 0.616979428830821, 'cosine_asn_motion': 0.2168416064553393, 'cosine_residue_motion': 0.6760548290232078, 'cosine_ionic_motion': 0.557822080474634, 'motion_component_glu': 1.7916674002097324, 'motion_component_asn': 0.55596798530823, 'motion_component_residue': 2.3476353855179624, 'motion_component_ionic': 8.751195018798747, 'ionic_contributions': [{'ion_id': 1327, 'distance': 12.443742752075195, 'force': [1.5750917196273804, 1.453436017036438, -0.059865642338991165], 'magnitude': 2.1440553665161133}, {'ion_id': 1330, 'distance': 6.1113481521606445, 'force': [8.851373672485352, -0.5448993444442749, 0.612082302570343], 'magnitude': 8.889227867126465}, {'ion_id': 1341, 'distance': 7.490889549255371, 'force': [-0.1118030920624733, 4.923777103424072, 3.27870774269104], 'magnitude': 5.9165873527526855}, {'ion_id': 1359, 'distance': 8.462321281433105, 'force': [1.5930393934249878, 2.9040167331695557, -3.243910789489746], 'magnitude': 4.636167049407959}, {'ion_id': 1374, 'distance': 12.411674499511719, 'force': [0.4613865613937378, 0.8184714913368225, -1.9395605325698853], 'magnitude': 2.155149221420288}], 'glu_contributions': [{'resid': 423, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 5.885604381561279, 'force': [-4.789684295654297, -5.065373420715332, -3.3144640922546387], 'magnitude': 7.7191162109375}, {'resid': 423, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 5.172755241394043, 'force': [6.550285339355469, 7.287144660949707, 2.6845054626464844], 'magnitude': 10.159492492675781}], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.012881755828857, 'force': [-4.670202732086182, 1.571510910987854, 8.02849292755127], 'magnitude': 9.420039176940918}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.714416027069092, 'force': [3.6295950412750244, -1.6445144414901733, -4.525853157043457], 'magnitude': 6.030068874359131}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.604116439819336, 'force': [3.857551336288452, -3.9069876670837402, -13.306673049926758], 'magnitude': 14.394887924194336}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.168186187744141, 'force': [-1.0959246158599854, 2.225980281829834, 4.5875444412231445], 'magnitude': 5.215515613555908}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.269467353820801, 'force': [-0.8467773795127869, 1.051544427871704, 7.522136211395264], 'magnitude': 7.642336845397949}]}, 6571: {'frame': 6571, 'ionic_force': [10.874882519245148, 11.021745204925537, -1.5739329904317856], 'ionic_force_magnitude': 15.563393017849684, 'motion_vector': [-0.7143974304199219, 2.6378211975097656, 0.46242523193359375], 'ionic_force_x': 10.874882519245148, 'ionic_force_y': 11.021745204925537, 'ionic_force_z': -1.5739329904317856, 'radial_force': 15.483602202642729, 'axial_force': -1.5739329904317856, 'glu_force': [7.676974296569824, 7.6012349128723145, 1.5161144137382507], 'glu_force_magnitude': 10.909322135971951, 'asn_force': [1.804943561553955, -2.185672402381897, -6.2858805656433105], 'asn_force_magnitude': 6.8954535453776495, 'residue_force': [9.48191785812378, 5.4155625104904175, -4.76976615190506], 'residue_force_magnitude': 11.915777470106393, 'total_force': [20.356800377368927, 16.437307715415955, -6.343699142336845], 'total_force_magnitude': 26.922609928159005, 'motion_component_total': 9.338087993671115, 'cosine_total_motion': 0.34684928461947456, 'cosine_glu_motion': 0.5049181651682594, 'cosine_asn_motion': -0.5212199278497726, 'cosine_residue_motion': 0.16064978735241064, 'cosine_ionic_motion': 0.4770052949537086, 'motion_component_glu': 5.5083149161244345, 'motion_component_asn': -3.5940477994131967, 'motion_component_residue': 1.9142671167112377, 'motion_component_ionic': 7.423820876959877, 'ionic_contributions': [{'ion_id': 1327, 'distance': 14.060022354125977, 'force': [0.9435466527938843, 1.3866626024246216, -0.0861724466085434], 'magnitude': 1.6794461011886597}, {'ion_id': 1330, 'distance': 6.742351531982422, 'force': [7.051734924316406, 1.6229393482208252, 0.9881018400192261], 'magnitude': 7.3032355308532715}, {'ion_id': 1341, 'distance': 8.82316780090332, 'force': [0.5937607288360596, 3.663236141204834, 2.101393938064575], 'magnitude': 4.264704704284668}, {'ion_id': 1359, 'distance': 8.525839805603027, 'force': [1.727158784866333, 3.3323826789855957, -2.602457046508789], 'magnitude': 4.5673441886901855}, {'ion_id': 1374, 'distance': 12.040011405944824, 'force': [0.5586814284324646, 1.0165244340896606, -1.9747992753982544], 'magnitude': 2.290257453918457}], 'glu_contributions': [{'resid': 423, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 5.272819995880127, 'force': [-7.410064220428467, -5.5089592933654785, -2.6905951499938965], 'magnitude': 9.617535591125488}, {'resid': 423, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 5.610739707946777, 'force': [5.298938274383545, 5.913795471191406, 3.393536329269409], 'magnitude': 8.635265350341797}, {'resid': 423, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 4.725030899047852, 'force': [9.788100242614746, 7.196398735046387, 0.813173234462738], 'magnitude': 12.176054954528809}], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.708808422088623, 'force': [-3.2005159854888916, 1.111762285232544, 6.424706935882568], 'magnitude': 7.263344764709473}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.992682933807373, 'force': [2.94905161857605, -1.6493879556655884, -4.318172454833984], 'magnitude': 5.483064651489258}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.889748573303223, 'force': [2.056407928466797, -1.6480467319488525, -8.392415046691895], 'magnitude': 8.796448707580566}]}, 6572: {'frame': 6572, 'ionic_force': [4.297864839434624, 8.788159370422363, -1.320813924074173], 'ionic_force_magnitude': 9.871572150372959, 'motion_vector': [0.8923988342285156, -0.882781982421875, -0.6154251098632812], 'ionic_force_x': 4.297864839434624, 'ionic_force_y': 8.788159370422363, 'ionic_force_z': -1.320813924074173, 'radial_force': 9.782810807635544, 'axial_force': -1.320813924074173, 'glu_force': [13.541619300842285, 3.0024799704551697, 4.42834997177124], 'glu_force_magnitude': 14.560241163332945, 'asn_force': [-1.4802942276000977, 2.662510633468628, 3.6407511234283447], 'asn_force_magnitude': 4.747136254242597, 'residue_force': [12.061325073242188, 5.664990603923798, 8.069101095199585], 'residue_force_magnitude': 15.578128050234941, 'total_force': [16.35918991267681, 14.453149974346161, 6.748287171125412], 'total_force_magnitude': 22.848545216795422, 'motion_component_total': -1.6545849266526034, 'cosine_total_motion': -0.07241532933293089, 'cosine_glu_motion': 0.32957797866470223, 'cosine_asn_motion': -0.8908319332372551, 'cosine_residue_motion': 0.03657912445813258, 'cosine_ionic_motion': -0.22533586115184634, 'motion_component_glu': 4.798734851481864, 'motion_component_asn': -4.228900566707594, 'motion_component_residue': 0.5698342847742701, 'motion_component_ionic': -2.2244192114268744, 'ionic_contributions': [{'ion_id': 1330, 'distance': 8.661239624023438, 'force': [3.4389588832855225, 2.7700512409210205, 0.2946772277355194], 'magnitude': 4.425658702850342}, {'ion_id': 1341, 'distance': 11.687585830688477, 'force': [-0.10774736106395721, 2.0299341678619385, 1.3322513103485107], 'magnitude': 2.430459976196289}, {'ion_id': 1359, 'distance': 10.02340030670166, 'force': [0.6919946074485779, 2.870731830596924, -1.4831961393356323], 'magnitude': 3.304516315460205}, {'ion_id': 1374, 'distance': 13.351118087768555, 'force': [0.2746587097644806, 1.1174421310424805, -1.4645463228225708], 'magnitude': 1.8625279664993286}], 'glu_contributions': [{'resid': 423, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 4.82476282119751, 'force': [-10.750345230102539, -0.609584391117096, -4.000533580780029], 'magnitude': 11.48676586151123}, {'resid': 423, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 4.59662389755249, 'force': [10.555639266967773, 2.346975326538086, 6.9713640213012695], 'magnitude': 12.865835189819336}, {'resid': 423, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 4.426905155181885, 'force': [13.73632526397705, 1.2650890350341797, 1.45751953125], 'magnitude': 13.871245384216309}], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.417150974273682, 'force': [-1.4802942276000977, 2.662510633468628, 3.6407511234283447], 'magnitude': 4.747136116027832}]}, 6573: {'frame': 6573, 'ionic_force': [6.707516588270664, 9.176944971084595, -0.1950500402599573], 'ionic_force_magnitude': 11.368603357600545, 'motion_vector': [-0.3231239318847656, -0.48430633544921875, 0.06146240234375], 'ionic_force_x': 6.707516588270664, 'ionic_force_y': 9.176944971084595, 'ionic_force_z': -0.1950500402599573, 'radial_force': 11.366930007008971, 'axial_force': -0.1950500402599573, 'glu_force': [14.778462409973145, 7.344141960144043, 6.265172243118286], 'glu_force_magnitude': 17.651961805127424, 'asn_force': [-0.33382272720336914, 2.524196147918701, 3.64918851852417], 'asn_force_magnitude': 4.449671971066376, 'residue_force': [14.444639682769775, 9.868338108062744, 9.914360761642456], 'residue_force_magnitude': 20.107865672221063, 'total_force': [21.15215627104044, 19.04528307914734, 9.719310721382499], 'total_force_magnitude': 30.07659427824487, 'motion_component_total': -26.409473335995354, 'cosine_total_motion': -0.8780739299029601, 'cosine_glu_motion': -0.7690050360806358, 'cosine_asn_motion': -0.3417756668672356, 'cosine_residue_motion': -0.7507130481258231, 'cosine_ionic_motion': -0.9952177809364312, 'motion_component_glu': -13.574447524846018, 'motion_component_asn': -1.5207896052516574, 'motion_component_residue': -15.095237130097676, 'motion_component_ionic': -11.314236205897675, 'ionic_contributions': [{'ion_id': 1327, 'distance': 14.697473526000977, 'force': [0.9881269335746765, 1.1771571636199951, 0.006705602630972862], 'magnitude': 1.5369250774383545}, {'ion_id': 1330, 'distance': 8.471452713012695, 'force': [4.258534908294678, 1.36393404006958, 1.1857856512069702], 'magnitude': 4.62617826461792}, {'ion_id': 1341, 'distance': 10.060464859008789, 'force': [-0.05445399135351181, 2.8371944427490234, 1.6453436613082886], 'magnitude': 3.28021240234375}, {'ion_id': 1359, 'distance': 9.740442276000977, 'force': [1.1280900239944458, 2.8237078189849854, -1.7318087816238403], 'magnitude': 3.499296188354492}, {'ion_id': 1374, 'distance': 14.094215393066406, 'force': [0.387218713760376, 0.9749515056610107, -1.3010761737823486], 'magnitude': 1.6713072061538696}], 'glu_contributions': [{'resid': 423, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 4.355980396270752, 'force': [-12.280144691467285, -3.5702157020568848, -5.91953182220459], 'magnitude': 14.092169761657715}, {'resid': 423, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 4.083305835723877, 'force': [11.299105644226074, 6.346077919006348, 9.893199920654297], 'magnitude': 16.303922653198242}, {'resid': 423, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 4.050694465637207, 'force': [15.759501457214355, 4.56827974319458, 2.291504144668579], 'magnitude': 16.5674991607666}], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.595292091369629, 'force': [-0.33382272720336914, 2.524196147918701, 3.64918851852417], 'magnitude': 4.449672222137451}]}, 6574: {'frame': 6574, 'ionic_force': [9.922765612602234, 10.655503034591675, -1.8789064027369022], 'ionic_force_magnitude': 14.680984694259426, 'motion_vector': [0.2715606689453125, -0.07678985595703125, -0.05289459228515625], 'ionic_force_x': 9.922765612602234, 'ionic_force_y': 10.655503034591675, 'ionic_force_z': -1.8789064027369022, 'radial_force': 14.560254885228959, 'axial_force': -1.8789064027369022, 'glu_force': [17.74110221862793, 5.849688529968262, 4.713434934616089], 'glu_force_magnitude': 19.26608503854134, 'asn_force': [-0.9105595350265503, 3.097674608230591, 3.3834304809570312], 'asn_force_magnitude': 4.676783987397049, 'residue_force': [16.83054268360138, 8.947363138198853, 8.09686541557312], 'residue_force_magnitude': 20.70945928094772, 'total_force': [26.753308296203613, 19.602866172790527, 6.217959012836218], 'total_force_magnitude': 33.744257011606635, 'motion_component_total': 18.915048441471637, 'cosine_total_motion': 0.5605412629166984, 'cosine_glu_motion': 0.7446615484621248, 'cosine_asn_motion': -0.4945642363207028, 'cosine_residue_motion': 0.5810746892609628, 'cosine_ionic_motion': 0.468722362180727, 'motion_component_glu': 14.346712717603172, 'motion_component_asn': -2.3129701011639128, 'motion_component_residue': 12.033742616439259, 'motion_component_ionic': 6.881305825032376, 'ionic_contributions': [{'ion_id': 1327, 'distance': 14.467777252197266, 'force': [0.8655595183372498, 1.3287378549575806, -0.03194442763924599], 'magnitude': 1.5861141681671143}, {'ion_id': 1330, 'distance': 6.830624103546143, 'force': [6.645339488983154, 1.9468575716018677, 1.6377795934677124], 'magnitude': 7.115694999694824}, {'ion_id': 1341, 'distance': 9.315082550048828, 'force': [0.7769212126731873, 3.7414112091064453, 0.19452917575836182], 'magnitude': 3.826173782348633}, {'ion_id': 1359, 'distance': 9.518845558166504, 'force': [1.2521162033081055, 2.632829427719116, -2.2195000648498535], 'magnitude': 3.664118766784668}, {'ion_id': 1374, 'distance': 13.530313491821289, 'force': [0.3828291893005371, 1.005666971206665, -1.459770679473877], 'magnitude': 1.8135199546813965}], 'glu_contributions': [{'resid': 423, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 4.296910762786865, 'force': [-13.159367561340332, -2.9600107669830322, -5.27313232421875], 'magnitude': 14.482283592224121}, {'resid': 423, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 4.145949363708496, 'force': [12.05315113067627, 6.673973083496094, 7.764817237854004], 'magnitude': 15.814953804016113}, {'resid': 423, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 3.7728400230407715, 'force': [18.847318649291992, 2.1357262134552, 2.221750020980835], 'magnitude': 19.097614288330078}], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.4577436447143555, 'force': [-0.9105595350265503, 3.097674608230591, 3.3834304809570312], 'magnitude': 4.676784038543701}]}, 6575: {'frame': 6575, 'ionic_force': [6.102406769990921, 8.403478920459747, -1.6997588761150837], 'ionic_force_magnitude': 10.52364036776126, 'motion_vector': [-0.7413291931152344, 0.8488311767578125, 0.4405517578125], 'ionic_force_x': 6.102406769990921, 'ionic_force_y': 8.403478920459747, 'ionic_force_z': -1.6997588761150837, 'radial_force': 10.385462259959464, 'axial_force': -1.6997588761150837, 'glu_force': [9.891911029815674, 5.041309118270874, 3.3797075748443604], 'glu_force_magnitude': 11.60547822104761, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [9.891911029815674, 5.041309118270874, 3.3797075748443604], 'residue_force_magnitude': 11.60547822104761, 'total_force': [15.994317799806595, 13.444788038730621, 1.6799486987292767], 'total_force_magnitude': 20.96193585807299, 'motion_component_total': 0.2441303387280822, 'cosine_total_motion': 0.011646364170800628, 'cosine_glu_motion': -0.11144418221079178, 'cosine_asn_motion': None, 'cosine_residue_motion': -0.11144418221079178, 'cosine_ionic_motion': 0.14609900324491662, 'motion_component_glu': -1.2933630295098055, 'motion_component_asn': None, 'motion_component_residue': -1.2933630295098055, 'motion_component_ionic': 1.5374933682378877, 'ionic_contributions': [{'ion_id': 1330, 'distance': 8.94628620147705, 'force': [3.698859691619873, 1.877339243888855, -0.03207122161984444], 'magnitude': 4.148131370544434}, {'ion_id': 1341, 'distance': 9.998907089233398, 'force': [0.6937668323516846, 2.8005433082580566, 1.644039273262024], 'magnitude': 3.320725917816162}, {'ion_id': 1359, 'distance': 9.653382301330566, 'force': [1.2716120481491089, 2.7411482334136963, -1.8873075246810913], 'magnitude': 3.5626986026763916}, {'ion_id': 1374, 'distance': 13.633832931518555, 'force': [0.4381681978702545, 0.9844481348991394, -1.4244194030761719], 'magnitude': 1.7860851287841797}], 'glu_contributions': [{'resid': 423, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 5.190161228179932, 'force': [-8.700726509094238, -2.7343060970306396, -3.918245792388916], 'magnitude': 9.926314353942871}, {'resid': 423, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 5.058320999145508, 'force': [7.884056568145752, 4.601932525634766, 5.435170650482178], 'magnitude': 10.624368667602539}, {'resid': 423, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 4.899733543395996, 'force': [10.70858097076416, 3.173682689666748, 1.8627827167510986], 'magnitude': 11.323246955871582}], 'asn_contributions': []}, 6576: {'frame': 6576, 'ionic_force': [5.697530130855739, 9.966541528701782, -1.1423418633639812], 'ionic_force_magnitude': 11.536842920320106, 'motion_vector': [0.1239013671875, -0.14241409301757812, -0.3520050048828125], 'ionic_force_x': 5.697530130855739, 'ionic_force_y': 9.966541528701782, 'ionic_force_z': -1.1423418633639812, 'radial_force': 11.480148066786693, 'axial_force': -1.1423418633639812, 'glu_force': [13.319981575012207, 3.524713158607483, 3.651986300945282], 'glu_force_magnitude': 14.254210463979316, 'asn_force': [-0.8843836188316345, 1.9354552030563354, 3.2343735694885254], 'asn_force_magnitude': 3.87160091116085, 'residue_force': [12.435597956180573, 5.460168361663818, 6.886359870433807], 'residue_force_magnitude': 15.22758967567087, 'total_force': [18.13312808703631, 15.4267098903656, 5.744018007069826], 'total_force_magnitude': 24.49055848950594, 'motion_component_total': -4.937551273368648, 'cosine_total_motion': -0.20161039918646034, 'cosine_glu_motion': -0.02408403683996421, 'cosine_asn_motion': -0.9853282746516491, 'cosine_residue_motion': -0.2730633583144382, 'cosine_ionic_motion': -0.06756220075795798, 'motion_component_glu': -0.3432989299390812, 'motion_component_asn': -3.8147978459338727, 'motion_component_residue': -4.158096775872954, 'motion_component_ionic': -0.7794544974956932, 'ionic_contributions': [{'ion_id': 1327, 'distance': 14.209431648254395, 'force': [0.8476411700248718, 1.4078731536865234, 0.05625929310917854], 'magnitude': 1.6443136930465698}, {'ion_id': 1330, 'distance': 9.042120933532715, 'force': [3.670255661010742, 1.709186315536499, 0.31133517622947693], 'magnitude': 4.060667991638184}, {'ion_id': 1341, 'distance': 10.431806564331055, 'force': [0.002328316681087017, 2.6095755100250244, 1.5804171562194824], 'magnitude': 3.050837278366089}, {'ion_id': 1359, 'distance': 9.570117950439453, 'force': [0.9095866680145264, 3.105701446533203, -1.6332862377166748], 'magnitude': 3.624962568283081}, {'ion_id': 1374, 'distance': 13.339473724365234, 'force': [0.2677183151245117, 1.1342051029205322, -1.4570672512054443], 'magnitude': 1.8657810688018799}], 'glu_contributions': [{'resid': 423, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 5.070013046264648, 'force': [-9.858771324157715, -1.6822232007980347, -2.860715866088867], 'magnitude': 10.402353286743164}, {'resid': 423, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 4.59600305557251, 'force': [10.842070579528809, 3.475238084793091, 5.999281883239746], 'magnitude': 12.86931037902832}, {'resid': 423, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 4.669345378875732, 'force': [12.336682319641113, 1.7316982746124268, 0.5134202837944031], 'magnitude': 12.4682035446167}], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.998483657836914, 'force': [-0.8843836188316345, 1.9354552030563354, 3.2343735694885254], 'magnitude': 3.871600866317749}]}, 6577: {'frame': 6577, 'ionic_force': [10.770041853189468, 11.033284544944763, -1.4359604306519032], 'ionic_force_magnitude': 15.48512679081343, 'motion_vector': [2.2769126892089844, -2.477092742919922, -0.91888427734375], 'ionic_force_x': 10.770041853189468, 'ionic_force_y': 11.033284544944763, 'ionic_force_z': -1.4359604306519032, 'radial_force': 15.41840359340648, 'axial_force': -1.4359604306519032, 'glu_force': [13.212784767150879, 2.444539189338684, 5.092426776885986], 'glu_force_magnitude': 14.369629905784363, 'asn_force': [1.5786161422729492, -2.0778887271881104, -2.204274892807007], 'asn_force_magnitude': 3.4159154395680664, 'residue_force': [14.791400909423828, 0.36665046215057373, 2.8881518840789795], 'residue_force_magnitude': 15.07519136628813, 'total_force': [25.561442762613297, 11.399935007095337, 1.4521914534270763], 'total_force_magnitude': 28.02596535874831, 'motion_component_total': 8.208090849579504, 'cosine_total_motion': 0.29287450920998687, 'cosine_glu_motion': 0.3860802336174297, 'cosine_asn_motion': 0.9037247256917464, 'cosine_residue_motion': 0.5727872439444326, 'cosine_ionic_motion': -0.027561057188422215, 'motion_component_glu': 5.547830071021231, 'motion_component_asn': 3.0870472436098524, 'motion_component_residue': 8.634877314631083, 'motion_component_ionic': -0.4267864650515779, 'ionic_contributions': [{'ion_id': 1327, 'distance': 14.401464462280273, 'force': [1.0223180055618286, 1.2306550741195679, 0.052624136209487915], 'magnitude': 1.6007546186447144}, {'ion_id': 1330, 'distance': 6.132602691650391, 'force': [7.852027416229248, 3.727412223815918, 1.5429376363754272], 'magnitude': 8.827717781066895}, {'ion_id': 1341, 'distance': 12.76302719116211, 'force': [0.4523809254169464, 1.9864200353622437, 0.05863363668322563], 'magnitude': 2.0381243228912354}, {'ion_id': 1359, 'distance': 9.616036415100098, 'force': [1.0853403806686401, 2.987722158432007, -1.669343113899231], 'magnitude': 3.5904252529144287}, {'ion_id': 1374, 'distance': 13.458894729614258, 'force': [0.3579751253128052, 1.1010750532150269, -1.420812726020813], 'magnitude': 1.832817792892456}], 'glu_contributions': [{'resid': 423, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 5.099560737609863, 'force': [-9.278050422668457, -1.1631405353546143, -4.276401519775391], 'magnitude': 10.282155990600586}, {'resid': 423, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 5.051114082336426, 'force': [8.281856536865234, 2.693467140197754, 6.138312816619873], 'magnitude': 10.654707908630371}, {'resid': 423, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 4.314971446990967, 'force': [14.208978652954102, 0.9142125844955444, 3.230515480041504], 'magnitude': 14.60024356842041}], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.497316360473633, 'force': [5.828977584838867, -5.851686000823975, -5.808055877685547], 'magnitude': 10.097164154052734}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.54962682723999, 'force': [-4.250361442565918, 3.7737972736358643, 3.60378098487854], 'magnitude': 6.730108261108398}]}, 6578: {'frame': 6578, 'ionic_force': [11.297083020210266, 8.097006931900978, -3.776877298951149], 'ionic_force_magnitude': 14.403138829856085, 'motion_vector': [-1.2792587280273438, 0.96728515625, 1.4186248779296875], 'ionic_force_x': 11.297083020210266, 'ionic_force_y': 8.097006931900978, 'ionic_force_z': -3.776877298951149, 'radial_force': 13.899122491034303, 'axial_force': -3.776877298951149, 'glu_force': [2.6663551330566406, 10.47876501083374, 5.669543266296387], 'glu_force_magnitude': 12.208918326217832, 'asn_force': [2.245582327246666, -1.485685408115387, 1.8394064903259277], 'asn_force_magnitude': 3.2608767773380647, 'residue_force': [4.911937460303307, 8.993079602718353, 7.5089497566223145], 'residue_force_magnitude': 12.703815836284706, 'total_force': [16.209020480513573, 17.09008653461933, 3.7320724576711655], 'total_force_magnitude': 23.848097775877076, 'motion_component_total': 0.5090037912467364, 'cosine_total_motion': 0.02134358035723948, 'cosine_glu_motion': 0.5649245542342627, 'cosine_asn_motion': -0.24352713209933802, 'cosine_residue_motion': 0.48040729274232874, 'cosine_ionic_motion': -0.38838770133661316, 'motion_component_glu': 6.897117743121129, 'motion_component_asn': -0.7941119697144705, 'motion_component_residue': 6.103005773406658, 'motion_component_ionic': -5.594001982159921, 'ionic_contributions': [{'ion_id': 1327, 'distance': 13.392813682556152, 'force': [1.3949049711227417, 1.2103792428970337, -0.1234259232878685], 'magnitude': 1.8509489297866821}, {'ion_id': 1330, 'distance': 8.506098747253418, 'force': [4.5826263427734375, 0.2037651091814041, 0.11392490565776825], 'magnitude': 4.588568687438965}, {'ion_id': 1341, 'distance': 8.48983097076416, 'force': [2.695676326751709, 3.7334976196289062, 0.10549106448888779], 'magnitude': 4.606170177459717}, {'ion_id': 1359, 'distance': 9.237970352172852, 'force': [2.0399694442749023, 2.267669677734375, -2.4146974086761475], 'magnitude': 3.8903167247772217}, {'ion_id': 1374, 'distance': 13.924551963806152, 'force': [0.5839059352874756, 0.681695282459259, -1.458169937133789], 'magnitude': 1.7122832536697388}], 'glu_contributions': [{'resid': 423, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 5.0896315574646, 'force': [-3.710625648498535, -7.19097900390625, -6.408683776855469], 'magnitude': 10.32231330871582}, {'resid': 423, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 5.841547966003418, 'force': [1.5748701095581055, 5.566060543060303, 5.477377414703369], 'magnitude': 7.966361045837402}, {'resid': 423, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 4.315155982971191, 'force': [4.80211067199707, 12.103683471679688, 6.600849628448486], 'magnitude': 14.598994255065918}], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.115440845489502, 'force': [-4.598389625549316, 1.912513017654419, 13.058960914611816], 'magnitude': 13.976385116577148}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.4282073974609375, 'force': [4.9736857414245605, -3.1048879623413086, -8.152250289916992], 'magnitude': 10.041766166687012}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.098162651062012, 'force': [0.6328785419464111, -4.629727363586426, -17.557466506958008], 'magnitude': 18.16864013671875}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.347646713256836, 'force': [-0.0689331442117691, 3.4609742164611816, 6.506396770477295], 'magnitude': 7.369958877563477}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.1376166343688965, 'force': [1.3063408136367798, 0.8754426836967468, 7.983765602111816], 'magnitude': 8.137164115905762}]}, 6579: {'frame': 6579, 'ionic_force': [9.608516097068787, 8.373697221279144, -1.9300379157066345], 'ionic_force_magnitude': 12.89059475343761, 'motion_vector': [2.924358367919922, -6.608238220214844, -2.4186172485351562], 'ionic_force_x': 9.608516097068787, 'ionic_force_y': 8.373697221279144, 'ionic_force_z': -1.9300379157066345, 'radial_force': 12.745288805723, 'axial_force': -1.9300379157066345, 'glu_force': [15.032806396484375, 17.933500289916992, 3.2542089223861694], 'glu_force_magnitude': 23.625951335621856, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [15.032806396484375, 17.933500289916992, 3.2542089223861694], 'residue_force_magnitude': 23.625951335621856, 'total_force': [24.64132249355316, 26.307197511196136, 1.324171006679535], 'total_force_magnitude': 36.06961108716455, 'motion_component_total': -13.777088051440614, 'cosine_total_motion': -0.38195831993162854, 'cosine_glu_motion': -0.4577796658542562, 'cosine_asn_motion': None, 'cosine_residue_motion': -0.4577796658542562, 'cosine_ionic_motion': -0.2297495189460466, 'motion_component_glu': -10.815480107909892, 'motion_component_asn': None, 'motion_component_residue': -10.815480107909892, 'motion_component_ionic': -2.9616079435307228, 'ionic_contributions': [{'ion_id': 1327, 'distance': 12.721465110778809, 'force': [1.3253157138824463, 1.</t>
+          <t>{6569: {'frame': 6569, 'motion_vector': [0.9375572204589844, 4.542621612548828, 3.9090347290039062], 'ionic_force': [8.93659296631813, 4.198592029511929, -11.964962244033813], 'ionic_force_magnitude': 15.51293622681027, 'radial_force': 9.87374644579897, 'axial_force': -11.964962244033813, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.24319716542959213, -5.893840670585632, -0.811901792883873], 'asn_force_magnitude': 5.954467837918879, 'residue_force': [0.24319716542959213, -5.893840670585632, -0.811901792883873], 'residue_force_magnitude': 5.954467837918879, 'total_force': [9.179790131747723, -1.6952486410737038, -12.776864036917686], 'total_force_magnitude': 15.823737530554393, 'cosine_total_motion': -0.5109080261412919, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.822811478701697, 'cosine_residue_motion': -0.822811478701697, 'cosine_ionic_motion': -0.20531703184656236, 'motion_component_total': -8.084474507913425, 'motion_component_glu': None, 'motion_component_asn': -4.89940448659973, 'motion_component_residue': -4.89940448659973, 'motion_component_ionic': -3.1850700213136953, 'motion_component_percent_total': 51.090802614129196, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 82.2811478701697, 'motion_component_percent_residue': 82.2811478701697, 'motion_component_percent_ionic': 20.531703184656237, 'ionic_contributions': [{'ion_id': 1327, 'distance': 10.281067848205566, 'force': [2.5776994228363037, 1.23420250415802, -1.3029985427856445], 'magnitude': 3.1409544944763184, 'cosine_ionic_motion': 0.15377314388751984, 'motion_component_ionic': 0.4829944372177124, 'motion_component_percent_ionic': 15.377314388751984}, {'ion_id': 1330, 'distance': 7.982583522796631, 'force': [3.5478971004486084, -3.1198573112487793, -2.1965181827545166], 'magnitude': 5.210160732269287, 'cosine_ionic_motion': -0.614861786365509, 'motion_component_ionic': -3.203528881072998, 'motion_component_percent_ionic': 61.4861786365509}, {'ion_id': 1341, 'distance': 6.964383125305176, 'force': [1.5748634338378906, 5.740958213806152, -3.378621816635132], 'magnitude': 6.844989776611328, 'cosine_ionic_motion': 0.3455697000026703, 'motion_component_ionic': 2.3654210567474365, 'motion_component_percent_ionic': 34.55697000026703}, {'ion_id': 1359, 'distance': 9.398062705993652, 'force': [1.0105098485946655, 0.24263377487659454, -3.6123909950256348], 'magnitude': 3.7589054107666016, 'cosine_ionic_motion': -0.5294201374053955, 'motion_component_ionic': -1.9900403022766113, 'motion_component_percent_ionic': 52.94201374053955}, {'ion_id': 1374, 'distance': 14.902193069458008, 'force': [0.22562316060066223, 0.10065484791994095, -1.4744327068328857], 'magnitude': 1.494987964630127, 'cosine_ionic_motion': -0.5618215203285217, 'motion_component_ionic': -0.8399164080619812, 'motion_component_percent_ionic': 56.18215203285217}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.862966537475586, 'force': [-3.78678035736084, 3.9053030014038086, -1.7953109741210938], 'magnitude': 5.728371620178223, 'cosine_with_motion': 0.20640410482883453, 'motion_component': 1.1823594570159912, 'motion_component_percent': 20.640410482883453}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.223381042480469, 'force': [4.336669921875, -1.6977781057357788, 2.0930356979370117], 'magnitude': 5.105874538421631, 'cosine_with_motion': 0.14643268287181854, 'motion_component': 0.7476668953895569, 'motion_component_percent': 14.643268287181854}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.000786304473877, 'force': [7.137111663818359, 9.86938190460205, -0.7356123328208923], 'magnitude': 12.201810836791992, 'cosine_with_motion': 0.6572846174240112, 'motion_component': 8.020062446594238, 'motion_component_percent': 65.72846174240112}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.115147590637207, 'force': [-5.323076248168945, -6.185309886932373, 1.0383859872817993], 'magnitude': 8.226264953613281, 'cosine_with_motion': -0.5817508101463318, 'motion_component': -4.7856364250183105, 'motion_component_percent': 58.17508101463318}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.198151111602783, 'force': [-2.1941421031951904, -4.665300369262695, 0.022443369030952454], 'magnitude': 5.155559539794922, 'cosine_with_motion': -0.7406410574913025, 'motion_component': -3.8184192180633545, 'motion_component_percent': 74.06410574913025}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.206618309020996, 'force': [0.07341428846120834, -7.1201372146606445, -1.4348435401916504], 'magnitude': 7.263643741607666, 'cosine_with_motion': -0.8598215579986572, 'motion_component': -6.2454376220703125, 'motion_component_percent': 85.98215579986572}]}, 6570: {'frame': 6570, 'motion_vector': [0.08165740966796875, 0.8572654724121094, 0.46636962890625], 'ionic_force': [12.369088254868984, 9.554802000522614, -1.3525469191372395], 'ionic_force_magnitude': 15.688147395227915, 'radial_force': 15.629734019679567, 'axial_force': -1.3525469191372395, 'glu_force': [1.7606010437011719, 2.221771240234375, -0.6299586296081543], 'glu_force_magnitude': 2.903933772321957, 'asn_force': [0.8742416501045227, -0.7024664878845215, 2.305647373199463], 'asn_force_magnitude': 2.5639359272259274, 'residue_force': [2.6348426938056946, 1.5193047523498535, 1.6756887435913086], 'residue_force_magnitude': 3.4725517587233625, 'total_force': [15.003930948674679, 11.074106752872467, 0.32314182445406914], 'total_force_magnitude': 18.650957212039412, 'cosine_total_motion': 0.5950810072714275, 'cosine_glu_motion': 0.616979428830821, 'cosine_asn_motion': 0.2168416064553393, 'cosine_residue_motion': 0.6760548290232078, 'cosine_ionic_motion': 0.557822080474634, 'motion_component_total': 11.09883040431671, 'motion_component_glu': 1.7916674002097324, 'motion_component_asn': 0.55596798530823, 'motion_component_residue': 2.3476353855179624, 'motion_component_ionic': 8.751195018798747, 'motion_component_percent_total': 59.508100727142754, 'motion_component_percent_glu': 61.6979428830821, 'motion_component_percent_asn': 21.68416064553393, 'motion_component_percent_residue': 67.60548290232077, 'motion_component_percent_ionic': 55.7822080474634, 'ionic_contributions': [{'ion_id': 1327, 'distance': 12.443742752075195, 'force': [1.5750917196273804, 1.453436017036438, -0.059865642338991165], 'magnitude': 2.1440553665161133, 'cosine_ionic_motion': 0.6413606405258179, 'motion_component_ionic': 1.375112771987915, 'motion_component_percent_ionic': 64.13606405258179}, {'ion_id': 1330, 'distance': 6.1113481521606445, 'force': [8.851373672485352, -0.5448993444442749, 0.612082302570343], 'magnitude': 8.889227867126465, 'cosine_ionic_motion': 0.062158212065696716, 'motion_component_ionic': 0.5525385141372681, 'motion_component_percent_ionic': 6.215821206569672}, {'ion_id': 1341, 'distance': 7.490889549255371, 'force': [-0.1118030920624733, 4.923777103424072, 3.27870774269104], 'magnitude': 5.9165873527526855, 'cosine_ionic_motion': 0.990800678730011, 'motion_component_ionic': 5.86215877532959, 'motion_component_percent_ionic': 99.0800678730011}, {'ion_id': 1359, 'distance': 8.462321281433105, 'force': [1.5930393934249878, 2.9040167331695557, -3.243910789489746], 'magnitude': 4.636167049407959, 'cosine_ionic_motion': 0.24375799298286438, 'motion_component_ionic': 1.1301027536392212, 'motion_component_percent_ionic': 24.375799298286438}, {'ion_id': 1374, 'distance': 12.411674499511719, 'force': [0.4613865613937378, 0.8184714913368225, -1.9395605325698853], 'magnitude': 2.155149221420288, 'cosine_ionic_motion': -0.07828592509031296, 'motion_component_ionic': -0.16871784627437592, 'motion_component_percent_ionic': 7.828592509031296}], 'glu_contributions': [{'resid': 423, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 5.885604381561279, 'force': [-4.789684295654297, -5.065373420715332, -3.3144640922546387], 'magnitude': 7.7191162109375, 'cosine_with_motion': -0.8306428790092468, 'motion_component': -6.411828994750977, 'motion_component_percent': 83.06428790092468}, {'resid': 423, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 5.172755241394043, 'force': [6.550285339355469, 7.287144660949707, 2.6845054626464844], 'magnitude': 10.159492492675781, 'cosine_with_motion': 0.8074710369110107, 'motion_component': 8.203495979309082, 'motion_component_percent': 80.74710369110107}], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.012881755828857, 'force': [-4.670202732086182, 1.571510910987854, 8.02849292755127], 'magnitude': 9.420039176940918, 'cosine_with_motion': 0.5105647444725037, 'motion_component': 4.809539794921875, 'motion_component_percent': 51.056474447250366}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.714416027069092, 'force': [3.6295950412750244, -1.6445144414901733, -4.525853157043457], 'magnitude': 6.030068874359131, 'cosine_with_motion': -0.5459633469581604, 'motion_component': -3.292196750640869, 'motion_component_percent': 54.59633469581604}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.604116439819336, 'force': [3.857551336288452, -3.9069876670837402, -13.306673049926758], 'magnitude': 14.394887924194336, 'cosine_with_motion': -0.6554586291313171, 'motion_component': -9.435253143310547, 'motion_component_percent': 65.54586291313171}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.168186187744141, 'force': [-1.0959246158599854, 2.225980281829834, 4.5875444412231445], 'magnitude': 5.215515613555908, 'cosine_with_motion': 0.7749630808830261, 'motion_component': 4.041831970214844, 'motion_component_percent': 77.49630808830261}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 4.269467353820801, 'force': [-0.8467773795127869, 1.051544427871704, 7.522136211395264], 'magnitude': 7.642336845397949, 'cosine_with_motion': 0.5799334049224854, 'motion_component': 4.432046413421631, 'motion_component_percent': 57.993340492248535}]}, 6571: {'frame': 6571, 'motion_vector': [-0.7143974304199219, 2.6378211975097656, 0.46242523193359375], 'ionic_force': [10.874882519245148, 11.021745204925537, -1.5739329904317856], 'ionic_force_magnitude': 15.563393017849684, 'radial_force': 15.483602202642729, 'axial_force': -1.5739329904317856, 'glu_force': [7.676974296569824, 7.6012349128723145, 1.5161144137382507], 'glu_force_magnitude': 10.909322135971951, 'asn_force': [1.804943561553955, -2.185672402381897, -6.2858805656433105], 'asn_force_magnitude': 6.8954535453776495, 'residue_force': [9.48191785812378, 5.4155625104904175, -4.76976615190506], 'residue_force_magnitude': 11.915777470106393, 'total_force': [20.356800377368927, 16.437307715415955, -6.343699142336845], 'total_force_magnitude': 26.922609928159005, 'cosine_total_motion': 0.34684928461947456, 'cosine_glu_motion': 0.5049181651682594, 'cosine_asn_motion': -0.5212199278497726, 'cosine_residue_motion': 0.16064978735241064, 'cosine_ionic_motion': 0.4770052949537086, 'motion_component_total': 9.338087993671115, 'motion_component_glu': 5.5083149161244345, 'motion_component_asn': -3.5940477994131967, 'motion_component_residue': 1.9142671167112377, 'motion_component_ionic': 7.423820876959877, 'motion_component_percent_total': 34.68492846194746, 'motion_component_percent_glu': 50.491816516825935, 'motion_component_percent_asn': 52.12199278497726, 'motion_component_percent_residue': 16.064978735241063, 'motion_component_percent_ionic': 47.70052949537086, 'ionic_contributions': [{'ion_id': 1327, 'distance': 14.060022354125977, 'force': [0.9435466527938843, 1.3866626024246216, -0.0861724466085434], 'magnitude': 1.6794461011886597, 'cosine_ionic_motion': 0.6324180960655212, 'motion_component_ionic': 1.0621120929718018, 'motion_component_percent_ionic': 63.241809606552124}, {'ion_id': 1330, 'distance': 6.742351531982422, 'force': [7.051734924316406, 1.6229393482208252, 0.9881018400192261], 'magnitude': 7.3032355308532715, 'cosine_ionic_motion': -0.014810262247920036, 'motion_component_ionic': -0.10816283524036407, 'motion_component_percent_ionic': 1.4810262247920036}, {'ion_id': 1341, 'distance': 8.82316780090332, 'force': [0.5937607288360596, 3.663236141204834, 2.101393938064575], 'magnitude': 4.264704704284668, 'cosine_ionic_motion': 0.8637998104095459, 'motion_component_ionic': 3.6838512420654297, 'motion_component_percent_ionic': 86.37998104095459}, {'ion_id': 1359, 'distance': 8.525839805603027, 'force': [1.727158784866333, 3.3323826789855957, -2.602457046508789], 'magnitude': 4.5673441886901855, 'cosine_ionic_motion': 0.5018377304077148, 'motion_component_ionic': 2.2920656204223633, 'motion_component_percent_ionic': 50.183773040771484}, {'ion_id': 1374, 'distance': 12.040011405944824, 'force': [0.5586814284324646, 1.0165244340896606, -1.9747992753982544], 'magnitude': 2.290257453918457, 'cosine_ionic_motion': 0.2156764268875122, 'motion_component_ionic': 0.49395453929901123, 'motion_component_percent_ionic': 21.56764268875122}], 'glu_contributions': [{'resid': 423, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 5.272819995880127, 'force': [-7.410064220428467, -5.5089592933654785, -2.6905951499938965], 'magnitude': 9.617535591125488, 'cosine_with_motion': -0.3932235836982727, 'motion_component': -3.78184175491333, 'motion_component_percent': 39.32235836982727}, {'resid': 423, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 5.610739707946777, 'force': [5.298938274383545, 5.913795471191406, 3.393536329269409], 'magnitude': 8.635265350341797, 'cosine_with_motion': 0.5591650605201721, 'motion_component': 4.82853889465332, 'motion_component_percent': 55.91650605201721}, {'resid': 423, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 4.725030899047852, 'force': [9.788100242614746, 7.196398735046387, 0.813173234462738], 'magnitude': 12.176054954528809, 'cosine_with_motion': 0.3664255738258362, 'motion_component': 4.461617946624756, 'motion_component_percent': 36.64255738258362}], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.708808422088623, 'force': [-3.2005159854888916, 1.111762285232544, 6.424706935882568], 'magnitude': 7.263344764709473, 'cosine_with_motion': 0.406820148229599, 'motion_component': 2.9548749923706055, 'motion_component_percent': 40.6820148229599}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.992682933807373, 'force': [2.94905161857605, -1.6493879556655884, -4.318172454833984], 'magnitude': 5.483064651489258, 'cosine_with_motion': -0.5563071966171265, 'motion_component': -3.0502681732177734, 'motion_component_percent': 55.63071966171265}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.889748573303223, 'force': [2.056407928466797, -1.6480467319488525, -8.392415046691895], 'magnitude': 8.796448707580566, 'cosine_with_motion': -0.3977349102497101, 'motion_component': -3.498654842376709, 'motion_component_percent': 39.77349102497101}]}, 6572: {'frame': 6572, 'motion_vector': [0.8923988342285156, -0.882781982421875, -0.6154251098632812], 'ionic_force': [4.297864839434624, 8.788159370422363, -1.320813924074173], 'ionic_force_magnitude': 9.871572150372959, 'radial_force': 9.782810807635544, 'axial_force': -1.320813924074173, 'glu_force': [13.541619300842285, 3.0024799704551697, 4.42834997177124], 'glu_force_magnitude': 14.560241163332945, 'asn_force': [-1.4802942276000977, 2.662510633468628, 3.6407511234283447], 'asn_force_magnitude': 4.747136254242597, 'residue_force': [12.061325073242188, 5.664990603923798, 8.069101095199585], 'residue_force_magnitude': 15.578128050234941, 'total_force': [16.35918991267681, 14.453149974346161, 6.748287171125412], 'total_force_magnitude': 22.848545216795422, 'cosine_total_motion': -0.07241532933293089, 'cosine_glu_motion': 0.32957797866470223, 'cosine_asn_motion': -0.8908319332372551, 'cosine_residue_motion': 0.03657912445813258, 'cosine_ionic_motion': -0.22533586115184634, 'motion_component_total': -1.6545849266526034, 'motion_component_glu': 4.798734851481864, 'motion_component_asn': -4.228900566707594, 'motion_component_residue': 0.5698342847742701, 'motion_component_ionic': -2.2244192114268744, 'motion_component_percent_total': 7.241532933293089, 'motion_component_percent_glu': 32.95779786647022, 'motion_component_percent_asn': 89.08319332372551, 'motion_component_percent_residue': 3.657912445813258, 'motion_component_percent_ionic': 22.533586115184633, 'ionic_contributions': [{'ion_id': 1330, 'distance': 8.661239624023438, 'force': [3.4389588832855225, 2.7700512409210205, 0.2946772277355194], 'magnitude': 4.425658702850342, 'cosine_ionic_motion': 0.07147438824176788, 'motion_component_ionic': 0.3163212537765503, 'motion_component_percent_ionic': 7.147438824176788}, {'ion_id': 1341, 'distance': 11.687585830688477, 'force': [-0.10774736106395721, 2.0299341678619385, 1.3322513103485107], 'magnitude': 2.430459976196289, 'cosine_ionic_motion': -0.7969983220100403, 'motion_component_ionic': -1.937072515487671, 'motion_component_percent_ionic': 79.69983220100403}, {'ion_id': 1359, 'distance': 10.02340030670166, 'force': [0.6919946074485779, 2.870731830596924, -1.4831961393356323], 'magnitude': 3.304516315460205, 'cosine_ionic_motion': -0.2173062562942505, 'motion_component_ionic': -0.7180920839309692, 'motion_component_percent_ionic': 21.73062562942505}, {'ion_id': 1374, 'distance': 13.351118087768555, 'force': [0.2746587097644806, 1.1174421310424805, -1.4645463228225708], 'magnitude': 1.8625279664993286, 'cosine_ionic_motion': 0.061434898525476456, 'motion_component_ionic': 0.1144242137670517, 'motion_component_percent_ionic': 6.143489852547646}], 'glu_contributions': [{'resid': 423, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 4.82476282119751, 'force': [-10.750345230102539, -0.609584391117096, -4.000533580780029], 'magnitude': 11.48676586151123, 'cosine_with_motion': -0.4105861186981201, 'motion_component': -4.716306686401367, 'motion_component_percent': 41.05861186981201}, {'resid': 423, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 4.59662389755249, 'force': [10.555639266967773, 2.346975326538086, 6.9713640213012695], 'magnitude': 12.865835189819336, 'cosine_with_motion': 0.16999481618404388, 'motion_component': 2.1871252059936523, 'motion_component_percent': 16.99948161840439}, {'resid': 423, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 4.426905155181885, 'force': [13.73632526397705, 1.2650890350341797, 1.45751953125], 'magnitude': 13.871245384216309, 'cosine_with_motion': 0.528281033039093, 'motion_component': 7.327916145324707, 'motion_component_percent': 52.8281033039093}], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.417150974273682, 'force': [-1.4802942276000977, 2.662510633468628, 3.6407511234283447], 'magnitude': 4.747136116027832, 'cosine_with_motion': -0.8908319473266602, 'motion_component': -4.22890043258667, 'motion_component_percent': 89.08319473266602}]}, 6573: {'frame': 6573, 'motion_vector': [-0.3231239318847656, -0.48430633544921875, 0.06146240234375], 'ionic_force': [6.707516588270664, 9.176944971084595, -0.1950500402599573], 'ionic_force_magnitude': 11.368603357600545, 'radial_force': 11.366930007008971, 'axial_force': -0.1950500402599573, 'glu_force': [14.778462409973145, 7.344141960144043, 6.265172243118286], 'glu_force_magnitude': 17.651961805127424, 'asn_force': [-0.33382272720336914, 2.524196147918701, 3.64918851852417], 'asn_force_magnitude': 4.449671971066376, 'residue_force': [14.444639682769775, 9.868338108062744, 9.914360761642456], 'residue_force_magnitude': 20.107865672221063, 'total_force': [21.15215627104044, 19.04528307914734, 9.719310721382499], 'total_force_magnitude': 30.07659427824487, 'cosine_total_motion': -0.8780739299029601, 'cosine_glu_motion': -0.7690050360806358, 'cosine_asn_motion': -0.3417756668672356, 'cosine_residue_motion': -0.7507130481258231, 'cosine_ionic_motion': -0.9952177809364312, 'motion_component_total': -26.409473335995354, 'motion_component_glu': -13.574447524846018, 'motion_component_asn': -1.5207896052516574, 'motion_component_residue': -15.095237130097676, 'motion_component_ionic': -11.314236205897675, 'motion_component_percent_total': 87.80739299029601, 'motion_component_percent_glu': 76.90050360806357, 'motion_component_percent_asn': 34.17756668672356, 'motion_component_percent_residue': 75.07130481258231, 'motion_component_percent_ionic': 99.52177809364312, 'ionic_contributions': [{'ion_id': 1327, 'distance': 14.697473526000977, 'force': [0.9881269335746765, 1.1771571636199951, 0.006705602630972862], 'magnitude': 1.5369250774383545, 'cosine_ionic_motion': -0.9880008697509766, 'motion_component_ionic': -1.518483281135559, 'motion_component_percent_ionic': 98.80008697509766}, {'ion_id': 1330, 'distance': 8.471452713012695, 'force': [4.258534908294678, 1.36393404006958, 1.1857856512069702], 'magnitude': 4.62617826461792, 'cosine_ionic_motion': -0.7250603437423706, 'motion_component_ionic': -3.3542585372924805, 'motion_component_percent_ionic': 72.50603437423706}, {'ion_id': 1341, 'distance': 10.060464859008789, 'force': [-0.05445399135351181, 2.8371944427490234, 1.6453436613082886], 'magnitude': 3.28021240234375, 'cosine_ionic_motion': -0.6537031531333923, 'motion_component_ionic': -2.144285202026367, 'motion_component_percent_ionic': 65.37031531333923}, {'ion_id': 1359, 'distance': 9.740442276000977, 'force': [1.1280900239944458, 2.8237078189849854, -1.7318087816238403], 'magnitude': 3.499296188354492, 'cosine_ionic_motion': -0.8974276185035706, 'motion_component_ionic': -3.1403651237487793, 'motion_component_percent_ionic': 89.74276185035706}, {'ion_id': 1374, 'distance': 14.094215393066406, 'force': [0.387218713760376, 0.9749515056610107, -1.3010761737823486], 'magnitude': 1.6713072061538696, 'cosine_ionic_motion': -0.6921791434288025, 'motion_component_ionic': -1.1568440198898315, 'motion_component_percent_ionic': 69.21791434288025}], 'glu_contributions': [{'resid': 423, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 4.355980396270752, 'force': [-12.280144691467285, -3.5702157020568848, -5.91953182220459], 'magnitude': 14.092169761657715, 'cosine_with_motion': 0.6464467644691467, 'motion_component': 9.109837532043457, 'motion_component_percent': 64.64467644691467}, {'resid': 423, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 4.083305835723877, 'force': [11.299105644226074, 6.346077919006348, 9.893199920654297], 'magnitude': 16.303922653198242, 'cosine_with_motion': -0.6407986879348755, 'motion_component': -10.447532653808594, 'motion_component_percent': 64.07986879348755}, {'resid': 423, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 4.050694465637207, 'force': [15.759501457214355, 4.56827974319458, 2.291504144668579], 'magnitude': 16.5674991607666, 'cosine_with_motion': -0.7385998368263245, 'motion_component': -12.2367525100708, 'motion_component_percent': 73.85998368263245}], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.595292091369629, 'force': [-0.33382272720336914, 2.524196147918701, 3.64918851852417], 'magnitude': 4.449672222137451, 'cosine_with_motion': -0.34177565574645996, 'motion_component': -1.520789623260498, 'motion_component_percent': 34.177565574645996}]}, 6574: {'frame': 6574, 'motion_vector': [0.2715606689453125, -0.07678985595703125, -0.05289459228515625], 'ionic_force': [9.922765612602234, 10.655503034591675, -1.8789064027369022], 'ionic_force_magnitude': 14.680984694259426, 'radial_force': 14.560254885228959, 'axial_force': -1.8789064027369022, 'glu_force': [17.74110221862793, 5.849688529968262, 4.713434934616089], 'glu_force_magnitude': 19.26608503854134, 'asn_force': [-0.9105595350265503, 3.097674608230591, 3.3834304809570312], 'asn_force_magnitude': 4.676783987397049, 'residue_force': [16.83054268360138, 8.947363138198853, 8.09686541557312], 'residue_force_magnitude': 20.70945928094772, 'total_force': [26.753308296203613, 19.602866172790527, 6.217959012836218], 'total_force_magnitude': 33.744257011606635, 'cosine_total_motion': 0.5605412629166984, 'cosine_glu_motion': 0.7446615484621248, 'cosine_asn_motion': -0.4945642363207028, 'cosine_residue_motion': 0.5810746892609628, 'cosine_ionic_motion': 0.468722362180727, 'motion_component_total': 18.915048441471637, 'motion_component_glu': 14.346712717603172, 'motion_component_asn': -2.3129701011639128, 'motion_component_residue': 12.033742616439259, 'motion_component_ionic': 6.881305825032376, 'motion_component_percent_total': 56.05412629166984, 'motion_component_percent_glu': 74.46615484621249, 'motion_component_percent_asn': 49.456423632070276, 'motion_component_percent_residue': 58.10746892609628, 'motion_component_percent_ionic': 46.8722362180727, 'ionic_contributions': [{'ion_id': 1327, 'distance': 14.467777252197266, 'force': [0.8655595183372498, 1.3287378549575806, -0.03194442763924599], 'magnitude': 1.5861141681671143, 'cosine_ionic_motion': 0.29579493403434753, 'motion_component_ionic': 0.46916455030441284, 'motion_component_percent_ionic': 29.579493403434753}, {'ion_id': 1330, 'distance': 6.830624103546143, 'force': [6.645339488983154, 1.9468575716018677, 1.6377795934677124], 'magnitude': 7.115694999694824, 'cosine_ionic_motion': 0.7677054405212402, 'motion_component_ionic': 5.462757587432861, 'motion_component_percent_ionic': 76.77054405212402}, {'ion_id': 1341, 'distance': 9.315082550048828, 'force': [0.7769212126731873, 3.7414112091064453, 0.19452917575836182], 'magnitude': 3.826173782348633, 'cosine_ionic_motion': -0.07883856445550919, 'motion_component_ionic': -0.3016500473022461, 'motion_component_percent_ionic': 7.883856445550919}, {'ion_id': 1359, 'distance': 9.518845558166504, 'force': [1.2521162033081055, 2.632829427719116, -2.2195000648498535], 'magnitude': 3.664118766784668, 'cosine_ionic_motion': 0.24262121319770813, 'motion_component_ionic': 0.888992965221405, 'motion_component_percent_ionic': 24.262121319770813}, {'ion_id': 1374, 'distance': 13.530313491821289, 'force': [0.3828291893005371, 1.005666971206665, -1.459770679473877], 'magnitude': 1.8135199546813965, 'cosine_ionic_motion': 0.19963432848453522, 'motion_component_ionic': 0.36204084753990173, 'motion_component_percent_ionic': 19.96343284845352}], 'glu_contributions': [{'resid': 423, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 4.296910762786865, 'force': [-13.159367561340332, -2.9600107669830322, -5.27313232421875], 'magnitude': 14.482283592224121, 'cosine_with_motion': -0.7376624941825867, 'motion_component': -10.683037757873535, 'motion_component_percent': 73.76624941825867}, {'resid': 423, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 4.145949363708496, 'force': [12.05315113067627, 6.673973083496094, 7.764817237854004], 'magnitude': 15.814953804016113, 'cosine_with_motion': 0.5175147652626038, 'motion_component': 8.18447208404541, 'motion_component_percent': 51.751476526260376}, {'resid': 423, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 3.7728400230407715, 'force': [18.847318649291992, 2.1357262134552, 2.221750020980835], 'magnitude': 19.097614288330078, 'cosine_with_motion': 0.8820618987083435, 'motion_component': 16.845277786254883, 'motion_component_percent': 88.20618987083435}], 'asn_contributions': [{'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.4577436447143555, 'force': [-0.9105595350265503, 3.097674608230591, 3.3834304809570312], 'magnitude': 4.676784038543701, 'cosine_with_motion': -0.4945642352104187, 'motion_component': -2.3129701614379883, 'motion_component_percent': 49.45642352104187}]}, 6575: {'frame': 6575, 'motion_vector': [-0.7413291931152344, 0.8488311767578125, 0.4405517578125], 'ionic_force': [6.102406769990921, 8.403478920459747, -1.6997588761150837], 'ionic_force_magnitude': 10.52364036776126, 'radial_force': 10.385462259959464, 'axial_force': -1.6997588761150837, 'glu_force': [9.891911029815674, 5.041309118270874, 3.3797075748443604], 'glu_force_magnitude': 11.60547822104761, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [9.891911029815674, 5.041309118270874, 3.3797075748443604], 'residue_force_magnitude': 11.60547822104761, 'total_force': [15.994317799806595, 13.444788038730621, 1.6799486987292767], 'total_force_magnitude': 20.96193585807299, 'cosine_total_motion': 0.011646364170800628, 'cosine_glu_motion': -0.11144418221079178, 'cosine_asn_motion': None, 'cosine_residue_motion': -0.11144418221079178, 'cosine_ionic_motion': 0.14609900324491662, 'motion_component_total': 0.2441303387280822, 'motion_component_glu': -1.2933630295098055, 'motion_component_asn': None, 'motion_component_residue': -1.2933630295098055, 'motion_component_ionic': 1.5374933682378877, 'motion_component_percent_total': 1.1646364170800627, 'motion_component_percent_glu': 11.144418221079178, 'motion_component_percent_asn': None, 'motion_component_percent_residue': 11.144418221079178, 'motion_component_percent_ionic': 14.609900324491662, 'ionic_contributions': [{'ion_id': 1330, 'distance': 8.94628620147705, 'force': [3.698859691619873, 1.877339243888855, -0.03207122161984444], 'magnitude': 4.148131370544434, 'cosine_ionic_motion': -0.23163475096225739, 'motion_component_ionic': -0.9608513712882996, 'motion_component_percent_ionic': 23.16347509622574}, {'ion_id': 1341, 'distance': 9.998907089233398, 'force': [0.6937668323516846, 2.8005433082580566, 1.644039273262024], 'magnitude': 3.320725917816162, 'cosine_ionic_motion': 0.6438655853271484, 'motion_component_ionic': 2.138101100921631, 'motion_component_percent_ionic': 64.38655853271484}, {'ion_id': 1359, 'distance': 9.653382301330566, 'force': [1.2716120481491089, 2.7411482334136963, -1.8873075246810913], 'magnitude': 3.5626986026763916, 'cosine_ionic_motion': 0.1281922161579132, 'motion_component_ionic': 0.45671021938323975, 'motion_component_percent_ionic': 12.81922161579132}, {'ion_id': 1374, 'distance': 13.633832931518555, 'force': [0.4381681978702545, 0.9844481348991394, -1.4244194030761719], 'magnitude': 1.7860851287841797, 'cosine_ionic_motion': -0.05400992929935455, 'motion_component_ionic': -0.09646633267402649, 'motion_component_percent_ionic': 5.400992929935455}], 'glu_contributions': [{'resid': 423, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.8054, 'distance': 5.190161228179932, 'force': [-8.700726509094238, -2.7343060970306396, -3.918245792388916], 'magnitude': 9.926314353942871, 'cosine_with_motion': 0.20006026327610016, 'motion_component': 1.98586106300354, 'motion_component_percent': 20.006026327610016}, {'resid': 423, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8188, 'distance': 5.058320999145508, 'force': [7.884056568145752, 4.601932525634766, 5.435170650482178], 'magnitude': 10.624368667602539, 'cosine_with_motion': 0.035474810749292374, 'motion_component': 0.3768974542617798, 'motion_component_percent': 3.5474810749292374}, {'resid': 423, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8188, 'distance': 4.899733543395996, 'force': [10.70858097076416, 3.173682689666748, 1.8627827167510986], 'magnitude': 11.323246955871582, 'cosine_with_motion': -0.32288628816604614, 'motion_component': -3.656121253967285, 'motion_component_percent': 32.288628816604614}], 'asn_contributions': []}, 6576: {'frame': 6576, 'motion_vector': [0.1239013671875, -0.14241409301757812, -0.3520050048828125], 'ionic_force': [5.697530130855739, 9.966541528701782, -1.1423418633639812], 'ionic_force_magnitude': 11.536842920320106, 'radial_force': 11.480148066786693, 'axial_force': -1.1423418633639812, 'glu_force': [13.319981575012207, 3.524713158607483, 3.651986300945282], 'glu_force_magnitude': 14.254210463979316, 'asn_force': [-0.8843836188316345, 1.9354552030563354, 3.2343735694885254], 'asn_force_magnitude': 3.87160091116085, 'residue_force': [12.435597956180573, 5.460168361663818, 6.886359870433807], 'residue_force_magnitude': 15.22758967567087, 'total_force': [18.13312808703631, 15.4267098903656, 5.744018007069826], 'total_force_magnitude': 24.49055848950594, 'cosine_total_motion': -0.20161039918646034, 'cosine_glu_motion': -0.02408403683996421, 'cosine_asn_motion': -0.9853282746516491, 'cosine_residue_motion': -0.2730633583144382, 'cosine_ionic_motion': -0.06756220075795798, 'motion_component_total': -4.937551273368648, 'motion_component_glu': -0.3432989299390</t>
         </is>
       </c>
     </row>
@@ -835,7 +835,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>{6716: {'frame': 6716, 'ionic_force': [3.5372003354132175, 2.635218560695648, -13.300951480865479], 'ionic_force_magnitude': 14.013260625986366, 'motion_vector': [2.1366920471191406, 6.534908294677734, 0.9935302734375], 'ionic_force_x': 3.5372003354132175, 'ionic_force_y': 2.635218560695648, 'ionic_force_z': -13.300951480865479, 'radial_force': 4.4109140861597185, 'axial_force': -13.300951480865479, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-3.9373409748077393, 5.4104814529418945, 0.5344047546386719], 'asn_force_magnitude': 6.712790175948345, 'residue_force': [-3.9373409748077393, 5.4104814529418945, 0.5344047546386719], 'residue_force_magnitude': 6.712790175948345, 'total_force': [-0.4001406393945217, 8.045700013637543, -12.766546726226807], 'total_force_magnitude': 15.095632366803141, 'motion_component_total': 5.619733723999221, 'cosine_total_motion': 0.37227547594214055, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.5891865868447074, 'cosine_residue_motion': 0.5891865868447074, 'cosine_ionic_motion': 0.11879089645564639, 'motion_component_glu': None, 'motion_component_asn': 3.955085931971688, 'motion_component_residue': 3.955085931971688, 'motion_component_ionic': 1.6646477920275329, 'ionic_contributions': [{'ion_id': 1327, 'distance': 10.33717155456543, 'force': [1.9013433456420898, -1.8896634578704834, -1.5707390308380127], 'magnitude': 3.106952667236328}, {'ion_id': 1330, 'distance': 10.157370567321777, 'force': [1.3640469312667847, -2.8642194271087646, -0.5391140580177307], 'magnitude': 3.217921733856201}, {'ion_id': 1341, 'distance': 5.020081996917725, 'force': [3.074054718017578, 10.045456886291504, -7.949360370635986], 'magnitude': 13.173964500427246}, {'ion_id': 1359, 'distance': 9.410994529724121, 'force': [-2.778268337249756, -2.3256843090057373, -0.9613978266716003], 'magnitude': 3.748582124710083}, {'ion_id': 1400, 'distance': 12.003229141235352, 'force': [-0.023976322263479233, -0.33067113161087036, -2.2803401947021484], 'magnitude': 2.3043153285980225}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.938302040100098, 'force': [-3.9373409748077393, 5.4104814529418945, 0.5344047546386719], 'magnitude': 6.712790489196777}]}, 6717: {'frame': 6717, 'ionic_force': [0.5450510084629059, 4.748510509729385, -11.099060416221619], 'ionic_force_magnitude': 12.084476603716624, 'motion_vector': [-2.882415771484375, -8.947956085205078, 1.36480712890625], 'ionic_force_x': 0.5450510084629059, 'ionic_force_y': 4.748510509729385, 'ionic_force_z': -11.099060416221619, 'radial_force': 4.779689599005029, 'axial_force': -11.099060416221619, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-3.165311813354492, 1.2545452266931534, 4.686738654971123], 'asn_force_magnitude': 5.792978665728073, 'residue_force': [-3.165311813354492, 1.2545452266931534, 4.686738654971123], 'residue_force_magnitude': 5.792978665728073, 'total_force': [-2.6202608048915863, 6.003055736422539, -6.412321761250496], 'total_force_magnitude': 9.166259609571034, 'motion_component_total': -5.780837510922945, 'cosine_total_motion': -0.6306648248198022, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.07804247690003732, 'cosine_residue_motion': 0.07804247690003732, 'cosine_ionic_motion': -0.5157803783333467, 'motion_component_glu': None, 'motion_component_asn': 0.4520984037024922, 'motion_component_residue': 0.4520984037024922, 'motion_component_ionic': -6.232935914625437, 'ionic_contributions': [{'ion_id': 1327, 'distance': 8.708318710327148, 'force': [3.7785017490386963, 0.381460577249527, -2.1780126094818115], 'magnitude': 4.377936363220215}, {'ion_id': 1330, 'distance': 6.242790222167969, 'force': [8.046460151672363, -2.481989860534668, -1.290306568145752], 'magnitude': 8.518842697143555}, {'ion_id': 1341, 'distance': 10.314593315124512, 'force': [0.29557427763938904, 3.0619518756866455, -0.5244418382644653], 'magnitude': 3.1205694675445557}, {'ion_id': 1359, 'distance': 4.99979305267334, 'force': [-12.195097923278809, 2.7431704998016357, -4.48800802230835], 'magnitude': 13.281100273132324}, {'ion_id': 1400, 'distance': 10.72553825378418, 'force': [0.6196127533912659, 1.0439174175262451, -2.6182913780212402], 'magnitude': 2.886023759841919}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.271315574645996, 'force': [7.994795322418213, 0.07383163273334503, 2.9413421154022217], 'magnitude': 8.51901912689209}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.926371097564697, 'force': [-7.612933158874512, 1.7408227920532227, -2.200620412826538], 'magnitude': 8.113565444946289}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.951241970062256, 'force': [-11.73505973815918, -2.9713551998138428, -2.8970422744750977], 'magnitude': 12.447225570678711}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.602412223815918, 'force': [6.388051509857178, 1.5452309846878052, 0.238634392619133], 'magnitude': 6.5766167640686035}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.571588039398193, 'force': [3.97037410736084, 1.6553090810775757, 1.2785794734954834], 'magnitude': 4.487614631652832}, {'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.140684127807617, 'force': [-13.08947467803955, -1.4339754581451416, 4.1507415771484375], 'magnitude': 13.80649471282959}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.798559665679932, 'force': [8.45839786529541, -0.44235149025917053, -1.1783984899520874], 'magnitude': 8.55153751373291}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.1781539916992188, 'force': [25.97951889038086, -0.468379408121109, -15.410722732543945], 'magnitude': 30.210018157958984}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.068876266479492, 'force': [-12.186545372009277, 4.896431922912598, 6.804714202880859], 'magnitude': 14.791587829589844}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 2.940152645111084, 'force': [-11.332436561584473, -3.341019630432129, 10.959510803222656], 'magnitude': 16.115129470825195}]}, 6718: {'frame': 6718, 'ionic_force': [-15.74527932703495, -6.038105010986328, -8.724657155573368], 'ionic_force_magnitude': 18.986631499356328, 'motion_vector': [-0.8591651916503906, -0.15292739868164062, -0.16278839111328125], 'ionic_force_x': -15.74527932703495, 'ionic_force_y': -6.038105010986328, 'ionic_force_z': -8.724657155573368, 'radial_force': 16.863348813626917, 'axial_force': -8.724657155573368, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-1.2443006038665771, -0.7628138065338135, 0.43168115615844727], 'asn_force_magnitude': 1.5220110107366598, 'residue_force': [-1.2443006038665771, -0.7628138065338135, 0.43168115615844727], 'residue_force_magnitude': 1.5220110107366598, 'total_force': [-16.989579930901527, -6.800918817520142, -8.29297599941492], 'total_force_magnitude': 20.091584654224352, 'motion_component_total': 19.13536938782027, 'cosine_total_motion': 0.9524071752994837, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.8255662530363957, 'cosine_residue_motion': 0.8255662530363957, 'cosine_ionic_motion': 0.9416545773910651, 'motion_component_glu': None, 'motion_component_asn': 1.2565209272140017, 'motion_component_residue': 1.2565209272140017, 'motion_component_ionic': 17.878848460606267, 'ionic_contributions': [{'ion_id': 1327, 'distance': 9.429652214050293, 'force': [1.6139215230941772, -3.2655608654022217, -0.8199719190597534], 'magnitude': 3.733762741088867}, {'ion_id': 1330, 'distance': 11.5631685256958, 'force': [0.40082046389579773, -2.4494481086730957, 0.07108324021100998], 'magnitude': 2.483043670654297}, {'ion_id': 1340, 'distance': 13.527496337890625, 'force': [-0.1447393149137497, -0.5571725368499756, -1.720524549484253], 'magnitude': 1.8142755031585693}, {'ion_id': 1341, 'distance': 4.54123067855835, 'force': [-15.274748802185059, 4.401199817657471, -2.545541286468506], 'magnitude': 16.098703384399414}, {'ion_id': 1359, 'distance': 11.682413101196289, 'force': [-1.6921180486679077, -1.7458655834197998, -0.0793391764163971], 'magnitude': 2.432612895965576}, {'ion_id': 1400, 'distance': 8.67500114440918, 'force': [-0.6484151482582092, -2.421257734298706, -3.6303634643554688], 'magnitude': 4.4116291999816895}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.763683319091797, 'force': [-5.116099834442139, 3.732774019241333, 3.266111135482788], 'magnitude': 7.125697135925293}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.472349166870117, 'force': [3.8717992305755615, -4.4955878257751465, -2.834429979324341], 'magnitude': 6.575342655181885}]}, 6719: {'frame': 6719, 'ionic_force': [-13.247648186981678, -7.324256241321564, -7.235395602881908], 'ionic_force_magnitude': 16.777838403822457, 'motion_vector': [3.021942138671875, 1.1164970397949219, -1.1178054809570312], 'ionic_force_x': -13.247648186981678, 'ionic_force_y': -7.324256241321564, 'ionic_force_z': -7.235395602881908, 'radial_force': 15.13753321960275, 'axial_force': -7.235395602881908, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [1.5103087425231934, -1.504694551229477, 0.6632749438285828], 'asn_force_magnitude': 2.2327274444840945, 'residue_force': [1.5103087425231934, -1.504694551229477, 0.6632749438285828], 'residue_force_magnitude': 2.2327274444840945, 'total_force': [-11.737339444458485, -8.82895079255104, -6.572120659053326], 'total_force_magnitude': 16.09062706325904, 'motion_component_total': -11.13799453572973, 'cosine_total_motion': -0.6922038831638803, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.2814250626997317, 'cosine_residue_motion': 0.2814250626997317, 'cosine_ionic_motion': -0.7013024987834178, 'motion_component_glu': None, 'motion_component_asn': 0.628345461055348, 'motion_component_residue': 0.628345461055348, 'motion_component_ionic': -11.766339996785078, 'ionic_contributions': [{'ion_id': 1327, 'distance': 9.7034273147583, 'force': [1.420046091079712, -3.122454881668091, -0.8165378570556641], 'magnitude': 3.5260443687438965}, {'ion_id': 1330, 'distance': 11.059231758117676, 'force': [0.10633199661970139, -2.712059497833252, -0.04335900396108627], 'magnitude': 2.714489459991455}, {'ion_id': 1340, 'distance': 13.822405815124512, 'force': [-0.22071534395217896, -0.5099888443946838, -1.6464329957962036], 'magnitude': 1.737683892250061}, {'ion_id': 1341, 'distance': 5.057727336883545, 'force': [-12.584758758544922, 2.7286531925201416, -1.619233250617981], 'magnitude': 12.978583335876465}, {'ion_id': 1359, 'distance': 11.801372528076172, 'force': [-1.4268096685409546, -1.9060715436935425, -0.11701104044914246], 'magnitude': 2.383817672729492}, {'ion_id': 1400, 'distance': 9.690614700317383, 'force': [-0.5417425036430359, -1.8023346662521362, -2.992821455001831], 'magnitude': 3.535374879837036}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.772884368896484, 'force': [-5.747104644775391, 2.5360307693481445, 3.315413236618042], 'magnitude': 7.103001594543457}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.1520514488220215, 'force': [5.1302103996276855, -3.7503409385681152, -3.8271894454956055], 'magnitude': 7.41832160949707}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.895623683929443, 'force': [6.665841102600098, -0.8980498909950256, 1.0680148601531982], 'magnitude': 6.810329437255859}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.814387798309326, 'force': [-9.020288467407227, -0.31253138184547424, -0.06685638427734375], 'magnitude': 9.025948524475098}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.516042709350586, 'force': [4.481650352478027, 0.9201968908309937, 0.17389267683029175], 'magnitude': 4.578448295593262}]}, 6720: {'frame': 6720, 'ionic_force': [-13.875824749469757, -1.1168307960033417, -19.71669438481331], 'ionic_force_magnitude': 24.135738251999413, 'motion_vector': [-2.0362319946289062, -3.377918243408203, 1.4120712280273438], 'ionic_force_x': -13.875824749469757, 'ionic_force_y': -1.1168307960033417, 'ionic_force_z': -19.71669438481331, 'radial_force': 13.920697665882228, 'axial_force': -19.71669438481331, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [2.0428948402404785, -10.723928928375244, -0.9626303017139435], 'asn_force_magnitude': 10.959139021241699, 'residue_force': [2.0428948402404785, -10.723928928375244, -0.9626303017139435], 'residue_force_magnitude': 10.959139021241699, 'total_force': [-11.832929909229279, -11.840759724378586, -20.679324686527252], 'total_force_magnitude': 26.60556878884596, 'motion_component_total': 8.328538715566472, 'cosine_total_motion': 0.31303742391923994, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.6687964913835129, 'cosine_residue_motion': 0.6687964913835129, 'cosine_ionic_motion': 0.041395252929257796, 'motion_component_glu': None, 'motion_component_asn': 7.329433725990594, 'motion_component_residue': 7.329433725990594, 'motion_component_ionic': 0.9991049895758781, 'ionic_contributions': [{'ion_id': 1327, 'distance': 9.959306716918945, 'force': [1.9507142305374146, -2.5765552520751953, -0.8716263175010681], 'magnitude': 3.3471860885620117}, {'ion_id': 1330, 'distance': 11.256476402282715, 'force': [0.7414261698722839, -2.502897262573242, -0.2262757122516632], 'magnitude': 2.620192527770996}, {'ion_id': 1340, 'distance': 14.40766429901123, 'force': [0.15693143010139465, -0.3897511661052704, -1.5432026386260986], 'magnitude': 1.5993773937225342}, {'ion_id': 1341, 'distance': 3.792005777359009, 'force': [-16.80057144165039, 8.428204536437988, -13.408795356750488], 'magnitude': 23.088733673095703}, {'ion_id': 1359, 'distance': 11.166389465332031, 'force': [-0.39115285873413086, -2.5806212425231934, -0.5263550877571106], 'magnitude': 2.6626408100128174}, {'ion_id': 1400, 'distance': 9.726400375366211, 'force': [0.46682772040367126, -1.4952104091644287, -3.14043927192688], 'magnitude': 3.5094075202941895}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.581059455871582, 'force': [-12.880091667175293, 12.077126502990723, 5.382866382598877], 'magnitude': 18.458847045898438}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.8597395420074463, 'force': [11.540397644042969, -20.39795684814453, -5.520225524902344], 'magnitude': 24.07758903503418}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.488231182098389, 'force': [11.634135246276855, -9.636543273925781, -1.1138628721237183], 'magnitude': 15.14783000946045}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.795572280883789, 'force': [-3.98441219329834, 4.548394203186035, -0.36021217703819275], 'magnitude': 6.05748987197876}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.235020160675049, 'force': [-4.267134189605713, 2.6850504875183105, 0.6488038897514343], 'magnitude': 5.083195686340332}]}, 6721: {'frame': 6721, 'ionic_force': [-14.872823670506477, -15.005800008773804, -8.68900191783905], 'ionic_force_magnitude': 22.84455454075444, 'motion_vector': [-1.2706642150878906, 0.12684249877929688, -0.00298309326171875], 'ionic_force_x': -14.872823670506477, 'ionic_force_y': -15.005800008773804, 'ionic_force_z': -8.68900191783905, 'radial_force': 21.127586654355333, 'axial_force': -8.68900191783905, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [4.620800018310547, 0.4382438585162163, -1.6210395097732544], 'asn_force_magnitude': 4.916464134008489, 'residue_force': [4.620800018310547, 0.4382438585162163, -1.6210395097732544], 'residue_force_magnitude': 4.916464134008489, 'total_force': [-10.25202365219593, -14.567556150257587, -10.310041427612305], 'total_force_magnitude': 20.5819006749905, 'motion_component_total': 8.778386988970396, 'cosine_total_motion': 0.4265100258518495, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.925587579998016, 'cosine_residue_motion': -0.925587579998016, 'cosine_ionic_motion': 0.5834653113999466, 'motion_component_glu': None, 'motion_component_asn': -4.550618139943959, 'motion_component_residue': -4.550618139943959, 'motion_component_ionic': 13.329005128914353, 'ionic_contributions': [{'ion_id': 1327, 'distance': 12.513692855834961, 'force': [0.9067454934120178, -1.875288724899292, -0.39515984058380127], 'magnitude': 2.120152473449707}, {'ion_id': 1340, 'distance': 14.38318157196045, 'force': [-0.07977347075939178, -0.7151584625244141, -1.4344524145126343], 'magnitude': 1.604826807975769}, {'ion_id': 1341, 'distance': 4.348263740539551, 'force': [-14.652536392211914, -8.457913398742676, -4.700499534606934], 'magnitude': 17.55926513671875}, {'ion_id': 1359, 'distance': 12.728078842163086, 'force': [-0.839736819267273, -1.8682215213775635, -0.06597363948822021], 'magnitude': 2.0493321418762207}, {'ion_id': 1400, 'distance': 10.5826416015625, 'force': [-0.20752248167991638, -2.0892179012298584, -2.092916488647461], 'magnitude': 2.964489221572876}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.330554962158203, 'force': [-7.216357231140137, -1.9429612159729004, 3.681042432785034], 'magnitude': 8.33072566986084}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.944515228271484, 'force': [7.308725357055664, 0.10142730921506882, -3.38248872756958], 'magnitude': 8.05412769317627}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.6264729499816895, 'force': [8.688624382019043, 3.4481146335601807, -2.35097599029541], 'magnitude': 9.638919830322266}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.66384220123291, 'force': [-4.160192489624023, -1.1683368682861328, 0.43138277530670166], 'magnitude': 4.342614650726318}]}, 6722: {'frame': 6722, 'ionic_force': [-6.684693541377783, -13.338738977909088, -3.4362437948584557], 'ionic_force_magnitude': 15.310612550797314, 'motion_vector': [1.3387413024902344, 0.14303207397460938, 0.6805572509765625], 'ionic_force_x': -6.684693541377783, 'ionic_force_y': -13.338738977909088, 'ionic_force_z': -3.4362437948584557, 'radial_force': 14.920022964557695, 'axial_force': -3.4362437948584557, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [2.985116481781006, 1.4708438366651535, -3.913796901702881], 'asn_force_magnitude': 5.137325003290676, 'residue_force': [2.985116481781006, 1.4708438366651535, -3.913796901702881], 'residue_force_magnitude': 5.137325003290676, 'total_force': [-3.699577059596777, -11.867895141243935, -7.3500406965613365], 'total_force_magnitude': 14.441499359296596, 'motion_component_total': -7.724025764867186, 'cosine_total_motion': -0.5348492959558876, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.19910838163365252, 'cosine_residue_motion': 0.19910838163365252, 'cosine_ionic_motion': -0.5712972099044454, 'motion_component_glu': None, 'motion_component_asn': 1.0228844673313051, 'motion_component_residue': 1.0228844673313051, 'motion_component_ionic': -8.74691023219849, 'ionic_contributions': [{'ion_id': 1327, 'distance': 11.797014236450195, 'force': [0.81926029920578, -2.1865475177764893, -0.4886828362941742], 'magnitude': 2.3855793476104736}, {'ion_id': 1330, 'distance': 14.756539344787598, 'force': [0.03506458178162575, -1.515844464302063, 0.15978533029556274], 'magnitude': 1.5246459245681763}, {'ion_id': 1340, 'distance': 13.889774322509766, 'force': [-0.26287201046943665, -0.7818873524665833, -1.5102778673171997], 'magnitude': 1.7208685874938965}, {'ion_id': 1341, 'distance': 6.538846492767334, 'force': [-5.845895767211914, -5.08392858505249, 0.5223320126533508], 'magnitude': 7.764898777008057}, {'ion_id': 1359, 'distance': 13.870075225830078, 'force': [-0.7654677033424377, -1.5446780920028687, -0.07922738045454025], 'magnitude': 1.7257601022720337}, {'ion_id': 1400, 'distance': 10.362624168395996, 'force': [-0.6647829413414001, -2.2258529663085938, -2.040173053741455], 'magnitude': 3.0917088985443115}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.159953594207764, 'force': [6.548040390014648, -0.21510781347751617, -3.4310414791107178], 'magnitude': 7.3956170082092285}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.989753723144531, 'force': [-8.02670669555664, 2.2843375205993652, -1.6406288146972656], 'magnitude': 8.505167961120605}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.473338603973389, 'force': [4.463782787322998, -0.5983858704566956, 1.1578733921051025], 'magnitude': 4.650171279907227}]}, 6723: {'frame': 6723, 'ionic_force': [-0.5762564726173878, -13.915500342845917, 1.1806349530816078], 'ionic_force_magnitude': 13.977378874682344, 'motion_vector': [-0.162322998046875, 2.1346893310546875, 1.369384765625], 'ionic_force_x': -0.5762564726173878, 'ionic_force_y': -13.915500342845917, 'ionic_force_z': 1.1806349530816078, 'radial_force': 13.92742694520342, 'axial_force': 1.1806349530816078, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [3.501002788543701, -1.5818647742271423, -3.6147671937942505], 'asn_force_magnitude': 5.27502213783626, 'residue_force': [3.501002788543701, -1.5818647742271423, -3.6147671937942505], 'residue_force_magnitude': 5.27502213783626, 'total_force': [2.9247463159263134, -15.497365117073059, -2.4341322407126427], 'total_force_magnitude': 15.957677348213121, 'motion_component_total': -14.515935554017787, 'cosine_total_motion': -0.9096521528330829, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.663531465362386, 'cosine_residue_motion': -0.663531465362386, 'cosine_ionic_motion': -0.7881157464389487, 'motion_component_glu': None, 'motion_component_asn': -3.5001431689375195, 'motion_component_residue': -3.5001431689375195, 'motion_component_ionic': -11.015792385080267, 'ionic_contributions': [{'ion_id': 1327, 'distance': 12.17466926574707, 'force': [0.9342626333236694, -2.013418436050415, -0.30056488513946533], 'magnitude': 2.239874839782715}, {'ion_id': 1340, 'distance': 13.355932235717773, 'force': [-0.046403419226408005, -0.8943821787834167, -1.6315449476242065], 'magnitude': 1.8611855506896973}, {'ion_id': 1341, 'distance': 6.2200493812561035, 'force': [-0.5979642868041992, -6.457273483276367, 5.619952201843262], 'magnitude': 8.581247329711914}, {'ion_id': 1359, 'distance': 12.868754386901855, 'force': [-0.7437009215354919, -1.8613765239715576, 0.03603336960077286], 'magnitude': 2.004772424697876}, {'ion_id': 1400, 'distance': 9.46842098236084, 'force': [-0.12245047837495804, -2.68904972076416, -2.543240785598755], 'magnitude': 3.703249454498291}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.37502908706665, 'force': [-6.257567882537842, 0.9548014998435974, 5.202266216278076], 'magnitude': 8.193434715270996}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.700689315795898, 'force': [5.8640546798706055, -2.441789388656616, -6.249997138977051], 'magnitude': 8.911337852478027}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.788921356201172, 'force': [8.019872665405273, -1.3474538326263428, -4.095949649810791], 'magnitude': 9.105536460876465}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.518486022949219, 'force': [-4.125356674194336, 1.2525769472122192, 1.5289133787155151], 'magnitude': 4.574395179748535}]}, 6725: {'frame': 6725, 'ionic_force': [-2.6017091274261475, -10.550699710845947, -2.3864916190505028], 'ionic_force_magnitude': 11.125713326343421, 'motion_vector': [-0.458587646484375, 0.23482513427734375, -0.8922119140625], 'ionic_force_x': -2.6017091274261475, 'ionic_force_y': -10.550699710845947, 'ionic_force_z': -2.3864916190505028, 'radial_force': 10.866745362443039, 'axial_force': -2.3864916190505028, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.4782562255859375, -0.024776041507720947, 1.0505620241165161], 'asn_force_magnitude': 1.1545663411256586, 'residue_force': [0.4782562255859375, -0.024776041507720947, 1.0505620241165161], 'residue_force_magnitude': 1.1545663411256586, 'total_force': [-2.12345290184021, -10.575475752353668, -1.3359295949339867], 'total_force_magnitude': 10.86896717713208, 'motion_component_total': -0.3083282267553735, 'cosine_total_motion': -0.02836775764711896, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.9772446113062414, 'cosine_residue_motion': -0.9772446113062414, 'cosine_ionic_motion': 0.0737000392202924, 'motion_component_glu': None, 'motion_component_asn': -1.1282937352606135, 'motion_component_residue': -1.1282937352606135, 'motion_component_ionic': 0.81996550850524, 'ionic_contributions': [{'ion_id': 1327, 'distance': 11.196022987365723, 'force': [1.0887424945831299, -2.387108087539673, -0.3622821271419525], 'magnitude': 2.648564338684082}, {'ion_id': 1340, 'distance': 14.0929594039917, 'force': [-0.1545937955379486, -0.8115612268447876, -1.4531803131103516], 'magnitude': 1.671605110168457}, {'ion_id': 1341, 'distance': 8.497982025146484, 'force': [-2.5049638748168945, -3.5627336502075195, 1.4722782373428345], 'magnitude': 4.5973381996154785}, {'ion_id': 1359, 'distance': 13.108739852905273, 'force': [-0.7145503759384155, -1.7946149110794067, 0.0394371822476387], 'magnitude': 1.9320404529571533}, {'ion_id': 1400, 'distance': 10.697546005249023, 'force': [-0.3163435757160187, -1.9946818351745605, -2.082744598388672], 'magnitude': 2.9011471271514893}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.987851619720459, 'force': [-5.124249458312988, -1.1166393756866455, 4.010436534881592], 'magnitude': 6.602152347564697}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.871133327484131, 'force': [5.938694953918457, 1.965562105178833, -5.453036308288574], 'magnitude': 8.298622131347656}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.624743461608887, 'force': [-4.118346214294434, -0.09200024604797363, 1.5552843809127808], 'magnitude': 4.403197765350342}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.920444011688232, 'force': [3.7821569442749023, -0.7816985249519348, 0.9378774166107178], 'magnitude': 3.9743399620056152}]}, 6726: {'frame': 6726, 'ionic_force': [-10.6773931235075, -23.184772670269012, 0.8381237238645554], 'ionic_force_magnitude': 25.539045774313546, 'motion_vector': [1.3153266906738281, 2.5401535034179688, 0.22161865234375], 'ionic_force_x': -10.6773931235075, 'ionic_force_y': -23.184772670269012, 'ionic_force_z': 0.8381237238645554, 'radial_force': 25.525289571050475, 'axial_force': 0.8381237238645554, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [1.1686220169067383, -0.646749883890152, -0.4897400736808777], 'asn_force_magnitude': 1.4226061192333068, 'residue_force': [1.1686220169067383, -0.646749883890152, -0.4897400736808777], 'residue_force_magnitude': 1.4226061192333068, 'total_force': [-9.508771106600761, -23.831522554159164, 0.3483836501836777], 'total_force_magnitude': 25.660856696042668, 'motion_component_total': -25.431789325206566, 'cosine_total_motion': -0.991073276564791, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.05249456983615419, 'cosine_residue_motion': -0.05249456983615419, 'cosine_ionic_motion': -0.9928761807708024, 'motion_component_glu': None, 'motion_component_asn': -0.07467909627543312, 'motion_component_residue': -0.07467909627543312, 'motion_component_ionic': -25.357110228931134, 'ionic_contributions': [{'ion_id': 1327, 'distance': 11.431077003479004, 'force': [0.9742769598960876, -2.260103225708008, -0.6310176849365234], 'magnitude': 2.5407607555389404}, {'ion_id': 1330, 'distance': 12.921623229980469, 'force': [0.2411656379699707, -1.9719339609146118, -0.08398731797933578], 'magnitude': 1.988400936126709}, {'ion_id': 1340, 'distance': 14.394261360168457, 'force': [-0.16953469812870026, -0.6895309090614319, -1.4364378452301025], 'magnitude': 1.602357268333435}, {'ion_id': 1341, 'distance': 4.1642889976501465, 'force': [-10.608416557312012, -15.084050178527832, 5.144473552703857], 'magnitude': 19.145042419433594}, {'ion_id': 1359, 'distance': 14.180342674255371, 'force': [-0.709636926651001, -1.48970365524292, -0.056744806468486786], 'magnitude': 1.651066780090332}, {'ion_id': 1400, 'distance': 11.039693832397461, 'force': [-0.4052475392818451, -1.689450740814209, -2.0981621742248535], 'magnitude': 2.7241060733795166}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.976112365722656, 'force': [-5.707995414733887, -1.4798458814620972, 3.02667498588562], 'magnitude': 6.628115653991699}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.871404647827148, 'force': [6.820507049560547, 1.5041851997375488, -4.47994327545166], 'magnitude': 8.297697067260742}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.900014877319336, 'force': [-3.927506446838379, -0.4829113185405731, 0.5973057150840759], 'magnitude': 4.001910209655762}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.897857189178467, 'force': [3.983616828918457, -0.18817788362503052, 0.3662225008010864], 'magnitude': 4.004838466644287}]}, 6727: {'frame': 6727, 'ionic_force': [0.19401593878865242, -14.893805980682373, -1.1919869855046272], 'ionic_force_magnitude': 14.942688237004964, 'motion_vector': [1.3554725646972656, -0.12535858154296875, 0.22263336181640625], 'ionic_force_x': 0.19401593878865242, 'ionic_force_y': -14.893805980682373, 'ionic_force_z': -1.1919869855046272, 'radial_force': 14.895069612952941, 'axial_force': -1.1919869855046272, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [3.7730207443237305, -1.0659925937652588, -11.357152342796326], 'asn_force_magnitude': 12.014863090545129, 'residue_force': [3.7730207443237305, -1.0659925937652588, -11.357152342796326], 'residue_force_magnitude': 12.014863090545129, 'total_force': [3.967036683112383, -15.959798574447632, -12.549139328300953], 'total_force_magnitude': 20.686552358070923, 'motion_component_total': 3.323358331395372, 'cosine_total_motion': 0.16065307905687595, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.16408857017293355, 'cosine_residue_motion': 0.16408857017293355, 'cosine_ionic_motion': 0.09046943927374791, 'motion_component_glu': None, 'motion_component_asn': 1.9715017053511037, 'motion_component_residue': 1.9715017053511037, 'motion_component_ionic': 1.3518566260442677, 'ionic_contributions': [{'ion_id': 1327, 'distance': 9.895651817321777, 'force': [1.8957453966140747, -2.660691499710083, -0.9064189195632935], 'magnitude': 3.3903872966766357}, {'ion_id': 1330, 'distance': 12.571402549743652, 'force': [0.34051114320755005, -2.0693624019622803, 0.12192656844854355], 'magnitude': 2.1007320880889893}, {'ion_id': 1340, 'distance': 13.898711204528809, 'force': [-0.058663200587034225, -0.5451574325561523, -1.6288467645645142], 'magnitude': 1.7186564207077026}, {'ion_id': 1341, 'distance': 7.175320148468018, 'force': [0.5644397139549255, -4.903802871704102, 4.149296760559082], 'magnitude': 6.448452472686768}, {'ion_id': 1359, 'distance': 9.4185209274292, 'force': [-2.4074673652648926, -2.86397123336792, 0.0936751663684845], 'magnitude': 3.74259352684021}, {'ion_id': 1400, 'distance': 9.675823211669922, 'force': [-0.14054974913597107, -1.850820541381836, -3.0216197967529297], 'magnitude': 3.546191930770874}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.9024887084960938, 'force': [-12.00053882598877, 1.6600605249404907, 9.737896919250488], 'magnitude': 15.543338775634766}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.896557092666626, 'force': [</t>
+          <t>{6716: {'frame': 6716, 'motion_vector': [2.1366920471191406, 6.534908294677734, 0.9935302734375], 'ionic_force': [3.5372003354132175, 2.635218560695648, -13.300951480865479], 'ionic_force_magnitude': 14.013260625986366, 'radial_force': 4.4109140861597185, 'axial_force': -13.300951480865479, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-3.9373409748077393, 5.4104814529418945, 0.5344047546386719], 'asn_force_magnitude': 6.712790175948345, 'residue_force': [-3.9373409748077393, 5.4104814529418945, 0.5344047546386719], 'residue_force_magnitude': 6.712790175948345, 'total_force': [-0.4001406393945217, 8.045700013637543, -12.766546726226807], 'total_force_magnitude': 15.095632366803141, 'cosine_total_motion': 0.37227547594214055, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.5891865868447074, 'cosine_residue_motion': 0.5891865868447074, 'cosine_ionic_motion': 0.11879089645564639, 'motion_component_total': 5.619733723999221, 'motion_component_glu': None, 'motion_component_asn': 3.955085931971688, 'motion_component_residue': 3.955085931971688, 'motion_component_ionic': 1.6646477920275329, 'motion_component_percent_total': 37.22754759421406, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 58.918658684470735, 'motion_component_percent_residue': 58.918658684470735, 'motion_component_percent_ionic': 11.879089645564639, 'ionic_contributions': [{'ion_id': 1327, 'distance': 10.33717155456543, 'force': [1.9013433456420898, -1.8896634578704834, -1.5707390308380127], 'magnitude': 3.106952667236328, 'cosine_ionic_motion': -0.4562221169471741, 'motion_component_ionic': -1.417460560798645, 'motion_component_percent_ionic': 45.62221169471741}, {'ion_id': 1330, 'distance': 10.157370567321777, 'force': [1.3640469312667847, -2.8642194271087646, -0.5391140580177307], 'magnitude': 3.217921733856201, 'cosine_ionic_motion': -0.7308927178382874, 'motion_component_ionic': -2.3519556522369385, 'motion_component_percent_ionic': 73.08927178382874}, {'ion_id': 1341, 'distance': 5.020081996917725, 'force': [3.074054718017578, 10.045456886291504, -7.949360370635986], 'magnitude': 13.173964500427246, 'cosine_ionic_motion': 0.7027862668037415, 'motion_component_ionic': 9.2584810256958, 'motion_component_percent_ionic': 70.27862668037415}, {'ion_id': 1359, 'distance': 9.410994529724121, 'force': [-2.778268337249756, -2.3256843090057373, -0.9613978266716003], 'magnitude': 3.748582124710083, 'cosine_ionic_motion': -0.848278284072876, 'motion_component_ionic': -3.1798408031463623, 'motion_component_percent_ionic': 84.8278284072876}, {'ion_id': 1400, 'distance': 12.003229141235352, 'force': [-0.023976322263479233, -0.33067113161087036, -2.2803401947021484], 'magnitude': 2.3043153285980225, 'cosine_ionic_motion': -0.2797257900238037, 'motion_component_ionic': -0.6445764303207397, 'motion_component_percent_ionic': 27.97257900238037}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.938302040100098, 'force': [-3.9373409748077393, 5.4104814529418945, 0.5344047546386719], 'magnitude': 6.712790489196777, 'cosine_with_motion': 0.5891865491867065, 'motion_component': 3.9550859928131104, 'motion_component_percent': 58.918654918670654}]}, 6717: {'frame': 6717, 'motion_vector': [-2.882415771484375, -8.947956085205078, 1.36480712890625], 'ionic_force': [0.5450510084629059, 4.748510509729385, -11.099060416221619], 'ionic_force_magnitude': 12.084476603716624, 'radial_force': 4.779689599005029, 'axial_force': -11.099060416221619, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-3.165311813354492, 1.2545452266931534, 4.686738654971123], 'asn_force_magnitude': 5.792978665728073, 'residue_force': [-3.165311813354492, 1.2545452266931534, 4.686738654971123], 'residue_force_magnitude': 5.792978665728073, 'total_force': [-2.6202608048915863, 6.003055736422539, -6.412321761250496], 'total_force_magnitude': 9.166259609571034, 'cosine_total_motion': -0.6306648248198022, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.07804247690003732, 'cosine_residue_motion': 0.07804247690003732, 'cosine_ionic_motion': -0.5157803783333467, 'motion_component_total': -5.780837510922945, 'motion_component_glu': None, 'motion_component_asn': 0.4520984037024922, 'motion_component_residue': 0.4520984037024922, 'motion_component_ionic': -6.232935914625437, 'motion_component_percent_total': 63.06648248198022, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 7.8042476900037325, 'motion_component_percent_residue': 7.8042476900037325, 'motion_component_percent_ionic': 51.57803783333467, 'ionic_contributions': [{'ion_id': 1327, 'distance': 8.708318710327148, 'force': [3.7785017490386963, 0.381460577249527, -2.1780126094818115], 'magnitude': 4.377936363220215, 'cosine_ionic_motion': -0.41544026136398315, 'motion_component_ionic': -1.8187710046768188, 'motion_component_percent_ionic': 41.544026136398315}, {'ion_id': 1330, 'distance': 6.242790222167969, 'force': [8.046460151672363, -2.481989860534668, -1.290306568145752], 'magnitude': 8.518842697143555, 'cosine_ionic_motion': -0.033927612006664276, 'motion_component_ionic': -0.2890239953994751, 'motion_component_percent_ionic': 3.3927612006664276}, {'ion_id': 1341, 'distance': 10.314593315124512, 'force': [0.29557427763938904, 3.0619518756866455, -0.5244418382644653], 'magnitude': 3.1205694675445557, 'cosine_ionic_motion': -0.9771509170532227, 'motion_component_ionic': -3.049267292022705, 'motion_component_percent_ionic': 97.71509170532227}, {'ion_id': 1359, 'distance': 4.99979305267334, 'force': [-12.195097923278809, 2.7431704998016357, -4.48800802230835], 'magnitude': 13.281100273132324, 'cosine_ionic_motion': 0.03551255166530609, 'motion_component_ionic': 0.4716457724571228, 'motion_component_percent_ionic': 3.551255166530609}, {'ion_id': 1400, 'distance': 10.72553825378418, 'force': [0.6196127533912659, 1.0439174175262451, -2.6182913780212402], 'magnitude': 2.886023759841919, 'cosine_ionic_motion': -0.5362116694450378, 'motion_component_ionic': -1.547519564628601, 'motion_component_percent_ionic': 53.621166944503784}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.271315574645996, 'force': [7.994795322418213, 0.07383163273334503, 2.9413421154022217], 'magnitude': 8.51901912689209, 'cosine_with_motion': -0.24331967532634735, 'motion_component': -2.072844982147217, 'motion_component_percent': 24.331967532634735}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.926371097564697, 'force': [-7.612933158874512, 1.7408227920532227, -2.200620412826538], 'magnitude': 8.113565444946289, 'cosine_with_motion': 0.04363911971449852, 'motion_component': 0.3540688455104828, 'motion_component_percent': 4.363911971449852}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.951241970062256, 'force': [-11.73505973815918, -2.9713551998138428, -2.8970422744750977], 'magnitude': 12.447225570678711, 'cosine_with_motion': 0.47749435901641846, 'motion_component': 5.943480014801025, 'motion_component_percent': 47.749435901641846}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.602412223815918, 'force': [6.388051509857178, 1.5452309846878052, 0.238634392619133], 'magnitude': 6.5766167640686035, 'cosine_with_motion': -0.5108417868614197, 'motion_component': -3.3596105575561523, 'motion_component_percent': 51.08417868614197}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.571588039398193, 'force': [3.97037410736084, 1.6553090810775757, 1.2785794734954834], 'magnitude': 4.487614631652832, 'cosine_with_motion': -0.5749781131744385, 'motion_component': -2.580280303955078, 'motion_component_percent': 57.49781131744385}, {'resid': 455, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 4.140684127807617, 'force': [-13.08947467803955, -1.4339754581451416, 4.1507415771484375], 'magnitude': 13.80649471282959, 'cosine_with_motion': 0.42870357632637024, 'motion_component': 5.918893814086914, 'motion_component_percent': 42.870357632637024}, {'resid': 455, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.798559665679932, 'force': [8.45839786529541, -0.44235149025917053, -1.1783984899520874], 'magnitude': 8.55153751373291, 'cosine_with_motion': -0.2712022066116333, 'motion_component': -2.3191957473754883, 'motion_component_percent': 27.12022066116333}, {'resid': 455, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 3.1781539916992188, 'force': [25.97951889038086, -0.468379408121109, -15.410722732543945], 'magnitude': 30.210018157958984, 'cosine_with_motion': -0.3196292221546173, 'motion_component': -9.656004905700684, 'motion_component_percent': 31.96292221546173}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 3.068876266479492, 'force': [-12.186545372009277, 4.896431922912598, 6.804714202880859], 'magnitude': 14.791587829589844, 'cosine_with_motion': 0.004275555722415447, 'motion_component': 0.06324225664138794, 'motion_component_percent': 0.4275555722415447}, {'resid': 455, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 2.940152645111084, 'force': [-11.332436561584473, -3.341019630432129, 10.959510803222656], 'magnitude': 16.115129470825195, 'cosine_with_motion': 0.506378173828125, 'motion_component': 8.16034984588623, 'motion_component_percent': 50.6378173828125}]}, 6718: {'frame': 6718, 'motion_vector': [-0.8591651916503906, -0.15292739868164062, -0.16278839111328125], 'ionic_force': [-15.74527932703495, -6.038105010986328, -8.724657155573368], 'ionic_force_magnitude': 18.986631499356328, 'radial_force': 16.863348813626917, 'axial_force': -8.724657155573368, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-1.2443006038665771, -0.7628138065338135, 0.43168115615844727], 'asn_force_magnitude': 1.5220110107366598, 'residue_force': [-1.2443006038665771, -0.7628138065338135, 0.43168115615844727], 'residue_force_magnitude': 1.5220110107366598, 'total_force': [-16.989579930901527, -6.800918817520142, -8.29297599941492], 'total_force_magnitude': 20.091584654224352, 'cosine_total_motion': 0.9524071752994837, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.8255662530363957, 'cosine_residue_motion': 0.8255662530363957, 'cosine_ionic_motion': 0.9416545773910651, 'motion_component_total': 19.13536938782027, 'motion_component_glu': None, 'motion_component_asn': 1.2565209272140017, 'motion_component_residue': 1.2565209272140017, 'motion_component_ionic': 17.878848460606267, 'motion_component_percent_total': 95.24071752994837, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 82.55662530363958, 'motion_component_percent_residue': 82.55662530363958, 'motion_component_percent_ionic': 94.1654577391065, 'ionic_contributions': [{'ion_id': 1327, 'distance': 9.429652214050293, 'force': [1.6139215230941772, -3.2655608654022217, -0.8199719190597534], 'magnitude': 3.733762741088867, 'cosine_ionic_motion': -0.2274065613746643, 'motion_component_ionic': -0.8490821719169617, 'motion_component_percent_ionic': 22.74065613746643}, {'ion_id': 1330, 'distance': 11.5631685256958, 'force': [0.40082046389579773, -2.4494481086730957, 0.07108324021100998], 'magnitude': 2.483043670654297, 'cosine_ionic_motion': 0.008458750322461128, 'motion_component_ionic': 0.021003445610404015, 'motion_component_percent_ionic': 0.8458750322461128}, {'ion_id': 1340, 'distance': 13.527496337890625, 'force': [-0.1447393149137497, -0.5571725368499756, -1.720524549484253], 'magnitude': 1.8142755031585693, 'cosine_ionic_motion': 0.3040179908275604, 'motion_component_ionic': 0.5515723824501038, 'motion_component_percent_ionic': 30.401799082756042}, {'ion_id': 1341, 'distance': 4.54123067855835, 'force': [-15.274748802185059, 4.401199817657471, -2.545541286468506], 'magnitude': 16.098703384399414, 'cosine_ionic_motion': 0.9001949429512024, 'motion_component_ionic': 14.491971015930176, 'motion_component_percent_ionic': 90.01949429512024}, {'ion_id': 1359, 'distance': 11.682413101196289, 'force': [-1.6921180486679077, -1.7458655834197998, -0.0793391764163971], 'magnitude': 2.432612895965576, 'cosine_ionic_motion': 0.8028370141983032, 'motion_component_ionic': 1.9529916048049927, 'motion_component_percent_ionic': 80.28370141983032}, {'ion_id': 1400, 'distance': 8.67500114440918, 'force': [-0.6484151482582092, -2.421257734298706, -3.6303634643554688], 'magnitude': 4.4116291999816895, 'cosine_ionic_motion': 0.387700617313385, 'motion_component_ionic': 1.7103914022445679, 'motion_component_percent_ionic': 38.7700617313385}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.763683319091797, 'force': [-5.116099834442139, 3.732774019241333, 3.266111135482788], 'magnitude': 7.125697135925293, 'cosine_with_motion': 0.5205867886543274, 'motion_component': 3.7095437049865723, 'motion_component_percent': 52.05867886543274}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.472349166870117, 'force': [3.8717992305755615, -4.4955878257751465, -2.834429979324341], 'magnitude': 6.575342655181885, 'cosine_with_motion': -0.3730638921260834, 'motion_component': -2.4530229568481445, 'motion_component_percent': 37.30638921260834}]}, 6719: {'frame': 6719, 'motion_vector': [3.021942138671875, 1.1164970397949219, -1.1178054809570312], 'ionic_force': [-13.247648186981678, -7.324256241321564, -7.235395602881908], 'ionic_force_magnitude': 16.777838403822457, 'radial_force': 15.13753321960275, 'axial_force': -7.235395602881908, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [1.5103087425231934, -1.504694551229477, 0.6632749438285828], 'asn_force_magnitude': 2.2327274444840945, 'residue_force': [1.5103087425231934, -1.504694551229477, 0.6632749438285828], 'residue_force_magnitude': 2.2327274444840945, 'total_force': [-11.737339444458485, -8.82895079255104, -6.572120659053326], 'total_force_magnitude': 16.09062706325904, 'cosine_total_motion': -0.6922038831638803, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.2814250626997317, 'cosine_residue_motion': 0.2814250626997317, 'cosine_ionic_motion': -0.7013024987834178, 'motion_component_total': -11.13799453572973, 'motion_component_glu': None, 'motion_component_asn': 0.628345461055348, 'motion_component_residue': 0.628345461055348, 'motion_component_ionic': -11.766339996785078, 'motion_component_percent_total': 69.22038831638802, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 28.142506269973172, 'motion_component_percent_residue': 28.142506269973172, 'motion_component_percent_ionic': 70.13024987834177, 'ionic_contributions': [{'ion_id': 1327, 'distance': 9.7034273147583, 'force': [1.420046091079712, -3.122454881668091, -0.8165378570556641], 'magnitude': 3.5260443687438965, 'cosine_ionic_motion': 0.1428672969341278, 'motion_component_ionic': 0.5037564039230347, 'motion_component_percent_ionic': 14.28672969341278}, {'ion_id': 1330, 'distance': 11.059231758117676, 'force': [0.10633199661970139, -2.712059497833252, -0.04335900396108627], 'magnitude': 2.714489459991455, 'cosine_ionic_motion': -0.2871740460395813, 'motion_component_ionic': -0.7795308828353882, 'motion_component_percent_ionic': 28.71740460395813}, {'ion_id': 1340, 'distance': 13.822405815124512, 'force': [-0.22071534395217896, -0.5099888443946838, -1.6464329957962036], 'magnitude': 1.737683892250061, 'cosine_ionic_motion': 0.10193220525979996, 'motion_component_ionic': 0.177125945687294, 'motion_component_percent_ionic': 10.193220525979996}, {'ion_id': 1341, 'distance': 5.057727336883545, 'force': [-12.584758758544922, 2.7286531925201416, -1.619233250617981], 'magnitude': 12.978583335876465, 'cosine_ionic_motion': -0.7495715618133545, 'motion_component_ionic': -9.728377342224121, 'motion_component_percent_ionic': 74.95715618133545}, {'ion_id': 1359, 'distance': 11.801372528076172, 'force': [-1.4268096685409546, -1.9060715436935425, -0.11701104044914246], 'magnitude': 2.383817672729492, 'cosine_ionic_motion': -0.7761324644088745, 'motion_component_ionic': -1.8501583337783813, 'motion_component_percent_ionic': 77.61324644088745}, {'ion_id': 1400, 'distance': 9.690614700317383, 'force': [-0.5417425036430359, -1.8023346662521362, -2.992821455001831], 'magnitude': 3.535374879837036, 'cosine_ionic_motion': -0.025218309834599495, 'motion_component_ionic': -0.08915618062019348, 'motion_component_percent_ionic': 2.5218309834599495}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.772884368896484, 'force': [-5.747104644775391, 2.5360307693481445, 3.315413236618042], 'magnitude': 7.103001594543457, 'cosine_with_motion': -0.7531351447105408, 'motion_component': -5.349520206451416, 'motion_component_percent': 75.31351447105408}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.1520514488220215, 'force': [5.1302103996276855, -3.7503409385681152, -3.8271894454956055], 'magnitude': 7.41832160949707, 'cosine_with_motion': 0.616447389125824, 'motion_component': 4.573005199432373, 'motion_component_percent': 61.6447389125824}, {'resid': 1105, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.895623683929443, 'force': [6.665841102600098, -0.8980498909950256, 1.0680148601531982], 'magnitude': 6.810329437255859, 'cosine_with_motion': 0.7728132605552673, 'motion_component': 5.263113021850586, 'motion_component_percent': 77.28132605552673}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.814387798309326, 'force': [-9.020288467407227, -0.31253138184547424, -0.06685638427734375], 'magnitude': 9.025948524475098, 'cosine_with_motion': -0.8945500254631042, 'motion_component': -8.074162483215332, 'motion_component_percent': 89.45500254631042}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.516042709350586, 'force': [4.481650352478027, 0.9201968908309937, 0.17389267683029175], 'magnitude': 4.578448295593262, 'cosine_with_motion': 0.9208163022994995, 'motion_component': 4.215909957885742, 'motion_component_percent': 92.08163022994995}]}, 6720: {'frame': 6720, 'motion_vector': [-2.0362319946289062, -3.377918243408203, 1.4120712280273438], 'ionic_force': [-13.875824749469757, -1.1168307960033417, -19.71669438481331], 'ionic_force_magnitude': 24.135738251999413, 'radial_force': 13.920697665882228, 'axial_force': -19.71669438481331, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [2.0428948402404785, -10.723928928375244, -0.9626303017139435], 'asn_force_magnitude': 10.959139021241699, 'residue_force': [2.0428948402404785, -10.723928928375244, -0.9626303017139435], 'residue_force_magnitude': 10.959139021241699, 'total_force': [-11.832929909229279, -11.840759724378586, -20.679324686527252], 'total_force_magnitude': 26.60556878884596, 'cosine_total_motion': 0.31303742391923994, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.6687964913835129, 'cosine_residue_motion': 0.6687964913835129, 'cosine_ionic_motion': 0.041395252929257796, 'motion_component_total': 8.328538715566472, 'motion_component_glu': None, 'motion_component_asn': 7.329433725990594, 'motion_component_residue': 7.329433725990594, 'motion_component_ionic': 0.9991049895758781, 'motion_component_percent_total': 31.303742391923993, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 66.8796491383513, 'motion_component_percent_residue': 66.8796491383513, 'motion_component_percent_ionic': 4.1395252929257795, 'ionic_contributions': [{'ion_id': 1327, 'distance': 9.959306716918945, 'force': [1.9507142305374146, -2.5765552520751953, -0.8716263175010681], 'magnitude': 3.3471860885620117, 'cosine_ionic_motion': 0.2496340274810791, 'motion_component_ionic': 0.8355715274810791, 'motion_component_percent_ionic': 24.96340274810791}, {'ion_id': 1330, 'distance': 11.256476402282715, 'force': [0.7414261698722839, -2.502897262573242, -0.2262757122516632], 'magnitude': 2.620192527770996, 'cosine_ionic_motion': 0.6035741567611694, 'motion_component_ionic': 1.5814805030822754, 'motion_component_percent_ionic': 60.35741567611694}, {'ion_id': 1340, 'distance': 14.40766429901123, 'force': [0.15693143010139465, -0.3897511661052704, -1.5432026386260986], 'magnitude': 1.5993773937225342, 'cosine_ionic_motion': -0.1764262169599533, 'motion_component_ionic': -0.2821721136569977, 'motion_component_percent_ionic': 17.64262169599533}, {'ion_id': 1341, 'distance': 3.792005777359009, 'force': [-16.80057144165039, 8.428204536437988, -13.408795356750488], 'magnitude': 23.088733673095703, 'cosine_ionic_motion': -0.13640636205673218, 'motion_component_ionic': -3.1494503021240234, 'motion_component_percent_ionic': 13.640636205673218}, {'ion_id': 1359, 'distance': 11.166389465332031, 'force': [-0.39115285873413086, -2.5806212425231934, -0.5263550877571106], 'magnitude': 2.6626408100128174, 'cosine_ionic_motion': 0.7862480282783508, 'motion_component_ionic': 2.093496084213257, 'motion_component_percent_ionic': 78.62480282783508}, {'ion_id': 1400, 'distance': 9.726400375366211, 'force': [0.46682772040367126, -1.4952104091644287, -3.14043927192688], 'magnitude': 3.5094075202941895, 'cosine_ionic_motion': -0.02274474687874317, 'motion_component_ionic': -0.07982058823108673, 'motion_component_percent_ionic': 2.274474687874317}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 3.581059455871582, 'force': [-12.880091667175293, 12.077126502990723, 5.382866382598877], 'magnitude': 18.458847045898438, 'cosine_with_motion': -0.09010312706232071, 'motion_component': -1.663199782371521, 'motion_component_percent': 9.010312706232071}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 2.8597395420074463, 'force': [11.540397644042969, -20.39795684814453, -5.520225524902344], 'magnitude': 24.07758903503418, 'cosine_with_motion': 0.3728472888469696, 'motion_component': 8.977263450622559, 'motion_component_percent': 37.28472888469696}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 4.488231182098389, 'force': [11.634135246276855, -9.636543273925781, -1.1138628721237183], 'magnitude': 15.14783000946045, 'cosine_with_motion': 0.11485788226127625, 'motion_component': 1.7398476600646973, 'motion_component_percent': 11.485788226127625}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 4.795572280883789, 'force': [-3.98441219329834, 4.548394203186035, -0.36021217703819275], 'magnitude': 6.05748987197876, 'cosine_with_motion': -0.30577322840690613, 'motion_component': -1.8522182703018188, 'motion_component_percent': 30.577322840690613}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.235020160675049, 'force': [-4.267134189605713, 2.6850504875183105, 0.6488038897514343], 'magnitude': 5.083195686340332, 'cosine_with_motion': 0.02513018250465393, 'motion_component': 0.12774163484573364, 'motion_component_percent': 2.513018250465393}]}, 6721: {'frame': 6721, 'motion_vector': [-1.2706642150878906, 0.12684249877929688, -0.00298309326171875], 'ionic_force': [-14.872823670506477, -15.005800008773804, -8.68900191783905], 'ionic_force_magnitude': 22.84455454075444, 'radial_force': 21.127586654355333, 'axial_force': -8.68900191783905, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [4.620800018310547, 0.4382438585162163, -1.6210395097732544], 'asn_force_magnitude': 4.916464134008489, 'residue_force': [4.620800018310547, 0.4382438585162163, -1.6210395097732544], 'residue_force_magnitude': 4.916464134008489, 'total_force': [-10.25202365219593, -14.567556150257587, -10.310041427612305], 'total_force_magnitude': 20.5819006749905, 'cosine_total_motion': 0.4265100258518495, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.925587579998016, 'cosine_residue_motion': -0.925587579998016, 'cosine_ionic_motion': 0.5834653113999466, 'motion_component_total': 8.778386988970396, 'motion_component_glu': None, 'motion_component_asn': -4.550618139943959, 'motion_component_residue': -4.550618139943959, 'motion_component_ionic': 13.329005128914353, 'motion_component_percent_total': 42.65100258518495, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 92.5587579998016, 'motion_component_percent_residue': 92.5587579998016, 'motion_component_percent_ionic': 58.34653113999466, 'ionic_contributions': [{'ion_id': 1327, 'distance': 12.513692855834961, 'force': [0.9067454934120178, -1.875288724899292, -0.39515984058380127], 'magnitude': 2.120152473449707, 'cosine_ionic_motion': -0.5129857063293457, 'motion_component_ionic': -1.0876078605651855, 'motion_component_percent_ionic': 51.29857063293457}, {'ion_id': 1340, 'distance': 14.38318157196045, 'force': [-0.07977347075939178, -0.7151584625244141, -1.4344524145126343], 'magnitude': 1.604826807975769, 'cosine_ionic_motion': 0.007286217994987965, 'motion_component_ionic': 0.011693118140101433, 'motion_component_percent_ionic': 0.7286217994987965}, {'ion_id': 1341, 'distance': 4.348263740539551, 'force': [-14.652536392211914, -8.457913398742676, -4.700499534606934], 'magnitude': 17.55926513671875, 'cosine_ionic_motion': 0.7831131219863892, 'motion_component_ionic': 13.750890731811523, 'motion_component_percent_ionic': 78.31131219863892}, {'ion_id': 1359, 'distance': 12.728078842163086, 'force': [-0.839736819267273, -1.8682215213775635, -0.06597363948822021], 'magnitude': 2.0493321418762207, 'cosine_ionic_motion': 0.3172573149204254, 'motion_component_ionic': 0.6501656174659729, 'motion_component_percent_ionic': 31.72573149204254}, {'ion_id': 1400, 'distance': 10.5826416015625, 'force': [-0.20752248167991638, -2.0892179012298584, -2.092916488647461], 'magnitude': 2.964489221572876, 'cosine_ionic_motion': 0.0013031262205913663, 'motion_component_ionic': 0.003863103687763214, 'motion_component_percent_ionic': 0.13031262205913663}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.713, 'distance': 5.330554962158203, 'force': [-7.216357231140137, -1.9429612159729004, 3.681042432785034], 'magnitude': 8.33072566986084, 'cosine_with_motion': 0.8377489447593689, 'motion_component': 6.9790568351745605, 'motion_component_percent': 83.77489447593689}, {'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 4.944515228271484, 'force': [7.308725357055664, 0.10142730921506882, -3.38248872756958], 'magnitude': 8.05412769317627, 'cosine_with_motion': -0.9007287621498108, 'motion_component': -7.254584312438965, 'motion_component_percent': 90.07287621498108}, {'resid': 780, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.6264729499816895, 'force': [8.688624382019043, 3.4481146335601807, -2.35097599029541], 'magnitude': 9.638919830322266, 'cosine_with_motion': -0.8608473539352417, 'motion_component': -8.297638893127441, 'motion_component_percent': 86.08473539352417}, {'resid': 780, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.4196, 'distance': 5.66384220123291, 'force': [-4.160192489624023, -1.1683368682861328, 0.43138277530670166], 'magnitude': 4.342614650726318, 'cosine_with_motion': 0.926296591758728, 'motion_component': 4.022549152374268, 'motion_component_percent': 92.6296591758728}]}, 6722: {'frame': 6722, 'motion_vector': [1.3387413024902344, 0.14303207397460938, 0.6805572509765625], 'ionic_force': [-6.684693541377783, -13.338738977909088, -3.4362437948584557], 'ionic_force_magnitude': 15.310612550797314, 'radial_force': 14.920022964557695, 'axial_force': -3.4362437948584557, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [2.985116481781006, 1.4708438366651535, -3.913796901702881], 'asn_force_magnitude': 5.137325003290676, 'residue_force': [2.985116481781006, 1.4708438366651535, -3.913796901702881], 'residue_force_magnitude': 5.137325003290676, 'total_force': [-3.699577059596777, -11.867895141243935, -7.3500406965613365], 'total_force_magnitude': 14.441499359296596, 'cosine_total_motion': -0.5348492959558876, 'cosine_glu_motion': None, 'cosine_asn_motion': 0.19910838163365252, 'cosine_residue_motion': 0.19910838163365252, 'cosine_ionic_motion': -0.5712972099044454, 'motion_component_total': -7.724025764867186, 'motion_component_glu': None, 'motion_component_asn': 1.0228844673313051, 'motion_component_residue': 1.0228844673313051, 'motion_component_ionic': -8.74691023219849, 'motion_component_percent_total': 53.48492959558876, 'motion_component_percent_glu': None, 'motion_component_percent_asn': 19.910838163365252, 'motion_component_percent_residue': 19.910838163365252, 'motion_component_percent_ionic': 57.12972099044455, 'ionic_contributions': [{'ion_id': 1327, 'distance': 11.797014236450195, 'force': [0.81926029920578, -2.1865475177764893, -0.4886828362941742], 'magnitude': 2.3855793476104736, 'cosine_ionic_motion': 0.125443696975708, 'motion_component_ionic': 0.2992558777332306, 'motion_component_percent_ionic': 12.5443696975708}, {'ion_id': 1330, 'distance': 14.756539344787598, 'force': [0.03506458178162575, -1.515844464302063, 0.15978533029556274], 'magnitude': 1.5246459245681763, 'cosine_ionic_motion': -0.026577014476060867, 'motion_component_ionic': -0.04052053764462471, 'motion_component_percent_ionic': 2.6577014476060867}, {'ion_id': 1340, 'distance': 13.889774322509766, 'force': [-0.26287201046943665, -0.7818873524665833, -1.5102778673171997], 'magnitude': 1.7208685874938965, 'cosine_ionic_motion': -0.5745508670806885, 'motion_component_ionic': -0.9887264966964722, 'motion_component_percent_ionic': 57.45508670806885}, {'ion_id': 1341, 'distance': 6.538846492767334, 'force': [-5.845895767211914, -5.08392858505249, 0.5223320126533508], 'magnitude': 7.764898777008057, 'cosine_ionic_motion': -0.6998288035392761, 'motion_component_ionic': -5.4340996742248535, 'motion_component_percent_ionic': 69.98288035392761}, {'ion_id': 1359, 'distance': 13.870075225830078, 'force': [-0.7654677033424377, -1.5446780920028687, -0.07922738045454025], 'magnitude': 1.7257601022720337, 'cosine_ionic_motion': -0.4991888105869293, 'motion_component_ionic': -0.8614801168441772, 'motion_component_percent_ionic': 49.91888105869293}, {'ion_id': 1400, 'distance': 10.362624168395996, 'force': [-0.6647829413414001, -2.2258529663085938, -2.040173053741455], 'magnitude': 3.0917088985443115, 'cosine_ionic_motion': -0.556759774684906, 'motion_component_ionic': -1.7213391065597534, 'motion_component_percent_ionic': 55.6759774684906}], 'glu_contributions': [], 'asn_contributions': [{'resid': 780, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.5931, 'distance': 5.159953594207764, 'force': [6.548040390014648, -0.21510781347751617, -3.4310414791107178], 'magnitude': 7.3956170082092285, 'cosine_with_motion': 0.5736640095710754, 'motion_component': 4.2425994873046875, 'motion_component_percent': 57.366400957107544}, {'resid': 1105, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9191, 'distance': 5.989753723144531, 'force': [-8.02670669555664, 2.2843375205993652, -1.6406288146972656], 'magnitude': 8.505167961120605, 'cosine_with_motion': -0.899046003818512, 'motion_component': -7.6465373039245605, 'motion_component_percent': 89.9046003818512}, {'resid': 1105, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4196, 'distance': 5.473338603973389, 'force': [4.463782787322998, -0.5983858704566956, 1.1578733921051025], 'magnitude': 4.650171279907227, 'cosine_with_motion': 0.9519698023796082, 'motion_component': 4.426822662353516, 'motion_component_percent': 95.19698023796082}]}, 6723: {'frame': 6723, 'motion_vector': [-0.162322998046875, 2.1346893310546875, 1.369384765625], 'ionic_force': [-0.5762564726173878, -13.915500342845917, 1.1806349530816078], 'ionic_force_magnitude': 13.977378874682344, 'radial_force': 13.92742694520342, 'axial_force': 1.1806349530816078, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [3.501002788543701, -1.5818647742271423, -3.6147671937942505], 'asn_force_magnitude': 5.27502213783626, 'residue_force': [3.501002788543701, -1.5818647742271423, -3.6147671937942505], 'residue_force_magnitude': 5.27502213783626, 'total_force': [2.9247463159263134, -15.497365117073059, -2.4341322407126427], 'total_force_magnitude': 15.957677348213121, 'cosine_total_motion': -0.9096521528330829, 'cosine_glu_motion': None, 'cosine_asn_motion': -0.663531465362386, 'cosine_residue_motion': -0.663531465362386, 'cosine_ionic_motion': -0.7881157464389487, 'motion_component_total': -14.515935554017787, 'motion_componen</t>
         </is>
       </c>
     </row>

</xml_diff>